<commit_message>
Updated testing data for 2020-06-11
</commit_message>
<xml_diff>
--- a/public/data/testing/covid-testing-latest-data-source-details.xlsx
+++ b/public/data/testing/covid-testing-latest-data-source-details.xlsx
@@ -585,13 +585,13 @@
     <t xml:space="preserve">France - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.santepubliquefrance.fr/content/download/257630/2628879</t>
+    <t xml:space="preserve">https://www.santepubliquefrance.fr/content/download/259223/2638086</t>
   </si>
   <si>
     <t xml:space="preserve">National Public Health Agency</t>
   </si>
   <si>
-    <t xml:space="preserve">Dividing 236,098 (weekly total) by 7</t>
+    <t xml:space="preserve">Dividing 194,099 (weekly total) by 7</t>
   </si>
   <si>
     <t xml:space="preserve">https://www.santepubliquefrance.fr/recherche/#search=COVID-19%20:%20point%20epidemiologique&amp;sort=dat</t>
@@ -3621,7 +3621,7 @@
         <v>174</v>
       </c>
       <c r="C25" s="1" t="n">
-        <v>43981</v>
+        <v>43988</v>
       </c>
       <c r="D25" t="s">
         <v>175</v>
@@ -3633,21 +3633,21 @@
         <v>177</v>
       </c>
       <c r="G25" t="n">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="H25"/>
       <c r="I25"/>
       <c r="J25" t="n">
-        <v>33728</v>
+        <v>27728</v>
       </c>
       <c r="K25" t="n">
-        <v>0.517</v>
+        <v>0.425</v>
       </c>
       <c r="L25" t="n">
-        <v>33728</v>
+        <v>27728</v>
       </c>
       <c r="M25" t="n">
-        <v>0.517</v>
+        <v>0.425</v>
       </c>
       <c r="N25" t="s">
         <v>176</v>

</xml_diff>

<commit_message>
Updated testing data for 2020-06-12
</commit_message>
<xml_diff>
--- a/public/data/testing/covid-testing-latest-data-source-details.xlsx
+++ b/public/data/testing/covid-testing-latest-data-source-details.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="609" uniqueCount="609">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="611" uniqueCount="611">
   <si>
     <t xml:space="preserve">ISO code</t>
   </si>
@@ -71,7 +71,7 @@
     <t xml:space="preserve">Argentina - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.argentina.gob.ar/sites/default/files/10-06-20_reporte-matutino-covid-19.pdf</t>
+    <t xml:space="preserve">https://www.argentina.gob.ar/sites/default/files/11-06-20_reporte_matutino_covid_19.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">Government of Argentina</t>
@@ -139,7 +139,7 @@
     <t xml:space="preserve">Bahrain - units unclear</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200611180616/https://www.moh.gov.bh/COVID19</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200612073353/https://www.moh.gov.bh/COVID19</t>
   </si>
   <si>
     <t xml:space="preserve">Ministry of Health</t>
@@ -280,7 +280,7 @@
     <t xml:space="preserve">Bulgaria - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200611180630/https://coronavirus.bg/</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200612073357/https://coronavirus.bg/</t>
   </si>
   <si>
     <t xml:space="preserve">Bulgaria COVID-10 Information Portal</t>
@@ -303,7 +303,7 @@
     <t xml:space="preserve">Canada - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200611180634/https://www.canada.ca/en/public-health/services/diseases/2019-novel-coronavirus-infection.html</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200612073358/https://www.canada.ca/en/public-health/services/diseases/2019-novel-coronavirus-infection.html</t>
   </si>
   <si>
     <t xml:space="preserve">Government of Canada</t>
@@ -639,7 +639,7 @@
     <t xml:space="preserve">To determine how many laboratory tests regarding SARS-CoV-2 are carried out per calendar week in Germany and how many tests are positive or negative, the RKI has started a Germany-wide laboratory query. However, the number of laboratories reporting data seems to vary from week to week.
 The report published on 27 May states that “from the beginning of the collection up to and including calendar week 22/2020”:
 – The cumulative total of samples tested was 4,348,880;
-- For calendar week 22 (which ends 31May), 169 labs reported 392,437 samples tested;
+- For calendar week 22 (which ends 31 May), 169 labs reported 392,437 samples tested;
 - For calendar week 21( which ends 24 May), 174 labs reported 346,470 samples tested;
 - For calendar week 20 (which ends 17 May), 182 labs reported 432,666 samples tested;
 - For calendar week 19 (which ends 10 May), 182 labs reported 403,875 samples tested;
@@ -933,7 +933,7 @@
     <t xml:space="preserve">Japan - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.mhlw.go.jp/stf/newpage_11796.html</t>
+    <t xml:space="preserve">https://www.mhlw.go.jp/stf/newpage_11820.html</t>
   </si>
   <si>
     <t xml:space="preserve">Ministry of Health, Labor and Welfare Press Release</t>
@@ -957,10 +957,10 @@
     <t xml:space="preserve">Japan - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.mhlw.go.jp/content/10906000/000638697.pdf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The cumulative total reported in the press release (533,747) does not sum to the cumulative total calculated from the weekly and daily figures reported by the MOH. See: https://www.mhlw.go.jp/content/10906000/000638697.pdf</t>
+    <t xml:space="preserve">https://www.mhlw.go.jp/content/10906000/000638974.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The cumulative total reported in the press release (540,823) does not sum to the cumulative total calculated from the weekly and daily figures reported by the MOH. See: https://www.mhlw.go.jp/content/10906000/000638974.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">On 11th April 2020, the MOH started providing a daily time series on the "Implementation status of PCR tests for new coronavirus in Japan (based on the date on which results were determined" (via Google translate). 
@@ -1033,7 +1033,7 @@
     <t xml:space="preserve">Lithuania - samples tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200611181044/http://sam.lrv.lt/lt/naujienos/koronavirusas</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200612073946/http://sam.lrv.lt/lt/naujienos/koronavirusas</t>
   </si>
   <si>
     <t xml:space="preserve">http://sam.lrv.lt/lt/naujienos/koronavirusas</t>
@@ -1070,13 +1070,13 @@
     <t xml:space="preserve">Malaysia - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.facebook.com/373560576236/videos/3043580832395340</t>
+    <t xml:space="preserve">https://www.facebook.com/kementeriankesihatanmalaysia/videos/270663217507305</t>
   </si>
   <si>
     <t xml:space="preserve">Ministry of Health Malaysia</t>
   </si>
   <si>
-    <t xml:space="preserve">Statistics on testing can be see at 27:22 timestamp on the MOH livestream</t>
+    <t xml:space="preserve">Statistics on testing can be see at 18:21 timestamp on the MOH livestream</t>
   </si>
   <si>
     <t xml:space="preserve">http://covid-19.moh.gov.my/terkini</t>
@@ -1126,10 +1126,16 @@
     <t xml:space="preserve">Health Secretary</t>
   </si>
   <si>
-    <t xml:space="preserve">The Mexican Health Secretary publishes a dataset on [datos.gob.mx](https://datos.gob.mx/busca/dataset/informacion-referente-a-casos-covid-19-en-mexico), the open data platform of the Mexican government.
-The file can be downloaded in CSV format, and gives detailed information on each case (1 row per case). The RESULTADO column gives the status of the case, with 1 = CONFIRMED and 2 = NEGATIVE. The resulting tally can also be found on the [government's COVID-19 dashboard](https://coronavirus.gob.mx/datos/). We do not include pending tests (RESULTADO = 3).
-While geographical coverage is complete, there is a time lag in the publication of the data, and recent days systematically show temporary low figures. Data starts on 1 January 2020; we do not know if this is because tests started on that date or because earlier data is not available.
-The notes to the data provide the following note "Information from the Epidemiological Surveillance System for Viral Respiratory Diseases, reported by the 475 viral respiratory disease monitoring units (USMER) throughout the country in the entire health sector (IMSS, ISSSTE, SEDENA, SEMAR, ETC).... Preliminary data subject to validation by the Ministry of Health through the General Directorate of Epidemiology. The information contained corresponds only to the data obtained from the epidemiological study of a suspected case of viral respiratory disease at the time it is identified in the medical units of the Health Sector". (via Google translate)</t>
+    <t xml:space="preserve">Government of Mexico</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://coronavirus.gob.mx/datos/#DownZCSV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Government of Mexico makes a dataset available along with [its COVID-19 dashboard](https://coronavirus.gob.mx/datos/#DownZCSV).
+The file can be downloaded in CSV format, and gives detailed information on each case (1 row per case). The RESULTADO column gives the status of the case, with 1 = CONFIRMED and 2 = NEGATIVE. The resulting tally can be found [on the dashboard](https://coronavirus.gob.mx/datos/). We do not include pending tests (RESULTADO = 3).
+While geographical coverage is complete, there is a time lag in the publication of the data, and recent days systematically show temporarily low figures. Data starts on 1 January 2020; we do not know if this is because tests started on that date or because earlier data is not available.
+The notes to the data provide the following note "Information from the Epidemiological Surveillance System for Viral Respiratory Diseases, reported by the 475 viral respiratory disease monitoring units (USMER) throughout the country in the entire health sector (IMSS, ISSSTE, SEDENA, SEMAR, ETC).... Preliminary data subject to validation by the Ministry of Health through the General Directorate of Epidemiology. The information contained corresponds only to the data obtained from the epidemiological study of a suspected case of viral respiratory disease at the time it is identified in the medical units of the Health Sector".</t>
   </si>
   <si>
     <t xml:space="preserve">MAR</t>
@@ -1286,7 +1292,7 @@
     <t xml:space="preserve">Pakistan - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200611181828/http://www.covid.gov.pk/</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200612074015/http://www.covid.gov.pk/</t>
   </si>
   <si>
     <t xml:space="preserve">Government of Pakistan</t>
@@ -1342,7 +1348,7 @@
     <t xml:space="preserve">Peru - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.gob.pe/institucion/minsa/noticias/185212-minsa-casos-confirmados-por-coronavirus-covid-19-ascienden-a-208-823-en-el-peru-comunicado-n-128</t>
+    <t xml:space="preserve">https://www.gob.pe/institucion/minsa/noticias/186578-minsa-casos-confirmados-por-coronavirus-covid-19-ascienden-a-214-788-en-el-peru-comunicado-n-129</t>
   </si>
   <si>
     <t xml:space="preserve">Ministry of Health, Government of Peru</t>
@@ -1466,7 +1472,7 @@
     <t xml:space="preserve">Russia - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://rospotrebnadzor.ru/about/info/news/news_details.php?ELEMENT_ID=14679</t>
+    <t xml:space="preserve">https://rospotrebnadzor.ru/about/info/news/news_details.php?ELEMENT_ID=14685</t>
   </si>
   <si>
     <t xml:space="preserve">Government of the Russian Federation</t>
@@ -1593,7 +1599,7 @@
     <t xml:space="preserve">Slovakia - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200611181919/https://korona.gov.sk/</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200612074024/https://korona.gov.sk/</t>
   </si>
   <si>
     <t xml:space="preserve">National Center of Health Information and the Office of the Government of the Slovak Republic</t>
@@ -1867,7 +1873,7 @@
     <t xml:space="preserve">Uganda - samples tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/MinofHealthUG/status/1270627010428239872/photo/1</t>
+    <t xml:space="preserve">https://twitter.com/MinofHealthUG/status/1270989725797679104/photo/1</t>
   </si>
   <si>
     <t xml:space="preserve">Press Release from the Office of the Director General</t>
@@ -1891,7 +1897,7 @@
     <t xml:space="preserve">Ukraine - units unclear</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200611182003/https://covid19.gov.ua/en</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200612074110/https://covid19.gov.ua/en</t>
   </si>
   <si>
     <t xml:space="preserve">Cabinet of Ministers of Ukraine</t>
@@ -1949,7 +1955,7 @@
     <t xml:space="preserve">United States - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200610165830/https://www.cdc.gov/coronavirus/2019-ncov/cases-updates/testing-in-us.html</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200612074112/https://www.cdc.gov/coronavirus/2019-ncov/cases-updates/testing-in-us.html</t>
   </si>
   <si>
     <t xml:space="preserve">United States CDC</t>
@@ -2003,7 +2009,7 @@
     <t xml:space="preserve">Uruguay - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.gub.uy/ministerio-salud-publica/comunicacion/noticias/actualizacion-informacion-relacion-coronavirus-covid-19-uruguay-50</t>
+    <t xml:space="preserve">https://www.gub.uy/ministerio-salud-publica/comunicacion/noticias/actualizacion-informacion-relacion-coronavirus-covid-19-uruguay-51</t>
   </si>
   <si>
     <t xml:space="preserve">https://www.gub.uy/ministerio-salud-publica/comunicacion/noticias</t>
@@ -2452,7 +2458,7 @@
         <v>18</v>
       </c>
       <c r="C2" s="1" t="n">
-        <v>43992</v>
+        <v>43993</v>
       </c>
       <c r="D2" t="s">
         <v>19</v>
@@ -2462,25 +2468,25 @@
       </c>
       <c r="F2"/>
       <c r="G2" t="n">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="H2" t="n">
-        <v>208519</v>
+        <v>214807</v>
       </c>
       <c r="I2" t="n">
-        <v>4.614</v>
+        <v>4.753</v>
       </c>
       <c r="J2" t="n">
-        <v>5468</v>
+        <v>6288</v>
       </c>
       <c r="K2" t="n">
-        <v>0.121</v>
+        <v>0.139</v>
       </c>
       <c r="L2" t="n">
-        <v>5082</v>
+        <v>5194</v>
       </c>
       <c r="M2" t="n">
-        <v>0.112</v>
+        <v>0.115</v>
       </c>
       <c r="N2" t="s">
         <v>20</v>
@@ -2605,7 +2611,7 @@
         <v>39</v>
       </c>
       <c r="C5" s="1" t="n">
-        <v>43993</v>
+        <v>43994</v>
       </c>
       <c r="D5" t="s">
         <v>40</v>
@@ -2615,25 +2621,25 @@
       </c>
       <c r="F5"/>
       <c r="G5" t="n">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="H5" t="n">
-        <v>393910</v>
+        <v>403036</v>
       </c>
       <c r="I5" t="n">
-        <v>231.496</v>
+        <v>236.859</v>
       </c>
       <c r="J5" t="n">
-        <v>7776</v>
+        <v>9126</v>
       </c>
       <c r="K5" t="n">
-        <v>4.57</v>
+        <v>5.363</v>
       </c>
       <c r="L5" t="n">
-        <v>6939</v>
+        <v>6988</v>
       </c>
       <c r="M5" t="n">
-        <v>4.078</v>
+        <v>4.107</v>
       </c>
       <c r="N5" t="s">
         <v>42</v>
@@ -2905,7 +2911,7 @@
         <v>81</v>
       </c>
       <c r="C11" s="1" t="n">
-        <v>43993</v>
+        <v>43994</v>
       </c>
       <c r="D11" t="s">
         <v>82</v>
@@ -2915,25 +2921,25 @@
       </c>
       <c r="F11"/>
       <c r="G11" t="n">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H11" t="n">
-        <v>95820</v>
+        <v>98460</v>
       </c>
       <c r="I11" t="n">
-        <v>13.79</v>
+        <v>14.17</v>
       </c>
       <c r="J11" t="n">
-        <v>2308</v>
+        <v>2640</v>
       </c>
       <c r="K11" t="n">
-        <v>0.332</v>
+        <v>0.38</v>
       </c>
       <c r="L11" t="n">
-        <v>1427</v>
+        <v>1510</v>
       </c>
       <c r="M11" t="n">
-        <v>0.205</v>
+        <v>0.217</v>
       </c>
       <c r="N11" t="s">
         <v>84</v>
@@ -2956,7 +2962,7 @@
         <v>88</v>
       </c>
       <c r="C12" s="1" t="n">
-        <v>43993</v>
+        <v>43994</v>
       </c>
       <c r="D12" t="s">
         <v>89</v>
@@ -2966,25 +2972,25 @@
       </c>
       <c r="F12"/>
       <c r="G12" t="n">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="H12" t="n">
-        <v>1989179</v>
+        <v>2028420</v>
       </c>
       <c r="I12" t="n">
-        <v>52.704</v>
+        <v>53.744</v>
       </c>
       <c r="J12" t="n">
-        <v>33536</v>
+        <v>39241</v>
       </c>
       <c r="K12" t="n">
-        <v>0.889</v>
+        <v>1.04</v>
       </c>
       <c r="L12" t="n">
-        <v>28830</v>
+        <v>29091</v>
       </c>
       <c r="M12" t="n">
-        <v>0.764</v>
+        <v>0.771</v>
       </c>
       <c r="N12" t="s">
         <v>90</v>
@@ -3060,7 +3066,7 @@
         <v>102</v>
       </c>
       <c r="C14" s="1" t="n">
-        <v>43992</v>
+        <v>43993</v>
       </c>
       <c r="D14" t="s">
         <v>103</v>
@@ -3070,25 +3076,25 @@
       </c>
       <c r="F14"/>
       <c r="G14" t="n">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="H14" t="n">
-        <v>444933</v>
+        <v>458324</v>
       </c>
       <c r="I14" t="n">
-        <v>8.744</v>
+        <v>9.007</v>
       </c>
       <c r="J14" t="n">
-        <v>12063</v>
+        <v>13391</v>
       </c>
       <c r="K14" t="n">
-        <v>0.237</v>
+        <v>0.263</v>
       </c>
       <c r="L14" t="n">
-        <v>11786</v>
+        <v>11962</v>
       </c>
       <c r="M14" t="n">
-        <v>0.232</v>
+        <v>0.235</v>
       </c>
       <c r="N14" t="s">
         <v>104</v>
@@ -3111,7 +3117,7 @@
         <v>109</v>
       </c>
       <c r="C15" s="1" t="n">
-        <v>43992</v>
+        <v>43993</v>
       </c>
       <c r="D15" t="s">
         <v>110</v>
@@ -3121,19 +3127,19 @@
       </c>
       <c r="F15"/>
       <c r="G15" t="n">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="H15" t="n">
-        <v>22360</v>
+        <v>22741</v>
       </c>
       <c r="I15" t="n">
-        <v>4.389</v>
+        <v>4.464</v>
       </c>
       <c r="J15" t="n">
-        <v>427</v>
+        <v>381</v>
       </c>
       <c r="K15" t="n">
-        <v>0.084</v>
+        <v>0.075</v>
       </c>
       <c r="L15" t="n">
         <v>320</v>
@@ -3266,7 +3272,7 @@
         <v>130</v>
       </c>
       <c r="C18" s="1" t="n">
-        <v>43992</v>
+        <v>43993</v>
       </c>
       <c r="D18" t="s">
         <v>131</v>
@@ -3276,25 +3282,25 @@
       </c>
       <c r="F18"/>
       <c r="G18" t="n">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="H18" t="n">
-        <v>487334</v>
+        <v>491193</v>
       </c>
       <c r="I18" t="n">
-        <v>45.507</v>
+        <v>45.867</v>
       </c>
       <c r="J18" t="n">
-        <v>3698</v>
+        <v>3546</v>
       </c>
       <c r="K18" t="n">
-        <v>0.345</v>
+        <v>0.331</v>
       </c>
       <c r="L18" t="n">
-        <v>3741</v>
+        <v>3576</v>
       </c>
       <c r="M18" t="n">
-        <v>0.349</v>
+        <v>0.334</v>
       </c>
       <c r="N18" t="s">
         <v>41</v>
@@ -3468,7 +3474,7 @@
         <v>154</v>
       </c>
       <c r="C22" s="1" t="n">
-        <v>43992</v>
+        <v>43993</v>
       </c>
       <c r="D22" t="s">
         <v>155</v>
@@ -3478,25 +3484,25 @@
       </c>
       <c r="F22"/>
       <c r="G22" t="n">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="H22" t="n">
-        <v>93838</v>
+        <v>94716</v>
       </c>
       <c r="I22" t="n">
-        <v>70.739</v>
+        <v>71.401</v>
       </c>
       <c r="J22" t="n">
-        <v>955</v>
+        <v>884</v>
       </c>
       <c r="K22" t="n">
-        <v>0.72</v>
+        <v>0.666</v>
       </c>
       <c r="L22" t="n">
-        <v>913</v>
+        <v>879</v>
       </c>
       <c r="M22" t="n">
-        <v>0.688</v>
+        <v>0.663</v>
       </c>
       <c r="N22" t="s">
         <v>157</v>
@@ -4484,7 +4490,7 @@
         <v>274</v>
       </c>
       <c r="C42" s="1" t="n">
-        <v>43992</v>
+        <v>43993</v>
       </c>
       <c r="D42" t="s">
         <v>275</v>
@@ -4496,18 +4502,18 @@
         <v>277</v>
       </c>
       <c r="G42" t="n">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="H42" t="n">
-        <v>324675</v>
+        <v>328730</v>
       </c>
       <c r="I42" t="n">
-        <v>2.567</v>
+        <v>2.599</v>
       </c>
       <c r="J42"/>
       <c r="K42"/>
       <c r="L42" t="n">
-        <v>3485</v>
+        <v>3585</v>
       </c>
       <c r="M42" t="n">
         <v>0.028</v>
@@ -4533,7 +4539,7 @@
         <v>281</v>
       </c>
       <c r="C43" s="1" t="n">
-        <v>43990</v>
+        <v>43991</v>
       </c>
       <c r="D43" t="s">
         <v>282</v>
@@ -4545,22 +4551,22 @@
         <v>283</v>
       </c>
       <c r="G43" t="n">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="H43" t="n">
-        <v>533756</v>
+        <v>540832</v>
       </c>
       <c r="I43" t="n">
-        <v>4.22</v>
+        <v>4.276</v>
       </c>
       <c r="J43" t="n">
-        <v>4235</v>
+        <v>6960</v>
       </c>
       <c r="K43" t="n">
-        <v>0.033</v>
+        <v>0.055</v>
       </c>
       <c r="L43" t="n">
-        <v>6033</v>
+        <v>6052</v>
       </c>
       <c r="M43" t="n">
         <v>0.048</v>
@@ -4688,7 +4694,7 @@
         <v>298</v>
       </c>
       <c r="C46" s="1" t="n">
-        <v>43993</v>
+        <v>43994</v>
       </c>
       <c r="D46" t="s">
         <v>299</v>
@@ -4700,25 +4706,25 @@
         <v>301</v>
       </c>
       <c r="G46" t="n">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="H46" t="n">
-        <v>123364</v>
+        <v>124662</v>
       </c>
       <c r="I46" t="n">
-        <v>65.403</v>
+        <v>66.092</v>
       </c>
       <c r="J46" t="n">
-        <v>1581</v>
+        <v>1298</v>
       </c>
       <c r="K46" t="n">
-        <v>0.838</v>
+        <v>0.688</v>
       </c>
       <c r="L46" t="n">
-        <v>1273</v>
+        <v>1314</v>
       </c>
       <c r="M46" t="n">
-        <v>0.675</v>
+        <v>0.697</v>
       </c>
       <c r="N46" t="s">
         <v>300</v>
@@ -4741,7 +4747,7 @@
         <v>304</v>
       </c>
       <c r="C47" s="1" t="n">
-        <v>43993</v>
+        <v>43994</v>
       </c>
       <c r="D47" t="s">
         <v>305</v>
@@ -4751,25 +4757,25 @@
       </c>
       <c r="F47"/>
       <c r="G47" t="n">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="H47" t="n">
-        <v>350788</v>
+        <v>356062</v>
       </c>
       <c r="I47" t="n">
-        <v>128.858</v>
+        <v>130.795</v>
       </c>
       <c r="J47" t="n">
-        <v>5396</v>
+        <v>5274</v>
       </c>
       <c r="K47" t="n">
-        <v>1.982</v>
+        <v>1.937</v>
       </c>
       <c r="L47" t="n">
-        <v>4250</v>
+        <v>4253</v>
       </c>
       <c r="M47" t="n">
-        <v>1.561</v>
+        <v>1.562</v>
       </c>
       <c r="N47" t="s">
         <v>41</v>
@@ -4843,7 +4849,7 @@
         <v>315</v>
       </c>
       <c r="C49" s="1" t="n">
-        <v>43992</v>
+        <v>43993</v>
       </c>
       <c r="D49" t="s">
         <v>316</v>
@@ -4855,25 +4861,25 @@
         <v>318</v>
       </c>
       <c r="G49" t="n">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="H49" t="n">
-        <v>625775</v>
+        <v>631608</v>
       </c>
       <c r="I49" t="n">
-        <v>19.334</v>
+        <v>19.515</v>
       </c>
       <c r="J49" t="n">
-        <v>5455</v>
+        <v>5833</v>
       </c>
       <c r="K49" t="n">
-        <v>0.169</v>
+        <v>0.18</v>
       </c>
       <c r="L49" t="n">
-        <v>7181</v>
+        <v>7017</v>
       </c>
       <c r="M49" t="n">
-        <v>0.222</v>
+        <v>0.217</v>
       </c>
       <c r="N49" t="s">
         <v>41</v>
@@ -4945,7 +4951,7 @@
         <v>330</v>
       </c>
       <c r="C51" s="1" t="n">
-        <v>43991</v>
+        <v>43992</v>
       </c>
       <c r="D51" t="s">
         <v>331</v>
@@ -4955,57 +4961,57 @@
       </c>
       <c r="F51"/>
       <c r="G51" t="n">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="H51" t="n">
-        <v>315727</v>
+        <v>325416</v>
       </c>
       <c r="I51" t="n">
-        <v>2.449</v>
+        <v>2.524</v>
       </c>
       <c r="J51" t="n">
-        <v>351</v>
+        <v>310</v>
       </c>
       <c r="K51" t="n">
-        <v>0.003</v>
+        <v>0.002</v>
       </c>
       <c r="L51" t="n">
-        <v>4053</v>
+        <v>4050</v>
       </c>
       <c r="M51" t="n">
         <v>0.031</v>
       </c>
       <c r="N51" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="O51" t="s">
-        <v>331</v>
+        <v>334</v>
       </c>
       <c r="P51" t="s">
         <v>243</v>
       </c>
       <c r="Q51" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="B52" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="C52" s="1" t="n">
         <v>43969</v>
       </c>
       <c r="D52" t="s">
-        <v>336</v>
+        <v>338</v>
       </c>
       <c r="E52" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="F52" t="s">
-        <v>338</v>
+        <v>340</v>
       </c>
       <c r="G52" t="n">
         <v>87</v>
@@ -5029,33 +5035,33 @@
         <v>0.103</v>
       </c>
       <c r="N52" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="O52" t="s">
-        <v>339</v>
+        <v>341</v>
       </c>
       <c r="P52" t="s">
         <v>243</v>
       </c>
       <c r="Q52" t="s">
-        <v>340</v>
+        <v>342</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>341</v>
+        <v>343</v>
       </c>
       <c r="B53" t="s">
-        <v>342</v>
+        <v>344</v>
       </c>
       <c r="C53" s="1" t="n">
         <v>43992</v>
       </c>
       <c r="D53" t="s">
-        <v>343</v>
+        <v>345</v>
       </c>
       <c r="E53" t="s">
-        <v>344</v>
+        <v>346</v>
       </c>
       <c r="F53"/>
       <c r="G53" t="n">
@@ -5080,36 +5086,36 @@
         <v>0.032</v>
       </c>
       <c r="N53" t="s">
-        <v>344</v>
+        <v>346</v>
       </c>
       <c r="O53" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="P53" t="s">
         <v>51</v>
       </c>
       <c r="Q53" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>347</v>
+        <v>349</v>
       </c>
       <c r="B54" t="s">
-        <v>348</v>
+        <v>350</v>
       </c>
       <c r="C54" s="1" t="n">
         <v>43992</v>
       </c>
       <c r="D54" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="E54" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="F54" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="G54" t="n">
         <v>111</v>
@@ -5133,33 +5139,33 @@
         <v>0.149</v>
       </c>
       <c r="N54" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="O54" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="P54" t="s">
         <v>92</v>
       </c>
       <c r="Q54" t="s">
-        <v>353</v>
+        <v>355</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="B55" t="s">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="C55" s="1" t="n">
         <v>43992</v>
       </c>
       <c r="D55" t="s">
-        <v>356</v>
+        <v>358</v>
       </c>
       <c r="E55" t="s">
-        <v>357</v>
+        <v>359</v>
       </c>
       <c r="F55"/>
       <c r="G55" t="n">
@@ -5184,84 +5190,84 @@
         <v>0.491</v>
       </c>
       <c r="N55" t="s">
-        <v>358</v>
+        <v>360</v>
       </c>
       <c r="O55" t="s">
-        <v>359</v>
+        <v>361</v>
       </c>
       <c r="P55" t="s">
         <v>92</v>
       </c>
       <c r="Q55" t="s">
-        <v>360</v>
+        <v>362</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>361</v>
+        <v>363</v>
       </c>
       <c r="B56" t="s">
-        <v>362</v>
+        <v>364</v>
       </c>
       <c r="C56" s="1" t="n">
-        <v>43992</v>
+        <v>43993</v>
       </c>
       <c r="D56" t="s">
-        <v>363</v>
+        <v>365</v>
       </c>
       <c r="E56" t="s">
         <v>41</v>
       </c>
       <c r="F56"/>
       <c r="G56" t="n">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="H56" t="n">
-        <v>301882</v>
+        <v>304832</v>
       </c>
       <c r="I56" t="n">
-        <v>62.602</v>
+        <v>63.214</v>
       </c>
       <c r="J56" t="n">
-        <v>3350</v>
+        <v>2950</v>
       </c>
       <c r="K56" t="n">
-        <v>0.695</v>
+        <v>0.612</v>
       </c>
       <c r="L56" t="n">
-        <v>2244</v>
+        <v>2264</v>
       </c>
       <c r="M56" t="n">
-        <v>0.465</v>
+        <v>0.469</v>
       </c>
       <c r="N56" t="s">
-        <v>364</v>
+        <v>366</v>
       </c>
       <c r="O56" t="s">
-        <v>363</v>
+        <v>365</v>
       </c>
       <c r="P56" t="s">
         <v>22</v>
       </c>
       <c r="Q56" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="s">
-        <v>366</v>
+        <v>368</v>
       </c>
       <c r="B57" t="s">
-        <v>367</v>
+        <v>369</v>
       </c>
       <c r="C57" s="1" t="n">
         <v>43993</v>
       </c>
       <c r="D57" t="s">
-        <v>368</v>
+        <v>370</v>
       </c>
       <c r="E57" t="s">
-        <v>369</v>
+        <v>371</v>
       </c>
       <c r="F57"/>
       <c r="G57" t="n">
@@ -5286,33 +5292,33 @@
         <v>0.01</v>
       </c>
       <c r="N57" t="s">
-        <v>369</v>
+        <v>371</v>
       </c>
       <c r="O57" t="s">
-        <v>370</v>
+        <v>372</v>
       </c>
       <c r="P57" t="s">
         <v>51</v>
       </c>
       <c r="Q57" t="s">
-        <v>371</v>
+        <v>373</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="s">
-        <v>372</v>
+        <v>374</v>
       </c>
       <c r="B58" t="s">
-        <v>373</v>
+        <v>375</v>
       </c>
       <c r="C58" s="1" t="n">
         <v>43993</v>
       </c>
       <c r="D58" t="s">
-        <v>374</v>
+        <v>376</v>
       </c>
       <c r="E58" t="s">
-        <v>375</v>
+        <v>377</v>
       </c>
       <c r="F58"/>
       <c r="G58" t="n">
@@ -5337,84 +5343,84 @@
         <v>0.479</v>
       </c>
       <c r="N58" t="s">
-        <v>375</v>
+        <v>377</v>
       </c>
       <c r="O58" t="s">
-        <v>376</v>
+        <v>378</v>
       </c>
       <c r="P58" t="s">
-        <v>377</v>
+        <v>379</v>
       </c>
       <c r="Q58" t="s">
-        <v>378</v>
+        <v>380</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="s">
-        <v>379</v>
+        <v>381</v>
       </c>
       <c r="B59" t="s">
-        <v>380</v>
+        <v>382</v>
       </c>
       <c r="C59" s="1" t="n">
-        <v>43993</v>
+        <v>43994</v>
       </c>
       <c r="D59" t="s">
-        <v>381</v>
+        <v>383</v>
       </c>
       <c r="E59" t="s">
-        <v>382</v>
+        <v>384</v>
       </c>
       <c r="F59"/>
       <c r="G59" t="n">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="H59" t="n">
-        <v>780825</v>
+        <v>809169</v>
       </c>
       <c r="I59" t="n">
-        <v>3.535</v>
+        <v>3.663</v>
       </c>
       <c r="J59" t="n">
-        <v>26573</v>
+        <v>28344</v>
       </c>
       <c r="K59" t="n">
-        <v>0.12</v>
+        <v>0.128</v>
       </c>
       <c r="L59" t="n">
-        <v>23616</v>
+        <v>24407</v>
       </c>
       <c r="M59" t="n">
-        <v>0.107</v>
+        <v>0.11</v>
       </c>
       <c r="N59" t="s">
-        <v>382</v>
+        <v>384</v>
       </c>
       <c r="O59" t="s">
-        <v>383</v>
+        <v>385</v>
       </c>
       <c r="P59" t="s">
         <v>22</v>
       </c>
       <c r="Q59" t="s">
-        <v>384</v>
+        <v>386</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="s">
-        <v>385</v>
+        <v>387</v>
       </c>
       <c r="B60" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="C60" s="1" t="n">
         <v>43991</v>
       </c>
       <c r="D60" t="s">
-        <v>387</v>
+        <v>389</v>
       </c>
       <c r="E60" t="s">
-        <v>388</v>
+        <v>390</v>
       </c>
       <c r="F60"/>
       <c r="G60" t="n">
@@ -5439,33 +5445,33 @@
         <v>0.365</v>
       </c>
       <c r="N60" t="s">
-        <v>388</v>
+        <v>390</v>
       </c>
       <c r="O60" t="s">
-        <v>389</v>
+        <v>391</v>
       </c>
       <c r="P60" t="s">
         <v>22</v>
       </c>
       <c r="Q60" t="s">
-        <v>390</v>
+        <v>392</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="s">
-        <v>391</v>
+        <v>393</v>
       </c>
       <c r="B61" t="s">
-        <v>392</v>
+        <v>394</v>
       </c>
       <c r="C61" s="1" t="n">
         <v>43992</v>
       </c>
       <c r="D61" t="s">
-        <v>393</v>
+        <v>395</v>
       </c>
       <c r="E61" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="F61"/>
       <c r="G61" t="n">
@@ -5490,136 +5496,140 @@
         <v>0.173</v>
       </c>
       <c r="N61" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="O61" t="s">
-        <v>395</v>
+        <v>397</v>
       </c>
       <c r="P61" t="s">
         <v>51</v>
       </c>
       <c r="Q61" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="s">
-        <v>397</v>
+        <v>399</v>
       </c>
       <c r="B62" t="s">
-        <v>398</v>
+        <v>400</v>
       </c>
       <c r="C62" s="1" t="n">
-        <v>43993</v>
+        <v>43994</v>
       </c>
       <c r="D62" t="s">
-        <v>399</v>
+        <v>401</v>
       </c>
       <c r="E62" t="s">
         <v>41</v>
       </c>
       <c r="F62"/>
       <c r="G62" t="n">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H62" t="n">
-        <v>175752</v>
+        <v>179364</v>
       </c>
       <c r="I62" t="n">
-        <v>5.33</v>
-      </c>
-      <c r="J62"/>
-      <c r="K62"/>
+        <v>5.44</v>
+      </c>
+      <c r="J62" t="n">
+        <v>3612</v>
+      </c>
+      <c r="K62" t="n">
+        <v>0.11</v>
+      </c>
       <c r="L62" t="n">
-        <v>3250</v>
+        <v>3656</v>
       </c>
       <c r="M62" t="n">
-        <v>0.099</v>
+        <v>0.111</v>
       </c>
       <c r="N62" t="s">
-        <v>400</v>
+        <v>402</v>
       </c>
       <c r="O62" t="s">
-        <v>401</v>
+        <v>403</v>
       </c>
       <c r="P62" t="s">
         <v>92</v>
       </c>
       <c r="Q62" t="s">
-        <v>402</v>
+        <v>404</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="s">
-        <v>403</v>
+        <v>405</v>
       </c>
       <c r="B63" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="C63" s="1" t="n">
-        <v>43989</v>
+        <v>43991</v>
       </c>
       <c r="D63" t="s">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="E63" t="s">
-        <v>406</v>
+        <v>408</v>
       </c>
       <c r="F63" t="s">
-        <v>407</v>
+        <v>409</v>
       </c>
       <c r="G63" t="n">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="H63" t="n">
-        <v>406344</v>
+        <v>427121</v>
       </c>
       <c r="I63" t="n">
-        <v>3.708</v>
+        <v>3.898</v>
       </c>
       <c r="J63" t="n">
-        <v>10472</v>
+        <v>10920</v>
       </c>
       <c r="K63" t="n">
-        <v>0.096</v>
+        <v>0.1</v>
       </c>
       <c r="L63" t="n">
-        <v>11073</v>
+        <v>11399</v>
       </c>
       <c r="M63" t="n">
-        <v>0.101</v>
+        <v>0.104</v>
       </c>
       <c r="N63" t="s">
         <v>213</v>
       </c>
       <c r="O63" t="s">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="P63" t="s">
         <v>92</v>
       </c>
       <c r="Q63" t="s">
-        <v>408</v>
+        <v>410</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="s">
-        <v>409</v>
+        <v>411</v>
       </c>
       <c r="B64" t="s">
-        <v>410</v>
+        <v>412</v>
       </c>
       <c r="C64" s="1" t="n">
         <v>43985</v>
       </c>
       <c r="D64" t="s">
-        <v>411</v>
+        <v>413</v>
       </c>
       <c r="E64" t="s">
-        <v>412</v>
+        <v>414</v>
       </c>
       <c r="F64" t="s">
-        <v>413</v>
+        <v>415</v>
       </c>
       <c r="G64" t="n">
         <v>91</v>
@@ -5643,30 +5653,30 @@
         <v>0.538</v>
       </c>
       <c r="N64" t="s">
-        <v>414</v>
+        <v>416</v>
       </c>
       <c r="O64" t="s">
-        <v>415</v>
+        <v>417</v>
       </c>
       <c r="P64" t="s">
         <v>51</v>
       </c>
       <c r="Q64" t="s">
-        <v>416</v>
+        <v>418</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="s">
-        <v>417</v>
+        <v>419</v>
       </c>
       <c r="B65" t="s">
-        <v>418</v>
+        <v>420</v>
       </c>
       <c r="C65" s="1" t="n">
         <v>43991</v>
       </c>
       <c r="D65" t="s">
-        <v>419</v>
+        <v>421</v>
       </c>
       <c r="E65" t="s">
         <v>41</v>
@@ -5694,84 +5704,84 @@
         <v>1.25</v>
       </c>
       <c r="N65" t="s">
-        <v>420</v>
+        <v>422</v>
       </c>
       <c r="O65" t="s">
-        <v>419</v>
+        <v>421</v>
       </c>
       <c r="P65" t="s">
-        <v>421</v>
+        <v>423</v>
       </c>
       <c r="Q65" t="s">
-        <v>422</v>
+        <v>424</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="s">
-        <v>423</v>
+        <v>425</v>
       </c>
       <c r="B66" t="s">
-        <v>424</v>
+        <v>426</v>
       </c>
       <c r="C66" s="1" t="n">
-        <v>43992</v>
+        <v>43993</v>
       </c>
       <c r="D66" t="s">
-        <v>425</v>
+        <v>427</v>
       </c>
       <c r="E66" t="s">
-        <v>426</v>
+        <v>428</v>
       </c>
       <c r="F66"/>
       <c r="G66" t="n">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="H66" t="n">
-        <v>269964</v>
+        <v>274793</v>
       </c>
       <c r="I66" t="n">
-        <v>93.703</v>
+        <v>95.379</v>
       </c>
       <c r="J66" t="n">
-        <v>4929</v>
+        <v>4829</v>
       </c>
       <c r="K66" t="n">
-        <v>1.711</v>
+        <v>1.676</v>
       </c>
       <c r="L66" t="n">
-        <v>4790</v>
+        <v>4815</v>
       </c>
       <c r="M66" t="n">
-        <v>1.663</v>
+        <v>1.671</v>
       </c>
       <c r="N66" t="s">
-        <v>426</v>
+        <v>428</v>
       </c>
       <c r="O66" t="s">
-        <v>427</v>
+        <v>429</v>
       </c>
       <c r="P66" t="s">
         <v>92</v>
       </c>
       <c r="Q66" t="s">
-        <v>428</v>
+        <v>430</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="s">
-        <v>429</v>
+        <v>431</v>
       </c>
       <c r="B67" t="s">
-        <v>430</v>
+        <v>432</v>
       </c>
       <c r="C67" s="1" t="n">
         <v>43993</v>
       </c>
       <c r="D67" t="s">
-        <v>431</v>
+        <v>433</v>
       </c>
       <c r="E67" t="s">
-        <v>432</v>
+        <v>434</v>
       </c>
       <c r="F67"/>
       <c r="G67" t="n">
@@ -5796,84 +5806,84 @@
         <v>0.436</v>
       </c>
       <c r="N67" t="s">
-        <v>432</v>
+        <v>434</v>
       </c>
       <c r="O67" t="s">
-        <v>433</v>
+        <v>435</v>
       </c>
       <c r="P67" t="s">
         <v>22</v>
       </c>
       <c r="Q67" t="s">
-        <v>434</v>
+        <v>436</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="s">
-        <v>435</v>
+        <v>437</v>
       </c>
       <c r="B68" t="s">
-        <v>436</v>
+        <v>438</v>
       </c>
       <c r="C68" s="1" t="n">
-        <v>43993</v>
+        <v>43994</v>
       </c>
       <c r="D68" t="s">
-        <v>437</v>
+        <v>439</v>
       </c>
       <c r="E68" t="s">
-        <v>438</v>
+        <v>440</v>
       </c>
       <c r="F68"/>
       <c r="G68" t="n">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="H68" t="n">
-        <v>13875097</v>
+        <v>14218674</v>
       </c>
       <c r="I68" t="n">
-        <v>95.078</v>
+        <v>97.432</v>
       </c>
       <c r="J68" t="n">
-        <v>329794</v>
+        <v>343577</v>
       </c>
       <c r="K68" t="n">
-        <v>2.26</v>
+        <v>2.354</v>
       </c>
       <c r="L68" t="n">
-        <v>306007</v>
+        <v>309287</v>
       </c>
       <c r="M68" t="n">
-        <v>2.097</v>
+        <v>2.119</v>
       </c>
       <c r="N68" t="s">
-        <v>438</v>
+        <v>440</v>
       </c>
       <c r="O68" t="s">
-        <v>439</v>
+        <v>441</v>
       </c>
       <c r="P68" t="s">
         <v>22</v>
       </c>
       <c r="Q68" t="s">
-        <v>440</v>
+        <v>442</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="s">
-        <v>441</v>
+        <v>443</v>
       </c>
       <c r="B69" t="s">
-        <v>442</v>
+        <v>444</v>
       </c>
       <c r="C69" s="1" t="n">
         <v>43992</v>
       </c>
       <c r="D69" t="s">
-        <v>443</v>
+        <v>445</v>
       </c>
       <c r="E69" t="s">
-        <v>444</v>
+        <v>446</v>
       </c>
       <c r="F69"/>
       <c r="G69" t="n">
@@ -5898,187 +5908,187 @@
         <v>0.122</v>
       </c>
       <c r="N69" t="s">
-        <v>444</v>
+        <v>446</v>
       </c>
       <c r="O69" t="s">
-        <v>445</v>
+        <v>447</v>
       </c>
       <c r="P69" t="s">
         <v>51</v>
       </c>
       <c r="Q69" t="s">
-        <v>446</v>
+        <v>448</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="s">
-        <v>447</v>
+        <v>449</v>
       </c>
       <c r="B70" t="s">
-        <v>448</v>
+        <v>450</v>
       </c>
       <c r="C70" s="1" t="n">
-        <v>43992</v>
+        <v>43993</v>
       </c>
       <c r="D70" t="s">
-        <v>449</v>
+        <v>451</v>
       </c>
       <c r="E70" t="s">
         <v>41</v>
       </c>
       <c r="F70"/>
       <c r="G70" t="n">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H70" t="n">
-        <v>1019812</v>
+        <v>1042312</v>
       </c>
       <c r="I70" t="n">
-        <v>29.293</v>
+        <v>29.94</v>
       </c>
       <c r="J70" t="n">
-        <v>22139</v>
+        <v>22500</v>
       </c>
       <c r="K70" t="n">
+        <v>0.646</v>
+      </c>
+      <c r="L70" t="n">
+        <v>22158</v>
+      </c>
+      <c r="M70" t="n">
         <v>0.636</v>
-      </c>
-      <c r="L70" t="n">
-        <v>21264</v>
-      </c>
-      <c r="M70" t="n">
-        <v>0.611</v>
       </c>
       <c r="N70" t="s">
         <v>41</v>
       </c>
       <c r="O70" t="s">
-        <v>449</v>
+        <v>451</v>
       </c>
       <c r="P70" t="s">
         <v>127</v>
       </c>
       <c r="Q70" t="s">
-        <v>450</v>
+        <v>452</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="s">
-        <v>451</v>
+        <v>453</v>
       </c>
       <c r="B71" t="s">
-        <v>452</v>
+        <v>454</v>
       </c>
       <c r="C71" s="1" t="n">
-        <v>43992</v>
+        <v>43993</v>
       </c>
       <c r="D71" t="s">
-        <v>453</v>
+        <v>455</v>
       </c>
       <c r="E71" t="s">
-        <v>454</v>
+        <v>456</v>
       </c>
       <c r="F71" t="s">
-        <v>455</v>
+        <v>457</v>
       </c>
       <c r="G71" t="n">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="H71" t="n">
-        <v>56739</v>
+        <v>57903</v>
       </c>
       <c r="I71" t="n">
-        <v>3.389</v>
+        <v>3.458</v>
       </c>
       <c r="J71" t="n">
-        <v>1205</v>
+        <v>1164</v>
       </c>
       <c r="K71" t="n">
-        <v>0.072</v>
+        <v>0.07</v>
       </c>
       <c r="L71" t="n">
-        <v>1299</v>
+        <v>1273</v>
       </c>
       <c r="M71" t="n">
-        <v>0.078</v>
+        <v>0.076</v>
       </c>
       <c r="N71" t="s">
-        <v>456</v>
+        <v>458</v>
       </c>
       <c r="O71" t="s">
-        <v>457</v>
+        <v>459</v>
       </c>
       <c r="P71" t="s">
-        <v>458</v>
+        <v>460</v>
       </c>
       <c r="Q71" t="s">
-        <v>459</v>
+        <v>461</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="s">
-        <v>460</v>
+        <v>462</v>
       </c>
       <c r="B72" t="s">
-        <v>461</v>
+        <v>463</v>
       </c>
       <c r="C72" s="1" t="n">
-        <v>43992</v>
+        <v>43993</v>
       </c>
       <c r="D72" t="s">
-        <v>462</v>
+        <v>464</v>
       </c>
       <c r="E72" t="s">
         <v>41</v>
       </c>
       <c r="F72" t="s">
-        <v>463</v>
+        <v>465</v>
       </c>
       <c r="G72" t="n">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="H72" t="n">
-        <v>287064</v>
+        <v>291996</v>
       </c>
       <c r="I72" t="n">
-        <v>42.187</v>
+        <v>42.912</v>
       </c>
       <c r="J72" t="n">
-        <v>5015</v>
+        <v>4932</v>
       </c>
       <c r="K72" t="n">
-        <v>0.737</v>
+        <v>0.725</v>
       </c>
       <c r="L72" t="n">
-        <v>4260</v>
+        <v>4390</v>
       </c>
       <c r="M72" t="n">
-        <v>0.626</v>
+        <v>0.645</v>
       </c>
       <c r="N72" t="s">
         <v>41</v>
       </c>
       <c r="O72" t="s">
-        <v>464</v>
+        <v>466</v>
       </c>
       <c r="P72" t="s">
         <v>92</v>
       </c>
       <c r="Q72" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="s">
-        <v>466</v>
+        <v>468</v>
       </c>
       <c r="B73" t="s">
-        <v>467</v>
+        <v>469</v>
       </c>
       <c r="C73" s="1" t="n">
         <v>43990</v>
       </c>
       <c r="D73" t="s">
-        <v>468</v>
+        <v>470</v>
       </c>
       <c r="E73" t="s">
         <v>41</v>
@@ -6105,27 +6115,27 @@
         <v>41</v>
       </c>
       <c r="O73" t="s">
-        <v>469</v>
+        <v>471</v>
       </c>
       <c r="P73" t="s">
         <v>92</v>
       </c>
       <c r="Q73" t="s">
-        <v>470</v>
+        <v>472</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="s">
-        <v>466</v>
+        <v>468</v>
       </c>
       <c r="B74" t="s">
-        <v>471</v>
+        <v>473</v>
       </c>
       <c r="C74" s="1" t="n">
         <v>43990</v>
       </c>
       <c r="D74" t="s">
-        <v>472</v>
+        <v>474</v>
       </c>
       <c r="E74" t="s">
         <v>41</v>
@@ -6152,81 +6162,81 @@
         <v>41</v>
       </c>
       <c r="O74" t="s">
-        <v>469</v>
+        <v>471</v>
       </c>
       <c r="P74" t="s">
-        <v>473</v>
+        <v>475</v>
       </c>
       <c r="Q74" t="s">
-        <v>470</v>
+        <v>472</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="s">
-        <v>474</v>
+        <v>476</v>
       </c>
       <c r="B75" t="s">
-        <v>475</v>
+        <v>477</v>
       </c>
       <c r="C75" s="1" t="n">
-        <v>43993</v>
+        <v>43994</v>
       </c>
       <c r="D75" t="s">
-        <v>476</v>
+        <v>478</v>
       </c>
       <c r="E75" t="s">
-        <v>477</v>
+        <v>479</v>
       </c>
       <c r="F75"/>
       <c r="G75" t="n">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="H75" t="n">
-        <v>193471</v>
+        <v>194733</v>
       </c>
       <c r="I75" t="n">
-        <v>35.437</v>
+        <v>35.668</v>
       </c>
       <c r="J75" t="n">
-        <v>1500</v>
+        <v>1262</v>
       </c>
       <c r="K75" t="n">
-        <v>0.275</v>
+        <v>0.231</v>
       </c>
       <c r="L75" t="n">
-        <v>1387</v>
+        <v>1305</v>
       </c>
       <c r="M75" t="n">
-        <v>0.254</v>
+        <v>0.239</v>
       </c>
       <c r="N75" t="s">
-        <v>478</v>
+        <v>480</v>
       </c>
       <c r="O75" t="s">
-        <v>479</v>
+        <v>481</v>
       </c>
       <c r="P75" t="s">
-        <v>480</v>
+        <v>482</v>
       </c>
       <c r="Q75" t="s">
-        <v>481</v>
+        <v>483</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="s">
-        <v>482</v>
+        <v>484</v>
       </c>
       <c r="B76" t="s">
-        <v>483</v>
+        <v>485</v>
       </c>
       <c r="C76" s="1" t="n">
         <v>43992</v>
       </c>
       <c r="D76" t="s">
-        <v>484</v>
+        <v>486</v>
       </c>
       <c r="E76" t="s">
-        <v>485</v>
+        <v>487</v>
       </c>
       <c r="F76"/>
       <c r="G76" t="n">
@@ -6251,36 +6261,36 @@
         <v>0.295</v>
       </c>
       <c r="N76" t="s">
-        <v>486</v>
+        <v>488</v>
       </c>
       <c r="O76" t="s">
-        <v>487</v>
+        <v>489</v>
       </c>
       <c r="P76" t="s">
         <v>22</v>
       </c>
       <c r="Q76" t="s">
-        <v>488</v>
+        <v>490</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="s">
-        <v>489</v>
+        <v>491</v>
       </c>
       <c r="B77" t="s">
-        <v>490</v>
+        <v>492</v>
       </c>
       <c r="C77" s="1" t="n">
         <v>43993</v>
       </c>
       <c r="D77" t="s">
-        <v>491</v>
+        <v>493</v>
       </c>
       <c r="E77" t="s">
-        <v>492</v>
+        <v>494</v>
       </c>
       <c r="F77" t="s">
-        <v>493</v>
+        <v>495</v>
       </c>
       <c r="G77" t="n">
         <v>103</v>
@@ -6304,33 +6314,33 @@
         <v>0.5</v>
       </c>
       <c r="N77" t="s">
-        <v>492</v>
+        <v>494</v>
       </c>
       <c r="O77" t="s">
-        <v>494</v>
+        <v>496</v>
       </c>
       <c r="P77" t="s">
         <v>92</v>
       </c>
       <c r="Q77" t="s">
-        <v>495</v>
+        <v>497</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="s">
-        <v>496</v>
+        <v>498</v>
       </c>
       <c r="B78" t="s">
-        <v>497</v>
+        <v>499</v>
       </c>
       <c r="C78" s="1" t="n">
         <v>43993</v>
       </c>
       <c r="D78" t="s">
-        <v>498</v>
+        <v>500</v>
       </c>
       <c r="E78" t="s">
-        <v>499</v>
+        <v>501</v>
       </c>
       <c r="F78"/>
       <c r="G78" t="n">
@@ -6355,33 +6365,33 @@
         <v>0.259</v>
       </c>
       <c r="N78" t="s">
-        <v>499</v>
+        <v>501</v>
       </c>
       <c r="O78" t="s">
-        <v>500</v>
+        <v>502</v>
       </c>
       <c r="P78" t="s">
         <v>243</v>
       </c>
       <c r="Q78" t="s">
-        <v>501</v>
+        <v>503</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="s">
-        <v>502</v>
+        <v>504</v>
       </c>
       <c r="B79" t="s">
-        <v>503</v>
+        <v>505</v>
       </c>
       <c r="C79" s="1" t="n">
         <v>43986</v>
       </c>
       <c r="D79" t="s">
-        <v>504</v>
+        <v>506</v>
       </c>
       <c r="E79" t="s">
-        <v>505</v>
+        <v>507</v>
       </c>
       <c r="F79"/>
       <c r="G79" t="n">
@@ -6402,33 +6412,33 @@
         <v>0.876</v>
       </c>
       <c r="N79" t="s">
-        <v>506</v>
+        <v>508</v>
       </c>
       <c r="O79" t="s">
-        <v>507</v>
+        <v>509</v>
       </c>
       <c r="P79" t="s">
         <v>22</v>
       </c>
       <c r="Q79" t="s">
-        <v>508</v>
+        <v>510</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="s">
-        <v>509</v>
+        <v>511</v>
       </c>
       <c r="B80" t="s">
-        <v>510</v>
+        <v>512</v>
       </c>
       <c r="C80" s="1" t="n">
         <v>43989</v>
       </c>
       <c r="D80" t="s">
-        <v>511</v>
+        <v>513</v>
       </c>
       <c r="E80" t="s">
-        <v>512</v>
+        <v>514</v>
       </c>
       <c r="F80"/>
       <c r="G80" t="n">
@@ -6449,33 +6459,33 @@
         <v>0.696</v>
       </c>
       <c r="N80" t="s">
-        <v>512</v>
+        <v>514</v>
       </c>
       <c r="O80" t="s">
-        <v>511</v>
+        <v>513</v>
       </c>
       <c r="P80" t="s">
         <v>92</v>
       </c>
       <c r="Q80" t="s">
-        <v>513</v>
+        <v>515</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="s">
-        <v>514</v>
+        <v>516</v>
       </c>
       <c r="B81" t="s">
-        <v>515</v>
+        <v>517</v>
       </c>
       <c r="C81" s="1" t="n">
         <v>43992</v>
       </c>
       <c r="D81" t="s">
-        <v>516</v>
+        <v>518</v>
       </c>
       <c r="E81" t="s">
-        <v>517</v>
+        <v>519</v>
       </c>
       <c r="F81"/>
       <c r="G81" t="n">
@@ -6500,33 +6510,33 @@
         <v>0.501</v>
       </c>
       <c r="N81" t="s">
-        <v>517</v>
+        <v>519</v>
       </c>
       <c r="O81" t="s">
-        <v>516</v>
+        <v>518</v>
       </c>
       <c r="P81" t="s">
-        <v>518</v>
+        <v>520</v>
       </c>
       <c r="Q81" t="s">
-        <v>519</v>
+        <v>521</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="s">
-        <v>520</v>
+        <v>522</v>
       </c>
       <c r="B82" t="s">
-        <v>521</v>
+        <v>523</v>
       </c>
       <c r="C82" s="1" t="n">
         <v>43991</v>
       </c>
       <c r="D82" t="s">
-        <v>522</v>
+        <v>524</v>
       </c>
       <c r="E82" t="s">
-        <v>523</v>
+        <v>525</v>
       </c>
       <c r="F82"/>
       <c r="G82" t="n">
@@ -6547,33 +6557,33 @@
         <v>0.006</v>
       </c>
       <c r="N82" t="s">
-        <v>523</v>
+        <v>525</v>
       </c>
       <c r="O82" t="s">
-        <v>524</v>
+        <v>526</v>
       </c>
       <c r="P82" t="s">
-        <v>525</v>
+        <v>527</v>
       </c>
       <c r="Q82" t="s">
-        <v>526</v>
+        <v>528</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="s">
-        <v>527</v>
+        <v>529</v>
       </c>
       <c r="B83" t="s">
-        <v>528</v>
+        <v>530</v>
       </c>
       <c r="C83" s="1" t="n">
         <v>43993</v>
       </c>
       <c r="D83" t="s">
-        <v>529</v>
+        <v>531</v>
       </c>
       <c r="E83" t="s">
-        <v>530</v>
+        <v>532</v>
       </c>
       <c r="F83"/>
       <c r="G83" t="n">
@@ -6598,36 +6608,36 @@
         <v>0.075</v>
       </c>
       <c r="N83" t="s">
-        <v>531</v>
+        <v>533</v>
       </c>
       <c r="O83" t="s">
-        <v>532</v>
+        <v>534</v>
       </c>
       <c r="P83" t="s">
         <v>92</v>
       </c>
       <c r="Q83" t="s">
-        <v>533</v>
+        <v>535</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="s">
-        <v>527</v>
+        <v>529</v>
       </c>
       <c r="B84" t="s">
-        <v>534</v>
+        <v>536</v>
       </c>
       <c r="C84" s="1" t="n">
         <v>43987</v>
       </c>
       <c r="D84" t="s">
-        <v>535</v>
+        <v>537</v>
       </c>
       <c r="E84" t="s">
-        <v>536</v>
+        <v>538</v>
       </c>
       <c r="F84" t="s">
-        <v>537</v>
+        <v>539</v>
       </c>
       <c r="G84" t="n">
         <v>10</v>
@@ -6647,33 +6657,33 @@
         <v>0.126</v>
       </c>
       <c r="N84" t="s">
-        <v>536</v>
+        <v>538</v>
       </c>
       <c r="O84" t="s">
-        <v>538</v>
+        <v>540</v>
       </c>
       <c r="P84" t="s">
         <v>51</v>
       </c>
       <c r="Q84" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="s">
-        <v>540</v>
+        <v>542</v>
       </c>
       <c r="B85" t="s">
-        <v>541</v>
+        <v>543</v>
       </c>
       <c r="C85" s="1" t="n">
         <v>43991</v>
       </c>
       <c r="D85" t="s">
-        <v>542</v>
+        <v>544</v>
       </c>
       <c r="E85" t="s">
-        <v>543</v>
+        <v>545</v>
       </c>
       <c r="F85"/>
       <c r="G85" t="n">
@@ -6694,33 +6704,33 @@
         <v>0.032</v>
       </c>
       <c r="N85" t="s">
-        <v>543</v>
+        <v>545</v>
       </c>
       <c r="O85" t="s">
-        <v>544</v>
+        <v>546</v>
       </c>
       <c r="P85" t="s">
-        <v>545</v>
+        <v>547</v>
       </c>
       <c r="Q85" t="s">
-        <v>546</v>
+        <v>548</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="s">
-        <v>547</v>
+        <v>549</v>
       </c>
       <c r="B86" t="s">
-        <v>548</v>
+        <v>550</v>
       </c>
       <c r="C86" s="1" t="n">
         <v>43993</v>
       </c>
       <c r="D86" t="s">
-        <v>549</v>
+        <v>551</v>
       </c>
       <c r="E86" t="s">
-        <v>550</v>
+        <v>552</v>
       </c>
       <c r="F86"/>
       <c r="G86" t="n">
@@ -6745,137 +6755,137 @@
         <v>0.493</v>
       </c>
       <c r="N86" t="s">
-        <v>550</v>
+        <v>552</v>
       </c>
       <c r="O86" t="s">
-        <v>551</v>
+        <v>553</v>
       </c>
       <c r="P86" t="s">
-        <v>552</v>
+        <v>554</v>
       </c>
       <c r="Q86" t="s">
-        <v>553</v>
+        <v>555</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="s">
-        <v>554</v>
+        <v>556</v>
       </c>
       <c r="B87" t="s">
-        <v>555</v>
+        <v>557</v>
       </c>
       <c r="C87" s="1" t="n">
-        <v>43991</v>
+        <v>43992</v>
       </c>
       <c r="D87" t="s">
-        <v>556</v>
+        <v>558</v>
       </c>
       <c r="E87" t="s">
-        <v>557</v>
+        <v>559</v>
       </c>
       <c r="F87" t="s">
-        <v>558</v>
+        <v>560</v>
       </c>
       <c r="G87" t="n">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H87" t="n">
-        <v>115101</v>
+        <v>117422</v>
       </c>
       <c r="I87" t="n">
-        <v>2.516</v>
+        <v>2.567</v>
       </c>
       <c r="J87" t="n">
-        <v>2423</v>
+        <v>2321</v>
       </c>
       <c r="K87" t="n">
-        <v>0.053</v>
+        <v>0.051</v>
       </c>
       <c r="L87" t="n">
-        <v>2084</v>
+        <v>2254</v>
       </c>
       <c r="M87" t="n">
-        <v>0.046</v>
+        <v>0.049</v>
       </c>
       <c r="N87" t="s">
-        <v>557</v>
+        <v>559</v>
       </c>
       <c r="O87" t="s">
-        <v>559</v>
+        <v>561</v>
       </c>
       <c r="P87" t="s">
         <v>51</v>
       </c>
       <c r="Q87" t="s">
-        <v>560</v>
+        <v>562</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="s">
-        <v>561</v>
+        <v>563</v>
       </c>
       <c r="B88" t="s">
-        <v>562</v>
+        <v>564</v>
       </c>
       <c r="C88" s="1" t="n">
-        <v>43993</v>
+        <v>43994</v>
       </c>
       <c r="D88" t="s">
-        <v>563</v>
+        <v>565</v>
       </c>
       <c r="E88" t="s">
-        <v>564</v>
+        <v>566</v>
       </c>
       <c r="F88"/>
       <c r="G88" t="n">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="H88" t="n">
-        <v>456509</v>
+        <v>468172</v>
       </c>
       <c r="I88" t="n">
-        <v>10.438</v>
+        <v>10.705</v>
       </c>
       <c r="J88" t="n">
-        <v>10569</v>
+        <v>11663</v>
       </c>
       <c r="K88" t="n">
-        <v>0.242</v>
+        <v>0.267</v>
       </c>
       <c r="L88" t="n">
-        <v>9170</v>
+        <v>9232</v>
       </c>
       <c r="M88" t="n">
-        <v>0.21</v>
+        <v>0.211</v>
       </c>
       <c r="N88" t="s">
-        <v>564</v>
+        <v>566</v>
       </c>
       <c r="O88" t="s">
-        <v>565</v>
+        <v>567</v>
       </c>
       <c r="P88" t="s">
-        <v>566</v>
+        <v>568</v>
       </c>
       <c r="Q88" t="s">
-        <v>567</v>
+        <v>569</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="s">
-        <v>568</v>
+        <v>570</v>
       </c>
       <c r="B89" t="s">
-        <v>569</v>
+        <v>571</v>
       </c>
       <c r="C89" s="1" t="n">
         <v>43973</v>
       </c>
       <c r="D89" t="s">
-        <v>570</v>
+        <v>572</v>
       </c>
       <c r="E89" t="s">
-        <v>571</v>
+        <v>573</v>
       </c>
       <c r="F89"/>
       <c r="G89" t="n">
@@ -6900,36 +6910,36 @@
         <v>1.012</v>
       </c>
       <c r="N89" t="s">
-        <v>571</v>
+        <v>573</v>
       </c>
       <c r="O89" t="s">
-        <v>572</v>
+        <v>574</v>
       </c>
       <c r="P89" t="s">
         <v>92</v>
       </c>
       <c r="Q89" t="s">
-        <v>573</v>
+        <v>575</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="s">
-        <v>568</v>
+        <v>570</v>
       </c>
       <c r="B90" t="s">
-        <v>574</v>
+        <v>576</v>
       </c>
       <c r="C90" s="1" t="n">
         <v>43992</v>
       </c>
       <c r="D90" t="s">
-        <v>575</v>
+        <v>577</v>
       </c>
       <c r="E90" t="s">
-        <v>571</v>
+        <v>573</v>
       </c>
       <c r="F90" t="s">
-        <v>576</v>
+        <v>578</v>
       </c>
       <c r="G90" t="n">
         <v>46</v>
@@ -6953,186 +6963,186 @@
         <v>1.142</v>
       </c>
       <c r="N90" t="s">
-        <v>571</v>
+        <v>573</v>
       </c>
       <c r="O90" t="s">
-        <v>572</v>
+        <v>574</v>
       </c>
       <c r="P90" t="s">
         <v>22</v>
       </c>
       <c r="Q90" t="s">
-        <v>577</v>
+        <v>579</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="s">
-        <v>578</v>
+        <v>580</v>
       </c>
       <c r="B91" t="s">
-        <v>579</v>
+        <v>581</v>
       </c>
       <c r="C91" s="1" t="n">
-        <v>43991</v>
+        <v>43993</v>
       </c>
       <c r="D91" t="s">
-        <v>580</v>
+        <v>582</v>
       </c>
       <c r="E91" t="s">
-        <v>581</v>
+        <v>583</v>
       </c>
       <c r="F91"/>
       <c r="G91" t="n">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="H91" t="n">
-        <v>21693633</v>
+        <v>22418881</v>
       </c>
       <c r="I91" t="n">
-        <v>65.539</v>
+        <v>67.73</v>
       </c>
       <c r="J91" t="n">
-        <v>879364</v>
+        <v>367990</v>
       </c>
       <c r="K91" t="n">
-        <v>2.657</v>
+        <v>1.112</v>
       </c>
       <c r="L91" t="n">
-        <v>397889</v>
+        <v>372520</v>
       </c>
       <c r="M91" t="n">
-        <v>1.202</v>
+        <v>1.125</v>
       </c>
       <c r="N91" t="s">
-        <v>581</v>
+        <v>583</v>
       </c>
       <c r="O91" t="s">
-        <v>582</v>
+        <v>584</v>
       </c>
       <c r="P91" t="s">
-        <v>583</v>
+        <v>585</v>
       </c>
       <c r="Q91" t="s">
-        <v>584</v>
+        <v>586</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="s">
-        <v>578</v>
+        <v>580</v>
       </c>
       <c r="B92" t="s">
-        <v>585</v>
+        <v>587</v>
       </c>
       <c r="C92" s="1" t="n">
-        <v>43992</v>
+        <v>43993</v>
       </c>
       <c r="D92" t="s">
-        <v>586</v>
+        <v>588</v>
       </c>
       <c r="E92" t="s">
-        <v>587</v>
+        <v>589</v>
       </c>
       <c r="F92"/>
       <c r="G92" t="n">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="H92" t="n">
-        <v>21467820</v>
+        <v>21933301</v>
       </c>
       <c r="I92" t="n">
-        <v>64.857</v>
+        <v>66.263</v>
       </c>
       <c r="J92" t="n">
-        <v>419637</v>
+        <v>446765</v>
       </c>
       <c r="K92" t="n">
-        <v>1.268</v>
+        <v>1.35</v>
       </c>
       <c r="L92" t="n">
-        <v>460724</v>
+        <v>449582</v>
       </c>
       <c r="M92" t="n">
-        <v>1.392</v>
+        <v>1.358</v>
       </c>
       <c r="N92" t="s">
-        <v>587</v>
+        <v>589</v>
       </c>
       <c r="O92" t="s">
-        <v>588</v>
+        <v>590</v>
       </c>
       <c r="P92" t="s">
-        <v>589</v>
+        <v>591</v>
       </c>
       <c r="Q92" t="s">
-        <v>590</v>
+        <v>592</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="s">
-        <v>591</v>
+        <v>593</v>
       </c>
       <c r="B93" t="s">
-        <v>592</v>
+        <v>594</v>
       </c>
       <c r="C93" s="1" t="n">
-        <v>43993</v>
+        <v>43994</v>
       </c>
       <c r="D93" t="s">
-        <v>593</v>
+        <v>595</v>
       </c>
       <c r="E93" t="s">
         <v>124</v>
       </c>
       <c r="F93"/>
       <c r="G93" t="n">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="H93" t="n">
-        <v>50473</v>
+        <v>51313</v>
       </c>
       <c r="I93" t="n">
-        <v>14.53</v>
+        <v>14.772</v>
       </c>
       <c r="J93" t="n">
-        <v>820</v>
+        <v>840</v>
       </c>
       <c r="K93" t="n">
-        <v>0.236</v>
+        <v>0.242</v>
       </c>
       <c r="L93" t="n">
-        <v>671</v>
+        <v>686</v>
       </c>
       <c r="M93" t="n">
-        <v>0.193</v>
+        <v>0.197</v>
       </c>
       <c r="N93" t="s">
         <v>124</v>
       </c>
       <c r="O93" t="s">
-        <v>594</v>
+        <v>596</v>
       </c>
       <c r="P93" t="s">
         <v>22</v>
       </c>
       <c r="Q93" t="s">
-        <v>595</v>
+        <v>597</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="s">
-        <v>596</v>
+        <v>598</v>
       </c>
       <c r="B94" t="s">
-        <v>597</v>
+        <v>599</v>
       </c>
       <c r="C94" s="1" t="n">
         <v>43950</v>
       </c>
       <c r="D94" t="s">
-        <v>598</v>
+        <v>600</v>
       </c>
       <c r="E94" t="s">
-        <v>599</v>
+        <v>601</v>
       </c>
       <c r="F94"/>
       <c r="G94" t="n">
@@ -7153,33 +7163,33 @@
         <v>0.112</v>
       </c>
       <c r="N94" t="s">
-        <v>599</v>
+        <v>601</v>
       </c>
       <c r="O94" t="s">
-        <v>600</v>
+        <v>602</v>
       </c>
       <c r="P94" t="s">
-        <v>601</v>
+        <v>603</v>
       </c>
       <c r="Q94" t="s">
-        <v>602</v>
+        <v>604</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="s">
-        <v>603</v>
+        <v>605</v>
       </c>
       <c r="B95" t="s">
-        <v>604</v>
+        <v>606</v>
       </c>
       <c r="C95" s="1" t="n">
         <v>43992</v>
       </c>
       <c r="D95" t="s">
-        <v>605</v>
+        <v>607</v>
       </c>
       <c r="E95" t="s">
-        <v>606</v>
+        <v>608</v>
       </c>
       <c r="F95"/>
       <c r="G95" t="n">
@@ -7204,16 +7214,16 @@
         <v>0.027</v>
       </c>
       <c r="N95" t="s">
-        <v>606</v>
+        <v>608</v>
       </c>
       <c r="O95" t="s">
-        <v>607</v>
+        <v>609</v>
       </c>
       <c r="P95" t="s">
         <v>22</v>
       </c>
       <c r="Q95" t="s">
-        <v>608</v>
+        <v>610</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated testing data for 2020-06-13
</commit_message>
<xml_diff>
--- a/public/data/testing/covid-testing-latest-data-source-details.xlsx
+++ b/public/data/testing/covid-testing-latest-data-source-details.xlsx
@@ -71,7 +71,7 @@
     <t xml:space="preserve">Argentina - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.argentina.gob.ar/sites/default/files/11-06-20_reporte_matutino_covid_19.pdf</t>
+    <t xml:space="preserve">https://www.argentina.gob.ar/sites/default/files/13-06-20-reporte-matutino-covid-19.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">Government of Argentina</t>
@@ -112,7 +112,7 @@
     <t xml:space="preserve">Austria - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200611180612/https://www.sozialministerium.at/Informationen-zum-Coronavirus/Neuartiges-Coronavirus-(2019-nCov).html</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200613164008/https://www.sozialministerium.at/Informationen-zum-Coronavirus/Neuartiges-Coronavirus-(2019-nCov).html</t>
   </si>
   <si>
     <t xml:space="preserve">Austrian Ministry for Health</t>
@@ -139,7 +139,7 @@
     <t xml:space="preserve">Bahrain - units unclear</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200612073353/https://www.moh.gov.bh/COVID19</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200613164010/https://www.moh.gov.bh/COVID19</t>
   </si>
   <si>
     <t xml:space="preserve">Ministry of Health</t>
@@ -187,7 +187,7 @@
     <t xml:space="preserve">Belarus - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">http://minzdrav.gov.by/ru/sobytiya/v-belarusi-na-8-iyunya-vyzdoroveli-i-vypisany-23-tys-880-patsientov/</t>
+    <t xml:space="preserve">http://minzdrav.gov.by/ru/sobytiya/v-belarusi-vyzdoroveli-i-vypisany-29111-patsientov/</t>
   </si>
   <si>
     <t xml:space="preserve">Belarus Ministry of Health</t>
@@ -233,7 +233,7 @@
     <t xml:space="preserve">Bolivia - units unclear</t>
   </si>
   <si>
-    <t xml:space="preserve">https://minsalud.gob.bo/4275-ministerio-de-salud-reporta-695-nuevos-contagios-de-coronavirus-en-bolivia-y-el-total-sube-a-14-644</t>
+    <t xml:space="preserve">https://minsalud.gob.bo/4284-ministerio-de-salud-reporta-884-nuevos-contagios-de-coronavirus-y-el-total-asciende-a-16-165</t>
   </si>
   <si>
     <t xml:space="preserve">https://www.minsalud.gob.bo/</t>
@@ -280,7 +280,7 @@
     <t xml:space="preserve">Bulgaria - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200612073357/https://coronavirus.bg/</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200612225405/https://coronavirus.bg/</t>
   </si>
   <si>
     <t xml:space="preserve">Bulgaria COVID-10 Information Portal</t>
@@ -303,7 +303,7 @@
     <t xml:space="preserve">Canada - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200612073358/https://www.canada.ca/en/public-health/services/diseases/2019-novel-coronavirus-infection.html</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200612225406/https://www.canada.ca/en/public-health/services/diseases/2019-novel-coronavirus-infection.html</t>
   </si>
   <si>
     <t xml:space="preserve">Government of Canada</t>
@@ -391,7 +391,7 @@
     <t xml:space="preserve">Croatia - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200611180652/https://www.koronavirus.hr/najnovije/ukupno-dosad-382-zarazene-osobe-u-hrvatskoj/35</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200613164311/https://www.koronavirus.hr/najnovije/ukupno-dosad-382-zarazene-osobe-u-hrvatskoj/35</t>
   </si>
   <si>
     <t xml:space="preserve">Government of Croatia</t>
@@ -454,7 +454,7 @@
     <t xml:space="preserve">Denmark - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://files.ssi.dk/Data-Epidemiologiske-Rapport-11062020-9ha2</t>
+    <t xml:space="preserve">https://files.ssi.dk/Data-Epidemiologiske-Rapport-12062020-12ju</t>
   </si>
   <si>
     <t xml:space="preserve">Statens Serum Institut</t>
@@ -473,7 +473,7 @@
     <t xml:space="preserve">Ecuador - units unclear</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.gestionderiesgos.gob.ec/wp-content/uploads/2020/06/INFOGRAFIA-NACIONALCOVI-19-COE-NACIONAL-10062020-08h00.pdf</t>
+    <t xml:space="preserve">https://www.gestionderiesgos.gob.ec/wp-content/uploads/2020/06/INFOGRAFIA-NACIONALCOVI-19-COE-NACIONAL-12062020-08h00.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">Government of Ecuador</t>
@@ -542,7 +542,7 @@
     <t xml:space="preserve">Ethiopia - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.ephi.gov.et/images/novel_coronavirus/confirmed-case-Press-release_June-11-Eng_V2.pdf</t>
+    <t xml:space="preserve">https://www.ephi.gov.et/images/novel_coronavirus/confirmed-case-Press-release_June-13-Eng_V2.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">Ethiopian Public Health Institute</t>
@@ -697,7 +697,7 @@
     <t xml:space="preserve">Greece - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://eody.gov.gr/wp-content/uploads/2020/06/covid-gr-daily-report-20200611.pdf</t>
+    <t xml:space="preserve">https://eody.gov.gr/wp-content/uploads/2020/06/covid-gr-daily-report-20200613.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">National Organization of Public Health</t>
@@ -876,7 +876,7 @@
     <t xml:space="preserve">Israel - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://govextra.gov.il/media/20524/covid19-data-israel-04062020.csv</t>
+    <t xml:space="preserve">https://govextra.gov.il/media/20556/covid19-data-israel-05062020.csv</t>
   </si>
   <si>
     <t xml:space="preserve">Israel Ministry of Health</t>
@@ -933,7 +933,7 @@
     <t xml:space="preserve">Japan - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.mhlw.go.jp/stf/newpage_11820.html</t>
+    <t xml:space="preserve">https://www.mhlw.go.jp/stf/newpage_11850.html</t>
   </si>
   <si>
     <t xml:space="preserve">Ministry of Health, Labor and Welfare Press Release</t>
@@ -957,10 +957,10 @@
     <t xml:space="preserve">Japan - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.mhlw.go.jp/content/10906000/000638974.pdf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The cumulative total reported in the press release (540,823) does not sum to the cumulative total calculated from the weekly and daily figures reported by the MOH. See: https://www.mhlw.go.jp/content/10906000/000638974.pdf</t>
+    <t xml:space="preserve">https://www.mhlw.go.jp/content/10906000/000639347.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The cumulative total reported in the press release (551,768) does not sum to the cumulative total calculated from the weekly and daily figures reported by the MOH. See: https://www.mhlw.go.jp/content/10906000/000639347.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">On 11th April 2020, the MOH started providing a daily time series on the "Implementation status of PCR tests for new coronavirus in Japan (based on the date on which results were determined" (via Google translate). 
@@ -1033,7 +1033,7 @@
     <t xml:space="preserve">Lithuania - samples tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200612073946/http://sam.lrv.lt/lt/naujienos/koronavirusas</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200613164427/http://sam.lrv.lt/lt/naujienos/koronavirusas</t>
   </si>
   <si>
     <t xml:space="preserve">http://sam.lrv.lt/lt/naujienos/koronavirusas</t>
@@ -1049,7 +1049,7 @@
     <t xml:space="preserve">Luxembourg - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200611181101/https://gouvernement.lu/en/dossiers.gouv_msan%2Ben%2Bdossiers%2B2020%2Bcorona-virus.html</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200613164428/https://gouvernement.lu/en/dossiers.gouv_msan%2Ben%2Bdossiers%2B2020%2Bcorona-virus.html</t>
   </si>
   <si>
     <t xml:space="preserve">Luxembourg Government situation update</t>
@@ -1070,13 +1070,13 @@
     <t xml:space="preserve">Malaysia - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.facebook.com/kementeriankesihatanmalaysia/videos/270663217507305</t>
+    <t xml:space="preserve">https://www.facebook.com/373560576236/videos/686827878765381</t>
   </si>
   <si>
     <t xml:space="preserve">Ministry of Health Malaysia</t>
   </si>
   <si>
-    <t xml:space="preserve">Statistics on testing can be see at 18:21 timestamp on the MOH livestream</t>
+    <t xml:space="preserve">Statistics on testing can be see at 38:11 timestamp on the MOH livestream</t>
   </si>
   <si>
     <t xml:space="preserve">http://covid-19.moh.gov.my/terkini</t>
@@ -1096,13 +1096,13 @@
     <t xml:space="preserve">Maldives - samples tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.facebook.com/MinistryOfHealthMV/videos/308883413841135/</t>
+    <t xml:space="preserve">https://www.facebook.com/561317043971945/videos/2629831207290787/</t>
   </si>
   <si>
     <t xml:space="preserve">Maldives Ministry of Health</t>
   </si>
   <si>
-    <t xml:space="preserve">Numbers visible in video at time: 1:05</t>
+    <t xml:space="preserve">Numbers visible in video at time: 0:59</t>
   </si>
   <si>
     <t xml:space="preserve">Maldives Ministry of Health Official Facebook page</t>
@@ -1133,8 +1133,8 @@
   </si>
   <si>
     <t xml:space="preserve">The Government of Mexico makes a dataset available along with [its COVID-19 dashboard](https://coronavirus.gob.mx/datos/#DownZCSV).
-The file can be downloaded in CSV format, and gives detailed information on each case (1 row per case). The RESULTADO column gives the status of the case, with 1 = CONFIRMED and 2 = NEGATIVE. The resulting tally can be found [on the dashboard](https://coronavirus.gob.mx/datos/). We do not include pending tests (RESULTADO = 3).
-While geographical coverage is complete, there is a time lag in the publication of the data, and recent days systematically show temporarily low figures. Data starts on 1 January 2020; we do not know if this is because tests started on that date or because earlier data is not available.
+The file can be downloaded in CSV format, and gives detailed information on each case (1 row per case). The RESULTADO column gives the status of the case, with 1 = POSITIVE, 2 = NEGATIVE, 3 = PENDING. We do not include pending tests in our time series, and we remove recent days where the proportion of pending tests (RESULTADO = 3) is above 50%, to avoid publishing a time series that drops substantially in the last few days.
+Data starts on 1 January 2020; we do not know if this is because tests started on that date or because earlier data is not available.
 The notes to the data provide the following note "Information from the Epidemiological Surveillance System for Viral Respiratory Diseases, reported by the 475 viral respiratory disease monitoring units (USMER) throughout the country in the entire health sector (IMSS, ISSSTE, SEDENA, SEMAR, ETC).... Preliminary data subject to validation by the Ministry of Health through the General Directorate of Epidemiology. The information contained corresponds only to the data obtained from the epidemiological study of a suspected case of viral respiratory disease at the time it is identified in the medical units of the Health Sector".</t>
   </si>
   <si>
@@ -1247,7 +1247,7 @@
     <t xml:space="preserve">Nigeria - samples tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200611181808/https://covid19.ncdc.gov.ng/</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200613164734/https://covid19.ncdc.gov.ng/</t>
   </si>
   <si>
     <t xml:space="preserve">Nigeria Centre for Disease Control</t>
@@ -1267,7 +1267,7 @@
     <t xml:space="preserve">Norway - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.fhi.no/contentassets/ca5914bd0aa14e15a17f8a7d48fa306a/2020.06.11---dagsrapport-norge-covid-19.pdf</t>
+    <t xml:space="preserve">https://www.fhi.no/contentassets/ca5914bd0aa14e15a17f8a7d48fa306a/2020.06.12---dagsrapport-norge-covid-19.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">Norwegian Institute of Public Health</t>
@@ -1292,7 +1292,7 @@
     <t xml:space="preserve">Pakistan - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200612074015/http://www.covid.gov.pk/</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200613164737/http://www.covid.gov.pk/</t>
   </si>
   <si>
     <t xml:space="preserve">Government of Pakistan</t>
@@ -1311,13 +1311,10 @@
     <t xml:space="preserve">Panama - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">http://minsa.gob.pa/covid-23</t>
+    <t xml:space="preserve">http://minsa.gob.pa/covid-19</t>
   </si>
   <si>
     <t xml:space="preserve">Panama Ministry of Health</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://minsa.gob.pa/covid-19</t>
   </si>
   <si>
     <t xml:space="preserve">The Panama Ministry of Health reports the cumulative number of tests performed ("pruebas realizadas") on [their official dashboard](http://minsa.gob.pa/covid-19) with a time series dating back to 9 March 2020. The page with testing numbers is not the first one shown but can be navigated to with the arrows at the bottom of the dashboard. The dashboard shows the cumulative number of total, positive, negative, and control tests ("prueba de control") performed. We report here the total of positive and negative numbers because: 1) the time series only includes positive and negative test numbers; and 2) the total they provide seems to include control tests, which we understand to be used for testing quality control.</t>
@@ -1348,7 +1345,7 @@
     <t xml:space="preserve">Peru - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.gob.pe/institucion/minsa/noticias/186578-minsa-casos-confirmados-por-coronavirus-covid-19-ascienden-a-214-788-en-el-peru-comunicado-n-129</t>
+    <t xml:space="preserve">https://www.gob.pe/institucion/minsa/noticias/186668-minsa-casos-confirmados-por-coronavirus-covid-19-ascienden-a-220-749-en-el-peru-comunicado-n-130</t>
   </si>
   <si>
     <t xml:space="preserve">Ministry of Health, Government of Peru</t>
@@ -1454,7 +1451,7 @@
     <t xml:space="preserve">Romania - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://gov.ro/ro/media/comunicate/buletin-de-presa-11-iunie-2020-ora-13-00&amp;page=1</t>
+    <t xml:space="preserve">https://gov.ro/ro/media/comunicate/buletin-de-presa-13-iunie-2020-ora-13-00&amp;page=1</t>
   </si>
   <si>
     <t xml:space="preserve">Ministry of Internal Affairs</t>
@@ -1472,7 +1469,7 @@
     <t xml:space="preserve">Russia - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://rospotrebnadzor.ru/about/info/news/news_details.php?ELEMENT_ID=14685</t>
+    <t xml:space="preserve">https://rospotrebnadzor.ru/about/info/news/news_details.php?ELEMENT_ID=14689</t>
   </si>
   <si>
     <t xml:space="preserve">Government of the Russian Federation</t>
@@ -1599,7 +1596,7 @@
     <t xml:space="preserve">Slovakia - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200612074024/https://korona.gov.sk/</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200613164748/https://korona.gov.sk/</t>
   </si>
   <si>
     <t xml:space="preserve">National Center of Health Information and the Office of the Government of the Slovak Republic</t>
@@ -1673,7 +1670,7 @@
     <t xml:space="preserve">South Korea - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.cdc.go.kr/board/board.es?mid=&amp;bid=0030&amp;act=view&amp;list_no=367497&amp;tag=&amp;nPage=1</t>
+    <t xml:space="preserve">https://www.cdc.go.kr/board/board.es?mid=&amp;bid=0030&amp;act=view&amp;list_no=367511&amp;tag=&amp;nPage=1</t>
   </si>
   <si>
     <t xml:space="preserve">South Korea CDC</t>
@@ -1719,10 +1716,13 @@
     <t xml:space="preserve">Sweden - people tested</t>
   </si>
   <si>
+    <t xml:space="preserve">https://www.folkhalsomyndigheten.se/smittskydd-beredskap/utbrott/aktuella-utbrott/covid-19/antal-individer-som-har-testats-for-covid-19/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Public Health Agency</t>
+  </si>
+  <si>
     <t xml:space="preserve">https://www.folkhalsomyndigheten.se/smittskydd-beredskap/utbrott/aktuella-utbrott/covid-19/bekraftade-fall-i-sverige</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Public Health Agency</t>
   </si>
   <si>
     <t xml:space="preserve">The weekly report gives the cumulative total of individuals "analyzed for the virus that causes covid-19 in Sweden", along with weekly totals.
@@ -1779,7 +1779,7 @@
     <t xml:space="preserve">Thailand - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200611181957/https://ddc.moph.go.th/viralpneumonia/eng/index.php</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200612230804/https://ddc.moph.go.th/viralpneumonia/eng/index.php</t>
   </si>
   <si>
     <t xml:space="preserve">Department of Disease Control</t>
@@ -1849,7 +1849,7 @@
     <t xml:space="preserve">Turkey - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200611182000/https://covid19.saglik.gov.tr/</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200612230807/https://covid19.saglik.gov.tr/</t>
   </si>
   <si>
     <t xml:space="preserve">Turkish Ministry of Health</t>
@@ -1873,7 +1873,7 @@
     <t xml:space="preserve">Uganda - samples tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/MinofHealthUG/status/1270989725797679104/photo/1</t>
+    <t xml:space="preserve">https://twitter.com/MinofHealthUG/status/1271351705649721344</t>
   </si>
   <si>
     <t xml:space="preserve">Press Release from the Office of the Director General</t>
@@ -1897,7 +1897,7 @@
     <t xml:space="preserve">Ukraine - units unclear</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200612074110/https://covid19.gov.ua/en</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200613164831/https://covid19.gov.ua/en</t>
   </si>
   <si>
     <t xml:space="preserve">Cabinet of Ministers of Ukraine</t>
@@ -1934,7 +1934,7 @@
     <t xml:space="preserve">United Kingdom - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://assets.publishing.service.gov.uk/government/uploads/system/uploads/attachment_data/file/891711/2020-06-11_COVID-19_UK_testing_time_series.csv</t>
+    <t xml:space="preserve">https://assets.publishing.service.gov.uk/government/uploads/system/uploads/attachment_data/file/892130/2020-06-13-covid-19-testing-time-series.csv</t>
   </si>
   <si>
     <t xml:space="preserve">Sum of pillar 1 + pillar 2 (tests processed only)</t>
@@ -1955,7 +1955,7 @@
     <t xml:space="preserve">United States - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200612074112/https://www.cdc.gov/coronavirus/2019-ncov/cases-updates/testing-in-us.html</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200612230811/https://www.cdc.gov/coronavirus/2019-ncov/cases-updates/testing-in-us.html</t>
   </si>
   <si>
     <t xml:space="preserve">United States CDC</t>
@@ -2009,7 +2009,7 @@
     <t xml:space="preserve">Uruguay - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.gub.uy/ministerio-salud-publica/comunicacion/noticias/actualizacion-informacion-relacion-coronavirus-covid-19-uruguay-51</t>
+    <t xml:space="preserve">https://www.gub.uy/ministerio-salud-publica/comunicacion/noticias/actualizacion-informacion-relacion-coronavirus-covid-19-uruguay-52</t>
   </si>
   <si>
     <t xml:space="preserve">https://www.gub.uy/ministerio-salud-publica/comunicacion/noticias</t>
@@ -2458,7 +2458,7 @@
         <v>18</v>
       </c>
       <c r="C2" s="1" t="n">
-        <v>43993</v>
+        <v>43995</v>
       </c>
       <c r="D2" t="s">
         <v>19</v>
@@ -2468,25 +2468,25 @@
       </c>
       <c r="F2"/>
       <c r="G2" t="n">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="H2" t="n">
-        <v>214807</v>
+        <v>228324</v>
       </c>
       <c r="I2" t="n">
-        <v>4.753</v>
+        <v>5.052</v>
       </c>
       <c r="J2" t="n">
-        <v>6288</v>
+        <v>7019</v>
       </c>
       <c r="K2" t="n">
-        <v>0.139</v>
+        <v>0.155</v>
       </c>
       <c r="L2" t="n">
-        <v>5194</v>
+        <v>5578</v>
       </c>
       <c r="M2" t="n">
-        <v>0.115</v>
+        <v>0.123</v>
       </c>
       <c r="N2" t="s">
         <v>20</v>
@@ -2560,7 +2560,7 @@
         <v>31</v>
       </c>
       <c r="C4" s="1" t="n">
-        <v>43993</v>
+        <v>43995</v>
       </c>
       <c r="D4" t="s">
         <v>32</v>
@@ -2570,25 +2570,21 @@
       </c>
       <c r="F4"/>
       <c r="G4" t="n">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="H4" t="n">
-        <v>512501</v>
+        <v>520976</v>
       </c>
       <c r="I4" t="n">
-        <v>56.904</v>
-      </c>
-      <c r="J4" t="n">
-        <v>6157</v>
-      </c>
-      <c r="K4" t="n">
-        <v>0.684</v>
-      </c>
+        <v>57.845</v>
+      </c>
+      <c r="J4"/>
+      <c r="K4"/>
       <c r="L4" t="n">
-        <v>5862</v>
+        <v>5009</v>
       </c>
       <c r="M4" t="n">
-        <v>0.651</v>
+        <v>0.556</v>
       </c>
       <c r="N4" t="s">
         <v>34</v>
@@ -2611,7 +2607,7 @@
         <v>39</v>
       </c>
       <c r="C5" s="1" t="n">
-        <v>43994</v>
+        <v>43995</v>
       </c>
       <c r="D5" t="s">
         <v>40</v>
@@ -2621,25 +2617,25 @@
       </c>
       <c r="F5"/>
       <c r="G5" t="n">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="H5" t="n">
-        <v>403036</v>
+        <v>410842</v>
       </c>
       <c r="I5" t="n">
-        <v>236.859</v>
+        <v>241.447</v>
       </c>
       <c r="J5" t="n">
-        <v>9126</v>
+        <v>7806</v>
       </c>
       <c r="K5" t="n">
-        <v>5.363</v>
+        <v>4.587</v>
       </c>
       <c r="L5" t="n">
-        <v>6988</v>
+        <v>7067</v>
       </c>
       <c r="M5" t="n">
-        <v>4.107</v>
+        <v>4.153</v>
       </c>
       <c r="N5" t="s">
         <v>42</v>
@@ -2713,7 +2709,7 @@
         <v>54</v>
       </c>
       <c r="C7" s="1" t="n">
-        <v>43990</v>
+        <v>43995</v>
       </c>
       <c r="D7" t="s">
         <v>55</v>
@@ -2723,25 +2719,21 @@
       </c>
       <c r="F7"/>
       <c r="G7" t="n">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="H7" t="n">
-        <v>632993</v>
+        <v>714324</v>
       </c>
       <c r="I7" t="n">
-        <v>66.988</v>
-      </c>
-      <c r="J7" t="n">
-        <v>10680</v>
-      </c>
-      <c r="K7" t="n">
-        <v>1.13</v>
-      </c>
+        <v>75.595</v>
+      </c>
+      <c r="J7"/>
+      <c r="K7"/>
       <c r="L7" t="n">
-        <v>11374</v>
+        <v>14841</v>
       </c>
       <c r="M7" t="n">
-        <v>1.204</v>
+        <v>1.571</v>
       </c>
       <c r="N7" t="s">
         <v>56</v>
@@ -2764,7 +2756,7 @@
         <v>60</v>
       </c>
       <c r="C8" s="1" t="n">
-        <v>43991</v>
+        <v>43993</v>
       </c>
       <c r="D8" t="s">
         <v>61</v>
@@ -2774,25 +2766,25 @@
       </c>
       <c r="F8"/>
       <c r="G8" t="n">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="H8" t="n">
-        <v>775013</v>
+        <v>794709</v>
       </c>
       <c r="I8" t="n">
-        <v>66.871</v>
+        <v>68.571</v>
       </c>
       <c r="J8" t="n">
-        <v>9191</v>
+        <v>8204</v>
       </c>
       <c r="K8" t="n">
-        <v>0.793</v>
+        <v>0.708</v>
       </c>
       <c r="L8" t="n">
-        <v>8407</v>
+        <v>8525</v>
       </c>
       <c r="M8" t="n">
-        <v>0.725</v>
+        <v>0.736</v>
       </c>
       <c r="N8" t="s">
         <v>62</v>
@@ -2815,7 +2807,7 @@
         <v>67</v>
       </c>
       <c r="C9" s="1" t="n">
-        <v>43991</v>
+        <v>43993</v>
       </c>
       <c r="D9" t="s">
         <v>68</v>
@@ -2825,25 +2817,25 @@
       </c>
       <c r="F9"/>
       <c r="G9" t="n">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="H9" t="n">
-        <v>39610</v>
+        <v>42741</v>
       </c>
       <c r="I9" t="n">
-        <v>3.393</v>
+        <v>3.662</v>
       </c>
       <c r="J9" t="n">
-        <v>1518</v>
+        <v>1706</v>
       </c>
       <c r="K9" t="n">
-        <v>0.13</v>
+        <v>0.146</v>
       </c>
       <c r="L9" t="n">
-        <v>1203</v>
+        <v>1256</v>
       </c>
       <c r="M9" t="n">
-        <v>0.103</v>
+        <v>0.108</v>
       </c>
       <c r="N9" t="s">
         <v>41</v>
@@ -2911,7 +2903,7 @@
         <v>81</v>
       </c>
       <c r="C11" s="1" t="n">
-        <v>43994</v>
+        <v>43995</v>
       </c>
       <c r="D11" t="s">
         <v>82</v>
@@ -2921,25 +2913,25 @@
       </c>
       <c r="F11"/>
       <c r="G11" t="n">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H11" t="n">
-        <v>98460</v>
+        <v>101102</v>
       </c>
       <c r="I11" t="n">
-        <v>14.17</v>
+        <v>14.55</v>
       </c>
       <c r="J11" t="n">
-        <v>2640</v>
+        <v>2642</v>
       </c>
       <c r="K11" t="n">
         <v>0.38</v>
       </c>
       <c r="L11" t="n">
-        <v>1510</v>
+        <v>1717</v>
       </c>
       <c r="M11" t="n">
-        <v>0.217</v>
+        <v>0.247</v>
       </c>
       <c r="N11" t="s">
         <v>84</v>
@@ -2962,7 +2954,7 @@
         <v>88</v>
       </c>
       <c r="C12" s="1" t="n">
-        <v>43994</v>
+        <v>43995</v>
       </c>
       <c r="D12" t="s">
         <v>89</v>
@@ -2972,25 +2964,25 @@
       </c>
       <c r="F12"/>
       <c r="G12" t="n">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H12" t="n">
-        <v>2028420</v>
+        <v>2072020</v>
       </c>
       <c r="I12" t="n">
-        <v>53.744</v>
+        <v>54.899</v>
       </c>
       <c r="J12" t="n">
-        <v>39241</v>
+        <v>43600</v>
       </c>
       <c r="K12" t="n">
-        <v>1.04</v>
+        <v>1.155</v>
       </c>
       <c r="L12" t="n">
-        <v>29091</v>
+        <v>34514</v>
       </c>
       <c r="M12" t="n">
-        <v>0.771</v>
+        <v>0.914</v>
       </c>
       <c r="N12" t="s">
         <v>90</v>
@@ -3013,7 +3005,7 @@
         <v>95</v>
       </c>
       <c r="C13" s="1" t="n">
-        <v>43993</v>
+        <v>43995</v>
       </c>
       <c r="D13" t="s">
         <v>96</v>
@@ -3025,25 +3017,25 @@
         <v>97</v>
       </c>
       <c r="G13" t="n">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="H13" t="n">
-        <v>781043</v>
+        <v>819999</v>
       </c>
       <c r="I13" t="n">
-        <v>40.858</v>
+        <v>42.895</v>
       </c>
       <c r="J13" t="n">
-        <v>19976</v>
+        <v>20223</v>
       </c>
       <c r="K13" t="n">
-        <v>1.045</v>
+        <v>1.058</v>
       </c>
       <c r="L13" t="n">
-        <v>19181</v>
+        <v>18927</v>
       </c>
       <c r="M13" t="n">
-        <v>1.003</v>
+        <v>0.99</v>
       </c>
       <c r="N13" t="s">
         <v>98</v>
@@ -3066,7 +3058,7 @@
         <v>102</v>
       </c>
       <c r="C14" s="1" t="n">
-        <v>43993</v>
+        <v>43994</v>
       </c>
       <c r="D14" t="s">
         <v>103</v>
@@ -3076,25 +3068,25 @@
       </c>
       <c r="F14"/>
       <c r="G14" t="n">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="H14" t="n">
-        <v>458324</v>
+        <v>470351</v>
       </c>
       <c r="I14" t="n">
-        <v>9.007</v>
+        <v>9.244</v>
       </c>
       <c r="J14" t="n">
-        <v>13391</v>
+        <v>12027</v>
       </c>
       <c r="K14" t="n">
-        <v>0.263</v>
+        <v>0.236</v>
       </c>
       <c r="L14" t="n">
-        <v>11962</v>
+        <v>11916</v>
       </c>
       <c r="M14" t="n">
-        <v>0.235</v>
+        <v>0.234</v>
       </c>
       <c r="N14" t="s">
         <v>104</v>
@@ -3117,7 +3109,7 @@
         <v>109</v>
       </c>
       <c r="C15" s="1" t="n">
-        <v>43993</v>
+        <v>43994</v>
       </c>
       <c r="D15" t="s">
         <v>110</v>
@@ -3127,25 +3119,25 @@
       </c>
       <c r="F15"/>
       <c r="G15" t="n">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="H15" t="n">
-        <v>22741</v>
+        <v>23224</v>
       </c>
       <c r="I15" t="n">
-        <v>4.464</v>
+        <v>4.559</v>
       </c>
       <c r="J15" t="n">
-        <v>381</v>
+        <v>483</v>
       </c>
       <c r="K15" t="n">
-        <v>0.075</v>
+        <v>0.095</v>
       </c>
       <c r="L15" t="n">
-        <v>320</v>
+        <v>326</v>
       </c>
       <c r="M15" t="n">
-        <v>0.063</v>
+        <v>0.064</v>
       </c>
       <c r="N15" t="s">
         <v>111</v>
@@ -3168,7 +3160,7 @@
         <v>115</v>
       </c>
       <c r="C16" s="1" t="n">
-        <v>43993</v>
+        <v>43995</v>
       </c>
       <c r="D16" t="s">
         <v>116</v>
@@ -3178,25 +3170,25 @@
       </c>
       <c r="F16"/>
       <c r="G16" t="n">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="H16" t="n">
-        <v>69606</v>
+        <v>69967</v>
       </c>
       <c r="I16" t="n">
-        <v>16.955</v>
+        <v>17.043</v>
       </c>
       <c r="J16" t="n">
-        <v>257</v>
+        <v>246</v>
       </c>
       <c r="K16" t="n">
-        <v>0.063</v>
+        <v>0.06</v>
       </c>
       <c r="L16" t="n">
-        <v>230</v>
+        <v>208</v>
       </c>
       <c r="M16" t="n">
-        <v>0.056</v>
+        <v>0.051</v>
       </c>
       <c r="N16" t="s">
         <v>117</v>
@@ -3219,7 +3211,7 @@
         <v>122</v>
       </c>
       <c r="C17" s="1" t="n">
-        <v>43992</v>
+        <v>43994</v>
       </c>
       <c r="D17" t="s">
         <v>123</v>
@@ -3231,25 +3223,25 @@
         <v>125</v>
       </c>
       <c r="G17" t="n">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="H17" t="n">
-        <v>127042</v>
+        <v>131628</v>
       </c>
       <c r="I17" t="n">
-        <v>11.216</v>
+        <v>11.621</v>
       </c>
       <c r="J17" t="n">
-        <v>2095</v>
+        <v>2496</v>
       </c>
       <c r="K17" t="n">
-        <v>0.185</v>
+        <v>0.22</v>
       </c>
       <c r="L17" t="n">
-        <v>2085</v>
+        <v>2166</v>
       </c>
       <c r="M17" t="n">
-        <v>0.184</v>
+        <v>0.191</v>
       </c>
       <c r="N17" t="s">
         <v>124</v>
@@ -3272,7 +3264,7 @@
         <v>130</v>
       </c>
       <c r="C18" s="1" t="n">
-        <v>43993</v>
+        <v>43994</v>
       </c>
       <c r="D18" t="s">
         <v>131</v>
@@ -3282,25 +3274,25 @@
       </c>
       <c r="F18"/>
       <c r="G18" t="n">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="H18" t="n">
-        <v>491193</v>
+        <v>494805</v>
       </c>
       <c r="I18" t="n">
-        <v>45.867</v>
+        <v>46.205</v>
       </c>
       <c r="J18" t="n">
-        <v>3546</v>
+        <v>3234</v>
       </c>
       <c r="K18" t="n">
-        <v>0.331</v>
+        <v>0.302</v>
       </c>
       <c r="L18" t="n">
-        <v>3576</v>
+        <v>3496</v>
       </c>
       <c r="M18" t="n">
-        <v>0.334</v>
+        <v>0.326</v>
       </c>
       <c r="N18" t="s">
         <v>41</v>
@@ -3323,7 +3315,7 @@
         <v>135</v>
       </c>
       <c r="C19" s="1" t="n">
-        <v>43992</v>
+        <v>43993</v>
       </c>
       <c r="D19" t="s">
         <v>136</v>
@@ -3333,25 +3325,25 @@
       </c>
       <c r="F19"/>
       <c r="G19" t="n">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="H19" t="n">
-        <v>732716</v>
+        <v>754640</v>
       </c>
       <c r="I19" t="n">
-        <v>126.5</v>
+        <v>130.285</v>
       </c>
       <c r="J19" t="n">
-        <v>4376</v>
+        <v>3914</v>
       </c>
       <c r="K19" t="n">
-        <v>0.755</v>
+        <v>0.676</v>
       </c>
       <c r="L19" t="n">
-        <v>9323</v>
+        <v>10757</v>
       </c>
       <c r="M19" t="n">
-        <v>1.61</v>
+        <v>1.857</v>
       </c>
       <c r="N19" t="s">
         <v>137</v>
@@ -3374,7 +3366,7 @@
         <v>141</v>
       </c>
       <c r="C20" s="1" t="n">
-        <v>43992</v>
+        <v>43994</v>
       </c>
       <c r="D20" t="s">
         <v>142</v>
@@ -3386,21 +3378,21 @@
         <v>144</v>
       </c>
       <c r="G20" t="n">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="H20" t="n">
-        <v>83400</v>
+        <v>87561</v>
       </c>
       <c r="I20" t="n">
-        <v>4.727</v>
+        <v>4.963</v>
       </c>
       <c r="J20"/>
       <c r="K20"/>
       <c r="L20" t="n">
-        <v>1239</v>
+        <v>1326</v>
       </c>
       <c r="M20" t="n">
-        <v>0.07</v>
+        <v>0.075</v>
       </c>
       <c r="N20" t="s">
         <v>143</v>
@@ -3474,7 +3466,7 @@
         <v>154</v>
       </c>
       <c r="C22" s="1" t="n">
-        <v>43993</v>
+        <v>43994</v>
       </c>
       <c r="D22" t="s">
         <v>155</v>
@@ -3484,25 +3476,25 @@
       </c>
       <c r="F22"/>
       <c r="G22" t="n">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="H22" t="n">
-        <v>94716</v>
+        <v>95380</v>
       </c>
       <c r="I22" t="n">
-        <v>71.401</v>
+        <v>71.901</v>
       </c>
       <c r="J22" t="n">
-        <v>884</v>
+        <v>666</v>
       </c>
       <c r="K22" t="n">
-        <v>0.666</v>
+        <v>0.502</v>
       </c>
       <c r="L22" t="n">
-        <v>879</v>
+        <v>852</v>
       </c>
       <c r="M22" t="n">
-        <v>0.663</v>
+        <v>0.642</v>
       </c>
       <c r="N22" t="s">
         <v>157</v>
@@ -3525,7 +3517,7 @@
         <v>162</v>
       </c>
       <c r="C23" s="1" t="n">
-        <v>43993</v>
+        <v>43995</v>
       </c>
       <c r="D23" t="s">
         <v>163</v>
@@ -3535,22 +3527,18 @@
       </c>
       <c r="F23"/>
       <c r="G23" t="n">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="H23" t="n">
-        <v>165151</v>
+        <v>176504</v>
       </c>
       <c r="I23" t="n">
-        <v>1.437</v>
-      </c>
-      <c r="J23" t="n">
-        <v>6630</v>
-      </c>
-      <c r="K23" t="n">
-        <v>0.058</v>
-      </c>
+        <v>1.535</v>
+      </c>
+      <c r="J23"/>
+      <c r="K23"/>
       <c r="L23" t="n">
-        <v>5608</v>
+        <v>5620</v>
       </c>
       <c r="M23" t="n">
         <v>0.049</v>
@@ -3576,7 +3564,7 @@
         <v>168</v>
       </c>
       <c r="C24" s="1" t="n">
-        <v>43991</v>
+        <v>43993</v>
       </c>
       <c r="D24" t="s">
         <v>169</v>
@@ -3586,25 +3574,25 @@
       </c>
       <c r="F24"/>
       <c r="G24" t="n">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="H24" t="n">
-        <v>211220</v>
+        <v>217103</v>
       </c>
       <c r="I24" t="n">
-        <v>38.121</v>
+        <v>39.183</v>
       </c>
       <c r="J24" t="n">
-        <v>2474</v>
+        <v>2604</v>
       </c>
       <c r="K24" t="n">
-        <v>0.447</v>
+        <v>0.47</v>
       </c>
       <c r="L24" t="n">
-        <v>2080</v>
+        <v>2096</v>
       </c>
       <c r="M24" t="n">
-        <v>0.375</v>
+        <v>0.378</v>
       </c>
       <c r="N24" t="s">
         <v>171</v>
@@ -3827,7 +3815,7 @@
         <v>201</v>
       </c>
       <c r="C29" s="1" t="n">
-        <v>43989</v>
+        <v>43991</v>
       </c>
       <c r="D29" t="s">
         <v>194</v>
@@ -3839,25 +3827,25 @@
         <v>202</v>
       </c>
       <c r="G29" t="n">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="H29" t="n">
-        <v>239395</v>
+        <v>242218</v>
       </c>
       <c r="I29" t="n">
-        <v>7.704</v>
+        <v>7.795</v>
       </c>
       <c r="J29" t="n">
-        <v>3952</v>
+        <v>2014</v>
       </c>
       <c r="K29" t="n">
-        <v>0.127</v>
+        <v>0.065</v>
       </c>
       <c r="L29" t="n">
-        <v>2796</v>
+        <v>2736</v>
       </c>
       <c r="M29" t="n">
-        <v>0.09</v>
+        <v>0.088</v>
       </c>
       <c r="N29" t="s">
         <v>197</v>
@@ -3880,7 +3868,7 @@
         <v>204</v>
       </c>
       <c r="C30" s="1" t="n">
-        <v>43993</v>
+        <v>43995</v>
       </c>
       <c r="D30" t="s">
         <v>205</v>
@@ -3890,21 +3878,25 @@
       </c>
       <c r="F30"/>
       <c r="G30" t="n">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="H30" t="n">
-        <v>237276</v>
+        <v>247452</v>
       </c>
       <c r="I30" t="n">
-        <v>22.765</v>
-      </c>
-      <c r="J30"/>
-      <c r="K30"/>
+        <v>23.741</v>
+      </c>
+      <c r="J30" t="n">
+        <v>3585</v>
+      </c>
+      <c r="K30" t="n">
+        <v>0.344</v>
+      </c>
       <c r="L30" t="n">
-        <v>6192</v>
+        <v>5104</v>
       </c>
       <c r="M30" t="n">
-        <v>0.594</v>
+        <v>0.49</v>
       </c>
       <c r="N30" t="s">
         <v>207</v>
@@ -3974,7 +3966,7 @@
         <v>218</v>
       </c>
       <c r="C32" s="1" t="n">
-        <v>43993</v>
+        <v>43994</v>
       </c>
       <c r="D32" t="s">
         <v>219</v>
@@ -3986,25 +3978,25 @@
         <v>221</v>
       </c>
       <c r="G32" t="n">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="H32" t="n">
-        <v>222247</v>
+        <v>226669</v>
       </c>
       <c r="I32" t="n">
-        <v>23.006</v>
+        <v>23.464</v>
       </c>
       <c r="J32" t="n">
-        <v>4558</v>
+        <v>4422</v>
       </c>
       <c r="K32" t="n">
-        <v>0.472</v>
+        <v>0.458</v>
       </c>
       <c r="L32" t="n">
-        <v>3765</v>
+        <v>3438</v>
       </c>
       <c r="M32" t="n">
-        <v>0.39</v>
+        <v>0.356</v>
       </c>
       <c r="N32" t="s">
         <v>220</v>
@@ -4027,7 +4019,7 @@
         <v>226</v>
       </c>
       <c r="C33" s="1" t="n">
-        <v>43992</v>
+        <v>43994</v>
       </c>
       <c r="D33" t="s">
         <v>227</v>
@@ -4037,25 +4029,25 @@
       </c>
       <c r="F33"/>
       <c r="G33" t="n">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="H33" t="n">
-        <v>62935</v>
+        <v>63083</v>
       </c>
       <c r="I33" t="n">
-        <v>184.425</v>
+        <v>184.859</v>
       </c>
       <c r="J33" t="n">
-        <v>65</v>
+        <v>79</v>
       </c>
       <c r="K33" t="n">
-        <v>0.19</v>
+        <v>0.232</v>
       </c>
       <c r="L33" t="n">
-        <v>185</v>
+        <v>51</v>
       </c>
       <c r="M33" t="n">
-        <v>0.542</v>
+        <v>0.149</v>
       </c>
       <c r="N33" t="s">
         <v>228</v>
@@ -4131,7 +4123,7 @@
         <v>237</v>
       </c>
       <c r="C35" s="1" t="n">
-        <v>43993</v>
+        <v>43995</v>
       </c>
       <c r="D35" t="s">
         <v>233</v>
@@ -4143,25 +4135,25 @@
         <v>235</v>
       </c>
       <c r="G35" t="n">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="H35" t="n">
-        <v>5213140</v>
+        <v>5507182</v>
       </c>
       <c r="I35" t="n">
-        <v>3.778</v>
+        <v>3.991</v>
       </c>
       <c r="J35" t="n">
-        <v>151808</v>
+        <v>143737</v>
       </c>
       <c r="K35" t="n">
-        <v>0.11</v>
+        <v>0.104</v>
       </c>
       <c r="L35" t="n">
-        <v>138632</v>
+        <v>140409</v>
       </c>
       <c r="M35" t="n">
-        <v>0.1</v>
+        <v>0.102</v>
       </c>
       <c r="N35" t="s">
         <v>234</v>
@@ -4184,7 +4176,7 @@
         <v>239</v>
       </c>
       <c r="C36" s="1" t="n">
-        <v>43993</v>
+        <v>43995</v>
       </c>
       <c r="D36" t="s">
         <v>240</v>
@@ -4194,25 +4186,25 @@
       </c>
       <c r="F36"/>
       <c r="G36" t="n">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="H36" t="n">
-        <v>294671</v>
+        <v>313275</v>
       </c>
       <c r="I36" t="n">
-        <v>1.077</v>
+        <v>1.145</v>
       </c>
       <c r="J36" t="n">
-        <v>7193</v>
+        <v>11128</v>
       </c>
       <c r="K36" t="n">
-        <v>0.026</v>
+        <v>0.041</v>
       </c>
       <c r="L36" t="n">
-        <v>6134</v>
+        <v>6934</v>
       </c>
       <c r="M36" t="n">
-        <v>0.022</v>
+        <v>0.025</v>
       </c>
       <c r="N36" t="s">
         <v>241</v>
@@ -4333,7 +4325,7 @@
         <v>258</v>
       </c>
       <c r="C39" s="1" t="n">
-        <v>43986</v>
+        <v>43987</v>
       </c>
       <c r="D39" t="s">
         <v>259</v>
@@ -4343,25 +4335,25 @@
       </c>
       <c r="F39"/>
       <c r="G39" t="n">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="H39" t="n">
-        <v>621147</v>
+        <v>637829</v>
       </c>
       <c r="I39" t="n">
-        <v>71.763</v>
+        <v>73.69</v>
       </c>
       <c r="J39" t="n">
-        <v>14604</v>
+        <v>16334</v>
       </c>
       <c r="K39" t="n">
-        <v>1.687</v>
+        <v>1.887</v>
       </c>
       <c r="L39" t="n">
-        <v>8001</v>
+        <v>10118</v>
       </c>
       <c r="M39" t="n">
-        <v>0.924</v>
+        <v>1.169</v>
       </c>
       <c r="N39" t="s">
         <v>41</v>
@@ -4384,7 +4376,7 @@
         <v>264</v>
       </c>
       <c r="C40" s="1" t="n">
-        <v>43993</v>
+        <v>43995</v>
       </c>
       <c r="D40" t="s">
         <v>265</v>
@@ -4396,25 +4388,25 @@
         <v>267</v>
       </c>
       <c r="G40" t="n">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="H40" t="n">
-        <v>2746545</v>
+        <v>2817076</v>
       </c>
       <c r="I40" t="n">
-        <v>45.426</v>
+        <v>46.593</v>
       </c>
       <c r="J40" t="n">
-        <v>32991</v>
+        <v>32880</v>
       </c>
       <c r="K40" t="n">
-        <v>0.546</v>
+        <v>0.544</v>
       </c>
       <c r="L40" t="n">
-        <v>31680</v>
+        <v>31112</v>
       </c>
       <c r="M40" t="n">
-        <v>0.524</v>
+        <v>0.515</v>
       </c>
       <c r="N40" t="s">
         <v>268</v>
@@ -4437,7 +4429,7 @@
         <v>271</v>
       </c>
       <c r="C41" s="1" t="n">
-        <v>43993</v>
+        <v>43995</v>
       </c>
       <c r="D41" t="s">
         <v>265</v>
@@ -4449,25 +4441,25 @@
         <v>267</v>
       </c>
       <c r="G41" t="n">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="H41" t="n">
-        <v>4443821</v>
+        <v>4564191</v>
       </c>
       <c r="I41" t="n">
-        <v>73.498</v>
+        <v>75.489</v>
       </c>
       <c r="J41" t="n">
-        <v>62472</v>
+        <v>49750</v>
       </c>
       <c r="K41" t="n">
-        <v>1.033</v>
+        <v>0.823</v>
       </c>
       <c r="L41" t="n">
-        <v>56325</v>
+        <v>53876</v>
       </c>
       <c r="M41" t="n">
-        <v>0.932</v>
+        <v>0.891</v>
       </c>
       <c r="N41" t="s">
         <v>268</v>
@@ -4490,7 +4482,7 @@
         <v>274</v>
       </c>
       <c r="C42" s="1" t="n">
-        <v>43993</v>
+        <v>43994</v>
       </c>
       <c r="D42" t="s">
         <v>275</v>
@@ -4502,18 +4494,18 @@
         <v>277</v>
       </c>
       <c r="G42" t="n">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="H42" t="n">
-        <v>328730</v>
+        <v>332207</v>
       </c>
       <c r="I42" t="n">
-        <v>2.599</v>
+        <v>2.627</v>
       </c>
       <c r="J42"/>
       <c r="K42"/>
       <c r="L42" t="n">
-        <v>3585</v>
+        <v>3535</v>
       </c>
       <c r="M42" t="n">
         <v>0.028</v>
@@ -4539,7 +4531,7 @@
         <v>281</v>
       </c>
       <c r="C43" s="1" t="n">
-        <v>43991</v>
+        <v>43992</v>
       </c>
       <c r="D43" t="s">
         <v>282</v>
@@ -4551,25 +4543,25 @@
         <v>283</v>
       </c>
       <c r="G43" t="n">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="H43" t="n">
-        <v>540832</v>
+        <v>551777</v>
       </c>
       <c r="I43" t="n">
-        <v>4.276</v>
+        <v>4.363</v>
       </c>
       <c r="J43" t="n">
-        <v>6960</v>
+        <v>7325</v>
       </c>
       <c r="K43" t="n">
-        <v>0.055</v>
+        <v>0.058</v>
       </c>
       <c r="L43" t="n">
-        <v>6052</v>
+        <v>6516</v>
       </c>
       <c r="M43" t="n">
-        <v>0.048</v>
+        <v>0.052</v>
       </c>
       <c r="N43" t="s">
         <v>278</v>
@@ -4694,7 +4686,7 @@
         <v>298</v>
       </c>
       <c r="C46" s="1" t="n">
-        <v>43994</v>
+        <v>43995</v>
       </c>
       <c r="D46" t="s">
         <v>299</v>
@@ -4706,25 +4698,25 @@
         <v>301</v>
       </c>
       <c r="G46" t="n">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="H46" t="n">
-        <v>124662</v>
+        <v>126054</v>
       </c>
       <c r="I46" t="n">
-        <v>66.092</v>
+        <v>66.83</v>
       </c>
       <c r="J46" t="n">
-        <v>1298</v>
+        <v>1392</v>
       </c>
       <c r="K46" t="n">
-        <v>0.688</v>
+        <v>0.738</v>
       </c>
       <c r="L46" t="n">
-        <v>1314</v>
+        <v>1360</v>
       </c>
       <c r="M46" t="n">
-        <v>0.697</v>
+        <v>0.721</v>
       </c>
       <c r="N46" t="s">
         <v>300</v>
@@ -4747,7 +4739,7 @@
         <v>304</v>
       </c>
       <c r="C47" s="1" t="n">
-        <v>43994</v>
+        <v>43995</v>
       </c>
       <c r="D47" t="s">
         <v>305</v>
@@ -4757,25 +4749,25 @@
       </c>
       <c r="F47"/>
       <c r="G47" t="n">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="H47" t="n">
-        <v>356062</v>
+        <v>360670</v>
       </c>
       <c r="I47" t="n">
-        <v>130.795</v>
+        <v>132.488</v>
       </c>
       <c r="J47" t="n">
-        <v>5274</v>
+        <v>4608</v>
       </c>
       <c r="K47" t="n">
-        <v>1.937</v>
+        <v>1.693</v>
       </c>
       <c r="L47" t="n">
-        <v>4253</v>
+        <v>4464</v>
       </c>
       <c r="M47" t="n">
-        <v>1.562</v>
+        <v>1.64</v>
       </c>
       <c r="N47" t="s">
         <v>41</v>
@@ -4798,7 +4790,7 @@
         <v>309</v>
       </c>
       <c r="C48" s="1" t="n">
-        <v>43993</v>
+        <v>43995</v>
       </c>
       <c r="D48" t="s">
         <v>310</v>
@@ -4808,25 +4800,25 @@
       </c>
       <c r="F48"/>
       <c r="G48" t="n">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="H48" t="n">
-        <v>98232</v>
+        <v>106062</v>
       </c>
       <c r="I48" t="n">
-        <v>156.926</v>
+        <v>169.435</v>
       </c>
       <c r="J48" t="n">
-        <v>7029</v>
+        <v>4185</v>
       </c>
       <c r="K48" t="n">
-        <v>11.229</v>
+        <v>6.686</v>
       </c>
       <c r="L48" t="n">
-        <v>2265</v>
+        <v>3018</v>
       </c>
       <c r="M48" t="n">
-        <v>3.618</v>
+        <v>4.821</v>
       </c>
       <c r="N48" t="s">
         <v>311</v>
@@ -4849,7 +4841,7 @@
         <v>315</v>
       </c>
       <c r="C49" s="1" t="n">
-        <v>43993</v>
+        <v>43994</v>
       </c>
       <c r="D49" t="s">
         <v>316</v>
@@ -4861,25 +4853,25 @@
         <v>318</v>
       </c>
       <c r="G49" t="n">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="H49" t="n">
-        <v>631608</v>
+        <v>640680</v>
       </c>
       <c r="I49" t="n">
-        <v>19.515</v>
+        <v>19.795</v>
       </c>
       <c r="J49" t="n">
-        <v>5833</v>
+        <v>9072</v>
       </c>
       <c r="K49" t="n">
-        <v>0.18</v>
+        <v>0.28</v>
       </c>
       <c r="L49" t="n">
-        <v>7017</v>
+        <v>7152</v>
       </c>
       <c r="M49" t="n">
-        <v>0.217</v>
+        <v>0.221</v>
       </c>
       <c r="N49" t="s">
         <v>41</v>
@@ -4902,7 +4894,7 @@
         <v>322</v>
       </c>
       <c r="C50" s="1" t="n">
-        <v>43991</v>
+        <v>43992</v>
       </c>
       <c r="D50" t="s">
         <v>323</v>
@@ -4914,21 +4906,25 @@
         <v>325</v>
       </c>
       <c r="G50" t="n">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="H50" t="n">
-        <v>31355</v>
+        <v>32127</v>
       </c>
       <c r="I50" t="n">
-        <v>58.007</v>
-      </c>
-      <c r="J50"/>
-      <c r="K50"/>
+        <v>59.435</v>
+      </c>
+      <c r="J50" t="n">
+        <v>772</v>
+      </c>
+      <c r="K50" t="n">
+        <v>1.428</v>
+      </c>
       <c r="L50" t="n">
-        <v>823</v>
+        <v>841</v>
       </c>
       <c r="M50" t="n">
-        <v>1.523</v>
+        <v>1.556</v>
       </c>
       <c r="N50" t="s">
         <v>326</v>
@@ -4951,7 +4947,7 @@
         <v>330</v>
       </c>
       <c r="C51" s="1" t="n">
-        <v>43992</v>
+        <v>43990</v>
       </c>
       <c r="D51" t="s">
         <v>331</v>
@@ -4961,25 +4957,25 @@
       </c>
       <c r="F51"/>
       <c r="G51" t="n">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="H51" t="n">
-        <v>325416</v>
+        <v>329283</v>
       </c>
       <c r="I51" t="n">
-        <v>2.524</v>
+        <v>2.554</v>
       </c>
       <c r="J51" t="n">
-        <v>310</v>
+        <v>7220</v>
       </c>
       <c r="K51" t="n">
-        <v>0.002</v>
+        <v>0.056</v>
       </c>
       <c r="L51" t="n">
-        <v>4050</v>
+        <v>6820</v>
       </c>
       <c r="M51" t="n">
-        <v>0.031</v>
+        <v>0.053</v>
       </c>
       <c r="N51" t="s">
         <v>333</v>
@@ -5210,7 +5206,7 @@
         <v>364</v>
       </c>
       <c r="C56" s="1" t="n">
-        <v>43993</v>
+        <v>43994</v>
       </c>
       <c r="D56" t="s">
         <v>365</v>
@@ -5220,25 +5216,25 @@
       </c>
       <c r="F56"/>
       <c r="G56" t="n">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="H56" t="n">
-        <v>304832</v>
+        <v>307810</v>
       </c>
       <c r="I56" t="n">
-        <v>63.214</v>
+        <v>63.831</v>
       </c>
       <c r="J56" t="n">
-        <v>2950</v>
+        <v>2978</v>
       </c>
       <c r="K56" t="n">
-        <v>0.612</v>
+        <v>0.618</v>
       </c>
       <c r="L56" t="n">
-        <v>2264</v>
+        <v>2259</v>
       </c>
       <c r="M56" t="n">
-        <v>0.469</v>
+        <v>0.468</v>
       </c>
       <c r="N56" t="s">
         <v>366</v>
@@ -5261,7 +5257,7 @@
         <v>369</v>
       </c>
       <c r="C57" s="1" t="n">
-        <v>43993</v>
+        <v>43995</v>
       </c>
       <c r="D57" t="s">
         <v>370</v>
@@ -5271,25 +5267,21 @@
       </c>
       <c r="F57"/>
       <c r="G57" t="n">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="H57" t="n">
-        <v>85375</v>
+        <v>90464</v>
       </c>
       <c r="I57" t="n">
-        <v>0.414</v>
-      </c>
-      <c r="J57" t="n">
-        <v>2440</v>
-      </c>
-      <c r="K57" t="n">
-        <v>0.012</v>
-      </c>
+        <v>0.439</v>
+      </c>
+      <c r="J57"/>
+      <c r="K57"/>
       <c r="L57" t="n">
-        <v>2006</v>
+        <v>2209</v>
       </c>
       <c r="M57" t="n">
-        <v>0.01</v>
+        <v>0.011</v>
       </c>
       <c r="N57" t="s">
         <v>371</v>
@@ -5312,7 +5304,7 @@
         <v>375</v>
       </c>
       <c r="C58" s="1" t="n">
-        <v>43993</v>
+        <v>43995</v>
       </c>
       <c r="D58" t="s">
         <v>376</v>
@@ -5322,25 +5314,21 @@
       </c>
       <c r="F58"/>
       <c r="G58" t="n">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="H58" t="n">
-        <v>272905</v>
+        <v>277253</v>
       </c>
       <c r="I58" t="n">
-        <v>50.34</v>
-      </c>
-      <c r="J58" t="n">
-        <v>5028</v>
-      </c>
-      <c r="K58" t="n">
-        <v>0.927</v>
-      </c>
+        <v>51.142</v>
+      </c>
+      <c r="J58"/>
+      <c r="K58"/>
       <c r="L58" t="n">
-        <v>2599</v>
+        <v>2615</v>
       </c>
       <c r="M58" t="n">
-        <v>0.479</v>
+        <v>0.482</v>
       </c>
       <c r="N58" t="s">
         <v>377</v>
@@ -5363,7 +5351,7 @@
         <v>382</v>
       </c>
       <c r="C59" s="1" t="n">
-        <v>43994</v>
+        <v>43995</v>
       </c>
       <c r="D59" t="s">
         <v>383</v>
@@ -5373,25 +5361,25 @@
       </c>
       <c r="F59"/>
       <c r="G59" t="n">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="H59" t="n">
-        <v>809169</v>
+        <v>839019</v>
       </c>
       <c r="I59" t="n">
-        <v>3.663</v>
+        <v>3.798</v>
       </c>
       <c r="J59" t="n">
-        <v>28344</v>
+        <v>29850</v>
       </c>
       <c r="K59" t="n">
-        <v>0.128</v>
+        <v>0.135</v>
       </c>
       <c r="L59" t="n">
-        <v>24407</v>
+        <v>25502</v>
       </c>
       <c r="M59" t="n">
-        <v>0.11</v>
+        <v>0.115</v>
       </c>
       <c r="N59" t="s">
         <v>384</v>
@@ -5414,7 +5402,7 @@
         <v>388</v>
       </c>
       <c r="C60" s="1" t="n">
-        <v>43991</v>
+        <v>43993</v>
       </c>
       <c r="D60" t="s">
         <v>389</v>
@@ -5424,54 +5412,54 @@
       </c>
       <c r="F60"/>
       <c r="G60" t="n">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="H60" t="n">
-        <v>78132</v>
+        <v>82391</v>
       </c>
       <c r="I60" t="n">
-        <v>18.108</v>
+        <v>19.095</v>
       </c>
       <c r="J60" t="n">
-        <v>1419</v>
+        <v>2218</v>
       </c>
       <c r="K60" t="n">
-        <v>0.329</v>
+        <v>0.514</v>
       </c>
       <c r="L60" t="n">
-        <v>1577</v>
+        <v>1735</v>
       </c>
       <c r="M60" t="n">
-        <v>0.365</v>
+        <v>0.402</v>
       </c>
       <c r="N60" t="s">
         <v>390</v>
       </c>
       <c r="O60" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="P60" t="s">
         <v>22</v>
       </c>
       <c r="Q60" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="s">
+        <v>392</v>
+      </c>
+      <c r="B61" t="s">
         <v>393</v>
-      </c>
-      <c r="B61" t="s">
-        <v>394</v>
       </c>
       <c r="C61" s="1" t="n">
         <v>43992</v>
       </c>
       <c r="D61" t="s">
+        <v>394</v>
+      </c>
+      <c r="E61" t="s">
         <v>395</v>
-      </c>
-      <c r="E61" t="s">
-        <v>396</v>
       </c>
       <c r="F61"/>
       <c r="G61" t="n">
@@ -5496,140 +5484,140 @@
         <v>0.173</v>
       </c>
       <c r="N61" t="s">
+        <v>395</v>
+      </c>
+      <c r="O61" t="s">
         <v>396</v>
-      </c>
-      <c r="O61" t="s">
-        <v>397</v>
       </c>
       <c r="P61" t="s">
         <v>51</v>
       </c>
       <c r="Q61" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="s">
+        <v>398</v>
+      </c>
+      <c r="B62" t="s">
         <v>399</v>
       </c>
-      <c r="B62" t="s">
+      <c r="C62" s="1" t="n">
+        <v>43995</v>
+      </c>
+      <c r="D62" t="s">
         <v>400</v>
-      </c>
-      <c r="C62" s="1" t="n">
-        <v>43994</v>
-      </c>
-      <c r="D62" t="s">
-        <v>401</v>
       </c>
       <c r="E62" t="s">
         <v>41</v>
       </c>
       <c r="F62"/>
       <c r="G62" t="n">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="H62" t="n">
-        <v>179364</v>
+        <v>183143</v>
       </c>
       <c r="I62" t="n">
-        <v>5.44</v>
+        <v>5.555</v>
       </c>
       <c r="J62" t="n">
-        <v>3612</v>
+        <v>3779</v>
       </c>
       <c r="K62" t="n">
-        <v>0.11</v>
+        <v>0.115</v>
       </c>
       <c r="L62" t="n">
-        <v>3656</v>
+        <v>3425</v>
       </c>
       <c r="M62" t="n">
-        <v>0.111</v>
+        <v>0.104</v>
       </c>
       <c r="N62" t="s">
+        <v>401</v>
+      </c>
+      <c r="O62" t="s">
         <v>402</v>
-      </c>
-      <c r="O62" t="s">
-        <v>403</v>
       </c>
       <c r="P62" t="s">
         <v>92</v>
       </c>
       <c r="Q62" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="s">
+        <v>404</v>
+      </c>
+      <c r="B63" t="s">
         <v>405</v>
       </c>
-      <c r="B63" t="s">
+      <c r="C63" s="1" t="n">
+        <v>43992</v>
+      </c>
+      <c r="D63" t="s">
         <v>406</v>
       </c>
-      <c r="C63" s="1" t="n">
-        <v>43991</v>
-      </c>
-      <c r="D63" t="s">
+      <c r="E63" t="s">
         <v>407</v>
       </c>
-      <c r="E63" t="s">
+      <c r="F63" t="s">
         <v>408</v>
       </c>
-      <c r="F63" t="s">
-        <v>409</v>
-      </c>
       <c r="G63" t="n">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="H63" t="n">
-        <v>427121</v>
+        <v>436448</v>
       </c>
       <c r="I63" t="n">
-        <v>3.898</v>
+        <v>3.983</v>
       </c>
       <c r="J63" t="n">
-        <v>10920</v>
+        <v>9327</v>
       </c>
       <c r="K63" t="n">
-        <v>0.1</v>
+        <v>0.085</v>
       </c>
       <c r="L63" t="n">
-        <v>11399</v>
+        <v>11300</v>
       </c>
       <c r="M63" t="n">
-        <v>0.104</v>
+        <v>0.103</v>
       </c>
       <c r="N63" t="s">
         <v>213</v>
       </c>
       <c r="O63" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="P63" t="s">
         <v>92</v>
       </c>
       <c r="Q63" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="s">
+        <v>410</v>
+      </c>
+      <c r="B64" t="s">
         <v>411</v>
-      </c>
-      <c r="B64" t="s">
-        <v>412</v>
       </c>
       <c r="C64" s="1" t="n">
         <v>43985</v>
       </c>
       <c r="D64" t="s">
+        <v>412</v>
+      </c>
+      <c r="E64" t="s">
         <v>413</v>
       </c>
-      <c r="E64" t="s">
+      <c r="F64" t="s">
         <v>414</v>
-      </c>
-      <c r="F64" t="s">
-        <v>415</v>
       </c>
       <c r="G64" t="n">
         <v>91</v>
@@ -5653,30 +5641,30 @@
         <v>0.538</v>
       </c>
       <c r="N64" t="s">
+        <v>415</v>
+      </c>
+      <c r="O64" t="s">
         <v>416</v>
-      </c>
-      <c r="O64" t="s">
-        <v>417</v>
       </c>
       <c r="P64" t="s">
         <v>51</v>
       </c>
       <c r="Q64" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="s">
+        <v>418</v>
+      </c>
+      <c r="B65" t="s">
         <v>419</v>
-      </c>
-      <c r="B65" t="s">
-        <v>420</v>
       </c>
       <c r="C65" s="1" t="n">
         <v>43991</v>
       </c>
       <c r="D65" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="E65" t="s">
         <v>41</v>
@@ -5704,186 +5692,182 @@
         <v>1.25</v>
       </c>
       <c r="N65" t="s">
+        <v>421</v>
+      </c>
+      <c r="O65" t="s">
+        <v>420</v>
+      </c>
+      <c r="P65" t="s">
         <v>422</v>
       </c>
-      <c r="O65" t="s">
-        <v>421</v>
-      </c>
-      <c r="P65" t="s">
+      <c r="Q65" t="s">
         <v>423</v>
-      </c>
-      <c r="Q65" t="s">
-        <v>424</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="s">
+        <v>424</v>
+      </c>
+      <c r="B66" t="s">
         <v>425</v>
       </c>
-      <c r="B66" t="s">
+      <c r="C66" s="1" t="n">
+        <v>43994</v>
+      </c>
+      <c r="D66" t="s">
         <v>426</v>
       </c>
-      <c r="C66" s="1" t="n">
-        <v>43993</v>
-      </c>
-      <c r="D66" t="s">
+      <c r="E66" t="s">
         <v>427</v>
-      </c>
-      <c r="E66" t="s">
-        <v>428</v>
       </c>
       <c r="F66"/>
       <c r="G66" t="n">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="H66" t="n">
-        <v>274793</v>
+        <v>280665</v>
       </c>
       <c r="I66" t="n">
-        <v>95.379</v>
+        <v>97.417</v>
       </c>
       <c r="J66" t="n">
-        <v>4829</v>
+        <v>5872</v>
       </c>
       <c r="K66" t="n">
-        <v>1.676</v>
+        <v>2.038</v>
       </c>
       <c r="L66" t="n">
-        <v>4815</v>
+        <v>4900</v>
       </c>
       <c r="M66" t="n">
-        <v>1.671</v>
+        <v>1.701</v>
       </c>
       <c r="N66" t="s">
+        <v>427</v>
+      </c>
+      <c r="O66" t="s">
         <v>428</v>
-      </c>
-      <c r="O66" t="s">
-        <v>429</v>
       </c>
       <c r="P66" t="s">
         <v>92</v>
       </c>
       <c r="Q66" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="s">
+        <v>430</v>
+      </c>
+      <c r="B67" t="s">
         <v>431</v>
       </c>
-      <c r="B67" t="s">
+      <c r="C67" s="1" t="n">
+        <v>43995</v>
+      </c>
+      <c r="D67" t="s">
         <v>432</v>
       </c>
-      <c r="C67" s="1" t="n">
-        <v>43993</v>
-      </c>
-      <c r="D67" t="s">
+      <c r="E67" t="s">
         <v>433</v>
-      </c>
-      <c r="E67" t="s">
-        <v>434</v>
       </c>
       <c r="F67"/>
       <c r="G67" t="n">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="H67" t="n">
-        <v>531619</v>
+        <v>552670</v>
       </c>
       <c r="I67" t="n">
-        <v>27.634</v>
-      </c>
-      <c r="J67" t="n">
-        <v>11055</v>
-      </c>
-      <c r="K67" t="n">
-        <v>0.575</v>
-      </c>
+        <v>28.729</v>
+      </c>
+      <c r="J67"/>
+      <c r="K67"/>
       <c r="L67" t="n">
-        <v>8396</v>
+        <v>8037</v>
       </c>
       <c r="M67" t="n">
-        <v>0.436</v>
+        <v>0.418</v>
       </c>
       <c r="N67" t="s">
+        <v>433</v>
+      </c>
+      <c r="O67" t="s">
         <v>434</v>
-      </c>
-      <c r="O67" t="s">
-        <v>435</v>
       </c>
       <c r="P67" t="s">
         <v>22</v>
       </c>
       <c r="Q67" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="s">
+        <v>436</v>
+      </c>
+      <c r="B68" t="s">
         <v>437</v>
       </c>
-      <c r="B68" t="s">
+      <c r="C68" s="1" t="n">
+        <v>43995</v>
+      </c>
+      <c r="D68" t="s">
         <v>438</v>
       </c>
-      <c r="C68" s="1" t="n">
-        <v>43994</v>
-      </c>
-      <c r="D68" t="s">
+      <c r="E68" t="s">
         <v>439</v>
-      </c>
-      <c r="E68" t="s">
-        <v>440</v>
       </c>
       <c r="F68"/>
       <c r="G68" t="n">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="H68" t="n">
-        <v>14218674</v>
+        <v>14574117</v>
       </c>
       <c r="I68" t="n">
-        <v>97.432</v>
+        <v>99.868</v>
       </c>
       <c r="J68" t="n">
-        <v>343577</v>
+        <v>355443</v>
       </c>
       <c r="K68" t="n">
-        <v>2.354</v>
+        <v>2.436</v>
       </c>
       <c r="L68" t="n">
-        <v>309287</v>
+        <v>312164</v>
       </c>
       <c r="M68" t="n">
-        <v>2.119</v>
+        <v>2.139</v>
       </c>
       <c r="N68" t="s">
+        <v>439</v>
+      </c>
+      <c r="O68" t="s">
         <v>440</v>
-      </c>
-      <c r="O68" t="s">
-        <v>441</v>
       </c>
       <c r="P68" t="s">
         <v>22</v>
       </c>
       <c r="Q68" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="s">
+        <v>442</v>
+      </c>
+      <c r="B69" t="s">
         <v>443</v>
-      </c>
-      <c r="B69" t="s">
-        <v>444</v>
       </c>
       <c r="C69" s="1" t="n">
         <v>43992</v>
       </c>
       <c r="D69" t="s">
+        <v>444</v>
+      </c>
+      <c r="E69" t="s">
         <v>445</v>
-      </c>
-      <c r="E69" t="s">
-        <v>446</v>
       </c>
       <c r="F69"/>
       <c r="G69" t="n">
@@ -5908,187 +5892,187 @@
         <v>0.122</v>
       </c>
       <c r="N69" t="s">
+        <v>445</v>
+      </c>
+      <c r="O69" t="s">
         <v>446</v>
-      </c>
-      <c r="O69" t="s">
-        <v>447</v>
       </c>
       <c r="P69" t="s">
         <v>51</v>
       </c>
       <c r="Q69" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="s">
+        <v>448</v>
+      </c>
+      <c r="B70" t="s">
         <v>449</v>
       </c>
-      <c r="B70" t="s">
+      <c r="C70" s="1" t="n">
+        <v>43994</v>
+      </c>
+      <c r="D70" t="s">
         <v>450</v>
-      </c>
-      <c r="C70" s="1" t="n">
-        <v>43993</v>
-      </c>
-      <c r="D70" t="s">
-        <v>451</v>
       </c>
       <c r="E70" t="s">
         <v>41</v>
       </c>
       <c r="F70"/>
       <c r="G70" t="n">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H70" t="n">
-        <v>1042312</v>
+        <v>1069636</v>
       </c>
       <c r="I70" t="n">
-        <v>29.94</v>
+        <v>30.724</v>
       </c>
       <c r="J70" t="n">
-        <v>22500</v>
+        <v>27324</v>
       </c>
       <c r="K70" t="n">
-        <v>0.646</v>
+        <v>0.785</v>
       </c>
       <c r="L70" t="n">
-        <v>22158</v>
+        <v>22952</v>
       </c>
       <c r="M70" t="n">
-        <v>0.636</v>
+        <v>0.659</v>
       </c>
       <c r="N70" t="s">
         <v>41</v>
       </c>
       <c r="O70" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="P70" t="s">
         <v>127</v>
       </c>
       <c r="Q70" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="s">
+        <v>452</v>
+      </c>
+      <c r="B71" t="s">
         <v>453</v>
       </c>
-      <c r="B71" t="s">
+      <c r="C71" s="1" t="n">
+        <v>43995</v>
+      </c>
+      <c r="D71" t="s">
         <v>454</v>
       </c>
-      <c r="C71" s="1" t="n">
-        <v>43993</v>
-      </c>
-      <c r="D71" t="s">
+      <c r="E71" t="s">
         <v>455</v>
       </c>
-      <c r="E71" t="s">
+      <c r="F71" t="s">
         <v>456</v>
       </c>
-      <c r="F71" t="s">
+      <c r="G71" t="n">
+        <v>103</v>
+      </c>
+      <c r="H71" t="n">
+        <v>60286</v>
+      </c>
+      <c r="I71" t="n">
+        <v>3.6</v>
+      </c>
+      <c r="J71" t="n">
+        <v>1378</v>
+      </c>
+      <c r="K71" t="n">
+        <v>0.082</v>
+      </c>
+      <c r="L71" t="n">
+        <v>1204</v>
+      </c>
+      <c r="M71" t="n">
+        <v>0.072</v>
+      </c>
+      <c r="N71" t="s">
         <v>457</v>
       </c>
-      <c r="G71" t="n">
-        <v>101</v>
-      </c>
-      <c r="H71" t="n">
-        <v>57903</v>
-      </c>
-      <c r="I71" t="n">
-        <v>3.458</v>
-      </c>
-      <c r="J71" t="n">
-        <v>1164</v>
-      </c>
-      <c r="K71" t="n">
-        <v>0.07</v>
-      </c>
-      <c r="L71" t="n">
-        <v>1273</v>
-      </c>
-      <c r="M71" t="n">
-        <v>0.076</v>
-      </c>
-      <c r="N71" t="s">
+      <c r="O71" t="s">
         <v>458</v>
       </c>
-      <c r="O71" t="s">
+      <c r="P71" t="s">
         <v>459</v>
       </c>
-      <c r="P71" t="s">
+      <c r="Q71" t="s">
         <v>460</v>
-      </c>
-      <c r="Q71" t="s">
-        <v>461</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="s">
+        <v>461</v>
+      </c>
+      <c r="B72" t="s">
         <v>462</v>
       </c>
-      <c r="B72" t="s">
+      <c r="C72" s="1" t="n">
+        <v>43994</v>
+      </c>
+      <c r="D72" t="s">
         <v>463</v>
-      </c>
-      <c r="C72" s="1" t="n">
-        <v>43993</v>
-      </c>
-      <c r="D72" t="s">
-        <v>464</v>
       </c>
       <c r="E72" t="s">
         <v>41</v>
       </c>
       <c r="F72" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="G72" t="n">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="H72" t="n">
-        <v>291996</v>
+        <v>297789</v>
       </c>
       <c r="I72" t="n">
-        <v>42.912</v>
+        <v>43.763</v>
       </c>
       <c r="J72" t="n">
-        <v>4932</v>
+        <v>5793</v>
       </c>
       <c r="K72" t="n">
-        <v>0.725</v>
+        <v>0.851</v>
       </c>
       <c r="L72" t="n">
-        <v>4390</v>
+        <v>4533</v>
       </c>
       <c r="M72" t="n">
-        <v>0.645</v>
+        <v>0.666</v>
       </c>
       <c r="N72" t="s">
         <v>41</v>
       </c>
       <c r="O72" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="P72" t="s">
         <v>92</v>
       </c>
       <c r="Q72" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="s">
+        <v>467</v>
+      </c>
+      <c r="B73" t="s">
         <v>468</v>
-      </c>
-      <c r="B73" t="s">
-        <v>469</v>
       </c>
       <c r="C73" s="1" t="n">
         <v>43990</v>
       </c>
       <c r="D73" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="E73" t="s">
         <v>41</v>
@@ -6115,27 +6099,27 @@
         <v>41</v>
       </c>
       <c r="O73" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="P73" t="s">
         <v>92</v>
       </c>
       <c r="Q73" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="B74" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="C74" s="1" t="n">
         <v>43990</v>
       </c>
       <c r="D74" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="E74" t="s">
         <v>41</v>
@@ -6162,236 +6146,232 @@
         <v>41</v>
       </c>
       <c r="O74" t="s">
+        <v>470</v>
+      </c>
+      <c r="P74" t="s">
+        <v>474</v>
+      </c>
+      <c r="Q74" t="s">
         <v>471</v>
-      </c>
-      <c r="P74" t="s">
-        <v>475</v>
-      </c>
-      <c r="Q74" t="s">
-        <v>472</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="s">
+        <v>475</v>
+      </c>
+      <c r="B75" t="s">
         <v>476</v>
       </c>
-      <c r="B75" t="s">
+      <c r="C75" s="1" t="n">
+        <v>43995</v>
+      </c>
+      <c r="D75" t="s">
         <v>477</v>
       </c>
-      <c r="C75" s="1" t="n">
-        <v>43994</v>
-      </c>
-      <c r="D75" t="s">
+      <c r="E75" t="s">
         <v>478</v>
-      </c>
-      <c r="E75" t="s">
-        <v>479</v>
       </c>
       <c r="F75"/>
       <c r="G75" t="n">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="H75" t="n">
-        <v>194733</v>
+        <v>196244</v>
       </c>
       <c r="I75" t="n">
-        <v>35.668</v>
+        <v>35.944</v>
       </c>
       <c r="J75" t="n">
-        <v>1262</v>
+        <v>1511</v>
       </c>
       <c r="K75" t="n">
-        <v>0.231</v>
+        <v>0.277</v>
       </c>
       <c r="L75" t="n">
-        <v>1305</v>
+        <v>1144</v>
       </c>
       <c r="M75" t="n">
-        <v>0.239</v>
+        <v>0.21</v>
       </c>
       <c r="N75" t="s">
+        <v>479</v>
+      </c>
+      <c r="O75" t="s">
         <v>480</v>
       </c>
-      <c r="O75" t="s">
+      <c r="P75" t="s">
         <v>481</v>
       </c>
-      <c r="P75" t="s">
+      <c r="Q75" t="s">
         <v>482</v>
-      </c>
-      <c r="Q75" t="s">
-        <v>483</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="s">
+        <v>483</v>
+      </c>
+      <c r="B76" t="s">
         <v>484</v>
       </c>
-      <c r="B76" t="s">
+      <c r="C76" s="1" t="n">
+        <v>43994</v>
+      </c>
+      <c r="D76" t="s">
         <v>485</v>
       </c>
-      <c r="C76" s="1" t="n">
-        <v>43992</v>
-      </c>
-      <c r="D76" t="s">
+      <c r="E76" t="s">
         <v>486</v>
-      </c>
-      <c r="E76" t="s">
-        <v>487</v>
       </c>
       <c r="F76"/>
       <c r="G76" t="n">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="H76" t="n">
-        <v>85626</v>
+        <v>87095</v>
       </c>
       <c r="I76" t="n">
-        <v>41.187</v>
+        <v>41.894</v>
       </c>
       <c r="J76" t="n">
-        <v>758</v>
+        <v>767</v>
       </c>
       <c r="K76" t="n">
-        <v>0.365</v>
+        <v>0.369</v>
       </c>
       <c r="L76" t="n">
-        <v>613</v>
+        <v>603</v>
       </c>
       <c r="M76" t="n">
-        <v>0.295</v>
+        <v>0.29</v>
       </c>
       <c r="N76" t="s">
+        <v>487</v>
+      </c>
+      <c r="O76" t="s">
         <v>488</v>
-      </c>
-      <c r="O76" t="s">
-        <v>489</v>
       </c>
       <c r="P76" t="s">
         <v>22</v>
       </c>
       <c r="Q76" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="s">
+        <v>490</v>
+      </c>
+      <c r="B77" t="s">
         <v>491</v>
       </c>
-      <c r="B77" t="s">
+      <c r="C77" s="1" t="n">
+        <v>43994</v>
+      </c>
+      <c r="D77" t="s">
         <v>492</v>
       </c>
-      <c r="C77" s="1" t="n">
-        <v>43993</v>
-      </c>
-      <c r="D77" t="s">
+      <c r="E77" t="s">
         <v>493</v>
       </c>
-      <c r="E77" t="s">
+      <c r="F77" t="s">
         <v>494</v>
       </c>
-      <c r="F77" t="s">
+      <c r="G77" t="n">
+        <v>104</v>
+      </c>
+      <c r="H77" t="n">
+        <v>1060425</v>
+      </c>
+      <c r="I77" t="n">
+        <v>17.88</v>
+      </c>
+      <c r="J77" t="n">
+        <v>32026</v>
+      </c>
+      <c r="K77" t="n">
+        <v>0.54</v>
+      </c>
+      <c r="L77" t="n">
+        <v>29936</v>
+      </c>
+      <c r="M77" t="n">
+        <v>0.505</v>
+      </c>
+      <c r="N77" t="s">
+        <v>493</v>
+      </c>
+      <c r="O77" t="s">
         <v>495</v>
-      </c>
-      <c r="G77" t="n">
-        <v>103</v>
-      </c>
-      <c r="H77" t="n">
-        <v>1028399</v>
-      </c>
-      <c r="I77" t="n">
-        <v>17.34</v>
-      </c>
-      <c r="J77" t="n">
-        <v>29999</v>
-      </c>
-      <c r="K77" t="n">
-        <v>0.506</v>
-      </c>
-      <c r="L77" t="n">
-        <v>29675</v>
-      </c>
-      <c r="M77" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="N77" t="s">
-        <v>494</v>
-      </c>
-      <c r="O77" t="s">
-        <v>496</v>
       </c>
       <c r="P77" t="s">
         <v>92</v>
       </c>
       <c r="Q77" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="s">
+        <v>497</v>
+      </c>
+      <c r="B78" t="s">
         <v>498</v>
       </c>
-      <c r="B78" t="s">
+      <c r="C78" s="1" t="n">
+        <v>43995</v>
+      </c>
+      <c r="D78" t="s">
         <v>499</v>
       </c>
-      <c r="C78" s="1" t="n">
-        <v>43993</v>
-      </c>
-      <c r="D78" t="s">
+      <c r="E78" t="s">
         <v>500</v>
-      </c>
-      <c r="E78" t="s">
-        <v>501</v>
       </c>
       <c r="F78"/>
       <c r="G78" t="n">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="H78" t="n">
-        <v>1066888</v>
+        <v>1094704</v>
       </c>
       <c r="I78" t="n">
-        <v>20.81</v>
-      </c>
-      <c r="J78" t="n">
-        <v>14916</v>
-      </c>
-      <c r="K78" t="n">
-        <v>0.291</v>
-      </c>
+        <v>21.352</v>
+      </c>
+      <c r="J78"/>
+      <c r="K78"/>
       <c r="L78" t="n">
-        <v>13290</v>
+        <v>12771</v>
       </c>
       <c r="M78" t="n">
-        <v>0.259</v>
+        <v>0.249</v>
       </c>
       <c r="N78" t="s">
+        <v>500</v>
+      </c>
+      <c r="O78" t="s">
         <v>501</v>
-      </c>
-      <c r="O78" t="s">
-        <v>502</v>
       </c>
       <c r="P78" t="s">
         <v>243</v>
       </c>
       <c r="Q78" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="s">
+        <v>503</v>
+      </c>
+      <c r="B79" t="s">
         <v>504</v>
-      </c>
-      <c r="B79" t="s">
-        <v>505</v>
       </c>
       <c r="C79" s="1" t="n">
         <v>43986</v>
       </c>
       <c r="D79" t="s">
+        <v>505</v>
+      </c>
+      <c r="E79" t="s">
         <v>506</v>
-      </c>
-      <c r="E79" t="s">
-        <v>507</v>
       </c>
       <c r="F79"/>
       <c r="G79" t="n">
@@ -6412,33 +6392,33 @@
         <v>0.876</v>
       </c>
       <c r="N79" t="s">
+        <v>507</v>
+      </c>
+      <c r="O79" t="s">
         <v>508</v>
-      </c>
-      <c r="O79" t="s">
-        <v>509</v>
       </c>
       <c r="P79" t="s">
         <v>22</v>
       </c>
       <c r="Q79" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="s">
+        <v>510</v>
+      </c>
+      <c r="B80" t="s">
         <v>511</v>
-      </c>
-      <c r="B80" t="s">
-        <v>512</v>
       </c>
       <c r="C80" s="1" t="n">
         <v>43989</v>
       </c>
       <c r="D80" t="s">
+        <v>512</v>
+      </c>
+      <c r="E80" t="s">
         <v>513</v>
-      </c>
-      <c r="E80" t="s">
-        <v>514</v>
       </c>
       <c r="F80"/>
       <c r="G80" t="n">
@@ -6459,10 +6439,10 @@
         <v>0.696</v>
       </c>
       <c r="N80" t="s">
+        <v>513</v>
+      </c>
+      <c r="O80" t="s">
         <v>514</v>
-      </c>
-      <c r="O80" t="s">
-        <v>513</v>
       </c>
       <c r="P80" t="s">
         <v>92</v>
@@ -6479,7 +6459,7 @@
         <v>517</v>
       </c>
       <c r="C81" s="1" t="n">
-        <v>43992</v>
+        <v>43994</v>
       </c>
       <c r="D81" t="s">
         <v>518</v>
@@ -6489,25 +6469,25 @@
       </c>
       <c r="F81"/>
       <c r="G81" t="n">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="H81" t="n">
-        <v>441628</v>
+        <v>453744</v>
       </c>
       <c r="I81" t="n">
-        <v>51.028</v>
+        <v>52.428</v>
       </c>
       <c r="J81" t="n">
-        <v>4917</v>
+        <v>4653</v>
       </c>
       <c r="K81" t="n">
-        <v>0.568</v>
+        <v>0.538</v>
       </c>
       <c r="L81" t="n">
-        <v>4339</v>
+        <v>4634</v>
       </c>
       <c r="M81" t="n">
-        <v>0.501</v>
+        <v>0.535</v>
       </c>
       <c r="N81" t="s">
         <v>519</v>
@@ -6577,7 +6557,7 @@
         <v>530</v>
       </c>
       <c r="C83" s="1" t="n">
-        <v>43993</v>
+        <v>43994</v>
       </c>
       <c r="D83" t="s">
         <v>531</v>
@@ -6587,25 +6567,25 @@
       </c>
       <c r="F83"/>
       <c r="G83" t="n">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="H83" t="n">
-        <v>254860</v>
+        <v>261606</v>
       </c>
       <c r="I83" t="n">
-        <v>3.651</v>
+        <v>3.748</v>
       </c>
       <c r="J83" t="n">
-        <v>4784</v>
+        <v>6746</v>
       </c>
       <c r="K83" t="n">
-        <v>0.069</v>
+        <v>0.097</v>
       </c>
       <c r="L83" t="n">
-        <v>5231</v>
+        <v>5317</v>
       </c>
       <c r="M83" t="n">
-        <v>0.075</v>
+        <v>0.076</v>
       </c>
       <c r="N83" t="s">
         <v>533</v>
@@ -6677,7 +6657,7 @@
         <v>543</v>
       </c>
       <c r="C85" s="1" t="n">
-        <v>43991</v>
+        <v>43993</v>
       </c>
       <c r="D85" t="s">
         <v>544</v>
@@ -6687,21 +6667,25 @@
       </c>
       <c r="F85"/>
       <c r="G85" t="n">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="H85" t="n">
-        <v>56210</v>
+        <v>58770</v>
       </c>
       <c r="I85" t="n">
-        <v>4.756</v>
-      </c>
-      <c r="J85"/>
-      <c r="K85"/>
+        <v>4.973</v>
+      </c>
+      <c r="J85" t="n">
+        <v>1497</v>
+      </c>
+      <c r="K85" t="n">
+        <v>0.127</v>
+      </c>
       <c r="L85" t="n">
-        <v>381</v>
+        <v>638</v>
       </c>
       <c r="M85" t="n">
-        <v>0.032</v>
+        <v>0.054</v>
       </c>
       <c r="N85" t="s">
         <v>545</v>
@@ -6724,7 +6708,7 @@
         <v>550</v>
       </c>
       <c r="C86" s="1" t="n">
-        <v>43993</v>
+        <v>43995</v>
       </c>
       <c r="D86" t="s">
         <v>551</v>
@@ -6734,25 +6718,21 @@
       </c>
       <c r="F86"/>
       <c r="G86" t="n">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="H86" t="n">
-        <v>2500890</v>
+        <v>2541903</v>
       </c>
       <c r="I86" t="n">
-        <v>29.653</v>
-      </c>
-      <c r="J86" t="n">
-        <v>49190</v>
-      </c>
-      <c r="K86" t="n">
-        <v>0.583</v>
-      </c>
+        <v>30.139</v>
+      </c>
+      <c r="J86"/>
+      <c r="K86"/>
       <c r="L86" t="n">
-        <v>41615</v>
+        <v>34092</v>
       </c>
       <c r="M86" t="n">
-        <v>0.493</v>
+        <v>0.404</v>
       </c>
       <c r="N86" t="s">
         <v>552</v>
@@ -6775,7 +6755,7 @@
         <v>557</v>
       </c>
       <c r="C87" s="1" t="n">
-        <v>43992</v>
+        <v>43993</v>
       </c>
       <c r="D87" t="s">
         <v>558</v>
@@ -6787,25 +6767,25 @@
         <v>560</v>
       </c>
       <c r="G87" t="n">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="H87" t="n">
-        <v>117422</v>
+        <v>119954</v>
       </c>
       <c r="I87" t="n">
-        <v>2.567</v>
+        <v>2.622</v>
       </c>
       <c r="J87" t="n">
-        <v>2321</v>
+        <v>2532</v>
       </c>
       <c r="K87" t="n">
-        <v>0.051</v>
+        <v>0.055</v>
       </c>
       <c r="L87" t="n">
-        <v>2254</v>
+        <v>2453</v>
       </c>
       <c r="M87" t="n">
-        <v>0.049</v>
+        <v>0.054</v>
       </c>
       <c r="N87" t="s">
         <v>559</v>
@@ -6828,7 +6808,7 @@
         <v>564</v>
       </c>
       <c r="C88" s="1" t="n">
-        <v>43994</v>
+        <v>43995</v>
       </c>
       <c r="D88" t="s">
         <v>565</v>
@@ -6838,22 +6818,22 @@
       </c>
       <c r="F88"/>
       <c r="G88" t="n">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="H88" t="n">
-        <v>468172</v>
+        <v>479111</v>
       </c>
       <c r="I88" t="n">
-        <v>10.705</v>
+        <v>10.955</v>
       </c>
       <c r="J88" t="n">
-        <v>11663</v>
+        <v>10939</v>
       </c>
       <c r="K88" t="n">
-        <v>0.267</v>
+        <v>0.25</v>
       </c>
       <c r="L88" t="n">
-        <v>9232</v>
+        <v>9224</v>
       </c>
       <c r="M88" t="n">
         <v>0.211</v>
@@ -6930,7 +6910,7 @@
         <v>576</v>
       </c>
       <c r="C90" s="1" t="n">
-        <v>43992</v>
+        <v>43994</v>
       </c>
       <c r="D90" t="s">
         <v>577</v>
@@ -6942,25 +6922,25 @@
         <v>578</v>
       </c>
       <c r="G90" t="n">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="H90" t="n">
-        <v>3633910</v>
+        <v>3792060</v>
       </c>
       <c r="I90" t="n">
-        <v>53.53</v>
+        <v>55.859</v>
       </c>
       <c r="J90" t="n">
-        <v>79982</v>
+        <v>76146</v>
       </c>
       <c r="K90" t="n">
-        <v>1.178</v>
+        <v>1.122</v>
       </c>
       <c r="L90" t="n">
-        <v>77510</v>
+        <v>77380</v>
       </c>
       <c r="M90" t="n">
-        <v>1.142</v>
+        <v>1.14</v>
       </c>
       <c r="N90" t="s">
         <v>573</v>
@@ -6983,7 +6963,7 @@
         <v>581</v>
       </c>
       <c r="C91" s="1" t="n">
-        <v>43993</v>
+        <v>43994</v>
       </c>
       <c r="D91" t="s">
         <v>582</v>
@@ -6993,25 +6973,25 @@
       </c>
       <c r="F91"/>
       <c r="G91" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H91" t="n">
-        <v>22418881</v>
+        <v>23290724</v>
       </c>
       <c r="I91" t="n">
-        <v>67.73</v>
+        <v>70.364</v>
       </c>
       <c r="J91" t="n">
-        <v>367990</v>
+        <v>871843</v>
       </c>
       <c r="K91" t="n">
-        <v>1.112</v>
+        <v>2.634</v>
       </c>
       <c r="L91" t="n">
-        <v>372520</v>
+        <v>415125</v>
       </c>
       <c r="M91" t="n">
-        <v>1.125</v>
+        <v>1.254</v>
       </c>
       <c r="N91" t="s">
         <v>583</v>
@@ -7034,7 +7014,7 @@
         <v>587</v>
       </c>
       <c r="C92" s="1" t="n">
-        <v>43993</v>
+        <v>43994</v>
       </c>
       <c r="D92" t="s">
         <v>588</v>
@@ -7044,25 +7024,25 @@
       </c>
       <c r="F92"/>
       <c r="G92" t="n">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="H92" t="n">
-        <v>21933301</v>
+        <v>22517262</v>
       </c>
       <c r="I92" t="n">
-        <v>66.263</v>
+        <v>68.027</v>
       </c>
       <c r="J92" t="n">
-        <v>446765</v>
+        <v>583961</v>
       </c>
       <c r="K92" t="n">
-        <v>1.35</v>
+        <v>1.764</v>
       </c>
       <c r="L92" t="n">
-        <v>449582</v>
+        <v>455881</v>
       </c>
       <c r="M92" t="n">
-        <v>1.358</v>
+        <v>1.377</v>
       </c>
       <c r="N92" t="s">
         <v>589</v>
@@ -7085,7 +7065,7 @@
         <v>594</v>
       </c>
       <c r="C93" s="1" t="n">
-        <v>43994</v>
+        <v>43995</v>
       </c>
       <c r="D93" t="s">
         <v>595</v>
@@ -7095,25 +7075,25 @@
       </c>
       <c r="F93"/>
       <c r="G93" t="n">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="H93" t="n">
-        <v>51313</v>
+        <v>52078</v>
       </c>
       <c r="I93" t="n">
-        <v>14.772</v>
+        <v>14.992</v>
       </c>
       <c r="J93" t="n">
-        <v>840</v>
+        <v>765</v>
       </c>
       <c r="K93" t="n">
-        <v>0.242</v>
+        <v>0.22</v>
       </c>
       <c r="L93" t="n">
-        <v>686</v>
+        <v>664</v>
       </c>
       <c r="M93" t="n">
-        <v>0.197</v>
+        <v>0.191</v>
       </c>
       <c r="N93" t="s">
         <v>124</v>

</xml_diff>

<commit_message>
Updated testing data for 2020-06-17
</commit_message>
<xml_diff>
--- a/public/data/testing/covid-testing-latest-data-source-details.xlsx
+++ b/public/data/testing/covid-testing-latest-data-source-details.xlsx
@@ -71,7 +71,7 @@
     <t xml:space="preserve">Argentina - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.argentina.gob.ar/sites/default/files/15-06-20-reporte-matutino-covid-19.pdf</t>
+    <t xml:space="preserve">https://www.argentina.gob.ar/sites/default/files/17-06-20_reporte-matutino-covid-19.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">Government of Argentina</t>
@@ -112,7 +112,7 @@
     <t xml:space="preserve">Austria - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200615193059/https://www.sozialministerium.at/Informationen-zum-Coronavirus/Neuartiges-Coronavirus-(2019-nCov).html</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200617152355/https://www.sozialministerium.at/Informationen-zum-Coronavirus/Neuartiges-Coronavirus-(2019-nCov).html</t>
   </si>
   <si>
     <t xml:space="preserve">Austrian Ministry for Health</t>
@@ -139,7 +139,7 @@
     <t xml:space="preserve">Bahrain - units unclear</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200615193101/https://www.moh.gov.bh/COVID19</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200616221820/https://www.moh.gov.bh/COVID19</t>
   </si>
   <si>
     <t xml:space="preserve">Ministry of Health</t>
@@ -187,7 +187,7 @@
     <t xml:space="preserve">Belarus - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">http://minzdrav.gov.by/ru/sobytiya/v-belarusi-vyzdoroveli-i-vypisany-30-420-patsientov/</t>
+    <t xml:space="preserve">http://minzdrav.gov.by/ru/sobytiya/v-belarusi-na-16-iyunya-vyzdoroveli-i-vypisany-31273-patsienta/</t>
   </si>
   <si>
     <t xml:space="preserve">Belarus Ministry of Health</t>
@@ -233,7 +233,7 @@
     <t xml:space="preserve">Bolivia - units unclear</t>
   </si>
   <si>
-    <t xml:space="preserve">https://minsalud.gob.bo/4293-ministerio-de-salud-reporta-617-nuevos-contagios-de-coronavirus-y-el-numero-de-recuperados-supera-los-3-000</t>
+    <t xml:space="preserve">https://minsalud.gob.bo/4306-ministerio-de-salud-reporta-810-nuevos-contagios-de-coronavirus-en-bolivia-y-el-numero-de-recuperados-sube-a-3-752</t>
   </si>
   <si>
     <t xml:space="preserve">https://www.minsalud.gob.bo/</t>
@@ -280,7 +280,7 @@
     <t xml:space="preserve">Bulgaria - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200615193217/https://coronavirus.bg/</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200616221837/https://coronavirus.bg/</t>
   </si>
   <si>
     <t xml:space="preserve">Bulgaria COVID-10 Information Portal</t>
@@ -303,7 +303,7 @@
     <t xml:space="preserve">Canada - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200615193219/https://www.canada.ca/en/public-health/services/diseases/2019-novel-coronavirus-infection.html</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200617152359/https://www.canada.ca/en/public-health/services/diseases/2019-novel-coronavirus-infection.html</t>
   </si>
   <si>
     <t xml:space="preserve">Government of Canada</t>
@@ -391,7 +391,7 @@
     <t xml:space="preserve">Croatia - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200615193223/https://www.koronavirus.hr/najnovije/ukupno-dosad-382-zarazene-osobe-u-hrvatskoj/35</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200617152415/https://www.koronavirus.hr/najnovije/ukupno-dosad-382-zarazene-osobe-u-hrvatskoj/35</t>
   </si>
   <si>
     <t xml:space="preserve">Government of Croatia</t>
@@ -454,7 +454,7 @@
     <t xml:space="preserve">Denmark - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://files.ssi.dk/Data-Epidemiologiske-Rapport-15062020-help</t>
+    <t xml:space="preserve">https://files.ssi.dk/Data-Epidemiologiske-Rapport-17062020-bbh6</t>
   </si>
   <si>
     <t xml:space="preserve">Statens Serum Institut</t>
@@ -473,7 +473,7 @@
     <t xml:space="preserve">Ecuador - units unclear</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.gestionderiesgos.gob.ec/wp-content/uploads/2020/06/INFOGRAFIA-NACIONALCOVI-19-COE-NACIONAL-14062020-08h00.pdf</t>
+    <t xml:space="preserve">https://www.gestionderiesgos.gob.ec/wp-content/uploads/2020/06/INFOGRAFIA-NACIONALCOVI-19-COE-NACIONAL-16062020-08h00.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">Government of Ecuador</t>
@@ -539,7 +539,7 @@
     <t xml:space="preserve">Ethiopia - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.ephi.gov.et/images/novel_coronavirus/confirmed-case-Press-release_June-15-Eng_V2.pdf</t>
+    <t xml:space="preserve">https://www.ephi.gov.et/images/novel_coronavirus/Confirmed-case-Press-release_June-17-Eng_V1.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">Ethiopian Public Health Institute</t>
@@ -694,7 +694,7 @@
     <t xml:space="preserve">Greece - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://eody.gov.gr/wp-content/uploads/2020/06/covid-gr-daily-report-20200615.pdf</t>
+    <t xml:space="preserve">https://eody.gov.gr/wp-content/uploads/2020/06/covid-gr-daily-report-20200617.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">National Organization of Public Health</t>
@@ -855,7 +855,7 @@
     <t xml:space="preserve">Ireland - units unclear</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.gov.ie/en/press-release/b8a62-statement-from-the-national-public-health-emergency-team-tuesday-9-june/</t>
+    <t xml:space="preserve">https://www.gov.ie/en/press-release/68c96-statement-from-the-national-public-health-emergency-team-tuesday-16-june/</t>
   </si>
   <si>
     <t xml:space="preserve">https://www.gov.ie/en/publications/?&amp;type=press-releases&amp;organisation=department-of-health</t>
@@ -876,7 +876,7 @@
     <t xml:space="preserve">Israel - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://govextra.gov.il/media/20608/covid19-data-israel-08062020.csv</t>
+    <t xml:space="preserve">https://govextra.gov.il/media/21014/covid19-data-israel-10062020.csv</t>
   </si>
   <si>
     <t xml:space="preserve">Israel Ministry of Health</t>
@@ -933,13 +933,13 @@
     <t xml:space="preserve">Japan - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.mhlw.go.jp/stf/newpage_11868.html</t>
+    <t xml:space="preserve">https://www.mhlw.go.jp/stf/newpage_11906.html</t>
   </si>
   <si>
     <t xml:space="preserve">Ministry of Health, Labor and Welfare Press Release</t>
   </si>
   <si>
-    <t xml:space="preserve">See Table: 国内の発生状況, column 1 '検査実施人数'.</t>
+    <t xml:space="preserve">See Table: 国内の発生状況, column 1 '検査実施人数'. Daily change figure provided for this date is not consistent with the cumulative totals for today and the previous day.</t>
   </si>
   <si>
     <t xml:space="preserve">Ministry of Health, Labor and Welfare</t>
@@ -957,10 +957,10 @@
     <t xml:space="preserve">Japan - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.mhlw.go.jp/content/10906000/000639750.pdf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The cumulative total reported in the press release (557, 393) does not sum to the cumulative total calculated from the weekly and daily figures reported by the MOH. See: https://www.mhlw.go.jp/content/10906000/000639750.pdf</t>
+    <t xml:space="preserve">https://www.mhlw.go.jp/content/10906000/000640398.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The cumulative total reported in the press release (561,066) does not sum to the cumulative total calculated from the weekly and daily figures reported by the MOH. See: https://www.mhlw.go.jp/content/10906000/000640038.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">On 11th April 2020, the MOH started providing a daily time series on the "Implementation status of PCR tests for new coronavirus in Japan (based on the date on which results were determined" (via Google translate). 
@@ -1015,7 +1015,7 @@
     <t xml:space="preserve">Kuwait - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/KUWAIT_MOH/status/1272474325338161155/photo/2</t>
+    <t xml:space="preserve">https://twitter.com/KUWAIT_MOH/status/1273214443044974593/photo/2</t>
   </si>
   <si>
     <t xml:space="preserve">Kuwait Ministry of Health</t>
@@ -1024,7 +1024,7 @@
     <t xml:space="preserve">https://twitter.com/KUWAIT_MOH</t>
   </si>
   <si>
-    <t xml:space="preserve">The Kuwait Ministry of Health provides daily reports of the daily ("NEW TESTS") and cumulative ("Total") number of tests performed on [their official Twitter account](https://twitter.com/KUWAIT_MOH). COVID-19 reports date back to early March 2020 but did not begin including testing numbers until 13 May; the cumulative total then was already 227,000. From 13 to 29 May, the daily number was termed "NP swab last 24 h" and the cumulative number "Total Investigations".</t>
+    <t xml:space="preserve">The Kuwait Ministry of Health provides daily reports of the daily ("NEW TESTS") and cumulative ("Total") number of tests performed on [their official Twitter account](https://twitter.com/KUWAIT_MOH). COVID-19 reports date back to early March 2020 but did not begin including testing numbers until 13 May; the cumulative total then was already 227,000. From 13 to 29 May, the daily number was termed "NP swab last 24 h" and the cumulative number "Total Investigations."</t>
   </si>
   <si>
     <t xml:space="preserve">LVA</t>
@@ -1051,7 +1051,7 @@
     <t xml:space="preserve">Lithuania - samples tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200615193338/http://sam.lrv.lt/lt/naujienos/koronavirusas</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200617152520/http://sam.lrv.lt/lt/naujienos/koronavirusas</t>
   </si>
   <si>
     <t xml:space="preserve">http://sam.lrv.lt/lt/naujienos/koronavirusas</t>
@@ -1067,7 +1067,7 @@
     <t xml:space="preserve">Luxembourg - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200615193339/https://gouvernement.lu/en/dossiers.gouv_msan%2Ben%2Bdossiers%2B2020%2Bcorona-virus.html</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200616221932/https://gouvernement.lu/en/dossiers.gouv_msan%2Ben%2Bdossiers%2B2020%2Bcorona-virus.html</t>
   </si>
   <si>
     <t xml:space="preserve">Luxembourg Government situation update</t>
@@ -1088,13 +1088,13 @@
     <t xml:space="preserve">Malaysia - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.facebook.com/373560576236/videos/271901207492240</t>
+    <t xml:space="preserve">https://www.facebook.com/373560576236/videos/573787186665171</t>
   </si>
   <si>
     <t xml:space="preserve">Ministry of Health Malaysia</t>
   </si>
   <si>
-    <t xml:space="preserve">Statistics on testing can be see at 00:00 timestamp on the MOH livestream</t>
+    <t xml:space="preserve">Statistics on testing can be see at 08:56 timestamp on the MOH livestream</t>
   </si>
   <si>
     <t xml:space="preserve">http://covid-19.moh.gov.my/terkini</t>
@@ -1113,13 +1113,13 @@
     <t xml:space="preserve">Maldives - samples tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.facebook.com/561317043971945/videos/2629831207290787/</t>
+    <t xml:space="preserve">https://www.facebook.com/561317043971945/videos/861915974295679/</t>
   </si>
   <si>
     <t xml:space="preserve">Maldives Ministry of Health</t>
   </si>
   <si>
-    <t xml:space="preserve">Numbers visible in video at time: 0:59</t>
+    <t xml:space="preserve">Numbers visible in video at time: 1:00</t>
   </si>
   <si>
     <t xml:space="preserve">Maldives Ministry of Health Official Facebook page</t>
@@ -1264,7 +1264,7 @@
     <t xml:space="preserve">Nigeria - samples tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200615193615/https://covid19.ncdc.gov.ng/</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200616143820/https://covid19.ncdc.gov.ng/</t>
   </si>
   <si>
     <t xml:space="preserve">Nigeria Centre for Disease Control</t>
@@ -1284,7 +1284,7 @@
     <t xml:space="preserve">Norway - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.fhi.no/contentassets/ca5914bd0aa14e15a17f8a7d48fa306a/2020.06.15-dagsrapport-norge-covid-19.pdf</t>
+    <t xml:space="preserve">https://www.fhi.no/contentassets/ca5914bd0aa14e15a17f8a7d48fa306a/2020.06.17-dagsrapport-covid-19.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">Norwegian Institute of Public Health</t>
@@ -1309,7 +1309,7 @@
     <t xml:space="preserve">Pakistan - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200615193617/http://www.covid.gov.pk/</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200617152733/http://www.covid.gov.pk/</t>
   </si>
   <si>
     <t xml:space="preserve">Government of Pakistan</t>
@@ -1362,7 +1362,7 @@
     <t xml:space="preserve">Peru - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.gob.pe/institucion/minsa/noticias/186742-minsa-casos-confirmados-por-coronavirus-covid-19-ascienden-a-229-736-en-el-peru-comunicado-n-132</t>
+    <t xml:space="preserve">https://www.gob.pe/institucion/minsa/noticias/187343-minsa-casos-confirmados-por-coronavirus-covid-19-ascienden-a-237-156-en-el-peru-comunicado-n-134</t>
   </si>
   <si>
     <t xml:space="preserve">Ministry of Health, Government of Peru</t>
@@ -1392,8 +1392,8 @@
     <t xml:space="preserve">The DOH reports the cumulative samples and unique individuals tested.</t>
   </si>
   <si>
-    <t xml:space="preserve">The Ministry of Health (MOH) provides a daily snapshot of testing capacity detailing the total number of individuals tested and the total number of tests conducted. 
-The total number of individuals tested is the sum of positive, negative, equivocal, and invalid individuals. No definitions of equivocal and invalid individual tests are given, hence our figures only report the sum of individuals who have tested positive or negative. From 22nd May, the DOH stopped reporting figures on equivocal and invalid individuals; the DOH provides the cumulative samples and unique indivdiuals tested, where cumulative unique individuals = cumulative positive + cumulative negative individuals. 
+    <t xml:space="preserve">The Department of Health (DOH) provides a daily snapshot of testing capacity detailing the total number of individuals tested and the total number of tests conducted. As of 15th June, the DOH provides a historical series dating back to 3rd April. These figures are subject to change as the DOH continues with its validation.
+In earlier versions of the DOH portal, the total number of individuals tested was reported as the sum of positive, negative, equivocal, and invalid individuals. No definitions of equivocal and invalid individual tests were given, hence our figures only reported the sum of individuals who have tested positive or negative. From 22nd May, the DOH stopped reporting figures on equivocal and invalid individuals; the DOH provided the cumulative samples and unique individuals tested, where cumulative unique individuals = cumulative positive + cumulative negative individuals. 
 The source provides a breakdown of both i) the number of individuals tested and ii) the total tests conducted, by laboratory. We are not aware of any aggregation issues. 
 The DOH used to report the number of cases tested in a previous dashboard, but stopped on 4th April. This previous breakdown of the test results and COVID-19 dashboard have both been removed. We became aware of this new tracker on the 13th April with data 'as of April 11 2020, 12am'. No previous snapshots of the dashboard are available using web archive, therefore the series starts from the 11th April - the earliest date from which we have access to the data.</t>
   </si>
@@ -1468,7 +1468,7 @@
     <t xml:space="preserve">Romania - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://gov.ro/ro/media/comunicate/buletin-de-presa-14-iunie-2020-ora-13-00&amp;page=1</t>
+    <t xml:space="preserve">https://gov.ro/ro/media/comunicate/buletin-de-presa-17-iunie-2020-ora-13-00&amp;page=1</t>
   </si>
   <si>
     <t xml:space="preserve">Ministry of Internal Affairs</t>
@@ -1486,7 +1486,7 @@
     <t xml:space="preserve">Russia - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://rospotrebnadzor.ru/about/info/news/news_details.php?ELEMENT_ID=14694</t>
+    <t xml:space="preserve">https://rospotrebnadzor.ru/about/info/news/news_details.php?ELEMENT_ID=14708</t>
   </si>
   <si>
     <t xml:space="preserve">Government of the Russian Federation</t>
@@ -1588,7 +1588,7 @@
     <t xml:space="preserve">Singapore - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200610165255/https://www.moh.gov.sg/covid-19</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200617152740/https://www.moh.gov.sg/covid-19</t>
   </si>
   <si>
     <t xml:space="preserve">https://www.moh.gov.sg/covid-19</t>
@@ -1601,7 +1601,7 @@
     <t xml:space="preserve">Singapore - swabs tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200610165257/https://www.moh.gov.sg/covid-19</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200617152742/https://www.moh.gov.sg/covid-19</t>
   </si>
   <si>
     <t xml:space="preserve">The number of swabs tested.</t>
@@ -1613,7 +1613,7 @@
     <t xml:space="preserve">Slovakia - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200614075654/https://korona.gov.sk/</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200617152744/https://korona.gov.sk/</t>
   </si>
   <si>
     <t xml:space="preserve">National Center of Health Information and the Office of the Government of the Slovak Republic</t>
@@ -1661,7 +1661,7 @@
     <t xml:space="preserve">ZAF</t>
   </si>
   <si>
-    <t xml:space="preserve">South Africa - units unclear</t>
+    <t xml:space="preserve">South Africa - people tested</t>
   </si>
   <si>
     <t xml:space="preserve">https://github.com/dsfsi/covid19za</t>
@@ -1687,7 +1687,7 @@
     <t xml:space="preserve">South Korea - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.cdc.go.kr/board/board.es?mid=&amp;bid=0030&amp;act=view&amp;list_no=367523&amp;tag=&amp;nPage=1</t>
+    <t xml:space="preserve">https://www.cdc.go.kr/board/board.es?mid=&amp;bid=0030&amp;act=view&amp;list_no=367536&amp;tag=&amp;nPage=1</t>
   </si>
   <si>
     <t xml:space="preserve">South Korea CDC</t>
@@ -1773,7 +1773,7 @@
     <t xml:space="preserve">Taiwan - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.cdc.gov.tw/Bulletin/Detail/aL2rUdFBmAyUJvtx5mkNpA?typeid=9</t>
+    <t xml:space="preserve">https://www.cdc.gov.tw/Bulletin/Detail/83k1oGCSBiSlnIdtc17cKQ?typeid=9</t>
   </si>
   <si>
     <t xml:space="preserve">Taiwan Centers for Disease Control (CDC)</t>
@@ -1796,7 +1796,7 @@
     <t xml:space="preserve">Thailand - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200615193709/https://ddc.moph.go.th/viralpneumonia/eng/index.php</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200617152826/https://ddc.moph.go.th/viralpneumonia/eng/index.php</t>
   </si>
   <si>
     <t xml:space="preserve">Department of Disease Control</t>
@@ -1866,7 +1866,7 @@
     <t xml:space="preserve">Turkey - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200614204731/https://covid19.saglik.gov.tr/</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200616222201/https://covid19.saglik.gov.tr/</t>
   </si>
   <si>
     <t xml:space="preserve">Turkish Ministry of Health</t>
@@ -1890,7 +1890,7 @@
     <t xml:space="preserve">Uganda - samples tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/MinofHealthUG/status/1272081495268696065</t>
+    <t xml:space="preserve">https://www.health.go.ug/cause/update-on-the-covid-19-outbreak-in-uganda-22/</t>
   </si>
   <si>
     <t xml:space="preserve">Press Release from the Office of the Director General</t>
@@ -1914,7 +1914,7 @@
     <t xml:space="preserve">Ukraine - units unclear</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200615193715/https://covid19.gov.ua/en</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200617152831/https://covid19.gov.ua/en</t>
   </si>
   <si>
     <t xml:space="preserve">Cabinet of Ministers of Ukraine</t>
@@ -1951,7 +1951,7 @@
     <t xml:space="preserve">United Kingdom - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://assets.publishing.service.gov.uk/government/uploads/system/uploads/attachment_data/file/892445/2020-06-15_COVID-19_UK_testing_time_series.csv</t>
+    <t xml:space="preserve">https://assets.publishing.service.gov.uk/government/uploads/system/uploads/attachment_data/file/893047/2020-06-17_COVID-19_UK_testing_time_series.csv</t>
   </si>
   <si>
     <t xml:space="preserve">Sum of pillar 1 + pillar 2 (tests processed only)</t>
@@ -1972,7 +1972,7 @@
     <t xml:space="preserve">United States - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200612230811/https://www.cdc.gov/coronavirus/2019-ncov/cases-updates/testing-in-us.html</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200616222205/https://www.cdc.gov/coronavirus/2019-ncov/cases-updates/testing-in-us.html</t>
   </si>
   <si>
     <t xml:space="preserve">United States CDC</t>
@@ -2012,7 +2012,7 @@
   <si>
     <t xml:space="preserve">This is a collaborative project launched in order to fill some of the important gaps in the testing figures being collated by the CDC.
 Testing data is gathered from individual states, as reported in state health department websites, data dashboards and press releases from officials.
-As of 26 May, there have been a number of media reports noting that the testing figures released by some states include antibody tests in addition to PCR tests – as discussed in [this article](https://www.theatlantic.com/health/archive/2020/05/cdc-and-states-are-misreporting-covid-19-test-data-pennsylvania-georgia-texas/611935/) in The Atlantic. Our dataset aims to report only PCR tests. But becasue some states do not disaggregate these types of tests we are not currently able to exclude the antibody tests.
+As of 26 May, there have been a number of media reports noting that the testing figures released by some states include antibody tests in addition to PCR tests – as discussed in [this article](https://www.theatlantic.com/health/archive/2020/05/cdc-and-states-are-misreporting-covid-19-test-data-pennsylvania-georgia-texas/611935/) in The Atlantic. Our dataset aims to report only PCR tests. But because some states do not disaggregate these types of tests we are not currently able to exclude the antibody tests.
 Other differences across states include: some report the number of tests performed, others the number of people tested; some include private labs, others not; some report negative test results, others only positive test results; some include pending tests, others do not (below we show figures that exclude explicitly pending results).
 Moreover, many states do not explicitly provide details about these important factors needed to interpret the data they provide. 
 There are issues in comparing the figures over time. The totals given for early on in the outbreak do not include all states. One significant uncertainty is the extent to which the rapid rise in tests seen from the mid-March in part reflects states beginning to report private lab tests.
@@ -2026,7 +2026,7 @@
     <t xml:space="preserve">Uruguay - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.gub.uy/ministerio-salud-publica/comunicacion/noticias/actualizacion-informacion-relacion-coronavirus-covid-19-uruguay-54</t>
+    <t xml:space="preserve">https://www.gub.uy/ministerio-salud-publica/comunicacion/noticias/actualizacion-informacion-relacion-coronavirus-covid-19-uruguay-56</t>
   </si>
   <si>
     <t xml:space="preserve">https://www.gub.uy/ministerio-salud-publica/comunicacion/noticias</t>
@@ -2475,7 +2475,7 @@
         <v>18</v>
       </c>
       <c r="C2" s="1" t="n">
-        <v>43997</v>
+        <v>43999</v>
       </c>
       <c r="D2" t="s">
         <v>19</v>
@@ -2485,25 +2485,25 @@
       </c>
       <c r="F2"/>
       <c r="G2" t="n">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="H2" t="n">
-        <v>239941</v>
+        <v>250615</v>
       </c>
       <c r="I2" t="n">
-        <v>5.309</v>
+        <v>5.545</v>
       </c>
       <c r="J2" t="n">
-        <v>5571</v>
+        <v>5556</v>
       </c>
       <c r="K2" t="n">
         <v>0.123</v>
       </c>
       <c r="L2" t="n">
-        <v>5917</v>
+        <v>6014</v>
       </c>
       <c r="M2" t="n">
-        <v>0.131</v>
+        <v>0.133</v>
       </c>
       <c r="N2" t="s">
         <v>20</v>
@@ -2577,7 +2577,7 @@
         <v>31</v>
       </c>
       <c r="C4" s="1" t="n">
-        <v>43997</v>
+        <v>43999</v>
       </c>
       <c r="D4" t="s">
         <v>32</v>
@@ -2587,25 +2587,25 @@
       </c>
       <c r="F4"/>
       <c r="G4" t="n">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="H4" t="n">
-        <v>527670</v>
+        <v>540615</v>
       </c>
       <c r="I4" t="n">
-        <v>58.588</v>
+        <v>60.026</v>
       </c>
       <c r="J4" t="n">
-        <v>2830</v>
+        <v>7915</v>
       </c>
       <c r="K4" t="n">
-        <v>0.314</v>
+        <v>0.879</v>
       </c>
       <c r="L4" t="n">
-        <v>4701</v>
+        <v>4896</v>
       </c>
       <c r="M4" t="n">
-        <v>0.522</v>
+        <v>0.544</v>
       </c>
       <c r="N4" t="s">
         <v>34</v>
@@ -2628,7 +2628,7 @@
         <v>39</v>
       </c>
       <c r="C5" s="1" t="n">
-        <v>43997</v>
+        <v>43998</v>
       </c>
       <c r="D5" t="s">
         <v>40</v>
@@ -2638,25 +2638,25 @@
       </c>
       <c r="F5"/>
       <c r="G5" t="n">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H5" t="n">
-        <v>425192</v>
+        <v>438080</v>
       </c>
       <c r="I5" t="n">
-        <v>249.88</v>
+        <v>257.454</v>
       </c>
       <c r="J5" t="n">
-        <v>6779</v>
+        <v>12888</v>
       </c>
       <c r="K5" t="n">
-        <v>3.984</v>
+        <v>7.574</v>
       </c>
       <c r="L5" t="n">
-        <v>7261</v>
+        <v>8549</v>
       </c>
       <c r="M5" t="n">
-        <v>4.267</v>
+        <v>5.024</v>
       </c>
       <c r="N5" t="s">
         <v>42</v>
@@ -2730,7 +2730,7 @@
         <v>54</v>
       </c>
       <c r="C7" s="1" t="n">
-        <v>43997</v>
+        <v>43998</v>
       </c>
       <c r="D7" t="s">
         <v>55</v>
@@ -2740,21 +2740,25 @@
       </c>
       <c r="F7"/>
       <c r="G7" t="n">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="H7" t="n">
-        <v>749917</v>
+        <v>760549</v>
       </c>
       <c r="I7" t="n">
-        <v>79.362</v>
-      </c>
-      <c r="J7"/>
-      <c r="K7"/>
+        <v>80.487</v>
+      </c>
+      <c r="J7" t="n">
+        <v>10632</v>
+      </c>
+      <c r="K7" t="n">
+        <v>1.125</v>
+      </c>
       <c r="L7" t="n">
-        <v>16703</v>
+        <v>15899</v>
       </c>
       <c r="M7" t="n">
-        <v>1.768</v>
+        <v>1.683</v>
       </c>
       <c r="N7" t="s">
         <v>56</v>
@@ -2777,7 +2781,7 @@
         <v>60</v>
       </c>
       <c r="C8" s="1" t="n">
-        <v>43995</v>
+        <v>43997</v>
       </c>
       <c r="D8" t="s">
         <v>61</v>
@@ -2787,25 +2791,25 @@
       </c>
       <c r="F8"/>
       <c r="G8" t="n">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="H8" t="n">
-        <v>814108</v>
+        <v>828172</v>
       </c>
       <c r="I8" t="n">
-        <v>70.245</v>
+        <v>71.458</v>
       </c>
       <c r="J8" t="n">
-        <v>8325</v>
+        <v>6758</v>
       </c>
       <c r="K8" t="n">
-        <v>0.718</v>
+        <v>0.583</v>
       </c>
       <c r="L8" t="n">
-        <v>8680</v>
+        <v>8814</v>
       </c>
       <c r="M8" t="n">
-        <v>0.749</v>
+        <v>0.761</v>
       </c>
       <c r="N8" t="s">
         <v>62</v>
@@ -2828,7 +2832,7 @@
         <v>67</v>
       </c>
       <c r="C9" s="1" t="n">
-        <v>43996</v>
+        <v>43998</v>
       </c>
       <c r="D9" t="s">
         <v>68</v>
@@ -2838,25 +2842,25 @@
       </c>
       <c r="F9"/>
       <c r="G9" t="n">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="H9" t="n">
-        <v>47372</v>
+        <v>50114</v>
       </c>
       <c r="I9" t="n">
-        <v>4.058</v>
+        <v>4.293</v>
       </c>
       <c r="J9" t="n">
-        <v>1303</v>
+        <v>1358</v>
       </c>
       <c r="K9" t="n">
-        <v>0.112</v>
+        <v>0.116</v>
       </c>
       <c r="L9" t="n">
-        <v>1442</v>
+        <v>1501</v>
       </c>
       <c r="M9" t="n">
-        <v>0.124</v>
+        <v>0.129</v>
       </c>
       <c r="N9" t="s">
         <v>41</v>
@@ -2924,7 +2928,7 @@
         <v>81</v>
       </c>
       <c r="C11" s="1" t="n">
-        <v>43997</v>
+        <v>43998</v>
       </c>
       <c r="D11" t="s">
         <v>82</v>
@@ -2934,25 +2938,25 @@
       </c>
       <c r="F11"/>
       <c r="G11" t="n">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="H11" t="n">
-        <v>104486</v>
+        <v>108325</v>
       </c>
       <c r="I11" t="n">
-        <v>15.037</v>
+        <v>15.59</v>
       </c>
       <c r="J11" t="n">
-        <v>1409</v>
+        <v>3839</v>
       </c>
       <c r="K11" t="n">
-        <v>0.203</v>
+        <v>0.552</v>
       </c>
       <c r="L11" t="n">
-        <v>2022</v>
+        <v>2370</v>
       </c>
       <c r="M11" t="n">
-        <v>0.291</v>
+        <v>0.341</v>
       </c>
       <c r="N11" t="s">
         <v>84</v>
@@ -2975,7 +2979,7 @@
         <v>88</v>
       </c>
       <c r="C12" s="1" t="n">
-        <v>43997</v>
+        <v>43999</v>
       </c>
       <c r="D12" t="s">
         <v>89</v>
@@ -2985,25 +2989,25 @@
       </c>
       <c r="F12"/>
       <c r="G12" t="n">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="H12" t="n">
-        <v>2152700</v>
+        <v>2216654</v>
       </c>
       <c r="I12" t="n">
-        <v>57.037</v>
+        <v>58.732</v>
       </c>
       <c r="J12" t="n">
-        <v>38852</v>
+        <v>33254</v>
       </c>
       <c r="K12" t="n">
-        <v>1.029</v>
+        <v>0.881</v>
       </c>
       <c r="L12" t="n">
-        <v>36565</v>
+        <v>37287</v>
       </c>
       <c r="M12" t="n">
-        <v>0.969</v>
+        <v>0.988</v>
       </c>
       <c r="N12" t="s">
         <v>90</v>
@@ -3026,7 +3030,7 @@
         <v>95</v>
       </c>
       <c r="C13" s="1" t="n">
-        <v>43997</v>
+        <v>43998</v>
       </c>
       <c r="D13" t="s">
         <v>96</v>
@@ -3038,25 +3042,25 @@
         <v>97</v>
       </c>
       <c r="G13" t="n">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="H13" t="n">
-        <v>858958</v>
+        <v>873533</v>
       </c>
       <c r="I13" t="n">
-        <v>44.933</v>
+        <v>45.696</v>
       </c>
       <c r="J13" t="n">
-        <v>18808</v>
+        <v>14575</v>
       </c>
       <c r="K13" t="n">
-        <v>0.984</v>
+        <v>0.762</v>
       </c>
       <c r="L13" t="n">
-        <v>18592</v>
+        <v>18134</v>
       </c>
       <c r="M13" t="n">
-        <v>0.973</v>
+        <v>0.949</v>
       </c>
       <c r="N13" t="s">
         <v>98</v>
@@ -3079,7 +3083,7 @@
         <v>102</v>
       </c>
       <c r="C14" s="1" t="n">
-        <v>43996</v>
+        <v>43998</v>
       </c>
       <c r="D14" t="s">
         <v>103</v>
@@ -3089,25 +3093,25 @@
       </c>
       <c r="F14"/>
       <c r="G14" t="n">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="H14" t="n">
-        <v>495024</v>
+        <v>519990</v>
       </c>
       <c r="I14" t="n">
-        <v>9.729</v>
+        <v>10.219</v>
       </c>
       <c r="J14" t="n">
-        <v>12192</v>
+        <v>12402</v>
       </c>
       <c r="K14" t="n">
-        <v>0.24</v>
+        <v>0.244</v>
       </c>
       <c r="L14" t="n">
-        <v>12044</v>
+        <v>12446</v>
       </c>
       <c r="M14" t="n">
-        <v>0.237</v>
+        <v>0.245</v>
       </c>
       <c r="N14" t="s">
         <v>104</v>
@@ -3130,7 +3134,7 @@
         <v>109</v>
       </c>
       <c r="C15" s="1" t="n">
-        <v>43996</v>
+        <v>43997</v>
       </c>
       <c r="D15" t="s">
         <v>110</v>
@@ -3140,25 +3144,25 @@
       </c>
       <c r="F15"/>
       <c r="G15" t="n">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="H15" t="n">
-        <v>24042</v>
+        <v>24279</v>
       </c>
       <c r="I15" t="n">
-        <v>4.72</v>
+        <v>4.766</v>
       </c>
       <c r="J15" t="n">
-        <v>308</v>
+        <v>237</v>
       </c>
       <c r="K15" t="n">
-        <v>0.06</v>
+        <v>0.047</v>
       </c>
       <c r="L15" t="n">
-        <v>357</v>
+        <v>368</v>
       </c>
       <c r="M15" t="n">
-        <v>0.07</v>
+        <v>0.072</v>
       </c>
       <c r="N15" t="s">
         <v>111</v>
@@ -3181,7 +3185,7 @@
         <v>115</v>
       </c>
       <c r="C16" s="1" t="n">
-        <v>43997</v>
+        <v>43999</v>
       </c>
       <c r="D16" t="s">
         <v>116</v>
@@ -3191,25 +3195,25 @@
       </c>
       <c r="F16"/>
       <c r="G16" t="n">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="H16" t="n">
-        <v>70254</v>
+        <v>70712</v>
       </c>
       <c r="I16" t="n">
-        <v>17.113</v>
+        <v>17.225</v>
       </c>
       <c r="J16" t="n">
-        <v>144</v>
+        <v>186</v>
       </c>
       <c r="K16" t="n">
-        <v>0.035</v>
+        <v>0.045</v>
       </c>
       <c r="L16" t="n">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="M16" t="n">
-        <v>0.048</v>
+        <v>0.047</v>
       </c>
       <c r="N16" t="s">
         <v>117</v>
@@ -3232,7 +3236,7 @@
         <v>122</v>
       </c>
       <c r="C17" s="1" t="n">
-        <v>43996</v>
+        <v>43998</v>
       </c>
       <c r="D17" t="s">
         <v>123</v>
@@ -3244,25 +3248,25 @@
         <v>125</v>
       </c>
       <c r="G17" t="n">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="H17" t="n">
-        <v>136249</v>
+        <v>141151</v>
       </c>
       <c r="I17" t="n">
-        <v>12.029</v>
+        <v>12.462</v>
       </c>
       <c r="J17" t="n">
-        <v>2486</v>
+        <v>2320</v>
       </c>
       <c r="K17" t="n">
-        <v>0.219</v>
+        <v>0.205</v>
       </c>
       <c r="L17" t="n">
-        <v>2245</v>
+        <v>2315</v>
       </c>
       <c r="M17" t="n">
-        <v>0.198</v>
+        <v>0.204</v>
       </c>
       <c r="N17" t="s">
         <v>124</v>
@@ -3285,7 +3289,7 @@
         <v>130</v>
       </c>
       <c r="C18" s="1" t="n">
-        <v>43996</v>
+        <v>43998</v>
       </c>
       <c r="D18" t="s">
         <v>131</v>
@@ -3295,25 +3299,25 @@
       </c>
       <c r="F18"/>
       <c r="G18" t="n">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="H18" t="n">
-        <v>497990</v>
+        <v>505272</v>
       </c>
       <c r="I18" t="n">
-        <v>46.502</v>
+        <v>47.182</v>
       </c>
       <c r="J18" t="n">
-        <v>1057</v>
+        <v>3592</v>
       </c>
       <c r="K18" t="n">
-        <v>0.099</v>
+        <v>0.335</v>
       </c>
       <c r="L18" t="n">
-        <v>3340</v>
+        <v>3061</v>
       </c>
       <c r="M18" t="n">
-        <v>0.312</v>
+        <v>0.286</v>
       </c>
       <c r="N18" t="s">
         <v>41</v>
@@ -3336,7 +3340,7 @@
         <v>135</v>
       </c>
       <c r="C19" s="1" t="n">
-        <v>43996</v>
+        <v>43998</v>
       </c>
       <c r="D19" t="s">
         <v>136</v>
@@ -3346,25 +3350,25 @@
       </c>
       <c r="F19"/>
       <c r="G19" t="n">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="H19" t="n">
-        <v>793096</v>
+        <v>821174</v>
       </c>
       <c r="I19" t="n">
-        <v>136.925</v>
+        <v>141.772</v>
       </c>
       <c r="J19" t="n">
-        <v>3185</v>
+        <v>5094</v>
       </c>
       <c r="K19" t="n">
-        <v>0.55</v>
+        <v>0.879</v>
       </c>
       <c r="L19" t="n">
-        <v>12608</v>
+        <v>11973</v>
       </c>
       <c r="M19" t="n">
-        <v>2.177</v>
+        <v>2.067</v>
       </c>
       <c r="N19" t="s">
         <v>137</v>
@@ -3387,7 +3391,7 @@
         <v>141</v>
       </c>
       <c r="C20" s="1" t="n">
-        <v>43996</v>
+        <v>43998</v>
       </c>
       <c r="D20" t="s">
         <v>142</v>
@@ -3399,21 +3403,21 @@
         <v>144</v>
       </c>
       <c r="G20" t="n">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="H20" t="n">
-        <v>89842</v>
+        <v>92964</v>
       </c>
       <c r="I20" t="n">
-        <v>5.092</v>
+        <v>5.269</v>
       </c>
       <c r="J20"/>
       <c r="K20"/>
       <c r="L20" t="n">
-        <v>1352</v>
+        <v>1526</v>
       </c>
       <c r="M20" t="n">
-        <v>0.077</v>
+        <v>0.086</v>
       </c>
       <c r="N20" t="s">
         <v>143</v>
@@ -3485,7 +3489,7 @@
         <v>153</v>
       </c>
       <c r="C22" s="1" t="n">
-        <v>43996</v>
+        <v>43998</v>
       </c>
       <c r="D22" t="s">
         <v>154</v>
@@ -3495,25 +3499,25 @@
       </c>
       <c r="F22"/>
       <c r="G22" t="n">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="H22" t="n">
-        <v>96639</v>
+        <v>99154</v>
       </c>
       <c r="I22" t="n">
-        <v>72.85</v>
+        <v>74.746</v>
       </c>
       <c r="J22" t="n">
-        <v>645</v>
+        <v>1455</v>
       </c>
       <c r="K22" t="n">
-        <v>0.486</v>
+        <v>1.097</v>
       </c>
       <c r="L22" t="n">
-        <v>861</v>
+        <v>897</v>
       </c>
       <c r="M22" t="n">
-        <v>0.649</v>
+        <v>0.676</v>
       </c>
       <c r="N22" t="s">
         <v>156</v>
@@ -3536,7 +3540,7 @@
         <v>161</v>
       </c>
       <c r="C23" s="1" t="n">
-        <v>43997</v>
+        <v>43999</v>
       </c>
       <c r="D23" t="s">
         <v>162</v>
@@ -3546,25 +3550,25 @@
       </c>
       <c r="F23"/>
       <c r="G23" t="n">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="H23" t="n">
-        <v>186985</v>
+        <v>197361</v>
       </c>
       <c r="I23" t="n">
-        <v>1.626</v>
+        <v>1.717</v>
       </c>
       <c r="J23" t="n">
-        <v>5636</v>
+        <v>5274</v>
       </c>
       <c r="K23" t="n">
-        <v>0.049</v>
+        <v>0.046</v>
       </c>
       <c r="L23" t="n">
-        <v>5607</v>
+        <v>5549</v>
       </c>
       <c r="M23" t="n">
-        <v>0.049</v>
+        <v>0.048</v>
       </c>
       <c r="N23" t="s">
         <v>163</v>
@@ -3587,7 +3591,7 @@
         <v>167</v>
       </c>
       <c r="C24" s="1" t="n">
-        <v>43995</v>
+        <v>43997</v>
       </c>
       <c r="D24" t="s">
         <v>168</v>
@@ -3597,25 +3601,25 @@
       </c>
       <c r="F24"/>
       <c r="G24" t="n">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="H24" t="n">
-        <v>219704</v>
+        <v>224016</v>
       </c>
       <c r="I24" t="n">
-        <v>39.653</v>
+        <v>40.431</v>
       </c>
       <c r="J24" t="n">
-        <v>1076</v>
+        <v>1625</v>
       </c>
       <c r="K24" t="n">
-        <v>0.194</v>
+        <v>0.293</v>
       </c>
       <c r="L24" t="n">
-        <v>1862</v>
+        <v>2086</v>
       </c>
       <c r="M24" t="n">
-        <v>0.336</v>
+        <v>0.376</v>
       </c>
       <c r="N24" t="s">
         <v>170</v>
@@ -3838,7 +3842,7 @@
         <v>200</v>
       </c>
       <c r="C29" s="1" t="n">
-        <v>43993</v>
+        <v>43995</v>
       </c>
       <c r="D29" t="s">
         <v>193</v>
@@ -3850,25 +3854,25 @@
         <v>201</v>
       </c>
       <c r="G29" t="n">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="H29" t="n">
-        <v>247592</v>
+        <v>254331</v>
       </c>
       <c r="I29" t="n">
-        <v>7.968</v>
+        <v>8.185</v>
       </c>
       <c r="J29" t="n">
-        <v>2144</v>
+        <v>3437</v>
       </c>
       <c r="K29" t="n">
-        <v>0.069</v>
+        <v>0.111</v>
       </c>
       <c r="L29" t="n">
-        <v>2643</v>
+        <v>2698</v>
       </c>
       <c r="M29" t="n">
-        <v>0.085</v>
+        <v>0.087</v>
       </c>
       <c r="N29" t="s">
         <v>196</v>
@@ -3891,7 +3895,7 @@
         <v>203</v>
       </c>
       <c r="C30" s="1" t="n">
-        <v>43997</v>
+        <v>43999</v>
       </c>
       <c r="D30" t="s">
         <v>204</v>
@@ -3901,25 +3905,25 @@
       </c>
       <c r="F30"/>
       <c r="G30" t="n">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="H30" t="n">
-        <v>254854</v>
+        <v>264930</v>
       </c>
       <c r="I30" t="n">
-        <v>24.451</v>
+        <v>25.418</v>
       </c>
       <c r="J30" t="n">
-        <v>3931</v>
+        <v>5194</v>
       </c>
       <c r="K30" t="n">
-        <v>0.377</v>
+        <v>0.498</v>
       </c>
       <c r="L30" t="n">
-        <v>3619</v>
+        <v>4345</v>
       </c>
       <c r="M30" t="n">
-        <v>0.347</v>
+        <v>0.417</v>
       </c>
       <c r="N30" t="s">
         <v>206</v>
@@ -4042,7 +4046,7 @@
         <v>225</v>
       </c>
       <c r="C33" s="1" t="n">
-        <v>43995</v>
+        <v>43998</v>
       </c>
       <c r="D33" t="s">
         <v>226</v>
@@ -4052,25 +4056,25 @@
       </c>
       <c r="F33"/>
       <c r="G33" t="n">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="H33" t="n">
-        <v>63143</v>
+        <v>63360</v>
       </c>
       <c r="I33" t="n">
-        <v>185.034</v>
+        <v>185.67</v>
       </c>
       <c r="J33" t="n">
-        <v>60</v>
+        <v>176</v>
       </c>
       <c r="K33" t="n">
-        <v>0.176</v>
+        <v>0.516</v>
       </c>
       <c r="L33" t="n">
-        <v>56</v>
+        <v>70</v>
       </c>
       <c r="M33" t="n">
-        <v>0.164</v>
+        <v>0.205</v>
       </c>
       <c r="N33" t="s">
         <v>227</v>
@@ -4146,7 +4150,7 @@
         <v>236</v>
       </c>
       <c r="C35" s="1" t="n">
-        <v>43997</v>
+        <v>43999</v>
       </c>
       <c r="D35" t="s">
         <v>232</v>
@@ -4158,25 +4162,25 @@
         <v>234</v>
       </c>
       <c r="G35" t="n">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="H35" t="n">
-        <v>5774133</v>
+        <v>6084256</v>
       </c>
       <c r="I35" t="n">
-        <v>4.184</v>
+        <v>4.409</v>
       </c>
       <c r="J35" t="n">
-        <v>115519</v>
+        <v>163187</v>
       </c>
       <c r="K35" t="n">
-        <v>0.084</v>
+        <v>0.118</v>
       </c>
       <c r="L35" t="n">
-        <v>142814</v>
+        <v>146132</v>
       </c>
       <c r="M35" t="n">
-        <v>0.103</v>
+        <v>0.106</v>
       </c>
       <c r="N35" t="s">
         <v>233</v>
@@ -4199,7 +4203,7 @@
         <v>238</v>
       </c>
       <c r="C36" s="1" t="n">
-        <v>43997</v>
+        <v>43999</v>
       </c>
       <c r="D36" t="s">
         <v>239</v>
@@ -4209,21 +4213,25 @@
       </c>
       <c r="F36"/>
       <c r="G36" t="n">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="H36" t="n">
-        <v>329190</v>
+        <v>348278</v>
       </c>
       <c r="I36" t="n">
-        <v>1.204</v>
-      </c>
-      <c r="J36"/>
-      <c r="K36"/>
+        <v>1.273</v>
+      </c>
+      <c r="J36" t="n">
+        <v>8969</v>
+      </c>
+      <c r="K36" t="n">
+        <v>0.033</v>
+      </c>
       <c r="L36" t="n">
-        <v>7823</v>
+        <v>8686</v>
       </c>
       <c r="M36" t="n">
-        <v>0.029</v>
+        <v>0.032</v>
       </c>
       <c r="N36" t="s">
         <v>240</v>
@@ -4297,7 +4305,7 @@
         <v>251</v>
       </c>
       <c r="C38" s="1" t="n">
-        <v>43991</v>
+        <v>43998</v>
       </c>
       <c r="D38" t="s">
         <v>252</v>
@@ -4307,21 +4315,21 @@
       </c>
       <c r="F38"/>
       <c r="G38" t="n">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H38" t="n">
-        <v>367780</v>
+        <v>386572</v>
       </c>
       <c r="I38" t="n">
-        <v>74.483</v>
+        <v>78.288</v>
       </c>
       <c r="J38"/>
       <c r="K38"/>
       <c r="L38" t="n">
-        <v>2766</v>
+        <v>2685</v>
       </c>
       <c r="M38" t="n">
-        <v>0.56</v>
+        <v>0.544</v>
       </c>
       <c r="N38" t="s">
         <v>212</v>
@@ -4344,7 +4352,7 @@
         <v>257</v>
       </c>
       <c r="C39" s="1" t="n">
-        <v>43990</v>
+        <v>43992</v>
       </c>
       <c r="D39" t="s">
         <v>258</v>
@@ -4354,25 +4362,25 @@
       </c>
       <c r="F39"/>
       <c r="G39" t="n">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="H39" t="n">
-        <v>679255</v>
+        <v>713594</v>
       </c>
       <c r="I39" t="n">
-        <v>78.476</v>
+        <v>82.444</v>
       </c>
       <c r="J39" t="n">
-        <v>14440</v>
+        <v>18480</v>
       </c>
       <c r="K39" t="n">
-        <v>1.668</v>
+        <v>2.135</v>
       </c>
       <c r="L39" t="n">
-        <v>13865</v>
+        <v>15137</v>
       </c>
       <c r="M39" t="n">
-        <v>1.602</v>
+        <v>1.749</v>
       </c>
       <c r="N39" t="s">
         <v>41</v>
@@ -4395,7 +4403,7 @@
         <v>263</v>
       </c>
       <c r="C40" s="1" t="n">
-        <v>43997</v>
+        <v>43998</v>
       </c>
       <c r="D40" t="s">
         <v>264</v>
@@ -4407,25 +4415,25 @@
         <v>266</v>
       </c>
       <c r="G40" t="n">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="H40" t="n">
-        <v>2864084</v>
+        <v>2891846</v>
       </c>
       <c r="I40" t="n">
-        <v>47.37</v>
+        <v>47.829</v>
       </c>
       <c r="J40" t="n">
-        <v>17463</v>
+        <v>27762</v>
       </c>
       <c r="K40" t="n">
-        <v>0.289</v>
+        <v>0.459</v>
       </c>
       <c r="L40" t="n">
-        <v>31514</v>
+        <v>30880</v>
       </c>
       <c r="M40" t="n">
-        <v>0.521</v>
+        <v>0.511</v>
       </c>
       <c r="N40" t="s">
         <v>267</v>
@@ -4448,7 +4456,7 @@
         <v>270</v>
       </c>
       <c r="C41" s="1" t="n">
-        <v>43996</v>
+        <v>43998</v>
       </c>
       <c r="D41" t="s">
         <v>264</v>
@@ -4460,25 +4468,25 @@
         <v>266</v>
       </c>
       <c r="G41" t="n">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="H41" t="n">
-        <v>4620718</v>
+        <v>4695707</v>
       </c>
       <c r="I41" t="n">
-        <v>76.424</v>
+        <v>77.664</v>
       </c>
       <c r="J41" t="n">
-        <v>56527</v>
+        <v>46882</v>
       </c>
       <c r="K41" t="n">
-        <v>0.935</v>
+        <v>0.775</v>
       </c>
       <c r="L41" t="n">
-        <v>54883</v>
+        <v>53865</v>
       </c>
       <c r="M41" t="n">
-        <v>0.908</v>
+        <v>0.891</v>
       </c>
       <c r="N41" t="s">
         <v>267</v>
@@ -4501,7 +4509,7 @@
         <v>273</v>
       </c>
       <c r="C42" s="1" t="n">
-        <v>43996</v>
+        <v>43998</v>
       </c>
       <c r="D42" t="s">
         <v>274</v>
@@ -4513,18 +4521,18 @@
         <v>276</v>
       </c>
       <c r="G42" t="n">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="H42" t="n">
-        <v>338758</v>
+        <v>344526</v>
       </c>
       <c r="I42" t="n">
-        <v>2.678</v>
+        <v>2.724</v>
       </c>
       <c r="J42"/>
       <c r="K42"/>
       <c r="L42" t="n">
-        <v>3468</v>
+        <v>3353</v>
       </c>
       <c r="M42" t="n">
         <v>0.027</v>
@@ -4550,7 +4558,7 @@
         <v>280</v>
       </c>
       <c r="C43" s="1" t="n">
-        <v>43993</v>
+        <v>43995</v>
       </c>
       <c r="D43" t="s">
         <v>281</v>
@@ -4562,25 +4570,25 @@
         <v>282</v>
       </c>
       <c r="G43" t="n">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="H43" t="n">
-        <v>557402</v>
+        <v>571831</v>
       </c>
       <c r="I43" t="n">
-        <v>4.407</v>
+        <v>4.521</v>
       </c>
       <c r="J43" t="n">
-        <v>5615</v>
+        <v>6468</v>
       </c>
       <c r="K43" t="n">
-        <v>0.044</v>
+        <v>0.051</v>
       </c>
       <c r="L43" t="n">
-        <v>6317</v>
+        <v>6483</v>
       </c>
       <c r="M43" t="n">
-        <v>0.05</v>
+        <v>0.051</v>
       </c>
       <c r="N43" t="s">
         <v>277</v>
@@ -4705,7 +4713,7 @@
         <v>297</v>
       </c>
       <c r="C46" s="1" t="n">
-        <v>43997</v>
+        <v>43999</v>
       </c>
       <c r="D46" t="s">
         <v>298</v>
@@ -4715,25 +4723,25 @@
       </c>
       <c r="F46"/>
       <c r="G46" t="n">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="H46" t="n">
-        <v>337387</v>
+        <v>343027</v>
       </c>
       <c r="I46" t="n">
-        <v>79.003</v>
+        <v>80.324</v>
       </c>
       <c r="J46" t="n">
-        <v>2775</v>
+        <v>2885</v>
       </c>
       <c r="K46" t="n">
-        <v>0.65</v>
+        <v>0.676</v>
       </c>
       <c r="L46" t="n">
-        <v>2729</v>
+        <v>2665</v>
       </c>
       <c r="M46" t="n">
-        <v>0.639</v>
+        <v>0.624</v>
       </c>
       <c r="N46" t="s">
         <v>299</v>
@@ -4756,7 +4764,7 @@
         <v>303</v>
       </c>
       <c r="C47" s="1" t="n">
-        <v>43996</v>
+        <v>43999</v>
       </c>
       <c r="D47" t="s">
         <v>304</v>
@@ -4768,25 +4776,25 @@
         <v>306</v>
       </c>
       <c r="G47" t="n">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="H47" t="n">
-        <v>127450</v>
+        <v>131646</v>
       </c>
       <c r="I47" t="n">
-        <v>67.57</v>
+        <v>69.794</v>
       </c>
       <c r="J47" t="n">
-        <v>1396</v>
+        <v>1810</v>
       </c>
       <c r="K47" t="n">
-        <v>0.74</v>
+        <v>0.96</v>
       </c>
       <c r="L47" t="n">
-        <v>1399</v>
+        <v>1409</v>
       </c>
       <c r="M47" t="n">
-        <v>0.742</v>
+        <v>0.747</v>
       </c>
       <c r="N47" t="s">
         <v>305</v>
@@ -4809,7 +4817,7 @@
         <v>309</v>
       </c>
       <c r="C48" s="1" t="n">
-        <v>43997</v>
+        <v>43999</v>
       </c>
       <c r="D48" t="s">
         <v>310</v>
@@ -4819,25 +4827,25 @@
       </c>
       <c r="F48"/>
       <c r="G48" t="n">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="H48" t="n">
-        <v>365136</v>
+        <v>375572</v>
       </c>
       <c r="I48" t="n">
-        <v>134.128</v>
+        <v>137.962</v>
       </c>
       <c r="J48" t="n">
-        <v>1608</v>
+        <v>6026</v>
       </c>
       <c r="K48" t="n">
-        <v>0.591</v>
+        <v>2.214</v>
       </c>
       <c r="L48" t="n">
-        <v>4207</v>
+        <v>4311</v>
       </c>
       <c r="M48" t="n">
-        <v>1.545</v>
+        <v>1.584</v>
       </c>
       <c r="N48" t="s">
         <v>41</v>
@@ -4860,7 +4868,7 @@
         <v>314</v>
       </c>
       <c r="C49" s="1" t="n">
-        <v>43997</v>
+        <v>43998</v>
       </c>
       <c r="D49" t="s">
         <v>315</v>
@@ -4870,25 +4878,25 @@
       </c>
       <c r="F49"/>
       <c r="G49" t="n">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="H49" t="n">
-        <v>110946</v>
+        <v>116869</v>
       </c>
       <c r="I49" t="n">
-        <v>177.237</v>
+        <v>186.699</v>
       </c>
       <c r="J49" t="n">
-        <v>4342</v>
+        <v>5923</v>
       </c>
       <c r="K49" t="n">
-        <v>6.936</v>
+        <v>9.462</v>
       </c>
       <c r="L49" t="n">
-        <v>3245</v>
+        <v>3994</v>
       </c>
       <c r="M49" t="n">
-        <v>5.184</v>
+        <v>6.38</v>
       </c>
       <c r="N49" t="s">
         <v>316</v>
@@ -4911,7 +4919,7 @@
         <v>320</v>
       </c>
       <c r="C50" s="1" t="n">
-        <v>43996</v>
+        <v>43998</v>
       </c>
       <c r="D50" t="s">
         <v>321</v>
@@ -4923,25 +4931,25 @@
         <v>323</v>
       </c>
       <c r="G50" t="n">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="H50" t="n">
-        <v>651344</v>
+        <v>659632</v>
       </c>
       <c r="I50" t="n">
-        <v>20.124</v>
+        <v>20.38</v>
       </c>
       <c r="J50" t="n">
-        <v>5289</v>
+        <v>3422</v>
       </c>
       <c r="K50" t="n">
-        <v>0.163</v>
+        <v>0.106</v>
       </c>
       <c r="L50" t="n">
-        <v>6357</v>
+        <v>5616</v>
       </c>
       <c r="M50" t="n">
-        <v>0.196</v>
+        <v>0.174</v>
       </c>
       <c r="N50" t="s">
         <v>41</v>
@@ -4964,7 +4972,7 @@
         <v>327</v>
       </c>
       <c r="C51" s="1" t="n">
-        <v>43992</v>
+        <v>43996</v>
       </c>
       <c r="D51" t="s">
         <v>328</v>
@@ -4976,25 +4984,25 @@
         <v>330</v>
       </c>
       <c r="G51" t="n">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="H51" t="n">
-        <v>32127</v>
+        <v>34741</v>
       </c>
       <c r="I51" t="n">
-        <v>59.435</v>
+        <v>64.271</v>
       </c>
       <c r="J51" t="n">
-        <v>772</v>
+        <v>629</v>
       </c>
       <c r="K51" t="n">
-        <v>1.428</v>
+        <v>1.164</v>
       </c>
       <c r="L51" t="n">
-        <v>841</v>
+        <v>737</v>
       </c>
       <c r="M51" t="n">
-        <v>1.556</v>
+        <v>1.363</v>
       </c>
       <c r="N51" t="s">
         <v>331</v>
@@ -5017,7 +5025,7 @@
         <v>335</v>
       </c>
       <c r="C52" s="1" t="n">
-        <v>43992</v>
+        <v>43993</v>
       </c>
       <c r="D52" t="s">
         <v>336</v>
@@ -5027,25 +5035,25 @@
       </c>
       <c r="F52"/>
       <c r="G52" t="n">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="H52" t="n">
-        <v>348058</v>
+        <v>363221</v>
       </c>
       <c r="I52" t="n">
-        <v>2.7</v>
+        <v>2.817</v>
       </c>
       <c r="J52" t="n">
-        <v>5866</v>
+        <v>7083</v>
       </c>
       <c r="K52" t="n">
-        <v>0.045</v>
+        <v>0.055</v>
       </c>
       <c r="L52" t="n">
-        <v>6833</v>
+        <v>7423</v>
       </c>
       <c r="M52" t="n">
-        <v>0.053</v>
+        <v>0.058</v>
       </c>
       <c r="N52" t="s">
         <v>338</v>
@@ -5272,7 +5280,7 @@
         <v>369</v>
       </c>
       <c r="C57" s="1" t="n">
-        <v>43995</v>
+        <v>43998</v>
       </c>
       <c r="D57" t="s">
         <v>370</v>
@@ -5282,25 +5290,25 @@
       </c>
       <c r="F57"/>
       <c r="G57" t="n">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="H57" t="n">
-        <v>310297</v>
+        <v>316251</v>
       </c>
       <c r="I57" t="n">
-        <v>64.347</v>
+        <v>65.582</v>
       </c>
       <c r="J57" t="n">
-        <v>2487</v>
+        <v>3603</v>
       </c>
       <c r="K57" t="n">
-        <v>0.516</v>
+        <v>0.747</v>
       </c>
       <c r="L57" t="n">
-        <v>2321</v>
+        <v>2531</v>
       </c>
       <c r="M57" t="n">
-        <v>0.481</v>
+        <v>0.525</v>
       </c>
       <c r="N57" t="s">
         <v>371</v>
@@ -5323,7 +5331,7 @@
         <v>374</v>
       </c>
       <c r="C58" s="1" t="n">
-        <v>43997</v>
+        <v>43998</v>
       </c>
       <c r="D58" t="s">
         <v>375</v>
@@ -5333,22 +5341,22 @@
       </c>
       <c r="F58"/>
       <c r="G58" t="n">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H58" t="n">
-        <v>94323</v>
+        <v>96402</v>
       </c>
       <c r="I58" t="n">
-        <v>0.458</v>
+        <v>0.468</v>
       </c>
       <c r="J58" t="n">
-        <v>1399</v>
+        <v>2079</v>
       </c>
       <c r="K58" t="n">
-        <v>0.007</v>
+        <v>0.01</v>
       </c>
       <c r="L58" t="n">
-        <v>2297</v>
+        <v>2351</v>
       </c>
       <c r="M58" t="n">
         <v>0.011</v>
@@ -5374,7 +5382,7 @@
         <v>380</v>
       </c>
       <c r="C59" s="1" t="n">
-        <v>43997</v>
+        <v>43999</v>
       </c>
       <c r="D59" t="s">
         <v>381</v>
@@ -5384,21 +5392,25 @@
       </c>
       <c r="F59"/>
       <c r="G59" t="n">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="H59" t="n">
-        <v>285867</v>
+        <v>292891</v>
       </c>
       <c r="I59" t="n">
-        <v>52.731</v>
-      </c>
-      <c r="J59"/>
-      <c r="K59"/>
+        <v>54.027</v>
+      </c>
+      <c r="J59" t="n">
+        <v>4350</v>
+      </c>
+      <c r="K59" t="n">
+        <v>0.802</v>
+      </c>
       <c r="L59" t="n">
-        <v>3376</v>
+        <v>3573</v>
       </c>
       <c r="M59" t="n">
-        <v>0.623</v>
+        <v>0.659</v>
       </c>
       <c r="N59" t="s">
         <v>382</v>
@@ -5421,7 +5433,7 @@
         <v>387</v>
       </c>
       <c r="C60" s="1" t="n">
-        <v>43997</v>
+        <v>43999</v>
       </c>
       <c r="D60" t="s">
         <v>388</v>
@@ -5431,25 +5443,25 @@
       </c>
       <c r="F60"/>
       <c r="G60" t="n">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="H60" t="n">
-        <v>897650</v>
+        <v>950782</v>
       </c>
       <c r="I60" t="n">
-        <v>4.064</v>
+        <v>4.304</v>
       </c>
       <c r="J60" t="n">
-        <v>29085</v>
+        <v>28117</v>
       </c>
       <c r="K60" t="n">
-        <v>0.132</v>
+        <v>0.127</v>
       </c>
       <c r="L60" t="n">
-        <v>27402</v>
+        <v>28076</v>
       </c>
       <c r="M60" t="n">
-        <v>0.124</v>
+        <v>0.127</v>
       </c>
       <c r="N60" t="s">
         <v>389</v>
@@ -5472,7 +5484,7 @@
         <v>393</v>
       </c>
       <c r="C61" s="1" t="n">
-        <v>43996</v>
+        <v>43998</v>
       </c>
       <c r="D61" t="s">
         <v>394</v>
@@ -5482,25 +5494,25 @@
       </c>
       <c r="F61"/>
       <c r="G61" t="n">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="H61" t="n">
-        <v>88966</v>
+        <v>92595</v>
       </c>
       <c r="I61" t="n">
-        <v>20.619</v>
+        <v>21.46</v>
       </c>
       <c r="J61" t="n">
-        <v>1880</v>
+        <v>1645</v>
       </c>
       <c r="K61" t="n">
-        <v>0.436</v>
+        <v>0.381</v>
       </c>
       <c r="L61" t="n">
-        <v>1987</v>
+        <v>2066</v>
       </c>
       <c r="M61" t="n">
-        <v>0.461</v>
+        <v>0.479</v>
       </c>
       <c r="N61" t="s">
         <v>395</v>
@@ -5574,7 +5586,7 @@
         <v>404</v>
       </c>
       <c r="C63" s="1" t="n">
-        <v>43996</v>
+        <v>43999</v>
       </c>
       <c r="D63" t="s">
         <v>405</v>
@@ -5584,25 +5596,21 @@
       </c>
       <c r="F63"/>
       <c r="G63" t="n">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="H63" t="n">
-        <v>191072</v>
+        <v>198817</v>
       </c>
       <c r="I63" t="n">
-        <v>5.795</v>
-      </c>
-      <c r="J63" t="n">
-        <v>7929</v>
-      </c>
-      <c r="K63" t="n">
-        <v>0.24</v>
-      </c>
+        <v>6.03</v>
+      </c>
+      <c r="J63"/>
+      <c r="K63"/>
       <c r="L63" t="n">
-        <v>3933</v>
+        <v>3583</v>
       </c>
       <c r="M63" t="n">
-        <v>0.119</v>
+        <v>0.109</v>
       </c>
       <c r="N63" t="s">
         <v>406</v>
@@ -5625,7 +5633,7 @@
         <v>410</v>
       </c>
       <c r="C64" s="1" t="n">
-        <v>43994</v>
+        <v>43997</v>
       </c>
       <c r="D64" t="s">
         <v>411</v>
@@ -5637,25 +5645,25 @@
         <v>413</v>
       </c>
       <c r="G64" t="n">
-        <v>42</v>
+        <v>74</v>
       </c>
       <c r="H64" t="n">
-        <v>457029</v>
+        <v>484181</v>
       </c>
       <c r="I64" t="n">
-        <v>4.171</v>
+        <v>4.418</v>
       </c>
       <c r="J64" t="n">
-        <v>10880</v>
+        <v>7263</v>
       </c>
       <c r="K64" t="n">
-        <v>0.099</v>
+        <v>0.066</v>
       </c>
       <c r="L64" t="n">
-        <v>10043</v>
+        <v>9677</v>
       </c>
       <c r="M64" t="n">
-        <v>0.092</v>
+        <v>0.088</v>
       </c>
       <c r="N64" t="s">
         <v>212</v>
@@ -5731,7 +5739,7 @@
         <v>424</v>
       </c>
       <c r="C66" s="1" t="n">
-        <v>43991</v>
+        <v>43996</v>
       </c>
       <c r="D66" t="s">
         <v>425</v>
@@ -5741,25 +5749,25 @@
       </c>
       <c r="F66"/>
       <c r="G66" t="n">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="H66" t="n">
-        <v>966328</v>
+        <v>1006454</v>
       </c>
       <c r="I66" t="n">
-        <v>94.769</v>
+        <v>98.704</v>
       </c>
       <c r="J66" t="n">
-        <v>11801</v>
+        <v>4726</v>
       </c>
       <c r="K66" t="n">
-        <v>1.157</v>
+        <v>0.463</v>
       </c>
       <c r="L66" t="n">
-        <v>12749</v>
+        <v>8601</v>
       </c>
       <c r="M66" t="n">
-        <v>1.25</v>
+        <v>0.844</v>
       </c>
       <c r="N66" t="s">
         <v>426</v>
@@ -5782,7 +5790,7 @@
         <v>430</v>
       </c>
       <c r="C67" s="1" t="n">
-        <v>43996</v>
+        <v>43998</v>
       </c>
       <c r="D67" t="s">
         <v>431</v>
@@ -5792,25 +5800,25 @@
       </c>
       <c r="F67"/>
       <c r="G67" t="n">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="H67" t="n">
-        <v>290714</v>
+        <v>300499</v>
       </c>
       <c r="I67" t="n">
-        <v>100.905</v>
+        <v>104.302</v>
       </c>
       <c r="J67" t="n">
-        <v>3884</v>
+        <v>5161</v>
       </c>
       <c r="K67" t="n">
-        <v>1.348</v>
+        <v>1.791</v>
       </c>
       <c r="L67" t="n">
-        <v>5028</v>
+        <v>5066</v>
       </c>
       <c r="M67" t="n">
-        <v>1.745</v>
+        <v>1.758</v>
       </c>
       <c r="N67" t="s">
         <v>432</v>
@@ -5833,7 +5841,7 @@
         <v>436</v>
       </c>
       <c r="C68" s="1" t="n">
-        <v>43996</v>
+        <v>43999</v>
       </c>
       <c r="D68" t="s">
         <v>437</v>
@@ -5843,25 +5851,25 @@
       </c>
       <c r="F68"/>
       <c r="G68" t="n">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="H68" t="n">
-        <v>560596</v>
+        <v>585353</v>
       </c>
       <c r="I68" t="n">
-        <v>29.141</v>
+        <v>30.427</v>
       </c>
       <c r="J68" t="n">
-        <v>7926</v>
+        <v>11715</v>
       </c>
       <c r="K68" t="n">
-        <v>0.412</v>
+        <v>0.609</v>
       </c>
       <c r="L68" t="n">
-        <v>8199</v>
+        <v>9256</v>
       </c>
       <c r="M68" t="n">
-        <v>0.426</v>
+        <v>0.481</v>
       </c>
       <c r="N68" t="s">
         <v>438</v>
@@ -5884,7 +5892,7 @@
         <v>442</v>
       </c>
       <c r="C69" s="1" t="n">
-        <v>43997</v>
+        <v>43999</v>
       </c>
       <c r="D69" t="s">
         <v>443</v>
@@ -5894,25 +5902,25 @@
       </c>
       <c r="F69"/>
       <c r="G69" t="n">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="H69" t="n">
-        <v>15161152</v>
+        <v>15679724</v>
       </c>
       <c r="I69" t="n">
-        <v>103.89</v>
+        <v>107.444</v>
       </c>
       <c r="J69" t="n">
-        <v>280980</v>
+        <v>284307</v>
       </c>
       <c r="K69" t="n">
-        <v>1.925</v>
+        <v>1.948</v>
       </c>
       <c r="L69" t="n">
-        <v>306447</v>
+        <v>304917</v>
       </c>
       <c r="M69" t="n">
-        <v>2.1</v>
+        <v>2.089</v>
       </c>
       <c r="N69" t="s">
         <v>444</v>
@@ -5986,7 +5994,7 @@
         <v>454</v>
       </c>
       <c r="C71" s="1" t="n">
-        <v>43996</v>
+        <v>43998</v>
       </c>
       <c r="D71" t="s">
         <v>455</v>
@@ -5996,25 +6004,25 @@
       </c>
       <c r="F71"/>
       <c r="G71" t="n">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="H71" t="n">
-        <v>1106398</v>
+        <v>1144282</v>
       </c>
       <c r="I71" t="n">
-        <v>31.78</v>
+        <v>32.869</v>
       </c>
       <c r="J71" t="n">
-        <v>19377</v>
+        <v>17629</v>
       </c>
       <c r="K71" t="n">
-        <v>0.557</v>
+        <v>0.506</v>
       </c>
       <c r="L71" t="n">
-        <v>21627</v>
+        <v>20944</v>
       </c>
       <c r="M71" t="n">
-        <v>0.621</v>
+        <v>0.602</v>
       </c>
       <c r="N71" t="s">
         <v>41</v>
@@ -6037,7 +6045,7 @@
         <v>458</v>
       </c>
       <c r="C72" s="1" t="n">
-        <v>43996</v>
+        <v>43998</v>
       </c>
       <c r="D72" t="s">
         <v>459</v>
@@ -6049,25 +6057,25 @@
         <v>461</v>
       </c>
       <c r="G72" t="n">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="H72" t="n">
-        <v>61509</v>
+        <v>63762</v>
       </c>
       <c r="I72" t="n">
-        <v>3.674</v>
+        <v>3.808</v>
       </c>
       <c r="J72" t="n">
-        <v>1223</v>
+        <v>999</v>
       </c>
       <c r="K72" t="n">
-        <v>0.073</v>
+        <v>0.06</v>
       </c>
       <c r="L72" t="n">
-        <v>1198</v>
+        <v>1175</v>
       </c>
       <c r="M72" t="n">
-        <v>0.072</v>
+        <v>0.07</v>
       </c>
       <c r="N72" t="s">
         <v>462</v>
@@ -6090,7 +6098,7 @@
         <v>467</v>
       </c>
       <c r="C73" s="1" t="n">
-        <v>43995</v>
+        <v>43998</v>
       </c>
       <c r="D73" t="s">
         <v>468</v>
@@ -6102,25 +6110,25 @@
         <v>469</v>
       </c>
       <c r="G73" t="n">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="H73" t="n">
-        <v>301126</v>
+        <v>313483</v>
       </c>
       <c r="I73" t="n">
-        <v>44.253</v>
+        <v>46.069</v>
       </c>
       <c r="J73" t="n">
-        <v>3337</v>
+        <v>5470</v>
       </c>
       <c r="K73" t="n">
-        <v>0.49</v>
+        <v>0.804</v>
       </c>
       <c r="L73" t="n">
-        <v>4563</v>
+        <v>4491</v>
       </c>
       <c r="M73" t="n">
-        <v>0.671</v>
+        <v>0.66</v>
       </c>
       <c r="N73" t="s">
         <v>41</v>
@@ -6143,7 +6151,7 @@
         <v>473</v>
       </c>
       <c r="C74" s="1" t="n">
-        <v>43990</v>
+        <v>43997</v>
       </c>
       <c r="D74" t="s">
         <v>474</v>
@@ -6153,21 +6161,21 @@
       </c>
       <c r="F74"/>
       <c r="G74" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H74" t="n">
-        <v>284963</v>
+        <v>340894</v>
       </c>
       <c r="I74" t="n">
-        <v>48.709</v>
+        <v>58.269</v>
       </c>
       <c r="J74"/>
       <c r="K74"/>
       <c r="L74" t="n">
-        <v>2939</v>
+        <v>7990</v>
       </c>
       <c r="M74" t="n">
-        <v>0.502</v>
+        <v>1.366</v>
       </c>
       <c r="N74" t="s">
         <v>41</v>
@@ -6190,7 +6198,7 @@
         <v>477</v>
       </c>
       <c r="C75" s="1" t="n">
-        <v>43990</v>
+        <v>43997</v>
       </c>
       <c r="D75" t="s">
         <v>478</v>
@@ -6200,21 +6208,21 @@
       </c>
       <c r="F75"/>
       <c r="G75" t="n">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="H75" t="n">
-        <v>488695</v>
+        <v>576189</v>
       </c>
       <c r="I75" t="n">
-        <v>83.533</v>
+        <v>98.488</v>
       </c>
       <c r="J75"/>
       <c r="K75"/>
       <c r="L75" t="n">
-        <v>11457</v>
+        <v>12499</v>
       </c>
       <c r="M75" t="n">
-        <v>1.958</v>
+        <v>2.136</v>
       </c>
       <c r="N75" t="s">
         <v>41</v>
@@ -6237,7 +6245,7 @@
         <v>481</v>
       </c>
       <c r="C76" s="1" t="n">
-        <v>43996</v>
+        <v>43999</v>
       </c>
       <c r="D76" t="s">
         <v>482</v>
@@ -6247,25 +6255,25 @@
       </c>
       <c r="F76"/>
       <c r="G76" t="n">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="H76" t="n">
-        <v>196723</v>
+        <v>198780</v>
       </c>
       <c r="I76" t="n">
-        <v>36.032</v>
+        <v>36.409</v>
       </c>
       <c r="J76" t="n">
-        <v>479</v>
+        <v>1163</v>
       </c>
       <c r="K76" t="n">
-        <v>0.088</v>
+        <v>0.213</v>
       </c>
       <c r="L76" t="n">
-        <v>1044</v>
+        <v>973</v>
       </c>
       <c r="M76" t="n">
-        <v>0.191</v>
+        <v>0.178</v>
       </c>
       <c r="N76" t="s">
         <v>484</v>
@@ -6288,7 +6296,7 @@
         <v>489</v>
       </c>
       <c r="C77" s="1" t="n">
-        <v>43996</v>
+        <v>43998</v>
       </c>
       <c r="D77" t="s">
         <v>490</v>
@@ -6298,19 +6306,19 @@
       </c>
       <c r="F77"/>
       <c r="G77" t="n">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="H77" t="n">
-        <v>87598</v>
+        <v>89151</v>
       </c>
       <c r="I77" t="n">
-        <v>42.136</v>
+        <v>42.883</v>
       </c>
       <c r="J77" t="n">
-        <v>212</v>
+        <v>986</v>
       </c>
       <c r="K77" t="n">
-        <v>0.102</v>
+        <v>0.474</v>
       </c>
       <c r="L77" t="n">
         <v>612</v>
@@ -6339,7 +6347,7 @@
         <v>496</v>
       </c>
       <c r="C78" s="1" t="n">
-        <v>43996</v>
+        <v>43998</v>
       </c>
       <c r="D78" t="s">
         <v>497</v>
@@ -6351,25 +6359,25 @@
         <v>499</v>
       </c>
       <c r="G78" t="n">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="H78" t="n">
-        <v>1121958</v>
+        <v>1172513</v>
       </c>
       <c r="I78" t="n">
-        <v>18.917</v>
+        <v>19.77</v>
       </c>
       <c r="J78" t="n">
-        <v>34071</v>
+        <v>23580</v>
       </c>
       <c r="K78" t="n">
-        <v>0.574</v>
+        <v>0.398</v>
       </c>
       <c r="L78" t="n">
-        <v>28842</v>
+        <v>29206</v>
       </c>
       <c r="M78" t="n">
-        <v>0.486</v>
+        <v>0.492</v>
       </c>
       <c r="N78" t="s">
         <v>498</v>
@@ -6392,7 +6400,7 @@
         <v>503</v>
       </c>
       <c r="C79" s="1" t="n">
-        <v>43997</v>
+        <v>43999</v>
       </c>
       <c r="D79" t="s">
         <v>504</v>
@@ -6402,25 +6410,25 @@
       </c>
       <c r="F79"/>
       <c r="G79" t="n">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="H79" t="n">
-        <v>1105719</v>
+        <v>1132823</v>
       </c>
       <c r="I79" t="n">
-        <v>21.567</v>
+        <v>22.096</v>
       </c>
       <c r="J79" t="n">
-        <v>5391</v>
+        <v>13056</v>
       </c>
       <c r="K79" t="n">
-        <v>0.105</v>
+        <v>0.255</v>
       </c>
       <c r="L79" t="n">
-        <v>12501</v>
+        <v>11550</v>
       </c>
       <c r="M79" t="n">
-        <v>0.244</v>
+        <v>0.225</v>
       </c>
       <c r="N79" t="s">
         <v>505</v>
@@ -6490,7 +6498,7 @@
         <v>516</v>
       </c>
       <c r="C81" s="1" t="n">
-        <v>43989</v>
+        <v>43996</v>
       </c>
       <c r="D81" t="s">
         <v>517</v>
@@ -6500,21 +6508,21 @@
       </c>
       <c r="F81"/>
       <c r="G81" t="n">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="H81" t="n">
-        <v>325000</v>
+        <v>385659</v>
       </c>
       <c r="I81" t="n">
-        <v>32.181</v>
+        <v>38.187</v>
       </c>
       <c r="J81"/>
       <c r="K81"/>
       <c r="L81" t="n">
-        <v>7029</v>
+        <v>8668</v>
       </c>
       <c r="M81" t="n">
-        <v>0.696</v>
+        <v>0.858</v>
       </c>
       <c r="N81" t="s">
         <v>518</v>
@@ -6537,7 +6545,7 @@
         <v>522</v>
       </c>
       <c r="C82" s="1" t="n">
-        <v>43995</v>
+        <v>43998</v>
       </c>
       <c r="D82" t="s">
         <v>523</v>
@@ -6547,25 +6555,25 @@
       </c>
       <c r="F82"/>
       <c r="G82" t="n">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="H82" t="n">
-        <v>459708</v>
+        <v>475224</v>
       </c>
       <c r="I82" t="n">
-        <v>53.117</v>
+        <v>54.91</v>
       </c>
       <c r="J82" t="n">
-        <v>4145</v>
+        <v>7477</v>
       </c>
       <c r="K82" t="n">
-        <v>0.479</v>
+        <v>0.864</v>
       </c>
       <c r="L82" t="n">
-        <v>5040</v>
+        <v>5443</v>
       </c>
       <c r="M82" t="n">
-        <v>0.582</v>
+        <v>0.629</v>
       </c>
       <c r="N82" t="s">
         <v>524</v>
@@ -6588,7 +6596,7 @@
         <v>528</v>
       </c>
       <c r="C83" s="1" t="n">
-        <v>43991</v>
+        <v>43998</v>
       </c>
       <c r="D83" t="s">
         <v>529</v>
@@ -6598,18 +6606,18 @@
       </c>
       <c r="F83"/>
       <c r="G83" t="n">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="H83" t="n">
-        <v>73751</v>
+        <v>74699</v>
       </c>
       <c r="I83" t="n">
-        <v>3.097</v>
+        <v>3.136</v>
       </c>
       <c r="J83"/>
       <c r="K83"/>
       <c r="L83" t="n">
-        <v>153</v>
+        <v>135</v>
       </c>
       <c r="M83" t="n">
         <v>0.006</v>
@@ -6635,7 +6643,7 @@
         <v>535</v>
       </c>
       <c r="C84" s="1" t="n">
-        <v>43997</v>
+        <v>43999</v>
       </c>
       <c r="D84" t="s">
         <v>536</v>
@@ -6645,25 +6653,25 @@
       </c>
       <c r="F84"/>
       <c r="G84" t="n">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="H84" t="n">
-        <v>271701</v>
+        <v>280461</v>
       </c>
       <c r="I84" t="n">
-        <v>3.893</v>
+        <v>4.018</v>
       </c>
       <c r="J84" t="n">
-        <v>4137</v>
+        <v>3888</v>
       </c>
       <c r="K84" t="n">
-        <v>0.059</v>
+        <v>0.056</v>
       </c>
       <c r="L84" t="n">
-        <v>4966</v>
+        <v>4341</v>
       </c>
       <c r="M84" t="n">
-        <v>0.071</v>
+        <v>0.062</v>
       </c>
       <c r="N84" t="s">
         <v>538</v>
@@ -6735,7 +6743,7 @@
         <v>548</v>
       </c>
       <c r="C86" s="1" t="n">
-        <v>43994</v>
+        <v>43997</v>
       </c>
       <c r="D86" t="s">
         <v>549</v>
@@ -6745,25 +6753,21 @@
       </c>
       <c r="F86"/>
       <c r="G86" t="n">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="H86" t="n">
-        <v>59887</v>
+        <v>67398</v>
       </c>
       <c r="I86" t="n">
-        <v>5.067</v>
-      </c>
-      <c r="J86" t="n">
-        <v>1117</v>
-      </c>
-      <c r="K86" t="n">
-        <v>0.095</v>
-      </c>
+        <v>5.703</v>
+      </c>
+      <c r="J86"/>
+      <c r="K86"/>
       <c r="L86" t="n">
-        <v>743</v>
+        <v>1653</v>
       </c>
       <c r="M86" t="n">
-        <v>0.063</v>
+        <v>0.14</v>
       </c>
       <c r="N86" t="s">
         <v>550</v>
@@ -6786,7 +6790,7 @@
         <v>555</v>
       </c>
       <c r="C87" s="1" t="n">
-        <v>43996</v>
+        <v>43998</v>
       </c>
       <c r="D87" t="s">
         <v>556</v>
@@ -6796,25 +6800,25 @@
       </c>
       <c r="F87"/>
       <c r="G87" t="n">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="H87" t="n">
-        <v>2632171</v>
+        <v>2721003</v>
       </c>
       <c r="I87" t="n">
-        <v>31.209</v>
+        <v>32.263</v>
       </c>
       <c r="J87" t="n">
-        <v>90268</v>
+        <v>46800</v>
       </c>
       <c r="K87" t="n">
-        <v>1.07</v>
+        <v>0.555</v>
       </c>
       <c r="L87" t="n">
-        <v>41940</v>
+        <v>43689</v>
       </c>
       <c r="M87" t="n">
-        <v>0.497</v>
+        <v>0.518</v>
       </c>
       <c r="N87" t="s">
         <v>557</v>
@@ -6837,7 +6841,7 @@
         <v>562</v>
       </c>
       <c r="C88" s="1" t="n">
-        <v>43995</v>
+        <v>43997</v>
       </c>
       <c r="D88" t="s">
         <v>563</v>
@@ -6849,25 +6853,25 @@
         <v>565</v>
       </c>
       <c r="G88" t="n">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="H88" t="n">
-        <v>125491</v>
+        <v>130380</v>
       </c>
       <c r="I88" t="n">
-        <v>2.744</v>
+        <v>2.85</v>
       </c>
       <c r="J88" t="n">
-        <v>2949</v>
+        <v>2212</v>
       </c>
       <c r="K88" t="n">
-        <v>0.064</v>
+        <v>0.048</v>
       </c>
       <c r="L88" t="n">
-        <v>2701</v>
+        <v>2529</v>
       </c>
       <c r="M88" t="n">
-        <v>0.059</v>
+        <v>0.055</v>
       </c>
       <c r="N88" t="s">
         <v>564</v>
@@ -6890,7 +6894,7 @@
         <v>569</v>
       </c>
       <c r="C89" s="1" t="n">
-        <v>43997</v>
+        <v>43999</v>
       </c>
       <c r="D89" t="s">
         <v>570</v>
@@ -6900,25 +6904,25 @@
       </c>
       <c r="F89"/>
       <c r="G89" t="n">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="H89" t="n">
-        <v>497284</v>
+        <v>571995</v>
       </c>
       <c r="I89" t="n">
-        <v>11.371</v>
+        <v>13.079</v>
       </c>
       <c r="J89" t="n">
-        <v>7950</v>
+        <v>64744</v>
       </c>
       <c r="K89" t="n">
-        <v>0.182</v>
+        <v>1.48</v>
       </c>
       <c r="L89" t="n">
-        <v>9457</v>
+        <v>18008</v>
       </c>
       <c r="M89" t="n">
-        <v>0.216</v>
+        <v>0.412</v>
       </c>
       <c r="N89" t="s">
         <v>571</v>
@@ -6992,7 +6996,7 @@
         <v>581</v>
       </c>
       <c r="C91" s="1" t="n">
-        <v>43996</v>
+        <v>43998</v>
       </c>
       <c r="D91" t="s">
         <v>582</v>
@@ -7004,25 +7008,25 @@
         <v>583</v>
       </c>
       <c r="G91" t="n">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="H91" t="n">
-        <v>3915362</v>
+        <v>4032084</v>
       </c>
       <c r="I91" t="n">
-        <v>57.676</v>
+        <v>59.395</v>
       </c>
       <c r="J91" t="n">
-        <v>47457</v>
+        <v>65301</v>
       </c>
       <c r="K91" t="n">
-        <v>0.699</v>
+        <v>0.962</v>
       </c>
       <c r="L91" t="n">
-        <v>74084</v>
+        <v>68268</v>
       </c>
       <c r="M91" t="n">
-        <v>1.091</v>
+        <v>1.006</v>
       </c>
       <c r="N91" t="s">
         <v>578</v>
@@ -7045,7 +7049,7 @@
         <v>586</v>
       </c>
       <c r="C92" s="1" t="n">
-        <v>43994</v>
+        <v>43998</v>
       </c>
       <c r="D92" t="s">
         <v>587</v>
@@ -7055,25 +7059,25 @@
       </c>
       <c r="F92"/>
       <c r="G92" t="n">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="H92" t="n">
-        <v>23290724</v>
+        <v>23765801</v>
       </c>
       <c r="I92" t="n">
-        <v>70.364</v>
+        <v>71.799</v>
       </c>
       <c r="J92" t="n">
-        <v>871843</v>
+        <v>297820</v>
       </c>
       <c r="K92" t="n">
-        <v>2.634</v>
+        <v>0.9</v>
       </c>
       <c r="L92" t="n">
-        <v>415125</v>
+        <v>296024</v>
       </c>
       <c r="M92" t="n">
-        <v>1.254</v>
+        <v>0.894</v>
       </c>
       <c r="N92" t="s">
         <v>588</v>
@@ -7096,7 +7100,7 @@
         <v>592</v>
       </c>
       <c r="C93" s="1" t="n">
-        <v>43996</v>
+        <v>43998</v>
       </c>
       <c r="D93" t="s">
         <v>593</v>
@@ -7106,25 +7110,25 @@
       </c>
       <c r="F93"/>
       <c r="G93" t="n">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="H93" t="n">
-        <v>23535104</v>
+        <v>24449307</v>
       </c>
       <c r="I93" t="n">
-        <v>71.102</v>
+        <v>73.864</v>
       </c>
       <c r="J93" t="n">
-        <v>485082</v>
+        <v>464715</v>
       </c>
       <c r="K93" t="n">
-        <v>1.465</v>
+        <v>1.404</v>
       </c>
       <c r="L93" t="n">
-        <v>467854</v>
+        <v>481920</v>
       </c>
       <c r="M93" t="n">
-        <v>1.413</v>
+        <v>1.456</v>
       </c>
       <c r="N93" t="s">
         <v>594</v>
@@ -7147,7 +7151,7 @@
         <v>599</v>
       </c>
       <c r="C94" s="1" t="n">
-        <v>43997</v>
+        <v>43999</v>
       </c>
       <c r="D94" t="s">
         <v>600</v>
@@ -7157,19 +7161,19 @@
       </c>
       <c r="F94"/>
       <c r="G94" t="n">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="H94" t="n">
-        <v>53265</v>
+        <v>54486</v>
       </c>
       <c r="I94" t="n">
-        <v>15.334</v>
+        <v>15.685</v>
       </c>
       <c r="J94" t="n">
-        <v>403</v>
+        <v>761</v>
       </c>
       <c r="K94" t="n">
-        <v>0.116</v>
+        <v>0.219</v>
       </c>
       <c r="L94" t="n">
         <v>690</v>

</xml_diff>

<commit_message>
Updated testing data for 2020-06-19
</commit_message>
<xml_diff>
--- a/public/data/testing/covid-testing-latest-data-source-details.xlsx
+++ b/public/data/testing/covid-testing-latest-data-source-details.xlsx
@@ -584,13 +584,13 @@
     <t xml:space="preserve">France - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.santepubliquefrance.fr/content/download/259223/2638086</t>
+    <t xml:space="preserve">https://www.santepubliquefrance.fr/content/download/260891/2645733</t>
   </si>
   <si>
     <t xml:space="preserve">National Public Health Agency</t>
   </si>
   <si>
-    <t xml:space="preserve">Dividing 194,099 (weekly total) by 7</t>
+    <t xml:space="preserve">Dividing 214,252 (weekly total) by 7</t>
   </si>
   <si>
     <t xml:space="preserve">https://www.santepubliquefrance.fr/recherche/#search=COVID-19%20:%20point%20epidemiologique&amp;sort=dat</t>
@@ -1677,7 +1677,7 @@
   <si>
     <t xml:space="preserve">The Government information website provides figures for the number of tests completed ("Opravljeni testi"). A time series of both cumulative and daily tests is available to download. This date back to the 12 March, where 3863 tests are reported to have already been performed (it is not known from which date this first cumulative figure dates back to).
 The same cumulative figure is published each day by the [National Insitute for Public Health (NIJZ)](https://www.nijz.si/sl/dnevno-spremljanje-okuzb-s-sars-cov-2-covid-19). Here they clarify that figures relate to the number of tests – including those for people who were tested several times.
-A footnote states that the figures relate to "Laboratory tests performed as part of routine testing and the COVID-19 National Survey are included." The later appears to refer to the prevalence study described on this [Government page](https://www.gov.si/en/news/2020-04-24-national-covid-19-prevalence-survey/). The description of the study states that "The survey is being conducted on a random sample of 3,000 persons" and that people will be tested with both a PCR and a serological test.
+A footnote states that the figures relate to "Laboratory tests performed as part of routine testing and the COVID-19 National Survey are included." The later appears to refer to the prevalence study described on this [Government page](https://www.gov.si/en/news/2020-04-24-national-covid-19-prevalence-survey/). The description of the study states that "The survey is being conducted on a random sample of 3,000 persons" and that people will be tested with both a PCR and a serological test. For this reason, the reported testing figures may include serological tests in addition to PCR tests.
 The volunteer-led [Sledilnik.org project](https://covid-19.sledilnik.org/#/) also presents the official data in a helpful website.</t>
   </si>
   <si>
@@ -1792,7 +1792,7 @@
     <t xml:space="preserve">The number of tests perfomed.</t>
   </si>
   <si>
-    <t xml:space="preserve">The Federal Office of Public Health presents a time series of daily positive and negative tests as a graphic. The data can be accessed by downloading the graphic software file. The graphic notes that "Since several tests can be taken and reported per person, the number of positive tests is higher than the number of positively tested people". (via Googl translate).
+    <t xml:space="preserve">The Federal Office of Public Health presents a time series of daily positive and negative tests as a graphic. The data can be accessed by downloading the graphic software file. The graphic notes that "Since several tests can be taken and reported per person, the number of positive tests is higher than the number of positively tested people". (via Google translate).
 The Federal Office of Public Health also publishes a [daily report](https://www.bag.admin.ch/bag/de/home/krankheiten/ausbrueche-epidemien-pandemien/aktuelle-ausbrueche-epidemien/novel-cov/situation-schweiz-und-international.html#316168418) on the epidemiological situation, in which very similar cumulative figures are provided, but often rounded-off. These reports present the figures as "The number of tests carried out on SARS-CoV-2, the causative agent of COVID-19".</t>
   </si>
   <si>
@@ -3658,7 +3658,7 @@
         <v>174</v>
       </c>
       <c r="C25" s="1" t="n">
-        <v>43988</v>
+        <v>43995</v>
       </c>
       <c r="D25" t="s">
         <v>175</v>
@@ -3670,21 +3670,21 @@
         <v>177</v>
       </c>
       <c r="G25" t="n">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="H25"/>
       <c r="I25"/>
       <c r="J25" t="n">
-        <v>27728</v>
+        <v>30607</v>
       </c>
       <c r="K25" t="n">
-        <v>0.425</v>
+        <v>0.469</v>
       </c>
       <c r="L25" t="n">
-        <v>27728</v>
+        <v>30607</v>
       </c>
       <c r="M25" t="n">
-        <v>0.425</v>
+        <v>0.469</v>
       </c>
       <c r="N25" t="s">
         <v>176</v>

</xml_diff>

<commit_message>
Updated testing data for 2020-06-26
</commit_message>
<xml_diff>
--- a/public/data/testing/covid-testing-latest-data-source-details.xlsx
+++ b/public/data/testing/covid-testing-latest-data-source-details.xlsx
@@ -139,7 +139,7 @@
     <t xml:space="preserve">Bahrain - units unclear</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200625192114/https://www.moh.gov.bh/COVID19</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200626061624/https://www.moh.gov.bh/COVID19</t>
   </si>
   <si>
     <t xml:space="preserve">Ministry of Health</t>
@@ -233,7 +233,7 @@
     <t xml:space="preserve">Bolivia - units unclear</t>
   </si>
   <si>
-    <t xml:space="preserve">https://minsalud.gob.bo/4332-bolivia-reporta-1-098-nuevos-contagios-de-coronavirus-y-el-total-sube-a-27-487</t>
+    <t xml:space="preserve">https://minsalud.gob.bo/4335-covid-19-bolivia-reporta-1-016-nuevos-contagios-y-37-fallecidos</t>
   </si>
   <si>
     <t xml:space="preserve">https://www.minsalud.gob.bo/</t>
@@ -280,7 +280,7 @@
     <t xml:space="preserve">Bulgaria - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200625192118/https://coronavirus.bg/</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200626061652/https://coronavirus.bg/</t>
   </si>
   <si>
     <t xml:space="preserve">Bulgaria COVID-10 Information Portal</t>
@@ -303,7 +303,7 @@
     <t xml:space="preserve">Canada - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200625192119/https://www.canada.ca/en/public-health/services/diseases/2019-novel-coronavirus-infection.html</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200626061653/https://www.canada.ca/en/public-health/services/diseases/2019-novel-coronavirus-infection.html</t>
   </si>
   <si>
     <t xml:space="preserve">Government of Canada</t>
@@ -472,7 +472,7 @@
     <t xml:space="preserve">Ecuador - units unclear</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.gestionderiesgos.gob.ec/wp-content/uploads/2020/06/INFOGRAFIA-NACIONALCOVI-19-COE-NACIONAL-24062020-08h00.pdf</t>
+    <t xml:space="preserve">https://www.gestionderiesgos.gob.ec/wp-content/uploads/2020/06/INFOGRAFIA-NACIONALCOVI-19-COE-NACIONAL-25062020-08h00.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">Government of Ecuador</t>
@@ -931,13 +931,13 @@
     <t xml:space="preserve">Japan - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.mhlw.go.jp/stf/newpage_12062.html</t>
+    <t xml:space="preserve">https://www.mhlw.go.jp/stf/newpage_12088.html</t>
   </si>
   <si>
     <t xml:space="preserve">Ministry of Health, Labor and Welfare Press Release</t>
   </si>
   <si>
-    <t xml:space="preserve">See Table: 国内の発生状況, column 1 '検査実施人数'. Daily change figure provided for this date is not consistent with the cumulative totals for today and the previous day.</t>
+    <t xml:space="preserve">See Table: 国内の発生状況, column 1 '検査実施人数'.</t>
   </si>
   <si>
     <t xml:space="preserve">Ministry of Health, Labor and Welfare</t>
@@ -955,7 +955,7 @@
     <t xml:space="preserve">Japan - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.mhlw.go.jp/content/10906000/000642776.pdf</t>
+    <t xml:space="preserve">https://www.mhlw.go.jp/content/10906000/000643532.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">The cumulative total reported in the press release matches the cumulative total calculated from the weekly and daily figures reported by the MOH.</t>
@@ -1013,7 +1013,7 @@
     <t xml:space="preserve">Kuwait - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/KUWAIT_MOH/status/1276117248256638977/photo/2</t>
+    <t xml:space="preserve">https://twitter.com/KUWAIT_MOH/status/1276481026156572673/photo/2</t>
   </si>
   <si>
     <t xml:space="preserve">Kuwait Ministry of Health</t>
@@ -1111,13 +1111,13 @@
     <t xml:space="preserve">Maldives - samples tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.facebook.com/561317043971945/videos/1638191456330288/</t>
+    <t xml:space="preserve">https://www.facebook.com/561317043971945/videos/594103654855023/</t>
   </si>
   <si>
     <t xml:space="preserve">Maldives Ministry of Health</t>
   </si>
   <si>
-    <t xml:space="preserve">Numbers visible in video at time: 2:23</t>
+    <t xml:space="preserve">Numbers visible in video at time: 1:24</t>
   </si>
   <si>
     <t xml:space="preserve">Maldives Ministry of Health Official Facebook page</t>
@@ -1305,7 +1305,7 @@
     <t xml:space="preserve">Oman - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/OmanVSCovid19/status/1275720140944965634</t>
+    <t xml:space="preserve">https://twitter.com/OmanVSCovid19/status/1276089447549997056</t>
   </si>
   <si>
     <t xml:space="preserve">Oman Ministry of Health</t>
@@ -1324,7 +1324,7 @@
     <t xml:space="preserve">Pakistan - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200625194421/http://www.covid.gov.pk/</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200626062509/http://www.covid.gov.pk/</t>
   </si>
   <si>
     <t xml:space="preserve">Government of Pakistan</t>
@@ -1377,7 +1377,7 @@
     <t xml:space="preserve">Peru - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.gob.pe/institucion/minsa/noticias/188228-minsa-casos-confirmados-por-coronavirus-covid-19-ascienden-a-260-810-en-el-peru-comunicado-n-143</t>
+    <t xml:space="preserve">https://www.gob.pe/institucion/minsa/noticias/188959-minsa-casos-confirmados-por-coronavirus-covid-19-ascienden-a-268-602-en-el-peru-comunicado-n-146</t>
   </si>
   <si>
     <t xml:space="preserve">Ministry of Health, Government of Peru</t>
@@ -1418,7 +1418,7 @@
     <t xml:space="preserve">Poland - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/MZ_GOV_PL/status/1275715366191280128</t>
+    <t xml:space="preserve">https://twitter.com/MZ_GOV_PL/status/1276077673983467521</t>
   </si>
   <si>
     <t xml:space="preserve">Poland Ministry of Health</t>
@@ -1746,7 +1746,7 @@
     <t xml:space="preserve">Sweden - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.folkhalsomyndigheten.se/globalassets/statistik-uppfoljning/smittsamma-sjukdomar/veckorapporter-covid-19/2020/covid-19-veckorapport-vecka-24_final.pdf</t>
+    <t xml:space="preserve">https://www.folkhalsomyndigheten.se/smittskydd-beredskap/utbrott/aktuella-utbrott/covid-19/antal-individer-som-har-testats-for-covid-19/</t>
   </si>
   <si>
     <t xml:space="preserve">Swedish Public Health Agency</t>
@@ -1903,7 +1903,7 @@
     <t xml:space="preserve">Uganda - samples tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/MinofHealthUG/status/1275713550615547904</t>
+    <t xml:space="preserve">https://twitter.com/MinofHealthUG/status/1276068542790668288</t>
   </si>
   <si>
     <t xml:space="preserve">Press Release from the Office of the Director General</t>
@@ -1985,7 +1985,7 @@
     <t xml:space="preserve">United States - tests performed (CDC)</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200624115618/https://www.cdc.gov/coronavirus/2019-ncov/cases-updates/testing-in-us.html</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200626063118/https://www.cdc.gov/coronavirus/2019-ncov/cases-updates/testing-in-us.html</t>
   </si>
   <si>
     <t xml:space="preserve">United States CDC</t>
@@ -2641,7 +2641,7 @@
         <v>39</v>
       </c>
       <c r="C5" s="1" t="n">
-        <v>44007</v>
+        <v>44008</v>
       </c>
       <c r="D5" t="s">
         <v>40</v>
@@ -2651,25 +2651,25 @@
       </c>
       <c r="F5"/>
       <c r="G5" t="n">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="H5" t="n">
-        <v>502763</v>
+        <v>511458</v>
       </c>
       <c r="I5" t="n">
-        <v>295.468</v>
+        <v>300.578</v>
       </c>
       <c r="J5" t="n">
-        <v>8735</v>
+        <v>8695</v>
       </c>
       <c r="K5" t="n">
-        <v>5.133</v>
+        <v>5.11</v>
       </c>
       <c r="L5" t="n">
-        <v>6914</v>
+        <v>7010</v>
       </c>
       <c r="M5" t="n">
-        <v>4.063</v>
+        <v>4.12</v>
       </c>
       <c r="N5" t="s">
         <v>42</v>
@@ -2845,7 +2845,7 @@
         <v>67</v>
       </c>
       <c r="C9" s="1" t="n">
-        <v>44006</v>
+        <v>44007</v>
       </c>
       <c r="D9" t="s">
         <v>68</v>
@@ -2855,25 +2855,25 @@
       </c>
       <c r="F9"/>
       <c r="G9" t="n">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="H9" t="n">
-        <v>64946</v>
+        <v>66597</v>
       </c>
       <c r="I9" t="n">
-        <v>5.564</v>
+        <v>5.705</v>
       </c>
       <c r="J9" t="n">
-        <v>1735</v>
+        <v>1651</v>
       </c>
       <c r="K9" t="n">
-        <v>0.149</v>
+        <v>0.141</v>
       </c>
       <c r="L9" t="n">
-        <v>1944</v>
+        <v>1977</v>
       </c>
       <c r="M9" t="n">
-        <v>0.167</v>
+        <v>0.169</v>
       </c>
       <c r="N9" t="s">
         <v>41</v>
@@ -2941,7 +2941,7 @@
         <v>81</v>
       </c>
       <c r="C11" s="1" t="n">
-        <v>44007</v>
+        <v>44008</v>
       </c>
       <c r="D11" t="s">
         <v>82</v>
@@ -2951,25 +2951,25 @@
       </c>
       <c r="F11"/>
       <c r="G11" t="n">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="H11" t="n">
-        <v>125518</v>
+        <v>128293</v>
       </c>
       <c r="I11" t="n">
-        <v>18.064</v>
+        <v>18.464</v>
       </c>
       <c r="J11" t="n">
-        <v>3016</v>
+        <v>2775</v>
       </c>
       <c r="K11" t="n">
-        <v>0.434</v>
+        <v>0.399</v>
       </c>
       <c r="L11" t="n">
-        <v>1862</v>
+        <v>1992</v>
       </c>
       <c r="M11" t="n">
-        <v>0.268</v>
+        <v>0.287</v>
       </c>
       <c r="N11" t="s">
         <v>84</v>
@@ -2992,7 +2992,7 @@
         <v>88</v>
       </c>
       <c r="C12" s="1" t="n">
-        <v>44007</v>
+        <v>44008</v>
       </c>
       <c r="D12" t="s">
         <v>89</v>
@@ -3002,25 +3002,25 @@
       </c>
       <c r="F12"/>
       <c r="G12" t="n">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="H12" t="n">
-        <v>2518574</v>
+        <v>2558287</v>
       </c>
       <c r="I12" t="n">
-        <v>66.731</v>
+        <v>67.783</v>
       </c>
       <c r="J12" t="n">
-        <v>35781</v>
+        <v>39713</v>
       </c>
       <c r="K12" t="n">
-        <v>0.948</v>
+        <v>1.052</v>
       </c>
       <c r="L12" t="n">
-        <v>37738</v>
+        <v>37560</v>
       </c>
       <c r="M12" t="n">
-        <v>1</v>
+        <v>0.995</v>
       </c>
       <c r="N12" t="s">
         <v>90</v>
@@ -3096,7 +3096,7 @@
         <v>102</v>
       </c>
       <c r="C14" s="1" t="n">
-        <v>44006</v>
+        <v>44007</v>
       </c>
       <c r="D14" t="s">
         <v>103</v>
@@ -3106,25 +3106,25 @@
       </c>
       <c r="F14"/>
       <c r="G14" t="n">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="H14" t="n">
-        <v>651592</v>
+        <v>670093</v>
       </c>
       <c r="I14" t="n">
-        <v>12.806</v>
+        <v>13.169</v>
       </c>
       <c r="J14" t="n">
-        <v>16981</v>
+        <v>18501</v>
       </c>
       <c r="K14" t="n">
-        <v>0.334</v>
+        <v>0.364</v>
       </c>
       <c r="L14" t="n">
-        <v>16625</v>
+        <v>17069</v>
       </c>
       <c r="M14" t="n">
-        <v>0.327</v>
+        <v>0.335</v>
       </c>
       <c r="N14" t="s">
         <v>104</v>
@@ -3147,7 +3147,7 @@
         <v>109</v>
       </c>
       <c r="C15" s="1" t="n">
-        <v>44002</v>
+        <v>44007</v>
       </c>
       <c r="D15" t="s">
         <v>110</v>
@@ -3157,25 +3157,25 @@
       </c>
       <c r="F15"/>
       <c r="G15" t="n">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="H15" t="n">
-        <v>26541</v>
+        <v>28943</v>
       </c>
       <c r="I15" t="n">
-        <v>5.21</v>
+        <v>5.682</v>
       </c>
       <c r="J15" t="n">
-        <v>457</v>
+        <v>703</v>
       </c>
       <c r="K15" t="n">
-        <v>0.09</v>
+        <v>0.138</v>
       </c>
       <c r="L15" t="n">
-        <v>401</v>
+        <v>498</v>
       </c>
       <c r="M15" t="n">
-        <v>0.079</v>
+        <v>0.098</v>
       </c>
       <c r="N15" t="s">
         <v>111</v>
@@ -3404,7 +3404,7 @@
         <v>141</v>
       </c>
       <c r="C20" s="1" t="n">
-        <v>44006</v>
+        <v>44007</v>
       </c>
       <c r="D20" t="s">
         <v>142</v>
@@ -3416,21 +3416,21 @@
         <v>144</v>
       </c>
       <c r="G20" t="n">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="H20" t="n">
-        <v>104572</v>
+        <v>106476</v>
       </c>
       <c r="I20" t="n">
-        <v>5.927</v>
+        <v>6.035</v>
       </c>
       <c r="J20"/>
       <c r="K20"/>
       <c r="L20" t="n">
-        <v>1478</v>
+        <v>1540</v>
       </c>
       <c r="M20" t="n">
-        <v>0.084</v>
+        <v>0.087</v>
       </c>
       <c r="N20" t="s">
         <v>143</v>
@@ -3855,7 +3855,7 @@
         <v>200</v>
       </c>
       <c r="C29" s="1" t="n">
-        <v>44003</v>
+        <v>44005</v>
       </c>
       <c r="D29" t="s">
         <v>194</v>
@@ -3865,25 +3865,25 @@
       </c>
       <c r="F29"/>
       <c r="G29" t="n">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="H29" t="n">
-        <v>277550</v>
+        <v>283124</v>
       </c>
       <c r="I29" t="n">
-        <v>8.932</v>
+        <v>9.112</v>
       </c>
       <c r="J29" t="n">
-        <v>7250</v>
+        <v>3008</v>
       </c>
       <c r="K29" t="n">
-        <v>0.233</v>
+        <v>0.097</v>
       </c>
       <c r="L29" t="n">
-        <v>3083</v>
+        <v>3115</v>
       </c>
       <c r="M29" t="n">
-        <v>0.099</v>
+        <v>0.1</v>
       </c>
       <c r="N29" t="s">
         <v>196</v>
@@ -4153,7 +4153,7 @@
         <v>235</v>
       </c>
       <c r="C35" s="1" t="n">
-        <v>44007</v>
+        <v>44008</v>
       </c>
       <c r="D35" t="s">
         <v>231</v>
@@ -4165,25 +4165,25 @@
         <v>233</v>
       </c>
       <c r="G35" t="n">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="H35" t="n">
-        <v>7560782</v>
+        <v>7776228</v>
       </c>
       <c r="I35" t="n">
-        <v>5.479</v>
+        <v>5.635</v>
       </c>
       <c r="J35" t="n">
-        <v>207871</v>
+        <v>215446</v>
       </c>
       <c r="K35" t="n">
-        <v>0.151</v>
+        <v>0.156</v>
       </c>
       <c r="L35" t="n">
-        <v>187302</v>
+        <v>192800</v>
       </c>
       <c r="M35" t="n">
-        <v>0.136</v>
+        <v>0.14</v>
       </c>
       <c r="N35" t="s">
         <v>232</v>
@@ -4512,7 +4512,7 @@
         <v>272</v>
       </c>
       <c r="C42" s="1" t="n">
-        <v>44006</v>
+        <v>44007</v>
       </c>
       <c r="D42" t="s">
         <v>273</v>
@@ -4524,21 +4524,21 @@
         <v>275</v>
       </c>
       <c r="G42" t="n">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="H42" t="n">
-        <v>429481</v>
+        <v>435495</v>
       </c>
       <c r="I42" t="n">
-        <v>3.396</v>
+        <v>3.443</v>
       </c>
       <c r="J42"/>
       <c r="K42"/>
       <c r="L42" t="n">
-        <v>11633</v>
+        <v>5580</v>
       </c>
       <c r="M42" t="n">
-        <v>0.092</v>
+        <v>0.044</v>
       </c>
       <c r="N42" t="s">
         <v>276</v>
@@ -4561,7 +4561,7 @@
         <v>279</v>
       </c>
       <c r="C43" s="1" t="n">
-        <v>44004</v>
+        <v>44005</v>
       </c>
       <c r="D43" t="s">
         <v>280</v>
@@ -4573,25 +4573,25 @@
         <v>281</v>
       </c>
       <c r="G43" t="n">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H43" t="n">
-        <v>627459</v>
+        <v>632744</v>
       </c>
       <c r="I43" t="n">
-        <v>4.961</v>
+        <v>5.003</v>
       </c>
       <c r="J43" t="n">
-        <v>4365</v>
+        <v>5261</v>
       </c>
       <c r="K43" t="n">
-        <v>0.035</v>
+        <v>0.042</v>
       </c>
       <c r="L43" t="n">
-        <v>6130</v>
+        <v>5780</v>
       </c>
       <c r="M43" t="n">
-        <v>0.048</v>
+        <v>0.046</v>
       </c>
       <c r="N43" t="s">
         <v>276</v>
@@ -4716,7 +4716,7 @@
         <v>296</v>
       </c>
       <c r="C46" s="1" t="n">
-        <v>44007</v>
+        <v>44008</v>
       </c>
       <c r="D46" t="s">
         <v>297</v>
@@ -4726,25 +4726,25 @@
       </c>
       <c r="F46"/>
       <c r="G46" t="n">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H46" t="n">
-        <v>368510</v>
+        <v>372284</v>
       </c>
       <c r="I46" t="n">
-        <v>86.291</v>
+        <v>87.174</v>
       </c>
       <c r="J46" t="n">
-        <v>3286</v>
+        <v>3774</v>
       </c>
       <c r="K46" t="n">
-        <v>0.769</v>
+        <v>0.884</v>
       </c>
       <c r="L46" t="n">
-        <v>3169</v>
+        <v>3267</v>
       </c>
       <c r="M46" t="n">
-        <v>0.742</v>
+        <v>0.765</v>
       </c>
       <c r="N46" t="s">
         <v>298</v>
@@ -4922,7 +4922,7 @@
         <v>319</v>
       </c>
       <c r="C50" s="1" t="n">
-        <v>44006</v>
+        <v>44007</v>
       </c>
       <c r="D50" t="s">
         <v>320</v>
@@ -4934,25 +4934,25 @@
         <v>322</v>
       </c>
       <c r="G50" t="n">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="H50" t="n">
-        <v>704336</v>
+        <v>716178</v>
       </c>
       <c r="I50" t="n">
-        <v>21.762</v>
+        <v>22.127</v>
       </c>
       <c r="J50" t="n">
-        <v>10733</v>
+        <v>11842</v>
       </c>
       <c r="K50" t="n">
-        <v>0.332</v>
+        <v>0.366</v>
       </c>
       <c r="L50" t="n">
-        <v>5715</v>
+        <v>6656</v>
       </c>
       <c r="M50" t="n">
-        <v>0.177</v>
+        <v>0.206</v>
       </c>
       <c r="N50" t="s">
         <v>41</v>
@@ -4975,7 +4975,7 @@
         <v>326</v>
       </c>
       <c r="C51" s="1" t="n">
-        <v>44005</v>
+        <v>44006</v>
       </c>
       <c r="D51" t="s">
         <v>327</v>
@@ -4987,25 +4987,25 @@
         <v>329</v>
       </c>
       <c r="G51" t="n">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="H51" t="n">
-        <v>43998</v>
+        <v>45185</v>
       </c>
       <c r="I51" t="n">
-        <v>81.396</v>
+        <v>83.592</v>
       </c>
       <c r="J51" t="n">
-        <v>1168</v>
+        <v>1187</v>
       </c>
       <c r="K51" t="n">
-        <v>2.161</v>
+        <v>2.196</v>
       </c>
       <c r="L51" t="n">
-        <v>1020</v>
+        <v>1099</v>
       </c>
       <c r="M51" t="n">
-        <v>1.887</v>
+        <v>2.033</v>
       </c>
       <c r="N51" t="s">
         <v>330</v>
@@ -5028,7 +5028,7 @@
         <v>334</v>
       </c>
       <c r="C52" s="1" t="n">
-        <v>44001</v>
+        <v>44003</v>
       </c>
       <c r="D52" t="s">
         <v>335</v>
@@ -5038,25 +5038,25 @@
       </c>
       <c r="F52"/>
       <c r="G52" t="n">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="H52" t="n">
-        <v>445597</v>
+        <v>456138</v>
       </c>
       <c r="I52" t="n">
-        <v>3.456</v>
+        <v>3.538</v>
       </c>
       <c r="J52" t="n">
-        <v>7647</v>
+        <v>2241</v>
       </c>
       <c r="K52" t="n">
-        <v>0.059</v>
+        <v>0.017</v>
       </c>
       <c r="L52" t="n">
-        <v>8139</v>
+        <v>8215</v>
       </c>
       <c r="M52" t="n">
-        <v>0.063</v>
+        <v>0.064</v>
       </c>
       <c r="N52" t="s">
         <v>337</v>
@@ -5285,7 +5285,7 @@
         <v>367</v>
       </c>
       <c r="C57" s="1" t="n">
-        <v>44006</v>
+        <v>44007</v>
       </c>
       <c r="D57" t="s">
         <v>368</v>
@@ -5295,25 +5295,25 @@
       </c>
       <c r="F57"/>
       <c r="G57" t="n">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="H57" t="n">
-        <v>368432</v>
+        <v>378257</v>
       </c>
       <c r="I57" t="n">
-        <v>76.403</v>
+        <v>78.44</v>
       </c>
       <c r="J57" t="n">
-        <v>10436</v>
+        <v>9825</v>
       </c>
       <c r="K57" t="n">
-        <v>2.164</v>
+        <v>2.037</v>
       </c>
       <c r="L57" t="n">
-        <v>6749</v>
+        <v>7257</v>
       </c>
       <c r="M57" t="n">
-        <v>1.4</v>
+        <v>1.505</v>
       </c>
       <c r="N57" t="s">
         <v>369</v>
@@ -5438,7 +5438,7 @@
         <v>385</v>
       </c>
       <c r="C60" s="1" t="n">
-        <v>44006</v>
+        <v>44007</v>
       </c>
       <c r="D60" t="s">
         <v>386</v>
@@ -5448,21 +5448,21 @@
       </c>
       <c r="F60"/>
       <c r="G60" t="n">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H60"/>
       <c r="I60"/>
       <c r="J60" t="n">
-        <v>3585</v>
+        <v>3835</v>
       </c>
       <c r="K60" t="n">
-        <v>0.702</v>
+        <v>0.751</v>
       </c>
       <c r="L60" t="n">
-        <v>3284</v>
+        <v>3496</v>
       </c>
       <c r="M60" t="n">
-        <v>0.643</v>
+        <v>0.685</v>
       </c>
       <c r="N60" t="s">
         <v>387</v>
@@ -5485,7 +5485,7 @@
         <v>391</v>
       </c>
       <c r="C61" s="1" t="n">
-        <v>44007</v>
+        <v>44008</v>
       </c>
       <c r="D61" t="s">
         <v>392</v>
@@ -5495,25 +5495,25 @@
       </c>
       <c r="F61"/>
       <c r="G61" t="n">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="H61" t="n">
-        <v>1171976</v>
+        <v>1193017</v>
       </c>
       <c r="I61" t="n">
-        <v>5.306</v>
+        <v>5.401</v>
       </c>
       <c r="J61" t="n">
-        <v>21835</v>
+        <v>21041</v>
       </c>
       <c r="K61" t="n">
-        <v>0.099</v>
+        <v>0.095</v>
       </c>
       <c r="L61" t="n">
-        <v>27138</v>
+        <v>25987</v>
       </c>
       <c r="M61" t="n">
-        <v>0.123</v>
+        <v>0.118</v>
       </c>
       <c r="N61" t="s">
         <v>393</v>
@@ -5638,7 +5638,7 @@
         <v>408</v>
       </c>
       <c r="C64" s="1" t="n">
-        <v>44006</v>
+        <v>44008</v>
       </c>
       <c r="D64" t="s">
         <v>409</v>
@@ -5648,21 +5648,21 @@
       </c>
       <c r="F64"/>
       <c r="G64" t="n">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="H64" t="n">
-        <v>222240</v>
+        <v>232730</v>
       </c>
       <c r="I64" t="n">
-        <v>6.74</v>
+        <v>7.058</v>
       </c>
       <c r="J64"/>
       <c r="K64"/>
       <c r="L64" t="n">
-        <v>3346</v>
+        <v>3360</v>
       </c>
       <c r="M64" t="n">
-        <v>0.101</v>
+        <v>0.102</v>
       </c>
       <c r="N64" t="s">
         <v>410</v>
@@ -5685,7 +5685,7 @@
         <v>414</v>
       </c>
       <c r="C65" s="1" t="n">
-        <v>44004</v>
+        <v>44005</v>
       </c>
       <c r="D65" t="s">
         <v>415</v>
@@ -5695,25 +5695,25 @@
       </c>
       <c r="F65"/>
       <c r="G65" t="n">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="H65" t="n">
-        <v>568633</v>
+        <v>580560</v>
       </c>
       <c r="I65" t="n">
-        <v>5.189</v>
+        <v>5.298</v>
       </c>
       <c r="J65" t="n">
-        <v>10470</v>
+        <v>11927</v>
       </c>
       <c r="K65" t="n">
-        <v>0.096</v>
+        <v>0.109</v>
       </c>
       <c r="L65" t="n">
-        <v>12065</v>
+        <v>12197</v>
       </c>
       <c r="M65" t="n">
-        <v>0.11</v>
+        <v>0.111</v>
       </c>
       <c r="N65" t="s">
         <v>211</v>
@@ -5736,7 +5736,7 @@
         <v>419</v>
       </c>
       <c r="C66" s="1" t="n">
-        <v>44006</v>
+        <v>44007</v>
       </c>
       <c r="D66" t="s">
         <v>420</v>
@@ -5746,25 +5746,25 @@
       </c>
       <c r="F66"/>
       <c r="G66" t="n">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="H66" t="n">
-        <v>1257001</v>
+        <v>1278454</v>
       </c>
       <c r="I66" t="n">
-        <v>33.213</v>
+        <v>33.78</v>
       </c>
       <c r="J66" t="n">
-        <v>19251</v>
+        <v>21453</v>
       </c>
       <c r="K66" t="n">
-        <v>0.509</v>
+        <v>0.567</v>
       </c>
       <c r="L66" t="n">
-        <v>18670</v>
+        <v>18748</v>
       </c>
       <c r="M66" t="n">
-        <v>0.493</v>
+        <v>0.495</v>
       </c>
       <c r="N66" t="s">
         <v>421</v>
@@ -5787,7 +5787,7 @@
         <v>424</v>
       </c>
       <c r="C67" s="1" t="n">
-        <v>44006</v>
+        <v>44007</v>
       </c>
       <c r="D67"/>
       <c r="E67"/>
@@ -5798,10 +5798,10 @@
       <c r="J67"/>
       <c r="K67"/>
       <c r="L67" t="n">
-        <v>15562</v>
+        <v>12155</v>
       </c>
       <c r="M67" t="n">
-        <v>0.411</v>
+        <v>0.321</v>
       </c>
       <c r="N67" t="s">
         <v>421</v>
@@ -5875,7 +5875,7 @@
         <v>433</v>
       </c>
       <c r="C69" s="1" t="n">
-        <v>44006</v>
+        <v>44007</v>
       </c>
       <c r="D69" t="s">
         <v>434</v>
@@ -5885,25 +5885,25 @@
       </c>
       <c r="F69"/>
       <c r="G69" t="n">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="H69" t="n">
-        <v>333172</v>
+        <v>337496</v>
       </c>
       <c r="I69" t="n">
-        <v>115.642</v>
+        <v>117.143</v>
       </c>
       <c r="J69" t="n">
-        <v>4231</v>
+        <v>4324</v>
       </c>
       <c r="K69" t="n">
-        <v>1.469</v>
+        <v>1.501</v>
       </c>
       <c r="L69" t="n">
-        <v>4053</v>
+        <v>3975</v>
       </c>
       <c r="M69" t="n">
-        <v>1.407</v>
+        <v>1.38</v>
       </c>
       <c r="N69" t="s">
         <v>435</v>
@@ -6075,7 +6075,7 @@
         <v>457</v>
       </c>
       <c r="C73" s="1" t="n">
-        <v>44006</v>
+        <v>44007</v>
       </c>
       <c r="D73" t="s">
         <v>458</v>
@@ -6085,25 +6085,25 @@
       </c>
       <c r="F73"/>
       <c r="G73" t="n">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H73" t="n">
-        <v>1380031</v>
+        <v>1417771</v>
       </c>
       <c r="I73" t="n">
-        <v>39.64</v>
+        <v>40.724</v>
       </c>
       <c r="J73" t="n">
-        <v>34511</v>
+        <v>37740</v>
       </c>
       <c r="K73" t="n">
-        <v>0.991</v>
+        <v>1.084</v>
       </c>
       <c r="L73" t="n">
-        <v>30324</v>
+        <v>31357</v>
       </c>
       <c r="M73" t="n">
-        <v>0.871</v>
+        <v>0.901</v>
       </c>
       <c r="N73" t="s">
         <v>41</v>
@@ -6428,7 +6428,7 @@
         <v>499</v>
       </c>
       <c r="C80" s="1" t="n">
-        <v>44006</v>
+        <v>44007</v>
       </c>
       <c r="D80" t="s">
         <v>500</v>
@@ -6440,25 +6440,25 @@
         <v>502</v>
       </c>
       <c r="G80" t="n">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="H80" t="n">
-        <v>1416894</v>
+        <v>1460012</v>
       </c>
       <c r="I80" t="n">
-        <v>23.89</v>
+        <v>24.617</v>
       </c>
       <c r="J80" t="n">
-        <v>34122</v>
+        <v>43118</v>
       </c>
       <c r="K80" t="n">
-        <v>0.575</v>
+        <v>0.727</v>
       </c>
       <c r="L80" t="n">
-        <v>29933</v>
+        <v>33131</v>
       </c>
       <c r="M80" t="n">
-        <v>0.505</v>
+        <v>0.559</v>
       </c>
       <c r="N80" t="s">
         <v>501</v>
@@ -6579,7 +6579,7 @@
         <v>519</v>
       </c>
       <c r="C83" s="1" t="n">
-        <v>43996</v>
+        <v>44003</v>
       </c>
       <c r="D83" t="s">
         <v>520</v>
@@ -6589,21 +6589,21 @@
       </c>
       <c r="F83"/>
       <c r="G83" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H83" t="n">
-        <v>382804</v>
+        <v>447462</v>
       </c>
       <c r="I83" t="n">
-        <v>37.904</v>
+        <v>44.306</v>
       </c>
       <c r="J83"/>
       <c r="K83"/>
       <c r="L83" t="n">
-        <v>8552</v>
+        <v>8829</v>
       </c>
       <c r="M83" t="n">
-        <v>0.847</v>
+        <v>0.874</v>
       </c>
       <c r="N83" t="s">
         <v>522</v>
@@ -6932,7 +6932,7 @@
         <v>566</v>
       </c>
       <c r="C90" s="1" t="n">
-        <v>44005</v>
+        <v>44006</v>
       </c>
       <c r="D90" t="s">
         <v>567</v>
@@ -6944,25 +6944,25 @@
         <v>569</v>
       </c>
       <c r="G90" t="n">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="H90" t="n">
-        <v>150073</v>
+        <v>153528</v>
       </c>
       <c r="I90" t="n">
-        <v>3.281</v>
+        <v>3.356</v>
       </c>
       <c r="J90" t="n">
-        <v>2196</v>
+        <v>3455</v>
       </c>
       <c r="K90" t="n">
-        <v>0.048</v>
+        <v>0.076</v>
       </c>
       <c r="L90" t="n">
-        <v>2452</v>
+        <v>2560</v>
       </c>
       <c r="M90" t="n">
-        <v>0.054</v>
+        <v>0.056</v>
       </c>
       <c r="N90" t="s">
         <v>568</v>
@@ -7140,7 +7140,7 @@
         <v>590</v>
       </c>
       <c r="C94" s="1" t="n">
-        <v>44005</v>
+        <v>44007</v>
       </c>
       <c r="D94" t="s">
         <v>591</v>
@@ -7150,25 +7150,25 @@
       </c>
       <c r="F94"/>
       <c r="G94" t="n">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="H94" t="n">
-        <v>29339757</v>
+        <v>31281178</v>
       </c>
       <c r="I94" t="n">
-        <v>88.639</v>
+        <v>94.504</v>
       </c>
       <c r="J94" t="n">
-        <v>2022722</v>
+        <v>1171117</v>
       </c>
       <c r="K94" t="n">
-        <v>6.111</v>
+        <v>3.538</v>
       </c>
       <c r="L94" t="n">
-        <v>796279</v>
+        <v>682954</v>
       </c>
       <c r="M94" t="n">
-        <v>2.406</v>
+        <v>2.063</v>
       </c>
       <c r="N94" t="s">
         <v>592</v>
@@ -7191,7 +7191,7 @@
         <v>596</v>
       </c>
       <c r="C95" s="1" t="n">
-        <v>44006</v>
+        <v>44007</v>
       </c>
       <c r="D95" t="s">
         <v>597</v>
@@ -7201,25 +7201,25 @@
       </c>
       <c r="F95"/>
       <c r="G95" t="n">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="H95" t="n">
-        <v>28567355</v>
+        <v>29207820</v>
       </c>
       <c r="I95" t="n">
-        <v>86.306</v>
+        <v>88.24</v>
       </c>
       <c r="J95" t="n">
-        <v>512394</v>
+        <v>637587</v>
       </c>
       <c r="K95" t="n">
-        <v>1.548</v>
+        <v>1.926</v>
       </c>
       <c r="L95" t="n">
-        <v>520869</v>
+        <v>538019</v>
       </c>
       <c r="M95" t="n">
-        <v>1.574</v>
+        <v>1.625</v>
       </c>
       <c r="N95" t="s">
         <v>598</v>

</xml_diff>

<commit_message>
Updated testing data for 2020-06-28
</commit_message>
<xml_diff>
--- a/public/data/testing/covid-testing-latest-data-source-details.xlsx
+++ b/public/data/testing/covid-testing-latest-data-source-details.xlsx
@@ -71,7 +71,7 @@
     <t xml:space="preserve">Argentina - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.argentina.gob.ar/sites/default/files/25-06-20_reporte_matutino_covid_19.pdf</t>
+    <t xml:space="preserve">https://www.argentina.gob.ar/sites/default/files/28-06-20_reporte-matutino-covid-19.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">Government of Argentina</t>
@@ -92,7 +92,7 @@
     <t xml:space="preserve">Australia - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.health.gov.au/sites/default/files/documents/2020/06/coronavirus-covid-19-at-a-glance-24-june-2020.pdf</t>
+    <t xml:space="preserve">https://www.health.gov.au/sites/default/files/documents/2020/06/coronavirus-covid-19-at-a-glance-28-june-2020.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">Australian Government Department of Health</t>
@@ -112,7 +112,7 @@
     <t xml:space="preserve">Austria - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200625192112/https://www.sozialministerium.at/Informationen-zum-Coronavirus/Neuartiges-Coronavirus-(2019-nCov).html</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200628172135/https://www.sozialministerium.at/Informationen-zum-Coronavirus/Neuartiges-Coronavirus-(2019-nCov).html</t>
   </si>
   <si>
     <t xml:space="preserve">Austrian Ministry for Health</t>
@@ -139,7 +139,7 @@
     <t xml:space="preserve">Bahrain - units unclear</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200626061624/https://www.moh.gov.bh/COVID19</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200628075454/https://www.moh.gov.bh/COVID19</t>
   </si>
   <si>
     <t xml:space="preserve">Ministry of Health</t>
@@ -187,7 +187,7 @@
     <t xml:space="preserve">Belarus - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">http://minzdrav.gov.by/ru/sobytiya/v-belarusi-vyzdoroveli-i-vypisany-41-448-patsientov/</t>
+    <t xml:space="preserve">http://minzdrav.gov.by/ru/sobytiya/v-belarusi-vyzdoroveli-i-vypisany-42-689-patsientov/</t>
   </si>
   <si>
     <t xml:space="preserve">Belarus Ministry of Health</t>
@@ -280,7 +280,7 @@
     <t xml:space="preserve">Bulgaria - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200626061652/https://coronavirus.bg/</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200628075458/https://coronavirus.bg/</t>
   </si>
   <si>
     <t xml:space="preserve">Bulgaria COVID-10 Information Portal</t>
@@ -303,7 +303,7 @@
     <t xml:space="preserve">Canada - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200626061653/https://www.canada.ca/en/public-health/services/diseases/2019-novel-coronavirus-infection.html</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200628075743/https://www.canada.ca/en/public-health/services/diseases/2019-novel-coronavirus-infection.html</t>
   </si>
   <si>
     <t xml:space="preserve">Government of Canada</t>
@@ -391,7 +391,7 @@
     <t xml:space="preserve">Croatia - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200625192126/https://www.koronavirus.hr/najnovije/ukupno-dosad-382-zarazene-osobe-u-hrvatskoj/35</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200628172149/https://www.koronavirus.hr/najnovije/ukupno-dosad-382-zarazene-osobe-u-hrvatskoj/35</t>
   </si>
   <si>
     <t xml:space="preserve">Government of Croatia</t>
@@ -454,7 +454,7 @@
     <t xml:space="preserve">Denmark - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://files.ssi.dk/Data-epidemiologisk-rapport-25062020-45t5</t>
+    <t xml:space="preserve">https://files.ssi.dk/Data-epidemiologisk-rapport-26062020-wd26</t>
   </si>
   <si>
     <t xml:space="preserve">Statens Serum Institut</t>
@@ -472,7 +472,7 @@
     <t xml:space="preserve">Ecuador - units unclear</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.gestionderiesgos.gob.ec/wp-content/uploads/2020/06/INFOGRAFIA-NACIONALCOVI-19-COE-NACIONAL-25062020-08h00.pdf</t>
+    <t xml:space="preserve">https://www.gestionderiesgos.gob.ec/wp-content/uploads/2020/06/INFOGRAFIA-NACIONALCOVI-19-COE-NACIONAL-26062020-08h00.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">Government of Ecuador</t>
@@ -497,7 +497,7 @@
     <t xml:space="preserve">El Salvador - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.facebook.com/nayibbukele/posts/3002101273209377</t>
+    <t xml:space="preserve">https://www.facebook.com/nayibbukele/posts/3012945928791578</t>
   </si>
   <si>
     <t xml:space="preserve">Government of El Salvador</t>
@@ -540,7 +540,7 @@
     <t xml:space="preserve">Ethiopia - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.ephi.gov.et/images/novel_coronavirus/confirmed-case-Press-release_June-25-Eng_V2.pdf</t>
+    <t xml:space="preserve">https://www.ephi.gov.et/images/novel_coronavirus/confirmed-case-Press-release_June-28-Eng_V3.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">Ethiopian Public Health Institute</t>
@@ -692,7 +692,7 @@
     <t xml:space="preserve">Greece - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://eody.gov.gr/covid-gr-daily-report-20200625/</t>
+    <t xml:space="preserve">https://eody.gov.gr/wp-content/uploads/2020/06/covid-gr-daily-report-20200628.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">National Organization of Public Health</t>
@@ -834,7 +834,7 @@
     <t xml:space="preserve">Iran - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">http://web.archive.org/web/20200624194143/http://irangov.ir/detail/341715</t>
+    <t xml:space="preserve">http://web.archive.org/web/20200628163113/http://irangov.ir/detail/341977</t>
   </si>
   <si>
     <t xml:space="preserve">Government of Iran</t>
@@ -874,7 +874,7 @@
     <t xml:space="preserve">Israel - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://govextra.gov.il/media/21345/covid19-data-israel-17062020.csv</t>
+    <t xml:space="preserve">https://govextra.gov.il/media/21474/covid19-data-israel-21062020.csv</t>
   </si>
   <si>
     <t xml:space="preserve">Israel Ministry of Health</t>
@@ -931,7 +931,7 @@
     <t xml:space="preserve">Japan - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.mhlw.go.jp/stf/newpage_12088.html</t>
+    <t xml:space="preserve">https://www.mhlw.go.jp/stf/newpage_12123.html</t>
   </si>
   <si>
     <t xml:space="preserve">Ministry of Health, Labor and Welfare Press Release</t>
@@ -955,7 +955,7 @@
     <t xml:space="preserve">Japan - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.mhlw.go.jp/content/10906000/000643532.pdf</t>
+    <t xml:space="preserve">https://www.mhlw.go.jp/content/10906000/000644327.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">The cumulative total reported in the press release matches the cumulative total calculated from the weekly and daily figures reported by the MOH.</t>
@@ -990,7 +990,7 @@
     <t xml:space="preserve">Kenya - units unclear</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/MOH_Kenya/status/1275776785960112129</t>
+    <t xml:space="preserve">https://twitter.com/MOH_Kenya/status/1277226471795445760</t>
   </si>
   <si>
     <t xml:space="preserve">Kenya Ministry of Health</t>
@@ -1049,7 +1049,7 @@
     <t xml:space="preserve">Lithuania - samples tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200625192619/http://sam.lrv.lt/lt/naujienos/koronavirusas</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200627121117/http://sam.lrv.lt/lt/naujienos/koronavirusas</t>
   </si>
   <si>
     <t xml:space="preserve">http://sam.lrv.lt/lt/naujienos/koronavirusas</t>
@@ -1065,7 +1065,7 @@
     <t xml:space="preserve">Luxembourg - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200625192624/https://gouvernement.lu/en/dossiers.gouv_msan%2Ben%2Bdossiers%2B2020%2Bcorona-virus.html</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200628172214/https://gouvernement.lu/en/dossiers.gouv_msan%2Ben%2Bdossiers%2B2020%2Bcorona-virus.html</t>
   </si>
   <si>
     <t xml:space="preserve">Luxembourg Government situation update</t>
@@ -1086,7 +1086,7 @@
     <t xml:space="preserve">Malaysia - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">http://covid-19.moh.gov.my/terkini/062020/situasi-terkini-24-jun-2020</t>
+    <t xml:space="preserve">http://covid-19.moh.gov.my/terkini/062020/situasi-terkini-27-jun-2020</t>
   </si>
   <si>
     <t xml:space="preserve">Ministry of Health Malaysia</t>
@@ -1221,7 +1221,7 @@
     <t xml:space="preserve">Netherlands - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.rivm.nl/sites/default/files/2020-06/COVID-19_WebSite_rapport_dagelijks_20200624_1123.pdf</t>
+    <t xml:space="preserve">https://www.rivm.nl/sites/default/files/2020-06/COVID-19_WebSite_rapport_dagelijks_20200628_1022.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">National Institute for Public Health and the Environment</t>
@@ -1260,7 +1260,7 @@
     <t xml:space="preserve">Nigeria - samples tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200625194341/https://covid19.ncdc.gov.ng/</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200628172254/https://covid19.ncdc.gov.ng/</t>
   </si>
   <si>
     <t xml:space="preserve">Nigeria Centre for Disease Control</t>
@@ -1305,7 +1305,7 @@
     <t xml:space="preserve">Oman - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/OmanVSCovid19/status/1276089447549997056</t>
+    <t xml:space="preserve">https://twitter.com/OmanVSCovid19/status/1276802996517482496</t>
   </si>
   <si>
     <t xml:space="preserve">Oman Ministry of Health</t>
@@ -1324,7 +1324,7 @@
     <t xml:space="preserve">Pakistan - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200626062509/http://www.covid.gov.pk/</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200628080315/http://www.covid.gov.pk/</t>
   </si>
   <si>
     <t xml:space="preserve">Government of Pakistan</t>
@@ -1377,7 +1377,7 @@
     <t xml:space="preserve">Peru - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.gob.pe/institucion/minsa/noticias/188959-minsa-casos-confirmados-por-coronavirus-covid-19-ascienden-a-268-602-en-el-peru-comunicado-n-146</t>
+    <t xml:space="preserve">https://www.gob.pe/institucion/minsa/noticias/189171-minsa-casos-confirmados-por-coronavirus-covid-19-ascienden-a-275-989-en-el-peru-comunicado-n-149</t>
   </si>
   <si>
     <t xml:space="preserve">Ministry of Health, Government of Peru</t>
@@ -1418,7 +1418,7 @@
     <t xml:space="preserve">Poland - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/MZ_GOV_PL/status/1276077673983467521</t>
+    <t xml:space="preserve">https://twitter.com/MZ_GOV_PL/status/1276802451555840002</t>
   </si>
   <si>
     <t xml:space="preserve">Poland Ministry of Health</t>
@@ -1482,7 +1482,7 @@
     <t xml:space="preserve">Romania - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://gov.ro/ro/media/comunicate/buletin-de-presa-25-iunie-2020-ora-13-00&amp;page=1</t>
+    <t xml:space="preserve">https://gov.ro/ro/media/comunicate/buletin-de-presa-28-iunie-2020-ora-13-00&amp;page=1</t>
   </si>
   <si>
     <t xml:space="preserve">Ministry of Internal Affairs</t>
@@ -1500,7 +1500,7 @@
     <t xml:space="preserve">Russia - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://rospotrebnadzor.ru/about/info/news/news_details.php?ELEMENT_ID=14762</t>
+    <t xml:space="preserve">https://rospotrebnadzor.ru/about/info/news/news_details.php?ELEMENT_ID=14783</t>
   </si>
   <si>
     <t xml:space="preserve">Government of the Russian Federation</t>
@@ -1520,7 +1520,7 @@
     <t xml:space="preserve">Rwanda - units unclear</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/RwandaHealth/status/1275860090940162048</t>
+    <t xml:space="preserve">https://twitter.com/RwandaHealth/status/1276952727147479041</t>
   </si>
   <si>
     <t xml:space="preserve">Rwanda Ministry of Health</t>
@@ -1626,7 +1626,7 @@
     <t xml:space="preserve">Slovakia - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200625194429/https://korona.gov.sk/</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200628080701/https://korona.gov.sk/</t>
   </si>
   <si>
     <t xml:space="preserve">National Health Information Centre</t>
@@ -1700,7 +1700,7 @@
     <t xml:space="preserve">South Korea - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.cdc.go.kr/board/board.es?mid=&amp;bid=0030&amp;act=view&amp;list_no=367612&amp;tag=&amp;nPage=1</t>
+    <t xml:space="preserve">https://www.cdc.go.kr/board/board.es?mid=&amp;bid=0030&amp;act=view&amp;list_no=367645&amp;tag=&amp;nPage=1</t>
   </si>
   <si>
     <t xml:space="preserve">South Korea CDC</t>
@@ -1746,7 +1746,7 @@
     <t xml:space="preserve">Sweden - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.folkhalsomyndigheten.se/smittskydd-beredskap/utbrott/aktuella-utbrott/covid-19/antal-individer-som-har-testats-for-covid-19/</t>
+    <t xml:space="preserve">https://www.folkhalsomyndigheten.se/globalassets/statistik-uppfoljning/smittsamma-sjukdomar/veckorapporter-covid-19/2020/covid-19-veckorapport-vecka-25-final.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">Swedish Public Health Agency</t>
@@ -1814,7 +1814,7 @@
     <t xml:space="preserve">Thailand - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200625194521/https://ddc.moph.go.th/viralpneumonia/eng/index.php</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200627121444/https://ddc.moph.go.th/viralpneumonia/eng/index.php</t>
   </si>
   <si>
     <t xml:space="preserve">Department of Disease Control</t>
@@ -1882,7 +1882,7 @@
     <t xml:space="preserve">Turkey - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200625194526/https://covid19.saglik.gov.tr/</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200628080858/https://covid19.saglik.gov.tr/</t>
   </si>
   <si>
     <t xml:space="preserve">Turkish Ministry of Health</t>
@@ -1903,7 +1903,7 @@
     <t xml:space="preserve">Uganda - samples tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/MinofHealthUG/status/1276068542790668288</t>
+    <t xml:space="preserve">https://twitter.com/MinofHealthUG/status/1276787476024250374</t>
   </si>
   <si>
     <t xml:space="preserve">Press Release from the Office of the Director General</t>
@@ -1927,7 +1927,7 @@
     <t xml:space="preserve">Ukraine - units unclear</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200625194529/https://covid19.gov.ua/en</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200628172444/https://covid19.gov.ua/en</t>
   </si>
   <si>
     <t xml:space="preserve">Cabinet of Ministers of Ukraine</t>
@@ -1964,7 +1964,7 @@
     <t xml:space="preserve">United Kingdom - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://assets.publishing.service.gov.uk/government/uploads/system/uploads/attachment_data/file/895414/2020-06-25_COVID-19_UK_testing_time_series.csv</t>
+    <t xml:space="preserve">https://assets.publishing.service.gov.uk/government/uploads/system/uploads/attachment_data/file/896043/2020-06-28-COVID-19-UK-testing-time-series.csv</t>
   </si>
   <si>
     <t xml:space="preserve">Sum of pillar 1 + pillar 2 (tests processed only)</t>
@@ -1985,7 +1985,7 @@
     <t xml:space="preserve">United States - tests performed (CDC)</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200626063118/https://www.cdc.gov/coronavirus/2019-ncov/cases-updates/testing-in-us.html</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200627121458/https://www.cdc.gov/coronavirus/2019-ncov/cases-updates/testing-in-us.html</t>
   </si>
   <si>
     <t xml:space="preserve">United States CDC</t>
@@ -2039,7 +2039,7 @@
     <t xml:space="preserve">Uruguay - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.gub.uy/ministerio-salud-publica/comunicacion/noticias/informacion-interes-actualizada-sobre-coronavirus-covid-19-uruguay-10</t>
+    <t xml:space="preserve">https://www.gub.uy/ministerio-salud-publica/comunicacion/noticias/informacion-interes-actualizada-sobre-coronavirus-covid-19-uruguay-13</t>
   </si>
   <si>
     <t xml:space="preserve">https://www.gub.uy/ministerio-salud-publica/comunicacion/noticias</t>
@@ -2078,7 +2078,7 @@
     <t xml:space="preserve">Zimbabwe - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/MoHCCZim/status/1275851683965304837</t>
+    <t xml:space="preserve">https://twitter.com/MoHCCZim/status/1276939070732677120</t>
   </si>
   <si>
     <t xml:space="preserve">Zimbabwe Ministry of Health and Child Care</t>
@@ -2488,7 +2488,7 @@
         <v>18</v>
       </c>
       <c r="C2" s="1" t="n">
-        <v>44007</v>
+        <v>44010</v>
       </c>
       <c r="D2" t="s">
         <v>19</v>
@@ -2498,25 +2498,25 @@
       </c>
       <c r="F2"/>
       <c r="G2" t="n">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="H2" t="n">
-        <v>309601</v>
+        <v>336951</v>
       </c>
       <c r="I2" t="n">
-        <v>6.85</v>
+        <v>7.455</v>
       </c>
       <c r="J2" t="n">
-        <v>9256</v>
+        <v>7915</v>
       </c>
       <c r="K2" t="n">
-        <v>0.205</v>
+        <v>0.175</v>
       </c>
       <c r="L2" t="n">
-        <v>7427</v>
+        <v>8183</v>
       </c>
       <c r="M2" t="n">
-        <v>0.164</v>
+        <v>0.181</v>
       </c>
       <c r="N2" t="s">
         <v>20</v>
@@ -2539,7 +2539,7 @@
         <v>25</v>
       </c>
       <c r="C3" s="1" t="n">
-        <v>44006</v>
+        <v>44010</v>
       </c>
       <c r="D3" t="s">
         <v>26</v>
@@ -2549,25 +2549,25 @@
       </c>
       <c r="F3"/>
       <c r="G3" t="n">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="H3" t="n">
-        <v>2180424</v>
+        <v>2379175</v>
       </c>
       <c r="I3" t="n">
-        <v>85.507</v>
+        <v>93.301</v>
       </c>
       <c r="J3" t="n">
-        <v>47603</v>
+        <v>43114</v>
       </c>
       <c r="K3" t="n">
-        <v>1.867</v>
+        <v>1.691</v>
       </c>
       <c r="L3" t="n">
-        <v>43472</v>
+        <v>48264</v>
       </c>
       <c r="M3" t="n">
-        <v>1.705</v>
+        <v>1.893</v>
       </c>
       <c r="N3" t="s">
         <v>27</v>
@@ -2590,7 +2590,7 @@
         <v>31</v>
       </c>
       <c r="C4" s="1" t="n">
-        <v>44007</v>
+        <v>44010</v>
       </c>
       <c r="D4" t="s">
         <v>32</v>
@@ -2600,25 +2600,25 @@
       </c>
       <c r="F4"/>
       <c r="G4" t="n">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="H4" t="n">
-        <v>584243</v>
+        <v>602520</v>
       </c>
       <c r="I4" t="n">
-        <v>64.87</v>
+        <v>66.899</v>
       </c>
       <c r="J4" t="n">
-        <v>5659</v>
+        <v>5025</v>
       </c>
       <c r="K4" t="n">
-        <v>0.628</v>
+        <v>0.558</v>
       </c>
       <c r="L4" t="n">
-        <v>5474</v>
+        <v>5991</v>
       </c>
       <c r="M4" t="n">
-        <v>0.608</v>
+        <v>0.665</v>
       </c>
       <c r="N4" t="s">
         <v>34</v>
@@ -2641,7 +2641,7 @@
         <v>39</v>
       </c>
       <c r="C5" s="1" t="n">
-        <v>44008</v>
+        <v>44010</v>
       </c>
       <c r="D5" t="s">
         <v>40</v>
@@ -2651,25 +2651,25 @@
       </c>
       <c r="F5"/>
       <c r="G5" t="n">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="H5" t="n">
-        <v>511458</v>
+        <v>529242</v>
       </c>
       <c r="I5" t="n">
-        <v>300.578</v>
+        <v>311.029</v>
       </c>
       <c r="J5" t="n">
-        <v>8695</v>
+        <v>8141</v>
       </c>
       <c r="K5" t="n">
-        <v>5.11</v>
+        <v>4.784</v>
       </c>
       <c r="L5" t="n">
-        <v>7010</v>
+        <v>7311</v>
       </c>
       <c r="M5" t="n">
-        <v>4.12</v>
+        <v>4.297</v>
       </c>
       <c r="N5" t="s">
         <v>42</v>
@@ -2692,7 +2692,7 @@
         <v>47</v>
       </c>
       <c r="C6" s="1" t="n">
-        <v>44006</v>
+        <v>44010</v>
       </c>
       <c r="D6" t="s">
         <v>48</v>
@@ -2702,25 +2702,25 @@
       </c>
       <c r="F6"/>
       <c r="G6" t="n">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="H6" t="n">
-        <v>663444</v>
+        <v>733197</v>
       </c>
       <c r="I6" t="n">
-        <v>4.028</v>
+        <v>4.452</v>
       </c>
       <c r="J6" t="n">
-        <v>16433</v>
+        <v>18099</v>
       </c>
       <c r="K6" t="n">
-        <v>0.1</v>
+        <v>0.11</v>
       </c>
       <c r="L6" t="n">
-        <v>15600</v>
+        <v>16862</v>
       </c>
       <c r="M6" t="n">
-        <v>0.095</v>
+        <v>0.102</v>
       </c>
       <c r="N6" t="s">
         <v>49</v>
@@ -2743,7 +2743,7 @@
         <v>54</v>
       </c>
       <c r="C7" s="1" t="n">
-        <v>44007</v>
+        <v>44008</v>
       </c>
       <c r="D7" t="s">
         <v>55</v>
@@ -2753,25 +2753,25 @@
       </c>
       <c r="F7"/>
       <c r="G7" t="n">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="H7" t="n">
-        <v>919139</v>
+        <v>939524</v>
       </c>
       <c r="I7" t="n">
-        <v>97.27</v>
+        <v>99.428</v>
       </c>
       <c r="J7" t="n">
-        <v>17235</v>
+        <v>20385</v>
       </c>
       <c r="K7" t="n">
-        <v>1.824</v>
+        <v>2.157</v>
       </c>
       <c r="L7" t="n">
-        <v>16958</v>
+        <v>16805</v>
       </c>
       <c r="M7" t="n">
-        <v>1.795</v>
+        <v>1.778</v>
       </c>
       <c r="N7" t="s">
         <v>56</v>
@@ -2794,7 +2794,7 @@
         <v>60</v>
       </c>
       <c r="C8" s="1" t="n">
-        <v>44005</v>
+        <v>44007</v>
       </c>
       <c r="D8" t="s">
         <v>61</v>
@@ -2804,25 +2804,25 @@
       </c>
       <c r="F8"/>
       <c r="G8" t="n">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="H8" t="n">
-        <v>905354</v>
+        <v>929914</v>
       </c>
       <c r="I8" t="n">
-        <v>78.118</v>
+        <v>80.237</v>
       </c>
       <c r="J8" t="n">
-        <v>10335</v>
+        <v>8805</v>
       </c>
       <c r="K8" t="n">
-        <v>0.892</v>
+        <v>0.76</v>
       </c>
       <c r="L8" t="n">
-        <v>9147</v>
+        <v>9582</v>
       </c>
       <c r="M8" t="n">
-        <v>0.789</v>
+        <v>0.827</v>
       </c>
       <c r="N8" t="s">
         <v>62</v>
@@ -2941,7 +2941,7 @@
         <v>81</v>
       </c>
       <c r="C11" s="1" t="n">
-        <v>44008</v>
+        <v>44010</v>
       </c>
       <c r="D11" t="s">
         <v>82</v>
@@ -2951,25 +2951,25 @@
       </c>
       <c r="F11"/>
       <c r="G11" t="n">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="H11" t="n">
-        <v>128293</v>
+        <v>132571</v>
       </c>
       <c r="I11" t="n">
-        <v>18.464</v>
+        <v>19.079</v>
       </c>
       <c r="J11" t="n">
-        <v>2775</v>
+        <v>1528</v>
       </c>
       <c r="K11" t="n">
-        <v>0.399</v>
+        <v>0.22</v>
       </c>
       <c r="L11" t="n">
-        <v>1992</v>
+        <v>2296</v>
       </c>
       <c r="M11" t="n">
-        <v>0.287</v>
+        <v>0.33</v>
       </c>
       <c r="N11" t="s">
         <v>84</v>
@@ -2992,7 +2992,7 @@
         <v>88</v>
       </c>
       <c r="C12" s="1" t="n">
-        <v>44008</v>
+        <v>44010</v>
       </c>
       <c r="D12" t="s">
         <v>89</v>
@@ -3002,25 +3002,25 @@
       </c>
       <c r="F12"/>
       <c r="G12" t="n">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="H12" t="n">
-        <v>2558287</v>
+        <v>2640239</v>
       </c>
       <c r="I12" t="n">
-        <v>67.783</v>
+        <v>69.955</v>
       </c>
       <c r="J12" t="n">
-        <v>39713</v>
+        <v>42072</v>
       </c>
       <c r="K12" t="n">
-        <v>1.052</v>
+        <v>1.115</v>
       </c>
       <c r="L12" t="n">
-        <v>37560</v>
+        <v>36791</v>
       </c>
       <c r="M12" t="n">
-        <v>0.995</v>
+        <v>0.975</v>
       </c>
       <c r="N12" t="s">
         <v>90</v>
@@ -3043,7 +3043,7 @@
         <v>95</v>
       </c>
       <c r="C13" s="1" t="n">
-        <v>44007</v>
+        <v>44009</v>
       </c>
       <c r="D13" t="s">
         <v>96</v>
@@ -3055,25 +3055,25 @@
         <v>97</v>
       </c>
       <c r="G13" t="n">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="H13" t="n">
-        <v>1025081</v>
+        <v>1061274</v>
       </c>
       <c r="I13" t="n">
-        <v>53.624</v>
+        <v>55.517</v>
       </c>
       <c r="J13" t="n">
-        <v>17446</v>
+        <v>17944</v>
       </c>
       <c r="K13" t="n">
-        <v>0.913</v>
+        <v>0.939</v>
       </c>
       <c r="L13" t="n">
-        <v>17416</v>
+        <v>16812</v>
       </c>
       <c r="M13" t="n">
-        <v>0.911</v>
+        <v>0.879</v>
       </c>
       <c r="N13" t="s">
         <v>98</v>
@@ -3096,7 +3096,7 @@
         <v>102</v>
       </c>
       <c r="C14" s="1" t="n">
-        <v>44007</v>
+        <v>44009</v>
       </c>
       <c r="D14" t="s">
         <v>103</v>
@@ -3106,25 +3106,25 @@
       </c>
       <c r="F14"/>
       <c r="G14" t="n">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="H14" t="n">
-        <v>670093</v>
+        <v>707688</v>
       </c>
       <c r="I14" t="n">
-        <v>13.169</v>
+        <v>13.908</v>
       </c>
       <c r="J14" t="n">
-        <v>18501</v>
+        <v>18729</v>
       </c>
       <c r="K14" t="n">
-        <v>0.364</v>
+        <v>0.368</v>
       </c>
       <c r="L14" t="n">
-        <v>17069</v>
+        <v>17409</v>
       </c>
       <c r="M14" t="n">
-        <v>0.335</v>
+        <v>0.342</v>
       </c>
       <c r="N14" t="s">
         <v>104</v>
@@ -3198,7 +3198,7 @@
         <v>115</v>
       </c>
       <c r="C16" s="1" t="n">
-        <v>44007</v>
+        <v>44010</v>
       </c>
       <c r="D16" t="s">
         <v>116</v>
@@ -3208,25 +3208,25 @@
       </c>
       <c r="F16"/>
       <c r="G16" t="n">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="H16" t="n">
-        <v>74657</v>
+        <v>77453</v>
       </c>
       <c r="I16" t="n">
-        <v>18.186</v>
+        <v>18.867</v>
       </c>
       <c r="J16" t="n">
-        <v>919</v>
+        <v>829</v>
       </c>
       <c r="K16" t="n">
-        <v>0.224</v>
+        <v>0.202</v>
       </c>
       <c r="L16" t="n">
-        <v>523</v>
+        <v>711</v>
       </c>
       <c r="M16" t="n">
-        <v>0.127</v>
+        <v>0.173</v>
       </c>
       <c r="N16" t="s">
         <v>117</v>
@@ -3249,7 +3249,7 @@
         <v>122</v>
       </c>
       <c r="C17" s="1" t="n">
-        <v>44006</v>
+        <v>44009</v>
       </c>
       <c r="D17" t="s">
         <v>123</v>
@@ -3261,25 +3261,25 @@
         <v>125</v>
       </c>
       <c r="G17" t="n">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="H17" t="n">
-        <v>159571</v>
+        <v>166335</v>
       </c>
       <c r="I17" t="n">
-        <v>14.088</v>
+        <v>14.685</v>
       </c>
       <c r="J17" t="n">
-        <v>2184</v>
+        <v>2373</v>
       </c>
       <c r="K17" t="n">
-        <v>0.193</v>
+        <v>0.21</v>
       </c>
       <c r="L17" t="n">
-        <v>2263</v>
+        <v>2167</v>
       </c>
       <c r="M17" t="n">
-        <v>0.2</v>
+        <v>0.191</v>
       </c>
       <c r="N17" t="s">
         <v>124</v>
@@ -3302,7 +3302,7 @@
         <v>130</v>
       </c>
       <c r="C18" s="1" t="n">
-        <v>44006</v>
+        <v>44009</v>
       </c>
       <c r="D18" t="s">
         <v>131</v>
@@ -3312,25 +3312,25 @@
       </c>
       <c r="F18"/>
       <c r="G18" t="n">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="H18" t="n">
-        <v>532987</v>
+        <v>543925</v>
       </c>
       <c r="I18" t="n">
-        <v>49.77</v>
+        <v>50.791</v>
       </c>
       <c r="J18" t="n">
-        <v>3765</v>
+        <v>2365</v>
       </c>
       <c r="K18" t="n">
-        <v>0.352</v>
+        <v>0.221</v>
       </c>
       <c r="L18" t="n">
-        <v>3301</v>
+        <v>3489</v>
       </c>
       <c r="M18" t="n">
-        <v>0.308</v>
+        <v>0.326</v>
       </c>
       <c r="N18" t="s">
         <v>41</v>
@@ -3353,7 +3353,7 @@
         <v>135</v>
       </c>
       <c r="C19" s="1" t="n">
-        <v>44006</v>
+        <v>44007</v>
       </c>
       <c r="D19" t="s">
         <v>136</v>
@@ -3363,25 +3363,25 @@
       </c>
       <c r="F19"/>
       <c r="G19" t="n">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="H19" t="n">
-        <v>960329</v>
+        <v>978592</v>
       </c>
       <c r="I19" t="n">
-        <v>165.797</v>
+        <v>168.95</v>
       </c>
       <c r="J19" t="n">
-        <v>5707</v>
+        <v>4136</v>
       </c>
       <c r="K19" t="n">
-        <v>0.985</v>
+        <v>0.714</v>
       </c>
       <c r="L19" t="n">
-        <v>14908</v>
+        <v>15015</v>
       </c>
       <c r="M19" t="n">
-        <v>2.574</v>
+        <v>2.592</v>
       </c>
       <c r="N19" t="s">
         <v>137</v>
@@ -3404,7 +3404,7 @@
         <v>141</v>
       </c>
       <c r="C20" s="1" t="n">
-        <v>44007</v>
+        <v>44008</v>
       </c>
       <c r="D20" t="s">
         <v>142</v>
@@ -3416,21 +3416,21 @@
         <v>144</v>
       </c>
       <c r="G20" t="n">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="H20" t="n">
-        <v>106476</v>
+        <v>108471</v>
       </c>
       <c r="I20" t="n">
-        <v>6.035</v>
+        <v>6.148</v>
       </c>
       <c r="J20"/>
       <c r="K20"/>
       <c r="L20" t="n">
-        <v>1540</v>
+        <v>1557</v>
       </c>
       <c r="M20" t="n">
-        <v>0.087</v>
+        <v>0.088</v>
       </c>
       <c r="N20" t="s">
         <v>143</v>
@@ -3453,7 +3453,7 @@
         <v>148</v>
       </c>
       <c r="C21" s="1" t="n">
-        <v>44005</v>
+        <v>44009</v>
       </c>
       <c r="D21" t="s">
         <v>149</v>
@@ -3463,25 +3463,25 @@
       </c>
       <c r="F21"/>
       <c r="G21" t="n">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="H21" t="n">
-        <v>147771</v>
+        <v>157799</v>
       </c>
       <c r="I21" t="n">
-        <v>22.782</v>
+        <v>24.328</v>
       </c>
       <c r="J21" t="n">
-        <v>2430</v>
+        <v>2498</v>
       </c>
       <c r="K21" t="n">
-        <v>0.375</v>
+        <v>0.385</v>
       </c>
       <c r="L21" t="n">
-        <v>2442</v>
+        <v>2481</v>
       </c>
       <c r="M21" t="n">
-        <v>0.376</v>
+        <v>0.383</v>
       </c>
       <c r="N21" t="s">
         <v>150</v>
@@ -3504,7 +3504,7 @@
         <v>154</v>
       </c>
       <c r="C22" s="1" t="n">
-        <v>44006</v>
+        <v>44009</v>
       </c>
       <c r="D22" t="s">
         <v>155</v>
@@ -3514,25 +3514,25 @@
       </c>
       <c r="F22"/>
       <c r="G22" t="n">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="H22" t="n">
-        <v>104300</v>
+        <v>105677</v>
       </c>
       <c r="I22" t="n">
-        <v>78.626</v>
+        <v>79.664</v>
       </c>
       <c r="J22" t="n">
-        <v>350</v>
+        <v>368</v>
       </c>
       <c r="K22" t="n">
-        <v>0.264</v>
+        <v>0.277</v>
       </c>
       <c r="L22" t="n">
-        <v>559</v>
+        <v>393</v>
       </c>
       <c r="M22" t="n">
-        <v>0.421</v>
+        <v>0.296</v>
       </c>
       <c r="N22" t="s">
         <v>157</v>
@@ -3555,7 +3555,7 @@
         <v>162</v>
       </c>
       <c r="C23" s="1" t="n">
-        <v>44007</v>
+        <v>44010</v>
       </c>
       <c r="D23" t="s">
         <v>163</v>
@@ -3565,25 +3565,25 @@
       </c>
       <c r="F23"/>
       <c r="G23" t="n">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="H23" t="n">
-        <v>232050</v>
+        <v>246911</v>
       </c>
       <c r="I23" t="n">
-        <v>2.018</v>
+        <v>2.148</v>
       </c>
       <c r="J23" t="n">
-        <v>4675</v>
+        <v>3895</v>
       </c>
       <c r="K23" t="n">
-        <v>0.041</v>
+        <v>0.034</v>
       </c>
       <c r="L23" t="n">
-        <v>4262</v>
+        <v>4369</v>
       </c>
       <c r="M23" t="n">
-        <v>0.037</v>
+        <v>0.038</v>
       </c>
       <c r="N23" t="s">
         <v>164</v>
@@ -3606,7 +3606,7 @@
         <v>168</v>
       </c>
       <c r="C24" s="1" t="n">
-        <v>44006</v>
+        <v>44008</v>
       </c>
       <c r="D24" t="s">
         <v>169</v>
@@ -3616,25 +3616,25 @@
       </c>
       <c r="F24"/>
       <c r="G24" t="n">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="H24" t="n">
-        <v>237875</v>
+        <v>239670</v>
       </c>
       <c r="I24" t="n">
-        <v>42.932</v>
+        <v>43.256</v>
       </c>
       <c r="J24" t="n">
-        <v>470</v>
+        <v>276</v>
       </c>
       <c r="K24" t="n">
-        <v>0.085</v>
+        <v>0.05</v>
       </c>
       <c r="L24" t="n">
-        <v>1230</v>
+        <v>1391</v>
       </c>
       <c r="M24" t="n">
-        <v>0.222</v>
+        <v>0.251</v>
       </c>
       <c r="N24" t="s">
         <v>171</v>
@@ -3855,7 +3855,7 @@
         <v>200</v>
       </c>
       <c r="C29" s="1" t="n">
-        <v>44005</v>
+        <v>44007</v>
       </c>
       <c r="D29" t="s">
         <v>194</v>
@@ -3865,25 +3865,25 @@
       </c>
       <c r="F29"/>
       <c r="G29" t="n">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="H29" t="n">
-        <v>283124</v>
+        <v>288465</v>
       </c>
       <c r="I29" t="n">
-        <v>9.112</v>
+        <v>9.283</v>
       </c>
       <c r="J29" t="n">
-        <v>3008</v>
+        <v>2012</v>
       </c>
       <c r="K29" t="n">
+        <v>0.065</v>
+      </c>
+      <c r="L29" t="n">
+        <v>3026</v>
+      </c>
+      <c r="M29" t="n">
         <v>0.097</v>
-      </c>
-      <c r="L29" t="n">
-        <v>3115</v>
-      </c>
-      <c r="M29" t="n">
-        <v>0.1</v>
       </c>
       <c r="N29" t="s">
         <v>196</v>
@@ -3906,7 +3906,7 @@
         <v>202</v>
       </c>
       <c r="C30" s="1" t="n">
-        <v>44007</v>
+        <v>44010</v>
       </c>
       <c r="D30" t="s">
         <v>203</v>
@@ -3916,21 +3916,25 @@
       </c>
       <c r="F30"/>
       <c r="G30" t="n">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="H30" t="n">
-        <v>291840</v>
+        <v>305137</v>
       </c>
       <c r="I30" t="n">
-        <v>27.999</v>
-      </c>
-      <c r="J30"/>
-      <c r="K30"/>
+        <v>29.275</v>
+      </c>
+      <c r="J30" t="n">
+        <v>3993</v>
+      </c>
+      <c r="K30" t="n">
+        <v>0.383</v>
+      </c>
       <c r="L30" t="n">
-        <v>3072</v>
+        <v>3142</v>
       </c>
       <c r="M30" t="n">
-        <v>0.295</v>
+        <v>0.301</v>
       </c>
       <c r="N30" t="s">
         <v>205</v>
@@ -4153,7 +4157,7 @@
         <v>235</v>
       </c>
       <c r="C35" s="1" t="n">
-        <v>44008</v>
+        <v>44010</v>
       </c>
       <c r="D35" t="s">
         <v>231</v>
@@ -4165,25 +4169,25 @@
         <v>233</v>
       </c>
       <c r="G35" t="n">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="H35" t="n">
-        <v>7776228</v>
+        <v>8227802</v>
       </c>
       <c r="I35" t="n">
-        <v>5.635</v>
+        <v>5.962</v>
       </c>
       <c r="J35" t="n">
-        <v>215446</v>
+        <v>231095</v>
       </c>
       <c r="K35" t="n">
-        <v>0.156</v>
+        <v>0.167</v>
       </c>
       <c r="L35" t="n">
-        <v>192800</v>
+        <v>202939</v>
       </c>
       <c r="M35" t="n">
-        <v>0.14</v>
+        <v>0.147</v>
       </c>
       <c r="N35" t="s">
         <v>232</v>
@@ -4206,7 +4210,7 @@
         <v>237</v>
       </c>
       <c r="C36" s="1" t="n">
-        <v>44007</v>
+        <v>44010</v>
       </c>
       <c r="D36" t="s">
         <v>238</v>
@@ -4216,25 +4220,25 @@
       </c>
       <c r="F36"/>
       <c r="G36" t="n">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="H36" t="n">
-        <v>427158</v>
+        <v>456636</v>
       </c>
       <c r="I36" t="n">
-        <v>1.562</v>
+        <v>1.669</v>
       </c>
       <c r="J36" t="n">
-        <v>13239</v>
+        <v>7067</v>
       </c>
       <c r="K36" t="n">
-        <v>0.048</v>
+        <v>0.026</v>
       </c>
       <c r="L36" t="n">
-        <v>9786</v>
+        <v>10504</v>
       </c>
       <c r="M36" t="n">
-        <v>0.036</v>
+        <v>0.038</v>
       </c>
       <c r="N36" t="s">
         <v>239</v>
@@ -4257,7 +4261,7 @@
         <v>244</v>
       </c>
       <c r="C37" s="1" t="n">
-        <v>44006</v>
+        <v>44010</v>
       </c>
       <c r="D37" t="s">
         <v>245</v>
@@ -4267,25 +4271,25 @@
       </c>
       <c r="F37"/>
       <c r="G37" t="n">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="H37" t="n">
-        <v>1502525</v>
+        <v>1610869</v>
       </c>
       <c r="I37" t="n">
-        <v>17.889</v>
+        <v>19.179</v>
       </c>
       <c r="J37" t="n">
-        <v>27194</v>
+        <v>27327</v>
       </c>
       <c r="K37" t="n">
-        <v>0.324</v>
+        <v>0.325</v>
       </c>
       <c r="L37" t="n">
-        <v>26086</v>
+        <v>26923</v>
       </c>
       <c r="M37" t="n">
-        <v>0.311</v>
+        <v>0.321</v>
       </c>
       <c r="N37" t="s">
         <v>246</v>
@@ -4355,7 +4359,7 @@
         <v>256</v>
       </c>
       <c r="C39" s="1" t="n">
-        <v>43999</v>
+        <v>44003</v>
       </c>
       <c r="D39" t="s">
         <v>257</v>
@@ -4365,25 +4369,25 @@
       </c>
       <c r="F39"/>
       <c r="G39" t="n">
-        <v>137</v>
+        <v>141</v>
       </c>
       <c r="H39" t="n">
-        <v>804739</v>
+        <v>850679</v>
       </c>
       <c r="I39" t="n">
-        <v>92.974</v>
+        <v>98.281</v>
       </c>
       <c r="J39" t="n">
-        <v>15996</v>
+        <v>9073</v>
       </c>
       <c r="K39" t="n">
-        <v>1.848</v>
+        <v>1.048</v>
       </c>
       <c r="L39" t="n">
-        <v>13022</v>
+        <v>13115</v>
       </c>
       <c r="M39" t="n">
-        <v>1.504</v>
+        <v>1.515</v>
       </c>
       <c r="N39" t="s">
         <v>41</v>
@@ -4406,7 +4410,7 @@
         <v>262</v>
       </c>
       <c r="C40" s="1" t="n">
-        <v>44007</v>
+        <v>44010</v>
       </c>
       <c r="D40" t="s">
         <v>263</v>
@@ -4418,25 +4422,25 @@
         <v>265</v>
       </c>
       <c r="G40" t="n">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="H40" t="n">
-        <v>3140785</v>
+        <v>3220020</v>
       </c>
       <c r="I40" t="n">
-        <v>51.947</v>
+        <v>53.257</v>
       </c>
       <c r="J40" t="n">
-        <v>29421</v>
+        <v>21183</v>
       </c>
       <c r="K40" t="n">
-        <v>0.487</v>
+        <v>0.35</v>
       </c>
       <c r="L40" t="n">
-        <v>26009</v>
+        <v>25467</v>
       </c>
       <c r="M40" t="n">
-        <v>0.43</v>
+        <v>0.421</v>
       </c>
       <c r="N40" t="s">
         <v>266</v>
@@ -4459,7 +4463,7 @@
         <v>269</v>
       </c>
       <c r="C41" s="1" t="n">
-        <v>44007</v>
+        <v>44010</v>
       </c>
       <c r="D41" t="s">
         <v>263</v>
@@ -4471,25 +4475,25 @@
         <v>265</v>
       </c>
       <c r="G41" t="n">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="H41" t="n">
-        <v>5163154</v>
+        <v>5314619</v>
       </c>
       <c r="I41" t="n">
-        <v>85.395</v>
+        <v>87.9</v>
       </c>
       <c r="J41" t="n">
-        <v>56061</v>
+        <v>37346</v>
       </c>
       <c r="K41" t="n">
-        <v>0.927</v>
+        <v>0.618</v>
       </c>
       <c r="L41" t="n">
-        <v>47370</v>
+        <v>47178</v>
       </c>
       <c r="M41" t="n">
-        <v>0.783</v>
+        <v>0.78</v>
       </c>
       <c r="N41" t="s">
         <v>266</v>
@@ -4512,7 +4516,7 @@
         <v>272</v>
       </c>
       <c r="C42" s="1" t="n">
-        <v>44007</v>
+        <v>44009</v>
       </c>
       <c r="D42" t="s">
         <v>273</v>
@@ -4524,21 +4528,21 @@
         <v>275</v>
       </c>
       <c r="G42" t="n">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="H42" t="n">
-        <v>435495</v>
+        <v>446589</v>
       </c>
       <c r="I42" t="n">
-        <v>3.443</v>
+        <v>3.531</v>
       </c>
       <c r="J42"/>
       <c r="K42"/>
       <c r="L42" t="n">
-        <v>5580</v>
+        <v>5367</v>
       </c>
       <c r="M42" t="n">
-        <v>0.044</v>
+        <v>0.042</v>
       </c>
       <c r="N42" t="s">
         <v>276</v>
@@ -4561,7 +4565,7 @@
         <v>279</v>
       </c>
       <c r="C43" s="1" t="n">
-        <v>44005</v>
+        <v>44007</v>
       </c>
       <c r="D43" t="s">
         <v>280</v>
@@ -4573,25 +4577,25 @@
         <v>281</v>
       </c>
       <c r="G43" t="n">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="H43" t="n">
-        <v>632744</v>
+        <v>653555</v>
       </c>
       <c r="I43" t="n">
-        <v>5.003</v>
+        <v>5.167</v>
       </c>
       <c r="J43" t="n">
-        <v>5261</v>
+        <v>5497</v>
       </c>
       <c r="K43" t="n">
-        <v>0.042</v>
+        <v>0.043</v>
       </c>
       <c r="L43" t="n">
-        <v>5780</v>
+        <v>6534</v>
       </c>
       <c r="M43" t="n">
-        <v>0.046</v>
+        <v>0.052</v>
       </c>
       <c r="N43" t="s">
         <v>276</v>
@@ -4665,7 +4669,7 @@
         <v>289</v>
       </c>
       <c r="C45" s="1" t="n">
-        <v>44006</v>
+        <v>44010</v>
       </c>
       <c r="D45" t="s">
         <v>290</v>
@@ -4675,22 +4679,22 @@
       </c>
       <c r="F45"/>
       <c r="G45" t="n">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="H45" t="n">
-        <v>151396</v>
+        <v>165196</v>
       </c>
       <c r="I45" t="n">
-        <v>2.816</v>
+        <v>3.072</v>
       </c>
       <c r="J45" t="n">
-        <v>4859</v>
+        <v>2718</v>
       </c>
       <c r="K45" t="n">
-        <v>0.09</v>
+        <v>0.051</v>
       </c>
       <c r="L45" t="n">
-        <v>3596</v>
+        <v>3598</v>
       </c>
       <c r="M45" t="n">
         <v>0.067</v>
@@ -4767,7 +4771,7 @@
         <v>302</v>
       </c>
       <c r="C47" s="1" t="n">
-        <v>44007</v>
+        <v>44009</v>
       </c>
       <c r="D47" t="s">
         <v>303</v>
@@ -4779,25 +4783,25 @@
         <v>305</v>
       </c>
       <c r="G47" t="n">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="H47" t="n">
-        <v>142794</v>
+        <v>146874</v>
       </c>
       <c r="I47" t="n">
-        <v>75.705</v>
+        <v>77.868</v>
       </c>
       <c r="J47" t="n">
-        <v>1081</v>
+        <v>1788</v>
       </c>
       <c r="K47" t="n">
-        <v>0.573</v>
+        <v>0.948</v>
       </c>
       <c r="L47" t="n">
-        <v>1320</v>
+        <v>1472</v>
       </c>
       <c r="M47" t="n">
-        <v>0.7</v>
+        <v>0.78</v>
       </c>
       <c r="N47" t="s">
         <v>304</v>
@@ -4820,7 +4824,7 @@
         <v>308</v>
       </c>
       <c r="C48" s="1" t="n">
-        <v>44007</v>
+        <v>44009</v>
       </c>
       <c r="D48" t="s">
         <v>309</v>
@@ -4830,25 +4834,25 @@
       </c>
       <c r="F48"/>
       <c r="G48" t="n">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="H48" t="n">
-        <v>406557</v>
+        <v>414792</v>
       </c>
       <c r="I48" t="n">
-        <v>149.344</v>
+        <v>152.369</v>
       </c>
       <c r="J48" t="n">
-        <v>2716</v>
+        <v>3925</v>
       </c>
       <c r="K48" t="n">
-        <v>0.998</v>
+        <v>1.442</v>
       </c>
       <c r="L48" t="n">
-        <v>3619</v>
+        <v>3476</v>
       </c>
       <c r="M48" t="n">
-        <v>1.329</v>
+        <v>1.277</v>
       </c>
       <c r="N48" t="s">
         <v>41</v>
@@ -4871,7 +4875,7 @@
         <v>313</v>
       </c>
       <c r="C49" s="1" t="n">
-        <v>44007</v>
+        <v>44010</v>
       </c>
       <c r="D49" t="s">
         <v>314</v>
@@ -4881,25 +4885,25 @@
       </c>
       <c r="F49"/>
       <c r="G49" t="n">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="H49" t="n">
-        <v>163090</v>
+        <v>177217</v>
       </c>
       <c r="I49" t="n">
-        <v>260.537</v>
+        <v>283.105</v>
       </c>
       <c r="J49" t="n">
-        <v>7001</v>
+        <v>4925</v>
       </c>
       <c r="K49" t="n">
-        <v>11.184</v>
+        <v>7.868</v>
       </c>
       <c r="L49" t="n">
-        <v>4370</v>
+        <v>4172</v>
       </c>
       <c r="M49" t="n">
-        <v>6.981</v>
+        <v>6.665</v>
       </c>
       <c r="N49" t="s">
         <v>315</v>
@@ -4922,7 +4926,7 @@
         <v>319</v>
       </c>
       <c r="C50" s="1" t="n">
-        <v>44007</v>
+        <v>44009</v>
       </c>
       <c r="D50" t="s">
         <v>320</v>
@@ -4934,25 +4938,25 @@
         <v>322</v>
       </c>
       <c r="G50" t="n">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="H50" t="n">
-        <v>716178</v>
+        <v>739458</v>
       </c>
       <c r="I50" t="n">
-        <v>22.127</v>
+        <v>22.847</v>
       </c>
       <c r="J50" t="n">
-        <v>11842</v>
+        <v>10342</v>
       </c>
       <c r="K50" t="n">
-        <v>0.366</v>
+        <v>0.32</v>
       </c>
       <c r="L50" t="n">
-        <v>6656</v>
+        <v>8519</v>
       </c>
       <c r="M50" t="n">
-        <v>0.206</v>
+        <v>0.263</v>
       </c>
       <c r="N50" t="s">
         <v>41</v>
@@ -5028,7 +5032,7 @@
         <v>334</v>
       </c>
       <c r="C52" s="1" t="n">
-        <v>44003</v>
+        <v>44005</v>
       </c>
       <c r="D52" t="s">
         <v>335</v>
@@ -5038,25 +5042,25 @@
       </c>
       <c r="F52"/>
       <c r="G52" t="n">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="H52" t="n">
-        <v>456138</v>
+        <v>477363</v>
       </c>
       <c r="I52" t="n">
-        <v>3.538</v>
+        <v>3.702</v>
       </c>
       <c r="J52" t="n">
-        <v>2241</v>
+        <v>7252</v>
       </c>
       <c r="K52" t="n">
-        <v>0.017</v>
+        <v>0.056</v>
       </c>
       <c r="L52" t="n">
-        <v>8215</v>
+        <v>7783</v>
       </c>
       <c r="M52" t="n">
-        <v>0.064</v>
+        <v>0.06</v>
       </c>
       <c r="N52" t="s">
         <v>337</v>
@@ -5130,7 +5134,7 @@
         <v>347</v>
       </c>
       <c r="C54" s="1" t="n">
-        <v>44004</v>
+        <v>44009</v>
       </c>
       <c r="D54" t="s">
         <v>348</v>
@@ -5140,22 +5144,22 @@
       </c>
       <c r="F54"/>
       <c r="G54" t="n">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="H54" t="n">
-        <v>64532</v>
+        <v>73278</v>
       </c>
       <c r="I54" t="n">
-        <v>1.186</v>
+        <v>1.347</v>
       </c>
       <c r="J54" t="n">
-        <v>1114</v>
+        <v>1586</v>
       </c>
       <c r="K54" t="n">
-        <v>0.02</v>
+        <v>0.029</v>
       </c>
       <c r="L54" t="n">
-        <v>1597</v>
+        <v>1601</v>
       </c>
       <c r="M54" t="n">
         <v>0.029</v>
@@ -5234,7 +5238,7 @@
         <v>360</v>
       </c>
       <c r="C56" s="1" t="n">
-        <v>44005</v>
+        <v>44007</v>
       </c>
       <c r="D56" t="s">
         <v>361</v>
@@ -5244,25 +5248,25 @@
       </c>
       <c r="F56"/>
       <c r="G56" t="n">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="H56" t="n">
-        <v>561863</v>
+        <v>581445</v>
       </c>
       <c r="I56" t="n">
-        <v>32.791</v>
+        <v>33.933</v>
       </c>
       <c r="J56" t="n">
-        <v>7459</v>
+        <v>7203</v>
       </c>
       <c r="K56" t="n">
-        <v>0.435</v>
+        <v>0.42</v>
       </c>
       <c r="L56" t="n">
-        <v>8544</v>
+        <v>8746</v>
       </c>
       <c r="M56" t="n">
-        <v>0.499</v>
+        <v>0.51</v>
       </c>
       <c r="N56" t="s">
         <v>363</v>
@@ -5285,7 +5289,7 @@
         <v>367</v>
       </c>
       <c r="C57" s="1" t="n">
-        <v>44007</v>
+        <v>44009</v>
       </c>
       <c r="D57" t="s">
         <v>368</v>
@@ -5295,25 +5299,25 @@
       </c>
       <c r="F57"/>
       <c r="G57" t="n">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="H57" t="n">
-        <v>378257</v>
+        <v>392756</v>
       </c>
       <c r="I57" t="n">
-        <v>78.44</v>
+        <v>81.447</v>
       </c>
       <c r="J57" t="n">
-        <v>9825</v>
+        <v>5321</v>
       </c>
       <c r="K57" t="n">
-        <v>2.037</v>
+        <v>1.103</v>
       </c>
       <c r="L57" t="n">
-        <v>7257</v>
+        <v>7377</v>
       </c>
       <c r="M57" t="n">
-        <v>1.505</v>
+        <v>1.53</v>
       </c>
       <c r="N57" t="s">
         <v>369</v>
@@ -5336,7 +5340,7 @@
         <v>372</v>
       </c>
       <c r="C58" s="1" t="n">
-        <v>44007</v>
+        <v>44010</v>
       </c>
       <c r="D58" t="s">
         <v>373</v>
@@ -5346,22 +5350,22 @@
       </c>
       <c r="F58"/>
       <c r="G58" t="n">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="H58" t="n">
-        <v>122155</v>
+        <v>130164</v>
       </c>
       <c r="I58" t="n">
-        <v>0.593</v>
+        <v>0.631</v>
       </c>
       <c r="J58" t="n">
-        <v>2047</v>
+        <v>3006</v>
       </c>
       <c r="K58" t="n">
-        <v>0.01</v>
+        <v>0.015</v>
       </c>
       <c r="L58" t="n">
-        <v>2307</v>
+        <v>2370</v>
       </c>
       <c r="M58" t="n">
         <v>0.011</v>
@@ -5387,7 +5391,7 @@
         <v>378</v>
       </c>
       <c r="C59" s="1" t="n">
-        <v>44005</v>
+        <v>44006</v>
       </c>
       <c r="D59" t="s">
         <v>379</v>
@@ -5397,25 +5401,25 @@
       </c>
       <c r="F59"/>
       <c r="G59" t="n">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="H59" t="n">
-        <v>300722</v>
+        <v>305073</v>
       </c>
       <c r="I59" t="n">
-        <v>55.471</v>
+        <v>56.274</v>
       </c>
       <c r="J59" t="n">
-        <v>3370</v>
+        <v>3623</v>
       </c>
       <c r="K59" t="n">
-        <v>0.622</v>
+        <v>0.668</v>
       </c>
       <c r="L59" t="n">
-        <v>3030</v>
+        <v>3012</v>
       </c>
       <c r="M59" t="n">
-        <v>0.559</v>
+        <v>0.556</v>
       </c>
       <c r="N59" t="s">
         <v>380</v>
@@ -5438,7 +5442,7 @@
         <v>385</v>
       </c>
       <c r="C60" s="1" t="n">
-        <v>44007</v>
+        <v>44009</v>
       </c>
       <c r="D60" t="s">
         <v>386</v>
@@ -5448,21 +5452,21 @@
       </c>
       <c r="F60"/>
       <c r="G60" t="n">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="H60"/>
       <c r="I60"/>
       <c r="J60" t="n">
-        <v>3835</v>
+        <v>2508</v>
       </c>
       <c r="K60" t="n">
-        <v>0.751</v>
+        <v>0.491</v>
       </c>
       <c r="L60" t="n">
-        <v>3496</v>
+        <v>3604</v>
       </c>
       <c r="M60" t="n">
-        <v>0.685</v>
+        <v>0.706</v>
       </c>
       <c r="N60" t="s">
         <v>387</v>
@@ -5485,7 +5489,7 @@
         <v>391</v>
       </c>
       <c r="C61" s="1" t="n">
-        <v>44008</v>
+        <v>44010</v>
       </c>
       <c r="D61" t="s">
         <v>392</v>
@@ -5495,25 +5499,25 @@
       </c>
       <c r="F61"/>
       <c r="G61" t="n">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="H61" t="n">
-        <v>1193017</v>
+        <v>1239153</v>
       </c>
       <c r="I61" t="n">
-        <v>5.401</v>
+        <v>5.61</v>
       </c>
       <c r="J61" t="n">
-        <v>21041</v>
+        <v>25013</v>
       </c>
       <c r="K61" t="n">
-        <v>0.095</v>
+        <v>0.113</v>
       </c>
       <c r="L61" t="n">
-        <v>25987</v>
+        <v>23930</v>
       </c>
       <c r="M61" t="n">
-        <v>0.118</v>
+        <v>0.108</v>
       </c>
       <c r="N61" t="s">
         <v>393</v>
@@ -5587,7 +5591,7 @@
         <v>402</v>
       </c>
       <c r="C63" s="1" t="n">
-        <v>44006</v>
+        <v>44009</v>
       </c>
       <c r="D63" t="s">
         <v>403</v>
@@ -5597,25 +5601,25 @@
       </c>
       <c r="F63"/>
       <c r="G63" t="n">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="H63" t="n">
-        <v>60811</v>
+        <v>65605</v>
       </c>
       <c r="I63" t="n">
-        <v>8.526</v>
+        <v>9.198</v>
       </c>
       <c r="J63" t="n">
-        <v>1357</v>
+        <v>1631</v>
       </c>
       <c r="K63" t="n">
-        <v>0.19</v>
+        <v>0.229</v>
       </c>
       <c r="L63" t="n">
-        <v>1376</v>
+        <v>1397</v>
       </c>
       <c r="M63" t="n">
-        <v>0.193</v>
+        <v>0.196</v>
       </c>
       <c r="N63" t="s">
         <v>404</v>
@@ -5638,7 +5642,7 @@
         <v>408</v>
       </c>
       <c r="C64" s="1" t="n">
-        <v>44008</v>
+        <v>44010</v>
       </c>
       <c r="D64" t="s">
         <v>409</v>
@@ -5648,21 +5652,25 @@
       </c>
       <c r="F64"/>
       <c r="G64" t="n">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="H64" t="n">
-        <v>232730</v>
+        <v>242809</v>
       </c>
       <c r="I64" t="n">
-        <v>7.058</v>
-      </c>
-      <c r="J64"/>
-      <c r="K64"/>
+        <v>7.364</v>
+      </c>
+      <c r="J64" t="n">
+        <v>4921</v>
+      </c>
+      <c r="K64" t="n">
+        <v>0.149</v>
+      </c>
       <c r="L64" t="n">
-        <v>3360</v>
+        <v>3958</v>
       </c>
       <c r="M64" t="n">
-        <v>0.102</v>
+        <v>0.12</v>
       </c>
       <c r="N64" t="s">
         <v>410</v>
@@ -5685,7 +5693,7 @@
         <v>414</v>
       </c>
       <c r="C65" s="1" t="n">
-        <v>44005</v>
+        <v>44007</v>
       </c>
       <c r="D65" t="s">
         <v>415</v>
@@ -5695,25 +5703,25 @@
       </c>
       <c r="F65"/>
       <c r="G65" t="n">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="H65" t="n">
-        <v>580560</v>
+        <v>610052</v>
       </c>
       <c r="I65" t="n">
-        <v>5.298</v>
+        <v>5.567</v>
       </c>
       <c r="J65" t="n">
-        <v>11927</v>
+        <v>13994</v>
       </c>
       <c r="K65" t="n">
-        <v>0.109</v>
+        <v>0.128</v>
       </c>
       <c r="L65" t="n">
-        <v>12197</v>
+        <v>12821</v>
       </c>
       <c r="M65" t="n">
-        <v>0.111</v>
+        <v>0.117</v>
       </c>
       <c r="N65" t="s">
         <v>211</v>
@@ -5736,7 +5744,7 @@
         <v>419</v>
       </c>
       <c r="C66" s="1" t="n">
-        <v>44007</v>
+        <v>44009</v>
       </c>
       <c r="D66" t="s">
         <v>420</v>
@@ -5746,25 +5754,25 @@
       </c>
       <c r="F66"/>
       <c r="G66" t="n">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="H66" t="n">
-        <v>1278454</v>
+        <v>1315933</v>
       </c>
       <c r="I66" t="n">
-        <v>33.78</v>
+        <v>34.77</v>
       </c>
       <c r="J66" t="n">
-        <v>21453</v>
+        <v>19143</v>
       </c>
       <c r="K66" t="n">
-        <v>0.567</v>
+        <v>0.506</v>
       </c>
       <c r="L66" t="n">
-        <v>18748</v>
+        <v>17933</v>
       </c>
       <c r="M66" t="n">
-        <v>0.495</v>
+        <v>0.474</v>
       </c>
       <c r="N66" t="s">
         <v>421</v>
@@ -5787,7 +5795,7 @@
         <v>424</v>
       </c>
       <c r="C67" s="1" t="n">
-        <v>44007</v>
+        <v>44009</v>
       </c>
       <c r="D67"/>
       <c r="E67"/>
@@ -5798,10 +5806,10 @@
       <c r="J67"/>
       <c r="K67"/>
       <c r="L67" t="n">
-        <v>12155</v>
+        <v>5091</v>
       </c>
       <c r="M67" t="n">
-        <v>0.321</v>
+        <v>0.135</v>
       </c>
       <c r="N67" t="s">
         <v>421</v>
@@ -5875,7 +5883,7 @@
         <v>433</v>
       </c>
       <c r="C69" s="1" t="n">
-        <v>44007</v>
+        <v>44009</v>
       </c>
       <c r="D69" t="s">
         <v>434</v>
@@ -5885,25 +5893,25 @@
       </c>
       <c r="F69"/>
       <c r="G69" t="n">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="H69" t="n">
-        <v>337496</v>
+        <v>345691</v>
       </c>
       <c r="I69" t="n">
-        <v>117.143</v>
+        <v>119.987</v>
       </c>
       <c r="J69" t="n">
-        <v>4324</v>
+        <v>3777</v>
       </c>
       <c r="K69" t="n">
-        <v>1.501</v>
+        <v>1.311</v>
       </c>
       <c r="L69" t="n">
-        <v>3975</v>
+        <v>4000</v>
       </c>
       <c r="M69" t="n">
-        <v>1.38</v>
+        <v>1.388</v>
       </c>
       <c r="N69" t="s">
         <v>435</v>
@@ -5926,7 +5934,7 @@
         <v>439</v>
       </c>
       <c r="C70" s="1" t="n">
-        <v>44007</v>
+        <v>44010</v>
       </c>
       <c r="D70" t="s">
         <v>440</v>
@@ -5936,21 +5944,25 @@
       </c>
       <c r="F70"/>
       <c r="G70" t="n">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="H70" t="n">
-        <v>663558</v>
+        <v>694909</v>
       </c>
       <c r="I70" t="n">
-        <v>34.493</v>
-      </c>
-      <c r="J70"/>
-      <c r="K70"/>
+        <v>36.122</v>
+      </c>
+      <c r="J70" t="n">
+        <v>17650</v>
+      </c>
+      <c r="K70" t="n">
+        <v>0.917</v>
+      </c>
       <c r="L70" t="n">
-        <v>9409</v>
+        <v>9797</v>
       </c>
       <c r="M70" t="n">
-        <v>0.489</v>
+        <v>0.509</v>
       </c>
       <c r="N70" t="s">
         <v>441</v>
@@ -5973,7 +5985,7 @@
         <v>445</v>
       </c>
       <c r="C71" s="1" t="n">
-        <v>44007</v>
+        <v>44010</v>
       </c>
       <c r="D71" t="s">
         <v>446</v>
@@ -5983,25 +5995,25 @@
       </c>
       <c r="F71"/>
       <c r="G71" t="n">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="H71" t="n">
-        <v>18115830</v>
+        <v>19044954</v>
       </c>
       <c r="I71" t="n">
-        <v>124.137</v>
+        <v>130.503</v>
       </c>
       <c r="J71" t="n">
-        <v>311875</v>
+        <v>337008</v>
       </c>
       <c r="K71" t="n">
-        <v>2.137</v>
+        <v>2.309</v>
       </c>
       <c r="L71" t="n">
-        <v>303448</v>
+        <v>292357</v>
       </c>
       <c r="M71" t="n">
-        <v>2.079</v>
+        <v>2.003</v>
       </c>
       <c r="N71" t="s">
         <v>447</v>
@@ -6024,7 +6036,7 @@
         <v>451</v>
       </c>
       <c r="C72" s="1" t="n">
-        <v>44006</v>
+        <v>44009</v>
       </c>
       <c r="D72" t="s">
         <v>452</v>
@@ -6034,25 +6046,25 @@
       </c>
       <c r="F72"/>
       <c r="G72" t="n">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="H72" t="n">
-        <v>121527</v>
+        <v>134749</v>
       </c>
       <c r="I72" t="n">
-        <v>9.383</v>
+        <v>10.404</v>
       </c>
       <c r="J72" t="n">
-        <v>3415</v>
+        <v>4702</v>
       </c>
       <c r="K72" t="n">
-        <v>0.264</v>
+        <v>0.363</v>
       </c>
       <c r="L72" t="n">
-        <v>3174</v>
+        <v>3821</v>
       </c>
       <c r="M72" t="n">
-        <v>0.245</v>
+        <v>0.295</v>
       </c>
       <c r="N72" t="s">
         <v>453</v>
@@ -6075,7 +6087,7 @@
         <v>457</v>
       </c>
       <c r="C73" s="1" t="n">
-        <v>44007</v>
+        <v>44009</v>
       </c>
       <c r="D73" t="s">
         <v>458</v>
@@ -6085,25 +6097,25 @@
       </c>
       <c r="F73"/>
       <c r="G73" t="n">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="H73" t="n">
-        <v>1417771</v>
+        <v>1500516</v>
       </c>
       <c r="I73" t="n">
-        <v>40.724</v>
+        <v>43.101</v>
       </c>
       <c r="J73" t="n">
-        <v>37740</v>
+        <v>44275</v>
       </c>
       <c r="K73" t="n">
-        <v>1.084</v>
+        <v>1.272</v>
       </c>
       <c r="L73" t="n">
-        <v>31357</v>
+        <v>35931</v>
       </c>
       <c r="M73" t="n">
-        <v>0.901</v>
+        <v>1.032</v>
       </c>
       <c r="N73" t="s">
         <v>41</v>
@@ -6126,7 +6138,7 @@
         <v>461</v>
       </c>
       <c r="C74" s="1" t="n">
-        <v>44007</v>
+        <v>44009</v>
       </c>
       <c r="D74" t="s">
         <v>462</v>
@@ -6138,25 +6150,25 @@
         <v>464</v>
       </c>
       <c r="G74" t="n">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="H74" t="n">
-        <v>74037</v>
+        <v>76103</v>
       </c>
       <c r="I74" t="n">
-        <v>4.422</v>
+        <v>4.545</v>
       </c>
       <c r="J74" t="n">
-        <v>985</v>
+        <v>1009</v>
       </c>
       <c r="K74" t="n">
-        <v>0.059</v>
+        <v>0.06</v>
       </c>
       <c r="L74" t="n">
-        <v>1128</v>
+        <v>1014</v>
       </c>
       <c r="M74" t="n">
-        <v>0.067</v>
+        <v>0.061</v>
       </c>
       <c r="N74" t="s">
         <v>465</v>
@@ -6179,7 +6191,7 @@
         <v>470</v>
       </c>
       <c r="C75" s="1" t="n">
-        <v>44006</v>
+        <v>44009</v>
       </c>
       <c r="D75" t="s">
         <v>471</v>
@@ -6191,25 +6203,25 @@
         <v>472</v>
       </c>
       <c r="G75" t="n">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="H75" t="n">
-        <v>359069</v>
+        <v>380808</v>
       </c>
       <c r="I75" t="n">
-        <v>52.769</v>
+        <v>55.963</v>
       </c>
       <c r="J75" t="n">
-        <v>7784</v>
+        <v>5933</v>
       </c>
       <c r="K75" t="n">
-        <v>1.144</v>
+        <v>0.872</v>
       </c>
       <c r="L75" t="n">
-        <v>5641</v>
+        <v>6322</v>
       </c>
       <c r="M75" t="n">
-        <v>0.829</v>
+        <v>0.929</v>
       </c>
       <c r="N75" t="s">
         <v>41</v>
@@ -6326,7 +6338,7 @@
         <v>484</v>
       </c>
       <c r="C78" s="1" t="n">
-        <v>44007</v>
+        <v>44010</v>
       </c>
       <c r="D78" t="s">
         <v>485</v>
@@ -6336,25 +6348,25 @@
       </c>
       <c r="F78"/>
       <c r="G78" t="n">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="H78" t="n">
-        <v>204847</v>
+        <v>208904</v>
       </c>
       <c r="I78" t="n">
-        <v>37.52</v>
+        <v>38.263</v>
       </c>
       <c r="J78" t="n">
-        <v>936</v>
+        <v>931</v>
       </c>
       <c r="K78" t="n">
         <v>0.171</v>
       </c>
       <c r="L78" t="n">
-        <v>754</v>
+        <v>993</v>
       </c>
       <c r="M78" t="n">
-        <v>0.138</v>
+        <v>0.182</v>
       </c>
       <c r="N78" t="s">
         <v>487</v>
@@ -6377,7 +6389,7 @@
         <v>492</v>
       </c>
       <c r="C79" s="1" t="n">
-        <v>44006</v>
+        <v>44009</v>
       </c>
       <c r="D79" t="s">
         <v>493</v>
@@ -6387,25 +6399,25 @@
       </c>
       <c r="F79"/>
       <c r="G79" t="n">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="H79" t="n">
-        <v>96599</v>
+        <v>98945</v>
       </c>
       <c r="I79" t="n">
-        <v>46.466</v>
+        <v>47.594</v>
       </c>
       <c r="J79" t="n">
-        <v>1212</v>
+        <v>625</v>
       </c>
       <c r="K79" t="n">
-        <v>0.583</v>
+        <v>0.301</v>
       </c>
       <c r="L79" t="n">
-        <v>928</v>
+        <v>861</v>
       </c>
       <c r="M79" t="n">
-        <v>0.446</v>
+        <v>0.414</v>
       </c>
       <c r="N79" t="s">
         <v>495</v>
@@ -6428,7 +6440,7 @@
         <v>499</v>
       </c>
       <c r="C80" s="1" t="n">
-        <v>44007</v>
+        <v>44009</v>
       </c>
       <c r="D80" t="s">
         <v>500</v>
@@ -6440,25 +6452,25 @@
         <v>502</v>
       </c>
       <c r="G80" t="n">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="H80" t="n">
-        <v>1460012</v>
+        <v>1529009</v>
       </c>
       <c r="I80" t="n">
-        <v>24.617</v>
+        <v>25.781</v>
       </c>
       <c r="J80" t="n">
-        <v>43118</v>
+        <v>35905</v>
       </c>
       <c r="K80" t="n">
-        <v>0.727</v>
+        <v>0.605</v>
       </c>
       <c r="L80" t="n">
-        <v>33131</v>
+        <v>33629</v>
       </c>
       <c r="M80" t="n">
-        <v>0.559</v>
+        <v>0.567</v>
       </c>
       <c r="N80" t="s">
         <v>501</v>
@@ -6481,7 +6493,7 @@
         <v>506</v>
       </c>
       <c r="C81" s="1" t="n">
-        <v>44007</v>
+        <v>44010</v>
       </c>
       <c r="D81" t="s">
         <v>507</v>
@@ -6491,25 +6503,25 @@
       </c>
       <c r="F81"/>
       <c r="G81" t="n">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="H81" t="n">
-        <v>1200233</v>
+        <v>1231829</v>
       </c>
       <c r="I81" t="n">
-        <v>23.41</v>
+        <v>24.027</v>
       </c>
       <c r="J81" t="n">
-        <v>13914</v>
+        <v>7915</v>
       </c>
       <c r="K81" t="n">
-        <v>0.271</v>
+        <v>0.154</v>
       </c>
       <c r="L81" t="n">
-        <v>10891</v>
+        <v>10977</v>
       </c>
       <c r="M81" t="n">
-        <v>0.212</v>
+        <v>0.214</v>
       </c>
       <c r="N81" t="s">
         <v>508</v>
@@ -6592,10 +6604,10 @@
         <v>18</v>
       </c>
       <c r="H83" t="n">
-        <v>447462</v>
+        <v>444607</v>
       </c>
       <c r="I83" t="n">
-        <v>44.306</v>
+        <v>44.024</v>
       </c>
       <c r="J83"/>
       <c r="K83"/>
@@ -6626,7 +6638,7 @@
         <v>527</v>
       </c>
       <c r="C84" s="1" t="n">
-        <v>44006</v>
+        <v>44009</v>
       </c>
       <c r="D84" t="s">
         <v>528</v>
@@ -6636,25 +6648,25 @@
       </c>
       <c r="F84"/>
       <c r="G84" t="n">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="H84" t="n">
-        <v>534490</v>
+        <v>562909</v>
       </c>
       <c r="I84" t="n">
-        <v>61.758</v>
+        <v>65.041</v>
       </c>
       <c r="J84" t="n">
-        <v>5816</v>
+        <v>4993</v>
       </c>
       <c r="K84" t="n">
-        <v>0.672</v>
+        <v>0.577</v>
       </c>
       <c r="L84" t="n">
-        <v>6593</v>
+        <v>7693</v>
       </c>
       <c r="M84" t="n">
-        <v>0.762</v>
+        <v>0.889</v>
       </c>
       <c r="N84" t="s">
         <v>529</v>
@@ -6728,7 +6740,7 @@
         <v>540</v>
       </c>
       <c r="C86" s="1" t="n">
-        <v>44007</v>
+        <v>44009</v>
       </c>
       <c r="D86" t="s">
         <v>541</v>
@@ -6738,25 +6750,25 @@
       </c>
       <c r="F86"/>
       <c r="G86" t="n">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="H86" t="n">
-        <v>302670</v>
+        <v>305324</v>
       </c>
       <c r="I86" t="n">
-        <v>4.336</v>
+        <v>4.374</v>
       </c>
       <c r="J86" t="n">
-        <v>2521</v>
+        <v>2502</v>
       </c>
       <c r="K86" t="n">
         <v>0.036</v>
       </c>
       <c r="L86" t="n">
-        <v>2585</v>
+        <v>2125</v>
       </c>
       <c r="M86" t="n">
-        <v>0.037</v>
+        <v>0.03</v>
       </c>
       <c r="N86" t="s">
         <v>543</v>
@@ -6881,7 +6893,7 @@
         <v>560</v>
       </c>
       <c r="C89" s="1" t="n">
-        <v>44007</v>
+        <v>44010</v>
       </c>
       <c r="D89" t="s">
         <v>561</v>
@@ -6891,25 +6903,25 @@
       </c>
       <c r="F89"/>
       <c r="G89" t="n">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="H89" t="n">
-        <v>3135424</v>
+        <v>3231835</v>
       </c>
       <c r="I89" t="n">
-        <v>37.176</v>
+        <v>38.32</v>
       </c>
       <c r="J89" t="n">
-        <v>52303</v>
+        <v>45213</v>
       </c>
       <c r="K89" t="n">
-        <v>0.62</v>
+        <v>0.536</v>
       </c>
       <c r="L89" t="n">
-        <v>44730</v>
+        <v>40942</v>
       </c>
       <c r="M89" t="n">
-        <v>0.53</v>
+        <v>0.485</v>
       </c>
       <c r="N89" t="s">
         <v>562</v>
@@ -6932,7 +6944,7 @@
         <v>566</v>
       </c>
       <c r="C90" s="1" t="n">
-        <v>44006</v>
+        <v>44008</v>
       </c>
       <c r="D90" t="s">
         <v>567</v>
@@ -6944,22 +6956,22 @@
         <v>569</v>
       </c>
       <c r="G90" t="n">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="H90" t="n">
-        <v>153528</v>
+        <v>158509</v>
       </c>
       <c r="I90" t="n">
-        <v>3.356</v>
+        <v>3.465</v>
       </c>
       <c r="J90" t="n">
-        <v>3455</v>
+        <v>2868</v>
       </c>
       <c r="K90" t="n">
-        <v>0.076</v>
+        <v>0.063</v>
       </c>
       <c r="L90" t="n">
-        <v>2560</v>
+        <v>2573</v>
       </c>
       <c r="M90" t="n">
         <v>0.056</v>
@@ -6985,7 +6997,7 @@
         <v>573</v>
       </c>
       <c r="C91" s="1" t="n">
-        <v>44007</v>
+        <v>44010</v>
       </c>
       <c r="D91" t="s">
         <v>574</v>
@@ -6995,25 +7007,25 @@
       </c>
       <c r="F91"/>
       <c r="G91" t="n">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="H91" t="n">
-        <v>606766</v>
+        <v>641911</v>
       </c>
       <c r="I91" t="n">
-        <v>13.874</v>
+        <v>14.678</v>
       </c>
       <c r="J91" t="n">
-        <v>12764</v>
+        <v>9945</v>
       </c>
       <c r="K91" t="n">
-        <v>0.292</v>
+        <v>0.227</v>
       </c>
       <c r="L91" t="n">
-        <v>10903</v>
+        <v>11245</v>
       </c>
       <c r="M91" t="n">
-        <v>0.249</v>
+        <v>0.257</v>
       </c>
       <c r="N91" t="s">
         <v>575</v>
@@ -7087,7 +7099,7 @@
         <v>585</v>
       </c>
       <c r="C93" s="1" t="n">
-        <v>44006</v>
+        <v>44009</v>
       </c>
       <c r="D93" t="s">
         <v>586</v>
@@ -7099,25 +7111,25 @@
         <v>587</v>
       </c>
       <c r="G93" t="n">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="H93" t="n">
-        <v>4537055</v>
+        <v>4797763</v>
       </c>
       <c r="I93" t="n">
-        <v>66.833</v>
+        <v>70.674</v>
       </c>
       <c r="J93" t="n">
-        <v>76026</v>
+        <v>75495</v>
       </c>
       <c r="K93" t="n">
-        <v>1.12</v>
+        <v>1.112</v>
       </c>
       <c r="L93" t="n">
-        <v>62391</v>
+        <v>70119</v>
       </c>
       <c r="M93" t="n">
-        <v>0.919</v>
+        <v>1.033</v>
       </c>
       <c r="N93" t="s">
         <v>582</v>
@@ -7140,7 +7152,7 @@
         <v>590</v>
       </c>
       <c r="C94" s="1" t="n">
-        <v>44007</v>
+        <v>44008</v>
       </c>
       <c r="D94" t="s">
         <v>591</v>
@@ -7150,25 +7162,25 @@
       </c>
       <c r="F94"/>
       <c r="G94" t="n">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H94" t="n">
-        <v>31281178</v>
+        <v>32297688</v>
       </c>
       <c r="I94" t="n">
-        <v>94.504</v>
+        <v>97.575</v>
       </c>
       <c r="J94" t="n">
-        <v>1171117</v>
+        <v>1016510</v>
       </c>
       <c r="K94" t="n">
-        <v>3.538</v>
+        <v>3.071</v>
       </c>
       <c r="L94" t="n">
-        <v>682954</v>
+        <v>788003</v>
       </c>
       <c r="M94" t="n">
-        <v>2.063</v>
+        <v>2.381</v>
       </c>
       <c r="N94" t="s">
         <v>592</v>
@@ -7191,7 +7203,7 @@
         <v>596</v>
       </c>
       <c r="C95" s="1" t="n">
-        <v>44007</v>
+        <v>44009</v>
       </c>
       <c r="D95" t="s">
         <v>597</v>
@@ -7201,25 +7213,25 @@
       </c>
       <c r="F95"/>
       <c r="G95" t="n">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="H95" t="n">
-        <v>29207820</v>
+        <v>30401644</v>
       </c>
       <c r="I95" t="n">
-        <v>88.24</v>
+        <v>91.847</v>
       </c>
       <c r="J95" t="n">
-        <v>637587</v>
+        <v>590877</v>
       </c>
       <c r="K95" t="n">
-        <v>1.926</v>
+        <v>1.785</v>
       </c>
       <c r="L95" t="n">
-        <v>538019</v>
+        <v>546033</v>
       </c>
       <c r="M95" t="n">
-        <v>1.625</v>
+        <v>1.65</v>
       </c>
       <c r="N95" t="s">
         <v>598</v>
@@ -7242,7 +7254,7 @@
         <v>603</v>
       </c>
       <c r="C96" s="1" t="n">
-        <v>44006</v>
+        <v>44009</v>
       </c>
       <c r="D96" t="s">
         <v>604</v>
@@ -7252,25 +7264,25 @@
       </c>
       <c r="F96"/>
       <c r="G96" t="n">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="H96" t="n">
-        <v>60318</v>
+        <v>64183</v>
       </c>
       <c r="I96" t="n">
-        <v>17.364</v>
+        <v>18.477</v>
       </c>
       <c r="J96" t="n">
-        <v>1473</v>
+        <v>1418</v>
       </c>
       <c r="K96" t="n">
-        <v>0.424</v>
+        <v>0.408</v>
       </c>
       <c r="L96" t="n">
-        <v>833</v>
+        <v>1044</v>
       </c>
       <c r="M96" t="n">
-        <v>0.24</v>
+        <v>0.301</v>
       </c>
       <c r="N96" t="s">
         <v>124</v>
@@ -7340,7 +7352,7 @@
         <v>615</v>
       </c>
       <c r="C98" s="1" t="n">
-        <v>44006</v>
+        <v>44009</v>
       </c>
       <c r="D98" t="s">
         <v>616</v>
@@ -7350,25 +7362,25 @@
       </c>
       <c r="F98"/>
       <c r="G98" t="n">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="H98" t="n">
-        <v>28253</v>
+        <v>29641</v>
       </c>
       <c r="I98" t="n">
-        <v>1.901</v>
+        <v>1.994</v>
       </c>
       <c r="J98" t="n">
-        <v>654</v>
+        <v>464</v>
       </c>
       <c r="K98" t="n">
-        <v>0.044</v>
+        <v>0.031</v>
       </c>
       <c r="L98" t="n">
-        <v>423</v>
+        <v>456</v>
       </c>
       <c r="M98" t="n">
-        <v>0.028</v>
+        <v>0.031</v>
       </c>
       <c r="N98" t="s">
         <v>617</v>

</xml_diff>

<commit_message>
Updated testing data for 2020-06-29
</commit_message>
<xml_diff>
--- a/public/data/testing/covid-testing-latest-data-source-details.xlsx
+++ b/public/data/testing/covid-testing-latest-data-source-details.xlsx
@@ -71,7 +71,7 @@
     <t xml:space="preserve">Argentina - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.argentina.gob.ar/sites/default/files/28-06-20_reporte-matutino-covid-19.pdf</t>
+    <t xml:space="preserve">https://www.argentina.gob.ar/sites/default/files/29-06-20-reporte-matutino-covid-19.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">Government of Argentina</t>
@@ -112,7 +112,7 @@
     <t xml:space="preserve">Austria - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200628172135/https://www.sozialministerium.at/Informationen-zum-Coronavirus/Neuartiges-Coronavirus-(2019-nCov).html</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200629202830/https://www.sozialministerium.at/Informationen-zum-Coronavirus/Neuartiges-Coronavirus-(2019-nCov).html</t>
   </si>
   <si>
     <t xml:space="preserve">Austrian Ministry for Health</t>
@@ -139,7 +139,7 @@
     <t xml:space="preserve">Bahrain - units unclear</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200628075454/https://www.moh.gov.bh/COVID19</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200629202832/https://www.moh.gov.bh/COVID19</t>
   </si>
   <si>
     <t xml:space="preserve">Ministry of Health</t>
@@ -187,7 +187,7 @@
     <t xml:space="preserve">Belarus - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">http://minzdrav.gov.by/ru/sobytiya/v-belarusi-vyzdoroveli-i-vypisany-42-689-patsientov/</t>
+    <t xml:space="preserve">http://minzdrav.gov.by/ru/sobytiya/v-belarusi-vyzdoroveli-i-vypisany-45-tys-213-patsientov/</t>
   </si>
   <si>
     <t xml:space="preserve">Belarus Ministry of Health</t>
@@ -233,7 +233,7 @@
     <t xml:space="preserve">Bolivia - units unclear</t>
   </si>
   <si>
-    <t xml:space="preserve">https://minsalud.gob.bo/4335-covid-19-bolivia-reporta-1-016-nuevos-contagios-y-37-fallecidos</t>
+    <t xml:space="preserve">https://minsalud.gob.bo/4346-ministerio-de-salud-reporta-848-nuevos-contagios-de-coronavirus-y-el-total-sube-a-31-524</t>
   </si>
   <si>
     <t xml:space="preserve">https://www.minsalud.gob.bo/</t>
@@ -280,7 +280,7 @@
     <t xml:space="preserve">Bulgaria - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200628075458/https://coronavirus.bg/</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200629203058/https://coronavirus.bg/</t>
   </si>
   <si>
     <t xml:space="preserve">Bulgaria COVID-10 Information Portal</t>
@@ -303,7 +303,7 @@
     <t xml:space="preserve">Canada - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200628075743/https://www.canada.ca/en/public-health/services/diseases/2019-novel-coronavirus-infection.html</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200629203059/https://www.canada.ca/en/public-health/services/diseases/2019-novel-coronavirus-infection.html</t>
   </si>
   <si>
     <t xml:space="preserve">Government of Canada</t>
@@ -391,7 +391,7 @@
     <t xml:space="preserve">Croatia - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200628172149/https://www.koronavirus.hr/najnovije/ukupno-dosad-382-zarazene-osobe-u-hrvatskoj/35</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200629203159/https://www.koronavirus.hr/najnovije/ukupno-dosad-382-zarazene-osobe-u-hrvatskoj/35</t>
   </si>
   <si>
     <t xml:space="preserve">Government of Croatia</t>
@@ -454,7 +454,7 @@
     <t xml:space="preserve">Denmark - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://files.ssi.dk/Data-epidemiologisk-rapport-26062020-wd26</t>
+    <t xml:space="preserve">https://files.ssi.dk/Data-Epidemiologiske-Rapport-29062020-bhht</t>
   </si>
   <si>
     <t xml:space="preserve">Statens Serum Institut</t>
@@ -472,7 +472,7 @@
     <t xml:space="preserve">Ecuador - units unclear</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.gestionderiesgos.gob.ec/wp-content/uploads/2020/06/INFOGRAFIA-NACIONALCOVI-19-COE-NACIONAL-26062020-08h00.pdf</t>
+    <t xml:space="preserve">https://www.gestionderiesgos.gob.ec/wp-content/uploads/2020/06/INFOGRAFIA-NACIONALCOVI-19-COE-NACIONAL-29062020-08h00-v1.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">Government of Ecuador</t>
@@ -540,7 +540,7 @@
     <t xml:space="preserve">Ethiopia - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.ephi.gov.et/images/novel_coronavirus/confirmed-case-Press-release_June-28-Eng_V3.pdf</t>
+    <t xml:space="preserve">https://www.ephi.gov.et/images/novel_coronavirus/confirmed-case-Press-release_June-29-Eng_V2-1.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">Ethiopian Public Health Institute</t>
@@ -692,7 +692,7 @@
     <t xml:space="preserve">Greece - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://eody.gov.gr/wp-content/uploads/2020/06/covid-gr-daily-report-20200628.pdf</t>
+    <t xml:space="preserve">https://eody.gov.gr/covid-gr-daily-report-20200629/</t>
   </si>
   <si>
     <t xml:space="preserve">National Organization of Public Health</t>
@@ -874,7 +874,7 @@
     <t xml:space="preserve">Israel - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://govextra.gov.il/media/21474/covid19-data-israel-21062020.csv</t>
+    <t xml:space="preserve">https://govextra.gov.il/media/21682/covid19-data-israel-22062020.csv</t>
   </si>
   <si>
     <t xml:space="preserve">Israel Ministry of Health</t>
@@ -931,7 +931,7 @@
     <t xml:space="preserve">Japan - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.mhlw.go.jp/stf/newpage_12123.html</t>
+    <t xml:space="preserve">https://www.mhlw.go.jp/stf/newpage_12134.html</t>
   </si>
   <si>
     <t xml:space="preserve">Ministry of Health, Labor and Welfare Press Release</t>
@@ -955,7 +955,7 @@
     <t xml:space="preserve">Japan - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.mhlw.go.jp/content/10906000/000644327.pdf</t>
+    <t xml:space="preserve">https://www.mhlw.go.jp/content/10906000/000644588.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">The cumulative total reported in the press release matches the cumulative total calculated from the weekly and daily figures reported by the MOH.</t>
@@ -1013,7 +1013,7 @@
     <t xml:space="preserve">Kuwait - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/KUWAIT_MOH/status/1276481026156572673/photo/2</t>
+    <t xml:space="preserve">https://twitter.com/KUWAIT_MOH/status/1277560169166143488/photo/2</t>
   </si>
   <si>
     <t xml:space="preserve">Kuwait Ministry of Health</t>
@@ -1049,7 +1049,7 @@
     <t xml:space="preserve">Lithuania - samples tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200627121117/http://sam.lrv.lt/lt/naujienos/koronavirusas</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200629203228/http://sam.lrv.lt/lt/naujienos/koronavirusas</t>
   </si>
   <si>
     <t xml:space="preserve">http://sam.lrv.lt/lt/naujienos/koronavirusas</t>
@@ -1086,7 +1086,7 @@
     <t xml:space="preserve">Malaysia - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">http://covid-19.moh.gov.my/terkini/062020/situasi-terkini-27-jun-2020</t>
+    <t xml:space="preserve">http://covid-19.moh.gov.my/terkini/062020/situasi-terkini-29-jun-2020</t>
   </si>
   <si>
     <t xml:space="preserve">Ministry of Health Malaysia</t>
@@ -1111,13 +1111,13 @@
     <t xml:space="preserve">Maldives - samples tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.facebook.com/561317043971945/videos/594103654855023/</t>
+    <t xml:space="preserve">https://www.facebook.com/561317043971945/videos/605238630096493/</t>
   </si>
   <si>
     <t xml:space="preserve">Maldives Ministry of Health</t>
   </si>
   <si>
-    <t xml:space="preserve">Numbers visible in video at time: 1:24</t>
+    <t xml:space="preserve">Numbers visible in video at time: 1:29</t>
   </si>
   <si>
     <t xml:space="preserve">Maldives Ministry of Health Official Facebook page</t>
@@ -1160,7 +1160,7 @@
     <t xml:space="preserve">Morocco - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/Ministere_Sante/status/1275839812776464385</t>
+    <t xml:space="preserve">https://twitter.com/Ministere_Sante/status/1277289459021762562</t>
   </si>
   <si>
     <t xml:space="preserve">Morocco Ministry of Health</t>
@@ -1260,7 +1260,7 @@
     <t xml:space="preserve">Nigeria - samples tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200628172254/https://covid19.ncdc.gov.ng/</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200629203502/https://covid19.ncdc.gov.ng/</t>
   </si>
   <si>
     <t xml:space="preserve">Nigeria Centre for Disease Control</t>
@@ -1305,7 +1305,7 @@
     <t xml:space="preserve">Oman - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/OmanVSCovid19/status/1276802996517482496</t>
+    <t xml:space="preserve">https://twitter.com/OmanVSCovid19/status/1277529318206439430</t>
   </si>
   <si>
     <t xml:space="preserve">Oman Ministry of Health</t>
@@ -1324,7 +1324,7 @@
     <t xml:space="preserve">Pakistan - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200628080315/http://www.covid.gov.pk/</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200629203709/http://www.covid.gov.pk/</t>
   </si>
   <si>
     <t xml:space="preserve">Government of Pakistan</t>
@@ -1377,7 +1377,7 @@
     <t xml:space="preserve">Peru - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.gob.pe/institucion/minsa/noticias/189171-minsa-casos-confirmados-por-coronavirus-covid-19-ascienden-a-275-989-en-el-peru-comunicado-n-149</t>
+    <t xml:space="preserve">https://www.gob.pe/institucion/minsa/noticias/189224-minsa-casos-confirmados-por-coronavirus-covid-19-ascienden-a-279-419-en-el-peru-comunicado-n-151</t>
   </si>
   <si>
     <t xml:space="preserve">Ministry of Health, Government of Peru</t>
@@ -1418,7 +1418,7 @@
     <t xml:space="preserve">Poland - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/MZ_GOV_PL/status/1276802451555840002</t>
+    <t xml:space="preserve">https://twitter.com/MZ_GOV_PL/status/1277527227203231745</t>
   </si>
   <si>
     <t xml:space="preserve">Poland Ministry of Health</t>
@@ -1500,7 +1500,7 @@
     <t xml:space="preserve">Russia - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://rospotrebnadzor.ru/about/info/news/news_details.php?ELEMENT_ID=14783</t>
+    <t xml:space="preserve">https://rospotrebnadzor.ru/about/info/news/news_details.php?ELEMENT_ID=14787</t>
   </si>
   <si>
     <t xml:space="preserve">Government of the Russian Federation</t>
@@ -1700,7 +1700,7 @@
     <t xml:space="preserve">South Korea - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.cdc.go.kr/board/board.es?mid=&amp;bid=0030&amp;act=view&amp;list_no=367645&amp;tag=&amp;nPage=1</t>
+    <t xml:space="preserve">https://www.cdc.go.kr/board/board.es?mid=&amp;bid=0030&amp;act=view&amp;list_no=367651&amp;tag=&amp;nPage=1</t>
   </si>
   <si>
     <t xml:space="preserve">South Korea CDC</t>
@@ -1814,7 +1814,7 @@
     <t xml:space="preserve">Thailand - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200627121444/https://ddc.moph.go.th/viralpneumonia/eng/index.php</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200629203756/https://ddc.moph.go.th/viralpneumonia/eng/index.php</t>
   </si>
   <si>
     <t xml:space="preserve">Department of Disease Control</t>
@@ -1882,7 +1882,7 @@
     <t xml:space="preserve">Turkey - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200628080858/https://covid19.saglik.gov.tr/</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200629203759/https://covid19.saglik.gov.tr/</t>
   </si>
   <si>
     <t xml:space="preserve">Turkish Ministry of Health</t>
@@ -1903,7 +1903,7 @@
     <t xml:space="preserve">Uganda - samples tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/MinofHealthUG/status/1276787476024250374</t>
+    <t xml:space="preserve">https://www.health.go.ug/cause/update-on-the-covid-19-outbreak-in-uganda-27/</t>
   </si>
   <si>
     <t xml:space="preserve">Press Release from the Office of the Director General</t>
@@ -1927,7 +1927,7 @@
     <t xml:space="preserve">Ukraine - units unclear</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200628172444/https://covid19.gov.ua/en</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200629203801/https://covid19.gov.ua/en</t>
   </si>
   <si>
     <t xml:space="preserve">Cabinet of Ministers of Ukraine</t>
@@ -1964,7 +1964,7 @@
     <t xml:space="preserve">United Kingdom - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://assets.publishing.service.gov.uk/government/uploads/system/uploads/attachment_data/file/896043/2020-06-28-COVID-19-UK-testing-time-series.csv</t>
+    <t xml:space="preserve">https://assets.publishing.service.gov.uk/government/uploads/system/uploads/attachment_data/file/896265/COVID-19_UK_testing_time_series_29_June.csv</t>
   </si>
   <si>
     <t xml:space="preserve">Sum of pillar 1 + pillar 2 (tests processed only)</t>
@@ -2488,7 +2488,7 @@
         <v>18</v>
       </c>
       <c r="C2" s="1" t="n">
-        <v>44010</v>
+        <v>44011</v>
       </c>
       <c r="D2" t="s">
         <v>19</v>
@@ -2498,25 +2498,25 @@
       </c>
       <c r="F2"/>
       <c r="G2" t="n">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="H2" t="n">
-        <v>336951</v>
+        <v>344409</v>
       </c>
       <c r="I2" t="n">
-        <v>7.455</v>
+        <v>7.62</v>
       </c>
       <c r="J2" t="n">
-        <v>7915</v>
+        <v>7458</v>
       </c>
       <c r="K2" t="n">
-        <v>0.175</v>
+        <v>0.165</v>
       </c>
       <c r="L2" t="n">
-        <v>8183</v>
+        <v>8431</v>
       </c>
       <c r="M2" t="n">
-        <v>0.181</v>
+        <v>0.187</v>
       </c>
       <c r="N2" t="s">
         <v>20</v>
@@ -2590,7 +2590,7 @@
         <v>31</v>
       </c>
       <c r="C4" s="1" t="n">
-        <v>44010</v>
+        <v>44011</v>
       </c>
       <c r="D4" t="s">
         <v>32</v>
@@ -2600,25 +2600,25 @@
       </c>
       <c r="F4"/>
       <c r="G4" t="n">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="H4" t="n">
-        <v>602520</v>
+        <v>606375</v>
       </c>
       <c r="I4" t="n">
-        <v>66.899</v>
+        <v>67.327</v>
       </c>
       <c r="J4" t="n">
-        <v>5025</v>
+        <v>3855</v>
       </c>
       <c r="K4" t="n">
-        <v>0.558</v>
+        <v>0.428</v>
       </c>
       <c r="L4" t="n">
-        <v>5991</v>
+        <v>5796</v>
       </c>
       <c r="M4" t="n">
-        <v>0.665</v>
+        <v>0.644</v>
       </c>
       <c r="N4" t="s">
         <v>34</v>
@@ -2641,7 +2641,7 @@
         <v>39</v>
       </c>
       <c r="C5" s="1" t="n">
-        <v>44010</v>
+        <v>44011</v>
       </c>
       <c r="D5" t="s">
         <v>40</v>
@@ -2651,25 +2651,25 @@
       </c>
       <c r="F5"/>
       <c r="G5" t="n">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="H5" t="n">
-        <v>529242</v>
+        <v>536516</v>
       </c>
       <c r="I5" t="n">
-        <v>311.029</v>
+        <v>315.304</v>
       </c>
       <c r="J5" t="n">
-        <v>8141</v>
+        <v>7274</v>
       </c>
       <c r="K5" t="n">
-        <v>4.784</v>
+        <v>4.275</v>
       </c>
       <c r="L5" t="n">
-        <v>7311</v>
+        <v>7257</v>
       </c>
       <c r="M5" t="n">
-        <v>4.297</v>
+        <v>4.265</v>
       </c>
       <c r="N5" t="s">
         <v>42</v>
@@ -2743,7 +2743,7 @@
         <v>54</v>
       </c>
       <c r="C7" s="1" t="n">
-        <v>44008</v>
+        <v>44011</v>
       </c>
       <c r="D7" t="s">
         <v>55</v>
@@ -2753,25 +2753,21 @@
       </c>
       <c r="F7"/>
       <c r="G7" t="n">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H7" t="n">
-        <v>939524</v>
+        <v>992007</v>
       </c>
       <c r="I7" t="n">
-        <v>99.428</v>
-      </c>
-      <c r="J7" t="n">
-        <v>20385</v>
-      </c>
-      <c r="K7" t="n">
-        <v>2.157</v>
-      </c>
+        <v>104.982</v>
+      </c>
+      <c r="J7"/>
+      <c r="K7"/>
       <c r="L7" t="n">
-        <v>16805</v>
+        <v>16481</v>
       </c>
       <c r="M7" t="n">
-        <v>1.778</v>
+        <v>1.744</v>
       </c>
       <c r="N7" t="s">
         <v>56</v>
@@ -2845,7 +2841,7 @@
         <v>67</v>
       </c>
       <c r="C9" s="1" t="n">
-        <v>44007</v>
+        <v>44010</v>
       </c>
       <c r="D9" t="s">
         <v>68</v>
@@ -2855,25 +2851,25 @@
       </c>
       <c r="F9"/>
       <c r="G9" t="n">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="H9" t="n">
-        <v>66597</v>
+        <v>72236</v>
       </c>
       <c r="I9" t="n">
-        <v>5.705</v>
+        <v>6.188</v>
       </c>
       <c r="J9" t="n">
-        <v>1651</v>
+        <v>1364</v>
       </c>
       <c r="K9" t="n">
-        <v>0.141</v>
+        <v>0.117</v>
       </c>
       <c r="L9" t="n">
-        <v>1977</v>
+        <v>1921</v>
       </c>
       <c r="M9" t="n">
-        <v>0.169</v>
+        <v>0.165</v>
       </c>
       <c r="N9" t="s">
         <v>41</v>
@@ -2941,7 +2937,7 @@
         <v>81</v>
       </c>
       <c r="C11" s="1" t="n">
-        <v>44010</v>
+        <v>44011</v>
       </c>
       <c r="D11" t="s">
         <v>82</v>
@@ -2951,25 +2947,25 @@
       </c>
       <c r="F11"/>
       <c r="G11" t="n">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="H11" t="n">
-        <v>132571</v>
+        <v>133605</v>
       </c>
       <c r="I11" t="n">
-        <v>19.079</v>
+        <v>19.228</v>
       </c>
       <c r="J11" t="n">
-        <v>1528</v>
+        <v>1034</v>
       </c>
       <c r="K11" t="n">
-        <v>0.22</v>
+        <v>0.149</v>
       </c>
       <c r="L11" t="n">
-        <v>2296</v>
+        <v>2404</v>
       </c>
       <c r="M11" t="n">
-        <v>0.33</v>
+        <v>0.346</v>
       </c>
       <c r="N11" t="s">
         <v>84</v>
@@ -2992,7 +2988,7 @@
         <v>88</v>
       </c>
       <c r="C12" s="1" t="n">
-        <v>44010</v>
+        <v>44011</v>
       </c>
       <c r="D12" t="s">
         <v>89</v>
@@ -3002,25 +2998,25 @@
       </c>
       <c r="F12"/>
       <c r="G12" t="n">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="H12" t="n">
-        <v>2640239</v>
+        <v>2676629</v>
       </c>
       <c r="I12" t="n">
-        <v>69.955</v>
+        <v>70.919</v>
       </c>
       <c r="J12" t="n">
-        <v>42072</v>
+        <v>36390</v>
       </c>
       <c r="K12" t="n">
-        <v>1.115</v>
+        <v>0.964</v>
       </c>
       <c r="L12" t="n">
-        <v>36791</v>
+        <v>37323</v>
       </c>
       <c r="M12" t="n">
-        <v>0.975</v>
+        <v>0.989</v>
       </c>
       <c r="N12" t="s">
         <v>90</v>
@@ -3043,7 +3039,7 @@
         <v>95</v>
       </c>
       <c r="C13" s="1" t="n">
-        <v>44009</v>
+        <v>44010</v>
       </c>
       <c r="D13" t="s">
         <v>96</v>
@@ -3055,25 +3051,25 @@
         <v>97</v>
       </c>
       <c r="G13" t="n">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="H13" t="n">
-        <v>1061274</v>
+        <v>1079644</v>
       </c>
       <c r="I13" t="n">
-        <v>55.517</v>
+        <v>56.478</v>
       </c>
       <c r="J13" t="n">
-        <v>17944</v>
+        <v>18370</v>
       </c>
       <c r="K13" t="n">
-        <v>0.939</v>
+        <v>0.961</v>
       </c>
       <c r="L13" t="n">
-        <v>16812</v>
+        <v>16562</v>
       </c>
       <c r="M13" t="n">
-        <v>0.879</v>
+        <v>0.866</v>
       </c>
       <c r="N13" t="s">
         <v>98</v>
@@ -3198,7 +3194,7 @@
         <v>115</v>
       </c>
       <c r="C16" s="1" t="n">
-        <v>44010</v>
+        <v>44011</v>
       </c>
       <c r="D16" t="s">
         <v>116</v>
@@ -3208,25 +3204,25 @@
       </c>
       <c r="F16"/>
       <c r="G16" t="n">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="H16" t="n">
-        <v>77453</v>
+        <v>78183</v>
       </c>
       <c r="I16" t="n">
-        <v>18.867</v>
+        <v>19.045</v>
       </c>
       <c r="J16" t="n">
-        <v>829</v>
+        <v>730</v>
       </c>
       <c r="K16" t="n">
-        <v>0.202</v>
+        <v>0.178</v>
       </c>
       <c r="L16" t="n">
-        <v>711</v>
+        <v>777</v>
       </c>
       <c r="M16" t="n">
-        <v>0.173</v>
+        <v>0.189</v>
       </c>
       <c r="N16" t="s">
         <v>117</v>
@@ -3249,7 +3245,7 @@
         <v>122</v>
       </c>
       <c r="C17" s="1" t="n">
-        <v>44009</v>
+        <v>44010</v>
       </c>
       <c r="D17" t="s">
         <v>123</v>
@@ -3261,25 +3257,25 @@
         <v>125</v>
       </c>
       <c r="G17" t="n">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="H17" t="n">
-        <v>166335</v>
+        <v>168545</v>
       </c>
       <c r="I17" t="n">
-        <v>14.685</v>
+        <v>14.88</v>
       </c>
       <c r="J17" t="n">
-        <v>2373</v>
+        <v>2210</v>
       </c>
       <c r="K17" t="n">
-        <v>0.21</v>
+        <v>0.195</v>
       </c>
       <c r="L17" t="n">
-        <v>2167</v>
+        <v>2187</v>
       </c>
       <c r="M17" t="n">
-        <v>0.191</v>
+        <v>0.193</v>
       </c>
       <c r="N17" t="s">
         <v>124</v>
@@ -3302,7 +3298,7 @@
         <v>130</v>
       </c>
       <c r="C18" s="1" t="n">
-        <v>44009</v>
+        <v>44010</v>
       </c>
       <c r="D18" t="s">
         <v>131</v>
@@ -3312,25 +3308,25 @@
       </c>
       <c r="F18"/>
       <c r="G18" t="n">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="H18" t="n">
-        <v>543925</v>
+        <v>545973</v>
       </c>
       <c r="I18" t="n">
-        <v>50.791</v>
+        <v>50.983</v>
       </c>
       <c r="J18" t="n">
-        <v>2365</v>
+        <v>1812</v>
       </c>
       <c r="K18" t="n">
-        <v>0.221</v>
+        <v>0.169</v>
       </c>
       <c r="L18" t="n">
-        <v>3489</v>
+        <v>3594</v>
       </c>
       <c r="M18" t="n">
-        <v>0.326</v>
+        <v>0.336</v>
       </c>
       <c r="N18" t="s">
         <v>41</v>
@@ -3353,7 +3349,7 @@
         <v>135</v>
       </c>
       <c r="C19" s="1" t="n">
-        <v>44007</v>
+        <v>44010</v>
       </c>
       <c r="D19" t="s">
         <v>136</v>
@@ -3363,25 +3359,25 @@
       </c>
       <c r="F19"/>
       <c r="G19" t="n">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="H19" t="n">
-        <v>978592</v>
+        <v>1018866</v>
       </c>
       <c r="I19" t="n">
-        <v>168.95</v>
+        <v>175.903</v>
       </c>
       <c r="J19" t="n">
-        <v>4136</v>
+        <v>3149</v>
       </c>
       <c r="K19" t="n">
-        <v>0.714</v>
+        <v>0.544</v>
       </c>
       <c r="L19" t="n">
-        <v>15015</v>
+        <v>14983</v>
       </c>
       <c r="M19" t="n">
-        <v>2.592</v>
+        <v>2.587</v>
       </c>
       <c r="N19" t="s">
         <v>137</v>
@@ -3404,7 +3400,7 @@
         <v>141</v>
       </c>
       <c r="C20" s="1" t="n">
-        <v>44008</v>
+        <v>44011</v>
       </c>
       <c r="D20" t="s">
         <v>142</v>
@@ -3416,21 +3412,21 @@
         <v>144</v>
       </c>
       <c r="G20" t="n">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="H20" t="n">
-        <v>108471</v>
+        <v>112845</v>
       </c>
       <c r="I20" t="n">
-        <v>6.148</v>
+        <v>6.396</v>
       </c>
       <c r="J20"/>
       <c r="K20"/>
       <c r="L20" t="n">
-        <v>1557</v>
+        <v>1727</v>
       </c>
       <c r="M20" t="n">
-        <v>0.088</v>
+        <v>0.098</v>
       </c>
       <c r="N20" t="s">
         <v>143</v>
@@ -3504,7 +3500,7 @@
         <v>154</v>
       </c>
       <c r="C22" s="1" t="n">
-        <v>44009</v>
+        <v>44010</v>
       </c>
       <c r="D22" t="s">
         <v>155</v>
@@ -3514,25 +3510,25 @@
       </c>
       <c r="F22"/>
       <c r="G22" t="n">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="H22" t="n">
-        <v>105677</v>
+        <v>106022</v>
       </c>
       <c r="I22" t="n">
-        <v>79.664</v>
+        <v>79.924</v>
       </c>
       <c r="J22" t="n">
-        <v>368</v>
+        <v>351</v>
       </c>
       <c r="K22" t="n">
-        <v>0.277</v>
+        <v>0.265</v>
       </c>
       <c r="L22" t="n">
-        <v>393</v>
+        <v>402</v>
       </c>
       <c r="M22" t="n">
-        <v>0.296</v>
+        <v>0.303</v>
       </c>
       <c r="N22" t="s">
         <v>157</v>
@@ -3555,7 +3551,7 @@
         <v>162</v>
       </c>
       <c r="C23" s="1" t="n">
-        <v>44010</v>
+        <v>44011</v>
       </c>
       <c r="D23" t="s">
         <v>163</v>
@@ -3565,25 +3561,25 @@
       </c>
       <c r="F23"/>
       <c r="G23" t="n">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="H23" t="n">
-        <v>246911</v>
+        <v>250604</v>
       </c>
       <c r="I23" t="n">
-        <v>2.148</v>
+        <v>2.18</v>
       </c>
       <c r="J23" t="n">
-        <v>3895</v>
+        <v>3693</v>
       </c>
       <c r="K23" t="n">
-        <v>0.034</v>
+        <v>0.032</v>
       </c>
       <c r="L23" t="n">
-        <v>4369</v>
+        <v>4434</v>
       </c>
       <c r="M23" t="n">
-        <v>0.038</v>
+        <v>0.039</v>
       </c>
       <c r="N23" t="s">
         <v>164</v>
@@ -3855,7 +3851,7 @@
         <v>200</v>
       </c>
       <c r="C29" s="1" t="n">
-        <v>44007</v>
+        <v>44009</v>
       </c>
       <c r="D29" t="s">
         <v>194</v>
@@ -3865,25 +3861,25 @@
       </c>
       <c r="F29"/>
       <c r="G29" t="n">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="H29" t="n">
-        <v>288465</v>
+        <v>294867</v>
       </c>
       <c r="I29" t="n">
-        <v>9.283</v>
+        <v>9.49</v>
       </c>
       <c r="J29" t="n">
-        <v>2012</v>
+        <v>4502</v>
       </c>
       <c r="K29" t="n">
-        <v>0.065</v>
+        <v>0.145</v>
       </c>
       <c r="L29" t="n">
-        <v>3026</v>
+        <v>3510</v>
       </c>
       <c r="M29" t="n">
-        <v>0.097</v>
+        <v>0.113</v>
       </c>
       <c r="N29" t="s">
         <v>196</v>
@@ -3906,7 +3902,7 @@
         <v>202</v>
       </c>
       <c r="C30" s="1" t="n">
-        <v>44010</v>
+        <v>44011</v>
       </c>
       <c r="D30" t="s">
         <v>203</v>
@@ -3916,25 +3912,25 @@
       </c>
       <c r="F30"/>
       <c r="G30" t="n">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="H30" t="n">
-        <v>305137</v>
+        <v>308392</v>
       </c>
       <c r="I30" t="n">
-        <v>29.275</v>
+        <v>29.587</v>
       </c>
       <c r="J30" t="n">
-        <v>3993</v>
+        <v>3255</v>
       </c>
       <c r="K30" t="n">
-        <v>0.383</v>
+        <v>0.312</v>
       </c>
       <c r="L30" t="n">
-        <v>3142</v>
+        <v>3200</v>
       </c>
       <c r="M30" t="n">
-        <v>0.301</v>
+        <v>0.307</v>
       </c>
       <c r="N30" t="s">
         <v>205</v>
@@ -4000,7 +3996,7 @@
         <v>216</v>
       </c>
       <c r="C32" s="1" t="n">
-        <v>44004</v>
+        <v>44011</v>
       </c>
       <c r="D32" t="s">
         <v>217</v>
@@ -4012,25 +4008,25 @@
         <v>219</v>
       </c>
       <c r="G32" t="n">
-        <v>109</v>
+        <v>116</v>
       </c>
       <c r="H32" t="n">
-        <v>258115</v>
+        <v>273879</v>
       </c>
       <c r="I32" t="n">
-        <v>26.719</v>
+        <v>28.351</v>
       </c>
       <c r="J32" t="n">
-        <v>1789</v>
+        <v>2685</v>
       </c>
       <c r="K32" t="n">
-        <v>0.185</v>
+        <v>0.278</v>
       </c>
       <c r="L32" t="n">
-        <v>3248</v>
+        <v>2252</v>
       </c>
       <c r="M32" t="n">
-        <v>0.336</v>
+        <v>0.233</v>
       </c>
       <c r="N32" t="s">
         <v>218</v>
@@ -4157,7 +4153,7 @@
         <v>235</v>
       </c>
       <c r="C35" s="1" t="n">
-        <v>44010</v>
+        <v>44011</v>
       </c>
       <c r="D35" t="s">
         <v>231</v>
@@ -4169,25 +4165,25 @@
         <v>233</v>
       </c>
       <c r="G35" t="n">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="H35" t="n">
-        <v>8227802</v>
+        <v>8398362</v>
       </c>
       <c r="I35" t="n">
-        <v>5.962</v>
+        <v>6.086</v>
       </c>
       <c r="J35" t="n">
-        <v>231095</v>
+        <v>170560</v>
       </c>
       <c r="K35" t="n">
-        <v>0.167</v>
+        <v>0.124</v>
       </c>
       <c r="L35" t="n">
-        <v>202939</v>
+        <v>206838</v>
       </c>
       <c r="M35" t="n">
-        <v>0.147</v>
+        <v>0.15</v>
       </c>
       <c r="N35" t="s">
         <v>232</v>
@@ -4210,7 +4206,7 @@
         <v>237</v>
       </c>
       <c r="C36" s="1" t="n">
-        <v>44010</v>
+        <v>44011</v>
       </c>
       <c r="D36" t="s">
         <v>238</v>
@@ -4220,22 +4216,22 @@
       </c>
       <c r="F36"/>
       <c r="G36" t="n">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="H36" t="n">
-        <v>456636</v>
+        <v>465683</v>
       </c>
       <c r="I36" t="n">
-        <v>1.669</v>
+        <v>1.703</v>
       </c>
       <c r="J36" t="n">
-        <v>7067</v>
+        <v>9047</v>
       </c>
       <c r="K36" t="n">
-        <v>0.026</v>
+        <v>0.033</v>
       </c>
       <c r="L36" t="n">
-        <v>10504</v>
+        <v>10367</v>
       </c>
       <c r="M36" t="n">
         <v>0.038</v>
@@ -4359,7 +4355,7 @@
         <v>256</v>
       </c>
       <c r="C39" s="1" t="n">
-        <v>44003</v>
+        <v>44004</v>
       </c>
       <c r="D39" t="s">
         <v>257</v>
@@ -4369,25 +4365,25 @@
       </c>
       <c r="F39"/>
       <c r="G39" t="n">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="H39" t="n">
-        <v>850679</v>
+        <v>864761</v>
       </c>
       <c r="I39" t="n">
-        <v>98.281</v>
+        <v>99.908</v>
       </c>
       <c r="J39" t="n">
-        <v>9073</v>
+        <v>14006</v>
       </c>
       <c r="K39" t="n">
-        <v>1.048</v>
+        <v>1.618</v>
       </c>
       <c r="L39" t="n">
-        <v>13115</v>
+        <v>13066</v>
       </c>
       <c r="M39" t="n">
-        <v>1.515</v>
+        <v>1.51</v>
       </c>
       <c r="N39" t="s">
         <v>41</v>
@@ -4410,7 +4406,7 @@
         <v>262</v>
       </c>
       <c r="C40" s="1" t="n">
-        <v>44010</v>
+        <v>44011</v>
       </c>
       <c r="D40" t="s">
         <v>263</v>
@@ -4422,25 +4418,25 @@
         <v>265</v>
       </c>
       <c r="G40" t="n">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="H40" t="n">
-        <v>3220020</v>
+        <v>3235504</v>
       </c>
       <c r="I40" t="n">
-        <v>53.257</v>
+        <v>53.513</v>
       </c>
       <c r="J40" t="n">
-        <v>21183</v>
+        <v>15484</v>
       </c>
       <c r="K40" t="n">
-        <v>0.35</v>
+        <v>0.256</v>
       </c>
       <c r="L40" t="n">
-        <v>25467</v>
+        <v>25372</v>
       </c>
       <c r="M40" t="n">
-        <v>0.421</v>
+        <v>0.42</v>
       </c>
       <c r="N40" t="s">
         <v>266</v>
@@ -4463,7 +4459,7 @@
         <v>269</v>
       </c>
       <c r="C41" s="1" t="n">
-        <v>44010</v>
+        <v>44011</v>
       </c>
       <c r="D41" t="s">
         <v>263</v>
@@ -4475,25 +4471,25 @@
         <v>265</v>
       </c>
       <c r="G41" t="n">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="H41" t="n">
-        <v>5314619</v>
+        <v>5341837</v>
       </c>
       <c r="I41" t="n">
-        <v>87.9</v>
+        <v>88.351</v>
       </c>
       <c r="J41" t="n">
-        <v>37346</v>
+        <v>27218</v>
       </c>
       <c r="K41" t="n">
-        <v>0.618</v>
+        <v>0.45</v>
       </c>
       <c r="L41" t="n">
-        <v>47178</v>
+        <v>46928</v>
       </c>
       <c r="M41" t="n">
-        <v>0.78</v>
+        <v>0.776</v>
       </c>
       <c r="N41" t="s">
         <v>266</v>
@@ -4516,7 +4512,7 @@
         <v>272</v>
       </c>
       <c r="C42" s="1" t="n">
-        <v>44009</v>
+        <v>44011</v>
       </c>
       <c r="D42" t="s">
         <v>273</v>
@@ -4528,21 +4524,21 @@
         <v>275</v>
       </c>
       <c r="G42" t="n">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="H42" t="n">
-        <v>446589</v>
+        <v>454609</v>
       </c>
       <c r="I42" t="n">
-        <v>3.531</v>
+        <v>3.594</v>
       </c>
       <c r="J42"/>
       <c r="K42"/>
       <c r="L42" t="n">
-        <v>5367</v>
+        <v>5237</v>
       </c>
       <c r="M42" t="n">
-        <v>0.042</v>
+        <v>0.041</v>
       </c>
       <c r="N42" t="s">
         <v>276</v>
@@ -4565,7 +4561,7 @@
         <v>279</v>
       </c>
       <c r="C43" s="1" t="n">
-        <v>44007</v>
+        <v>44009</v>
       </c>
       <c r="D43" t="s">
         <v>280</v>
@@ -4577,25 +4573,25 @@
         <v>281</v>
       </c>
       <c r="G43" t="n">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="H43" t="n">
-        <v>653555</v>
+        <v>657245</v>
       </c>
       <c r="I43" t="n">
-        <v>5.167</v>
+        <v>5.197</v>
       </c>
       <c r="J43" t="n">
-        <v>5497</v>
+        <v>1694</v>
       </c>
       <c r="K43" t="n">
-        <v>0.043</v>
+        <v>0.013</v>
       </c>
       <c r="L43" t="n">
-        <v>6534</v>
+        <v>5104</v>
       </c>
       <c r="M43" t="n">
-        <v>0.052</v>
+        <v>0.04</v>
       </c>
       <c r="N43" t="s">
         <v>276</v>
@@ -4720,7 +4716,7 @@
         <v>296</v>
       </c>
       <c r="C46" s="1" t="n">
-        <v>44008</v>
+        <v>44011</v>
       </c>
       <c r="D46" t="s">
         <v>297</v>
@@ -4730,25 +4726,25 @@
       </c>
       <c r="F46"/>
       <c r="G46" t="n">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="H46" t="n">
-        <v>372284</v>
+        <v>382842</v>
       </c>
       <c r="I46" t="n">
-        <v>87.174</v>
+        <v>89.647</v>
       </c>
       <c r="J46" t="n">
-        <v>3774</v>
+        <v>3504</v>
       </c>
       <c r="K46" t="n">
-        <v>0.884</v>
+        <v>0.821</v>
       </c>
       <c r="L46" t="n">
-        <v>3267</v>
+        <v>3607</v>
       </c>
       <c r="M46" t="n">
-        <v>0.765</v>
+        <v>0.845</v>
       </c>
       <c r="N46" t="s">
         <v>298</v>
@@ -4771,7 +4767,7 @@
         <v>302</v>
       </c>
       <c r="C47" s="1" t="n">
-        <v>44009</v>
+        <v>44011</v>
       </c>
       <c r="D47" t="s">
         <v>303</v>
@@ -4783,25 +4779,25 @@
         <v>305</v>
       </c>
       <c r="G47" t="n">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="H47" t="n">
-        <v>146874</v>
+        <v>148777</v>
       </c>
       <c r="I47" t="n">
-        <v>77.868</v>
+        <v>78.876</v>
       </c>
       <c r="J47" t="n">
-        <v>1788</v>
+        <v>861</v>
       </c>
       <c r="K47" t="n">
-        <v>0.948</v>
+        <v>0.456</v>
       </c>
       <c r="L47" t="n">
-        <v>1472</v>
+        <v>1393</v>
       </c>
       <c r="M47" t="n">
-        <v>0.78</v>
+        <v>0.739</v>
       </c>
       <c r="N47" t="s">
         <v>304</v>
@@ -4824,7 +4820,7 @@
         <v>308</v>
       </c>
       <c r="C48" s="1" t="n">
-        <v>44009</v>
+        <v>44011</v>
       </c>
       <c r="D48" t="s">
         <v>309</v>
@@ -4834,25 +4830,25 @@
       </c>
       <c r="F48"/>
       <c r="G48" t="n">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="H48" t="n">
-        <v>414792</v>
+        <v>418368</v>
       </c>
       <c r="I48" t="n">
-        <v>152.369</v>
+        <v>153.682</v>
       </c>
       <c r="J48" t="n">
-        <v>3925</v>
+        <v>1629</v>
       </c>
       <c r="K48" t="n">
-        <v>1.442</v>
+        <v>0.598</v>
       </c>
       <c r="L48" t="n">
-        <v>3476</v>
+        <v>3415</v>
       </c>
       <c r="M48" t="n">
-        <v>1.277</v>
+        <v>1.254</v>
       </c>
       <c r="N48" t="s">
         <v>41</v>
@@ -4926,7 +4922,7 @@
         <v>319</v>
       </c>
       <c r="C50" s="1" t="n">
-        <v>44009</v>
+        <v>44011</v>
       </c>
       <c r="D50" t="s">
         <v>320</v>
@@ -4938,25 +4934,25 @@
         <v>322</v>
       </c>
       <c r="G50" t="n">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="H50" t="n">
-        <v>739458</v>
+        <v>756171</v>
       </c>
       <c r="I50" t="n">
-        <v>22.847</v>
+        <v>23.363</v>
       </c>
       <c r="J50" t="n">
-        <v>10342</v>
+        <v>6221</v>
       </c>
       <c r="K50" t="n">
-        <v>0.32</v>
+        <v>0.192</v>
       </c>
       <c r="L50" t="n">
-        <v>8519</v>
+        <v>9895</v>
       </c>
       <c r="M50" t="n">
-        <v>0.263</v>
+        <v>0.306</v>
       </c>
       <c r="N50" t="s">
         <v>41</v>
@@ -4979,7 +4975,7 @@
         <v>326</v>
       </c>
       <c r="C51" s="1" t="n">
-        <v>44006</v>
+        <v>44007</v>
       </c>
       <c r="D51" t="s">
         <v>327</v>
@@ -4991,25 +4987,25 @@
         <v>329</v>
       </c>
       <c r="G51" t="n">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="H51" t="n">
-        <v>45185</v>
+        <v>46182</v>
       </c>
       <c r="I51" t="n">
-        <v>83.592</v>
+        <v>85.436</v>
       </c>
       <c r="J51" t="n">
-        <v>1187</v>
+        <v>997</v>
       </c>
       <c r="K51" t="n">
-        <v>2.196</v>
+        <v>1.844</v>
       </c>
       <c r="L51" t="n">
-        <v>1099</v>
+        <v>1080</v>
       </c>
       <c r="M51" t="n">
-        <v>2.033</v>
+        <v>1.998</v>
       </c>
       <c r="N51" t="s">
         <v>330</v>
@@ -5045,22 +5041,22 @@
         <v>175</v>
       </c>
       <c r="H52" t="n">
-        <v>477363</v>
+        <v>480602</v>
       </c>
       <c r="I52" t="n">
-        <v>3.702</v>
+        <v>3.728</v>
       </c>
       <c r="J52" t="n">
-        <v>7252</v>
+        <v>8357</v>
       </c>
       <c r="K52" t="n">
-        <v>0.056</v>
+        <v>0.065</v>
       </c>
       <c r="L52" t="n">
-        <v>7783</v>
+        <v>8181</v>
       </c>
       <c r="M52" t="n">
-        <v>0.06</v>
+        <v>0.063</v>
       </c>
       <c r="N52" t="s">
         <v>337</v>
@@ -5083,7 +5079,7 @@
         <v>341</v>
       </c>
       <c r="C53" s="1" t="n">
-        <v>44006</v>
+        <v>44010</v>
       </c>
       <c r="D53" t="s">
         <v>342</v>
@@ -5093,25 +5089,25 @@
       </c>
       <c r="F53"/>
       <c r="G53" t="n">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="H53" t="n">
-        <v>591757</v>
+        <v>646195</v>
       </c>
       <c r="I53" t="n">
-        <v>16.032</v>
+        <v>17.507</v>
       </c>
       <c r="J53" t="n">
-        <v>16581</v>
+        <v>12701</v>
       </c>
       <c r="K53" t="n">
-        <v>0.449</v>
+        <v>0.344</v>
       </c>
       <c r="L53" t="n">
-        <v>17146</v>
+        <v>15429</v>
       </c>
       <c r="M53" t="n">
-        <v>0.465</v>
+        <v>0.418</v>
       </c>
       <c r="N53" t="s">
         <v>343</v>
@@ -5289,7 +5285,7 @@
         <v>367</v>
       </c>
       <c r="C57" s="1" t="n">
-        <v>44009</v>
+        <v>44010</v>
       </c>
       <c r="D57" t="s">
         <v>368</v>
@@ -5299,25 +5295,25 @@
       </c>
       <c r="F57"/>
       <c r="G57" t="n">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="H57" t="n">
-        <v>392756</v>
+        <v>395510</v>
       </c>
       <c r="I57" t="n">
-        <v>81.447</v>
+        <v>82.018</v>
       </c>
       <c r="J57" t="n">
-        <v>5321</v>
+        <v>2754</v>
       </c>
       <c r="K57" t="n">
-        <v>1.103</v>
+        <v>0.571</v>
       </c>
       <c r="L57" t="n">
-        <v>7377</v>
+        <v>7284</v>
       </c>
       <c r="M57" t="n">
-        <v>1.53</v>
+        <v>1.511</v>
       </c>
       <c r="N57" t="s">
         <v>369</v>
@@ -5340,7 +5336,7 @@
         <v>372</v>
       </c>
       <c r="C58" s="1" t="n">
-        <v>44010</v>
+        <v>44011</v>
       </c>
       <c r="D58" t="s">
         <v>373</v>
@@ -5350,22 +5346,22 @@
       </c>
       <c r="F58"/>
       <c r="G58" t="n">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="H58" t="n">
-        <v>130164</v>
+        <v>132304</v>
       </c>
       <c r="I58" t="n">
-        <v>0.631</v>
+        <v>0.642</v>
       </c>
       <c r="J58" t="n">
-        <v>3006</v>
+        <v>2140</v>
       </c>
       <c r="K58" t="n">
-        <v>0.015</v>
+        <v>0.01</v>
       </c>
       <c r="L58" t="n">
-        <v>2370</v>
+        <v>2363</v>
       </c>
       <c r="M58" t="n">
         <v>0.011</v>
@@ -5391,7 +5387,7 @@
         <v>378</v>
       </c>
       <c r="C59" s="1" t="n">
-        <v>44006</v>
+        <v>44009</v>
       </c>
       <c r="D59" t="s">
         <v>379</v>
@@ -5401,25 +5397,25 @@
       </c>
       <c r="F59"/>
       <c r="G59" t="n">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="H59" t="n">
-        <v>305073</v>
+        <v>312008</v>
       </c>
       <c r="I59" t="n">
-        <v>56.274</v>
+        <v>57.553</v>
       </c>
       <c r="J59" t="n">
-        <v>3623</v>
+        <v>619</v>
       </c>
       <c r="K59" t="n">
-        <v>0.668</v>
+        <v>0.114</v>
       </c>
       <c r="L59" t="n">
-        <v>3012</v>
+        <v>2831</v>
       </c>
       <c r="M59" t="n">
-        <v>0.556</v>
+        <v>0.522</v>
       </c>
       <c r="N59" t="s">
         <v>380</v>
@@ -5442,7 +5438,7 @@
         <v>385</v>
       </c>
       <c r="C60" s="1" t="n">
-        <v>44009</v>
+        <v>44011</v>
       </c>
       <c r="D60" t="s">
         <v>386</v>
@@ -5452,21 +5448,21 @@
       </c>
       <c r="F60"/>
       <c r="G60" t="n">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="H60"/>
       <c r="I60"/>
       <c r="J60" t="n">
-        <v>2508</v>
+        <v>3191</v>
       </c>
       <c r="K60" t="n">
-        <v>0.491</v>
+        <v>0.625</v>
       </c>
       <c r="L60" t="n">
-        <v>3604</v>
+        <v>3481</v>
       </c>
       <c r="M60" t="n">
-        <v>0.706</v>
+        <v>0.682</v>
       </c>
       <c r="N60" t="s">
         <v>387</v>
@@ -5489,7 +5485,7 @@
         <v>391</v>
       </c>
       <c r="C61" s="1" t="n">
-        <v>44010</v>
+        <v>44011</v>
       </c>
       <c r="D61" t="s">
         <v>392</v>
@@ -5499,25 +5495,25 @@
       </c>
       <c r="F61"/>
       <c r="G61" t="n">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="H61" t="n">
-        <v>1239153</v>
+        <v>1262162</v>
       </c>
       <c r="I61" t="n">
-        <v>5.61</v>
+        <v>5.714</v>
       </c>
       <c r="J61" t="n">
-        <v>25013</v>
+        <v>23009</v>
       </c>
       <c r="K61" t="n">
-        <v>0.113</v>
+        <v>0.104</v>
       </c>
       <c r="L61" t="n">
-        <v>23930</v>
+        <v>22857</v>
       </c>
       <c r="M61" t="n">
-        <v>0.108</v>
+        <v>0.103</v>
       </c>
       <c r="N61" t="s">
         <v>393</v>
@@ -5540,7 +5536,7 @@
         <v>397</v>
       </c>
       <c r="C62" s="1" t="n">
-        <v>44006</v>
+        <v>44007</v>
       </c>
       <c r="D62" t="s">
         <v>398</v>
@@ -5550,25 +5546,25 @@
       </c>
       <c r="F62"/>
       <c r="G62" t="n">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="H62" t="n">
-        <v>111197</v>
+        <v>114421</v>
       </c>
       <c r="I62" t="n">
-        <v>25.771</v>
+        <v>26.518</v>
       </c>
       <c r="J62" t="n">
-        <v>2295</v>
+        <v>3224</v>
       </c>
       <c r="K62" t="n">
-        <v>0.532</v>
+        <v>0.747</v>
       </c>
       <c r="L62" t="n">
-        <v>2359</v>
+        <v>2470</v>
       </c>
       <c r="M62" t="n">
-        <v>0.547</v>
+        <v>0.572</v>
       </c>
       <c r="N62" t="s">
         <v>399</v>
@@ -5642,7 +5638,7 @@
         <v>408</v>
       </c>
       <c r="C64" s="1" t="n">
-        <v>44010</v>
+        <v>44011</v>
       </c>
       <c r="D64" t="s">
         <v>409</v>
@@ -5652,25 +5648,25 @@
       </c>
       <c r="F64"/>
       <c r="G64" t="n">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="H64" t="n">
-        <v>242809</v>
+        <v>245315</v>
       </c>
       <c r="I64" t="n">
-        <v>7.364</v>
+        <v>7.44</v>
       </c>
       <c r="J64" t="n">
-        <v>4921</v>
+        <v>2506</v>
       </c>
       <c r="K64" t="n">
-        <v>0.149</v>
+        <v>0.076</v>
       </c>
       <c r="L64" t="n">
-        <v>3958</v>
+        <v>3871</v>
       </c>
       <c r="M64" t="n">
-        <v>0.12</v>
+        <v>0.117</v>
       </c>
       <c r="N64" t="s">
         <v>410</v>
@@ -5693,7 +5689,7 @@
         <v>414</v>
       </c>
       <c r="C65" s="1" t="n">
-        <v>44007</v>
+        <v>44009</v>
       </c>
       <c r="D65" t="s">
         <v>415</v>
@@ -5703,25 +5699,25 @@
       </c>
       <c r="F65"/>
       <c r="G65" t="n">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="H65" t="n">
-        <v>610052</v>
+        <v>636291</v>
       </c>
       <c r="I65" t="n">
-        <v>5.567</v>
+        <v>5.807</v>
       </c>
       <c r="J65" t="n">
-        <v>13994</v>
+        <v>12127</v>
       </c>
       <c r="K65" t="n">
-        <v>0.128</v>
+        <v>0.111</v>
       </c>
       <c r="L65" t="n">
-        <v>12821</v>
+        <v>12703</v>
       </c>
       <c r="M65" t="n">
-        <v>0.117</v>
+        <v>0.116</v>
       </c>
       <c r="N65" t="s">
         <v>211</v>
@@ -5744,7 +5740,7 @@
         <v>419</v>
       </c>
       <c r="C66" s="1" t="n">
-        <v>44009</v>
+        <v>44011</v>
       </c>
       <c r="D66" t="s">
         <v>420</v>
@@ -5754,25 +5750,25 @@
       </c>
       <c r="F66"/>
       <c r="G66" t="n">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="H66" t="n">
-        <v>1315933</v>
+        <v>1338503</v>
       </c>
       <c r="I66" t="n">
-        <v>34.77</v>
+        <v>35.367</v>
       </c>
       <c r="J66" t="n">
-        <v>19143</v>
+        <v>7752</v>
       </c>
       <c r="K66" t="n">
-        <v>0.506</v>
+        <v>0.205</v>
       </c>
       <c r="L66" t="n">
-        <v>17933</v>
+        <v>16976</v>
       </c>
       <c r="M66" t="n">
-        <v>0.474</v>
+        <v>0.449</v>
       </c>
       <c r="N66" t="s">
         <v>421</v>
@@ -5795,7 +5791,7 @@
         <v>424</v>
       </c>
       <c r="C67" s="1" t="n">
-        <v>44009</v>
+        <v>44010</v>
       </c>
       <c r="D67"/>
       <c r="E67"/>
@@ -5806,10 +5802,10 @@
       <c r="J67"/>
       <c r="K67"/>
       <c r="L67" t="n">
-        <v>5091</v>
+        <v>2028</v>
       </c>
       <c r="M67" t="n">
-        <v>0.135</v>
+        <v>0.054</v>
       </c>
       <c r="N67" t="s">
         <v>421</v>
@@ -5883,7 +5879,7 @@
         <v>433</v>
       </c>
       <c r="C69" s="1" t="n">
-        <v>44009</v>
+        <v>44011</v>
       </c>
       <c r="D69" t="s">
         <v>434</v>
@@ -5893,25 +5889,25 @@
       </c>
       <c r="F69"/>
       <c r="G69" t="n">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="H69" t="n">
-        <v>345691</v>
+        <v>352659</v>
       </c>
       <c r="I69" t="n">
-        <v>119.987</v>
+        <v>122.406</v>
       </c>
       <c r="J69" t="n">
-        <v>3777</v>
+        <v>3506</v>
       </c>
       <c r="K69" t="n">
-        <v>1.311</v>
+        <v>1.217</v>
       </c>
       <c r="L69" t="n">
-        <v>4000</v>
+        <v>4013</v>
       </c>
       <c r="M69" t="n">
-        <v>1.388</v>
+        <v>1.393</v>
       </c>
       <c r="N69" t="s">
         <v>435</v>
@@ -5985,7 +5981,7 @@
         <v>445</v>
       </c>
       <c r="C71" s="1" t="n">
-        <v>44010</v>
+        <v>44011</v>
       </c>
       <c r="D71" t="s">
         <v>446</v>
@@ -5995,25 +5991,25 @@
       </c>
       <c r="F71"/>
       <c r="G71" t="n">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="H71" t="n">
-        <v>19044954</v>
+        <v>19334442</v>
       </c>
       <c r="I71" t="n">
-        <v>130.503</v>
+        <v>132.487</v>
       </c>
       <c r="J71" t="n">
-        <v>337008</v>
+        <v>289488</v>
       </c>
       <c r="K71" t="n">
-        <v>2.309</v>
+        <v>1.984</v>
       </c>
       <c r="L71" t="n">
-        <v>292357</v>
+        <v>292107</v>
       </c>
       <c r="M71" t="n">
-        <v>2.003</v>
+        <v>2.002</v>
       </c>
       <c r="N71" t="s">
         <v>447</v>
@@ -6087,7 +6083,7 @@
         <v>457</v>
       </c>
       <c r="C73" s="1" t="n">
-        <v>44009</v>
+        <v>44011</v>
       </c>
       <c r="D73" t="s">
         <v>458</v>
@@ -6097,25 +6093,25 @@
       </c>
       <c r="F73"/>
       <c r="G73" t="n">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="H73" t="n">
-        <v>1500516</v>
+        <v>1591141</v>
       </c>
       <c r="I73" t="n">
-        <v>43.101</v>
+        <v>45.704</v>
       </c>
       <c r="J73" t="n">
-        <v>44275</v>
+        <v>45104</v>
       </c>
       <c r="K73" t="n">
-        <v>1.272</v>
+        <v>1.296</v>
       </c>
       <c r="L73" t="n">
-        <v>35931</v>
+        <v>38982</v>
       </c>
       <c r="M73" t="n">
-        <v>1.032</v>
+        <v>1.12</v>
       </c>
       <c r="N73" t="s">
         <v>41</v>
@@ -6138,7 +6134,7 @@
         <v>461</v>
       </c>
       <c r="C74" s="1" t="n">
-        <v>44009</v>
+        <v>44011</v>
       </c>
       <c r="D74" t="s">
         <v>462</v>
@@ -6150,25 +6146,25 @@
         <v>464</v>
       </c>
       <c r="G74" t="n">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="H74" t="n">
-        <v>76103</v>
+        <v>78238</v>
       </c>
       <c r="I74" t="n">
-        <v>4.545</v>
+        <v>4.673</v>
       </c>
       <c r="J74" t="n">
-        <v>1009</v>
+        <v>956</v>
       </c>
       <c r="K74" t="n">
-        <v>0.06</v>
+        <v>0.057</v>
       </c>
       <c r="L74" t="n">
-        <v>1014</v>
+        <v>1031</v>
       </c>
       <c r="M74" t="n">
-        <v>0.061</v>
+        <v>0.062</v>
       </c>
       <c r="N74" t="s">
         <v>465</v>
@@ -6191,7 +6187,7 @@
         <v>470</v>
       </c>
       <c r="C75" s="1" t="n">
-        <v>44009</v>
+        <v>44010</v>
       </c>
       <c r="D75" t="s">
         <v>471</v>
@@ -6203,25 +6199,25 @@
         <v>472</v>
       </c>
       <c r="G75" t="n">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="H75" t="n">
-        <v>380808</v>
+        <v>385713</v>
       </c>
       <c r="I75" t="n">
-        <v>55.963</v>
+        <v>56.684</v>
       </c>
       <c r="J75" t="n">
-        <v>5933</v>
+        <v>4905</v>
       </c>
       <c r="K75" t="n">
-        <v>0.872</v>
+        <v>0.721</v>
       </c>
       <c r="L75" t="n">
-        <v>6322</v>
+        <v>6556</v>
       </c>
       <c r="M75" t="n">
-        <v>0.929</v>
+        <v>0.963</v>
       </c>
       <c r="N75" t="s">
         <v>41</v>
@@ -6440,7 +6436,7 @@
         <v>499</v>
       </c>
       <c r="C80" s="1" t="n">
-        <v>44009</v>
+        <v>44010</v>
       </c>
       <c r="D80" t="s">
         <v>500</v>
@@ -6452,25 +6448,25 @@
         <v>502</v>
       </c>
       <c r="G80" t="n">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="H80" t="n">
-        <v>1529009</v>
+        <v>1567084</v>
       </c>
       <c r="I80" t="n">
-        <v>25.781</v>
+        <v>26.423</v>
       </c>
       <c r="J80" t="n">
-        <v>35905</v>
+        <v>38075</v>
       </c>
       <c r="K80" t="n">
-        <v>0.605</v>
+        <v>0.642</v>
       </c>
       <c r="L80" t="n">
-        <v>33629</v>
+        <v>34146</v>
       </c>
       <c r="M80" t="n">
-        <v>0.567</v>
+        <v>0.576</v>
       </c>
       <c r="N80" t="s">
         <v>501</v>
@@ -6493,7 +6489,7 @@
         <v>506</v>
       </c>
       <c r="C81" s="1" t="n">
-        <v>44010</v>
+        <v>44011</v>
       </c>
       <c r="D81" t="s">
         <v>507</v>
@@ -6503,25 +6499,25 @@
       </c>
       <c r="F81"/>
       <c r="G81" t="n">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="H81" t="n">
-        <v>1231829</v>
+        <v>1240949</v>
       </c>
       <c r="I81" t="n">
-        <v>24.027</v>
+        <v>24.205</v>
       </c>
       <c r="J81" t="n">
-        <v>7915</v>
+        <v>9120</v>
       </c>
       <c r="K81" t="n">
-        <v>0.154</v>
+        <v>0.178</v>
       </c>
       <c r="L81" t="n">
-        <v>10977</v>
+        <v>11279</v>
       </c>
       <c r="M81" t="n">
-        <v>0.214</v>
+        <v>0.22</v>
       </c>
       <c r="N81" t="s">
         <v>508</v>
@@ -6651,22 +6647,22 @@
         <v>154</v>
       </c>
       <c r="H84" t="n">
-        <v>562909</v>
+        <v>564747</v>
       </c>
       <c r="I84" t="n">
-        <v>65.041</v>
+        <v>65.254</v>
       </c>
       <c r="J84" t="n">
-        <v>4993</v>
+        <v>5714</v>
       </c>
       <c r="K84" t="n">
-        <v>0.577</v>
+        <v>0.66</v>
       </c>
       <c r="L84" t="n">
-        <v>7693</v>
+        <v>7953</v>
       </c>
       <c r="M84" t="n">
-        <v>0.889</v>
+        <v>0.919</v>
       </c>
       <c r="N84" t="s">
         <v>529</v>
@@ -6740,7 +6736,7 @@
         <v>540</v>
       </c>
       <c r="C86" s="1" t="n">
-        <v>44009</v>
+        <v>44011</v>
       </c>
       <c r="D86" t="s">
         <v>541</v>
@@ -6750,22 +6746,18 @@
       </c>
       <c r="F86"/>
       <c r="G86" t="n">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="H86" t="n">
-        <v>305324</v>
+        <v>309371</v>
       </c>
       <c r="I86" t="n">
-        <v>4.374</v>
-      </c>
-      <c r="J86" t="n">
-        <v>2502</v>
-      </c>
-      <c r="K86" t="n">
-        <v>0.036</v>
-      </c>
+        <v>4.432</v>
+      </c>
+      <c r="J86"/>
+      <c r="K86"/>
       <c r="L86" t="n">
-        <v>2125</v>
+        <v>2078</v>
       </c>
       <c r="M86" t="n">
         <v>0.03</v>
@@ -6893,7 +6885,7 @@
         <v>560</v>
       </c>
       <c r="C89" s="1" t="n">
-        <v>44010</v>
+        <v>44011</v>
       </c>
       <c r="D89" t="s">
         <v>561</v>
@@ -6903,25 +6895,25 @@
       </c>
       <c r="F89"/>
       <c r="G89" t="n">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="H89" t="n">
-        <v>3231835</v>
+        <v>3331158</v>
       </c>
       <c r="I89" t="n">
-        <v>38.32</v>
+        <v>39.497</v>
       </c>
       <c r="J89" t="n">
-        <v>45213</v>
+        <v>51014</v>
       </c>
       <c r="K89" t="n">
-        <v>0.536</v>
+        <v>0.605</v>
       </c>
       <c r="L89" t="n">
-        <v>40942</v>
+        <v>49215</v>
       </c>
       <c r="M89" t="n">
-        <v>0.485</v>
+        <v>0.584</v>
       </c>
       <c r="N89" t="s">
         <v>562</v>
@@ -6944,7 +6936,7 @@
         <v>566</v>
       </c>
       <c r="C90" s="1" t="n">
-        <v>44008</v>
+        <v>44010</v>
       </c>
       <c r="D90" t="s">
         <v>567</v>
@@ -6956,25 +6948,25 @@
         <v>569</v>
       </c>
       <c r="G90" t="n">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="H90" t="n">
-        <v>158509</v>
+        <v>164225</v>
       </c>
       <c r="I90" t="n">
-        <v>3.465</v>
+        <v>3.59</v>
       </c>
       <c r="J90" t="n">
-        <v>2868</v>
+        <v>2330</v>
       </c>
       <c r="K90" t="n">
-        <v>0.063</v>
+        <v>0.051</v>
       </c>
       <c r="L90" t="n">
-        <v>2573</v>
+        <v>2652</v>
       </c>
       <c r="M90" t="n">
-        <v>0.056</v>
+        <v>0.058</v>
       </c>
       <c r="N90" t="s">
         <v>568</v>
@@ -6997,7 +6989,7 @@
         <v>573</v>
       </c>
       <c r="C91" s="1" t="n">
-        <v>44010</v>
+        <v>44011</v>
       </c>
       <c r="D91" t="s">
         <v>574</v>
@@ -7007,25 +6999,25 @@
       </c>
       <c r="F91"/>
       <c r="G91" t="n">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="H91" t="n">
-        <v>641911</v>
+        <v>649150</v>
       </c>
       <c r="I91" t="n">
-        <v>14.678</v>
+        <v>14.843</v>
       </c>
       <c r="J91" t="n">
-        <v>9945</v>
+        <v>7239</v>
       </c>
       <c r="K91" t="n">
-        <v>0.227</v>
+        <v>0.166</v>
       </c>
       <c r="L91" t="n">
-        <v>11245</v>
+        <v>11366</v>
       </c>
       <c r="M91" t="n">
-        <v>0.257</v>
+        <v>0.26</v>
       </c>
       <c r="N91" t="s">
         <v>575</v>
@@ -7099,7 +7091,7 @@
         <v>585</v>
       </c>
       <c r="C93" s="1" t="n">
-        <v>44009</v>
+        <v>44010</v>
       </c>
       <c r="D93" t="s">
         <v>586</v>
@@ -7111,25 +7103,25 @@
         <v>587</v>
       </c>
       <c r="G93" t="n">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="H93" t="n">
-        <v>4797763</v>
+        <v>4852547</v>
       </c>
       <c r="I93" t="n">
-        <v>70.674</v>
+        <v>71.481</v>
       </c>
       <c r="J93" t="n">
-        <v>75495</v>
+        <v>54311</v>
       </c>
       <c r="K93" t="n">
-        <v>1.112</v>
+        <v>0.8</v>
       </c>
       <c r="L93" t="n">
-        <v>70119</v>
+        <v>71735</v>
       </c>
       <c r="M93" t="n">
-        <v>1.033</v>
+        <v>1.057</v>
       </c>
       <c r="N93" t="s">
         <v>582</v>
@@ -7203,7 +7195,7 @@
         <v>596</v>
       </c>
       <c r="C95" s="1" t="n">
-        <v>44009</v>
+        <v>44010</v>
       </c>
       <c r="D95" t="s">
         <v>597</v>
@@ -7213,25 +7205,25 @@
       </c>
       <c r="F95"/>
       <c r="G95" t="n">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="H95" t="n">
-        <v>30401644</v>
+        <v>30988013</v>
       </c>
       <c r="I95" t="n">
-        <v>91.847</v>
+        <v>93.619</v>
       </c>
       <c r="J95" t="n">
-        <v>590877</v>
+        <v>586369</v>
       </c>
       <c r="K95" t="n">
-        <v>1.785</v>
+        <v>1.771</v>
       </c>
       <c r="L95" t="n">
-        <v>546033</v>
+        <v>556632</v>
       </c>
       <c r="M95" t="n">
-        <v>1.65</v>
+        <v>1.682</v>
       </c>
       <c r="N95" t="s">
         <v>598</v>

</xml_diff>

<commit_message>
Updated testing data for 2020-07-01
</commit_message>
<xml_diff>
--- a/public/data/testing/covid-testing-latest-data-source-details.xlsx
+++ b/public/data/testing/covid-testing-latest-data-source-details.xlsx
@@ -5808,19 +5808,33 @@
       <c r="C67" s="1" t="n">
         <v>44013</v>
       </c>
-      <c r="D67"/>
-      <c r="E67"/>
+      <c r="D67" t="s">
+        <v>418</v>
+      </c>
+      <c r="E67" t="s">
+        <v>419</v>
+      </c>
       <c r="F67"/>
-      <c r="G67"/>
-      <c r="H67"/>
-      <c r="I67"/>
-      <c r="J67"/>
-      <c r="K67"/>
+      <c r="G67" t="n">
+        <v>116</v>
+      </c>
+      <c r="H67" t="n">
+        <v>1546510</v>
+      </c>
+      <c r="I67" t="n">
+        <v>40.863</v>
+      </c>
+      <c r="J67" t="n">
+        <v>25104</v>
+      </c>
+      <c r="K67" t="n">
+        <v>0.663</v>
+      </c>
       <c r="L67" t="n">
-        <v>0</v>
+        <v>20980</v>
       </c>
       <c r="M67" t="n">
-        <v>0</v>
+        <v>0.554</v>
       </c>
       <c r="N67" t="s">
         <v>419</v>

</xml_diff>

<commit_message>
Updated testing data for 2020-07-04
</commit_message>
<xml_diff>
--- a/public/data/testing/covid-testing-latest-data-source-details.xlsx
+++ b/public/data/testing/covid-testing-latest-data-source-details.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="628" uniqueCount="628">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="627" uniqueCount="627">
   <si>
     <t xml:space="preserve">ISO code</t>
   </si>
@@ -71,7 +71,7 @@
     <t xml:space="preserve">Argentina - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.argentina.gob.ar/sites/default/files/3-07-20-reporte-matutino-covid-19.pdf</t>
+    <t xml:space="preserve">https://www.argentina.gob.ar/sites/default/files/4-07-20-reporte-matutino-covid-19.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">Government of Argentina</t>
@@ -112,7 +112,7 @@
     <t xml:space="preserve">Austria - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200703151001/https://www.sozialministerium.at/Informationen-zum-Coronavirus/Neuartiges-Coronavirus-(2019-nCov).html</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200704151529/https://www.sozialministerium.at/Informationen-zum-Coronavirus/Neuartiges-Coronavirus-(2019-nCov).html</t>
   </si>
   <si>
     <t xml:space="preserve">Austrian Ministry for Health</t>
@@ -139,7 +139,7 @@
     <t xml:space="preserve">Bahrain - units unclear</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200703151004/https://www.moh.gov.bh/COVID19</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200704151532/https://www.moh.gov.bh/COVID19</t>
   </si>
   <si>
     <t xml:space="preserve">Ministry of Health</t>
@@ -233,7 +233,7 @@
     <t xml:space="preserve">Bolivia - units unclear</t>
   </si>
   <si>
-    <t xml:space="preserve">https://minsalud.gob.bo/4356-ministerio-de-salud-reporta-1-008-nuevos-contagios-de-coronavirus-y-el-numero-de-recuperados-alcanza-los-9-764</t>
+    <t xml:space="preserve">https://minsalud.gob.bo/4360-bolivia-acumula-35-528-contagios-de-covid-19-tras-registrar-record-de-1-301-nuevos-infectados</t>
   </si>
   <si>
     <t xml:space="preserve">https://www.minsalud.gob.bo/</t>
@@ -279,7 +279,7 @@
     <t xml:space="preserve">Bulgaria - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200703151010/https://coronavirus.bg/</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200704151537/https://coronavirus.bg/</t>
   </si>
   <si>
     <t xml:space="preserve">Bulgaria COVID-10 Information Portal</t>
@@ -301,7 +301,7 @@
     <t xml:space="preserve">Canada - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200703151011/https://www.canada.ca/en/public-health/services/diseases/2019-novel-coronavirus-infection.html</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200704151538/https://www.canada.ca/en/public-health/services/diseases/2019-novel-coronavirus-infection.html</t>
   </si>
   <si>
     <t xml:space="preserve">Government of Canada</t>
@@ -389,7 +389,7 @@
     <t xml:space="preserve">Croatia - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200703151017/https://www.koronavirus.hr/najnovije/ukupno-dosad-382-zarazene-osobe-u-hrvatskoj/35</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200704151542/https://www.koronavirus.hr/najnovije/ukupno-dosad-382-zarazene-osobe-u-hrvatskoj/35</t>
   </si>
   <si>
     <t xml:space="preserve">Government of Croatia</t>
@@ -485,7 +485,7 @@
     <t xml:space="preserve">The Government of Ecuador publish daily updates in the form of situation reports and summary infographics. These report the number and status of confirmed cases, deaths and number of samples tested. This data is available daily from 18th March; reports and infographics prior to this date do not include the number of samples tested. But all figures are dated cumulative since 29th February.
 The source reports the number of confirmed ('confirmados') and negative ('descartados') cases, which we sum to get the number of cases tested.
 On 24 April 2020, the number of tests suddenly jumped from 23,383 to 45,857, because of what we assume to be the inclusion of rapid tests ("pruebas rápidas"), as made clear by the subsequent infographic published on 27 April. We therefore do not include the 24 April infographic in our time series; and from 27 April onwards, we include only PCR tests.
-On 11 May 2020, the Government of Ecuador published a [report](https://www.gestionderiesgos.gob.ec/wp-content/uploads/2020/05/BP-VARIACIONES-INFOGRAFIA-No.-074-11052020.pdf) detailing "a reclassification of the records by identity card of the persons and not by the number of tests that have been carried out" (via google translate). This suggests the government is moving towards reporting figures on the number of people tested, where previously they reported the number of cases tested. The reclassification partially explains the fall in the cumulative total after 4 May 2020.
+On 11 May 2020, the Government of Ecuador published a [report](https://www.gestionderiesgos.gob.ec/wp-content/uploads/2020/05/BP-VARIACIONES-INFOGRAFIA-No.-074-11052020.pdf) detailing "a reclassification of the records by identity card of the persons and not by the number of tests that have been carried out". This suggests the government is moving towards reporting figures on the number of people tested, where previously they reported the number of cases tested. The reclassification partially explains the fall in the cumulative total after 4 May 2020.
 The most recently published situation report is dated 24th May, as of 26th May.</t>
   </si>
   <si>
@@ -691,7 +691,7 @@
     <t xml:space="preserve">Greece - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://eody.gov.gr/wp-content/uploads/2020/07/covid-gr-daily-report-20200702.pdf</t>
+    <t xml:space="preserve">https://eody.gov.gr/covid-gr-daily-report-20200704/</t>
   </si>
   <si>
     <t xml:space="preserve">National Organization of Public Health</t>
@@ -833,7 +833,7 @@
     <t xml:space="preserve">Iran - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">http://web.archive.org/web/20200630133927/http://irangov.ir/detail/342192</t>
+    <t xml:space="preserve">http://irangov.ir/detail/342430</t>
   </si>
   <si>
     <t xml:space="preserve">Government of Iran</t>
@@ -926,7 +926,7 @@
     <t xml:space="preserve">Japan - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.mhlw.go.jp/stf/newpage_12198.html</t>
+    <t xml:space="preserve">https://www.mhlw.go.jp/stf/newpage_12236.html</t>
   </si>
   <si>
     <t xml:space="preserve">Ministry of Health, Labor and Welfare Press Release</t>
@@ -949,10 +949,10 @@
     <t xml:space="preserve">Japan - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.mhlw.go.jp/content/10906000/000645672.pdf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The cumulative total reported in the press release (684,802) does not sum to the cumulative total calculated from the weekly and daily figures reported by the MOH. See: https://www.mhlw.go.jp/content/10906000/000645672.pdf</t>
+    <t xml:space="preserve">https://www.mhlw.go.jp/content/10906000/000646181.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The cumulative total reported in the press release (701,541) does not sum to the cumulative total calculated from the weekly and daily figures reported by the MOH. See: https://www.mhlw.go.jp/content/10906000/000646181.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">On 11th April 2020, the MOH started providing a daily time series on the "Implementation status of PCR tests for new coronavirus in Japan (based on the date on which results were determined" (via Google translate). 
@@ -1006,7 +1006,7 @@
     <t xml:space="preserve">Kuwait - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/KUWAIT_MOH/status/1278672859569819649/photo/2</t>
+    <t xml:space="preserve">https://twitter.com/KUWAIT_MOH/status/1278998384817385472/photo/2</t>
   </si>
   <si>
     <t xml:space="preserve">Kuwait Ministry of Health</t>
@@ -1058,7 +1058,7 @@
     <t xml:space="preserve">Luxembourg - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200702185357/https://gouvernement.lu/en/dossiers.gouv_msan%2Ben%2Bdossiers%2B2020%2Bcorona-virus.html</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200704165139/https://gouvernement.lu/en/dossiers.gouv_msan%2Ben%2Bdossiers%2B2020%2Bcorona-virus.html</t>
   </si>
   <si>
     <t xml:space="preserve">Luxembourg Government situation update</t>
@@ -1079,7 +1079,7 @@
     <t xml:space="preserve">Malaysia - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">http://covid-19.moh.gov.my/terkini/072020/situasi-terkini-02-julai-2020</t>
+    <t xml:space="preserve">http://covid-19.moh.gov.my/terkini/072020/situasi-terkini-03-julai-2020</t>
   </si>
   <si>
     <t xml:space="preserve">Ministry of Health Malaysia</t>
@@ -1104,7 +1104,7 @@
     <t xml:space="preserve">Maldives - samples tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/HPA_MV/status/1278735503207120897/photo/1</t>
+    <t xml:space="preserve">https://twitter.com/HPA_MV/status/1279097457494970377/photo/1</t>
   </si>
   <si>
     <t xml:space="preserve">Maldives Health Protection Agency</t>
@@ -1127,7 +1127,7 @@
     <t xml:space="preserve">Malta - samples tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.facebook.com/sahhagovmt/photos/a.102565371462015/174534604265091</t>
+    <t xml:space="preserve">https://www.facebook.com/sahhagovmt/photos/a.102565371462015/174913164227235/</t>
   </si>
   <si>
     <t xml:space="preserve">Malta Ministry of Health</t>
@@ -1170,7 +1170,7 @@
     <t xml:space="preserve">Morocco - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/Ministere_Sante/status/1278740249896722433</t>
+    <t xml:space="preserve">https://twitter.com/Ministere_Sante/status/1279104329266462722/photo/1</t>
   </si>
   <si>
     <t xml:space="preserve">Morocco Ministry of Health</t>
@@ -1270,7 +1270,7 @@
     <t xml:space="preserve">Nigeria - samples tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200703151316/https://covid19.ncdc.gov.ng/</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200704151638/https://covid19.ncdc.gov.ng/</t>
   </si>
   <si>
     <t xml:space="preserve">Nigeria Centre for Disease Control</t>
@@ -1315,7 +1315,7 @@
     <t xml:space="preserve">Oman - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/OmanVSCovid19/status/1278619811820568577</t>
+    <t xml:space="preserve">https://twitter.com/OmanVSCovid19/status/1278977212365049858</t>
   </si>
   <si>
     <t xml:space="preserve">Oman Ministry of Health</t>
@@ -1334,7 +1334,7 @@
     <t xml:space="preserve">Pakistan - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200703151318/http://www.covid.gov.pk/</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200704151639/http://www.covid.gov.pk/</t>
   </si>
   <si>
     <t xml:space="preserve">Government of Pakistan</t>
@@ -1387,7 +1387,7 @@
     <t xml:space="preserve">Peru - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.gob.pe/institucion/minsa/noticias/189644-minsa-casos-confirmados-por-coronavirus-covid-19-ascienden-a-292-004-en-el-peru-comunicado-n-155</t>
+    <t xml:space="preserve">https://www.gob.pe/institucion/minsa/noticias/189954-minsa-casos-confirmados-por-coronavirus-covid-19-ascienden-a-295-599-en-el-peru-comunicado-n-156</t>
   </si>
   <si>
     <t xml:space="preserve">Ministry of Health, Government of Peru</t>
@@ -1428,7 +1428,7 @@
     <t xml:space="preserve">Poland - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/MZ_GOV_PL/status/1278614392225927168</t>
+    <t xml:space="preserve">https://twitter.com/MZ_GOV_PL/status/1278976776300105728</t>
   </si>
   <si>
     <t xml:space="preserve">Poland Ministry of Health</t>
@@ -1492,7 +1492,7 @@
     <t xml:space="preserve">Romania - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://gov.ro/ro/media/comunicate/buletin-de-presa-3-iulie-2020-ora-13-00&amp;page=1</t>
+    <t xml:space="preserve">https://gov.ro/ro/media/comunicate/buletin-de-presa-4-iulie-2020-ora-13-00&amp;page=1</t>
   </si>
   <si>
     <t xml:space="preserve">Ministry of Internal Affairs</t>
@@ -1510,7 +1510,7 @@
     <t xml:space="preserve">Russia - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://rospotrebnadzor.ru/about/info/news/news_details.php?ELEMENT_ID=14825</t>
+    <t xml:space="preserve">https://rospotrebnadzor.ru/about/info/news/news_details.php?ELEMENT_ID=14837</t>
   </si>
   <si>
     <t xml:space="preserve">Government of the Russian Federation</t>
@@ -1621,7 +1621,7 @@
 No other information is given on how the data was collected and aggregated, and whether coverage was complete.</t>
   </si>
   <si>
-    <t xml:space="preserve">Singapore - swabs tested</t>
+    <t xml:space="preserve">Singapore - samples tested</t>
   </si>
   <si>
     <t xml:space="preserve">https://web.archive.org/web/20200701194830/https://www.moh.gov.sg/covid-19</t>
@@ -1636,7 +1636,7 @@
     <t xml:space="preserve">Slovakia - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200703151331/https://korona.gov.sk/</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200704151649/https://korona.gov.sk/</t>
   </si>
   <si>
     <t xml:space="preserve">National Health Information Centre</t>
@@ -1710,7 +1710,7 @@
     <t xml:space="preserve">South Korea - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.cdc.go.kr/board/board.es?mid=&amp;bid=0030&amp;act=view&amp;list_no=367702&amp;tag=&amp;nPage=1</t>
+    <t xml:space="preserve">https://www.cdc.go.kr/board/board.es?mid=&amp;bid=0030&amp;act=view&amp;list_no=367707&amp;tag=&amp;nPage=1</t>
   </si>
   <si>
     <t xml:space="preserve">South Korea CDC</t>
@@ -1756,7 +1756,7 @@
     <t xml:space="preserve">Sweden - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.folkhalsomyndigheten.se/globalassets/statistik-uppfoljning/smittsamma-sjukdomar/veckorapporter-covid-19/2020/covid-19-veckorapport-vecka-25-final.pdf</t>
+    <t xml:space="preserve">https://www.folkhalsomyndigheten.se/smittskydd-beredskap/utbrott/aktuella-utbrott/covid-19/antal-individer-som-har-testats-for-covid-19/</t>
   </si>
   <si>
     <t xml:space="preserve">Swedish Public Health Agency</t>
@@ -1766,9 +1766,6 @@
   </si>
   <si>
     <t xml:space="preserve">https://www.folkhalsomyndigheten.se/folkhalsorapportering-statistik/statistik-a-o/sjukdomsstatistik/covid-19-veckorapporter/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">People tested</t>
   </si>
   <si>
     <t xml:space="preserve">The Swedish Public Health Agency provides weekly reports on COVID-19 on the number of people tested. 
@@ -1823,7 +1820,7 @@
     <t xml:space="preserve">Thailand - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200703151409/https://ddc.moph.go.th/viralpneumonia/eng/index.php</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200704151745/https://ddc.moph.go.th/viralpneumonia/eng/index.php</t>
   </si>
   <si>
     <t xml:space="preserve">Department of Disease Control</t>
@@ -1906,7 +1903,7 @@
     <t xml:space="preserve">Turkey - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200702190545/https://covid19.saglik.gov.tr/</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200704151748/https://covid19.saglik.gov.tr/</t>
   </si>
   <si>
     <t xml:space="preserve">Turkish Ministry of Health</t>
@@ -1927,7 +1924,7 @@
     <t xml:space="preserve">Uganda - samples tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/MinofHealthUG/status/1278247741232209920</t>
+    <t xml:space="preserve">https://twitter.com/MinofHealthUG/status/1278977810720264193</t>
   </si>
   <si>
     <t xml:space="preserve">Press Release from the Office of the Director General</t>
@@ -2006,10 +2003,10 @@
     <t xml:space="preserve">USA</t>
   </si>
   <si>
-    <t xml:space="preserve">United States - tests performed (CDC)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200703151414/https://www.cdc.gov/coronavirus/2019-ncov/cases-updates/testing-in-us.html</t>
+    <t xml:space="preserve">United States - tests performed (CDC) (incl. non-PCR)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://web.archive.org/web/20200704151751/https://www.cdc.gov/coronavirus/2019-ncov/cases-updates/testing-in-us.html</t>
   </si>
   <si>
     <t xml:space="preserve">United States CDC</t>
@@ -2032,7 +2029,7 @@
 The CDC previously published a time series that only covered public health labs and did not include private lab tests, which were occurring in significant numbers. Daily figures were provided since 18 January. This data is still visible on [this page of the CDC website](https://www.cdc.gov/coronavirus/2019-ncov/cases-updates/previous-testing-in-us.html).</t>
   </si>
   <si>
-    <t xml:space="preserve">United States - units unclear</t>
+    <t xml:space="preserve">United States - units unclear (incl. non-PCR)</t>
   </si>
   <si>
     <t xml:space="preserve">https://covidtracking.com/api/us/daily.csv</t>
@@ -2512,7 +2509,7 @@
         <v>18</v>
       </c>
       <c r="C2" s="1" t="n">
-        <v>44015</v>
+        <v>44016</v>
       </c>
       <c r="D2" t="s">
         <v>19</v>
@@ -2522,25 +2519,25 @@
       </c>
       <c r="F2"/>
       <c r="G2" t="n">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="H2" t="n">
-        <v>381431</v>
+        <v>390382</v>
       </c>
       <c r="I2" t="n">
-        <v>8.44</v>
+        <v>8.638</v>
       </c>
       <c r="J2" t="n">
-        <v>9323</v>
+        <v>8951</v>
       </c>
       <c r="K2" t="n">
-        <v>0.206</v>
+        <v>0.198</v>
       </c>
       <c r="L2" t="n">
-        <v>8959</v>
+        <v>8764</v>
       </c>
       <c r="M2" t="n">
-        <v>0.198</v>
+        <v>0.194</v>
       </c>
       <c r="N2" t="s">
         <v>20</v>
@@ -2614,7 +2611,7 @@
         <v>31</v>
       </c>
       <c r="C4" s="1" t="n">
-        <v>44015</v>
+        <v>44016</v>
       </c>
       <c r="D4" t="s">
         <v>32</v>
@@ -2624,25 +2621,25 @@
       </c>
       <c r="F4"/>
       <c r="G4" t="n">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="H4" t="n">
-        <v>635505</v>
+        <v>642679</v>
       </c>
       <c r="I4" t="n">
-        <v>70.561</v>
+        <v>71.358</v>
       </c>
       <c r="J4" t="n">
-        <v>6805</v>
+        <v>7174</v>
       </c>
       <c r="K4" t="n">
-        <v>0.756</v>
+        <v>0.797</v>
       </c>
       <c r="L4" t="n">
-        <v>6438</v>
+        <v>6455</v>
       </c>
       <c r="M4" t="n">
-        <v>0.715</v>
+        <v>0.717</v>
       </c>
       <c r="N4" t="s">
         <v>34</v>
@@ -2665,7 +2662,7 @@
         <v>39</v>
       </c>
       <c r="C5" s="1" t="n">
-        <v>44015</v>
+        <v>44016</v>
       </c>
       <c r="D5" t="s">
         <v>40</v>
@@ -2675,25 +2672,25 @@
       </c>
       <c r="F5"/>
       <c r="G5" t="n">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="H5" t="n">
-        <v>574105</v>
+        <v>584070</v>
       </c>
       <c r="I5" t="n">
-        <v>337.395</v>
+        <v>343.251</v>
       </c>
       <c r="J5" t="n">
-        <v>9740</v>
+        <v>9965</v>
       </c>
       <c r="K5" t="n">
-        <v>5.724</v>
+        <v>5.856</v>
       </c>
       <c r="L5" t="n">
-        <v>8950</v>
+        <v>8996</v>
       </c>
       <c r="M5" t="n">
-        <v>5.26</v>
+        <v>5.287</v>
       </c>
       <c r="N5" t="s">
         <v>42</v>
@@ -2814,7 +2811,7 @@
         <v>60</v>
       </c>
       <c r="C8" s="1" t="n">
-        <v>44013</v>
+        <v>44014</v>
       </c>
       <c r="D8" t="s">
         <v>61</v>
@@ -2824,25 +2821,25 @@
       </c>
       <c r="F8"/>
       <c r="G8" t="n">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="H8" t="n">
-        <v>987972</v>
+        <v>997812</v>
       </c>
       <c r="I8" t="n">
-        <v>85.246</v>
+        <v>86.095</v>
       </c>
       <c r="J8" t="n">
-        <v>9599</v>
+        <v>8653</v>
       </c>
       <c r="K8" t="n">
-        <v>0.828</v>
+        <v>0.747</v>
       </c>
       <c r="L8" t="n">
-        <v>9228</v>
+        <v>9027</v>
       </c>
       <c r="M8" t="n">
-        <v>0.796</v>
+        <v>0.779</v>
       </c>
       <c r="N8" t="s">
         <v>62</v>
@@ -2865,7 +2862,7 @@
         <v>67</v>
       </c>
       <c r="C9" s="1" t="n">
-        <v>44013</v>
+        <v>44014</v>
       </c>
       <c r="D9" t="s">
         <v>68</v>
@@ -2875,25 +2872,25 @@
       </c>
       <c r="F9"/>
       <c r="G9" t="n">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="H9" t="n">
-        <v>77413</v>
+        <v>79567</v>
       </c>
       <c r="I9" t="n">
-        <v>6.632</v>
+        <v>6.816</v>
       </c>
       <c r="J9" t="n">
-        <v>1947</v>
+        <v>2154</v>
       </c>
       <c r="K9" t="n">
-        <v>0.167</v>
+        <v>0.185</v>
       </c>
       <c r="L9" t="n">
-        <v>1781</v>
+        <v>1853</v>
       </c>
       <c r="M9" t="n">
-        <v>0.153</v>
+        <v>0.159</v>
       </c>
       <c r="N9" t="s">
         <v>41</v>
@@ -2961,7 +2958,7 @@
         <v>81</v>
       </c>
       <c r="C11" s="1" t="n">
-        <v>44015</v>
+        <v>44016</v>
       </c>
       <c r="D11" t="s">
         <v>82</v>
@@ -2971,25 +2968,25 @@
       </c>
       <c r="F11"/>
       <c r="G11" t="n">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="H11" t="n">
-        <v>147524</v>
+        <v>150062</v>
       </c>
       <c r="I11" t="n">
-        <v>21.231</v>
+        <v>21.596</v>
       </c>
       <c r="J11" t="n">
-        <v>3155</v>
+        <v>2538</v>
       </c>
       <c r="K11" t="n">
-        <v>0.454</v>
+        <v>0.365</v>
       </c>
       <c r="L11" t="n">
-        <v>2747</v>
+        <v>2717</v>
       </c>
       <c r="M11" t="n">
-        <v>0.395</v>
+        <v>0.391</v>
       </c>
       <c r="N11" t="s">
         <v>84</v>
@@ -3012,7 +3009,7 @@
         <v>88</v>
       </c>
       <c r="C12" s="1" t="n">
-        <v>44015</v>
+        <v>44016</v>
       </c>
       <c r="D12" t="s">
         <v>89</v>
@@ -3022,21 +3019,25 @@
       </c>
       <c r="F12"/>
       <c r="G12" t="n">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="H12" t="n">
-        <v>2848168</v>
+        <v>2885670</v>
       </c>
       <c r="I12" t="n">
-        <v>75.464</v>
-      </c>
-      <c r="J12"/>
-      <c r="K12"/>
+        <v>76.457</v>
+      </c>
+      <c r="J12" t="n">
+        <v>37502</v>
+      </c>
+      <c r="K12" t="n">
+        <v>0.994</v>
+      </c>
       <c r="L12" t="n">
-        <v>41412</v>
+        <v>41072</v>
       </c>
       <c r="M12" t="n">
-        <v>1.097</v>
+        <v>1.088</v>
       </c>
       <c r="N12" t="s">
         <v>90</v>
@@ -3059,7 +3060,7 @@
         <v>95</v>
       </c>
       <c r="C13" s="1" t="n">
-        <v>44014</v>
+        <v>44015</v>
       </c>
       <c r="D13" t="s">
         <v>96</v>
@@ -3071,25 +3072,25 @@
         <v>97</v>
       </c>
       <c r="G13" t="n">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="H13" t="n">
-        <v>1131008</v>
+        <v>1146593</v>
       </c>
       <c r="I13" t="n">
-        <v>59.165</v>
+        <v>59.98</v>
       </c>
       <c r="J13" t="n">
-        <v>10831</v>
+        <v>15585</v>
       </c>
       <c r="K13" t="n">
-        <v>0.567</v>
+        <v>0.815</v>
       </c>
       <c r="L13" t="n">
-        <v>15132</v>
+        <v>14752</v>
       </c>
       <c r="M13" t="n">
-        <v>0.792</v>
+        <v>0.772</v>
       </c>
       <c r="N13" t="s">
         <v>98</v>
@@ -3163,7 +3164,7 @@
         <v>109</v>
       </c>
       <c r="C15" s="1" t="n">
-        <v>44013</v>
+        <v>44014</v>
       </c>
       <c r="D15" t="s">
         <v>110</v>
@@ -3173,25 +3174,25 @@
       </c>
       <c r="F15"/>
       <c r="G15" t="n">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="H15" t="n">
-        <v>33401</v>
+        <v>34660</v>
       </c>
       <c r="I15" t="n">
-        <v>6.557</v>
+        <v>6.804</v>
       </c>
       <c r="J15" t="n">
-        <v>853</v>
+        <v>1259</v>
       </c>
       <c r="K15" t="n">
-        <v>0.167</v>
+        <v>0.247</v>
       </c>
       <c r="L15" t="n">
-        <v>737</v>
+        <v>817</v>
       </c>
       <c r="M15" t="n">
-        <v>0.145</v>
+        <v>0.16</v>
       </c>
       <c r="N15" t="s">
         <v>111</v>
@@ -3214,7 +3215,7 @@
         <v>115</v>
       </c>
       <c r="C16" s="1" t="n">
-        <v>44015</v>
+        <v>44016</v>
       </c>
       <c r="D16" t="s">
         <v>116</v>
@@ -3224,25 +3225,25 @@
       </c>
       <c r="F16"/>
       <c r="G16" t="n">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="H16" t="n">
-        <v>82902</v>
+        <v>84166</v>
       </c>
       <c r="I16" t="n">
-        <v>20.194</v>
+        <v>20.502</v>
       </c>
       <c r="J16" t="n">
-        <v>1465</v>
+        <v>1264</v>
       </c>
       <c r="K16" t="n">
-        <v>0.357</v>
+        <v>0.308</v>
       </c>
       <c r="L16" t="n">
-        <v>1037</v>
+        <v>1077</v>
       </c>
       <c r="M16" t="n">
-        <v>0.253</v>
+        <v>0.262</v>
       </c>
       <c r="N16" t="s">
         <v>117</v>
@@ -3265,7 +3266,7 @@
         <v>122</v>
       </c>
       <c r="C17" s="1" t="n">
-        <v>44014</v>
+        <v>44015</v>
       </c>
       <c r="D17" t="s">
         <v>123</v>
@@ -3277,25 +3278,25 @@
         <v>125</v>
       </c>
       <c r="G17" t="n">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="H17" t="n">
-        <v>178062</v>
+        <v>180697</v>
       </c>
       <c r="I17" t="n">
-        <v>15.721</v>
+        <v>15.953</v>
       </c>
       <c r="J17" t="n">
-        <v>2690</v>
+        <v>2635</v>
       </c>
       <c r="K17" t="n">
-        <v>0.237</v>
+        <v>0.233</v>
       </c>
       <c r="L17" t="n">
-        <v>2341</v>
+        <v>2391</v>
       </c>
       <c r="M17" t="n">
-        <v>0.207</v>
+        <v>0.211</v>
       </c>
       <c r="N17" t="s">
         <v>124</v>
@@ -3318,7 +3319,7 @@
         <v>130</v>
       </c>
       <c r="C18" s="1" t="n">
-        <v>44013</v>
+        <v>44015</v>
       </c>
       <c r="D18" t="s">
         <v>131</v>
@@ -3328,25 +3329,25 @@
       </c>
       <c r="F18"/>
       <c r="G18" t="n">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="H18" t="n">
-        <v>560189</v>
+        <v>570080</v>
       </c>
       <c r="I18" t="n">
-        <v>52.31</v>
+        <v>53.234</v>
       </c>
       <c r="J18" t="n">
-        <v>4100</v>
+        <v>4840</v>
       </c>
       <c r="K18" t="n">
-        <v>0.383</v>
+        <v>0.452</v>
       </c>
       <c r="L18" t="n">
-        <v>3793</v>
+        <v>3981</v>
       </c>
       <c r="M18" t="n">
-        <v>0.354</v>
+        <v>0.372</v>
       </c>
       <c r="N18" t="s">
         <v>41</v>
@@ -3524,7 +3525,7 @@
         <v>154</v>
       </c>
       <c r="C22" s="1" t="n">
-        <v>44014</v>
+        <v>44015</v>
       </c>
       <c r="D22" t="s">
         <v>155</v>
@@ -3534,25 +3535,25 @@
       </c>
       <c r="F22"/>
       <c r="G22" t="n">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="H22" t="n">
-        <v>108539</v>
+        <v>108802</v>
       </c>
       <c r="I22" t="n">
-        <v>81.821</v>
+        <v>82.019</v>
       </c>
       <c r="J22" t="n">
-        <v>393</v>
+        <v>266</v>
       </c>
       <c r="K22" t="n">
-        <v>0.296</v>
+        <v>0.201</v>
       </c>
       <c r="L22" t="n">
-        <v>526</v>
+        <v>500</v>
       </c>
       <c r="M22" t="n">
-        <v>0.397</v>
+        <v>0.377</v>
       </c>
       <c r="N22" t="s">
         <v>157</v>
@@ -3626,7 +3627,7 @@
         <v>168</v>
       </c>
       <c r="C24" s="1" t="n">
-        <v>44014</v>
+        <v>44016</v>
       </c>
       <c r="D24" t="s">
         <v>169</v>
@@ -3636,25 +3637,25 @@
       </c>
       <c r="F24"/>
       <c r="G24" t="n">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="H24" t="n">
-        <v>251528</v>
+        <v>255108</v>
       </c>
       <c r="I24" t="n">
-        <v>45.396</v>
+        <v>46.042</v>
       </c>
       <c r="J24" t="n">
-        <v>311</v>
+        <v>65</v>
       </c>
       <c r="K24" t="n">
-        <v>0.056</v>
+        <v>0.012</v>
       </c>
       <c r="L24" t="n">
-        <v>1584</v>
+        <v>1613</v>
       </c>
       <c r="M24" t="n">
-        <v>0.286</v>
+        <v>0.291</v>
       </c>
       <c r="N24" t="s">
         <v>171</v>
@@ -3926,7 +3927,7 @@
         <v>202</v>
       </c>
       <c r="C30" s="1" t="n">
-        <v>44014</v>
+        <v>44016</v>
       </c>
       <c r="D30" t="s">
         <v>203</v>
@@ -3936,25 +3937,21 @@
       </c>
       <c r="F30"/>
       <c r="G30" t="n">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="H30" t="n">
-        <v>320427</v>
+        <v>331703</v>
       </c>
       <c r="I30" t="n">
-        <v>30.742</v>
-      </c>
-      <c r="J30" t="n">
-        <v>4445</v>
-      </c>
-      <c r="K30" t="n">
-        <v>0.426</v>
-      </c>
+        <v>31.824</v>
+      </c>
+      <c r="J30"/>
+      <c r="K30"/>
       <c r="L30" t="n">
-        <v>4084</v>
+        <v>4366</v>
       </c>
       <c r="M30" t="n">
-        <v>0.392</v>
+        <v>0.419</v>
       </c>
       <c r="N30" t="s">
         <v>205</v>
@@ -4177,7 +4174,7 @@
         <v>235</v>
       </c>
       <c r="C35" s="1" t="n">
-        <v>44015</v>
+        <v>44016</v>
       </c>
       <c r="D35" t="s">
         <v>231</v>
@@ -4189,25 +4186,25 @@
         <v>233</v>
       </c>
       <c r="G35" t="n">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="H35" t="n">
-        <v>9297749</v>
+        <v>9540132</v>
       </c>
       <c r="I35" t="n">
-        <v>6.737</v>
+        <v>6.913</v>
       </c>
       <c r="J35" t="n">
-        <v>241576</v>
+        <v>242383</v>
       </c>
       <c r="K35" t="n">
-        <v>0.175</v>
+        <v>0.176</v>
       </c>
       <c r="L35" t="n">
-        <v>217360</v>
+        <v>220489</v>
       </c>
       <c r="M35" t="n">
-        <v>0.158</v>
+        <v>0.16</v>
       </c>
       <c r="N35" t="s">
         <v>232</v>
@@ -4230,7 +4227,7 @@
         <v>237</v>
       </c>
       <c r="C36" s="1" t="n">
-        <v>44013</v>
+        <v>44016</v>
       </c>
       <c r="D36" t="s">
         <v>238</v>
@@ -4240,25 +4237,21 @@
       </c>
       <c r="F36"/>
       <c r="G36" t="n">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="H36" t="n">
-        <v>492318</v>
+        <v>529669</v>
       </c>
       <c r="I36" t="n">
-        <v>1.8</v>
-      </c>
-      <c r="J36" t="n">
-        <v>15000</v>
-      </c>
-      <c r="K36" t="n">
-        <v>0.055</v>
-      </c>
+        <v>1.936</v>
+      </c>
+      <c r="J36"/>
+      <c r="K36"/>
       <c r="L36" t="n">
-        <v>11200</v>
+        <v>11443</v>
       </c>
       <c r="M36" t="n">
-        <v>0.041</v>
+        <v>0.042</v>
       </c>
       <c r="N36" t="s">
         <v>239</v>
@@ -4281,7 +4274,7 @@
         <v>244</v>
       </c>
       <c r="C37" s="1" t="n">
-        <v>44012</v>
+        <v>44016</v>
       </c>
       <c r="D37" t="s">
         <v>245</v>
@@ -4291,25 +4284,25 @@
       </c>
       <c r="F37"/>
       <c r="G37" t="n">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="H37" t="n">
-        <v>1666587</v>
+        <v>1769520</v>
       </c>
       <c r="I37" t="n">
-        <v>19.842</v>
+        <v>21.067</v>
       </c>
       <c r="J37" t="n">
-        <v>27509</v>
+        <v>24562</v>
       </c>
       <c r="K37" t="n">
-        <v>0.328</v>
+        <v>0.292</v>
       </c>
       <c r="L37" t="n">
-        <v>27322</v>
+        <v>26568</v>
       </c>
       <c r="M37" t="n">
-        <v>0.325</v>
+        <v>0.316</v>
       </c>
       <c r="N37" t="s">
         <v>246</v>
@@ -4332,7 +4325,7 @@
         <v>250</v>
       </c>
       <c r="C38" s="1" t="n">
-        <v>44014</v>
+        <v>44015</v>
       </c>
       <c r="D38" t="s">
         <v>251</v>
@@ -4342,25 +4335,25 @@
       </c>
       <c r="F38"/>
       <c r="G38" t="n">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="H38" t="n">
-        <v>438034</v>
+        <v>445962</v>
       </c>
       <c r="I38" t="n">
-        <v>88.71</v>
+        <v>90.316</v>
       </c>
       <c r="J38" t="n">
-        <v>3773</v>
+        <v>8000</v>
       </c>
       <c r="K38" t="n">
-        <v>0.764</v>
+        <v>1.62</v>
       </c>
       <c r="L38" t="n">
-        <v>3814</v>
+        <v>4429</v>
       </c>
       <c r="M38" t="n">
-        <v>0.772</v>
+        <v>0.897</v>
       </c>
       <c r="N38" t="s">
         <v>252</v>
@@ -4434,7 +4427,7 @@
         <v>261</v>
       </c>
       <c r="C40" s="1" t="n">
-        <v>44014</v>
+        <v>44016</v>
       </c>
       <c r="D40" t="s">
         <v>262</v>
@@ -4446,25 +4439,25 @@
         <v>264</v>
       </c>
       <c r="G40" t="n">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="H40" t="n">
-        <v>3322447</v>
+        <v>3377073</v>
       </c>
       <c r="I40" t="n">
-        <v>54.951</v>
+        <v>55.855</v>
       </c>
       <c r="J40" t="n">
-        <v>29147</v>
+        <v>28946</v>
       </c>
       <c r="K40" t="n">
-        <v>0.482</v>
+        <v>0.479</v>
       </c>
       <c r="L40" t="n">
-        <v>25952</v>
+        <v>25462</v>
       </c>
       <c r="M40" t="n">
-        <v>0.429</v>
+        <v>0.421</v>
       </c>
       <c r="N40" t="s">
         <v>265</v>
@@ -4487,7 +4480,7 @@
         <v>268</v>
       </c>
       <c r="C41" s="1" t="n">
-        <v>44014</v>
+        <v>44016</v>
       </c>
       <c r="D41" t="s">
         <v>262</v>
@@ -4499,25 +4492,25 @@
         <v>264</v>
       </c>
       <c r="G41" t="n">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="H41" t="n">
-        <v>5498719</v>
+        <v>5600826</v>
       </c>
       <c r="I41" t="n">
-        <v>90.945</v>
+        <v>92.634</v>
       </c>
       <c r="J41" t="n">
-        <v>53243</v>
+        <v>52011</v>
       </c>
       <c r="K41" t="n">
-        <v>0.881</v>
+        <v>0.86</v>
       </c>
       <c r="L41" t="n">
-        <v>47938</v>
+        <v>46222</v>
       </c>
       <c r="M41" t="n">
-        <v>0.793</v>
+        <v>0.764</v>
       </c>
       <c r="N41" t="s">
         <v>265</v>
@@ -4540,7 +4533,7 @@
         <v>271</v>
       </c>
       <c r="C42" s="1" t="n">
-        <v>44014</v>
+        <v>44015</v>
       </c>
       <c r="D42" t="s">
         <v>272</v>
@@ -4552,25 +4545,25 @@
         <v>274</v>
       </c>
       <c r="G42" t="n">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="H42" t="n">
-        <v>475308</v>
+        <v>481877</v>
       </c>
       <c r="I42" t="n">
-        <v>3.758</v>
+        <v>3.81</v>
       </c>
       <c r="J42" t="n">
-        <v>7864</v>
+        <v>6569</v>
       </c>
       <c r="K42" t="n">
-        <v>0.062</v>
+        <v>0.052</v>
       </c>
       <c r="L42" t="n">
-        <v>5688</v>
+        <v>5877</v>
       </c>
       <c r="M42" t="n">
-        <v>0.045</v>
+        <v>0.046</v>
       </c>
       <c r="N42" t="s">
         <v>275</v>
@@ -4593,7 +4586,7 @@
         <v>278</v>
       </c>
       <c r="C43" s="1" t="n">
-        <v>44012</v>
+        <v>44013</v>
       </c>
       <c r="D43" t="s">
         <v>279</v>
@@ -4605,25 +4598,25 @@
         <v>280</v>
       </c>
       <c r="G43" t="n">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H43" t="n">
-        <v>674736</v>
+        <v>691481</v>
       </c>
       <c r="I43" t="n">
-        <v>5.335</v>
+        <v>5.467</v>
       </c>
       <c r="J43" t="n">
-        <v>4883</v>
+        <v>9348</v>
       </c>
       <c r="K43" t="n">
-        <v>0.039</v>
+        <v>0.074</v>
       </c>
       <c r="L43" t="n">
-        <v>6216</v>
+        <v>7101</v>
       </c>
       <c r="M43" t="n">
-        <v>0.049</v>
+        <v>0.056</v>
       </c>
       <c r="N43" t="s">
         <v>275</v>
@@ -4748,7 +4741,7 @@
         <v>295</v>
       </c>
       <c r="C46" s="1" t="n">
-        <v>44014</v>
+        <v>44015</v>
       </c>
       <c r="D46" t="s">
         <v>296</v>
@@ -4758,25 +4751,25 @@
       </c>
       <c r="F46"/>
       <c r="G46" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="H46" t="n">
-        <v>395349</v>
+        <v>399498</v>
       </c>
       <c r="I46" t="n">
-        <v>92.575</v>
+        <v>93.547</v>
       </c>
       <c r="J46" t="n">
-        <v>4312</v>
+        <v>4149</v>
       </c>
       <c r="K46" t="n">
-        <v>1.01</v>
+        <v>0.972</v>
       </c>
       <c r="L46" t="n">
-        <v>3834</v>
+        <v>3888</v>
       </c>
       <c r="M46" t="n">
-        <v>0.898</v>
+        <v>0.91</v>
       </c>
       <c r="N46" t="s">
         <v>297</v>
@@ -4799,7 +4792,7 @@
         <v>301</v>
       </c>
       <c r="C47" s="1" t="n">
-        <v>44015</v>
+        <v>44016</v>
       </c>
       <c r="D47" t="s">
         <v>302</v>
@@ -4811,25 +4804,25 @@
         <v>304</v>
       </c>
       <c r="G47" t="n">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="H47" t="n">
-        <v>155599</v>
+        <v>156784</v>
       </c>
       <c r="I47" t="n">
-        <v>82.493</v>
+        <v>83.122</v>
       </c>
       <c r="J47" t="n">
-        <v>1105</v>
+        <v>1185</v>
       </c>
       <c r="K47" t="n">
-        <v>0.586</v>
+        <v>0.628</v>
       </c>
       <c r="L47" t="n">
-        <v>1502</v>
+        <v>1416</v>
       </c>
       <c r="M47" t="n">
-        <v>0.796</v>
+        <v>0.751</v>
       </c>
       <c r="N47" t="s">
         <v>303</v>
@@ -4903,7 +4896,7 @@
         <v>312</v>
       </c>
       <c r="C49" s="1" t="n">
-        <v>44014</v>
+        <v>44016</v>
       </c>
       <c r="D49" t="s">
         <v>313</v>
@@ -4913,25 +4906,25 @@
       </c>
       <c r="F49"/>
       <c r="G49" t="n">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="H49" t="n">
-        <v>198947</v>
+        <v>219471</v>
       </c>
       <c r="I49" t="n">
-        <v>317.819</v>
+        <v>350.606</v>
       </c>
       <c r="J49" t="n">
-        <v>7665</v>
+        <v>11662</v>
       </c>
       <c r="K49" t="n">
-        <v>12.245</v>
+        <v>18.63</v>
       </c>
       <c r="L49" t="n">
-        <v>5122</v>
+        <v>6740</v>
       </c>
       <c r="M49" t="n">
-        <v>8.182</v>
+        <v>10.767</v>
       </c>
       <c r="N49" t="s">
         <v>314</v>
@@ -4954,7 +4947,7 @@
         <v>318</v>
       </c>
       <c r="C50" s="1" t="n">
-        <v>44014</v>
+        <v>44015</v>
       </c>
       <c r="D50" t="s">
         <v>319</v>
@@ -4966,25 +4959,25 @@
         <v>321</v>
       </c>
       <c r="G50" t="n">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="H50" t="n">
-        <v>782638</v>
+        <v>790859</v>
       </c>
       <c r="I50" t="n">
-        <v>24.181</v>
+        <v>24.435</v>
       </c>
       <c r="J50" t="n">
-        <v>8727</v>
+        <v>8221</v>
       </c>
       <c r="K50" t="n">
-        <v>0.27</v>
+        <v>0.254</v>
       </c>
       <c r="L50" t="n">
-        <v>9494</v>
+        <v>8820</v>
       </c>
       <c r="M50" t="n">
-        <v>0.293</v>
+        <v>0.273</v>
       </c>
       <c r="N50" t="s">
         <v>41</v>
@@ -5007,7 +5000,7 @@
         <v>325</v>
       </c>
       <c r="C51" s="1" t="n">
-        <v>44014</v>
+        <v>44015</v>
       </c>
       <c r="D51" t="s">
         <v>326</v>
@@ -5017,25 +5010,25 @@
       </c>
       <c r="F51"/>
       <c r="G51" t="n">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="H51" t="n">
-        <v>52962</v>
+        <v>53867</v>
       </c>
       <c r="I51" t="n">
-        <v>97.979</v>
+        <v>99.654</v>
       </c>
       <c r="J51" t="n">
-        <v>1386</v>
+        <v>905</v>
       </c>
       <c r="K51" t="n">
-        <v>2.564</v>
+        <v>1.674</v>
       </c>
       <c r="L51" t="n">
-        <v>969</v>
+        <v>997</v>
       </c>
       <c r="M51" t="n">
-        <v>1.793</v>
+        <v>1.844</v>
       </c>
       <c r="N51" t="s">
         <v>328</v>
@@ -5058,7 +5051,7 @@
         <v>332</v>
       </c>
       <c r="C52" s="1" t="n">
-        <v>44014</v>
+        <v>44015</v>
       </c>
       <c r="D52" t="s">
         <v>333</v>
@@ -5068,25 +5061,25 @@
       </c>
       <c r="F52"/>
       <c r="G52" t="n">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H52" t="n">
-        <v>97158</v>
+        <v>98139</v>
       </c>
       <c r="I52" t="n">
-        <v>220.044</v>
+        <v>222.266</v>
       </c>
       <c r="J52" t="n">
-        <v>892</v>
+        <v>981</v>
       </c>
       <c r="K52" t="n">
-        <v>2.02</v>
+        <v>2.222</v>
       </c>
       <c r="L52" t="n">
-        <v>798</v>
+        <v>803</v>
       </c>
       <c r="M52" t="n">
-        <v>1.807</v>
+        <v>1.819</v>
       </c>
       <c r="N52" t="s">
         <v>334</v>
@@ -5109,7 +5102,7 @@
         <v>338</v>
       </c>
       <c r="C53" s="1" t="n">
-        <v>44008</v>
+        <v>44011</v>
       </c>
       <c r="D53" t="s">
         <v>339</v>
@@ -5119,25 +5112,25 @@
       </c>
       <c r="F53"/>
       <c r="G53" t="n">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="H53" t="n">
-        <v>520421</v>
+        <v>539594</v>
       </c>
       <c r="I53" t="n">
-        <v>4.036</v>
+        <v>4.185</v>
       </c>
       <c r="J53" t="n">
-        <v>9477</v>
+        <v>7715</v>
       </c>
       <c r="K53" t="n">
-        <v>0.074</v>
+        <v>0.06</v>
       </c>
       <c r="L53" t="n">
-        <v>8715</v>
+        <v>8356</v>
       </c>
       <c r="M53" t="n">
-        <v>0.068</v>
+        <v>0.065</v>
       </c>
       <c r="N53" t="s">
         <v>341</v>
@@ -5160,7 +5153,7 @@
         <v>345</v>
       </c>
       <c r="C54" s="1" t="n">
-        <v>44014</v>
+        <v>44015</v>
       </c>
       <c r="D54" t="s">
         <v>346</v>
@@ -5170,25 +5163,25 @@
       </c>
       <c r="F54"/>
       <c r="G54" t="n">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="H54" t="n">
-        <v>715853</v>
+        <v>732494</v>
       </c>
       <c r="I54" t="n">
-        <v>19.394</v>
+        <v>19.845</v>
       </c>
       <c r="J54" t="n">
-        <v>17725</v>
+        <v>16641</v>
       </c>
       <c r="K54" t="n">
-        <v>0.48</v>
+        <v>0.451</v>
       </c>
       <c r="L54" t="n">
-        <v>15680</v>
+        <v>16008</v>
       </c>
       <c r="M54" t="n">
-        <v>0.425</v>
+        <v>0.434</v>
       </c>
       <c r="N54" t="s">
         <v>347</v>
@@ -5366,7 +5359,7 @@
         <v>371</v>
       </c>
       <c r="C58" s="1" t="n">
-        <v>44014</v>
+        <v>44015</v>
       </c>
       <c r="D58" t="s">
         <v>372</v>
@@ -5376,25 +5369,25 @@
       </c>
       <c r="F58"/>
       <c r="G58" t="n">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="H58" t="n">
-        <v>409032</v>
+        <v>411932</v>
       </c>
       <c r="I58" t="n">
-        <v>84.822</v>
+        <v>85.423</v>
       </c>
       <c r="J58" t="n">
-        <v>3703</v>
+        <v>2900</v>
       </c>
       <c r="K58" t="n">
-        <v>0.768</v>
+        <v>0.601</v>
       </c>
       <c r="L58" t="n">
-        <v>4396</v>
+        <v>3500</v>
       </c>
       <c r="M58" t="n">
-        <v>0.912</v>
+        <v>0.726</v>
       </c>
       <c r="N58" t="s">
         <v>373</v>
@@ -5417,7 +5410,7 @@
         <v>376</v>
       </c>
       <c r="C59" s="1" t="n">
-        <v>44015</v>
+        <v>44016</v>
       </c>
       <c r="D59" t="s">
         <v>377</v>
@@ -5427,25 +5420,25 @@
       </c>
       <c r="F59"/>
       <c r="G59" t="n">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H59" t="n">
-        <v>144833</v>
+        <v>148188</v>
       </c>
       <c r="I59" t="n">
-        <v>0.703</v>
+        <v>0.719</v>
       </c>
       <c r="J59" t="n">
-        <v>3308</v>
+        <v>3355</v>
       </c>
       <c r="K59" t="n">
         <v>0.016</v>
       </c>
       <c r="L59" t="n">
-        <v>2882</v>
+        <v>3004</v>
       </c>
       <c r="M59" t="n">
-        <v>0.014</v>
+        <v>0.015</v>
       </c>
       <c r="N59" t="s">
         <v>378</v>
@@ -5519,7 +5512,7 @@
         <v>389</v>
       </c>
       <c r="C61" s="1" t="n">
-        <v>44014</v>
+        <v>44015</v>
       </c>
       <c r="D61" t="s">
         <v>390</v>
@@ -5529,21 +5522,21 @@
       </c>
       <c r="F61"/>
       <c r="G61" t="n">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H61"/>
       <c r="I61"/>
       <c r="J61" t="n">
-        <v>4049</v>
+        <v>3834</v>
       </c>
       <c r="K61" t="n">
-        <v>0.793</v>
+        <v>0.751</v>
       </c>
       <c r="L61" t="n">
-        <v>3387</v>
+        <v>3361</v>
       </c>
       <c r="M61" t="n">
-        <v>0.663</v>
+        <v>0.658</v>
       </c>
       <c r="N61" t="s">
         <v>391</v>
@@ -5566,7 +5559,7 @@
         <v>395</v>
       </c>
       <c r="C62" s="1" t="n">
-        <v>44015</v>
+        <v>44016</v>
       </c>
       <c r="D62" t="s">
         <v>396</v>
@@ -5576,25 +5569,25 @@
       </c>
       <c r="F62"/>
       <c r="G62" t="n">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="H62" t="n">
-        <v>1350773</v>
+        <v>1372825</v>
       </c>
       <c r="I62" t="n">
-        <v>6.115</v>
+        <v>6.215</v>
       </c>
       <c r="J62" t="n">
-        <v>23135</v>
+        <v>22052</v>
       </c>
       <c r="K62" t="n">
-        <v>0.105</v>
+        <v>0.1</v>
       </c>
       <c r="L62" t="n">
-        <v>22537</v>
+        <v>22669</v>
       </c>
       <c r="M62" t="n">
-        <v>0.102</v>
+        <v>0.103</v>
       </c>
       <c r="N62" t="s">
         <v>397</v>
@@ -5617,7 +5610,7 @@
         <v>401</v>
       </c>
       <c r="C63" s="1" t="n">
-        <v>44013</v>
+        <v>44014</v>
       </c>
       <c r="D63" t="s">
         <v>402</v>
@@ -5627,25 +5620,25 @@
       </c>
       <c r="F63"/>
       <c r="G63" t="n">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="H63" t="n">
-        <v>130556</v>
+        <v>132903</v>
       </c>
       <c r="I63" t="n">
-        <v>30.258</v>
+        <v>30.802</v>
       </c>
       <c r="J63" t="n">
-        <v>2670</v>
+        <v>2347</v>
       </c>
       <c r="K63" t="n">
-        <v>0.619</v>
+        <v>0.544</v>
       </c>
       <c r="L63" t="n">
-        <v>2766</v>
+        <v>2640</v>
       </c>
       <c r="M63" t="n">
-        <v>0.641</v>
+        <v>0.612</v>
       </c>
       <c r="N63" t="s">
         <v>403</v>
@@ -5719,7 +5712,7 @@
         <v>412</v>
       </c>
       <c r="C65" s="1" t="n">
-        <v>44015</v>
+        <v>44016</v>
       </c>
       <c r="D65" t="s">
         <v>413</v>
@@ -5729,25 +5722,25 @@
       </c>
       <c r="F65"/>
       <c r="G65" t="n">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="H65" t="n">
-        <v>255999</v>
+        <v>259036</v>
       </c>
       <c r="I65" t="n">
-        <v>7.764</v>
+        <v>7.856</v>
       </c>
       <c r="J65" t="n">
-        <v>3261</v>
+        <v>3037</v>
       </c>
       <c r="K65" t="n">
-        <v>0.099</v>
+        <v>0.092</v>
       </c>
       <c r="L65" t="n">
-        <v>3324</v>
+        <v>3021</v>
       </c>
       <c r="M65" t="n">
-        <v>0.101</v>
+        <v>0.092</v>
       </c>
       <c r="N65" t="s">
         <v>414</v>
@@ -5770,7 +5763,7 @@
         <v>418</v>
       </c>
       <c r="C66" s="1" t="n">
-        <v>44012</v>
+        <v>44013</v>
       </c>
       <c r="D66" t="s">
         <v>419</v>
@@ -5780,25 +5773,25 @@
       </c>
       <c r="F66"/>
       <c r="G66" t="n">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="H66" t="n">
-        <v>681667</v>
+        <v>704549</v>
       </c>
       <c r="I66" t="n">
-        <v>6.221</v>
+        <v>6.429</v>
       </c>
       <c r="J66" t="n">
-        <v>14989</v>
+        <v>22882</v>
       </c>
       <c r="K66" t="n">
-        <v>0.137</v>
+        <v>0.209</v>
       </c>
       <c r="L66" t="n">
-        <v>14444</v>
+        <v>15499</v>
       </c>
       <c r="M66" t="n">
-        <v>0.132</v>
+        <v>0.141</v>
       </c>
       <c r="N66" t="s">
         <v>211</v>
@@ -5821,7 +5814,7 @@
         <v>423</v>
       </c>
       <c r="C67" s="1" t="n">
-        <v>44014</v>
+        <v>44015</v>
       </c>
       <c r="D67" t="s">
         <v>424</v>
@@ -5831,25 +5824,25 @@
       </c>
       <c r="F67"/>
       <c r="G67" t="n">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="H67" t="n">
-        <v>1396177</v>
+        <v>1419434</v>
       </c>
       <c r="I67" t="n">
-        <v>36.89</v>
+        <v>37.505</v>
       </c>
       <c r="J67" t="n">
-        <v>18803</v>
+        <v>23257</v>
       </c>
       <c r="K67" t="n">
-        <v>0.497</v>
+        <v>0.615</v>
       </c>
       <c r="L67" t="n">
-        <v>16818</v>
+        <v>17521</v>
       </c>
       <c r="M67" t="n">
-        <v>0.444</v>
+        <v>0.463</v>
       </c>
       <c r="N67" t="s">
         <v>425</v>
@@ -5872,7 +5865,7 @@
         <v>428</v>
       </c>
       <c r="C68" s="1" t="n">
-        <v>44014</v>
+        <v>44015</v>
       </c>
       <c r="D68" t="s">
         <v>424</v>
@@ -5882,25 +5875,25 @@
       </c>
       <c r="F68"/>
       <c r="G68" t="n">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="H68" t="n">
-        <v>1569693</v>
+        <v>1597497</v>
       </c>
       <c r="I68" t="n">
-        <v>41.475</v>
+        <v>42.21</v>
       </c>
       <c r="J68" t="n">
-        <v>23183</v>
+        <v>27804</v>
       </c>
       <c r="K68" t="n">
-        <v>0.613</v>
+        <v>0.735</v>
       </c>
       <c r="L68" t="n">
-        <v>20693</v>
+        <v>21481</v>
       </c>
       <c r="M68" t="n">
-        <v>0.547</v>
+        <v>0.568</v>
       </c>
       <c r="N68" t="s">
         <v>425</v>
@@ -5974,7 +5967,7 @@
         <v>437</v>
       </c>
       <c r="C70" s="1" t="n">
-        <v>44014</v>
+        <v>44015</v>
       </c>
       <c r="D70" t="s">
         <v>438</v>
@@ -5984,25 +5977,25 @@
       </c>
       <c r="F70"/>
       <c r="G70" t="n">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="H70" t="n">
-        <v>366095</v>
+        <v>372005</v>
       </c>
       <c r="I70" t="n">
-        <v>127.07</v>
+        <v>129.121</v>
       </c>
       <c r="J70" t="n">
-        <v>5593</v>
+        <v>5910</v>
       </c>
       <c r="K70" t="n">
-        <v>1.941</v>
+        <v>2.051</v>
       </c>
       <c r="L70" t="n">
-        <v>4086</v>
+        <v>4299</v>
       </c>
       <c r="M70" t="n">
-        <v>1.418</v>
+        <v>1.492</v>
       </c>
       <c r="N70" t="s">
         <v>439</v>
@@ -6025,7 +6018,7 @@
         <v>443</v>
       </c>
       <c r="C71" s="1" t="n">
-        <v>44015</v>
+        <v>44016</v>
       </c>
       <c r="D71" t="s">
         <v>444</v>
@@ -6035,25 +6028,25 @@
       </c>
       <c r="F71"/>
       <c r="G71" t="n">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="H71" t="n">
-        <v>747592</v>
+        <v>759037</v>
       </c>
       <c r="I71" t="n">
-        <v>38.861</v>
+        <v>39.456</v>
       </c>
       <c r="J71" t="n">
-        <v>12371</v>
+        <v>11445</v>
       </c>
       <c r="K71" t="n">
-        <v>0.643</v>
+        <v>0.595</v>
       </c>
       <c r="L71" t="n">
-        <v>10316</v>
+        <v>11683</v>
       </c>
       <c r="M71" t="n">
-        <v>0.536</v>
+        <v>0.607</v>
       </c>
       <c r="N71" t="s">
         <v>445</v>
@@ -6076,7 +6069,7 @@
         <v>449</v>
       </c>
       <c r="C72" s="1" t="n">
-        <v>44015</v>
+        <v>44016</v>
       </c>
       <c r="D72" t="s">
         <v>450</v>
@@ -6086,25 +6079,25 @@
       </c>
       <c r="F72"/>
       <c r="G72" t="n">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="H72" t="n">
-        <v>20451110</v>
+        <v>20752406</v>
       </c>
       <c r="I72" t="n">
-        <v>140.139</v>
+        <v>142.204</v>
       </c>
       <c r="J72" t="n">
-        <v>282206</v>
+        <v>301296</v>
       </c>
       <c r="K72" t="n">
-        <v>1.934</v>
+        <v>2.065</v>
       </c>
       <c r="L72" t="n">
-        <v>292627</v>
+        <v>292066</v>
       </c>
       <c r="M72" t="n">
-        <v>2.005</v>
+        <v>2.001</v>
       </c>
       <c r="N72" t="s">
         <v>451</v>
@@ -6178,7 +6171,7 @@
         <v>461</v>
       </c>
       <c r="C74" s="1" t="n">
-        <v>44014</v>
+        <v>44015</v>
       </c>
       <c r="D74" t="s">
         <v>462</v>
@@ -6188,25 +6181,25 @@
       </c>
       <c r="F74"/>
       <c r="G74" t="n">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="H74" t="n">
-        <v>1727701</v>
+        <v>1771628</v>
       </c>
       <c r="I74" t="n">
-        <v>49.627</v>
+        <v>50.889</v>
       </c>
       <c r="J74" t="n">
-        <v>53214</v>
+        <v>43927</v>
       </c>
       <c r="K74" t="n">
-        <v>1.529</v>
+        <v>1.262</v>
       </c>
       <c r="L74" t="n">
-        <v>44276</v>
+        <v>45055</v>
       </c>
       <c r="M74" t="n">
-        <v>1.272</v>
+        <v>1.294</v>
       </c>
       <c r="N74" t="s">
         <v>41</v>
@@ -6229,7 +6222,7 @@
         <v>465</v>
       </c>
       <c r="C75" s="1" t="n">
-        <v>44014</v>
+        <v>44015</v>
       </c>
       <c r="D75" t="s">
         <v>466</v>
@@ -6241,25 +6234,25 @@
         <v>468</v>
       </c>
       <c r="G75" t="n">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="H75" t="n">
-        <v>81579</v>
+        <v>82657</v>
       </c>
       <c r="I75" t="n">
-        <v>4.872</v>
+        <v>4.937</v>
       </c>
       <c r="J75" t="n">
-        <v>1160</v>
+        <v>1078</v>
       </c>
       <c r="K75" t="n">
-        <v>0.069</v>
+        <v>0.064</v>
       </c>
       <c r="L75" t="n">
-        <v>1077</v>
+        <v>1080</v>
       </c>
       <c r="M75" t="n">
-        <v>0.064</v>
+        <v>0.065</v>
       </c>
       <c r="N75" t="s">
         <v>469</v>
@@ -6429,7 +6422,7 @@
         <v>488</v>
       </c>
       <c r="C79" s="1" t="n">
-        <v>44015</v>
+        <v>44016</v>
       </c>
       <c r="D79" t="s">
         <v>489</v>
@@ -6439,25 +6432,25 @@
       </c>
       <c r="F79"/>
       <c r="G79" t="n">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="H79" t="n">
-        <v>215322</v>
+        <v>217538</v>
       </c>
       <c r="I79" t="n">
-        <v>39.439</v>
+        <v>39.845</v>
       </c>
       <c r="J79" t="n">
-        <v>1801</v>
+        <v>2216</v>
       </c>
       <c r="K79" t="n">
-        <v>0.33</v>
+        <v>0.406</v>
       </c>
       <c r="L79" t="n">
-        <v>1280</v>
+        <v>1366</v>
       </c>
       <c r="M79" t="n">
-        <v>0.234</v>
+        <v>0.25</v>
       </c>
       <c r="N79" t="s">
         <v>491</v>
@@ -6480,7 +6473,7 @@
         <v>496</v>
       </c>
       <c r="C80" s="1" t="n">
-        <v>44014</v>
+        <v>44015</v>
       </c>
       <c r="D80" t="s">
         <v>497</v>
@@ -6490,25 +6483,25 @@
       </c>
       <c r="F80"/>
       <c r="G80" t="n">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="H80" t="n">
-        <v>104201</v>
+        <v>105652</v>
       </c>
       <c r="I80" t="n">
-        <v>50.122</v>
+        <v>50.82</v>
       </c>
       <c r="J80" t="n">
-        <v>1274</v>
+        <v>1451</v>
       </c>
       <c r="K80" t="n">
-        <v>0.613</v>
+        <v>0.698</v>
       </c>
       <c r="L80" t="n">
-        <v>966</v>
+        <v>1047</v>
       </c>
       <c r="M80" t="n">
-        <v>0.465</v>
+        <v>0.504</v>
       </c>
       <c r="N80" t="s">
         <v>499</v>
@@ -6531,7 +6524,7 @@
         <v>503</v>
       </c>
       <c r="C81" s="1" t="n">
-        <v>44014</v>
+        <v>44015</v>
       </c>
       <c r="D81" t="s">
         <v>504</v>
@@ -6543,25 +6536,25 @@
         <v>506</v>
       </c>
       <c r="G81" t="n">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="H81" t="n">
-        <v>1706127</v>
+        <v>1745153</v>
       </c>
       <c r="I81" t="n">
-        <v>28.767</v>
+        <v>29.425</v>
       </c>
       <c r="J81" t="n">
-        <v>39188</v>
+        <v>39026</v>
       </c>
       <c r="K81" t="n">
-        <v>0.661</v>
+        <v>0.658</v>
       </c>
       <c r="L81" t="n">
-        <v>35159</v>
+        <v>36007</v>
       </c>
       <c r="M81" t="n">
-        <v>0.593</v>
+        <v>0.607</v>
       </c>
       <c r="N81" t="s">
         <v>505</v>
@@ -6584,7 +6577,7 @@
         <v>510</v>
       </c>
       <c r="C82" s="1" t="n">
-        <v>44015</v>
+        <v>44016</v>
       </c>
       <c r="D82" t="s">
         <v>511</v>
@@ -6594,25 +6587,25 @@
       </c>
       <c r="F82"/>
       <c r="G82" t="n">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="H82" t="n">
-        <v>1286201</v>
+        <v>1297202</v>
       </c>
       <c r="I82" t="n">
-        <v>25.087</v>
+        <v>25.302</v>
       </c>
       <c r="J82" t="n">
-        <v>10021</v>
+        <v>11001</v>
       </c>
       <c r="K82" t="n">
-        <v>0.195</v>
+        <v>0.215</v>
       </c>
       <c r="L82" t="n">
-        <v>10398</v>
+        <v>10470</v>
       </c>
       <c r="M82" t="n">
-        <v>0.203</v>
+        <v>0.204</v>
       </c>
       <c r="N82" t="s">
         <v>512</v>
@@ -6682,7 +6675,7 @@
         <v>523</v>
       </c>
       <c r="C84" s="1" t="n">
-        <v>44003</v>
+        <v>44010</v>
       </c>
       <c r="D84" t="s">
         <v>524</v>
@@ -6692,21 +6685,21 @@
       </c>
       <c r="F84"/>
       <c r="G84" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H84" t="n">
-        <v>444607</v>
+        <v>520208</v>
       </c>
       <c r="I84" t="n">
-        <v>44.024</v>
+        <v>51.509</v>
       </c>
       <c r="J84"/>
       <c r="K84"/>
       <c r="L84" t="n">
-        <v>8829</v>
+        <v>10736</v>
       </c>
       <c r="M84" t="n">
-        <v>0.874</v>
+        <v>1.063</v>
       </c>
       <c r="N84" t="s">
         <v>526</v>
@@ -6715,78 +6708,78 @@
         <v>527</v>
       </c>
       <c r="P84" t="s">
+        <v>92</v>
+      </c>
+      <c r="Q84" t="s">
         <v>528</v>
-      </c>
-      <c r="Q84" t="s">
-        <v>529</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="s">
+        <v>529</v>
+      </c>
+      <c r="B85" t="s">
         <v>530</v>
       </c>
-      <c r="B85" t="s">
+      <c r="C85" s="1" t="n">
+        <v>44015</v>
+      </c>
+      <c r="D85" t="s">
         <v>531</v>
       </c>
-      <c r="C85" s="1" t="n">
-        <v>44014</v>
-      </c>
-      <c r="D85" t="s">
+      <c r="E85" t="s">
         <v>532</v>
-      </c>
-      <c r="E85" t="s">
-        <v>533</v>
       </c>
       <c r="F85"/>
       <c r="G85" t="n">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="H85" t="n">
-        <v>614283</v>
+        <v>624396</v>
       </c>
       <c r="I85" t="n">
-        <v>70.977</v>
+        <v>72.146</v>
       </c>
       <c r="J85" t="n">
-        <v>7410</v>
+        <v>6708</v>
       </c>
       <c r="K85" t="n">
-        <v>0.856</v>
+        <v>0.775</v>
       </c>
       <c r="L85" t="n">
-        <v>9305</v>
+        <v>9292</v>
       </c>
       <c r="M85" t="n">
-        <v>1.075</v>
+        <v>1.074</v>
       </c>
       <c r="N85" t="s">
+        <v>532</v>
+      </c>
+      <c r="O85" t="s">
+        <v>531</v>
+      </c>
+      <c r="P85" t="s">
         <v>533</v>
       </c>
-      <c r="O85" t="s">
-        <v>532</v>
-      </c>
-      <c r="P85" t="s">
+      <c r="Q85" t="s">
         <v>534</v>
-      </c>
-      <c r="Q85" t="s">
-        <v>535</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="s">
+        <v>535</v>
+      </c>
+      <c r="B86" t="s">
         <v>536</v>
-      </c>
-      <c r="B86" t="s">
-        <v>537</v>
       </c>
       <c r="C86" s="1" t="n">
         <v>44014</v>
       </c>
       <c r="D86" t="s">
+        <v>537</v>
+      </c>
+      <c r="E86" t="s">
         <v>538</v>
-      </c>
-      <c r="E86" t="s">
-        <v>539</v>
       </c>
       <c r="F86"/>
       <c r="G86" t="n">
@@ -6811,84 +6804,84 @@
         <v>0.007</v>
       </c>
       <c r="N86" t="s">
+        <v>538</v>
+      </c>
+      <c r="O86" t="s">
         <v>539</v>
       </c>
-      <c r="O86" t="s">
+      <c r="P86" t="s">
         <v>540</v>
       </c>
-      <c r="P86" t="s">
+      <c r="Q86" t="s">
         <v>541</v>
-      </c>
-      <c r="Q86" t="s">
-        <v>542</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="s">
+        <v>542</v>
+      </c>
+      <c r="B87" t="s">
         <v>543</v>
       </c>
-      <c r="B87" t="s">
+      <c r="C87" s="1" t="n">
+        <v>44016</v>
+      </c>
+      <c r="D87" t="s">
         <v>544</v>
       </c>
-      <c r="C87" s="1" t="n">
-        <v>44015</v>
-      </c>
-      <c r="D87" t="s">
+      <c r="E87" t="s">
         <v>545</v>
-      </c>
-      <c r="E87" t="s">
-        <v>546</v>
       </c>
       <c r="F87"/>
       <c r="G87" t="n">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="H87" t="n">
-        <v>317273</v>
+        <v>318619</v>
       </c>
       <c r="I87" t="n">
-        <v>4.545</v>
+        <v>4.565</v>
       </c>
       <c r="J87" t="n">
-        <v>1828</v>
+        <v>1346</v>
       </c>
       <c r="K87" t="n">
-        <v>0.026</v>
+        <v>0.019</v>
       </c>
       <c r="L87" t="n">
-        <v>2064</v>
+        <v>1899</v>
       </c>
       <c r="M87" t="n">
-        <v>0.03</v>
+        <v>0.027</v>
       </c>
       <c r="N87" t="s">
+        <v>546</v>
+      </c>
+      <c r="O87" t="s">
         <v>547</v>
-      </c>
-      <c r="O87" t="s">
-        <v>548</v>
       </c>
       <c r="P87" t="s">
         <v>92</v>
       </c>
       <c r="Q87" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="B88" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="C88" s="1" t="n">
         <v>44008</v>
       </c>
       <c r="D88" t="s">
+        <v>550</v>
+      </c>
+      <c r="E88" t="s">
         <v>551</v>
-      </c>
-      <c r="E88" t="s">
-        <v>552</v>
       </c>
       <c r="F88"/>
       <c r="G88" t="n">
@@ -6909,33 +6902,33 @@
         <v>0.072</v>
       </c>
       <c r="N88" t="s">
+        <v>551</v>
+      </c>
+      <c r="O88" t="s">
         <v>552</v>
-      </c>
-      <c r="O88" t="s">
-        <v>553</v>
       </c>
       <c r="P88" t="s">
         <v>51</v>
       </c>
       <c r="Q88" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="s">
+        <v>554</v>
+      </c>
+      <c r="B89" t="s">
         <v>555</v>
-      </c>
-      <c r="B89" t="s">
-        <v>556</v>
       </c>
       <c r="C89" s="1" t="n">
         <v>44014</v>
       </c>
       <c r="D89" t="s">
+        <v>556</v>
+      </c>
+      <c r="E89" t="s">
         <v>557</v>
-      </c>
-      <c r="E89" t="s">
-        <v>558</v>
       </c>
       <c r="F89"/>
       <c r="G89" t="n">
@@ -6960,36 +6953,36 @@
         <v>0.053</v>
       </c>
       <c r="N89" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="O89" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="P89" t="s">
         <v>51</v>
       </c>
       <c r="Q89" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="s">
+        <v>559</v>
+      </c>
+      <c r="B90" t="s">
         <v>560</v>
-      </c>
-      <c r="B90" t="s">
-        <v>561</v>
       </c>
       <c r="C90" s="1" t="n">
         <v>44004</v>
       </c>
       <c r="D90" t="s">
+        <v>561</v>
+      </c>
+      <c r="E90" t="s">
         <v>562</v>
       </c>
-      <c r="E90" t="s">
+      <c r="F90" t="s">
         <v>563</v>
-      </c>
-      <c r="F90" t="s">
-        <v>564</v>
       </c>
       <c r="G90" t="n">
         <v>76</v>
@@ -7013,137 +7006,133 @@
         <v>0.063</v>
       </c>
       <c r="N90" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="O90" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="P90" t="s">
         <v>22</v>
       </c>
       <c r="Q90" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="s">
+        <v>566</v>
+      </c>
+      <c r="B91" t="s">
         <v>567</v>
       </c>
-      <c r="B91" t="s">
+      <c r="C91" s="1" t="n">
+        <v>44016</v>
+      </c>
+      <c r="D91" t="s">
         <v>568</v>
       </c>
-      <c r="C91" s="1" t="n">
-        <v>44014</v>
-      </c>
-      <c r="D91" t="s">
+      <c r="E91" t="s">
         <v>569</v>
-      </c>
-      <c r="E91" t="s">
-        <v>570</v>
       </c>
       <c r="F91"/>
       <c r="G91" t="n">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="H91" t="n">
-        <v>3483677</v>
+        <v>3535818</v>
       </c>
       <c r="I91" t="n">
-        <v>41.306</v>
-      </c>
-      <c r="J91" t="n">
-        <v>49714</v>
-      </c>
-      <c r="K91" t="n">
-        <v>0.589</v>
-      </c>
+        <v>41.924</v>
+      </c>
+      <c r="J91"/>
+      <c r="K91"/>
       <c r="L91" t="n">
-        <v>49750</v>
+        <v>49885</v>
       </c>
       <c r="M91" t="n">
-        <v>0.59</v>
+        <v>0.591</v>
       </c>
       <c r="N91" t="s">
+        <v>569</v>
+      </c>
+      <c r="O91" t="s">
         <v>570</v>
-      </c>
-      <c r="O91" t="s">
-        <v>571</v>
       </c>
       <c r="P91" t="s">
         <v>22</v>
       </c>
       <c r="Q91" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="s">
+        <v>572</v>
+      </c>
+      <c r="B92" t="s">
         <v>573</v>
       </c>
-      <c r="B92" t="s">
+      <c r="C92" s="1" t="n">
+        <v>44014</v>
+      </c>
+      <c r="D92" t="s">
         <v>574</v>
       </c>
-      <c r="C92" s="1" t="n">
-        <v>44012</v>
-      </c>
-      <c r="D92" t="s">
+      <c r="E92" t="s">
         <v>575</v>
       </c>
-      <c r="E92" t="s">
+      <c r="F92" t="s">
         <v>576</v>
       </c>
-      <c r="F92" t="s">
-        <v>577</v>
-      </c>
       <c r="G92" t="n">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="H92" t="n">
-        <v>168454</v>
+        <v>173761</v>
       </c>
       <c r="I92" t="n">
-        <v>3.683</v>
+        <v>3.799</v>
       </c>
       <c r="J92" t="n">
-        <v>2059</v>
+        <v>3349</v>
       </c>
       <c r="K92" t="n">
-        <v>0.045</v>
+        <v>0.073</v>
       </c>
       <c r="L92" t="n">
-        <v>2626</v>
+        <v>2589</v>
       </c>
       <c r="M92" t="n">
         <v>0.057</v>
       </c>
       <c r="N92" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="O92" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="P92" t="s">
         <v>51</v>
       </c>
       <c r="Q92" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="s">
+        <v>579</v>
+      </c>
+      <c r="B93" t="s">
         <v>580</v>
-      </c>
-      <c r="B93" t="s">
-        <v>581</v>
       </c>
       <c r="C93" s="1" t="n">
         <v>44015</v>
       </c>
       <c r="D93" t="s">
+        <v>581</v>
+      </c>
+      <c r="E93" t="s">
         <v>582</v>
-      </c>
-      <c r="E93" t="s">
-        <v>583</v>
       </c>
       <c r="F93"/>
       <c r="G93" t="n">
@@ -7168,33 +7157,33 @@
         <v>0.234</v>
       </c>
       <c r="N93" t="s">
+        <v>582</v>
+      </c>
+      <c r="O93" t="s">
         <v>583</v>
       </c>
-      <c r="O93" t="s">
+      <c r="P93" t="s">
         <v>584</v>
       </c>
-      <c r="P93" t="s">
+      <c r="Q93" t="s">
         <v>585</v>
-      </c>
-      <c r="Q93" t="s">
-        <v>586</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="s">
+        <v>586</v>
+      </c>
+      <c r="B94" t="s">
         <v>587</v>
-      </c>
-      <c r="B94" t="s">
-        <v>588</v>
       </c>
       <c r="C94" s="1" t="n">
         <v>43973</v>
       </c>
       <c r="D94" t="s">
+        <v>588</v>
+      </c>
+      <c r="E94" t="s">
         <v>589</v>
-      </c>
-      <c r="E94" t="s">
-        <v>590</v>
       </c>
       <c r="F94"/>
       <c r="G94" t="n">
@@ -7219,36 +7208,36 @@
         <v>1.012</v>
       </c>
       <c r="N94" t="s">
+        <v>589</v>
+      </c>
+      <c r="O94" t="s">
         <v>590</v>
-      </c>
-      <c r="O94" t="s">
-        <v>591</v>
       </c>
       <c r="P94" t="s">
         <v>92</v>
       </c>
       <c r="Q94" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="B95" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
       <c r="C95" s="1" t="n">
         <v>44012</v>
       </c>
       <c r="D95" t="s">
+        <v>593</v>
+      </c>
+      <c r="E95" t="s">
+        <v>589</v>
+      </c>
+      <c r="F95" t="s">
         <v>594</v>
-      </c>
-      <c r="E95" t="s">
-        <v>590</v>
-      </c>
-      <c r="F95" t="s">
-        <v>595</v>
       </c>
       <c r="G95" t="n">
         <v>66</v>
@@ -7272,132 +7261,132 @@
         <v>1.131</v>
       </c>
       <c r="N95" t="s">
+        <v>589</v>
+      </c>
+      <c r="O95" t="s">
         <v>590</v>
-      </c>
-      <c r="O95" t="s">
-        <v>591</v>
       </c>
       <c r="P95" t="s">
         <v>22</v>
       </c>
       <c r="Q95" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="s">
+        <v>596</v>
+      </c>
+      <c r="B96" t="s">
         <v>597</v>
       </c>
-      <c r="B96" t="s">
+      <c r="C96" s="1" t="n">
+        <v>44015</v>
+      </c>
+      <c r="D96" t="s">
         <v>598</v>
       </c>
-      <c r="C96" s="1" t="n">
-        <v>44014</v>
-      </c>
-      <c r="D96" t="s">
+      <c r="E96" t="s">
         <v>599</v>
-      </c>
-      <c r="E96" t="s">
-        <v>600</v>
       </c>
       <c r="F96"/>
       <c r="G96" t="n">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H96" t="n">
-        <v>35542936</v>
+        <v>36255888</v>
       </c>
       <c r="I96" t="n">
-        <v>107.38</v>
+        <v>109.534</v>
       </c>
       <c r="J96" t="n">
-        <v>67347</v>
+        <v>712952</v>
       </c>
       <c r="K96" t="n">
-        <v>0.203</v>
+        <v>2.154</v>
       </c>
       <c r="L96" t="n">
-        <v>608823</v>
+        <v>565457</v>
       </c>
       <c r="M96" t="n">
-        <v>1.839</v>
+        <v>1.708</v>
       </c>
       <c r="N96" t="s">
+        <v>599</v>
+      </c>
+      <c r="O96" t="s">
         <v>600</v>
       </c>
-      <c r="O96" t="s">
+      <c r="P96" t="s">
         <v>601</v>
       </c>
-      <c r="P96" t="s">
+      <c r="Q96" t="s">
         <v>602</v>
-      </c>
-      <c r="Q96" t="s">
-        <v>603</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
       <c r="B97" t="s">
+        <v>603</v>
+      </c>
+      <c r="C97" s="1" t="n">
+        <v>44015</v>
+      </c>
+      <c r="D97" t="s">
         <v>604</v>
       </c>
-      <c r="C97" s="1" t="n">
-        <v>44014</v>
-      </c>
-      <c r="D97" t="s">
+      <c r="E97" t="s">
         <v>605</v>
-      </c>
-      <c r="E97" t="s">
-        <v>606</v>
       </c>
       <c r="F97"/>
       <c r="G97" t="n">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="H97" t="n">
-        <v>33462181</v>
+        <v>34213497</v>
       </c>
       <c r="I97" t="n">
-        <v>101.093</v>
+        <v>103.363</v>
       </c>
       <c r="J97" t="n">
-        <v>634822</v>
+        <v>721054</v>
       </c>
       <c r="K97" t="n">
-        <v>1.918</v>
+        <v>2.178</v>
       </c>
       <c r="L97" t="n">
-        <v>607766</v>
+        <v>628961</v>
       </c>
       <c r="M97" t="n">
-        <v>1.836</v>
+        <v>1.9</v>
       </c>
       <c r="N97" t="s">
+        <v>605</v>
+      </c>
+      <c r="O97" t="s">
         <v>606</v>
       </c>
-      <c r="O97" t="s">
+      <c r="P97" t="s">
         <v>607</v>
       </c>
-      <c r="P97" t="s">
+      <c r="Q97" t="s">
         <v>608</v>
-      </c>
-      <c r="Q97" t="s">
-        <v>609</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="s">
+        <v>609</v>
+      </c>
+      <c r="B98" t="s">
         <v>610</v>
-      </c>
-      <c r="B98" t="s">
-        <v>611</v>
       </c>
       <c r="C98" s="1" t="n">
         <v>44014</v>
       </c>
       <c r="D98" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="E98" t="s">
         <v>124</v>
@@ -7424,30 +7413,30 @@
         <v>124</v>
       </c>
       <c r="O98" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="P98" t="s">
         <v>22</v>
       </c>
       <c r="Q98" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="s">
+        <v>614</v>
+      </c>
+      <c r="B99" t="s">
         <v>615</v>
-      </c>
-      <c r="B99" t="s">
-        <v>616</v>
       </c>
       <c r="C99" s="1" t="n">
         <v>43950</v>
       </c>
       <c r="D99" t="s">
+        <v>616</v>
+      </c>
+      <c r="E99" t="s">
         <v>617</v>
-      </c>
-      <c r="E99" t="s">
-        <v>618</v>
       </c>
       <c r="F99"/>
       <c r="G99" t="n">
@@ -7468,33 +7457,33 @@
         <v>0.112</v>
       </c>
       <c r="N99" t="s">
+        <v>617</v>
+      </c>
+      <c r="O99" t="s">
         <v>618</v>
       </c>
-      <c r="O99" t="s">
+      <c r="P99" t="s">
         <v>619</v>
       </c>
-      <c r="P99" t="s">
+      <c r="Q99" t="s">
         <v>620</v>
-      </c>
-      <c r="Q99" t="s">
-        <v>621</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="s">
+        <v>621</v>
+      </c>
+      <c r="B100" t="s">
         <v>622</v>
-      </c>
-      <c r="B100" t="s">
-        <v>623</v>
       </c>
       <c r="C100" s="1" t="n">
         <v>44011</v>
       </c>
       <c r="D100" t="s">
+        <v>623</v>
+      </c>
+      <c r="E100" t="s">
         <v>624</v>
-      </c>
-      <c r="E100" t="s">
-        <v>625</v>
       </c>
       <c r="F100"/>
       <c r="G100" t="n">
@@ -7519,16 +7508,16 @@
         <v>0.03</v>
       </c>
       <c r="N100" t="s">
+        <v>624</v>
+      </c>
+      <c r="O100" t="s">
         <v>625</v>
-      </c>
-      <c r="O100" t="s">
-        <v>626</v>
       </c>
       <c r="P100" t="s">
         <v>22</v>
       </c>
       <c r="Q100" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated testing data for 2020-07-05
</commit_message>
<xml_diff>
--- a/public/data/testing/covid-testing-latest-data-source-details.xlsx
+++ b/public/data/testing/covid-testing-latest-data-source-details.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="627" uniqueCount="627">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="624" uniqueCount="624">
   <si>
     <t xml:space="preserve">ISO code</t>
   </si>
@@ -112,7 +112,7 @@
     <t xml:space="preserve">Austria - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200704151529/https://www.sozialministerium.at/Informationen-zum-Coronavirus/Neuartiges-Coronavirus-(2019-nCov).html</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200705082020/https://www.sozialministerium.at/Informationen-zum-Coronavirus/Neuartiges-Coronavirus-(2019-nCov).html</t>
   </si>
   <si>
     <t xml:space="preserve">Austrian Ministry for Health</t>
@@ -139,7 +139,7 @@
     <t xml:space="preserve">Bahrain - units unclear</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200704151532/https://www.moh.gov.bh/COVID19</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200705082023/https://www.moh.gov.bh/COVID19</t>
   </si>
   <si>
     <t xml:space="preserve">Ministry of Health</t>
@@ -279,7 +279,7 @@
     <t xml:space="preserve">Bulgaria - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200704151537/https://coronavirus.bg/</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200705082027/https://coronavirus.bg/</t>
   </si>
   <si>
     <t xml:space="preserve">Bulgaria COVID-10 Information Portal</t>
@@ -470,7 +470,7 @@
     <t xml:space="preserve">Ecuador - units unclear</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.gestionderiesgos.gob.ec/wp-content/uploads/2020/07/INFOGRAFIA-NACIONALCOVI-19-COE-NACIONAL-02072020-08h00.pdf</t>
+    <t xml:space="preserve">https://www.gestionderiesgos.gob.ec/wp-content/uploads/2020/07/INFOGRAFIA-NACIONALCOVI-19-COE-NACIONAL-04072020-08h00.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">Government of Ecuador</t>
@@ -869,7 +869,7 @@
     <t xml:space="preserve">Israel - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://govextra.gov.il/media/21876/covid19-data-israel-26062020.csv</t>
+    <t xml:space="preserve">https://govextra.gov.il/media/21883/covid19-data-israel-28062020.csv</t>
   </si>
   <si>
     <t xml:space="preserve">Israel Ministry of Health</t>
@@ -926,7 +926,7 @@
     <t xml:space="preserve">Japan - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.mhlw.go.jp/stf/newpage_12236.html</t>
+    <t xml:space="preserve">https://www.mhlw.go.jp/stf/newpage_12245.html</t>
   </si>
   <si>
     <t xml:space="preserve">Ministry of Health, Labor and Welfare Press Release</t>
@@ -949,10 +949,10 @@
     <t xml:space="preserve">Japan - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.mhlw.go.jp/content/10906000/000646181.pdf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The cumulative total reported in the press release (701,541) does not sum to the cumulative total calculated from the weekly and daily figures reported by the MOH. See: https://www.mhlw.go.jp/content/10906000/000646181.pdf</t>
+    <t xml:space="preserve">https://www.mhlw.go.jp/content/10906000/000646587.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The cumulative total reported in the press release (708,438) does not sum to the cumulative total calculated from the weekly and daily figures reported by the MOH. See: https://www.mhlw.go.jp/content/10906000/000646587.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">On 11th April 2020, the MOH started providing a daily time series on the "Implementation status of PCR tests for new coronavirus in Japan (based on the date on which results were determined" (via Google translate). 
@@ -1079,7 +1079,7 @@
     <t xml:space="preserve">Malaysia - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">http://covid-19.moh.gov.my/terkini/072020/situasi-terkini-03-julai-2020</t>
+    <t xml:space="preserve">http://covid-19.moh.gov.my/terkini/072020/situasi-terkini-04-julai-2020</t>
   </si>
   <si>
     <t xml:space="preserve">Ministry of Health Malaysia</t>
@@ -1127,7 +1127,7 @@
     <t xml:space="preserve">Malta - samples tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.facebook.com/sahhagovmt/photos/a.102565371462015/174913164227235/</t>
+    <t xml:space="preserve">https://www.facebook.com/sahhagovmt/photos/a.102565371462015/175299484188603/</t>
   </si>
   <si>
     <t xml:space="preserve">Malta Ministry of Health</t>
@@ -1315,7 +1315,7 @@
     <t xml:space="preserve">Oman - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/OmanVSCovid19/status/1278977212365049858</t>
+    <t xml:space="preserve">https://twitter.com/OmanVSCovid19/status/1279343523708514305</t>
   </si>
   <si>
     <t xml:space="preserve">Oman Ministry of Health</t>
@@ -1334,7 +1334,7 @@
     <t xml:space="preserve">Pakistan - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200704151639/http://www.covid.gov.pk/</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200705083543/http://www.covid.gov.pk/</t>
   </si>
   <si>
     <t xml:space="preserve">Government of Pakistan</t>
@@ -1387,7 +1387,7 @@
     <t xml:space="preserve">Peru - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.gob.pe/institucion/minsa/noticias/189954-minsa-casos-confirmados-por-coronavirus-covid-19-ascienden-a-295-599-en-el-peru-comunicado-n-156</t>
+    <t xml:space="preserve">https://www.gob.pe/institucion/minsa/noticias/192057-minsa-casos-confirmados-por-coronavirus-covid-19-ascienden-a-299-080-en-el-peru-comunicado-n-157</t>
   </si>
   <si>
     <t xml:space="preserve">Ministry of Health, Government of Peru</t>
@@ -1428,7 +1428,7 @@
     <t xml:space="preserve">Poland - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/MZ_GOV_PL/status/1278976776300105728</t>
+    <t xml:space="preserve">https://twitter.com/MZ_GOV_PL/status/1279339163503013888</t>
   </si>
   <si>
     <t xml:space="preserve">Poland Ministry of Health</t>
@@ -1710,7 +1710,7 @@
     <t xml:space="preserve">South Korea - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.cdc.go.kr/board/board.es?mid=&amp;bid=0030&amp;act=view&amp;list_no=367707&amp;tag=&amp;nPage=1</t>
+    <t xml:space="preserve">https://www.cdc.go.kr/board/board.es?mid=&amp;bid=0030&amp;act=view&amp;list_no=367712&amp;tag=&amp;nPage=1</t>
   </si>
   <si>
     <t xml:space="preserve">South Korea CDC</t>
@@ -1903,7 +1903,7 @@
     <t xml:space="preserve">Turkey - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200704151748/https://covid19.saglik.gov.tr/</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200704195450/https://covid19.saglik.gov.tr/</t>
   </si>
   <si>
     <t xml:space="preserve">Turkish Ministry of Health</t>
@@ -1924,7 +1924,7 @@
     <t xml:space="preserve">Uganda - samples tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/MinofHealthUG/status/1278977810720264193</t>
+    <t xml:space="preserve">https://twitter.com/MinofHealthUG/status/1279324518629150720</t>
   </si>
   <si>
     <t xml:space="preserve">Press Release from the Office of the Director General</t>
@@ -1948,7 +1948,7 @@
     <t xml:space="preserve">Ukraine - units unclear</t>
   </si>
   <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200703151413/https://covid19.gov.ua/en</t>
+    <t xml:space="preserve">https://web.archive.org/web/20200705083633/https://covid19.gov.ua/en</t>
   </si>
   <si>
     <t xml:space="preserve">Cabinet of Ministers of Ukraine</t>
@@ -1967,33 +1967,24 @@
     <t xml:space="preserve">GBR</t>
   </si>
   <si>
-    <t xml:space="preserve">United Kingdom - people tested</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200522162805/https://www.gov.uk/guidance/coronavirus-covid-19-information-for-the-public</t>
+    <t xml:space="preserve">United Kingdom - tests performed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://assets.publishing.service.gov.uk/government/uploads/system/uploads/attachment_data/file/897767/2020-07-04_COVID-19_UK_testing_time_series.csv</t>
   </si>
   <si>
     <t xml:space="preserve">Public Health England/Department of Health and Social Care</t>
   </si>
   <si>
+    <t xml:space="preserve">Sum of pillar 1 + pillar 2 (tests processed only)</t>
+  </si>
+  <si>
     <t xml:space="preserve">https://www.gov.uk/guidance/coronavirus-covid-19-information-for-the-public#number-of-cases</t>
   </si>
   <si>
-    <t xml:space="preserve">The figures we provide relate to the daily updates provided for the cumulative total and daily number of people tested. It is not clear the exact date that the cumulative figures date back to. As of 2 June 2020, the source notes that "reporting on the number of people tested has been temporarily paused to ensure consistent reporting across all pillars. This is due to a small percentage of cases where the same person has had more than one test or tested positive more than once for coronavirus in pillar 2. Corrections will be made to any figures if they have subsequently been found to have an error."</t>
-  </si>
-  <si>
-    <t xml:space="preserve">United Kingdom - tests performed</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://assets.publishing.service.gov.uk/government/uploads/system/uploads/attachment_data/file/897065/2020-07-01_COVID-19_UK_testing_time_series.csv</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sum of pillar 1 + pillar 2 (tests processed only)</t>
-  </si>
-  <si>
     <t xml:space="preserve">Since early June 2020, the United Kingdom has been publishing a full retrospective time series in CSV format, with testing data going back to 20 March 2020. In our time series for "tests performed", we aggregate the data for the United Kingdom based only on two "pillars":
-- Pillar 1: swab testing in Public Health England (PHE) labs and NHS hospitals for those with a clinical need, and health and care workers;
-- Pillar 2: swab testing for the wider population, as set out in government guidance. For this pillar we exclude "Delivery (tests sent out)", since we aim to include completed tests in the dataset, not only distributed tests. The source does not make it clear how many of these delivered tests are being returned and processed.
+- pillar 1: swab (antigen) testing in Public Health England (PHE) labs and NHS hospitals for those with a clinical need and health and care workers;
+- pillar 2: swab (antigen) testing for the wider population. For this pillar we exclude "Delivery (tests sent out)", since we aim to include completed tests in the dataset, not only distributed tests. The source does not make it clear how many of these delivered tests are being returned and processed.
 These combined criteria mean that our time series starts on 26 April 2020. We do not include other pillars, i.e.
 - Pillar 3: this pillar consists (fully) of serology tests, which we aim not to include;
 - Pillar 4: this pillar consists (partly) of serology tests, which we aim not to include, and positive tests results from this pillar seem not to be included in the government's total for positive cases.
@@ -2611,7 +2602,7 @@
         <v>31</v>
       </c>
       <c r="C4" s="1" t="n">
-        <v>44016</v>
+        <v>44017</v>
       </c>
       <c r="D4" t="s">
         <v>32</v>
@@ -2621,25 +2612,25 @@
       </c>
       <c r="F4"/>
       <c r="G4" t="n">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="H4" t="n">
-        <v>642679</v>
+        <v>647804</v>
       </c>
       <c r="I4" t="n">
-        <v>71.358</v>
+        <v>71.927</v>
       </c>
       <c r="J4" t="n">
-        <v>7174</v>
+        <v>5125</v>
       </c>
       <c r="K4" t="n">
-        <v>0.797</v>
+        <v>0.569</v>
       </c>
       <c r="L4" t="n">
-        <v>6455</v>
+        <v>6469</v>
       </c>
       <c r="M4" t="n">
-        <v>0.717</v>
+        <v>0.718</v>
       </c>
       <c r="N4" t="s">
         <v>34</v>
@@ -2662,7 +2653,7 @@
         <v>39</v>
       </c>
       <c r="C5" s="1" t="n">
-        <v>44016</v>
+        <v>44017</v>
       </c>
       <c r="D5" t="s">
         <v>40</v>
@@ -2672,25 +2663,25 @@
       </c>
       <c r="F5"/>
       <c r="G5" t="n">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="H5" t="n">
-        <v>584070</v>
+        <v>592350</v>
       </c>
       <c r="I5" t="n">
-        <v>343.251</v>
+        <v>348.117</v>
       </c>
       <c r="J5" t="n">
-        <v>9965</v>
+        <v>8280</v>
       </c>
       <c r="K5" t="n">
-        <v>5.856</v>
+        <v>4.866</v>
       </c>
       <c r="L5" t="n">
-        <v>8996</v>
+        <v>9015</v>
       </c>
       <c r="M5" t="n">
-        <v>5.287</v>
+        <v>5.298</v>
       </c>
       <c r="N5" t="s">
         <v>42</v>
@@ -2958,7 +2949,7 @@
         <v>81</v>
       </c>
       <c r="C11" s="1" t="n">
-        <v>44016</v>
+        <v>44017</v>
       </c>
       <c r="D11" t="s">
         <v>82</v>
@@ -2968,25 +2959,25 @@
       </c>
       <c r="F11"/>
       <c r="G11" t="n">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H11" t="n">
-        <v>150062</v>
+        <v>152653</v>
       </c>
       <c r="I11" t="n">
-        <v>21.596</v>
+        <v>21.969</v>
       </c>
       <c r="J11" t="n">
-        <v>2538</v>
+        <v>2591</v>
       </c>
       <c r="K11" t="n">
-        <v>0.365</v>
+        <v>0.373</v>
       </c>
       <c r="L11" t="n">
-        <v>2717</v>
+        <v>2869</v>
       </c>
       <c r="M11" t="n">
-        <v>0.391</v>
+        <v>0.413</v>
       </c>
       <c r="N11" t="s">
         <v>84</v>
@@ -3060,7 +3051,7 @@
         <v>95</v>
       </c>
       <c r="C13" s="1" t="n">
-        <v>44015</v>
+        <v>44016</v>
       </c>
       <c r="D13" t="s">
         <v>96</v>
@@ -3072,25 +3063,25 @@
         <v>97</v>
       </c>
       <c r="G13" t="n">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="H13" t="n">
-        <v>1146593</v>
+        <v>1163907</v>
       </c>
       <c r="I13" t="n">
-        <v>59.98</v>
+        <v>60.886</v>
       </c>
       <c r="J13" t="n">
-        <v>15585</v>
+        <v>17314</v>
       </c>
       <c r="K13" t="n">
-        <v>0.815</v>
+        <v>0.906</v>
       </c>
       <c r="L13" t="n">
-        <v>14752</v>
+        <v>14662</v>
       </c>
       <c r="M13" t="n">
-        <v>0.772</v>
+        <v>0.767</v>
       </c>
       <c r="N13" t="s">
         <v>98</v>
@@ -3113,7 +3104,7 @@
         <v>102</v>
       </c>
       <c r="C14" s="1" t="n">
-        <v>44014</v>
+        <v>44016</v>
       </c>
       <c r="D14" t="s">
         <v>103</v>
@@ -3123,25 +3114,25 @@
       </c>
       <c r="F14"/>
       <c r="G14" t="n">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="H14" t="n">
-        <v>798108</v>
+        <v>839731</v>
       </c>
       <c r="I14" t="n">
-        <v>15.685</v>
+        <v>16.503</v>
       </c>
       <c r="J14" t="n">
-        <v>19335</v>
+        <v>21028</v>
       </c>
       <c r="K14" t="n">
-        <v>0.38</v>
+        <v>0.413</v>
       </c>
       <c r="L14" t="n">
-        <v>18288</v>
+        <v>18863</v>
       </c>
       <c r="M14" t="n">
-        <v>0.359</v>
+        <v>0.371</v>
       </c>
       <c r="N14" t="s">
         <v>104</v>
@@ -3421,7 +3412,7 @@
         <v>141</v>
       </c>
       <c r="C20" s="1" t="n">
-        <v>44014</v>
+        <v>44016</v>
       </c>
       <c r="D20" t="s">
         <v>142</v>
@@ -3433,25 +3424,25 @@
         <v>144</v>
       </c>
       <c r="G20" t="n">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="H20" t="n">
-        <v>120346</v>
+        <v>124735</v>
       </c>
       <c r="I20" t="n">
-        <v>6.821</v>
+        <v>7.07</v>
       </c>
       <c r="J20" t="n">
-        <v>2743</v>
+        <v>2104</v>
       </c>
       <c r="K20" t="n">
-        <v>0.155</v>
+        <v>0.119</v>
       </c>
       <c r="L20" t="n">
-        <v>1981</v>
+        <v>2114</v>
       </c>
       <c r="M20" t="n">
-        <v>0.112</v>
+        <v>0.12</v>
       </c>
       <c r="N20" t="s">
         <v>143</v>
@@ -3525,7 +3516,7 @@
         <v>154</v>
       </c>
       <c r="C22" s="1" t="n">
-        <v>44015</v>
+        <v>44016</v>
       </c>
       <c r="D22" t="s">
         <v>155</v>
@@ -3535,25 +3526,25 @@
       </c>
       <c r="F22"/>
       <c r="G22" t="n">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="H22" t="n">
-        <v>108802</v>
+        <v>109090</v>
       </c>
       <c r="I22" t="n">
-        <v>82.019</v>
+        <v>82.237</v>
       </c>
       <c r="J22" t="n">
-        <v>266</v>
+        <v>288</v>
       </c>
       <c r="K22" t="n">
-        <v>0.201</v>
+        <v>0.217</v>
       </c>
       <c r="L22" t="n">
-        <v>500</v>
+        <v>489</v>
       </c>
       <c r="M22" t="n">
-        <v>0.377</v>
+        <v>0.369</v>
       </c>
       <c r="N22" t="s">
         <v>157</v>
@@ -3876,7 +3867,7 @@
         <v>200</v>
       </c>
       <c r="C29" s="1" t="n">
-        <v>44011</v>
+        <v>44013</v>
       </c>
       <c r="D29" t="s">
         <v>194</v>
@@ -3886,25 +3877,21 @@
       </c>
       <c r="F29"/>
       <c r="G29" t="n">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="H29" t="n">
-        <v>300520</v>
+        <v>307133</v>
       </c>
       <c r="I29" t="n">
-        <v>9.671</v>
-      </c>
-      <c r="J29" t="n">
-        <v>2929</v>
-      </c>
-      <c r="K29" t="n">
-        <v>0.094</v>
-      </c>
+        <v>9.884</v>
+      </c>
+      <c r="J29"/>
+      <c r="K29"/>
       <c r="L29" t="n">
-        <v>2915</v>
+        <v>2954</v>
       </c>
       <c r="M29" t="n">
-        <v>0.094</v>
+        <v>0.095</v>
       </c>
       <c r="N29" t="s">
         <v>196</v>
@@ -4174,7 +4161,7 @@
         <v>235</v>
       </c>
       <c r="C35" s="1" t="n">
-        <v>44016</v>
+        <v>44017</v>
       </c>
       <c r="D35" t="s">
         <v>231</v>
@@ -4186,25 +4173,25 @@
         <v>233</v>
       </c>
       <c r="G35" t="n">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="H35" t="n">
-        <v>9540132</v>
+        <v>9789066</v>
       </c>
       <c r="I35" t="n">
-        <v>6.913</v>
+        <v>7.094</v>
       </c>
       <c r="J35" t="n">
-        <v>242383</v>
+        <v>248934</v>
       </c>
       <c r="K35" t="n">
-        <v>0.176</v>
+        <v>0.18</v>
       </c>
       <c r="L35" t="n">
-        <v>220489</v>
+        <v>223038</v>
       </c>
       <c r="M35" t="n">
-        <v>0.16</v>
+        <v>0.162</v>
       </c>
       <c r="N35" t="s">
         <v>232</v>
@@ -4325,7 +4312,7 @@
         <v>250</v>
       </c>
       <c r="C38" s="1" t="n">
-        <v>44015</v>
+        <v>44016</v>
       </c>
       <c r="D38" t="s">
         <v>251</v>
@@ -4335,25 +4322,25 @@
       </c>
       <c r="F38"/>
       <c r="G38" t="n">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="H38" t="n">
-        <v>445962</v>
+        <v>454216</v>
       </c>
       <c r="I38" t="n">
-        <v>90.316</v>
+        <v>91.988</v>
       </c>
       <c r="J38" t="n">
-        <v>8000</v>
+        <v>8254</v>
       </c>
       <c r="K38" t="n">
-        <v>1.62</v>
+        <v>1.672</v>
       </c>
       <c r="L38" t="n">
-        <v>4429</v>
+        <v>5036</v>
       </c>
       <c r="M38" t="n">
-        <v>0.897</v>
+        <v>1.02</v>
       </c>
       <c r="N38" t="s">
         <v>252</v>
@@ -4376,7 +4363,7 @@
         <v>255</v>
       </c>
       <c r="C39" s="1" t="n">
-        <v>44008</v>
+        <v>44010</v>
       </c>
       <c r="D39" t="s">
         <v>256</v>
@@ -4386,25 +4373,25 @@
       </c>
       <c r="F39"/>
       <c r="G39" t="n">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="H39" t="n">
-        <v>938272</v>
+        <v>959146</v>
       </c>
       <c r="I39" t="n">
-        <v>108.401</v>
+        <v>110.813</v>
       </c>
       <c r="J39" t="n">
-        <v>16529</v>
+        <v>10386</v>
       </c>
       <c r="K39" t="n">
-        <v>1.91</v>
+        <v>1.2</v>
       </c>
       <c r="L39" t="n">
-        <v>14655</v>
+        <v>15472</v>
       </c>
       <c r="M39" t="n">
-        <v>1.693</v>
+        <v>1.788</v>
       </c>
       <c r="N39" t="s">
         <v>41</v>
@@ -4533,7 +4520,7 @@
         <v>271</v>
       </c>
       <c r="C42" s="1" t="n">
-        <v>44015</v>
+        <v>44016</v>
       </c>
       <c r="D42" t="s">
         <v>272</v>
@@ -4545,25 +4532,25 @@
         <v>274</v>
       </c>
       <c r="G42" t="n">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="H42" t="n">
-        <v>481877</v>
+        <v>490287</v>
       </c>
       <c r="I42" t="n">
-        <v>3.81</v>
+        <v>3.877</v>
       </c>
       <c r="J42" t="n">
-        <v>6569</v>
+        <v>8410</v>
       </c>
       <c r="K42" t="n">
-        <v>0.052</v>
+        <v>0.066</v>
       </c>
       <c r="L42" t="n">
-        <v>5877</v>
+        <v>6243</v>
       </c>
       <c r="M42" t="n">
-        <v>0.046</v>
+        <v>0.049</v>
       </c>
       <c r="N42" t="s">
         <v>275</v>
@@ -4586,7 +4573,7 @@
         <v>278</v>
       </c>
       <c r="C43" s="1" t="n">
-        <v>44013</v>
+        <v>44014</v>
       </c>
       <c r="D43" t="s">
         <v>279</v>
@@ -4598,22 +4585,22 @@
         <v>280</v>
       </c>
       <c r="G43" t="n">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H43" t="n">
-        <v>691481</v>
+        <v>698378</v>
       </c>
       <c r="I43" t="n">
-        <v>5.467</v>
+        <v>5.522</v>
       </c>
       <c r="J43" t="n">
-        <v>9348</v>
+        <v>6869</v>
       </c>
       <c r="K43" t="n">
-        <v>0.074</v>
+        <v>0.054</v>
       </c>
       <c r="L43" t="n">
-        <v>7101</v>
+        <v>7020</v>
       </c>
       <c r="M43" t="n">
         <v>0.056</v>
@@ -4792,7 +4779,7 @@
         <v>301</v>
       </c>
       <c r="C47" s="1" t="n">
-        <v>44016</v>
+        <v>44017</v>
       </c>
       <c r="D47" t="s">
         <v>302</v>
@@ -4804,19 +4791,19 @@
         <v>304</v>
       </c>
       <c r="G47" t="n">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="H47" t="n">
-        <v>156784</v>
+        <v>157826</v>
       </c>
       <c r="I47" t="n">
-        <v>83.122</v>
+        <v>83.674</v>
       </c>
       <c r="J47" t="n">
-        <v>1185</v>
+        <v>1042</v>
       </c>
       <c r="K47" t="n">
-        <v>0.628</v>
+        <v>0.552</v>
       </c>
       <c r="L47" t="n">
         <v>1416</v>
@@ -4947,7 +4934,7 @@
         <v>318</v>
       </c>
       <c r="C50" s="1" t="n">
-        <v>44015</v>
+        <v>44016</v>
       </c>
       <c r="D50" t="s">
         <v>319</v>
@@ -4959,25 +4946,25 @@
         <v>321</v>
       </c>
       <c r="G50" t="n">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="H50" t="n">
-        <v>790859</v>
+        <v>797796</v>
       </c>
       <c r="I50" t="n">
-        <v>24.435</v>
+        <v>24.649</v>
       </c>
       <c r="J50" t="n">
-        <v>8221</v>
+        <v>6937</v>
       </c>
       <c r="K50" t="n">
-        <v>0.254</v>
+        <v>0.214</v>
       </c>
       <c r="L50" t="n">
-        <v>8820</v>
+        <v>8334</v>
       </c>
       <c r="M50" t="n">
-        <v>0.273</v>
+        <v>0.257</v>
       </c>
       <c r="N50" t="s">
         <v>41</v>
@@ -5051,7 +5038,7 @@
         <v>332</v>
       </c>
       <c r="C52" s="1" t="n">
-        <v>44015</v>
+        <v>44016</v>
       </c>
       <c r="D52" t="s">
         <v>333</v>
@@ -5061,25 +5048,25 @@
       </c>
       <c r="F52"/>
       <c r="G52" t="n">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="H52" t="n">
-        <v>98139</v>
+        <v>99126</v>
       </c>
       <c r="I52" t="n">
-        <v>222.266</v>
+        <v>224.501</v>
       </c>
       <c r="J52" t="n">
-        <v>981</v>
+        <v>987</v>
       </c>
       <c r="K52" t="n">
-        <v>2.222</v>
+        <v>2.235</v>
       </c>
       <c r="L52" t="n">
-        <v>803</v>
+        <v>820</v>
       </c>
       <c r="M52" t="n">
-        <v>1.819</v>
+        <v>1.857</v>
       </c>
       <c r="N52" t="s">
         <v>334</v>
@@ -5102,7 +5089,7 @@
         <v>338</v>
       </c>
       <c r="C53" s="1" t="n">
-        <v>44011</v>
+        <v>44012</v>
       </c>
       <c r="D53" t="s">
         <v>339</v>
@@ -5112,22 +5099,22 @@
       </c>
       <c r="F53"/>
       <c r="G53" t="n">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="H53" t="n">
-        <v>539594</v>
+        <v>552671</v>
       </c>
       <c r="I53" t="n">
-        <v>4.185</v>
+        <v>4.287</v>
       </c>
       <c r="J53" t="n">
-        <v>7715</v>
+        <v>7574</v>
       </c>
       <c r="K53" t="n">
-        <v>0.06</v>
+        <v>0.059</v>
       </c>
       <c r="L53" t="n">
-        <v>8356</v>
+        <v>8421</v>
       </c>
       <c r="M53" t="n">
         <v>0.065</v>
@@ -5461,7 +5448,7 @@
         <v>382</v>
       </c>
       <c r="C60" s="1" t="n">
-        <v>44012</v>
+        <v>44013</v>
       </c>
       <c r="D60" t="s">
         <v>383</v>
@@ -5471,25 +5458,25 @@
       </c>
       <c r="F60"/>
       <c r="G60" t="n">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="H60" t="n">
-        <v>322909</v>
+        <v>327386</v>
       </c>
       <c r="I60" t="n">
-        <v>59.564</v>
+        <v>60.389</v>
       </c>
       <c r="J60" t="n">
-        <v>3737</v>
+        <v>3826</v>
       </c>
       <c r="K60" t="n">
-        <v>0.689</v>
+        <v>0.706</v>
       </c>
       <c r="L60" t="n">
-        <v>3055</v>
+        <v>3116</v>
       </c>
       <c r="M60" t="n">
-        <v>0.564</v>
+        <v>0.575</v>
       </c>
       <c r="N60" t="s">
         <v>384</v>
@@ -5512,7 +5499,7 @@
         <v>389</v>
       </c>
       <c r="C61" s="1" t="n">
-        <v>44015</v>
+        <v>44016</v>
       </c>
       <c r="D61" t="s">
         <v>390</v>
@@ -5522,21 +5509,21 @@
       </c>
       <c r="F61"/>
       <c r="G61" t="n">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H61"/>
       <c r="I61"/>
       <c r="J61" t="n">
-        <v>3834</v>
+        <v>2992</v>
       </c>
       <c r="K61" t="n">
-        <v>0.751</v>
+        <v>0.586</v>
       </c>
       <c r="L61" t="n">
-        <v>3361</v>
+        <v>3430</v>
       </c>
       <c r="M61" t="n">
-        <v>0.658</v>
+        <v>0.672</v>
       </c>
       <c r="N61" t="s">
         <v>391</v>
@@ -5559,7 +5546,7 @@
         <v>395</v>
       </c>
       <c r="C62" s="1" t="n">
-        <v>44016</v>
+        <v>44017</v>
       </c>
       <c r="D62" t="s">
         <v>396</v>
@@ -5569,22 +5556,22 @@
       </c>
       <c r="F62"/>
       <c r="G62" t="n">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="H62" t="n">
-        <v>1372825</v>
+        <v>1398352</v>
       </c>
       <c r="I62" t="n">
-        <v>6.215</v>
+        <v>6.33</v>
       </c>
       <c r="J62" t="n">
-        <v>22052</v>
+        <v>25527</v>
       </c>
       <c r="K62" t="n">
-        <v>0.1</v>
+        <v>0.116</v>
       </c>
       <c r="L62" t="n">
-        <v>22669</v>
+        <v>22743</v>
       </c>
       <c r="M62" t="n">
         <v>0.103</v>
@@ -5712,7 +5699,7 @@
         <v>412</v>
       </c>
       <c r="C65" s="1" t="n">
-        <v>44016</v>
+        <v>44017</v>
       </c>
       <c r="D65" t="s">
         <v>413</v>
@@ -5722,25 +5709,25 @@
       </c>
       <c r="F65"/>
       <c r="G65" t="n">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="H65" t="n">
-        <v>259036</v>
+        <v>261603</v>
       </c>
       <c r="I65" t="n">
-        <v>7.856</v>
+        <v>7.934</v>
       </c>
       <c r="J65" t="n">
-        <v>3037</v>
+        <v>2567</v>
       </c>
       <c r="K65" t="n">
-        <v>0.092</v>
+        <v>0.078</v>
       </c>
       <c r="L65" t="n">
-        <v>3021</v>
+        <v>2685</v>
       </c>
       <c r="M65" t="n">
-        <v>0.092</v>
+        <v>0.081</v>
       </c>
       <c r="N65" t="s">
         <v>414</v>
@@ -5763,7 +5750,7 @@
         <v>418</v>
       </c>
       <c r="C66" s="1" t="n">
-        <v>44013</v>
+        <v>44015</v>
       </c>
       <c r="D66" t="s">
         <v>419</v>
@@ -5773,25 +5760,21 @@
       </c>
       <c r="F66"/>
       <c r="G66" t="n">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="H66" t="n">
-        <v>704549</v>
+        <v>738502</v>
       </c>
       <c r="I66" t="n">
-        <v>6.429</v>
-      </c>
-      <c r="J66" t="n">
-        <v>22882</v>
-      </c>
-      <c r="K66" t="n">
-        <v>0.209</v>
-      </c>
+        <v>6.739</v>
+      </c>
+      <c r="J66"/>
+      <c r="K66"/>
       <c r="L66" t="n">
-        <v>15499</v>
+        <v>16334</v>
       </c>
       <c r="M66" t="n">
-        <v>0.141</v>
+        <v>0.149</v>
       </c>
       <c r="N66" t="s">
         <v>211</v>
@@ -5814,7 +5797,7 @@
         <v>423</v>
       </c>
       <c r="C67" s="1" t="n">
-        <v>44015</v>
+        <v>44016</v>
       </c>
       <c r="D67" t="s">
         <v>424</v>
@@ -5824,25 +5807,25 @@
       </c>
       <c r="F67"/>
       <c r="G67" t="n">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="H67" t="n">
-        <v>1419434</v>
+        <v>1437849</v>
       </c>
       <c r="I67" t="n">
-        <v>37.505</v>
+        <v>37.991</v>
       </c>
       <c r="J67" t="n">
-        <v>23257</v>
+        <v>18415</v>
       </c>
       <c r="K67" t="n">
-        <v>0.615</v>
+        <v>0.487</v>
       </c>
       <c r="L67" t="n">
-        <v>17521</v>
+        <v>17417</v>
       </c>
       <c r="M67" t="n">
-        <v>0.463</v>
+        <v>0.46</v>
       </c>
       <c r="N67" t="s">
         <v>425</v>
@@ -5865,7 +5848,7 @@
         <v>428</v>
       </c>
       <c r="C68" s="1" t="n">
-        <v>44015</v>
+        <v>44016</v>
       </c>
       <c r="D68" t="s">
         <v>424</v>
@@ -5875,25 +5858,25 @@
       </c>
       <c r="F68"/>
       <c r="G68" t="n">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="H68" t="n">
-        <v>1597497</v>
+        <v>1620160</v>
       </c>
       <c r="I68" t="n">
-        <v>42.21</v>
+        <v>42.809</v>
       </c>
       <c r="J68" t="n">
-        <v>27804</v>
+        <v>22663</v>
       </c>
       <c r="K68" t="n">
-        <v>0.735</v>
+        <v>0.599</v>
       </c>
       <c r="L68" t="n">
-        <v>21481</v>
+        <v>21457</v>
       </c>
       <c r="M68" t="n">
-        <v>0.568</v>
+        <v>0.567</v>
       </c>
       <c r="N68" t="s">
         <v>425</v>
@@ -5967,7 +5950,7 @@
         <v>437</v>
       </c>
       <c r="C70" s="1" t="n">
-        <v>44015</v>
+        <v>44016</v>
       </c>
       <c r="D70" t="s">
         <v>438</v>
@@ -5977,25 +5960,25 @@
       </c>
       <c r="F70"/>
       <c r="G70" t="n">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="H70" t="n">
-        <v>372005</v>
+        <v>376881</v>
       </c>
       <c r="I70" t="n">
-        <v>129.121</v>
+        <v>130.813</v>
       </c>
       <c r="J70" t="n">
-        <v>5910</v>
+        <v>4876</v>
       </c>
       <c r="K70" t="n">
-        <v>2.051</v>
+        <v>1.692</v>
       </c>
       <c r="L70" t="n">
-        <v>4299</v>
+        <v>4456</v>
       </c>
       <c r="M70" t="n">
-        <v>1.492</v>
+        <v>1.547</v>
       </c>
       <c r="N70" t="s">
         <v>439</v>
@@ -6171,7 +6154,7 @@
         <v>461</v>
       </c>
       <c r="C74" s="1" t="n">
-        <v>44015</v>
+        <v>44016</v>
       </c>
       <c r="D74" t="s">
         <v>462</v>
@@ -6181,25 +6164,25 @@
       </c>
       <c r="F74"/>
       <c r="G74" t="n">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="H74" t="n">
-        <v>1771628</v>
+        <v>1823763</v>
       </c>
       <c r="I74" t="n">
-        <v>50.889</v>
+        <v>52.386</v>
       </c>
       <c r="J74" t="n">
-        <v>43927</v>
+        <v>52135</v>
       </c>
       <c r="K74" t="n">
-        <v>1.262</v>
+        <v>1.498</v>
       </c>
       <c r="L74" t="n">
-        <v>45055</v>
+        <v>46178</v>
       </c>
       <c r="M74" t="n">
-        <v>1.294</v>
+        <v>1.326</v>
       </c>
       <c r="N74" t="s">
         <v>41</v>
@@ -6222,7 +6205,7 @@
         <v>465</v>
       </c>
       <c r="C75" s="1" t="n">
-        <v>44015</v>
+        <v>44016</v>
       </c>
       <c r="D75" t="s">
         <v>466</v>
@@ -6234,25 +6217,25 @@
         <v>468</v>
       </c>
       <c r="G75" t="n">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="H75" t="n">
-        <v>82657</v>
+        <v>83616</v>
       </c>
       <c r="I75" t="n">
-        <v>4.937</v>
+        <v>4.994</v>
       </c>
       <c r="J75" t="n">
-        <v>1078</v>
+        <v>959</v>
       </c>
       <c r="K75" t="n">
+        <v>0.057</v>
+      </c>
+      <c r="L75" t="n">
+        <v>1073</v>
+      </c>
+      <c r="M75" t="n">
         <v>0.064</v>
-      </c>
-      <c r="L75" t="n">
-        <v>1080</v>
-      </c>
-      <c r="M75" t="n">
-        <v>0.065</v>
       </c>
       <c r="N75" t="s">
         <v>469</v>
@@ -6275,7 +6258,7 @@
         <v>474</v>
       </c>
       <c r="C76" s="1" t="n">
-        <v>44015</v>
+        <v>44016</v>
       </c>
       <c r="D76" t="s">
         <v>475</v>
@@ -6287,25 +6270,25 @@
         <v>476</v>
       </c>
       <c r="G76" t="n">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="H76" t="n">
-        <v>426981</v>
+        <v>434415</v>
       </c>
       <c r="I76" t="n">
-        <v>62.749</v>
+        <v>63.841</v>
       </c>
       <c r="J76" t="n">
-        <v>8102</v>
+        <v>7434</v>
       </c>
       <c r="K76" t="n">
-        <v>1.191</v>
+        <v>1.092</v>
       </c>
       <c r="L76" t="n">
-        <v>7444</v>
+        <v>7658</v>
       </c>
       <c r="M76" t="n">
-        <v>1.094</v>
+        <v>1.125</v>
       </c>
       <c r="N76" t="s">
         <v>41</v>
@@ -6524,7 +6507,7 @@
         <v>503</v>
       </c>
       <c r="C81" s="1" t="n">
-        <v>44015</v>
+        <v>44016</v>
       </c>
       <c r="D81" t="s">
         <v>504</v>
@@ -6536,25 +6519,25 @@
         <v>506</v>
       </c>
       <c r="G81" t="n">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="H81" t="n">
-        <v>1745153</v>
+        <v>1792078</v>
       </c>
       <c r="I81" t="n">
-        <v>29.425</v>
+        <v>30.216</v>
       </c>
       <c r="J81" t="n">
-        <v>39026</v>
+        <v>46925</v>
       </c>
       <c r="K81" t="n">
-        <v>0.658</v>
+        <v>0.791</v>
       </c>
       <c r="L81" t="n">
-        <v>36007</v>
+        <v>37581</v>
       </c>
       <c r="M81" t="n">
-        <v>0.607</v>
+        <v>0.634</v>
       </c>
       <c r="N81" t="s">
         <v>505</v>
@@ -6577,7 +6560,7 @@
         <v>510</v>
       </c>
       <c r="C82" s="1" t="n">
-        <v>44016</v>
+        <v>44017</v>
       </c>
       <c r="D82" t="s">
         <v>511</v>
@@ -6587,25 +6570,25 @@
       </c>
       <c r="F82"/>
       <c r="G82" t="n">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="H82" t="n">
-        <v>1297202</v>
+        <v>1303734</v>
       </c>
       <c r="I82" t="n">
-        <v>25.302</v>
+        <v>25.429</v>
       </c>
       <c r="J82" t="n">
-        <v>11001</v>
+        <v>6532</v>
       </c>
       <c r="K82" t="n">
-        <v>0.215</v>
+        <v>0.127</v>
       </c>
       <c r="L82" t="n">
-        <v>10470</v>
+        <v>10272</v>
       </c>
       <c r="M82" t="n">
-        <v>0.204</v>
+        <v>0.2</v>
       </c>
       <c r="N82" t="s">
         <v>512</v>
@@ -7039,18 +7022,18 @@
         <v>104</v>
       </c>
       <c r="H91" t="n">
-        <v>3535818</v>
+        <v>3584066</v>
       </c>
       <c r="I91" t="n">
-        <v>41.924</v>
+        <v>42.496</v>
       </c>
       <c r="J91"/>
       <c r="K91"/>
       <c r="L91" t="n">
-        <v>49885</v>
+        <v>56778</v>
       </c>
       <c r="M91" t="n">
-        <v>0.591</v>
+        <v>0.673</v>
       </c>
       <c r="N91" t="s">
         <v>569</v>
@@ -7073,7 +7056,7 @@
         <v>573</v>
       </c>
       <c r="C92" s="1" t="n">
-        <v>44014</v>
+        <v>44015</v>
       </c>
       <c r="D92" t="s">
         <v>574</v>
@@ -7085,25 +7068,25 @@
         <v>576</v>
       </c>
       <c r="G92" t="n">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H92" t="n">
-        <v>173761</v>
+        <v>178894</v>
       </c>
       <c r="I92" t="n">
-        <v>3.799</v>
+        <v>3.911</v>
       </c>
       <c r="J92" t="n">
-        <v>3349</v>
+        <v>5133</v>
       </c>
       <c r="K92" t="n">
-        <v>0.073</v>
+        <v>0.112</v>
       </c>
       <c r="L92" t="n">
-        <v>2589</v>
+        <v>2912</v>
       </c>
       <c r="M92" t="n">
-        <v>0.057</v>
+        <v>0.064</v>
       </c>
       <c r="N92" t="s">
         <v>575</v>
@@ -7126,7 +7109,7 @@
         <v>580</v>
       </c>
       <c r="C93" s="1" t="n">
-        <v>44015</v>
+        <v>44017</v>
       </c>
       <c r="D93" t="s">
         <v>581</v>
@@ -7136,25 +7119,21 @@
       </c>
       <c r="F93"/>
       <c r="G93" t="n">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="H93" t="n">
-        <v>690953</v>
+        <v>715770</v>
       </c>
       <c r="I93" t="n">
-        <v>15.799</v>
-      </c>
-      <c r="J93" t="n">
-        <v>13696</v>
-      </c>
-      <c r="K93" t="n">
-        <v>0.313</v>
-      </c>
+        <v>16.367</v>
+      </c>
+      <c r="J93"/>
+      <c r="K93"/>
       <c r="L93" t="n">
-        <v>10227</v>
+        <v>10551</v>
       </c>
       <c r="M93" t="n">
-        <v>0.234</v>
+        <v>0.241</v>
       </c>
       <c r="N93" t="s">
         <v>582</v>
@@ -7177,7 +7156,7 @@
         <v>587</v>
       </c>
       <c r="C94" s="1" t="n">
-        <v>43973</v>
+        <v>44011</v>
       </c>
       <c r="D94" t="s">
         <v>588</v>
@@ -7185,339 +7164,288 @@
       <c r="E94" t="s">
         <v>589</v>
       </c>
-      <c r="F94"/>
+      <c r="F94" t="s">
+        <v>590</v>
+      </c>
       <c r="G94" t="n">
-        <v>117</v>
+        <v>65</v>
       </c>
       <c r="H94" t="n">
-        <v>2144626</v>
+        <v>4905196</v>
       </c>
       <c r="I94" t="n">
-        <v>31.592</v>
+        <v>72.256</v>
       </c>
       <c r="J94" t="n">
-        <v>80297</v>
+        <v>50414</v>
       </c>
       <c r="K94" t="n">
-        <v>1.183</v>
+        <v>0.743</v>
       </c>
       <c r="L94" t="n">
-        <v>68733</v>
+        <v>71684</v>
       </c>
       <c r="M94" t="n">
-        <v>1.012</v>
+        <v>1.056</v>
       </c>
       <c r="N94" t="s">
         <v>589</v>
       </c>
       <c r="O94" t="s">
-        <v>590</v>
+        <v>591</v>
       </c>
       <c r="P94" t="s">
-        <v>92</v>
+        <v>22</v>
       </c>
       <c r="Q94" t="s">
-        <v>591</v>
+        <v>592</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="s">
-        <v>586</v>
+        <v>593</v>
       </c>
       <c r="B95" t="s">
-        <v>592</v>
+        <v>594</v>
       </c>
       <c r="C95" s="1" t="n">
-        <v>44012</v>
+        <v>44015</v>
       </c>
       <c r="D95" t="s">
-        <v>593</v>
+        <v>595</v>
       </c>
       <c r="E95" t="s">
-        <v>589</v>
-      </c>
-      <c r="F95" t="s">
-        <v>594</v>
-      </c>
+        <v>596</v>
+      </c>
+      <c r="F95"/>
       <c r="G95" t="n">
-        <v>66</v>
+        <v>35</v>
       </c>
       <c r="H95" t="n">
-        <v>4998914</v>
+        <v>36255888</v>
       </c>
       <c r="I95" t="n">
-        <v>73.637</v>
+        <v>109.534</v>
       </c>
       <c r="J95" t="n">
-        <v>93855</v>
+        <v>712952</v>
       </c>
       <c r="K95" t="n">
-        <v>1.383</v>
+        <v>2.154</v>
       </c>
       <c r="L95" t="n">
-        <v>76793</v>
+        <v>565457</v>
       </c>
       <c r="M95" t="n">
-        <v>1.131</v>
+        <v>1.708</v>
       </c>
       <c r="N95" t="s">
-        <v>589</v>
+        <v>596</v>
       </c>
       <c r="O95" t="s">
-        <v>590</v>
+        <v>597</v>
       </c>
       <c r="P95" t="s">
-        <v>22</v>
+        <v>598</v>
       </c>
       <c r="Q95" t="s">
-        <v>595</v>
+        <v>599</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="s">
-        <v>596</v>
+        <v>593</v>
       </c>
       <c r="B96" t="s">
-        <v>597</v>
+        <v>600</v>
       </c>
       <c r="C96" s="1" t="n">
-        <v>44015</v>
+        <v>44016</v>
       </c>
       <c r="D96" t="s">
-        <v>598</v>
+        <v>601</v>
       </c>
       <c r="E96" t="s">
-        <v>599</v>
+        <v>602</v>
       </c>
       <c r="F96"/>
       <c r="G96" t="n">
-        <v>35</v>
+        <v>120</v>
       </c>
       <c r="H96" t="n">
-        <v>36255888</v>
+        <v>34858427</v>
       </c>
       <c r="I96" t="n">
-        <v>109.534</v>
+        <v>105.312</v>
       </c>
       <c r="J96" t="n">
-        <v>712952</v>
+        <v>644930</v>
       </c>
       <c r="K96" t="n">
-        <v>2.154</v>
+        <v>1.948</v>
       </c>
       <c r="L96" t="n">
-        <v>565457</v>
+        <v>636683</v>
       </c>
       <c r="M96" t="n">
-        <v>1.708</v>
+        <v>1.923</v>
       </c>
       <c r="N96" t="s">
-        <v>599</v>
+        <v>602</v>
       </c>
       <c r="O96" t="s">
-        <v>600</v>
+        <v>603</v>
       </c>
       <c r="P96" t="s">
-        <v>601</v>
+        <v>604</v>
       </c>
       <c r="Q96" t="s">
-        <v>602</v>
+        <v>605</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="s">
-        <v>596</v>
+        <v>606</v>
       </c>
       <c r="B97" t="s">
-        <v>603</v>
+        <v>607</v>
       </c>
       <c r="C97" s="1" t="n">
-        <v>44015</v>
+        <v>44014</v>
       </c>
       <c r="D97" t="s">
-        <v>604</v>
+        <v>608</v>
       </c>
       <c r="E97" t="s">
-        <v>605</v>
+        <v>124</v>
       </c>
       <c r="F97"/>
       <c r="G97" t="n">
-        <v>119</v>
+        <v>91</v>
       </c>
       <c r="H97" t="n">
-        <v>34213497</v>
+        <v>68449</v>
       </c>
       <c r="I97" t="n">
-        <v>103.363</v>
-      </c>
-      <c r="J97" t="n">
-        <v>721054</v>
-      </c>
-      <c r="K97" t="n">
-        <v>2.178</v>
-      </c>
+        <v>19.705</v>
+      </c>
+      <c r="J97"/>
+      <c r="K97"/>
       <c r="L97" t="n">
-        <v>628961</v>
+        <v>977</v>
       </c>
       <c r="M97" t="n">
-        <v>1.9</v>
+        <v>0.281</v>
       </c>
       <c r="N97" t="s">
-        <v>605</v>
+        <v>124</v>
       </c>
       <c r="O97" t="s">
-        <v>606</v>
+        <v>609</v>
       </c>
       <c r="P97" t="s">
-        <v>607</v>
+        <v>22</v>
       </c>
       <c r="Q97" t="s">
-        <v>608</v>
+        <v>610</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="s">
-        <v>609</v>
+        <v>611</v>
       </c>
       <c r="B98" t="s">
-        <v>610</v>
+        <v>612</v>
       </c>
       <c r="C98" s="1" t="n">
-        <v>44014</v>
+        <v>43950</v>
       </c>
       <c r="D98" t="s">
-        <v>611</v>
+        <v>613</v>
       </c>
       <c r="E98" t="s">
-        <v>124</v>
+        <v>614</v>
       </c>
       <c r="F98"/>
       <c r="G98" t="n">
-        <v>91</v>
+        <v>37</v>
       </c>
       <c r="H98" t="n">
-        <v>68449</v>
+        <v>261004</v>
       </c>
       <c r="I98" t="n">
-        <v>19.705</v>
+        <v>2.681</v>
       </c>
       <c r="J98"/>
       <c r="K98"/>
       <c r="L98" t="n">
-        <v>977</v>
+        <v>10906</v>
       </c>
       <c r="M98" t="n">
-        <v>0.281</v>
+        <v>0.112</v>
       </c>
       <c r="N98" t="s">
-        <v>124</v>
+        <v>614</v>
       </c>
       <c r="O98" t="s">
-        <v>612</v>
+        <v>615</v>
       </c>
       <c r="P98" t="s">
-        <v>22</v>
+        <v>616</v>
       </c>
       <c r="Q98" t="s">
-        <v>613</v>
+        <v>617</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="s">
-        <v>614</v>
+        <v>618</v>
       </c>
       <c r="B99" t="s">
-        <v>615</v>
+        <v>619</v>
       </c>
       <c r="C99" s="1" t="n">
-        <v>43950</v>
+        <v>44011</v>
       </c>
       <c r="D99" t="s">
-        <v>616</v>
+        <v>620</v>
       </c>
       <c r="E99" t="s">
-        <v>617</v>
+        <v>621</v>
       </c>
       <c r="F99"/>
       <c r="G99" t="n">
-        <v>37</v>
+        <v>53</v>
       </c>
       <c r="H99" t="n">
-        <v>261004</v>
+        <v>30371</v>
       </c>
       <c r="I99" t="n">
-        <v>2.681</v>
-      </c>
-      <c r="J99"/>
-      <c r="K99"/>
+        <v>2.043</v>
+      </c>
+      <c r="J99" t="n">
+        <v>272</v>
+      </c>
+      <c r="K99" t="n">
+        <v>0.018</v>
+      </c>
       <c r="L99" t="n">
-        <v>10906</v>
+        <v>450</v>
       </c>
       <c r="M99" t="n">
-        <v>0.112</v>
+        <v>0.03</v>
       </c>
       <c r="N99" t="s">
-        <v>617</v>
+        <v>621</v>
       </c>
       <c r="O99" t="s">
-        <v>618</v>
+        <v>622</v>
       </c>
       <c r="P99" t="s">
-        <v>619</v>
+        <v>22</v>
       </c>
       <c r="Q99" t="s">
-        <v>620</v>
-      </c>
-    </row>
-    <row r="100">
-      <c r="A100" t="s">
-        <v>621</v>
-      </c>
-      <c r="B100" t="s">
-        <v>622</v>
-      </c>
-      <c r="C100" s="1" t="n">
-        <v>44011</v>
-      </c>
-      <c r="D100" t="s">
         <v>623</v>
-      </c>
-      <c r="E100" t="s">
-        <v>624</v>
-      </c>
-      <c r="F100"/>
-      <c r="G100" t="n">
-        <v>53</v>
-      </c>
-      <c r="H100" t="n">
-        <v>30371</v>
-      </c>
-      <c r="I100" t="n">
-        <v>2.043</v>
-      </c>
-      <c r="J100" t="n">
-        <v>272</v>
-      </c>
-      <c r="K100" t="n">
-        <v>0.018</v>
-      </c>
-      <c r="L100" t="n">
-        <v>450</v>
-      </c>
-      <c r="M100" t="n">
-        <v>0.03</v>
-      </c>
-      <c r="N100" t="s">
-        <v>624</v>
-      </c>
-      <c r="O100" t="s">
-        <v>625</v>
-      </c>
-      <c r="P100" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q100" t="s">
-        <v>626</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated testing data for 2020-07-13
</commit_message>
<xml_diff>
--- a/public/data/testing/covid-testing-latest-data-source-details.xlsx
+++ b/public/data/testing/covid-testing-latest-data-source-details.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="624" uniqueCount="624">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="623" uniqueCount="623">
   <si>
     <t xml:space="preserve">ISO code</t>
   </si>
@@ -71,7 +71,7 @@
     <t xml:space="preserve">Argentina - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.argentina.gob.ar/sites/default/files/11-07-20_reporte-matutino-covid-19.pdf</t>
+    <t xml:space="preserve">https://www.argentina.gob.ar/sites/default/files/13-07-20-reporte-matutino-covid-19_0.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">Government of Argentina</t>
@@ -184,7 +184,7 @@
     <t xml:space="preserve">Belarus - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">http://minzdrav.gov.by/ru/sobytiya/v-belarusi-vyzdoroveli-i-vypisany-51-120-patsientov/</t>
+    <t xml:space="preserve">http://minzdrav.gov.by/ru/sobytiya/v-belarusi-na-12-iyulya-vyzdoroveli-i-vypisany-55-380-patsientov/</t>
   </si>
   <si>
     <t xml:space="preserve">Belarus Ministry of Health</t>
@@ -230,7 +230,7 @@
     <t xml:space="preserve">Bolivia - units unclear</t>
   </si>
   <si>
-    <t xml:space="preserve">https://minsalud.gob.bo/4378-bolivia-reporta-1-129-contagios-nuevos-de-covid-19-y-61-fallecidos</t>
+    <t xml:space="preserve">https://minsalud.gob.bo/4391-bolivia-registra-987-nuevos-contagios-de-coronavirus-y-el-numero-de-pacientes-recuperados-sube-a-14-843</t>
   </si>
   <si>
     <t xml:space="preserve">https://www.minsalud.gob.bo/</t>
@@ -440,7 +440,7 @@
     <t xml:space="preserve">Denmark - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://files.ssi.dk/Data-Epidemiologiske-Rapport-10072020-y4g5</t>
+    <t xml:space="preserve">https://files.ssi.dk/Data-Epidemiologiske-Rapport-13072020-13ma</t>
   </si>
   <si>
     <t xml:space="preserve">Statens Serum Institut</t>
@@ -458,7 +458,7 @@
     <t xml:space="preserve">Ecuador - units unclear</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.gestionderiesgos.gob.ec/wp-content/uploads/2020/07/INFOGRAFIA-NACIONALCOVI-19-COE-NACIONAL-10072020-08h00.pdf</t>
+    <t xml:space="preserve">https://www.gestionderiesgos.gob.ec/wp-content/uploads/2020/07/INFOGRAFIA-NACIONALCOVI-19-COE-NACIONAL-12072020-08h00.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">Government of Ecuador</t>
@@ -695,7 +695,7 @@
     <t xml:space="preserve">Greece - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://eody.gov.gr/covid-gr-daily-report-20200711/</t>
+    <t xml:space="preserve">https://eody.gov.gr/covid-gr-daily-report-20200713-2/</t>
   </si>
   <si>
     <t xml:space="preserve">National Organization of Public Health</t>
@@ -835,7 +835,7 @@
     <t xml:space="preserve">Iran - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">http://irangov.ir/detail/342917</t>
+    <t xml:space="preserve">http://irangov.ir/detail/343055</t>
   </si>
   <si>
     <t xml:space="preserve">Government of Iran</t>
@@ -871,7 +871,7 @@
     <t xml:space="preserve">Israel - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://govextra.gov.il/media/22028/covid19-data-israel-02072020.csv</t>
+    <t xml:space="preserve">https://govextra.gov.il/media/22086/covid19-data-israel-05072020.csv</t>
   </si>
   <si>
     <t xml:space="preserve">Israel Ministry of Health</t>
@@ -928,13 +928,13 @@
     <t xml:space="preserve">Japan - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.mhlw.go.jp/stf/newpage_12375.html</t>
+    <t xml:space="preserve">https://www.mhlw.go.jp/stf/newpage_12378.html</t>
   </si>
   <si>
     <t xml:space="preserve">Ministry of Health, Labor and Welfare Press Release</t>
   </si>
   <si>
-    <t xml:space="preserve">See Table: 国内の発生状況, column 1 '検査実施人数'. Daily change figure provided for this date is not consistent with the cumulative totals for today and the previous day.</t>
+    <t xml:space="preserve">See Table: 国内の発生状況, column 1 '検査実施人数'.</t>
   </si>
   <si>
     <t xml:space="preserve">Ministry of Health, Labor and Welfare</t>
@@ -951,10 +951,10 @@
     <t xml:space="preserve">Japan - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.mhlw.go.jp/content/10906000/000648215.pdf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The cumulative total reported in the press release (778,122) does not sum to the cumulative total calculated from the weekly and daily figures reported by the MOH. See: https://www.mhlw.go.jp/content/10906000/000648215.pdf</t>
+    <t xml:space="preserve">https://www.mhlw.go.jp/content/10906000/000648431.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The cumulative total reported in the press release (784,070) does not sum to the cumulative total calculated from the weekly and daily figures reported by the MOH. See: https://www.mhlw.go.jp/content/10906000/000648431.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">On 11th April 2020, the MOH started providing a daily time series on the "Implementation status of PCR tests for new coronavirus in Japan (based on the date on which results were determined" (via Google translate). 
@@ -1008,7 +1008,7 @@
     <t xml:space="preserve">Kuwait - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/KUWAIT_MOH/status/1281533396255150080/photo/2</t>
+    <t xml:space="preserve">https://twitter.com/KUWAIT_MOH/status/1282610505316794369/photo/2</t>
   </si>
   <si>
     <t xml:space="preserve">Kuwait Ministry of Health</t>
@@ -1042,9 +1042,6 @@
   </si>
   <si>
     <t xml:space="preserve">Lithuania - samples tested</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://web.archive.org/web/20200710094631/http://sam.lrv.lt/lt/naujienos/koronavirusas</t>
   </si>
   <si>
     <t xml:space="preserve">http://sam.lrv.lt/lt/naujienos/koronavirusas</t>
@@ -1077,7 +1074,7 @@
     <t xml:space="preserve">Malaysia - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">http://covid-19.moh.gov.my/terkini/072020/situasi-terkini-11-julai-2020</t>
+    <t xml:space="preserve">http://covid-19.moh.gov.my/terkini/072020/situasi-terkini-13-julai-2020</t>
   </si>
   <si>
     <t xml:space="preserve">Ministry of Health Malaysia</t>
@@ -1102,7 +1099,7 @@
     <t xml:space="preserve">Maldives - samples tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/HPA_MV/status/1281278721022976010</t>
+    <t xml:space="preserve">https://twitter.com/HPA_MV/status/1282722654819102723/photo/1</t>
   </si>
   <si>
     <t xml:space="preserve">Maldives Health Protection Agency</t>
@@ -1167,7 +1164,7 @@
     <t xml:space="preserve">Morocco - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/Ministere_Sante/status/1281641168200019968</t>
+    <t xml:space="preserve">https://twitter.com/Ministere_Sante/status/1282362441544929281</t>
   </si>
   <si>
     <t xml:space="preserve">Morocco Ministry of Health</t>
@@ -1309,7 +1306,7 @@
     <t xml:space="preserve">Oman - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/OmanVSCovid19/status/1281876118203760644</t>
+    <t xml:space="preserve">https://twitter.com/OmanVSCovid19/status/1282602504522473477</t>
   </si>
   <si>
     <t xml:space="preserve">Oman Ministry of Health</t>
@@ -1369,7 +1366,7 @@
   </si>
   <si>
     <t xml:space="preserve">The Paraguay Ministry of Public Health and Social Welfare maintains an [official dashboard](https://www.mspbs.gov.py/reporte-covid19.html) that reports the weekly and daily number of PCR tests conducted, alongside the percentage of postive tests ('confirmados'). Weekly figures are provided in the chart titled "Cantidad de pruebas vs confirmados". Daily figures are available by clicking on the "+" symbol that appears when hovering over the bottom-left corner of this chart.
-The fact that the percentage shown equates to the number of confirmed case demonstrates that the testing figures equate to the number of people tested and do not include tests pending results.
+The fact that the percentage shown equates to the number of confirmed case suggests that the testing figures equate to the number of people tested and do not include tests pending results.
 The reported figures are cumulative from March 7th 2020, when the first case in Paraguay was confirmed.</t>
   </si>
   <si>
@@ -1379,7 +1376,7 @@
     <t xml:space="preserve">Peru - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.gob.pe/institucion/minsa/noticias/201740-minsa-casos-confirmados-por-coronavirus-covid-19-ascienden-a-319-646-en-el-peru-comunicado-n-166</t>
+    <t xml:space="preserve">https://www.gob.pe/institucion/minsa/noticias/206653-minsa-casos-confirmados-por-coronavirus-covid-19-ascienden-a-326-326-en-el-peru-comunicado-n-168</t>
   </si>
   <si>
     <t xml:space="preserve">Ministry of Health, Government of Peru</t>
@@ -1416,7 +1413,7 @@
     <t xml:space="preserve">Poland - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/MZ_GOV_PL/status/1281875878511878145</t>
+    <t xml:space="preserve">https://twitter.com/MZ_GOV_PL/status/1282600656147111936</t>
   </si>
   <si>
     <t xml:space="preserve">Poland Ministry of Health</t>
@@ -1480,7 +1477,7 @@
     <t xml:space="preserve">Romania - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://gov.ro/ro/media/comunicate/buletin-de-presa-11-iulie-2020-ora-13-00&amp;page=1</t>
+    <t xml:space="preserve">https://gov.ro/ro/media/comunicate/buletin-de-presa-13-iulie-2020-ora-13-00&amp;page=1</t>
   </si>
   <si>
     <t xml:space="preserve">Ministry of Internal Affairs</t>
@@ -1502,7 +1499,7 @@
     <t xml:space="preserve">Russia - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://rospotrebnadzor.ru/about/info/news/news_details.php?ELEMENT_ID=14887</t>
+    <t xml:space="preserve">https://rospotrebnadzor.ru/about/info/news/news_details.php?ELEMENT_ID=14892</t>
   </si>
   <si>
     <t xml:space="preserve">Government of the Russian Federation</t>
@@ -1572,10 +1569,10 @@
     <t xml:space="preserve">http://www.sante.gouv.sn/actualites</t>
   </si>
   <si>
-    <t xml:space="preserve">The figures are labelled as the number of 'tests performed'. Note that from other countries, we see that such a label can be consistent with figures relating to the number of individuals tested.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The Senegalese Ministry for Health and Social Action publishes daily press releases detailing the number of tests performed and the number of positive confirmed cases. It is not totally clear whether the number of tests performed is equivalent to the number of people tested. It is also unclear whether the reported figures include pending test results.
+    <t xml:space="preserve">The figures are labelled as the number of 'tests performed', but this appears to equate to the number of people tested.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Senegalese Ministry for Health and Social Action publishes daily press releases detailing the number of tests performed (tests réalisés) and the number of positive confirmed cases (cas positifs). The fact that the number of tests with positive results (son revenus positifs) equals the number ofn confirmed cases implies that the testing figures equal the number of people tested.
 The daily press releases date back to February 28th 2020. We construct a daily time series of the number of tests performed using data contained in [this unofficial github repository](https://github.com/senegalouvert/COVID-19), which we have cross-checked against official data for a sample of dates.</t>
   </si>
   <si>
@@ -1609,8 +1606,8 @@
     <t xml:space="preserve">https://www.moh.gov.sg/covid-19</t>
   </si>
   <si>
-    <t xml:space="preserve">Singapore's Ministry of Health has started reporting testing numbers since 10 April 2020. The dashboard gives a cumulative total of swabs tested, and unique persons tested.
-No other information is given on how the data was collected and aggregated, and whether coverage was complete.</t>
+    <t xml:space="preserve">The Ministry of Health dashboard gives a cumulative total of swabs tested, and unique persons tested.
+No other information is provided.</t>
   </si>
   <si>
     <t xml:space="preserve">Singapore - samples tested</t>
@@ -1664,7 +1661,7 @@
     <t xml:space="preserve">https://www.gov.si/teme/koronavirus</t>
   </si>
   <si>
-    <t xml:space="preserve">The Government information website provides figures for the number of tests completed ("Opravljeni testi"). A time series of both cumulative and daily tests is available to download. This date back to the 12 March, where 3863 tests are reported to have already been performed (it is not known from which date this first cumulative figure dates back to).
+    <t xml:space="preserve">The Government information website provides figures for the number of tests completed ("Opravljeni testi"). A time series of both cumulative and daily tests is available to download. This dates back to the 12 March, where 3863 tests are reported to have already been performed (it is not known from which date this first cumulative figure dates back to).
 The same cumulative figure is published each day by the [National Insitute for Public Health (NIJZ)](https://www.nijz.si/sl/dnevno-spremljanje-okuzb-s-sars-cov-2-covid-19). Here they clarify that figures relate to the number of tests – including those for people who were tested several times.
 A footnote states that the figures relate to "Laboratory tests performed as part of routine testing and the COVID-19 National Survey are included." The later appears to refer to the prevalence study described on this [Government page](https://www.gov.si/en/news/2020-04-24-national-covid-19-prevalence-survey/). The description of the study states that "The survey is being conducted on a random sample of 3,000 persons" and that people will be tested with both a PCR and a serological test. For this reason, the reported testing figures may include serological tests in addition to PCR tests.
 The volunteer-led [Sledilnik.org project](https://covid-19.sledilnik.org/#/) also presents the official data in a helpful website.</t>
@@ -1689,8 +1686,9 @@
   </si>
   <si>
     <t xml:space="preserve">The South African National Institute for Communicable Diseases (NICD) publishes daily updates on the number of confirmed cases, deaths and tests conducted nationally and by province. These updates are published on its [website](https://www.nicd.ac.za/media/alerts/) and on its offical Twitter account ([@nicd_sa](https://twitter.com/nicd_sa)).
-The NICD reports the number of 'tests conducted' in addition to the number of 'positive cases' (and sometimes the number of 'negative cases'). This is suggestive that 'tests conducted' refers to the number of people tested, but this was unclear from the available documentation until April 18th 2020. On April 18th, the official twitter account for the [Department for Health](https://twitter.com/HealthZA/status/1251605326681575427) clarified that repeat tests for COVID-19 are not counted and that the number 'tests conducted' refers to people tested.
-The NICD began publishing daily updates on 7th February 2020, allowing us to develop a time series from this date forward. We do not know the first date of testing. As of 7th February, 42 people had been tested.</t>
+The NICD reports the number of 'tests processed', which is also labelled as 'total tested'. On April 18th, the official twitter account for the [Department for Health](https://twitter.com/HealthZA/status/1251605326681575427) clarified that repeat tests for COVID-19 are not counted and that the testing figures refer to the number of people tested.
+The NICD began publishing daily updates on 7th February 2020, allowing us to develop a time series from this date forward. We do not know the first date of testing. As of 7th February, 42 people had been tested.
+We source this data from the [Data Repository for South Africa](https://github.com/dsfsi/covid19za) repo – created, maintained and hosted by Data Science for Social Impact research group, led by Dr. Vukosi Marivate, at the University of Pretoria.</t>
   </si>
   <si>
     <t xml:space="preserve">KOR</t>
@@ -1699,7 +1697,7 @@
     <t xml:space="preserve">South Korea - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.cdc.go.kr/board/board.es?mid=&amp;bid=0030&amp;act=view&amp;list_no=367767&amp;tag=&amp;nPage=1</t>
+    <t xml:space="preserve">https://www.cdc.go.kr/board/board.es?mid=&amp;bid=0030&amp;act=view&amp;list_no=367792&amp;tag=&amp;nPage=1</t>
   </si>
   <si>
     <t xml:space="preserve">South Korea CDC</t>
@@ -1708,9 +1706,8 @@
     <t xml:space="preserve">https://www.cdc.go.kr/board/board.es?mid=&amp;bid=0030</t>
   </si>
   <si>
-    <t xml:space="preserve">KCDC have provided daily updates in English since 21 January. The figures they provide relate to ‘cases’, where this signifies an individual considered eligible for testing due to their symptoms, travel history or contact history.
-The figures do not include those cases pending test results. The daily updates show the change each day and the current total. These form a consistent chain all the way back to 21 January. The daily test figures we provide relate to the daily change in the number of tests with results.
-We are not aware of any significant issues affecting comparisons over time.</t>
+    <t xml:space="preserve">KCDC have provided daily updates in English since 21 January.
+The daily updates show the change each day and the current total. These form a consistent chain all the way back to 21 January. The daily test figures we provide relate to the daily change in the number of tests with results (the figures do not include those cases pending test results).</t>
   </si>
   <si>
     <t xml:space="preserve">ESP</t>
@@ -1719,7 +1716,7 @@
     <t xml:space="preserve">Spain - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.mscbs.gob.es/profesionales/saludPublica/ccayes/alertasActual/nCov-China/documentos/COVID-19_pruebas_diagnosticas_02_07_2020.pdf</t>
+    <t xml:space="preserve">https://www.mscbs.gob.es/profesionales/saludPublica/ccayes/alertasActual/nCov-China/documentos/COVID-19_pruebas_diagnosticas_09_07_2020.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">Ministry of Health, Consumption and Social Welfare</t>
@@ -1736,7 +1733,7 @@
 The second is another Ministry of Health press release published on 27 April and relating to testing conducted up to 23 April. It provides a breakdown across Autonomous Communities (regions), with a total for Spain of 1,035,522 PCR tests. The same release provides a figure of 310,038 antibody tests conducted nationwide. These are different to the PCR tests, as we discuss [here](https://ourworldindata.org/covid-testing#different-types-of-tests-for-covid-19). Our database aims to not include antibody tests. So in order to provide the data that is most comparable to the other countries in our database, we include only the PCR tests count for this observation.
 One aspect of the 27 April press release that is not totally clear is whether the figures provided for each Autonomous Community relate to the 23 April. Comparing the regional breakdowns provided in the Ministry of Health release to those collected from official sources by CIVIO (as of 28 April) suggests that the figure of 203,892 provided for Madrid in the Ministry of Health update—ostensibly dating to the 23 April—may date back to 14 April.
 Further data points are collected from the [Ministry of Health's press releases](https://www.mscbs.gob.es/gabinete/notasPrensa.do?metodo=verHistorico) or [its Twitter account](https://twitter.com/sanidadgob).
-[CIVIO](https://datos.civio.es/dataset/pcr-coronavirus-covid19-espana-comunidades-autonomas/) is a non-profit investigative data journalism organisation who are collating information on tests performed within each Autonomous Community, as released through official channels (communication offices, web pages, press releases and social networks of the different regions). We do not report these figures because their data are not complete: For some autonomous communities, figures are available only irregular intervals. The figures they provide are broadly in-line with those of the Ministry of Health releases, although with somewhat lower figures for some Autonomous Communities. This may be due to the Ministry of Health having access to more recent estimates for these Autonomous Communities.</t>
+[CIVIO](https://datos.civio.es/dataset/pcr-coronavirus-covid19-espana-comunidades-autonomas/) is a non-profit investigative data journalism organisation who are collating information on tests performed within each Autonomous Community, as released through official channels (communication offices, web pages, press releases and social networks of the different regions).</t>
   </si>
   <si>
     <t xml:space="preserve">SWE</t>
@@ -1773,8 +1770,9 @@
     <t xml:space="preserve">The number of tests perfomed.</t>
   </si>
   <si>
-    <t xml:space="preserve">The Federal Office of Public Health presents a time series of daily positive and negative tests as a graphic. The data can be accessed by downloading the graphic software file. The graphic notes that "Since several tests can be taken and reported per person, the number of positive tests is higher than the number of positively tested people". (via Google translate).
-The Federal Office of Public Health also publishes a [daily report](https://www.bag.admin.ch/bag/de/home/krankheiten/ausbrueche-epidemien-pandemien/aktuelle-ausbrueche-epidemien/novel-cov/situation-schweiz-und-international.html#316168418) on the epidemiological situation, in which very similar cumulative figures are provided, but often rounded-off. These reports present the figures as "The number of tests carried out on SARS-CoV-2, the causative agent of COVID-19".</t>
+    <t xml:space="preserve">The Federal Office of Public Health presents a time series of daily positive and negative tests, downloadable as a csv file on [their website](https://www.bag.admin.ch/bag/de/home/krankheiten/ausbrueche-epidemien-pandemien/aktuelle-ausbrueche-epidemien/novel-cov/situation-schweiz-und-international.html). A note states that: "The data published here is based on information that laboratories, doctors and hospitals have given us. They refer to reports that we received this morning and can therefore deviate from the figures that the cantons communicate." (via Google translate).
+At this page they also make available daily situation reports, which present the same figures, making it explicit that the numbers refer to PCR tests. 
+The data can also be accessed by downloading the graphic software file in their [visualization here](https://covid-19-schweiz.bagapps.ch/de-3.html). This graphic notes that "Since several tests can be taken and reported per person, the number of positive tests is higher than the number of positively tested people". (via Google translate).</t>
   </si>
   <si>
     <t xml:space="preserve">TWN</t>
@@ -1795,8 +1793,8 @@
     <t xml:space="preserve">The figures are labelled in the source only as 'tested'. It is unclear whether this relates to the number of individuals tested, or the number of samples tested.</t>
   </si>
   <si>
-    <t xml:space="preserve">The Taiwanese Centers for Disease Control (CDC) host a dashboard in which they publish the total 'tested' to date, and 'new from yesterday'. It is not clear whether this represents the total number of tests performed, or the number of people tested. The number 'tested' is greater than the sum of confirmed cases and 'excluded' (i.e. negative) test results. This would suggest it does not equal the total number of people tested, or if it does, pending results without a reported outcome are also included.
-Although the CDC only show the last day's figures on this dashboard, we can construct a time-series by looking at previous versions on web archive. Where possible we have tried to take the total test counts at the same time every day (those published at 00:30h). Unfortunately this time of publishing from CDC was not always completely consistent. This may lead to small discrepancies between 'total tested' and 'new from 'yesterday' figures. Wherever possible we took the total test count as of 00:30 as the prefered figure; where a day of data was missing we used the 'new from yesterday' figure to calculate the total for the previous day. If there are small discrepancies with other sources, this timing issue is likely to be the cause. In any case it is likely to be minor.
+    <t xml:space="preserve">The Taiwanese Centers for Disease Control (CDC) host a dashboard in which they publish the total 'tested' to date, and 'new from yesterday'. It is not clear whether this represents the total number of tests performed, or the number of people tested. The number 'tested' appears to be somewhat greater than the sum of confirmed cases and 'excluded' (i.e. negative) test results. This either suggests that the figure relates to the number of tests performed, or that it relates to the number of people tested but includes some pending results or is affected by reporting delays.
+Although the CDC only show the last day's figures on this dashboard, we can construct a time-series of cumulative tests by looking at previous versions on web archive. Where possible we have tried to take the total test counts at the same time every day (those published at 00:30h), but a complete sequence of archives are not available on this basis. As such, day-to-day variation will be affected by differences in the time of publishing of the data used. Where no data was retreivable for a day, we used the 'new from yesterday' figure to calculate the total for the previous day.
 The date from which the total test figures date back to is not known; the CDC dashboard is unavailable in web archives prior to 21st March.</t>
   </si>
   <si>
@@ -1904,7 +1902,7 @@
     <t xml:space="preserve">Uganda - samples tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/MinofHealthUG/status/1281874535642468352</t>
+    <t xml:space="preserve">https://twitter.com/MinofHealthUG/status/1282586117896843264</t>
   </si>
   <si>
     <t xml:space="preserve">Press Release from the Office of the Director General</t>
@@ -1947,13 +1945,13 @@
     <t xml:space="preserve">United Arab Emirates - samples tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.doh.gov.ae/covid-19/Media-Center/news/News-Listing/News136</t>
+    <t xml:space="preserve">https://www.doh.gov.ae/covid-19/Media-Center/news/News-Listing/News138</t>
   </si>
   <si>
     <t xml:space="preserve">UAE Department of Health</t>
   </si>
   <si>
-    <t xml:space="preserve">"The Ministry of Health and Prevention, MoHAP, announced on Friday that it conducted over 47,000 additional COVID-19 tests"</t>
+    <t xml:space="preserve">"The Ministry of Health and Prevention, MoHAP, announced that it conducted over 50,000 additional COVID-19 tests"</t>
   </si>
   <si>
     <t xml:space="preserve">https://www.doh.gov.ae/en/covid-19/Media%20Center/news/News%20Listing</t>
@@ -1971,7 +1969,7 @@
     <t xml:space="preserve">United Kingdom - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://assets.publishing.service.gov.uk/government/uploads/system/uploads/attachment_data/file/899759/2020-07-11_COVID-19_UK_testing_time_series.csv</t>
+    <t xml:space="preserve">https://assets.publishing.service.gov.uk/government/uploads/system/uploads/attachment_data/file/899965/2020-07-13_COVID-19_UK_testing_time_series.csv</t>
   </si>
   <si>
     <t xml:space="preserve">Public Health England/Department of Health and Social Care</t>
@@ -2050,7 +2048,7 @@
     <t xml:space="preserve">Uruguay - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.gub.uy/ministerio-salud-publica/comunicacion/noticias/informacion-interes-actualizada-sobre-coronavirus-covid-19-uruguay-23</t>
+    <t xml:space="preserve">https://www.gub.uy/ministerio-salud-publica/comunicacion/noticias/informacion-interes-actualizada-sobre-coronavirus-covid-19-uruguay-25</t>
   </si>
   <si>
     <t xml:space="preserve">https://www.gub.uy/ministerio-salud-publica/comunicacion/noticias</t>
@@ -2499,7 +2497,7 @@
         <v>18</v>
       </c>
       <c r="C2" s="1" t="n">
-        <v>44023</v>
+        <v>44025</v>
       </c>
       <c r="D2" t="s">
         <v>19</v>
@@ -2509,25 +2507,25 @@
       </c>
       <c r="F2"/>
       <c r="G2" t="n">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="H2" t="n">
-        <v>456042</v>
+        <v>474422</v>
       </c>
       <c r="I2" t="n">
-        <v>10.09</v>
+        <v>10.497</v>
       </c>
       <c r="J2" t="n">
-        <v>10309</v>
+        <v>8114</v>
       </c>
       <c r="K2" t="n">
-        <v>0.228</v>
+        <v>0.18</v>
       </c>
       <c r="L2" t="n">
-        <v>9380</v>
+        <v>9745</v>
       </c>
       <c r="M2" t="n">
-        <v>0.208</v>
+        <v>0.216</v>
       </c>
       <c r="N2" t="s">
         <v>20</v>
@@ -2601,7 +2599,7 @@
         <v>31</v>
       </c>
       <c r="C4" s="1" t="n">
-        <v>44023</v>
+        <v>44025</v>
       </c>
       <c r="D4" t="s">
         <v>32</v>
@@ -2611,25 +2609,25 @@
       </c>
       <c r="F4"/>
       <c r="G4" t="n">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="H4" t="n">
-        <v>691709</v>
+        <v>700616</v>
       </c>
       <c r="I4" t="n">
-        <v>76.802</v>
+        <v>77.791</v>
       </c>
       <c r="J4" t="n">
-        <v>8225</v>
+        <v>3876</v>
       </c>
       <c r="K4" t="n">
-        <v>0.913</v>
+        <v>0.43</v>
       </c>
       <c r="L4" t="n">
-        <v>7004</v>
+        <v>6644</v>
       </c>
       <c r="M4" t="n">
-        <v>0.778</v>
+        <v>0.738</v>
       </c>
       <c r="N4" t="s">
         <v>34</v>
@@ -2652,7 +2650,7 @@
         <v>39</v>
       </c>
       <c r="C5" s="1" t="n">
-        <v>44023</v>
+        <v>44025</v>
       </c>
       <c r="D5" t="s">
         <v>32</v>
@@ -2662,25 +2660,25 @@
       </c>
       <c r="F5"/>
       <c r="G5" t="n">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="H5" t="n">
-        <v>649020</v>
+        <v>666248</v>
       </c>
       <c r="I5" t="n">
-        <v>381.421</v>
+        <v>391.546</v>
       </c>
       <c r="J5" t="n">
-        <v>8801</v>
+        <v>9589</v>
       </c>
       <c r="K5" t="n">
-        <v>5.172</v>
+        <v>5.635</v>
       </c>
       <c r="L5" t="n">
-        <v>9279</v>
+        <v>7736</v>
       </c>
       <c r="M5" t="n">
-        <v>5.453</v>
+        <v>4.546</v>
       </c>
       <c r="N5" t="s">
         <v>41</v>
@@ -2754,7 +2752,7 @@
         <v>53</v>
       </c>
       <c r="C7" s="1" t="n">
-        <v>44018</v>
+        <v>44024</v>
       </c>
       <c r="D7" t="s">
         <v>54</v>
@@ -2764,21 +2762,21 @@
       </c>
       <c r="F7"/>
       <c r="G7" t="n">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H7" t="n">
-        <v>1074240</v>
+        <v>1134653</v>
       </c>
       <c r="I7" t="n">
-        <v>113.684</v>
+        <v>120.078</v>
       </c>
       <c r="J7"/>
       <c r="K7"/>
       <c r="L7" t="n">
-        <v>11748</v>
+        <v>10076</v>
       </c>
       <c r="M7" t="n">
-        <v>1.243</v>
+        <v>1.066</v>
       </c>
       <c r="N7" t="s">
         <v>55</v>
@@ -2852,7 +2850,7 @@
         <v>66</v>
       </c>
       <c r="C9" s="1" t="n">
-        <v>44021</v>
+        <v>44024</v>
       </c>
       <c r="D9" t="s">
         <v>67</v>
@@ -2862,25 +2860,25 @@
       </c>
       <c r="F9"/>
       <c r="G9" t="n">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="H9" t="n">
-        <v>94859</v>
+        <v>101623</v>
       </c>
       <c r="I9" t="n">
-        <v>8.126</v>
+        <v>8.706</v>
       </c>
       <c r="J9" t="n">
-        <v>2031</v>
+        <v>1869</v>
       </c>
       <c r="K9" t="n">
-        <v>0.174</v>
+        <v>0.16</v>
       </c>
       <c r="L9" t="n">
-        <v>2185</v>
+        <v>2106</v>
       </c>
       <c r="M9" t="n">
-        <v>0.187</v>
+        <v>0.18</v>
       </c>
       <c r="N9" t="s">
         <v>40</v>
@@ -2948,7 +2946,7 @@
         <v>80</v>
       </c>
       <c r="C11" s="1" t="n">
-        <v>44023</v>
+        <v>44024</v>
       </c>
       <c r="D11" t="s">
         <v>32</v>
@@ -2958,25 +2956,25 @@
       </c>
       <c r="F11"/>
       <c r="G11" t="n">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="H11" t="n">
-        <v>172330</v>
+        <v>175136</v>
       </c>
       <c r="I11" t="n">
-        <v>24.801</v>
+        <v>25.205</v>
       </c>
       <c r="J11" t="n">
-        <v>4540</v>
+        <v>2806</v>
       </c>
       <c r="K11" t="n">
-        <v>0.653</v>
+        <v>0.404</v>
       </c>
       <c r="L11" t="n">
-        <v>3181</v>
+        <v>3080</v>
       </c>
       <c r="M11" t="n">
-        <v>0.458</v>
+        <v>0.443</v>
       </c>
       <c r="N11" t="s">
         <v>82</v>
@@ -2999,7 +2997,7 @@
         <v>86</v>
       </c>
       <c r="C12" s="1" t="n">
-        <v>44023</v>
+        <v>44025</v>
       </c>
       <c r="D12" t="s">
         <v>32</v>
@@ -3009,25 +3007,25 @@
       </c>
       <c r="F12"/>
       <c r="G12" t="n">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="H12" t="n">
-        <v>3142626</v>
+        <v>3212803</v>
       </c>
       <c r="I12" t="n">
-        <v>83.266</v>
+        <v>85.125</v>
       </c>
       <c r="J12" t="n">
-        <v>44509</v>
+        <v>29363</v>
       </c>
       <c r="K12" t="n">
-        <v>1.179</v>
+        <v>0.778</v>
       </c>
       <c r="L12" t="n">
-        <v>36708</v>
+        <v>38851</v>
       </c>
       <c r="M12" t="n">
-        <v>0.973</v>
+        <v>1.029</v>
       </c>
       <c r="N12" t="s">
         <v>87</v>
@@ -3050,7 +3048,7 @@
         <v>92</v>
       </c>
       <c r="C13" s="1" t="n">
-        <v>44022</v>
+        <v>44025</v>
       </c>
       <c r="D13" t="s">
         <v>93</v>
@@ -3062,25 +3060,25 @@
         <v>94</v>
       </c>
       <c r="G13" t="n">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="H13" t="n">
-        <v>1255359</v>
+        <v>1310265</v>
       </c>
       <c r="I13" t="n">
-        <v>65.67</v>
+        <v>68.542</v>
       </c>
       <c r="J13" t="n">
-        <v>17727</v>
+        <v>17467</v>
       </c>
       <c r="K13" t="n">
-        <v>0.927</v>
+        <v>0.914</v>
       </c>
       <c r="L13" t="n">
-        <v>15538</v>
+        <v>16001</v>
       </c>
       <c r="M13" t="n">
-        <v>0.813</v>
+        <v>0.837</v>
       </c>
       <c r="N13" t="s">
         <v>95</v>
@@ -3103,7 +3101,7 @@
         <v>99</v>
       </c>
       <c r="C14" s="1" t="n">
-        <v>44021</v>
+        <v>44024</v>
       </c>
       <c r="D14" t="s">
         <v>100</v>
@@ -3113,25 +3111,25 @@
       </c>
       <c r="F14"/>
       <c r="G14" t="n">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="H14" t="n">
-        <v>945240</v>
+        <v>1031230</v>
       </c>
       <c r="I14" t="n">
-        <v>18.577</v>
+        <v>20.267</v>
       </c>
       <c r="J14" t="n">
-        <v>21526</v>
+        <v>25137</v>
       </c>
       <c r="K14" t="n">
-        <v>0.423</v>
+        <v>0.494</v>
       </c>
       <c r="L14" t="n">
-        <v>21019</v>
+        <v>24357</v>
       </c>
       <c r="M14" t="n">
-        <v>0.413</v>
+        <v>0.479</v>
       </c>
       <c r="N14" t="s">
         <v>101</v>
@@ -3154,7 +3152,7 @@
         <v>106</v>
       </c>
       <c r="C15" s="1" t="n">
-        <v>44022</v>
+        <v>44023</v>
       </c>
       <c r="D15" t="s">
         <v>107</v>
@@ -3164,25 +3162,25 @@
       </c>
       <c r="F15"/>
       <c r="G15" t="n">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="H15" t="n">
-        <v>44255</v>
+        <v>45850</v>
       </c>
       <c r="I15" t="n">
-        <v>8.687</v>
+        <v>9.001</v>
       </c>
       <c r="J15" t="n">
-        <v>1367</v>
+        <v>1595</v>
       </c>
       <c r="K15" t="n">
-        <v>0.268</v>
+        <v>0.313</v>
       </c>
       <c r="L15" t="n">
-        <v>1237</v>
+        <v>1323</v>
       </c>
       <c r="M15" t="n">
-        <v>0.243</v>
+        <v>0.26</v>
       </c>
       <c r="N15" t="s">
         <v>108</v>
@@ -3205,7 +3203,7 @@
         <v>112</v>
       </c>
       <c r="C16" s="1" t="n">
-        <v>44023</v>
+        <v>44025</v>
       </c>
       <c r="D16" t="s">
         <v>32</v>
@@ -3215,25 +3213,25 @@
       </c>
       <c r="F16"/>
       <c r="G16" t="n">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="H16" t="n">
-        <v>92808</v>
+        <v>94175</v>
       </c>
       <c r="I16" t="n">
-        <v>22.607</v>
+        <v>22.94</v>
       </c>
       <c r="J16" t="n">
-        <v>1322</v>
+        <v>604</v>
       </c>
       <c r="K16" t="n">
-        <v>0.322</v>
+        <v>0.147</v>
       </c>
       <c r="L16" t="n">
-        <v>1235</v>
+        <v>1168</v>
       </c>
       <c r="M16" t="n">
-        <v>0.301</v>
+        <v>0.285</v>
       </c>
       <c r="N16" t="s">
         <v>113</v>
@@ -3256,7 +3254,7 @@
         <v>118</v>
       </c>
       <c r="C17" s="1" t="n">
-        <v>44022</v>
+        <v>44024</v>
       </c>
       <c r="D17" t="s">
         <v>119</v>
@@ -3268,25 +3266,25 @@
         <v>121</v>
       </c>
       <c r="G17" t="n">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="H17" t="n">
-        <v>202014</v>
+        <v>208098</v>
       </c>
       <c r="I17" t="n">
-        <v>17.835</v>
+        <v>18.372</v>
       </c>
       <c r="J17" t="n">
-        <v>3339</v>
+        <v>2978</v>
       </c>
       <c r="K17" t="n">
-        <v>0.295</v>
+        <v>0.263</v>
       </c>
       <c r="L17" t="n">
-        <v>3045</v>
+        <v>3083</v>
       </c>
       <c r="M17" t="n">
-        <v>0.269</v>
+        <v>0.272</v>
       </c>
       <c r="N17" t="s">
         <v>120</v>
@@ -3309,7 +3307,7 @@
         <v>126</v>
       </c>
       <c r="C18" s="1" t="n">
-        <v>44022</v>
+        <v>44024</v>
       </c>
       <c r="D18" t="s">
         <v>127</v>
@@ -3319,25 +3317,25 @@
       </c>
       <c r="F18"/>
       <c r="G18" t="n">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="H18" t="n">
-        <v>594454</v>
+        <v>598642</v>
       </c>
       <c r="I18" t="n">
-        <v>55.51</v>
+        <v>55.901</v>
       </c>
       <c r="J18" t="n">
-        <v>5281</v>
+        <v>1441</v>
       </c>
       <c r="K18" t="n">
-        <v>0.493</v>
+        <v>0.135</v>
       </c>
       <c r="L18" t="n">
-        <v>3428</v>
+        <v>3568</v>
       </c>
       <c r="M18" t="n">
-        <v>0.32</v>
+        <v>0.333</v>
       </c>
       <c r="N18" t="s">
         <v>40</v>
@@ -3360,7 +3358,7 @@
         <v>131</v>
       </c>
       <c r="C19" s="1" t="n">
-        <v>44021</v>
+        <v>44024</v>
       </c>
       <c r="D19" t="s">
         <v>132</v>
@@ -3370,25 +3368,25 @@
       </c>
       <c r="F19"/>
       <c r="G19" t="n">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="H19" t="n">
-        <v>1184480</v>
+        <v>1222188</v>
       </c>
       <c r="I19" t="n">
-        <v>204.496</v>
+        <v>211.006</v>
       </c>
       <c r="J19" t="n">
-        <v>4113</v>
+        <v>3312</v>
       </c>
       <c r="K19" t="n">
-        <v>0.71</v>
+        <v>0.572</v>
       </c>
       <c r="L19" t="n">
-        <v>12408</v>
+        <v>12983</v>
       </c>
       <c r="M19" t="n">
-        <v>2.142</v>
+        <v>2.241</v>
       </c>
       <c r="N19" t="s">
         <v>133</v>
@@ -3411,7 +3409,7 @@
         <v>137</v>
       </c>
       <c r="C20" s="1" t="n">
-        <v>44022</v>
+        <v>44024</v>
       </c>
       <c r="D20" t="s">
         <v>138</v>
@@ -3423,25 +3421,21 @@
         <v>140</v>
       </c>
       <c r="G20" t="n">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="H20" t="n">
-        <v>134811</v>
+        <v>139271</v>
       </c>
       <c r="I20" t="n">
-        <v>7.641</v>
-      </c>
-      <c r="J20" t="n">
-        <v>1604</v>
-      </c>
-      <c r="K20" t="n">
-        <v>0.091</v>
-      </c>
+        <v>7.894</v>
+      </c>
+      <c r="J20"/>
+      <c r="K20"/>
       <c r="L20" t="n">
-        <v>1740</v>
+        <v>1934</v>
       </c>
       <c r="M20" t="n">
-        <v>0.099</v>
+        <v>0.11</v>
       </c>
       <c r="N20" t="s">
         <v>139</v>
@@ -3515,7 +3509,7 @@
         <v>150</v>
       </c>
       <c r="C22" s="1" t="n">
-        <v>44022</v>
+        <v>44024</v>
       </c>
       <c r="D22" t="s">
         <v>151</v>
@@ -3525,25 +3519,25 @@
       </c>
       <c r="F22"/>
       <c r="G22" t="n">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="H22" t="n">
-        <v>111802</v>
+        <v>112175</v>
       </c>
       <c r="I22" t="n">
-        <v>84.281</v>
+        <v>84.562</v>
       </c>
       <c r="J22" t="n">
-        <v>339</v>
+        <v>220</v>
       </c>
       <c r="K22" t="n">
-        <v>0.256</v>
+        <v>0.166</v>
       </c>
       <c r="L22" t="n">
-        <v>429</v>
+        <v>400</v>
       </c>
       <c r="M22" t="n">
-        <v>0.323</v>
+        <v>0.302</v>
       </c>
       <c r="N22" t="s">
         <v>153</v>
@@ -3668,7 +3662,7 @@
         <v>169</v>
       </c>
       <c r="C25" s="1" t="n">
-        <v>44021</v>
+        <v>44023</v>
       </c>
       <c r="D25" t="s">
         <v>170</v>
@@ -3678,25 +3672,25 @@
       </c>
       <c r="F25"/>
       <c r="G25" t="n">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="H25" t="n">
-        <v>278618</v>
+        <v>278862</v>
       </c>
       <c r="I25" t="n">
-        <v>50.286</v>
+        <v>50.33</v>
       </c>
       <c r="J25" t="n">
-        <v>4135</v>
+        <v>81</v>
       </c>
       <c r="K25" t="n">
-        <v>0.746</v>
+        <v>0.015</v>
       </c>
       <c r="L25" t="n">
-        <v>3037</v>
+        <v>2266</v>
       </c>
       <c r="M25" t="n">
-        <v>0.548</v>
+        <v>0.409</v>
       </c>
       <c r="N25" t="s">
         <v>172</v>
@@ -3917,7 +3911,7 @@
         <v>201</v>
       </c>
       <c r="C30" s="1" t="n">
-        <v>44019</v>
+        <v>44021</v>
       </c>
       <c r="D30" t="s">
         <v>195</v>
@@ -3927,25 +3921,25 @@
       </c>
       <c r="F30"/>
       <c r="G30" t="n">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="H30" t="n">
-        <v>325450</v>
+        <v>328383</v>
       </c>
       <c r="I30" t="n">
-        <v>10.474</v>
+        <v>10.568</v>
       </c>
       <c r="J30" t="n">
-        <v>2540</v>
+        <v>1374</v>
       </c>
       <c r="K30" t="n">
-        <v>0.082</v>
+        <v>0.044</v>
       </c>
       <c r="L30" t="n">
-        <v>3089</v>
+        <v>2603</v>
       </c>
       <c r="M30" t="n">
-        <v>0.099</v>
+        <v>0.084</v>
       </c>
       <c r="N30" t="s">
         <v>197</v>
@@ -3968,7 +3962,7 @@
         <v>203</v>
       </c>
       <c r="C31" s="1" t="n">
-        <v>44023</v>
+        <v>44025</v>
       </c>
       <c r="D31" t="s">
         <v>204</v>
@@ -3978,25 +3972,25 @@
       </c>
       <c r="F31"/>
       <c r="G31" t="n">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="H31" t="n">
-        <v>371167</v>
+        <v>382452</v>
       </c>
       <c r="I31" t="n">
-        <v>35.61</v>
+        <v>36.693</v>
       </c>
       <c r="J31" t="n">
-        <v>7755</v>
+        <v>8520</v>
       </c>
       <c r="K31" t="n">
-        <v>0.744</v>
+        <v>0.817</v>
       </c>
       <c r="L31" t="n">
-        <v>5638</v>
+        <v>6018</v>
       </c>
       <c r="M31" t="n">
-        <v>0.541</v>
+        <v>0.577</v>
       </c>
       <c r="N31" t="s">
         <v>206</v>
@@ -4066,7 +4060,7 @@
         <v>218</v>
       </c>
       <c r="C33" s="1" t="n">
-        <v>44020</v>
+        <v>44025</v>
       </c>
       <c r="D33" t="s">
         <v>219</v>
@@ -4078,21 +4072,25 @@
         <v>221</v>
       </c>
       <c r="G33" t="n">
-        <v>124</v>
+        <v>130</v>
       </c>
       <c r="H33" t="n">
-        <v>288693</v>
+        <v>295561</v>
       </c>
       <c r="I33" t="n">
-        <v>29.884</v>
-      </c>
-      <c r="J33"/>
-      <c r="K33"/>
+        <v>30.595</v>
+      </c>
+      <c r="J33" t="n">
+        <v>1136</v>
+      </c>
+      <c r="K33" t="n">
+        <v>0.118</v>
+      </c>
       <c r="L33" t="n">
-        <v>1563</v>
+        <v>1354</v>
       </c>
       <c r="M33" t="n">
-        <v>0.162</v>
+        <v>0.14</v>
       </c>
       <c r="N33" t="s">
         <v>220</v>
@@ -4115,7 +4113,7 @@
         <v>226</v>
       </c>
       <c r="C34" s="1" t="n">
-        <v>44022</v>
+        <v>44023</v>
       </c>
       <c r="D34" t="s">
         <v>227</v>
@@ -4125,25 +4123,25 @@
       </c>
       <c r="F34"/>
       <c r="G34" t="n">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="H34" t="n">
-        <v>67729</v>
+        <v>67792</v>
       </c>
       <c r="I34" t="n">
-        <v>198.473</v>
+        <v>198.658</v>
       </c>
       <c r="J34" t="n">
-        <v>211</v>
+        <v>63</v>
       </c>
       <c r="K34" t="n">
-        <v>0.618</v>
+        <v>0.185</v>
       </c>
       <c r="L34" t="n">
-        <v>152</v>
+        <v>140</v>
       </c>
       <c r="M34" t="n">
-        <v>0.445</v>
+        <v>0.41</v>
       </c>
       <c r="N34" t="s">
         <v>228</v>
@@ -4219,7 +4217,7 @@
         <v>236</v>
       </c>
       <c r="C36" s="1" t="n">
-        <v>44023</v>
+        <v>44025</v>
       </c>
       <c r="D36" t="s">
         <v>232</v>
@@ -4231,25 +4229,25 @@
         <v>234</v>
       </c>
       <c r="G36" t="n">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="H36" t="n">
-        <v>11307002</v>
+        <v>11806256</v>
       </c>
       <c r="I36" t="n">
-        <v>8.193</v>
+        <v>8.555</v>
       </c>
       <c r="J36" t="n">
-        <v>282511</v>
+        <v>219103</v>
       </c>
       <c r="K36" t="n">
-        <v>0.205</v>
+        <v>0.159</v>
       </c>
       <c r="L36" t="n">
-        <v>252410</v>
+        <v>262371</v>
       </c>
       <c r="M36" t="n">
-        <v>0.183</v>
+        <v>0.19</v>
       </c>
       <c r="N36" t="s">
         <v>233</v>
@@ -4272,7 +4270,7 @@
         <v>238</v>
       </c>
       <c r="C37" s="1" t="n">
-        <v>44023</v>
+        <v>44025</v>
       </c>
       <c r="D37" t="s">
         <v>239</v>
@@ -4282,25 +4280,25 @@
       </c>
       <c r="F37"/>
       <c r="G37" t="n">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="H37" t="n">
-        <v>610093</v>
+        <v>630149</v>
       </c>
       <c r="I37" t="n">
-        <v>2.23</v>
+        <v>2.304</v>
       </c>
       <c r="J37" t="n">
-        <v>12625</v>
+        <v>9062</v>
       </c>
       <c r="K37" t="n">
-        <v>0.046</v>
+        <v>0.033</v>
       </c>
       <c r="L37" t="n">
-        <v>11489</v>
+        <v>11152</v>
       </c>
       <c r="M37" t="n">
-        <v>0.042</v>
+        <v>0.041</v>
       </c>
       <c r="N37" t="s">
         <v>240</v>
@@ -4323,7 +4321,7 @@
         <v>245</v>
       </c>
       <c r="C38" s="1" t="n">
-        <v>44023</v>
+        <v>44025</v>
       </c>
       <c r="D38" t="s">
         <v>246</v>
@@ -4333,25 +4331,25 @@
       </c>
       <c r="F38"/>
       <c r="G38" t="n">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="H38" t="n">
-        <v>1947114</v>
+        <v>1997967</v>
       </c>
       <c r="I38" t="n">
-        <v>23.182</v>
+        <v>23.787</v>
       </c>
       <c r="J38" t="n">
-        <v>24613</v>
+        <v>25760</v>
       </c>
       <c r="K38" t="n">
-        <v>0.293</v>
+        <v>0.307</v>
       </c>
       <c r="L38" t="n">
-        <v>25371</v>
+        <v>25423</v>
       </c>
       <c r="M38" t="n">
-        <v>0.302</v>
+        <v>0.303</v>
       </c>
       <c r="N38" t="s">
         <v>247</v>
@@ -4374,7 +4372,7 @@
         <v>251</v>
       </c>
       <c r="C39" s="1" t="n">
-        <v>44023</v>
+        <v>44025</v>
       </c>
       <c r="D39" t="s">
         <v>252</v>
@@ -4384,25 +4382,25 @@
       </c>
       <c r="F39"/>
       <c r="G39" t="n">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="H39" t="n">
-        <v>500578</v>
+        <v>516958</v>
       </c>
       <c r="I39" t="n">
-        <v>101.377</v>
+        <v>104.694</v>
       </c>
       <c r="J39" t="n">
-        <v>8929</v>
+        <v>7663</v>
       </c>
       <c r="K39" t="n">
-        <v>1.808</v>
+        <v>1.552</v>
       </c>
       <c r="L39" t="n">
-        <v>6608</v>
+        <v>7015</v>
       </c>
       <c r="M39" t="n">
-        <v>1.338</v>
+        <v>1.421</v>
       </c>
       <c r="N39" t="s">
         <v>253</v>
@@ -4425,7 +4423,7 @@
         <v>256</v>
       </c>
       <c r="C40" s="1" t="n">
-        <v>44014</v>
+        <v>44017</v>
       </c>
       <c r="D40" t="s">
         <v>257</v>
@@ -4435,25 +4433,25 @@
       </c>
       <c r="F40"/>
       <c r="G40" t="n">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="H40" t="n">
-        <v>1047501</v>
+        <v>1106807</v>
       </c>
       <c r="I40" t="n">
-        <v>121.021</v>
+        <v>127.873</v>
       </c>
       <c r="J40" t="n">
-        <v>25040</v>
+        <v>21056</v>
       </c>
       <c r="K40" t="n">
-        <v>2.893</v>
+        <v>2.433</v>
       </c>
       <c r="L40" t="n">
-        <v>17964</v>
+        <v>21094</v>
       </c>
       <c r="M40" t="n">
-        <v>2.075</v>
+        <v>2.437</v>
       </c>
       <c r="N40" t="s">
         <v>40</v>
@@ -4476,7 +4474,7 @@
         <v>262</v>
       </c>
       <c r="C41" s="1" t="n">
-        <v>44023</v>
+        <v>44025</v>
       </c>
       <c r="D41" t="s">
         <v>263</v>
@@ -4488,25 +4486,25 @@
         <v>265</v>
       </c>
       <c r="G41" t="n">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="H41" t="n">
-        <v>3545826</v>
+        <v>3582893</v>
       </c>
       <c r="I41" t="n">
-        <v>58.646</v>
+        <v>59.259</v>
       </c>
       <c r="J41" t="n">
-        <v>25449</v>
+        <v>14006</v>
       </c>
       <c r="K41" t="n">
-        <v>0.421</v>
+        <v>0.232</v>
       </c>
       <c r="L41" t="n">
-        <v>24108</v>
+        <v>24412</v>
       </c>
       <c r="M41" t="n">
-        <v>0.399</v>
+        <v>0.404</v>
       </c>
       <c r="N41" t="s">
         <v>266</v>
@@ -4529,7 +4527,7 @@
         <v>269</v>
       </c>
       <c r="C42" s="1" t="n">
-        <v>44023</v>
+        <v>44025</v>
       </c>
       <c r="D42" t="s">
         <v>263</v>
@@ -4541,25 +4539,25 @@
         <v>265</v>
       </c>
       <c r="G42" t="n">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="H42" t="n">
-        <v>5900552</v>
+        <v>5962744</v>
       </c>
       <c r="I42" t="n">
-        <v>97.591</v>
+        <v>98.62</v>
       </c>
       <c r="J42" t="n">
-        <v>45931</v>
+        <v>23933</v>
       </c>
       <c r="K42" t="n">
-        <v>0.76</v>
+        <v>0.396</v>
       </c>
       <c r="L42" t="n">
-        <v>42818</v>
+        <v>43184</v>
       </c>
       <c r="M42" t="n">
-        <v>0.708</v>
+        <v>0.714</v>
       </c>
       <c r="N42" t="s">
         <v>266</v>
@@ -4582,7 +4580,7 @@
         <v>272</v>
       </c>
       <c r="C43" s="1" t="n">
-        <v>44023</v>
+        <v>44025</v>
       </c>
       <c r="D43" t="s">
         <v>273</v>
@@ -4594,25 +4592,25 @@
         <v>275</v>
       </c>
       <c r="G43" t="n">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="H43" t="n">
-        <v>551658</v>
+        <v>562105</v>
       </c>
       <c r="I43" t="n">
-        <v>4.362</v>
+        <v>4.444</v>
       </c>
       <c r="J43" t="n">
-        <v>11247</v>
+        <v>3483</v>
       </c>
       <c r="K43" t="n">
-        <v>0.089</v>
+        <v>0.028</v>
       </c>
       <c r="L43" t="n">
-        <v>8767</v>
+        <v>8887</v>
       </c>
       <c r="M43" t="n">
-        <v>0.069</v>
+        <v>0.07</v>
       </c>
       <c r="N43" t="s">
         <v>276</v>
@@ -4635,7 +4633,7 @@
         <v>279</v>
       </c>
       <c r="C44" s="1" t="n">
-        <v>44021</v>
+        <v>44023</v>
       </c>
       <c r="D44" t="s">
         <v>280</v>
@@ -4647,25 +4645,25 @@
         <v>281</v>
       </c>
       <c r="G44" t="n">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="H44" t="n">
-        <v>768069</v>
+        <v>774017</v>
       </c>
       <c r="I44" t="n">
-        <v>6.073</v>
+        <v>6.12</v>
       </c>
       <c r="J44" t="n">
-        <v>7500</v>
+        <v>2838</v>
       </c>
       <c r="K44" t="n">
-        <v>0.059</v>
+        <v>0.022</v>
       </c>
       <c r="L44" t="n">
-        <v>9728</v>
+        <v>7664</v>
       </c>
       <c r="M44" t="n">
-        <v>0.077</v>
+        <v>0.061</v>
       </c>
       <c r="N44" t="s">
         <v>276</v>
@@ -4790,7 +4788,7 @@
         <v>296</v>
       </c>
       <c r="C47" s="1" t="n">
-        <v>44022</v>
+        <v>44025</v>
       </c>
       <c r="D47" t="s">
         <v>297</v>
@@ -4800,25 +4798,25 @@
       </c>
       <c r="F47"/>
       <c r="G47" t="n">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="H47" t="n">
-        <v>427006</v>
+        <v>437422</v>
       </c>
       <c r="I47" t="n">
-        <v>99.988</v>
+        <v>102.427</v>
       </c>
       <c r="J47" t="n">
-        <v>4121</v>
+        <v>4086</v>
       </c>
       <c r="K47" t="n">
-        <v>0.965</v>
+        <v>0.957</v>
       </c>
       <c r="L47" t="n">
-        <v>3930</v>
+        <v>4012</v>
       </c>
       <c r="M47" t="n">
-        <v>0.92</v>
+        <v>0.939</v>
       </c>
       <c r="N47" t="s">
         <v>298</v>
@@ -4841,7 +4839,7 @@
         <v>302</v>
       </c>
       <c r="C48" s="1" t="n">
-        <v>44023</v>
+        <v>44025</v>
       </c>
       <c r="D48" t="s">
         <v>303</v>
@@ -4853,25 +4851,25 @@
         <v>305</v>
       </c>
       <c r="G48" t="n">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="H48" t="n">
-        <v>167480</v>
+        <v>169943</v>
       </c>
       <c r="I48" t="n">
-        <v>88.792</v>
+        <v>90.098</v>
       </c>
       <c r="J48" t="n">
-        <v>1870</v>
+        <v>996</v>
       </c>
       <c r="K48" t="n">
-        <v>0.991</v>
+        <v>0.528</v>
       </c>
       <c r="L48" t="n">
-        <v>1528</v>
+        <v>1632</v>
       </c>
       <c r="M48" t="n">
-        <v>0.81</v>
+        <v>0.865</v>
       </c>
       <c r="N48" t="s">
         <v>304</v>
@@ -4894,219 +4892,215 @@
         <v>308</v>
       </c>
       <c r="C49" s="1" t="n">
-        <v>44022</v>
+        <v>44025</v>
       </c>
       <c r="D49" t="s">
-        <v>309</v>
+        <v>32</v>
       </c>
       <c r="E49" t="s">
         <v>40</v>
       </c>
       <c r="F49"/>
       <c r="G49" t="n">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="H49" t="n">
-        <v>455833</v>
+        <v>461666</v>
       </c>
       <c r="I49" t="n">
-        <v>167.445</v>
-      </c>
-      <c r="J49" t="n">
-        <v>3846</v>
-      </c>
-      <c r="K49" t="n">
-        <v>1.413</v>
-      </c>
+        <v>169.587</v>
+      </c>
+      <c r="J49"/>
+      <c r="K49"/>
       <c r="L49" t="n">
-        <v>2736</v>
+        <v>2742</v>
       </c>
       <c r="M49" t="n">
-        <v>1.005</v>
+        <v>1.007</v>
       </c>
       <c r="N49" t="s">
         <v>40</v>
       </c>
       <c r="O49" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="P49" t="s">
         <v>50</v>
       </c>
       <c r="Q49" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
+        <v>311</v>
+      </c>
+      <c r="B50" t="s">
         <v>312</v>
       </c>
-      <c r="B50" t="s">
-        <v>313</v>
-      </c>
       <c r="C50" s="1" t="n">
-        <v>44023</v>
+        <v>44025</v>
       </c>
       <c r="D50" t="s">
         <v>32</v>
       </c>
       <c r="E50" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="F50"/>
       <c r="G50" t="n">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="H50" t="n">
-        <v>273866</v>
+        <v>281431</v>
       </c>
       <c r="I50" t="n">
-        <v>437.502</v>
+        <v>449.588</v>
       </c>
       <c r="J50" t="n">
-        <v>7429</v>
+        <v>3043</v>
       </c>
       <c r="K50" t="n">
-        <v>11.868</v>
+        <v>4.861</v>
       </c>
       <c r="L50" t="n">
-        <v>7771</v>
+        <v>7810</v>
       </c>
       <c r="M50" t="n">
-        <v>12.414</v>
+        <v>12.477</v>
       </c>
       <c r="N50" t="s">
+        <v>313</v>
+      </c>
+      <c r="O50" t="s">
         <v>314</v>
-      </c>
-      <c r="O50" t="s">
-        <v>315</v>
       </c>
       <c r="P50" t="s">
         <v>22</v>
       </c>
       <c r="Q50" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
+        <v>316</v>
+      </c>
+      <c r="B51" t="s">
         <v>317</v>
       </c>
-      <c r="B51" t="s">
+      <c r="C51" s="1" t="n">
+        <v>44025</v>
+      </c>
+      <c r="D51" t="s">
         <v>318</v>
       </c>
-      <c r="C51" s="1" t="n">
-        <v>44023</v>
-      </c>
-      <c r="D51" t="s">
+      <c r="E51" t="s">
         <v>319</v>
       </c>
-      <c r="E51" t="s">
+      <c r="F51" t="s">
         <v>320</v>
       </c>
-      <c r="F51" t="s">
-        <v>321</v>
-      </c>
       <c r="G51" t="n">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="H51" t="n">
-        <v>842476</v>
+        <v>850423</v>
       </c>
       <c r="I51" t="n">
-        <v>26.03</v>
+        <v>26.275</v>
       </c>
       <c r="J51" t="n">
-        <v>6221</v>
+        <v>2913</v>
       </c>
       <c r="K51" t="n">
-        <v>0.192</v>
+        <v>0.09</v>
       </c>
       <c r="L51" t="n">
-        <v>6383</v>
+        <v>5767</v>
       </c>
       <c r="M51" t="n">
-        <v>0.197</v>
+        <v>0.178</v>
       </c>
       <c r="N51" t="s">
         <v>40</v>
       </c>
       <c r="O51" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="P51" t="s">
         <v>89</v>
       </c>
       <c r="Q51" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
+        <v>323</v>
+      </c>
+      <c r="B52" t="s">
         <v>324</v>
       </c>
-      <c r="B52" t="s">
+      <c r="C52" s="1" t="n">
+        <v>44025</v>
+      </c>
+      <c r="D52" t="s">
         <v>325</v>
       </c>
-      <c r="C52" s="1" t="n">
-        <v>44021</v>
-      </c>
-      <c r="D52" t="s">
+      <c r="E52" t="s">
         <v>326</v>
-      </c>
-      <c r="E52" t="s">
-        <v>327</v>
       </c>
       <c r="F52"/>
       <c r="G52" t="n">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="H52" t="n">
-        <v>59530</v>
+        <v>62767</v>
       </c>
       <c r="I52" t="n">
-        <v>110.13</v>
+        <v>116.119</v>
       </c>
       <c r="J52" t="n">
-        <v>947</v>
+        <v>948</v>
       </c>
       <c r="K52" t="n">
-        <v>1.752</v>
+        <v>1.754</v>
       </c>
       <c r="L52" t="n">
-        <v>938</v>
+        <v>836</v>
       </c>
       <c r="M52" t="n">
-        <v>1.735</v>
+        <v>1.547</v>
       </c>
       <c r="N52" t="s">
+        <v>327</v>
+      </c>
+      <c r="O52" t="s">
         <v>328</v>
-      </c>
-      <c r="O52" t="s">
-        <v>329</v>
       </c>
       <c r="P52" t="s">
         <v>50</v>
       </c>
       <c r="Q52" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
+        <v>330</v>
+      </c>
+      <c r="B53" t="s">
         <v>331</v>
-      </c>
-      <c r="B53" t="s">
-        <v>332</v>
       </c>
       <c r="C53" s="1" t="n">
         <v>44019</v>
       </c>
       <c r="D53" t="s">
+        <v>332</v>
+      </c>
+      <c r="E53" t="s">
         <v>333</v>
-      </c>
-      <c r="E53" t="s">
-        <v>334</v>
       </c>
       <c r="F53"/>
       <c r="G53" t="n">
@@ -5131,33 +5125,33 @@
         <v>1.875</v>
       </c>
       <c r="N53" t="s">
+        <v>333</v>
+      </c>
+      <c r="O53" t="s">
         <v>334</v>
-      </c>
-      <c r="O53" t="s">
-        <v>335</v>
       </c>
       <c r="P53" t="s">
         <v>22</v>
       </c>
       <c r="Q53" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
+        <v>336</v>
+      </c>
+      <c r="B54" t="s">
         <v>337</v>
-      </c>
-      <c r="B54" t="s">
-        <v>338</v>
       </c>
       <c r="C54" s="1" t="n">
         <v>44018</v>
       </c>
       <c r="D54" t="s">
+        <v>338</v>
+      </c>
+      <c r="E54" t="s">
         <v>339</v>
-      </c>
-      <c r="E54" t="s">
-        <v>340</v>
       </c>
       <c r="F54"/>
       <c r="G54" t="n">
@@ -5182,84 +5176,84 @@
         <v>0.071</v>
       </c>
       <c r="N54" t="s">
+        <v>340</v>
+      </c>
+      <c r="O54" t="s">
         <v>341</v>
-      </c>
-      <c r="O54" t="s">
-        <v>342</v>
       </c>
       <c r="P54" t="s">
         <v>242</v>
       </c>
       <c r="Q54" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
+        <v>343</v>
+      </c>
+      <c r="B55" t="s">
         <v>344</v>
       </c>
-      <c r="B55" t="s">
+      <c r="C55" s="1" t="n">
+        <v>44024</v>
+      </c>
+      <c r="D55" t="s">
         <v>345</v>
       </c>
-      <c r="C55" s="1" t="n">
-        <v>44022</v>
-      </c>
-      <c r="D55" t="s">
+      <c r="E55" t="s">
         <v>346</v>
-      </c>
-      <c r="E55" t="s">
-        <v>347</v>
       </c>
       <c r="F55"/>
       <c r="G55" t="n">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="H55" t="n">
-        <v>849097</v>
+        <v>878626</v>
       </c>
       <c r="I55" t="n">
-        <v>23.004</v>
+        <v>23.804</v>
       </c>
       <c r="J55" t="n">
-        <v>13833</v>
+        <v>14032</v>
       </c>
       <c r="K55" t="n">
-        <v>0.375</v>
+        <v>0.38</v>
       </c>
       <c r="L55" t="n">
-        <v>16658</v>
+        <v>16149</v>
       </c>
       <c r="M55" t="n">
-        <v>0.451</v>
+        <v>0.438</v>
       </c>
       <c r="N55" t="s">
+        <v>346</v>
+      </c>
+      <c r="O55" t="s">
         <v>347</v>
-      </c>
-      <c r="O55" t="s">
-        <v>348</v>
       </c>
       <c r="P55" t="s">
         <v>242</v>
       </c>
       <c r="Q55" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
+        <v>349</v>
+      </c>
+      <c r="B56" t="s">
         <v>350</v>
-      </c>
-      <c r="B56" t="s">
-        <v>351</v>
       </c>
       <c r="C56" s="1" t="n">
         <v>44021</v>
       </c>
       <c r="D56" t="s">
+        <v>351</v>
+      </c>
+      <c r="E56" t="s">
         <v>352</v>
-      </c>
-      <c r="E56" t="s">
-        <v>353</v>
       </c>
       <c r="F56"/>
       <c r="G56" t="n">
@@ -5284,36 +5278,36 @@
         <v>0.024</v>
       </c>
       <c r="N56" t="s">
+        <v>352</v>
+      </c>
+      <c r="O56" t="s">
         <v>353</v>
-      </c>
-      <c r="O56" t="s">
-        <v>354</v>
       </c>
       <c r="P56" t="s">
         <v>50</v>
       </c>
       <c r="Q56" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="s">
+        <v>355</v>
+      </c>
+      <c r="B57" t="s">
         <v>356</v>
-      </c>
-      <c r="B57" t="s">
-        <v>357</v>
       </c>
       <c r="C57" s="1" t="n">
         <v>43996</v>
       </c>
       <c r="D57" t="s">
+        <v>357</v>
+      </c>
+      <c r="E57" t="s">
         <v>358</v>
       </c>
-      <c r="E57" t="s">
+      <c r="F57" t="s">
         <v>359</v>
-      </c>
-      <c r="F57" t="s">
-        <v>360</v>
       </c>
       <c r="G57" t="n">
         <v>115</v>
@@ -5337,33 +5331,33 @@
         <v>0.182</v>
       </c>
       <c r="N57" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="O57" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="P57" t="s">
         <v>89</v>
       </c>
       <c r="Q57" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="s">
+        <v>362</v>
+      </c>
+      <c r="B58" t="s">
         <v>363</v>
-      </c>
-      <c r="B58" t="s">
-        <v>364</v>
       </c>
       <c r="C58" s="1" t="n">
         <v>44018</v>
       </c>
       <c r="D58" t="s">
+        <v>364</v>
+      </c>
+      <c r="E58" t="s">
         <v>365</v>
-      </c>
-      <c r="E58" t="s">
-        <v>366</v>
       </c>
       <c r="F58"/>
       <c r="G58" t="n">
@@ -5388,335 +5382,335 @@
         <v>0.49</v>
       </c>
       <c r="N58" t="s">
+        <v>366</v>
+      </c>
+      <c r="O58" t="s">
         <v>367</v>
-      </c>
-      <c r="O58" t="s">
-        <v>368</v>
       </c>
       <c r="P58" t="s">
         <v>89</v>
       </c>
       <c r="Q58" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="s">
+        <v>369</v>
+      </c>
+      <c r="B59" t="s">
         <v>370</v>
       </c>
-      <c r="B59" t="s">
+      <c r="C59" s="1" t="n">
+        <v>44024</v>
+      </c>
+      <c r="D59" t="s">
         <v>371</v>
-      </c>
-      <c r="C59" s="1" t="n">
-        <v>44022</v>
-      </c>
-      <c r="D59" t="s">
-        <v>372</v>
       </c>
       <c r="E59" t="s">
         <v>40</v>
       </c>
       <c r="F59"/>
       <c r="G59" t="n">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="H59" t="n">
-        <v>426776</v>
+        <v>429643</v>
       </c>
       <c r="I59" t="n">
-        <v>88.502</v>
+        <v>89.096</v>
       </c>
       <c r="J59" t="n">
-        <v>2057</v>
+        <v>1043</v>
       </c>
       <c r="K59" t="n">
-        <v>0.427</v>
+        <v>0.216</v>
       </c>
       <c r="L59" t="n">
-        <v>2121</v>
+        <v>2051</v>
       </c>
       <c r="M59" t="n">
-        <v>0.44</v>
+        <v>0.425</v>
       </c>
       <c r="N59" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="O59" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="P59" t="s">
         <v>22</v>
       </c>
       <c r="Q59" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="s">
+        <v>374</v>
+      </c>
+      <c r="B60" t="s">
         <v>375</v>
       </c>
-      <c r="B60" t="s">
-        <v>376</v>
-      </c>
       <c r="C60" s="1" t="n">
-        <v>44023</v>
+        <v>44025</v>
       </c>
       <c r="D60" t="s">
         <v>32</v>
       </c>
       <c r="E60" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="F60"/>
       <c r="G60" t="n">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="H60" t="n">
-        <v>178265</v>
+        <v>183294</v>
       </c>
       <c r="I60" t="n">
-        <v>0.865</v>
+        <v>0.889</v>
       </c>
       <c r="J60" t="n">
-        <v>2609</v>
+        <v>2046</v>
       </c>
       <c r="K60" t="n">
-        <v>0.013</v>
+        <v>0.01</v>
       </c>
       <c r="L60" t="n">
-        <v>4297</v>
+        <v>4335</v>
       </c>
       <c r="M60" t="n">
         <v>0.021</v>
       </c>
       <c r="N60" t="s">
+        <v>376</v>
+      </c>
+      <c r="O60" t="s">
         <v>377</v>
-      </c>
-      <c r="O60" t="s">
-        <v>378</v>
       </c>
       <c r="P60" t="s">
         <v>50</v>
       </c>
       <c r="Q60" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="s">
+        <v>379</v>
+      </c>
+      <c r="B61" t="s">
         <v>380</v>
       </c>
-      <c r="B61" t="s">
+      <c r="C61" s="1" t="n">
+        <v>44023</v>
+      </c>
+      <c r="D61" t="s">
         <v>381</v>
       </c>
-      <c r="C61" s="1" t="n">
-        <v>44020</v>
-      </c>
-      <c r="D61" t="s">
+      <c r="E61" t="s">
         <v>382</v>
-      </c>
-      <c r="E61" t="s">
-        <v>383</v>
       </c>
       <c r="F61"/>
       <c r="G61" t="n">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="H61" t="n">
-        <v>351563</v>
+        <v>360090</v>
       </c>
       <c r="I61" t="n">
-        <v>64.849</v>
+        <v>66.422</v>
       </c>
       <c r="J61" t="n">
-        <v>3707</v>
+        <v>776</v>
       </c>
       <c r="K61" t="n">
-        <v>0.684</v>
+        <v>0.143</v>
       </c>
       <c r="L61" t="n">
-        <v>3353</v>
+        <v>3284</v>
       </c>
       <c r="M61" t="n">
-        <v>0.618</v>
+        <v>0.606</v>
       </c>
       <c r="N61" t="s">
+        <v>382</v>
+      </c>
+      <c r="O61" t="s">
         <v>383</v>
       </c>
-      <c r="O61" t="s">
+      <c r="P61" t="s">
         <v>384</v>
       </c>
-      <c r="P61" t="s">
+      <c r="Q61" t="s">
         <v>385</v>
-      </c>
-      <c r="Q61" t="s">
-        <v>386</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="s">
+        <v>386</v>
+      </c>
+      <c r="B62" t="s">
         <v>387</v>
       </c>
-      <c r="B62" t="s">
+      <c r="C62" s="1" t="n">
+        <v>44025</v>
+      </c>
+      <c r="D62" t="s">
         <v>388</v>
       </c>
-      <c r="C62" s="1" t="n">
-        <v>44023</v>
-      </c>
-      <c r="D62" t="s">
+      <c r="E62" t="s">
         <v>389</v>
-      </c>
-      <c r="E62" t="s">
-        <v>390</v>
       </c>
       <c r="F62"/>
       <c r="G62" t="n">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="H62"/>
       <c r="I62"/>
       <c r="J62" t="n">
-        <v>3833</v>
+        <v>6173</v>
       </c>
       <c r="K62" t="n">
-        <v>0.751</v>
+        <v>1.209</v>
       </c>
       <c r="L62" t="n">
-        <v>4175</v>
+        <v>4514</v>
       </c>
       <c r="M62" t="n">
-        <v>0.818</v>
+        <v>0.884</v>
       </c>
       <c r="N62" t="s">
+        <v>389</v>
+      </c>
+      <c r="O62" t="s">
         <v>390</v>
-      </c>
-      <c r="O62" t="s">
-        <v>391</v>
       </c>
       <c r="P62" t="s">
         <v>89</v>
       </c>
       <c r="Q62" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="s">
+        <v>392</v>
+      </c>
+      <c r="B63" t="s">
         <v>393</v>
       </c>
-      <c r="B63" t="s">
-        <v>394</v>
-      </c>
       <c r="C63" s="1" t="n">
-        <v>44023</v>
+        <v>44025</v>
       </c>
       <c r="D63" t="s">
         <v>32</v>
       </c>
       <c r="E63" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="F63"/>
       <c r="G63" t="n">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="H63" t="n">
-        <v>1538427</v>
+        <v>1585170</v>
       </c>
       <c r="I63" t="n">
-        <v>6.965</v>
+        <v>7.176</v>
       </c>
       <c r="J63" t="n">
-        <v>23569</v>
+        <v>22532</v>
       </c>
       <c r="K63" t="n">
-        <v>0.107</v>
+        <v>0.102</v>
       </c>
       <c r="L63" t="n">
-        <v>23657</v>
+        <v>23507</v>
       </c>
       <c r="M63" t="n">
-        <v>0.107</v>
+        <v>0.106</v>
       </c>
       <c r="N63" t="s">
+        <v>394</v>
+      </c>
+      <c r="O63" t="s">
         <v>395</v>
-      </c>
-      <c r="O63" t="s">
-        <v>396</v>
       </c>
       <c r="P63" t="s">
         <v>22</v>
       </c>
       <c r="Q63" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="s">
+        <v>397</v>
+      </c>
+      <c r="B64" t="s">
         <v>398</v>
       </c>
-      <c r="B64" t="s">
+      <c r="C64" s="1" t="n">
+        <v>44024</v>
+      </c>
+      <c r="D64" t="s">
         <v>399</v>
       </c>
-      <c r="C64" s="1" t="n">
-        <v>44021</v>
-      </c>
-      <c r="D64" t="s">
+      <c r="E64" t="s">
         <v>400</v>
-      </c>
-      <c r="E64" t="s">
-        <v>401</v>
       </c>
       <c r="F64"/>
       <c r="G64" t="n">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="H64" t="n">
-        <v>152642</v>
+        <v>162005</v>
       </c>
       <c r="I64" t="n">
-        <v>35.377</v>
+        <v>37.547</v>
       </c>
       <c r="J64" t="n">
-        <v>2498</v>
+        <v>3435</v>
       </c>
       <c r="K64" t="n">
-        <v>0.579</v>
+        <v>0.796</v>
       </c>
       <c r="L64" t="n">
-        <v>2820</v>
+        <v>2863</v>
       </c>
       <c r="M64" t="n">
-        <v>0.654</v>
+        <v>0.664</v>
       </c>
       <c r="N64" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="O64" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="P64" t="s">
         <v>22</v>
       </c>
       <c r="Q64" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="s">
+        <v>402</v>
+      </c>
+      <c r="B65" t="s">
         <v>403</v>
-      </c>
-      <c r="B65" t="s">
-        <v>404</v>
       </c>
       <c r="C65" s="1" t="n">
         <v>44022</v>
       </c>
       <c r="D65" t="s">
+        <v>404</v>
+      </c>
+      <c r="E65" t="s">
         <v>405</v>
-      </c>
-      <c r="E65" t="s">
-        <v>406</v>
       </c>
       <c r="F65"/>
       <c r="G65" t="n">
@@ -5741,234 +5735,230 @@
         <v>0.263</v>
       </c>
       <c r="N65" t="s">
+        <v>405</v>
+      </c>
+      <c r="O65" t="s">
         <v>406</v>
-      </c>
-      <c r="O65" t="s">
-        <v>407</v>
       </c>
       <c r="P65" t="s">
         <v>89</v>
       </c>
       <c r="Q65" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="s">
+        <v>408</v>
+      </c>
+      <c r="B66" t="s">
         <v>409</v>
       </c>
-      <c r="B66" t="s">
+      <c r="C66" s="1" t="n">
+        <v>44024</v>
+      </c>
+      <c r="D66" t="s">
         <v>410</v>
-      </c>
-      <c r="C66" s="1" t="n">
-        <v>44023</v>
-      </c>
-      <c r="D66" t="s">
-        <v>411</v>
       </c>
       <c r="E66" t="s">
         <v>40</v>
       </c>
       <c r="F66"/>
       <c r="G66" t="n">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="H66" t="n">
-        <v>283886</v>
+        <v>290234</v>
       </c>
       <c r="I66" t="n">
-        <v>8.61</v>
+        <v>8.802</v>
       </c>
       <c r="J66" t="n">
-        <v>4113</v>
+        <v>6348</v>
       </c>
       <c r="K66" t="n">
-        <v>0.125</v>
+        <v>0.193</v>
       </c>
       <c r="L66" t="n">
-        <v>3550</v>
+        <v>4090</v>
       </c>
       <c r="M66" t="n">
-        <v>0.108</v>
+        <v>0.124</v>
       </c>
       <c r="N66" t="s">
+        <v>411</v>
+      </c>
+      <c r="O66" t="s">
         <v>412</v>
-      </c>
-      <c r="O66" t="s">
-        <v>413</v>
       </c>
       <c r="P66" t="s">
         <v>89</v>
       </c>
       <c r="Q66" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="s">
+        <v>414</v>
+      </c>
+      <c r="B67" t="s">
         <v>415</v>
       </c>
-      <c r="B67" t="s">
+      <c r="C67" s="1" t="n">
+        <v>44023</v>
+      </c>
+      <c r="D67" t="s">
         <v>416</v>
       </c>
-      <c r="C67" s="1" t="n">
-        <v>44021</v>
-      </c>
-      <c r="D67" t="s">
+      <c r="E67" t="s">
         <v>417</v>
-      </c>
-      <c r="E67" t="s">
-        <v>418</v>
       </c>
       <c r="F67"/>
       <c r="G67" t="n">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="H67" t="n">
-        <v>870162</v>
+        <v>910924</v>
       </c>
       <c r="I67" t="n">
-        <v>7.941</v>
-      </c>
-      <c r="J67" t="n">
-        <v>23742</v>
-      </c>
-      <c r="K67" t="n">
-        <v>0.217</v>
-      </c>
+        <v>8.313</v>
+      </c>
+      <c r="J67"/>
+      <c r="K67"/>
       <c r="L67" t="n">
-        <v>21234</v>
+        <v>21405</v>
       </c>
       <c r="M67" t="n">
-        <v>0.194</v>
+        <v>0.195</v>
       </c>
       <c r="N67" t="s">
         <v>213</v>
       </c>
       <c r="O67" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="P67" t="s">
         <v>89</v>
       </c>
       <c r="Q67" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="s">
+        <v>419</v>
+      </c>
+      <c r="B68" t="s">
         <v>420</v>
       </c>
-      <c r="B68" t="s">
+      <c r="C68" s="1" t="n">
+        <v>44025</v>
+      </c>
+      <c r="D68" t="s">
         <v>421</v>
       </c>
-      <c r="C68" s="1" t="n">
-        <v>44023</v>
-      </c>
-      <c r="D68" t="s">
+      <c r="E68" t="s">
         <v>422</v>
-      </c>
-      <c r="E68" t="s">
-        <v>423</v>
       </c>
       <c r="F68"/>
       <c r="G68" t="n">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="H68" t="n">
-        <v>1581440</v>
+        <v>1605344</v>
       </c>
       <c r="I68" t="n">
-        <v>41.786</v>
+        <v>42.417</v>
       </c>
       <c r="J68" t="n">
-        <v>32734</v>
+        <v>10709</v>
       </c>
       <c r="K68" t="n">
-        <v>0.865</v>
+        <v>0.283</v>
       </c>
       <c r="L68" t="n">
-        <v>20513</v>
+        <v>20062</v>
       </c>
       <c r="M68" t="n">
-        <v>0.542</v>
+        <v>0.53</v>
       </c>
       <c r="N68" t="s">
+        <v>422</v>
+      </c>
+      <c r="O68" t="s">
         <v>423</v>
-      </c>
-      <c r="O68" t="s">
-        <v>424</v>
       </c>
       <c r="P68" t="s">
         <v>89</v>
       </c>
       <c r="Q68" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="B69" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="C69" s="1" t="n">
-        <v>44023</v>
+        <v>44025</v>
       </c>
       <c r="D69" t="s">
+        <v>421</v>
+      </c>
+      <c r="E69" t="s">
         <v>422</v>
-      </c>
-      <c r="E69" t="s">
-        <v>423</v>
       </c>
       <c r="F69"/>
       <c r="G69" t="n">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="H69" t="n">
-        <v>1779643</v>
+        <v>1813365</v>
       </c>
       <c r="I69" t="n">
-        <v>47.023</v>
+        <v>47.914</v>
       </c>
       <c r="J69" t="n">
-        <v>35012</v>
+        <v>15753</v>
       </c>
       <c r="K69" t="n">
-        <v>0.925</v>
+        <v>0.416</v>
       </c>
       <c r="L69" t="n">
-        <v>22783</v>
+        <v>22529</v>
       </c>
       <c r="M69" t="n">
-        <v>0.602</v>
+        <v>0.595</v>
       </c>
       <c r="N69" t="s">
+        <v>422</v>
+      </c>
+      <c r="O69" t="s">
         <v>423</v>
-      </c>
-      <c r="O69" t="s">
-        <v>424</v>
       </c>
       <c r="P69" t="s">
         <v>50</v>
       </c>
       <c r="Q69" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="s">
+        <v>427</v>
+      </c>
+      <c r="B70" t="s">
         <v>428</v>
-      </c>
-      <c r="B70" t="s">
-        <v>429</v>
       </c>
       <c r="C70" s="1" t="n">
         <v>44019</v>
       </c>
       <c r="D70" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="E70" t="s">
         <v>40</v>
@@ -5996,186 +5986,186 @@
         <v>1.312</v>
       </c>
       <c r="N70" t="s">
+        <v>430</v>
+      </c>
+      <c r="O70" t="s">
+        <v>429</v>
+      </c>
+      <c r="P70" t="s">
         <v>431</v>
       </c>
-      <c r="O70" t="s">
-        <v>430</v>
-      </c>
-      <c r="P70" t="s">
+      <c r="Q70" t="s">
         <v>432</v>
-      </c>
-      <c r="Q70" t="s">
-        <v>433</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="s">
+        <v>433</v>
+      </c>
+      <c r="B71" t="s">
         <v>434</v>
       </c>
-      <c r="B71" t="s">
+      <c r="C71" s="1" t="n">
+        <v>44024</v>
+      </c>
+      <c r="D71" t="s">
         <v>435</v>
       </c>
-      <c r="C71" s="1" t="n">
-        <v>44023</v>
-      </c>
-      <c r="D71" t="s">
+      <c r="E71" t="s">
         <v>436</v>
-      </c>
-      <c r="E71" t="s">
-        <v>437</v>
       </c>
       <c r="F71"/>
       <c r="G71" t="n">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="H71" t="n">
-        <v>409199</v>
+        <v>412682</v>
       </c>
       <c r="I71" t="n">
-        <v>142.031</v>
+        <v>143.24</v>
       </c>
       <c r="J71" t="n">
-        <v>4331</v>
+        <v>3483</v>
       </c>
       <c r="K71" t="n">
-        <v>1.503</v>
+        <v>1.209</v>
       </c>
       <c r="L71" t="n">
-        <v>4617</v>
+        <v>4464</v>
       </c>
       <c r="M71" t="n">
-        <v>1.603</v>
+        <v>1.549</v>
       </c>
       <c r="N71" t="s">
+        <v>436</v>
+      </c>
+      <c r="O71" t="s">
         <v>437</v>
-      </c>
-      <c r="O71" t="s">
-        <v>438</v>
       </c>
       <c r="P71" t="s">
         <v>89</v>
       </c>
       <c r="Q71" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="s">
+        <v>439</v>
+      </c>
+      <c r="B72" t="s">
         <v>440</v>
       </c>
-      <c r="B72" t="s">
+      <c r="C72" s="1" t="n">
+        <v>44025</v>
+      </c>
+      <c r="D72" t="s">
         <v>441</v>
       </c>
-      <c r="C72" s="1" t="n">
-        <v>44023</v>
-      </c>
-      <c r="D72" t="s">
+      <c r="E72" t="s">
         <v>442</v>
-      </c>
-      <c r="E72" t="s">
-        <v>443</v>
       </c>
       <c r="F72"/>
       <c r="G72" t="n">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="H72" t="n">
-        <v>838953</v>
+        <v>854241</v>
       </c>
       <c r="I72" t="n">
-        <v>43.61</v>
+        <v>44.405</v>
       </c>
       <c r="J72" t="n">
-        <v>14610</v>
+        <v>6655</v>
       </c>
       <c r="K72" t="n">
-        <v>0.759</v>
+        <v>0.346</v>
       </c>
       <c r="L72" t="n">
-        <v>11417</v>
+        <v>12482</v>
       </c>
       <c r="M72" t="n">
-        <v>0.593</v>
+        <v>0.649</v>
       </c>
       <c r="N72" t="s">
+        <v>443</v>
+      </c>
+      <c r="O72" t="s">
         <v>444</v>
-      </c>
-      <c r="O72" t="s">
-        <v>445</v>
       </c>
       <c r="P72" t="s">
         <v>22</v>
       </c>
       <c r="Q72" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="s">
+        <v>446</v>
+      </c>
+      <c r="B73" t="s">
         <v>447</v>
       </c>
-      <c r="B73" t="s">
+      <c r="C73" s="1" t="n">
+        <v>44025</v>
+      </c>
+      <c r="D73" t="s">
         <v>448</v>
       </c>
-      <c r="C73" s="1" t="n">
-        <v>44023</v>
-      </c>
-      <c r="D73" t="s">
+      <c r="E73" t="s">
         <v>449</v>
-      </c>
-      <c r="E73" t="s">
-        <v>450</v>
       </c>
       <c r="F73"/>
       <c r="G73" t="n">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="H73" t="n">
-        <v>22708416</v>
+        <v>23292630</v>
       </c>
       <c r="I73" t="n">
-        <v>155.607</v>
+        <v>159.61</v>
       </c>
       <c r="J73" t="n">
-        <v>320221</v>
+        <v>261574</v>
       </c>
       <c r="K73" t="n">
-        <v>2.194</v>
+        <v>1.792</v>
       </c>
       <c r="L73" t="n">
-        <v>279430</v>
+        <v>279605</v>
       </c>
       <c r="M73" t="n">
-        <v>1.915</v>
+        <v>1.916</v>
       </c>
       <c r="N73" t="s">
+        <v>449</v>
+      </c>
+      <c r="O73" t="s">
         <v>450</v>
-      </c>
-      <c r="O73" t="s">
-        <v>451</v>
       </c>
       <c r="P73" t="s">
         <v>22</v>
       </c>
       <c r="Q73" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="s">
+        <v>452</v>
+      </c>
+      <c r="B74" t="s">
         <v>453</v>
-      </c>
-      <c r="B74" t="s">
-        <v>454</v>
       </c>
       <c r="C74" s="1" t="n">
         <v>44022</v>
       </c>
       <c r="D74" t="s">
+        <v>454</v>
+      </c>
+      <c r="E74" t="s">
         <v>455</v>
-      </c>
-      <c r="E74" t="s">
-        <v>456</v>
       </c>
       <c r="F74"/>
       <c r="G74" t="n">
@@ -6200,187 +6190,187 @@
         <v>0.247</v>
       </c>
       <c r="N74" t="s">
+        <v>455</v>
+      </c>
+      <c r="O74" t="s">
         <v>456</v>
-      </c>
-      <c r="O74" t="s">
-        <v>457</v>
       </c>
       <c r="P74" t="s">
         <v>50</v>
       </c>
       <c r="Q74" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="s">
+        <v>458</v>
+      </c>
+      <c r="B75" t="s">
         <v>459</v>
       </c>
-      <c r="B75" t="s">
+      <c r="C75" s="1" t="n">
+        <v>44025</v>
+      </c>
+      <c r="D75" t="s">
         <v>460</v>
-      </c>
-      <c r="C75" s="1" t="n">
-        <v>44023</v>
-      </c>
-      <c r="D75" t="s">
-        <v>461</v>
       </c>
       <c r="E75" t="s">
         <v>40</v>
       </c>
       <c r="F75"/>
       <c r="G75" t="n">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="H75" t="n">
-        <v>2217002</v>
+        <v>2327586</v>
       </c>
       <c r="I75" t="n">
-        <v>63.682</v>
+        <v>66.858</v>
       </c>
       <c r="J75" t="n">
-        <v>46842</v>
+        <v>66155</v>
       </c>
       <c r="K75" t="n">
-        <v>1.345</v>
+        <v>1.9</v>
       </c>
       <c r="L75" t="n">
-        <v>56177</v>
+        <v>56171</v>
       </c>
       <c r="M75" t="n">
-        <v>1.614</v>
+        <v>1.613</v>
       </c>
       <c r="N75" t="s">
         <v>40</v>
       </c>
       <c r="O75" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="P75" t="s">
         <v>123</v>
       </c>
       <c r="Q75" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="s">
+        <v>462</v>
+      </c>
+      <c r="B76" t="s">
         <v>463</v>
       </c>
-      <c r="B76" t="s">
+      <c r="C76" s="1" t="n">
+        <v>44025</v>
+      </c>
+      <c r="D76" t="s">
         <v>464</v>
       </c>
-      <c r="C76" s="1" t="n">
-        <v>44023</v>
-      </c>
-      <c r="D76" t="s">
+      <c r="E76" t="s">
         <v>465</v>
       </c>
-      <c r="E76" t="s">
+      <c r="F76" t="s">
         <v>466</v>
       </c>
-      <c r="F76" t="s">
-        <v>467</v>
-      </c>
       <c r="G76" t="n">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="H76" t="n">
-        <v>89229</v>
+        <v>91047</v>
       </c>
       <c r="I76" t="n">
-        <v>5.329</v>
+        <v>5.438</v>
       </c>
       <c r="J76" t="n">
-        <v>700</v>
+        <v>710</v>
       </c>
       <c r="K76" t="n">
         <v>0.042</v>
       </c>
       <c r="L76" t="n">
-        <v>802</v>
+        <v>834</v>
       </c>
       <c r="M76" t="n">
-        <v>0.048</v>
+        <v>0.05</v>
       </c>
       <c r="N76" t="s">
+        <v>467</v>
+      </c>
+      <c r="O76" t="s">
         <v>468</v>
       </c>
-      <c r="O76" t="s">
+      <c r="P76" t="s">
         <v>469</v>
       </c>
-      <c r="P76" t="s">
+      <c r="Q76" t="s">
         <v>470</v>
-      </c>
-      <c r="Q76" t="s">
-        <v>471</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="s">
+        <v>471</v>
+      </c>
+      <c r="B77" t="s">
         <v>472</v>
       </c>
-      <c r="B77" t="s">
+      <c r="C77" s="1" t="n">
+        <v>44025</v>
+      </c>
+      <c r="D77" t="s">
         <v>473</v>
-      </c>
-      <c r="C77" s="1" t="n">
-        <v>44023</v>
-      </c>
-      <c r="D77" t="s">
-        <v>474</v>
       </c>
       <c r="E77" t="s">
         <v>40</v>
       </c>
       <c r="F77" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="G77" t="n">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="H77" t="n">
-        <v>487378</v>
+        <v>498343</v>
       </c>
       <c r="I77" t="n">
-        <v>71.625</v>
+        <v>73.236</v>
       </c>
       <c r="J77" t="n">
-        <v>7032</v>
+        <v>6915</v>
       </c>
       <c r="K77" t="n">
-        <v>1.033</v>
+        <v>1.016</v>
       </c>
       <c r="L77" t="n">
-        <v>7566</v>
+        <v>7289</v>
       </c>
       <c r="M77" t="n">
-        <v>1.112</v>
+        <v>1.071</v>
       </c>
       <c r="N77" t="s">
         <v>40</v>
       </c>
       <c r="O77" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="P77" t="s">
         <v>89</v>
       </c>
       <c r="Q77" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="s">
+        <v>477</v>
+      </c>
+      <c r="B78" t="s">
         <v>478</v>
-      </c>
-      <c r="B78" t="s">
-        <v>479</v>
       </c>
       <c r="C78" s="1" t="n">
         <v>44018</v>
       </c>
       <c r="D78" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="E78" t="s">
         <v>40</v>
@@ -6407,27 +6397,27 @@
         <v>40</v>
       </c>
       <c r="O78" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="P78" t="s">
         <v>89</v>
       </c>
       <c r="Q78" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B79" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="C79" s="1" t="n">
         <v>44018</v>
       </c>
       <c r="D79" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="E79" t="s">
         <v>40</v>
@@ -6454,274 +6444,274 @@
         <v>40</v>
       </c>
       <c r="O79" t="s">
+        <v>480</v>
+      </c>
+      <c r="P79" t="s">
+        <v>484</v>
+      </c>
+      <c r="Q79" t="s">
         <v>481</v>
-      </c>
-      <c r="P79" t="s">
-        <v>485</v>
-      </c>
-      <c r="Q79" t="s">
-        <v>482</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="s">
+        <v>485</v>
+      </c>
+      <c r="B80" t="s">
         <v>486</v>
       </c>
-      <c r="B80" t="s">
-        <v>487</v>
-      </c>
       <c r="C80" s="1" t="n">
-        <v>44023</v>
+        <v>44024</v>
       </c>
       <c r="D80" t="s">
         <v>32</v>
       </c>
       <c r="E80" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="F80"/>
       <c r="G80" t="n">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="H80" t="n">
-        <v>228829</v>
+        <v>229789</v>
       </c>
       <c r="I80" t="n">
-        <v>41.913</v>
+        <v>42.089</v>
       </c>
       <c r="J80" t="n">
-        <v>2879</v>
+        <v>960</v>
       </c>
       <c r="K80" t="n">
-        <v>0.527</v>
+        <v>0.176</v>
       </c>
       <c r="L80" t="n">
-        <v>1613</v>
+        <v>1635</v>
       </c>
       <c r="M80" t="n">
-        <v>0.295</v>
+        <v>0.299</v>
       </c>
       <c r="N80" t="s">
+        <v>488</v>
+      </c>
+      <c r="O80" t="s">
         <v>489</v>
       </c>
-      <c r="O80" t="s">
+      <c r="P80" t="s">
         <v>490</v>
       </c>
-      <c r="P80" t="s">
+      <c r="Q80" t="s">
         <v>491</v>
-      </c>
-      <c r="Q80" t="s">
-        <v>492</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="s">
+        <v>492</v>
+      </c>
+      <c r="B81" t="s">
         <v>493</v>
       </c>
-      <c r="B81" t="s">
+      <c r="C81" s="1" t="n">
+        <v>44024</v>
+      </c>
+      <c r="D81" t="s">
         <v>494</v>
       </c>
-      <c r="C81" s="1" t="n">
-        <v>44022</v>
-      </c>
-      <c r="D81" t="s">
+      <c r="E81" t="s">
         <v>495</v>
-      </c>
-      <c r="E81" t="s">
-        <v>496</v>
       </c>
       <c r="F81"/>
       <c r="G81" t="n">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="H81" t="n">
-        <v>113665</v>
+        <v>114665</v>
       </c>
       <c r="I81" t="n">
-        <v>54.675</v>
+        <v>55.156</v>
       </c>
       <c r="J81" t="n">
-        <v>1169</v>
+        <v>450</v>
       </c>
       <c r="K81" t="n">
-        <v>0.562</v>
+        <v>0.216</v>
       </c>
       <c r="L81" t="n">
-        <v>1145</v>
+        <v>1110</v>
       </c>
       <c r="M81" t="n">
-        <v>0.551</v>
+        <v>0.534</v>
       </c>
       <c r="N81" t="s">
+        <v>496</v>
+      </c>
+      <c r="O81" t="s">
         <v>497</v>
-      </c>
-      <c r="O81" t="s">
-        <v>498</v>
       </c>
       <c r="P81" t="s">
         <v>22</v>
       </c>
       <c r="Q81" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="s">
+        <v>499</v>
+      </c>
+      <c r="B82" t="s">
         <v>500</v>
       </c>
-      <c r="B82" t="s">
+      <c r="C82" s="1" t="n">
+        <v>44024</v>
+      </c>
+      <c r="D82" t="s">
         <v>501</v>
       </c>
-      <c r="C82" s="1" t="n">
-        <v>44022</v>
-      </c>
-      <c r="D82" t="s">
+      <c r="E82" t="s">
         <v>502</v>
       </c>
-      <c r="E82" t="s">
+      <c r="F82" t="s">
         <v>503</v>
       </c>
-      <c r="F82" t="s">
+      <c r="G82" t="n">
+        <v>134</v>
+      </c>
+      <c r="H82" t="n">
+        <v>2154391</v>
+      </c>
+      <c r="I82" t="n">
+        <v>36.325</v>
+      </c>
+      <c r="J82" t="n">
+        <v>45821</v>
+      </c>
+      <c r="K82" t="n">
+        <v>0.773</v>
+      </c>
+      <c r="L82" t="n">
+        <v>46319</v>
+      </c>
+      <c r="M82" t="n">
+        <v>0.781</v>
+      </c>
+      <c r="N82" t="s">
+        <v>502</v>
+      </c>
+      <c r="O82" t="s">
         <v>504</v>
-      </c>
-      <c r="G82" t="n">
-        <v>132</v>
-      </c>
-      <c r="H82" t="n">
-        <v>2057232</v>
-      </c>
-      <c r="I82" t="n">
-        <v>34.687</v>
-      </c>
-      <c r="J82" t="n">
-        <v>56663</v>
-      </c>
-      <c r="K82" t="n">
-        <v>0.955</v>
-      </c>
-      <c r="L82" t="n">
-        <v>44583</v>
-      </c>
-      <c r="M82" t="n">
-        <v>0.752</v>
-      </c>
-      <c r="N82" t="s">
-        <v>503</v>
-      </c>
-      <c r="O82" t="s">
-        <v>505</v>
       </c>
       <c r="P82" t="s">
         <v>89</v>
       </c>
       <c r="Q82" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="s">
+        <v>506</v>
+      </c>
+      <c r="B83" t="s">
         <v>507</v>
       </c>
-      <c r="B83" t="s">
+      <c r="C83" s="1" t="n">
+        <v>44025</v>
+      </c>
+      <c r="D83" t="s">
         <v>508</v>
       </c>
-      <c r="C83" s="1" t="n">
-        <v>44023</v>
-      </c>
-      <c r="D83" t="s">
+      <c r="E83" t="s">
         <v>509</v>
-      </c>
-      <c r="E83" t="s">
-        <v>510</v>
       </c>
       <c r="F83"/>
       <c r="G83" t="n">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="H83" t="n">
-        <v>1373414</v>
+        <v>1386467</v>
       </c>
       <c r="I83" t="n">
-        <v>26.788</v>
+        <v>27.043</v>
       </c>
       <c r="J83" t="n">
-        <v>12436</v>
+        <v>7273</v>
       </c>
       <c r="K83" t="n">
-        <v>0.243</v>
+        <v>0.142</v>
       </c>
       <c r="L83" t="n">
-        <v>10887</v>
+        <v>10903</v>
       </c>
       <c r="M83" t="n">
-        <v>0.212</v>
+        <v>0.213</v>
       </c>
       <c r="N83" t="s">
+        <v>509</v>
+      </c>
+      <c r="O83" t="s">
         <v>510</v>
-      </c>
-      <c r="O83" t="s">
-        <v>511</v>
       </c>
       <c r="P83" t="s">
         <v>89</v>
       </c>
       <c r="Q83" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="s">
+        <v>512</v>
+      </c>
+      <c r="B84" t="s">
         <v>513</v>
       </c>
-      <c r="B84" t="s">
+      <c r="C84" s="1" t="n">
+        <v>44021</v>
+      </c>
+      <c r="D84" t="s">
         <v>514</v>
       </c>
-      <c r="C84" s="1" t="n">
-        <v>44014</v>
-      </c>
-      <c r="D84" t="s">
+      <c r="E84" t="s">
         <v>515</v>
-      </c>
-      <c r="E84" t="s">
-        <v>516</v>
       </c>
       <c r="F84"/>
       <c r="G84" t="n">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H84" t="n">
-        <v>3644458</v>
+        <v>3849701</v>
       </c>
       <c r="I84" t="n">
-        <v>77.948</v>
+        <v>82.338</v>
       </c>
       <c r="J84"/>
       <c r="K84"/>
       <c r="L84" t="n">
-        <v>24904</v>
+        <v>29320</v>
       </c>
       <c r="M84" t="n">
-        <v>0.533</v>
+        <v>0.627</v>
       </c>
       <c r="N84" t="s">
+        <v>516</v>
+      </c>
+      <c r="O84" t="s">
         <v>517</v>
-      </c>
-      <c r="O84" t="s">
-        <v>518</v>
       </c>
       <c r="P84" t="s">
         <v>22</v>
       </c>
       <c r="Q84" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="s">
+        <v>519</v>
+      </c>
+      <c r="B85" t="s">
         <v>520</v>
-      </c>
-      <c r="B85" t="s">
-        <v>521</v>
       </c>
       <c r="C85" s="1" t="n">
         <v>44017</v>
@@ -6730,7 +6720,7 @@
         <v>32</v>
       </c>
       <c r="E85" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="F85"/>
       <c r="G85" t="n">
@@ -6751,84 +6741,84 @@
         <v>1.129</v>
       </c>
       <c r="N85" t="s">
+        <v>522</v>
+      </c>
+      <c r="O85" t="s">
         <v>523</v>
-      </c>
-      <c r="O85" t="s">
-        <v>524</v>
       </c>
       <c r="P85" t="s">
         <v>89</v>
       </c>
       <c r="Q85" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="s">
+        <v>525</v>
+      </c>
+      <c r="B86" t="s">
         <v>526</v>
       </c>
-      <c r="B86" t="s">
+      <c r="C86" s="1" t="n">
+        <v>44023</v>
+      </c>
+      <c r="D86" t="s">
         <v>527</v>
       </c>
-      <c r="C86" s="1" t="n">
-        <v>44022</v>
-      </c>
-      <c r="D86" t="s">
+      <c r="E86" t="s">
         <v>528</v>
-      </c>
-      <c r="E86" t="s">
-        <v>529</v>
       </c>
       <c r="F86"/>
       <c r="G86" t="n">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="H86" t="n">
-        <v>678679</v>
+        <v>684766</v>
       </c>
       <c r="I86" t="n">
-        <v>78.418</v>
+        <v>79.121</v>
       </c>
       <c r="J86" t="n">
-        <v>5966</v>
+        <v>4455</v>
       </c>
       <c r="K86" t="n">
-        <v>0.689</v>
+        <v>0.515</v>
       </c>
       <c r="L86" t="n">
-        <v>7044</v>
+        <v>7036</v>
       </c>
       <c r="M86" t="n">
-        <v>0.814</v>
+        <v>0.813</v>
       </c>
       <c r="N86" t="s">
+        <v>528</v>
+      </c>
+      <c r="O86" t="s">
+        <v>527</v>
+      </c>
+      <c r="P86" t="s">
         <v>529</v>
       </c>
-      <c r="O86" t="s">
-        <v>528</v>
-      </c>
-      <c r="P86" t="s">
+      <c r="Q86" t="s">
         <v>530</v>
-      </c>
-      <c r="Q86" t="s">
-        <v>531</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="s">
+        <v>531</v>
+      </c>
+      <c r="B87" t="s">
         <v>532</v>
-      </c>
-      <c r="B87" t="s">
-        <v>533</v>
       </c>
       <c r="C87" s="1" t="n">
         <v>44019</v>
       </c>
       <c r="D87" t="s">
+        <v>533</v>
+      </c>
+      <c r="E87" t="s">
         <v>534</v>
-      </c>
-      <c r="E87" t="s">
-        <v>535</v>
       </c>
       <c r="F87"/>
       <c r="G87" t="n">
@@ -6849,84 +6839,84 @@
         <v>0.006</v>
       </c>
       <c r="N87" t="s">
+        <v>534</v>
+      </c>
+      <c r="O87" t="s">
         <v>535</v>
       </c>
-      <c r="O87" t="s">
+      <c r="P87" t="s">
         <v>536</v>
       </c>
-      <c r="P87" t="s">
+      <c r="Q87" t="s">
         <v>537</v>
-      </c>
-      <c r="Q87" t="s">
-        <v>538</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="s">
+        <v>538</v>
+      </c>
+      <c r="B88" t="s">
         <v>539</v>
       </c>
-      <c r="B88" t="s">
-        <v>540</v>
-      </c>
       <c r="C88" s="1" t="n">
-        <v>44023</v>
+        <v>44024</v>
       </c>
       <c r="D88" t="s">
         <v>32</v>
       </c>
       <c r="E88" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="F88"/>
       <c r="G88" t="n">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="H88" t="n">
-        <v>329887</v>
+        <v>331018</v>
       </c>
       <c r="I88" t="n">
-        <v>4.726</v>
+        <v>4.742</v>
       </c>
       <c r="J88" t="n">
-        <v>1443</v>
+        <v>1131</v>
       </c>
       <c r="K88" t="n">
-        <v>0.021</v>
+        <v>0.016</v>
       </c>
       <c r="L88" t="n">
-        <v>1610</v>
+        <v>1621</v>
       </c>
       <c r="M88" t="n">
         <v>0.023</v>
       </c>
       <c r="N88" t="s">
+        <v>541</v>
+      </c>
+      <c r="O88" t="s">
         <v>542</v>
-      </c>
-      <c r="O88" t="s">
-        <v>543</v>
       </c>
       <c r="P88" t="s">
         <v>89</v>
       </c>
       <c r="Q88" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="B89" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="C89" s="1" t="n">
         <v>44008</v>
       </c>
       <c r="D89" t="s">
+        <v>545</v>
+      </c>
+      <c r="E89" t="s">
         <v>546</v>
-      </c>
-      <c r="E89" t="s">
-        <v>547</v>
       </c>
       <c r="F89"/>
       <c r="G89" t="n">
@@ -6947,33 +6937,33 @@
         <v>0.072</v>
       </c>
       <c r="N89" t="s">
+        <v>546</v>
+      </c>
+      <c r="O89" t="s">
         <v>547</v>
-      </c>
-      <c r="O89" t="s">
-        <v>548</v>
       </c>
       <c r="P89" t="s">
         <v>50</v>
       </c>
       <c r="Q89" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="s">
+        <v>549</v>
+      </c>
+      <c r="B90" t="s">
         <v>550</v>
-      </c>
-      <c r="B90" t="s">
-        <v>551</v>
       </c>
       <c r="C90" s="1" t="n">
         <v>44022</v>
       </c>
       <c r="D90" t="s">
+        <v>551</v>
+      </c>
+      <c r="E90" t="s">
         <v>552</v>
-      </c>
-      <c r="E90" t="s">
-        <v>553</v>
       </c>
       <c r="F90"/>
       <c r="G90" t="n">
@@ -6998,36 +6988,36 @@
         <v>0.04</v>
       </c>
       <c r="N90" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="O90" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="P90" t="s">
         <v>50</v>
       </c>
       <c r="Q90" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="s">
+        <v>554</v>
+      </c>
+      <c r="B91" t="s">
         <v>555</v>
-      </c>
-      <c r="B91" t="s">
-        <v>556</v>
       </c>
       <c r="C91" s="1" t="n">
         <v>44004</v>
       </c>
       <c r="D91" t="s">
+        <v>556</v>
+      </c>
+      <c r="E91" t="s">
         <v>557</v>
       </c>
-      <c r="E91" t="s">
+      <c r="F91" t="s">
         <v>558</v>
-      </c>
-      <c r="F91" t="s">
-        <v>559</v>
       </c>
       <c r="G91" t="n">
         <v>76</v>
@@ -7051,281 +7041,281 @@
         <v>0.063</v>
       </c>
       <c r="N91" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
       <c r="O91" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="P91" t="s">
         <v>22</v>
       </c>
       <c r="Q91" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="s">
+        <v>561</v>
+      </c>
+      <c r="B92" t="s">
         <v>562</v>
       </c>
-      <c r="B92" t="s">
-        <v>563</v>
-      </c>
       <c r="C92" s="1" t="n">
-        <v>44023</v>
+        <v>44025</v>
       </c>
       <c r="D92" t="s">
         <v>32</v>
       </c>
       <c r="E92" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="F92"/>
       <c r="G92" t="n">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="H92" t="n">
-        <v>3930223</v>
+        <v>4021947</v>
       </c>
       <c r="I92" t="n">
-        <v>46.6</v>
+        <v>47.688</v>
       </c>
       <c r="J92" t="n">
-        <v>48813</v>
+        <v>46492</v>
       </c>
       <c r="K92" t="n">
-        <v>0.579</v>
+        <v>0.551</v>
       </c>
       <c r="L92" t="n">
-        <v>49451</v>
+        <v>48468</v>
       </c>
       <c r="M92" t="n">
-        <v>0.586</v>
+        <v>0.575</v>
       </c>
       <c r="N92" t="s">
+        <v>563</v>
+      </c>
+      <c r="O92" t="s">
         <v>564</v>
-      </c>
-      <c r="O92" t="s">
-        <v>565</v>
       </c>
       <c r="P92" t="s">
         <v>22</v>
       </c>
       <c r="Q92" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="s">
+        <v>566</v>
+      </c>
+      <c r="B93" t="s">
         <v>567</v>
       </c>
-      <c r="B93" t="s">
+      <c r="C93" s="1" t="n">
+        <v>44024</v>
+      </c>
+      <c r="D93" t="s">
         <v>568</v>
       </c>
-      <c r="C93" s="1" t="n">
-        <v>44022</v>
-      </c>
-      <c r="D93" t="s">
+      <c r="E93" t="s">
         <v>569</v>
       </c>
-      <c r="E93" t="s">
+      <c r="F93" t="s">
         <v>570</v>
       </c>
-      <c r="F93" t="s">
+      <c r="G93" t="n">
+        <v>95</v>
+      </c>
+      <c r="H93" t="n">
+        <v>201759</v>
+      </c>
+      <c r="I93" t="n">
+        <v>4.411</v>
+      </c>
+      <c r="J93" t="n">
+        <v>1702</v>
+      </c>
+      <c r="K93" t="n">
+        <v>0.037</v>
+      </c>
+      <c r="L93" t="n">
+        <v>2523</v>
+      </c>
+      <c r="M93" t="n">
+        <v>0.055</v>
+      </c>
+      <c r="N93" t="s">
+        <v>569</v>
+      </c>
+      <c r="O93" t="s">
         <v>571</v>
-      </c>
-      <c r="G93" t="n">
-        <v>93</v>
-      </c>
-      <c r="H93" t="n">
-        <v>197765</v>
-      </c>
-      <c r="I93" t="n">
-        <v>4.324</v>
-      </c>
-      <c r="J93" t="n">
-        <v>2436</v>
-      </c>
-      <c r="K93" t="n">
-        <v>0.053</v>
-      </c>
-      <c r="L93" t="n">
-        <v>2696</v>
-      </c>
-      <c r="M93" t="n">
-        <v>0.059</v>
-      </c>
-      <c r="N93" t="s">
-        <v>570</v>
-      </c>
-      <c r="O93" t="s">
-        <v>572</v>
       </c>
       <c r="P93" t="s">
         <v>50</v>
       </c>
       <c r="Q93" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="s">
+        <v>573</v>
+      </c>
+      <c r="B94" t="s">
         <v>574</v>
       </c>
-      <c r="B94" t="s">
-        <v>575</v>
-      </c>
       <c r="C94" s="1" t="n">
-        <v>44023</v>
+        <v>44025</v>
       </c>
       <c r="D94" t="s">
         <v>32</v>
       </c>
       <c r="E94" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="F94"/>
       <c r="G94" t="n">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="H94" t="n">
-        <v>786843</v>
+        <v>803657</v>
       </c>
       <c r="I94" t="n">
-        <v>17.992</v>
+        <v>18.376</v>
       </c>
       <c r="J94" t="n">
-        <v>13012</v>
+        <v>6977</v>
       </c>
       <c r="K94" t="n">
-        <v>0.298</v>
+        <v>0.16</v>
       </c>
       <c r="L94" t="n">
-        <v>11926</v>
+        <v>11592</v>
       </c>
       <c r="M94" t="n">
-        <v>0.273</v>
+        <v>0.265</v>
       </c>
       <c r="N94" t="s">
+        <v>575</v>
+      </c>
+      <c r="O94" t="s">
         <v>576</v>
       </c>
-      <c r="O94" t="s">
+      <c r="P94" t="s">
         <v>577</v>
       </c>
-      <c r="P94" t="s">
+      <c r="Q94" t="s">
         <v>578</v>
-      </c>
-      <c r="Q94" t="s">
-        <v>579</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="s">
+        <v>579</v>
+      </c>
+      <c r="B95" t="s">
         <v>580</v>
       </c>
-      <c r="B95" t="s">
+      <c r="C95" s="1" t="n">
+        <v>44024</v>
+      </c>
+      <c r="D95" t="s">
         <v>581</v>
       </c>
-      <c r="C95" s="1" t="n">
-        <v>44022</v>
-      </c>
-      <c r="D95" t="s">
+      <c r="E95" t="s">
         <v>582</v>
       </c>
-      <c r="E95" t="s">
+      <c r="F95" t="s">
         <v>583</v>
       </c>
-      <c r="F95" t="s">
-        <v>584</v>
-      </c>
       <c r="G95" t="n">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="H95"/>
       <c r="I95"/>
       <c r="J95" t="n">
-        <v>47000</v>
+        <v>50000</v>
       </c>
       <c r="K95" t="n">
-        <v>4.752</v>
+        <v>5.055</v>
       </c>
       <c r="L95" t="n">
-        <v>47287</v>
+        <v>46716</v>
       </c>
       <c r="M95" t="n">
-        <v>4.781</v>
+        <v>4.723</v>
       </c>
       <c r="N95" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
       <c r="O95" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="P95" t="s">
         <v>50</v>
       </c>
       <c r="Q95" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="s">
+        <v>586</v>
+      </c>
+      <c r="B96" t="s">
         <v>587</v>
       </c>
-      <c r="B96" t="s">
+      <c r="C96" s="1" t="n">
+        <v>44024</v>
+      </c>
+      <c r="D96" t="s">
         <v>588</v>
       </c>
-      <c r="C96" s="1" t="n">
-        <v>44022</v>
-      </c>
-      <c r="D96" t="s">
+      <c r="E96" t="s">
         <v>589</v>
       </c>
-      <c r="E96" t="s">
+      <c r="F96" t="s">
         <v>590</v>
       </c>
-      <c r="F96" t="s">
+      <c r="G96" t="n">
+        <v>104</v>
+      </c>
+      <c r="H96" t="n">
+        <v>7188816</v>
+      </c>
+      <c r="I96" t="n">
+        <v>105.895</v>
+      </c>
+      <c r="J96" t="n">
+        <v>86609</v>
+      </c>
+      <c r="K96" t="n">
+        <v>1.276</v>
+      </c>
+      <c r="L96" t="n">
+        <v>107957</v>
+      </c>
+      <c r="M96" t="n">
+        <v>1.59</v>
+      </c>
+      <c r="N96" t="s">
+        <v>589</v>
+      </c>
+      <c r="O96" t="s">
         <v>591</v>
-      </c>
-      <c r="G96" t="n">
-        <v>102</v>
-      </c>
-      <c r="H96" t="n">
-        <v>6977736</v>
-      </c>
-      <c r="I96" t="n">
-        <v>102.786</v>
-      </c>
-      <c r="J96" t="n">
-        <v>128125</v>
-      </c>
-      <c r="K96" t="n">
-        <v>1.887</v>
-      </c>
-      <c r="L96" t="n">
-        <v>102232</v>
-      </c>
-      <c r="M96" t="n">
-        <v>1.506</v>
-      </c>
-      <c r="N96" t="s">
-        <v>590</v>
-      </c>
-      <c r="O96" t="s">
-        <v>592</v>
       </c>
       <c r="P96" t="s">
         <v>22</v>
       </c>
       <c r="Q96" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="s">
+        <v>593</v>
+      </c>
+      <c r="B97" t="s">
         <v>594</v>
-      </c>
-      <c r="B97" t="s">
-        <v>595</v>
       </c>
       <c r="C97" s="1" t="n">
         <v>44022</v>
@@ -7334,7 +7324,7 @@
         <v>32</v>
       </c>
       <c r="E97" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
       <c r="F97"/>
       <c r="G97" t="n">
@@ -7359,135 +7349,135 @@
         <v>1.956</v>
       </c>
       <c r="N97" t="s">
+        <v>595</v>
+      </c>
+      <c r="O97" t="s">
         <v>596</v>
       </c>
-      <c r="O97" t="s">
+      <c r="P97" t="s">
         <v>597</v>
       </c>
-      <c r="P97" t="s">
+      <c r="Q97" t="s">
         <v>598</v>
-      </c>
-      <c r="Q97" t="s">
-        <v>599</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="B98" t="s">
+        <v>599</v>
+      </c>
+      <c r="C98" s="1" t="n">
+        <v>44024</v>
+      </c>
+      <c r="D98" t="s">
         <v>600</v>
       </c>
-      <c r="C98" s="1" t="n">
-        <v>44022</v>
-      </c>
-      <c r="D98" t="s">
+      <c r="E98" t="s">
         <v>601</v>
-      </c>
-      <c r="E98" t="s">
-        <v>602</v>
       </c>
       <c r="F98"/>
       <c r="G98" t="n">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="H98" t="n">
-        <v>38919421</v>
+        <v>40282176</v>
       </c>
       <c r="I98" t="n">
-        <v>117.58</v>
+        <v>121.697</v>
       </c>
       <c r="J98" t="n">
-        <v>823375</v>
+        <v>728781</v>
       </c>
       <c r="K98" t="n">
-        <v>2.488</v>
+        <v>2.202</v>
       </c>
       <c r="L98" t="n">
-        <v>657534</v>
+        <v>666622</v>
       </c>
       <c r="M98" t="n">
-        <v>1.986</v>
+        <v>2.014</v>
       </c>
       <c r="N98" t="s">
+        <v>601</v>
+      </c>
+      <c r="O98" t="s">
         <v>602</v>
       </c>
-      <c r="O98" t="s">
+      <c r="P98" t="s">
         <v>603</v>
       </c>
-      <c r="P98" t="s">
+      <c r="Q98" t="s">
         <v>604</v>
-      </c>
-      <c r="Q98" t="s">
-        <v>605</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="s">
+        <v>605</v>
+      </c>
+      <c r="B99" t="s">
         <v>606</v>
       </c>
-      <c r="B99" t="s">
+      <c r="C99" s="1" t="n">
+        <v>44024</v>
+      </c>
+      <c r="D99" t="s">
         <v>607</v>
-      </c>
-      <c r="C99" s="1" t="n">
-        <v>44022</v>
-      </c>
-      <c r="D99" t="s">
-        <v>608</v>
       </c>
       <c r="E99" t="s">
         <v>120</v>
       </c>
       <c r="F99"/>
       <c r="G99" t="n">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="H99" t="n">
-        <v>77259</v>
+        <v>78586</v>
       </c>
       <c r="I99" t="n">
-        <v>22.241</v>
+        <v>22.623</v>
       </c>
       <c r="J99" t="n">
-        <v>1224</v>
+        <v>469</v>
       </c>
       <c r="K99" t="n">
-        <v>0.352</v>
+        <v>0.135</v>
       </c>
       <c r="L99" t="n">
-        <v>1112</v>
+        <v>1008</v>
       </c>
       <c r="M99" t="n">
-        <v>0.32</v>
+        <v>0.29</v>
       </c>
       <c r="N99" t="s">
         <v>120</v>
       </c>
       <c r="O99" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="P99" t="s">
         <v>22</v>
       </c>
       <c r="Q99" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="s">
+        <v>610</v>
+      </c>
+      <c r="B100" t="s">
         <v>611</v>
-      </c>
-      <c r="B100" t="s">
-        <v>612</v>
       </c>
       <c r="C100" s="1" t="n">
         <v>43950</v>
       </c>
       <c r="D100" t="s">
+        <v>612</v>
+      </c>
+      <c r="E100" t="s">
         <v>613</v>
-      </c>
-      <c r="E100" t="s">
-        <v>614</v>
       </c>
       <c r="F100"/>
       <c r="G100" t="n">
@@ -7508,33 +7498,33 @@
         <v>0.112</v>
       </c>
       <c r="N100" t="s">
+        <v>613</v>
+      </c>
+      <c r="O100" t="s">
         <v>614</v>
       </c>
-      <c r="O100" t="s">
+      <c r="P100" t="s">
         <v>615</v>
       </c>
-      <c r="P100" t="s">
+      <c r="Q100" t="s">
         <v>616</v>
-      </c>
-      <c r="Q100" t="s">
-        <v>617</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="s">
+        <v>617</v>
+      </c>
+      <c r="B101" t="s">
         <v>618</v>
-      </c>
-      <c r="B101" t="s">
-        <v>619</v>
       </c>
       <c r="C101" s="1" t="n">
         <v>44022</v>
       </c>
       <c r="D101" t="s">
+        <v>619</v>
+      </c>
+      <c r="E101" t="s">
         <v>620</v>
-      </c>
-      <c r="E101" t="s">
-        <v>621</v>
       </c>
       <c r="F101"/>
       <c r="G101" t="n">
@@ -7559,16 +7549,16 @@
         <v>0.037</v>
       </c>
       <c r="N101" t="s">
+        <v>620</v>
+      </c>
+      <c r="O101" t="s">
         <v>621</v>
-      </c>
-      <c r="O101" t="s">
-        <v>622</v>
       </c>
       <c r="P101" t="s">
         <v>22</v>
       </c>
       <c r="Q101" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated testing data for 2020-07-20
</commit_message>
<xml_diff>
--- a/public/data/testing/covid-testing-latest-data-source-details.xlsx
+++ b/public/data/testing/covid-testing-latest-data-source-details.xlsx
@@ -1790,7 +1790,7 @@
     <t xml:space="preserve">Spain - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.mscbs.gob.es/profesionales/saludPublica/ccayes/alertasActual/nCov-China/documentos/COVID-19_pruebas_diagnosticas_09_07_2020.pdf</t>
+    <t xml:space="preserve">https://www.mscbs.gob.es/en/profesionales/saludPublica/ccayes/alertasActual/nCov-China/documentos/COVID-19_pruebas_diagnosticas_16_07_2020.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">Ministry of Health, Consumption and Social Welfare</t>
@@ -6756,7 +6756,7 @@
         <v>519</v>
       </c>
       <c r="C84" s="1" t="n">
-        <v>44021</v>
+        <v>44028</v>
       </c>
       <c r="D84" t="s">
         <v>520</v>
@@ -6766,21 +6766,21 @@
       </c>
       <c r="F84"/>
       <c r="G84" t="n">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H84" t="n">
-        <v>3849701</v>
+        <v>4073664</v>
       </c>
       <c r="I84" t="n">
-        <v>82.338</v>
+        <v>87.128</v>
       </c>
       <c r="J84"/>
       <c r="K84"/>
       <c r="L84" t="n">
-        <v>29320</v>
+        <v>31995</v>
       </c>
       <c r="M84" t="n">
-        <v>0.627</v>
+        <v>0.684</v>
       </c>
       <c r="N84" t="s">
         <v>522</v>

</xml_diff>

<commit_message>
Updated testing data for 2020-07-22
</commit_message>
<xml_diff>
--- a/public/data/testing/covid-testing-latest-data-source-details.xlsx
+++ b/public/data/testing/covid-testing-latest-data-source-details.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="634" uniqueCount="634">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="632" uniqueCount="632">
   <si>
     <t xml:space="preserve">ISO code</t>
   </si>
@@ -71,7 +71,7 @@
     <t xml:space="preserve">Argentina - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.argentina.gob.ar/sites/default/files/20-07-20-reporte-matutino-covid-19.pdf</t>
+    <t xml:space="preserve">https://www.argentina.gob.ar/sites/default/files/22-07-20-reporte-matutino-covid-19.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">Government of Argentina</t>
@@ -232,7 +232,7 @@
     <t xml:space="preserve">Bolivia - units unclear</t>
   </si>
   <si>
-    <t xml:space="preserve">https://minsalud.gob.bo/4406-bolivia-supera-los-2-000-contagios-diarios-de-coronavirus-y-registra-un-total-de-58-138-casos</t>
+    <t xml:space="preserve">https://minsalud.gob.bo/4409-bolivia-suma-1-409-contagios-nuevos-de-coronavirus-con-cifras-altas-en-santa-cruz-y-la-paz</t>
   </si>
   <si>
     <t xml:space="preserve">https://www.minsalud.gob.bo/</t>
@@ -253,13 +253,13 @@
     <t xml:space="preserve">Brazil - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.saude.gov.br/noticias/agencia-saude/47151-laboratorios-publicos-ampliam-em-869-capacidade-de-testagem-para-covid-19-no-brasil</t>
+    <t xml:space="preserve">https://www.saude.gov.br/noticias/agencia-saude/47230-portaria-torna-obrigatoria-notificacao-de-resultados-de-testes-da-covid-19</t>
   </si>
   <si>
     <t xml:space="preserve">Ministry of Health press release</t>
   </si>
   <si>
-    <t xml:space="preserve">Until June 30, 1.4 million RT-PCR exams were performed for Covid-19, 860,604 of which in the national network of public health laboratories and 618,067 in the main private laboratories in the country.</t>
+    <t xml:space="preserve">Until July 21, 2,536,552 million RT-PCR exams were performed for Covid-19, with 1,406,132 in the national network of public health laboratories and 1,130,420 in the main private laboratories in the country.</t>
   </si>
   <si>
     <t xml:space="preserve">Brazil Ministry of Health</t>
@@ -453,7 +453,7 @@
     <t xml:space="preserve">Democratic Republic of Congo - samples tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/CMR_Covid19_RDC/status/1284770764730839040/photo/1</t>
+    <t xml:space="preserve">https://twitter.com/CMR_Covid19_RDC/status/1285506737114624001/photo/1</t>
   </si>
   <si>
     <t xml:space="preserve">DRC COVID-19 Pandemic Response Multisectoral Committee</t>
@@ -471,7 +471,7 @@
     <t xml:space="preserve">Denmark - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://files.ssi.dk/Data-epidemiologisk-rapport-20072020-hj10</t>
+    <t xml:space="preserve">https://files.ssi.dk/Data-Epidemiologiske-Rapport-22072020-gz34</t>
   </si>
   <si>
     <t xml:space="preserve">Statens Serum Institut</t>
@@ -489,7 +489,7 @@
     <t xml:space="preserve">Ecuador - units unclear</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.gestionderiesgos.gob.ec/wp-content/uploads/2020/07/INFOGRAFIA-NACIONALCOVI-19-COE-NACIONAL-19072020-08h00.pdf</t>
+    <t xml:space="preserve">https://www.gestionderiesgos.gob.ec/wp-content/uploads/2020/07/INFOGRAFIA-NACIONALCOVI-19-COE-NACIONAL-08h00-220720201.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">Government of Ecuador</t>
@@ -655,7 +655,7 @@
     <t xml:space="preserve">Germany - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.rki.de/DE/Content/InfAZ/N/Neuartiges_Coronavirus/Situationsberichte/2020-07-15-de.pdf?__blob=publicationFile</t>
+    <t xml:space="preserve">https://www.rki.de/DE/Content/InfAZ/N/Neuartiges_Coronavirus/Situationsberichte/2020-07-22-de.pdf?__blob=publicationFile</t>
   </si>
   <si>
     <t xml:space="preserve">Robert Koch Institut</t>
@@ -671,13 +671,14 @@
   </si>
   <si>
     <t xml:space="preserve">To determine how many laboratory tests regarding SARS-CoV-2 are carried out per calendar week in Germany and how many tests are positive or negative, the RKI has started a Germany-wide laboratory query. However, the number of laboratories reporting data seems to vary from week to week.
-The report published on 15th July states that “from the beginning of the collection up to and including calendar week 28/2020”:
-– The cumulative total of samples tested was 6,884,614;
-- For calendar week 28 (which ends 12th July), 171 labs reported 503,220 samples tested;
-- For calendar week 27 (which ends 5th July), 146 labs reported 499,486 samples tested;
-- For calendar week 26 (which ends 28 June), 176 labs reported 462,641 samples tested;
-- For calendar week 25 (which ends 21 June), 172 labs reported 384,142 samples tested;
-- For calendar week 24 (which ends 14 June), 170 labs reported 325,430 samples tested;
+The report published on 22nd July states that “from the beginning of the collection up to and including calendar week 29/2020”:
+– The cumulative total of samples tested was 7,418,812;
+- For calendar week 29 (which ends 19th July), 168 labs reported 531,571 samples tested;
+- For calendar week 28 (which ends 12th July), 175 labs reported 504,596 samples tested;
+- For calendar week 27 (which ends 5th July), 148 labs reported 500,122 samples tested;
+- For calendar week 26 (which ends 28 June), 177 labs reported 462,942 samples tested;
+- For calendar week 25 (which ends 21 June), 173 labs reported 384,311 samples tested;
+- For calendar week 24 (which ends 14 June), 171 labs reported 325,575 samples tested;
 - For calendar week 23 (which ends 7 June), 176 labs reported 340,986 samples tested;
 - For calendar week 22 (which ends 31 May), 178 labs reported 405,269 samples tested;
 - For calendar week 21( which ends 24 May), 179 labs reported 353,467 samples tested;
@@ -729,7 +730,7 @@
     <t xml:space="preserve">Greece - samples tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://eody.gov.gr/covid-gr-daily-report-20200719-new/</t>
+    <t xml:space="preserve">https://eody.gov.gr/covid-gr-daily-report-20200722/</t>
   </si>
   <si>
     <t xml:space="preserve">National Organization of Public Health</t>
@@ -872,7 +873,7 @@
     <t xml:space="preserve">Iran - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">http://irangov.ir/detail/343561</t>
+    <t xml:space="preserve">http://irangov.ir/detail/343755</t>
   </si>
   <si>
     <t xml:space="preserve">Government of Iran</t>
@@ -909,7 +910,7 @@
     <t xml:space="preserve">Israel - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://govextra.gov.il/media/22630/covid19-data-israel-13072020.csv</t>
+    <t xml:space="preserve">https://govextra.gov.il/media/22812/covid19-data-israel-15072020.csv</t>
   </si>
   <si>
     <t xml:space="preserve">Israel Ministry of Health</t>
@@ -968,7 +969,7 @@
     <t xml:space="preserve">Japan - people tested (incl. non-PCR)</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.mhlw.go.jp/stf/newpage_12545.html</t>
+    <t xml:space="preserve">https://www.mhlw.go.jp/stf/newpage_12601.html</t>
   </si>
   <si>
     <t xml:space="preserve">Ministry of Health, Labor and Welfare Press Release</t>
@@ -993,10 +994,10 @@
     <t xml:space="preserve">Japan - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.mhlw.go.jp/content/10906000/000650558.pdf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The cumulative total reported in the press release (877,982) does not sum to the cumulative total calculated from the weekly and daily figures reported by the MOH. See: https://www.mhlw.go.jp/content/10906000/000650558.pdf</t>
+    <t xml:space="preserve">https://www.mhlw.go.jp/content/10906000/000651651.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The cumulative total reported in the press release (925,078) does not sum to the cumulative total calculated from the weekly and daily figures reported by the MOH. See: https://www.mhlw.go.jp/content/10906000/000651651.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">On 11th April 2020, the MOH started providing a daily time series on the "Implementation status of PCR tests for new coronavirus in Japan (based on the date on which results were determined" (via Google translate). 
@@ -1051,7 +1052,7 @@
     <t xml:space="preserve">Kuwait - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/KUWAIT_MOH/status/1284450396220661760/photo/1</t>
+    <t xml:space="preserve">https://twitter.com/KUWAIT_MOH/status/1285537534559363073/photo/1</t>
   </si>
   <si>
     <t xml:space="preserve">Kuwait Ministry of Health</t>
@@ -1123,7 +1124,7 @@
     <t xml:space="preserve">Malaysia - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">http://covid-19.moh.gov.my/terkini/072020/situasi-terkini-20-julai-2020</t>
+    <t xml:space="preserve">http://covid-19.moh.gov.my/terkini/072020/situasi-terkini-22-julai-2020</t>
   </si>
   <si>
     <t xml:space="preserve">Ministry of Health Malaysia</t>
@@ -1149,7 +1150,7 @@
     <t xml:space="preserve">Maldives - samples tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/HPA_MV/status/1284895969772003328/photo/1</t>
+    <t xml:space="preserve">https://twitter.com/HPA_MV/status/1285620754772615169/photo/1</t>
   </si>
   <si>
     <t xml:space="preserve">Maldives Health Protection Agency</t>
@@ -1216,7 +1217,7 @@
     <t xml:space="preserve">Morocco - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/Ministere_Sante/status/1284903347787571201/photo/1</t>
+    <t xml:space="preserve">https://twitter.com/Ministere_Sante/status/1285624495139676160/photo/1</t>
   </si>
   <si>
     <t xml:space="preserve">Morocco Ministry of Health</t>
@@ -1256,7 +1257,7 @@
     <t xml:space="preserve">Nepal - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://drive.google.com/drive/folders/1OSUvO0GfeoHOobLoBeBT35baYepNH9yC</t>
+    <t xml:space="preserve">https://drive.google.com/drive/folders/1aX11-9i_J2fMbpxJ7l9N0oykgYWrCeGp</t>
   </si>
   <si>
     <t xml:space="preserve">Ministry of Health and Population</t>
@@ -1315,7 +1316,7 @@
     <t xml:space="preserve">Nigeria - samples tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://covid19.ncdc.gov.ng/</t>
+    <t xml:space="preserve">http://covid19.ncdc.gov.ng/</t>
   </si>
   <si>
     <t xml:space="preserve">Nigeria Centre for Disease Control</t>
@@ -1362,7 +1363,7 @@
     <t xml:space="preserve">Oman - units unclear</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/OmanVSCovid19/status/1285137530615214081</t>
+    <t xml:space="preserve">https://twitter.com/OmanVSCovid19/status/1285862401297047552</t>
   </si>
   <si>
     <t xml:space="preserve">Oman Ministry of Health</t>
@@ -1440,7 +1441,7 @@
     <t xml:space="preserve">Peru - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.gob.pe/institucion/minsa/noticias/212460-minsa-casos-confirmados-por-coronavirus-covid-19-ascienden-a-353-590-en-el-peru-comunicado-n-176</t>
+    <t xml:space="preserve">https://www.gob.pe/institucion/minsa/noticias/214384-minsa-casos-confirmados-por-coronavirus-covid-19-ascienden-a-362-087-en-el-peru-comunicado-n-179</t>
   </si>
   <si>
     <t xml:space="preserve">Ministry of Health, Government of Peru</t>
@@ -1478,7 +1479,7 @@
     <t xml:space="preserve">Poland - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/MZ_GOV_PL/status/1285137375027486720</t>
+    <t xml:space="preserve">https://twitter.com/MZ_GOV_PL/status/1285862151341527040</t>
   </si>
   <si>
     <t xml:space="preserve">Poland Ministry of Health</t>
@@ -1545,7 +1546,7 @@
     <t xml:space="preserve">Romania - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://gov.ro/ro/media/comunicate/buletin-de-presa-18-iulie-2020-ora-13-00&amp;page=1</t>
+    <t xml:space="preserve">https://gov.ro/ro/media/comunicate/informare-21-iulie-ora-13-00&amp;page=1</t>
   </si>
   <si>
     <t xml:space="preserve">Ministry of Internal Affairs</t>
@@ -1568,7 +1569,7 @@
     <t xml:space="preserve">Russia - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://rospotrebnadzor.ru/about/info/news/news_details.php?ELEMENT_ID=14964</t>
+    <t xml:space="preserve">https://rospotrebnadzor.ru/about/info/news/news_details.php?ELEMENT_ID=14985</t>
   </si>
   <si>
     <t xml:space="preserve">Government of the Russian Federation</t>
@@ -1693,16 +1694,13 @@
     <t xml:space="preserve">Slovakia - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://korona.gov.sk/</t>
+    <t xml:space="preserve">https://www.korona.gov.sk/</t>
   </si>
   <si>
     <t xml:space="preserve">National Health Information Centre</t>
   </si>
   <si>
     <t xml:space="preserve">National Center of Health Information and the Slovak Republic Government coronavirus information website</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.korona.gov.sk/</t>
   </si>
   <si>
     <t xml:space="preserve">The number of completed laboratory tests.</t>
@@ -1770,7 +1768,7 @@
     <t xml:space="preserve">South Korea - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.cdc.go.kr/board/board.es?mid=&amp;bid=0030&amp;act=view&amp;list_no=367840&amp;tag=&amp;nPage=1</t>
+    <t xml:space="preserve">https://www.cdc.go.kr/board/board.es?mid=&amp;bid=0030&amp;act=view&amp;list_no=367861&amp;tag=&amp;nPage=1</t>
   </si>
   <si>
     <t xml:space="preserve">South Korea CDC</t>
@@ -1865,24 +1863,19 @@
     <t xml:space="preserve">TWN</t>
   </si>
   <si>
-    <t xml:space="preserve">Taiwan - units unclear</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.cdc.gov.tw/Bulletin/Detail/VTXOjOkSvTvT4YSsYY2pEg?typeid=9</t>
+    <t xml:space="preserve">Taiwan - people tested</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.cdc.gov.tw/Bulletin/Detail/-DA6xPL6BCxG4JdT4Xvz4A?typeid=9</t>
   </si>
   <si>
     <t xml:space="preserve">Taiwan Centers for Disease Control (CDC)</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.cdc.gov.tw/en</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The figures are labelled in the source only as 'tested'. It is unclear whether this relates to the number of individuals tested, or the number of samples tested.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The Taiwanese Centers for Disease Control (CDC) host a dashboard in which they publish the total 'tested' to date, and 'new from yesterday'. It is not clear whether this represents the total number of tests performed, or the number of people tested. The number 'tested' appears to be somewhat greater than the sum of confirmed cases and 'excluded' (i.e. negative) test results. This either suggests that the figure relates to the number of tests performed, or that it relates to the number of people tested but includes some pending results or is affected by reporting delays.
-Although the CDC only show the last day's figures on this dashboard, we can construct a time-series of cumulative tests by looking at previous versions on web archive. Where possible we have tried to take the total test counts at the same time every day (those published at 00:30h), but a complete sequence of archives are not available on this basis. As such, day-to-day variation will be affected by differences in the time of publishing of the data used. Where no data was retreivable for a day, we used the 'new from yesterday' figure to calculate the total for the previous day.
-The date from which the total test figures date back to is not known; the CDC dashboard is unavailable in web archives prior to 21st March.
+    <t xml:space="preserve">https://www.cdc.gov.tw/En</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Taiwan Centers for Disease Control (CDC) publishes regular press releases (usually several times per week) that include the cumulative total of reported cases related to COVID-19. We construct a time series of cumulative tests on the basis of these press releases, and derive the daily number of tests based on the change in the cumulative total. The date from which the cumulative total of tests date back to is not known.
 Note that, due to the way the data is presented by the official source, the time series may be impacted by retrospective revisions made by the source – see our [FAQ here](https://ourworldindata.org/coronavirus-testing#does-your-data-reflect-retrospective-updates-made-by-the-source).</t>
   </si>
   <si>
@@ -2000,7 +1993,7 @@
     <t xml:space="preserve">Uganda - samples tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/MinofHealthUG/status/1285137201962061826/photo/1</t>
+    <t xml:space="preserve">https://twitter.com/MinofHealthUG/status/1285871129584906241/photo/1</t>
   </si>
   <si>
     <t xml:space="preserve">Uganda Ministry of Health</t>
@@ -2064,7 +2057,7 @@
     <t xml:space="preserve">United Kingdom - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://assets.publishing.service.gov.uk/government/uploads/system/uploads/attachment_data/file/902206/2020-07-20-COVID-19-UK-testing-time-series.csv</t>
+    <t xml:space="preserve">https://assets.publishing.service.gov.uk/government/uploads/system/uploads/attachment_data/file/903002/2020-07-22_COVID-19_UK_testing_time_series.csv</t>
   </si>
   <si>
     <t xml:space="preserve">Public Health England/Department of Health and Social Care</t>
@@ -2144,7 +2137,7 @@
     <t xml:space="preserve">Uruguay - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.gub.uy/ministerio-salud-publica/comunicacion/noticias/informacion-interes-actualizada-sobre-coronavirus-covid-19-uruguay-29</t>
+    <t xml:space="preserve">https://www.gub.uy/ministerio-salud-publica/comunicacion/noticias/informacion-interes-actualizada-sobre-coronavirus-covid-19-uruguay-31</t>
   </si>
   <si>
     <t xml:space="preserve">https://www.gub.uy/ministerio-salud-publica/comunicacion/noticias</t>
@@ -2596,7 +2589,7 @@
         <v>18</v>
       </c>
       <c r="C2" s="1" t="n">
-        <v>44032</v>
+        <v>44034</v>
       </c>
       <c r="D2" t="s">
         <v>19</v>
@@ -2606,25 +2599,21 @@
       </c>
       <c r="F2"/>
       <c r="G2" t="n">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="H2" t="n">
-        <v>552306</v>
+        <v>578202</v>
       </c>
       <c r="I2" t="n">
-        <v>12.22</v>
-      </c>
-      <c r="J2" t="n">
-        <v>11068</v>
-      </c>
-      <c r="K2" t="n">
-        <v>0.245</v>
-      </c>
+        <v>12.793</v>
+      </c>
+      <c r="J2"/>
+      <c r="K2"/>
       <c r="L2" t="n">
-        <v>11126</v>
+        <v>11877</v>
       </c>
       <c r="M2" t="n">
-        <v>0.246</v>
+        <v>0.263</v>
       </c>
       <c r="N2" t="s">
         <v>20</v>
@@ -2698,7 +2687,7 @@
         <v>31</v>
       </c>
       <c r="C4" s="1" t="n">
-        <v>44032</v>
+        <v>44034</v>
       </c>
       <c r="D4" t="s">
         <v>32</v>
@@ -2708,25 +2697,25 @@
       </c>
       <c r="F4"/>
       <c r="G4" t="n">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="H4" t="n">
-        <v>798436</v>
+        <v>814681</v>
       </c>
       <c r="I4" t="n">
-        <v>88.652</v>
+        <v>90.456</v>
       </c>
       <c r="J4" t="n">
-        <v>49767</v>
+        <v>9081</v>
       </c>
       <c r="K4" t="n">
-        <v>5.526</v>
+        <v>1.008</v>
       </c>
       <c r="L4" t="n">
-        <v>13974</v>
+        <v>14055</v>
       </c>
       <c r="M4" t="n">
-        <v>1.552</v>
+        <v>1.561</v>
       </c>
       <c r="N4" t="s">
         <v>34</v>
@@ -2749,7 +2738,7 @@
         <v>38</v>
       </c>
       <c r="C5" s="1" t="n">
-        <v>44032</v>
+        <v>44033</v>
       </c>
       <c r="D5" t="s">
         <v>39</v>
@@ -2759,25 +2748,25 @@
       </c>
       <c r="F5"/>
       <c r="G5" t="n">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="H5" t="n">
-        <v>726140</v>
+        <v>744694</v>
       </c>
       <c r="I5" t="n">
-        <v>426.744</v>
+        <v>437.648</v>
       </c>
       <c r="J5" t="n">
-        <v>8417</v>
+        <v>18554</v>
       </c>
       <c r="K5" t="n">
-        <v>4.947</v>
+        <v>10.904</v>
       </c>
       <c r="L5" t="n">
-        <v>8556</v>
+        <v>9892</v>
       </c>
       <c r="M5" t="n">
-        <v>5.028</v>
+        <v>5.813</v>
       </c>
       <c r="N5" t="s">
         <v>41</v>
@@ -2898,7 +2887,7 @@
         <v>58</v>
       </c>
       <c r="C8" s="1" t="n">
-        <v>44028</v>
+        <v>44032</v>
       </c>
       <c r="D8" t="s">
         <v>59</v>
@@ -2908,25 +2897,25 @@
       </c>
       <c r="F8"/>
       <c r="G8" t="n">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="H8" t="n">
-        <v>1110824</v>
+        <v>1138257</v>
       </c>
       <c r="I8" t="n">
-        <v>95.846</v>
+        <v>98.214</v>
       </c>
       <c r="J8" t="n">
-        <v>8754</v>
+        <v>5787</v>
       </c>
       <c r="K8" t="n">
-        <v>0.755</v>
+        <v>0.499</v>
       </c>
       <c r="L8" t="n">
-        <v>8089</v>
+        <v>8323</v>
       </c>
       <c r="M8" t="n">
-        <v>0.698</v>
+        <v>0.718</v>
       </c>
       <c r="N8" t="s">
         <v>60</v>
@@ -2949,7 +2938,7 @@
         <v>65</v>
       </c>
       <c r="C9" s="1" t="n">
-        <v>44030</v>
+        <v>44032</v>
       </c>
       <c r="D9" t="s">
         <v>66</v>
@@ -2959,25 +2948,25 @@
       </c>
       <c r="F9"/>
       <c r="G9" t="n">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="H9" t="n">
-        <v>117164</v>
+        <v>121787</v>
       </c>
       <c r="I9" t="n">
-        <v>10.037</v>
+        <v>10.433</v>
       </c>
       <c r="J9" t="n">
-        <v>2982</v>
+        <v>2023</v>
       </c>
       <c r="K9" t="n">
-        <v>0.255</v>
+        <v>0.173</v>
       </c>
       <c r="L9" t="n">
-        <v>2487</v>
+        <v>2637</v>
       </c>
       <c r="M9" t="n">
-        <v>0.213</v>
+        <v>0.226</v>
       </c>
       <c r="N9" t="s">
         <v>40</v>
@@ -3000,7 +2989,7 @@
         <v>71</v>
       </c>
       <c r="C10" s="1" t="n">
-        <v>44012</v>
+        <v>44033</v>
       </c>
       <c r="D10" t="s">
         <v>72</v>
@@ -3012,18 +3001,22 @@
         <v>74</v>
       </c>
       <c r="G10" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H10" t="n">
-        <v>1478671</v>
+        <v>2536552</v>
       </c>
       <c r="I10" t="n">
-        <v>6.957</v>
+        <v>11.933</v>
       </c>
       <c r="J10"/>
       <c r="K10"/>
-      <c r="L10"/>
-      <c r="M10"/>
+      <c r="L10" t="n">
+        <v>50375</v>
+      </c>
+      <c r="M10" t="n">
+        <v>0.237</v>
+      </c>
       <c r="N10" t="s">
         <v>75</v>
       </c>
@@ -3045,7 +3038,7 @@
         <v>79</v>
       </c>
       <c r="C11" s="1" t="n">
-        <v>44032</v>
+        <v>44033</v>
       </c>
       <c r="D11" t="s">
         <v>80</v>
@@ -3055,25 +3048,25 @@
       </c>
       <c r="F11"/>
       <c r="G11" t="n">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="H11" t="n">
-        <v>206521</v>
+        <v>215572</v>
       </c>
       <c r="I11" t="n">
-        <v>29.722</v>
+        <v>31.024</v>
       </c>
       <c r="J11" t="n">
-        <v>3155</v>
+        <v>9051</v>
       </c>
       <c r="K11" t="n">
-        <v>0.454</v>
+        <v>1.303</v>
       </c>
       <c r="L11" t="n">
-        <v>4312</v>
+        <v>5128</v>
       </c>
       <c r="M11" t="n">
-        <v>0.621</v>
+        <v>0.738</v>
       </c>
       <c r="N11" t="s">
         <v>82</v>
@@ -3096,7 +3089,7 @@
         <v>85</v>
       </c>
       <c r="C12" s="1" t="n">
-        <v>44032</v>
+        <v>44034</v>
       </c>
       <c r="D12" t="s">
         <v>86</v>
@@ -3106,25 +3099,25 @@
       </c>
       <c r="F12"/>
       <c r="G12" t="n">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="H12" t="n">
-        <v>3520466</v>
+        <v>3616652</v>
       </c>
       <c r="I12" t="n">
-        <v>93.277</v>
+        <v>95.825</v>
       </c>
       <c r="J12" t="n">
-        <v>38738</v>
+        <v>43098</v>
       </c>
       <c r="K12" t="n">
-        <v>1.026</v>
+        <v>1.142</v>
       </c>
       <c r="L12" t="n">
-        <v>43952</v>
+        <v>44892</v>
       </c>
       <c r="M12" t="n">
-        <v>1.165</v>
+        <v>1.189</v>
       </c>
       <c r="N12" t="s">
         <v>87</v>
@@ -3147,7 +3140,7 @@
         <v>91</v>
       </c>
       <c r="C13" s="1" t="n">
-        <v>44032</v>
+        <v>44034</v>
       </c>
       <c r="D13" t="s">
         <v>92</v>
@@ -3159,25 +3152,25 @@
         <v>93</v>
       </c>
       <c r="G13" t="n">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="H13" t="n">
-        <v>1420390</v>
+        <v>1445773</v>
       </c>
       <c r="I13" t="n">
-        <v>74.303</v>
+        <v>75.631</v>
       </c>
       <c r="J13" t="n">
-        <v>16343</v>
+        <v>12793</v>
       </c>
       <c r="K13" t="n">
-        <v>0.855</v>
+        <v>0.669</v>
       </c>
       <c r="L13" t="n">
-        <v>15732</v>
+        <v>15866</v>
       </c>
       <c r="M13" t="n">
-        <v>0.823</v>
+        <v>0.83</v>
       </c>
       <c r="N13" t="s">
         <v>94</v>
@@ -3200,7 +3193,7 @@
         <v>98</v>
       </c>
       <c r="C14" s="1" t="n">
-        <v>44031</v>
+        <v>44032</v>
       </c>
       <c r="D14" t="s">
         <v>99</v>
@@ -3210,25 +3203,25 @@
       </c>
       <c r="F14"/>
       <c r="G14" t="n">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="H14" t="n">
-        <v>1210063</v>
+        <v>1236536</v>
       </c>
       <c r="I14" t="n">
-        <v>23.781</v>
+        <v>24.302</v>
       </c>
       <c r="J14" t="n">
-        <v>24079</v>
+        <v>26473</v>
       </c>
       <c r="K14" t="n">
-        <v>0.473</v>
+        <v>0.52</v>
       </c>
       <c r="L14" t="n">
-        <v>25548</v>
+        <v>25675</v>
       </c>
       <c r="M14" t="n">
-        <v>0.502</v>
+        <v>0.505</v>
       </c>
       <c r="N14" t="s">
         <v>100</v>
@@ -3251,7 +3244,7 @@
         <v>105</v>
       </c>
       <c r="C15" s="1" t="n">
-        <v>44030</v>
+        <v>44033</v>
       </c>
       <c r="D15" t="s">
         <v>106</v>
@@ -3261,25 +3254,25 @@
       </c>
       <c r="F15"/>
       <c r="G15" t="n">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="H15" t="n">
-        <v>56508</v>
+        <v>60253</v>
       </c>
       <c r="I15" t="n">
-        <v>11.093</v>
+        <v>11.828</v>
       </c>
       <c r="J15" t="n">
-        <v>1116</v>
+        <v>1104</v>
       </c>
       <c r="K15" t="n">
-        <v>0.219</v>
+        <v>0.217</v>
       </c>
       <c r="L15" t="n">
-        <v>1523</v>
+        <v>1332</v>
       </c>
       <c r="M15" t="n">
-        <v>0.299</v>
+        <v>0.261</v>
       </c>
       <c r="N15" t="s">
         <v>107</v>
@@ -3302,7 +3295,7 @@
         <v>111</v>
       </c>
       <c r="C16" s="1" t="n">
-        <v>44032</v>
+        <v>44034</v>
       </c>
       <c r="D16" t="s">
         <v>112</v>
@@ -3312,25 +3305,25 @@
       </c>
       <c r="F16"/>
       <c r="G16" t="n">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="H16" t="n">
-        <v>104132</v>
+        <v>106805</v>
       </c>
       <c r="I16" t="n">
-        <v>25.365</v>
+        <v>26.017</v>
       </c>
       <c r="J16" t="n">
-        <v>1028</v>
+        <v>1279</v>
       </c>
       <c r="K16" t="n">
-        <v>0.25</v>
+        <v>0.312</v>
       </c>
       <c r="L16" t="n">
-        <v>1422</v>
+        <v>1297</v>
       </c>
       <c r="M16" t="n">
-        <v>0.346</v>
+        <v>0.316</v>
       </c>
       <c r="N16" t="s">
         <v>113</v>
@@ -3353,7 +3346,7 @@
         <v>118</v>
       </c>
       <c r="C17" s="1" t="n">
-        <v>44031</v>
+        <v>44033</v>
       </c>
       <c r="D17" t="s">
         <v>119</v>
@@ -3365,25 +3358,25 @@
         <v>121</v>
       </c>
       <c r="G17" t="n">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="H17" t="n">
-        <v>229357</v>
+        <v>234817</v>
       </c>
       <c r="I17" t="n">
-        <v>20.249</v>
+        <v>20.731</v>
       </c>
       <c r="J17" t="n">
-        <v>2914</v>
+        <v>2714</v>
       </c>
       <c r="K17" t="n">
-        <v>0.257</v>
+        <v>0.24</v>
       </c>
       <c r="L17" t="n">
-        <v>3037</v>
+        <v>2860</v>
       </c>
       <c r="M17" t="n">
-        <v>0.268</v>
+        <v>0.253</v>
       </c>
       <c r="N17" t="s">
         <v>120</v>
@@ -3406,7 +3399,7 @@
         <v>126</v>
       </c>
       <c r="C18" s="1" t="n">
-        <v>44031</v>
+        <v>44033</v>
       </c>
       <c r="D18" t="s">
         <v>127</v>
@@ -3416,25 +3409,25 @@
       </c>
       <c r="F18"/>
       <c r="G18" t="n">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="H18" t="n">
-        <v>626610</v>
+        <v>638484</v>
       </c>
       <c r="I18" t="n">
-        <v>58.513</v>
+        <v>59.621</v>
       </c>
       <c r="J18" t="n">
-        <v>1830</v>
+        <v>6089</v>
       </c>
       <c r="K18" t="n">
-        <v>0.171</v>
+        <v>0.569</v>
       </c>
       <c r="L18" t="n">
-        <v>3934</v>
+        <v>4313</v>
       </c>
       <c r="M18" t="n">
-        <v>0.367</v>
+        <v>0.403</v>
       </c>
       <c r="N18" t="s">
         <v>40</v>
@@ -3457,7 +3450,7 @@
         <v>131</v>
       </c>
       <c r="C19" s="1" t="n">
-        <v>44030</v>
+        <v>44032</v>
       </c>
       <c r="D19" t="s">
         <v>132</v>
@@ -3467,18 +3460,18 @@
       </c>
       <c r="F19"/>
       <c r="G19" t="n">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="H19"/>
       <c r="I19"/>
       <c r="J19" t="n">
-        <v>435</v>
+        <v>649</v>
       </c>
       <c r="K19" t="n">
-        <v>0.005</v>
+        <v>0.007</v>
       </c>
       <c r="L19" t="n">
-        <v>544</v>
+        <v>541</v>
       </c>
       <c r="M19" t="n">
         <v>0.006</v>
@@ -3504,7 +3497,7 @@
         <v>137</v>
       </c>
       <c r="C20" s="1" t="n">
-        <v>44031</v>
+        <v>44033</v>
       </c>
       <c r="D20" t="s">
         <v>138</v>
@@ -3514,25 +3507,25 @@
       </c>
       <c r="F20"/>
       <c r="G20" t="n">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="H20" t="n">
-        <v>1309722</v>
+        <v>1347145</v>
       </c>
       <c r="I20" t="n">
-        <v>226.118</v>
+        <v>232.579</v>
       </c>
       <c r="J20" t="n">
-        <v>2912</v>
+        <v>4332</v>
       </c>
       <c r="K20" t="n">
-        <v>0.503</v>
+        <v>0.748</v>
       </c>
       <c r="L20" t="n">
-        <v>11554</v>
+        <v>11899</v>
       </c>
       <c r="M20" t="n">
-        <v>1.995</v>
+        <v>2.054</v>
       </c>
       <c r="N20" t="s">
         <v>139</v>
@@ -3555,7 +3548,7 @@
         <v>143</v>
       </c>
       <c r="C21" s="1" t="n">
-        <v>44031</v>
+        <v>44034</v>
       </c>
       <c r="D21" t="s">
         <v>144</v>
@@ -3567,25 +3560,25 @@
         <v>146</v>
       </c>
       <c r="G21" t="n">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="H21" t="n">
-        <v>154150</v>
+        <v>161443</v>
       </c>
       <c r="I21" t="n">
-        <v>8.737</v>
+        <v>9.151</v>
       </c>
       <c r="J21" t="n">
-        <v>1702</v>
+        <v>2291</v>
       </c>
       <c r="K21" t="n">
-        <v>0.096</v>
+        <v>0.13</v>
       </c>
       <c r="L21" t="n">
-        <v>2126</v>
+        <v>2319</v>
       </c>
       <c r="M21" t="n">
-        <v>0.121</v>
+        <v>0.131</v>
       </c>
       <c r="N21" t="s">
         <v>145</v>
@@ -3659,7 +3652,7 @@
         <v>156</v>
       </c>
       <c r="C23" s="1" t="n">
-        <v>44031</v>
+        <v>44033</v>
       </c>
       <c r="D23" t="s">
         <v>157</v>
@@ -3669,25 +3662,25 @@
       </c>
       <c r="F23"/>
       <c r="G23" t="n">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="H23" t="n">
-        <v>114542</v>
+        <v>115518</v>
       </c>
       <c r="I23" t="n">
-        <v>86.347</v>
+        <v>87.082</v>
       </c>
       <c r="J23" t="n">
-        <v>106</v>
+        <v>588</v>
       </c>
       <c r="K23" t="n">
-        <v>0.08</v>
+        <v>0.443</v>
       </c>
       <c r="L23" t="n">
-        <v>339</v>
+        <v>343</v>
       </c>
       <c r="M23" t="n">
-        <v>0.256</v>
+        <v>0.259</v>
       </c>
       <c r="N23" t="s">
         <v>159</v>
@@ -3761,7 +3754,7 @@
         <v>170</v>
       </c>
       <c r="C25" s="1" t="n">
-        <v>44024</v>
+        <v>44031</v>
       </c>
       <c r="D25" t="s">
         <v>171</v>
@@ -3771,25 +3764,25 @@
       </c>
       <c r="F25"/>
       <c r="G25" t="n">
-        <v>117</v>
+        <v>124</v>
       </c>
       <c r="H25" t="n">
-        <v>5937</v>
+        <v>6414</v>
       </c>
       <c r="I25" t="n">
-        <v>6.623</v>
+        <v>7.155</v>
       </c>
       <c r="J25" t="n">
-        <v>97</v>
+        <v>13</v>
       </c>
       <c r="K25" t="n">
-        <v>0.108</v>
+        <v>0.015</v>
       </c>
       <c r="L25" t="n">
-        <v>89</v>
+        <v>68</v>
       </c>
       <c r="M25" t="n">
-        <v>0.099</v>
+        <v>0.076</v>
       </c>
       <c r="N25" t="s">
         <v>172</v>
@@ -3812,7 +3805,7 @@
         <v>175</v>
       </c>
       <c r="C26" s="1" t="n">
-        <v>44030</v>
+        <v>44032</v>
       </c>
       <c r="D26" t="s">
         <v>176</v>
@@ -3822,25 +3815,25 @@
       </c>
       <c r="F26"/>
       <c r="G26" t="n">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="H26" t="n">
-        <v>311294</v>
+        <v>320650</v>
       </c>
       <c r="I26" t="n">
-        <v>56.183</v>
+        <v>57.872</v>
       </c>
       <c r="J26" t="n">
-        <v>1707</v>
+        <v>2657</v>
       </c>
       <c r="K26" t="n">
-        <v>0.308</v>
+        <v>0.48</v>
       </c>
       <c r="L26" t="n">
-        <v>3445</v>
+        <v>4029</v>
       </c>
       <c r="M26" t="n">
-        <v>0.622</v>
+        <v>0.727</v>
       </c>
       <c r="N26" t="s">
         <v>178</v>
@@ -3961,7 +3954,7 @@
         <v>192</v>
       </c>
       <c r="C29" s="1" t="n">
-        <v>44024</v>
+        <v>44031</v>
       </c>
       <c r="D29" t="s">
         <v>193</v>
@@ -3973,21 +3966,21 @@
         <v>195</v>
       </c>
       <c r="G29" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H29" t="n">
-        <v>6884614</v>
+        <v>7418812</v>
       </c>
       <c r="I29" t="n">
-        <v>82.171</v>
+        <v>88.547</v>
       </c>
       <c r="J29"/>
       <c r="K29"/>
       <c r="L29" t="n">
-        <v>71889</v>
+        <v>75939</v>
       </c>
       <c r="M29" t="n">
-        <v>0.858</v>
+        <v>0.906</v>
       </c>
       <c r="N29" t="s">
         <v>194</v>
@@ -4010,7 +4003,7 @@
         <v>200</v>
       </c>
       <c r="C30" s="1" t="n">
-        <v>44028</v>
+        <v>44030</v>
       </c>
       <c r="D30" t="s">
         <v>201</v>
@@ -4020,25 +4013,25 @@
       </c>
       <c r="F30"/>
       <c r="G30" t="n">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="H30" t="n">
-        <v>346990</v>
+        <v>353752</v>
       </c>
       <c r="I30" t="n">
-        <v>11.167</v>
+        <v>11.385</v>
       </c>
       <c r="J30" t="n">
-        <v>2853</v>
+        <v>4000</v>
       </c>
       <c r="K30" t="n">
-        <v>0.092</v>
+        <v>0.129</v>
       </c>
       <c r="L30" t="n">
-        <v>2658</v>
+        <v>2807</v>
       </c>
       <c r="M30" t="n">
-        <v>0.086</v>
+        <v>0.09</v>
       </c>
       <c r="N30" t="s">
         <v>203</v>
@@ -4061,7 +4054,7 @@
         <v>208</v>
       </c>
       <c r="C31" s="1" t="n">
-        <v>44031</v>
+        <v>44034</v>
       </c>
       <c r="D31" t="s">
         <v>209</v>
@@ -4071,25 +4064,25 @@
       </c>
       <c r="F31"/>
       <c r="G31" t="n">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="H31" t="n">
-        <v>410766</v>
+        <v>424675</v>
       </c>
       <c r="I31" t="n">
-        <v>39.409</v>
+        <v>40.744</v>
       </c>
       <c r="J31" t="n">
-        <v>4726</v>
+        <v>4769</v>
       </c>
       <c r="K31" t="n">
-        <v>0.453</v>
+        <v>0.458</v>
       </c>
       <c r="L31" t="n">
-        <v>5262</v>
+        <v>4700</v>
       </c>
       <c r="M31" t="n">
-        <v>0.505</v>
+        <v>0.451</v>
       </c>
       <c r="N31" t="s">
         <v>211</v>
@@ -4159,7 +4152,7 @@
         <v>222</v>
       </c>
       <c r="C33" s="1" t="n">
-        <v>44032</v>
+        <v>44033</v>
       </c>
       <c r="D33" t="s">
         <v>223</v>
@@ -4171,25 +4164,25 @@
         <v>225</v>
       </c>
       <c r="G33" t="n">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="H33" t="n">
-        <v>310070</v>
+        <v>310830</v>
       </c>
       <c r="I33" t="n">
-        <v>32.097</v>
+        <v>32.176</v>
       </c>
       <c r="J33" t="n">
-        <v>2224</v>
+        <v>760</v>
       </c>
       <c r="K33" t="n">
-        <v>0.23</v>
+        <v>0.079</v>
       </c>
       <c r="L33" t="n">
-        <v>2073</v>
+        <v>2067</v>
       </c>
       <c r="M33" t="n">
-        <v>0.215</v>
+        <v>0.214</v>
       </c>
       <c r="N33" t="s">
         <v>224</v>
@@ -4212,7 +4205,7 @@
         <v>230</v>
       </c>
       <c r="C34" s="1" t="n">
-        <v>44031</v>
+        <v>44033</v>
       </c>
       <c r="D34" t="s">
         <v>231</v>
@@ -4222,25 +4215,25 @@
       </c>
       <c r="F34"/>
       <c r="G34" t="n">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="H34" t="n">
-        <v>68614</v>
+        <v>68704</v>
       </c>
       <c r="I34" t="n">
-        <v>201.067</v>
+        <v>201.33</v>
       </c>
       <c r="J34" t="n">
-        <v>39</v>
+        <v>64</v>
       </c>
       <c r="K34" t="n">
-        <v>0.114</v>
+        <v>0.188</v>
       </c>
       <c r="L34" t="n">
-        <v>113</v>
+        <v>91</v>
       </c>
       <c r="M34" t="n">
-        <v>0.331</v>
+        <v>0.267</v>
       </c>
       <c r="N34" t="s">
         <v>232</v>
@@ -4316,7 +4309,7 @@
         <v>240</v>
       </c>
       <c r="C36" s="1" t="n">
-        <v>44031</v>
+        <v>44034</v>
       </c>
       <c r="D36" t="s">
         <v>236</v>
@@ -4328,25 +4321,25 @@
         <v>238</v>
       </c>
       <c r="G36" t="n">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="H36" t="n">
-        <v>13791869</v>
+        <v>14724546</v>
       </c>
       <c r="I36" t="n">
-        <v>9.994</v>
+        <v>10.67</v>
       </c>
       <c r="J36" t="n">
-        <v>358127</v>
+        <v>343243</v>
       </c>
       <c r="K36" t="n">
-        <v>0.26</v>
+        <v>0.249</v>
       </c>
       <c r="L36" t="n">
-        <v>314959</v>
+        <v>330269</v>
       </c>
       <c r="M36" t="n">
-        <v>0.228</v>
+        <v>0.239</v>
       </c>
       <c r="N36" t="s">
         <v>237</v>
@@ -4369,7 +4362,7 @@
         <v>242</v>
       </c>
       <c r="C37" s="1" t="n">
-        <v>44032</v>
+        <v>44034</v>
       </c>
       <c r="D37" t="s">
         <v>243</v>
@@ -4379,25 +4372,25 @@
       </c>
       <c r="F37"/>
       <c r="G37" t="n">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="H37" t="n">
-        <v>720497</v>
+        <v>749626</v>
       </c>
       <c r="I37" t="n">
-        <v>2.634</v>
+        <v>2.741</v>
       </c>
       <c r="J37" t="n">
-        <v>13259</v>
+        <v>11782</v>
       </c>
       <c r="K37" t="n">
+        <v>0.043</v>
+      </c>
+      <c r="L37" t="n">
+        <v>13139</v>
+      </c>
+      <c r="M37" t="n">
         <v>0.048</v>
-      </c>
-      <c r="L37" t="n">
-        <v>12907</v>
-      </c>
-      <c r="M37" t="n">
-        <v>0.047</v>
       </c>
       <c r="N37" t="s">
         <v>244</v>
@@ -4420,7 +4413,7 @@
         <v>249</v>
       </c>
       <c r="C38" s="1" t="n">
-        <v>44032</v>
+        <v>44034</v>
       </c>
       <c r="D38" t="s">
         <v>250</v>
@@ -4430,25 +4423,25 @@
       </c>
       <c r="F38"/>
       <c r="G38" t="n">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="H38" t="n">
-        <v>2175217</v>
+        <v>2228277</v>
       </c>
       <c r="I38" t="n">
-        <v>25.898</v>
+        <v>26.529</v>
       </c>
       <c r="J38" t="n">
-        <v>26218</v>
+        <v>26319</v>
       </c>
       <c r="K38" t="n">
-        <v>0.312</v>
+        <v>0.313</v>
       </c>
       <c r="L38" t="n">
-        <v>25321</v>
+        <v>25747</v>
       </c>
       <c r="M38" t="n">
-        <v>0.301</v>
+        <v>0.307</v>
       </c>
       <c r="N38" t="s">
         <v>251</v>
@@ -4471,7 +4464,7 @@
         <v>255</v>
       </c>
       <c r="C39" s="1" t="n">
-        <v>44032</v>
+        <v>44034</v>
       </c>
       <c r="D39" t="s">
         <v>256</v>
@@ -4481,25 +4474,25 @@
       </c>
       <c r="F39"/>
       <c r="G39" t="n">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="H39" t="n">
-        <v>567819</v>
+        <v>579088</v>
       </c>
       <c r="I39" t="n">
-        <v>114.994</v>
+        <v>117.277</v>
       </c>
       <c r="J39" t="n">
-        <v>8402</v>
+        <v>4599</v>
       </c>
       <c r="K39" t="n">
-        <v>1.702</v>
+        <v>0.931</v>
       </c>
       <c r="L39" t="n">
-        <v>7266</v>
+        <v>7335</v>
       </c>
       <c r="M39" t="n">
-        <v>1.472</v>
+        <v>1.485</v>
       </c>
       <c r="N39" t="s">
         <v>257</v>
@@ -4522,7 +4515,7 @@
         <v>260</v>
       </c>
       <c r="C40" s="1" t="n">
-        <v>44025</v>
+        <v>44027</v>
       </c>
       <c r="D40" t="s">
         <v>261</v>
@@ -4532,25 +4525,25 @@
       </c>
       <c r="F40"/>
       <c r="G40" t="n">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="H40" t="n">
-        <v>1317541</v>
+        <v>1379993</v>
       </c>
       <c r="I40" t="n">
-        <v>152.219</v>
+        <v>159.435</v>
       </c>
       <c r="J40" t="n">
-        <v>29184</v>
+        <v>30629</v>
       </c>
       <c r="K40" t="n">
-        <v>3.372</v>
+        <v>3.539</v>
       </c>
       <c r="L40" t="n">
-        <v>26439</v>
+        <v>27063</v>
       </c>
       <c r="M40" t="n">
-        <v>3.055</v>
+        <v>3.127</v>
       </c>
       <c r="N40" t="s">
         <v>40</v>
@@ -4573,7 +4566,7 @@
         <v>266</v>
       </c>
       <c r="C41" s="1" t="n">
-        <v>44032</v>
+        <v>44034</v>
       </c>
       <c r="D41" t="s">
         <v>267</v>
@@ -4585,25 +4578,25 @@
         <v>269</v>
       </c>
       <c r="G41" t="n">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="H41" t="n">
-        <v>3754568</v>
+        <v>3807771</v>
       </c>
       <c r="I41" t="n">
-        <v>62.098</v>
+        <v>62.978</v>
       </c>
       <c r="J41" t="n">
-        <v>14121</v>
+        <v>29288</v>
       </c>
       <c r="K41" t="n">
-        <v>0.234</v>
+        <v>0.484</v>
       </c>
       <c r="L41" t="n">
-        <v>24525</v>
+        <v>24609</v>
       </c>
       <c r="M41" t="n">
-        <v>0.406</v>
+        <v>0.407</v>
       </c>
       <c r="N41" t="s">
         <v>270</v>
@@ -4626,7 +4619,7 @@
         <v>273</v>
       </c>
       <c r="C42" s="1" t="n">
-        <v>44032</v>
+        <v>44034</v>
       </c>
       <c r="D42" t="s">
         <v>267</v>
@@ -4638,25 +4631,25 @@
         <v>269</v>
       </c>
       <c r="G42" t="n">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="H42" t="n">
-        <v>6262302</v>
+        <v>6354730</v>
       </c>
       <c r="I42" t="n">
-        <v>103.574</v>
+        <v>105.103</v>
       </c>
       <c r="J42" t="n">
-        <v>24253</v>
+        <v>49318</v>
       </c>
       <c r="K42" t="n">
-        <v>0.401</v>
+        <v>0.816</v>
       </c>
       <c r="L42" t="n">
-        <v>42794</v>
+        <v>43096</v>
       </c>
       <c r="M42" t="n">
-        <v>0.708</v>
+        <v>0.713</v>
       </c>
       <c r="N42" t="s">
         <v>270</v>
@@ -4679,7 +4672,7 @@
         <v>276</v>
       </c>
       <c r="C43" s="1" t="n">
-        <v>44032</v>
+        <v>44034</v>
       </c>
       <c r="D43" t="s">
         <v>277</v>
@@ -4691,25 +4684,25 @@
         <v>279</v>
       </c>
       <c r="G43" t="n">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="H43" t="n">
-        <v>639821</v>
+        <v>670619</v>
       </c>
       <c r="I43" t="n">
-        <v>5.059</v>
+        <v>5.302</v>
       </c>
       <c r="J43" t="n">
-        <v>4824</v>
+        <v>13084</v>
       </c>
       <c r="K43" t="n">
-        <v>0.038</v>
+        <v>0.103</v>
       </c>
       <c r="L43" t="n">
-        <v>11102</v>
+        <v>11988</v>
       </c>
       <c r="M43" t="n">
-        <v>0.088</v>
+        <v>0.095</v>
       </c>
       <c r="N43" t="s">
         <v>280</v>
@@ -4732,7 +4725,7 @@
         <v>283</v>
       </c>
       <c r="C44" s="1" t="n">
-        <v>44030</v>
+        <v>44032</v>
       </c>
       <c r="D44" t="s">
         <v>284</v>
@@ -4744,25 +4737,25 @@
         <v>285</v>
       </c>
       <c r="G44" t="n">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="H44" t="n">
-        <v>868062</v>
+        <v>911548</v>
       </c>
       <c r="I44" t="n">
-        <v>6.863</v>
+        <v>7.207</v>
       </c>
       <c r="J44" t="n">
-        <v>3373</v>
+        <v>9553</v>
       </c>
       <c r="K44" t="n">
-        <v>0.027</v>
+        <v>0.076</v>
       </c>
       <c r="L44" t="n">
-        <v>9832</v>
+        <v>13850</v>
       </c>
       <c r="M44" t="n">
-        <v>0.078</v>
+        <v>0.11</v>
       </c>
       <c r="N44" t="s">
         <v>280</v>
@@ -4883,7 +4876,7 @@
         <v>300</v>
       </c>
       <c r="C47" s="1" t="n">
-        <v>44030</v>
+        <v>44033</v>
       </c>
       <c r="D47" t="s">
         <v>301</v>
@@ -4893,25 +4886,25 @@
       </c>
       <c r="F47"/>
       <c r="G47" t="n">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="H47" t="n">
-        <v>457340</v>
+        <v>466861</v>
       </c>
       <c r="I47" t="n">
-        <v>107.091</v>
+        <v>109.321</v>
       </c>
       <c r="J47" t="n">
-        <v>4370</v>
+        <v>4157</v>
       </c>
       <c r="K47" t="n">
-        <v>1.023</v>
+        <v>0.973</v>
       </c>
       <c r="L47" t="n">
-        <v>3977</v>
+        <v>3674</v>
       </c>
       <c r="M47" t="n">
-        <v>0.931</v>
+        <v>0.86</v>
       </c>
       <c r="N47" t="s">
         <v>302</v>
@@ -4934,7 +4927,7 @@
         <v>306</v>
       </c>
       <c r="C48" s="1" t="n">
-        <v>44032</v>
+        <v>44034</v>
       </c>
       <c r="D48" t="s">
         <v>307</v>
@@ -4946,25 +4939,25 @@
         <v>309</v>
       </c>
       <c r="G48" t="n">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="H48" t="n">
-        <v>182225</v>
+        <v>185223</v>
       </c>
       <c r="I48" t="n">
-        <v>96.609</v>
+        <v>98.199</v>
       </c>
       <c r="J48" t="n">
-        <v>1297</v>
+        <v>1613</v>
       </c>
       <c r="K48" t="n">
-        <v>0.688</v>
+        <v>0.855</v>
       </c>
       <c r="L48" t="n">
-        <v>1755</v>
+        <v>1595</v>
       </c>
       <c r="M48" t="n">
-        <v>0.93</v>
+        <v>0.846</v>
       </c>
       <c r="N48" t="s">
         <v>308</v>
@@ -4987,7 +4980,7 @@
         <v>312</v>
       </c>
       <c r="C49" s="1" t="n">
-        <v>44032</v>
+        <v>44034</v>
       </c>
       <c r="D49" t="s">
         <v>313</v>
@@ -4997,21 +4990,25 @@
       </c>
       <c r="F49"/>
       <c r="G49" t="n">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="H49" t="n">
-        <v>482607</v>
+        <v>489869</v>
       </c>
       <c r="I49" t="n">
-        <v>177.28</v>
-      </c>
-      <c r="J49"/>
-      <c r="K49"/>
+        <v>179.947</v>
+      </c>
+      <c r="J49" t="n">
+        <v>3645</v>
+      </c>
+      <c r="K49" t="n">
+        <v>1.339</v>
+      </c>
       <c r="L49" t="n">
-        <v>2992</v>
+        <v>2967</v>
       </c>
       <c r="M49" t="n">
-        <v>1.099</v>
+        <v>1.09</v>
       </c>
       <c r="N49" t="s">
         <v>40</v>
@@ -5034,7 +5031,7 @@
         <v>316</v>
       </c>
       <c r="C50" s="1" t="n">
-        <v>44031</v>
+        <v>44034</v>
       </c>
       <c r="D50" t="s">
         <v>317</v>
@@ -5044,25 +5041,25 @@
       </c>
       <c r="F50"/>
       <c r="G50" t="n">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="H50" t="n">
-        <v>344744</v>
+        <v>370539</v>
       </c>
       <c r="I50" t="n">
-        <v>550.73</v>
+        <v>591.938</v>
       </c>
       <c r="J50" t="n">
-        <v>11287</v>
+        <v>12902</v>
       </c>
       <c r="K50" t="n">
-        <v>18.031</v>
+        <v>20.611</v>
       </c>
       <c r="L50" t="n">
-        <v>9479</v>
+        <v>9675</v>
       </c>
       <c r="M50" t="n">
-        <v>15.143</v>
+        <v>15.456</v>
       </c>
       <c r="N50" t="s">
         <v>318</v>
@@ -5085,7 +5082,7 @@
         <v>322</v>
       </c>
       <c r="C51" s="1" t="n">
-        <v>44032</v>
+        <v>44034</v>
       </c>
       <c r="D51" t="s">
         <v>323</v>
@@ -5097,25 +5094,25 @@
         <v>325</v>
       </c>
       <c r="G51" t="n">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="H51" t="n">
-        <v>895758</v>
+        <v>909627</v>
       </c>
       <c r="I51" t="n">
-        <v>27.676</v>
+        <v>28.104</v>
       </c>
       <c r="J51" t="n">
-        <v>6014</v>
+        <v>7188</v>
       </c>
       <c r="K51" t="n">
-        <v>0.186</v>
+        <v>0.222</v>
       </c>
       <c r="L51" t="n">
-        <v>6476</v>
+        <v>6819</v>
       </c>
       <c r="M51" t="n">
-        <v>0.2</v>
+        <v>0.211</v>
       </c>
       <c r="N51" t="s">
         <v>40</v>
@@ -5138,7 +5135,7 @@
         <v>329</v>
       </c>
       <c r="C52" s="1" t="n">
-        <v>44031</v>
+        <v>44033</v>
       </c>
       <c r="D52" t="s">
         <v>330</v>
@@ -5148,25 +5145,25 @@
       </c>
       <c r="F52"/>
       <c r="G52" t="n">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="H52" t="n">
-        <v>67264</v>
+        <v>68696</v>
       </c>
       <c r="I52" t="n">
-        <v>124.438</v>
+        <v>127.087</v>
       </c>
       <c r="J52" t="n">
-        <v>658</v>
+        <v>711</v>
       </c>
       <c r="K52" t="n">
-        <v>1.217</v>
+        <v>1.315</v>
       </c>
       <c r="L52" t="n">
-        <v>778</v>
+        <v>734</v>
       </c>
       <c r="M52" t="n">
-        <v>1.439</v>
+        <v>1.358</v>
       </c>
       <c r="N52" t="s">
         <v>332</v>
@@ -5240,7 +5237,7 @@
         <v>342</v>
       </c>
       <c r="C54" s="1" t="n">
-        <v>44027</v>
+        <v>44029</v>
       </c>
       <c r="D54" t="s">
         <v>343</v>
@@ -5250,25 +5247,25 @@
       </c>
       <c r="F54"/>
       <c r="G54" t="n">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="H54" t="n">
-        <v>731117</v>
+        <v>758257</v>
       </c>
       <c r="I54" t="n">
-        <v>5.671</v>
+        <v>5.881</v>
       </c>
       <c r="J54" t="n">
-        <v>8995</v>
+        <v>7450</v>
       </c>
       <c r="K54" t="n">
-        <v>0.07</v>
+        <v>0.058</v>
       </c>
       <c r="L54" t="n">
-        <v>9283</v>
+        <v>9365</v>
       </c>
       <c r="M54" t="n">
-        <v>0.072</v>
+        <v>0.073</v>
       </c>
       <c r="N54" t="s">
         <v>345</v>
@@ -5291,7 +5288,7 @@
         <v>349</v>
       </c>
       <c r="C55" s="1" t="n">
-        <v>44031</v>
+        <v>44033</v>
       </c>
       <c r="D55" t="s">
         <v>350</v>
@@ -5301,25 +5298,25 @@
       </c>
       <c r="F55"/>
       <c r="G55" t="n">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="H55" t="n">
-        <v>1009326</v>
+        <v>1046806</v>
       </c>
       <c r="I55" t="n">
-        <v>27.345</v>
+        <v>28.361</v>
       </c>
       <c r="J55" t="n">
-        <v>18812</v>
+        <v>19033</v>
       </c>
       <c r="K55" t="n">
+        <v>0.516</v>
+      </c>
+      <c r="L55" t="n">
+        <v>18809</v>
+      </c>
+      <c r="M55" t="n">
         <v>0.51</v>
-      </c>
-      <c r="L55" t="n">
-        <v>18671</v>
-      </c>
-      <c r="M55" t="n">
-        <v>0.506</v>
       </c>
       <c r="N55" t="s">
         <v>351</v>
@@ -5393,7 +5390,7 @@
         <v>361</v>
       </c>
       <c r="C57" s="1" t="n">
-        <v>44031</v>
+        <v>44033</v>
       </c>
       <c r="D57" t="s">
         <v>362</v>
@@ -5403,25 +5400,25 @@
       </c>
       <c r="F57"/>
       <c r="G57" t="n">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="H57" t="n">
-        <v>315570</v>
+        <v>323416</v>
       </c>
       <c r="I57" t="n">
-        <v>10.831</v>
+        <v>11.1</v>
       </c>
       <c r="J57" t="n">
-        <v>3741</v>
+        <v>3544</v>
       </c>
       <c r="K57" t="n">
-        <v>0.128</v>
+        <v>0.122</v>
       </c>
       <c r="L57" t="n">
-        <v>4579</v>
+        <v>4240</v>
       </c>
       <c r="M57" t="n">
-        <v>0.157</v>
+        <v>0.146</v>
       </c>
       <c r="N57" t="s">
         <v>363</v>
@@ -5495,7 +5492,7 @@
         <v>374</v>
       </c>
       <c r="C59" s="1" t="n">
-        <v>44030</v>
+        <v>44033</v>
       </c>
       <c r="D59" t="s">
         <v>375</v>
@@ -5505,25 +5502,25 @@
       </c>
       <c r="F59"/>
       <c r="G59" t="n">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="H59" t="n">
-        <v>442488</v>
+        <v>446367</v>
       </c>
       <c r="I59" t="n">
-        <v>91.76</v>
+        <v>92.564</v>
       </c>
       <c r="J59" t="n">
-        <v>1365</v>
+        <v>2191</v>
       </c>
       <c r="K59" t="n">
-        <v>0.283</v>
+        <v>0.454</v>
       </c>
       <c r="L59" t="n">
-        <v>1984</v>
+        <v>1863</v>
       </c>
       <c r="M59" t="n">
-        <v>0.411</v>
+        <v>0.386</v>
       </c>
       <c r="N59" t="s">
         <v>376</v>
@@ -5546,7 +5543,7 @@
         <v>379</v>
       </c>
       <c r="C60" s="1" t="n">
-        <v>44031</v>
+        <v>44034</v>
       </c>
       <c r="D60" t="s">
         <v>380</v>
@@ -5556,25 +5553,25 @@
       </c>
       <c r="F60"/>
       <c r="G60" t="n">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="H60" t="n">
-        <v>212201</v>
+        <v>247825</v>
       </c>
       <c r="I60" t="n">
-        <v>1.029</v>
+        <v>1.202</v>
       </c>
       <c r="J60" t="n">
-        <v>2755</v>
+        <v>29602</v>
       </c>
       <c r="K60" t="n">
-        <v>0.013</v>
+        <v>0.144</v>
       </c>
       <c r="L60" t="n">
-        <v>4422</v>
+        <v>6973</v>
       </c>
       <c r="M60" t="n">
-        <v>0.021</v>
+        <v>0.034</v>
       </c>
       <c r="N60" t="s">
         <v>381</v>
@@ -5648,7 +5645,7 @@
         <v>392</v>
       </c>
       <c r="C62" s="1" t="n">
-        <v>44032</v>
+        <v>44034</v>
       </c>
       <c r="D62" t="s">
         <v>393</v>
@@ -5658,21 +5655,21 @@
       </c>
       <c r="F62"/>
       <c r="G62" t="n">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="H62"/>
       <c r="I62"/>
       <c r="J62" t="n">
-        <v>3957</v>
+        <v>4798</v>
       </c>
       <c r="K62" t="n">
-        <v>0.775</v>
+        <v>0.94</v>
       </c>
       <c r="L62" t="n">
-        <v>4280</v>
+        <v>4400</v>
       </c>
       <c r="M62" t="n">
-        <v>0.838</v>
+        <v>0.862</v>
       </c>
       <c r="N62" t="s">
         <v>394</v>
@@ -5695,7 +5692,7 @@
         <v>399</v>
       </c>
       <c r="C63" s="1" t="n">
-        <v>44032</v>
+        <v>44034</v>
       </c>
       <c r="D63" t="s">
         <v>400</v>
@@ -5705,25 +5702,25 @@
       </c>
       <c r="F63"/>
       <c r="G63" t="n">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="H63" t="n">
-        <v>1740768</v>
+        <v>1776882</v>
       </c>
       <c r="I63" t="n">
-        <v>7.881</v>
+        <v>8.044</v>
       </c>
       <c r="J63" t="n">
-        <v>19108</v>
+        <v>18331</v>
       </c>
       <c r="K63" t="n">
-        <v>0.087</v>
+        <v>0.083</v>
       </c>
       <c r="L63" t="n">
-        <v>22228</v>
+        <v>21278</v>
       </c>
       <c r="M63" t="n">
-        <v>0.101</v>
+        <v>0.096</v>
       </c>
       <c r="N63" t="s">
         <v>401</v>
@@ -5746,7 +5743,7 @@
         <v>404</v>
       </c>
       <c r="C64" s="1" t="n">
-        <v>44030</v>
+        <v>44032</v>
       </c>
       <c r="D64" t="s">
         <v>405</v>
@@ -5756,25 +5753,25 @@
       </c>
       <c r="F64"/>
       <c r="G64" t="n">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="H64" t="n">
-        <v>180296</v>
+        <v>186986</v>
       </c>
       <c r="I64" t="n">
-        <v>41.786</v>
+        <v>43.336</v>
       </c>
       <c r="J64" t="n">
-        <v>2477</v>
+        <v>2920</v>
       </c>
       <c r="K64" t="n">
-        <v>0.574</v>
+        <v>0.677</v>
       </c>
       <c r="L64" t="n">
-        <v>3104</v>
+        <v>3057</v>
       </c>
       <c r="M64" t="n">
-        <v>0.719</v>
+        <v>0.708</v>
       </c>
       <c r="N64" t="s">
         <v>406</v>
@@ -5848,7 +5845,7 @@
         <v>416</v>
       </c>
       <c r="C66" s="1" t="n">
-        <v>44032</v>
+        <v>44033</v>
       </c>
       <c r="D66" t="s">
         <v>417</v>
@@ -5858,21 +5855,25 @@
       </c>
       <c r="F66"/>
       <c r="G66" t="n">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="H66" t="n">
-        <v>326510</v>
+        <v>334511</v>
       </c>
       <c r="I66" t="n">
-        <v>9.903</v>
-      </c>
-      <c r="J66"/>
-      <c r="K66"/>
+        <v>10.145</v>
+      </c>
+      <c r="J66" t="n">
+        <v>8001</v>
+      </c>
+      <c r="K66" t="n">
+        <v>0.243</v>
+      </c>
       <c r="L66" t="n">
-        <v>4949</v>
+        <v>5859</v>
       </c>
       <c r="M66" t="n">
-        <v>0.15</v>
+        <v>0.178</v>
       </c>
       <c r="N66" t="s">
         <v>418</v>
@@ -5895,7 +5896,7 @@
         <v>422</v>
       </c>
       <c r="C67" s="1" t="n">
-        <v>44031</v>
+        <v>44032</v>
       </c>
       <c r="D67" t="s">
         <v>423</v>
@@ -5905,21 +5906,25 @@
       </c>
       <c r="F67"/>
       <c r="G67" t="n">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="H67" t="n">
-        <v>1088641</v>
+        <v>1110901</v>
       </c>
       <c r="I67" t="n">
-        <v>9.935</v>
-      </c>
-      <c r="J67"/>
-      <c r="K67"/>
+        <v>10.138</v>
+      </c>
+      <c r="J67" t="n">
+        <v>22260</v>
+      </c>
+      <c r="K67" t="n">
+        <v>0.203</v>
+      </c>
       <c r="L67" t="n">
-        <v>22828</v>
+        <v>23448</v>
       </c>
       <c r="M67" t="n">
-        <v>0.208</v>
+        <v>0.214</v>
       </c>
       <c r="N67" t="s">
         <v>217</v>
@@ -5942,7 +5947,7 @@
         <v>427</v>
       </c>
       <c r="C68" s="1" t="n">
-        <v>44032</v>
+        <v>44034</v>
       </c>
       <c r="D68" t="s">
         <v>428</v>
@@ -5952,25 +5957,25 @@
       </c>
       <c r="F68"/>
       <c r="G68" t="n">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="H68" t="n">
-        <v>1725447</v>
+        <v>1761265</v>
       </c>
       <c r="I68" t="n">
-        <v>45.591</v>
+        <v>46.537</v>
       </c>
       <c r="J68" t="n">
-        <v>10091</v>
+        <v>19656</v>
       </c>
       <c r="K68" t="n">
-        <v>0.267</v>
+        <v>0.519</v>
       </c>
       <c r="L68" t="n">
-        <v>17158</v>
+        <v>17054</v>
       </c>
       <c r="M68" t="n">
-        <v>0.453</v>
+        <v>0.451</v>
       </c>
       <c r="N68" t="s">
         <v>429</v>
@@ -5993,7 +5998,7 @@
         <v>432</v>
       </c>
       <c r="C69" s="1" t="n">
-        <v>44032</v>
+        <v>44034</v>
       </c>
       <c r="D69" t="s">
         <v>428</v>
@@ -6003,25 +6008,25 @@
       </c>
       <c r="F69"/>
       <c r="G69" t="n">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="H69" t="n">
-        <v>1971736</v>
+        <v>2017513</v>
       </c>
       <c r="I69" t="n">
-        <v>52.098</v>
+        <v>53.308</v>
       </c>
       <c r="J69" t="n">
-        <v>15464</v>
+        <v>25511</v>
       </c>
       <c r="K69" t="n">
-        <v>0.409</v>
+        <v>0.674</v>
       </c>
       <c r="L69" t="n">
-        <v>22624</v>
+        <v>22417</v>
       </c>
       <c r="M69" t="n">
-        <v>0.598</v>
+        <v>0.592</v>
       </c>
       <c r="N69" t="s">
         <v>429</v>
@@ -6044,7 +6049,7 @@
         <v>435</v>
       </c>
       <c r="C70" s="1" t="n">
-        <v>44023</v>
+        <v>44032</v>
       </c>
       <c r="D70" t="s">
         <v>436</v>
@@ -6054,25 +6059,25 @@
       </c>
       <c r="F70"/>
       <c r="G70" t="n">
-        <v>133</v>
+        <v>142</v>
       </c>
       <c r="H70" t="n">
-        <v>1360164</v>
+        <v>1480458</v>
       </c>
       <c r="I70" t="n">
-        <v>133.392</v>
+        <v>145.19</v>
       </c>
       <c r="J70" t="n">
-        <v>11992</v>
+        <v>13413</v>
       </c>
       <c r="K70" t="n">
-        <v>1.176</v>
+        <v>1.315</v>
       </c>
       <c r="L70" t="n">
-        <v>13593</v>
+        <v>14124</v>
       </c>
       <c r="M70" t="n">
-        <v>1.333</v>
+        <v>1.385</v>
       </c>
       <c r="N70" t="s">
         <v>437</v>
@@ -6095,7 +6100,7 @@
         <v>441</v>
       </c>
       <c r="C71" s="1" t="n">
-        <v>44032</v>
+        <v>44034</v>
       </c>
       <c r="D71" t="s">
         <v>442</v>
@@ -6105,25 +6110,25 @@
       </c>
       <c r="F71"/>
       <c r="G71" t="n">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="H71" t="n">
-        <v>446036</v>
+        <v>455798</v>
       </c>
       <c r="I71" t="n">
-        <v>154.817</v>
+        <v>158.205</v>
       </c>
       <c r="J71" t="n">
-        <v>4336</v>
+        <v>4630</v>
       </c>
       <c r="K71" t="n">
-        <v>1.505</v>
+        <v>1.607</v>
       </c>
       <c r="L71" t="n">
-        <v>4196</v>
+        <v>4420</v>
       </c>
       <c r="M71" t="n">
-        <v>1.456</v>
+        <v>1.534</v>
       </c>
       <c r="N71" t="s">
         <v>443</v>
@@ -6146,7 +6151,7 @@
         <v>447</v>
       </c>
       <c r="C72" s="1" t="n">
-        <v>44030</v>
+        <v>44033</v>
       </c>
       <c r="D72" t="s">
         <v>448</v>
@@ -6156,25 +6161,25 @@
       </c>
       <c r="F72"/>
       <c r="G72" t="n">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="H72" t="n">
-        <v>943733</v>
+        <v>984396</v>
       </c>
       <c r="I72" t="n">
-        <v>49.056</v>
+        <v>51.17</v>
       </c>
       <c r="J72" t="n">
-        <v>18732</v>
+        <v>17204</v>
       </c>
       <c r="K72" t="n">
-        <v>0.974</v>
+        <v>0.894</v>
       </c>
       <c r="L72" t="n">
-        <v>14969</v>
+        <v>16260</v>
       </c>
       <c r="M72" t="n">
-        <v>0.778</v>
+        <v>0.845</v>
       </c>
       <c r="N72" t="s">
         <v>450</v>
@@ -6197,7 +6202,7 @@
         <v>454</v>
       </c>
       <c r="C73" s="1" t="n">
-        <v>44031</v>
+        <v>44033</v>
       </c>
       <c r="D73" t="s">
         <v>455</v>
@@ -6207,25 +6212,25 @@
       </c>
       <c r="F73"/>
       <c r="G73" t="n">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="H73" t="n">
-        <v>25251614</v>
+        <v>25704372</v>
       </c>
       <c r="I73" t="n">
-        <v>173.034</v>
+        <v>176.136</v>
       </c>
       <c r="J73" t="n">
-        <v>259874</v>
+        <v>255205</v>
       </c>
       <c r="K73" t="n">
-        <v>1.781</v>
+        <v>1.749</v>
       </c>
       <c r="L73" t="n">
-        <v>279855</v>
+        <v>278532</v>
       </c>
       <c r="M73" t="n">
-        <v>1.918</v>
+        <v>1.909</v>
       </c>
       <c r="N73" t="s">
         <v>456</v>
@@ -6299,7 +6304,7 @@
         <v>466</v>
       </c>
       <c r="C75" s="1" t="n">
-        <v>44032</v>
+        <v>44034</v>
       </c>
       <c r="D75" t="s">
         <v>467</v>
@@ -6309,25 +6314,25 @@
       </c>
       <c r="F75"/>
       <c r="G75" t="n">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="H75" t="n">
-        <v>2719136</v>
+        <v>2827766</v>
       </c>
       <c r="I75" t="n">
-        <v>78.105</v>
+        <v>81.225</v>
       </c>
       <c r="J75" t="n">
-        <v>57498</v>
+        <v>52180</v>
       </c>
       <c r="K75" t="n">
-        <v>1.652</v>
+        <v>1.499</v>
       </c>
       <c r="L75" t="n">
-        <v>55936</v>
+        <v>57196</v>
       </c>
       <c r="M75" t="n">
-        <v>1.607</v>
+        <v>1.643</v>
       </c>
       <c r="N75" t="s">
         <v>40</v>
@@ -6350,7 +6355,7 @@
         <v>470</v>
       </c>
       <c r="C76" s="1" t="n">
-        <v>44031</v>
+        <v>44033</v>
       </c>
       <c r="D76" t="s">
         <v>471</v>
@@ -6362,25 +6367,25 @@
         <v>473</v>
       </c>
       <c r="G76" t="n">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="H76" t="n">
-        <v>96364</v>
+        <v>97372</v>
       </c>
       <c r="I76" t="n">
-        <v>5.755</v>
+        <v>5.815</v>
       </c>
       <c r="J76" t="n">
-        <v>712</v>
+        <v>369</v>
       </c>
       <c r="K76" t="n">
-        <v>0.043</v>
+        <v>0.022</v>
       </c>
       <c r="L76" t="n">
-        <v>861</v>
+        <v>794</v>
       </c>
       <c r="M76" t="n">
-        <v>0.051</v>
+        <v>0.047</v>
       </c>
       <c r="N76" t="s">
         <v>474</v>
@@ -6403,7 +6408,7 @@
         <v>479</v>
       </c>
       <c r="C77" s="1" t="n">
-        <v>44032</v>
+        <v>44034</v>
       </c>
       <c r="D77" t="s">
         <v>480</v>
@@ -6415,25 +6420,25 @@
         <v>481</v>
       </c>
       <c r="G77" t="n">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="H77" t="n">
-        <v>558440</v>
+        <v>580271</v>
       </c>
       <c r="I77" t="n">
-        <v>82.068</v>
+        <v>85.276</v>
       </c>
       <c r="J77" t="n">
-        <v>8349</v>
+        <v>11521</v>
       </c>
       <c r="K77" t="n">
-        <v>1.227</v>
+        <v>1.693</v>
       </c>
       <c r="L77" t="n">
-        <v>8585</v>
+        <v>9268</v>
       </c>
       <c r="M77" t="n">
-        <v>1.262</v>
+        <v>1.362</v>
       </c>
       <c r="N77" t="s">
         <v>40</v>
@@ -6456,7 +6461,7 @@
         <v>485</v>
       </c>
       <c r="C78" s="1" t="n">
-        <v>44025</v>
+        <v>44032</v>
       </c>
       <c r="D78" t="s">
         <v>486</v>
@@ -6466,21 +6471,21 @@
       </c>
       <c r="F78"/>
       <c r="G78" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H78" t="n">
-        <v>519911</v>
+        <v>571496</v>
       </c>
       <c r="I78" t="n">
-        <v>88.868</v>
+        <v>97.686</v>
       </c>
       <c r="J78"/>
       <c r="K78"/>
       <c r="L78" t="n">
-        <v>7558</v>
+        <v>7369</v>
       </c>
       <c r="M78" t="n">
-        <v>1.292</v>
+        <v>1.26</v>
       </c>
       <c r="N78" t="s">
         <v>40</v>
@@ -6503,7 +6508,7 @@
         <v>488</v>
       </c>
       <c r="C79" s="1" t="n">
-        <v>44025</v>
+        <v>44032</v>
       </c>
       <c r="D79" t="s">
         <v>486</v>
@@ -6513,21 +6518,21 @@
       </c>
       <c r="F79"/>
       <c r="G79" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H79" t="n">
-        <v>1009532</v>
+        <v>1170049</v>
       </c>
       <c r="I79" t="n">
-        <v>172.559</v>
+        <v>199.997</v>
       </c>
       <c r="J79"/>
       <c r="K79"/>
       <c r="L79" t="n">
-        <v>20445</v>
+        <v>22931</v>
       </c>
       <c r="M79" t="n">
-        <v>3.495</v>
+        <v>3.92</v>
       </c>
       <c r="N79" t="s">
         <v>40</v>
@@ -6550,7 +6555,7 @@
         <v>491</v>
       </c>
       <c r="C80" s="1" t="n">
-        <v>44031</v>
+        <v>44034</v>
       </c>
       <c r="D80" t="s">
         <v>492</v>
@@ -6560,209 +6565,209 @@
       </c>
       <c r="F80"/>
       <c r="G80" t="n">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="H80" t="n">
-        <v>240205</v>
+        <v>246133</v>
       </c>
       <c r="I80" t="n">
-        <v>43.996</v>
+        <v>45.082</v>
       </c>
       <c r="J80" t="n">
-        <v>410</v>
+        <v>2571</v>
       </c>
       <c r="K80" t="n">
-        <v>0.075</v>
+        <v>0.471</v>
       </c>
       <c r="L80" t="n">
-        <v>1488</v>
+        <v>1814</v>
       </c>
       <c r="M80" t="n">
-        <v>0.273</v>
+        <v>0.332</v>
       </c>
       <c r="N80" t="s">
         <v>494</v>
       </c>
       <c r="O80" t="s">
+        <v>492</v>
+      </c>
+      <c r="P80" t="s">
         <v>495</v>
       </c>
-      <c r="P80" t="s">
+      <c r="Q80" t="s">
         <v>496</v>
-      </c>
-      <c r="Q80" t="s">
-        <v>497</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="s">
+        <v>497</v>
+      </c>
+      <c r="B81" t="s">
         <v>498</v>
       </c>
-      <c r="B81" t="s">
+      <c r="C81" s="1" t="n">
+        <v>44033</v>
+      </c>
+      <c r="D81" t="s">
         <v>499</v>
       </c>
-      <c r="C81" s="1" t="n">
-        <v>44031</v>
-      </c>
-      <c r="D81" t="s">
+      <c r="E81" t="s">
         <v>500</v>
-      </c>
-      <c r="E81" t="s">
-        <v>501</v>
       </c>
       <c r="F81"/>
       <c r="G81" t="n">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="H81" t="n">
-        <v>120907</v>
+        <v>122971</v>
       </c>
       <c r="I81" t="n">
-        <v>58.158</v>
+        <v>59.151</v>
       </c>
       <c r="J81" t="n">
-        <v>371</v>
+        <v>1150</v>
       </c>
       <c r="K81" t="n">
-        <v>0.178</v>
+        <v>0.553</v>
       </c>
       <c r="L81" t="n">
-        <v>892</v>
+        <v>855</v>
       </c>
       <c r="M81" t="n">
-        <v>0.429</v>
+        <v>0.411</v>
       </c>
       <c r="N81" t="s">
+        <v>501</v>
+      </c>
+      <c r="O81" t="s">
         <v>502</v>
-      </c>
-      <c r="O81" t="s">
-        <v>503</v>
       </c>
       <c r="P81" t="s">
         <v>22</v>
       </c>
       <c r="Q81" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="s">
+        <v>504</v>
+      </c>
+      <c r="B82" t="s">
         <v>505</v>
       </c>
-      <c r="B82" t="s">
+      <c r="C82" s="1" t="n">
+        <v>44033</v>
+      </c>
+      <c r="D82" t="s">
         <v>506</v>
       </c>
-      <c r="C82" s="1" t="n">
-        <v>44031</v>
-      </c>
-      <c r="D82" t="s">
+      <c r="E82" t="s">
         <v>507</v>
       </c>
-      <c r="E82" t="s">
+      <c r="F82" t="s">
         <v>508</v>
       </c>
-      <c r="F82" t="s">
+      <c r="G82" t="n">
+        <v>143</v>
+      </c>
+      <c r="H82" t="n">
+        <v>2536921</v>
+      </c>
+      <c r="I82" t="n">
+        <v>42.775</v>
+      </c>
+      <c r="J82" t="n">
+        <v>31275</v>
+      </c>
+      <c r="K82" t="n">
+        <v>0.527</v>
+      </c>
+      <c r="L82" t="n">
+        <v>43455</v>
+      </c>
+      <c r="M82" t="n">
+        <v>0.733</v>
+      </c>
+      <c r="N82" t="s">
+        <v>507</v>
+      </c>
+      <c r="O82" t="s">
         <v>509</v>
-      </c>
-      <c r="G82" t="n">
-        <v>141</v>
-      </c>
-      <c r="H82" t="n">
-        <v>2471747</v>
-      </c>
-      <c r="I82" t="n">
-        <v>41.676</v>
-      </c>
-      <c r="J82" t="n">
-        <v>49006</v>
-      </c>
-      <c r="K82" t="n">
-        <v>0.826</v>
-      </c>
-      <c r="L82" t="n">
-        <v>45337</v>
-      </c>
-      <c r="M82" t="n">
-        <v>0.764</v>
-      </c>
-      <c r="N82" t="s">
-        <v>508</v>
-      </c>
-      <c r="O82" t="s">
-        <v>510</v>
       </c>
       <c r="P82" t="s">
         <v>88</v>
       </c>
       <c r="Q82" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="s">
+        <v>511</v>
+      </c>
+      <c r="B83" t="s">
         <v>512</v>
       </c>
-      <c r="B83" t="s">
+      <c r="C83" s="1" t="n">
+        <v>44034</v>
+      </c>
+      <c r="D83" t="s">
         <v>513</v>
       </c>
-      <c r="C83" s="1" t="n">
-        <v>44031</v>
-      </c>
-      <c r="D83" t="s">
+      <c r="E83" t="s">
         <v>514</v>
-      </c>
-      <c r="E83" t="s">
-        <v>515</v>
       </c>
       <c r="F83"/>
       <c r="G83" t="n">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="H83" t="n">
-        <v>1443346</v>
+        <v>1470320</v>
       </c>
       <c r="I83" t="n">
-        <v>28.152</v>
+        <v>28.678</v>
       </c>
       <c r="J83" t="n">
-        <v>6065</v>
+        <v>11794</v>
       </c>
       <c r="K83" t="n">
-        <v>0.118</v>
+        <v>0.23</v>
       </c>
       <c r="L83" t="n">
-        <v>9005</v>
+        <v>8900</v>
       </c>
       <c r="M83" t="n">
-        <v>0.176</v>
+        <v>0.174</v>
       </c>
       <c r="N83" t="s">
+        <v>514</v>
+      </c>
+      <c r="O83" t="s">
         <v>515</v>
-      </c>
-      <c r="O83" t="s">
-        <v>516</v>
       </c>
       <c r="P83" t="s">
         <v>88</v>
       </c>
       <c r="Q83" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="s">
+        <v>517</v>
+      </c>
+      <c r="B84" t="s">
         <v>518</v>
-      </c>
-      <c r="B84" t="s">
-        <v>519</v>
       </c>
       <c r="C84" s="1" t="n">
         <v>44028</v>
       </c>
       <c r="D84" t="s">
+        <v>519</v>
+      </c>
+      <c r="E84" t="s">
         <v>520</v>
-      </c>
-      <c r="E84" t="s">
-        <v>521</v>
       </c>
       <c r="F84"/>
       <c r="G84" t="n">
@@ -6783,33 +6788,33 @@
         <v>0.684</v>
       </c>
       <c r="N84" t="s">
+        <v>521</v>
+      </c>
+      <c r="O84" t="s">
         <v>522</v>
-      </c>
-      <c r="O84" t="s">
-        <v>523</v>
       </c>
       <c r="P84" t="s">
         <v>22</v>
       </c>
       <c r="Q84" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="s">
+        <v>524</v>
+      </c>
+      <c r="B85" t="s">
         <v>525</v>
-      </c>
-      <c r="B85" t="s">
-        <v>526</v>
       </c>
       <c r="C85" s="1" t="n">
         <v>44017</v>
       </c>
       <c r="D85" t="s">
+        <v>526</v>
+      </c>
+      <c r="E85" t="s">
         <v>527</v>
-      </c>
-      <c r="E85" t="s">
-        <v>528</v>
       </c>
       <c r="F85"/>
       <c r="G85" t="n">
@@ -6830,229 +6835,229 @@
         <v>1.098</v>
       </c>
       <c r="N85" t="s">
+        <v>528</v>
+      </c>
+      <c r="O85" t="s">
         <v>529</v>
-      </c>
-      <c r="O85" t="s">
-        <v>530</v>
       </c>
       <c r="P85" t="s">
         <v>88</v>
       </c>
       <c r="Q85" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="B86" t="s">
+        <v>531</v>
+      </c>
+      <c r="C86" s="1" t="n">
+        <v>44031</v>
+      </c>
+      <c r="D86" t="s">
         <v>532</v>
       </c>
-      <c r="C86" s="1" t="n">
-        <v>44024</v>
-      </c>
-      <c r="D86" t="s">
-        <v>533</v>
-      </c>
       <c r="E86" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="F86"/>
       <c r="G86" t="n">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="H86"/>
       <c r="I86"/>
       <c r="J86" t="n">
-        <v>11686</v>
+        <v>9913</v>
       </c>
       <c r="K86" t="n">
-        <v>1.157</v>
+        <v>0.982</v>
       </c>
       <c r="L86" t="n">
-        <v>11686</v>
+        <v>9913</v>
       </c>
       <c r="M86" t="n">
-        <v>1.157</v>
+        <v>0.982</v>
       </c>
       <c r="N86" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="O86" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="P86" t="s">
         <v>49</v>
       </c>
       <c r="Q86" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="s">
+        <v>534</v>
+      </c>
+      <c r="B87" t="s">
         <v>535</v>
       </c>
-      <c r="B87" t="s">
+      <c r="C87" s="1" t="n">
+        <v>44033</v>
+      </c>
+      <c r="D87" t="s">
         <v>536</v>
       </c>
-      <c r="C87" s="1" t="n">
-        <v>44030</v>
-      </c>
-      <c r="D87" t="s">
+      <c r="E87" t="s">
         <v>537</v>
-      </c>
-      <c r="E87" t="s">
-        <v>538</v>
       </c>
       <c r="F87"/>
       <c r="G87" t="n">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="H87" t="n">
-        <v>727158</v>
+        <v>739616</v>
       </c>
       <c r="I87" t="n">
-        <v>84.02</v>
+        <v>85.459</v>
       </c>
       <c r="J87" t="n">
-        <v>3364</v>
+        <v>4641</v>
       </c>
       <c r="K87" t="n">
-        <v>0.389</v>
+        <v>0.536</v>
       </c>
       <c r="L87" t="n">
-        <v>5976</v>
+        <v>5252</v>
       </c>
       <c r="M87" t="n">
-        <v>0.69</v>
+        <v>0.607</v>
       </c>
       <c r="N87" t="s">
+        <v>537</v>
+      </c>
+      <c r="O87" t="s">
+        <v>536</v>
+      </c>
+      <c r="P87" t="s">
         <v>538</v>
       </c>
-      <c r="O87" t="s">
-        <v>537</v>
-      </c>
-      <c r="P87" t="s">
+      <c r="Q87" t="s">
         <v>539</v>
-      </c>
-      <c r="Q87" t="s">
-        <v>540</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="s">
+        <v>540</v>
+      </c>
+      <c r="B88" t="s">
         <v>541</v>
       </c>
-      <c r="B88" t="s">
+      <c r="C88" s="1" t="n">
+        <v>44033</v>
+      </c>
+      <c r="D88" t="s">
         <v>542</v>
       </c>
-      <c r="C88" s="1" t="n">
-        <v>44030</v>
-      </c>
-      <c r="D88" t="s">
+      <c r="E88" t="s">
         <v>543</v>
-      </c>
-      <c r="E88" t="s">
-        <v>544</v>
       </c>
       <c r="F88"/>
       <c r="G88" t="n">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="H88" t="n">
-        <v>79506</v>
+        <v>79951</v>
       </c>
       <c r="I88" t="n">
-        <v>3.338</v>
+        <v>3.357</v>
       </c>
       <c r="J88"/>
       <c r="K88"/>
       <c r="L88" t="n">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="M88" t="n">
         <v>0.006</v>
       </c>
       <c r="N88" t="s">
+        <v>543</v>
+      </c>
+      <c r="O88" t="s">
         <v>544</v>
       </c>
-      <c r="O88" t="s">
+      <c r="P88" t="s">
+        <v>88</v>
+      </c>
+      <c r="Q88" t="s">
         <v>545</v>
-      </c>
-      <c r="P88" t="s">
-        <v>546</v>
-      </c>
-      <c r="Q88" t="s">
-        <v>547</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="s">
+        <v>546</v>
+      </c>
+      <c r="B89" t="s">
+        <v>547</v>
+      </c>
+      <c r="C89" s="1" t="n">
+        <v>44034</v>
+      </c>
+      <c r="D89" t="s">
         <v>548</v>
       </c>
-      <c r="B89" t="s">
+      <c r="E89" t="s">
         <v>549</v>
-      </c>
-      <c r="C89" s="1" t="n">
-        <v>44031</v>
-      </c>
-      <c r="D89" t="s">
-        <v>550</v>
-      </c>
-      <c r="E89" t="s">
-        <v>551</v>
       </c>
       <c r="F89"/>
       <c r="G89" t="n">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="H89" t="n">
-        <v>348650</v>
+        <v>355830</v>
       </c>
       <c r="I89" t="n">
-        <v>4.995</v>
+        <v>5.098</v>
       </c>
       <c r="J89" t="n">
-        <v>5823</v>
+        <v>2993</v>
       </c>
       <c r="K89" t="n">
-        <v>0.083</v>
+        <v>0.043</v>
       </c>
       <c r="L89" t="n">
-        <v>2519</v>
+        <v>2726</v>
       </c>
       <c r="M89" t="n">
-        <v>0.036</v>
+        <v>0.039</v>
       </c>
       <c r="N89" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
       <c r="O89" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
       <c r="P89" t="s">
         <v>88</v>
       </c>
       <c r="Q89" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="B90" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="C90" s="1" t="n">
         <v>44008</v>
       </c>
       <c r="D90" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="E90" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="F90"/>
       <c r="G90" t="n">
@@ -7073,34 +7078,34 @@
         <v>0.072</v>
       </c>
       <c r="N90" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="O90" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="P90" t="s">
         <v>49</v>
       </c>
       <c r="Q90" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="B91" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="C91" s="1" t="n">
         <v>44031</v>
       </c>
       <c r="D91"/>
       <c r="E91" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="F91" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="G91" t="n">
         <v>132</v>
@@ -7124,36 +7129,36 @@
         <v>0.045</v>
       </c>
       <c r="N91" t="s">
+        <v>560</v>
+      </c>
+      <c r="O91" t="s">
         <v>562</v>
-      </c>
-      <c r="O91" t="s">
-        <v>564</v>
       </c>
       <c r="P91" t="s">
         <v>49</v>
       </c>
       <c r="Q91" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="B92" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
       <c r="C92" s="1" t="n">
         <v>44004</v>
       </c>
       <c r="D92" t="s">
+        <v>566</v>
+      </c>
+      <c r="E92" t="s">
+        <v>567</v>
+      </c>
+      <c r="F92" t="s">
         <v>568</v>
-      </c>
-      <c r="E92" t="s">
-        <v>569</v>
-      </c>
-      <c r="F92" t="s">
-        <v>570</v>
       </c>
       <c r="G92" t="n">
         <v>76</v>
@@ -7177,43 +7182,43 @@
         <v>0.063</v>
       </c>
       <c r="N92" t="s">
+        <v>567</v>
+      </c>
+      <c r="O92" t="s">
         <v>569</v>
-      </c>
-      <c r="O92" t="s">
-        <v>571</v>
       </c>
       <c r="P92" t="s">
         <v>22</v>
       </c>
       <c r="Q92" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="s">
+        <v>571</v>
+      </c>
+      <c r="B93" t="s">
+        <v>572</v>
+      </c>
+      <c r="C93" s="1" t="n">
+        <v>44034</v>
+      </c>
+      <c r="D93" t="s">
         <v>573</v>
       </c>
-      <c r="B93" t="s">
+      <c r="E93" t="s">
         <v>574</v>
-      </c>
-      <c r="C93" s="1" t="n">
-        <v>44032</v>
-      </c>
-      <c r="D93" t="s">
-        <v>575</v>
-      </c>
-      <c r="E93" t="s">
-        <v>576</v>
       </c>
       <c r="F93"/>
       <c r="G93" t="n">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="H93" t="n">
-        <v>4316781</v>
+        <v>4403031</v>
       </c>
       <c r="I93" t="n">
-        <v>51.184</v>
+        <v>52.206</v>
       </c>
       <c r="J93" t="n">
         <v>43404</v>
@@ -7222,386 +7227,394 @@
         <v>0.515</v>
       </c>
       <c r="L93" t="n">
-        <v>42119</v>
+        <v>42219</v>
       </c>
       <c r="M93" t="n">
-        <v>0.499</v>
+        <v>0.501</v>
       </c>
       <c r="N93" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="O93" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="P93" t="s">
         <v>22</v>
       </c>
       <c r="Q93" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="s">
+        <v>576</v>
+      </c>
+      <c r="B94" t="s">
+        <v>577</v>
+      </c>
+      <c r="C94" s="1" t="n">
+        <v>44033</v>
+      </c>
+      <c r="D94" t="s">
         <v>578</v>
       </c>
-      <c r="B94" t="s">
+      <c r="E94" t="s">
         <v>579</v>
-      </c>
-      <c r="C94" s="1" t="n">
-        <v>44031</v>
-      </c>
-      <c r="D94" t="s">
-        <v>580</v>
-      </c>
-      <c r="E94" t="s">
-        <v>581</v>
       </c>
       <c r="F94"/>
       <c r="G94" t="n">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="H94"/>
       <c r="I94"/>
       <c r="J94" t="n">
-        <v>2196</v>
+        <v>2098</v>
       </c>
       <c r="K94" t="n">
-        <v>0.048</v>
-      </c>
-      <c r="L94"/>
-      <c r="M94"/>
+        <v>0.046</v>
+      </c>
+      <c r="L94" t="n">
+        <v>2788</v>
+      </c>
+      <c r="M94" t="n">
+        <v>0.061</v>
+      </c>
       <c r="N94" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="O94" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
       <c r="P94" t="s">
         <v>49</v>
       </c>
       <c r="Q94" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="s">
+        <v>582</v>
+      </c>
+      <c r="B95" t="s">
+        <v>583</v>
+      </c>
+      <c r="C95" s="1" t="n">
+        <v>44034</v>
+      </c>
+      <c r="D95" t="s">
         <v>584</v>
       </c>
-      <c r="B95" t="s">
+      <c r="E95" t="s">
         <v>585</v>
-      </c>
-      <c r="C95" s="1" t="n">
-        <v>44031</v>
-      </c>
-      <c r="D95" t="s">
-        <v>586</v>
-      </c>
-      <c r="E95" t="s">
-        <v>587</v>
       </c>
       <c r="F95"/>
       <c r="G95" t="n">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="H95" t="n">
-        <v>877262</v>
+        <v>907360</v>
       </c>
       <c r="I95" t="n">
-        <v>20.059</v>
+        <v>20.747</v>
       </c>
       <c r="J95" t="n">
-        <v>12666</v>
+        <v>12967</v>
       </c>
       <c r="K95" t="n">
-        <v>0.29</v>
+        <v>0.296</v>
       </c>
       <c r="L95" t="n">
-        <v>11512</v>
+        <v>11458</v>
       </c>
       <c r="M95" t="n">
-        <v>0.263</v>
+        <v>0.262</v>
       </c>
       <c r="N95" t="s">
+        <v>585</v>
+      </c>
+      <c r="O95" t="s">
+        <v>586</v>
+      </c>
+      <c r="P95" t="s">
         <v>587</v>
       </c>
-      <c r="O95" t="s">
+      <c r="Q95" t="s">
         <v>588</v>
-      </c>
-      <c r="P95" t="s">
-        <v>589</v>
-      </c>
-      <c r="Q95" t="s">
-        <v>590</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="s">
+        <v>589</v>
+      </c>
+      <c r="B96" t="s">
+        <v>590</v>
+      </c>
+      <c r="C96" s="1" t="n">
+        <v>44034</v>
+      </c>
+      <c r="D96" t="s">
         <v>591</v>
       </c>
-      <c r="B96" t="s">
+      <c r="E96" t="s">
         <v>592</v>
-      </c>
-      <c r="C96" s="1" t="n">
-        <v>44032</v>
-      </c>
-      <c r="D96" t="s">
-        <v>593</v>
-      </c>
-      <c r="E96" t="s">
-        <v>594</v>
       </c>
       <c r="F96"/>
       <c r="G96" t="n">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="H96" t="n">
-        <v>4536152</v>
+        <v>4623216</v>
       </c>
       <c r="I96" t="n">
-        <v>458.642</v>
+        <v>467.445</v>
       </c>
       <c r="J96" t="n">
-        <v>27224</v>
+        <v>47014</v>
       </c>
       <c r="K96" t="n">
-        <v>2.753</v>
+        <v>4.753</v>
       </c>
       <c r="L96" t="n">
-        <v>45815</v>
+        <v>43779</v>
       </c>
       <c r="M96" t="n">
-        <v>4.632</v>
+        <v>4.426</v>
       </c>
       <c r="N96" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="O96" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="P96" t="s">
         <v>49</v>
       </c>
       <c r="Q96" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="s">
+        <v>595</v>
+      </c>
+      <c r="B97" t="s">
+        <v>596</v>
+      </c>
+      <c r="C97" s="1" t="n">
+        <v>44033</v>
+      </c>
+      <c r="D97" t="s">
         <v>597</v>
       </c>
-      <c r="B97" t="s">
+      <c r="E97" t="s">
         <v>598</v>
       </c>
-      <c r="C97" s="1" t="n">
-        <v>44031</v>
-      </c>
-      <c r="D97" t="s">
+      <c r="F97" t="s">
         <v>599</v>
       </c>
-      <c r="E97" t="s">
+      <c r="G97" t="n">
+        <v>113</v>
+      </c>
+      <c r="H97" t="n">
+        <v>8256935</v>
+      </c>
+      <c r="I97" t="n">
+        <v>121.629</v>
+      </c>
+      <c r="J97" t="n">
+        <v>121694</v>
+      </c>
+      <c r="K97" t="n">
+        <v>1.793</v>
+      </c>
+      <c r="L97" t="n">
+        <v>125906</v>
+      </c>
+      <c r="M97" t="n">
+        <v>1.855</v>
+      </c>
+      <c r="N97" t="s">
+        <v>598</v>
+      </c>
+      <c r="O97" t="s">
         <v>600</v>
-      </c>
-      <c r="F97" t="s">
-        <v>601</v>
-      </c>
-      <c r="G97" t="n">
-        <v>111</v>
-      </c>
-      <c r="H97" t="n">
-        <v>8050171</v>
-      </c>
-      <c r="I97" t="n">
-        <v>118.584</v>
-      </c>
-      <c r="J97" t="n">
-        <v>102572</v>
-      </c>
-      <c r="K97" t="n">
-        <v>1.511</v>
-      </c>
-      <c r="L97" t="n">
-        <v>123051</v>
-      </c>
-      <c r="M97" t="n">
-        <v>1.813</v>
-      </c>
-      <c r="N97" t="s">
-        <v>600</v>
-      </c>
-      <c r="O97" t="s">
-        <v>602</v>
       </c>
       <c r="P97" t="s">
         <v>22</v>
       </c>
       <c r="Q97" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="s">
+        <v>602</v>
+      </c>
+      <c r="B98" t="s">
+        <v>603</v>
+      </c>
+      <c r="C98" s="1" t="n">
+        <v>44033</v>
+      </c>
+      <c r="D98" t="s">
         <v>604</v>
       </c>
-      <c r="B98" t="s">
+      <c r="E98" t="s">
         <v>605</v>
-      </c>
-      <c r="C98" s="1" t="n">
-        <v>44029</v>
-      </c>
-      <c r="D98" t="s">
-        <v>606</v>
-      </c>
-      <c r="E98" t="s">
-        <v>607</v>
       </c>
       <c r="F98"/>
       <c r="G98" t="n">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="H98" t="n">
-        <v>47313367</v>
+        <v>50343272</v>
       </c>
       <c r="I98" t="n">
-        <v>142.94</v>
+        <v>152.093</v>
       </c>
       <c r="J98" t="n">
-        <v>761762</v>
+        <v>1740157</v>
       </c>
       <c r="K98" t="n">
-        <v>2.301</v>
+        <v>5.257</v>
       </c>
       <c r="L98" t="n">
-        <v>932216</v>
+        <v>963952</v>
       </c>
       <c r="M98" t="n">
-        <v>2.816</v>
+        <v>2.912</v>
       </c>
       <c r="N98" t="s">
+        <v>605</v>
+      </c>
+      <c r="O98" t="s">
+        <v>604</v>
+      </c>
+      <c r="P98" t="s">
+        <v>606</v>
+      </c>
+      <c r="Q98" t="s">
         <v>607</v>
-      </c>
-      <c r="O98" t="s">
-        <v>606</v>
-      </c>
-      <c r="P98" t="s">
-        <v>608</v>
-      </c>
-      <c r="Q98" t="s">
-        <v>609</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
       <c r="B99" t="s">
+        <v>608</v>
+      </c>
+      <c r="C99" s="1" t="n">
+        <v>44033</v>
+      </c>
+      <c r="D99" t="s">
+        <v>609</v>
+      </c>
+      <c r="E99" t="s">
         <v>610</v>
-      </c>
-      <c r="C99" s="1" t="n">
-        <v>44031</v>
-      </c>
-      <c r="D99" t="s">
-        <v>611</v>
-      </c>
-      <c r="E99" t="s">
-        <v>612</v>
       </c>
       <c r="F99"/>
       <c r="G99" t="n">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="H99" t="n">
-        <v>45734327</v>
+        <v>47224382</v>
       </c>
       <c r="I99" t="n">
-        <v>138.169</v>
+        <v>142.671</v>
       </c>
       <c r="J99" t="n">
-        <v>768823</v>
+        <v>749355</v>
       </c>
       <c r="K99" t="n">
-        <v>2.323</v>
+        <v>2.264</v>
       </c>
       <c r="L99" t="n">
-        <v>778879</v>
+        <v>778209</v>
       </c>
       <c r="M99" t="n">
-        <v>2.353</v>
+        <v>2.351</v>
       </c>
       <c r="N99" t="s">
+        <v>610</v>
+      </c>
+      <c r="O99" t="s">
+        <v>611</v>
+      </c>
+      <c r="P99" t="s">
         <v>612</v>
       </c>
-      <c r="O99" t="s">
+      <c r="Q99" t="s">
         <v>613</v>
-      </c>
-      <c r="P99" t="s">
-        <v>614</v>
-      </c>
-      <c r="Q99" t="s">
-        <v>615</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="s">
+        <v>614</v>
+      </c>
+      <c r="B100" t="s">
+        <v>615</v>
+      </c>
+      <c r="C100" s="1" t="n">
+        <v>44033</v>
+      </c>
+      <c r="D100" t="s">
         <v>616</v>
-      </c>
-      <c r="B100" t="s">
-        <v>617</v>
-      </c>
-      <c r="C100" s="1" t="n">
-        <v>44031</v>
-      </c>
-      <c r="D100" t="s">
-        <v>618</v>
       </c>
       <c r="E100" t="s">
         <v>120</v>
       </c>
       <c r="F100"/>
       <c r="G100" t="n">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="H100" t="n">
-        <v>88616</v>
+        <v>92056</v>
       </c>
       <c r="I100" t="n">
-        <v>25.51</v>
-      </c>
-      <c r="J100"/>
-      <c r="K100"/>
+        <v>26.501</v>
+      </c>
+      <c r="J100" t="n">
+        <v>1407</v>
+      </c>
+      <c r="K100" t="n">
+        <v>0.405</v>
+      </c>
       <c r="L100" t="n">
-        <v>1433</v>
+        <v>1516</v>
       </c>
       <c r="M100" t="n">
-        <v>0.413</v>
+        <v>0.436</v>
       </c>
       <c r="N100" t="s">
         <v>120</v>
       </c>
       <c r="O100" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
       <c r="P100" t="s">
         <v>22</v>
       </c>
       <c r="Q100" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
       <c r="B101" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
       <c r="C101" s="1" t="n">
         <v>43950</v>
       </c>
       <c r="D101" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
       <c r="E101" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
       <c r="F101"/>
       <c r="G101" t="n">
@@ -7622,33 +7635,33 @@
         <v>0.112</v>
       </c>
       <c r="N101" t="s">
+        <v>622</v>
+      </c>
+      <c r="O101" t="s">
+        <v>623</v>
+      </c>
+      <c r="P101" t="s">
         <v>624</v>
       </c>
-      <c r="O101" t="s">
+      <c r="Q101" t="s">
         <v>625</v>
-      </c>
-      <c r="P101" t="s">
-        <v>626</v>
-      </c>
-      <c r="Q101" t="s">
-        <v>627</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
       <c r="B102" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
       <c r="C102" s="1" t="n">
         <v>44031</v>
       </c>
       <c r="D102" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
       <c r="E102" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="F102"/>
       <c r="G102" t="n">
@@ -7673,16 +7686,16 @@
         <v>0.043</v>
       </c>
       <c r="N102" t="s">
-        <v>631</v>
+        <v>629</v>
       </c>
       <c r="O102" t="s">
-        <v>632</v>
+        <v>630</v>
       </c>
       <c r="P102" t="s">
         <v>22</v>
       </c>
       <c r="Q102" t="s">
-        <v>633</v>
+        <v>631</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated testing data for 2020-08-03
</commit_message>
<xml_diff>
--- a/public/data/testing/covid-testing-latest-data-source-details.xlsx
+++ b/public/data/testing/covid-testing-latest-data-source-details.xlsx
@@ -104,7 +104,7 @@
     <t xml:space="preserve">Australia - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.health.gov.au/sites/default/files/documents/2020/07/coronavirus-covid-19-at-a-glance-30-july-2020.pdf</t>
+    <t xml:space="preserve">https://www.health.gov.au/sites/default/files/documents/2020/08/coronavirus-covid-19-at-a-glance-2-august-2020.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">Australian Government Department of Health</t>
@@ -196,7 +196,7 @@
     <t xml:space="preserve">Belarus - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">http://minzdrav.gov.by/ru/sobytiya/v-belarusi-na-31-iyulya-vyzdoroveli-i-vypisany-62-444-patsienta/</t>
+    <t xml:space="preserve">http://minzdrav.gov.by/ru/sobytiya/u-belarusi-na-2-zhni-nya-vypisanyya-62-tys-896-patsyenta/</t>
   </si>
   <si>
     <t xml:space="preserve">Belarus Ministry of Health</t>
@@ -243,7 +243,7 @@
     <t xml:space="preserve">Bolivia - units unclear</t>
   </si>
   <si>
-    <t xml:space="preserve">https://minsalud.gob.bo/4451-covid-19-se-reportan-1-207-contagios-nuevos-y-el-numero-de-pacientes-recuperados-supera-los-22-500</t>
+    <t xml:space="preserve">https://minsalud.gob.bo/4457-ministerio-de-salud-reporta-1-700-contagios-nuevos-de-coronavirus-y-86-fallecidos</t>
   </si>
   <si>
     <t xml:space="preserve">https://www.minsalud.gob.bo/</t>
@@ -383,6 +383,7 @@
     <t xml:space="preserve">The Costa Rican Ministry of Health produce daily update reports of confirmed cases, deaths and test results.
 These daily reports state the daily number of people who have been tested – given as the number of confirmed cases (‘Confirma contagio’) and number of people with negative results (‘Descarta contagio’) (thus the figures do not include pending tests). We can use these daily updates to construct a full time-series. This figures have been collected and are made available for download by the news website [El Observador](https://observador.cr/covid19-estadisticas/), from which we take our data.
 Daily reports with figures on testing are only available dating back to 11th March. We therefore do not know the first date of testing, or daily figures prior to this date.
+For the number of new tests reported on 25 March 2020, we noticed a discrepancy between data published by El Observador and the official data from the Ministry of Health. We there replaced the number of discarded tests for that day (5) with the official number (65) (official reports: [24 March](https://www.ministeriodesalud.go.cr/sobre_ministerio/prensa/img_cvd/img_datos_marzo_2020_14.jpeg), [25 March](https://www.ministeriodesalud.go.cr/sobre_ministerio/prensa/img_cvd/img_datos_marzo_2020_15.jpeg)).
 Our data for this series is sourced from a non-official repository of official data. As explained in our [FAQ here](https://ourworldindata.org/coronavirus-testing#do-you-rely-on-any-non-official-sources) we regularly audit the accuracy of this repository against direct official channels. Note that, due to the way the data is presented by the official source, the time series may be impacted by retrospective revisions made by the source – see our [FAQ here](https://ourworldindata.org/coronavirus-testing#does-your-data-reflect-retrospective-updates-made-by-the-source).</t>
   </si>
   <si>
@@ -392,7 +393,7 @@
     <t xml:space="preserve">Cote d'Ivoire - samples tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.facebook.com/Mshpci/posts/1656954844470203</t>
+    <t xml:space="preserve">https://www.facebook.com/Mshpci/posts/1657886101043744</t>
   </si>
   <si>
     <t xml:space="preserve">Ministry of Health and Public Hygiene</t>
@@ -474,7 +475,7 @@
     <t xml:space="preserve">Democratic Republic of Congo - samples tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/CMR_Covid19_RDC/status/1288809742090080258/photo/1</t>
+    <t xml:space="preserve">https://twitter.com/CMR_Covid19_RDC/status/1289257564119511043/photo/1</t>
   </si>
   <si>
     <t xml:space="preserve">DRC COVID-19 Pandemic Response Multisectoral Committee</t>
@@ -492,7 +493,7 @@
     <t xml:space="preserve">Denmark - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://files.ssi.dk/Data-Epidemiologiske-Rapport-31072020-we21</t>
+    <t xml:space="preserve">https://files.ssi.dk/Data-epidemiologisk-rapport-03082020-mm79</t>
   </si>
   <si>
     <t xml:space="preserve">Statens Serum Institut</t>
@@ -510,7 +511,7 @@
     <t xml:space="preserve">Ecuador - units unclear</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.gestionderiesgos.gob.ec/wp-content/uploads/2020/07/INFOGRAFIA-NACIONALCOVI-19-COE-NACIONAL-08h00-31072020.pdf</t>
+    <t xml:space="preserve">https://www.gestionderiesgos.gob.ec/wp-content/uploads/2020/08/INFOGRAFIA-NACIONALCOVI-19-COE-NACIONAL-08h00-01082020.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">Government of Ecuador</t>
@@ -748,7 +749,7 @@
     <t xml:space="preserve">Greece - samples tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://eody.gov.gr/covid-gr-daily-report-20200729</t>
+    <t xml:space="preserve">https://eody.gov.gr/covid-gr-daily-report-20200802</t>
   </si>
   <si>
     <t xml:space="preserve">National Organization of Public Health</t>
@@ -888,7 +889,7 @@
     <t xml:space="preserve">Iran - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">http://irangov.ir/detail/344270</t>
+    <t xml:space="preserve">http://irangov.ir/detail/344480</t>
   </si>
   <si>
     <t xml:space="preserve">Government of Iran</t>
@@ -925,7 +926,7 @@
     <t xml:space="preserve">Israel - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://govextra.gov.il/media/23395/covid19-data-israel-23072020.xlsx</t>
+    <t xml:space="preserve">https://govextra.gov.il/media/23626/covid19-data-israel-27072020.csv</t>
   </si>
   <si>
     <t xml:space="preserve">Israel Ministry of Health</t>
@@ -984,13 +985,13 @@
     <t xml:space="preserve">Japan - people tested (incl. non-PCR)</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.mhlw.go.jp/stf/newpage_12763.html</t>
+    <t xml:space="preserve">https://www.mhlw.go.jp/stf/newpage_12781.html</t>
   </si>
   <si>
     <t xml:space="preserve">Ministry of Health, Labor and Welfare Press Release</t>
   </si>
   <si>
-    <t xml:space="preserve">See Table: 国内の発生状況, column 1 '検査実施人数'.</t>
+    <t xml:space="preserve">See Table: 国内の発生状況, column 1 '検査実施人数'. Daily change figure provided for this date is not consistent with the cumulative totals for today and the previous day.</t>
   </si>
   <si>
     <t xml:space="preserve">Ministry of Health, Labor and Welfare</t>
@@ -1009,10 +1010,10 @@
     <t xml:space="preserve">Japan - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.mhlw.go.jp/content/10906000/000654713.pdf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The cumulative total reported in the press release (1,084,347) does not sum to the cumulative total calculated from the weekly and daily figures reported by the MOH. See: https://www.mhlw.go.jp/content/10906000/000654713.pdf</t>
+    <t xml:space="preserve">https://www.mhlw.go.jp/content/10906000/000655354.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The cumulative total reported in the press release (1,101,541) does not sum to the cumulative total calculated from the weekly and daily figures reported by the MOH. See: https://www.mhlw.go.jp/content/10906000/000655354.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">On 11th April 2020, the MOH started providing a daily time series on the "Implementation status of PCR tests for new coronavirus in Japan (based on the date on which results were determined" (via Google translate). 
@@ -1067,7 +1068,7 @@
     <t xml:space="preserve">Kuwait - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/KUWAIT_MOH/status/1288806619275558914/photo/1</t>
+    <t xml:space="preserve">https://twitter.com/KUWAIT_MOH/status/1289161413970112513/photo/1</t>
   </si>
   <si>
     <t xml:space="preserve">Kuwait Ministry of Health</t>
@@ -1133,7 +1134,7 @@
     <t xml:space="preserve">Malaysia - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">http://covid-19.moh.gov.my/terkini/072020/situasi-terkini-31-julai-2020</t>
+    <t xml:space="preserve">http://covid-19.moh.gov.my/terkini/082020/situasi-terkini-02-ogos-2020</t>
   </si>
   <si>
     <t xml:space="preserve">Ministry of Health Malaysia</t>
@@ -1159,7 +1160,7 @@
     <t xml:space="preserve">Maldives - samples tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/HPA_MV/status/1288528885559119872/photo/1</t>
+    <t xml:space="preserve">https://twitter.com/HPA_MV/status/1289244995736580096/photo/1</t>
   </si>
   <si>
     <t xml:space="preserve">Maldives Health Protection Agency</t>
@@ -1226,7 +1227,7 @@
     <t xml:space="preserve">Morocco - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/Ministere_Sante/status/1288522745270149122/photo/1</t>
+    <t xml:space="preserve">https://twitter.com/Ministere_Sante/status/1288885676889591816/photo/1</t>
   </si>
   <si>
     <t xml:space="preserve">Morocco Ministry of Health</t>
@@ -1266,7 +1267,7 @@
     <t xml:space="preserve">Nepal - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://drive.google.com/drive/folders/1z8ddX6wpS4mWEZgB5DUVqKGZyo9oqaT0</t>
+    <t xml:space="preserve">https://drive.google.com/drive/folders/1mgqdZykT84Gd8Xl2ozjs93bjIJ-UqW_k</t>
   </si>
   <si>
     <t xml:space="preserve">Ministry of Health and Population</t>
@@ -1488,7 +1489,7 @@
     <t xml:space="preserve">Poland - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/MZ_GOV_PL/status/1289123640336941057</t>
+    <t xml:space="preserve">https://twitter.com/MZ_GOV_PL/status/1289848411890413568</t>
   </si>
   <si>
     <t xml:space="preserve">Poland Ministry of Health</t>
@@ -1555,7 +1556,7 @@
     <t xml:space="preserve">Romania - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://gov.ro/ro/media/comunicate/buletin-de-presa-31-iulie-2020-ora-13-00&amp;page=1</t>
+    <t xml:space="preserve">https://gov.ro/ro/media/comunicate/buletin-de-presa-3-august-2020-ora-13-00&amp;page=1</t>
   </si>
   <si>
     <t xml:space="preserve">Ministry of Internal Affairs</t>
@@ -1578,7 +1579,7 @@
     <t xml:space="preserve">Russia - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://rospotrebnadzor.ru/about/info/news/news_details.php?ELEMENT_ID=15054</t>
+    <t xml:space="preserve">https://rospotrebnadzor.ru/about/info/news/news_details.php?ELEMENT_ID=15070</t>
   </si>
   <si>
     <t xml:space="preserve">Government of the Russian Federation</t>
@@ -1780,7 +1781,7 @@
     <t xml:space="preserve">South Korea - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.cdc.go.kr/board/board.es?mid=&amp;bid=0030&amp;act=view&amp;list_no=367938&amp;tag=&amp;nPage=1</t>
+    <t xml:space="preserve">https://www.cdc.go.kr/board/board.es?mid=&amp;bid=0030&amp;act=view&amp;list_no=367974&amp;tag=&amp;nPage=1</t>
   </si>
   <si>
     <t xml:space="preserve">South Korea CDC</t>
@@ -1895,7 +1896,7 @@
     <t xml:space="preserve">Thailand - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://ddc.moph.go.th/viralpneumonia/file/situation/situation-no210-310763.pdf</t>
+    <t xml:space="preserve">https://ddc.moph.go.th/viralpneumonia/file/situation/situation-no212-020863.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">Department of Disease Control</t>
@@ -1983,7 +1984,7 @@
     <t xml:space="preserve">Uganda - samples tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/MinofHealthUG/status/1289228240893153281/photo/2</t>
+    <t xml:space="preserve">https://twitter.com/MinofHealthUG/status/1289536809718824960/photo/2</t>
   </si>
   <si>
     <t xml:space="preserve">Uganda Ministry of Health</t>
@@ -1992,10 +1993,9 @@
     <t xml:space="preserve">https://twitter.com/MinofHealthUG</t>
   </si>
   <si>
-    <t xml:space="preserve">The Uganda Ministry of Health publishes a daily press release detailing the number of cumulative and daily samples tested. As a result of missing daily testing figures (for 17/05, 03/06, 14/07) and retrospective revisions by the MOH to cumulative totals, we report only the daily number of samples tested.  
-From 12 June, the press releases regularly include the official cumulative number of samples tested. Prior to this date, only daily testing figures were reported - with the exception of reports from 06-14/04. 
-The earliest press release we could find that lists the cumulative and daily figures is for 1st April. However, we cannot say with certainty when testing began and the precise date from which cumulative totals begin.
-Note that, due to the way the data is presented by the official source, the time series may be impacted by retrospective revisions made by the source – see our [FAQ here](https://ourworldindata.org/coronavirus-testing#does-your-data-reflect-retrospective-updates-made-by-the-source).</t>
+    <t xml:space="preserve">The Uganda Ministry of Health publishes a daily press release detailing the number of cumulative and daily samples tested. As a result of changes in the way the data is published, we only report the cumulative total of samples tested when it is published by the official source.
+From late June 2020, the press releases regularly include the official cumulative number of samples tested. Prior to this date, only daily testing figures were reported - with the exception of reports from 6–14 April 2020.
+The earliest press release we could find that lists the cumulative and daily figures is for 1 April 2020. However, we cannot say with certainty when testing began and the precise date from which cumulative totals begin.</t>
   </si>
   <si>
     <t xml:space="preserve">UKR</t>
@@ -2044,7 +2044,7 @@
     <t xml:space="preserve">United Kingdom - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://assets.publishing.service.gov.uk/government/uploads/system/uploads/attachment_data/file/905963/2020-07-31_COVID-19_UK_testing_time_series.csv</t>
+    <t xml:space="preserve">https://assets.publishing.service.gov.uk/government/uploads/system/uploads/attachment_data/file/906109/2020-08-02-COVID-19-UK-testing-time-series.csv</t>
   </si>
   <si>
     <t xml:space="preserve">Public Health England/Department of Health and Social Care</t>
@@ -2124,7 +2124,7 @@
     <t xml:space="preserve">Uruguay - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.gub.uy/ministerio-salud-publica/comunicacion/noticias/informe-situacion-sobre-coronavirus-covid-19-uruguay-8</t>
+    <t xml:space="preserve">https://www.gub.uy/ministerio-salud-publica/comunicacion/noticias/informe-situacion-sobre-coronavirus-covid-19-uruguay-11</t>
   </si>
   <si>
     <t xml:space="preserve">https://www.gub.uy/ministerio-salud-publica/comunicacion/noticias</t>
@@ -2576,7 +2576,7 @@
         <v>18</v>
       </c>
       <c r="C2" s="1" t="n">
-        <v>44040</v>
+        <v>44044</v>
       </c>
       <c r="D2" t="s">
         <v>19</v>
@@ -2586,25 +2586,25 @@
       </c>
       <c r="F2"/>
       <c r="G2" t="n">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="H2" t="n">
-        <v>574629</v>
+        <v>626413</v>
       </c>
       <c r="I2" t="n">
-        <v>12.714</v>
+        <v>13.86</v>
       </c>
       <c r="J2" t="n">
-        <v>10394</v>
+        <v>7298</v>
       </c>
       <c r="K2" t="n">
-        <v>0.23</v>
+        <v>0.161</v>
       </c>
       <c r="L2" t="n">
-        <v>10883</v>
+        <v>10921</v>
       </c>
       <c r="M2" t="n">
-        <v>0.241</v>
+        <v>0.242</v>
       </c>
       <c r="N2" t="s">
         <v>20</v>
@@ -2627,7 +2627,7 @@
         <v>23</v>
       </c>
       <c r="C3" s="1" t="n">
-        <v>44040</v>
+        <v>44044</v>
       </c>
       <c r="D3" t="s">
         <v>24</v>
@@ -2637,25 +2637,25 @@
       </c>
       <c r="F3"/>
       <c r="G3" t="n">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="H3" t="n">
-        <v>704951</v>
+        <v>767023</v>
       </c>
       <c r="I3" t="n">
-        <v>15.598</v>
+        <v>16.971</v>
       </c>
       <c r="J3" t="n">
-        <v>12289</v>
+        <v>8495</v>
       </c>
       <c r="K3" t="n">
-        <v>0.272</v>
+        <v>0.188</v>
       </c>
       <c r="L3" t="n">
-        <v>13029</v>
+        <v>12936</v>
       </c>
       <c r="M3" t="n">
-        <v>0.288</v>
+        <v>0.286</v>
       </c>
       <c r="N3" t="s">
         <v>20</v>
@@ -2678,7 +2678,7 @@
         <v>28</v>
       </c>
       <c r="C4" s="1" t="n">
-        <v>44042</v>
+        <v>44044</v>
       </c>
       <c r="D4" t="s">
         <v>29</v>
@@ -2688,21 +2688,21 @@
       </c>
       <c r="F4"/>
       <c r="G4" t="n">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="H4" t="n">
-        <v>4164454</v>
+        <v>4346382</v>
       </c>
       <c r="I4" t="n">
-        <v>163.313</v>
+        <v>170.447</v>
       </c>
       <c r="J4"/>
       <c r="K4"/>
       <c r="L4" t="n">
-        <v>63517</v>
+        <v>69554</v>
       </c>
       <c r="M4" t="n">
-        <v>2.491</v>
+        <v>2.728</v>
       </c>
       <c r="N4" t="s">
         <v>30</v>
@@ -2725,7 +2725,7 @@
         <v>34</v>
       </c>
       <c r="C5" s="1" t="n">
-        <v>44042</v>
+        <v>44045</v>
       </c>
       <c r="D5" t="s">
         <v>35</v>
@@ -2735,25 +2735,25 @@
       </c>
       <c r="F5"/>
       <c r="G5" t="n">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="H5" t="n">
-        <v>890461</v>
+        <v>910437</v>
       </c>
       <c r="I5" t="n">
-        <v>98.87</v>
+        <v>101.088</v>
       </c>
       <c r="J5" t="n">
-        <v>10425</v>
+        <v>5123</v>
       </c>
       <c r="K5" t="n">
-        <v>1.158</v>
+        <v>0.569</v>
       </c>
       <c r="L5" t="n">
-        <v>9204</v>
+        <v>8934</v>
       </c>
       <c r="M5" t="n">
-        <v>1.022</v>
+        <v>0.992</v>
       </c>
       <c r="N5" t="s">
         <v>37</v>
@@ -2776,7 +2776,7 @@
         <v>41</v>
       </c>
       <c r="C6" s="1" t="n">
-        <v>44042</v>
+        <v>44045</v>
       </c>
       <c r="D6" t="s">
         <v>42</v>
@@ -2786,25 +2786,25 @@
       </c>
       <c r="F6"/>
       <c r="G6" t="n">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="H6" t="n">
-        <v>826672</v>
+        <v>842992</v>
       </c>
       <c r="I6" t="n">
-        <v>485.825</v>
+        <v>495.416</v>
       </c>
       <c r="J6" t="n">
-        <v>9064</v>
+        <v>7425</v>
       </c>
       <c r="K6" t="n">
-        <v>5.327</v>
+        <v>4.364</v>
       </c>
       <c r="L6" t="n">
-        <v>9420</v>
+        <v>7650</v>
       </c>
       <c r="M6" t="n">
-        <v>5.536</v>
+        <v>4.496</v>
       </c>
       <c r="N6" t="s">
         <v>44</v>
@@ -2878,7 +2878,7 @@
         <v>55</v>
       </c>
       <c r="C8" s="1" t="n">
-        <v>44043</v>
+        <v>44045</v>
       </c>
       <c r="D8" t="s">
         <v>56</v>
@@ -2888,21 +2888,21 @@
       </c>
       <c r="F8"/>
       <c r="G8" t="n">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="H8" t="n">
-        <v>1299428</v>
+        <v>1319976</v>
       </c>
       <c r="I8" t="n">
-        <v>137.515</v>
+        <v>139.69</v>
       </c>
       <c r="J8"/>
       <c r="K8"/>
       <c r="L8" t="n">
-        <v>9821</v>
+        <v>9802</v>
       </c>
       <c r="M8" t="n">
-        <v>1.039</v>
+        <v>1.037</v>
       </c>
       <c r="N8" t="s">
         <v>57</v>
@@ -2925,7 +2925,7 @@
         <v>61</v>
       </c>
       <c r="C9" s="1" t="n">
-        <v>44041</v>
+        <v>44044</v>
       </c>
       <c r="D9" t="s">
         <v>62</v>
@@ -2935,25 +2935,25 @@
       </c>
       <c r="F9"/>
       <c r="G9" t="n">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="H9" t="n">
-        <v>1248474</v>
+        <v>1702556</v>
       </c>
       <c r="I9" t="n">
-        <v>107.724</v>
+        <v>146.904</v>
       </c>
       <c r="J9" t="n">
-        <v>15122</v>
+        <v>17168</v>
       </c>
       <c r="K9" t="n">
-        <v>1.305</v>
+        <v>1.481</v>
       </c>
       <c r="L9" t="n">
-        <v>12357</v>
+        <v>19120</v>
       </c>
       <c r="M9" t="n">
-        <v>1.066</v>
+        <v>1.65</v>
       </c>
       <c r="N9" t="s">
         <v>63</v>
@@ -2976,7 +2976,7 @@
         <v>68</v>
       </c>
       <c r="C10" s="1" t="n">
-        <v>44041</v>
+        <v>44042</v>
       </c>
       <c r="D10" t="s">
         <v>69</v>
@@ -2986,25 +2986,25 @@
       </c>
       <c r="F10"/>
       <c r="G10" t="n">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="H10" t="n">
-        <v>144153</v>
+        <v>147458</v>
       </c>
       <c r="I10" t="n">
-        <v>12.349</v>
+        <v>12.632</v>
       </c>
       <c r="J10" t="n">
-        <v>2035</v>
+        <v>3305</v>
       </c>
       <c r="K10" t="n">
-        <v>0.174</v>
+        <v>0.283</v>
       </c>
       <c r="L10" t="n">
-        <v>2427</v>
+        <v>2579</v>
       </c>
       <c r="M10" t="n">
-        <v>0.208</v>
+        <v>0.221</v>
       </c>
       <c r="N10" t="s">
         <v>43</v>
@@ -3076,7 +3076,7 @@
         <v>82</v>
       </c>
       <c r="C12" s="1" t="n">
-        <v>44042</v>
+        <v>44044</v>
       </c>
       <c r="D12" t="s">
         <v>83</v>
@@ -3086,25 +3086,25 @@
       </c>
       <c r="F12"/>
       <c r="G12" t="n">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="H12" t="n">
-        <v>261463</v>
+        <v>271000</v>
       </c>
       <c r="I12" t="n">
-        <v>37.629</v>
+        <v>39.002</v>
       </c>
       <c r="J12" t="n">
-        <v>6639</v>
+        <v>3955</v>
       </c>
       <c r="K12" t="n">
-        <v>0.955</v>
+        <v>0.569</v>
       </c>
       <c r="L12" t="n">
-        <v>5673</v>
+        <v>5030</v>
       </c>
       <c r="M12" t="n">
-        <v>0.816</v>
+        <v>0.724</v>
       </c>
       <c r="N12" t="s">
         <v>85</v>
@@ -3127,7 +3127,7 @@
         <v>88</v>
       </c>
       <c r="C13" s="1" t="n">
-        <v>44042</v>
+        <v>44045</v>
       </c>
       <c r="D13" t="s">
         <v>89</v>
@@ -3137,25 +3137,25 @@
       </c>
       <c r="F13"/>
       <c r="G13" t="n">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="H13" t="n">
-        <v>3996625</v>
+        <v>4143459</v>
       </c>
       <c r="I13" t="n">
-        <v>105.893</v>
+        <v>109.783</v>
       </c>
       <c r="J13" t="n">
-        <v>50060</v>
+        <v>44707</v>
       </c>
       <c r="K13" t="n">
-        <v>1.326</v>
+        <v>1.185</v>
       </c>
       <c r="L13" t="n">
-        <v>48121</v>
+        <v>54505</v>
       </c>
       <c r="M13" t="n">
-        <v>1.275</v>
+        <v>1.444</v>
       </c>
       <c r="N13" t="s">
         <v>90</v>
@@ -3178,7 +3178,7 @@
         <v>93</v>
       </c>
       <c r="C14" s="1" t="n">
-        <v>44043</v>
+        <v>44045</v>
       </c>
       <c r="D14" t="s">
         <v>94</v>
@@ -3190,25 +3190,25 @@
         <v>95</v>
       </c>
       <c r="G14" t="n">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="H14" t="n">
-        <v>1623992</v>
+        <v>1673289</v>
       </c>
       <c r="I14" t="n">
-        <v>84.954</v>
+        <v>87.532</v>
       </c>
       <c r="J14" t="n">
-        <v>22874</v>
+        <v>24899</v>
       </c>
       <c r="K14" t="n">
-        <v>1.197</v>
+        <v>1.303</v>
       </c>
       <c r="L14" t="n">
-        <v>19754</v>
+        <v>21248</v>
       </c>
       <c r="M14" t="n">
-        <v>1.033</v>
+        <v>1.112</v>
       </c>
       <c r="N14" t="s">
         <v>96</v>
@@ -3231,7 +3231,7 @@
         <v>100</v>
       </c>
       <c r="C15" s="1" t="n">
-        <v>44041</v>
+        <v>44045</v>
       </c>
       <c r="D15" t="s">
         <v>101</v>
@@ -3241,25 +3241,25 @@
       </c>
       <c r="F15"/>
       <c r="G15" t="n">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="H15" t="n">
-        <v>1502809</v>
+        <v>1647395</v>
       </c>
       <c r="I15" t="n">
-        <v>29.535</v>
+        <v>32.376</v>
       </c>
       <c r="J15" t="n">
-        <v>32196</v>
+        <v>37666</v>
       </c>
       <c r="K15" t="n">
-        <v>0.633</v>
+        <v>0.74</v>
       </c>
       <c r="L15" t="n">
-        <v>30044</v>
+        <v>34039</v>
       </c>
       <c r="M15" t="n">
-        <v>0.59</v>
+        <v>0.669</v>
       </c>
       <c r="N15" t="s">
         <v>102</v>
@@ -3282,7 +3282,7 @@
         <v>106</v>
       </c>
       <c r="C16" s="1" t="n">
-        <v>44042</v>
+        <v>44043</v>
       </c>
       <c r="D16" t="s">
         <v>107</v>
@@ -3292,25 +3292,25 @@
       </c>
       <c r="F16"/>
       <c r="G16" t="n">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="H16" t="n">
-        <v>74924</v>
+        <v>76728</v>
       </c>
       <c r="I16" t="n">
-        <v>14.708</v>
+        <v>15.062</v>
       </c>
       <c r="J16" t="n">
-        <v>1840</v>
+        <v>1744</v>
       </c>
       <c r="K16" t="n">
-        <v>0.361</v>
+        <v>0.342</v>
       </c>
       <c r="L16" t="n">
-        <v>1659</v>
+        <v>1693</v>
       </c>
       <c r="M16" t="n">
-        <v>0.326</v>
+        <v>0.332</v>
       </c>
       <c r="N16" t="s">
         <v>108</v>
@@ -3333,7 +3333,7 @@
         <v>112</v>
       </c>
       <c r="C17" s="1" t="n">
-        <v>44043</v>
+        <v>44044</v>
       </c>
       <c r="D17" t="s">
         <v>113</v>
@@ -3343,25 +3343,25 @@
       </c>
       <c r="F17"/>
       <c r="G17" t="n">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="H17" t="n">
-        <v>100685</v>
+        <v>101583</v>
       </c>
       <c r="I17" t="n">
-        <v>3.817</v>
+        <v>3.851</v>
       </c>
       <c r="J17" t="n">
-        <v>951</v>
+        <v>898</v>
       </c>
       <c r="K17" t="n">
-        <v>0.036</v>
+        <v>0.034</v>
       </c>
       <c r="L17" t="n">
-        <v>1290</v>
+        <v>1132</v>
       </c>
       <c r="M17" t="n">
-        <v>0.049</v>
+        <v>0.043</v>
       </c>
       <c r="N17" t="s">
         <v>114</v>
@@ -3384,7 +3384,7 @@
         <v>118</v>
       </c>
       <c r="C18" s="1" t="n">
-        <v>44043</v>
+        <v>44046</v>
       </c>
       <c r="D18" t="s">
         <v>119</v>
@@ -3394,25 +3394,25 @@
       </c>
       <c r="F18"/>
       <c r="G18" t="n">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="H18" t="n">
-        <v>118955</v>
+        <v>122083</v>
       </c>
       <c r="I18" t="n">
-        <v>28.976</v>
+        <v>29.738</v>
       </c>
       <c r="J18" t="n">
-        <v>1785</v>
+        <v>763</v>
       </c>
       <c r="K18" t="n">
-        <v>0.435</v>
+        <v>0.186</v>
       </c>
       <c r="L18" t="n">
-        <v>1371</v>
+        <v>1321</v>
       </c>
       <c r="M18" t="n">
-        <v>0.334</v>
+        <v>0.322</v>
       </c>
       <c r="N18" t="s">
         <v>120</v>
@@ -3435,7 +3435,7 @@
         <v>125</v>
       </c>
       <c r="C19" s="1" t="n">
-        <v>44042</v>
+        <v>44045</v>
       </c>
       <c r="D19" t="s">
         <v>126</v>
@@ -3447,25 +3447,25 @@
         <v>128</v>
       </c>
       <c r="G19" t="n">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="H19" t="n">
-        <v>264147</v>
+        <v>274474</v>
       </c>
       <c r="I19" t="n">
-        <v>23.321</v>
+        <v>24.233</v>
       </c>
       <c r="J19" t="n">
-        <v>3696</v>
+        <v>3485</v>
       </c>
       <c r="K19" t="n">
-        <v>0.326</v>
+        <v>0.308</v>
       </c>
       <c r="L19" t="n">
-        <v>3322</v>
+        <v>3437</v>
       </c>
       <c r="M19" t="n">
-        <v>0.293</v>
+        <v>0.303</v>
       </c>
       <c r="N19" t="s">
         <v>127</v>
@@ -3488,7 +3488,7 @@
         <v>132</v>
       </c>
       <c r="C20" s="1" t="n">
-        <v>44042</v>
+        <v>44044</v>
       </c>
       <c r="D20" t="s">
         <v>133</v>
@@ -3498,25 +3498,25 @@
       </c>
       <c r="F20"/>
       <c r="G20" t="n">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="H20" t="n">
-        <v>690799</v>
+        <v>703504</v>
       </c>
       <c r="I20" t="n">
-        <v>64.507</v>
+        <v>65.693</v>
       </c>
       <c r="J20" t="n">
-        <v>7205</v>
+        <v>4528</v>
       </c>
       <c r="K20" t="n">
-        <v>0.673</v>
+        <v>0.423</v>
       </c>
       <c r="L20" t="n">
-        <v>5736</v>
+        <v>6183</v>
       </c>
       <c r="M20" t="n">
-        <v>0.536</v>
+        <v>0.577</v>
       </c>
       <c r="N20" t="s">
         <v>43</v>
@@ -3539,7 +3539,7 @@
         <v>137</v>
       </c>
       <c r="C21" s="1" t="n">
-        <v>44041</v>
+        <v>44042</v>
       </c>
       <c r="D21" t="s">
         <v>138</v>
@@ -3549,21 +3549,21 @@
       </c>
       <c r="F21"/>
       <c r="G21" t="n">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="H21"/>
       <c r="I21"/>
       <c r="J21" t="n">
-        <v>637</v>
+        <v>364</v>
       </c>
       <c r="K21" t="n">
-        <v>0.007</v>
+        <v>0.004</v>
       </c>
       <c r="L21" t="n">
-        <v>434</v>
+        <v>394</v>
       </c>
       <c r="M21" t="n">
-        <v>0.005</v>
+        <v>0.004</v>
       </c>
       <c r="N21" t="s">
         <v>139</v>
@@ -3586,7 +3586,7 @@
         <v>143</v>
       </c>
       <c r="C22" s="1" t="n">
-        <v>44042</v>
+        <v>44045</v>
       </c>
       <c r="D22" t="s">
         <v>144</v>
@@ -3596,25 +3596,25 @@
       </c>
       <c r="F22"/>
       <c r="G22" t="n">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="H22" t="n">
-        <v>1504512</v>
+        <v>1557930</v>
       </c>
       <c r="I22" t="n">
-        <v>259.748</v>
+        <v>268.97</v>
       </c>
       <c r="J22" t="n">
-        <v>4548</v>
+        <v>3364</v>
       </c>
       <c r="K22" t="n">
-        <v>0.785</v>
+        <v>0.581</v>
       </c>
       <c r="L22" t="n">
-        <v>15138</v>
+        <v>16963</v>
       </c>
       <c r="M22" t="n">
-        <v>2.614</v>
+        <v>2.929</v>
       </c>
       <c r="N22" t="s">
         <v>145</v>
@@ -3637,7 +3637,7 @@
         <v>149</v>
       </c>
       <c r="C23" s="1" t="n">
-        <v>44043</v>
+        <v>44044</v>
       </c>
       <c r="D23" t="s">
         <v>150</v>
@@ -3649,25 +3649,25 @@
         <v>152</v>
       </c>
       <c r="G23" t="n">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="H23" t="n">
-        <v>181594</v>
+        <v>184045</v>
       </c>
       <c r="I23" t="n">
-        <v>10.293</v>
+        <v>10.432</v>
       </c>
       <c r="J23" t="n">
-        <v>2501</v>
+        <v>2451</v>
       </c>
       <c r="K23" t="n">
-        <v>0.142</v>
+        <v>0.139</v>
       </c>
       <c r="L23" t="n">
-        <v>2269</v>
+        <v>2323</v>
       </c>
       <c r="M23" t="n">
-        <v>0.129</v>
+        <v>0.132</v>
       </c>
       <c r="N23" t="s">
         <v>151</v>
@@ -3741,7 +3741,7 @@
         <v>162</v>
       </c>
       <c r="C25" s="1" t="n">
-        <v>44042</v>
+        <v>44045</v>
       </c>
       <c r="D25" t="s">
         <v>163</v>
@@ -3751,25 +3751,25 @@
       </c>
       <c r="F25"/>
       <c r="G25" t="n">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="H25" t="n">
-        <v>119217</v>
+        <v>120346</v>
       </c>
       <c r="I25" t="n">
-        <v>89.871</v>
+        <v>90.722</v>
       </c>
       <c r="J25" t="n">
-        <v>721</v>
+        <v>257</v>
       </c>
       <c r="K25" t="n">
-        <v>0.544</v>
+        <v>0.194</v>
       </c>
       <c r="L25" t="n">
-        <v>421</v>
+        <v>479</v>
       </c>
       <c r="M25" t="n">
-        <v>0.317</v>
+        <v>0.361</v>
       </c>
       <c r="N25" t="s">
         <v>165</v>
@@ -3839,7 +3839,7 @@
         <v>176</v>
       </c>
       <c r="C27" s="1" t="n">
-        <v>44039</v>
+        <v>44046</v>
       </c>
       <c r="D27" t="s">
         <v>177</v>
@@ -3849,25 +3849,21 @@
       </c>
       <c r="F27"/>
       <c r="G27" t="n">
-        <v>131</v>
+        <v>137</v>
       </c>
       <c r="H27" t="n">
-        <v>6719</v>
+        <v>6996</v>
       </c>
       <c r="I27" t="n">
-        <v>7.495</v>
-      </c>
-      <c r="J27" t="n">
-        <v>26</v>
-      </c>
-      <c r="K27" t="n">
-        <v>0.029</v>
-      </c>
+        <v>7.804</v>
+      </c>
+      <c r="J27"/>
+      <c r="K27"/>
       <c r="L27" t="n">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="M27" t="n">
-        <v>0.049</v>
+        <v>0.045</v>
       </c>
       <c r="N27" t="s">
         <v>178</v>
@@ -3890,7 +3886,7 @@
         <v>181</v>
       </c>
       <c r="C28" s="1" t="n">
-        <v>44041</v>
+        <v>44044</v>
       </c>
       <c r="D28" t="s">
         <v>182</v>
@@ -3900,25 +3896,25 @@
       </c>
       <c r="F28"/>
       <c r="G28" t="n">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="H28" t="n">
-        <v>359193</v>
+        <v>367775</v>
       </c>
       <c r="I28" t="n">
-        <v>64.828</v>
+        <v>66.377</v>
       </c>
       <c r="J28" t="n">
-        <v>3244</v>
+        <v>407</v>
       </c>
       <c r="K28" t="n">
-        <v>0.585</v>
+        <v>0.073</v>
       </c>
       <c r="L28" t="n">
-        <v>3919</v>
+        <v>3238</v>
       </c>
       <c r="M28" t="n">
-        <v>0.707</v>
+        <v>0.584</v>
       </c>
       <c r="N28" t="s">
         <v>184</v>
@@ -3941,7 +3937,7 @@
         <v>187</v>
       </c>
       <c r="C29" s="1" t="n">
-        <v>44040</v>
+        <v>44042</v>
       </c>
       <c r="D29" t="s">
         <v>188</v>
@@ -3951,21 +3947,21 @@
       </c>
       <c r="F29"/>
       <c r="G29" t="n">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="H29"/>
       <c r="I29"/>
       <c r="J29" t="n">
-        <v>90194</v>
+        <v>88662</v>
       </c>
       <c r="K29" t="n">
-        <v>1.382</v>
+        <v>1.358</v>
       </c>
       <c r="L29" t="n">
-        <v>68413</v>
+        <v>72468</v>
       </c>
       <c r="M29" t="n">
-        <v>1.048</v>
+        <v>1.11</v>
       </c>
       <c r="N29" t="s">
         <v>189</v>
@@ -4086,7 +4082,7 @@
         <v>205</v>
       </c>
       <c r="C32" s="1" t="n">
-        <v>44039</v>
+        <v>44042</v>
       </c>
       <c r="D32" t="s">
         <v>206</v>
@@ -4096,25 +4092,21 @@
       </c>
       <c r="F32"/>
       <c r="G32" t="n">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="H32" t="n">
-        <v>387336</v>
+        <v>396731</v>
       </c>
       <c r="I32" t="n">
-        <v>12.465</v>
-      </c>
-      <c r="J32" t="n">
-        <v>4584</v>
-      </c>
-      <c r="K32" t="n">
-        <v>0.148</v>
-      </c>
+        <v>12.768</v>
+      </c>
+      <c r="J32"/>
+      <c r="K32"/>
       <c r="L32" t="n">
-        <v>3685</v>
+        <v>3451</v>
       </c>
       <c r="M32" t="n">
-        <v>0.119</v>
+        <v>0.111</v>
       </c>
       <c r="N32" t="s">
         <v>208</v>
@@ -4137,7 +4129,7 @@
         <v>213</v>
       </c>
       <c r="C33" s="1" t="n">
-        <v>44041</v>
+        <v>44045</v>
       </c>
       <c r="D33" t="s">
         <v>214</v>
@@ -4147,25 +4139,25 @@
       </c>
       <c r="F33"/>
       <c r="G33" t="n">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="H33" t="n">
-        <v>511429</v>
+        <v>545439</v>
       </c>
       <c r="I33" t="n">
-        <v>49.067</v>
+        <v>52.33</v>
       </c>
       <c r="J33" t="n">
-        <v>53889</v>
+        <v>5946</v>
       </c>
       <c r="K33" t="n">
-        <v>5.17</v>
+        <v>0.57</v>
       </c>
       <c r="L33" t="n">
-        <v>12393</v>
+        <v>13965</v>
       </c>
       <c r="M33" t="n">
-        <v>1.189</v>
+        <v>1.34</v>
       </c>
       <c r="N33" t="s">
         <v>216</v>
@@ -4231,7 +4223,7 @@
         <v>227</v>
       </c>
       <c r="C35" s="1" t="n">
-        <v>44040</v>
+        <v>44046</v>
       </c>
       <c r="D35" t="s">
         <v>228</v>
@@ -4243,25 +4235,25 @@
         <v>230</v>
       </c>
       <c r="G35" t="n">
-        <v>145</v>
+        <v>151</v>
       </c>
       <c r="H35" t="n">
-        <v>330239</v>
+        <v>346962</v>
       </c>
       <c r="I35" t="n">
-        <v>34.185</v>
+        <v>35.916</v>
       </c>
       <c r="J35" t="n">
-        <v>1656</v>
+        <v>1965</v>
       </c>
       <c r="K35" t="n">
-        <v>0.171</v>
+        <v>0.203</v>
       </c>
       <c r="L35" t="n">
-        <v>2773</v>
+        <v>2626</v>
       </c>
       <c r="M35" t="n">
-        <v>0.287</v>
+        <v>0.272</v>
       </c>
       <c r="N35" t="s">
         <v>229</v>
@@ -4284,7 +4276,7 @@
         <v>235</v>
       </c>
       <c r="C36" s="1" t="n">
-        <v>44042</v>
+        <v>44045</v>
       </c>
       <c r="D36" t="s">
         <v>236</v>
@@ -4294,25 +4286,25 @@
       </c>
       <c r="F36"/>
       <c r="G36" t="n">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="H36" t="n">
-        <v>70606</v>
+        <v>73961</v>
       </c>
       <c r="I36" t="n">
-        <v>206.904</v>
+        <v>216.736</v>
       </c>
       <c r="J36" t="n">
-        <v>1138</v>
+        <v>1205</v>
       </c>
       <c r="K36" t="n">
-        <v>3.335</v>
+        <v>3.531</v>
       </c>
       <c r="L36" t="n">
-        <v>255</v>
+        <v>715</v>
       </c>
       <c r="M36" t="n">
-        <v>0.747</v>
+        <v>2.095</v>
       </c>
       <c r="N36" t="s">
         <v>237</v>
@@ -4388,7 +4380,7 @@
         <v>245</v>
       </c>
       <c r="C38" s="1" t="n">
-        <v>44043</v>
+        <v>44046</v>
       </c>
       <c r="D38" t="s">
         <v>241</v>
@@ -4400,22 +4392,22 @@
         <v>243</v>
       </c>
       <c r="G38" t="n">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="H38" t="n">
-        <v>18832970</v>
+        <v>20202858</v>
       </c>
       <c r="I38" t="n">
-        <v>13.647</v>
+        <v>14.64</v>
       </c>
       <c r="J38" t="n">
-        <v>642588</v>
+        <v>381027</v>
       </c>
       <c r="K38" t="n">
-        <v>0.466</v>
+        <v>0.276</v>
       </c>
       <c r="L38" t="n">
-        <v>486400</v>
+        <v>485151</v>
       </c>
       <c r="M38" t="n">
         <v>0.352</v>
@@ -4441,7 +4433,7 @@
         <v>247</v>
       </c>
       <c r="C39" s="1" t="n">
-        <v>44043</v>
+        <v>44046</v>
       </c>
       <c r="D39" t="s">
         <v>248</v>
@@ -4451,25 +4443,25 @@
       </c>
       <c r="F39"/>
       <c r="G39" t="n">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="H39" t="n">
-        <v>866539</v>
+        <v>894531</v>
       </c>
       <c r="I39" t="n">
-        <v>3.168</v>
+        <v>3.27</v>
       </c>
       <c r="J39" t="n">
-        <v>10536</v>
+        <v>12179</v>
       </c>
       <c r="K39" t="n">
-        <v>0.039</v>
+        <v>0.045</v>
       </c>
       <c r="L39" t="n">
-        <v>12777</v>
+        <v>13155</v>
       </c>
       <c r="M39" t="n">
-        <v>0.047</v>
+        <v>0.048</v>
       </c>
       <c r="N39" t="s">
         <v>249</v>
@@ -4492,7 +4484,7 @@
         <v>253</v>
       </c>
       <c r="C40" s="1" t="n">
-        <v>44043</v>
+        <v>44046</v>
       </c>
       <c r="D40" t="s">
         <v>254</v>
@@ -4502,21 +4494,25 @@
       </c>
       <c r="F40"/>
       <c r="G40" t="n">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="H40" t="n">
-        <v>2456909</v>
+        <v>2534658</v>
       </c>
       <c r="I40" t="n">
-        <v>29.251</v>
-      </c>
-      <c r="J40"/>
-      <c r="K40"/>
+        <v>30.177</v>
+      </c>
+      <c r="J40" t="n">
+        <v>26240</v>
+      </c>
+      <c r="K40" t="n">
+        <v>0.312</v>
+      </c>
       <c r="L40" t="n">
-        <v>25504</v>
+        <v>25710</v>
       </c>
       <c r="M40" t="n">
-        <v>0.304</v>
+        <v>0.306</v>
       </c>
       <c r="N40" t="s">
         <v>255</v>
@@ -4539,7 +4535,7 @@
         <v>259</v>
       </c>
       <c r="C41" s="1" t="n">
-        <v>44043</v>
+        <v>44044</v>
       </c>
       <c r="D41" t="s">
         <v>260</v>
@@ -4549,25 +4545,25 @@
       </c>
       <c r="F41"/>
       <c r="G41" t="n">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="H41" t="n">
-        <v>632854</v>
+        <v>636085</v>
       </c>
       <c r="I41" t="n">
-        <v>128.165</v>
+        <v>128.82</v>
       </c>
       <c r="J41" t="n">
-        <v>3856</v>
+        <v>3231</v>
       </c>
       <c r="K41" t="n">
-        <v>0.781</v>
+        <v>0.654</v>
       </c>
       <c r="L41" t="n">
-        <v>5807</v>
+        <v>4999</v>
       </c>
       <c r="M41" t="n">
-        <v>1.176</v>
+        <v>1.012</v>
       </c>
       <c r="N41" t="s">
         <v>261</v>
@@ -4590,7 +4586,7 @@
         <v>264</v>
       </c>
       <c r="C42" s="1" t="n">
-        <v>44035</v>
+        <v>44039</v>
       </c>
       <c r="D42" t="s">
         <v>265</v>
@@ -4600,25 +4596,25 @@
       </c>
       <c r="F42"/>
       <c r="G42" t="n">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="H42" t="n">
-        <v>1596095</v>
+        <v>1676396</v>
       </c>
       <c r="I42" t="n">
-        <v>184.402</v>
+        <v>193.679</v>
       </c>
       <c r="J42" t="n">
-        <v>32255</v>
+        <v>28234</v>
       </c>
       <c r="K42" t="n">
-        <v>3.727</v>
+        <v>3.262</v>
       </c>
       <c r="L42" t="n">
-        <v>26388</v>
+        <v>24501</v>
       </c>
       <c r="M42" t="n">
-        <v>3.049</v>
+        <v>2.831</v>
       </c>
       <c r="N42" t="s">
         <v>43</v>
@@ -4641,7 +4637,7 @@
         <v>270</v>
       </c>
       <c r="C43" s="1" t="n">
-        <v>44043</v>
+        <v>44046</v>
       </c>
       <c r="D43" t="s">
         <v>271</v>
@@ -4653,25 +4649,25 @@
         <v>273</v>
       </c>
       <c r="G43" t="n">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="H43" t="n">
-        <v>4061667</v>
+        <v>4131535</v>
       </c>
       <c r="I43" t="n">
-        <v>67.177</v>
+        <v>68.333</v>
       </c>
       <c r="J43" t="n">
-        <v>29686</v>
+        <v>13467</v>
       </c>
       <c r="K43" t="n">
-        <v>0.491</v>
+        <v>0.223</v>
       </c>
       <c r="L43" t="n">
-        <v>27415</v>
+        <v>27024</v>
       </c>
       <c r="M43" t="n">
-        <v>0.453</v>
+        <v>0.447</v>
       </c>
       <c r="N43" t="s">
         <v>274</v>
@@ -4694,7 +4690,7 @@
         <v>277</v>
       </c>
       <c r="C44" s="1" t="n">
-        <v>44043</v>
+        <v>44046</v>
       </c>
       <c r="D44" t="s">
         <v>271</v>
@@ -4706,25 +4702,25 @@
         <v>273</v>
       </c>
       <c r="G44" t="n">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="H44" t="n">
-        <v>6820613</v>
+        <v>6940801</v>
       </c>
       <c r="I44" t="n">
-        <v>112.809</v>
+        <v>114.796</v>
       </c>
       <c r="J44" t="n">
-        <v>68444</v>
+        <v>24036</v>
       </c>
       <c r="K44" t="n">
-        <v>1.132</v>
+        <v>0.398</v>
       </c>
       <c r="L44" t="n">
-        <v>50320</v>
+        <v>50668</v>
       </c>
       <c r="M44" t="n">
-        <v>0.832</v>
+        <v>0.838</v>
       </c>
       <c r="N44" t="s">
         <v>274</v>
@@ -4747,7 +4743,7 @@
         <v>280</v>
       </c>
       <c r="C45" s="1" t="n">
-        <v>44043</v>
+        <v>44045</v>
       </c>
       <c r="D45" t="s">
         <v>281</v>
@@ -4759,25 +4755,25 @@
         <v>283</v>
       </c>
       <c r="G45" t="n">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="H45" t="n">
-        <v>806067</v>
+        <v>836404</v>
       </c>
       <c r="I45" t="n">
-        <v>6.373</v>
+        <v>6.613</v>
       </c>
       <c r="J45" t="n">
-        <v>20843</v>
+        <v>11656</v>
       </c>
       <c r="K45" t="n">
-        <v>0.165</v>
+        <v>0.092</v>
       </c>
       <c r="L45" t="n">
-        <v>15508</v>
+        <v>17303</v>
       </c>
       <c r="M45" t="n">
-        <v>0.123</v>
+        <v>0.137</v>
       </c>
       <c r="N45" t="s">
         <v>284</v>
@@ -4800,7 +4796,7 @@
         <v>287</v>
       </c>
       <c r="C46" s="1" t="n">
-        <v>44041</v>
+        <v>44042</v>
       </c>
       <c r="D46" t="s">
         <v>288</v>
@@ -4812,25 +4808,25 @@
         <v>289</v>
       </c>
       <c r="G46" t="n">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="H46" t="n">
-        <v>1074305</v>
+        <v>1091499</v>
       </c>
       <c r="I46" t="n">
-        <v>8.494</v>
+        <v>8.63</v>
       </c>
       <c r="J46" t="n">
-        <v>19935</v>
+        <v>17194</v>
       </c>
       <c r="K46" t="n">
-        <v>0.158</v>
+        <v>0.136</v>
       </c>
       <c r="L46" t="n">
-        <v>15297</v>
+        <v>15754</v>
       </c>
       <c r="M46" t="n">
-        <v>0.121</v>
+        <v>0.125</v>
       </c>
       <c r="N46" t="s">
         <v>284</v>
@@ -4955,7 +4951,7 @@
         <v>304</v>
       </c>
       <c r="C49" s="1" t="n">
-        <v>44042</v>
+        <v>44043</v>
       </c>
       <c r="D49" t="s">
         <v>305</v>
@@ -4965,25 +4961,25 @@
       </c>
       <c r="F49"/>
       <c r="G49" t="n">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="H49" t="n">
-        <v>502168</v>
+        <v>505088</v>
       </c>
       <c r="I49" t="n">
-        <v>117.588</v>
+        <v>118.272</v>
       </c>
       <c r="J49" t="n">
-        <v>3811</v>
+        <v>2920</v>
       </c>
       <c r="K49" t="n">
-        <v>0.892</v>
+        <v>0.684</v>
       </c>
       <c r="L49" t="n">
-        <v>3909</v>
+        <v>3668</v>
       </c>
       <c r="M49" t="n">
-        <v>0.915</v>
+        <v>0.859</v>
       </c>
       <c r="N49" t="s">
         <v>306</v>
@@ -5006,7 +5002,7 @@
         <v>310</v>
       </c>
       <c r="C50" s="1" t="n">
-        <v>44043</v>
+        <v>44046</v>
       </c>
       <c r="D50" t="s">
         <v>311</v>
@@ -5018,25 +5014,25 @@
         <v>313</v>
       </c>
       <c r="G50" t="n">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="H50" t="n">
-        <v>198508</v>
+        <v>201997</v>
       </c>
       <c r="I50" t="n">
-        <v>105.242</v>
+        <v>107.092</v>
       </c>
       <c r="J50" t="n">
-        <v>1473</v>
+        <v>687</v>
       </c>
       <c r="K50" t="n">
-        <v>0.781</v>
+        <v>0.364</v>
       </c>
       <c r="L50" t="n">
-        <v>1432</v>
+        <v>1447</v>
       </c>
       <c r="M50" t="n">
-        <v>0.759</v>
+        <v>0.767</v>
       </c>
       <c r="N50" t="s">
         <v>312</v>
@@ -5059,7 +5055,7 @@
         <v>316</v>
       </c>
       <c r="C51" s="1" t="n">
-        <v>44042</v>
+        <v>44045</v>
       </c>
       <c r="D51" t="s">
         <v>317</v>
@@ -5069,25 +5065,21 @@
       </c>
       <c r="F51"/>
       <c r="G51" t="n">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="H51" t="n">
-        <v>519929</v>
+        <v>527729</v>
       </c>
       <c r="I51" t="n">
-        <v>190.99</v>
-      </c>
-      <c r="J51" t="n">
-        <v>4132</v>
-      </c>
-      <c r="K51" t="n">
-        <v>1.518</v>
-      </c>
+        <v>193.855</v>
+      </c>
+      <c r="J51"/>
+      <c r="K51"/>
       <c r="L51" t="n">
-        <v>3723</v>
+        <v>3386</v>
       </c>
       <c r="M51" t="n">
-        <v>1.368</v>
+        <v>1.244</v>
       </c>
       <c r="N51" t="s">
         <v>43</v>
@@ -5110,7 +5102,7 @@
         <v>320</v>
       </c>
       <c r="C52" s="1" t="n">
-        <v>44042</v>
+        <v>44044</v>
       </c>
       <c r="D52" t="s">
         <v>321</v>
@@ -5120,25 +5112,25 @@
       </c>
       <c r="F52"/>
       <c r="G52" t="n">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="H52" t="n">
-        <v>425227</v>
+        <v>432505</v>
       </c>
       <c r="I52" t="n">
-        <v>679.302</v>
+        <v>690.929</v>
       </c>
       <c r="J52" t="n">
-        <v>4962</v>
+        <v>3004</v>
       </c>
       <c r="K52" t="n">
-        <v>7.927</v>
+        <v>4.799</v>
       </c>
       <c r="L52" t="n">
-        <v>5187</v>
+        <v>4552</v>
       </c>
       <c r="M52" t="n">
-        <v>8.286</v>
+        <v>7.272</v>
       </c>
       <c r="N52" t="s">
         <v>322</v>
@@ -5161,7 +5153,7 @@
         <v>325</v>
       </c>
       <c r="C53" s="1" t="n">
-        <v>44043</v>
+        <v>44045</v>
       </c>
       <c r="D53" t="s">
         <v>326</v>
@@ -5173,25 +5165,25 @@
         <v>328</v>
       </c>
       <c r="G53" t="n">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="H53" t="n">
-        <v>970644</v>
+        <v>979178</v>
       </c>
       <c r="I53" t="n">
-        <v>29.99</v>
+        <v>30.253</v>
       </c>
       <c r="J53" t="n">
-        <v>7565</v>
+        <v>4504</v>
       </c>
       <c r="K53" t="n">
-        <v>0.234</v>
+        <v>0.139</v>
       </c>
       <c r="L53" t="n">
-        <v>6494</v>
+        <v>5933</v>
       </c>
       <c r="M53" t="n">
-        <v>0.201</v>
+        <v>0.183</v>
       </c>
       <c r="N53" t="s">
         <v>43</v>
@@ -5214,7 +5206,7 @@
         <v>332</v>
       </c>
       <c r="C54" s="1" t="n">
-        <v>44041</v>
+        <v>44043</v>
       </c>
       <c r="D54" t="s">
         <v>333</v>
@@ -5224,25 +5216,25 @@
       </c>
       <c r="F54"/>
       <c r="G54" t="n">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="H54" t="n">
-        <v>76937</v>
+        <v>78900</v>
       </c>
       <c r="I54" t="n">
-        <v>142.333</v>
+        <v>145.965</v>
       </c>
       <c r="J54" t="n">
-        <v>1387</v>
+        <v>860</v>
       </c>
       <c r="K54" t="n">
-        <v>2.566</v>
+        <v>1.591</v>
       </c>
       <c r="L54" t="n">
-        <v>1081</v>
+        <v>1151</v>
       </c>
       <c r="M54" t="n">
-        <v>2</v>
+        <v>2.129</v>
       </c>
       <c r="N54" t="s">
         <v>335</v>
@@ -5316,7 +5308,7 @@
         <v>345</v>
       </c>
       <c r="C56" s="1" t="n">
-        <v>44033</v>
+        <v>44042</v>
       </c>
       <c r="D56" t="s">
         <v>346</v>
@@ -5326,25 +5318,25 @@
       </c>
       <c r="F56"/>
       <c r="G56" t="n">
-        <v>203</v>
+        <v>212</v>
       </c>
       <c r="H56" t="n">
-        <v>809561</v>
+        <v>920079</v>
       </c>
       <c r="I56" t="n">
-        <v>6.279</v>
+        <v>7.136</v>
       </c>
       <c r="J56" t="n">
-        <v>9300</v>
+        <v>5960</v>
       </c>
       <c r="K56" t="n">
-        <v>0.072</v>
+        <v>0.046</v>
       </c>
       <c r="L56" t="n">
-        <v>10361</v>
+        <v>8499</v>
       </c>
       <c r="M56" t="n">
-        <v>0.08</v>
+        <v>0.066</v>
       </c>
       <c r="N56" t="s">
         <v>348</v>
@@ -5367,7 +5359,7 @@
         <v>352</v>
       </c>
       <c r="C57" s="1" t="n">
-        <v>44041</v>
+        <v>44043</v>
       </c>
       <c r="D57" t="s">
         <v>353</v>
@@ -5377,25 +5369,25 @@
       </c>
       <c r="F57"/>
       <c r="G57" t="n">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="H57" t="n">
-        <v>1210035</v>
+        <v>1252365</v>
       </c>
       <c r="I57" t="n">
-        <v>32.783</v>
+        <v>33.93</v>
       </c>
       <c r="J57" t="n">
-        <v>21234</v>
+        <v>21170</v>
       </c>
       <c r="K57" t="n">
-        <v>0.575</v>
+        <v>0.574</v>
       </c>
       <c r="L57" t="n">
-        <v>20600</v>
+        <v>21013</v>
       </c>
       <c r="M57" t="n">
-        <v>0.558</v>
+        <v>0.569</v>
       </c>
       <c r="N57" t="s">
         <v>354</v>
@@ -5469,7 +5461,7 @@
         <v>364</v>
       </c>
       <c r="C59" s="1" t="n">
-        <v>44041</v>
+        <v>44043</v>
       </c>
       <c r="D59" t="s">
         <v>365</v>
@@ -5479,25 +5471,25 @@
       </c>
       <c r="F59"/>
       <c r="G59" t="n">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="H59" t="n">
-        <v>358344</v>
+        <v>375416</v>
       </c>
       <c r="I59" t="n">
-        <v>12.299</v>
+        <v>12.885</v>
       </c>
       <c r="J59" t="n">
-        <v>6037</v>
+        <v>10768</v>
       </c>
       <c r="K59" t="n">
-        <v>0.207</v>
+        <v>0.37</v>
       </c>
       <c r="L59" t="n">
-        <v>4390</v>
+        <v>5762</v>
       </c>
       <c r="M59" t="n">
-        <v>0.151</v>
+        <v>0.198</v>
       </c>
       <c r="N59" t="s">
         <v>366</v>
@@ -5567,7 +5559,7 @@
         <v>377</v>
       </c>
       <c r="C61" s="1" t="n">
-        <v>44042</v>
+        <v>44045</v>
       </c>
       <c r="D61" t="s">
         <v>378</v>
@@ -5577,25 +5569,25 @@
       </c>
       <c r="F61"/>
       <c r="G61" t="n">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="H61" t="n">
-        <v>465066</v>
+        <v>472161</v>
       </c>
       <c r="I61" t="n">
-        <v>96.442</v>
+        <v>97.913</v>
       </c>
       <c r="J61" t="n">
-        <v>2476</v>
+        <v>1692</v>
       </c>
       <c r="K61" t="n">
-        <v>0.513</v>
+        <v>0.351</v>
       </c>
       <c r="L61" t="n">
-        <v>1921</v>
+        <v>2276</v>
       </c>
       <c r="M61" t="n">
-        <v>0.398</v>
+        <v>0.472</v>
       </c>
       <c r="N61" t="s">
         <v>379</v>
@@ -5618,7 +5610,7 @@
         <v>382</v>
       </c>
       <c r="C62" s="1" t="n">
-        <v>44042</v>
+        <v>44044</v>
       </c>
       <c r="D62" t="s">
         <v>383</v>
@@ -5628,25 +5620,21 @@
       </c>
       <c r="F62"/>
       <c r="G62" t="n">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H62" t="n">
-        <v>279675</v>
+        <v>286091</v>
       </c>
       <c r="I62" t="n">
-        <v>1.357</v>
-      </c>
-      <c r="J62" t="n">
-        <v>3622</v>
-      </c>
-      <c r="K62" t="n">
+        <v>1.388</v>
+      </c>
+      <c r="J62"/>
+      <c r="K62"/>
+      <c r="L62" t="n">
+        <v>3796</v>
+      </c>
+      <c r="M62" t="n">
         <v>0.018</v>
-      </c>
-      <c r="L62" t="n">
-        <v>3969</v>
-      </c>
-      <c r="M62" t="n">
-        <v>0.019</v>
       </c>
       <c r="N62" t="s">
         <v>384</v>
@@ -5669,7 +5657,7 @@
         <v>388</v>
       </c>
       <c r="C63" s="1" t="n">
-        <v>44039</v>
+        <v>44041</v>
       </c>
       <c r="D63" t="s">
         <v>389</v>
@@ -5679,25 +5667,25 @@
       </c>
       <c r="F63"/>
       <c r="G63" t="n">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="H63" t="n">
-        <v>414789</v>
+        <v>424857</v>
       </c>
       <c r="I63" t="n">
-        <v>76.512</v>
+        <v>78.369</v>
       </c>
       <c r="J63" t="n">
-        <v>4822</v>
+        <v>4366</v>
       </c>
       <c r="K63" t="n">
-        <v>0.889</v>
+        <v>0.805</v>
       </c>
       <c r="L63" t="n">
-        <v>3273</v>
+        <v>3549</v>
       </c>
       <c r="M63" t="n">
-        <v>0.604</v>
+        <v>0.655</v>
       </c>
       <c r="N63" t="s">
         <v>390</v>
@@ -5767,7 +5755,7 @@
         <v>402</v>
       </c>
       <c r="C65" s="1" t="n">
-        <v>44042</v>
+        <v>44045</v>
       </c>
       <c r="D65" t="s">
         <v>403</v>
@@ -5777,25 +5765,25 @@
       </c>
       <c r="F65"/>
       <c r="G65" t="n">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="H65" t="n">
-        <v>1973237</v>
+        <v>2021196</v>
       </c>
       <c r="I65" t="n">
-        <v>8.933</v>
+        <v>9.15</v>
       </c>
       <c r="J65" t="n">
-        <v>20507</v>
+        <v>11026</v>
       </c>
       <c r="K65" t="n">
-        <v>0.093</v>
+        <v>0.05</v>
       </c>
       <c r="L65" t="n">
-        <v>24850</v>
+        <v>21859</v>
       </c>
       <c r="M65" t="n">
-        <v>0.112</v>
+        <v>0.099</v>
       </c>
       <c r="N65" t="s">
         <v>404</v>
@@ -5818,7 +5806,7 @@
         <v>407</v>
       </c>
       <c r="C66" s="1" t="n">
-        <v>44041</v>
+        <v>44042</v>
       </c>
       <c r="D66" t="s">
         <v>408</v>
@@ -5828,25 +5816,25 @@
       </c>
       <c r="F66"/>
       <c r="G66" t="n">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="H66" t="n">
-        <v>214105</v>
+        <v>217323</v>
       </c>
       <c r="I66" t="n">
-        <v>49.621</v>
+        <v>50.367</v>
       </c>
       <c r="J66" t="n">
-        <v>3167</v>
+        <v>3218</v>
       </c>
       <c r="K66" t="n">
-        <v>0.734</v>
+        <v>0.746</v>
       </c>
       <c r="L66" t="n">
-        <v>3193</v>
+        <v>3221</v>
       </c>
       <c r="M66" t="n">
-        <v>0.74</v>
+        <v>0.747</v>
       </c>
       <c r="N66" t="s">
         <v>409</v>
@@ -5971,7 +5959,7 @@
         <v>425</v>
       </c>
       <c r="C69" s="1" t="n">
-        <v>44042</v>
+        <v>44043</v>
       </c>
       <c r="D69" t="s">
         <v>426</v>
@@ -5981,25 +5969,25 @@
       </c>
       <c r="F69"/>
       <c r="G69" t="n">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="H69" t="n">
-        <v>1398744</v>
+        <v>1435618</v>
       </c>
       <c r="I69" t="n">
-        <v>12.764</v>
+        <v>13.101</v>
       </c>
       <c r="J69" t="n">
-        <v>32875</v>
+        <v>36874</v>
       </c>
       <c r="K69" t="n">
-        <v>0.3</v>
+        <v>0.336</v>
       </c>
       <c r="L69" t="n">
-        <v>30638</v>
+        <v>32151</v>
       </c>
       <c r="M69" t="n">
-        <v>0.28</v>
+        <v>0.293</v>
       </c>
       <c r="N69" t="s">
         <v>222</v>
@@ -6022,7 +6010,7 @@
         <v>430</v>
       </c>
       <c r="C70" s="1" t="n">
-        <v>44043</v>
+        <v>44045</v>
       </c>
       <c r="D70" t="s">
         <v>431</v>
@@ -6032,25 +6020,25 @@
       </c>
       <c r="F70"/>
       <c r="G70" t="n">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="H70" t="n">
-        <v>1931574</v>
+        <v>1969570</v>
       </c>
       <c r="I70" t="n">
-        <v>51.037</v>
+        <v>52.041</v>
       </c>
       <c r="J70" t="n">
-        <v>22394</v>
+        <v>16734</v>
       </c>
       <c r="K70" t="n">
-        <v>0.592</v>
+        <v>0.442</v>
       </c>
       <c r="L70" t="n">
-        <v>18747</v>
+        <v>19366</v>
       </c>
       <c r="M70" t="n">
-        <v>0.495</v>
+        <v>0.512</v>
       </c>
       <c r="N70" t="s">
         <v>432</v>
@@ -6073,7 +6061,7 @@
         <v>435</v>
       </c>
       <c r="C71" s="1" t="n">
-        <v>44043</v>
+        <v>44045</v>
       </c>
       <c r="D71" t="s">
         <v>431</v>
@@ -6083,25 +6071,25 @@
       </c>
       <c r="F71"/>
       <c r="G71" t="n">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="H71" t="n">
-        <v>2245168</v>
+        <v>2297427</v>
       </c>
       <c r="I71" t="n">
-        <v>59.323</v>
+        <v>60.704</v>
       </c>
       <c r="J71" t="n">
-        <v>35127</v>
+        <v>23874</v>
       </c>
       <c r="K71" t="n">
-        <v>0.928</v>
+        <v>0.631</v>
       </c>
       <c r="L71" t="n">
-        <v>25169</v>
+        <v>26093</v>
       </c>
       <c r="M71" t="n">
-        <v>0.665</v>
+        <v>0.689</v>
       </c>
       <c r="N71" t="s">
         <v>432</v>
@@ -6124,7 +6112,7 @@
         <v>438</v>
       </c>
       <c r="C72" s="1" t="n">
-        <v>44040</v>
+        <v>44042</v>
       </c>
       <c r="D72" t="s">
         <v>439</v>
@@ -6134,25 +6122,25 @@
       </c>
       <c r="F72"/>
       <c r="G72" t="n">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="H72" t="n">
-        <v>1591873</v>
+        <v>1622951</v>
       </c>
       <c r="I72" t="n">
-        <v>156.116</v>
+        <v>159.164</v>
       </c>
       <c r="J72" t="n">
-        <v>16743</v>
+        <v>14479</v>
       </c>
       <c r="K72" t="n">
-        <v>1.642</v>
+        <v>1.42</v>
       </c>
       <c r="L72" t="n">
-        <v>13469</v>
+        <v>13448</v>
       </c>
       <c r="M72" t="n">
-        <v>1.321</v>
+        <v>1.319</v>
       </c>
       <c r="N72" t="s">
         <v>440</v>
@@ -6175,7 +6163,7 @@
         <v>444</v>
       </c>
       <c r="C73" s="1" t="n">
-        <v>44043</v>
+        <v>44045</v>
       </c>
       <c r="D73" t="s">
         <v>445</v>
@@ -6185,25 +6173,25 @@
       </c>
       <c r="F73"/>
       <c r="G73" t="n">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="H73" t="n">
-        <v>495377</v>
+        <v>500536</v>
       </c>
       <c r="I73" t="n">
-        <v>171.943</v>
+        <v>173.733</v>
       </c>
       <c r="J73" t="n">
-        <v>2808</v>
+        <v>1870</v>
       </c>
       <c r="K73" t="n">
-        <v>0.975</v>
+        <v>0.649</v>
       </c>
       <c r="L73" t="n">
-        <v>4386</v>
+        <v>4013</v>
       </c>
       <c r="M73" t="n">
-        <v>1.522</v>
+        <v>1.393</v>
       </c>
       <c r="N73" t="s">
         <v>446</v>
@@ -6226,7 +6214,7 @@
         <v>450</v>
       </c>
       <c r="C74" s="1" t="n">
-        <v>44042</v>
+        <v>44045</v>
       </c>
       <c r="D74" t="s">
         <v>451</v>
@@ -6236,25 +6224,25 @@
       </c>
       <c r="F74"/>
       <c r="G74" t="n">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="H74" t="n">
-        <v>1202607</v>
+        <v>1248318</v>
       </c>
       <c r="I74" t="n">
-        <v>62.513</v>
+        <v>64.889</v>
       </c>
       <c r="J74" t="n">
-        <v>24977</v>
+        <v>8045</v>
       </c>
       <c r="K74" t="n">
-        <v>1.298</v>
+        <v>0.418</v>
       </c>
       <c r="L74" t="n">
-        <v>24559</v>
+        <v>20774</v>
       </c>
       <c r="M74" t="n">
-        <v>1.277</v>
+        <v>1.08</v>
       </c>
       <c r="N74" t="s">
         <v>453</v>
@@ -6277,7 +6265,7 @@
         <v>457</v>
       </c>
       <c r="C75" s="1" t="n">
-        <v>44042</v>
+        <v>44045</v>
       </c>
       <c r="D75" t="s">
         <v>458</v>
@@ -6287,25 +6275,25 @@
       </c>
       <c r="F75"/>
       <c r="G75" t="n">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="H75" t="n">
-        <v>28161461</v>
+        <v>29029900</v>
       </c>
       <c r="I75" t="n">
-        <v>192.973</v>
+        <v>198.924</v>
       </c>
       <c r="J75" t="n">
-        <v>303611</v>
+        <v>236640</v>
       </c>
       <c r="K75" t="n">
-        <v>2.08</v>
+        <v>1.622</v>
       </c>
       <c r="L75" t="n">
-        <v>265830</v>
+        <v>269705</v>
       </c>
       <c r="M75" t="n">
-        <v>1.822</v>
+        <v>1.848</v>
       </c>
       <c r="N75" t="s">
         <v>459</v>
@@ -6379,7 +6367,7 @@
         <v>469</v>
       </c>
       <c r="C77" s="1" t="n">
-        <v>44043</v>
+        <v>44045</v>
       </c>
       <c r="D77" t="s">
         <v>470</v>
@@ -6389,25 +6377,25 @@
       </c>
       <c r="F77"/>
       <c r="G77" t="n">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="H77" t="n">
-        <v>3341253</v>
+        <v>3423066</v>
       </c>
       <c r="I77" t="n">
-        <v>95.975</v>
+        <v>98.325</v>
       </c>
       <c r="J77" t="n">
-        <v>60849</v>
+        <v>36666</v>
       </c>
       <c r="K77" t="n">
-        <v>1.748</v>
+        <v>1.053</v>
       </c>
       <c r="L77" t="n">
-        <v>57659</v>
+        <v>53628</v>
       </c>
       <c r="M77" t="n">
-        <v>1.656</v>
+        <v>1.54</v>
       </c>
       <c r="N77" t="s">
         <v>43</v>
@@ -6430,7 +6418,7 @@
         <v>474</v>
       </c>
       <c r="C78" s="1" t="n">
-        <v>44042</v>
+        <v>44046</v>
       </c>
       <c r="D78" t="s">
         <v>475</v>
@@ -6442,25 +6430,25 @@
         <v>477</v>
       </c>
       <c r="G78" t="n">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="H78" t="n">
-        <v>109487</v>
+        <v>113572</v>
       </c>
       <c r="I78" t="n">
-        <v>6.539</v>
+        <v>6.783</v>
       </c>
       <c r="J78" t="n">
-        <v>1547</v>
+        <v>946</v>
       </c>
       <c r="K78" t="n">
-        <v>0.092</v>
+        <v>0.056</v>
       </c>
       <c r="L78" t="n">
-        <v>1386</v>
+        <v>1203</v>
       </c>
       <c r="M78" t="n">
-        <v>0.083</v>
+        <v>0.072</v>
       </c>
       <c r="N78" t="s">
         <v>478</v>
@@ -6483,7 +6471,7 @@
         <v>483</v>
       </c>
       <c r="C79" s="1" t="n">
-        <v>44043</v>
+        <v>44046</v>
       </c>
       <c r="D79" t="s">
         <v>484</v>
@@ -6495,25 +6483,25 @@
         <v>485</v>
       </c>
       <c r="G79" t="n">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="H79" t="n">
-        <v>668984</v>
+        <v>693656</v>
       </c>
       <c r="I79" t="n">
-        <v>98.314</v>
+        <v>101.939</v>
       </c>
       <c r="J79" t="n">
-        <v>9436</v>
+        <v>7168</v>
       </c>
       <c r="K79" t="n">
-        <v>1.387</v>
+        <v>1.053</v>
       </c>
       <c r="L79" t="n">
-        <v>9571</v>
+        <v>8912</v>
       </c>
       <c r="M79" t="n">
-        <v>1.407</v>
+        <v>1.31</v>
       </c>
       <c r="N79" t="s">
         <v>43</v>
@@ -6630,7 +6618,7 @@
         <v>495</v>
       </c>
       <c r="C82" s="1" t="n">
-        <v>44043</v>
+        <v>44046</v>
       </c>
       <c r="D82" t="s">
         <v>496</v>
@@ -6640,25 +6628,25 @@
       </c>
       <c r="F82"/>
       <c r="G82" t="n">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="H82" t="n">
-        <v>261562</v>
+        <v>265797</v>
       </c>
       <c r="I82" t="n">
-        <v>47.908</v>
+        <v>48.684</v>
       </c>
       <c r="J82" t="n">
-        <v>2176</v>
+        <v>766</v>
       </c>
       <c r="K82" t="n">
-        <v>0.399</v>
+        <v>0.14</v>
       </c>
       <c r="L82" t="n">
-        <v>1590</v>
+        <v>1729</v>
       </c>
       <c r="M82" t="n">
-        <v>0.291</v>
+        <v>0.317</v>
       </c>
       <c r="N82" t="s">
         <v>498</v>
@@ -6681,7 +6669,7 @@
         <v>502</v>
       </c>
       <c r="C83" s="1" t="n">
-        <v>44042</v>
+        <v>44045</v>
       </c>
       <c r="D83" t="s">
         <v>503</v>
@@ -6691,25 +6679,25 @@
       </c>
       <c r="F83"/>
       <c r="G83" t="n">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="H83" t="n">
-        <v>130161</v>
+        <v>131699</v>
       </c>
       <c r="I83" t="n">
-        <v>62.61</v>
+        <v>63.349</v>
       </c>
       <c r="J83" t="n">
-        <v>917</v>
+        <v>272</v>
       </c>
       <c r="K83" t="n">
-        <v>0.441</v>
+        <v>0.131</v>
       </c>
       <c r="L83" t="n">
-        <v>772</v>
+        <v>732</v>
       </c>
       <c r="M83" t="n">
-        <v>0.371</v>
+        <v>0.352</v>
       </c>
       <c r="N83" t="s">
         <v>505</v>
@@ -6732,7 +6720,7 @@
         <v>509</v>
       </c>
       <c r="C84" s="1" t="n">
-        <v>44042</v>
+        <v>44045</v>
       </c>
       <c r="D84" t="s">
         <v>510</v>
@@ -6744,25 +6732,25 @@
         <v>512</v>
       </c>
       <c r="G84" t="n">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="H84" t="n">
-        <v>2918049</v>
+        <v>3036779</v>
       </c>
       <c r="I84" t="n">
-        <v>49.201</v>
+        <v>51.203</v>
       </c>
       <c r="J84" t="n">
-        <v>44886</v>
+        <v>34794</v>
       </c>
       <c r="K84" t="n">
-        <v>0.757</v>
+        <v>0.587</v>
       </c>
       <c r="L84" t="n">
-        <v>40849</v>
+        <v>37572</v>
       </c>
       <c r="M84" t="n">
-        <v>0.689</v>
+        <v>0.633</v>
       </c>
       <c r="N84" t="s">
         <v>511</v>
@@ -6785,7 +6773,7 @@
         <v>516</v>
       </c>
       <c r="C85" s="1" t="n">
-        <v>44042</v>
+        <v>44046</v>
       </c>
       <c r="D85" t="s">
         <v>517</v>
@@ -6795,25 +6783,25 @@
       </c>
       <c r="F85"/>
       <c r="G85" t="n">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="H85" t="n">
-        <v>1537197</v>
+        <v>1562356</v>
       </c>
       <c r="I85" t="n">
-        <v>29.983</v>
+        <v>30.474</v>
       </c>
       <c r="J85" t="n">
-        <v>9216</v>
+        <v>3878</v>
       </c>
       <c r="K85" t="n">
-        <v>0.18</v>
+        <v>0.076</v>
       </c>
       <c r="L85" t="n">
-        <v>8252</v>
+        <v>7736</v>
       </c>
       <c r="M85" t="n">
-        <v>0.161</v>
+        <v>0.151</v>
       </c>
       <c r="N85" t="s">
         <v>518</v>
@@ -6977,7 +6965,7 @@
         <v>539</v>
       </c>
       <c r="C89" s="1" t="n">
-        <v>44042</v>
+        <v>44045</v>
       </c>
       <c r="D89" t="s">
         <v>540</v>
@@ -6987,25 +6975,25 @@
       </c>
       <c r="F89"/>
       <c r="G89" t="n">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="H89" t="n">
-        <v>791725</v>
+        <v>803725</v>
       </c>
       <c r="I89" t="n">
-        <v>91.48</v>
+        <v>92.867</v>
       </c>
       <c r="J89" t="n">
-        <v>5239</v>
+        <v>1596</v>
       </c>
       <c r="K89" t="n">
-        <v>0.605</v>
+        <v>0.184</v>
       </c>
       <c r="L89" t="n">
-        <v>5107</v>
+        <v>5256</v>
       </c>
       <c r="M89" t="n">
-        <v>0.59</v>
+        <v>0.607</v>
       </c>
       <c r="N89" t="s">
         <v>541</v>
@@ -7028,7 +7016,7 @@
         <v>545</v>
       </c>
       <c r="C90" s="1" t="n">
-        <v>44043</v>
+        <v>44045</v>
       </c>
       <c r="D90" t="s">
         <v>546</v>
@@ -7038,22 +7026,22 @@
       </c>
       <c r="F90"/>
       <c r="G90" t="n">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="H90" t="n">
-        <v>81826</v>
+        <v>82062</v>
       </c>
       <c r="I90" t="n">
-        <v>3.436</v>
+        <v>3.446</v>
       </c>
       <c r="J90" t="n">
-        <v>238</v>
+        <v>130</v>
       </c>
       <c r="K90" t="n">
-        <v>0.01</v>
+        <v>0.005</v>
       </c>
       <c r="L90" t="n">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="M90" t="n">
         <v>0.009</v>
@@ -7079,7 +7067,7 @@
         <v>550</v>
       </c>
       <c r="C91" s="1" t="n">
-        <v>44043</v>
+        <v>44045</v>
       </c>
       <c r="D91" t="s">
         <v>551</v>
@@ -7089,25 +7077,25 @@
       </c>
       <c r="F91"/>
       <c r="G91" t="n">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="H91" t="n">
-        <v>375346</v>
+        <v>377680</v>
       </c>
       <c r="I91" t="n">
-        <v>5.377</v>
+        <v>5.411</v>
       </c>
       <c r="J91" t="n">
-        <v>2682</v>
+        <v>1040</v>
       </c>
       <c r="K91" t="n">
-        <v>0.038</v>
+        <v>0.015</v>
       </c>
       <c r="L91" t="n">
-        <v>1926</v>
+        <v>1744</v>
       </c>
       <c r="M91" t="n">
-        <v>0.028</v>
+        <v>0.025</v>
       </c>
       <c r="N91" t="s">
         <v>552</v>
@@ -7130,7 +7118,7 @@
         <v>555</v>
       </c>
       <c r="C92" s="1" t="n">
-        <v>44043</v>
+        <v>44045</v>
       </c>
       <c r="D92" t="s">
         <v>551</v>
@@ -7140,25 +7128,25 @@
       </c>
       <c r="F92"/>
       <c r="G92" t="n">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="H92" t="n">
-        <v>727691</v>
+        <v>730025</v>
       </c>
       <c r="I92" t="n">
-        <v>10.425</v>
+        <v>10.459</v>
       </c>
       <c r="J92" t="n">
-        <v>20233</v>
+        <v>1040</v>
       </c>
       <c r="K92" t="n">
-        <v>0.29</v>
+        <v>0.015</v>
       </c>
       <c r="L92" t="n">
-        <v>4434</v>
+        <v>4252</v>
       </c>
       <c r="M92" t="n">
-        <v>0.064</v>
+        <v>0.061</v>
       </c>
       <c r="N92" t="s">
         <v>552</v>
@@ -7181,7 +7169,7 @@
         <v>558</v>
       </c>
       <c r="C93" s="1" t="n">
-        <v>44031</v>
+        <v>44044</v>
       </c>
       <c r="D93"/>
       <c r="E93" t="s">
@@ -7191,25 +7179,25 @@
         <v>560</v>
       </c>
       <c r="G93" t="n">
-        <v>132</v>
+        <v>145</v>
       </c>
       <c r="H93" t="n">
-        <v>38063</v>
+        <v>42943</v>
       </c>
       <c r="I93" t="n">
-        <v>4.598</v>
+        <v>5.187</v>
       </c>
       <c r="J93" t="n">
-        <v>319</v>
+        <v>410</v>
       </c>
       <c r="K93" t="n">
-        <v>0.039</v>
+        <v>0.05</v>
       </c>
       <c r="L93" t="n">
-        <v>370</v>
+        <v>362</v>
       </c>
       <c r="M93" t="n">
-        <v>0.045</v>
+        <v>0.044</v>
       </c>
       <c r="N93" t="s">
         <v>559</v>
@@ -7232,7 +7220,7 @@
         <v>564</v>
       </c>
       <c r="C94" s="1" t="n">
-        <v>44040</v>
+        <v>44041</v>
       </c>
       <c r="D94" t="s">
         <v>565</v>
@@ -7242,25 +7230,25 @@
       </c>
       <c r="F94"/>
       <c r="G94" t="n">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="H94" t="n">
-        <v>90943</v>
+        <v>92530</v>
       </c>
       <c r="I94" t="n">
-        <v>7.695</v>
+        <v>7.829</v>
       </c>
       <c r="J94" t="n">
-        <v>1561</v>
+        <v>1587</v>
       </c>
       <c r="K94" t="n">
-        <v>0.132</v>
+        <v>0.134</v>
       </c>
       <c r="L94" t="n">
-        <v>1058</v>
+        <v>1142</v>
       </c>
       <c r="M94" t="n">
-        <v>0.09</v>
+        <v>0.097</v>
       </c>
       <c r="N94" t="s">
         <v>566</v>
@@ -7283,7 +7271,7 @@
         <v>569</v>
       </c>
       <c r="C95" s="1" t="n">
-        <v>44042</v>
+        <v>44044</v>
       </c>
       <c r="D95" t="s">
         <v>570</v>
@@ -7293,25 +7281,25 @@
       </c>
       <c r="F95"/>
       <c r="G95" t="n">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="H95" t="n">
-        <v>4800823</v>
+        <v>4885916</v>
       </c>
       <c r="I95" t="n">
-        <v>56.923</v>
+        <v>57.932</v>
       </c>
       <c r="J95" t="n">
-        <v>46492</v>
+        <v>40247</v>
       </c>
       <c r="K95" t="n">
-        <v>0.551</v>
+        <v>0.477</v>
       </c>
       <c r="L95" t="n">
-        <v>50636</v>
+        <v>50699</v>
       </c>
       <c r="M95" t="n">
-        <v>0.6</v>
+        <v>0.601</v>
       </c>
       <c r="N95" t="s">
         <v>571</v>
@@ -7334,7 +7322,7 @@
         <v>574</v>
       </c>
       <c r="C96" s="1" t="n">
-        <v>44042</v>
+        <v>44043</v>
       </c>
       <c r="D96" t="s">
         <v>575</v>
@@ -7344,21 +7332,25 @@
       </c>
       <c r="F96"/>
       <c r="G96" t="n">
-        <v>113</v>
-      </c>
-      <c r="H96"/>
-      <c r="I96"/>
+        <v>31</v>
+      </c>
+      <c r="H96" t="n">
+        <v>275355</v>
+      </c>
+      <c r="I96" t="n">
+        <v>6.02</v>
+      </c>
       <c r="J96" t="n">
-        <v>3229</v>
+        <v>2550</v>
       </c>
       <c r="K96" t="n">
-        <v>0.071</v>
+        <v>0.056</v>
       </c>
       <c r="L96" t="n">
-        <v>2395</v>
+        <v>2443</v>
       </c>
       <c r="M96" t="n">
-        <v>0.052</v>
+        <v>0.053</v>
       </c>
       <c r="N96" t="s">
         <v>576</v>
@@ -7381,7 +7373,7 @@
         <v>580</v>
       </c>
       <c r="C97" s="1" t="n">
-        <v>44043</v>
+        <v>44046</v>
       </c>
       <c r="D97" t="s">
         <v>581</v>
@@ -7391,25 +7383,25 @@
       </c>
       <c r="F97"/>
       <c r="G97" t="n">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="H97" t="n">
-        <v>1029220</v>
+        <v>1067006</v>
       </c>
       <c r="I97" t="n">
-        <v>23.534</v>
+        <v>24.398</v>
       </c>
       <c r="J97" t="n">
-        <v>15427</v>
+        <v>8623</v>
       </c>
       <c r="K97" t="n">
-        <v>0.353</v>
+        <v>0.197</v>
       </c>
       <c r="L97" t="n">
-        <v>13173</v>
+        <v>13757</v>
       </c>
       <c r="M97" t="n">
-        <v>0.301</v>
+        <v>0.315</v>
       </c>
       <c r="N97" t="s">
         <v>582</v>
@@ -7432,7 +7424,7 @@
         <v>587</v>
       </c>
       <c r="C98" s="1" t="n">
-        <v>44043</v>
+        <v>44045</v>
       </c>
       <c r="D98" t="s">
         <v>588</v>
@@ -7442,25 +7434,25 @@
       </c>
       <c r="F98"/>
       <c r="G98" t="n">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="H98" t="n">
-        <v>5076384</v>
+        <v>5162080</v>
       </c>
       <c r="I98" t="n">
-        <v>513.264</v>
+        <v>521.928</v>
       </c>
       <c r="J98" t="n">
-        <v>54727</v>
+        <v>42428</v>
       </c>
       <c r="K98" t="n">
-        <v>5.533</v>
+        <v>4.29</v>
       </c>
       <c r="L98" t="n">
-        <v>50301</v>
+        <v>47716</v>
       </c>
       <c r="M98" t="n">
-        <v>5.086</v>
+        <v>4.824</v>
       </c>
       <c r="N98" t="s">
         <v>589</v>
@@ -7483,7 +7475,7 @@
         <v>592</v>
       </c>
       <c r="C99" s="1" t="n">
-        <v>44042</v>
+        <v>44044</v>
       </c>
       <c r="D99" t="s">
         <v>593</v>
@@ -7495,25 +7487,25 @@
         <v>595</v>
       </c>
       <c r="G99" t="n">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="H99" t="n">
-        <v>9415384</v>
+        <v>9693382</v>
       </c>
       <c r="I99" t="n">
-        <v>138.694</v>
+        <v>142.789</v>
       </c>
       <c r="J99" t="n">
-        <v>154034</v>
+        <v>130999</v>
       </c>
       <c r="K99" t="n">
-        <v>2.269</v>
+        <v>1.93</v>
       </c>
       <c r="L99" t="n">
-        <v>127529</v>
+        <v>127907</v>
       </c>
       <c r="M99" t="n">
-        <v>1.879</v>
+        <v>1.884</v>
       </c>
       <c r="N99" t="s">
         <v>594</v>
@@ -7587,7 +7579,7 @@
         <v>604</v>
       </c>
       <c r="C101" s="1" t="n">
-        <v>44042</v>
+        <v>44045</v>
       </c>
       <c r="D101" t="s">
         <v>605</v>
@@ -7597,25 +7589,25 @@
       </c>
       <c r="F101"/>
       <c r="G101" t="n">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="H101" t="n">
-        <v>54466962</v>
+        <v>56812162</v>
       </c>
       <c r="I101" t="n">
-        <v>164.551</v>
+        <v>171.637</v>
       </c>
       <c r="J101" t="n">
-        <v>625815</v>
+        <v>725902</v>
       </c>
       <c r="K101" t="n">
-        <v>1.891</v>
+        <v>2.193</v>
       </c>
       <c r="L101" t="n">
-        <v>794101</v>
+        <v>760095</v>
       </c>
       <c r="M101" t="n">
-        <v>2.399</v>
+        <v>2.296</v>
       </c>
       <c r="N101" t="s">
         <v>606</v>
@@ -7638,7 +7630,7 @@
         <v>611</v>
       </c>
       <c r="C102" s="1" t="n">
-        <v>44042</v>
+        <v>44045</v>
       </c>
       <c r="D102" t="s">
         <v>612</v>
@@ -7648,25 +7640,25 @@
       </c>
       <c r="F102"/>
       <c r="G102" t="n">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="H102" t="n">
-        <v>110951</v>
+        <v>117053</v>
       </c>
       <c r="I102" t="n">
-        <v>31.94</v>
+        <v>33.697</v>
       </c>
       <c r="J102" t="n">
-        <v>1640</v>
+        <v>1853</v>
       </c>
       <c r="K102" t="n">
-        <v>0.472</v>
+        <v>0.533</v>
       </c>
       <c r="L102" t="n">
-        <v>1926</v>
+        <v>2007</v>
       </c>
       <c r="M102" t="n">
-        <v>0.554</v>
+        <v>0.578</v>
       </c>
       <c r="N102" t="s">
         <v>127</v>

</xml_diff>

<commit_message>
Updated testing data for 2020-08-04
</commit_message>
<xml_diff>
--- a/public/data/testing/covid-testing-latest-data-source-details.xlsx
+++ b/public/data/testing/covid-testing-latest-data-source-details.xlsx
@@ -104,7 +104,7 @@
     <t xml:space="preserve">Australia - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.health.gov.au/sites/default/files/documents/2020/08/coronavirus-covid-19-at-a-glance-2-august-2020.pdf</t>
+    <t xml:space="preserve">https://www.health.gov.au/sites/default/files/documents/2020/08/coronavirus-covid-19-at-a-glance-3-august-2020.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">Australian Government Department of Health</t>
@@ -243,7 +243,7 @@
     <t xml:space="preserve">Bolivia - units unclear</t>
   </si>
   <si>
-    <t xml:space="preserve">https://minsalud.gob.bo/4457-ministerio-de-salud-reporta-1-700-contagios-nuevos-de-coronavirus-y-86-fallecidos</t>
+    <t xml:space="preserve">https://minsalud.gob.bo/4471-reporte-covid-140</t>
   </si>
   <si>
     <t xml:space="preserve">https://www.minsalud.gob.bo/</t>
@@ -475,7 +475,7 @@
     <t xml:space="preserve">Democratic Republic of Congo - samples tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/CMR_Covid19_RDC/status/1289257564119511043/photo/1</t>
+    <t xml:space="preserve">https://twitter.com/CMR_Covid19_RDC/status/1290204955307999232/photo/1</t>
   </si>
   <si>
     <t xml:space="preserve">DRC COVID-19 Pandemic Response Multisectoral Committee</t>
@@ -511,7 +511,7 @@
     <t xml:space="preserve">Ecuador - units unclear</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.gestionderiesgos.gob.ec/wp-content/uploads/2020/08/INFOGRAFIA-NACIONALCOVI-19-COE-NACIONAL-08h00-01082020.pdf</t>
+    <t xml:space="preserve">https://www.gestionderiesgos.gob.ec/wp-content/uploads/2020/08/INFOGRAFIA-NACIONALCOVI-19-COE-NACIONAL-08h00-03082020-v2.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">Government of Ecuador</t>
@@ -889,7 +889,7 @@
     <t xml:space="preserve">Iran - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">http://irangov.ir/detail/344480</t>
+    <t xml:space="preserve">http://irangov.ir/detail/344549</t>
   </si>
   <si>
     <t xml:space="preserve">Government of Iran</t>
@@ -926,7 +926,7 @@
     <t xml:space="preserve">Israel - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://govextra.gov.il/media/23626/covid19-data-israel-27072020.csv</t>
+    <t xml:space="preserve">https://govextra.gov.il/media/23824/covid19-data-israel-28072020.csv</t>
   </si>
   <si>
     <t xml:space="preserve">Israel Ministry of Health</t>
@@ -985,13 +985,13 @@
     <t xml:space="preserve">Japan - people tested (incl. non-PCR)</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.mhlw.go.jp/stf/newpage_12781.html</t>
+    <t xml:space="preserve">https://www.mhlw.go.jp/stf/newpage_12800.html</t>
   </si>
   <si>
     <t xml:space="preserve">Ministry of Health, Labor and Welfare Press Release</t>
   </si>
   <si>
-    <t xml:space="preserve">See Table: 国内の発生状況, column 1 '検査実施人数'. Daily change figure provided for this date is not consistent with the cumulative totals for today and the previous day.</t>
+    <t xml:space="preserve">See Table: 国内の発生状況, column 1 '検査実施人数'.</t>
   </si>
   <si>
     <t xml:space="preserve">Ministry of Health, Labor and Welfare</t>
@@ -1010,10 +1010,10 @@
     <t xml:space="preserve">Japan - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.mhlw.go.jp/content/10906000/000655354.pdf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The cumulative total reported in the press release (1,101,541) does not sum to the cumulative total calculated from the weekly and daily figures reported by the MOH. See: https://www.mhlw.go.jp/content/10906000/000655354.pdf</t>
+    <t xml:space="preserve">https://www.mhlw.go.jp/content/10906000/000655738.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The cumulative total reported in the press release (1,110,207) does not sum to the cumulative total calculated from the weekly and daily figures reported by the MOH. See: https://www.mhlw.go.jp/content/10906000/000655738.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">On 11th April 2020, the MOH started providing a daily time series on the "Implementation status of PCR tests for new coronavirus in Japan (based on the date on which results were determined" (via Google translate). 
@@ -1068,7 +1068,7 @@
     <t xml:space="preserve">Kuwait - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/KUWAIT_MOH/status/1289161413970112513/photo/1</t>
+    <t xml:space="preserve">https://twitter.com/KUWAIT_MOH/status/1290225953763811330/photo/1</t>
   </si>
   <si>
     <t xml:space="preserve">Kuwait Ministry of Health</t>
@@ -1077,7 +1077,7 @@
     <t xml:space="preserve">https://twitter.com/KUWAIT_MOH</t>
   </si>
   <si>
-    <t xml:space="preserve">The Kuwait Ministry of Health provides daily reports of the daily ("NEW TESTS") and cumulative ("Total") number of tests performed on [their official Twitter account](https://twitter.com/KUWAIT_MOH). COVID-19 reports date back to early March 2020 but did not begin including testing numbers until 13 May; the cumulative total then was already 227,000. From 13 to 29 May, the daily number was termed "NP swab last 24 h" and the cumulative number "Total Investigations."
+    <t xml:space="preserve">The Kuwait Ministry of Health provides daily reports of the daily ("NEW TESTS") and cumulative ("Total") number of tests performed on [their official Twitter account](https://twitter.com/KUWAIT_MOH). COVID-19 reports date back to early March 2020 but did not begin including testing numbers until 13 May; the cumulative total then was already 227,000. From 13–29 May 2020, the daily number was termed "NP swab last 24 h" and the cumulative number "Total Investigations."
 Note that, due to the way the data is presented by the official source, the time series may be impacted by retrospective revisions made by the source – see our [FAQ here](https://ourworldindata.org/coronavirus-testing#does-your-data-reflect-retrospective-updates-made-by-the-source).</t>
   </si>
   <si>
@@ -1134,7 +1134,7 @@
     <t xml:space="preserve">Malaysia - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">http://covid-19.moh.gov.my/terkini/082020/situasi-terkini-02-ogos-2020</t>
+    <t xml:space="preserve">http://covid-19.moh.gov.my/terkini/082020/situasi-terkini-03-ogos-2020</t>
   </si>
   <si>
     <t xml:space="preserve">Ministry of Health Malaysia</t>
@@ -1160,7 +1160,7 @@
     <t xml:space="preserve">Maldives - samples tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/HPA_MV/status/1289244995736580096/photo/1</t>
+    <t xml:space="preserve">https://twitter.com/HPA_MV/status/1290345598428647425/photo/1</t>
   </si>
   <si>
     <t xml:space="preserve">Maldives Health Protection Agency</t>
@@ -1173,8 +1173,8 @@
   </si>
   <si>
     <t xml:space="preserve">The Maldives Health Protection Agency, part of the Ministry of Health, provides daily updates on their official Twitter page ([@HPA_MV](https://twitter.com/HPA_MV)) with the cumulative total of samples tested. They note that the total includes “repeated samples,” and likely also includes pending tests. This is our source starting 26 June 2020.
-Before the 26th, our source was daily update videos posted to the Maldives Ministry of Health [official Facebook page](https://www.facebook.com/MinistryOfHealthMV). Toward the end of these videos they report the number of positive, pending, and total “Laboratory Sample[s]” tested; before 16 June the number of negative samples was also reported. The positive, negative, and total numbers are cumulative, while the pending numbers are current as of that day.
-From 16-25 June, we used the reported total, which likely includes pending tests. Before the 16th when negative numbers were reported, we used the total of positive and negative numbers rather than the reported total, since the latter generally included pending values and occasionally contained discrepant numbers that did not match any combination of the positive, negative, or pending numbers. It is not clear when testing first began; data is only available from 16 March where it was reported that 221 tests had been conducted.
+Before the 26th, our source was daily update videos posted to the Maldives Ministry of Health [official Facebook page](https://www.facebook.com/MinistryOfHealthMV). Toward the end of these videos they report the number of positive, pending, and total “Laboratory Sample[s]” tested; before 16 June 2020 the number of negative samples was also reported. The positive, negative, and total numbers are cumulative, while the pending numbers are current as of that day.
+From 16–25 June 2020, we used the reported total, which likely includes pending tests. Before the 16th when negative numbers were reported, we used the total of positive and negative numbers rather than the reported total, since the latter generally included pending values and occasionally contained discrepant numbers that did not match any combination of the positive, negative, or pending numbers. It is not clear when testing first began; data is only available from 16 March 2020 where it was reported that 221 tests had been conducted.
 Note that, due to the way the data is presented by the official source, the time series may be impacted by retrospective revisions made by the source – see our [FAQ here](https://ourworldindata.org/coronavirus-testing#does-your-data-reflect-retrospective-updates-made-by-the-source).</t>
   </si>
   <si>
@@ -1227,7 +1227,7 @@
     <t xml:space="preserve">Morocco - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/Ministere_Sante/status/1288885676889591816/photo/1</t>
+    <t xml:space="preserve">https://twitter.com/Ministere_Sante/status/1290335589095661568/photo/1</t>
   </si>
   <si>
     <t xml:space="preserve">Morocco Ministry of Health</t>
@@ -1237,7 +1237,7 @@
   </si>
   <si>
     <t xml:space="preserve">The Morocco Ministry of Health [provides daily updates](http://www.covidmaroc.ma/pages/Accueil.aspx) of the cumulative number of both confirmed cases (“Cas confirmés”) and cases excluded following a negative laboratory result (“Cas exclus suite à un résultat négatif du laboratoire”); we add these two numbers together to derive a cumulative total. We construct a time series of the cumulative total number of cases tested to date using updates from the Ministry of Health's official Twitter page, ([@Ministere_Sante](https://twitter.com/Ministere_Sante)). There are usually two updates per day, and we use the later one. The earliest reported numbers are from 7 February 2020, at which point 9 cases had been tested.
-From 2 March to 18 May we used data stored in [this unofficial GitHub repository](https://github.com/RedaElmar/COVID-19_Morocco) instead of the official source to automate data collection. We have cross-checked a sample of the figures reported in the unofficial source against official data reported by the Ministry of Health to ensure accuracy.
+From 2 March to 18 May 2020 we used data stored in [this unofficial GitHub repository](https://github.com/RedaElmar/COVID-19_Morocco) instead of the official source to automate data collection. We have cross-checked a sample of the figures reported in the unofficial source against official data reported by the Ministry of Health to ensure accuracy.
 Our data for this series is sourced from a non-official repository of official data. As explained in our [FAQ here](https://ourworldindata.org/coronavirus-testing#do-you-rely-on-any-non-official-sources) we regularly audit the accuracy of this repository against direct official channels. Note that, due to the way the data is presented by the official source, the time series may be impacted by retrospective revisions made by the source – see our [FAQ here](https://ourworldindata.org/coronavirus-testing#does-your-data-reflect-retrospective-updates-made-by-the-source).</t>
   </si>
   <si>
@@ -1267,7 +1267,7 @@
     <t xml:space="preserve">Nepal - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://drive.google.com/drive/folders/1mgqdZykT84Gd8Xl2ozjs93bjIJ-UqW_k</t>
+    <t xml:space="preserve">https://drive.google.com/drive/folders/1vzjKFByfG1hg1XPooiWaWjkwT1hhd-wi</t>
   </si>
   <si>
     <t xml:space="preserve">Ministry of Health and Population</t>
@@ -1556,7 +1556,7 @@
     <t xml:space="preserve">Romania - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://gov.ro/ro/media/comunicate/buletin-de-presa-3-august-2020-ora-13-00&amp;page=1</t>
+    <t xml:space="preserve">https://gov.ro/ro/media/comunicate/buletin-de-presa-4-august-2020-ora-13-00&amp;page=1</t>
   </si>
   <si>
     <t xml:space="preserve">Ministry of Internal Affairs</t>
@@ -1579,7 +1579,7 @@
     <t xml:space="preserve">Russia - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://rospotrebnadzor.ru/about/info/news/news_details.php?ELEMENT_ID=15070</t>
+    <t xml:space="preserve">https://rospotrebnadzor.ru/about/info/news/news_details.php?ELEMENT_ID=15082</t>
   </si>
   <si>
     <t xml:space="preserve">Government of the Russian Federation</t>
@@ -1781,7 +1781,7 @@
     <t xml:space="preserve">South Korea - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.cdc.go.kr/board/board.es?mid=&amp;bid=0030&amp;act=view&amp;list_no=367974&amp;tag=&amp;nPage=1</t>
+    <t xml:space="preserve">https://www.cdc.go.kr/board/board.es?mid=&amp;bid=0030&amp;act=view&amp;list_no=367981&amp;tag=&amp;nPage=1</t>
   </si>
   <si>
     <t xml:space="preserve">South Korea CDC</t>
@@ -2124,7 +2124,7 @@
     <t xml:space="preserve">Uruguay - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.gub.uy/ministerio-salud-publica/comunicacion/noticias/informe-situacion-sobre-coronavirus-covid-19-uruguay-11</t>
+    <t xml:space="preserve">https://www.gub.uy/ministerio-salud-publica/comunicacion/noticias/informe-situacion-sobre-coronavirus-covid-19-uruguay-12</t>
   </si>
   <si>
     <t xml:space="preserve">https://www.gub.uy/ministerio-salud-publica/comunicacion/noticias</t>
@@ -2576,7 +2576,7 @@
         <v>18</v>
       </c>
       <c r="C2" s="1" t="n">
-        <v>44044</v>
+        <v>44045</v>
       </c>
       <c r="D2" t="s">
         <v>19</v>
@@ -2586,25 +2586,25 @@
       </c>
       <c r="F2"/>
       <c r="G2" t="n">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="H2" t="n">
-        <v>626413</v>
+        <v>637893</v>
       </c>
       <c r="I2" t="n">
-        <v>13.86</v>
+        <v>14.114</v>
       </c>
       <c r="J2" t="n">
-        <v>7298</v>
+        <v>6799</v>
       </c>
       <c r="K2" t="n">
-        <v>0.161</v>
+        <v>0.15</v>
       </c>
       <c r="L2" t="n">
-        <v>10921</v>
+        <v>11478</v>
       </c>
       <c r="M2" t="n">
-        <v>0.242</v>
+        <v>0.254</v>
       </c>
       <c r="N2" t="s">
         <v>20</v>
@@ -2627,7 +2627,7 @@
         <v>23</v>
       </c>
       <c r="C3" s="1" t="n">
-        <v>44044</v>
+        <v>44045</v>
       </c>
       <c r="D3" t="s">
         <v>24</v>
@@ -2637,25 +2637,25 @@
       </c>
       <c r="F3"/>
       <c r="G3" t="n">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="H3" t="n">
-        <v>767023</v>
+        <v>781133</v>
       </c>
       <c r="I3" t="n">
-        <v>16.971</v>
+        <v>17.283</v>
       </c>
       <c r="J3" t="n">
-        <v>8495</v>
+        <v>8177</v>
       </c>
       <c r="K3" t="n">
-        <v>0.188</v>
+        <v>0.181</v>
       </c>
       <c r="L3" t="n">
-        <v>12936</v>
+        <v>13657</v>
       </c>
       <c r="M3" t="n">
-        <v>0.286</v>
+        <v>0.302</v>
       </c>
       <c r="N3" t="s">
         <v>20</v>
@@ -2678,7 +2678,7 @@
         <v>28</v>
       </c>
       <c r="C4" s="1" t="n">
-        <v>44044</v>
+        <v>44046</v>
       </c>
       <c r="D4" t="s">
         <v>29</v>
@@ -2688,21 +2688,21 @@
       </c>
       <c r="F4"/>
       <c r="G4" t="n">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="H4" t="n">
-        <v>4346382</v>
+        <v>4386911</v>
       </c>
       <c r="I4" t="n">
-        <v>170.447</v>
+        <v>172.037</v>
       </c>
       <c r="J4"/>
       <c r="K4"/>
       <c r="L4" t="n">
-        <v>69554</v>
+        <v>57117</v>
       </c>
       <c r="M4" t="n">
-        <v>2.728</v>
+        <v>2.24</v>
       </c>
       <c r="N4" t="s">
         <v>30</v>
@@ -2725,7 +2725,7 @@
         <v>34</v>
       </c>
       <c r="C5" s="1" t="n">
-        <v>44045</v>
+        <v>44046</v>
       </c>
       <c r="D5" t="s">
         <v>35</v>
@@ -2735,25 +2735,25 @@
       </c>
       <c r="F5"/>
       <c r="G5" t="n">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="H5" t="n">
-        <v>910437</v>
+        <v>916778</v>
       </c>
       <c r="I5" t="n">
-        <v>101.088</v>
+        <v>101.792</v>
       </c>
       <c r="J5" t="n">
-        <v>5123</v>
+        <v>6341</v>
       </c>
       <c r="K5" t="n">
-        <v>0.569</v>
+        <v>0.704</v>
       </c>
       <c r="L5" t="n">
-        <v>8934</v>
+        <v>7939</v>
       </c>
       <c r="M5" t="n">
-        <v>0.992</v>
+        <v>0.881</v>
       </c>
       <c r="N5" t="s">
         <v>37</v>
@@ -2776,7 +2776,7 @@
         <v>41</v>
       </c>
       <c r="C6" s="1" t="n">
-        <v>44045</v>
+        <v>44046</v>
       </c>
       <c r="D6" t="s">
         <v>42</v>
@@ -2786,25 +2786,25 @@
       </c>
       <c r="F6"/>
       <c r="G6" t="n">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="H6" t="n">
-        <v>842992</v>
+        <v>850648</v>
       </c>
       <c r="I6" t="n">
-        <v>495.416</v>
+        <v>499.916</v>
       </c>
       <c r="J6" t="n">
-        <v>7425</v>
+        <v>7656</v>
       </c>
       <c r="K6" t="n">
-        <v>4.364</v>
+        <v>4.499</v>
       </c>
       <c r="L6" t="n">
-        <v>7650</v>
+        <v>7407</v>
       </c>
       <c r="M6" t="n">
-        <v>4.496</v>
+        <v>4.353</v>
       </c>
       <c r="N6" t="s">
         <v>44</v>
@@ -2925,7 +2925,7 @@
         <v>61</v>
       </c>
       <c r="C9" s="1" t="n">
-        <v>44044</v>
+        <v>44045</v>
       </c>
       <c r="D9" t="s">
         <v>62</v>
@@ -2935,25 +2935,25 @@
       </c>
       <c r="F9"/>
       <c r="G9" t="n">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="H9" t="n">
-        <v>1702556</v>
+        <v>1728163</v>
       </c>
       <c r="I9" t="n">
-        <v>146.904</v>
+        <v>149.113</v>
       </c>
       <c r="J9" t="n">
-        <v>17168</v>
+        <v>10877</v>
       </c>
       <c r="K9" t="n">
-        <v>1.481</v>
+        <v>0.939</v>
       </c>
       <c r="L9" t="n">
-        <v>19120</v>
+        <v>20284</v>
       </c>
       <c r="M9" t="n">
-        <v>1.65</v>
+        <v>1.75</v>
       </c>
       <c r="N9" t="s">
         <v>63</v>
@@ -2976,7 +2976,7 @@
         <v>68</v>
       </c>
       <c r="C10" s="1" t="n">
-        <v>44042</v>
+        <v>44045</v>
       </c>
       <c r="D10" t="s">
         <v>69</v>
@@ -2986,25 +2986,25 @@
       </c>
       <c r="F10"/>
       <c r="G10" t="n">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="H10" t="n">
-        <v>147458</v>
+        <v>156924</v>
       </c>
       <c r="I10" t="n">
-        <v>12.632</v>
+        <v>13.443</v>
       </c>
       <c r="J10" t="n">
-        <v>3305</v>
+        <v>2970</v>
       </c>
       <c r="K10" t="n">
-        <v>0.283</v>
+        <v>0.254</v>
       </c>
       <c r="L10" t="n">
-        <v>2579</v>
+        <v>2857</v>
       </c>
       <c r="M10" t="n">
-        <v>0.221</v>
+        <v>0.245</v>
       </c>
       <c r="N10" t="s">
         <v>43</v>
@@ -3076,7 +3076,7 @@
         <v>82</v>
       </c>
       <c r="C12" s="1" t="n">
-        <v>44044</v>
+        <v>44046</v>
       </c>
       <c r="D12" t="s">
         <v>83</v>
@@ -3086,25 +3086,25 @@
       </c>
       <c r="F12"/>
       <c r="G12" t="n">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="H12" t="n">
-        <v>271000</v>
+        <v>276628</v>
       </c>
       <c r="I12" t="n">
-        <v>39.002</v>
+        <v>39.811</v>
       </c>
       <c r="J12" t="n">
-        <v>3955</v>
+        <v>4137</v>
       </c>
       <c r="K12" t="n">
-        <v>0.569</v>
+        <v>0.595</v>
       </c>
       <c r="L12" t="n">
-        <v>5030</v>
+        <v>4786</v>
       </c>
       <c r="M12" t="n">
-        <v>0.724</v>
+        <v>0.689</v>
       </c>
       <c r="N12" t="s">
         <v>85</v>
@@ -3127,7 +3127,7 @@
         <v>88</v>
       </c>
       <c r="C13" s="1" t="n">
-        <v>44045</v>
+        <v>44046</v>
       </c>
       <c r="D13" t="s">
         <v>89</v>
@@ -3137,25 +3137,25 @@
       </c>
       <c r="F13"/>
       <c r="G13" t="n">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="H13" t="n">
-        <v>4143459</v>
+        <v>4178195</v>
       </c>
       <c r="I13" t="n">
-        <v>109.783</v>
+        <v>110.704</v>
       </c>
       <c r="J13" t="n">
-        <v>44707</v>
+        <v>34736</v>
       </c>
       <c r="K13" t="n">
-        <v>1.185</v>
+        <v>0.92</v>
       </c>
       <c r="L13" t="n">
-        <v>54505</v>
+        <v>44895</v>
       </c>
       <c r="M13" t="n">
-        <v>1.444</v>
+        <v>1.19</v>
       </c>
       <c r="N13" t="s">
         <v>90</v>
@@ -3539,7 +3539,7 @@
         <v>137</v>
       </c>
       <c r="C21" s="1" t="n">
-        <v>44042</v>
+        <v>44045</v>
       </c>
       <c r="D21" t="s">
         <v>138</v>
@@ -3549,18 +3549,18 @@
       </c>
       <c r="F21"/>
       <c r="G21" t="n">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="H21"/>
       <c r="I21"/>
       <c r="J21" t="n">
-        <v>364</v>
+        <v>237</v>
       </c>
       <c r="K21" t="n">
-        <v>0.004</v>
+        <v>0.003</v>
       </c>
       <c r="L21" t="n">
-        <v>394</v>
+        <v>347</v>
       </c>
       <c r="M21" t="n">
         <v>0.004</v>
@@ -3637,7 +3637,7 @@
         <v>149</v>
       </c>
       <c r="C23" s="1" t="n">
-        <v>44044</v>
+        <v>44046</v>
       </c>
       <c r="D23" t="s">
         <v>150</v>
@@ -3649,25 +3649,25 @@
         <v>152</v>
       </c>
       <c r="G23" t="n">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="H23" t="n">
-        <v>184045</v>
+        <v>186336</v>
       </c>
       <c r="I23" t="n">
-        <v>10.432</v>
+        <v>10.561</v>
       </c>
       <c r="J23" t="n">
-        <v>2451</v>
+        <v>1413</v>
       </c>
       <c r="K23" t="n">
-        <v>0.139</v>
+        <v>0.08</v>
       </c>
       <c r="L23" t="n">
-        <v>2323</v>
+        <v>2229</v>
       </c>
       <c r="M23" t="n">
-        <v>0.132</v>
+        <v>0.126</v>
       </c>
       <c r="N23" t="s">
         <v>151</v>
@@ -3741,7 +3741,7 @@
         <v>162</v>
       </c>
       <c r="C25" s="1" t="n">
-        <v>44045</v>
+        <v>44046</v>
       </c>
       <c r="D25" t="s">
         <v>163</v>
@@ -3751,25 +3751,25 @@
       </c>
       <c r="F25"/>
       <c r="G25" t="n">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="H25" t="n">
-        <v>120346</v>
+        <v>120988</v>
       </c>
       <c r="I25" t="n">
-        <v>90.722</v>
+        <v>91.206</v>
       </c>
       <c r="J25" t="n">
-        <v>257</v>
+        <v>645</v>
       </c>
       <c r="K25" t="n">
-        <v>0.194</v>
+        <v>0.486</v>
       </c>
       <c r="L25" t="n">
-        <v>479</v>
+        <v>532</v>
       </c>
       <c r="M25" t="n">
-        <v>0.361</v>
+        <v>0.401</v>
       </c>
       <c r="N25" t="s">
         <v>165</v>
@@ -3886,7 +3886,7 @@
         <v>181</v>
       </c>
       <c r="C28" s="1" t="n">
-        <v>44044</v>
+        <v>44045</v>
       </c>
       <c r="D28" t="s">
         <v>182</v>
@@ -3896,25 +3896,25 @@
       </c>
       <c r="F28"/>
       <c r="G28" t="n">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="H28" t="n">
-        <v>367775</v>
+        <v>380510</v>
       </c>
       <c r="I28" t="n">
-        <v>66.377</v>
+        <v>68.675</v>
       </c>
       <c r="J28" t="n">
-        <v>407</v>
+        <v>4424</v>
       </c>
       <c r="K28" t="n">
-        <v>0.073</v>
+        <v>0.798</v>
       </c>
       <c r="L28" t="n">
-        <v>3238</v>
+        <v>4728</v>
       </c>
       <c r="M28" t="n">
-        <v>0.584</v>
+        <v>0.853</v>
       </c>
       <c r="N28" t="s">
         <v>184</v>
@@ -4437,7 +4437,7 @@
         <v>247</v>
       </c>
       <c r="C39" s="1" t="n">
-        <v>44046</v>
+        <v>44047</v>
       </c>
       <c r="D39" t="s">
         <v>248</v>
@@ -4447,25 +4447,25 @@
       </c>
       <c r="F39"/>
       <c r="G39" t="n">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="H39" t="n">
-        <v>894531</v>
+        <v>907987</v>
       </c>
       <c r="I39" t="n">
-        <v>3.27</v>
+        <v>3.32</v>
       </c>
       <c r="J39" t="n">
-        <v>12179</v>
+        <v>13456</v>
       </c>
       <c r="K39" t="n">
-        <v>0.045</v>
+        <v>0.049</v>
       </c>
       <c r="L39" t="n">
-        <v>13155</v>
+        <v>14292</v>
       </c>
       <c r="M39" t="n">
-        <v>0.048</v>
+        <v>0.052</v>
       </c>
       <c r="N39" t="s">
         <v>249</v>
@@ -4488,7 +4488,7 @@
         <v>253</v>
       </c>
       <c r="C40" s="1" t="n">
-        <v>44046</v>
+        <v>44047</v>
       </c>
       <c r="D40" t="s">
         <v>254</v>
@@ -4498,25 +4498,25 @@
       </c>
       <c r="F40"/>
       <c r="G40" t="n">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="H40" t="n">
-        <v>2534658</v>
+        <v>2560374</v>
       </c>
       <c r="I40" t="n">
-        <v>30.177</v>
+        <v>30.483</v>
       </c>
       <c r="J40" t="n">
-        <v>26240</v>
+        <v>25716</v>
       </c>
       <c r="K40" t="n">
-        <v>0.312</v>
+        <v>0.306</v>
       </c>
       <c r="L40" t="n">
-        <v>25710</v>
+        <v>25750</v>
       </c>
       <c r="M40" t="n">
-        <v>0.306</v>
+        <v>0.307</v>
       </c>
       <c r="N40" t="s">
         <v>255</v>
@@ -4590,7 +4590,7 @@
         <v>264</v>
       </c>
       <c r="C42" s="1" t="n">
-        <v>44039</v>
+        <v>44040</v>
       </c>
       <c r="D42" t="s">
         <v>265</v>
@@ -4600,25 +4600,25 @@
       </c>
       <c r="F42"/>
       <c r="G42" t="n">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="H42" t="n">
-        <v>1676396</v>
+        <v>1702868</v>
       </c>
       <c r="I42" t="n">
-        <v>193.679</v>
+        <v>196.737</v>
       </c>
       <c r="J42" t="n">
-        <v>28234</v>
+        <v>26194</v>
       </c>
       <c r="K42" t="n">
-        <v>3.262</v>
+        <v>3.026</v>
       </c>
       <c r="L42" t="n">
-        <v>24501</v>
+        <v>23972</v>
       </c>
       <c r="M42" t="n">
-        <v>2.831</v>
+        <v>2.77</v>
       </c>
       <c r="N42" t="s">
         <v>43</v>
@@ -4747,7 +4747,7 @@
         <v>280</v>
       </c>
       <c r="C45" s="1" t="n">
-        <v>44045</v>
+        <v>44046</v>
       </c>
       <c r="D45" t="s">
         <v>281</v>
@@ -4759,25 +4759,25 @@
         <v>283</v>
       </c>
       <c r="G45" t="n">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="H45" t="n">
-        <v>836404</v>
+        <v>849115</v>
       </c>
       <c r="I45" t="n">
-        <v>6.613</v>
+        <v>6.714</v>
       </c>
       <c r="J45" t="n">
-        <v>11656</v>
+        <v>12711</v>
       </c>
       <c r="K45" t="n">
-        <v>0.092</v>
+        <v>0.101</v>
       </c>
       <c r="L45" t="n">
-        <v>17303</v>
+        <v>18373</v>
       </c>
       <c r="M45" t="n">
-        <v>0.137</v>
+        <v>0.145</v>
       </c>
       <c r="N45" t="s">
         <v>284</v>
@@ -4800,7 +4800,7 @@
         <v>287</v>
       </c>
       <c r="C46" s="1" t="n">
-        <v>44042</v>
+        <v>44044</v>
       </c>
       <c r="D46" t="s">
         <v>288</v>
@@ -4812,25 +4812,25 @@
         <v>289</v>
       </c>
       <c r="G46" t="n">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="H46" t="n">
-        <v>1091499</v>
+        <v>1100165</v>
       </c>
       <c r="I46" t="n">
-        <v>8.63</v>
+        <v>8.699</v>
       </c>
       <c r="J46" t="n">
-        <v>17194</v>
+        <v>3318</v>
       </c>
       <c r="K46" t="n">
-        <v>0.136</v>
+        <v>0.026</v>
       </c>
       <c r="L46" t="n">
-        <v>15754</v>
+        <v>13364</v>
       </c>
       <c r="M46" t="n">
-        <v>0.125</v>
+        <v>0.106</v>
       </c>
       <c r="N46" t="s">
         <v>284</v>
@@ -4955,7 +4955,7 @@
         <v>304</v>
       </c>
       <c r="C49" s="1" t="n">
-        <v>44043</v>
+        <v>44046</v>
       </c>
       <c r="D49" t="s">
         <v>305</v>
@@ -4965,25 +4965,25 @@
       </c>
       <c r="F49"/>
       <c r="G49" t="n">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="H49" t="n">
-        <v>505088</v>
+        <v>511599</v>
       </c>
       <c r="I49" t="n">
-        <v>118.272</v>
+        <v>119.797</v>
       </c>
       <c r="J49" t="n">
-        <v>2920</v>
+        <v>2038</v>
       </c>
       <c r="K49" t="n">
-        <v>0.684</v>
+        <v>0.477</v>
       </c>
       <c r="L49" t="n">
-        <v>3668</v>
+        <v>3148</v>
       </c>
       <c r="M49" t="n">
-        <v>0.859</v>
+        <v>0.737</v>
       </c>
       <c r="N49" t="s">
         <v>306</v>
@@ -5006,7 +5006,7 @@
         <v>310</v>
       </c>
       <c r="C50" s="1" t="n">
-        <v>44046</v>
+        <v>44047</v>
       </c>
       <c r="D50" t="s">
         <v>311</v>
@@ -5018,25 +5018,25 @@
         <v>313</v>
       </c>
       <c r="G50" t="n">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="H50" t="n">
-        <v>201997</v>
+        <v>203868</v>
       </c>
       <c r="I50" t="n">
-        <v>107.092</v>
+        <v>108.084</v>
       </c>
       <c r="J50" t="n">
-        <v>687</v>
+        <v>1871</v>
       </c>
       <c r="K50" t="n">
-        <v>0.364</v>
+        <v>0.992</v>
       </c>
       <c r="L50" t="n">
-        <v>1447</v>
+        <v>1489</v>
       </c>
       <c r="M50" t="n">
-        <v>0.767</v>
+        <v>0.789</v>
       </c>
       <c r="N50" t="s">
         <v>312</v>
@@ -5059,7 +5059,7 @@
         <v>316</v>
       </c>
       <c r="C51" s="1" t="n">
-        <v>44045</v>
+        <v>44046</v>
       </c>
       <c r="D51" t="s">
         <v>317</v>
@@ -5069,21 +5069,25 @@
       </c>
       <c r="F51"/>
       <c r="G51" t="n">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="H51" t="n">
-        <v>527729</v>
+        <v>531518</v>
       </c>
       <c r="I51" t="n">
-        <v>193.855</v>
-      </c>
-      <c r="J51"/>
-      <c r="K51"/>
+        <v>195.247</v>
+      </c>
+      <c r="J51" t="n">
+        <v>3789</v>
+      </c>
+      <c r="K51" t="n">
+        <v>1.392</v>
+      </c>
       <c r="L51" t="n">
-        <v>3386</v>
+        <v>3443</v>
       </c>
       <c r="M51" t="n">
-        <v>1.244</v>
+        <v>1.265</v>
       </c>
       <c r="N51" t="s">
         <v>43</v>
@@ -5157,7 +5161,7 @@
         <v>325</v>
       </c>
       <c r="C53" s="1" t="n">
-        <v>44045</v>
+        <v>44046</v>
       </c>
       <c r="D53" t="s">
         <v>326</v>
@@ -5169,25 +5173,25 @@
         <v>328</v>
       </c>
       <c r="G53" t="n">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="H53" t="n">
-        <v>979178</v>
+        <v>983297</v>
       </c>
       <c r="I53" t="n">
-        <v>30.253</v>
+        <v>30.381</v>
       </c>
       <c r="J53" t="n">
-        <v>4504</v>
+        <v>4119</v>
       </c>
       <c r="K53" t="n">
-        <v>0.139</v>
+        <v>0.127</v>
       </c>
       <c r="L53" t="n">
-        <v>5933</v>
+        <v>5722</v>
       </c>
       <c r="M53" t="n">
-        <v>0.183</v>
+        <v>0.177</v>
       </c>
       <c r="N53" t="s">
         <v>43</v>
@@ -5210,7 +5214,7 @@
         <v>332</v>
       </c>
       <c r="C54" s="1" t="n">
-        <v>44043</v>
+        <v>44046</v>
       </c>
       <c r="D54" t="s">
         <v>333</v>
@@ -5220,25 +5224,25 @@
       </c>
       <c r="F54"/>
       <c r="G54" t="n">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="H54" t="n">
-        <v>78900</v>
+        <v>82208</v>
       </c>
       <c r="I54" t="n">
-        <v>145.965</v>
+        <v>152.084</v>
       </c>
       <c r="J54" t="n">
-        <v>860</v>
+        <v>1209</v>
       </c>
       <c r="K54" t="n">
-        <v>1.591</v>
+        <v>2.237</v>
       </c>
       <c r="L54" t="n">
-        <v>1151</v>
+        <v>1157</v>
       </c>
       <c r="M54" t="n">
-        <v>2.129</v>
+        <v>2.14</v>
       </c>
       <c r="N54" t="s">
         <v>335</v>
@@ -5312,7 +5316,7 @@
         <v>345</v>
       </c>
       <c r="C56" s="1" t="n">
-        <v>44042</v>
+        <v>44043</v>
       </c>
       <c r="D56" t="s">
         <v>346</v>
@@ -5322,25 +5326,25 @@
       </c>
       <c r="F56"/>
       <c r="G56" t="n">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="H56" t="n">
-        <v>920079</v>
+        <v>931145</v>
       </c>
       <c r="I56" t="n">
-        <v>7.136</v>
+        <v>7.222</v>
       </c>
       <c r="J56" t="n">
-        <v>5960</v>
+        <v>4259</v>
       </c>
       <c r="K56" t="n">
-        <v>0.046</v>
+        <v>0.033</v>
       </c>
       <c r="L56" t="n">
-        <v>8499</v>
+        <v>8104</v>
       </c>
       <c r="M56" t="n">
-        <v>0.066</v>
+        <v>0.063</v>
       </c>
       <c r="N56" t="s">
         <v>348</v>
@@ -5363,7 +5367,7 @@
         <v>352</v>
       </c>
       <c r="C57" s="1" t="n">
-        <v>44043</v>
+        <v>44046</v>
       </c>
       <c r="D57" t="s">
         <v>353</v>
@@ -5373,25 +5377,25 @@
       </c>
       <c r="F57"/>
       <c r="G57" t="n">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="H57" t="n">
-        <v>1252365</v>
+        <v>1316861</v>
       </c>
       <c r="I57" t="n">
-        <v>33.93</v>
+        <v>35.677</v>
       </c>
       <c r="J57" t="n">
-        <v>21170</v>
+        <v>21667</v>
       </c>
       <c r="K57" t="n">
-        <v>0.574</v>
+        <v>0.587</v>
       </c>
       <c r="L57" t="n">
-        <v>21013</v>
+        <v>21250</v>
       </c>
       <c r="M57" t="n">
-        <v>0.569</v>
+        <v>0.576</v>
       </c>
       <c r="N57" t="s">
         <v>354</v>
@@ -5465,7 +5469,7 @@
         <v>364</v>
       </c>
       <c r="C59" s="1" t="n">
-        <v>44043</v>
+        <v>44046</v>
       </c>
       <c r="D59" t="s">
         <v>365</v>
@@ -5475,25 +5479,25 @@
       </c>
       <c r="F59"/>
       <c r="G59" t="n">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="H59" t="n">
-        <v>375416</v>
+        <v>398907</v>
       </c>
       <c r="I59" t="n">
-        <v>12.885</v>
+        <v>13.691</v>
       </c>
       <c r="J59" t="n">
-        <v>10768</v>
+        <v>7637</v>
       </c>
       <c r="K59" t="n">
-        <v>0.37</v>
+        <v>0.262</v>
       </c>
       <c r="L59" t="n">
-        <v>5762</v>
+        <v>7376</v>
       </c>
       <c r="M59" t="n">
-        <v>0.198</v>
+        <v>0.253</v>
       </c>
       <c r="N59" t="s">
         <v>366</v>
@@ -5563,7 +5567,7 @@
         <v>377</v>
       </c>
       <c r="C61" s="1" t="n">
-        <v>44045</v>
+        <v>44046</v>
       </c>
       <c r="D61" t="s">
         <v>378</v>
@@ -5573,25 +5577,25 @@
       </c>
       <c r="F61"/>
       <c r="G61" t="n">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="H61" t="n">
-        <v>472161</v>
+        <v>473769</v>
       </c>
       <c r="I61" t="n">
-        <v>97.913</v>
+        <v>98.247</v>
       </c>
       <c r="J61" t="n">
-        <v>1692</v>
+        <v>1608</v>
       </c>
       <c r="K61" t="n">
-        <v>0.351</v>
+        <v>0.333</v>
       </c>
       <c r="L61" t="n">
-        <v>2276</v>
+        <v>2348</v>
       </c>
       <c r="M61" t="n">
-        <v>0.472</v>
+        <v>0.487</v>
       </c>
       <c r="N61" t="s">
         <v>379</v>
@@ -5665,7 +5669,7 @@
         <v>388</v>
       </c>
       <c r="C63" s="1" t="n">
-        <v>44041</v>
+        <v>44044</v>
       </c>
       <c r="D63" t="s">
         <v>389</v>
@@ -5675,25 +5679,25 @@
       </c>
       <c r="F63"/>
       <c r="G63" t="n">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="H63" t="n">
-        <v>424857</v>
+        <v>434986</v>
       </c>
       <c r="I63" t="n">
-        <v>78.369</v>
+        <v>80.237</v>
       </c>
       <c r="J63" t="n">
-        <v>4366</v>
+        <v>1372</v>
       </c>
       <c r="K63" t="n">
-        <v>0.805</v>
+        <v>0.253</v>
       </c>
       <c r="L63" t="n">
-        <v>3549</v>
+        <v>3726</v>
       </c>
       <c r="M63" t="n">
-        <v>0.655</v>
+        <v>0.687</v>
       </c>
       <c r="N63" t="s">
         <v>390</v>
@@ -5763,7 +5767,7 @@
         <v>402</v>
       </c>
       <c r="C65" s="1" t="n">
-        <v>44045</v>
+        <v>44046</v>
       </c>
       <c r="D65" t="s">
         <v>403</v>
@@ -5773,25 +5777,25 @@
       </c>
       <c r="F65"/>
       <c r="G65" t="n">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="H65" t="n">
-        <v>2021196</v>
+        <v>2031955</v>
       </c>
       <c r="I65" t="n">
-        <v>9.15</v>
+        <v>9.199</v>
       </c>
       <c r="J65" t="n">
-        <v>11026</v>
+        <v>10759</v>
       </c>
       <c r="K65" t="n">
-        <v>0.05</v>
+        <v>0.049</v>
       </c>
       <c r="L65" t="n">
-        <v>21859</v>
+        <v>17444</v>
       </c>
       <c r="M65" t="n">
-        <v>0.099</v>
+        <v>0.079</v>
       </c>
       <c r="N65" t="s">
         <v>404</v>
@@ -5814,7 +5818,7 @@
         <v>407</v>
       </c>
       <c r="C66" s="1" t="n">
-        <v>44042</v>
+        <v>44045</v>
       </c>
       <c r="D66" t="s">
         <v>408</v>
@@ -5824,25 +5828,25 @@
       </c>
       <c r="F66"/>
       <c r="G66" t="n">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="H66" t="n">
-        <v>217323</v>
+        <v>227309</v>
       </c>
       <c r="I66" t="n">
-        <v>50.367</v>
+        <v>52.682</v>
       </c>
       <c r="J66" t="n">
-        <v>3218</v>
+        <v>3220</v>
       </c>
       <c r="K66" t="n">
         <v>0.746</v>
       </c>
       <c r="L66" t="n">
-        <v>3221</v>
+        <v>3157</v>
       </c>
       <c r="M66" t="n">
-        <v>0.747</v>
+        <v>0.732</v>
       </c>
       <c r="N66" t="s">
         <v>409</v>
@@ -5967,7 +5971,7 @@
         <v>425</v>
       </c>
       <c r="C69" s="1" t="n">
-        <v>44043</v>
+        <v>44045</v>
       </c>
       <c r="D69" t="s">
         <v>426</v>
@@ -5977,25 +5981,21 @@
       </c>
       <c r="F69"/>
       <c r="G69" t="n">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="H69" t="n">
-        <v>1435618</v>
+        <v>1480583</v>
       </c>
       <c r="I69" t="n">
-        <v>13.101</v>
-      </c>
-      <c r="J69" t="n">
-        <v>36874</v>
-      </c>
-      <c r="K69" t="n">
-        <v>0.336</v>
-      </c>
+        <v>13.511</v>
+      </c>
+      <c r="J69"/>
+      <c r="K69"/>
       <c r="L69" t="n">
-        <v>32151</v>
+        <v>29508</v>
       </c>
       <c r="M69" t="n">
-        <v>0.293</v>
+        <v>0.269</v>
       </c>
       <c r="N69" t="s">
         <v>222</v>
@@ -6222,7 +6222,7 @@
         <v>450</v>
       </c>
       <c r="C74" s="1" t="n">
-        <v>44045</v>
+        <v>44046</v>
       </c>
       <c r="D74" t="s">
         <v>451</v>
@@ -6232,25 +6232,25 @@
       </c>
       <c r="F74"/>
       <c r="G74" t="n">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="H74" t="n">
-        <v>1248318</v>
+        <v>1268899</v>
       </c>
       <c r="I74" t="n">
-        <v>64.889</v>
+        <v>65.959</v>
       </c>
       <c r="J74" t="n">
-        <v>8045</v>
+        <v>20581</v>
       </c>
       <c r="K74" t="n">
-        <v>0.418</v>
+        <v>1.07</v>
       </c>
       <c r="L74" t="n">
-        <v>20774</v>
+        <v>19600</v>
       </c>
       <c r="M74" t="n">
-        <v>1.08</v>
+        <v>1.019</v>
       </c>
       <c r="N74" t="s">
         <v>453</v>
@@ -6273,7 +6273,7 @@
         <v>457</v>
       </c>
       <c r="C75" s="1" t="n">
-        <v>44045</v>
+        <v>44046</v>
       </c>
       <c r="D75" t="s">
         <v>458</v>
@@ -6283,25 +6283,25 @@
       </c>
       <c r="F75"/>
       <c r="G75" t="n">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="H75" t="n">
-        <v>29029900</v>
+        <v>29201862</v>
       </c>
       <c r="I75" t="n">
-        <v>198.924</v>
+        <v>200.103</v>
       </c>
       <c r="J75" t="n">
-        <v>236640</v>
+        <v>171962</v>
       </c>
       <c r="K75" t="n">
-        <v>1.622</v>
+        <v>1.178</v>
       </c>
       <c r="L75" t="n">
-        <v>269705</v>
+        <v>267756</v>
       </c>
       <c r="M75" t="n">
-        <v>1.848</v>
+        <v>1.835</v>
       </c>
       <c r="N75" t="s">
         <v>459</v>
@@ -6626,7 +6626,7 @@
         <v>495</v>
       </c>
       <c r="C82" s="1" t="n">
-        <v>44046</v>
+        <v>44047</v>
       </c>
       <c r="D82" t="s">
         <v>496</v>
@@ -6636,25 +6636,25 @@
       </c>
       <c r="F82"/>
       <c r="G82" t="n">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="H82" t="n">
-        <v>265797</v>
+        <v>267117</v>
       </c>
       <c r="I82" t="n">
-        <v>48.684</v>
+        <v>48.926</v>
       </c>
       <c r="J82" t="n">
-        <v>766</v>
+        <v>1320</v>
       </c>
       <c r="K82" t="n">
-        <v>0.14</v>
+        <v>0.242</v>
       </c>
       <c r="L82" t="n">
-        <v>1729</v>
+        <v>1697</v>
       </c>
       <c r="M82" t="n">
-        <v>0.317</v>
+        <v>0.311</v>
       </c>
       <c r="N82" t="s">
         <v>498</v>
@@ -6677,7 +6677,7 @@
         <v>502</v>
       </c>
       <c r="C83" s="1" t="n">
-        <v>44045</v>
+        <v>44046</v>
       </c>
       <c r="D83" t="s">
         <v>503</v>
@@ -6687,25 +6687,25 @@
       </c>
       <c r="F83"/>
       <c r="G83" t="n">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="H83" t="n">
-        <v>131699</v>
+        <v>132589</v>
       </c>
       <c r="I83" t="n">
-        <v>63.349</v>
+        <v>63.777</v>
       </c>
       <c r="J83" t="n">
-        <v>272</v>
+        <v>890</v>
       </c>
       <c r="K83" t="n">
-        <v>0.131</v>
+        <v>0.428</v>
       </c>
       <c r="L83" t="n">
-        <v>732</v>
+        <v>735</v>
       </c>
       <c r="M83" t="n">
-        <v>0.352</v>
+        <v>0.354</v>
       </c>
       <c r="N83" t="s">
         <v>505</v>
@@ -6743,22 +6743,22 @@
         <v>155</v>
       </c>
       <c r="H84" t="n">
-        <v>3036779</v>
+        <v>3058695</v>
       </c>
       <c r="I84" t="n">
-        <v>51.203</v>
+        <v>51.572</v>
       </c>
       <c r="J84" t="n">
-        <v>34794</v>
+        <v>56710</v>
       </c>
       <c r="K84" t="n">
-        <v>0.587</v>
+        <v>0.956</v>
       </c>
       <c r="L84" t="n">
-        <v>37572</v>
+        <v>40702</v>
       </c>
       <c r="M84" t="n">
-        <v>0.633</v>
+        <v>0.686</v>
       </c>
       <c r="N84" t="s">
         <v>511</v>
@@ -6781,7 +6781,7 @@
         <v>516</v>
       </c>
       <c r="C85" s="1" t="n">
-        <v>44046</v>
+        <v>44047</v>
       </c>
       <c r="D85" t="s">
         <v>517</v>
@@ -6791,25 +6791,25 @@
       </c>
       <c r="F85"/>
       <c r="G85" t="n">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="H85" t="n">
-        <v>1562356</v>
+        <v>1571056</v>
       </c>
       <c r="I85" t="n">
-        <v>30.474</v>
+        <v>30.643</v>
       </c>
       <c r="J85" t="n">
-        <v>3878</v>
+        <v>8700</v>
       </c>
       <c r="K85" t="n">
-        <v>0.076</v>
+        <v>0.17</v>
       </c>
       <c r="L85" t="n">
-        <v>7736</v>
+        <v>7685</v>
       </c>
       <c r="M85" t="n">
-        <v>0.151</v>
+        <v>0.15</v>
       </c>
       <c r="N85" t="s">
         <v>518</v>
@@ -6973,7 +6973,7 @@
         <v>539</v>
       </c>
       <c r="C89" s="1" t="n">
-        <v>44045</v>
+        <v>44046</v>
       </c>
       <c r="D89" t="s">
         <v>540</v>
@@ -6983,25 +6983,25 @@
       </c>
       <c r="F89"/>
       <c r="G89" t="n">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="H89" t="n">
-        <v>803725</v>
+        <v>808031</v>
       </c>
       <c r="I89" t="n">
-        <v>92.867</v>
+        <v>93.364</v>
       </c>
       <c r="J89" t="n">
-        <v>1596</v>
+        <v>3625</v>
       </c>
       <c r="K89" t="n">
-        <v>0.184</v>
+        <v>0.419</v>
       </c>
       <c r="L89" t="n">
-        <v>5256</v>
+        <v>5081</v>
       </c>
       <c r="M89" t="n">
-        <v>0.607</v>
+        <v>0.587</v>
       </c>
       <c r="N89" t="s">
         <v>541</v>
@@ -7587,7 +7587,7 @@
         <v>604</v>
       </c>
       <c r="C101" s="1" t="n">
-        <v>44045</v>
+        <v>44046</v>
       </c>
       <c r="D101" t="s">
         <v>605</v>
@@ -7597,25 +7597,25 @@
       </c>
       <c r="F101"/>
       <c r="G101" t="n">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="H101" t="n">
-        <v>56812162</v>
+        <v>57543852</v>
       </c>
       <c r="I101" t="n">
-        <v>171.637</v>
+        <v>173.847</v>
       </c>
       <c r="J101" t="n">
-        <v>725902</v>
+        <v>731690</v>
       </c>
       <c r="K101" t="n">
-        <v>2.193</v>
+        <v>2.211</v>
       </c>
       <c r="L101" t="n">
-        <v>760095</v>
+        <v>755931</v>
       </c>
       <c r="M101" t="n">
-        <v>2.296</v>
+        <v>2.284</v>
       </c>
       <c r="N101" t="s">
         <v>606</v>
@@ -7638,7 +7638,7 @@
         <v>611</v>
       </c>
       <c r="C102" s="1" t="n">
-        <v>44045</v>
+        <v>44046</v>
       </c>
       <c r="D102" t="s">
         <v>612</v>
@@ -7648,25 +7648,25 @@
       </c>
       <c r="F102"/>
       <c r="G102" t="n">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="H102" t="n">
-        <v>117053</v>
+        <v>119042</v>
       </c>
       <c r="I102" t="n">
-        <v>33.697</v>
+        <v>34.269</v>
       </c>
       <c r="J102" t="n">
-        <v>1853</v>
+        <v>1989</v>
       </c>
       <c r="K102" t="n">
-        <v>0.533</v>
+        <v>0.573</v>
       </c>
       <c r="L102" t="n">
-        <v>2007</v>
+        <v>2012</v>
       </c>
       <c r="M102" t="n">
-        <v>0.578</v>
+        <v>0.579</v>
       </c>
       <c r="N102" t="s">
         <v>127</v>

</xml_diff>

<commit_message>
Updated testing data for 2020-08-07
</commit_message>
<xml_diff>
--- a/public/data/testing/covid-testing-latest-data-source-details.xlsx
+++ b/public/data/testing/covid-testing-latest-data-source-details.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="624" uniqueCount="624">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="623" uniqueCount="623">
   <si>
     <t xml:space="preserve">ISO code</t>
   </si>
@@ -110,7 +110,7 @@
     <t xml:space="preserve">Australia - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.health.gov.au/sites/default/files/documents/2020/08/coronavirus-covid-19-at-a-glance-5-august-2020.pdf</t>
+    <t xml:space="preserve">https://www.health.gov.au/sites/default/files/documents/2020/08/coronavirus-covid-19-at-a-glance-6-august-2020.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">Australian Government Department of Health</t>
@@ -202,7 +202,7 @@
     <t xml:space="preserve">Belarus - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">http://minzdrav.gov.by/ru/sobytiya/u-belarusi-na-4-zhni-nya-vypisanyya-63-tys-163-patsyenta/</t>
+    <t xml:space="preserve">http://minzdrav.gov.by/ru/sobytiya/u-belarusi-na-6-zhni-nya-vypisanyya-63-tys-756-patsyenta/</t>
   </si>
   <si>
     <t xml:space="preserve">Belarus Ministry of Health</t>
@@ -245,7 +245,7 @@
     <t xml:space="preserve">Bolivia - units unclear</t>
   </si>
   <si>
-    <t xml:space="preserve">https://minsalud.gob.bo/4471-reporte-covid-140</t>
+    <t xml:space="preserve">https://minsalud.gob.bo/4481-ministerio-de-salud-reporta-1-780-nuevos-contagios-de-covid-19-y-supera-los-85-000-casos-positivos</t>
   </si>
   <si>
     <t xml:space="preserve">https://www.minsalud.gob.bo/</t>
@@ -473,7 +473,7 @@
     <t xml:space="preserve">Democratic Republic of Congo - samples tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/CMR_Covid19_RDC/status/1290204955307999232/photo/1</t>
+    <t xml:space="preserve">https://twitter.com/CMR_Covid19_RDC/status/1291289739681828864/photo/1</t>
   </si>
   <si>
     <t xml:space="preserve">DRC COVID-19 Pandemic Response Multisectoral Committee</t>
@@ -491,7 +491,7 @@
     <t xml:space="preserve">Denmark - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://files.ssi.dk/Data-epidemiologiske-rapport-05082020-zx41</t>
+    <t xml:space="preserve">https://files.ssi.dk/Data-epidemiologiske-rapport-07082020-qw54</t>
   </si>
   <si>
     <t xml:space="preserve">Statens Serum Institut</t>
@@ -752,7 +752,7 @@
     <t xml:space="preserve">Greece - samples tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://eody.gov.gr/covid-gr-daily-report-20200804</t>
+    <t xml:space="preserve">https://eody.gov.gr/covid-gr-daily-report-20200806</t>
   </si>
   <si>
     <t xml:space="preserve">National Organization of Public Health</t>
@@ -988,13 +988,13 @@
     <t xml:space="preserve">Japan - people tested (incl. non-PCR)</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.mhlw.go.jp/stf/newpage_12851.html</t>
+    <t xml:space="preserve">https://www.mhlw.go.jp/stf/newpage_12870.html</t>
   </si>
   <si>
     <t xml:space="preserve">Ministry of Health, Labor and Welfare Press Release</t>
   </si>
   <si>
-    <t xml:space="preserve">See Table: 国内の発生状況, column 1 '検査実施人数'. Daily change figure provided for this date is not consistent with the cumulative totals for today and the previous day.</t>
+    <t xml:space="preserve">See Table: 国内の発生状況, column 1 '検査実施人数'.</t>
   </si>
   <si>
     <t xml:space="preserve">Ministry of Health, Labor and Welfare</t>
@@ -1013,10 +1013,10 @@
     <t xml:space="preserve">Japan - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.mhlw.go.jp/content/10906000/000656910.pdf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The cumulative total reported in the press release (1,184,681) does not sum to the cumulative total calculated from the weekly and daily figures reported by the MOH. See: https://www.mhlw.go.jp/content/10906000/000656910.pdf</t>
+    <t xml:space="preserve">https://www.mhlw.go.jp/content/10906000/000657349.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The cumulative total reported in the press release (1,215,318) does not sum to the cumulative total calculated from the weekly and daily figures reported by the MOH. See: https://www.mhlw.go.jp/content/10906000/000657349.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">On 11 April 2020, the MOH started providing a daily time series on the "Implementation status of PCR tests for new coronavirus in Japan (based on the date on which results were determined" (via Google translate). 
@@ -1069,7 +1069,7 @@
     <t xml:space="preserve">Kuwait - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/KUWAIT_MOH/status/1290225953763811330/photo/1</t>
+    <t xml:space="preserve">https://twitter.com/KUWAIT_MOH/status/1291341316073435136/photo/1</t>
   </si>
   <si>
     <t xml:space="preserve">Kuwait Ministry of Health</t>
@@ -1135,7 +1135,7 @@
     <t xml:space="preserve">Malaysia - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">http://covid-19.moh.gov.my/terkini/082020/situasi-terkini-05-ogos-2020</t>
+    <t xml:space="preserve">http://covid-19.moh.gov.my/terkini/082020/situasi-terkini-06-ogos-2020</t>
   </si>
   <si>
     <t xml:space="preserve">Ministry of Health Malaysia</t>
@@ -1161,7 +1161,7 @@
     <t xml:space="preserve">Maldives - samples tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/HPA_MV/status/1290345598428647425/photo/1</t>
+    <t xml:space="preserve">https://twitter.com/HPA_MV/status/1291418563312521216/photo/1</t>
   </si>
   <si>
     <t xml:space="preserve">Maldives Health Protection Agency</t>
@@ -1228,7 +1228,7 @@
     <t xml:space="preserve">Morocco - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/Ministere_Sante/status/1290335589095661568/photo/1</t>
+    <t xml:space="preserve">https://twitter.com/Ministere_Sante/status/1291422913153859586/photo/1</t>
   </si>
   <si>
     <t xml:space="preserve">Morocco Ministry of Health</t>
@@ -1268,7 +1268,7 @@
     <t xml:space="preserve">Nepal - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://drive.google.com/drive/folders/1vzjKFByfG1hg1XPooiWaWjkwT1hhd-wi</t>
+    <t xml:space="preserve">https://drive.google.com/drive/folders/1b1dQwSgV6Fw10kpUdBwFDiFIN1YehzQ8</t>
   </si>
   <si>
     <t xml:space="preserve">Ministry of Health and Population</t>
@@ -1472,13 +1472,17 @@
     <t xml:space="preserve">Philippines - people tested</t>
   </si>
   <si>
+    <t xml:space="preserve">https://drive.google.com/drive/folders/1e_Hv_hquoc8v0M5WZNNes3QnDwkFqaGO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Philippines Department of Health</t>
+  </si>
+  <si>
     <t xml:space="preserve">http://www.doh.gov.ph/covid19tracker</t>
   </si>
   <si>
-    <t xml:space="preserve">Department of Health (DOH) Philippines</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The Department of Health (DOH) [dashboard](http://www.doh.gov.ph/covid19tracker) provides a time series of both individuals tested and samples tested dating back to 3 April 2020.
+    <t xml:space="preserve">As part of its COVID-19 dashboard, the Philippines Department of Health provides a 'COVID-19 DOH Data Drop' as a series of CSV files shared on Google Drive.
+Among these files, the 'Testing Aggregates' file includes a time series of cumulative unique individuals tested since 3 April 2020.
 The source provides a breakdown by laboratory. Data for recent days may be incomplete due to delays in reporting.</t>
   </si>
   <si>
@@ -1488,7 +1492,7 @@
     <t xml:space="preserve">Poland - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/MZ_GOV_PL/status/1290935579882840065</t>
+    <t xml:space="preserve">https://twitter.com/MZ_GOV_PL/status/1291297967392120832</t>
   </si>
   <si>
     <t xml:space="preserve">Poland Ministry of Health</t>
@@ -1555,7 +1559,7 @@
     <t xml:space="preserve">Romania - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://gov.ro/ro/media/comunicate/buletin-de-presa-5-august-2020-ora-13-00&amp;page=1</t>
+    <t xml:space="preserve">https://gov.ro/ro/media/comunicate/buletin-de-presa-7-august-2020-ora-13-00&amp;page=1</t>
   </si>
   <si>
     <t xml:space="preserve">Ministry of Internal Affairs</t>
@@ -1578,7 +1582,7 @@
     <t xml:space="preserve">Russia - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://rospotrebnadzor.ru/about/info/news/news_details.php?ELEMENT_ID=15098</t>
+    <t xml:space="preserve">https://rospotrebnadzor.ru/about/info/news/news_details.php?ELEMENT_ID=15103</t>
   </si>
   <si>
     <t xml:space="preserve">Government of the Russian Federation</t>
@@ -1772,7 +1776,7 @@
     <t xml:space="preserve">South Korea - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.cdc.go.kr/board/board.es?mid=&amp;bid=0030&amp;act=view&amp;list_no=367996&amp;tag=&amp;nPage=1</t>
+    <t xml:space="preserve">https://www.cdc.go.kr/board/board.es?mid=&amp;bid=0030&amp;act=view&amp;list_no=368060&amp;tag=&amp;nPage=1</t>
   </si>
   <si>
     <t xml:space="preserve">South Korea CDC</t>
@@ -1814,9 +1818,10 @@
 ---
 Daily case reports (e.g. [5 August 2020](https://www.mscbs.gob.es/profesionales/saludPublica/ccayes/alertasActual/nCov-China/documentos/Actualizacion_178_COVID-19.pdf)) published by the Ministry of Health note that "total cases [are] confirmed by PCR until 10 May, and by PCR and IgM (only if compatible symptoms) according to the new surveillance strategy from 11 May".
 This could have indicated that Spain included positive antibody tests in their figures for confirmed cases. As we explain in [this FAQ](https://ourworldindata.org/coronavirus-testing#why-do-you-not-report-the-positive-rate-or-tests-per-case-for-all-countries-in-the-dataset), we do not present figures for the positive rate or number of tests per confirmed case for countries where we believe this to be the case.
-However, this footnote importantly says that positive IgM results are only counted if they have "compatible symptoms", i.e. if they are actively infected by the virus.
+However, this footnote importantly says that positive IgM results are only counted if they have "compatible symptoms", i.e. if patients are actively infected by the virus.
 [This report](https://www.mscbs.gob.es/profesionales/saludPublica/ccayes/alertasActual/nCov-China/documentos/COVID19_Estrategia_vigilancia_y_control_e_indicadores.pdf) published on 9 July 2020 also makes clear on page 4 that IgM tests included in new confirmed cases do not correspond to massive serology testing for past infections, but rather to active, symptomatic infections with a negative PCR result but for which further IgM testing came back positive.
-In the same way, the documentation published by the Carlos III Health Institute on [its COVID-19 website](https://cnecovid.isciii.es/covid19/#documentaci%C3%B3n-y-datos) states that "as of May 11, the Ministry of Health is counting the confirmed cases diagnosed by PCR (and in some specific cases those diagnosed by IgM by ELISA)", i.e. the inclusion of IgM does not mean the inclusion of massive antibody testing results, but rather specific instances where current infections are confirmed via IgM instead of PCR.</t>
+In the same way, the documentation published by the Carlos III Health Institute on [its COVID-19 website](https://cnecovid.isciii.es/covid19/#documentaci%C3%B3n-y-datos) states that "as of May 11, the Ministry of Health is counting the confirmed cases diagnosed by PCR (and in some specific cases those diagnosed by IgM by ELISA)", i.e. the inclusion of IgM does not mean the inclusion of massive antibody testing results, but rather specific instances where current infections are confirmed via IgM instead of PCR.
+Pending new information that would prove otherwise, we therefore do not exclude Spain from the calculation of the positive rate and number of tests per case, as IgM tests for active cases represent a very small number and therefore should not affect these ratios.</t>
   </si>
   <si>
     <t xml:space="preserve">SWE</t>
@@ -1893,7 +1898,7 @@
     <t xml:space="preserve">Thailand - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://ddc.moph.go.th/viralpneumonia/file/situation/situation-no215-050863.pdf</t>
+    <t xml:space="preserve">https://ddc.moph.go.th/viralpneumonia/file/situation/situation-no216-060863n.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">Department of Disease Control</t>
@@ -1911,12 +1916,9 @@
     <t xml:space="preserve">Thailand - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://ddc.moph.go.th/viralpneumonia/file/situation/situation-no214-040863.pdf</t>
-  </si>
-  <si>
     <t xml:space="preserve">The Thailand Department of Disease Control (DDC) issues daily situation reports which detail the status of confirmed cases, deaths and people being assessed.
 We provide the figures reported as "number of laboratory examinations". The reported figures include PCR tests only. It is unclear whether pending test results are included. 
-Prior to 1 July 2020, we collected data from the [World Health Organization Country Office for Thailand](https://www.who.int/thailand), which provides COVID-19 situation reports that periodically report the cumulative number of samples tested to date. The reported figures include samples tested in both public and private labs. However, reporting delays appear to affect the figures. For example, [the figures for 1 May 2020](https://www.who.int/docs/default-source/searo/thailand/2020-05-04-tha-sitrep-71-covid19-final.pdf) reflect only 121 of 142 public and private laboratories certified for PCR testing. The earliest figure we have found is for 10 April 2020, at which point 100,498 samples had been tested. The reported figures are cumulative, but the situation reports do not state an exact date.
+Prior to 1 July 2020, we collected data from the [World Health Organization Country Office for Thailand](https://www.who.int/thailand), which provides COVID-19 situation reports that periodically report the cumulative number of samples tested to date. The reported figures include samples tested in both public and private labs. However, reporting delays appear to affect the figures. For example, [the figures for 1 May 2020](https://www.who.int/docs/default-source/searo/thailand/2020-05-04-tha-sitrep-71-covid19-final.pdf) reflect only 121 of 142 public and private laboratories certified for PCR testing. The earliest figure we have found is for 10 April 2020, at which point 100,498 samples had been tested. The reported figures are cumulative, but the situation reports do not state an exact reference date.
 Note that, due to the way the data is presented by the official source, the time series may be impacted by retrospective revisions made by the source – see our [FAQ here](https://ourworldindata.org/coronavirus-testing#does-your-data-reflect-retrospective-updates-made-by-the-source).</t>
   </si>
   <si>
@@ -1984,7 +1986,7 @@
     <t xml:space="preserve">Uganda - samples tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/MinofHealthUG/status/1290952941759864835/photo/1</t>
+    <t xml:space="preserve">https://twitter.com/MinofHealthUG/status/1291296042483318784/photo/1</t>
   </si>
   <si>
     <t xml:space="preserve">Uganda Ministry of Health</t>
@@ -2013,10 +2015,10 @@
     <t xml:space="preserve">https://www.kmu.gov.ua/en</t>
   </si>
   <si>
-    <t xml:space="preserve">It is unclear whether the reported figures relate to the number of people tested or the number of tests performed.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The Cabinet of Ministers of Ukraine reports daily snapshots [here](https://covid19.gov.ua) that include the cumulative number "tested" (протестовано). As such it is unclear whether this refers to the number of people tested or the number of tests performed. Similarly, it is unclear whether this includes tests pending results.
+    <t xml:space="preserve">The Cabinet of Ministers of Ukraine provides [daily snapshots](https://covid19.gov.ua) that report the cumulative number of tests performed to date. 
+It is unclear whether the reported figures include tests pending results.
+In the daily snapshots, the wording used to report the cumulative testing figures does not make it clear as to whether the reported figures relate to the number of tests performed or the number of persons tested. For example, the cumulative testing figure reported on 6 August 2020 is "1,116,641 tested" (translated from "протестовано"). The [english version](https://covid19.gov.ua/en) of the same page reports the same figure as "total of tests", which is also unclear. [A more detailed dashboard](https://covid19.gov.ua/analitichni-paneli-dashbordy) on the same web domain provides testing figures in downloadable csv files dating back to 1 June 2020, where each csv file contains separate columns for the cumulative number of PCR tests and non-PCR tests. The cumulative PCR testing figures reported in these csv files are described as "The number of laboratory tests performed by PCR on COVID-19" ("Кількість проведених лабораторних досліджень методом ПЛР на COVID-19"), making it clear that the figures refer to the number of tests performed (which may or may not be equivalent to the number of people tested).
+The cumulative PCR testing figures provided in the csv files tend to be approximately 2% smaller than the testing figures provided in the daily snapshots. Nevertheless, we assume that this discrepancy is due to small differences in the reference date, reporting laboratories included, or other minor details, rather than the possibility that the daily snapshot figures include non-PCR tests or refer to a metric other than the number of tests performed. The cumulative number of non-PCR tests reported in the csv files are much larger than the size of this discrepancy.
 The earliest reported figure that we have been able to find is from 9 April 2020, at which point 20,608 cumulative tests were reported.
 Note that, due to the way the data is presented by the official source, the time series may be impacted by retrospective revisions made by the source – see our [FAQ here](https://ourworldindata.org/coronavirus-testing#does-your-data-reflect-retrospective-updates-made-by-the-source).</t>
   </si>
@@ -2044,7 +2046,7 @@
     <t xml:space="preserve">United Kingdom - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://assets.publishing.service.gov.uk/government/uploads/system/uploads/attachment_data/file/907127/2020-08-05_COVID-19_UK_testing_time_series.csv</t>
+    <t xml:space="preserve">https://assets.publishing.service.gov.uk/government/uploads/system/uploads/attachment_data/file/907557/2020-08-06_COVID-19_UK_testing_time_series.csv</t>
   </si>
   <si>
     <t xml:space="preserve">Public Health England/Department of Health and Social Care</t>
@@ -2582,7 +2584,7 @@
         <v>20</v>
       </c>
       <c r="C2" s="1" t="n">
-        <v>44048</v>
+        <v>44049</v>
       </c>
       <c r="D2" t="s">
         <v>21</v>
@@ -2592,31 +2594,31 @@
       </c>
       <c r="F2"/>
       <c r="G2" t="n">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="H2" t="n">
-        <v>671066</v>
+        <v>686800</v>
       </c>
       <c r="I2" t="n">
-        <v>14.848</v>
+        <v>15.196</v>
       </c>
       <c r="J2" t="n">
-        <v>4454</v>
+        <v>4566</v>
       </c>
       <c r="K2" t="n">
-        <v>0.099</v>
+        <v>0.101</v>
       </c>
       <c r="L2" t="n">
-        <v>10525</v>
+        <v>10804</v>
       </c>
       <c r="M2" t="n">
-        <v>0.233</v>
+        <v>0.239</v>
       </c>
       <c r="N2" t="n">
-        <v>0.534</v>
+        <v>0.531</v>
       </c>
       <c r="O2" t="n">
-        <v>1.873</v>
+        <v>1.882</v>
       </c>
       <c r="P2" t="s">
         <v>22</v>
@@ -2639,7 +2641,7 @@
         <v>25</v>
       </c>
       <c r="C3" s="1" t="n">
-        <v>44048</v>
+        <v>44049</v>
       </c>
       <c r="D3" t="s">
         <v>26</v>
@@ -2649,31 +2651,31 @@
       </c>
       <c r="F3"/>
       <c r="G3" t="n">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="H3" t="n">
-        <v>821034</v>
+        <v>839717</v>
       </c>
       <c r="I3" t="n">
-        <v>18.166</v>
+        <v>18.58</v>
       </c>
       <c r="J3" t="n">
-        <v>6009</v>
+        <v>6086</v>
       </c>
       <c r="K3" t="n">
-        <v>0.133</v>
+        <v>0.135</v>
       </c>
       <c r="L3" t="n">
-        <v>12517</v>
+        <v>12822</v>
       </c>
       <c r="M3" t="n">
-        <v>0.277</v>
+        <v>0.284</v>
       </c>
       <c r="N3" t="n">
-        <v>0.449</v>
+        <v>0.448</v>
       </c>
       <c r="O3" t="n">
-        <v>2.228</v>
+        <v>2.234</v>
       </c>
       <c r="P3" t="s">
         <v>22</v>
@@ -2696,7 +2698,7 @@
         <v>30</v>
       </c>
       <c r="C4" s="1" t="n">
-        <v>44048</v>
+        <v>44049</v>
       </c>
       <c r="D4" t="s">
         <v>31</v>
@@ -2706,31 +2708,31 @@
       </c>
       <c r="F4"/>
       <c r="G4" t="n">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="H4" t="n">
-        <v>4552081</v>
+        <v>4632089</v>
       </c>
       <c r="I4" t="n">
-        <v>178.514</v>
+        <v>181.651</v>
       </c>
       <c r="J4" t="n">
-        <v>70464</v>
+        <v>80008</v>
       </c>
       <c r="K4" t="n">
-        <v>2.763</v>
+        <v>3.138</v>
       </c>
       <c r="L4" t="n">
-        <v>60104</v>
+        <v>66805</v>
       </c>
       <c r="M4" t="n">
-        <v>2.357</v>
+        <v>2.62</v>
       </c>
       <c r="N4" t="n">
         <v>0.008</v>
       </c>
       <c r="O4" t="n">
-        <v>122.84</v>
+        <v>121.086</v>
       </c>
       <c r="P4" t="s">
         <v>32</v>
@@ -2753,7 +2755,7 @@
         <v>36</v>
       </c>
       <c r="C5" s="1" t="n">
-        <v>44049</v>
+        <v>44050</v>
       </c>
       <c r="D5" t="s">
         <v>37</v>
@@ -2763,27 +2765,31 @@
       </c>
       <c r="F5"/>
       <c r="G5" t="n">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="H5" t="n">
-        <v>937275</v>
+        <v>947305</v>
       </c>
       <c r="I5" t="n">
-        <v>104.068</v>
-      </c>
-      <c r="J5"/>
-      <c r="K5"/>
+        <v>105.181</v>
+      </c>
+      <c r="J5" t="n">
+        <v>10030</v>
+      </c>
+      <c r="K5" t="n">
+        <v>1.114</v>
+      </c>
       <c r="L5" t="n">
-        <v>6688</v>
+        <v>7069</v>
       </c>
       <c r="M5" t="n">
-        <v>0.743</v>
+        <v>0.785</v>
       </c>
       <c r="N5" t="n">
-        <v>0.016</v>
+        <v>0.014</v>
       </c>
       <c r="O5" t="n">
-        <v>64.219</v>
+        <v>72.769</v>
       </c>
       <c r="P5" t="s">
         <v>39</v>
@@ -2806,7 +2812,7 @@
         <v>43</v>
       </c>
       <c r="C6" s="1" t="n">
-        <v>44049</v>
+        <v>44050</v>
       </c>
       <c r="D6" t="s">
         <v>44</v>
@@ -2816,27 +2822,31 @@
       </c>
       <c r="F6"/>
       <c r="G6" t="n">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="H6" t="n">
-        <v>867534</v>
+        <v>876700</v>
       </c>
       <c r="I6" t="n">
-        <v>509.839</v>
-      </c>
-      <c r="J6"/>
-      <c r="K6"/>
+        <v>515.226</v>
+      </c>
+      <c r="J6" t="n">
+        <v>9166</v>
+      </c>
+      <c r="K6" t="n">
+        <v>5.387</v>
+      </c>
       <c r="L6" t="n">
-        <v>5837</v>
+        <v>6529</v>
       </c>
       <c r="M6" t="n">
-        <v>3.43</v>
+        <v>3.837</v>
       </c>
       <c r="N6" t="n">
-        <v>0.054</v>
+        <v>0.047</v>
       </c>
       <c r="O6" t="n">
-        <v>18.547</v>
+        <v>21.417</v>
       </c>
       <c r="P6" t="s">
         <v>46</v>
@@ -2916,7 +2926,7 @@
         <v>57</v>
       </c>
       <c r="C8" s="1" t="n">
-        <v>44047</v>
+        <v>44049</v>
       </c>
       <c r="D8" t="s">
         <v>58</v>
@@ -2926,27 +2936,27 @@
       </c>
       <c r="F8"/>
       <c r="G8" t="n">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="H8" t="n">
-        <v>1325776</v>
+        <v>1344303</v>
       </c>
       <c r="I8" t="n">
-        <v>140.304</v>
+        <v>142.265</v>
       </c>
       <c r="J8"/>
       <c r="K8"/>
       <c r="L8" t="n">
-        <v>8255</v>
+        <v>7960</v>
       </c>
       <c r="M8" t="n">
-        <v>0.874</v>
+        <v>0.842</v>
       </c>
       <c r="N8" t="n">
-        <v>0.016</v>
+        <v>0.015</v>
       </c>
       <c r="O8" t="n">
-        <v>63.153</v>
+        <v>64.942</v>
       </c>
       <c r="P8" t="s">
         <v>59</v>
@@ -2969,7 +2979,7 @@
         <v>63</v>
       </c>
       <c r="C9" s="1" t="n">
-        <v>44047</v>
+        <v>44048</v>
       </c>
       <c r="D9" t="s">
         <v>64</v>
@@ -2979,31 +2989,31 @@
       </c>
       <c r="F9"/>
       <c r="G9" t="n">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="H9" t="n">
-        <v>1766422</v>
+        <v>1791162</v>
       </c>
       <c r="I9" t="n">
-        <v>152.414</v>
+        <v>154.549</v>
       </c>
       <c r="J9" t="n">
-        <v>20716</v>
+        <v>22266</v>
       </c>
       <c r="K9" t="n">
-        <v>1.787</v>
+        <v>1.921</v>
       </c>
       <c r="L9" t="n">
-        <v>20027</v>
+        <v>19948</v>
       </c>
       <c r="M9" t="n">
-        <v>1.728</v>
+        <v>1.721</v>
       </c>
       <c r="N9" t="n">
-        <v>0.025</v>
+        <v>0.027</v>
       </c>
       <c r="O9" t="n">
-        <v>39.247</v>
+        <v>37.526</v>
       </c>
       <c r="P9" t="s">
         <v>65</v>
@@ -3026,7 +3036,7 @@
         <v>69</v>
       </c>
       <c r="C10" s="1" t="n">
-        <v>44045</v>
+        <v>44048</v>
       </c>
       <c r="D10" t="s">
         <v>70</v>
@@ -3036,31 +3046,31 @@
       </c>
       <c r="F10"/>
       <c r="G10" t="n">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="H10" t="n">
-        <v>156924</v>
+        <v>166104</v>
       </c>
       <c r="I10" t="n">
-        <v>13.443</v>
+        <v>14.23</v>
       </c>
       <c r="J10" t="n">
-        <v>2970</v>
+        <v>3443</v>
       </c>
       <c r="K10" t="n">
-        <v>0.254</v>
+        <v>0.295</v>
       </c>
       <c r="L10" t="n">
-        <v>2857</v>
+        <v>3136</v>
       </c>
       <c r="M10" t="n">
-        <v>0.245</v>
+        <v>0.269</v>
       </c>
       <c r="N10" t="n">
-        <v>0.526</v>
+        <v>0.503</v>
       </c>
       <c r="O10" t="n">
-        <v>1.902</v>
+        <v>1.989</v>
       </c>
       <c r="P10" t="s">
         <v>45</v>
@@ -3134,7 +3144,7 @@
         <v>82</v>
       </c>
       <c r="C12" s="1" t="n">
-        <v>44049</v>
+        <v>44050</v>
       </c>
       <c r="D12" t="s">
         <v>83</v>
@@ -3144,27 +3154,31 @@
       </c>
       <c r="F12"/>
       <c r="G12" t="n">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="H12" t="n">
-        <v>287654</v>
+        <v>294087</v>
       </c>
       <c r="I12" t="n">
-        <v>41.398</v>
-      </c>
-      <c r="J12"/>
-      <c r="K12"/>
+        <v>42.324</v>
+      </c>
+      <c r="J12" t="n">
+        <v>6433</v>
+      </c>
+      <c r="K12" t="n">
+        <v>0.926</v>
+      </c>
       <c r="L12" t="n">
-        <v>3742</v>
+        <v>3863</v>
       </c>
       <c r="M12" t="n">
-        <v>0.539</v>
+        <v>0.556</v>
       </c>
       <c r="N12" t="n">
         <v>0.048</v>
       </c>
       <c r="O12" t="n">
-        <v>20.805</v>
+        <v>20.849</v>
       </c>
       <c r="P12" t="s">
         <v>85</v>
@@ -3187,7 +3201,7 @@
         <v>88</v>
       </c>
       <c r="C13" s="1" t="n">
-        <v>44049</v>
+        <v>44050</v>
       </c>
       <c r="D13" t="s">
         <v>89</v>
@@ -3197,27 +3211,31 @@
       </c>
       <c r="F13"/>
       <c r="G13" t="n">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="H13" t="n">
-        <v>4272606</v>
+        <v>4319172</v>
       </c>
       <c r="I13" t="n">
-        <v>113.205</v>
-      </c>
-      <c r="J13"/>
-      <c r="K13"/>
+        <v>114.439</v>
+      </c>
+      <c r="J13" t="n">
+        <v>46566</v>
+      </c>
+      <c r="K13" t="n">
+        <v>1.234</v>
+      </c>
       <c r="L13" t="n">
-        <v>39426</v>
+        <v>38402</v>
       </c>
       <c r="M13" t="n">
-        <v>1.045</v>
+        <v>1.017</v>
       </c>
       <c r="N13" t="n">
         <v>0.01</v>
       </c>
       <c r="O13" t="n">
-        <v>101.613</v>
+        <v>97.361</v>
       </c>
       <c r="P13" t="s">
         <v>90</v>
@@ -3240,7 +3258,7 @@
         <v>93</v>
       </c>
       <c r="C14" s="1" t="n">
-        <v>44048</v>
+        <v>44049</v>
       </c>
       <c r="D14" t="s">
         <v>94</v>
@@ -3252,31 +3270,31 @@
         <v>95</v>
       </c>
       <c r="G14" t="n">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="H14" t="n">
-        <v>1737813</v>
+        <v>1760615</v>
       </c>
       <c r="I14" t="n">
-        <v>90.908</v>
+        <v>92.101</v>
       </c>
       <c r="J14" t="n">
-        <v>21398</v>
+        <v>22802</v>
       </c>
       <c r="K14" t="n">
-        <v>1.119</v>
+        <v>1.193</v>
       </c>
       <c r="L14" t="n">
-        <v>22427</v>
+        <v>22785</v>
       </c>
       <c r="M14" t="n">
-        <v>1.173</v>
+        <v>1.192</v>
       </c>
       <c r="N14" t="n">
-        <v>0.084</v>
+        <v>0.082</v>
       </c>
       <c r="O14" t="n">
-        <v>11.927</v>
+        <v>12.131</v>
       </c>
       <c r="P14" t="s">
         <v>96</v>
@@ -3356,7 +3374,7 @@
         <v>106</v>
       </c>
       <c r="C16" s="1" t="n">
-        <v>44047</v>
+        <v>44048</v>
       </c>
       <c r="D16" t="s">
         <v>107</v>
@@ -3366,31 +3384,31 @@
       </c>
       <c r="F16"/>
       <c r="G16" t="n">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="H16" t="n">
-        <v>83540</v>
+        <v>85339</v>
       </c>
       <c r="I16" t="n">
-        <v>16.399</v>
+        <v>16.752</v>
       </c>
       <c r="J16" t="n">
-        <v>1584</v>
+        <v>1799</v>
       </c>
       <c r="K16" t="n">
-        <v>0.311</v>
+        <v>0.353</v>
       </c>
       <c r="L16" t="n">
-        <v>1722</v>
+        <v>1742</v>
       </c>
       <c r="M16" t="n">
-        <v>0.338</v>
+        <v>0.342</v>
       </c>
       <c r="N16" t="n">
-        <v>0.295</v>
+        <v>0.286</v>
       </c>
       <c r="O16" t="n">
-        <v>3.385</v>
+        <v>3.491</v>
       </c>
       <c r="P16" t="s">
         <v>108</v>
@@ -3470,7 +3488,7 @@
         <v>118</v>
       </c>
       <c r="C18" s="1" t="n">
-        <v>44048</v>
+        <v>44050</v>
       </c>
       <c r="D18" t="s">
         <v>119</v>
@@ -3480,31 +3498,31 @@
       </c>
       <c r="F18"/>
       <c r="G18" t="n">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="H18" t="n">
-        <v>124383</v>
+        <v>126410</v>
       </c>
       <c r="I18" t="n">
-        <v>30.298</v>
+        <v>30.792</v>
       </c>
       <c r="J18" t="n">
-        <v>1184</v>
+        <v>1093</v>
       </c>
       <c r="K18" t="n">
-        <v>0.288</v>
+        <v>0.266</v>
       </c>
       <c r="L18" t="n">
-        <v>1237</v>
+        <v>1065</v>
       </c>
       <c r="M18" t="n">
-        <v>0.301</v>
+        <v>0.259</v>
       </c>
       <c r="N18" t="n">
-        <v>0.046</v>
+        <v>0.045</v>
       </c>
       <c r="O18" t="n">
-        <v>21.922</v>
+        <v>22.387</v>
       </c>
       <c r="P18" t="s">
         <v>120</v>
@@ -3527,7 +3545,7 @@
         <v>124</v>
       </c>
       <c r="C19" s="1" t="n">
-        <v>44047</v>
+        <v>44048</v>
       </c>
       <c r="D19" t="s">
         <v>125</v>
@@ -3539,31 +3557,31 @@
         <v>127</v>
       </c>
       <c r="G19" t="n">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="H19" t="n">
-        <v>281595</v>
+        <v>285471</v>
       </c>
       <c r="I19" t="n">
-        <v>24.861</v>
+        <v>25.204</v>
       </c>
       <c r="J19" t="n">
-        <v>3732</v>
+        <v>3876</v>
       </c>
       <c r="K19" t="n">
-        <v>0.329</v>
+        <v>0.342</v>
       </c>
       <c r="L19" t="n">
-        <v>3514</v>
+        <v>3574</v>
       </c>
       <c r="M19" t="n">
-        <v>0.31</v>
+        <v>0.316</v>
       </c>
       <c r="N19" t="n">
         <v>0.006</v>
       </c>
       <c r="O19" t="n">
-        <v>178.246</v>
+        <v>171.356</v>
       </c>
       <c r="P19" t="s">
         <v>126</v>
@@ -3586,7 +3604,7 @@
         <v>131</v>
       </c>
       <c r="C20" s="1" t="n">
-        <v>44047</v>
+        <v>44048</v>
       </c>
       <c r="D20" t="s">
         <v>132</v>
@@ -3596,31 +3614,31 @@
       </c>
       <c r="F20"/>
       <c r="G20" t="n">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="H20" t="n">
-        <v>722003</v>
+        <v>728670</v>
       </c>
       <c r="I20" t="n">
-        <v>67.42</v>
+        <v>68.043</v>
       </c>
       <c r="J20" t="n">
-        <v>8040</v>
+        <v>6575</v>
       </c>
       <c r="K20" t="n">
-        <v>0.751</v>
+        <v>0.614</v>
       </c>
       <c r="L20" t="n">
-        <v>6525</v>
+        <v>6434</v>
       </c>
       <c r="M20" t="n">
-        <v>0.609</v>
+        <v>0.601</v>
       </c>
       <c r="N20" t="n">
         <v>0.033</v>
       </c>
       <c r="O20" t="n">
-        <v>30.613</v>
+        <v>30.288</v>
       </c>
       <c r="P20" t="s">
         <v>45</v>
@@ -3643,7 +3661,7 @@
         <v>136</v>
       </c>
       <c r="C21" s="1" t="n">
-        <v>44045</v>
+        <v>44048</v>
       </c>
       <c r="D21" t="s">
         <v>137</v>
@@ -3653,27 +3671,27 @@
       </c>
       <c r="F21"/>
       <c r="G21" t="n">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="H21"/>
       <c r="I21"/>
       <c r="J21" t="n">
-        <v>237</v>
+        <v>489</v>
       </c>
       <c r="K21" t="n">
-        <v>0.003</v>
+        <v>0.005</v>
       </c>
       <c r="L21" t="n">
-        <v>347</v>
+        <v>367</v>
       </c>
       <c r="M21" t="n">
         <v>0.004</v>
       </c>
       <c r="N21" t="n">
-        <v>0.117</v>
+        <v>0.118</v>
       </c>
       <c r="O21" t="n">
-        <v>8.583</v>
+        <v>8.451</v>
       </c>
       <c r="P21" t="s">
         <v>138</v>
@@ -3696,7 +3714,7 @@
         <v>142</v>
       </c>
       <c r="C22" s="1" t="n">
-        <v>44047</v>
+        <v>44049</v>
       </c>
       <c r="D22" t="s">
         <v>143</v>
@@ -3706,31 +3724,31 @@
       </c>
       <c r="F22"/>
       <c r="G22" t="n">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="H22" t="n">
-        <v>1598560</v>
+        <v>1648030</v>
       </c>
       <c r="I22" t="n">
-        <v>275.985</v>
+        <v>284.526</v>
       </c>
       <c r="J22" t="n">
-        <v>5030</v>
+        <v>5406</v>
       </c>
       <c r="K22" t="n">
-        <v>0.868</v>
+        <v>0.933</v>
       </c>
       <c r="L22" t="n">
-        <v>16896</v>
+        <v>18141</v>
       </c>
       <c r="M22" t="n">
-        <v>2.917</v>
+        <v>3.132</v>
       </c>
       <c r="N22" t="n">
         <v>0.004</v>
       </c>
       <c r="O22" t="n">
-        <v>263.412</v>
+        <v>230.466</v>
       </c>
       <c r="P22" t="s">
         <v>144</v>
@@ -3865,7 +3883,7 @@
         <v>162</v>
       </c>
       <c r="C25" s="1" t="n">
-        <v>44047</v>
+        <v>44049</v>
       </c>
       <c r="D25" t="s">
         <v>163</v>
@@ -3875,13 +3893,13 @@
       </c>
       <c r="F25"/>
       <c r="G25" t="n">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="H25" t="n">
-        <v>121946</v>
+        <v>123839</v>
       </c>
       <c r="I25" t="n">
-        <v>91.928</v>
+        <v>93.355</v>
       </c>
       <c r="J25" t="n">
         <v>961</v>
@@ -3890,16 +3908,16 @@
         <v>0.724</v>
       </c>
       <c r="L25" t="n">
-        <v>590</v>
+        <v>663</v>
       </c>
       <c r="M25" t="n">
-        <v>0.445</v>
+        <v>0.5</v>
       </c>
       <c r="N25" t="n">
-        <v>0.01</v>
+        <v>0.015</v>
       </c>
       <c r="O25" t="n">
-        <v>98.333</v>
+        <v>65.366</v>
       </c>
       <c r="P25" t="s">
         <v>165</v>
@@ -4026,7 +4044,7 @@
         <v>181</v>
       </c>
       <c r="C28" s="1" t="n">
-        <v>44047</v>
+        <v>44048</v>
       </c>
       <c r="D28" t="s">
         <v>182</v>
@@ -4036,31 +4054,31 @@
       </c>
       <c r="F28"/>
       <c r="G28" t="n">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="H28" t="n">
-        <v>389288</v>
+        <v>398287</v>
       </c>
       <c r="I28" t="n">
-        <v>70.259</v>
+        <v>71.884</v>
       </c>
       <c r="J28" t="n">
-        <v>3885</v>
+        <v>6998</v>
       </c>
       <c r="K28" t="n">
-        <v>0.701</v>
+        <v>1.263</v>
       </c>
       <c r="L28" t="n">
-        <v>4740</v>
+        <v>5284</v>
       </c>
       <c r="M28" t="n">
-        <v>0.855</v>
+        <v>0.954</v>
       </c>
       <c r="N28" t="n">
         <v>0.002</v>
       </c>
       <c r="O28" t="n">
-        <v>487.941</v>
+        <v>468.203</v>
       </c>
       <c r="P28" t="s">
         <v>184</v>
@@ -4083,7 +4101,7 @@
         <v>187</v>
       </c>
       <c r="C29" s="1" t="n">
-        <v>44044</v>
+        <v>44046</v>
       </c>
       <c r="D29" t="s">
         <v>188</v>
@@ -4093,27 +4111,27 @@
       </c>
       <c r="F29"/>
       <c r="G29" t="n">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="H29"/>
       <c r="I29"/>
       <c r="J29" t="n">
-        <v>41090</v>
+        <v>94697</v>
       </c>
       <c r="K29" t="n">
-        <v>0.63</v>
+        <v>1.451</v>
       </c>
       <c r="L29" t="n">
-        <v>75058</v>
+        <v>75886</v>
       </c>
       <c r="M29" t="n">
-        <v>1.15</v>
+        <v>1.163</v>
       </c>
       <c r="N29" t="n">
         <v>0.014</v>
       </c>
       <c r="O29" t="n">
-        <v>71.087</v>
+        <v>71.871</v>
       </c>
       <c r="P29" t="s">
         <v>189</v>
@@ -4246,7 +4264,7 @@
         <v>205</v>
       </c>
       <c r="C32" s="1" t="n">
-        <v>44045</v>
+        <v>44046</v>
       </c>
       <c r="D32" t="s">
         <v>206</v>
@@ -4256,31 +4274,31 @@
       </c>
       <c r="F32"/>
       <c r="G32" t="n">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="H32" t="n">
-        <v>405817</v>
+        <v>407588</v>
       </c>
       <c r="I32" t="n">
-        <v>13.06</v>
+        <v>13.117</v>
       </c>
       <c r="J32" t="n">
-        <v>3253</v>
+        <v>1771</v>
       </c>
       <c r="K32" t="n">
-        <v>0.105</v>
+        <v>0.057</v>
       </c>
       <c r="L32" t="n">
-        <v>3295</v>
+        <v>2893</v>
       </c>
       <c r="M32" t="n">
-        <v>0.106</v>
+        <v>0.093</v>
       </c>
       <c r="N32" t="n">
-        <v>0.224</v>
+        <v>0.2</v>
       </c>
       <c r="O32" t="n">
-        <v>4.467</v>
+        <v>5.006</v>
       </c>
       <c r="P32" t="s">
         <v>208</v>
@@ -4303,7 +4321,7 @@
         <v>213</v>
       </c>
       <c r="C33" s="1" t="n">
-        <v>44047</v>
+        <v>44049</v>
       </c>
       <c r="D33" t="s">
         <v>214</v>
@@ -4313,31 +4331,31 @@
       </c>
       <c r="F33"/>
       <c r="G33" t="n">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="H33" t="n">
-        <v>599709</v>
+        <v>619393</v>
       </c>
       <c r="I33" t="n">
-        <v>57.537</v>
+        <v>59.425</v>
       </c>
       <c r="J33" t="n">
-        <v>34853</v>
+        <v>9810</v>
       </c>
       <c r="K33" t="n">
-        <v>3.344</v>
+        <v>0.941</v>
       </c>
       <c r="L33" t="n">
-        <v>20310</v>
+        <v>14215</v>
       </c>
       <c r="M33" t="n">
-        <v>1.949</v>
+        <v>1.364</v>
       </c>
       <c r="N33" t="n">
-        <v>0.004</v>
+        <v>0.006</v>
       </c>
       <c r="O33" t="n">
-        <v>278.765</v>
+        <v>156.209</v>
       </c>
       <c r="P33" t="s">
         <v>216</v>
@@ -4360,7 +4378,7 @@
         <v>220</v>
       </c>
       <c r="C34" s="1" t="n">
-        <v>44040</v>
+        <v>44047</v>
       </c>
       <c r="D34" t="s">
         <v>221</v>
@@ -4370,13 +4388,13 @@
       </c>
       <c r="F34"/>
       <c r="G34" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H34" t="n">
-        <v>593962</v>
+        <v>692430</v>
       </c>
       <c r="I34" t="n">
-        <v>79.227</v>
+        <v>92.361</v>
       </c>
       <c r="J34"/>
       <c r="K34"/>
@@ -4464,7 +4482,7 @@
         <v>235</v>
       </c>
       <c r="C36" s="1" t="n">
-        <v>44047</v>
+        <v>44049</v>
       </c>
       <c r="D36" t="s">
         <v>236</v>
@@ -4474,31 +4492,31 @@
       </c>
       <c r="F36"/>
       <c r="G36" t="n">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="H36" t="n">
-        <v>75343</v>
+        <v>77245</v>
       </c>
       <c r="I36" t="n">
-        <v>220.785</v>
+        <v>226.359</v>
       </c>
       <c r="J36" t="n">
-        <v>615</v>
+        <v>1077</v>
       </c>
       <c r="K36" t="n">
-        <v>1.802</v>
+        <v>3.156</v>
       </c>
       <c r="L36" t="n">
-        <v>890</v>
+        <v>948</v>
       </c>
       <c r="M36" t="n">
-        <v>2.608</v>
+        <v>2.778</v>
       </c>
       <c r="N36" t="n">
         <v>0.01</v>
       </c>
       <c r="O36" t="n">
-        <v>102.131</v>
+        <v>102.092</v>
       </c>
       <c r="P36" t="s">
         <v>237</v>
@@ -4580,7 +4598,7 @@
         <v>245</v>
       </c>
       <c r="C38" s="1" t="n">
-        <v>44049</v>
+        <v>44050</v>
       </c>
       <c r="D38" t="s">
         <v>241</v>
@@ -4592,31 +4610,31 @@
         <v>243</v>
       </c>
       <c r="G38" t="n">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="H38" t="n">
-        <v>22149351</v>
+        <v>22788393</v>
       </c>
       <c r="I38" t="n">
-        <v>16.05</v>
+        <v>16.513</v>
       </c>
       <c r="J38" t="n">
-        <v>664949</v>
+        <v>639042</v>
       </c>
       <c r="K38" t="n">
-        <v>0.482</v>
+        <v>0.463</v>
       </c>
       <c r="L38" t="n">
-        <v>565567</v>
+        <v>565060</v>
       </c>
       <c r="M38" t="n">
-        <v>0.41</v>
+        <v>0.409</v>
       </c>
       <c r="N38" t="n">
-        <v>0.096</v>
+        <v>0.098</v>
       </c>
       <c r="O38" t="n">
-        <v>10.398</v>
+        <v>10.189</v>
       </c>
       <c r="P38" t="s">
         <v>242</v>
@@ -4639,7 +4657,7 @@
         <v>247</v>
       </c>
       <c r="C39" s="1" t="n">
-        <v>44048</v>
+        <v>44050</v>
       </c>
       <c r="D39" t="s">
         <v>248</v>
@@ -4649,31 +4667,31 @@
       </c>
       <c r="F39"/>
       <c r="G39" t="n">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="H39" t="n">
-        <v>922709</v>
+        <v>951910</v>
       </c>
       <c r="I39" t="n">
-        <v>3.373</v>
+        <v>3.48</v>
       </c>
       <c r="J39" t="n">
-        <v>14722</v>
+        <v>15599</v>
       </c>
       <c r="K39" t="n">
-        <v>0.054</v>
+        <v>0.057</v>
       </c>
       <c r="L39" t="n">
-        <v>11669</v>
+        <v>12196</v>
       </c>
       <c r="M39" t="n">
-        <v>0.043</v>
+        <v>0.045</v>
       </c>
       <c r="N39" t="n">
-        <v>0.159</v>
+        <v>0.145</v>
       </c>
       <c r="O39" t="n">
-        <v>6.281</v>
+        <v>6.875</v>
       </c>
       <c r="P39" t="s">
         <v>249</v>
@@ -4753,7 +4771,7 @@
         <v>259</v>
       </c>
       <c r="C41" s="1" t="n">
-        <v>44048</v>
+        <v>44049</v>
       </c>
       <c r="D41" t="s">
         <v>260</v>
@@ -4763,31 +4781,31 @@
       </c>
       <c r="F41"/>
       <c r="G41" t="n">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="H41" t="n">
-        <v>648084</v>
+        <v>652917</v>
       </c>
       <c r="I41" t="n">
-        <v>131.25</v>
+        <v>132.228</v>
       </c>
       <c r="J41" t="n">
-        <v>3761</v>
+        <v>4833</v>
       </c>
       <c r="K41" t="n">
-        <v>0.762</v>
+        <v>0.979</v>
       </c>
       <c r="L41" t="n">
-        <v>3353</v>
+        <v>3417</v>
       </c>
       <c r="M41" t="n">
-        <v>0.679</v>
+        <v>0.692</v>
       </c>
       <c r="N41" t="n">
-        <v>0.014</v>
+        <v>0.015</v>
       </c>
       <c r="O41" t="n">
-        <v>72.441</v>
+        <v>66.258</v>
       </c>
       <c r="P41" t="s">
         <v>261</v>
@@ -4867,7 +4885,7 @@
         <v>270</v>
       </c>
       <c r="C43" s="1" t="n">
-        <v>44048</v>
+        <v>44049</v>
       </c>
       <c r="D43" t="s">
         <v>271</v>
@@ -4879,31 +4897,31 @@
         <v>273</v>
       </c>
       <c r="G43" t="n">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="H43" t="n">
-        <v>4184765</v>
+        <v>4216934</v>
       </c>
       <c r="I43" t="n">
-        <v>69.213</v>
+        <v>69.745</v>
       </c>
       <c r="J43" t="n">
-        <v>29739</v>
+        <v>32169</v>
       </c>
       <c r="K43" t="n">
-        <v>0.492</v>
+        <v>0.532</v>
       </c>
       <c r="L43" t="n">
-        <v>26597</v>
+        <v>26422</v>
       </c>
       <c r="M43" t="n">
-        <v>0.44</v>
+        <v>0.437</v>
       </c>
       <c r="N43" t="n">
-        <v>0.01</v>
+        <v>0.011</v>
       </c>
       <c r="O43" t="n">
-        <v>96.416</v>
+        <v>91.245</v>
       </c>
       <c r="P43" t="s">
         <v>274</v>
@@ -4926,7 +4944,7 @@
         <v>277</v>
       </c>
       <c r="C44" s="1" t="n">
-        <v>44048</v>
+        <v>44049</v>
       </c>
       <c r="D44" t="s">
         <v>271</v>
@@ -4938,31 +4956,31 @@
         <v>273</v>
       </c>
       <c r="G44" t="n">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="H44" t="n">
-        <v>7041040</v>
+        <v>7099713</v>
       </c>
       <c r="I44" t="n">
-        <v>116.454</v>
+        <v>117.425</v>
       </c>
       <c r="J44" t="n">
-        <v>56451</v>
+        <v>58673</v>
       </c>
       <c r="K44" t="n">
-        <v>0.934</v>
+        <v>0.97</v>
       </c>
       <c r="L44" t="n">
-        <v>50104</v>
+        <v>49649</v>
       </c>
       <c r="M44" t="n">
-        <v>0.829</v>
+        <v>0.821</v>
       </c>
       <c r="N44" t="n">
         <v>0.006</v>
       </c>
       <c r="O44" t="n">
-        <v>181.63</v>
+        <v>171.457</v>
       </c>
       <c r="P44" t="s">
         <v>274</v>
@@ -4985,7 +5003,7 @@
         <v>280</v>
       </c>
       <c r="C45" s="1" t="n">
-        <v>44048</v>
+        <v>44049</v>
       </c>
       <c r="D45" t="s">
         <v>281</v>
@@ -4997,31 +5015,31 @@
         <v>283</v>
       </c>
       <c r="G45" t="n">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="H45" t="n">
-        <v>897340</v>
+        <v>938739</v>
       </c>
       <c r="I45" t="n">
-        <v>7.095</v>
+        <v>7.422</v>
       </c>
       <c r="J45" t="n">
-        <v>20206</v>
+        <v>41399</v>
       </c>
       <c r="K45" t="n">
-        <v>0.16</v>
+        <v>0.327</v>
       </c>
       <c r="L45" t="n">
-        <v>18856</v>
+        <v>21931</v>
       </c>
       <c r="M45" t="n">
-        <v>0.149</v>
+        <v>0.173</v>
       </c>
       <c r="N45" t="n">
-        <v>0.074</v>
+        <v>0.064</v>
       </c>
       <c r="O45" t="n">
-        <v>13.474</v>
+        <v>15.659</v>
       </c>
       <c r="P45" t="s">
         <v>284</v>
@@ -5044,7 +5062,7 @@
         <v>287</v>
       </c>
       <c r="C46" s="1" t="n">
-        <v>44046</v>
+        <v>44047</v>
       </c>
       <c r="D46" t="s">
         <v>288</v>
@@ -5056,31 +5074,31 @@
         <v>289</v>
       </c>
       <c r="G46" t="n">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="H46" t="n">
-        <v>1174639</v>
+        <v>1205258</v>
       </c>
       <c r="I46" t="n">
-        <v>9.287</v>
+        <v>9.53</v>
       </c>
       <c r="J46" t="n">
-        <v>15849</v>
+        <v>15602</v>
       </c>
       <c r="K46" t="n">
-        <v>0.125</v>
+        <v>0.123</v>
       </c>
       <c r="L46" t="n">
-        <v>19943</v>
+        <v>21090</v>
       </c>
       <c r="M46" t="n">
-        <v>0.158</v>
+        <v>0.167</v>
       </c>
       <c r="N46" t="n">
-        <v>0.058</v>
+        <v>0.067</v>
       </c>
       <c r="O46" t="n">
-        <v>17.271</v>
+        <v>14.959</v>
       </c>
       <c r="P46" t="s">
         <v>284</v>
@@ -5217,7 +5235,7 @@
         <v>303</v>
       </c>
       <c r="C49" s="1" t="n">
-        <v>44046</v>
+        <v>44049</v>
       </c>
       <c r="D49" t="s">
         <v>304</v>
@@ -5227,31 +5245,31 @@
       </c>
       <c r="F49"/>
       <c r="G49" t="n">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="H49" t="n">
-        <v>511599</v>
+        <v>522200</v>
       </c>
       <c r="I49" t="n">
-        <v>119.797</v>
+        <v>122.279</v>
       </c>
       <c r="J49" t="n">
-        <v>2038</v>
+        <v>3599</v>
       </c>
       <c r="K49" t="n">
-        <v>0.477</v>
+        <v>0.843</v>
       </c>
       <c r="L49" t="n">
-        <v>3148</v>
+        <v>2862</v>
       </c>
       <c r="M49" t="n">
-        <v>0.737</v>
+        <v>0.67</v>
       </c>
       <c r="N49" t="n">
-        <v>0.188</v>
+        <v>0.176</v>
       </c>
       <c r="O49" t="n">
-        <v>5.325</v>
+        <v>5.688</v>
       </c>
       <c r="P49" t="s">
         <v>305</v>
@@ -5274,7 +5292,7 @@
         <v>309</v>
       </c>
       <c r="C50" s="1" t="n">
-        <v>44049</v>
+        <v>44050</v>
       </c>
       <c r="D50" t="s">
         <v>310</v>
@@ -5286,31 +5304,31 @@
         <v>312</v>
       </c>
       <c r="G50" t="n">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="H50" t="n">
-        <v>207909</v>
+        <v>210046</v>
       </c>
       <c r="I50" t="n">
-        <v>110.226</v>
+        <v>111.359</v>
       </c>
       <c r="J50" t="n">
-        <v>1829</v>
+        <v>2137</v>
       </c>
       <c r="K50" t="n">
-        <v>0.97</v>
+        <v>1.133</v>
       </c>
       <c r="L50" t="n">
-        <v>1553</v>
+        <v>1648</v>
       </c>
       <c r="M50" t="n">
-        <v>0.823</v>
+        <v>0.874</v>
       </c>
       <c r="N50" t="n">
-        <v>0.003</v>
+        <v>0.004</v>
       </c>
       <c r="O50" t="n">
-        <v>329.424</v>
+        <v>245.447</v>
       </c>
       <c r="P50" t="s">
         <v>311</v>
@@ -5333,7 +5351,7 @@
         <v>315</v>
       </c>
       <c r="C51" s="1" t="n">
-        <v>44049</v>
+        <v>44050</v>
       </c>
       <c r="D51" t="s">
         <v>316</v>
@@ -5343,27 +5361,31 @@
       </c>
       <c r="F51"/>
       <c r="G51" t="n">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="H51" t="n">
-        <v>540784</v>
+        <v>545362</v>
       </c>
       <c r="I51" t="n">
-        <v>198.65</v>
-      </c>
-      <c r="J51"/>
-      <c r="K51"/>
+        <v>200.332</v>
+      </c>
+      <c r="J51" t="n">
+        <v>4578</v>
+      </c>
+      <c r="K51" t="n">
+        <v>1.682</v>
+      </c>
       <c r="L51" t="n">
-        <v>2979</v>
+        <v>3262</v>
       </c>
       <c r="M51" t="n">
-        <v>1.094</v>
+        <v>1.198</v>
       </c>
       <c r="N51" t="n">
         <v>0.005</v>
       </c>
       <c r="O51" t="n">
-        <v>200.51</v>
+        <v>209.486</v>
       </c>
       <c r="P51" t="s">
         <v>45</v>
@@ -5386,7 +5408,7 @@
         <v>319</v>
       </c>
       <c r="C52" s="1" t="n">
-        <v>44047</v>
+        <v>44048</v>
       </c>
       <c r="D52" t="s">
         <v>320</v>
@@ -5396,31 +5418,31 @@
       </c>
       <c r="F52"/>
       <c r="G52" t="n">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="H52" t="n">
-        <v>439318</v>
+        <v>442746</v>
       </c>
       <c r="I52" t="n">
-        <v>701.813</v>
+        <v>707.289</v>
       </c>
       <c r="J52" t="n">
-        <v>3416</v>
+        <v>3428</v>
       </c>
       <c r="K52" t="n">
-        <v>5.457</v>
+        <v>5.476</v>
       </c>
       <c r="L52" t="n">
-        <v>3287</v>
+        <v>3212</v>
       </c>
       <c r="M52" t="n">
-        <v>5.251</v>
+        <v>5.131</v>
       </c>
       <c r="N52" t="n">
         <v>0.024</v>
       </c>
       <c r="O52" t="n">
-        <v>42.374</v>
+        <v>41.483</v>
       </c>
       <c r="P52" t="s">
         <v>321</v>
@@ -5443,7 +5465,7 @@
         <v>324</v>
       </c>
       <c r="C53" s="1" t="n">
-        <v>44048</v>
+        <v>44049</v>
       </c>
       <c r="D53" t="s">
         <v>325</v>
@@ -5455,31 +5477,31 @@
         <v>327</v>
       </c>
       <c r="G53" t="n">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="H53" t="n">
-        <v>1001090</v>
+        <v>1012660</v>
       </c>
       <c r="I53" t="n">
-        <v>30.93</v>
+        <v>31.288</v>
       </c>
       <c r="J53" t="n">
-        <v>9757</v>
+        <v>11570</v>
       </c>
       <c r="K53" t="n">
-        <v>0.301</v>
+        <v>0.357</v>
       </c>
       <c r="L53" t="n">
-        <v>6565</v>
+        <v>7083</v>
       </c>
       <c r="M53" t="n">
-        <v>0.203</v>
+        <v>0.219</v>
       </c>
       <c r="N53" t="n">
         <v>0.001</v>
       </c>
       <c r="O53" t="n">
-        <v>778.898</v>
+        <v>740.015</v>
       </c>
       <c r="P53" t="s">
         <v>45</v>
@@ -5502,7 +5524,7 @@
         <v>331</v>
       </c>
       <c r="C54" s="1" t="n">
-        <v>44046</v>
+        <v>44049</v>
       </c>
       <c r="D54" t="s">
         <v>332</v>
@@ -5512,31 +5534,31 @@
       </c>
       <c r="F54"/>
       <c r="G54" t="n">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="H54" t="n">
-        <v>82208</v>
+        <v>85587</v>
       </c>
       <c r="I54" t="n">
-        <v>152.084</v>
+        <v>158.336</v>
       </c>
       <c r="J54" t="n">
-        <v>1209</v>
+        <v>1443</v>
       </c>
       <c r="K54" t="n">
-        <v>2.237</v>
+        <v>2.67</v>
       </c>
       <c r="L54" t="n">
-        <v>1157</v>
+        <v>1078</v>
       </c>
       <c r="M54" t="n">
-        <v>2.14</v>
+        <v>1.994</v>
       </c>
       <c r="N54" t="n">
-        <v>0.106</v>
+        <v>0.136</v>
       </c>
       <c r="O54" t="n">
-        <v>9.396</v>
+        <v>7.348</v>
       </c>
       <c r="P54" t="s">
         <v>334</v>
@@ -5559,7 +5581,7 @@
         <v>338</v>
       </c>
       <c r="C55" s="1" t="n">
-        <v>44041</v>
+        <v>44049</v>
       </c>
       <c r="D55" t="s">
         <v>339</v>
@@ -5569,31 +5591,31 @@
       </c>
       <c r="F55"/>
       <c r="G55" t="n">
-        <v>159</v>
+        <v>167</v>
       </c>
       <c r="H55" t="n">
-        <v>125685</v>
+        <v>138427</v>
       </c>
       <c r="I55" t="n">
-        <v>284.652</v>
+        <v>313.51</v>
       </c>
       <c r="J55" t="n">
-        <v>1722</v>
+        <v>1717</v>
       </c>
       <c r="K55" t="n">
-        <v>3.9</v>
+        <v>3.889</v>
       </c>
       <c r="L55" t="n">
-        <v>1254</v>
+        <v>1633</v>
       </c>
       <c r="M55" t="n">
-        <v>2.84</v>
+        <v>3.698</v>
       </c>
       <c r="N55" t="n">
-        <v>0.004</v>
+        <v>0.011</v>
       </c>
       <c r="O55" t="n">
-        <v>283.161</v>
+        <v>94.471</v>
       </c>
       <c r="P55" t="s">
         <v>340</v>
@@ -5616,7 +5638,7 @@
         <v>344</v>
       </c>
       <c r="C56" s="1" t="n">
-        <v>44045</v>
+        <v>44046</v>
       </c>
       <c r="D56" t="s">
         <v>345</v>
@@ -5626,31 +5648,31 @@
       </c>
       <c r="F56"/>
       <c r="G56" t="n">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="H56" t="n">
-        <v>952323</v>
+        <v>965013</v>
       </c>
       <c r="I56" t="n">
-        <v>7.386</v>
+        <v>7.485</v>
       </c>
       <c r="J56" t="n">
-        <v>1743</v>
+        <v>6053</v>
       </c>
       <c r="K56" t="n">
-        <v>0.014</v>
+        <v>0.047</v>
       </c>
       <c r="L56" t="n">
-        <v>9226</v>
+        <v>8915</v>
       </c>
       <c r="M56" t="n">
-        <v>0.072</v>
+        <v>0.069</v>
       </c>
       <c r="N56" t="n">
-        <v>0.761</v>
+        <v>0.778</v>
       </c>
       <c r="O56" t="n">
-        <v>1.314</v>
+        <v>1.286</v>
       </c>
       <c r="P56" t="s">
         <v>347</v>
@@ -5673,7 +5695,7 @@
         <v>351</v>
       </c>
       <c r="C57" s="1" t="n">
-        <v>44046</v>
+        <v>44049</v>
       </c>
       <c r="D57" t="s">
         <v>352</v>
@@ -5683,31 +5705,31 @@
       </c>
       <c r="F57"/>
       <c r="G57" t="n">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="H57" t="n">
-        <v>1316861</v>
+        <v>1383816</v>
       </c>
       <c r="I57" t="n">
-        <v>35.677</v>
+        <v>37.491</v>
       </c>
       <c r="J57" t="n">
-        <v>21667</v>
+        <v>22266</v>
       </c>
       <c r="K57" t="n">
-        <v>0.587</v>
+        <v>0.603</v>
       </c>
       <c r="L57" t="n">
-        <v>21250</v>
+        <v>21803</v>
       </c>
       <c r="M57" t="n">
-        <v>0.576</v>
+        <v>0.591</v>
       </c>
       <c r="N57" t="n">
-        <v>0.035</v>
+        <v>0.041</v>
       </c>
       <c r="O57" t="n">
-        <v>28.285</v>
+        <v>24.276</v>
       </c>
       <c r="P57" t="s">
         <v>353</v>
@@ -5787,7 +5809,7 @@
         <v>363</v>
       </c>
       <c r="C59" s="1" t="n">
-        <v>44046</v>
+        <v>44049</v>
       </c>
       <c r="D59" t="s">
         <v>364</v>
@@ -5797,31 +5819,31 @@
       </c>
       <c r="F59"/>
       <c r="G59" t="n">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="H59" t="n">
-        <v>398907</v>
+        <v>419575</v>
       </c>
       <c r="I59" t="n">
-        <v>13.691</v>
+        <v>14.4</v>
       </c>
       <c r="J59" t="n">
-        <v>7637</v>
+        <v>6622</v>
       </c>
       <c r="K59" t="n">
-        <v>0.262</v>
+        <v>0.227</v>
       </c>
       <c r="L59" t="n">
-        <v>7376</v>
+        <v>7847</v>
       </c>
       <c r="M59" t="n">
-        <v>0.253</v>
+        <v>0.269</v>
       </c>
       <c r="N59" t="n">
-        <v>0.033</v>
+        <v>0.039</v>
       </c>
       <c r="O59" t="n">
-        <v>30.036</v>
+        <v>25.947</v>
       </c>
       <c r="P59" t="s">
         <v>365</v>
@@ -5897,7 +5919,7 @@
         <v>376</v>
       </c>
       <c r="C61" s="1" t="n">
-        <v>44048</v>
+        <v>44049</v>
       </c>
       <c r="D61" t="s">
         <v>377</v>
@@ -5907,31 +5929,31 @@
       </c>
       <c r="F61"/>
       <c r="G61" t="n">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="H61" t="n">
-        <v>482929</v>
+        <v>486943</v>
       </c>
       <c r="I61" t="n">
-        <v>100.146</v>
+        <v>100.979</v>
       </c>
       <c r="J61" t="n">
-        <v>5020</v>
+        <v>4014</v>
       </c>
       <c r="K61" t="n">
-        <v>1.041</v>
+        <v>0.832</v>
       </c>
       <c r="L61" t="n">
-        <v>2906</v>
+        <v>3125</v>
       </c>
       <c r="M61" t="n">
-        <v>0.603</v>
+        <v>0.648</v>
       </c>
       <c r="N61" t="n">
         <v>0</v>
       </c>
       <c r="O61" t="n">
-        <v>2034.2</v>
+        <v>2430.556</v>
       </c>
       <c r="P61" t="s">
         <v>378</v>
@@ -5954,7 +5976,7 @@
         <v>381</v>
       </c>
       <c r="C62" s="1" t="n">
-        <v>44047</v>
+        <v>44050</v>
       </c>
       <c r="D62" t="s">
         <v>382</v>
@@ -5964,31 +5986,31 @@
       </c>
       <c r="F62"/>
       <c r="G62" t="n">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="H62" t="n">
-        <v>304221</v>
+        <v>310729</v>
       </c>
       <c r="I62" t="n">
-        <v>1.476</v>
+        <v>1.507</v>
       </c>
       <c r="J62" t="n">
-        <v>15088</v>
+        <v>3835</v>
       </c>
       <c r="K62" t="n">
-        <v>0.073</v>
+        <v>0.019</v>
       </c>
       <c r="L62" t="n">
-        <v>4496</v>
+        <v>3978</v>
       </c>
       <c r="M62" t="n">
-        <v>0.022</v>
+        <v>0.019</v>
       </c>
       <c r="N62" t="n">
-        <v>0.094</v>
+        <v>0.092</v>
       </c>
       <c r="O62" t="n">
-        <v>10.672</v>
+        <v>10.899</v>
       </c>
       <c r="P62" t="s">
         <v>383</v>
@@ -6113,7 +6135,7 @@
         <v>401</v>
       </c>
       <c r="C65" s="1" t="n">
-        <v>44049</v>
+        <v>44050</v>
       </c>
       <c r="D65" t="s">
         <v>402</v>
@@ -6123,27 +6145,31 @@
       </c>
       <c r="F65"/>
       <c r="G65" t="n">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="H65" t="n">
-        <v>2058872</v>
+        <v>2079333</v>
       </c>
       <c r="I65" t="n">
-        <v>9.321</v>
-      </c>
-      <c r="J65"/>
-      <c r="K65"/>
+        <v>9.413</v>
+      </c>
+      <c r="J65" t="n">
+        <v>20461</v>
+      </c>
+      <c r="K65" t="n">
+        <v>0.093</v>
+      </c>
       <c r="L65" t="n">
-        <v>12234</v>
+        <v>12518</v>
       </c>
       <c r="M65" t="n">
-        <v>0.055</v>
+        <v>0.057</v>
       </c>
       <c r="N65" t="n">
-        <v>0.052</v>
+        <v>0.05</v>
       </c>
       <c r="O65" t="n">
-        <v>19.197</v>
+        <v>20.19</v>
       </c>
       <c r="P65" t="s">
         <v>403</v>
@@ -6166,7 +6192,7 @@
         <v>406</v>
       </c>
       <c r="C66" s="1" t="n">
-        <v>44045</v>
+        <v>44048</v>
       </c>
       <c r="D66" t="s">
         <v>407</v>
@@ -6176,31 +6202,31 @@
       </c>
       <c r="F66"/>
       <c r="G66" t="n">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="H66" t="n">
-        <v>227309</v>
+        <v>235074</v>
       </c>
       <c r="I66" t="n">
-        <v>52.682</v>
+        <v>54.481</v>
       </c>
       <c r="J66" t="n">
-        <v>3220</v>
+        <v>2557</v>
       </c>
       <c r="K66" t="n">
-        <v>0.746</v>
+        <v>0.593</v>
       </c>
       <c r="L66" t="n">
-        <v>3157</v>
+        <v>2996</v>
       </c>
       <c r="M66" t="n">
-        <v>0.732</v>
+        <v>0.694</v>
       </c>
       <c r="N66" t="n">
-        <v>0.34</v>
+        <v>0.343</v>
       </c>
       <c r="O66" t="n">
-        <v>2.939</v>
+        <v>2.912</v>
       </c>
       <c r="P66" t="s">
         <v>408</v>
@@ -6333,7 +6359,7 @@
         <v>423</v>
       </c>
       <c r="C69" s="1" t="n">
-        <v>44047</v>
+        <v>44049</v>
       </c>
       <c r="D69" t="s">
         <v>424</v>
@@ -6343,398 +6369,402 @@
       </c>
       <c r="F69"/>
       <c r="G69" t="n">
-        <v>113</v>
+        <v>126</v>
       </c>
       <c r="H69" t="n">
-        <v>1534595</v>
+        <v>1591000</v>
       </c>
       <c r="I69" t="n">
-        <v>14.004</v>
+        <v>14.519</v>
       </c>
       <c r="J69" t="n">
-        <v>25188</v>
+        <v>27732</v>
       </c>
       <c r="K69" t="n">
-        <v>0.23</v>
+        <v>0.253</v>
       </c>
       <c r="L69" t="n">
-        <v>29545</v>
+        <v>25521</v>
       </c>
       <c r="M69" t="n">
-        <v>0.27</v>
+        <v>0.233</v>
       </c>
       <c r="N69" t="n">
-        <v>0.117</v>
+        <v>0.171</v>
       </c>
       <c r="O69" t="n">
-        <v>8.514</v>
+        <v>5.858</v>
       </c>
       <c r="P69" t="s">
         <v>222</v>
       </c>
       <c r="Q69" t="s">
-        <v>424</v>
+        <v>426</v>
       </c>
       <c r="R69" t="s">
         <v>23</v>
       </c>
       <c r="S69" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="B70" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="C70" s="1" t="n">
-        <v>44048</v>
+        <v>44049</v>
       </c>
       <c r="D70" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="E70" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="F70"/>
       <c r="G70" t="n">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="H70" t="n">
-        <v>2027951</v>
+        <v>2049229</v>
       </c>
       <c r="I70" t="n">
-        <v>53.583</v>
+        <v>54.146</v>
       </c>
       <c r="J70" t="n">
-        <v>28422</v>
+        <v>21278</v>
       </c>
       <c r="K70" t="n">
-        <v>0.751</v>
+        <v>0.562</v>
       </c>
       <c r="L70" t="n">
-        <v>20126</v>
+        <v>20007</v>
       </c>
       <c r="M70" t="n">
-        <v>0.532</v>
+        <v>0.529</v>
       </c>
       <c r="N70" t="n">
-        <v>0.03</v>
+        <v>0.031</v>
       </c>
       <c r="O70" t="n">
-        <v>33.188</v>
+        <v>32.026</v>
       </c>
       <c r="P70" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="Q70" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="R70" t="s">
         <v>23</v>
       </c>
       <c r="S70" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="B71" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="C71" s="1" t="n">
-        <v>44048</v>
+        <v>44049</v>
       </c>
       <c r="D71" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="E71" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="F71"/>
       <c r="G71" t="n">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="H71" t="n">
-        <v>2374686</v>
+        <v>2403336</v>
       </c>
       <c r="I71" t="n">
-        <v>62.745</v>
+        <v>63.502</v>
       </c>
       <c r="J71" t="n">
-        <v>33647</v>
+        <v>28650</v>
       </c>
       <c r="K71" t="n">
-        <v>0.889</v>
+        <v>0.757</v>
       </c>
       <c r="L71" t="n">
-        <v>26816</v>
+        <v>27614</v>
       </c>
       <c r="M71" t="n">
-        <v>0.709</v>
+        <v>0.73</v>
       </c>
       <c r="N71" t="n">
         <v>0.023</v>
       </c>
       <c r="O71" t="n">
-        <v>44.22</v>
+        <v>44.203</v>
       </c>
       <c r="P71" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="Q71" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="R71" t="s">
         <v>54</v>
       </c>
       <c r="S71" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="B72" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="C72" s="1" t="n">
-        <v>44047</v>
+        <v>44048</v>
       </c>
       <c r="D72" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="E72" t="s">
         <v>45</v>
       </c>
       <c r="F72"/>
       <c r="G72" t="n">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="H72" t="n">
-        <v>1688567</v>
+        <v>1705474</v>
       </c>
       <c r="I72" t="n">
-        <v>165.599</v>
+        <v>167.257</v>
       </c>
       <c r="J72" t="n">
-        <v>17087</v>
+        <v>16864</v>
       </c>
       <c r="K72" t="n">
-        <v>1.676</v>
+        <v>1.654</v>
       </c>
       <c r="L72" t="n">
-        <v>13817</v>
+        <v>13858</v>
       </c>
       <c r="M72" t="n">
-        <v>1.355</v>
+        <v>1.359</v>
       </c>
       <c r="N72" t="n">
         <v>0.013</v>
       </c>
       <c r="O72" t="n">
-        <v>76.157</v>
+        <v>76.323</v>
       </c>
       <c r="P72" t="s">
+        <v>439</v>
+      </c>
+      <c r="Q72" t="s">
         <v>438</v>
       </c>
-      <c r="Q72" t="s">
-        <v>437</v>
-      </c>
       <c r="R72" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="S72" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="B73" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="C73" s="1" t="n">
-        <v>44048</v>
+        <v>44049</v>
       </c>
       <c r="D73" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="E73" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="F73"/>
       <c r="G73" t="n">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="H73" t="n">
-        <v>508079</v>
+        <v>511000</v>
       </c>
       <c r="I73" t="n">
-        <v>176.351</v>
+        <v>177.365</v>
       </c>
       <c r="J73" t="n">
-        <v>2931</v>
+        <v>2921</v>
       </c>
       <c r="K73" t="n">
-        <v>1.017</v>
+        <v>1.014</v>
       </c>
       <c r="L73" t="n">
-        <v>2949</v>
+        <v>2633</v>
       </c>
       <c r="M73" t="n">
-        <v>1.024</v>
+        <v>0.914</v>
       </c>
       <c r="N73" t="n">
-        <v>0.08</v>
+        <v>0.09</v>
       </c>
       <c r="O73" t="n">
-        <v>12.451</v>
+        <v>11.157</v>
       </c>
       <c r="P73" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="Q73" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="R73" t="s">
         <v>23</v>
       </c>
       <c r="S73" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="B74" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="C74" s="1" t="n">
-        <v>44048</v>
+        <v>44050</v>
       </c>
       <c r="D74" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="E74" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="F74"/>
       <c r="G74" t="n">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="H74" t="n">
-        <v>1295222</v>
+        <v>1343315</v>
       </c>
       <c r="I74" t="n">
-        <v>67.327</v>
-      </c>
-      <c r="J74"/>
-      <c r="K74"/>
+        <v>69.827</v>
+      </c>
+      <c r="J74" t="n">
+        <v>23946</v>
+      </c>
+      <c r="K74" t="n">
+        <v>1.245</v>
+      </c>
       <c r="L74" t="n">
-        <v>16799</v>
+        <v>16751</v>
       </c>
       <c r="M74" t="n">
-        <v>0.873</v>
+        <v>0.871</v>
       </c>
       <c r="N74" t="n">
-        <v>0.07</v>
+        <v>0.071</v>
       </c>
       <c r="O74" t="n">
-        <v>14.362</v>
+        <v>14.121</v>
       </c>
       <c r="P74" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="Q74" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="R74" t="s">
         <v>27</v>
       </c>
       <c r="S74" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="B75" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="C75" s="1" t="n">
-        <v>44048</v>
+        <v>44049</v>
       </c>
       <c r="D75" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="E75" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="F75"/>
       <c r="G75" t="n">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="H75" t="n">
-        <v>29716907</v>
+        <v>30038123</v>
       </c>
       <c r="I75" t="n">
-        <v>203.632</v>
+        <v>205.833</v>
       </c>
       <c r="J75" t="n">
-        <v>283017</v>
+        <v>321216</v>
       </c>
       <c r="K75" t="n">
-        <v>1.939</v>
+        <v>2.201</v>
       </c>
       <c r="L75" t="n">
-        <v>265580</v>
+        <v>268095</v>
       </c>
       <c r="M75" t="n">
-        <v>1.82</v>
+        <v>1.837</v>
       </c>
       <c r="N75" t="n">
         <v>0.02</v>
       </c>
       <c r="O75" t="n">
-        <v>49.041</v>
+        <v>48.931</v>
       </c>
       <c r="P75" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="Q75" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="R75" t="s">
         <v>27</v>
       </c>
       <c r="S75" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="B76" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="C76" s="1" t="n">
         <v>44046</v>
       </c>
       <c r="D76" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="E76" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="F76"/>
       <c r="G76" t="n">
@@ -6765,205 +6795,205 @@
         <v>112.407</v>
       </c>
       <c r="P76" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="Q76" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="R76" t="s">
         <v>54</v>
       </c>
       <c r="S76" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="B77" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="C77" s="1" t="n">
-        <v>44048</v>
+        <v>44049</v>
       </c>
       <c r="D77" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="E77" t="s">
         <v>45</v>
       </c>
       <c r="F77"/>
       <c r="G77" t="n">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="H77" t="n">
-        <v>3570851</v>
+        <v>3626417</v>
       </c>
       <c r="I77" t="n">
-        <v>102.57</v>
+        <v>104.166</v>
       </c>
       <c r="J77" t="n">
-        <v>52099</v>
+        <v>55566</v>
       </c>
       <c r="K77" t="n">
-        <v>1.497</v>
+        <v>1.596</v>
       </c>
       <c r="L77" t="n">
-        <v>48915</v>
+        <v>49430</v>
       </c>
       <c r="M77" t="n">
-        <v>1.405</v>
+        <v>1.42</v>
       </c>
       <c r="N77" t="n">
-        <v>0.031</v>
+        <v>0.03</v>
       </c>
       <c r="O77" t="n">
-        <v>32.29</v>
+        <v>33.81</v>
       </c>
       <c r="P77" t="s">
         <v>45</v>
       </c>
       <c r="Q77" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="R77" t="s">
         <v>27</v>
       </c>
       <c r="S77" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="B78" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="C78" s="1" t="n">
-        <v>44048</v>
+        <v>44049</v>
       </c>
       <c r="D78" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="E78" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="F78" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="G78" t="n">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="H78" t="n">
-        <v>115891</v>
+        <v>117808</v>
       </c>
       <c r="I78" t="n">
-        <v>6.921</v>
+        <v>7.036</v>
       </c>
       <c r="J78" t="n">
-        <v>1241</v>
+        <v>1917</v>
       </c>
       <c r="K78" t="n">
-        <v>0.074</v>
+        <v>0.114</v>
       </c>
       <c r="L78" t="n">
-        <v>1136</v>
+        <v>1189</v>
       </c>
       <c r="M78" t="n">
-        <v>0.068</v>
+        <v>0.071</v>
       </c>
       <c r="N78" t="n">
-        <v>0.079</v>
+        <v>0.069</v>
       </c>
       <c r="O78" t="n">
-        <v>12.683</v>
+        <v>14.425</v>
       </c>
       <c r="P78" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="Q78" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="R78" t="s">
         <v>27</v>
       </c>
       <c r="S78" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="B79" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="C79" s="1" t="n">
-        <v>44048</v>
+        <v>44049</v>
       </c>
       <c r="D79" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="E79" t="s">
         <v>45</v>
       </c>
       <c r="F79" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="G79" t="n">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="H79" t="n">
-        <v>713104</v>
+        <v>723137</v>
       </c>
       <c r="I79" t="n">
-        <v>104.797</v>
+        <v>106.272</v>
       </c>
       <c r="J79" t="n">
-        <v>9858</v>
+        <v>10033</v>
       </c>
       <c r="K79" t="n">
-        <v>1.449</v>
+        <v>1.474</v>
       </c>
       <c r="L79" t="n">
-        <v>8909</v>
+        <v>9084</v>
       </c>
       <c r="M79" t="n">
-        <v>1.309</v>
+        <v>1.335</v>
       </c>
       <c r="N79" t="n">
-        <v>0.036</v>
+        <v>0.034</v>
       </c>
       <c r="O79" t="n">
-        <v>28.117</v>
+        <v>29.7</v>
       </c>
       <c r="P79" t="s">
         <v>45</v>
       </c>
       <c r="Q79" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
       <c r="R79" t="s">
         <v>23</v>
       </c>
       <c r="S79" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="B80" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
       <c r="C80" s="1" t="n">
         <v>44046</v>
       </c>
       <c r="D80" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="E80" t="s">
         <v>45</v>
@@ -6996,27 +7026,27 @@
         <v>45</v>
       </c>
       <c r="Q80" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="R80" t="s">
         <v>23</v>
       </c>
       <c r="S80" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="B81" t="s">
-        <v>488</v>
+        <v>489</v>
       </c>
       <c r="C81" s="1" t="n">
         <v>44046</v>
       </c>
       <c r="D81" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="E81" t="s">
         <v>45</v>
@@ -7049,260 +7079,260 @@
         <v>45</v>
       </c>
       <c r="Q81" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="R81" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c r="S81" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="B82" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="C82" s="1" t="n">
-        <v>44049</v>
+        <v>44050</v>
       </c>
       <c r="D82" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="E82" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
       <c r="F82"/>
       <c r="G82" t="n">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="H82" t="n">
-        <v>272322</v>
+        <v>274795</v>
       </c>
       <c r="I82" t="n">
-        <v>49.879</v>
+        <v>50.332</v>
       </c>
       <c r="J82" t="n">
-        <v>2667</v>
+        <v>2473</v>
       </c>
       <c r="K82" t="n">
-        <v>0.488</v>
+        <v>0.453</v>
       </c>
       <c r="L82" t="n">
-        <v>1848</v>
+        <v>1890</v>
       </c>
       <c r="M82" t="n">
-        <v>0.338</v>
+        <v>0.346</v>
       </c>
       <c r="N82" t="n">
-        <v>0.013</v>
+        <v>0.016</v>
       </c>
       <c r="O82" t="n">
-        <v>75.209</v>
+        <v>61.535</v>
       </c>
       <c r="P82" t="s">
-        <v>494</v>
+        <v>495</v>
       </c>
       <c r="Q82" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="R82" t="s">
         <v>27</v>
       </c>
       <c r="S82" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="B83" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="C83" s="1" t="n">
-        <v>44048</v>
+        <v>44049</v>
       </c>
       <c r="D83" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="E83" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c r="F83"/>
       <c r="G83" t="n">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="H83" t="n">
-        <v>134334</v>
+        <v>135087</v>
       </c>
       <c r="I83" t="n">
-        <v>64.617</v>
+        <v>64.979</v>
       </c>
       <c r="J83" t="n">
-        <v>771</v>
+        <v>753</v>
       </c>
       <c r="K83" t="n">
-        <v>0.371</v>
+        <v>0.362</v>
       </c>
       <c r="L83" t="n">
-        <v>727</v>
+        <v>704</v>
       </c>
       <c r="M83" t="n">
-        <v>0.35</v>
+        <v>0.339</v>
       </c>
       <c r="N83" t="n">
-        <v>0.017</v>
+        <v>0.019</v>
       </c>
       <c r="O83" t="n">
-        <v>57.18</v>
+        <v>52.989</v>
       </c>
       <c r="P83" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="Q83" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="R83" t="s">
         <v>27</v>
       </c>
       <c r="S83" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
       <c r="B84" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="C84" s="1" t="n">
-        <v>44048</v>
+        <v>44049</v>
       </c>
       <c r="D84" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="E84" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="F84" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="G84" t="n">
         <v>158</v>
       </c>
       <c r="H84" t="n">
-        <v>3113191</v>
+        <v>3149807</v>
       </c>
       <c r="I84" t="n">
-        <v>52.491</v>
+        <v>53.109</v>
       </c>
       <c r="J84" t="n">
-        <v>34989</v>
+        <v>36616</v>
       </c>
       <c r="K84" t="n">
-        <v>0.59</v>
+        <v>0.617</v>
       </c>
       <c r="L84" t="n">
-        <v>34290</v>
+        <v>33108</v>
       </c>
       <c r="M84" t="n">
-        <v>0.578</v>
+        <v>0.558</v>
       </c>
       <c r="N84" t="n">
-        <v>0.256</v>
+        <v>0.254</v>
       </c>
       <c r="O84" t="n">
-        <v>3.899</v>
+        <v>3.945</v>
       </c>
       <c r="P84" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="Q84" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
       <c r="R84" t="s">
         <v>23</v>
       </c>
       <c r="S84" t="s">
-        <v>509</v>
+        <v>510</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
       <c r="B85" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
       <c r="C85" s="1" t="n">
-        <v>44049</v>
+        <v>44050</v>
       </c>
       <c r="D85" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="E85" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
       <c r="F85"/>
       <c r="G85" t="n">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="H85" t="n">
-        <v>1588456</v>
+        <v>1596584</v>
       </c>
       <c r="I85" t="n">
-        <v>30.983</v>
+        <v>31.141</v>
       </c>
       <c r="J85" t="n">
-        <v>8759</v>
+        <v>8128</v>
       </c>
       <c r="K85" t="n">
-        <v>0.171</v>
+        <v>0.159</v>
       </c>
       <c r="L85" t="n">
-        <v>7323</v>
+        <v>7303</v>
       </c>
       <c r="M85" t="n">
-        <v>0.143</v>
+        <v>0.142</v>
       </c>
       <c r="N85" t="n">
         <v>0.004</v>
       </c>
       <c r="O85" t="n">
-        <v>222.874</v>
+        <v>238.883</v>
       </c>
       <c r="P85" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
       <c r="Q85" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="R85" t="s">
         <v>23</v>
       </c>
       <c r="S85" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="B86" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
       <c r="C86" s="1" t="n">
         <v>44042</v>
       </c>
       <c r="D86" t="s">
-        <v>518</v>
+        <v>519</v>
       </c>
       <c r="E86" t="s">
-        <v>519</v>
+        <v>520</v>
       </c>
       <c r="F86"/>
       <c r="G86" t="n">
@@ -7329,33 +7359,33 @@
         <v>20.013</v>
       </c>
       <c r="P86" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="Q86" t="s">
-        <v>521</v>
+        <v>522</v>
       </c>
       <c r="R86" t="s">
         <v>27</v>
       </c>
       <c r="S86" t="s">
-        <v>522</v>
+        <v>523</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
       <c r="B87" t="s">
-        <v>524</v>
+        <v>525</v>
       </c>
       <c r="C87" s="1" t="n">
         <v>44017</v>
       </c>
       <c r="D87" t="s">
-        <v>525</v>
+        <v>526</v>
       </c>
       <c r="E87" t="s">
-        <v>526</v>
+        <v>527</v>
       </c>
       <c r="F87"/>
       <c r="G87" t="n">
@@ -7382,33 +7412,33 @@
         <v>12.36</v>
       </c>
       <c r="P87" t="s">
-        <v>527</v>
+        <v>528</v>
       </c>
       <c r="Q87" t="s">
-        <v>528</v>
+        <v>529</v>
       </c>
       <c r="R87" t="s">
         <v>23</v>
       </c>
       <c r="S87" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
       <c r="B88" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c r="C88" s="1" t="n">
         <v>44045</v>
       </c>
       <c r="D88" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
       <c r="E88" t="s">
-        <v>526</v>
+        <v>527</v>
       </c>
       <c r="F88"/>
       <c r="G88" t="n">
@@ -7435,109 +7465,109 @@
         <v>37.166</v>
       </c>
       <c r="P88" t="s">
-        <v>527</v>
+        <v>528</v>
       </c>
       <c r="Q88" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
       <c r="R88" t="s">
         <v>54</v>
       </c>
       <c r="S88" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="s">
-        <v>533</v>
+        <v>534</v>
       </c>
       <c r="B89" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="C89" s="1" t="n">
-        <v>44047</v>
+        <v>44049</v>
       </c>
       <c r="D89" t="s">
-        <v>535</v>
+        <v>536</v>
       </c>
       <c r="E89" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
       <c r="F89"/>
       <c r="G89" t="n">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="H89" t="n">
-        <v>815937</v>
+        <v>829158</v>
       </c>
       <c r="I89" t="n">
-        <v>94.278</v>
+        <v>95.805</v>
       </c>
       <c r="J89" t="n">
-        <v>5232</v>
+        <v>4483</v>
       </c>
       <c r="K89" t="n">
-        <v>0.605</v>
+        <v>0.518</v>
       </c>
       <c r="L89" t="n">
-        <v>5164</v>
+        <v>5062</v>
       </c>
       <c r="M89" t="n">
-        <v>0.597</v>
+        <v>0.585</v>
       </c>
       <c r="N89" t="n">
-        <v>0.031</v>
+        <v>0.032</v>
       </c>
       <c r="O89" t="n">
-        <v>31.792</v>
+        <v>31.525</v>
       </c>
       <c r="P89" t="s">
+        <v>537</v>
+      </c>
+      <c r="Q89" t="s">
         <v>536</v>
       </c>
-      <c r="Q89" t="s">
-        <v>535</v>
-      </c>
       <c r="R89" t="s">
-        <v>537</v>
+        <v>538</v>
       </c>
       <c r="S89" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
       <c r="B90" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
       <c r="C90" s="1" t="n">
-        <v>44048</v>
+        <v>44049</v>
       </c>
       <c r="D90" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
       <c r="E90" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
       <c r="F90"/>
       <c r="G90" t="n">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="H90" t="n">
-        <v>82737</v>
+        <v>82955</v>
       </c>
       <c r="I90" t="n">
-        <v>3.474</v>
+        <v>3.483</v>
       </c>
       <c r="J90" t="n">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="K90" t="n">
         <v>0.009</v>
       </c>
       <c r="L90" t="n">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="M90" t="n">
         <v>0.008</v>
@@ -7546,127 +7576,127 @@
         <v>0.007</v>
       </c>
       <c r="O90" t="n">
-        <v>150.111</v>
+        <v>136.5</v>
       </c>
       <c r="P90" t="s">
+        <v>543</v>
+      </c>
+      <c r="Q90" t="s">
         <v>542</v>
-      </c>
-      <c r="Q90" t="s">
-        <v>541</v>
       </c>
       <c r="R90" t="s">
         <v>23</v>
       </c>
       <c r="S90" t="s">
-        <v>543</v>
+        <v>544</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="B91" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
       <c r="C91" s="1" t="n">
-        <v>44048</v>
+        <v>44049</v>
       </c>
       <c r="D91" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
       <c r="E91" t="s">
-        <v>547</v>
+        <v>548</v>
       </c>
       <c r="F91"/>
       <c r="G91" t="n">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="H91" t="n">
-        <v>381770</v>
+        <v>383217</v>
       </c>
       <c r="I91" t="n">
-        <v>5.469</v>
+        <v>5.49</v>
       </c>
       <c r="J91" t="n">
-        <v>1140</v>
+        <v>1447</v>
       </c>
       <c r="K91" t="n">
-        <v>0.016</v>
+        <v>0.021</v>
       </c>
       <c r="L91" t="n">
-        <v>1670</v>
+        <v>1508</v>
       </c>
       <c r="M91" t="n">
-        <v>0.024</v>
+        <v>0.022</v>
       </c>
       <c r="N91" t="n">
-        <v>0.003</v>
+        <v>0.002</v>
       </c>
       <c r="O91" t="n">
-        <v>389.667</v>
+        <v>406</v>
       </c>
       <c r="P91" t="s">
-        <v>547</v>
+        <v>548</v>
       </c>
       <c r="Q91" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
       <c r="R91" t="s">
         <v>23</v>
       </c>
       <c r="S91" t="s">
-        <v>549</v>
+        <v>550</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="B92" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="C92" s="1" t="n">
-        <v>44047</v>
+        <v>44049</v>
       </c>
       <c r="D92" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="E92" t="s">
-        <v>547</v>
+        <v>548</v>
       </c>
       <c r="F92"/>
       <c r="G92" t="n">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="H92" t="n">
-        <v>752163</v>
+        <v>754750</v>
       </c>
       <c r="I92" t="n">
-        <v>10.776</v>
+        <v>10.813</v>
       </c>
       <c r="J92" t="n">
-        <v>20714</v>
+        <v>1447</v>
       </c>
       <c r="K92" t="n">
-        <v>0.297</v>
+        <v>0.021</v>
       </c>
       <c r="L92" t="n">
-        <v>7023</v>
+        <v>6756</v>
       </c>
       <c r="M92" t="n">
-        <v>0.101</v>
+        <v>0.097</v>
       </c>
       <c r="N92" t="n">
-        <v>0</v>
+        <v>0.001</v>
       </c>
       <c r="O92" t="n">
-        <v>2048.375</v>
+        <v>1818.923</v>
       </c>
       <c r="P92" t="s">
-        <v>547</v>
+        <v>548</v>
       </c>
       <c r="Q92" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
       <c r="R92" t="s">
         <v>27</v>
@@ -7810,24 +7840,24 @@
         <v>130</v>
       </c>
       <c r="H95" t="n">
-        <v>5027308</v>
+        <v>5081802</v>
       </c>
       <c r="I95" t="n">
-        <v>59.608</v>
+        <v>60.254</v>
       </c>
       <c r="J95"/>
       <c r="K95"/>
       <c r="L95" t="n">
-        <v>32355</v>
+        <v>40140</v>
       </c>
       <c r="M95" t="n">
-        <v>0.384</v>
+        <v>0.476</v>
       </c>
       <c r="N95" t="n">
-        <v>0.032</v>
+        <v>0.026</v>
       </c>
       <c r="O95" t="n">
-        <v>31.509</v>
+        <v>39.09</v>
       </c>
       <c r="P95" t="s">
         <v>567</v>
@@ -7850,7 +7880,7 @@
         <v>570</v>
       </c>
       <c r="C96" s="1" t="n">
-        <v>44047</v>
+        <v>44048</v>
       </c>
       <c r="D96" t="s">
         <v>571</v>
@@ -7860,31 +7890,31 @@
       </c>
       <c r="F96"/>
       <c r="G96" t="n">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="H96" t="n">
-        <v>284790</v>
+        <v>288367</v>
       </c>
       <c r="I96" t="n">
-        <v>6.226</v>
+        <v>6.304</v>
       </c>
       <c r="J96" t="n">
-        <v>2278</v>
+        <v>3577</v>
       </c>
       <c r="K96" t="n">
-        <v>0.05</v>
+        <v>0.078</v>
       </c>
       <c r="L96" t="n">
-        <v>2562</v>
+        <v>2648</v>
       </c>
       <c r="M96" t="n">
-        <v>0.056</v>
+        <v>0.058</v>
       </c>
       <c r="N96" t="n">
         <v>0.004</v>
       </c>
       <c r="O96" t="n">
-        <v>267.672</v>
+        <v>272.588</v>
       </c>
       <c r="P96" t="s">
         <v>572</v>
@@ -7907,7 +7937,7 @@
         <v>576</v>
       </c>
       <c r="C97" s="1" t="n">
-        <v>44049</v>
+        <v>44050</v>
       </c>
       <c r="D97" t="s">
         <v>577</v>
@@ -7917,31 +7947,31 @@
       </c>
       <c r="F97"/>
       <c r="G97" t="n">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="H97" t="n">
-        <v>1116641</v>
+        <v>1135051</v>
       </c>
       <c r="I97" t="n">
-        <v>25.533</v>
+        <v>25.954</v>
       </c>
       <c r="J97" t="n">
-        <v>17976</v>
+        <v>18410</v>
       </c>
       <c r="K97" t="n">
-        <v>0.411</v>
+        <v>0.421</v>
       </c>
       <c r="L97" t="n">
-        <v>14693</v>
+        <v>15119</v>
       </c>
       <c r="M97" t="n">
-        <v>0.336</v>
+        <v>0.346</v>
       </c>
       <c r="N97" t="n">
-        <v>0.077</v>
+        <v>0.076</v>
       </c>
       <c r="O97" t="n">
-        <v>13.031</v>
+        <v>13.206</v>
       </c>
       <c r="P97" t="s">
         <v>578</v>
@@ -7950,250 +7980,254 @@
         <v>579</v>
       </c>
       <c r="R97" t="s">
+        <v>40</v>
+      </c>
+      <c r="S97" t="s">
         <v>580</v>
-      </c>
-      <c r="S97" t="s">
-        <v>581</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="s">
+        <v>581</v>
+      </c>
+      <c r="B98" t="s">
         <v>582</v>
       </c>
-      <c r="B98" t="s">
+      <c r="C98" s="1" t="n">
+        <v>44049</v>
+      </c>
+      <c r="D98" t="s">
         <v>583</v>
       </c>
-      <c r="C98" s="1" t="n">
-        <v>44048</v>
-      </c>
-      <c r="D98" t="s">
+      <c r="E98" t="s">
         <v>584</v>
-      </c>
-      <c r="E98" t="s">
-        <v>585</v>
       </c>
       <c r="F98"/>
       <c r="G98" t="n">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="H98" t="n">
-        <v>5262658</v>
+        <v>5313387</v>
       </c>
       <c r="I98" t="n">
-        <v>532.098</v>
+        <v>537.227</v>
       </c>
       <c r="J98" t="n">
-        <v>43369</v>
+        <v>50729</v>
       </c>
       <c r="K98" t="n">
-        <v>4.385</v>
+        <v>5.129</v>
       </c>
       <c r="L98" t="n">
-        <v>42323</v>
+        <v>41676</v>
       </c>
       <c r="M98" t="n">
-        <v>4.279</v>
+        <v>4.214</v>
       </c>
       <c r="N98" t="n">
         <v>0.006</v>
       </c>
       <c r="O98" t="n">
-        <v>164.043</v>
+        <v>173.135</v>
       </c>
       <c r="P98" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
       <c r="Q98" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="R98" t="s">
         <v>54</v>
       </c>
       <c r="S98" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="s">
+        <v>586</v>
+      </c>
+      <c r="B99" t="s">
         <v>587</v>
       </c>
-      <c r="B99" t="s">
+      <c r="C99" s="1" t="n">
+        <v>44048</v>
+      </c>
+      <c r="D99" t="s">
         <v>588</v>
       </c>
-      <c r="C99" s="1" t="n">
-        <v>44047</v>
-      </c>
-      <c r="D99" t="s">
+      <c r="E99" t="s">
         <v>589</v>
       </c>
-      <c r="E99" t="s">
+      <c r="F99" t="s">
         <v>590</v>
       </c>
-      <c r="F99" t="s">
+      <c r="G99" t="n">
+        <v>128</v>
+      </c>
+      <c r="H99" t="n">
+        <v>10236970</v>
+      </c>
+      <c r="I99" t="n">
+        <v>150.796</v>
+      </c>
+      <c r="J99" t="n">
+        <v>152551</v>
+      </c>
+      <c r="K99" t="n">
+        <v>2.247</v>
+      </c>
+      <c r="L99" t="n">
+        <v>139426</v>
+      </c>
+      <c r="M99" t="n">
+        <v>2.054</v>
+      </c>
+      <c r="N99" t="n">
+        <v>0.006</v>
+      </c>
+      <c r="O99" t="n">
+        <v>174.251</v>
+      </c>
+      <c r="P99" t="s">
+        <v>589</v>
+      </c>
+      <c r="Q99" t="s">
         <v>591</v>
-      </c>
-      <c r="G99" t="n">
-        <v>127</v>
-      </c>
-      <c r="H99" t="n">
-        <v>10083427</v>
-      </c>
-      <c r="I99" t="n">
-        <v>148.535</v>
-      </c>
-      <c r="J99" t="n">
-        <v>140745</v>
-      </c>
-      <c r="K99" t="n">
-        <v>2.073</v>
-      </c>
-      <c r="L99" t="n">
-        <v>137992</v>
-      </c>
-      <c r="M99" t="n">
-        <v>2.033</v>
-      </c>
-      <c r="N99" t="n">
-        <v>0.005</v>
-      </c>
-      <c r="O99" t="n">
-        <v>193.15</v>
-      </c>
-      <c r="P99" t="s">
-        <v>590</v>
-      </c>
-      <c r="Q99" t="s">
-        <v>592</v>
       </c>
       <c r="R99" t="s">
         <v>27</v>
       </c>
       <c r="S99" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="s">
+        <v>593</v>
+      </c>
+      <c r="B100" t="s">
         <v>594</v>
       </c>
-      <c r="B100" t="s">
+      <c r="C100" s="1" t="n">
+        <v>44049</v>
+      </c>
+      <c r="D100" t="s">
         <v>595</v>
       </c>
-      <c r="C100" s="1" t="n">
-        <v>44048</v>
-      </c>
-      <c r="D100" t="s">
+      <c r="E100" t="s">
         <v>596</v>
-      </c>
-      <c r="E100" t="s">
-        <v>597</v>
       </c>
       <c r="F100"/>
       <c r="G100" t="n">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="H100" t="n">
-        <v>63537614</v>
+        <v>64920920</v>
       </c>
       <c r="I100" t="n">
-        <v>191.955</v>
-      </c>
-      <c r="J100"/>
-      <c r="K100"/>
+        <v>196.134</v>
+      </c>
+      <c r="J100" t="n">
+        <v>1383306</v>
+      </c>
+      <c r="K100" t="n">
+        <v>4.179</v>
+      </c>
       <c r="L100" t="n">
-        <v>815036</v>
+        <v>896217</v>
       </c>
       <c r="M100" t="n">
-        <v>2.462</v>
+        <v>2.708</v>
       </c>
       <c r="N100" t="n">
-        <v>0.073</v>
+        <v>0.063</v>
       </c>
       <c r="O100" t="n">
-        <v>13.613</v>
+        <v>15.806</v>
       </c>
       <c r="P100" t="s">
+        <v>596</v>
+      </c>
+      <c r="Q100" t="s">
+        <v>595</v>
+      </c>
+      <c r="R100" t="s">
         <v>597</v>
       </c>
-      <c r="Q100" t="s">
-        <v>596</v>
-      </c>
-      <c r="R100" t="s">
+      <c r="S100" t="s">
         <v>598</v>
-      </c>
-      <c r="S100" t="s">
-        <v>599</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="B101" t="s">
+        <v>599</v>
+      </c>
+      <c r="C101" s="1" t="n">
+        <v>44049</v>
+      </c>
+      <c r="D101" t="s">
         <v>600</v>
       </c>
-      <c r="C101" s="1" t="n">
-        <v>44048</v>
-      </c>
-      <c r="D101" t="s">
+      <c r="E101" t="s">
         <v>601</v>
-      </c>
-      <c r="E101" t="s">
-        <v>602</v>
       </c>
       <c r="F101"/>
       <c r="G101" t="n">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="H101" t="n">
-        <v>58920975</v>
+        <v>59652675</v>
       </c>
       <c r="I101" t="n">
-        <v>178.008</v>
+        <v>180.218</v>
       </c>
       <c r="J101" t="n">
-        <v>681537</v>
+        <v>731700</v>
       </c>
       <c r="K101" t="n">
-        <v>2.059</v>
+        <v>2.211</v>
       </c>
       <c r="L101" t="n">
-        <v>725690</v>
+        <v>715096</v>
       </c>
       <c r="M101" t="n">
-        <v>2.192</v>
+        <v>2.16</v>
       </c>
       <c r="N101" t="n">
-        <v>0.083</v>
+        <v>0.079</v>
       </c>
       <c r="O101" t="n">
-        <v>12.121</v>
+        <v>12.612</v>
       </c>
       <c r="P101" t="s">
+        <v>601</v>
+      </c>
+      <c r="Q101" t="s">
         <v>602</v>
       </c>
-      <c r="Q101" t="s">
+      <c r="R101" t="s">
         <v>603</v>
       </c>
-      <c r="R101" t="s">
+      <c r="S101" t="s">
         <v>604</v>
-      </c>
-      <c r="S101" t="s">
-        <v>605</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="s">
+        <v>605</v>
+      </c>
+      <c r="B102" t="s">
         <v>606</v>
-      </c>
-      <c r="B102" t="s">
-        <v>607</v>
       </c>
       <c r="C102" s="1" t="n">
         <v>44048</v>
       </c>
       <c r="D102" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
       <c r="E102" t="s">
         <v>126</v>
@@ -8226,30 +8260,30 @@
         <v>126</v>
       </c>
       <c r="Q102" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="R102" t="s">
         <v>27</v>
       </c>
       <c r="S102" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="s">
+        <v>610</v>
+      </c>
+      <c r="B103" t="s">
         <v>611</v>
-      </c>
-      <c r="B103" t="s">
-        <v>612</v>
       </c>
       <c r="C103" s="1" t="n">
         <v>43950</v>
       </c>
       <c r="D103" t="s">
+        <v>612</v>
+      </c>
+      <c r="E103" t="s">
         <v>613</v>
-      </c>
-      <c r="E103" t="s">
-        <v>614</v>
       </c>
       <c r="F103"/>
       <c r="G103" t="n">
@@ -8276,33 +8310,33 @@
         <v>38171</v>
       </c>
       <c r="P103" t="s">
+        <v>613</v>
+      </c>
+      <c r="Q103" t="s">
         <v>614</v>
       </c>
-      <c r="Q103" t="s">
+      <c r="R103" t="s">
         <v>615</v>
       </c>
-      <c r="R103" t="s">
+      <c r="S103" t="s">
         <v>616</v>
-      </c>
-      <c r="S103" t="s">
-        <v>617</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="s">
+        <v>617</v>
+      </c>
+      <c r="B104" t="s">
         <v>618</v>
-      </c>
-      <c r="B104" t="s">
-        <v>619</v>
       </c>
       <c r="C104" s="1" t="n">
         <v>44046</v>
       </c>
       <c r="D104" t="s">
+        <v>619</v>
+      </c>
+      <c r="E104" t="s">
         <v>620</v>
-      </c>
-      <c r="E104" t="s">
-        <v>621</v>
       </c>
       <c r="F104"/>
       <c r="G104" t="n">
@@ -8333,16 +8367,16 @@
         <v>6.955</v>
       </c>
       <c r="P104" t="s">
+        <v>620</v>
+      </c>
+      <c r="Q104" t="s">
         <v>621</v>
-      </c>
-      <c r="Q104" t="s">
-        <v>622</v>
       </c>
       <c r="R104" t="s">
         <v>27</v>
       </c>
       <c r="S104" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated testing data for 2020-08-10
</commit_message>
<xml_diff>
--- a/public/data/testing/covid-testing-latest-data-source-details.xlsx
+++ b/public/data/testing/covid-testing-latest-data-source-details.xlsx
@@ -491,7 +491,7 @@
     <t xml:space="preserve">Denmark - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://files.ssi.dk/Data-epidemiologiske-rapport-07082020-qw54</t>
+    <t xml:space="preserve">https://files.ssi.dk/Data-Epidemiologiske-Rapport-10082020-lz41</t>
   </si>
   <si>
     <t xml:space="preserve">Statens Serum Institut</t>
@@ -886,7 +886,7 @@
     <t xml:space="preserve">Iran - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">http://irangov.ir/detail/344795</t>
+    <t xml:space="preserve">http://irangov.ir/detail/344872</t>
   </si>
   <si>
     <t xml:space="preserve">Government of Iran</t>
@@ -1791,7 +1791,7 @@
     <t xml:space="preserve">Spain - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.mscbs.gob.es/profesionales/saludPublica/ccayes/alertasActual/nCov-China/documentos/COVID-19_pruebas_diagnosticas_30_07_2020.pdf</t>
+    <t xml:space="preserve">https://www.mscbs.gob.es/profesionales/saludPublica/ccayes/alertasActual/nCov-China/documentos/COVID-19_pruebas_diagnosticas_06_08_2020.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">Ministry of Health, Consumption and Social Welfare</t>
@@ -3476,7 +3476,7 @@
         <v>118</v>
       </c>
       <c r="C18" s="1" t="n">
-        <v>44052</v>
+        <v>44053</v>
       </c>
       <c r="D18" t="s">
         <v>119</v>
@@ -3486,31 +3486,31 @@
       </c>
       <c r="F18"/>
       <c r="G18" t="n">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="H18" t="n">
-        <v>128132</v>
+        <v>129379</v>
       </c>
       <c r="I18" t="n">
-        <v>31.212</v>
+        <v>31.515</v>
       </c>
       <c r="J18" t="n">
-        <v>727</v>
+        <v>1247</v>
       </c>
       <c r="K18" t="n">
-        <v>0.177</v>
+        <v>0.304</v>
       </c>
       <c r="L18" t="n">
-        <v>973</v>
+        <v>1042</v>
       </c>
       <c r="M18" t="n">
-        <v>0.237</v>
+        <v>0.254</v>
       </c>
       <c r="N18" t="n">
         <v>0.047</v>
       </c>
       <c r="O18" t="n">
-        <v>21.351</v>
+        <v>21.203</v>
       </c>
       <c r="P18" t="s">
         <v>120</v>
@@ -3702,7 +3702,7 @@
         <v>142</v>
       </c>
       <c r="C22" s="1" t="n">
-        <v>44049</v>
+        <v>44052</v>
       </c>
       <c r="D22" t="s">
         <v>143</v>
@@ -3712,31 +3712,31 @@
       </c>
       <c r="F22"/>
       <c r="G22" t="n">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="H22" t="n">
-        <v>1648030</v>
+        <v>1721479</v>
       </c>
       <c r="I22" t="n">
-        <v>284.526</v>
+        <v>297.206</v>
       </c>
       <c r="J22" t="n">
-        <v>5406</v>
+        <v>3826</v>
       </c>
       <c r="K22" t="n">
-        <v>0.933</v>
+        <v>0.661</v>
       </c>
       <c r="L22" t="n">
-        <v>18141</v>
+        <v>21501</v>
       </c>
       <c r="M22" t="n">
-        <v>3.132</v>
+        <v>3.712</v>
       </c>
       <c r="N22" t="n">
         <v>0.004</v>
       </c>
       <c r="O22" t="n">
-        <v>230.466</v>
+        <v>230.485</v>
       </c>
       <c r="P22" t="s">
         <v>144</v>
@@ -4474,7 +4474,7 @@
         <v>233</v>
       </c>
       <c r="C36" s="1" t="n">
-        <v>44051</v>
+        <v>44052</v>
       </c>
       <c r="D36" t="s">
         <v>234</v>
@@ -4484,31 +4484,31 @@
       </c>
       <c r="F36"/>
       <c r="G36" t="n">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="H36" t="n">
-        <v>78235</v>
+        <v>78467</v>
       </c>
       <c r="I36" t="n">
-        <v>229.26</v>
+        <v>229.94</v>
       </c>
       <c r="J36" t="n">
-        <v>396</v>
+        <v>232</v>
       </c>
       <c r="K36" t="n">
-        <v>1.16</v>
+        <v>0.68</v>
       </c>
       <c r="L36" t="n">
-        <v>783</v>
+        <v>644</v>
       </c>
       <c r="M36" t="n">
-        <v>2.295</v>
+        <v>1.887</v>
       </c>
       <c r="N36" t="n">
-        <v>0.012</v>
+        <v>0.014</v>
       </c>
       <c r="O36" t="n">
-        <v>81.806</v>
+        <v>72.71</v>
       </c>
       <c r="P36" t="s">
         <v>235</v>
@@ -4706,7 +4706,7 @@
         <v>251</v>
       </c>
       <c r="C40" s="1" t="n">
-        <v>44052</v>
+        <v>44053</v>
       </c>
       <c r="D40" t="s">
         <v>252</v>
@@ -4716,31 +4716,31 @@
       </c>
       <c r="F40"/>
       <c r="G40" t="n">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="H40" t="n">
-        <v>2686498</v>
+        <v>2711817</v>
       </c>
       <c r="I40" t="n">
-        <v>31.985</v>
+        <v>32.286</v>
       </c>
       <c r="J40" t="n">
-        <v>24533</v>
+        <v>25319</v>
       </c>
       <c r="K40" t="n">
-        <v>0.292</v>
+        <v>0.301</v>
       </c>
       <c r="L40" t="n">
-        <v>25440</v>
+        <v>25308</v>
       </c>
       <c r="M40" t="n">
-        <v>0.303</v>
+        <v>0.301</v>
       </c>
       <c r="N40" t="n">
-        <v>0.101</v>
+        <v>0.098</v>
       </c>
       <c r="O40" t="n">
-        <v>9.926</v>
+        <v>10.255</v>
       </c>
       <c r="P40" t="s">
         <v>253</v>
@@ -5964,7 +5964,7 @@
         <v>379</v>
       </c>
       <c r="C62" s="1" t="n">
-        <v>44052</v>
+        <v>44053</v>
       </c>
       <c r="D62" t="s">
         <v>380</v>
@@ -5974,31 +5974,31 @@
       </c>
       <c r="F62"/>
       <c r="G62" t="n">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="H62" t="n">
-        <v>317496</v>
+        <v>319851</v>
       </c>
       <c r="I62" t="n">
-        <v>1.54</v>
+        <v>1.552</v>
       </c>
       <c r="J62" t="n">
-        <v>2864</v>
+        <v>2355</v>
       </c>
       <c r="K62" t="n">
-        <v>0.014</v>
+        <v>0.011</v>
       </c>
       <c r="L62" t="n">
-        <v>4281</v>
+        <v>4388</v>
       </c>
       <c r="M62" t="n">
         <v>0.021</v>
       </c>
       <c r="N62" t="n">
-        <v>0.087</v>
+        <v>0.089</v>
       </c>
       <c r="O62" t="n">
-        <v>11.512</v>
+        <v>11.227</v>
       </c>
       <c r="P62" t="s">
         <v>381</v>
@@ -6021,7 +6021,7 @@
         <v>385</v>
       </c>
       <c r="C63" s="1" t="n">
-        <v>44048</v>
+        <v>44051</v>
       </c>
       <c r="D63" t="s">
         <v>386</v>
@@ -6031,31 +6031,31 @@
       </c>
       <c r="F63"/>
       <c r="G63" t="n">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="H63" t="n">
-        <v>458479</v>
+        <v>474531</v>
       </c>
       <c r="I63" t="n">
-        <v>84.571</v>
+        <v>87.532</v>
       </c>
       <c r="J63" t="n">
-        <v>6219</v>
+        <v>1990</v>
       </c>
       <c r="K63" t="n">
-        <v>1.147</v>
+        <v>0.367</v>
       </c>
       <c r="L63" t="n">
-        <v>4717</v>
+        <v>5463</v>
       </c>
       <c r="M63" t="n">
-        <v>0.87</v>
+        <v>1.008</v>
       </c>
       <c r="N63" t="n">
-        <v>0.006</v>
+        <v>0.007</v>
       </c>
       <c r="O63" t="n">
-        <v>164.274</v>
+        <v>147.081</v>
       </c>
       <c r="P63" t="s">
         <v>387</v>
@@ -7306,7 +7306,7 @@
         <v>516</v>
       </c>
       <c r="C86" s="1" t="n">
-        <v>44042</v>
+        <v>44049</v>
       </c>
       <c r="D86" t="s">
         <v>517</v>
@@ -7316,27 +7316,27 @@
       </c>
       <c r="F86"/>
       <c r="G86" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H86" t="n">
-        <v>4652493</v>
+        <v>4983935</v>
       </c>
       <c r="I86" t="n">
-        <v>99.508</v>
+        <v>106.597</v>
       </c>
       <c r="J86"/>
       <c r="K86"/>
       <c r="L86" t="n">
-        <v>43639</v>
+        <v>47349</v>
       </c>
       <c r="M86" t="n">
-        <v>0.933</v>
+        <v>1.013</v>
       </c>
       <c r="N86" t="n">
-        <v>0.05</v>
+        <v>0.074</v>
       </c>
       <c r="O86" t="n">
-        <v>20.013</v>
+        <v>13.57</v>
       </c>
       <c r="P86" t="s">
         <v>519</v>

</xml_diff>

<commit_message>
Updated testing data for 2020-08-12
</commit_message>
<xml_diff>
--- a/public/data/testing/covid-testing-latest-data-source-details.xlsx
+++ b/public/data/testing/covid-testing-latest-data-source-details.xlsx
@@ -110,7 +110,7 @@
     <t xml:space="preserve">Australia - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.health.gov.au/sites/default/files/documents/2020/08/coronavirus-covid-19-at-a-glance-9-august-2020.pdf</t>
+    <t xml:space="preserve">https://www.health.gov.au/sites/default/files/documents/2020/08/coronavirus-covid-19-at-a-glance-11-august-2020.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">Australian Government Department of Health</t>
@@ -202,7 +202,7 @@
     <t xml:space="preserve">Belarus - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">http://minzdrav.gov.by/ru/sobytiya/u-belarusi-na-8-zhni-nya-vypisanyya-64-tys-744-patsyenta/</t>
+    <t xml:space="preserve">http://minzdrav.gov.by/ru/sobytiya/u-belarusi-na-11-zhni-nya-vypisanyya-65-tys-219-patsyenta/</t>
   </si>
   <si>
     <t xml:space="preserve">Belarus Ministry of Health</t>
@@ -245,7 +245,7 @@
     <t xml:space="preserve">Bolivia - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://minsalud.gob.bo/4481-ministerio-de-salud-reporta-1-780-nuevos-contagios-de-covid-19-y-supera-los-85-000-casos-positivos</t>
+    <t xml:space="preserve">https://minsalud.gob.bo/4501-bolivia-reporta-1-636-contagios-nuevos-de-coronavirus-y-acumula-91-635-casos-en-cinco-meses</t>
   </si>
   <si>
     <t xml:space="preserve">https://www.minsalud.gob.bo/</t>
@@ -394,7 +394,7 @@
     <t xml:space="preserve">Cote d'Ivoire - samples tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.facebook.com/Mshpci/posts/1664126360419718</t>
+    <t xml:space="preserve">https://www.facebook.com/Mshpci/posts/1665844576914563</t>
   </si>
   <si>
     <t xml:space="preserve">Ministry of Health and Public Hygiene</t>
@@ -473,7 +473,7 @@
     <t xml:space="preserve">Democratic Republic of Congo - samples tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/CMR_Covid19_RDC/status/1291289739681828864/photo/1</t>
+    <t xml:space="preserve">https://twitter.com/CMR_Covid19_RDC/status/1293140045390589954/photo/1</t>
   </si>
   <si>
     <t xml:space="preserve">DRC COVID-19 Pandemic Response Multisectoral Committee</t>
@@ -491,7 +491,7 @@
     <t xml:space="preserve">Denmark - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://files.ssi.dk/Data-Epidemiologiske-Rapport-10082020-lz41</t>
+    <t xml:space="preserve">https://files.ssi.dk/Data-Epidemiologiske-Rapport-11082020-lok5</t>
   </si>
   <si>
     <t xml:space="preserve">Statens Serum Institut</t>
@@ -509,7 +509,7 @@
     <t xml:space="preserve">Ecuador - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.gestionderiesgos.gob.ec/wp-content/uploads/2020/08/INFOGRAFIA-NACIONALCOVI-19-COE-NACIONAL-08h00-08082020.pdf</t>
+    <t xml:space="preserve">https://www.gestionderiesgos.gob.ec/wp-content/uploads/2020/08/INFOGRAFIA-NACIONALCOVI-19-COE-NACIONAL-08h00-09082020.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">Government of Ecuador</t>
@@ -535,7 +535,7 @@
     <t xml:space="preserve">El Salvador - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.facebook.com/nayibbukele/posts/3126341627452007</t>
+    <t xml:space="preserve">https://www.facebook.com/nayibbukele/posts/3138372252915611</t>
   </si>
   <si>
     <t xml:space="preserve">Government of El Salvador</t>
@@ -579,7 +579,7 @@
     <t xml:space="preserve">Ethiopia - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.ephi.gov.et/images/novel_coronavirus/EPHI_-PHEOC_COVID-19_Weekly-bulletin_12_English_07202020.pdf</t>
+    <t xml:space="preserve">https://www.ephi.gov.et/images/novel_coronavirus/EPHI_-PHEOC_COVID-19_Weekly--bulletin_14_English_08032020.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">Ethiopian Public Health Institute</t>
@@ -746,7 +746,7 @@
     <t xml:space="preserve">Greece - samples tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://eody.gov.gr/covid-gr-daily-report-20200809</t>
+    <t xml:space="preserve">https://eody.gov.gr/covid-gr-daily-report-20200811</t>
   </si>
   <si>
     <t xml:space="preserve">National Organization of Public Health</t>
@@ -871,12 +871,11 @@
     <t xml:space="preserve">https://covid19.kemkes.go.id/</t>
   </si>
   <si>
-    <t xml:space="preserve">The Indonesian Ministry of Health updates its COVID-19 dashboard twice a day but doesn't keep time series of past data. The two URLs ([1](https://infeksiemerging.kemkes.go.id/), [2](https://covid19.kemkes.go.id/)) seem to lead to the exact same dashboard.
+    <t xml:space="preserve">The Indonesian Ministry of Health updates its COVID-19 dashboard twice a day but doesn't keep time series of past data. We found past values using Internet Archive's Wayback Machine. The two dashboard URLs ([1](https://infeksiemerging.kemkes.go.id/), [2](https://covid19.kemkes.go.id/)) seem to lead to the exact same dashboard.
 The dashboard shows the latest number of "Kasus dg Spesimen Diperiksa", which translates to "Cases with Specimens Checked".
-We found past values using Internet Archive's Wayback Machine.
-There is some reason to believe that non-PCR tests are included in the cumulative number of specimens checked to date. [Official COVID-19 diagnostic guidelines](https://covid19.kemkes.go.id/download/Pedoman_Penanganan_Cepat_Medis_dan_Kesehatan_Masyarakat_COVID-19_di_Indonesia.pdf.pdf) published on 23 March 2020 state that: 
+[Official diagnostic guidelines](https://covid19.kemkes.go.id/download/Pedoman_Penanganan_Cepat_Medis_dan_Kesehatan_Masyarakat_COVID-19_di_Indonesia.pdf.pdf) published on 23 March 2020 provide some reason to be concerned that serological (antibody) tests are included in the cumulative testing figures, stating that:
 "Handling of COVID-19 in Indonesia uses antibodies and / or antigen Rapid Tests (RT) in case of contact from a positive patient. RT antibodies are also used for case detection...in areas that do not have facilities for RT-PCR inspection. RT antibody examination results are confirmed using RT-PCR." (translated)
-We cannot find explicit confirmation of whether the reported testing figures include or exclude non-PCR tests.
+However, testing figures provided by the [National Agency for Disaster Countermeasure (BNPB)](https://www.bnpb.go.id/) via [twitter](https://twitter.com/bnpb_indonesia?lang=en) explicitly report the number of PCR tests conducted to date, which match the cumulative testing figures provided in the Ministry of Health dashboard. The PCR testing figures reported by the BNPB include a small number of "rapid molecular tests" ("Test Cepat Molekular"), which are diagnostic tests not to be confused with serological (antibody) tests. Of 998,406 cumulative people tested as of 11 August 2020, 26,184 (2.6%) were tested via rapid molecular testing ([source](https://twitter.com/BNPB_Indonesia/status/1293105682791542784)). These rapid molecular testing figures are included in the time series we construct.
 Note that, due to the way the data is presented by the official source, the time series may be impacted by retrospective revisions made by the source – see our [FAQ here](https://ourworldindata.org/coronavirus-testing#does-your-data-reflect-retrospective-updates-made-by-the-source).</t>
   </si>
   <si>
@@ -886,7 +885,7 @@
     <t xml:space="preserve">Iran - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">http://irangov.ir/detail/344872</t>
+    <t xml:space="preserve">http://irangov.ir/detail/344937</t>
   </si>
   <si>
     <t xml:space="preserve">Government of Iran</t>
@@ -923,7 +922,7 @@
     <t xml:space="preserve">Israel - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://govextra.gov.il/media/24033/covid19-data-israel-03082020.csv</t>
+    <t xml:space="preserve">https://govextra.gov.il/media/24250/covid19-data-israel-05082020.csv</t>
   </si>
   <si>
     <t xml:space="preserve">Israel Ministry of Health</t>
@@ -982,7 +981,7 @@
     <t xml:space="preserve">Japan - people tested (incl. non-PCR)</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.mhlw.go.jp/stf/newpage_12907.html</t>
+    <t xml:space="preserve">https://www.mhlw.go.jp/stf/newpage_12918.html</t>
   </si>
   <si>
     <t xml:space="preserve">Ministry of Health, Labor and Welfare Press Release</t>
@@ -1007,10 +1006,10 @@
     <t xml:space="preserve">Japan - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.mhlw.go.jp/content/10906000/000657894.pdf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The cumulative total reported in the press release (1,284,151) does not sum to the cumulative total calculated from the weekly and daily figures reported by the MOH. See: https://www.mhlw.go.jp/content/10906000/000657894.pdf</t>
+    <t xml:space="preserve">https://www.mhlw.go.jp/content/10906000/000658097.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The cumulative total reported in the press release (1,298,747) does not sum to the cumulative total calculated from the weekly and daily figures reported by the MOH. See: https://www.mhlw.go.jp/content/10906000/000658097.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">On 11 April 2020, the MOH started providing a daily time series on the "Implementation status of PCR tests for new coronavirus in Japan (based on the date on which results were determined" (via Google translate). 
@@ -1041,7 +1040,7 @@
     <t xml:space="preserve">Kenya - samples tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/MOH_Kenya/status/1291395868684419082</t>
+    <t xml:space="preserve">https://twitter.com/MOH_Kenya/status/1293167082423672835</t>
   </si>
   <si>
     <t xml:space="preserve">Kenya Ministry of Health</t>
@@ -1063,7 +1062,7 @@
     <t xml:space="preserve">Kuwait - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/KUWAIT_MOH/status/1291341316073435136/photo/1</t>
+    <t xml:space="preserve">https://twitter.com/KUWAIT_MOH/status/1293147679262998531/photo/1</t>
   </si>
   <si>
     <t xml:space="preserve">Kuwait Ministry of Health</t>
@@ -1129,7 +1128,7 @@
     <t xml:space="preserve">Malaysia - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">http://covid-19.moh.gov.my/terkini/082020/situasi-terkini-09-ogos-2020</t>
+    <t xml:space="preserve">http://covid-19.moh.gov.my/terkini/082020/situasi-terkini-11-ogos-2020</t>
   </si>
   <si>
     <t xml:space="preserve">Ministry of Health Malaysia</t>
@@ -1155,7 +1154,7 @@
     <t xml:space="preserve">Maldives - samples tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/HPA_MV/status/1291418563312521216/photo/1</t>
+    <t xml:space="preserve">https://twitter.com/HPA_MV/status/1292869546123165696/photo/1</t>
   </si>
   <si>
     <t xml:space="preserve">Maldives Health Protection Agency</t>
@@ -1222,7 +1221,7 @@
     <t xml:space="preserve">Morocco - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/Ministere_Sante/status/1291422913153859586/photo/1</t>
+    <t xml:space="preserve">https://twitter.com/Ministere_Sante/status/1292875556942381065/photo/1</t>
   </si>
   <si>
     <t xml:space="preserve">Morocco Ministry of Health</t>
@@ -1262,7 +1261,7 @@
     <t xml:space="preserve">Nepal - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://drive.google.com/drive/folders/1b1dQwSgV6Fw10kpUdBwFDiFIN1YehzQ8</t>
+    <t xml:space="preserve">https://drive.google.com/drive/folders/1O3VC_AWT2bSfZ1VrDY7e8OZ_mzsNjix-</t>
   </si>
   <si>
     <t xml:space="preserve">Ministry of Health and Population</t>
@@ -1282,7 +1281,7 @@
     <t xml:space="preserve">Netherlands - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.rivm.nl/sites/default/files/2020-08/COVID-19_WebSite_rapport_wekelijks_20200804_1306.pdf</t>
+    <t xml:space="preserve">https://www.rivm.nl/sites/default/files/2020-08/COVID-19_WebSite_rapport_wekelijks_20200811_1158_0.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">National Institute for Public Health and the Environment</t>
@@ -1382,6 +1381,7 @@
   <si>
     <t xml:space="preserve">The Oman Ministry of Health provides daily statements, including the total number of tests within the last 24 hours. It is unclear whether tests refer to samples or individuals tested. 
 The earliest observation on testing figures begins from 4 June 2020. No cumulative total is provided by the source, therefore this time series is only visible on our graphs for daily tests.
+The daily statements issued by the MOH do not provide test figures after 6 August 2020. 
 Note that, due to the way the data is presented by the official source, the time series may be impacted by retrospective revisions made by the source – see our [FAQ here](https://ourworldindata.org/coronavirus-testing#does-your-data-reflect-retrospective-updates-made-by-the-source).</t>
   </si>
   <si>
@@ -1486,7 +1486,7 @@
     <t xml:space="preserve">Poland - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/MZ_GOV_PL/status/1292385128732188673</t>
+    <t xml:space="preserve">https://twitter.com/MZ_GOV_PL/status/1293109904773980161</t>
   </si>
   <si>
     <t xml:space="preserve">Poland Ministry of Health</t>
@@ -1554,7 +1554,7 @@
     <t xml:space="preserve">Romania - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://gov.ro/ro/media/comunicate/buletin-de-presa-9-august-2020-ora-13-00&amp;page=1</t>
+    <t xml:space="preserve">https://gov.ro/ro/media/comunicate/buletin-de-presa-11-august-2020-ora-13-00&amp;page=1</t>
   </si>
   <si>
     <t xml:space="preserve">Ministry of Internal Affairs</t>
@@ -1577,7 +1577,7 @@
     <t xml:space="preserve">Russia - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://rospotrebnadzor.ru/about/info/news/news_details.php?ELEMENT_ID=15126</t>
+    <t xml:space="preserve">https://rospotrebnadzor.ru/about/info/news/news_details.php?ELEMENT_ID=15149</t>
   </si>
   <si>
     <t xml:space="preserve">Government of the Russian Federation</t>
@@ -1597,7 +1597,7 @@
     <t xml:space="preserve">Rwanda - samples tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/RwandaHealth/status/1291455527701094401</t>
+    <t xml:space="preserve">https://twitter.com/RwandaHealth/status/1292893993995575296</t>
   </si>
   <si>
     <t xml:space="preserve">Rwanda Ministry of Health</t>
@@ -1624,7 +1624,7 @@
   </si>
   <si>
     <t xml:space="preserve">The Saudi Arabian Ministry of Health provides a dashboard detailing the total number of tests performed. 
-The dashboard reports testing figures as "total tests", making it unclear whether the figures refer to the number of samples tested, tests performed, or people tested. Nevertheless, corresponding press  releases from [the Ministry of Health](https://www.moh.gov.sa/en/Ministry/MediaCenter/News/Pages/default.aspx) imply that the figures refer to the total number of tests performed. For example, the [26 July 2020 press release](https://www.moh.gov.sa/en/Ministry/MediaCenter/News/Pages/News-2020-07-26-004.aspx) states that "...57,216 new Polymerase Chain Reaction (PCR) tests for Novel Coronavirus (COVID-19) have been conducted in the Kingdom’s laboratories, bringing the total number to 3,056,956 lab tests". This 3,056,956 figure differs slightly from the figure of 3,047,668 tests reported on the official dashboard on 26 July 2020, but we assume this small discrepancy is due to differences in reporting time rather than a substantive difference in units (e.g. tests performed vs. people tested).
+The dashboard reports testing figures as "total tests", making it unclear whether the figures refer to the number of samples tested, tests performed, or people tested. Nevertheless, corresponding press releases from [the Ministry of Health](https://www.moh.gov.sa/en/Ministry/MediaCenter/News/Pages/default.aspx) imply that the figures refer to the total number of tests performed. For example, the [26 July 2020 press release](https://www.moh.gov.sa/en/Ministry/MediaCenter/News/Pages/News-2020-07-26-004.aspx) states that "...57,216 new Polymerase Chain Reaction (PCR) tests for Novel Coronavirus (COVID-19) have been conducted in the Kingdom’s laboratories, bringing the total number to 3,056,956 lab tests". This 3,056,956 figure differs slightly from the figure of 3,047,668 tests reported on the official dashboard on 26 July 2020, but we assume this small discrepancy is due to differences in reporting time rather than a substantive difference in units (e.g. tests performed vs. people tested).
 The exact date these cumulative figures date back to is unknown.
 Note that, due to the way the data is presented by the official source, the time series may be impacted by retrospective revisions made by the source – see our [FAQ here](https://ourworldindata.org/coronavirus-testing#does-your-data-reflect-retrospective-updates-made-by-the-source).</t>
   </si>
@@ -1771,7 +1771,7 @@
     <t xml:space="preserve">South Korea - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.cdc.go.kr/board/board.es?mid=&amp;bid=0030&amp;act=view&amp;list_no=368076&amp;tag=&amp;nPage=1</t>
+    <t xml:space="preserve">https://www.cdc.go.kr/board/board.es?mid=&amp;bid=0030&amp;act=view&amp;list_no=368103&amp;tag=&amp;nPage=1</t>
   </si>
   <si>
     <t xml:space="preserve">South Korea CDC</t>
@@ -1893,7 +1893,7 @@
     <t xml:space="preserve">Thailand - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://ddc.moph.go.th/viralpneumonia/file/situation/situation-no219-090863.pdf</t>
+    <t xml:space="preserve">https://ddc.moph.go.th/viralpneumonia/file/situation/situation-no221-110863n.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">Department of Disease Control</t>
@@ -1981,7 +1981,7 @@
     <t xml:space="preserve">Uganda - samples tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/MinofHealthUG/status/1292465720111124480/photo/2</t>
+    <t xml:space="preserve">https://twitter.com/MinofHealthUG/status/1293106352869515265/photo/1</t>
   </si>
   <si>
     <t xml:space="preserve">Uganda Ministry of Health</t>
@@ -2041,7 +2041,7 @@
     <t xml:space="preserve">United Kingdom - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://assets.publishing.service.gov.uk/government/uploads/system/uploads/attachment_data/file/907964/2020-08-09_COVID-19_UK_testing_time_series.csv</t>
+    <t xml:space="preserve">https://assets.publishing.service.gov.uk/government/uploads/system/uploads/attachment_data/file/908596/2020-08-11_COVID-19_UK_testing_time_series.csv</t>
   </si>
   <si>
     <t xml:space="preserve">Public Health England/Department of Health and Social Care</t>
@@ -2121,7 +2121,7 @@
     <t xml:space="preserve">Uruguay - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.gub.uy/ministerio-salud-publica/comunicacion/noticias/informe-situacion-sobre-coronavirus-covid-19-0</t>
+    <t xml:space="preserve">https://www.gub.uy/ministerio-salud-publica/comunicacion/noticias/informe-situacion-sobre-coronavirus-covid-19-uruguay-10-agosto</t>
   </si>
   <si>
     <t xml:space="preserve">https://www.gub.uy/ministerio-salud-publica/comunicacion/noticias</t>
@@ -2159,7 +2159,7 @@
     <t xml:space="preserve">Zimbabwe - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/MoHCCZim/status/1291223430046584833</t>
+    <t xml:space="preserve">https://twitter.com/MoHCCZim/status/1292530449500319744</t>
   </si>
   <si>
     <t xml:space="preserve">Zimbabwe Ministry of Health and Child Care</t>
@@ -2576,7 +2576,7 @@
         <v>20</v>
       </c>
       <c r="C2" s="1" t="n">
-        <v>44052</v>
+        <v>44054</v>
       </c>
       <c r="D2" t="s">
         <v>21</v>
@@ -2586,31 +2586,31 @@
       </c>
       <c r="F2"/>
       <c r="G2" t="n">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="H2" t="n">
-        <v>725776</v>
+        <v>757987</v>
       </c>
       <c r="I2" t="n">
-        <v>16.058</v>
+        <v>16.771</v>
       </c>
       <c r="J2" t="n">
-        <v>2230</v>
+        <v>4595</v>
       </c>
       <c r="K2" t="n">
-        <v>0.049</v>
+        <v>0.102</v>
       </c>
       <c r="L2" t="n">
-        <v>11233</v>
+        <v>11658</v>
       </c>
       <c r="M2" t="n">
-        <v>0.249</v>
+        <v>0.258</v>
       </c>
       <c r="N2" t="n">
-        <v>0.564</v>
+        <v>0.546</v>
       </c>
       <c r="O2" t="n">
-        <v>1.772</v>
+        <v>1.831</v>
       </c>
       <c r="P2" t="s">
         <v>22</v>
@@ -2633,7 +2633,7 @@
         <v>25</v>
       </c>
       <c r="C3" s="1" t="n">
-        <v>44052</v>
+        <v>44054</v>
       </c>
       <c r="D3" t="s">
         <v>26</v>
@@ -2643,31 +2643,31 @@
       </c>
       <c r="F3"/>
       <c r="G3" t="n">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="H3" t="n">
-        <v>884840</v>
+        <v>923656</v>
       </c>
       <c r="I3" t="n">
-        <v>19.578</v>
+        <v>20.437</v>
       </c>
       <c r="J3" t="n">
-        <v>2754</v>
+        <v>5829</v>
       </c>
       <c r="K3" t="n">
-        <v>0.061</v>
+        <v>0.129</v>
       </c>
       <c r="L3" t="n">
-        <v>13173</v>
+        <v>13597</v>
       </c>
       <c r="M3" t="n">
-        <v>0.291</v>
+        <v>0.301</v>
       </c>
       <c r="N3" t="n">
-        <v>0.481</v>
+        <v>0.468</v>
       </c>
       <c r="O3" t="n">
-        <v>2.078</v>
+        <v>2.135</v>
       </c>
       <c r="P3" t="s">
         <v>22</v>
@@ -2690,7 +2690,7 @@
         <v>30</v>
       </c>
       <c r="C4" s="1" t="n">
-        <v>44052</v>
+        <v>44054</v>
       </c>
       <c r="D4" t="s">
         <v>31</v>
@@ -2700,27 +2700,31 @@
       </c>
       <c r="F4"/>
       <c r="G4" t="n">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="H4" t="n">
-        <v>4857414</v>
+        <v>4980172</v>
       </c>
       <c r="I4" t="n">
-        <v>190.488</v>
-      </c>
-      <c r="J4"/>
-      <c r="K4"/>
+        <v>195.302</v>
+      </c>
+      <c r="J4" t="n">
+        <v>61626</v>
+      </c>
+      <c r="K4" t="n">
+        <v>2.417</v>
+      </c>
       <c r="L4" t="n">
-        <v>70110</v>
+        <v>71222</v>
       </c>
       <c r="M4" t="n">
-        <v>2.749</v>
+        <v>2.793</v>
       </c>
       <c r="N4" t="n">
-        <v>0.007</v>
+        <v>0.006</v>
       </c>
       <c r="O4" t="n">
-        <v>143.668</v>
+        <v>161.921</v>
       </c>
       <c r="P4" t="s">
         <v>32</v>
@@ -2743,7 +2747,7 @@
         <v>36</v>
       </c>
       <c r="C5" s="1" t="n">
-        <v>44053</v>
+        <v>44055</v>
       </c>
       <c r="D5" t="s">
         <v>37</v>
@@ -2753,32 +2757,28 @@
       </c>
       <c r="F5"/>
       <c r="G5" t="n">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="H5" t="n">
-        <v>965758</v>
+        <v>983018</v>
       </c>
       <c r="I5" t="n">
-        <v>107.23</v>
+        <v>109.147</v>
       </c>
       <c r="J5" t="n">
-        <v>3890</v>
+        <v>8510</v>
       </c>
       <c r="K5" t="n">
-        <v>0.432</v>
+        <v>0.945</v>
       </c>
       <c r="L5" t="n">
-        <v>6997</v>
+        <v>7490</v>
       </c>
       <c r="M5" t="n">
-        <v>0.777</v>
-      </c>
-      <c r="N5" t="n">
-        <v>0.014</v>
-      </c>
-      <c r="O5" t="n">
-        <v>69.771</v>
-      </c>
+        <v>0.832</v>
+      </c>
+      <c r="N5"/>
+      <c r="O5"/>
       <c r="P5" t="s">
         <v>39</v>
       </c>
@@ -2800,7 +2800,7 @@
         <v>43</v>
       </c>
       <c r="C6" s="1" t="n">
-        <v>44053</v>
+        <v>44055</v>
       </c>
       <c r="D6" t="s">
         <v>44</v>
@@ -2810,32 +2810,28 @@
       </c>
       <c r="F6"/>
       <c r="G6" t="n">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="H6" t="n">
-        <v>902059</v>
+        <v>923342</v>
       </c>
       <c r="I6" t="n">
-        <v>530.129</v>
+        <v>542.637</v>
       </c>
       <c r="J6" t="n">
-        <v>9133</v>
+        <v>11231</v>
       </c>
       <c r="K6" t="n">
-        <v>5.367</v>
+        <v>6.6</v>
       </c>
       <c r="L6" t="n">
-        <v>7344</v>
+        <v>8636</v>
       </c>
       <c r="M6" t="n">
-        <v>4.316</v>
-      </c>
-      <c r="N6" t="n">
-        <v>0.048</v>
-      </c>
-      <c r="O6" t="n">
-        <v>20.771</v>
-      </c>
+        <v>5.075</v>
+      </c>
+      <c r="N6"/>
+      <c r="O6"/>
       <c r="P6" t="s">
         <v>46</v>
       </c>
@@ -2857,7 +2853,7 @@
         <v>50</v>
       </c>
       <c r="C7" s="1" t="n">
-        <v>44050</v>
+        <v>44053</v>
       </c>
       <c r="D7" t="s">
         <v>51</v>
@@ -2867,31 +2863,31 @@
       </c>
       <c r="F7"/>
       <c r="G7" t="n">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="H7" t="n">
-        <v>1237823</v>
+        <v>1273168</v>
       </c>
       <c r="I7" t="n">
-        <v>7.516</v>
+        <v>7.731</v>
       </c>
       <c r="J7" t="n">
-        <v>12699</v>
+        <v>12849</v>
       </c>
       <c r="K7" t="n">
-        <v>0.077</v>
+        <v>0.078</v>
       </c>
       <c r="L7" t="n">
-        <v>8716</v>
+        <v>11375</v>
       </c>
       <c r="M7" t="n">
-        <v>0.053</v>
+        <v>0.069</v>
       </c>
       <c r="N7" t="n">
-        <v>0.242</v>
+        <v>0.212</v>
       </c>
       <c r="O7" t="n">
-        <v>4.133</v>
+        <v>4.724</v>
       </c>
       <c r="P7" t="s">
         <v>52</v>
@@ -2914,7 +2910,7 @@
         <v>57</v>
       </c>
       <c r="C8" s="1" t="n">
-        <v>44051</v>
+        <v>44054</v>
       </c>
       <c r="D8" t="s">
         <v>58</v>
@@ -2924,27 +2920,27 @@
       </c>
       <c r="F8"/>
       <c r="G8" t="n">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="H8" t="n">
-        <v>1363011</v>
+        <v>1377540</v>
       </c>
       <c r="I8" t="n">
-        <v>144.244</v>
+        <v>145.782</v>
       </c>
       <c r="J8"/>
       <c r="K8"/>
       <c r="L8" t="n">
-        <v>7616</v>
+        <v>7395</v>
       </c>
       <c r="M8" t="n">
-        <v>0.806</v>
+        <v>0.783</v>
       </c>
       <c r="N8" t="n">
         <v>0.015</v>
       </c>
       <c r="O8" t="n">
-        <v>66.144</v>
+        <v>66.28</v>
       </c>
       <c r="P8" t="s">
         <v>59</v>
@@ -2967,7 +2963,7 @@
         <v>63</v>
       </c>
       <c r="C9" s="1" t="n">
-        <v>44051</v>
+        <v>44053</v>
       </c>
       <c r="D9" t="s">
         <v>64</v>
@@ -2977,31 +2973,31 @@
       </c>
       <c r="F9"/>
       <c r="G9" t="n">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="H9" t="n">
-        <v>1859125</v>
+        <v>1888061</v>
       </c>
       <c r="I9" t="n">
-        <v>160.413</v>
+        <v>162.91</v>
       </c>
       <c r="J9" t="n">
-        <v>13202</v>
+        <v>12454</v>
       </c>
       <c r="K9" t="n">
-        <v>1.139</v>
+        <v>1.075</v>
       </c>
       <c r="L9" t="n">
-        <v>18889</v>
+        <v>19031</v>
       </c>
       <c r="M9" t="n">
-        <v>1.63</v>
+        <v>1.642</v>
       </c>
       <c r="N9" t="n">
-        <v>0.029</v>
+        <v>0.03</v>
       </c>
       <c r="O9" t="n">
-        <v>34.087</v>
+        <v>33.751</v>
       </c>
       <c r="P9" t="s">
         <v>65</v>
@@ -3024,7 +3020,7 @@
         <v>69</v>
       </c>
       <c r="C10" s="1" t="n">
-        <v>44048</v>
+        <v>44053</v>
       </c>
       <c r="D10" t="s">
         <v>70</v>
@@ -3034,31 +3030,31 @@
       </c>
       <c r="F10"/>
       <c r="G10" t="n">
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="H10" t="n">
-        <v>166104</v>
+        <v>179553</v>
       </c>
       <c r="I10" t="n">
-        <v>14.23</v>
+        <v>15.382</v>
       </c>
       <c r="J10" t="n">
-        <v>3443</v>
+        <v>3245</v>
       </c>
       <c r="K10" t="n">
-        <v>0.295</v>
+        <v>0.278</v>
       </c>
       <c r="L10" t="n">
-        <v>3136</v>
+        <v>2818</v>
       </c>
       <c r="M10" t="n">
-        <v>0.269</v>
+        <v>0.241</v>
       </c>
       <c r="N10" t="n">
-        <v>0.503</v>
+        <v>0.499</v>
       </c>
       <c r="O10" t="n">
-        <v>1.989</v>
+        <v>2.003</v>
       </c>
       <c r="P10" t="s">
         <v>45</v>
@@ -3132,7 +3128,7 @@
         <v>82</v>
       </c>
       <c r="C12" s="1" t="n">
-        <v>44052</v>
+        <v>44055</v>
       </c>
       <c r="D12" t="s">
         <v>83</v>
@@ -3142,32 +3138,28 @@
       </c>
       <c r="F12"/>
       <c r="G12" t="n">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="H12" t="n">
-        <v>303536</v>
+        <v>313866</v>
       </c>
       <c r="I12" t="n">
-        <v>43.684</v>
+        <v>45.171</v>
       </c>
       <c r="J12" t="n">
-        <v>3612</v>
+        <v>5388</v>
       </c>
       <c r="K12" t="n">
-        <v>0.52</v>
+        <v>0.775</v>
       </c>
       <c r="L12" t="n">
-        <v>4435</v>
+        <v>4152</v>
       </c>
       <c r="M12" t="n">
-        <v>0.638</v>
-      </c>
-      <c r="N12" t="n">
-        <v>0.049</v>
-      </c>
-      <c r="O12" t="n">
-        <v>20.601</v>
-      </c>
+        <v>0.598</v>
+      </c>
+      <c r="N12"/>
+      <c r="O12"/>
       <c r="P12" t="s">
         <v>85</v>
       </c>
@@ -3189,7 +3181,7 @@
         <v>88</v>
       </c>
       <c r="C13" s="1" t="n">
-        <v>44053</v>
+        <v>44055</v>
       </c>
       <c r="D13" t="s">
         <v>89</v>
@@ -3199,32 +3191,28 @@
       </c>
       <c r="F13"/>
       <c r="G13" t="n">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="H13" t="n">
-        <v>4447810</v>
+        <v>4541747</v>
       </c>
       <c r="I13" t="n">
-        <v>117.847</v>
+        <v>120.336</v>
       </c>
       <c r="J13" t="n">
-        <v>43772</v>
+        <v>36529</v>
       </c>
       <c r="K13" t="n">
-        <v>1.16</v>
+        <v>0.968</v>
       </c>
       <c r="L13" t="n">
-        <v>38516</v>
+        <v>41026</v>
       </c>
       <c r="M13" t="n">
-        <v>1.021</v>
-      </c>
-      <c r="N13" t="n">
-        <v>0.01</v>
-      </c>
-      <c r="O13" t="n">
-        <v>104.46</v>
-      </c>
+        <v>1.087</v>
+      </c>
+      <c r="N13"/>
+      <c r="O13"/>
       <c r="P13" t="s">
         <v>90</v>
       </c>
@@ -3246,7 +3234,7 @@
         <v>93</v>
       </c>
       <c r="C14" s="1" t="n">
-        <v>44052</v>
+        <v>44054</v>
       </c>
       <c r="D14" t="s">
         <v>94</v>
@@ -3258,31 +3246,31 @@
         <v>95</v>
       </c>
       <c r="G14" t="n">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="H14" t="n">
-        <v>1841355</v>
+        <v>1889616</v>
       </c>
       <c r="I14" t="n">
-        <v>96.324</v>
+        <v>98.849</v>
       </c>
       <c r="J14" t="n">
-        <v>28460</v>
+        <v>22249</v>
       </c>
       <c r="K14" t="n">
-        <v>1.489</v>
+        <v>1.164</v>
       </c>
       <c r="L14" t="n">
-        <v>24009</v>
+        <v>24743</v>
       </c>
       <c r="M14" t="n">
-        <v>1.256</v>
+        <v>1.294</v>
       </c>
       <c r="N14" t="n">
-        <v>0.08</v>
+        <v>0.078</v>
       </c>
       <c r="O14" t="n">
-        <v>12.575</v>
+        <v>12.781</v>
       </c>
       <c r="P14" t="s">
         <v>96</v>
@@ -3305,7 +3293,7 @@
         <v>100</v>
       </c>
       <c r="C15" s="1" t="n">
-        <v>44052</v>
+        <v>44054</v>
       </c>
       <c r="D15" t="s">
         <v>101</v>
@@ -3315,31 +3303,31 @@
       </c>
       <c r="F15"/>
       <c r="G15" t="n">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="H15" t="n">
-        <v>1909111</v>
+        <v>1982831</v>
       </c>
       <c r="I15" t="n">
-        <v>37.52</v>
+        <v>38.969</v>
       </c>
       <c r="J15" t="n">
-        <v>31743</v>
+        <v>40101</v>
       </c>
       <c r="K15" t="n">
-        <v>0.624</v>
+        <v>0.788</v>
       </c>
       <c r="L15" t="n">
-        <v>37388</v>
+        <v>37046</v>
       </c>
       <c r="M15" t="n">
-        <v>0.735</v>
+        <v>0.728</v>
       </c>
       <c r="N15" t="n">
-        <v>0.27</v>
+        <v>0.269</v>
       </c>
       <c r="O15" t="n">
-        <v>3.702</v>
+        <v>3.717</v>
       </c>
       <c r="P15" t="s">
         <v>102</v>
@@ -3362,7 +3350,7 @@
         <v>106</v>
       </c>
       <c r="C16" s="1" t="n">
-        <v>44049</v>
+        <v>44053</v>
       </c>
       <c r="D16" t="s">
         <v>107</v>
@@ -3372,31 +3360,31 @@
       </c>
       <c r="F16"/>
       <c r="G16" t="n">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="H16" t="n">
-        <v>87224</v>
+        <v>94259</v>
       </c>
       <c r="I16" t="n">
-        <v>17.123</v>
+        <v>18.504</v>
       </c>
       <c r="J16" t="n">
-        <v>1885</v>
+        <v>1476</v>
       </c>
       <c r="K16" t="n">
-        <v>0.37</v>
+        <v>0.29</v>
       </c>
       <c r="L16" t="n">
-        <v>1749</v>
+        <v>1758</v>
       </c>
       <c r="M16" t="n">
-        <v>0.343</v>
+        <v>0.345</v>
       </c>
       <c r="N16" t="n">
-        <v>0.295</v>
+        <v>0.35</v>
       </c>
       <c r="O16" t="n">
-        <v>3.385</v>
+        <v>2.855</v>
       </c>
       <c r="P16" t="s">
         <v>108</v>
@@ -3419,7 +3407,7 @@
         <v>112</v>
       </c>
       <c r="C17" s="1" t="n">
-        <v>44051</v>
+        <v>44052</v>
       </c>
       <c r="D17" t="s">
         <v>113</v>
@@ -3429,31 +3417,31 @@
       </c>
       <c r="F17"/>
       <c r="G17" t="n">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="H17" t="n">
-        <v>106753</v>
+        <v>109677</v>
       </c>
       <c r="I17" t="n">
-        <v>4.047</v>
+        <v>4.158</v>
       </c>
       <c r="J17" t="n">
-        <v>1245</v>
+        <v>2924</v>
       </c>
       <c r="K17" t="n">
-        <v>0.047</v>
+        <v>0.111</v>
       </c>
       <c r="L17" t="n">
-        <v>739</v>
+        <v>999</v>
       </c>
       <c r="M17" t="n">
-        <v>0.028</v>
+        <v>0.038</v>
       </c>
       <c r="N17" t="n">
-        <v>0.092</v>
+        <v>0.073</v>
       </c>
       <c r="O17" t="n">
-        <v>10.845</v>
+        <v>13.685</v>
       </c>
       <c r="P17" t="s">
         <v>114</v>
@@ -3476,7 +3464,7 @@
         <v>118</v>
       </c>
       <c r="C18" s="1" t="n">
-        <v>44053</v>
+        <v>44054</v>
       </c>
       <c r="D18" t="s">
         <v>119</v>
@@ -3486,31 +3474,31 @@
       </c>
       <c r="F18"/>
       <c r="G18" t="n">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="H18" t="n">
-        <v>129379</v>
+        <v>130688</v>
       </c>
       <c r="I18" t="n">
-        <v>31.515</v>
+        <v>31.834</v>
       </c>
       <c r="J18" t="n">
-        <v>1247</v>
+        <v>1309</v>
       </c>
       <c r="K18" t="n">
-        <v>0.304</v>
+        <v>0.319</v>
       </c>
       <c r="L18" t="n">
-        <v>1042</v>
+        <v>1070</v>
       </c>
       <c r="M18" t="n">
-        <v>0.254</v>
+        <v>0.261</v>
       </c>
       <c r="N18" t="n">
         <v>0.047</v>
       </c>
       <c r="O18" t="n">
-        <v>21.203</v>
+        <v>21.218</v>
       </c>
       <c r="P18" t="s">
         <v>120</v>
@@ -3533,7 +3521,7 @@
         <v>124</v>
       </c>
       <c r="C19" s="1" t="n">
-        <v>44051</v>
+        <v>44053</v>
       </c>
       <c r="D19" t="s">
         <v>125</v>
@@ -3545,31 +3533,31 @@
         <v>127</v>
       </c>
       <c r="G19" t="n">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="H19" t="n">
-        <v>297331</v>
+        <v>305652</v>
       </c>
       <c r="I19" t="n">
-        <v>26.251</v>
+        <v>26.985</v>
       </c>
       <c r="J19" t="n">
-        <v>4262</v>
+        <v>4054</v>
       </c>
       <c r="K19" t="n">
-        <v>0.376</v>
+        <v>0.358</v>
       </c>
       <c r="L19" t="n">
-        <v>3763</v>
+        <v>3970</v>
       </c>
       <c r="M19" t="n">
-        <v>0.332</v>
+        <v>0.351</v>
       </c>
       <c r="N19" t="n">
-        <v>0.008</v>
+        <v>0.011</v>
       </c>
       <c r="O19" t="n">
-        <v>119.19</v>
+        <v>90.521</v>
       </c>
       <c r="P19" t="s">
         <v>126</v>
@@ -3592,7 +3580,7 @@
         <v>131</v>
       </c>
       <c r="C20" s="1" t="n">
-        <v>44051</v>
+        <v>44053</v>
       </c>
       <c r="D20" t="s">
         <v>132</v>
@@ -3602,31 +3590,31 @@
       </c>
       <c r="F20"/>
       <c r="G20" t="n">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="H20" t="n">
-        <v>748872</v>
+        <v>757957</v>
       </c>
       <c r="I20" t="n">
-        <v>69.929</v>
+        <v>70.778</v>
       </c>
       <c r="J20" t="n">
-        <v>5106</v>
+        <v>5673</v>
       </c>
       <c r="K20" t="n">
-        <v>0.477</v>
+        <v>0.53</v>
       </c>
       <c r="L20" t="n">
-        <v>6420</v>
+        <v>6281</v>
       </c>
       <c r="M20" t="n">
-        <v>0.599</v>
+        <v>0.587</v>
       </c>
       <c r="N20" t="n">
-        <v>0.033</v>
+        <v>0.035</v>
       </c>
       <c r="O20" t="n">
-        <v>30.242</v>
+        <v>28.275</v>
       </c>
       <c r="P20" t="s">
         <v>45</v>
@@ -3649,7 +3637,7 @@
         <v>136</v>
       </c>
       <c r="C21" s="1" t="n">
-        <v>44048</v>
+        <v>44053</v>
       </c>
       <c r="D21" t="s">
         <v>137</v>
@@ -3659,27 +3647,27 @@
       </c>
       <c r="F21"/>
       <c r="G21" t="n">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="H21"/>
       <c r="I21"/>
       <c r="J21" t="n">
-        <v>489</v>
+        <v>299</v>
       </c>
       <c r="K21" t="n">
-        <v>0.005</v>
+        <v>0.003</v>
       </c>
       <c r="L21" t="n">
-        <v>367</v>
+        <v>359</v>
       </c>
       <c r="M21" t="n">
         <v>0.004</v>
       </c>
       <c r="N21" t="n">
-        <v>0.118</v>
+        <v>0.135</v>
       </c>
       <c r="O21" t="n">
-        <v>8.451</v>
+        <v>7.413</v>
       </c>
       <c r="P21" t="s">
         <v>138</v>
@@ -3702,7 +3690,7 @@
         <v>142</v>
       </c>
       <c r="C22" s="1" t="n">
-        <v>44052</v>
+        <v>44053</v>
       </c>
       <c r="D22" t="s">
         <v>143</v>
@@ -3712,31 +3700,31 @@
       </c>
       <c r="F22"/>
       <c r="G22" t="n">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="H22" t="n">
-        <v>1721479</v>
+        <v>1745491</v>
       </c>
       <c r="I22" t="n">
-        <v>297.206</v>
+        <v>301.352</v>
       </c>
       <c r="J22" t="n">
-        <v>3826</v>
+        <v>6541</v>
       </c>
       <c r="K22" t="n">
-        <v>0.661</v>
+        <v>1.129</v>
       </c>
       <c r="L22" t="n">
-        <v>21501</v>
+        <v>21583</v>
       </c>
       <c r="M22" t="n">
-        <v>3.712</v>
+        <v>3.726</v>
       </c>
       <c r="N22" t="n">
         <v>0.004</v>
       </c>
       <c r="O22" t="n">
-        <v>230.485</v>
+        <v>231.364</v>
       </c>
       <c r="P22" t="s">
         <v>144</v>
@@ -3759,7 +3747,7 @@
         <v>148</v>
       </c>
       <c r="C23" s="1" t="n">
-        <v>44051</v>
+        <v>44052</v>
       </c>
       <c r="D23" t="s">
         <v>149</v>
@@ -3771,25 +3759,25 @@
         <v>151</v>
       </c>
       <c r="G23" t="n">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="H23" t="n">
-        <v>202394</v>
+        <v>204729</v>
       </c>
       <c r="I23" t="n">
-        <v>11.472</v>
+        <v>11.604</v>
       </c>
       <c r="J23" t="n">
-        <v>4537</v>
+        <v>2335</v>
       </c>
       <c r="K23" t="n">
-        <v>0.257</v>
+        <v>0.132</v>
       </c>
       <c r="L23" t="n">
-        <v>2621</v>
+        <v>2829</v>
       </c>
       <c r="M23" t="n">
-        <v>0.149</v>
+        <v>0.16</v>
       </c>
       <c r="N23"/>
       <c r="O23"/>
@@ -3814,7 +3802,7 @@
         <v>155</v>
       </c>
       <c r="C24" s="1" t="n">
-        <v>44049</v>
+        <v>44053</v>
       </c>
       <c r="D24" t="s">
         <v>156</v>
@@ -3824,31 +3812,31 @@
       </c>
       <c r="F24"/>
       <c r="G24" t="n">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="H24" t="n">
-        <v>256176</v>
+        <v>266079</v>
       </c>
       <c r="I24" t="n">
-        <v>39.496</v>
+        <v>41.022</v>
       </c>
       <c r="J24" t="n">
-        <v>2464</v>
+        <v>2492</v>
       </c>
       <c r="K24" t="n">
-        <v>0.38</v>
+        <v>0.384</v>
       </c>
       <c r="L24" t="n">
-        <v>2466</v>
+        <v>2470</v>
       </c>
       <c r="M24" t="n">
-        <v>0.38</v>
+        <v>0.381</v>
       </c>
       <c r="N24" t="n">
-        <v>0.166</v>
+        <v>0.172</v>
       </c>
       <c r="O24" t="n">
-        <v>6.036</v>
+        <v>5.812</v>
       </c>
       <c r="P24" t="s">
         <v>157</v>
@@ -3871,7 +3859,7 @@
         <v>161</v>
       </c>
       <c r="C25" s="1" t="n">
-        <v>44052</v>
+        <v>44054</v>
       </c>
       <c r="D25" t="s">
         <v>162</v>
@@ -3881,31 +3869,31 @@
       </c>
       <c r="F25"/>
       <c r="G25" t="n">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="H25" t="n">
-        <v>126738</v>
+        <v>129633</v>
       </c>
       <c r="I25" t="n">
-        <v>95.54</v>
+        <v>97.723</v>
       </c>
       <c r="J25" t="n">
-        <v>1120</v>
+        <v>1427</v>
       </c>
       <c r="K25" t="n">
-        <v>0.844</v>
+        <v>1.076</v>
       </c>
       <c r="L25" t="n">
-        <v>916</v>
+        <v>1103</v>
       </c>
       <c r="M25" t="n">
-        <v>0.691</v>
+        <v>0.831</v>
       </c>
       <c r="N25" t="n">
-        <v>0.012</v>
+        <v>0.01</v>
       </c>
       <c r="O25" t="n">
-        <v>85.493</v>
+        <v>98.987</v>
       </c>
       <c r="P25" t="s">
         <v>164</v>
@@ -3928,7 +3916,7 @@
         <v>169</v>
       </c>
       <c r="C26" s="1" t="n">
-        <v>44031</v>
+        <v>44045</v>
       </c>
       <c r="D26" t="s">
         <v>170</v>
@@ -3938,27 +3926,27 @@
       </c>
       <c r="F26"/>
       <c r="G26" t="n">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="H26" t="n">
-        <v>331266</v>
+        <v>437319</v>
       </c>
       <c r="I26" t="n">
-        <v>2.881</v>
+        <v>3.804</v>
       </c>
       <c r="J26"/>
       <c r="K26"/>
       <c r="L26" t="n">
-        <v>5959</v>
+        <v>7575</v>
       </c>
       <c r="M26" t="n">
-        <v>0.052</v>
+        <v>0.066</v>
       </c>
       <c r="N26" t="n">
-        <v>0.042</v>
+        <v>0.1</v>
       </c>
       <c r="O26" t="n">
-        <v>23.904</v>
+        <v>9.993</v>
       </c>
       <c r="P26" t="s">
         <v>171</v>
@@ -4049,28 +4037,28 @@
         <v>168</v>
       </c>
       <c r="H28" t="n">
-        <v>408540</v>
+        <v>431048</v>
       </c>
       <c r="I28" t="n">
-        <v>73.734</v>
+        <v>77.796</v>
       </c>
       <c r="J28" t="n">
-        <v>64</v>
+        <v>6326</v>
       </c>
       <c r="K28" t="n">
-        <v>0.012</v>
+        <v>1.142</v>
       </c>
       <c r="L28" t="n">
-        <v>3247</v>
+        <v>6463</v>
       </c>
       <c r="M28" t="n">
-        <v>0.586</v>
+        <v>1.166</v>
       </c>
       <c r="N28" t="n">
-        <v>0.006</v>
+        <v>0.003</v>
       </c>
       <c r="O28" t="n">
-        <v>173.504</v>
+        <v>345.351</v>
       </c>
       <c r="P28" t="s">
         <v>183</v>
@@ -4093,7 +4081,7 @@
         <v>186</v>
       </c>
       <c r="C29" s="1" t="n">
-        <v>44049</v>
+        <v>44050</v>
       </c>
       <c r="D29" t="s">
         <v>187</v>
@@ -4103,27 +4091,27 @@
       </c>
       <c r="F29"/>
       <c r="G29" t="n">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H29"/>
       <c r="I29"/>
       <c r="J29" t="n">
-        <v>93162</v>
+        <v>95552</v>
       </c>
       <c r="K29" t="n">
-        <v>1.427</v>
+        <v>1.464</v>
       </c>
       <c r="L29" t="n">
-        <v>76232</v>
+        <v>76597</v>
       </c>
       <c r="M29" t="n">
-        <v>1.168</v>
+        <v>1.173</v>
       </c>
       <c r="N29" t="n">
         <v>0.017</v>
       </c>
       <c r="O29" t="n">
-        <v>60.413</v>
+        <v>59.181</v>
       </c>
       <c r="P29" t="s">
         <v>188</v>
@@ -4256,7 +4244,7 @@
         <v>204</v>
       </c>
       <c r="C32" s="1" t="n">
-        <v>44049</v>
+        <v>44050</v>
       </c>
       <c r="D32" t="s">
         <v>205</v>
@@ -4266,31 +4254,31 @@
       </c>
       <c r="F32"/>
       <c r="G32" t="n">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="H32" t="n">
-        <v>413835</v>
+        <v>415671</v>
       </c>
       <c r="I32" t="n">
-        <v>13.318</v>
+        <v>13.377</v>
       </c>
       <c r="J32" t="n">
-        <v>2296</v>
+        <v>1836</v>
       </c>
       <c r="K32" t="n">
-        <v>0.074</v>
+        <v>0.059</v>
       </c>
       <c r="L32" t="n">
-        <v>2443</v>
+        <v>2318</v>
       </c>
       <c r="M32" t="n">
-        <v>0.079</v>
+        <v>0.075</v>
       </c>
       <c r="N32" t="n">
-        <v>0.23</v>
+        <v>0.305</v>
       </c>
       <c r="O32" t="n">
-        <v>4.348</v>
+        <v>3.275</v>
       </c>
       <c r="P32" t="s">
         <v>207</v>
@@ -4313,7 +4301,7 @@
         <v>211</v>
       </c>
       <c r="C33" s="1" t="n">
-        <v>44052</v>
+        <v>44054</v>
       </c>
       <c r="D33" t="s">
         <v>212</v>
@@ -4323,31 +4311,31 @@
       </c>
       <c r="F33"/>
       <c r="G33" t="n">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="H33" t="n">
-        <v>650998</v>
+        <v>668739</v>
       </c>
       <c r="I33" t="n">
-        <v>62.457</v>
+        <v>64.16</v>
       </c>
       <c r="J33" t="n">
-        <v>10701</v>
+        <v>10561</v>
       </c>
       <c r="K33" t="n">
-        <v>1.027</v>
+        <v>1.013</v>
       </c>
       <c r="L33" t="n">
-        <v>15080</v>
+        <v>9861</v>
       </c>
       <c r="M33" t="n">
-        <v>1.447</v>
+        <v>0.946</v>
       </c>
       <c r="N33" t="n">
-        <v>0.008</v>
+        <v>0.015</v>
       </c>
       <c r="O33" t="n">
-        <v>126.571</v>
+        <v>68.208</v>
       </c>
       <c r="P33" t="s">
         <v>214</v>
@@ -4474,7 +4462,7 @@
         <v>233</v>
       </c>
       <c r="C36" s="1" t="n">
-        <v>44052</v>
+        <v>44053</v>
       </c>
       <c r="D36" t="s">
         <v>234</v>
@@ -4484,31 +4472,31 @@
       </c>
       <c r="F36"/>
       <c r="G36" t="n">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="H36" t="n">
-        <v>78467</v>
+        <v>78812</v>
       </c>
       <c r="I36" t="n">
-        <v>229.94</v>
+        <v>230.951</v>
       </c>
       <c r="J36" t="n">
-        <v>232</v>
+        <v>345</v>
       </c>
       <c r="K36" t="n">
-        <v>0.68</v>
+        <v>1.011</v>
       </c>
       <c r="L36" t="n">
-        <v>644</v>
+        <v>583</v>
       </c>
       <c r="M36" t="n">
-        <v>1.887</v>
+        <v>1.708</v>
       </c>
       <c r="N36" t="n">
-        <v>0.014</v>
+        <v>0.012</v>
       </c>
       <c r="O36" t="n">
-        <v>72.71</v>
+        <v>80.02</v>
       </c>
       <c r="P36" t="s">
         <v>235</v>
@@ -4590,7 +4578,7 @@
         <v>243</v>
       </c>
       <c r="C38" s="1" t="n">
-        <v>44053</v>
+        <v>44054</v>
       </c>
       <c r="D38" t="s">
         <v>239</v>
@@ -4602,31 +4590,31 @@
         <v>241</v>
       </c>
       <c r="G38" t="n">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="H38" t="n">
-        <v>24583558</v>
+        <v>25281848</v>
       </c>
       <c r="I38" t="n">
-        <v>17.814</v>
+        <v>18.32</v>
       </c>
       <c r="J38" t="n">
-        <v>477023</v>
+        <v>698290</v>
       </c>
       <c r="K38" t="n">
-        <v>0.346</v>
+        <v>0.506</v>
       </c>
       <c r="L38" t="n">
-        <v>625814</v>
+        <v>631014</v>
       </c>
       <c r="M38" t="n">
-        <v>0.453</v>
+        <v>0.457</v>
       </c>
       <c r="N38" t="n">
-        <v>0.094</v>
+        <v>0.093</v>
       </c>
       <c r="O38" t="n">
-        <v>10.649</v>
+        <v>10.697</v>
       </c>
       <c r="P38" t="s">
         <v>240</v>
@@ -4649,7 +4637,7 @@
         <v>245</v>
       </c>
       <c r="C39" s="1" t="n">
-        <v>44053</v>
+        <v>44054</v>
       </c>
       <c r="D39" t="s">
         <v>246</v>
@@ -4659,22 +4647,22 @@
       </c>
       <c r="F39"/>
       <c r="G39" t="n">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="H39" t="n">
-        <v>984893</v>
+        <v>998406</v>
       </c>
       <c r="I39" t="n">
-        <v>3.601</v>
+        <v>3.65</v>
       </c>
       <c r="J39" t="n">
-        <v>12299</v>
+        <v>13513</v>
       </c>
       <c r="K39" t="n">
-        <v>0.045</v>
+        <v>0.049</v>
       </c>
       <c r="L39" t="n">
-        <v>12909</v>
+        <v>12917</v>
       </c>
       <c r="M39" t="n">
         <v>0.047</v>
@@ -4706,7 +4694,7 @@
         <v>251</v>
       </c>
       <c r="C40" s="1" t="n">
-        <v>44053</v>
+        <v>44054</v>
       </c>
       <c r="D40" t="s">
         <v>252</v>
@@ -4716,31 +4704,31 @@
       </c>
       <c r="F40"/>
       <c r="G40" t="n">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="H40" t="n">
-        <v>2711817</v>
+        <v>2736514</v>
       </c>
       <c r="I40" t="n">
-        <v>32.286</v>
+        <v>32.58</v>
       </c>
       <c r="J40" t="n">
-        <v>25319</v>
+        <v>24697</v>
       </c>
       <c r="K40" t="n">
-        <v>0.301</v>
+        <v>0.294</v>
       </c>
       <c r="L40" t="n">
-        <v>25308</v>
+        <v>25163</v>
       </c>
       <c r="M40" t="n">
-        <v>0.301</v>
+        <v>0.3</v>
       </c>
       <c r="N40" t="n">
-        <v>0.098</v>
+        <v>0.095</v>
       </c>
       <c r="O40" t="n">
-        <v>10.255</v>
+        <v>10.479</v>
       </c>
       <c r="P40" t="s">
         <v>253</v>
@@ -4763,7 +4751,7 @@
         <v>257</v>
       </c>
       <c r="C41" s="1" t="n">
-        <v>44051</v>
+        <v>44054</v>
       </c>
       <c r="D41" t="s">
         <v>258</v>
@@ -4773,31 +4761,31 @@
       </c>
       <c r="F41"/>
       <c r="G41" t="n">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="H41" t="n">
-        <v>662242</v>
+        <v>674695</v>
       </c>
       <c r="I41" t="n">
-        <v>134.117</v>
+        <v>136.639</v>
       </c>
       <c r="J41" t="n">
-        <v>4345</v>
+        <v>3937</v>
       </c>
       <c r="K41" t="n">
-        <v>0.88</v>
+        <v>0.797</v>
       </c>
       <c r="L41" t="n">
-        <v>3726</v>
+        <v>4339</v>
       </c>
       <c r="M41" t="n">
-        <v>0.755</v>
+        <v>0.879</v>
       </c>
       <c r="N41" t="n">
-        <v>0.016</v>
+        <v>0.018</v>
       </c>
       <c r="O41" t="n">
-        <v>64.4</v>
+        <v>54.237</v>
       </c>
       <c r="P41" t="s">
         <v>259</v>
@@ -4820,7 +4808,7 @@
         <v>262</v>
       </c>
       <c r="C42" s="1" t="n">
-        <v>44046</v>
+        <v>44048</v>
       </c>
       <c r="D42" t="s">
         <v>263</v>
@@ -4830,31 +4818,31 @@
       </c>
       <c r="F42"/>
       <c r="G42" t="n">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="H42" t="n">
-        <v>1815205</v>
+        <v>1867725</v>
       </c>
       <c r="I42" t="n">
-        <v>209.716</v>
+        <v>215.784</v>
       </c>
       <c r="J42" t="n">
-        <v>23575</v>
+        <v>25796</v>
       </c>
       <c r="K42" t="n">
-        <v>2.724</v>
+        <v>2.98</v>
       </c>
       <c r="L42" t="n">
-        <v>19790</v>
+        <v>19726</v>
       </c>
       <c r="M42" t="n">
-        <v>2.286</v>
+        <v>2.279</v>
       </c>
       <c r="N42" t="n">
-        <v>0.08</v>
+        <v>0.073</v>
       </c>
       <c r="O42" t="n">
-        <v>12.515</v>
+        <v>13.689</v>
       </c>
       <c r="P42" t="s">
         <v>45</v>
@@ -4877,7 +4865,7 @@
         <v>268</v>
       </c>
       <c r="C43" s="1" t="n">
-        <v>44052</v>
+        <v>44054</v>
       </c>
       <c r="D43" t="s">
         <v>269</v>
@@ -4889,31 +4877,31 @@
         <v>271</v>
       </c>
       <c r="G43" t="n">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="H43" t="n">
-        <v>4296730</v>
+        <v>4329697</v>
       </c>
       <c r="I43" t="n">
-        <v>71.065</v>
+        <v>71.61</v>
       </c>
       <c r="J43" t="n">
-        <v>22773</v>
+        <v>22063</v>
       </c>
       <c r="K43" t="n">
-        <v>0.377</v>
+        <v>0.365</v>
       </c>
       <c r="L43" t="n">
-        <v>25523</v>
+        <v>24953</v>
       </c>
       <c r="M43" t="n">
-        <v>0.422</v>
+        <v>0.413</v>
       </c>
       <c r="N43" t="n">
-        <v>0.013</v>
+        <v>0.015</v>
       </c>
       <c r="O43" t="n">
-        <v>78.671</v>
+        <v>67.285</v>
       </c>
       <c r="P43" t="s">
         <v>272</v>
@@ -4936,7 +4924,7 @@
         <v>275</v>
       </c>
       <c r="C44" s="1" t="n">
-        <v>44052</v>
+        <v>44054</v>
       </c>
       <c r="D44" t="s">
         <v>269</v>
@@ -4948,31 +4936,31 @@
         <v>271</v>
       </c>
       <c r="G44" t="n">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="H44" t="n">
-        <v>7249844</v>
+        <v>7316918</v>
       </c>
       <c r="I44" t="n">
-        <v>119.908</v>
+        <v>121.017</v>
       </c>
       <c r="J44" t="n">
-        <v>37637</v>
+        <v>40642</v>
       </c>
       <c r="K44" t="n">
-        <v>0.622</v>
+        <v>0.672</v>
       </c>
       <c r="L44" t="n">
-        <v>47583</v>
+        <v>47476</v>
       </c>
       <c r="M44" t="n">
-        <v>0.787</v>
+        <v>0.785</v>
       </c>
       <c r="N44" t="n">
-        <v>0.007</v>
+        <v>0.008</v>
       </c>
       <c r="O44" t="n">
-        <v>146.667</v>
+        <v>128.017</v>
       </c>
       <c r="P44" t="s">
         <v>272</v>
@@ -4995,7 +4983,7 @@
         <v>278</v>
       </c>
       <c r="C45" s="1" t="n">
-        <v>44052</v>
+        <v>44054</v>
       </c>
       <c r="D45" t="s">
         <v>279</v>
@@ -5007,31 +4995,31 @@
         <v>281</v>
       </c>
       <c r="G45" t="n">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="H45" t="n">
-        <v>1001281</v>
+        <v>1024235</v>
       </c>
       <c r="I45" t="n">
-        <v>7.917</v>
+        <v>8.098</v>
       </c>
       <c r="J45" t="n">
-        <v>15180</v>
+        <v>8038</v>
       </c>
       <c r="K45" t="n">
-        <v>0.12</v>
+        <v>0.064</v>
       </c>
       <c r="L45" t="n">
-        <v>23554</v>
+        <v>21014</v>
       </c>
       <c r="M45" t="n">
-        <v>0.186</v>
+        <v>0.166</v>
       </c>
       <c r="N45" t="n">
-        <v>0.065</v>
+        <v>0.057</v>
       </c>
       <c r="O45" t="n">
-        <v>15.406</v>
+        <v>17.553</v>
       </c>
       <c r="P45" t="s">
         <v>282</v>
@@ -5054,7 +5042,7 @@
         <v>285</v>
       </c>
       <c r="C46" s="1" t="n">
-        <v>44049</v>
+        <v>44052</v>
       </c>
       <c r="D46" t="s">
         <v>286</v>
@@ -5066,31 +5054,31 @@
         <v>287</v>
       </c>
       <c r="G46" t="n">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="H46" t="n">
-        <v>1274091</v>
+        <v>1288757</v>
       </c>
       <c r="I46" t="n">
-        <v>10.074</v>
+        <v>10.19</v>
       </c>
       <c r="J46" t="n">
-        <v>25224</v>
+        <v>4546</v>
       </c>
       <c r="K46" t="n">
-        <v>0.199</v>
+        <v>0.036</v>
       </c>
       <c r="L46" t="n">
-        <v>23530</v>
+        <v>16662</v>
       </c>
       <c r="M46" t="n">
-        <v>0.186</v>
+        <v>0.132</v>
       </c>
       <c r="N46" t="n">
-        <v>0.06</v>
+        <v>0.092</v>
       </c>
       <c r="O46" t="n">
-        <v>16.8</v>
+        <v>10.898</v>
       </c>
       <c r="P46" t="s">
         <v>282</v>
@@ -5113,7 +5101,7 @@
         <v>290</v>
       </c>
       <c r="C47" s="1" t="n">
-        <v>44050</v>
+        <v>44054</v>
       </c>
       <c r="D47" t="s">
         <v>291</v>
@@ -5123,31 +5111,31 @@
       </c>
       <c r="F47"/>
       <c r="G47" t="n">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="H47" t="n">
-        <v>2183308</v>
+        <v>2236924</v>
       </c>
       <c r="I47" t="n">
-        <v>116.277</v>
+        <v>119.133</v>
       </c>
       <c r="J47" t="n">
-        <v>19595</v>
+        <v>10055</v>
       </c>
       <c r="K47" t="n">
-        <v>1.044</v>
+        <v>0.536</v>
       </c>
       <c r="L47" t="n">
-        <v>15740</v>
+        <v>15795</v>
       </c>
       <c r="M47" t="n">
-        <v>0.838</v>
+        <v>0.841</v>
       </c>
       <c r="N47" t="n">
-        <v>0.071</v>
+        <v>0.057</v>
       </c>
       <c r="O47" t="n">
-        <v>14.046</v>
+        <v>17.428</v>
       </c>
       <c r="P47" t="s">
         <v>292</v>
@@ -5170,7 +5158,7 @@
         <v>295</v>
       </c>
       <c r="C48" s="1" t="n">
-        <v>44049</v>
+        <v>44054</v>
       </c>
       <c r="D48" t="s">
         <v>296</v>
@@ -5180,31 +5168,31 @@
       </c>
       <c r="F48"/>
       <c r="G48" t="n">
-        <v>124</v>
+        <v>129</v>
       </c>
       <c r="H48" t="n">
-        <v>335318</v>
+        <v>362501</v>
       </c>
       <c r="I48" t="n">
-        <v>6.236</v>
+        <v>6.742</v>
       </c>
       <c r="J48" t="n">
-        <v>6195</v>
+        <v>4171</v>
       </c>
       <c r="K48" t="n">
-        <v>0.115</v>
+        <v>0.078</v>
       </c>
       <c r="L48" t="n">
-        <v>5720</v>
+        <v>5654</v>
       </c>
       <c r="M48" t="n">
-        <v>0.106</v>
+        <v>0.105</v>
       </c>
       <c r="N48" t="n">
-        <v>0.119</v>
+        <v>0.109</v>
       </c>
       <c r="O48" t="n">
-        <v>8.433</v>
+        <v>9.138</v>
       </c>
       <c r="P48" t="s">
         <v>45</v>
@@ -5227,7 +5215,7 @@
         <v>301</v>
       </c>
       <c r="C49" s="1" t="n">
-        <v>44049</v>
+        <v>44054</v>
       </c>
       <c r="D49" t="s">
         <v>302</v>
@@ -5237,31 +5225,31 @@
       </c>
       <c r="F49"/>
       <c r="G49" t="n">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="H49" t="n">
-        <v>522200</v>
+        <v>539461</v>
       </c>
       <c r="I49" t="n">
-        <v>122.279</v>
+        <v>126.321</v>
       </c>
       <c r="J49" t="n">
-        <v>3599</v>
+        <v>3658</v>
       </c>
       <c r="K49" t="n">
-        <v>0.843</v>
+        <v>0.857</v>
       </c>
       <c r="L49" t="n">
-        <v>2862</v>
+        <v>3630</v>
       </c>
       <c r="M49" t="n">
-        <v>0.67</v>
+        <v>0.85</v>
       </c>
       <c r="N49" t="n">
-        <v>0.176</v>
+        <v>0.161</v>
       </c>
       <c r="O49" t="n">
-        <v>5.688</v>
+        <v>6.196</v>
       </c>
       <c r="P49" t="s">
         <v>303</v>
@@ -5284,7 +5272,7 @@
         <v>307</v>
       </c>
       <c r="C50" s="1" t="n">
-        <v>44052</v>
+        <v>44055</v>
       </c>
       <c r="D50" t="s">
         <v>308</v>
@@ -5296,32 +5284,28 @@
         <v>310</v>
       </c>
       <c r="G50" t="n">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="H50" t="n">
-        <v>213534</v>
+        <v>218756</v>
       </c>
       <c r="I50" t="n">
-        <v>113.208</v>
+        <v>115.977</v>
       </c>
       <c r="J50" t="n">
-        <v>1597</v>
+        <v>2226</v>
       </c>
       <c r="K50" t="n">
-        <v>0.847</v>
+        <v>1.18</v>
       </c>
       <c r="L50" t="n">
-        <v>1746</v>
+        <v>1811</v>
       </c>
       <c r="M50" t="n">
-        <v>0.926</v>
-      </c>
-      <c r="N50" t="n">
-        <v>0.004</v>
-      </c>
-      <c r="O50" t="n">
-        <v>244.44</v>
-      </c>
+        <v>0.96</v>
+      </c>
+      <c r="N50"/>
+      <c r="O50"/>
       <c r="P50" t="s">
         <v>309</v>
       </c>
@@ -5343,7 +5327,7 @@
         <v>313</v>
       </c>
       <c r="C51" s="1" t="n">
-        <v>44053</v>
+        <v>44055</v>
       </c>
       <c r="D51" t="s">
         <v>314</v>
@@ -5353,28 +5337,24 @@
       </c>
       <c r="F51"/>
       <c r="G51" t="n">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="H51" t="n">
-        <v>553388</v>
+        <v>561555</v>
       </c>
       <c r="I51" t="n">
-        <v>203.28</v>
+        <v>206.28</v>
       </c>
       <c r="J51"/>
       <c r="K51"/>
       <c r="L51" t="n">
-        <v>3124</v>
+        <v>3282</v>
       </c>
       <c r="M51" t="n">
-        <v>1.148</v>
-      </c>
-      <c r="N51" t="n">
-        <v>0.006</v>
-      </c>
-      <c r="O51" t="n">
-        <v>154</v>
-      </c>
+        <v>1.206</v>
+      </c>
+      <c r="N51"/>
+      <c r="O51"/>
       <c r="P51" t="s">
         <v>45</v>
       </c>
@@ -5396,7 +5376,7 @@
         <v>317</v>
       </c>
       <c r="C52" s="1" t="n">
-        <v>44048</v>
+        <v>44053</v>
       </c>
       <c r="D52" t="s">
         <v>318</v>
@@ -5406,31 +5386,31 @@
       </c>
       <c r="F52"/>
       <c r="G52" t="n">
-        <v>160</v>
+        <v>165</v>
       </c>
       <c r="H52" t="n">
-        <v>443164</v>
+        <v>451407</v>
       </c>
       <c r="I52" t="n">
-        <v>707.957</v>
+        <v>721.125</v>
       </c>
       <c r="J52" t="n">
-        <v>3846</v>
+        <v>1596</v>
       </c>
       <c r="K52" t="n">
-        <v>6.144</v>
+        <v>2.55</v>
       </c>
       <c r="L52" t="n">
-        <v>3271</v>
+        <v>2214</v>
       </c>
       <c r="M52" t="n">
-        <v>5.225</v>
+        <v>3.537</v>
       </c>
       <c r="N52" t="n">
-        <v>0.024</v>
+        <v>0.027</v>
       </c>
       <c r="O52" t="n">
-        <v>42.245</v>
+        <v>37.077</v>
       </c>
       <c r="P52" t="s">
         <v>319</v>
@@ -5453,7 +5433,7 @@
         <v>322</v>
       </c>
       <c r="C53" s="1" t="n">
-        <v>44052</v>
+        <v>44054</v>
       </c>
       <c r="D53" t="s">
         <v>323</v>
@@ -5465,31 +5445,31 @@
         <v>325</v>
       </c>
       <c r="G53" t="n">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="H53" t="n">
-        <v>1045976</v>
+        <v>1063304</v>
       </c>
       <c r="I53" t="n">
-        <v>32.317</v>
+        <v>32.853</v>
       </c>
       <c r="J53" t="n">
-        <v>9637</v>
+        <v>9773</v>
       </c>
       <c r="K53" t="n">
-        <v>0.298</v>
+        <v>0.302</v>
       </c>
       <c r="L53" t="n">
-        <v>9543</v>
+        <v>10282</v>
       </c>
       <c r="M53" t="n">
-        <v>0.295</v>
+        <v>0.318</v>
       </c>
       <c r="N53" t="n">
         <v>0.001</v>
       </c>
       <c r="O53" t="n">
-        <v>785.894</v>
+        <v>773.914</v>
       </c>
       <c r="P53" t="s">
         <v>45</v>
@@ -5512,7 +5492,7 @@
         <v>329</v>
       </c>
       <c r="C54" s="1" t="n">
-        <v>44049</v>
+        <v>44053</v>
       </c>
       <c r="D54" t="s">
         <v>330</v>
@@ -5522,31 +5502,31 @@
       </c>
       <c r="F54"/>
       <c r="G54" t="n">
-        <v>127</v>
+        <v>131</v>
       </c>
       <c r="H54" t="n">
-        <v>85587</v>
+        <v>89555</v>
       </c>
       <c r="I54" t="n">
-        <v>158.336</v>
+        <v>165.676</v>
       </c>
       <c r="J54" t="n">
-        <v>1443</v>
+        <v>1163</v>
       </c>
       <c r="K54" t="n">
-        <v>2.67</v>
+        <v>2.152</v>
       </c>
       <c r="L54" t="n">
-        <v>1078</v>
+        <v>1050</v>
       </c>
       <c r="M54" t="n">
-        <v>1.994</v>
+        <v>1.942</v>
       </c>
       <c r="N54" t="n">
-        <v>0.136</v>
+        <v>0.119</v>
       </c>
       <c r="O54" t="n">
-        <v>7.348</v>
+        <v>8.381</v>
       </c>
       <c r="P54" t="s">
         <v>332</v>
@@ -5626,7 +5606,7 @@
         <v>342</v>
       </c>
       <c r="C56" s="1" t="n">
-        <v>44048</v>
+        <v>44050</v>
       </c>
       <c r="D56" t="s">
         <v>343</v>
@@ -5636,31 +5616,31 @@
       </c>
       <c r="F56"/>
       <c r="G56" t="n">
-        <v>218</v>
+        <v>220</v>
       </c>
       <c r="H56" t="n">
-        <v>998821</v>
+        <v>1026126</v>
       </c>
       <c r="I56" t="n">
-        <v>7.747</v>
+        <v>7.959</v>
       </c>
       <c r="J56" t="n">
-        <v>8663</v>
+        <v>7187</v>
       </c>
       <c r="K56" t="n">
-        <v>0.067</v>
+        <v>0.056</v>
       </c>
       <c r="L56" t="n">
-        <v>9438</v>
+        <v>9168</v>
       </c>
       <c r="M56" t="n">
-        <v>0.073</v>
+        <v>0.071</v>
       </c>
       <c r="N56" t="n">
-        <v>0.715</v>
+        <v>0.725</v>
       </c>
       <c r="O56" t="n">
-        <v>1.398</v>
+        <v>1.38</v>
       </c>
       <c r="P56" t="s">
         <v>345</v>
@@ -5683,7 +5663,7 @@
         <v>349</v>
       </c>
       <c r="C57" s="1" t="n">
-        <v>44049</v>
+        <v>44053</v>
       </c>
       <c r="D57" t="s">
         <v>350</v>
@@ -5693,31 +5673,31 @@
       </c>
       <c r="F57"/>
       <c r="G57" t="n">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="H57" t="n">
-        <v>1383816</v>
+        <v>1472095</v>
       </c>
       <c r="I57" t="n">
-        <v>37.491</v>
+        <v>39.883</v>
       </c>
       <c r="J57" t="n">
-        <v>22266</v>
+        <v>22127</v>
       </c>
       <c r="K57" t="n">
-        <v>0.603</v>
+        <v>0.599</v>
       </c>
       <c r="L57" t="n">
-        <v>21803</v>
+        <v>22176</v>
       </c>
       <c r="M57" t="n">
-        <v>0.591</v>
+        <v>0.601</v>
       </c>
       <c r="N57" t="n">
-        <v>0.041</v>
+        <v>0.05</v>
       </c>
       <c r="O57" t="n">
-        <v>24.276</v>
+        <v>20.16</v>
       </c>
       <c r="P57" t="s">
         <v>351</v>
@@ -5740,7 +5720,7 @@
         <v>355</v>
       </c>
       <c r="C58" s="1" t="n">
-        <v>44046</v>
+        <v>44052</v>
       </c>
       <c r="D58" t="s">
         <v>356</v>
@@ -5750,31 +5730,31 @@
       </c>
       <c r="F58"/>
       <c r="G58" t="n">
-        <v>118</v>
+        <v>124</v>
       </c>
       <c r="H58" t="n">
-        <v>120292</v>
+        <v>126828</v>
       </c>
       <c r="I58" t="n">
-        <v>2.211</v>
+        <v>2.331</v>
       </c>
       <c r="J58" t="n">
-        <v>1150</v>
+        <v>1001</v>
       </c>
       <c r="K58" t="n">
-        <v>0.021</v>
+        <v>0.018</v>
       </c>
       <c r="L58" t="n">
-        <v>1130</v>
+        <v>1098</v>
       </c>
       <c r="M58" t="n">
-        <v>0.021</v>
+        <v>0.02</v>
       </c>
       <c r="N58" t="n">
-        <v>0</v>
+        <v>0.001</v>
       </c>
       <c r="O58" t="n">
-        <v>2636.667</v>
+        <v>1281</v>
       </c>
       <c r="P58" t="s">
         <v>357</v>
@@ -5797,7 +5777,7 @@
         <v>361</v>
       </c>
       <c r="C59" s="1" t="n">
-        <v>44049</v>
+        <v>44054</v>
       </c>
       <c r="D59" t="s">
         <v>362</v>
@@ -5807,31 +5787,31 @@
       </c>
       <c r="F59"/>
       <c r="G59" t="n">
-        <v>168</v>
+        <v>173</v>
       </c>
       <c r="H59" t="n">
-        <v>419575</v>
+        <v>462698</v>
       </c>
       <c r="I59" t="n">
-        <v>14.4</v>
+        <v>15.88</v>
       </c>
       <c r="J59" t="n">
-        <v>6622</v>
+        <v>10462</v>
       </c>
       <c r="K59" t="n">
-        <v>0.227</v>
+        <v>0.359</v>
       </c>
       <c r="L59" t="n">
-        <v>7847</v>
+        <v>8015</v>
       </c>
       <c r="M59" t="n">
-        <v>0.269</v>
+        <v>0.275</v>
       </c>
       <c r="N59" t="n">
-        <v>0.039</v>
+        <v>0.046</v>
       </c>
       <c r="O59" t="n">
-        <v>25.947</v>
+        <v>21.916</v>
       </c>
       <c r="P59" t="s">
         <v>363</v>
@@ -5854,7 +5834,7 @@
         <v>367</v>
       </c>
       <c r="C60" s="1" t="n">
-        <v>44045</v>
+        <v>44052</v>
       </c>
       <c r="D60" t="s">
         <v>368</v>
@@ -5864,27 +5844,27 @@
       </c>
       <c r="F60"/>
       <c r="G60" t="n">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H60" t="n">
-        <v>1079860</v>
+        <v>1195475</v>
       </c>
       <c r="I60" t="n">
-        <v>63.021</v>
+        <v>69.769</v>
       </c>
       <c r="J60"/>
       <c r="K60"/>
       <c r="L60" t="n">
-        <v>16504</v>
+        <v>15822</v>
       </c>
       <c r="M60" t="n">
-        <v>0.963</v>
+        <v>0.923</v>
       </c>
       <c r="N60" t="n">
-        <v>0.017</v>
+        <v>0.029</v>
       </c>
       <c r="O60" t="n">
-        <v>57.764</v>
+        <v>34.026</v>
       </c>
       <c r="P60" t="s">
         <v>370</v>
@@ -5907,7 +5887,7 @@
         <v>374</v>
       </c>
       <c r="C61" s="1" t="n">
-        <v>44052</v>
+        <v>44054</v>
       </c>
       <c r="D61" t="s">
         <v>375</v>
@@ -5917,31 +5897,31 @@
       </c>
       <c r="F61"/>
       <c r="G61" t="n">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="H61" t="n">
-        <v>496606</v>
+        <v>502705</v>
       </c>
       <c r="I61" t="n">
-        <v>102.983</v>
+        <v>104.247</v>
       </c>
       <c r="J61" t="n">
-        <v>2125</v>
+        <v>4225</v>
       </c>
       <c r="K61" t="n">
-        <v>0.441</v>
+        <v>0.876</v>
       </c>
       <c r="L61" t="n">
-        <v>3492</v>
+        <v>3542</v>
       </c>
       <c r="M61" t="n">
-        <v>0.724</v>
+        <v>0.735</v>
       </c>
       <c r="N61" t="n">
         <v>0</v>
       </c>
       <c r="O61" t="n">
-        <v>6111</v>
+        <v>8264.667</v>
       </c>
       <c r="P61" t="s">
         <v>376</v>
@@ -6021,7 +6001,7 @@
         <v>385</v>
       </c>
       <c r="C63" s="1" t="n">
-        <v>44051</v>
+        <v>44053</v>
       </c>
       <c r="D63" t="s">
         <v>386</v>
@@ -6031,31 +6011,31 @@
       </c>
       <c r="F63"/>
       <c r="G63" t="n">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="H63" t="n">
-        <v>474531</v>
+        <v>480209</v>
       </c>
       <c r="I63" t="n">
-        <v>87.532</v>
+        <v>88.579</v>
       </c>
       <c r="J63" t="n">
-        <v>1990</v>
+        <v>1796</v>
       </c>
       <c r="K63" t="n">
-        <v>0.367</v>
+        <v>0.331</v>
       </c>
       <c r="L63" t="n">
-        <v>5463</v>
+        <v>4973</v>
       </c>
       <c r="M63" t="n">
-        <v>1.008</v>
+        <v>0.917</v>
       </c>
       <c r="N63" t="n">
         <v>0.007</v>
       </c>
       <c r="O63" t="n">
-        <v>147.081</v>
+        <v>133.888</v>
       </c>
       <c r="P63" t="s">
         <v>387</v>
@@ -6123,7 +6103,7 @@
         <v>399</v>
       </c>
       <c r="C65" s="1" t="n">
-        <v>44053</v>
+        <v>44055</v>
       </c>
       <c r="D65" t="s">
         <v>400</v>
@@ -6133,32 +6113,28 @@
       </c>
       <c r="F65"/>
       <c r="G65" t="n">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="H65" t="n">
-        <v>2147584</v>
+        <v>2186442</v>
       </c>
       <c r="I65" t="n">
-        <v>9.722</v>
+        <v>9.898</v>
       </c>
       <c r="J65" t="n">
-        <v>20495</v>
+        <v>20631</v>
       </c>
       <c r="K65" t="n">
         <v>0.093</v>
       </c>
       <c r="L65" t="n">
-        <v>16518</v>
+        <v>19296</v>
       </c>
       <c r="M65" t="n">
-        <v>0.075</v>
-      </c>
-      <c r="N65" t="n">
-        <v>0.04</v>
-      </c>
-      <c r="O65" t="n">
-        <v>24.968</v>
-      </c>
+        <v>0.087</v>
+      </c>
+      <c r="N65"/>
+      <c r="O65"/>
       <c r="P65" t="s">
         <v>401</v>
       </c>
@@ -6180,7 +6156,7 @@
         <v>404</v>
       </c>
       <c r="C66" s="1" t="n">
-        <v>44048</v>
+        <v>44052</v>
       </c>
       <c r="D66" t="s">
         <v>405</v>
@@ -6190,31 +6166,31 @@
       </c>
       <c r="F66"/>
       <c r="G66" t="n">
-        <v>149</v>
+        <v>153</v>
       </c>
       <c r="H66" t="n">
-        <v>235074</v>
+        <v>248090</v>
       </c>
       <c r="I66" t="n">
-        <v>54.481</v>
+        <v>57.498</v>
       </c>
       <c r="J66" t="n">
-        <v>2557</v>
+        <v>2861</v>
       </c>
       <c r="K66" t="n">
-        <v>0.593</v>
+        <v>0.663</v>
       </c>
       <c r="L66" t="n">
-        <v>2996</v>
+        <v>2969</v>
       </c>
       <c r="M66" t="n">
-        <v>0.694</v>
+        <v>0.688</v>
       </c>
       <c r="N66" t="n">
-        <v>0.343</v>
+        <v>0.35</v>
       </c>
       <c r="O66" t="n">
-        <v>2.912</v>
+        <v>2.86</v>
       </c>
       <c r="P66" t="s">
         <v>406</v>
@@ -6237,7 +6213,7 @@
         <v>409</v>
       </c>
       <c r="C67" s="1" t="n">
-        <v>44049</v>
+        <v>44053</v>
       </c>
       <c r="D67" t="s">
         <v>410</v>
@@ -6247,31 +6223,31 @@
       </c>
       <c r="F67"/>
       <c r="G67" t="n">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="H67" t="n">
-        <v>135277</v>
+        <v>140236</v>
       </c>
       <c r="I67" t="n">
-        <v>18.966</v>
+        <v>19.661</v>
       </c>
       <c r="J67" t="n">
-        <v>1455</v>
+        <v>1821</v>
       </c>
       <c r="K67" t="n">
-        <v>0.204</v>
+        <v>0.255</v>
       </c>
       <c r="L67" t="n">
-        <v>1417</v>
+        <v>1350</v>
       </c>
       <c r="M67" t="n">
-        <v>0.199</v>
+        <v>0.189</v>
       </c>
       <c r="N67" t="n">
-        <v>0.12</v>
+        <v>0.134</v>
       </c>
       <c r="O67" t="n">
-        <v>8.307</v>
+        <v>7.482</v>
       </c>
       <c r="P67" t="s">
         <v>411</v>
@@ -6404,7 +6380,7 @@
         <v>427</v>
       </c>
       <c r="C70" s="1" t="n">
-        <v>44052</v>
+        <v>44054</v>
       </c>
       <c r="D70" t="s">
         <v>428</v>
@@ -6414,31 +6390,31 @@
       </c>
       <c r="F70"/>
       <c r="G70" t="n">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="H70" t="n">
-        <v>2123622</v>
+        <v>2158532</v>
       </c>
       <c r="I70" t="n">
-        <v>56.111</v>
+        <v>57.034</v>
       </c>
       <c r="J70" t="n">
-        <v>20842</v>
+        <v>20511</v>
       </c>
       <c r="K70" t="n">
-        <v>0.551</v>
+        <v>0.542</v>
       </c>
       <c r="L70" t="n">
-        <v>22007</v>
+        <v>22715</v>
       </c>
       <c r="M70" t="n">
-        <v>0.581</v>
+        <v>0.6</v>
       </c>
       <c r="N70" t="n">
         <v>0.031</v>
       </c>
       <c r="O70" t="n">
-        <v>31.954</v>
+        <v>32.181</v>
       </c>
       <c r="P70" t="s">
         <v>429</v>
@@ -6461,7 +6437,7 @@
         <v>432</v>
       </c>
       <c r="C71" s="1" t="n">
-        <v>44052</v>
+        <v>44054</v>
       </c>
       <c r="D71" t="s">
         <v>428</v>
@@ -6471,19 +6447,19 @@
       </c>
       <c r="F71"/>
       <c r="G71" t="n">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="H71" t="n">
-        <v>2219459</v>
+        <v>2257525</v>
       </c>
       <c r="I71" t="n">
-        <v>58.644</v>
+        <v>59.649</v>
       </c>
       <c r="J71" t="n">
-        <v>20374</v>
+        <v>23142</v>
       </c>
       <c r="K71" t="n">
-        <v>0.538</v>
+        <v>0.611</v>
       </c>
       <c r="L71"/>
       <c r="M71"/>
@@ -6510,7 +6486,7 @@
         <v>435</v>
       </c>
       <c r="C72" s="1" t="n">
-        <v>44048</v>
+        <v>44053</v>
       </c>
       <c r="D72" t="s">
         <v>436</v>
@@ -6520,31 +6496,31 @@
       </c>
       <c r="F72"/>
       <c r="G72" t="n">
-        <v>158</v>
+        <v>163</v>
       </c>
       <c r="H72" t="n">
-        <v>1705474</v>
+        <v>1766454</v>
       </c>
       <c r="I72" t="n">
-        <v>167.257</v>
+        <v>173.238</v>
       </c>
       <c r="J72" t="n">
-        <v>16864</v>
+        <v>12903</v>
       </c>
       <c r="K72" t="n">
-        <v>1.654</v>
+        <v>1.265</v>
       </c>
       <c r="L72" t="n">
-        <v>13858</v>
+        <v>13566</v>
       </c>
       <c r="M72" t="n">
-        <v>1.359</v>
+        <v>1.33</v>
       </c>
       <c r="N72" t="n">
         <v>0.013</v>
       </c>
       <c r="O72" t="n">
-        <v>76.323</v>
+        <v>78.807</v>
       </c>
       <c r="P72" t="s">
         <v>437</v>
@@ -6567,7 +6543,7 @@
         <v>441</v>
       </c>
       <c r="C73" s="1" t="n">
-        <v>44052</v>
+        <v>44054</v>
       </c>
       <c r="D73" t="s">
         <v>442</v>
@@ -6577,31 +6553,31 @@
       </c>
       <c r="F73"/>
       <c r="G73" t="n">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="H73" t="n">
-        <v>520360</v>
+        <v>529289</v>
       </c>
       <c r="I73" t="n">
-        <v>180.614</v>
+        <v>183.713</v>
       </c>
       <c r="J73" t="n">
-        <v>3535</v>
+        <v>4823</v>
       </c>
       <c r="K73" t="n">
-        <v>1.227</v>
+        <v>1.674</v>
       </c>
       <c r="L73" t="n">
-        <v>2832</v>
+        <v>3449</v>
       </c>
       <c r="M73" t="n">
-        <v>0.983</v>
+        <v>1.197</v>
       </c>
       <c r="N73" t="n">
-        <v>0.088</v>
+        <v>0.08</v>
       </c>
       <c r="O73" t="n">
-        <v>11.4</v>
+        <v>12.445</v>
       </c>
       <c r="P73" t="s">
         <v>443</v>
@@ -6624,7 +6600,7 @@
         <v>447</v>
       </c>
       <c r="C74" s="1" t="n">
-        <v>44052</v>
+        <v>44054</v>
       </c>
       <c r="D74" t="s">
         <v>448</v>
@@ -6634,31 +6610,31 @@
       </c>
       <c r="F74"/>
       <c r="G74" t="n">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="H74" t="n">
-        <v>1378727</v>
+        <v>1404845</v>
       </c>
       <c r="I74" t="n">
-        <v>71.668</v>
+        <v>73.026</v>
       </c>
       <c r="J74" t="n">
-        <v>13968</v>
+        <v>19511</v>
       </c>
       <c r="K74" t="n">
-        <v>0.726</v>
+        <v>1.014</v>
       </c>
       <c r="L74" t="n">
-        <v>18630</v>
+        <v>17541</v>
       </c>
       <c r="M74" t="n">
-        <v>0.968</v>
+        <v>0.912</v>
       </c>
       <c r="N74" t="n">
-        <v>0.065</v>
+        <v>0.07</v>
       </c>
       <c r="O74" t="n">
-        <v>15.321</v>
+        <v>14.381</v>
       </c>
       <c r="P74" t="s">
         <v>450</v>
@@ -6681,7 +6657,7 @@
         <v>454</v>
       </c>
       <c r="C75" s="1" t="n">
-        <v>44052</v>
+        <v>44054</v>
       </c>
       <c r="D75" t="s">
         <v>455</v>
@@ -6691,31 +6667,31 @@
       </c>
       <c r="F75"/>
       <c r="G75" t="n">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="H75" t="n">
-        <v>30886160</v>
+        <v>31307764</v>
       </c>
       <c r="I75" t="n">
-        <v>211.644</v>
+        <v>214.533</v>
       </c>
       <c r="J75" t="n">
-        <v>246140</v>
+        <v>244577</v>
       </c>
       <c r="K75" t="n">
-        <v>1.687</v>
+        <v>1.676</v>
       </c>
       <c r="L75" t="n">
-        <v>265180</v>
+        <v>267696</v>
       </c>
       <c r="M75" t="n">
-        <v>1.817</v>
+        <v>1.834</v>
       </c>
       <c r="N75" t="n">
-        <v>0.02</v>
+        <v>0.022</v>
       </c>
       <c r="O75" t="n">
-        <v>50.3</v>
+        <v>45.334</v>
       </c>
       <c r="P75" t="s">
         <v>456</v>
@@ -6738,7 +6714,7 @@
         <v>460</v>
       </c>
       <c r="C76" s="1" t="n">
-        <v>44049</v>
+        <v>44053</v>
       </c>
       <c r="D76" t="s">
         <v>461</v>
@@ -6748,31 +6724,31 @@
       </c>
       <c r="F76"/>
       <c r="G76" t="n">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="H76" t="n">
-        <v>286251</v>
+        <v>304500</v>
       </c>
       <c r="I76" t="n">
-        <v>22.101</v>
+        <v>23.51</v>
       </c>
       <c r="J76" t="n">
-        <v>3196</v>
+        <v>5720</v>
       </c>
       <c r="K76" t="n">
-        <v>0.247</v>
+        <v>0.442</v>
       </c>
       <c r="L76" t="n">
-        <v>3747</v>
+        <v>4159</v>
       </c>
       <c r="M76" t="n">
-        <v>0.289</v>
+        <v>0.321</v>
       </c>
       <c r="N76" t="n">
-        <v>0.006</v>
+        <v>0.003</v>
       </c>
       <c r="O76" t="n">
-        <v>156.125</v>
+        <v>373.244</v>
       </c>
       <c r="P76" t="s">
         <v>462</v>
@@ -6795,7 +6771,7 @@
         <v>466</v>
       </c>
       <c r="C77" s="1" t="n">
-        <v>44052</v>
+        <v>44054</v>
       </c>
       <c r="D77" t="s">
         <v>467</v>
@@ -6805,31 +6781,31 @@
       </c>
       <c r="F77"/>
       <c r="G77" t="n">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="H77" t="n">
-        <v>3803986</v>
+        <v>3933427</v>
       </c>
       <c r="I77" t="n">
-        <v>109.266</v>
+        <v>112.984</v>
       </c>
       <c r="J77" t="n">
-        <v>58424</v>
+        <v>60828</v>
       </c>
       <c r="K77" t="n">
-        <v>1.678</v>
+        <v>1.747</v>
       </c>
       <c r="L77" t="n">
-        <v>54417</v>
+        <v>59239</v>
       </c>
       <c r="M77" t="n">
-        <v>1.563</v>
+        <v>1.702</v>
       </c>
       <c r="N77" t="n">
-        <v>0.026</v>
+        <v>0.024</v>
       </c>
       <c r="O77" t="n">
-        <v>38.933</v>
+        <v>42.082</v>
       </c>
       <c r="P77" t="s">
         <v>45</v>
@@ -6852,7 +6828,7 @@
         <v>470</v>
       </c>
       <c r="C78" s="1" t="n">
-        <v>44052</v>
+        <v>44054</v>
       </c>
       <c r="D78" t="s">
         <v>471</v>
@@ -6864,31 +6840,31 @@
         <v>473</v>
       </c>
       <c r="G78" t="n">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="H78" t="n">
-        <v>122751</v>
+        <v>125029</v>
       </c>
       <c r="I78" t="n">
-        <v>7.331</v>
+        <v>7.467</v>
       </c>
       <c r="J78" t="n">
-        <v>1656</v>
+        <v>876</v>
       </c>
       <c r="K78" t="n">
-        <v>0.099</v>
+        <v>0.052</v>
       </c>
       <c r="L78" t="n">
-        <v>1446</v>
+        <v>1483</v>
       </c>
       <c r="M78" t="n">
-        <v>0.086</v>
+        <v>0.089</v>
       </c>
       <c r="N78" t="n">
-        <v>0.074</v>
+        <v>0.089</v>
       </c>
       <c r="O78" t="n">
-        <v>13.514</v>
+        <v>11.211</v>
       </c>
       <c r="P78" t="s">
         <v>474</v>
@@ -6911,7 +6887,7 @@
         <v>478</v>
       </c>
       <c r="C79" s="1" t="n">
-        <v>44052</v>
+        <v>44054</v>
       </c>
       <c r="D79" t="s">
         <v>479</v>
@@ -6923,31 +6899,31 @@
         <v>480</v>
       </c>
       <c r="G79" t="n">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="H79" t="n">
-        <v>747324</v>
+        <v>762229</v>
       </c>
       <c r="I79" t="n">
-        <v>109.826</v>
+        <v>112.017</v>
       </c>
       <c r="J79" t="n">
-        <v>6251</v>
+        <v>8086</v>
       </c>
       <c r="K79" t="n">
-        <v>0.919</v>
+        <v>1.188</v>
       </c>
       <c r="L79" t="n">
-        <v>8691</v>
+        <v>8426</v>
       </c>
       <c r="M79" t="n">
-        <v>1.277</v>
+        <v>1.238</v>
       </c>
       <c r="N79" t="n">
-        <v>0.033</v>
+        <v>0.031</v>
       </c>
       <c r="O79" t="n">
-        <v>30.71</v>
+        <v>32.569</v>
       </c>
       <c r="P79" t="s">
         <v>45</v>
@@ -6970,7 +6946,7 @@
         <v>484</v>
       </c>
       <c r="C80" s="1" t="n">
-        <v>44046</v>
+        <v>44054</v>
       </c>
       <c r="D80" t="s">
         <v>485</v>
@@ -6980,27 +6956,27 @@
       </c>
       <c r="F80"/>
       <c r="G80" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H80" t="n">
-        <v>650702</v>
+        <v>686738</v>
       </c>
       <c r="I80" t="n">
-        <v>111.225</v>
+        <v>117.384</v>
       </c>
       <c r="J80"/>
       <c r="K80"/>
       <c r="L80" t="n">
-        <v>4913</v>
+        <v>4504</v>
       </c>
       <c r="M80" t="n">
-        <v>0.84</v>
+        <v>0.77</v>
       </c>
       <c r="N80" t="n">
         <v>0.071</v>
       </c>
       <c r="O80" t="n">
-        <v>14.003</v>
+        <v>14.069</v>
       </c>
       <c r="P80" t="s">
         <v>45</v>
@@ -7023,7 +6999,7 @@
         <v>487</v>
       </c>
       <c r="C81" s="1" t="n">
-        <v>44046</v>
+        <v>44054</v>
       </c>
       <c r="D81" t="s">
         <v>485</v>
@@ -7033,27 +7009,27 @@
       </c>
       <c r="F81"/>
       <c r="G81" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="H81" t="n">
-        <v>1474372</v>
+        <v>1610906</v>
       </c>
       <c r="I81" t="n">
-        <v>252.015</v>
+        <v>275.352</v>
       </c>
       <c r="J81"/>
       <c r="K81"/>
       <c r="L81" t="n">
-        <v>21897</v>
+        <v>17067</v>
       </c>
       <c r="M81" t="n">
-        <v>3.743</v>
+        <v>2.917</v>
       </c>
       <c r="N81" t="n">
-        <v>0.016</v>
+        <v>0.019</v>
       </c>
       <c r="O81" t="n">
-        <v>62.41</v>
+        <v>53.311</v>
       </c>
       <c r="P81" t="s">
         <v>45</v>
@@ -7076,7 +7052,7 @@
         <v>490</v>
       </c>
       <c r="C82" s="1" t="n">
-        <v>44053</v>
+        <v>44055</v>
       </c>
       <c r="D82" t="s">
         <v>491</v>
@@ -7086,32 +7062,28 @@
       </c>
       <c r="F82"/>
       <c r="G82" t="n">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="H82" t="n">
-        <v>279526</v>
+        <v>284111</v>
       </c>
       <c r="I82" t="n">
-        <v>51.199</v>
+        <v>52.038</v>
       </c>
       <c r="J82" t="n">
-        <v>564</v>
+        <v>3131</v>
       </c>
       <c r="K82" t="n">
-        <v>0.103</v>
+        <v>0.573</v>
       </c>
       <c r="L82" t="n">
-        <v>1961</v>
+        <v>2065</v>
       </c>
       <c r="M82" t="n">
-        <v>0.359</v>
-      </c>
-      <c r="N82" t="n">
-        <v>0.018</v>
-      </c>
-      <c r="O82" t="n">
-        <v>54.472</v>
-      </c>
+        <v>0.378</v>
+      </c>
+      <c r="N82"/>
+      <c r="O82"/>
       <c r="P82" t="s">
         <v>493</v>
       </c>
@@ -7133,7 +7105,7 @@
         <v>496</v>
       </c>
       <c r="C83" s="1" t="n">
-        <v>44052</v>
+        <v>44054</v>
       </c>
       <c r="D83" t="s">
         <v>497</v>
@@ -7143,31 +7115,31 @@
       </c>
       <c r="F83"/>
       <c r="G83" t="n">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="H83" t="n">
-        <v>136542</v>
+        <v>138718</v>
       </c>
       <c r="I83" t="n">
-        <v>65.679</v>
+        <v>66.726</v>
       </c>
       <c r="J83" t="n">
-        <v>322</v>
+        <v>1118</v>
       </c>
       <c r="K83" t="n">
-        <v>0.155</v>
+        <v>0.538</v>
       </c>
       <c r="L83" t="n">
-        <v>692</v>
+        <v>736</v>
       </c>
       <c r="M83" t="n">
-        <v>0.333</v>
+        <v>0.354</v>
       </c>
       <c r="N83" t="n">
-        <v>0.016</v>
+        <v>0.014</v>
       </c>
       <c r="O83" t="n">
-        <v>63.737</v>
+        <v>69.622</v>
       </c>
       <c r="P83" t="s">
         <v>499</v>
@@ -7190,7 +7162,7 @@
         <v>503</v>
       </c>
       <c r="C84" s="1" t="n">
-        <v>44052</v>
+        <v>44054</v>
       </c>
       <c r="D84" t="s">
         <v>504</v>
@@ -7202,31 +7174,31 @@
         <v>506</v>
       </c>
       <c r="G84" t="n">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="H84" t="n">
-        <v>3250583</v>
+        <v>3278977</v>
       </c>
       <c r="I84" t="n">
-        <v>54.808</v>
+        <v>55.287</v>
       </c>
       <c r="J84" t="n">
-        <v>30318</v>
+        <v>11483</v>
       </c>
       <c r="K84" t="n">
-        <v>0.511</v>
+        <v>0.194</v>
       </c>
       <c r="L84" t="n">
-        <v>30543</v>
+        <v>28682</v>
       </c>
       <c r="M84" t="n">
-        <v>0.515</v>
+        <v>0.484</v>
       </c>
       <c r="N84" t="n">
         <v>0.233</v>
       </c>
       <c r="O84" t="n">
-        <v>4.285</v>
+        <v>4.296</v>
       </c>
       <c r="P84" t="s">
         <v>505</v>
@@ -7249,7 +7221,7 @@
         <v>510</v>
       </c>
       <c r="C85" s="1" t="n">
-        <v>44053</v>
+        <v>44055</v>
       </c>
       <c r="D85" t="s">
         <v>511</v>
@@ -7259,32 +7231,28 @@
       </c>
       <c r="F85"/>
       <c r="G85" t="n">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="H85" t="n">
-        <v>1611907</v>
+        <v>1629277</v>
       </c>
       <c r="I85" t="n">
-        <v>31.44</v>
+        <v>31.779</v>
       </c>
       <c r="J85" t="n">
-        <v>4060</v>
+        <v>8922</v>
       </c>
       <c r="K85" t="n">
-        <v>0.079</v>
+        <v>0.174</v>
       </c>
       <c r="L85" t="n">
-        <v>7079</v>
+        <v>7083</v>
       </c>
       <c r="M85" t="n">
         <v>0.138</v>
       </c>
-      <c r="N85" t="n">
-        <v>0.005</v>
-      </c>
-      <c r="O85" t="n">
-        <v>209.084</v>
-      </c>
+      <c r="N85"/>
+      <c r="O85"/>
       <c r="P85" t="s">
         <v>512</v>
       </c>
@@ -7465,7 +7433,7 @@
         <v>533</v>
       </c>
       <c r="C89" s="1" t="n">
-        <v>44051</v>
+        <v>44053</v>
       </c>
       <c r="D89" t="s">
         <v>534</v>
@@ -7475,31 +7443,31 @@
       </c>
       <c r="F89"/>
       <c r="G89" t="n">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="H89" t="n">
-        <v>840986</v>
+        <v>847325</v>
       </c>
       <c r="I89" t="n">
-        <v>97.172</v>
+        <v>97.904</v>
       </c>
       <c r="J89" t="n">
-        <v>3555</v>
+        <v>4098</v>
       </c>
       <c r="K89" t="n">
-        <v>0.411</v>
+        <v>0.474</v>
       </c>
       <c r="L89" t="n">
-        <v>5499</v>
+        <v>5209</v>
       </c>
       <c r="M89" t="n">
-        <v>0.635</v>
+        <v>0.602</v>
       </c>
       <c r="N89" t="n">
         <v>0.029</v>
       </c>
       <c r="O89" t="n">
-        <v>34.678</v>
+        <v>34.628</v>
       </c>
       <c r="P89" t="s">
         <v>535</v>
@@ -7522,7 +7490,7 @@
         <v>539</v>
       </c>
       <c r="C90" s="1" t="n">
-        <v>44052</v>
+        <v>44054</v>
       </c>
       <c r="D90" t="s">
         <v>540</v>
@@ -7532,31 +7500,31 @@
       </c>
       <c r="F90"/>
       <c r="G90" t="n">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="H90" t="n">
-        <v>83434</v>
+        <v>83828</v>
       </c>
       <c r="I90" t="n">
-        <v>3.503</v>
+        <v>3.52</v>
       </c>
       <c r="J90" t="n">
-        <v>142</v>
+        <v>148</v>
       </c>
       <c r="K90" t="n">
         <v>0.006</v>
       </c>
       <c r="L90" t="n">
-        <v>196</v>
+        <v>186</v>
       </c>
       <c r="M90" t="n">
         <v>0.008</v>
       </c>
       <c r="N90" t="n">
-        <v>0.004</v>
+        <v>0.003</v>
       </c>
       <c r="O90" t="n">
-        <v>228.667</v>
+        <v>325.5</v>
       </c>
       <c r="P90" t="s">
         <v>541</v>
@@ -7579,7 +7547,7 @@
         <v>544</v>
       </c>
       <c r="C91" s="1" t="n">
-        <v>44052</v>
+        <v>44054</v>
       </c>
       <c r="D91" t="s">
         <v>545</v>
@@ -7589,31 +7557,31 @@
       </c>
       <c r="F91"/>
       <c r="G91" t="n">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="H91" t="n">
-        <v>386931</v>
+        <v>389247</v>
       </c>
       <c r="I91" t="n">
-        <v>5.543</v>
+        <v>5.577</v>
       </c>
       <c r="J91" t="n">
-        <v>1071</v>
+        <v>1485</v>
       </c>
       <c r="K91" t="n">
-        <v>0.015</v>
+        <v>0.021</v>
       </c>
       <c r="L91" t="n">
-        <v>1322</v>
+        <v>1231</v>
       </c>
       <c r="M91" t="n">
-        <v>0.019</v>
+        <v>0.018</v>
       </c>
       <c r="N91" t="n">
-        <v>0.004</v>
+        <v>0.003</v>
       </c>
       <c r="O91" t="n">
-        <v>272.176</v>
+        <v>287.233</v>
       </c>
       <c r="P91" t="s">
         <v>546</v>
@@ -7636,7 +7604,7 @@
         <v>549</v>
       </c>
       <c r="C92" s="1" t="n">
-        <v>44052</v>
+        <v>44054</v>
       </c>
       <c r="D92" t="s">
         <v>545</v>
@@ -7646,31 +7614,31 @@
       </c>
       <c r="F92"/>
       <c r="G92" t="n">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="H92" t="n">
-        <v>758464</v>
+        <v>777518</v>
       </c>
       <c r="I92" t="n">
-        <v>10.866</v>
+        <v>11.139</v>
       </c>
       <c r="J92" t="n">
-        <v>1071</v>
+        <v>18223</v>
       </c>
       <c r="K92" t="n">
-        <v>0.015</v>
+        <v>0.261</v>
       </c>
       <c r="L92" t="n">
-        <v>4063</v>
+        <v>3622</v>
       </c>
       <c r="M92" t="n">
-        <v>0.058</v>
+        <v>0.052</v>
       </c>
       <c r="N92" t="n">
         <v>0.001</v>
       </c>
       <c r="O92" t="n">
-        <v>836.5</v>
+        <v>845.133</v>
       </c>
       <c r="P92" t="s">
         <v>546</v>
@@ -7693,7 +7661,7 @@
         <v>552</v>
       </c>
       <c r="C93" s="1" t="n">
-        <v>44051</v>
+        <v>44052</v>
       </c>
       <c r="D93"/>
       <c r="E93" t="s">
@@ -7703,31 +7671,31 @@
         <v>554</v>
       </c>
       <c r="G93" t="n">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="H93" t="n">
-        <v>47078</v>
+        <v>47661</v>
       </c>
       <c r="I93" t="n">
-        <v>5.687</v>
+        <v>5.757</v>
       </c>
       <c r="J93" t="n">
-        <v>1062</v>
+        <v>583</v>
       </c>
       <c r="K93" t="n">
-        <v>0.128</v>
+        <v>0.07</v>
       </c>
       <c r="L93" t="n">
-        <v>591</v>
+        <v>614</v>
       </c>
       <c r="M93" t="n">
-        <v>0.071</v>
+        <v>0.074</v>
       </c>
       <c r="N93" t="n">
-        <v>0.021</v>
+        <v>0.02</v>
       </c>
       <c r="O93" t="n">
-        <v>47.552</v>
+        <v>48.841</v>
       </c>
       <c r="P93" t="s">
         <v>553</v>
@@ -7750,7 +7718,7 @@
         <v>558</v>
       </c>
       <c r="C94" s="1" t="n">
-        <v>44049</v>
+        <v>44051</v>
       </c>
       <c r="D94" t="s">
         <v>559</v>
@@ -7760,31 +7728,31 @@
       </c>
       <c r="F94"/>
       <c r="G94" t="n">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="H94" t="n">
-        <v>100095</v>
+        <v>102028</v>
       </c>
       <c r="I94" t="n">
-        <v>8.469</v>
+        <v>8.633</v>
       </c>
       <c r="J94" t="n">
-        <v>1382</v>
+        <v>650</v>
       </c>
       <c r="K94" t="n">
-        <v>0.117</v>
+        <v>0.055</v>
       </c>
       <c r="L94" t="n">
-        <v>1033</v>
+        <v>1260</v>
       </c>
       <c r="M94" t="n">
-        <v>0.087</v>
+        <v>0.107</v>
       </c>
       <c r="N94" t="n">
-        <v>0.016</v>
+        <v>0.014</v>
       </c>
       <c r="O94" t="n">
-        <v>63.991</v>
+        <v>72.893</v>
       </c>
       <c r="P94" t="s">
         <v>560</v>
@@ -7807,7 +7775,7 @@
         <v>563</v>
       </c>
       <c r="C95" s="1" t="n">
-        <v>44052</v>
+        <v>44054</v>
       </c>
       <c r="D95" t="s">
         <v>564</v>
@@ -7817,31 +7785,31 @@
       </c>
       <c r="F95"/>
       <c r="G95" t="n">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="H95" t="n">
-        <v>5263816</v>
+        <v>5387751</v>
       </c>
       <c r="I95" t="n">
-        <v>62.413</v>
+        <v>63.882</v>
       </c>
       <c r="J95" t="n">
-        <v>61446</v>
+        <v>61716</v>
       </c>
       <c r="K95" t="n">
-        <v>0.729</v>
+        <v>0.732</v>
       </c>
       <c r="L95" t="n">
-        <v>48086</v>
+        <v>54025</v>
       </c>
       <c r="M95" t="n">
-        <v>0.57</v>
+        <v>0.641</v>
       </c>
       <c r="N95" t="n">
-        <v>0.023</v>
+        <v>0.022</v>
       </c>
       <c r="O95" t="n">
-        <v>43.416</v>
+        <v>46.425</v>
       </c>
       <c r="P95" t="s">
         <v>565</v>
@@ -7864,7 +7832,7 @@
         <v>568</v>
       </c>
       <c r="C96" s="1" t="n">
-        <v>44051</v>
+        <v>44053</v>
       </c>
       <c r="D96" t="s">
         <v>569</v>
@@ -7874,31 +7842,31 @@
       </c>
       <c r="F96"/>
       <c r="G96" t="n">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="H96" t="n">
-        <v>296601</v>
+        <v>301286</v>
       </c>
       <c r="I96" t="n">
-        <v>6.484</v>
+        <v>6.587</v>
       </c>
       <c r="J96" t="n">
-        <v>3204</v>
+        <v>2250</v>
       </c>
       <c r="K96" t="n">
-        <v>0.07</v>
+        <v>0.049</v>
       </c>
       <c r="L96" t="n">
-        <v>2650</v>
+        <v>2682</v>
       </c>
       <c r="M96" t="n">
-        <v>0.058</v>
+        <v>0.059</v>
       </c>
       <c r="N96" t="n">
         <v>0.005</v>
       </c>
       <c r="O96" t="n">
-        <v>185.5</v>
+        <v>185.881</v>
       </c>
       <c r="P96" t="s">
         <v>570</v>
@@ -7921,7 +7889,7 @@
         <v>574</v>
       </c>
       <c r="C97" s="1" t="n">
-        <v>44053</v>
+        <v>44055</v>
       </c>
       <c r="D97" t="s">
         <v>575</v>
@@ -7931,32 +7899,28 @@
       </c>
       <c r="F97"/>
       <c r="G97" t="n">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="H97" t="n">
-        <v>1179434</v>
+        <v>1214941</v>
       </c>
       <c r="I97" t="n">
-        <v>26.969</v>
+        <v>27.78</v>
       </c>
       <c r="J97" t="n">
-        <v>10083</v>
+        <v>19380</v>
       </c>
       <c r="K97" t="n">
-        <v>0.231</v>
+        <v>0.443</v>
       </c>
       <c r="L97" t="n">
-        <v>16061</v>
+        <v>16611</v>
       </c>
       <c r="M97" t="n">
-        <v>0.367</v>
-      </c>
-      <c r="N97" t="n">
-        <v>0.087</v>
-      </c>
-      <c r="O97" t="n">
-        <v>11.485</v>
-      </c>
+        <v>0.38</v>
+      </c>
+      <c r="N97"/>
+      <c r="O97"/>
       <c r="P97" t="s">
         <v>576</v>
       </c>
@@ -7978,7 +7942,7 @@
         <v>580</v>
       </c>
       <c r="C98" s="1" t="n">
-        <v>44052</v>
+        <v>44054</v>
       </c>
       <c r="D98" t="s">
         <v>581</v>
@@ -7988,31 +7952,31 @@
       </c>
       <c r="F98"/>
       <c r="G98" t="n">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="H98" t="n">
-        <v>5500701</v>
+        <v>5623764</v>
       </c>
       <c r="I98" t="n">
-        <v>556.166</v>
+        <v>568.608</v>
       </c>
       <c r="J98" t="n">
-        <v>61544</v>
+        <v>64110</v>
       </c>
       <c r="K98" t="n">
-        <v>6.223</v>
+        <v>6.482</v>
       </c>
       <c r="L98" t="n">
-        <v>48374</v>
+        <v>57782</v>
       </c>
       <c r="M98" t="n">
-        <v>4.891</v>
+        <v>5.842</v>
       </c>
       <c r="N98" t="n">
-        <v>0.005</v>
+        <v>0.004</v>
       </c>
       <c r="O98" t="n">
-        <v>219.882</v>
+        <v>262.475</v>
       </c>
       <c r="P98" t="s">
         <v>582</v>
@@ -8035,7 +7999,7 @@
         <v>585</v>
       </c>
       <c r="C99" s="1" t="n">
-        <v>44051</v>
+        <v>44053</v>
       </c>
       <c r="D99" t="s">
         <v>586</v>
@@ -8047,31 +8011,31 @@
         <v>588</v>
       </c>
       <c r="G99" t="n">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="H99" t="n">
-        <v>10703374</v>
+        <v>10993551</v>
       </c>
       <c r="I99" t="n">
-        <v>157.667</v>
+        <v>161.941</v>
       </c>
       <c r="J99" t="n">
-        <v>146826</v>
+        <v>135827</v>
       </c>
       <c r="K99" t="n">
-        <v>2.163</v>
+        <v>2.001</v>
       </c>
       <c r="L99" t="n">
-        <v>144285</v>
+        <v>150223</v>
       </c>
       <c r="M99" t="n">
-        <v>2.125</v>
+        <v>2.213</v>
       </c>
       <c r="N99" t="n">
         <v>0.006</v>
       </c>
       <c r="O99" t="n">
-        <v>173.419</v>
+        <v>171.543</v>
       </c>
       <c r="P99" t="s">
         <v>587</v>
@@ -8151,7 +8115,7 @@
         <v>597</v>
       </c>
       <c r="C101" s="1" t="n">
-        <v>44052</v>
+        <v>44054</v>
       </c>
       <c r="D101" t="s">
         <v>598</v>
@@ -8161,31 +8125,31 @@
       </c>
       <c r="F101"/>
       <c r="G101" t="n">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="H101" t="n">
-        <v>61792571</v>
+        <v>63252257</v>
       </c>
       <c r="I101" t="n">
-        <v>186.683</v>
+        <v>191.093</v>
       </c>
       <c r="J101" t="n">
-        <v>711984</v>
+        <v>739083</v>
       </c>
       <c r="K101" t="n">
-        <v>2.151</v>
+        <v>2.233</v>
       </c>
       <c r="L101" t="n">
-        <v>711487</v>
+        <v>716117</v>
       </c>
       <c r="M101" t="n">
-        <v>2.149</v>
+        <v>2.163</v>
       </c>
       <c r="N101" t="n">
         <v>0.076</v>
       </c>
       <c r="O101" t="n">
-        <v>13.191</v>
+        <v>13.163</v>
       </c>
       <c r="P101" t="s">
         <v>599</v>
@@ -8208,7 +8172,7 @@
         <v>604</v>
       </c>
       <c r="C102" s="1" t="n">
-        <v>44051</v>
+        <v>44053</v>
       </c>
       <c r="D102" t="s">
         <v>605</v>
@@ -8218,31 +8182,27 @@
       </c>
       <c r="F102"/>
       <c r="G102" t="n">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="H102" t="n">
-        <v>130767</v>
+        <v>133237</v>
       </c>
       <c r="I102" t="n">
-        <v>37.645</v>
-      </c>
-      <c r="J102" t="n">
-        <v>1953</v>
-      </c>
-      <c r="K102" t="n">
-        <v>0.562</v>
-      </c>
+        <v>38.356</v>
+      </c>
+      <c r="J102"/>
+      <c r="K102"/>
       <c r="L102" t="n">
-        <v>2224</v>
+        <v>2028</v>
       </c>
       <c r="M102" t="n">
-        <v>0.64</v>
+        <v>0.584</v>
       </c>
       <c r="N102" t="n">
-        <v>0.004</v>
+        <v>0.005</v>
       </c>
       <c r="O102" t="n">
-        <v>255.213</v>
+        <v>211.881</v>
       </c>
       <c r="P102" t="s">
         <v>126</v>
@@ -8318,7 +8278,7 @@
         <v>615</v>
       </c>
       <c r="C104" s="1" t="n">
-        <v>44048</v>
+        <v>44052</v>
       </c>
       <c r="D104" t="s">
         <v>616</v>
@@ -8328,31 +8288,31 @@
       </c>
       <c r="F104"/>
       <c r="G104" t="n">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="H104" t="n">
-        <v>67374</v>
+        <v>71608</v>
       </c>
       <c r="I104" t="n">
-        <v>4.533</v>
+        <v>4.818</v>
       </c>
       <c r="J104" t="n">
-        <v>1660</v>
+        <v>1293</v>
       </c>
       <c r="K104" t="n">
-        <v>0.112</v>
+        <v>0.087</v>
       </c>
       <c r="L104" t="n">
-        <v>1369</v>
+        <v>1203</v>
       </c>
       <c r="M104" t="n">
-        <v>0.092</v>
+        <v>0.081</v>
       </c>
       <c r="N104" t="n">
-        <v>0.147</v>
+        <v>0.109</v>
       </c>
       <c r="O104" t="n">
-        <v>6.825</v>
+        <v>9.193</v>
       </c>
       <c r="P104" t="s">
         <v>617</v>

</xml_diff>

<commit_message>
Updated testing data for 2020-08-14
</commit_message>
<xml_diff>
--- a/public/data/testing/covid-testing-latest-data-source-details.xlsx
+++ b/public/data/testing/covid-testing-latest-data-source-details.xlsx
@@ -110,7 +110,7 @@
     <t xml:space="preserve">Australia - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.health.gov.au/sites/default/files/documents/2020/08/coronavirus-covid-19-at-a-glance-11-august-2020.pdf</t>
+    <t xml:space="preserve">https://www.health.gov.au/sites/default/files/documents/2020/08/coronavirus-covid-19-at-a-glance-13-august-2020.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">Australian Government Department of Health</t>
@@ -202,7 +202,7 @@
     <t xml:space="preserve">Belarus - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">http://minzdrav.gov.by/ru/sobytiya/u-belarusi-na-11-zhni-nya-vypisanyya-65-tys-219-patsyenta/</t>
+    <t xml:space="preserve">http://minzdrav.gov.by/ru/sobytiya/u-belarusi-na-12-zhni-nya-vypisanyya-65-tys-893-patsyenta/</t>
   </si>
   <si>
     <t xml:space="preserve">Belarus Ministry of Health</t>
@@ -245,7 +245,7 @@
     <t xml:space="preserve">Bolivia - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://minsalud.gob.bo/4501-bolivia-reporta-1-636-contagios-nuevos-de-coronavirus-y-acumula-91-635-casos-en-cinco-meses</t>
+    <t xml:space="preserve">https://minsalud.gob.bo/4504-coronavirus-se-reportan-1-743-contagios-nuevos-y-el-numero-de-pacientes-recuperados-llega-a-32-830</t>
   </si>
   <si>
     <t xml:space="preserve">https://www.minsalud.gob.bo/</t>
@@ -394,7 +394,7 @@
     <t xml:space="preserve">Cote d'Ivoire - samples tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.facebook.com/Mshpci/posts/1665844576914563</t>
+    <t xml:space="preserve">https://www.facebook.com/Mshpci/posts/1666768260155528</t>
   </si>
   <si>
     <t xml:space="preserve">Ministry of Health and Public Hygiene</t>
@@ -473,7 +473,7 @@
     <t xml:space="preserve">Democratic Republic of Congo - samples tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/CMR_Covid19_RDC/status/1293140045390589954/photo/1</t>
+    <t xml:space="preserve">https://twitter.com/CMR_Covid19_RDC/status/1293864579861291008/photo/1</t>
   </si>
   <si>
     <t xml:space="preserve">DRC COVID-19 Pandemic Response Multisectoral Committee</t>
@@ -491,7 +491,7 @@
     <t xml:space="preserve">Denmark - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://files.ssi.dk/Data-Epidemiologiske-Rapport-11082020-lok5</t>
+    <t xml:space="preserve">https://www.ssi.dk/-/media/arkiv/dk/sygdomme-beredskab-og-forskning/sygdomsovervaagning/covid19/13_08_2020_zp09/data-epidemiologiske-rapport-13082020-13yt.zip?la=da</t>
   </si>
   <si>
     <t xml:space="preserve">Statens Serum Institut</t>
@@ -509,7 +509,7 @@
     <t xml:space="preserve">Ecuador - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.gestionderiesgos.gob.ec/wp-content/uploads/2020/08/INFOGRAFIA-NACIONALCOVI-19-COE-NACIONAL-08h00-09082020.pdf</t>
+    <t xml:space="preserve">https://www.gestionderiesgos.gob.ec/wp-content/uploads/2020/08/INFOGRAFIA-NACIONALCOVI-19-COE-NACIONAL-08h00-13082020.xlsm.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">Government of Ecuador</t>
@@ -672,7 +672,7 @@
     <t xml:space="preserve">Germany - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.rki.de/DE/Content/InfAZ/N/Neuartiges_Coronavirus/Situationsberichte/2020-08-05-de.pdf?__blob=publicationFile</t>
+    <t xml:space="preserve">https://www.rki.de/DE/Content/InfAZ/N/Neuartiges_Coronavirus/Situationsberichte/2020-08-12-de.pdf?__blob=publicationFile</t>
   </si>
   <si>
     <t xml:space="preserve">Robert Koch Institut</t>
@@ -688,12 +688,13 @@
   </si>
   <si>
     <t xml:space="preserve">To determine how many laboratory tests regarding SARS-CoV-2 are carried out per calendar week in Germany and how many tests are positive or negative, the RKI has started a Germany-wide laboratory query. However, the number of laboratories reporting data seems to vary from week to week.
-The report published on 2 August 2020 states that “from the beginning of the collection up to and including calendar week 31/2020”:
-– The cumulative total of samples tested was 8,586,648;
-- For calendar week 31 (which ends 2 August), 161 labs reported 573,802 samples tested;
-- For calendar week 30 (which ends 26 July), 176 labs reported 569,868 samples tested;
-- For calendar week 29 (which ends 19 July), 173 labs reported 537,334 samples tested;
-- For calendar week 28 (which ends 12 July), 177 labs reported 509,298 samples tested;
+The report published on 12 August 2020 states that “from the beginning of the collection up to and including calendar week 32/2020”:
+– The cumulative total of samples tested was 9,265,361;
+- For calendar week 32 (which ends 9 August), 139 labs reported 672,171 samples tested;
+- For calendar week 31 (which ends 2 August), 165 labs reported 577,916 samples tested;
+- For calendar week 30 (which ends 26 July), 179 labs reported 570,681 samples tested;
+- For calendar week 29 (which ends 19 July), 175 labs reported 538,144 samples tested;
+- For calendar week 28 (which ends 12 July), 178 labs reported 510,103 samples tested;
 - For calendar week 27 (which ends 5 July), 150 labs reported 505,518 samples tested;
 - For calendar week 26 (which ends 28 June), 180 labs reported 467,004 samples tested;
 - For calendar week 25 (which ends 21 June), 175 labs reported 387,484 samples tested;
@@ -746,7 +747,7 @@
     <t xml:space="preserve">Greece - samples tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://eody.gov.gr/covid-gr-daily-report-20200811</t>
+    <t xml:space="preserve">https://eody.gov.gr/covid-gr-daily-report-20200813</t>
   </si>
   <si>
     <t xml:space="preserve">National Organization of Public Health</t>
@@ -885,7 +886,7 @@
     <t xml:space="preserve">Iran - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">http://irangov.ir/detail/344937</t>
+    <t xml:space="preserve">http://irangov.ir/detail/345030</t>
   </si>
   <si>
     <t xml:space="preserve">Government of Iran</t>
@@ -922,7 +923,7 @@
     <t xml:space="preserve">Israel - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://govextra.gov.il/media/24250/covid19-data-israel-05082020.csv</t>
+    <t xml:space="preserve">https://govextra.gov.il/media/24300/covid19-data-israel-06082020.csv</t>
   </si>
   <si>
     <t xml:space="preserve">Israel Ministry of Health</t>
@@ -981,7 +982,7 @@
     <t xml:space="preserve">Japan - people tested (incl. non-PCR)</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.mhlw.go.jp/stf/newpage_12918.html</t>
+    <t xml:space="preserve">https://www.mhlw.go.jp/stf/newpage_12978.html</t>
   </si>
   <si>
     <t xml:space="preserve">Ministry of Health, Labor and Welfare Press Release</t>
@@ -1006,10 +1007,10 @@
     <t xml:space="preserve">Japan - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.mhlw.go.jp/content/10906000/000658097.pdf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The cumulative total reported in the press release (1,298,747) does not sum to the cumulative total calculated from the weekly and daily figures reported by the MOH. See: https://www.mhlw.go.jp/content/10906000/000658097.pdf</t>
+    <t xml:space="preserve">https://www.mhlw.go.jp/content/10906000/000659117.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The cumulative total reported in the press release matches the cumulative total calculated from the weekly and daily figures reported by the MOH.</t>
   </si>
   <si>
     <t xml:space="preserve">On 11 April 2020, the MOH started providing a daily time series on the "Implementation status of PCR tests for new coronavirus in Japan (based on the date on which results were determined" (via Google translate). 
@@ -1062,7 +1063,7 @@
     <t xml:space="preserve">Kuwait - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/KUWAIT_MOH/status/1293147679262998531/photo/1</t>
+    <t xml:space="preserve">https://twitter.com/KUWAIT_MOH/status/1293849840422715392/photo/1</t>
   </si>
   <si>
     <t xml:space="preserve">Kuwait Ministry of Health</t>
@@ -1128,7 +1129,7 @@
     <t xml:space="preserve">Malaysia - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">http://covid-19.moh.gov.my/terkini/082020/situasi-terkini-11-ogos-2020</t>
+    <t xml:space="preserve">http://covid-19.moh.gov.my/terkini/082020/situasi-terkini-13-ogos-2020</t>
   </si>
   <si>
     <t xml:space="preserve">Ministry of Health Malaysia</t>
@@ -1154,7 +1155,7 @@
     <t xml:space="preserve">Maldives - samples tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/HPA_MV/status/1292869546123165696/photo/1</t>
+    <t xml:space="preserve">https://twitter.com/HPA_MV/status/1293962737379409927/photo/11</t>
   </si>
   <si>
     <t xml:space="preserve">Maldives Health Protection Agency</t>
@@ -1221,7 +1222,7 @@
     <t xml:space="preserve">Morocco - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/Ministere_Sante/status/1292875556942381065/photo/1</t>
+    <t xml:space="preserve">https://twitter.com/Ministere_Sante/status/1293960058716422146/photo/1</t>
   </si>
   <si>
     <t xml:space="preserve">Morocco Ministry of Health</t>
@@ -1261,7 +1262,7 @@
     <t xml:space="preserve">Nepal - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://drive.google.com/drive/folders/1O3VC_AWT2bSfZ1VrDY7e8OZ_mzsNjix-</t>
+    <t xml:space="preserve">https://drive.google.com/drive/folders/1hNjlpuQLYfn8PocMYmHBp1zXFvTDfyVX</t>
   </si>
   <si>
     <t xml:space="preserve">Ministry of Health and Population</t>
@@ -1486,7 +1487,7 @@
     <t xml:space="preserve">Poland - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/MZ_GOV_PL/status/1293109904773980161</t>
+    <t xml:space="preserve">https://twitter.com/MZ_GOV_PL/status/1293834678718234624</t>
   </si>
   <si>
     <t xml:space="preserve">Poland Ministry of Health</t>
@@ -1554,7 +1555,7 @@
     <t xml:space="preserve">Romania - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://gov.ro/ro/media/comunicate/buletin-de-presa-11-august-2020-ora-13-00&amp;page=1</t>
+    <t xml:space="preserve">https://gov.ro/ro/media/comunicate/buletin-de-presa-13-august-2020-ora-13-00&amp;page=1</t>
   </si>
   <si>
     <t xml:space="preserve">Ministry of Internal Affairs</t>
@@ -1577,7 +1578,7 @@
     <t xml:space="preserve">Russia - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://rospotrebnadzor.ru/about/info/news/news_details.php?ELEMENT_ID=15149</t>
+    <t xml:space="preserve">https://rospotrebnadzor.ru/about/info/news/news_details.php?ELEMENT_ID=15169</t>
   </si>
   <si>
     <t xml:space="preserve">Government of the Russian Federation</t>
@@ -1771,7 +1772,7 @@
     <t xml:space="preserve">South Korea - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.cdc.go.kr/board/board.es?mid=&amp;bid=0030&amp;act=view&amp;list_no=368103&amp;tag=&amp;nPage=1</t>
+    <t xml:space="preserve">https://www.cdc.go.kr/board/board.es?mid=&amp;bid=0030&amp;act=view&amp;list_no=368119&amp;tag=&amp;nPage=1</t>
   </si>
   <si>
     <t xml:space="preserve">South Korea CDC</t>
@@ -1893,7 +1894,7 @@
     <t xml:space="preserve">Thailand - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://ddc.moph.go.th/viralpneumonia/file/situation/situation-no221-110863n.pdf</t>
+    <t xml:space="preserve">https://ddc.moph.go.th/viralpneumonia/file/situation/situation-no223-130863.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">Department of Disease Control</t>
@@ -1981,7 +1982,7 @@
     <t xml:space="preserve">Uganda - samples tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/MinofHealthUG/status/1293106352869515265/photo/1</t>
+    <t xml:space="preserve">https://twitter.com/MinofHealthUG/status/1293840039407910914/photo/2</t>
   </si>
   <si>
     <t xml:space="preserve">Uganda Ministry of Health</t>
@@ -2041,7 +2042,7 @@
     <t xml:space="preserve">United Kingdom - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://assets.publishing.service.gov.uk/government/uploads/system/uploads/attachment_data/file/908596/2020-08-11_COVID-19_UK_testing_time_series.csv</t>
+    <t xml:space="preserve">https://assets.publishing.service.gov.uk/government/uploads/system/uploads/attachment_data/file/909375/2020-08-13_COVID-19_UK_testing_time_series.csv</t>
   </si>
   <si>
     <t xml:space="preserve">Public Health England/Department of Health and Social Care</t>
@@ -2121,7 +2122,7 @@
     <t xml:space="preserve">Uruguay - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.gub.uy/ministerio-salud-publica/comunicacion/noticias/informe-situacion-sobre-coronavirus-covid-19-uruguay-10-agosto</t>
+    <t xml:space="preserve">https://www.gub.uy/ministerio-salud-publica/comunicacion/noticias/informe-situacion-sobre-coronavirus-covid-19-uruguay-13-agosto</t>
   </si>
   <si>
     <t xml:space="preserve">https://www.gub.uy/ministerio-salud-publica/comunicacion/noticias</t>
@@ -2576,7 +2577,7 @@
         <v>20</v>
       </c>
       <c r="C2" s="1" t="n">
-        <v>44054</v>
+        <v>44056</v>
       </c>
       <c r="D2" t="s">
         <v>21</v>
@@ -2586,31 +2587,31 @@
       </c>
       <c r="F2"/>
       <c r="G2" t="n">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="H2" t="n">
-        <v>757987</v>
+        <v>793114</v>
       </c>
       <c r="I2" t="n">
-        <v>16.771</v>
+        <v>17.548</v>
       </c>
       <c r="J2" t="n">
-        <v>4595</v>
+        <v>4563</v>
       </c>
       <c r="K2" t="n">
-        <v>0.102</v>
+        <v>0.101</v>
       </c>
       <c r="L2" t="n">
-        <v>11658</v>
+        <v>11808</v>
       </c>
       <c r="M2" t="n">
-        <v>0.258</v>
+        <v>0.261</v>
       </c>
       <c r="N2" t="n">
-        <v>0.546</v>
+        <v>0.573</v>
       </c>
       <c r="O2" t="n">
-        <v>1.831</v>
+        <v>1.745</v>
       </c>
       <c r="P2" t="s">
         <v>22</v>
@@ -2633,7 +2634,7 @@
         <v>25</v>
       </c>
       <c r="C3" s="1" t="n">
-        <v>44054</v>
+        <v>44056</v>
       </c>
       <c r="D3" t="s">
         <v>26</v>
@@ -2643,31 +2644,31 @@
       </c>
       <c r="F3"/>
       <c r="G3" t="n">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="H3" t="n">
-        <v>923656</v>
+        <v>966220</v>
       </c>
       <c r="I3" t="n">
-        <v>20.437</v>
+        <v>21.379</v>
       </c>
       <c r="J3" t="n">
-        <v>5829</v>
+        <v>5449</v>
       </c>
       <c r="K3" t="n">
-        <v>0.129</v>
+        <v>0.121</v>
       </c>
       <c r="L3" t="n">
-        <v>13597</v>
+        <v>13871</v>
       </c>
       <c r="M3" t="n">
-        <v>0.301</v>
+        <v>0.307</v>
       </c>
       <c r="N3" t="n">
-        <v>0.468</v>
+        <v>0.488</v>
       </c>
       <c r="O3" t="n">
-        <v>2.135</v>
+        <v>2.049</v>
       </c>
       <c r="P3" t="s">
         <v>22</v>
@@ -2690,7 +2691,7 @@
         <v>30</v>
       </c>
       <c r="C4" s="1" t="n">
-        <v>44054</v>
+        <v>44056</v>
       </c>
       <c r="D4" t="s">
         <v>31</v>
@@ -2700,31 +2701,27 @@
       </c>
       <c r="F4"/>
       <c r="G4" t="n">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="H4" t="n">
-        <v>4980172</v>
+        <v>5109785</v>
       </c>
       <c r="I4" t="n">
-        <v>195.302</v>
-      </c>
-      <c r="J4" t="n">
-        <v>61626</v>
-      </c>
-      <c r="K4" t="n">
-        <v>2.417</v>
-      </c>
+        <v>200.385</v>
+      </c>
+      <c r="J4"/>
+      <c r="K4"/>
       <c r="L4" t="n">
-        <v>71222</v>
+        <v>68242</v>
       </c>
       <c r="M4" t="n">
-        <v>2.793</v>
+        <v>2.676</v>
       </c>
       <c r="N4" t="n">
         <v>0.006</v>
       </c>
       <c r="O4" t="n">
-        <v>161.921</v>
+        <v>178.045</v>
       </c>
       <c r="P4" t="s">
         <v>32</v>
@@ -2747,7 +2744,7 @@
         <v>36</v>
       </c>
       <c r="C5" s="1" t="n">
-        <v>44055</v>
+        <v>44056</v>
       </c>
       <c r="D5" t="s">
         <v>37</v>
@@ -2757,28 +2754,32 @@
       </c>
       <c r="F5"/>
       <c r="G5" t="n">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="H5" t="n">
-        <v>983018</v>
+        <v>991508</v>
       </c>
       <c r="I5" t="n">
-        <v>109.147</v>
+        <v>110.089</v>
       </c>
       <c r="J5" t="n">
-        <v>8510</v>
+        <v>8490</v>
       </c>
       <c r="K5" t="n">
-        <v>0.945</v>
+        <v>0.943</v>
       </c>
       <c r="L5" t="n">
-        <v>7490</v>
+        <v>7748</v>
       </c>
       <c r="M5" t="n">
-        <v>0.832</v>
-      </c>
-      <c r="N5"/>
-      <c r="O5"/>
+        <v>0.86</v>
+      </c>
+      <c r="N5" t="n">
+        <v>0.017</v>
+      </c>
+      <c r="O5" t="n">
+        <v>58.57</v>
+      </c>
       <c r="P5" t="s">
         <v>39</v>
       </c>
@@ -2800,7 +2801,7 @@
         <v>43</v>
       </c>
       <c r="C6" s="1" t="n">
-        <v>44055</v>
+        <v>44057</v>
       </c>
       <c r="D6" t="s">
         <v>44</v>
@@ -2810,28 +2811,28 @@
       </c>
       <c r="F6"/>
       <c r="G6" t="n">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="H6" t="n">
-        <v>923342</v>
+        <v>944798</v>
       </c>
       <c r="I6" t="n">
-        <v>542.637</v>
-      </c>
-      <c r="J6" t="n">
-        <v>11231</v>
-      </c>
-      <c r="K6" t="n">
-        <v>6.6</v>
-      </c>
+        <v>555.246</v>
+      </c>
+      <c r="J6"/>
+      <c r="K6"/>
       <c r="L6" t="n">
-        <v>8636</v>
+        <v>9728</v>
       </c>
       <c r="M6" t="n">
-        <v>5.075</v>
-      </c>
-      <c r="N6"/>
-      <c r="O6"/>
+        <v>5.717</v>
+      </c>
+      <c r="N6" t="n">
+        <v>0.042</v>
+      </c>
+      <c r="O6" t="n">
+        <v>24.003</v>
+      </c>
       <c r="P6" t="s">
         <v>46</v>
       </c>
@@ -2910,7 +2911,7 @@
         <v>57</v>
       </c>
       <c r="C8" s="1" t="n">
-        <v>44054</v>
+        <v>44055</v>
       </c>
       <c r="D8" t="s">
         <v>58</v>
@@ -2920,27 +2921,31 @@
       </c>
       <c r="F8"/>
       <c r="G8" t="n">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="H8" t="n">
-        <v>1377540</v>
+        <v>1384026</v>
       </c>
       <c r="I8" t="n">
-        <v>145.782</v>
-      </c>
-      <c r="J8"/>
-      <c r="K8"/>
+        <v>146.468</v>
+      </c>
+      <c r="J8" t="n">
+        <v>6486</v>
+      </c>
+      <c r="K8" t="n">
+        <v>0.686</v>
+      </c>
       <c r="L8" t="n">
-        <v>7395</v>
+        <v>6998</v>
       </c>
       <c r="M8" t="n">
-        <v>0.783</v>
+        <v>0.741</v>
       </c>
       <c r="N8" t="n">
         <v>0.015</v>
       </c>
       <c r="O8" t="n">
-        <v>66.28</v>
+        <v>64.882</v>
       </c>
       <c r="P8" t="s">
         <v>59</v>
@@ -2963,7 +2968,7 @@
         <v>63</v>
       </c>
       <c r="C9" s="1" t="n">
-        <v>44053</v>
+        <v>44055</v>
       </c>
       <c r="D9" t="s">
         <v>64</v>
@@ -2973,31 +2978,31 @@
       </c>
       <c r="F9"/>
       <c r="G9" t="n">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="H9" t="n">
-        <v>1888061</v>
+        <v>1923861</v>
       </c>
       <c r="I9" t="n">
-        <v>162.91</v>
+        <v>165.999</v>
       </c>
       <c r="J9" t="n">
-        <v>12454</v>
+        <v>18728</v>
       </c>
       <c r="K9" t="n">
-        <v>1.075</v>
+        <v>1.616</v>
       </c>
       <c r="L9" t="n">
-        <v>19031</v>
+        <v>18676</v>
       </c>
       <c r="M9" t="n">
-        <v>1.642</v>
+        <v>1.611</v>
       </c>
       <c r="N9" t="n">
         <v>0.03</v>
       </c>
       <c r="O9" t="n">
-        <v>33.751</v>
+        <v>32.98</v>
       </c>
       <c r="P9" t="s">
         <v>65</v>
@@ -3020,7 +3025,7 @@
         <v>69</v>
       </c>
       <c r="C10" s="1" t="n">
-        <v>44053</v>
+        <v>44055</v>
       </c>
       <c r="D10" t="s">
         <v>70</v>
@@ -3030,31 +3035,31 @@
       </c>
       <c r="F10"/>
       <c r="G10" t="n">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="H10" t="n">
-        <v>179553</v>
+        <v>186964</v>
       </c>
       <c r="I10" t="n">
-        <v>15.382</v>
+        <v>16.017</v>
       </c>
       <c r="J10" t="n">
-        <v>3245</v>
+        <v>3652</v>
       </c>
       <c r="K10" t="n">
-        <v>0.278</v>
+        <v>0.313</v>
       </c>
       <c r="L10" t="n">
-        <v>2818</v>
+        <v>2980</v>
       </c>
       <c r="M10" t="n">
-        <v>0.241</v>
+        <v>0.255</v>
       </c>
       <c r="N10" t="n">
-        <v>0.499</v>
+        <v>0.478</v>
       </c>
       <c r="O10" t="n">
-        <v>2.003</v>
+        <v>2.093</v>
       </c>
       <c r="P10" t="s">
         <v>45</v>
@@ -3128,7 +3133,7 @@
         <v>82</v>
       </c>
       <c r="C12" s="1" t="n">
-        <v>44055</v>
+        <v>44057</v>
       </c>
       <c r="D12" t="s">
         <v>83</v>
@@ -3138,28 +3143,32 @@
       </c>
       <c r="F12"/>
       <c r="G12" t="n">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="H12" t="n">
-        <v>313866</v>
+        <v>324851</v>
       </c>
       <c r="I12" t="n">
-        <v>45.171</v>
+        <v>46.752</v>
       </c>
       <c r="J12" t="n">
-        <v>5388</v>
+        <v>5877</v>
       </c>
       <c r="K12" t="n">
-        <v>0.775</v>
+        <v>0.846</v>
       </c>
       <c r="L12" t="n">
-        <v>4152</v>
+        <v>4395</v>
       </c>
       <c r="M12" t="n">
-        <v>0.598</v>
-      </c>
-      <c r="N12"/>
-      <c r="O12"/>
+        <v>0.633</v>
+      </c>
+      <c r="N12" t="n">
+        <v>0.044</v>
+      </c>
+      <c r="O12" t="n">
+        <v>22.755</v>
+      </c>
       <c r="P12" t="s">
         <v>85</v>
       </c>
@@ -3181,7 +3190,7 @@
         <v>88</v>
       </c>
       <c r="C13" s="1" t="n">
-        <v>44055</v>
+        <v>44057</v>
       </c>
       <c r="D13" t="s">
         <v>89</v>
@@ -3191,28 +3200,32 @@
       </c>
       <c r="F13"/>
       <c r="G13" t="n">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="H13" t="n">
-        <v>4541747</v>
+        <v>4635105</v>
       </c>
       <c r="I13" t="n">
-        <v>120.336</v>
+        <v>122.81</v>
       </c>
       <c r="J13" t="n">
-        <v>36529</v>
+        <v>54022</v>
       </c>
       <c r="K13" t="n">
-        <v>0.968</v>
+        <v>1.431</v>
       </c>
       <c r="L13" t="n">
-        <v>41026</v>
+        <v>45133</v>
       </c>
       <c r="M13" t="n">
-        <v>1.087</v>
-      </c>
-      <c r="N13"/>
-      <c r="O13"/>
+        <v>1.196</v>
+      </c>
+      <c r="N13" t="n">
+        <v>0.009</v>
+      </c>
+      <c r="O13" t="n">
+        <v>117.534</v>
+      </c>
       <c r="P13" t="s">
         <v>90</v>
       </c>
@@ -3234,7 +3247,7 @@
         <v>93</v>
       </c>
       <c r="C14" s="1" t="n">
-        <v>44054</v>
+        <v>44056</v>
       </c>
       <c r="D14" t="s">
         <v>94</v>
@@ -3246,31 +3259,31 @@
         <v>95</v>
       </c>
       <c r="G14" t="n">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="H14" t="n">
-        <v>1889616</v>
+        <v>1932592</v>
       </c>
       <c r="I14" t="n">
-        <v>98.849</v>
+        <v>101.097</v>
       </c>
       <c r="J14" t="n">
-        <v>22249</v>
+        <v>23628</v>
       </c>
       <c r="K14" t="n">
-        <v>1.164</v>
+        <v>1.236</v>
       </c>
       <c r="L14" t="n">
-        <v>24743</v>
+        <v>24568</v>
       </c>
       <c r="M14" t="n">
-        <v>1.294</v>
+        <v>1.285</v>
       </c>
       <c r="N14" t="n">
         <v>0.078</v>
       </c>
       <c r="O14" t="n">
-        <v>12.781</v>
+        <v>12.791</v>
       </c>
       <c r="P14" t="s">
         <v>96</v>
@@ -3293,7 +3306,7 @@
         <v>100</v>
       </c>
       <c r="C15" s="1" t="n">
-        <v>44054</v>
+        <v>44055</v>
       </c>
       <c r="D15" t="s">
         <v>101</v>
@@ -3303,31 +3316,31 @@
       </c>
       <c r="F15"/>
       <c r="G15" t="n">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="H15" t="n">
-        <v>1982831</v>
+        <v>2023256</v>
       </c>
       <c r="I15" t="n">
-        <v>38.969</v>
+        <v>39.763</v>
       </c>
       <c r="J15" t="n">
-        <v>40101</v>
+        <v>40425</v>
       </c>
       <c r="K15" t="n">
-        <v>0.788</v>
+        <v>0.794</v>
       </c>
       <c r="L15" t="n">
-        <v>37046</v>
+        <v>37355</v>
       </c>
       <c r="M15" t="n">
-        <v>0.728</v>
+        <v>0.734</v>
       </c>
       <c r="N15" t="n">
-        <v>0.269</v>
+        <v>0.289</v>
       </c>
       <c r="O15" t="n">
-        <v>3.717</v>
+        <v>3.465</v>
       </c>
       <c r="P15" t="s">
         <v>102</v>
@@ -3350,7 +3363,7 @@
         <v>106</v>
       </c>
       <c r="C16" s="1" t="n">
-        <v>44053</v>
+        <v>44055</v>
       </c>
       <c r="D16" t="s">
         <v>107</v>
@@ -3360,31 +3373,31 @@
       </c>
       <c r="F16"/>
       <c r="G16" t="n">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="H16" t="n">
-        <v>94259</v>
+        <v>97283</v>
       </c>
       <c r="I16" t="n">
-        <v>18.504</v>
+        <v>19.097</v>
       </c>
       <c r="J16" t="n">
-        <v>1476</v>
+        <v>1721</v>
       </c>
       <c r="K16" t="n">
-        <v>0.29</v>
+        <v>0.338</v>
       </c>
       <c r="L16" t="n">
-        <v>1758</v>
+        <v>1706</v>
       </c>
       <c r="M16" t="n">
-        <v>0.345</v>
+        <v>0.335</v>
       </c>
       <c r="N16" t="n">
-        <v>0.35</v>
+        <v>0.391</v>
       </c>
       <c r="O16" t="n">
-        <v>2.855</v>
+        <v>2.557</v>
       </c>
       <c r="P16" t="s">
         <v>108</v>
@@ -3407,7 +3420,7 @@
         <v>112</v>
       </c>
       <c r="C17" s="1" t="n">
-        <v>44052</v>
+        <v>44054</v>
       </c>
       <c r="D17" t="s">
         <v>113</v>
@@ -3417,31 +3430,31 @@
       </c>
       <c r="F17"/>
       <c r="G17" t="n">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="H17" t="n">
-        <v>109677</v>
+        <v>110359</v>
       </c>
       <c r="I17" t="n">
-        <v>4.158</v>
+        <v>4.184</v>
       </c>
       <c r="J17" t="n">
-        <v>2924</v>
+        <v>682</v>
       </c>
       <c r="K17" t="n">
-        <v>0.111</v>
+        <v>0.026</v>
       </c>
       <c r="L17" t="n">
-        <v>999</v>
+        <v>962</v>
       </c>
       <c r="M17" t="n">
-        <v>0.038</v>
+        <v>0.036</v>
       </c>
       <c r="N17" t="n">
-        <v>0.073</v>
+        <v>0.086</v>
       </c>
       <c r="O17" t="n">
-        <v>13.685</v>
+        <v>11.651</v>
       </c>
       <c r="P17" t="s">
         <v>114</v>
@@ -3464,7 +3477,7 @@
         <v>118</v>
       </c>
       <c r="C18" s="1" t="n">
-        <v>44054</v>
+        <v>44056</v>
       </c>
       <c r="D18" t="s">
         <v>119</v>
@@ -3474,31 +3487,31 @@
       </c>
       <c r="F18"/>
       <c r="G18" t="n">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="H18" t="n">
-        <v>130688</v>
+        <v>133493</v>
       </c>
       <c r="I18" t="n">
-        <v>31.834</v>
+        <v>32.517</v>
       </c>
       <c r="J18" t="n">
-        <v>1309</v>
+        <v>1201</v>
       </c>
       <c r="K18" t="n">
-        <v>0.319</v>
+        <v>0.293</v>
       </c>
       <c r="L18" t="n">
-        <v>1070</v>
+        <v>1168</v>
       </c>
       <c r="M18" t="n">
-        <v>0.261</v>
+        <v>0.285</v>
       </c>
       <c r="N18" t="n">
-        <v>0.047</v>
+        <v>0.06</v>
       </c>
       <c r="O18" t="n">
-        <v>21.218</v>
+        <v>16.551</v>
       </c>
       <c r="P18" t="s">
         <v>120</v>
@@ -3521,7 +3534,7 @@
         <v>124</v>
       </c>
       <c r="C19" s="1" t="n">
-        <v>44053</v>
+        <v>44055</v>
       </c>
       <c r="D19" t="s">
         <v>125</v>
@@ -3533,31 +3546,31 @@
         <v>127</v>
       </c>
       <c r="G19" t="n">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="H19" t="n">
-        <v>305652</v>
+        <v>314499</v>
       </c>
       <c r="I19" t="n">
-        <v>26.985</v>
+        <v>27.766</v>
       </c>
       <c r="J19" t="n">
-        <v>4054</v>
+        <v>4591</v>
       </c>
       <c r="K19" t="n">
-        <v>0.358</v>
+        <v>0.405</v>
       </c>
       <c r="L19" t="n">
-        <v>3970</v>
+        <v>4147</v>
       </c>
       <c r="M19" t="n">
-        <v>0.351</v>
+        <v>0.366</v>
       </c>
       <c r="N19" t="n">
-        <v>0.011</v>
+        <v>0.014</v>
       </c>
       <c r="O19" t="n">
-        <v>90.521</v>
+        <v>74.054</v>
       </c>
       <c r="P19" t="s">
         <v>126</v>
@@ -3580,7 +3593,7 @@
         <v>131</v>
       </c>
       <c r="C20" s="1" t="n">
-        <v>44053</v>
+        <v>44055</v>
       </c>
       <c r="D20" t="s">
         <v>132</v>
@@ -3590,31 +3603,31 @@
       </c>
       <c r="F20"/>
       <c r="G20" t="n">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="H20" t="n">
-        <v>757957</v>
+        <v>775991</v>
       </c>
       <c r="I20" t="n">
-        <v>70.778</v>
+        <v>72.462</v>
       </c>
       <c r="J20" t="n">
-        <v>5673</v>
+        <v>7507</v>
       </c>
       <c r="K20" t="n">
-        <v>0.53</v>
+        <v>0.701</v>
       </c>
       <c r="L20" t="n">
-        <v>6281</v>
+        <v>6649</v>
       </c>
       <c r="M20" t="n">
-        <v>0.587</v>
+        <v>0.621</v>
       </c>
       <c r="N20" t="n">
-        <v>0.035</v>
+        <v>0.032</v>
       </c>
       <c r="O20" t="n">
-        <v>28.275</v>
+        <v>31.091</v>
       </c>
       <c r="P20" t="s">
         <v>45</v>
@@ -3637,7 +3650,7 @@
         <v>136</v>
       </c>
       <c r="C21" s="1" t="n">
-        <v>44053</v>
+        <v>44055</v>
       </c>
       <c r="D21" t="s">
         <v>137</v>
@@ -3647,27 +3660,27 @@
       </c>
       <c r="F21"/>
       <c r="G21" t="n">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="H21"/>
       <c r="I21"/>
       <c r="J21" t="n">
-        <v>299</v>
+        <v>413</v>
       </c>
       <c r="K21" t="n">
-        <v>0.003</v>
+        <v>0.005</v>
       </c>
       <c r="L21" t="n">
-        <v>359</v>
+        <v>365</v>
       </c>
       <c r="M21" t="n">
         <v>0.004</v>
       </c>
       <c r="N21" t="n">
-        <v>0.135</v>
+        <v>0.126</v>
       </c>
       <c r="O21" t="n">
-        <v>7.413</v>
+        <v>7.96</v>
       </c>
       <c r="P21" t="s">
         <v>138</v>
@@ -3690,7 +3703,7 @@
         <v>142</v>
       </c>
       <c r="C22" s="1" t="n">
-        <v>44053</v>
+        <v>44055</v>
       </c>
       <c r="D22" t="s">
         <v>143</v>
@@ -3700,31 +3713,31 @@
       </c>
       <c r="F22"/>
       <c r="G22" t="n">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="H22" t="n">
-        <v>1745491</v>
+        <v>1800366</v>
       </c>
       <c r="I22" t="n">
-        <v>301.352</v>
+        <v>310.826</v>
       </c>
       <c r="J22" t="n">
-        <v>6541</v>
+        <v>5975</v>
       </c>
       <c r="K22" t="n">
-        <v>1.129</v>
+        <v>1.032</v>
       </c>
       <c r="L22" t="n">
-        <v>21583</v>
+        <v>22307</v>
       </c>
       <c r="M22" t="n">
-        <v>3.726</v>
+        <v>3.851</v>
       </c>
       <c r="N22" t="n">
-        <v>0.004</v>
+        <v>0.006</v>
       </c>
       <c r="O22" t="n">
-        <v>231.364</v>
+        <v>176.24</v>
       </c>
       <c r="P22" t="s">
         <v>144</v>
@@ -3747,7 +3760,7 @@
         <v>148</v>
       </c>
       <c r="C23" s="1" t="n">
-        <v>44052</v>
+        <v>44056</v>
       </c>
       <c r="D23" t="s">
         <v>149</v>
@@ -3759,25 +3772,25 @@
         <v>151</v>
       </c>
       <c r="G23" t="n">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="H23" t="n">
-        <v>204729</v>
+        <v>214477</v>
       </c>
       <c r="I23" t="n">
-        <v>11.604</v>
+        <v>12.156</v>
       </c>
       <c r="J23" t="n">
-        <v>2335</v>
+        <v>3285</v>
       </c>
       <c r="K23" t="n">
-        <v>0.132</v>
+        <v>0.186</v>
       </c>
       <c r="L23" t="n">
-        <v>2829</v>
+        <v>2875</v>
       </c>
       <c r="M23" t="n">
-        <v>0.16</v>
+        <v>0.163</v>
       </c>
       <c r="N23"/>
       <c r="O23"/>
@@ -3859,7 +3872,7 @@
         <v>161</v>
       </c>
       <c r="C25" s="1" t="n">
-        <v>44054</v>
+        <v>44056</v>
       </c>
       <c r="D25" t="s">
         <v>162</v>
@@ -3869,31 +3882,31 @@
       </c>
       <c r="F25"/>
       <c r="G25" t="n">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="H25" t="n">
-        <v>129633</v>
+        <v>132270</v>
       </c>
       <c r="I25" t="n">
-        <v>97.723</v>
+        <v>99.711</v>
       </c>
       <c r="J25" t="n">
-        <v>1427</v>
+        <v>1451</v>
       </c>
       <c r="K25" t="n">
-        <v>1.076</v>
+        <v>1.094</v>
       </c>
       <c r="L25" t="n">
-        <v>1103</v>
+        <v>1207</v>
       </c>
       <c r="M25" t="n">
-        <v>0.831</v>
+        <v>0.91</v>
       </c>
       <c r="N25" t="n">
-        <v>0.01</v>
+        <v>0.007</v>
       </c>
       <c r="O25" t="n">
-        <v>98.987</v>
+        <v>138.508</v>
       </c>
       <c r="P25" t="s">
         <v>164</v>
@@ -4024,7 +4037,7 @@
         <v>180</v>
       </c>
       <c r="C28" s="1" t="n">
-        <v>44053</v>
+        <v>44054</v>
       </c>
       <c r="D28" t="s">
         <v>181</v>
@@ -4034,31 +4047,31 @@
       </c>
       <c r="F28"/>
       <c r="G28" t="n">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="H28" t="n">
-        <v>431048</v>
+        <v>440037</v>
       </c>
       <c r="I28" t="n">
-        <v>77.796</v>
+        <v>79.419</v>
       </c>
       <c r="J28" t="n">
-        <v>6326</v>
+        <v>6996</v>
       </c>
       <c r="K28" t="n">
-        <v>1.142</v>
+        <v>1.263</v>
       </c>
       <c r="L28" t="n">
-        <v>6463</v>
+        <v>6616</v>
       </c>
       <c r="M28" t="n">
-        <v>1.166</v>
+        <v>1.194</v>
       </c>
       <c r="N28" t="n">
         <v>0.003</v>
       </c>
       <c r="O28" t="n">
-        <v>345.351</v>
+        <v>343.052</v>
       </c>
       <c r="P28" t="s">
         <v>183</v>
@@ -4081,7 +4094,7 @@
         <v>186</v>
       </c>
       <c r="C29" s="1" t="n">
-        <v>44050</v>
+        <v>44053</v>
       </c>
       <c r="D29" t="s">
         <v>187</v>
@@ -4091,27 +4104,27 @@
       </c>
       <c r="F29"/>
       <c r="G29" t="n">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="H29"/>
       <c r="I29"/>
       <c r="J29" t="n">
-        <v>95552</v>
+        <v>97453</v>
       </c>
       <c r="K29" t="n">
-        <v>1.464</v>
+        <v>1.493</v>
       </c>
       <c r="L29" t="n">
-        <v>76597</v>
+        <v>77189</v>
       </c>
       <c r="M29" t="n">
-        <v>1.173</v>
+        <v>1.183</v>
       </c>
       <c r="N29" t="n">
-        <v>0.017</v>
+        <v>0.019</v>
       </c>
       <c r="O29" t="n">
-        <v>59.181</v>
+        <v>54.021</v>
       </c>
       <c r="P29" t="s">
         <v>188</v>
@@ -4189,7 +4202,7 @@
         <v>196</v>
       </c>
       <c r="C31" s="1" t="n">
-        <v>44045</v>
+        <v>44052</v>
       </c>
       <c r="D31" t="s">
         <v>197</v>
@@ -4201,27 +4214,27 @@
         <v>199</v>
       </c>
       <c r="G31" t="n">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H31" t="n">
-        <v>8586648</v>
+        <v>9265361</v>
       </c>
       <c r="I31" t="n">
-        <v>102.486</v>
+        <v>110.586</v>
       </c>
       <c r="J31"/>
       <c r="K31"/>
       <c r="L31" t="n">
-        <v>81972</v>
+        <v>96024</v>
       </c>
       <c r="M31" t="n">
-        <v>0.978</v>
+        <v>1.146</v>
       </c>
       <c r="N31" t="n">
-        <v>0.008</v>
+        <v>0.009</v>
       </c>
       <c r="O31" t="n">
-        <v>124.093</v>
+        <v>112.065</v>
       </c>
       <c r="P31" t="s">
         <v>198</v>
@@ -4244,7 +4257,7 @@
         <v>204</v>
       </c>
       <c r="C32" s="1" t="n">
-        <v>44050</v>
+        <v>44054</v>
       </c>
       <c r="D32" t="s">
         <v>205</v>
@@ -4254,31 +4267,31 @@
       </c>
       <c r="F32"/>
       <c r="G32" t="n">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="H32" t="n">
-        <v>415671</v>
+        <v>421588</v>
       </c>
       <c r="I32" t="n">
-        <v>13.377</v>
+        <v>13.568</v>
       </c>
       <c r="J32" t="n">
-        <v>1836</v>
+        <v>1998</v>
       </c>
       <c r="K32" t="n">
-        <v>0.059</v>
+        <v>0.064</v>
       </c>
       <c r="L32" t="n">
-        <v>2318</v>
+        <v>1745</v>
       </c>
       <c r="M32" t="n">
-        <v>0.075</v>
+        <v>0.056</v>
       </c>
       <c r="N32" t="n">
-        <v>0.305</v>
+        <v>0.278</v>
       </c>
       <c r="O32" t="n">
-        <v>3.275</v>
+        <v>3.593</v>
       </c>
       <c r="P32" t="s">
         <v>207</v>
@@ -4301,7 +4314,7 @@
         <v>211</v>
       </c>
       <c r="C33" s="1" t="n">
-        <v>44054</v>
+        <v>44056</v>
       </c>
       <c r="D33" t="s">
         <v>212</v>
@@ -4311,31 +4324,31 @@
       </c>
       <c r="F33"/>
       <c r="G33" t="n">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="H33" t="n">
-        <v>668739</v>
+        <v>687338</v>
       </c>
       <c r="I33" t="n">
-        <v>64.16</v>
+        <v>65.944</v>
       </c>
       <c r="J33" t="n">
-        <v>10561</v>
+        <v>7553</v>
       </c>
       <c r="K33" t="n">
-        <v>1.013</v>
+        <v>0.725</v>
       </c>
       <c r="L33" t="n">
-        <v>9861</v>
+        <v>9706</v>
       </c>
       <c r="M33" t="n">
-        <v>0.946</v>
+        <v>0.931</v>
       </c>
       <c r="N33" t="n">
-        <v>0.015</v>
+        <v>0.018</v>
       </c>
       <c r="O33" t="n">
-        <v>68.208</v>
+        <v>56.43</v>
       </c>
       <c r="P33" t="s">
         <v>214</v>
@@ -4358,7 +4371,7 @@
         <v>218</v>
       </c>
       <c r="C34" s="1" t="n">
-        <v>44047</v>
+        <v>44054</v>
       </c>
       <c r="D34" t="s">
         <v>219</v>
@@ -4371,15 +4384,19 @@
         <v>8</v>
       </c>
       <c r="H34" t="n">
-        <v>692430</v>
+        <v>780410</v>
       </c>
       <c r="I34" t="n">
-        <v>92.361</v>
+        <v>104.096</v>
       </c>
       <c r="J34"/>
       <c r="K34"/>
-      <c r="L34"/>
-      <c r="M34"/>
+      <c r="L34" t="n">
+        <v>12322</v>
+      </c>
+      <c r="M34" t="n">
+        <v>1.644</v>
+      </c>
       <c r="N34"/>
       <c r="O34"/>
       <c r="P34" t="s">
@@ -4462,7 +4479,7 @@
         <v>233</v>
       </c>
       <c r="C36" s="1" t="n">
-        <v>44053</v>
+        <v>44055</v>
       </c>
       <c r="D36" t="s">
         <v>234</v>
@@ -4472,31 +4489,31 @@
       </c>
       <c r="F36"/>
       <c r="G36" t="n">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="H36" t="n">
-        <v>78812</v>
+        <v>80724</v>
       </c>
       <c r="I36" t="n">
-        <v>230.951</v>
+        <v>236.554</v>
       </c>
       <c r="J36" t="n">
-        <v>345</v>
+        <v>722</v>
       </c>
       <c r="K36" t="n">
-        <v>1.011</v>
+        <v>2.116</v>
       </c>
       <c r="L36" t="n">
-        <v>583</v>
+        <v>651</v>
       </c>
       <c r="M36" t="n">
-        <v>1.708</v>
+        <v>1.908</v>
       </c>
       <c r="N36" t="n">
-        <v>0.012</v>
+        <v>0.011</v>
       </c>
       <c r="O36" t="n">
-        <v>80.02</v>
+        <v>91.14</v>
       </c>
       <c r="P36" t="s">
         <v>235</v>
@@ -4519,7 +4536,7 @@
         <v>238</v>
       </c>
       <c r="C37" s="1" t="n">
-        <v>43945</v>
+        <v>43944</v>
       </c>
       <c r="D37" t="s">
         <v>239</v>
@@ -4552,10 +4569,10 @@
         <v>0.021</v>
       </c>
       <c r="N37" t="n">
-        <v>0.047</v>
+        <v>0.043</v>
       </c>
       <c r="O37" t="n">
-        <v>21.385</v>
+        <v>22.991</v>
       </c>
       <c r="P37" t="s">
         <v>240</v>
@@ -4578,7 +4595,7 @@
         <v>243</v>
       </c>
       <c r="C38" s="1" t="n">
-        <v>44054</v>
+        <v>44056</v>
       </c>
       <c r="D38" t="s">
         <v>239</v>
@@ -4590,31 +4607,31 @@
         <v>241</v>
       </c>
       <c r="G38" t="n">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="H38" t="n">
-        <v>25281848</v>
+        <v>27694416</v>
       </c>
       <c r="I38" t="n">
-        <v>18.32</v>
+        <v>20.068</v>
       </c>
       <c r="J38" t="n">
-        <v>698290</v>
+        <v>848728</v>
       </c>
       <c r="K38" t="n">
-        <v>0.506</v>
+        <v>0.615</v>
       </c>
       <c r="L38" t="n">
-        <v>631014</v>
+        <v>700860</v>
       </c>
       <c r="M38" t="n">
-        <v>0.457</v>
+        <v>0.508</v>
       </c>
       <c r="N38" t="n">
-        <v>0.093</v>
+        <v>0.088</v>
       </c>
       <c r="O38" t="n">
-        <v>10.697</v>
+        <v>11.354</v>
       </c>
       <c r="P38" t="s">
         <v>240</v>
@@ -4637,7 +4654,7 @@
         <v>245</v>
       </c>
       <c r="C39" s="1" t="n">
-        <v>44054</v>
+        <v>44056</v>
       </c>
       <c r="D39" t="s">
         <v>246</v>
@@ -4647,31 +4664,31 @@
       </c>
       <c r="F39"/>
       <c r="G39" t="n">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="H39" t="n">
-        <v>998406</v>
+        <v>1026954</v>
       </c>
       <c r="I39" t="n">
-        <v>3.65</v>
+        <v>3.755</v>
       </c>
       <c r="J39" t="n">
-        <v>13513</v>
+        <v>14850</v>
       </c>
       <c r="K39" t="n">
-        <v>0.049</v>
+        <v>0.054</v>
       </c>
       <c r="L39" t="n">
-        <v>12917</v>
+        <v>12949</v>
       </c>
       <c r="M39" t="n">
         <v>0.047</v>
       </c>
       <c r="N39" t="n">
-        <v>0.154</v>
+        <v>0.153</v>
       </c>
       <c r="O39" t="n">
-        <v>6.482</v>
+        <v>6.546</v>
       </c>
       <c r="P39" t="s">
         <v>247</v>
@@ -4694,7 +4711,7 @@
         <v>251</v>
       </c>
       <c r="C40" s="1" t="n">
-        <v>44054</v>
+        <v>44055</v>
       </c>
       <c r="D40" t="s">
         <v>252</v>
@@ -4704,19 +4721,19 @@
       </c>
       <c r="F40"/>
       <c r="G40" t="n">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="H40" t="n">
-        <v>2736514</v>
+        <v>2763225</v>
       </c>
       <c r="I40" t="n">
-        <v>32.58</v>
+        <v>32.898</v>
       </c>
       <c r="J40" t="n">
-        <v>24697</v>
+        <v>26711</v>
       </c>
       <c r="K40" t="n">
-        <v>0.294</v>
+        <v>0.318</v>
       </c>
       <c r="L40" t="n">
         <v>25163</v>
@@ -4725,10 +4742,10 @@
         <v>0.3</v>
       </c>
       <c r="N40" t="n">
-        <v>0.095</v>
+        <v>0.093</v>
       </c>
       <c r="O40" t="n">
-        <v>10.479</v>
+        <v>10.738</v>
       </c>
       <c r="P40" t="s">
         <v>253</v>
@@ -4751,7 +4768,7 @@
         <v>257</v>
       </c>
       <c r="C41" s="1" t="n">
-        <v>44054</v>
+        <v>44056</v>
       </c>
       <c r="D41" t="s">
         <v>258</v>
@@ -4761,31 +4778,31 @@
       </c>
       <c r="F41"/>
       <c r="G41" t="n">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="H41" t="n">
-        <v>674695</v>
+        <v>687699</v>
       </c>
       <c r="I41" t="n">
-        <v>136.639</v>
+        <v>139.272</v>
       </c>
       <c r="J41" t="n">
-        <v>3937</v>
+        <v>7072</v>
       </c>
       <c r="K41" t="n">
-        <v>0.797</v>
+        <v>1.432</v>
       </c>
       <c r="L41" t="n">
-        <v>4339</v>
+        <v>4969</v>
       </c>
       <c r="M41" t="n">
-        <v>0.879</v>
+        <v>1.006</v>
       </c>
       <c r="N41" t="n">
-        <v>0.018</v>
+        <v>0.015</v>
       </c>
       <c r="O41" t="n">
-        <v>54.237</v>
+        <v>65.015</v>
       </c>
       <c r="P41" t="s">
         <v>259</v>
@@ -4808,7 +4825,7 @@
         <v>262</v>
       </c>
       <c r="C42" s="1" t="n">
-        <v>44048</v>
+        <v>44049</v>
       </c>
       <c r="D42" t="s">
         <v>263</v>
@@ -4818,31 +4835,31 @@
       </c>
       <c r="F42"/>
       <c r="G42" t="n">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="H42" t="n">
-        <v>1867725</v>
+        <v>1896525</v>
       </c>
       <c r="I42" t="n">
-        <v>215.784</v>
+        <v>219.111</v>
       </c>
       <c r="J42" t="n">
-        <v>25796</v>
+        <v>28799</v>
       </c>
       <c r="K42" t="n">
-        <v>2.98</v>
+        <v>3.327</v>
       </c>
       <c r="L42" t="n">
-        <v>19726</v>
+        <v>20704</v>
       </c>
       <c r="M42" t="n">
-        <v>2.279</v>
+        <v>2.392</v>
       </c>
       <c r="N42" t="n">
-        <v>0.073</v>
+        <v>0.067</v>
       </c>
       <c r="O42" t="n">
-        <v>13.689</v>
+        <v>14.837</v>
       </c>
       <c r="P42" t="s">
         <v>45</v>
@@ -4865,7 +4882,7 @@
         <v>268</v>
       </c>
       <c r="C43" s="1" t="n">
-        <v>44054</v>
+        <v>44056</v>
       </c>
       <c r="D43" t="s">
         <v>269</v>
@@ -4877,31 +4894,31 @@
         <v>271</v>
       </c>
       <c r="G43" t="n">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="H43" t="n">
-        <v>4329697</v>
+        <v>4382656</v>
       </c>
       <c r="I43" t="n">
-        <v>71.61</v>
+        <v>72.486</v>
       </c>
       <c r="J43" t="n">
-        <v>22063</v>
+        <v>25629</v>
       </c>
       <c r="K43" t="n">
-        <v>0.365</v>
+        <v>0.424</v>
       </c>
       <c r="L43" t="n">
-        <v>24953</v>
+        <v>23675</v>
       </c>
       <c r="M43" t="n">
-        <v>0.413</v>
+        <v>0.392</v>
       </c>
       <c r="N43" t="n">
-        <v>0.015</v>
+        <v>0.018</v>
       </c>
       <c r="O43" t="n">
-        <v>67.285</v>
+        <v>56.95</v>
       </c>
       <c r="P43" t="s">
         <v>272</v>
@@ -4924,7 +4941,7 @@
         <v>275</v>
       </c>
       <c r="C44" s="1" t="n">
-        <v>44054</v>
+        <v>44056</v>
       </c>
       <c r="D44" t="s">
         <v>269</v>
@@ -4936,31 +4953,31 @@
         <v>271</v>
       </c>
       <c r="G44" t="n">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="H44" t="n">
-        <v>7316918</v>
+        <v>7420764</v>
       </c>
       <c r="I44" t="n">
-        <v>121.017</v>
+        <v>122.735</v>
       </c>
       <c r="J44" t="n">
-        <v>40642</v>
+        <v>51188</v>
       </c>
       <c r="K44" t="n">
-        <v>0.672</v>
+        <v>0.847</v>
       </c>
       <c r="L44" t="n">
-        <v>47476</v>
+        <v>45864</v>
       </c>
       <c r="M44" t="n">
-        <v>0.785</v>
+        <v>0.759</v>
       </c>
       <c r="N44" t="n">
-        <v>0.008</v>
+        <v>0.009</v>
       </c>
       <c r="O44" t="n">
-        <v>128.017</v>
+        <v>110.326</v>
       </c>
       <c r="P44" t="s">
         <v>272</v>
@@ -4983,7 +5000,7 @@
         <v>278</v>
       </c>
       <c r="C45" s="1" t="n">
-        <v>44054</v>
+        <v>44056</v>
       </c>
       <c r="D45" t="s">
         <v>279</v>
@@ -4995,31 +5012,31 @@
         <v>281</v>
       </c>
       <c r="G45" t="n">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="H45" t="n">
-        <v>1024235</v>
+        <v>1085322</v>
       </c>
       <c r="I45" t="n">
-        <v>8.098</v>
+        <v>8.581</v>
       </c>
       <c r="J45" t="n">
-        <v>8038</v>
+        <v>27158</v>
       </c>
       <c r="K45" t="n">
-        <v>0.064</v>
+        <v>0.215</v>
       </c>
       <c r="L45" t="n">
-        <v>21014</v>
+        <v>20940</v>
       </c>
       <c r="M45" t="n">
         <v>0.166</v>
       </c>
       <c r="N45" t="n">
-        <v>0.057</v>
+        <v>0.056</v>
       </c>
       <c r="O45" t="n">
-        <v>17.553</v>
+        <v>17.917</v>
       </c>
       <c r="P45" t="s">
         <v>282</v>
@@ -5042,7 +5059,7 @@
         <v>285</v>
       </c>
       <c r="C46" s="1" t="n">
-        <v>44052</v>
+        <v>44054</v>
       </c>
       <c r="D46" t="s">
         <v>286</v>
@@ -5054,31 +5071,31 @@
         <v>287</v>
       </c>
       <c r="G46" t="n">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="H46" t="n">
-        <v>1288757</v>
+        <v>1405649</v>
       </c>
       <c r="I46" t="n">
-        <v>10.19</v>
+        <v>11.114</v>
       </c>
       <c r="J46" t="n">
-        <v>4546</v>
+        <v>22672</v>
       </c>
       <c r="K46" t="n">
-        <v>0.036</v>
+        <v>0.179</v>
       </c>
       <c r="L46" t="n">
-        <v>16662</v>
+        <v>24256</v>
       </c>
       <c r="M46" t="n">
-        <v>0.132</v>
+        <v>0.192</v>
       </c>
       <c r="N46" t="n">
-        <v>0.092</v>
+        <v>0.049</v>
       </c>
       <c r="O46" t="n">
-        <v>10.898</v>
+        <v>20.262</v>
       </c>
       <c r="P46" t="s">
         <v>282</v>
@@ -5215,7 +5232,7 @@
         <v>301</v>
       </c>
       <c r="C49" s="1" t="n">
-        <v>44054</v>
+        <v>44056</v>
       </c>
       <c r="D49" t="s">
         <v>302</v>
@@ -5225,31 +5242,31 @@
       </c>
       <c r="F49"/>
       <c r="G49" t="n">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="H49" t="n">
-        <v>539461</v>
+        <v>548005</v>
       </c>
       <c r="I49" t="n">
-        <v>126.321</v>
+        <v>128.321</v>
       </c>
       <c r="J49" t="n">
-        <v>3658</v>
+        <v>4147</v>
       </c>
       <c r="K49" t="n">
-        <v>0.857</v>
+        <v>0.971</v>
       </c>
       <c r="L49" t="n">
-        <v>3630</v>
+        <v>3686</v>
       </c>
       <c r="M49" t="n">
-        <v>0.85</v>
+        <v>0.863</v>
       </c>
       <c r="N49" t="n">
-        <v>0.161</v>
+        <v>0.169</v>
       </c>
       <c r="O49" t="n">
-        <v>6.196</v>
+        <v>5.918</v>
       </c>
       <c r="P49" t="s">
         <v>303</v>
@@ -5272,7 +5289,7 @@
         <v>307</v>
       </c>
       <c r="C50" s="1" t="n">
-        <v>44055</v>
+        <v>44057</v>
       </c>
       <c r="D50" t="s">
         <v>308</v>
@@ -5284,28 +5301,32 @@
         <v>310</v>
       </c>
       <c r="G50" t="n">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="H50" t="n">
-        <v>218756</v>
+        <v>222531</v>
       </c>
       <c r="I50" t="n">
-        <v>115.977</v>
+        <v>117.978</v>
       </c>
       <c r="J50" t="n">
-        <v>2226</v>
+        <v>1704</v>
       </c>
       <c r="K50" t="n">
-        <v>1.18</v>
+        <v>0.903</v>
       </c>
       <c r="L50" t="n">
-        <v>1811</v>
+        <v>1784</v>
       </c>
       <c r="M50" t="n">
-        <v>0.96</v>
-      </c>
-      <c r="N50"/>
-      <c r="O50"/>
+        <v>0.946</v>
+      </c>
+      <c r="N50" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="O50" t="n">
+        <v>390.25</v>
+      </c>
       <c r="P50" t="s">
         <v>309</v>
       </c>
@@ -5327,7 +5348,7 @@
         <v>313</v>
       </c>
       <c r="C51" s="1" t="n">
-        <v>44055</v>
+        <v>44057</v>
       </c>
       <c r="D51" t="s">
         <v>314</v>
@@ -5337,24 +5358,32 @@
       </c>
       <c r="F51"/>
       <c r="G51" t="n">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="H51" t="n">
-        <v>561555</v>
+        <v>570657</v>
       </c>
       <c r="I51" t="n">
-        <v>206.28</v>
-      </c>
-      <c r="J51"/>
-      <c r="K51"/>
+        <v>209.624</v>
+      </c>
+      <c r="J51" t="n">
+        <v>4875</v>
+      </c>
+      <c r="K51" t="n">
+        <v>1.791</v>
+      </c>
       <c r="L51" t="n">
-        <v>3282</v>
+        <v>3614</v>
       </c>
       <c r="M51" t="n">
-        <v>1.206</v>
-      </c>
-      <c r="N51"/>
-      <c r="O51"/>
+        <v>1.328</v>
+      </c>
+      <c r="N51" t="n">
+        <v>0.006</v>
+      </c>
+      <c r="O51" t="n">
+        <v>159.107</v>
+      </c>
       <c r="P51" t="s">
         <v>45</v>
       </c>
@@ -5376,7 +5405,7 @@
         <v>317</v>
       </c>
       <c r="C52" s="1" t="n">
-        <v>44053</v>
+        <v>44055</v>
       </c>
       <c r="D52" t="s">
         <v>318</v>
@@ -5386,31 +5415,31 @@
       </c>
       <c r="F52"/>
       <c r="G52" t="n">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="H52" t="n">
-        <v>451407</v>
+        <v>455347</v>
       </c>
       <c r="I52" t="n">
-        <v>721.125</v>
+        <v>727.419</v>
       </c>
       <c r="J52" t="n">
-        <v>1596</v>
+        <v>1649</v>
       </c>
       <c r="K52" t="n">
-        <v>2.55</v>
+        <v>2.634</v>
       </c>
       <c r="L52" t="n">
-        <v>2214</v>
+        <v>1740</v>
       </c>
       <c r="M52" t="n">
-        <v>3.537</v>
+        <v>2.78</v>
       </c>
       <c r="N52" t="n">
         <v>0.027</v>
       </c>
       <c r="O52" t="n">
-        <v>37.077</v>
+        <v>37.477</v>
       </c>
       <c r="P52" t="s">
         <v>319</v>
@@ -5433,7 +5462,7 @@
         <v>322</v>
       </c>
       <c r="C53" s="1" t="n">
-        <v>44054</v>
+        <v>44056</v>
       </c>
       <c r="D53" t="s">
         <v>323</v>
@@ -5445,31 +5474,31 @@
         <v>325</v>
       </c>
       <c r="G53" t="n">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="H53" t="n">
-        <v>1063304</v>
+        <v>1085040</v>
       </c>
       <c r="I53" t="n">
-        <v>32.853</v>
+        <v>33.524</v>
       </c>
       <c r="J53" t="n">
-        <v>9773</v>
+        <v>11020</v>
       </c>
       <c r="K53" t="n">
-        <v>0.302</v>
+        <v>0.34</v>
       </c>
       <c r="L53" t="n">
-        <v>10282</v>
+        <v>10340</v>
       </c>
       <c r="M53" t="n">
-        <v>0.318</v>
+        <v>0.319</v>
       </c>
       <c r="N53" t="n">
         <v>0.001</v>
       </c>
       <c r="O53" t="n">
-        <v>773.914</v>
+        <v>795.385</v>
       </c>
       <c r="P53" t="s">
         <v>45</v>
@@ -5492,7 +5521,7 @@
         <v>329</v>
       </c>
       <c r="C54" s="1" t="n">
-        <v>44053</v>
+        <v>44056</v>
       </c>
       <c r="D54" t="s">
         <v>330</v>
@@ -5502,31 +5531,31 @@
       </c>
       <c r="F54"/>
       <c r="G54" t="n">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="H54" t="n">
-        <v>89555</v>
+        <v>93098</v>
       </c>
       <c r="I54" t="n">
-        <v>165.676</v>
+        <v>172.231</v>
       </c>
       <c r="J54" t="n">
-        <v>1163</v>
+        <v>1195</v>
       </c>
       <c r="K54" t="n">
-        <v>2.152</v>
+        <v>2.211</v>
       </c>
       <c r="L54" t="n">
-        <v>1050</v>
+        <v>1073</v>
       </c>
       <c r="M54" t="n">
-        <v>1.942</v>
+        <v>1.985</v>
       </c>
       <c r="N54" t="n">
-        <v>0.119</v>
+        <v>0.103</v>
       </c>
       <c r="O54" t="n">
-        <v>8.381</v>
+        <v>9.729</v>
       </c>
       <c r="P54" t="s">
         <v>332</v>
@@ -5606,7 +5635,7 @@
         <v>342</v>
       </c>
       <c r="C56" s="1" t="n">
-        <v>44050</v>
+        <v>44053</v>
       </c>
       <c r="D56" t="s">
         <v>343</v>
@@ -5616,31 +5645,31 @@
       </c>
       <c r="F56"/>
       <c r="G56" t="n">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="H56" t="n">
-        <v>1026126</v>
+        <v>1054609</v>
       </c>
       <c r="I56" t="n">
-        <v>7.959</v>
+        <v>8.18</v>
       </c>
       <c r="J56" t="n">
-        <v>7187</v>
+        <v>7727</v>
       </c>
       <c r="K56" t="n">
-        <v>0.056</v>
+        <v>0.06</v>
       </c>
       <c r="L56" t="n">
-        <v>9168</v>
+        <v>9383</v>
       </c>
       <c r="M56" t="n">
-        <v>0.071</v>
+        <v>0.073</v>
       </c>
       <c r="N56" t="n">
-        <v>0.725</v>
+        <v>0.628</v>
       </c>
       <c r="O56" t="n">
-        <v>1.38</v>
+        <v>1.593</v>
       </c>
       <c r="P56" t="s">
         <v>345</v>
@@ -5663,7 +5692,7 @@
         <v>349</v>
       </c>
       <c r="C57" s="1" t="n">
-        <v>44053</v>
+        <v>44056</v>
       </c>
       <c r="D57" t="s">
         <v>350</v>
@@ -5673,31 +5702,31 @@
       </c>
       <c r="F57"/>
       <c r="G57" t="n">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="H57" t="n">
-        <v>1472095</v>
+        <v>1538520</v>
       </c>
       <c r="I57" t="n">
-        <v>39.883</v>
+        <v>41.682</v>
       </c>
       <c r="J57" t="n">
-        <v>22127</v>
+        <v>22118</v>
       </c>
       <c r="K57" t="n">
         <v>0.599</v>
       </c>
       <c r="L57" t="n">
-        <v>22176</v>
+        <v>22101</v>
       </c>
       <c r="M57" t="n">
-        <v>0.601</v>
+        <v>0.599</v>
       </c>
       <c r="N57" t="n">
-        <v>0.05</v>
+        <v>0.053</v>
       </c>
       <c r="O57" t="n">
-        <v>20.16</v>
+        <v>18.881</v>
       </c>
       <c r="P57" t="s">
         <v>351</v>
@@ -5777,7 +5806,7 @@
         <v>361</v>
       </c>
       <c r="C59" s="1" t="n">
-        <v>44054</v>
+        <v>44056</v>
       </c>
       <c r="D59" t="s">
         <v>362</v>
@@ -5787,31 +5816,31 @@
       </c>
       <c r="F59"/>
       <c r="G59" t="n">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="H59" t="n">
-        <v>462698</v>
+        <v>483038</v>
       </c>
       <c r="I59" t="n">
-        <v>15.88</v>
+        <v>16.578</v>
       </c>
       <c r="J59" t="n">
-        <v>10462</v>
+        <v>9859</v>
       </c>
       <c r="K59" t="n">
-        <v>0.359</v>
+        <v>0.338</v>
       </c>
       <c r="L59" t="n">
-        <v>8015</v>
+        <v>9066</v>
       </c>
       <c r="M59" t="n">
-        <v>0.275</v>
+        <v>0.311</v>
       </c>
       <c r="N59" t="n">
-        <v>0.046</v>
+        <v>0.048</v>
       </c>
       <c r="O59" t="n">
-        <v>21.916</v>
+        <v>20.862</v>
       </c>
       <c r="P59" t="s">
         <v>363</v>
@@ -5887,7 +5916,7 @@
         <v>374</v>
       </c>
       <c r="C61" s="1" t="n">
-        <v>44054</v>
+        <v>44056</v>
       </c>
       <c r="D61" t="s">
         <v>375</v>
@@ -5897,31 +5926,31 @@
       </c>
       <c r="F61"/>
       <c r="G61" t="n">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="H61" t="n">
-        <v>502705</v>
+        <v>524414</v>
       </c>
       <c r="I61" t="n">
-        <v>104.247</v>
+        <v>108.749</v>
       </c>
       <c r="J61" t="n">
-        <v>4225</v>
+        <v>15703</v>
       </c>
       <c r="K61" t="n">
-        <v>0.876</v>
+        <v>3.256</v>
       </c>
       <c r="L61" t="n">
-        <v>3542</v>
+        <v>5353</v>
       </c>
       <c r="M61" t="n">
-        <v>0.735</v>
+        <v>1.11</v>
       </c>
       <c r="N61" t="n">
-        <v>0</v>
+        <v>0.001</v>
       </c>
       <c r="O61" t="n">
-        <v>8264.667</v>
+        <v>1972.158</v>
       </c>
       <c r="P61" t="s">
         <v>376</v>
@@ -5944,7 +5973,7 @@
         <v>379</v>
       </c>
       <c r="C62" s="1" t="n">
-        <v>44053</v>
+        <v>44056</v>
       </c>
       <c r="D62" t="s">
         <v>380</v>
@@ -5954,31 +5983,31 @@
       </c>
       <c r="F62"/>
       <c r="G62" t="n">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="H62" t="n">
-        <v>319851</v>
+        <v>341421</v>
       </c>
       <c r="I62" t="n">
-        <v>1.552</v>
+        <v>1.656</v>
       </c>
       <c r="J62" t="n">
-        <v>2355</v>
+        <v>3337</v>
       </c>
       <c r="K62" t="n">
-        <v>0.011</v>
+        <v>0.016</v>
       </c>
       <c r="L62" t="n">
-        <v>4388</v>
+        <v>4932</v>
       </c>
       <c r="M62" t="n">
-        <v>0.021</v>
+        <v>0.024</v>
       </c>
       <c r="N62" t="n">
-        <v>0.089</v>
+        <v>0.083</v>
       </c>
       <c r="O62" t="n">
-        <v>11.227</v>
+        <v>12.101</v>
       </c>
       <c r="P62" t="s">
         <v>381</v>
@@ -6103,7 +6132,7 @@
         <v>399</v>
       </c>
       <c r="C65" s="1" t="n">
-        <v>44055</v>
+        <v>44057</v>
       </c>
       <c r="D65" t="s">
         <v>400</v>
@@ -6113,28 +6142,32 @@
       </c>
       <c r="F65"/>
       <c r="G65" t="n">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="H65" t="n">
-        <v>2186442</v>
+        <v>2229409</v>
       </c>
       <c r="I65" t="n">
-        <v>9.898</v>
+        <v>10.093</v>
       </c>
       <c r="J65" t="n">
-        <v>20631</v>
+        <v>23745</v>
       </c>
       <c r="K65" t="n">
-        <v>0.093</v>
+        <v>0.107</v>
       </c>
       <c r="L65" t="n">
-        <v>19296</v>
+        <v>21439</v>
       </c>
       <c r="M65" t="n">
-        <v>0.087</v>
-      </c>
-      <c r="N65"/>
-      <c r="O65"/>
+        <v>0.097</v>
+      </c>
+      <c r="N65" t="n">
+        <v>0.031</v>
+      </c>
+      <c r="O65" t="n">
+        <v>32.239</v>
+      </c>
       <c r="P65" t="s">
         <v>401</v>
       </c>
@@ -6380,7 +6413,7 @@
         <v>427</v>
       </c>
       <c r="C70" s="1" t="n">
-        <v>44054</v>
+        <v>44056</v>
       </c>
       <c r="D70" t="s">
         <v>428</v>
@@ -6390,31 +6423,31 @@
       </c>
       <c r="F70"/>
       <c r="G70" t="n">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="H70" t="n">
-        <v>2158532</v>
+        <v>2207204</v>
       </c>
       <c r="I70" t="n">
-        <v>57.034</v>
+        <v>58.32</v>
       </c>
       <c r="J70" t="n">
-        <v>20511</v>
+        <v>25177</v>
       </c>
       <c r="K70" t="n">
-        <v>0.542</v>
+        <v>0.665</v>
       </c>
       <c r="L70" t="n">
-        <v>22715</v>
+        <v>22568</v>
       </c>
       <c r="M70" t="n">
-        <v>0.6</v>
+        <v>0.596</v>
       </c>
       <c r="N70" t="n">
         <v>0.031</v>
       </c>
       <c r="O70" t="n">
-        <v>32.181</v>
+        <v>32.326</v>
       </c>
       <c r="P70" t="s">
         <v>429</v>
@@ -6437,7 +6470,7 @@
         <v>432</v>
       </c>
       <c r="C71" s="1" t="n">
-        <v>44054</v>
+        <v>44056</v>
       </c>
       <c r="D71" t="s">
         <v>428</v>
@@ -6447,19 +6480,19 @@
       </c>
       <c r="F71"/>
       <c r="G71" t="n">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="H71" t="n">
-        <v>2257525</v>
+        <v>2307735</v>
       </c>
       <c r="I71" t="n">
-        <v>59.649</v>
+        <v>60.976</v>
       </c>
       <c r="J71" t="n">
-        <v>23142</v>
+        <v>26131</v>
       </c>
       <c r="K71" t="n">
-        <v>0.611</v>
+        <v>0.69</v>
       </c>
       <c r="L71"/>
       <c r="M71"/>
@@ -6486,7 +6519,7 @@
         <v>435</v>
       </c>
       <c r="C72" s="1" t="n">
-        <v>44053</v>
+        <v>44055</v>
       </c>
       <c r="D72" t="s">
         <v>436</v>
@@ -6496,31 +6529,31 @@
       </c>
       <c r="F72"/>
       <c r="G72" t="n">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="H72" t="n">
-        <v>1766454</v>
+        <v>1799226</v>
       </c>
       <c r="I72" t="n">
-        <v>173.238</v>
+        <v>176.452</v>
       </c>
       <c r="J72" t="n">
-        <v>12903</v>
+        <v>15899</v>
       </c>
       <c r="K72" t="n">
-        <v>1.265</v>
+        <v>1.559</v>
       </c>
       <c r="L72" t="n">
-        <v>13566</v>
+        <v>13380</v>
       </c>
       <c r="M72" t="n">
-        <v>1.33</v>
+        <v>1.312</v>
       </c>
       <c r="N72" t="n">
         <v>0.013</v>
       </c>
       <c r="O72" t="n">
-        <v>78.807</v>
+        <v>74.098</v>
       </c>
       <c r="P72" t="s">
         <v>437</v>
@@ -6543,7 +6576,7 @@
         <v>441</v>
       </c>
       <c r="C73" s="1" t="n">
-        <v>44054</v>
+        <v>44056</v>
       </c>
       <c r="D73" t="s">
         <v>442</v>
@@ -6553,31 +6586,31 @@
       </c>
       <c r="F73"/>
       <c r="G73" t="n">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="H73" t="n">
-        <v>529289</v>
+        <v>538602</v>
       </c>
       <c r="I73" t="n">
-        <v>183.713</v>
+        <v>186.946</v>
       </c>
       <c r="J73" t="n">
-        <v>4823</v>
+        <v>4607</v>
       </c>
       <c r="K73" t="n">
-        <v>1.674</v>
+        <v>1.599</v>
       </c>
       <c r="L73" t="n">
-        <v>3449</v>
+        <v>3943</v>
       </c>
       <c r="M73" t="n">
-        <v>1.197</v>
+        <v>1.369</v>
       </c>
       <c r="N73" t="n">
-        <v>0.08</v>
+        <v>0.077</v>
       </c>
       <c r="O73" t="n">
-        <v>12.445</v>
+        <v>12.94</v>
       </c>
       <c r="P73" t="s">
         <v>443</v>
@@ -6600,7 +6633,7 @@
         <v>447</v>
       </c>
       <c r="C74" s="1" t="n">
-        <v>44054</v>
+        <v>44056</v>
       </c>
       <c r="D74" t="s">
         <v>448</v>
@@ -6610,31 +6643,31 @@
       </c>
       <c r="F74"/>
       <c r="G74" t="n">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="H74" t="n">
-        <v>1404845</v>
+        <v>1450269</v>
       </c>
       <c r="I74" t="n">
-        <v>73.026</v>
+        <v>75.387</v>
       </c>
       <c r="J74" t="n">
-        <v>19511</v>
+        <v>22643</v>
       </c>
       <c r="K74" t="n">
-        <v>1.014</v>
+        <v>1.177</v>
       </c>
       <c r="L74" t="n">
-        <v>17541</v>
+        <v>18700</v>
       </c>
       <c r="M74" t="n">
-        <v>0.912</v>
+        <v>0.972</v>
       </c>
       <c r="N74" t="n">
-        <v>0.07</v>
+        <v>0.066</v>
       </c>
       <c r="O74" t="n">
-        <v>14.381</v>
+        <v>15.173</v>
       </c>
       <c r="P74" t="s">
         <v>450</v>
@@ -6657,7 +6690,7 @@
         <v>454</v>
       </c>
       <c r="C75" s="1" t="n">
-        <v>44054</v>
+        <v>44056</v>
       </c>
       <c r="D75" t="s">
         <v>455</v>
@@ -6667,31 +6700,31 @@
       </c>
       <c r="F75"/>
       <c r="G75" t="n">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="H75" t="n">
-        <v>31307764</v>
+        <v>31903055</v>
       </c>
       <c r="I75" t="n">
-        <v>214.533</v>
+        <v>218.612</v>
       </c>
       <c r="J75" t="n">
-        <v>244577</v>
+        <v>304753</v>
       </c>
       <c r="K75" t="n">
-        <v>1.676</v>
+        <v>2.088</v>
       </c>
       <c r="L75" t="n">
-        <v>267696</v>
+        <v>266419</v>
       </c>
       <c r="M75" t="n">
-        <v>1.834</v>
+        <v>1.826</v>
       </c>
       <c r="N75" t="n">
-        <v>0.022</v>
+        <v>0.019</v>
       </c>
       <c r="O75" t="n">
-        <v>45.334</v>
+        <v>52.744</v>
       </c>
       <c r="P75" t="s">
         <v>456</v>
@@ -6771,7 +6804,7 @@
         <v>466</v>
       </c>
       <c r="C77" s="1" t="n">
-        <v>44054</v>
+        <v>44056</v>
       </c>
       <c r="D77" t="s">
         <v>467</v>
@@ -6781,31 +6814,31 @@
       </c>
       <c r="F77"/>
       <c r="G77" t="n">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="H77" t="n">
-        <v>3933427</v>
+        <v>4071857</v>
       </c>
       <c r="I77" t="n">
-        <v>112.984</v>
+        <v>116.961</v>
       </c>
       <c r="J77" t="n">
-        <v>60828</v>
+        <v>70754</v>
       </c>
       <c r="K77" t="n">
-        <v>1.747</v>
+        <v>2.032</v>
       </c>
       <c r="L77" t="n">
-        <v>59239</v>
+        <v>63634</v>
       </c>
       <c r="M77" t="n">
-        <v>1.702</v>
+        <v>1.828</v>
       </c>
       <c r="N77" t="n">
-        <v>0.024</v>
+        <v>0.023</v>
       </c>
       <c r="O77" t="n">
-        <v>42.082</v>
+        <v>43.615</v>
       </c>
       <c r="P77" t="s">
         <v>45</v>
@@ -6828,7 +6861,7 @@
         <v>470</v>
       </c>
       <c r="C78" s="1" t="n">
-        <v>44054</v>
+        <v>44056</v>
       </c>
       <c r="D78" t="s">
         <v>471</v>
@@ -6840,31 +6873,31 @@
         <v>473</v>
       </c>
       <c r="G78" t="n">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="H78" t="n">
-        <v>125029</v>
+        <v>128601</v>
       </c>
       <c r="I78" t="n">
-        <v>7.467</v>
+        <v>7.68</v>
       </c>
       <c r="J78" t="n">
-        <v>876</v>
+        <v>1730</v>
       </c>
       <c r="K78" t="n">
-        <v>0.052</v>
+        <v>0.103</v>
       </c>
       <c r="L78" t="n">
-        <v>1483</v>
+        <v>1542</v>
       </c>
       <c r="M78" t="n">
-        <v>0.089</v>
+        <v>0.092</v>
       </c>
       <c r="N78" t="n">
-        <v>0.089</v>
+        <v>0.097</v>
       </c>
       <c r="O78" t="n">
-        <v>11.211</v>
+        <v>10.29</v>
       </c>
       <c r="P78" t="s">
         <v>474</v>
@@ -6887,7 +6920,7 @@
         <v>478</v>
       </c>
       <c r="C79" s="1" t="n">
-        <v>44054</v>
+        <v>44055</v>
       </c>
       <c r="D79" t="s">
         <v>479</v>
@@ -6899,31 +6932,31 @@
         <v>480</v>
       </c>
       <c r="G79" t="n">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="H79" t="n">
-        <v>762229</v>
+        <v>770997</v>
       </c>
       <c r="I79" t="n">
-        <v>112.017</v>
+        <v>113.305</v>
       </c>
       <c r="J79" t="n">
-        <v>8086</v>
+        <v>8768</v>
       </c>
       <c r="K79" t="n">
-        <v>1.188</v>
+        <v>1.289</v>
       </c>
       <c r="L79" t="n">
-        <v>8426</v>
+        <v>8270</v>
       </c>
       <c r="M79" t="n">
-        <v>1.238</v>
+        <v>1.215</v>
       </c>
       <c r="N79" t="n">
-        <v>0.031</v>
+        <v>0.03</v>
       </c>
       <c r="O79" t="n">
-        <v>32.569</v>
+        <v>32.911</v>
       </c>
       <c r="P79" t="s">
         <v>45</v>
@@ -7052,7 +7085,7 @@
         <v>490</v>
       </c>
       <c r="C82" s="1" t="n">
-        <v>44055</v>
+        <v>44057</v>
       </c>
       <c r="D82" t="s">
         <v>491</v>
@@ -7062,28 +7095,32 @@
       </c>
       <c r="F82"/>
       <c r="G82" t="n">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="H82" t="n">
-        <v>284111</v>
+        <v>289590</v>
       </c>
       <c r="I82" t="n">
-        <v>52.038</v>
+        <v>53.042</v>
       </c>
       <c r="J82" t="n">
-        <v>3131</v>
+        <v>2738</v>
       </c>
       <c r="K82" t="n">
-        <v>0.573</v>
+        <v>0.501</v>
       </c>
       <c r="L82" t="n">
-        <v>2065</v>
+        <v>2114</v>
       </c>
       <c r="M82" t="n">
-        <v>0.378</v>
-      </c>
-      <c r="N82"/>
-      <c r="O82"/>
+        <v>0.387</v>
+      </c>
+      <c r="N82" t="n">
+        <v>0.018</v>
+      </c>
+      <c r="O82" t="n">
+        <v>57.135</v>
+      </c>
       <c r="P82" t="s">
         <v>493</v>
       </c>
@@ -7105,7 +7142,7 @@
         <v>496</v>
       </c>
       <c r="C83" s="1" t="n">
-        <v>44054</v>
+        <v>44055</v>
       </c>
       <c r="D83" t="s">
         <v>497</v>
@@ -7115,31 +7152,31 @@
       </c>
       <c r="F83"/>
       <c r="G83" t="n">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="H83" t="n">
-        <v>138718</v>
+        <v>139574</v>
       </c>
       <c r="I83" t="n">
-        <v>66.726</v>
+        <v>67.137</v>
       </c>
       <c r="J83" t="n">
-        <v>1118</v>
+        <v>856</v>
       </c>
       <c r="K83" t="n">
-        <v>0.538</v>
+        <v>0.412</v>
       </c>
       <c r="L83" t="n">
-        <v>736</v>
+        <v>749</v>
       </c>
       <c r="M83" t="n">
-        <v>0.354</v>
+        <v>0.36</v>
       </c>
       <c r="N83" t="n">
-        <v>0.014</v>
+        <v>0.016</v>
       </c>
       <c r="O83" t="n">
-        <v>69.622</v>
+        <v>63.939</v>
       </c>
       <c r="P83" t="s">
         <v>499</v>
@@ -7162,7 +7199,7 @@
         <v>503</v>
       </c>
       <c r="C84" s="1" t="n">
-        <v>44054</v>
+        <v>44056</v>
       </c>
       <c r="D84" t="s">
         <v>504</v>
@@ -7174,31 +7211,31 @@
         <v>506</v>
       </c>
       <c r="G84" t="n">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="H84" t="n">
-        <v>3278977</v>
+        <v>3315497</v>
       </c>
       <c r="I84" t="n">
-        <v>55.287</v>
+        <v>55.902</v>
       </c>
       <c r="J84" t="n">
-        <v>11483</v>
+        <v>20063</v>
       </c>
       <c r="K84" t="n">
-        <v>0.194</v>
+        <v>0.338</v>
       </c>
       <c r="L84" t="n">
-        <v>28682</v>
+        <v>23670</v>
       </c>
       <c r="M84" t="n">
-        <v>0.484</v>
+        <v>0.399</v>
       </c>
       <c r="N84" t="n">
-        <v>0.233</v>
+        <v>0.236</v>
       </c>
       <c r="O84" t="n">
-        <v>4.296</v>
+        <v>4.244</v>
       </c>
       <c r="P84" t="s">
         <v>505</v>
@@ -7221,7 +7258,7 @@
         <v>510</v>
       </c>
       <c r="C85" s="1" t="n">
-        <v>44055</v>
+        <v>44056</v>
       </c>
       <c r="D85" t="s">
         <v>511</v>
@@ -7231,28 +7268,32 @@
       </c>
       <c r="F85"/>
       <c r="G85" t="n">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="H85" t="n">
-        <v>1629277</v>
+        <v>1637100</v>
       </c>
       <c r="I85" t="n">
-        <v>31.779</v>
+        <v>31.931</v>
       </c>
       <c r="J85" t="n">
-        <v>8922</v>
+        <v>7823</v>
       </c>
       <c r="K85" t="n">
-        <v>0.174</v>
+        <v>0.153</v>
       </c>
       <c r="L85" t="n">
-        <v>7083</v>
+        <v>6949</v>
       </c>
       <c r="M85" t="n">
-        <v>0.138</v>
-      </c>
-      <c r="N85"/>
-      <c r="O85"/>
+        <v>0.136</v>
+      </c>
+      <c r="N85" t="n">
+        <v>0.006</v>
+      </c>
+      <c r="O85" t="n">
+        <v>179.494</v>
+      </c>
       <c r="P85" t="s">
         <v>512</v>
       </c>
@@ -7380,7 +7421,7 @@
         <v>529</v>
       </c>
       <c r="C88" s="1" t="n">
-        <v>44045</v>
+        <v>44052</v>
       </c>
       <c r="D88" t="s">
         <v>530</v>
@@ -7390,27 +7431,27 @@
       </c>
       <c r="F88"/>
       <c r="G88" t="n">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="H88"/>
       <c r="I88"/>
       <c r="J88" t="n">
-        <v>7566</v>
+        <v>7674</v>
       </c>
       <c r="K88" t="n">
-        <v>0.749</v>
+        <v>0.76</v>
       </c>
       <c r="L88" t="n">
-        <v>7566</v>
+        <v>7674</v>
       </c>
       <c r="M88" t="n">
-        <v>0.749</v>
+        <v>0.76</v>
       </c>
       <c r="N88" t="n">
-        <v>0.027</v>
+        <v>0.035</v>
       </c>
       <c r="O88" t="n">
-        <v>37.166</v>
+        <v>28.258</v>
       </c>
       <c r="P88" t="s">
         <v>526</v>
@@ -7433,7 +7474,7 @@
         <v>533</v>
       </c>
       <c r="C89" s="1" t="n">
-        <v>44053</v>
+        <v>44055</v>
       </c>
       <c r="D89" t="s">
         <v>534</v>
@@ -7443,31 +7484,31 @@
       </c>
       <c r="F89"/>
       <c r="G89" t="n">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="H89" t="n">
-        <v>847325</v>
+        <v>861555</v>
       </c>
       <c r="I89" t="n">
-        <v>97.904</v>
+        <v>99.549</v>
       </c>
       <c r="J89" t="n">
-        <v>4098</v>
+        <v>4806</v>
       </c>
       <c r="K89" t="n">
-        <v>0.474</v>
+        <v>0.555</v>
       </c>
       <c r="L89" t="n">
-        <v>5209</v>
+        <v>5228</v>
       </c>
       <c r="M89" t="n">
-        <v>0.602</v>
+        <v>0.604</v>
       </c>
       <c r="N89" t="n">
-        <v>0.029</v>
+        <v>0.031</v>
       </c>
       <c r="O89" t="n">
-        <v>34.628</v>
+        <v>31.85</v>
       </c>
       <c r="P89" t="s">
         <v>535</v>
@@ -7490,7 +7531,7 @@
         <v>539</v>
       </c>
       <c r="C90" s="1" t="n">
-        <v>44054</v>
+        <v>44056</v>
       </c>
       <c r="D90" t="s">
         <v>540</v>
@@ -7500,22 +7541,22 @@
       </c>
       <c r="F90"/>
       <c r="G90" t="n">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="H90" t="n">
-        <v>83828</v>
+        <v>84249</v>
       </c>
       <c r="I90" t="n">
-        <v>3.52</v>
+        <v>3.537</v>
       </c>
       <c r="J90" t="n">
-        <v>148</v>
+        <v>230</v>
       </c>
       <c r="K90" t="n">
-        <v>0.006</v>
+        <v>0.01</v>
       </c>
       <c r="L90" t="n">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="M90" t="n">
         <v>0.008</v>
@@ -7524,7 +7565,7 @@
         <v>0.003</v>
       </c>
       <c r="O90" t="n">
-        <v>325.5</v>
+        <v>323.75</v>
       </c>
       <c r="P90" t="s">
         <v>541</v>
@@ -7547,7 +7588,7 @@
         <v>544</v>
       </c>
       <c r="C91" s="1" t="n">
-        <v>44054</v>
+        <v>44056</v>
       </c>
       <c r="D91" t="s">
         <v>545</v>
@@ -7557,31 +7598,31 @@
       </c>
       <c r="F91"/>
       <c r="G91" t="n">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="H91" t="n">
-        <v>389247</v>
+        <v>391136</v>
       </c>
       <c r="I91" t="n">
-        <v>5.577</v>
+        <v>5.604</v>
       </c>
       <c r="J91" t="n">
-        <v>1485</v>
+        <v>1384</v>
       </c>
       <c r="K91" t="n">
-        <v>0.021</v>
+        <v>0.02</v>
       </c>
       <c r="L91" t="n">
-        <v>1231</v>
+        <v>1131</v>
       </c>
       <c r="M91" t="n">
-        <v>0.018</v>
+        <v>0.016</v>
       </c>
       <c r="N91" t="n">
         <v>0.003</v>
       </c>
       <c r="O91" t="n">
-        <v>287.233</v>
+        <v>304.5</v>
       </c>
       <c r="P91" t="s">
         <v>546</v>
@@ -7604,7 +7645,7 @@
         <v>549</v>
       </c>
       <c r="C92" s="1" t="n">
-        <v>44054</v>
+        <v>44056</v>
       </c>
       <c r="D92" t="s">
         <v>545</v>
@@ -7614,31 +7655,31 @@
       </c>
       <c r="F92"/>
       <c r="G92" t="n">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="H92" t="n">
-        <v>777518</v>
+        <v>779407</v>
       </c>
       <c r="I92" t="n">
-        <v>11.139</v>
+        <v>11.166</v>
       </c>
       <c r="J92" t="n">
-        <v>18223</v>
+        <v>1384</v>
       </c>
       <c r="K92" t="n">
-        <v>0.261</v>
+        <v>0.02</v>
       </c>
       <c r="L92" t="n">
-        <v>3622</v>
+        <v>3522</v>
       </c>
       <c r="M92" t="n">
-        <v>0.052</v>
+        <v>0.05</v>
       </c>
       <c r="N92" t="n">
         <v>0.001</v>
       </c>
       <c r="O92" t="n">
-        <v>845.133</v>
+        <v>948.231</v>
       </c>
       <c r="P92" t="s">
         <v>546</v>
@@ -7718,7 +7759,7 @@
         <v>558</v>
       </c>
       <c r="C94" s="1" t="n">
-        <v>44051</v>
+        <v>44053</v>
       </c>
       <c r="D94" t="s">
         <v>559</v>
@@ -7728,31 +7769,31 @@
       </c>
       <c r="F94"/>
       <c r="G94" t="n">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="H94" t="n">
-        <v>102028</v>
+        <v>104206</v>
       </c>
       <c r="I94" t="n">
-        <v>8.633</v>
+        <v>8.817</v>
       </c>
       <c r="J94" t="n">
-        <v>650</v>
+        <v>1202</v>
       </c>
       <c r="K94" t="n">
-        <v>0.055</v>
+        <v>0.102</v>
       </c>
       <c r="L94" t="n">
-        <v>1260</v>
+        <v>1244</v>
       </c>
       <c r="M94" t="n">
-        <v>0.107</v>
+        <v>0.105</v>
       </c>
       <c r="N94" t="n">
-        <v>0.014</v>
+        <v>0.016</v>
       </c>
       <c r="O94" t="n">
-        <v>72.893</v>
+        <v>64.029</v>
       </c>
       <c r="P94" t="s">
         <v>560</v>
@@ -7775,7 +7816,7 @@
         <v>563</v>
       </c>
       <c r="C95" s="1" t="n">
-        <v>44054</v>
+        <v>44056</v>
       </c>
       <c r="D95" t="s">
         <v>564</v>
@@ -7785,31 +7826,31 @@
       </c>
       <c r="F95"/>
       <c r="G95" t="n">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="H95" t="n">
-        <v>5387751</v>
+        <v>5521880</v>
       </c>
       <c r="I95" t="n">
-        <v>63.882</v>
+        <v>65.472</v>
       </c>
       <c r="J95" t="n">
-        <v>61716</v>
+        <v>66892</v>
       </c>
       <c r="K95" t="n">
-        <v>0.732</v>
+        <v>0.793</v>
       </c>
       <c r="L95" t="n">
-        <v>54025</v>
+        <v>62868</v>
       </c>
       <c r="M95" t="n">
-        <v>0.641</v>
+        <v>0.745</v>
       </c>
       <c r="N95" t="n">
-        <v>0.022</v>
+        <v>0.019</v>
       </c>
       <c r="O95" t="n">
-        <v>46.425</v>
+        <v>53.149</v>
       </c>
       <c r="P95" t="s">
         <v>565</v>
@@ -7832,7 +7873,7 @@
         <v>568</v>
       </c>
       <c r="C96" s="1" t="n">
-        <v>44053</v>
+        <v>44055</v>
       </c>
       <c r="D96" t="s">
         <v>569</v>
@@ -7842,31 +7883,31 @@
       </c>
       <c r="F96"/>
       <c r="G96" t="n">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="H96" t="n">
-        <v>301286</v>
+        <v>308503</v>
       </c>
       <c r="I96" t="n">
-        <v>6.587</v>
+        <v>6.745</v>
       </c>
       <c r="J96" t="n">
-        <v>2250</v>
+        <v>4108</v>
       </c>
       <c r="K96" t="n">
-        <v>0.049</v>
+        <v>0.09</v>
       </c>
       <c r="L96" t="n">
-        <v>2682</v>
+        <v>2877</v>
       </c>
       <c r="M96" t="n">
-        <v>0.059</v>
+        <v>0.063</v>
       </c>
       <c r="N96" t="n">
         <v>0.005</v>
       </c>
       <c r="O96" t="n">
-        <v>185.881</v>
+        <v>183.082</v>
       </c>
       <c r="P96" t="s">
         <v>570</v>
@@ -7889,7 +7930,7 @@
         <v>574</v>
       </c>
       <c r="C97" s="1" t="n">
-        <v>44055</v>
+        <v>44057</v>
       </c>
       <c r="D97" t="s">
         <v>575</v>
@@ -7899,28 +7940,32 @@
       </c>
       <c r="F97"/>
       <c r="G97" t="n">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="H97" t="n">
-        <v>1214941</v>
+        <v>1252842</v>
       </c>
       <c r="I97" t="n">
-        <v>27.78</v>
+        <v>28.647</v>
       </c>
       <c r="J97" t="n">
-        <v>19380</v>
+        <v>18917</v>
       </c>
       <c r="K97" t="n">
-        <v>0.443</v>
+        <v>0.433</v>
       </c>
       <c r="L97" t="n">
-        <v>16611</v>
+        <v>16827</v>
       </c>
       <c r="M97" t="n">
-        <v>0.38</v>
-      </c>
-      <c r="N97"/>
-      <c r="O97"/>
+        <v>0.385</v>
+      </c>
+      <c r="N97" t="n">
+        <v>0.094</v>
+      </c>
+      <c r="O97" t="n">
+        <v>10.646</v>
+      </c>
       <c r="P97" t="s">
         <v>576</v>
       </c>
@@ -7942,7 +7987,7 @@
         <v>580</v>
       </c>
       <c r="C98" s="1" t="n">
-        <v>44054</v>
+        <v>44056</v>
       </c>
       <c r="D98" t="s">
         <v>581</v>
@@ -7952,31 +7997,31 @@
       </c>
       <c r="F98"/>
       <c r="G98" t="n">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="H98" t="n">
-        <v>5623764</v>
+        <v>5765358</v>
       </c>
       <c r="I98" t="n">
-        <v>568.608</v>
+        <v>582.925</v>
       </c>
       <c r="J98" t="n">
-        <v>64110</v>
+        <v>68964</v>
       </c>
       <c r="K98" t="n">
-        <v>6.482</v>
+        <v>6.973</v>
       </c>
       <c r="L98" t="n">
-        <v>57782</v>
+        <v>64567</v>
       </c>
       <c r="M98" t="n">
-        <v>5.842</v>
+        <v>6.528</v>
       </c>
       <c r="N98" t="n">
         <v>0.004</v>
       </c>
       <c r="O98" t="n">
-        <v>262.475</v>
+        <v>281.425</v>
       </c>
       <c r="P98" t="s">
         <v>582</v>
@@ -7999,7 +8044,7 @@
         <v>585</v>
       </c>
       <c r="C99" s="1" t="n">
-        <v>44053</v>
+        <v>44055</v>
       </c>
       <c r="D99" t="s">
         <v>586</v>
@@ -8011,31 +8056,31 @@
         <v>588</v>
       </c>
       <c r="G99" t="n">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="H99" t="n">
-        <v>10993551</v>
+        <v>11310805</v>
       </c>
       <c r="I99" t="n">
-        <v>161.941</v>
+        <v>166.615</v>
       </c>
       <c r="J99" t="n">
-        <v>135827</v>
+        <v>167983</v>
       </c>
       <c r="K99" t="n">
-        <v>2.001</v>
+        <v>2.474</v>
       </c>
       <c r="L99" t="n">
-        <v>150223</v>
+        <v>153405</v>
       </c>
       <c r="M99" t="n">
-        <v>2.213</v>
+        <v>2.26</v>
       </c>
       <c r="N99" t="n">
         <v>0.006</v>
       </c>
       <c r="O99" t="n">
-        <v>171.543</v>
+        <v>165.307</v>
       </c>
       <c r="P99" t="s">
         <v>587</v>
@@ -8058,7 +8103,7 @@
         <v>592</v>
       </c>
       <c r="C100" s="1" t="n">
-        <v>44050</v>
+        <v>44056</v>
       </c>
       <c r="D100" t="s">
         <v>593</v>
@@ -8068,31 +8113,27 @@
       </c>
       <c r="F100"/>
       <c r="G100" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="H100" t="n">
-        <v>65756307</v>
+        <v>69155988</v>
       </c>
       <c r="I100" t="n">
-        <v>198.658</v>
-      </c>
-      <c r="J100" t="n">
-        <v>835387</v>
-      </c>
-      <c r="K100" t="n">
-        <v>2.524</v>
-      </c>
+        <v>208.929</v>
+      </c>
+      <c r="J100"/>
+      <c r="K100"/>
       <c r="L100" t="n">
-        <v>899125</v>
+        <v>605010</v>
       </c>
       <c r="M100" t="n">
-        <v>2.716</v>
+        <v>1.828</v>
       </c>
       <c r="N100" t="n">
-        <v>0.062</v>
+        <v>0.088</v>
       </c>
       <c r="O100" t="n">
-        <v>16.195</v>
+        <v>11.346</v>
       </c>
       <c r="P100" t="s">
         <v>594</v>
@@ -8115,7 +8156,7 @@
         <v>597</v>
       </c>
       <c r="C101" s="1" t="n">
-        <v>44054</v>
+        <v>44056</v>
       </c>
       <c r="D101" t="s">
         <v>598</v>
@@ -8125,31 +8166,31 @@
       </c>
       <c r="F101"/>
       <c r="G101" t="n">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="H101" t="n">
-        <v>63252257</v>
+        <v>64612034</v>
       </c>
       <c r="I101" t="n">
-        <v>191.093</v>
+        <v>195.201</v>
       </c>
       <c r="J101" t="n">
-        <v>739083</v>
+        <v>880729</v>
       </c>
       <c r="K101" t="n">
-        <v>2.233</v>
+        <v>2.661</v>
       </c>
       <c r="L101" t="n">
-        <v>716117</v>
+        <v>708480</v>
       </c>
       <c r="M101" t="n">
-        <v>2.163</v>
+        <v>2.14</v>
       </c>
       <c r="N101" t="n">
-        <v>0.076</v>
+        <v>0.075</v>
       </c>
       <c r="O101" t="n">
-        <v>13.163</v>
+        <v>13.287</v>
       </c>
       <c r="P101" t="s">
         <v>599</v>
@@ -8172,7 +8213,7 @@
         <v>604</v>
       </c>
       <c r="C102" s="1" t="n">
-        <v>44053</v>
+        <v>44056</v>
       </c>
       <c r="D102" t="s">
         <v>605</v>
@@ -8182,27 +8223,31 @@
       </c>
       <c r="F102"/>
       <c r="G102" t="n">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="H102" t="n">
-        <v>133237</v>
+        <v>138700</v>
       </c>
       <c r="I102" t="n">
-        <v>38.356</v>
-      </c>
-      <c r="J102"/>
-      <c r="K102"/>
+        <v>39.928</v>
+      </c>
+      <c r="J102" t="n">
+        <v>1514</v>
+      </c>
+      <c r="K102" t="n">
+        <v>0.436</v>
+      </c>
       <c r="L102" t="n">
-        <v>2028</v>
+        <v>1749</v>
       </c>
       <c r="M102" t="n">
-        <v>0.584</v>
+        <v>0.503</v>
       </c>
       <c r="N102" t="n">
-        <v>0.005</v>
+        <v>0.007</v>
       </c>
       <c r="O102" t="n">
-        <v>211.881</v>
+        <v>145.75</v>
       </c>
       <c r="P102" t="s">
         <v>126</v>

</xml_diff>

<commit_message>
Updated testing data for 2020-08-19
</commit_message>
<xml_diff>
--- a/public/data/testing/covid-testing-latest-data-source-details.xlsx
+++ b/public/data/testing/covid-testing-latest-data-source-details.xlsx
@@ -110,7 +110,7 @@
     <t xml:space="preserve">Australia - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.health.gov.au/sites/default/files/documents/2020/08/coronavirus-covid-19-at-a-glance-16-august-2020.pdf</t>
+    <t xml:space="preserve">https://www.health.gov.au/sites/default/files/documents/2020/08/coronavirus-covid-19-at-a-glance-18-august-2020.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">Australian Government Department of Health</t>
@@ -245,7 +245,7 @@
     <t xml:space="preserve">Bolivia - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://minsalud.gob.bo/4512-bolivia-supera-los-99-000-contagios-de-coronavirus-59-505-son-casos-activos</t>
+    <t xml:space="preserve">https://minsalud.gob.bo/4517-bolivia-inicia-la-semana-con-879-contagios-nuevos-y-65-fallecidos-por-covid-19</t>
   </si>
   <si>
     <t xml:space="preserve">https://www.minsalud.gob.bo/</t>
@@ -400,7 +400,7 @@
     <t xml:space="preserve">Cote d'Ivoire - samples tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.facebook.com/Mshpci/posts/1671198983045789</t>
+    <t xml:space="preserve">https://www.facebook.com/Mshpci/posts/1672992029533151</t>
   </si>
   <si>
     <t xml:space="preserve">Ministry of Health and Public Hygiene</t>
@@ -479,7 +479,7 @@
     <t xml:space="preserve">Democratic Republic of Congo - samples tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/CMR_Covid19_RDC/status/1294958152409120768/photo/1</t>
+    <t xml:space="preserve">https://twitter.com/CMR_Covid19_RDC/status/1295660670885732352/photo/1</t>
   </si>
   <si>
     <t xml:space="preserve">DRC COVID-19 Pandemic Response Multisectoral Committee</t>
@@ -497,7 +497,7 @@
     <t xml:space="preserve">Denmark - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://files.ssi.dk/Data-Epidemiologiske-Rapport-14082020-yy6p</t>
+    <t xml:space="preserve">https://files.ssi.dk/Data-Epidemiologiske-Rapport-18082020-jq34</t>
   </si>
   <si>
     <t xml:space="preserve">Statens Serum Institut</t>
@@ -515,7 +515,7 @@
     <t xml:space="preserve">Ecuador - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.gestionderiesgos.gob.ec/wp-content/uploads/2020/08/INFOGRAFIA-NACIONAL-COVID-19-171.pdf</t>
+    <t xml:space="preserve">https://www.gestionderiesgos.gob.ec/wp-content/uploads/2020/08/INFOGRAFIA-NACIONALCOVI-19-COE-NACIONAL-08h00-18082020-3.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">Government of Ecuador</t>
@@ -541,7 +541,7 @@
     <t xml:space="preserve">El Salvador - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.facebook.com/nayibbukele/posts/3147014742051362</t>
+    <t xml:space="preserve">https://www.facebook.com/nayibbukele/posts/3155527237866779</t>
   </si>
   <si>
     <t xml:space="preserve">Government of El Salvador</t>
@@ -585,7 +585,7 @@
     <t xml:space="preserve">Ethiopia - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.ephi.gov.et/images/novel_coronavirus/EPHI_-PHEOC_COVID-19_Weekly--bulletin_14_English_08032020.pdf</t>
+    <t xml:space="preserve">https://www.ephi.gov.et/images/novel_coronavirus/EPHI_%20PHEOC_COVID-19_Weekly%20%20bulletin_15_English_08102020.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">Ethiopian Public Health Institute</t>
@@ -753,7 +753,7 @@
     <t xml:space="preserve">Greece - samples tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://eody.gov.gr/covid-gr-daily-report-15-08-2020/</t>
+    <t xml:space="preserve">https://eody.gov.gr/covid-gr-daily-report-18-08-2020/</t>
   </si>
   <si>
     <t xml:space="preserve">National Organization of Public Health</t>
@@ -892,7 +892,7 @@
     <t xml:space="preserve">Iran - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">http://irangov.ir/detail/345249</t>
+    <t xml:space="preserve">http://irangov.ir/detail/345395</t>
   </si>
   <si>
     <t xml:space="preserve">Government of Iran</t>
@@ -912,7 +912,7 @@
     <t xml:space="preserve">Iraq - samples tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://moh.gov.iq/index.php?name=News&amp;file=article&amp;sid=16328</t>
+    <t xml:space="preserve">https://moh.gov.iq/index.php?name=News&amp;file=article&amp;sid=16340</t>
   </si>
   <si>
     <t xml:space="preserve">Ministry of Health and Environment</t>
@@ -950,7 +950,7 @@
     <t xml:space="preserve">Israel - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://govextra.gov.il/media/24518/covid19-data-israel-10082020.csv</t>
+    <t xml:space="preserve">https://govextra.gov.il/media/24691/covid-19-data-israel-12082020.xlsx</t>
   </si>
   <si>
     <t xml:space="preserve">Israel Ministry of Health</t>
@@ -1009,7 +1009,7 @@
     <t xml:space="preserve">Japan - people tested (incl. non-PCR)</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.mhlw.go.jp/stf/newpage_12999.html</t>
+    <t xml:space="preserve">https://www.mhlw.go.jp/stf/newpage_13032.html</t>
   </si>
   <si>
     <t xml:space="preserve">Ministry of Health, Labor and Welfare Press Release</t>
@@ -1034,7 +1034,7 @@
     <t xml:space="preserve">Japan - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.mhlw.go.jp/content/10906000/000659503.pdf</t>
+    <t xml:space="preserve">https://www.mhlw.go.jp/content/10906000/000660170.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">The cumulative total reported in the press release matches the cumulative total calculated from the weekly and daily figures reported by the MOH.</t>
@@ -1068,7 +1068,7 @@
     <t xml:space="preserve">Kenya - samples tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/MOH_Kenya/status/1293931264047820800</t>
+    <t xml:space="preserve">https://twitter.com/MOH_Kenya/status/1295334203220008960</t>
   </si>
   <si>
     <t xml:space="preserve">Kenya Ministry of Health</t>
@@ -1090,7 +1090,7 @@
     <t xml:space="preserve">Kuwait - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/KUWAIT_MOH/status/1294948815569661955/photo/1</t>
+    <t xml:space="preserve">https://twitter.com/KUWAIT_MOH/status/1295691983760039936/photo/1</t>
   </si>
   <si>
     <t xml:space="preserve">Kuwait Ministry of Health</t>
@@ -1156,7 +1156,7 @@
     <t xml:space="preserve">Malaysia - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">http://covid-19.moh.gov.my/terkini/082020/situasi-terkini-16-ogos-2020</t>
+    <t xml:space="preserve">http://covid-19.moh.gov.my/terkini/082020/situasi-terkini-18-ogos-2020</t>
   </si>
   <si>
     <t xml:space="preserve">Ministry of Health Malaysia</t>
@@ -1182,7 +1182,7 @@
     <t xml:space="preserve">Maldives - samples tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/HPA_MV/status/1294681728737521664/photo/1</t>
+    <t xml:space="preserve">https://twitter.com/HPA_MV/status/1295405246894809088/photo/1</t>
   </si>
   <si>
     <t xml:space="preserve">Maldives Health Protection Agency</t>
@@ -1249,7 +1249,7 @@
     <t xml:space="preserve">Morocco - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/Ministere_Sante/status/1294684996578480130/photo/1</t>
+    <t xml:space="preserve">https://twitter.com/Ministere_Sante/status/1295411930010652676/photo/1</t>
   </si>
   <si>
     <t xml:space="preserve">Morocco Ministry of Health</t>
@@ -1289,7 +1289,7 @@
     <t xml:space="preserve">Nepal - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://drive.google.com/drive/folders/1OcGKoZxTqdTWw6h0MfrEeXwg0PXaBaWa</t>
+    <t xml:space="preserve">https://drive.google.com/drive/folders/1E5lyqxrn1X_dl2PWiJ2JUPWvN3bjy3Uy</t>
   </si>
   <si>
     <t xml:space="preserve">Ministry of Health and Population</t>
@@ -1309,7 +1309,7 @@
     <t xml:space="preserve">Netherlands - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.rivm.nl/sites/default/files/2020-08/COVID-19_WebSite_rapport_wekelijks_20200811_1158_0.pdf</t>
+    <t xml:space="preserve">https://www.rivm.nl/sites/default/files/2020-08/COVID-19_WebSite_rapport_wekelijks_20200818_1224_1.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">National Institute for Public Health and the Environment</t>
@@ -1494,7 +1494,7 @@
     <t xml:space="preserve">Philippines - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://drive.google.com/drive/folders/1e_Hv_hquoc8v0M5WZNNes3QnDwkFqaGO</t>
+    <t xml:space="preserve">https://drive.google.com/drive/folders/1pP9BFBJuu4UF5KpPMvnXeWJjq5bHJk8f</t>
   </si>
   <si>
     <t xml:space="preserve">Philippines Department of Health</t>
@@ -1514,7 +1514,7 @@
     <t xml:space="preserve">Poland - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/MZ_GOV_PL/status/1294921843875426305</t>
+    <t xml:space="preserve">https://twitter.com/MZ_GOV_PL/status/1295646617828122634</t>
   </si>
   <si>
     <t xml:space="preserve">Poland Ministry of Health</t>
@@ -1582,7 +1582,7 @@
     <t xml:space="preserve">Romania - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://gov.ro/ro/media/comunicate/buletin-de-presa-15-august-2020-ora-13-00&amp;page=1</t>
+    <t xml:space="preserve">https://gov.ro/ro/media/comunicate/buletin-de-presa-18-august-2020-ora-13-00&amp;page=1</t>
   </si>
   <si>
     <t xml:space="preserve">Ministry of Internal Affairs</t>
@@ -1605,7 +1605,7 @@
     <t xml:space="preserve">Russia - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://rospotrebnadzor.ru/about/info/news/news_details.php?ELEMENT_ID=15186</t>
+    <t xml:space="preserve">https://rospotrebnadzor.ru/about/info/news/news_details.php?ELEMENT_ID=15197</t>
   </si>
   <si>
     <t xml:space="preserve">Government of the Russian Federation</t>
@@ -1625,7 +1625,7 @@
     <t xml:space="preserve">Rwanda - samples tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/RwandaHealth/status/1293999179661025282</t>
+    <t xml:space="preserve">https://twitter.com/RwandaHealth/status/1295093748729352192</t>
   </si>
   <si>
     <t xml:space="preserve">Rwanda Ministry of Health</t>
@@ -1799,7 +1799,7 @@
     <t xml:space="preserve">South Korea - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.cdc.go.kr/board/board.es?mid=&amp;bid=0030&amp;act=view&amp;list_no=368145&amp;tag=&amp;nPage=1</t>
+    <t xml:space="preserve">https://www.cdc.go.kr/board/board.es?mid=&amp;bid=0030&amp;act=view&amp;list_no=368152&amp;tag=&amp;nPage=1</t>
   </si>
   <si>
     <t xml:space="preserve">South Korea CDC</t>
@@ -1819,7 +1819,7 @@
     <t xml:space="preserve">Spain - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.mscbs.gob.es/profesionales/saludPublica/ccayes/alertasActual/nCov-China/documentos/COVID-19_pruebas_diagnosticas_06_08_2020.pdf</t>
+    <t xml:space="preserve">https://www.mscbs.gob.es/profesionales/saludPublica/ccayes/alertasActual/nCov-China/documentos/COVID-19_pruebas_diagnosticas_13_08_2020.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">Ministry of Health, Consumption and Social Welfare</t>
@@ -1921,7 +1921,7 @@
     <t xml:space="preserve">Thailand - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://ddc.moph.go.th/viralpneumonia/file/situation/situation-no226-160863.pdf</t>
+    <t xml:space="preserve">https://ddc.moph.go.th/viralpneumonia/file/situation/situation-no228-180863.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">Department of Disease Control</t>
@@ -2009,7 +2009,7 @@
     <t xml:space="preserve">Uganda - samples tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/MinofHealthUG/status/1294203346044289024/photo/2</t>
+    <t xml:space="preserve">https://twitter.com/MinofHealthUG/status/1295711251406913537/photo/1</t>
   </si>
   <si>
     <t xml:space="preserve">Uganda Ministry of Health</t>
@@ -2069,7 +2069,7 @@
     <t xml:space="preserve">United Kingdom - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://assets.publishing.service.gov.uk/government/uploads/system/uploads/attachment_data/file/909658/2020-08-16_COVID-19_UK_testing_time_series.csv</t>
+    <t xml:space="preserve">https://assets.publishing.service.gov.uk/government/uploads/system/uploads/attachment_data/file/910211/2020-08-18_COVID-19_UK_testing_time_series.csv</t>
   </si>
   <si>
     <t xml:space="preserve">Public Health England/Department of Health and Social Care</t>
@@ -2187,7 +2187,7 @@
     <t xml:space="preserve">Zimbabwe - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/MoHCCZim/status/1294026974579523590</t>
+    <t xml:space="preserve">https://twitter.com/MoHCCZim/status/1295057062544781315</t>
   </si>
   <si>
     <t xml:space="preserve">Zimbabwe Ministry of Health and Child Care</t>
@@ -2604,7 +2604,7 @@
         <v>20</v>
       </c>
       <c r="C2" s="1" t="n">
-        <v>44059</v>
+        <v>44061</v>
       </c>
       <c r="D2" t="s">
         <v>21</v>
@@ -2614,31 +2614,31 @@
       </c>
       <c r="F2"/>
       <c r="G2" t="n">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="H2" t="n">
-        <v>838189</v>
+        <v>866234</v>
       </c>
       <c r="I2" t="n">
-        <v>18.546</v>
+        <v>19.166</v>
       </c>
       <c r="J2" t="n">
-        <v>1924</v>
+        <v>3667</v>
       </c>
       <c r="K2" t="n">
-        <v>0.043</v>
+        <v>0.081</v>
       </c>
       <c r="L2" t="n">
-        <v>12244</v>
+        <v>11332</v>
       </c>
       <c r="M2" t="n">
-        <v>0.271</v>
+        <v>0.251</v>
       </c>
       <c r="N2" t="n">
-        <v>0.546</v>
+        <v>0.606</v>
       </c>
       <c r="O2" t="n">
-        <v>1.833</v>
+        <v>1.65</v>
       </c>
       <c r="P2" t="s">
         <v>22</v>
@@ -2661,7 +2661,7 @@
         <v>25</v>
       </c>
       <c r="C3" s="1" t="n">
-        <v>44059</v>
+        <v>44061</v>
       </c>
       <c r="D3" t="s">
         <v>26</v>
@@ -2671,31 +2671,31 @@
       </c>
       <c r="F3"/>
       <c r="G3" t="n">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="H3" t="n">
-        <v>1019021</v>
+        <v>1052565</v>
       </c>
       <c r="I3" t="n">
-        <v>22.547</v>
+        <v>23.289</v>
       </c>
       <c r="J3" t="n">
-        <v>2219</v>
+        <v>4823</v>
       </c>
       <c r="K3" t="n">
-        <v>0.049</v>
+        <v>0.107</v>
       </c>
       <c r="L3" t="n">
-        <v>14463</v>
+        <v>13314</v>
       </c>
       <c r="M3" t="n">
-        <v>0.32</v>
+        <v>0.295</v>
       </c>
       <c r="N3" t="n">
-        <v>0.462</v>
+        <v>0.516</v>
       </c>
       <c r="O3" t="n">
-        <v>2.165</v>
+        <v>1.939</v>
       </c>
       <c r="P3" t="s">
         <v>22</v>
@@ -2718,7 +2718,7 @@
         <v>30</v>
       </c>
       <c r="C4" s="1" t="n">
-        <v>44058</v>
+        <v>44060</v>
       </c>
       <c r="D4" t="s">
         <v>31</v>
@@ -2728,27 +2728,31 @@
       </c>
       <c r="F4"/>
       <c r="G4" t="n">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="H4" t="n">
-        <v>5297558</v>
+        <v>5380613</v>
       </c>
       <c r="I4" t="n">
-        <v>207.748</v>
-      </c>
-      <c r="J4"/>
-      <c r="K4"/>
+        <v>211.005</v>
+      </c>
+      <c r="J4" t="n">
+        <v>44516</v>
+      </c>
+      <c r="K4" t="n">
+        <v>1.746</v>
+      </c>
       <c r="L4" t="n">
-        <v>73607</v>
+        <v>66010</v>
       </c>
       <c r="M4" t="n">
-        <v>2.887</v>
+        <v>2.589</v>
       </c>
       <c r="N4" t="n">
         <v>0.005</v>
       </c>
       <c r="O4" t="n">
-        <v>208.518</v>
+        <v>209.651</v>
       </c>
       <c r="P4" t="s">
         <v>32</v>
@@ -2771,7 +2775,7 @@
         <v>36</v>
       </c>
       <c r="C5" s="1" t="n">
-        <v>44060</v>
+        <v>44062</v>
       </c>
       <c r="D5" t="s">
         <v>37</v>
@@ -2781,31 +2785,31 @@
       </c>
       <c r="F5"/>
       <c r="G5" t="n">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="H5" t="n">
-        <v>1024067</v>
+        <v>1048216</v>
       </c>
       <c r="I5" t="n">
-        <v>113.704</v>
+        <v>116.386</v>
       </c>
       <c r="J5" t="n">
-        <v>5577</v>
+        <v>10328</v>
       </c>
       <c r="K5" t="n">
-        <v>0.619</v>
+        <v>1.147</v>
       </c>
       <c r="L5" t="n">
-        <v>8330</v>
+        <v>9314</v>
       </c>
       <c r="M5" t="n">
-        <v>0.925</v>
+        <v>1.034</v>
       </c>
       <c r="N5" t="n">
-        <v>0.023</v>
+        <v>0.025</v>
       </c>
       <c r="O5" t="n">
-        <v>42.812</v>
+        <v>40.37</v>
       </c>
       <c r="P5" t="s">
         <v>39</v>
@@ -2828,7 +2832,7 @@
         <v>43</v>
       </c>
       <c r="C6" s="1" t="n">
-        <v>44060</v>
+        <v>44062</v>
       </c>
       <c r="D6" t="s">
         <v>44</v>
@@ -2838,31 +2842,31 @@
       </c>
       <c r="F6"/>
       <c r="G6" t="n">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="H6" t="n">
-        <v>972003</v>
+        <v>991140</v>
       </c>
       <c r="I6" t="n">
-        <v>571.235</v>
+        <v>582.481</v>
       </c>
       <c r="J6" t="n">
-        <v>9669</v>
+        <v>9932</v>
       </c>
       <c r="K6" t="n">
-        <v>5.682</v>
+        <v>5.837</v>
       </c>
       <c r="L6" t="n">
-        <v>9992</v>
+        <v>8197</v>
       </c>
       <c r="M6" t="n">
-        <v>5.872</v>
+        <v>4.817</v>
       </c>
       <c r="N6" t="n">
-        <v>0.035</v>
+        <v>0.041</v>
       </c>
       <c r="O6" t="n">
-        <v>28.914</v>
+        <v>24.099</v>
       </c>
       <c r="P6" t="s">
         <v>46</v>
@@ -2885,7 +2889,7 @@
         <v>50</v>
       </c>
       <c r="C7" s="1" t="n">
-        <v>44055</v>
+        <v>44058</v>
       </c>
       <c r="D7" t="s">
         <v>51</v>
@@ -2895,31 +2899,31 @@
       </c>
       <c r="F7"/>
       <c r="G7" t="n">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="H7" t="n">
-        <v>1302739</v>
+        <v>1341648</v>
       </c>
       <c r="I7" t="n">
-        <v>7.91</v>
+        <v>8.147</v>
       </c>
       <c r="J7" t="n">
-        <v>14751</v>
+        <v>12891</v>
       </c>
       <c r="K7" t="n">
-        <v>0.09</v>
+        <v>0.078</v>
       </c>
       <c r="L7" t="n">
-        <v>12903</v>
+        <v>13155</v>
       </c>
       <c r="M7" t="n">
-        <v>0.078</v>
+        <v>0.08</v>
       </c>
       <c r="N7" t="n">
-        <v>0.216</v>
+        <v>0.21</v>
       </c>
       <c r="O7" t="n">
-        <v>4.636</v>
+        <v>4.752</v>
       </c>
       <c r="P7" t="s">
         <v>52</v>
@@ -2999,7 +3003,7 @@
         <v>63</v>
       </c>
       <c r="C9" s="1" t="n">
-        <v>44058</v>
+        <v>44060</v>
       </c>
       <c r="D9" t="s">
         <v>64</v>
@@ -3009,31 +3013,31 @@
       </c>
       <c r="F9"/>
       <c r="G9" t="n">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="H9" t="n">
-        <v>1998820</v>
+        <v>2022851</v>
       </c>
       <c r="I9" t="n">
-        <v>172.466</v>
+        <v>174.54</v>
       </c>
       <c r="J9" t="n">
-        <v>11914</v>
+        <v>13331</v>
       </c>
       <c r="K9" t="n">
-        <v>1.028</v>
+        <v>1.15</v>
       </c>
       <c r="L9" t="n">
-        <v>18026</v>
+        <v>17610</v>
       </c>
       <c r="M9" t="n">
-        <v>1.555</v>
+        <v>1.519</v>
       </c>
       <c r="N9" t="n">
-        <v>0.029</v>
+        <v>0.03</v>
       </c>
       <c r="O9" t="n">
-        <v>34.973</v>
+        <v>33.434</v>
       </c>
       <c r="P9" t="s">
         <v>65</v>
@@ -3056,7 +3060,7 @@
         <v>69</v>
       </c>
       <c r="C10" s="1" t="n">
-        <v>44058</v>
+        <v>44060</v>
       </c>
       <c r="D10" t="s">
         <v>70</v>
@@ -3066,31 +3070,31 @@
       </c>
       <c r="F10"/>
       <c r="G10" t="n">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="H10" t="n">
-        <v>195977</v>
+        <v>200211</v>
       </c>
       <c r="I10" t="n">
-        <v>16.789</v>
+        <v>17.152</v>
       </c>
       <c r="J10" t="n">
-        <v>3552</v>
+        <v>1513</v>
       </c>
       <c r="K10" t="n">
-        <v>0.304</v>
+        <v>0.13</v>
       </c>
       <c r="L10" t="n">
-        <v>3119</v>
+        <v>2951</v>
       </c>
       <c r="M10" t="n">
-        <v>0.267</v>
+        <v>0.253</v>
       </c>
       <c r="N10" t="n">
-        <v>0.392</v>
+        <v>0.501</v>
       </c>
       <c r="O10" t="n">
-        <v>2.548</v>
+        <v>1.997</v>
       </c>
       <c r="P10" t="s">
         <v>45</v>
@@ -3164,7 +3168,7 @@
         <v>82</v>
       </c>
       <c r="C12" s="1" t="n">
-        <v>44059</v>
+        <v>44062</v>
       </c>
       <c r="D12" t="s">
         <v>83</v>
@@ -3174,31 +3178,31 @@
       </c>
       <c r="F12"/>
       <c r="G12" t="n">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="H12" t="n">
-        <v>333530</v>
+        <v>343230</v>
       </c>
       <c r="I12" t="n">
-        <v>48.001</v>
+        <v>49.397</v>
       </c>
       <c r="J12" t="n">
-        <v>2745</v>
+        <v>3667</v>
       </c>
       <c r="K12" t="n">
-        <v>0.395</v>
+        <v>0.528</v>
       </c>
       <c r="L12" t="n">
-        <v>4285</v>
+        <v>4195</v>
       </c>
       <c r="M12" t="n">
-        <v>0.617</v>
+        <v>0.604</v>
       </c>
       <c r="N12" t="n">
-        <v>0.033</v>
+        <v>0.032</v>
       </c>
       <c r="O12" t="n">
-        <v>30.298</v>
+        <v>31.008</v>
       </c>
       <c r="P12" t="s">
         <v>85</v>
@@ -3221,7 +3225,7 @@
         <v>88</v>
       </c>
       <c r="C13" s="1" t="n">
-        <v>44060</v>
+        <v>44062</v>
       </c>
       <c r="D13" t="s">
         <v>89</v>
@@ -3231,31 +3235,31 @@
       </c>
       <c r="F13"/>
       <c r="G13" t="n">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="H13" t="n">
-        <v>4778360</v>
+        <v>4880172</v>
       </c>
       <c r="I13" t="n">
-        <v>126.605</v>
+        <v>129.303</v>
       </c>
       <c r="J13" t="n">
-        <v>37214</v>
+        <v>40129</v>
       </c>
       <c r="K13" t="n">
-        <v>0.986</v>
+        <v>1.063</v>
       </c>
       <c r="L13" t="n">
-        <v>47221</v>
+        <v>48346</v>
       </c>
       <c r="M13" t="n">
-        <v>1.251</v>
+        <v>1.281</v>
       </c>
       <c r="N13" t="n">
         <v>0.008</v>
       </c>
       <c r="O13" t="n">
-        <v>125.397</v>
+        <v>123.152</v>
       </c>
       <c r="P13" t="s">
         <v>90</v>
@@ -3278,7 +3282,7 @@
         <v>93</v>
       </c>
       <c r="C14" s="1" t="n">
-        <v>44059</v>
+        <v>44061</v>
       </c>
       <c r="D14" t="s">
         <v>94</v>
@@ -3290,31 +3294,31 @@
         <v>95</v>
       </c>
       <c r="G14" t="n">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="H14" t="n">
-        <v>2019591</v>
+        <v>2068079</v>
       </c>
       <c r="I14" t="n">
-        <v>105.648</v>
+        <v>108.185</v>
       </c>
       <c r="J14" t="n">
-        <v>30882</v>
+        <v>23199</v>
       </c>
       <c r="K14" t="n">
-        <v>1.615</v>
+        <v>1.214</v>
       </c>
       <c r="L14" t="n">
-        <v>25462</v>
+        <v>25495</v>
       </c>
       <c r="M14" t="n">
-        <v>1.332</v>
+        <v>1.334</v>
       </c>
       <c r="N14" t="n">
-        <v>0.072</v>
+        <v>0.07</v>
       </c>
       <c r="O14" t="n">
-        <v>13.839</v>
+        <v>14.325</v>
       </c>
       <c r="P14" t="s">
         <v>96</v>
@@ -3337,7 +3341,7 @@
         <v>100</v>
       </c>
       <c r="C15" s="1" t="n">
-        <v>44058</v>
+        <v>44061</v>
       </c>
       <c r="D15" t="s">
         <v>101</v>
@@ -3347,31 +3351,31 @@
       </c>
       <c r="F15"/>
       <c r="G15" t="n">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="H15" t="n">
-        <v>2143097</v>
+        <v>2246595</v>
       </c>
       <c r="I15" t="n">
-        <v>42.118</v>
+        <v>44.152</v>
       </c>
       <c r="J15" t="n">
-        <v>38331</v>
+        <v>35883</v>
       </c>
       <c r="K15" t="n">
-        <v>0.753</v>
+        <v>0.705</v>
       </c>
       <c r="L15" t="n">
-        <v>37961</v>
+        <v>37681</v>
       </c>
       <c r="M15" t="n">
-        <v>0.746</v>
+        <v>0.741</v>
       </c>
       <c r="N15" t="n">
-        <v>0.293</v>
+        <v>0.3</v>
       </c>
       <c r="O15" t="n">
-        <v>3.41</v>
+        <v>3.337</v>
       </c>
       <c r="P15" t="s">
         <v>102</v>
@@ -3394,7 +3398,7 @@
         <v>106</v>
       </c>
       <c r="C16" s="1" t="n">
-        <v>44058</v>
+        <v>44060</v>
       </c>
       <c r="D16" t="s">
         <v>107</v>
@@ -3404,19 +3408,19 @@
       </c>
       <c r="F16"/>
       <c r="G16" t="n">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="H16" t="n">
-        <v>104406</v>
+        <v>106613</v>
       </c>
       <c r="I16" t="n">
-        <v>20.495</v>
+        <v>20.929</v>
       </c>
       <c r="J16" t="n">
-        <v>2404</v>
+        <v>1535</v>
       </c>
       <c r="K16" t="n">
-        <v>0.472</v>
+        <v>0.301</v>
       </c>
       <c r="L16" t="n">
         <v>1866</v>
@@ -3447,7 +3451,7 @@
         <v>112</v>
       </c>
       <c r="C17" s="1" t="n">
-        <v>44059</v>
+        <v>44061</v>
       </c>
       <c r="D17" t="s">
         <v>113</v>
@@ -3457,31 +3461,31 @@
       </c>
       <c r="F17"/>
       <c r="G17" t="n">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="H17" t="n">
-        <v>113388</v>
+        <v>115338</v>
       </c>
       <c r="I17" t="n">
-        <v>4.299</v>
+        <v>4.372</v>
       </c>
       <c r="J17" t="n">
-        <v>457</v>
+        <v>918</v>
       </c>
       <c r="K17" t="n">
-        <v>0.017</v>
+        <v>0.035</v>
       </c>
       <c r="L17" t="n">
-        <v>647</v>
+        <v>711</v>
       </c>
       <c r="M17" t="n">
-        <v>0.025</v>
+        <v>0.027</v>
       </c>
       <c r="N17" t="n">
-        <v>0.082</v>
+        <v>0.046</v>
       </c>
       <c r="O17" t="n">
-        <v>12.142</v>
+        <v>21.829</v>
       </c>
       <c r="P17" t="s">
         <v>114</v>
@@ -3504,7 +3508,7 @@
         <v>118</v>
       </c>
       <c r="C18" s="1" t="n">
-        <v>44059</v>
+        <v>44061</v>
       </c>
       <c r="D18" t="s">
         <v>119</v>
@@ -3514,31 +3518,31 @@
       </c>
       <c r="F18"/>
       <c r="G18" t="n">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="H18" t="n">
-        <v>137657</v>
+        <v>140471</v>
       </c>
       <c r="I18" t="n">
-        <v>33.532</v>
+        <v>34.217</v>
       </c>
       <c r="J18" t="n">
-        <v>1377</v>
+        <v>1824</v>
       </c>
       <c r="K18" t="n">
-        <v>0.335</v>
+        <v>0.444</v>
       </c>
       <c r="L18" t="n">
-        <v>1361</v>
+        <v>1398</v>
       </c>
       <c r="M18" t="n">
-        <v>0.332</v>
+        <v>0.341</v>
       </c>
       <c r="N18" t="n">
-        <v>0.092</v>
+        <v>0.103</v>
       </c>
       <c r="O18" t="n">
-        <v>10.863</v>
+        <v>9.718</v>
       </c>
       <c r="P18" t="s">
         <v>120</v>
@@ -3561,7 +3565,7 @@
         <v>124</v>
       </c>
       <c r="C19" s="1" t="n">
-        <v>44058</v>
+        <v>44060</v>
       </c>
       <c r="D19" t="s">
         <v>125</v>
@@ -3573,31 +3577,31 @@
         <v>127</v>
       </c>
       <c r="G19" t="n">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="H19" t="n">
-        <v>327689</v>
+        <v>336333</v>
       </c>
       <c r="I19" t="n">
-        <v>28.931</v>
+        <v>29.694</v>
       </c>
       <c r="J19" t="n">
-        <v>3646</v>
+        <v>4294</v>
       </c>
       <c r="K19" t="n">
-        <v>0.322</v>
+        <v>0.379</v>
       </c>
       <c r="L19" t="n">
-        <v>4337</v>
+        <v>4383</v>
       </c>
       <c r="M19" t="n">
-        <v>0.383</v>
+        <v>0.387</v>
       </c>
       <c r="N19" t="n">
-        <v>0.013</v>
+        <v>0.012</v>
       </c>
       <c r="O19" t="n">
-        <v>75.897</v>
+        <v>84.521</v>
       </c>
       <c r="P19" t="s">
         <v>126</v>
@@ -3620,7 +3624,7 @@
         <v>131</v>
       </c>
       <c r="C20" s="1" t="n">
-        <v>44058</v>
+        <v>44060</v>
       </c>
       <c r="D20" t="s">
         <v>132</v>
@@ -3630,31 +3634,31 @@
       </c>
       <c r="F20"/>
       <c r="G20" t="n">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="H20" t="n">
-        <v>795760</v>
+        <v>805609</v>
       </c>
       <c r="I20" t="n">
-        <v>74.308</v>
+        <v>75.227</v>
       </c>
       <c r="J20" t="n">
-        <v>4581</v>
+        <v>6808</v>
       </c>
       <c r="K20" t="n">
-        <v>0.428</v>
+        <v>0.636</v>
       </c>
       <c r="L20" t="n">
-        <v>6318</v>
+        <v>6417</v>
       </c>
       <c r="M20" t="n">
-        <v>0.59</v>
+        <v>0.599</v>
       </c>
       <c r="N20" t="n">
         <v>0.037</v>
       </c>
       <c r="O20" t="n">
-        <v>27.083</v>
+        <v>27.109</v>
       </c>
       <c r="P20" t="s">
         <v>45</v>
@@ -3677,7 +3681,7 @@
         <v>136</v>
       </c>
       <c r="C21" s="1" t="n">
-        <v>44058</v>
+        <v>44060</v>
       </c>
       <c r="D21" t="s">
         <v>137</v>
@@ -3687,27 +3691,27 @@
       </c>
       <c r="F21"/>
       <c r="G21" t="n">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="H21"/>
       <c r="I21"/>
       <c r="J21" t="n">
-        <v>437</v>
+        <v>333</v>
       </c>
       <c r="K21" t="n">
-        <v>0.005</v>
+        <v>0.004</v>
       </c>
       <c r="L21" t="n">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="M21" t="n">
         <v>0.004</v>
       </c>
       <c r="N21" t="n">
-        <v>0.093</v>
+        <v>0.083</v>
       </c>
       <c r="O21" t="n">
-        <v>10.724</v>
+        <v>11.982</v>
       </c>
       <c r="P21" t="s">
         <v>138</v>
@@ -3730,7 +3734,7 @@
         <v>142</v>
       </c>
       <c r="C22" s="1" t="n">
-        <v>44056</v>
+        <v>44060</v>
       </c>
       <c r="D22" t="s">
         <v>143</v>
@@ -3740,31 +3744,31 @@
       </c>
       <c r="F22"/>
       <c r="G22" t="n">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="H22" t="n">
-        <v>1834329</v>
+        <v>1956472</v>
       </c>
       <c r="I22" t="n">
-        <v>316.689</v>
+        <v>337.777</v>
       </c>
       <c r="J22" t="n">
-        <v>5777</v>
+        <v>7796</v>
       </c>
       <c r="K22" t="n">
-        <v>0.997</v>
+        <v>1.346</v>
       </c>
       <c r="L22" t="n">
-        <v>23323</v>
+        <v>26521</v>
       </c>
       <c r="M22" t="n">
-        <v>4.027</v>
+        <v>4.579</v>
       </c>
       <c r="N22" t="n">
-        <v>0.005</v>
+        <v>0.006</v>
       </c>
       <c r="O22" t="n">
-        <v>184.476</v>
+        <v>157.997</v>
       </c>
       <c r="P22" t="s">
         <v>144</v>
@@ -3787,7 +3791,7 @@
         <v>148</v>
       </c>
       <c r="C23" s="1" t="n">
-        <v>44059</v>
+        <v>44061</v>
       </c>
       <c r="D23" t="s">
         <v>149</v>
@@ -3799,25 +3803,25 @@
         <v>151</v>
       </c>
       <c r="G23" t="n">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="H23" t="n">
-        <v>223842</v>
+        <v>228038</v>
       </c>
       <c r="I23" t="n">
-        <v>12.687</v>
+        <v>12.925</v>
       </c>
       <c r="J23" t="n">
-        <v>2679</v>
+        <v>3203</v>
       </c>
       <c r="K23" t="n">
-        <v>0.152</v>
+        <v>0.182</v>
       </c>
       <c r="L23" t="n">
-        <v>2730</v>
+        <v>2929</v>
       </c>
       <c r="M23" t="n">
-        <v>0.155</v>
+        <v>0.166</v>
       </c>
       <c r="N23"/>
       <c r="O23"/>
@@ -3842,7 +3846,7 @@
         <v>155</v>
       </c>
       <c r="C24" s="1" t="n">
-        <v>44056</v>
+        <v>44059</v>
       </c>
       <c r="D24" t="s">
         <v>156</v>
@@ -3852,31 +3856,31 @@
       </c>
       <c r="F24"/>
       <c r="G24" t="n">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="H24" t="n">
-        <v>273509</v>
+        <v>280943</v>
       </c>
       <c r="I24" t="n">
-        <v>42.168</v>
+        <v>43.314</v>
       </c>
       <c r="J24" t="n">
-        <v>2452</v>
+        <v>2498</v>
       </c>
       <c r="K24" t="n">
-        <v>0.378</v>
+        <v>0.385</v>
       </c>
       <c r="L24" t="n">
-        <v>2476</v>
+        <v>2479</v>
       </c>
       <c r="M24" t="n">
         <v>0.382</v>
       </c>
       <c r="N24" t="n">
-        <v>0.17</v>
+        <v>0.152</v>
       </c>
       <c r="O24" t="n">
-        <v>5.889</v>
+        <v>6.571</v>
       </c>
       <c r="P24" t="s">
         <v>157</v>
@@ -3899,7 +3903,7 @@
         <v>161</v>
       </c>
       <c r="C25" s="1" t="n">
-        <v>44058</v>
+        <v>44061</v>
       </c>
       <c r="D25" t="s">
         <v>162</v>
@@ -3909,31 +3913,31 @@
       </c>
       <c r="F25"/>
       <c r="G25" t="n">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="H25" t="n">
-        <v>134550</v>
+        <v>137286</v>
       </c>
       <c r="I25" t="n">
-        <v>101.429</v>
+        <v>103.492</v>
       </c>
       <c r="J25" t="n">
-        <v>1045</v>
+        <v>1162</v>
       </c>
       <c r="K25" t="n">
-        <v>0.788</v>
+        <v>0.876</v>
       </c>
       <c r="L25" t="n">
-        <v>1279</v>
+        <v>1095</v>
       </c>
       <c r="M25" t="n">
-        <v>0.964</v>
+        <v>0.825</v>
       </c>
       <c r="N25" t="n">
-        <v>0.005</v>
+        <v>0.004</v>
       </c>
       <c r="O25" t="n">
-        <v>203.477</v>
+        <v>225.441</v>
       </c>
       <c r="P25" t="s">
         <v>164</v>
@@ -3956,7 +3960,7 @@
         <v>169</v>
       </c>
       <c r="C26" s="1" t="n">
-        <v>44045</v>
+        <v>44052</v>
       </c>
       <c r="D26" t="s">
         <v>170</v>
@@ -3966,27 +3970,27 @@
       </c>
       <c r="F26"/>
       <c r="G26" t="n">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="H26" t="n">
-        <v>437319</v>
+        <v>497971</v>
       </c>
       <c r="I26" t="n">
-        <v>3.804</v>
+        <v>4.332</v>
       </c>
       <c r="J26"/>
       <c r="K26"/>
       <c r="L26" t="n">
-        <v>7575</v>
+        <v>8665</v>
       </c>
       <c r="M26" t="n">
-        <v>0.066</v>
+        <v>0.075</v>
       </c>
       <c r="N26" t="n">
-        <v>0.1</v>
+        <v>0.07</v>
       </c>
       <c r="O26" t="n">
-        <v>9.993</v>
+        <v>14.258</v>
       </c>
       <c r="P26" t="s">
         <v>171</v>
@@ -4064,7 +4068,7 @@
         <v>180</v>
       </c>
       <c r="C28" s="1" t="n">
-        <v>44059</v>
+        <v>44061</v>
       </c>
       <c r="D28" t="s">
         <v>181</v>
@@ -4074,31 +4078,31 @@
       </c>
       <c r="F28"/>
       <c r="G28" t="n">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="H28" t="n">
-        <v>470320</v>
+        <v>510300</v>
       </c>
       <c r="I28" t="n">
-        <v>84.884</v>
+        <v>92.1</v>
       </c>
       <c r="J28" t="n">
-        <v>454</v>
+        <v>731</v>
       </c>
       <c r="K28" t="n">
-        <v>0.082</v>
+        <v>0.132</v>
       </c>
       <c r="L28" t="n">
-        <v>5946</v>
+        <v>9140</v>
       </c>
       <c r="M28" t="n">
-        <v>1.073</v>
+        <v>1.65</v>
       </c>
       <c r="N28" t="n">
-        <v>0.004</v>
+        <v>0.002</v>
       </c>
       <c r="O28" t="n">
-        <v>273.829</v>
+        <v>423.709</v>
       </c>
       <c r="P28" t="s">
         <v>183</v>
@@ -4121,7 +4125,7 @@
         <v>186</v>
       </c>
       <c r="C29" s="1" t="n">
-        <v>44055</v>
+        <v>44057</v>
       </c>
       <c r="D29" t="s">
         <v>187</v>
@@ -4131,27 +4135,27 @@
       </c>
       <c r="F29"/>
       <c r="G29" t="n">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="H29"/>
       <c r="I29"/>
       <c r="J29" t="n">
-        <v>92940</v>
+        <v>111580</v>
       </c>
       <c r="K29" t="n">
-        <v>1.424</v>
+        <v>1.709</v>
       </c>
       <c r="L29" t="n">
-        <v>76986</v>
+        <v>80395</v>
       </c>
       <c r="M29" t="n">
-        <v>1.179</v>
+        <v>1.232</v>
       </c>
       <c r="N29" t="n">
-        <v>0.022</v>
+        <v>0.024</v>
       </c>
       <c r="O29" t="n">
-        <v>45.523</v>
+        <v>40.982</v>
       </c>
       <c r="P29" t="s">
         <v>188</v>
@@ -4284,7 +4288,7 @@
         <v>204</v>
       </c>
       <c r="C32" s="1" t="n">
-        <v>44057</v>
+        <v>44059</v>
       </c>
       <c r="D32" t="s">
         <v>205</v>
@@ -4294,31 +4298,31 @@
       </c>
       <c r="F32"/>
       <c r="G32" t="n">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="H32" t="n">
-        <v>425969</v>
+        <v>428695</v>
       </c>
       <c r="I32" t="n">
-        <v>13.709</v>
+        <v>13.796</v>
       </c>
       <c r="J32" t="n">
-        <v>1654</v>
+        <v>1574</v>
       </c>
       <c r="K32" t="n">
-        <v>0.053</v>
+        <v>0.051</v>
       </c>
       <c r="L32" t="n">
-        <v>1471</v>
+        <v>1481</v>
       </c>
       <c r="M32" t="n">
-        <v>0.047</v>
+        <v>0.048</v>
       </c>
       <c r="N32" t="n">
-        <v>0.17</v>
+        <v>0.162</v>
       </c>
       <c r="O32" t="n">
-        <v>5.884</v>
+        <v>6.182</v>
       </c>
       <c r="P32" t="s">
         <v>207</v>
@@ -4341,7 +4345,7 @@
         <v>211</v>
       </c>
       <c r="C33" s="1" t="n">
-        <v>44058</v>
+        <v>44061</v>
       </c>
       <c r="D33" t="s">
         <v>212</v>
@@ -4351,31 +4355,31 @@
       </c>
       <c r="F33"/>
       <c r="G33" t="n">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="H33" t="n">
-        <v>715503</v>
+        <v>740871</v>
       </c>
       <c r="I33" t="n">
-        <v>68.646</v>
+        <v>71.08</v>
       </c>
       <c r="J33" t="n">
-        <v>10582</v>
+        <v>13910</v>
       </c>
       <c r="K33" t="n">
-        <v>1.015</v>
+        <v>1.335</v>
       </c>
       <c r="L33" t="n">
-        <v>10744</v>
+        <v>10305</v>
       </c>
       <c r="M33" t="n">
-        <v>1.031</v>
+        <v>0.989</v>
       </c>
       <c r="N33" t="n">
-        <v>0.018</v>
+        <v>0.02</v>
       </c>
       <c r="O33" t="n">
-        <v>55.219</v>
+        <v>48.971</v>
       </c>
       <c r="P33" t="s">
         <v>214</v>
@@ -4506,7 +4510,7 @@
         <v>233</v>
       </c>
       <c r="C36" s="1" t="n">
-        <v>44058</v>
+        <v>44060</v>
       </c>
       <c r="D36" t="s">
         <v>234</v>
@@ -4516,31 +4520,31 @@
       </c>
       <c r="F36"/>
       <c r="G36" t="n">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="H36" t="n">
-        <v>81936</v>
+        <v>82477</v>
       </c>
       <c r="I36" t="n">
-        <v>240.105</v>
+        <v>241.691</v>
       </c>
       <c r="J36" t="n">
-        <v>347</v>
+        <v>383</v>
       </c>
       <c r="K36" t="n">
-        <v>1.017</v>
+        <v>1.122</v>
       </c>
       <c r="L36" t="n">
-        <v>529</v>
+        <v>524</v>
       </c>
       <c r="M36" t="n">
-        <v>1.55</v>
+        <v>1.536</v>
       </c>
       <c r="N36" t="n">
-        <v>0.008</v>
+        <v>0.014</v>
       </c>
       <c r="O36" t="n">
-        <v>119.452</v>
+        <v>69.208</v>
       </c>
       <c r="P36" t="s">
         <v>235</v>
@@ -4622,7 +4626,7 @@
         <v>243</v>
       </c>
       <c r="C38" s="1" t="n">
-        <v>44059</v>
+        <v>44061</v>
       </c>
       <c r="D38" t="s">
         <v>239</v>
@@ -4634,31 +4638,31 @@
         <v>241</v>
       </c>
       <c r="G38" t="n">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="H38" t="n">
-        <v>30041400</v>
+        <v>31742782</v>
       </c>
       <c r="I38" t="n">
-        <v>21.769</v>
+        <v>23.002</v>
       </c>
       <c r="J38" t="n">
-        <v>731697</v>
+        <v>801518</v>
       </c>
       <c r="K38" t="n">
-        <v>0.53</v>
+        <v>0.581</v>
       </c>
       <c r="L38" t="n">
-        <v>779692</v>
+        <v>818212</v>
       </c>
       <c r="M38" t="n">
-        <v>0.565</v>
+        <v>0.593</v>
       </c>
       <c r="N38" t="n">
-        <v>0.08</v>
+        <v>0.076</v>
       </c>
       <c r="O38" t="n">
-        <v>12.499</v>
+        <v>13.195</v>
       </c>
       <c r="P38" t="s">
         <v>240</v>
@@ -4681,7 +4685,7 @@
         <v>245</v>
       </c>
       <c r="C39" s="1" t="n">
-        <v>44059</v>
+        <v>44062</v>
       </c>
       <c r="D39" t="s">
         <v>246</v>
@@ -4691,31 +4695,31 @@
       </c>
       <c r="F39"/>
       <c r="G39" t="n">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="H39" t="n">
-        <v>1061721</v>
+        <v>1096294</v>
       </c>
       <c r="I39" t="n">
-        <v>3.882</v>
+        <v>4.008</v>
       </c>
       <c r="J39" t="n">
-        <v>9218</v>
+        <v>14940</v>
       </c>
       <c r="K39" t="n">
-        <v>0.034</v>
+        <v>0.055</v>
       </c>
       <c r="L39" t="n">
-        <v>12732</v>
+        <v>12027</v>
       </c>
       <c r="M39" t="n">
-        <v>0.047</v>
+        <v>0.044</v>
       </c>
       <c r="N39" t="n">
-        <v>0.157</v>
+        <v>0.169</v>
       </c>
       <c r="O39" t="n">
-        <v>6.382</v>
+        <v>5.901</v>
       </c>
       <c r="P39" t="s">
         <v>247</v>
@@ -4738,7 +4742,7 @@
         <v>251</v>
       </c>
       <c r="C40" s="1" t="n">
-        <v>44059</v>
+        <v>44061</v>
       </c>
       <c r="D40" t="s">
         <v>252</v>
@@ -4748,31 +4752,31 @@
       </c>
       <c r="F40"/>
       <c r="G40" t="n">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="H40" t="n">
-        <v>2861825</v>
+        <v>2914049</v>
       </c>
       <c r="I40" t="n">
-        <v>34.072</v>
+        <v>34.694</v>
       </c>
       <c r="J40" t="n">
-        <v>25573</v>
+        <v>26111</v>
       </c>
       <c r="K40" t="n">
-        <v>0.304</v>
+        <v>0.311</v>
       </c>
       <c r="L40" t="n">
-        <v>25047</v>
+        <v>25362</v>
       </c>
       <c r="M40" t="n">
-        <v>0.298</v>
+        <v>0.302</v>
       </c>
       <c r="N40" t="n">
-        <v>0.093</v>
+        <v>0.094</v>
       </c>
       <c r="O40" t="n">
-        <v>10.705</v>
+        <v>10.691</v>
       </c>
       <c r="P40" t="s">
         <v>253</v>
@@ -4795,7 +4799,7 @@
         <v>257</v>
       </c>
       <c r="C41" s="1" t="n">
-        <v>44059</v>
+        <v>44060</v>
       </c>
       <c r="D41" t="s">
         <v>258</v>
@@ -4805,31 +4809,31 @@
       </c>
       <c r="F41"/>
       <c r="G41" t="n">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="H41" t="n">
-        <v>1282928</v>
+        <v>1304331</v>
       </c>
       <c r="I41" t="n">
-        <v>31.896</v>
+        <v>32.428</v>
       </c>
       <c r="J41" t="n">
-        <v>19278</v>
+        <v>21403</v>
       </c>
       <c r="K41" t="n">
-        <v>0.479</v>
+        <v>0.532</v>
       </c>
       <c r="L41" t="n">
-        <v>19649</v>
+        <v>19897</v>
       </c>
       <c r="M41" t="n">
-        <v>0.489</v>
+        <v>0.495</v>
       </c>
       <c r="N41" t="n">
-        <v>0.183</v>
+        <v>0.193</v>
       </c>
       <c r="O41" t="n">
-        <v>5.459</v>
+        <v>5.194</v>
       </c>
       <c r="P41" t="s">
         <v>260</v>
@@ -4852,7 +4856,7 @@
         <v>264</v>
       </c>
       <c r="C42" s="1" t="n">
-        <v>44058</v>
+        <v>44061</v>
       </c>
       <c r="D42" t="s">
         <v>265</v>
@@ -4862,31 +4866,31 @@
       </c>
       <c r="F42"/>
       <c r="G42" t="n">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="H42" t="n">
-        <v>709689</v>
+        <v>729913</v>
       </c>
       <c r="I42" t="n">
-        <v>143.726</v>
+        <v>147.822</v>
       </c>
       <c r="J42" t="n">
-        <v>10653</v>
+        <v>4339</v>
       </c>
       <c r="K42" t="n">
-        <v>2.157</v>
+        <v>0.879</v>
       </c>
       <c r="L42" t="n">
-        <v>6702</v>
+        <v>7876</v>
       </c>
       <c r="M42" t="n">
-        <v>1.357</v>
+        <v>1.595</v>
       </c>
       <c r="N42" t="n">
-        <v>0.011</v>
+        <v>0.01</v>
       </c>
       <c r="O42" t="n">
-        <v>89.36</v>
+        <v>101.16</v>
       </c>
       <c r="P42" t="s">
         <v>266</v>
@@ -4909,7 +4913,7 @@
         <v>269</v>
       </c>
       <c r="C43" s="1" t="n">
-        <v>44053</v>
+        <v>44055</v>
       </c>
       <c r="D43" t="s">
         <v>270</v>
@@ -4919,31 +4923,31 @@
       </c>
       <c r="F43"/>
       <c r="G43" t="n">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="H43" t="n">
-        <v>1966932</v>
+        <v>2021151</v>
       </c>
       <c r="I43" t="n">
-        <v>227.245</v>
+        <v>233.509</v>
       </c>
       <c r="J43" t="n">
-        <v>24348</v>
+        <v>26229</v>
       </c>
       <c r="K43" t="n">
-        <v>2.813</v>
+        <v>3.03</v>
       </c>
       <c r="L43" t="n">
-        <v>21582</v>
+        <v>21872</v>
       </c>
       <c r="M43" t="n">
-        <v>2.493</v>
+        <v>2.527</v>
       </c>
       <c r="N43" t="n">
-        <v>0.066</v>
+        <v>0.067</v>
       </c>
       <c r="O43" t="n">
-        <v>15.142</v>
+        <v>14.84</v>
       </c>
       <c r="P43" t="s">
         <v>45</v>
@@ -4966,7 +4970,7 @@
         <v>275</v>
       </c>
       <c r="C44" s="1" t="n">
-        <v>44059</v>
+        <v>44061</v>
       </c>
       <c r="D44" t="s">
         <v>276</v>
@@ -4978,31 +4982,31 @@
         <v>278</v>
       </c>
       <c r="G44" t="n">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="H44" t="n">
-        <v>4455931</v>
+        <v>4509997</v>
       </c>
       <c r="I44" t="n">
-        <v>73.698</v>
+        <v>74.592</v>
       </c>
       <c r="J44" t="n">
-        <v>22470</v>
+        <v>32687</v>
       </c>
       <c r="K44" t="n">
-        <v>0.372</v>
+        <v>0.541</v>
       </c>
       <c r="L44" t="n">
-        <v>22743</v>
+        <v>25757</v>
       </c>
       <c r="M44" t="n">
-        <v>0.376</v>
+        <v>0.426</v>
       </c>
       <c r="N44" t="n">
-        <v>0.021</v>
+        <v>0.019</v>
       </c>
       <c r="O44" t="n">
-        <v>47.736</v>
+        <v>52.874</v>
       </c>
       <c r="P44" t="s">
         <v>279</v>
@@ -5025,7 +5029,7 @@
         <v>282</v>
       </c>
       <c r="C45" s="1" t="n">
-        <v>44059</v>
+        <v>44061</v>
       </c>
       <c r="D45" t="s">
         <v>276</v>
@@ -5037,31 +5041,31 @@
         <v>278</v>
       </c>
       <c r="G45" t="n">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="H45" t="n">
-        <v>7557417</v>
+        <v>7642059</v>
       </c>
       <c r="I45" t="n">
-        <v>124.995</v>
+        <v>126.395</v>
       </c>
       <c r="J45" t="n">
-        <v>36807</v>
+        <v>53976</v>
       </c>
       <c r="K45" t="n">
-        <v>0.609</v>
+        <v>0.893</v>
       </c>
       <c r="L45" t="n">
-        <v>43939</v>
+        <v>46449</v>
       </c>
       <c r="M45" t="n">
-        <v>0.727</v>
+        <v>0.768</v>
       </c>
       <c r="N45" t="n">
-        <v>0.011</v>
+        <v>0.01</v>
       </c>
       <c r="O45" t="n">
-        <v>92.226</v>
+        <v>95.35</v>
       </c>
       <c r="P45" t="s">
         <v>279</v>
@@ -5084,7 +5088,7 @@
         <v>285</v>
       </c>
       <c r="C46" s="1" t="n">
-        <v>44058</v>
+        <v>44061</v>
       </c>
       <c r="D46" t="s">
         <v>286</v>
@@ -5096,31 +5100,31 @@
         <v>288</v>
       </c>
       <c r="G46" t="n">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="H46" t="n">
-        <v>1164029</v>
+        <v>1214145</v>
       </c>
       <c r="I46" t="n">
-        <v>9.204</v>
+        <v>9.6</v>
       </c>
       <c r="J46" t="n">
-        <v>56492</v>
+        <v>27677</v>
       </c>
       <c r="K46" t="n">
-        <v>0.447</v>
+        <v>0.219</v>
       </c>
       <c r="L46" t="n">
-        <v>25418</v>
+        <v>27130</v>
       </c>
       <c r="M46" t="n">
-        <v>0.201</v>
+        <v>0.215</v>
       </c>
       <c r="N46" t="n">
-        <v>0.046</v>
+        <v>0.041</v>
       </c>
       <c r="O46" t="n">
-        <v>21.864</v>
+        <v>24.6</v>
       </c>
       <c r="P46" t="s">
         <v>289</v>
@@ -5143,7 +5147,7 @@
         <v>292</v>
       </c>
       <c r="C47" s="1" t="n">
-        <v>44056</v>
+        <v>44059</v>
       </c>
       <c r="D47" t="s">
         <v>293</v>
@@ -5155,31 +5159,31 @@
         <v>294</v>
       </c>
       <c r="G47" t="n">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="H47" t="n">
-        <v>1463078</v>
+        <v>1488614</v>
       </c>
       <c r="I47" t="n">
-        <v>11.568</v>
+        <v>11.77</v>
       </c>
       <c r="J47" t="n">
-        <v>19476</v>
+        <v>8590</v>
       </c>
       <c r="K47" t="n">
-        <v>0.154</v>
+        <v>0.068</v>
       </c>
       <c r="L47" t="n">
-        <v>22650</v>
+        <v>18297</v>
       </c>
       <c r="M47" t="n">
-        <v>0.179</v>
+        <v>0.145</v>
       </c>
       <c r="N47" t="n">
-        <v>0.052</v>
+        <v>0.062</v>
       </c>
       <c r="O47" t="n">
-        <v>19.38</v>
+        <v>16.149</v>
       </c>
       <c r="P47" t="s">
         <v>289</v>
@@ -5202,7 +5206,7 @@
         <v>297</v>
       </c>
       <c r="C48" s="1" t="n">
-        <v>44054</v>
+        <v>44057</v>
       </c>
       <c r="D48" t="s">
         <v>298</v>
@@ -5212,31 +5216,31 @@
       </c>
       <c r="F48"/>
       <c r="G48" t="n">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="H48" t="n">
-        <v>2236924</v>
+        <v>2291327</v>
       </c>
       <c r="I48" t="n">
-        <v>119.133</v>
+        <v>122.03</v>
       </c>
       <c r="J48" t="n">
-        <v>10055</v>
+        <v>19573</v>
       </c>
       <c r="K48" t="n">
-        <v>0.536</v>
+        <v>1.042</v>
       </c>
       <c r="L48" t="n">
-        <v>15795</v>
+        <v>15431</v>
       </c>
       <c r="M48" t="n">
-        <v>0.841</v>
+        <v>0.822</v>
       </c>
       <c r="N48" t="n">
-        <v>0.121</v>
+        <v>0.098</v>
       </c>
       <c r="O48" t="n">
-        <v>8.235</v>
+        <v>10.206</v>
       </c>
       <c r="P48" t="s">
         <v>299</v>
@@ -5259,7 +5263,7 @@
         <v>302</v>
       </c>
       <c r="C49" s="1" t="n">
-        <v>44056</v>
+        <v>44060</v>
       </c>
       <c r="D49" t="s">
         <v>303</v>
@@ -5269,31 +5273,31 @@
       </c>
       <c r="F49"/>
       <c r="G49" t="n">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="H49" t="n">
-        <v>375859</v>
+        <v>394566</v>
       </c>
       <c r="I49" t="n">
-        <v>6.99</v>
+        <v>7.338</v>
       </c>
       <c r="J49" t="n">
-        <v>6768</v>
+        <v>3150</v>
       </c>
       <c r="K49" t="n">
-        <v>0.126</v>
+        <v>0.059</v>
       </c>
       <c r="L49" t="n">
-        <v>5792</v>
+        <v>5177</v>
       </c>
       <c r="M49" t="n">
-        <v>0.108</v>
+        <v>0.096</v>
       </c>
       <c r="N49" t="n">
-        <v>0.104</v>
+        <v>0.102</v>
       </c>
       <c r="O49" t="n">
-        <v>9.583</v>
+        <v>9.837</v>
       </c>
       <c r="P49" t="s">
         <v>45</v>
@@ -5316,7 +5320,7 @@
         <v>308</v>
       </c>
       <c r="C50" s="1" t="n">
-        <v>44059</v>
+        <v>44061</v>
       </c>
       <c r="D50" t="s">
         <v>309</v>
@@ -5326,31 +5330,31 @@
       </c>
       <c r="F50"/>
       <c r="G50" t="n">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="H50" t="n">
-        <v>558800</v>
+        <v>568440</v>
       </c>
       <c r="I50" t="n">
-        <v>130.849</v>
+        <v>133.107</v>
       </c>
       <c r="J50" t="n">
-        <v>2863</v>
+        <v>5306</v>
       </c>
       <c r="K50" t="n">
-        <v>0.67</v>
+        <v>1.242</v>
       </c>
       <c r="L50" t="n">
-        <v>3778</v>
+        <v>4140</v>
       </c>
       <c r="M50" t="n">
-        <v>0.885</v>
+        <v>0.969</v>
       </c>
       <c r="N50" t="n">
-        <v>0.17</v>
+        <v>0.153</v>
       </c>
       <c r="O50" t="n">
-        <v>5.88</v>
+        <v>6.546</v>
       </c>
       <c r="P50" t="s">
         <v>310</v>
@@ -5373,7 +5377,7 @@
         <v>314</v>
       </c>
       <c r="C51" s="1" t="n">
-        <v>44060</v>
+        <v>44062</v>
       </c>
       <c r="D51" t="s">
         <v>315</v>
@@ -5385,31 +5389,31 @@
         <v>317</v>
       </c>
       <c r="G51" t="n">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="H51" t="n">
-        <v>226524</v>
+        <v>230921</v>
       </c>
       <c r="I51" t="n">
-        <v>120.095</v>
+        <v>122.426</v>
       </c>
       <c r="J51" t="n">
-        <v>888</v>
+        <v>2163</v>
       </c>
       <c r="K51" t="n">
-        <v>0.471</v>
+        <v>1.147</v>
       </c>
       <c r="L51" t="n">
-        <v>1760</v>
+        <v>1738</v>
       </c>
       <c r="M51" t="n">
-        <v>0.933</v>
+        <v>0.921</v>
       </c>
       <c r="N51" t="n">
-        <v>0.003</v>
+        <v>0.002</v>
       </c>
       <c r="O51" t="n">
-        <v>385</v>
+        <v>608.3</v>
       </c>
       <c r="P51" t="s">
         <v>316</v>
@@ -5432,7 +5436,7 @@
         <v>320</v>
       </c>
       <c r="C52" s="1" t="n">
-        <v>44060</v>
+        <v>44062</v>
       </c>
       <c r="D52" t="s">
         <v>321</v>
@@ -5442,27 +5446,31 @@
       </c>
       <c r="F52"/>
       <c r="G52" t="n">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="H52" t="n">
-        <v>580453</v>
+        <v>589505</v>
       </c>
       <c r="I52" t="n">
-        <v>213.222</v>
-      </c>
-      <c r="J52"/>
-      <c r="K52"/>
+        <v>216.547</v>
+      </c>
+      <c r="J52" t="n">
+        <v>4864</v>
+      </c>
+      <c r="K52" t="n">
+        <v>1.787</v>
+      </c>
       <c r="L52" t="n">
-        <v>3866</v>
+        <v>3993</v>
       </c>
       <c r="M52" t="n">
-        <v>1.42</v>
+        <v>1.467</v>
       </c>
       <c r="N52" t="n">
-        <v>0.006</v>
+        <v>0.007</v>
       </c>
       <c r="O52" t="n">
-        <v>165.012</v>
+        <v>146.34</v>
       </c>
       <c r="P52" t="s">
         <v>45</v>
@@ -5485,7 +5493,7 @@
         <v>324</v>
       </c>
       <c r="C53" s="1" t="n">
-        <v>44056</v>
+        <v>44060</v>
       </c>
       <c r="D53" t="s">
         <v>325</v>
@@ -5495,31 +5503,31 @@
       </c>
       <c r="F53"/>
       <c r="G53" t="n">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="H53" t="n">
-        <v>456963</v>
+        <v>462207</v>
       </c>
       <c r="I53" t="n">
-        <v>730.001</v>
+        <v>738.378</v>
       </c>
       <c r="J53" t="n">
-        <v>1616</v>
+        <v>1231</v>
       </c>
       <c r="K53" t="n">
-        <v>2.582</v>
+        <v>1.967</v>
       </c>
       <c r="L53" t="n">
-        <v>1649</v>
+        <v>1543</v>
       </c>
       <c r="M53" t="n">
-        <v>2.634</v>
+        <v>2.465</v>
       </c>
       <c r="N53" t="n">
-        <v>0.025</v>
+        <v>0.03</v>
       </c>
       <c r="O53" t="n">
-        <v>39.396</v>
+        <v>33.132</v>
       </c>
       <c r="P53" t="s">
         <v>326</v>
@@ -5542,7 +5550,7 @@
         <v>329</v>
       </c>
       <c r="C54" s="1" t="n">
-        <v>44059</v>
+        <v>44061</v>
       </c>
       <c r="D54" t="s">
         <v>330</v>
@@ -5554,31 +5562,31 @@
         <v>332</v>
       </c>
       <c r="G54" t="n">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="H54" t="n">
-        <v>1114246</v>
+        <v>1129091</v>
       </c>
       <c r="I54" t="n">
-        <v>34.426</v>
+        <v>34.885</v>
       </c>
       <c r="J54" t="n">
-        <v>8029</v>
+        <v>8425</v>
       </c>
       <c r="K54" t="n">
-        <v>0.248</v>
+        <v>0.26</v>
       </c>
       <c r="L54" t="n">
-        <v>9753</v>
+        <v>9398</v>
       </c>
       <c r="M54" t="n">
-        <v>0.301</v>
+        <v>0.29</v>
       </c>
       <c r="N54" t="n">
         <v>0.002</v>
       </c>
       <c r="O54" t="n">
-        <v>650.2</v>
+        <v>557.508</v>
       </c>
       <c r="P54" t="s">
         <v>45</v>
@@ -5601,7 +5609,7 @@
         <v>336</v>
       </c>
       <c r="C55" s="1" t="n">
-        <v>44058</v>
+        <v>44060</v>
       </c>
       <c r="D55" t="s">
         <v>337</v>
@@ -5611,31 +5619,31 @@
       </c>
       <c r="F55"/>
       <c r="G55" t="n">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="H55" t="n">
-        <v>94865</v>
+        <v>97211</v>
       </c>
       <c r="I55" t="n">
-        <v>175.5</v>
+        <v>179.84</v>
       </c>
       <c r="J55" t="n">
-        <v>818</v>
+        <v>1036</v>
       </c>
       <c r="K55" t="n">
-        <v>1.513</v>
+        <v>1.917</v>
       </c>
       <c r="L55" t="n">
-        <v>1033</v>
+        <v>1094</v>
       </c>
       <c r="M55" t="n">
-        <v>1.911</v>
+        <v>2.024</v>
       </c>
       <c r="N55" t="n">
-        <v>0.111</v>
+        <v>0.097</v>
       </c>
       <c r="O55" t="n">
-        <v>9.005</v>
+        <v>10.293</v>
       </c>
       <c r="P55" t="s">
         <v>339</v>
@@ -5658,7 +5666,7 @@
         <v>343</v>
       </c>
       <c r="C56" s="1" t="n">
-        <v>44057</v>
+        <v>44060</v>
       </c>
       <c r="D56" t="s">
         <v>344</v>
@@ -5668,31 +5676,31 @@
       </c>
       <c r="F56"/>
       <c r="G56" t="n">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="H56" t="n">
-        <v>154515</v>
+        <v>161047</v>
       </c>
       <c r="I56" t="n">
-        <v>349.946</v>
+        <v>364.74</v>
       </c>
       <c r="J56" t="n">
-        <v>2435</v>
+        <v>2123</v>
       </c>
       <c r="K56" t="n">
-        <v>5.515</v>
+        <v>4.808</v>
       </c>
       <c r="L56" t="n">
-        <v>2077</v>
+        <v>2255</v>
       </c>
       <c r="M56" t="n">
-        <v>4.704</v>
+        <v>5.107</v>
       </c>
       <c r="N56" t="n">
-        <v>0.021</v>
+        <v>0.014</v>
       </c>
       <c r="O56" t="n">
-        <v>48.625</v>
+        <v>72.742</v>
       </c>
       <c r="P56" t="s">
         <v>345</v>
@@ -5715,7 +5723,7 @@
         <v>349</v>
       </c>
       <c r="C57" s="1" t="n">
-        <v>44055</v>
+        <v>44057</v>
       </c>
       <c r="D57" t="s">
         <v>350</v>
@@ -5725,31 +5733,31 @@
       </c>
       <c r="F57"/>
       <c r="G57" t="n">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="H57" t="n">
-        <v>1087111</v>
+        <v>1111567</v>
       </c>
       <c r="I57" t="n">
-        <v>8.432</v>
+        <v>8.621</v>
       </c>
       <c r="J57" t="n">
-        <v>8872</v>
+        <v>6848</v>
       </c>
       <c r="K57" t="n">
-        <v>0.069</v>
+        <v>0.053</v>
       </c>
       <c r="L57" t="n">
-        <v>9731</v>
+        <v>9288</v>
       </c>
       <c r="M57" t="n">
-        <v>0.075</v>
+        <v>0.072</v>
       </c>
       <c r="N57" t="n">
-        <v>0.625</v>
+        <v>0.662</v>
       </c>
       <c r="O57" t="n">
-        <v>1.6</v>
+        <v>1.51</v>
       </c>
       <c r="P57" t="s">
         <v>352</v>
@@ -5772,7 +5780,7 @@
         <v>356</v>
       </c>
       <c r="C58" s="1" t="n">
-        <v>44058</v>
+        <v>44060</v>
       </c>
       <c r="D58" t="s">
         <v>357</v>
@@ -5782,31 +5790,31 @@
       </c>
       <c r="F58"/>
       <c r="G58" t="n">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="H58" t="n">
-        <v>1583234</v>
+        <v>1626810</v>
       </c>
       <c r="I58" t="n">
-        <v>42.894</v>
+        <v>44.074</v>
       </c>
       <c r="J58" t="n">
-        <v>22707</v>
+        <v>21197</v>
       </c>
       <c r="K58" t="n">
-        <v>0.615</v>
+        <v>0.574</v>
       </c>
       <c r="L58" t="n">
-        <v>22228</v>
+        <v>22102</v>
       </c>
       <c r="M58" t="n">
-        <v>0.602</v>
+        <v>0.599</v>
       </c>
       <c r="N58" t="n">
-        <v>0.055</v>
+        <v>0.06</v>
       </c>
       <c r="O58" t="n">
-        <v>18.137</v>
+        <v>16.722</v>
       </c>
       <c r="P58" t="s">
         <v>358</v>
@@ -5829,7 +5837,7 @@
         <v>362</v>
       </c>
       <c r="C59" s="1" t="n">
-        <v>44052</v>
+        <v>44057</v>
       </c>
       <c r="D59" t="s">
         <v>363</v>
@@ -5839,31 +5847,31 @@
       </c>
       <c r="F59"/>
       <c r="G59" t="n">
-        <v>124</v>
+        <v>129</v>
       </c>
       <c r="H59" t="n">
-        <v>126828</v>
+        <v>134035</v>
       </c>
       <c r="I59" t="n">
-        <v>2.331</v>
+        <v>2.463</v>
       </c>
       <c r="J59" t="n">
-        <v>1001</v>
+        <v>1736</v>
       </c>
       <c r="K59" t="n">
-        <v>0.018</v>
+        <v>0.032</v>
       </c>
       <c r="L59" t="n">
-        <v>1098</v>
+        <v>1324</v>
       </c>
       <c r="M59" t="n">
-        <v>0.02</v>
+        <v>0.024</v>
       </c>
       <c r="N59" t="n">
         <v>0.001</v>
       </c>
       <c r="O59" t="n">
-        <v>1281</v>
+        <v>926.8</v>
       </c>
       <c r="P59" t="s">
         <v>364</v>
@@ -5886,7 +5894,7 @@
         <v>368</v>
       </c>
       <c r="C60" s="1" t="n">
-        <v>44059</v>
+        <v>44061</v>
       </c>
       <c r="D60" t="s">
         <v>369</v>
@@ -5896,31 +5904,31 @@
       </c>
       <c r="F60"/>
       <c r="G60" t="n">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="H60" t="n">
-        <v>517907</v>
+        <v>542866</v>
       </c>
       <c r="I60" t="n">
-        <v>17.775</v>
+        <v>18.632</v>
       </c>
       <c r="J60" t="n">
-        <v>12247</v>
+        <v>13439</v>
       </c>
       <c r="K60" t="n">
-        <v>0.42</v>
+        <v>0.461</v>
       </c>
       <c r="L60" t="n">
-        <v>10586</v>
+        <v>11453</v>
       </c>
       <c r="M60" t="n">
-        <v>0.363</v>
+        <v>0.393</v>
       </c>
       <c r="N60" t="n">
-        <v>0.046</v>
+        <v>0.049</v>
       </c>
       <c r="O60" t="n">
-        <v>21.623</v>
+        <v>20.395</v>
       </c>
       <c r="P60" t="s">
         <v>370</v>
@@ -5943,7 +5951,7 @@
         <v>374</v>
       </c>
       <c r="C61" s="1" t="n">
-        <v>44052</v>
+        <v>44059</v>
       </c>
       <c r="D61" t="s">
         <v>375</v>
@@ -5953,27 +5961,27 @@
       </c>
       <c r="F61"/>
       <c r="G61" t="n">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H61" t="n">
-        <v>1195475</v>
+        <v>1312787</v>
       </c>
       <c r="I61" t="n">
-        <v>69.769</v>
+        <v>76.615</v>
       </c>
       <c r="J61"/>
       <c r="K61"/>
       <c r="L61" t="n">
-        <v>15822</v>
+        <v>15892</v>
       </c>
       <c r="M61" t="n">
-        <v>0.923</v>
+        <v>0.927</v>
       </c>
       <c r="N61" t="n">
-        <v>0.029</v>
+        <v>0.04</v>
       </c>
       <c r="O61" t="n">
-        <v>34.026</v>
+        <v>24.999</v>
       </c>
       <c r="P61" t="s">
         <v>377</v>
@@ -5996,7 +6004,7 @@
         <v>381</v>
       </c>
       <c r="C62" s="1" t="n">
-        <v>44059</v>
+        <v>44061</v>
       </c>
       <c r="D62" t="s">
         <v>382</v>
@@ -6006,31 +6014,31 @@
       </c>
       <c r="F62"/>
       <c r="G62" t="n">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="H62" t="n">
-        <v>597956</v>
+        <v>639415</v>
       </c>
       <c r="I62" t="n">
-        <v>124</v>
+        <v>132.597</v>
       </c>
       <c r="J62" t="n">
-        <v>26014</v>
+        <v>23038</v>
       </c>
       <c r="K62" t="n">
-        <v>5.395</v>
+        <v>4.777</v>
       </c>
       <c r="L62" t="n">
-        <v>14479</v>
+        <v>19530</v>
       </c>
       <c r="M62" t="n">
-        <v>3.003</v>
+        <v>4.05</v>
       </c>
       <c r="N62" t="n">
         <v>0.001</v>
       </c>
       <c r="O62" t="n">
-        <v>1949.096</v>
+        <v>1872.74</v>
       </c>
       <c r="P62" t="s">
         <v>383</v>
@@ -6053,7 +6061,7 @@
         <v>386</v>
       </c>
       <c r="C63" s="1" t="n">
-        <v>44060</v>
+        <v>44061</v>
       </c>
       <c r="D63" t="s">
         <v>387</v>
@@ -6063,31 +6071,31 @@
       </c>
       <c r="F63"/>
       <c r="G63" t="n">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="H63" t="n">
-        <v>352625</v>
+        <v>355196</v>
       </c>
       <c r="I63" t="n">
-        <v>1.711</v>
+        <v>1.723</v>
       </c>
       <c r="J63" t="n">
-        <v>2036</v>
+        <v>2571</v>
       </c>
       <c r="K63" t="n">
-        <v>0.01</v>
+        <v>0.012</v>
       </c>
       <c r="L63" t="n">
-        <v>4682</v>
+        <v>3747</v>
       </c>
       <c r="M63" t="n">
-        <v>0.023</v>
+        <v>0.018</v>
       </c>
       <c r="N63" t="n">
-        <v>0.076</v>
+        <v>0.1</v>
       </c>
       <c r="O63" t="n">
-        <v>13.157</v>
+        <v>10.019</v>
       </c>
       <c r="P63" t="s">
         <v>388</v>
@@ -6110,7 +6118,7 @@
         <v>392</v>
       </c>
       <c r="C64" s="1" t="n">
-        <v>44055</v>
+        <v>44060</v>
       </c>
       <c r="D64" t="s">
         <v>393</v>
@@ -6120,31 +6128,31 @@
       </c>
       <c r="F64"/>
       <c r="G64" t="n">
-        <v>171</v>
+        <v>176</v>
       </c>
       <c r="H64" t="n">
-        <v>509147</v>
+        <v>544872</v>
       </c>
       <c r="I64" t="n">
-        <v>93.917</v>
+        <v>100.507</v>
       </c>
       <c r="J64" t="n">
-        <v>8493</v>
+        <v>1984</v>
       </c>
       <c r="K64" t="n">
-        <v>1.567</v>
+        <v>0.366</v>
       </c>
       <c r="L64" t="n">
-        <v>7077</v>
+        <v>7826</v>
       </c>
       <c r="M64" t="n">
-        <v>1.305</v>
+        <v>1.444</v>
       </c>
       <c r="N64" t="n">
         <v>0.007</v>
       </c>
       <c r="O64" t="n">
-        <v>141.137</v>
+        <v>143.408</v>
       </c>
       <c r="P64" t="s">
         <v>394</v>
@@ -6212,7 +6220,7 @@
         <v>406</v>
       </c>
       <c r="C66" s="1" t="n">
-        <v>44060</v>
+        <v>44062</v>
       </c>
       <c r="D66" t="s">
         <v>407</v>
@@ -6222,31 +6230,31 @@
       </c>
       <c r="F66"/>
       <c r="G66" t="n">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="H66" t="n">
-        <v>2299601</v>
+        <v>2340072</v>
       </c>
       <c r="I66" t="n">
-        <v>10.411</v>
+        <v>10.594</v>
       </c>
       <c r="J66" t="n">
-        <v>22448</v>
+        <v>22859</v>
       </c>
       <c r="K66" t="n">
-        <v>0.102</v>
+        <v>0.103</v>
       </c>
       <c r="L66" t="n">
-        <v>21717</v>
+        <v>21947</v>
       </c>
       <c r="M66" t="n">
-        <v>0.098</v>
+        <v>0.099</v>
       </c>
       <c r="N66" t="n">
-        <v>0.03</v>
+        <v>0.025</v>
       </c>
       <c r="O66" t="n">
-        <v>33.374</v>
+        <v>39.281</v>
       </c>
       <c r="P66" t="s">
         <v>408</v>
@@ -6269,7 +6277,7 @@
         <v>411</v>
       </c>
       <c r="C67" s="1" t="n">
-        <v>44056</v>
+        <v>44057</v>
       </c>
       <c r="D67" t="s">
         <v>412</v>
@@ -6279,31 +6287,31 @@
       </c>
       <c r="F67"/>
       <c r="G67" t="n">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="H67" t="n">
-        <v>259583</v>
+        <v>262275</v>
       </c>
       <c r="I67" t="n">
-        <v>60.162</v>
+        <v>60.785</v>
       </c>
       <c r="J67" t="n">
-        <v>3134</v>
+        <v>2692</v>
       </c>
       <c r="K67" t="n">
-        <v>0.726</v>
+        <v>0.624</v>
       </c>
       <c r="L67" t="n">
-        <v>2986</v>
+        <v>2889</v>
       </c>
       <c r="M67" t="n">
-        <v>0.692</v>
+        <v>0.67</v>
       </c>
       <c r="N67" t="n">
-        <v>0.342</v>
+        <v>0.348</v>
       </c>
       <c r="O67" t="n">
-        <v>2.925</v>
+        <v>2.877</v>
       </c>
       <c r="P67" t="s">
         <v>413</v>
@@ -6326,7 +6334,7 @@
         <v>416</v>
       </c>
       <c r="C68" s="1" t="n">
-        <v>44056</v>
+        <v>44058</v>
       </c>
       <c r="D68" t="s">
         <v>417</v>
@@ -6336,31 +6344,31 @@
       </c>
       <c r="F68"/>
       <c r="G68" t="n">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="H68" t="n">
-        <v>146284</v>
+        <v>151427</v>
       </c>
       <c r="I68" t="n">
-        <v>20.509</v>
+        <v>21.23</v>
       </c>
       <c r="J68" t="n">
-        <v>1767</v>
+        <v>2078</v>
       </c>
       <c r="K68" t="n">
-        <v>0.248</v>
+        <v>0.291</v>
       </c>
       <c r="L68" t="n">
-        <v>1572</v>
+        <v>2018</v>
       </c>
       <c r="M68" t="n">
-        <v>0.22</v>
+        <v>0.283</v>
       </c>
       <c r="N68" t="n">
-        <v>0.178</v>
+        <v>0.182</v>
       </c>
       <c r="O68" t="n">
-        <v>5.62</v>
+        <v>5.499</v>
       </c>
       <c r="P68" t="s">
         <v>418</v>
@@ -6436,7 +6444,7 @@
         <v>428</v>
       </c>
       <c r="C70" s="1" t="n">
-        <v>44049</v>
+        <v>44059</v>
       </c>
       <c r="D70" t="s">
         <v>429</v>
@@ -6446,31 +6454,31 @@
       </c>
       <c r="F70"/>
       <c r="G70" t="n">
-        <v>126</v>
+        <v>136</v>
       </c>
       <c r="H70" t="n">
-        <v>1591000</v>
+        <v>1948932</v>
       </c>
       <c r="I70" t="n">
-        <v>14.519</v>
+        <v>17.785</v>
       </c>
       <c r="J70" t="n">
-        <v>27732</v>
+        <v>25312</v>
       </c>
       <c r="K70" t="n">
-        <v>0.253</v>
+        <v>0.231</v>
       </c>
       <c r="L70" t="n">
-        <v>25521</v>
+        <v>30570</v>
       </c>
       <c r="M70" t="n">
-        <v>0.233</v>
+        <v>0.279</v>
       </c>
       <c r="N70" t="n">
-        <v>0.171</v>
+        <v>0.145</v>
       </c>
       <c r="O70" t="n">
-        <v>5.858</v>
+        <v>6.896</v>
       </c>
       <c r="P70" t="s">
         <v>220</v>
@@ -6493,7 +6501,7 @@
         <v>434</v>
       </c>
       <c r="C71" s="1" t="n">
-        <v>44059</v>
+        <v>44061</v>
       </c>
       <c r="D71" t="s">
         <v>435</v>
@@ -6503,31 +6511,31 @@
       </c>
       <c r="F71"/>
       <c r="G71" t="n">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="H71" t="n">
-        <v>2272730</v>
+        <v>2305392</v>
       </c>
       <c r="I71" t="n">
-        <v>60.051</v>
+        <v>60.914</v>
       </c>
       <c r="J71" t="n">
-        <v>16004</v>
+        <v>19884</v>
       </c>
       <c r="K71" t="n">
-        <v>0.423</v>
+        <v>0.525</v>
       </c>
       <c r="L71" t="n">
-        <v>21301</v>
+        <v>20980</v>
       </c>
       <c r="M71" t="n">
-        <v>0.563</v>
+        <v>0.554</v>
       </c>
       <c r="N71" t="n">
         <v>0.033</v>
       </c>
       <c r="O71" t="n">
-        <v>30.288</v>
+        <v>30.162</v>
       </c>
       <c r="P71" t="s">
         <v>436</v>
@@ -6550,7 +6558,7 @@
         <v>439</v>
       </c>
       <c r="C72" s="1" t="n">
-        <v>44059</v>
+        <v>44061</v>
       </c>
       <c r="D72" t="s">
         <v>435</v>
@@ -6560,31 +6568,31 @@
       </c>
       <c r="F72"/>
       <c r="G72" t="n">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="H72" t="n">
-        <v>2375706</v>
+        <v>2409394</v>
       </c>
       <c r="I72" t="n">
-        <v>62.772</v>
+        <v>63.662</v>
       </c>
       <c r="J72" t="n">
-        <v>16613</v>
+        <v>20530</v>
       </c>
       <c r="K72" t="n">
-        <v>0.439</v>
+        <v>0.542</v>
       </c>
       <c r="L72" t="n">
-        <v>22321</v>
+        <v>21696</v>
       </c>
       <c r="M72" t="n">
-        <v>0.59</v>
+        <v>0.573</v>
       </c>
       <c r="N72" t="n">
         <v>0.032</v>
       </c>
       <c r="O72" t="n">
-        <v>31.738</v>
+        <v>31.192</v>
       </c>
       <c r="P72" t="s">
         <v>436</v>
@@ -6664,7 +6672,7 @@
         <v>448</v>
       </c>
       <c r="C74" s="1" t="n">
-        <v>44059</v>
+        <v>44061</v>
       </c>
       <c r="D74" t="s">
         <v>449</v>
@@ -6674,31 +6682,31 @@
       </c>
       <c r="F74"/>
       <c r="G74" t="n">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="H74" t="n">
-        <v>551273</v>
+        <v>560990</v>
       </c>
       <c r="I74" t="n">
-        <v>191.344</v>
+        <v>194.717</v>
       </c>
       <c r="J74" t="n">
-        <v>4988</v>
+        <v>5020</v>
       </c>
       <c r="K74" t="n">
-        <v>1.731</v>
+        <v>1.742</v>
       </c>
       <c r="L74" t="n">
-        <v>4416</v>
+        <v>4529</v>
       </c>
       <c r="M74" t="n">
-        <v>1.533</v>
+        <v>1.572</v>
       </c>
       <c r="N74" t="n">
-        <v>0.07</v>
+        <v>0.066</v>
       </c>
       <c r="O74" t="n">
-        <v>14.318</v>
+        <v>15.054</v>
       </c>
       <c r="P74" t="s">
         <v>450</v>
@@ -6721,7 +6729,7 @@
         <v>454</v>
       </c>
       <c r="C75" s="1" t="n">
-        <v>44058</v>
+        <v>44061</v>
       </c>
       <c r="D75" t="s">
         <v>455</v>
@@ -6731,31 +6739,31 @@
       </c>
       <c r="F75"/>
       <c r="G75" t="n">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="H75" t="n">
-        <v>1502042</v>
+        <v>1542094</v>
       </c>
       <c r="I75" t="n">
-        <v>78.078</v>
+        <v>80.16</v>
       </c>
       <c r="J75" t="n">
-        <v>23986</v>
+        <v>21344</v>
       </c>
       <c r="K75" t="n">
-        <v>1.247</v>
+        <v>1.109</v>
       </c>
       <c r="L75" t="n">
-        <v>19612</v>
+        <v>19607</v>
       </c>
       <c r="M75" t="n">
         <v>1.019</v>
       </c>
       <c r="N75" t="n">
-        <v>0.064</v>
+        <v>0.063</v>
       </c>
       <c r="O75" t="n">
-        <v>15.648</v>
+        <v>15.872</v>
       </c>
       <c r="P75" t="s">
         <v>457</v>
@@ -6778,7 +6786,7 @@
         <v>461</v>
       </c>
       <c r="C76" s="1" t="n">
-        <v>44059</v>
+        <v>44061</v>
       </c>
       <c r="D76" t="s">
         <v>462</v>
@@ -6788,31 +6796,31 @@
       </c>
       <c r="F76"/>
       <c r="G76" t="n">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="H76" t="n">
-        <v>32784478</v>
+        <v>33217468</v>
       </c>
       <c r="I76" t="n">
-        <v>224.652</v>
+        <v>227.619</v>
       </c>
       <c r="J76" t="n">
-        <v>250660</v>
+        <v>248709</v>
       </c>
       <c r="K76" t="n">
-        <v>1.718</v>
+        <v>1.704</v>
       </c>
       <c r="L76" t="n">
-        <v>271188</v>
+        <v>272815</v>
       </c>
       <c r="M76" t="n">
-        <v>1.858</v>
+        <v>1.869</v>
       </c>
       <c r="N76" t="n">
-        <v>0.019</v>
+        <v>0.018</v>
       </c>
       <c r="O76" t="n">
-        <v>53.418</v>
+        <v>54.422</v>
       </c>
       <c r="P76" t="s">
         <v>463</v>
@@ -6835,7 +6843,7 @@
         <v>467</v>
       </c>
       <c r="C77" s="1" t="n">
-        <v>44056</v>
+        <v>44059</v>
       </c>
       <c r="D77" t="s">
         <v>468</v>
@@ -6845,31 +6853,31 @@
       </c>
       <c r="F77"/>
       <c r="G77" t="n">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="H77" t="n">
-        <v>319295</v>
+        <v>334270</v>
       </c>
       <c r="I77" t="n">
-        <v>24.652</v>
+        <v>25.808</v>
       </c>
       <c r="J77" t="n">
-        <v>4756</v>
+        <v>4796</v>
       </c>
       <c r="K77" t="n">
-        <v>0.367</v>
+        <v>0.37</v>
       </c>
       <c r="L77" t="n">
-        <v>4721</v>
+        <v>5070</v>
       </c>
       <c r="M77" t="n">
-        <v>0.364</v>
+        <v>0.391</v>
       </c>
       <c r="N77" t="n">
-        <v>0.003</v>
+        <v>0.006</v>
       </c>
       <c r="O77" t="n">
-        <v>388.788</v>
+        <v>162.798</v>
       </c>
       <c r="P77" t="s">
         <v>469</v>
@@ -6892,7 +6900,7 @@
         <v>473</v>
       </c>
       <c r="C78" s="1" t="n">
-        <v>44059</v>
+        <v>44061</v>
       </c>
       <c r="D78" t="s">
         <v>474</v>
@@ -6902,31 +6910,31 @@
       </c>
       <c r="F78"/>
       <c r="G78" t="n">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="H78" t="n">
-        <v>4262092</v>
+        <v>4378417</v>
       </c>
       <c r="I78" t="n">
-        <v>122.425</v>
+        <v>125.766</v>
       </c>
       <c r="J78" t="n">
-        <v>60016</v>
+        <v>60712</v>
       </c>
       <c r="K78" t="n">
-        <v>1.724</v>
+        <v>1.744</v>
       </c>
       <c r="L78" t="n">
-        <v>65444</v>
+        <v>63570</v>
       </c>
       <c r="M78" t="n">
-        <v>1.88</v>
+        <v>1.826</v>
       </c>
       <c r="N78" t="n">
         <v>0.022</v>
       </c>
       <c r="O78" t="n">
-        <v>45.569</v>
+        <v>44.646</v>
       </c>
       <c r="P78" t="s">
         <v>45</v>
@@ -6949,7 +6957,7 @@
         <v>477</v>
       </c>
       <c r="C79" s="1" t="n">
-        <v>44059</v>
+        <v>44061</v>
       </c>
       <c r="D79" t="s">
         <v>478</v>
@@ -6961,31 +6969,31 @@
         <v>480</v>
       </c>
       <c r="G79" t="n">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="H79" t="n">
-        <v>133756</v>
+        <v>135731</v>
       </c>
       <c r="I79" t="n">
-        <v>7.988</v>
+        <v>8.106</v>
       </c>
       <c r="J79" t="n">
-        <v>1317</v>
+        <v>926</v>
       </c>
       <c r="K79" t="n">
-        <v>0.079</v>
+        <v>0.055</v>
       </c>
       <c r="L79" t="n">
-        <v>1572</v>
+        <v>1529</v>
       </c>
       <c r="M79" t="n">
-        <v>0.094</v>
+        <v>0.091</v>
       </c>
       <c r="N79" t="n">
-        <v>0.091</v>
+        <v>0.086</v>
       </c>
       <c r="O79" t="n">
-        <v>11.015</v>
+        <v>11.571</v>
       </c>
       <c r="P79" t="s">
         <v>481</v>
@@ -7008,7 +7016,7 @@
         <v>485</v>
       </c>
       <c r="C80" s="1" t="n">
-        <v>44059</v>
+        <v>44060</v>
       </c>
       <c r="D80" t="s">
         <v>486</v>
@@ -7020,31 +7028,31 @@
         <v>487</v>
       </c>
       <c r="G80" t="n">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="H80" t="n">
-        <v>804568</v>
+        <v>811920</v>
       </c>
       <c r="I80" t="n">
-        <v>118.239</v>
+        <v>119.319</v>
       </c>
       <c r="J80" t="n">
-        <v>6559</v>
+        <v>7352</v>
       </c>
       <c r="K80" t="n">
-        <v>0.964</v>
+        <v>1.08</v>
       </c>
       <c r="L80" t="n">
-        <v>8178</v>
+        <v>8254</v>
       </c>
       <c r="M80" t="n">
-        <v>1.202</v>
+        <v>1.213</v>
       </c>
       <c r="N80" t="n">
-        <v>0.028</v>
+        <v>0.027</v>
       </c>
       <c r="O80" t="n">
-        <v>35.601</v>
+        <v>36.499</v>
       </c>
       <c r="P80" t="s">
         <v>45</v>
@@ -7067,7 +7075,7 @@
         <v>491</v>
       </c>
       <c r="C81" s="1" t="n">
-        <v>44054</v>
+        <v>44061</v>
       </c>
       <c r="D81" t="s">
         <v>492</v>
@@ -7077,27 +7085,27 @@
       </c>
       <c r="F81"/>
       <c r="G81" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H81" t="n">
-        <v>686738</v>
+        <v>731313</v>
       </c>
       <c r="I81" t="n">
-        <v>117.384</v>
+        <v>125.003</v>
       </c>
       <c r="J81"/>
       <c r="K81"/>
       <c r="L81" t="n">
-        <v>4504</v>
+        <v>6368</v>
       </c>
       <c r="M81" t="n">
-        <v>0.77</v>
+        <v>1.088</v>
       </c>
       <c r="N81" t="n">
-        <v>0.071</v>
+        <v>0.012</v>
       </c>
       <c r="O81" t="n">
-        <v>14.069</v>
+        <v>81.641</v>
       </c>
       <c r="P81" t="s">
         <v>45</v>
@@ -7120,7 +7128,7 @@
         <v>494</v>
       </c>
       <c r="C82" s="1" t="n">
-        <v>44054</v>
+        <v>44061</v>
       </c>
       <c r="D82" t="s">
         <v>492</v>
@@ -7130,27 +7138,27 @@
       </c>
       <c r="F82"/>
       <c r="G82" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H82" t="n">
-        <v>1610906</v>
+        <v>1745928</v>
       </c>
       <c r="I82" t="n">
-        <v>275.352</v>
+        <v>298.432</v>
       </c>
       <c r="J82"/>
       <c r="K82"/>
       <c r="L82" t="n">
-        <v>17067</v>
+        <v>19289</v>
       </c>
       <c r="M82" t="n">
-        <v>2.917</v>
+        <v>3.297</v>
       </c>
       <c r="N82" t="n">
-        <v>0.019</v>
+        <v>0.004</v>
       </c>
       <c r="O82" t="n">
-        <v>53.311</v>
+        <v>247.295</v>
       </c>
       <c r="P82" t="s">
         <v>45</v>
@@ -7173,7 +7181,7 @@
         <v>497</v>
       </c>
       <c r="C83" s="1" t="n">
-        <v>44059</v>
+        <v>44062</v>
       </c>
       <c r="D83" t="s">
         <v>498</v>
@@ -7183,31 +7191,31 @@
       </c>
       <c r="F83"/>
       <c r="G83" t="n">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="H83" t="n">
-        <v>294838</v>
+        <v>300586</v>
       </c>
       <c r="I83" t="n">
-        <v>54.003</v>
+        <v>55.056</v>
       </c>
       <c r="J83" t="n">
-        <v>2013</v>
+        <v>3684</v>
       </c>
       <c r="K83" t="n">
-        <v>0.369</v>
+        <v>0.675</v>
       </c>
       <c r="L83" t="n">
-        <v>2268</v>
+        <v>2354</v>
       </c>
       <c r="M83" t="n">
-        <v>0.415</v>
+        <v>0.431</v>
       </c>
       <c r="N83" t="n">
-        <v>0.018</v>
+        <v>0.019</v>
       </c>
       <c r="O83" t="n">
-        <v>54.934</v>
+        <v>53.674</v>
       </c>
       <c r="P83" t="s">
         <v>500</v>
@@ -7230,7 +7238,7 @@
         <v>503</v>
       </c>
       <c r="C84" s="1" t="n">
-        <v>44057</v>
+        <v>44061</v>
       </c>
       <c r="D84" t="s">
         <v>504</v>
@@ -7240,31 +7248,31 @@
       </c>
       <c r="F84"/>
       <c r="G84" t="n">
-        <v>156</v>
+        <v>160</v>
       </c>
       <c r="H84" t="n">
-        <v>141545</v>
+        <v>144555</v>
       </c>
       <c r="I84" t="n">
-        <v>68.085</v>
+        <v>69.533</v>
       </c>
       <c r="J84" t="n">
-        <v>1034</v>
+        <v>1092</v>
       </c>
       <c r="K84" t="n">
-        <v>0.497</v>
+        <v>0.525</v>
       </c>
       <c r="L84" t="n">
-        <v>804</v>
+        <v>834</v>
       </c>
       <c r="M84" t="n">
-        <v>0.387</v>
+        <v>0.401</v>
       </c>
       <c r="N84" t="n">
-        <v>0.019</v>
+        <v>0.031</v>
       </c>
       <c r="O84" t="n">
-        <v>51.633</v>
+        <v>31.902</v>
       </c>
       <c r="P84" t="s">
         <v>506</v>
@@ -7287,7 +7295,7 @@
         <v>510</v>
       </c>
       <c r="C85" s="1" t="n">
-        <v>44059</v>
+        <v>44061</v>
       </c>
       <c r="D85" t="s">
         <v>511</v>
@@ -7299,31 +7307,31 @@
         <v>513</v>
       </c>
       <c r="G85" t="n">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="H85" t="n">
-        <v>3400638</v>
+        <v>3430347</v>
       </c>
       <c r="I85" t="n">
-        <v>57.338</v>
+        <v>57.839</v>
       </c>
       <c r="J85" t="n">
-        <v>22609</v>
+        <v>14677</v>
       </c>
       <c r="K85" t="n">
-        <v>0.381</v>
+        <v>0.247</v>
       </c>
       <c r="L85" t="n">
-        <v>21436</v>
+        <v>21624</v>
       </c>
       <c r="M85" t="n">
-        <v>0.361</v>
+        <v>0.365</v>
       </c>
       <c r="N85" t="n">
-        <v>0.203</v>
+        <v>0.174</v>
       </c>
       <c r="O85" t="n">
-        <v>4.925</v>
+        <v>5.758</v>
       </c>
       <c r="P85" t="s">
         <v>512</v>
@@ -7346,7 +7354,7 @@
         <v>517</v>
       </c>
       <c r="C86" s="1" t="n">
-        <v>44060</v>
+        <v>44061</v>
       </c>
       <c r="D86" t="s">
         <v>518</v>
@@ -7356,31 +7364,31 @@
       </c>
       <c r="F86"/>
       <c r="G86" t="n">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="H86" t="n">
-        <v>1665506</v>
+        <v>1671823</v>
       </c>
       <c r="I86" t="n">
-        <v>32.486</v>
+        <v>32.609</v>
       </c>
       <c r="J86" t="n">
-        <v>5724</v>
+        <v>6317</v>
       </c>
       <c r="K86" t="n">
-        <v>0.112</v>
+        <v>0.123</v>
       </c>
       <c r="L86" t="n">
-        <v>7657</v>
+        <v>7353</v>
       </c>
       <c r="M86" t="n">
-        <v>0.149</v>
+        <v>0.143</v>
       </c>
       <c r="N86" t="n">
-        <v>0.017</v>
+        <v>0.021</v>
       </c>
       <c r="O86" t="n">
-        <v>60.291</v>
+        <v>46.749</v>
       </c>
       <c r="P86" t="s">
         <v>519</v>
@@ -7403,7 +7411,7 @@
         <v>523</v>
       </c>
       <c r="C87" s="1" t="n">
-        <v>44049</v>
+        <v>44056</v>
       </c>
       <c r="D87" t="s">
         <v>524</v>
@@ -7413,27 +7421,27 @@
       </c>
       <c r="F87"/>
       <c r="G87" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="H87" t="n">
-        <v>4983935</v>
+        <v>5367311</v>
       </c>
       <c r="I87" t="n">
-        <v>106.597</v>
+        <v>114.797</v>
       </c>
       <c r="J87"/>
       <c r="K87"/>
       <c r="L87" t="n">
-        <v>47349</v>
+        <v>54768</v>
       </c>
       <c r="M87" t="n">
-        <v>1.013</v>
+        <v>1.171</v>
       </c>
       <c r="N87" t="n">
-        <v>0.074</v>
+        <v>0.072</v>
       </c>
       <c r="O87" t="n">
-        <v>13.57</v>
+        <v>13.952</v>
       </c>
       <c r="P87" t="s">
         <v>526</v>
@@ -7509,7 +7517,7 @@
         <v>536</v>
       </c>
       <c r="C89" s="1" t="n">
-        <v>44052</v>
+        <v>44059</v>
       </c>
       <c r="D89" t="s">
         <v>537</v>
@@ -7519,27 +7527,27 @@
       </c>
       <c r="F89"/>
       <c r="G89" t="n">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="H89"/>
       <c r="I89"/>
       <c r="J89" t="n">
-        <v>7674</v>
+        <v>8070</v>
       </c>
       <c r="K89" t="n">
-        <v>0.76</v>
+        <v>0.799</v>
       </c>
       <c r="L89" t="n">
-        <v>7674</v>
+        <v>8070</v>
       </c>
       <c r="M89" t="n">
-        <v>0.76</v>
+        <v>0.799</v>
       </c>
       <c r="N89" t="n">
         <v>0.035</v>
       </c>
       <c r="O89" t="n">
-        <v>28.258</v>
+        <v>28.661</v>
       </c>
       <c r="P89" t="s">
         <v>533</v>
@@ -7562,7 +7570,7 @@
         <v>540</v>
       </c>
       <c r="C90" s="1" t="n">
-        <v>44058</v>
+        <v>44060</v>
       </c>
       <c r="D90" t="s">
         <v>541</v>
@@ -7572,31 +7580,31 @@
       </c>
       <c r="F90"/>
       <c r="G90" t="n">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="H90" t="n">
-        <v>881683</v>
+        <v>890289</v>
       </c>
       <c r="I90" t="n">
-        <v>101.874</v>
+        <v>102.869</v>
       </c>
       <c r="J90" t="n">
-        <v>3808</v>
+        <v>5100</v>
       </c>
       <c r="K90" t="n">
-        <v>0.44</v>
+        <v>0.589</v>
       </c>
       <c r="L90" t="n">
-        <v>5750</v>
+        <v>5824</v>
       </c>
       <c r="M90" t="n">
-        <v>0.664</v>
+        <v>0.673</v>
       </c>
       <c r="N90" t="n">
-        <v>0.035</v>
+        <v>0.037</v>
       </c>
       <c r="O90" t="n">
-        <v>28.75</v>
+        <v>26.874</v>
       </c>
       <c r="P90" t="s">
         <v>542</v>
@@ -7619,7 +7627,7 @@
         <v>546</v>
       </c>
       <c r="C91" s="1" t="n">
-        <v>44059</v>
+        <v>44061</v>
       </c>
       <c r="D91" t="s">
         <v>547</v>
@@ -7629,31 +7637,31 @@
       </c>
       <c r="F91"/>
       <c r="G91" t="n">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="H91" t="n">
-        <v>84704</v>
+        <v>85128</v>
       </c>
       <c r="I91" t="n">
-        <v>3.556</v>
+        <v>3.574</v>
       </c>
       <c r="J91" t="n">
-        <v>124</v>
+        <v>166</v>
       </c>
       <c r="K91" t="n">
-        <v>0.005</v>
+        <v>0.007</v>
       </c>
       <c r="L91" t="n">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="M91" t="n">
         <v>0.008</v>
       </c>
       <c r="N91" t="n">
-        <v>0.003</v>
+        <v>0.004</v>
       </c>
       <c r="O91" t="n">
-        <v>318.5</v>
+        <v>260.4</v>
       </c>
       <c r="P91" t="s">
         <v>548</v>
@@ -7676,7 +7684,7 @@
         <v>551</v>
       </c>
       <c r="C92" s="1" t="n">
-        <v>44059</v>
+        <v>44061</v>
       </c>
       <c r="D92" t="s">
         <v>552</v>
@@ -7686,31 +7694,31 @@
       </c>
       <c r="F92"/>
       <c r="G92" t="n">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="H92" t="n">
-        <v>394115</v>
+        <v>397276</v>
       </c>
       <c r="I92" t="n">
-        <v>5.646</v>
+        <v>5.692</v>
       </c>
       <c r="J92" t="n">
-        <v>998</v>
+        <v>1868</v>
       </c>
       <c r="K92" t="n">
-        <v>0.014</v>
+        <v>0.027</v>
       </c>
       <c r="L92" t="n">
-        <v>1026</v>
+        <v>1147</v>
       </c>
       <c r="M92" t="n">
-        <v>0.015</v>
+        <v>0.016</v>
       </c>
       <c r="N92" t="n">
-        <v>0.004</v>
+        <v>0.003</v>
       </c>
       <c r="O92" t="n">
-        <v>276.231</v>
+        <v>297.37</v>
       </c>
       <c r="P92" t="s">
         <v>553</v>
@@ -7733,7 +7741,7 @@
         <v>556</v>
       </c>
       <c r="C93" s="1" t="n">
-        <v>44059</v>
+        <v>44061</v>
       </c>
       <c r="D93" t="s">
         <v>552</v>
@@ -7743,31 +7751,31 @@
       </c>
       <c r="F93"/>
       <c r="G93" t="n">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="H93" t="n">
-        <v>782386</v>
+        <v>785547</v>
       </c>
       <c r="I93" t="n">
-        <v>11.209</v>
+        <v>11.254</v>
       </c>
       <c r="J93" t="n">
-        <v>998</v>
+        <v>1868</v>
       </c>
       <c r="K93" t="n">
-        <v>0.014</v>
+        <v>0.027</v>
       </c>
       <c r="L93" t="n">
-        <v>3417</v>
+        <v>1147</v>
       </c>
       <c r="M93" t="n">
-        <v>0.049</v>
+        <v>0.016</v>
       </c>
       <c r="N93" t="n">
-        <v>0.001</v>
+        <v>0.003</v>
       </c>
       <c r="O93" t="n">
-        <v>919.962</v>
+        <v>297.37</v>
       </c>
       <c r="P93" t="s">
         <v>553</v>
@@ -7847,7 +7855,7 @@
         <v>565</v>
       </c>
       <c r="C95" s="1" t="n">
-        <v>44057</v>
+        <v>44059</v>
       </c>
       <c r="D95" t="s">
         <v>566</v>
@@ -7857,31 +7865,31 @@
       </c>
       <c r="F95"/>
       <c r="G95" t="n">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="H95" t="n">
-        <v>109697</v>
+        <v>112048</v>
       </c>
       <c r="I95" t="n">
-        <v>9.282</v>
+        <v>9.481</v>
       </c>
       <c r="J95" t="n">
-        <v>1508</v>
+        <v>1404</v>
       </c>
       <c r="K95" t="n">
-        <v>0.128</v>
+        <v>0.119</v>
       </c>
       <c r="L95" t="n">
-        <v>1188</v>
+        <v>1292</v>
       </c>
       <c r="M95" t="n">
-        <v>0.101</v>
+        <v>0.109</v>
       </c>
       <c r="N95" t="n">
-        <v>0.025</v>
+        <v>0.038</v>
       </c>
       <c r="O95" t="n">
-        <v>40.566</v>
+        <v>26.214</v>
       </c>
       <c r="P95" t="s">
         <v>567</v>
@@ -7904,7 +7912,7 @@
         <v>570</v>
       </c>
       <c r="C96" s="1" t="n">
-        <v>44059</v>
+        <v>44061</v>
       </c>
       <c r="D96" t="s">
         <v>571</v>
@@ -7914,31 +7922,31 @@
       </c>
       <c r="F96"/>
       <c r="G96" t="n">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="H96" t="n">
-        <v>5725242</v>
+        <v>5882406</v>
       </c>
       <c r="I96" t="n">
-        <v>67.884</v>
+        <v>69.747</v>
       </c>
       <c r="J96" t="n">
-        <v>65956</v>
+        <v>82318</v>
       </c>
       <c r="K96" t="n">
-        <v>0.782</v>
+        <v>0.976</v>
       </c>
       <c r="L96" t="n">
-        <v>65918</v>
+        <v>70665</v>
       </c>
       <c r="M96" t="n">
-        <v>0.782</v>
+        <v>0.838</v>
       </c>
       <c r="N96" t="n">
-        <v>0.018</v>
+        <v>0.017</v>
       </c>
       <c r="O96" t="n">
-        <v>54.317</v>
+        <v>57.888</v>
       </c>
       <c r="P96" t="s">
         <v>572</v>
@@ -7961,7 +7969,7 @@
         <v>575</v>
       </c>
       <c r="C97" s="1" t="n">
-        <v>44056</v>
+        <v>44060</v>
       </c>
       <c r="D97" t="s">
         <v>576</v>
@@ -7971,31 +7979,31 @@
       </c>
       <c r="F97"/>
       <c r="G97" t="n">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="H97" t="n">
-        <v>312792</v>
+        <v>329542</v>
       </c>
       <c r="I97" t="n">
-        <v>6.838</v>
+        <v>7.205</v>
       </c>
       <c r="J97" t="n">
-        <v>4289</v>
+        <v>3905</v>
       </c>
       <c r="K97" t="n">
-        <v>0.094</v>
+        <v>0.085</v>
       </c>
       <c r="L97" t="n">
-        <v>3156</v>
+        <v>4037</v>
       </c>
       <c r="M97" t="n">
-        <v>0.069</v>
+        <v>0.088</v>
       </c>
       <c r="N97" t="n">
-        <v>0.005</v>
+        <v>0.008</v>
       </c>
       <c r="O97" t="n">
-        <v>185.647</v>
+        <v>130.226</v>
       </c>
       <c r="P97" t="s">
         <v>577</v>
@@ -8018,7 +8026,7 @@
         <v>581</v>
       </c>
       <c r="C98" s="1" t="n">
-        <v>44060</v>
+        <v>44062</v>
       </c>
       <c r="D98" t="s">
         <v>582</v>
@@ -8028,31 +8036,31 @@
       </c>
       <c r="F98"/>
       <c r="G98" t="n">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="H98" t="n">
-        <v>1300289</v>
+        <v>1335000</v>
       </c>
       <c r="I98" t="n">
-        <v>29.732</v>
+        <v>30.526</v>
       </c>
       <c r="J98" t="n">
-        <v>10700</v>
+        <v>19591</v>
       </c>
       <c r="K98" t="n">
-        <v>0.245</v>
+        <v>0.448</v>
       </c>
       <c r="L98" t="n">
-        <v>17265</v>
+        <v>17151</v>
       </c>
       <c r="M98" t="n">
-        <v>0.395</v>
+        <v>0.392</v>
       </c>
       <c r="N98" t="n">
-        <v>0.09</v>
+        <v>0.082</v>
       </c>
       <c r="O98" t="n">
-        <v>11.125</v>
+        <v>12.142</v>
       </c>
       <c r="P98" t="s">
         <v>583</v>
@@ -8075,7 +8083,7 @@
         <v>587</v>
       </c>
       <c r="C99" s="1" t="n">
-        <v>44059</v>
+        <v>44061</v>
       </c>
       <c r="D99" t="s">
         <v>588</v>
@@ -8085,31 +8093,31 @@
       </c>
       <c r="F99"/>
       <c r="G99" t="n">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="H99" t="n">
-        <v>5990528</v>
+        <v>6121609</v>
       </c>
       <c r="I99" t="n">
-        <v>605.691</v>
+        <v>618.945</v>
       </c>
       <c r="J99" t="n">
-        <v>65186</v>
+        <v>59759</v>
       </c>
       <c r="K99" t="n">
-        <v>6.591</v>
+        <v>6.042</v>
       </c>
       <c r="L99" t="n">
-        <v>69975</v>
+        <v>71121</v>
       </c>
       <c r="M99" t="n">
-        <v>7.075</v>
+        <v>7.191</v>
       </c>
       <c r="N99" t="n">
         <v>0.004</v>
       </c>
       <c r="O99" t="n">
-        <v>271.823</v>
+        <v>271.011</v>
       </c>
       <c r="P99" t="s">
         <v>589</v>
@@ -8132,7 +8140,7 @@
         <v>592</v>
       </c>
       <c r="C100" s="1" t="n">
-        <v>44058</v>
+        <v>44060</v>
       </c>
       <c r="D100" t="s">
         <v>593</v>
@@ -8144,31 +8152,31 @@
         <v>595</v>
       </c>
       <c r="G100" t="n">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="H100" t="n">
-        <v>11814098</v>
+        <v>12118924</v>
       </c>
       <c r="I100" t="n">
-        <v>174.028</v>
+        <v>178.519</v>
       </c>
       <c r="J100" t="n">
-        <v>174914</v>
+        <v>140608</v>
       </c>
       <c r="K100" t="n">
-        <v>2.577</v>
+        <v>2.071</v>
       </c>
       <c r="L100" t="n">
-        <v>158675</v>
+        <v>160768</v>
       </c>
       <c r="M100" t="n">
-        <v>2.337</v>
+        <v>2.368</v>
       </c>
       <c r="N100" t="n">
         <v>0.007</v>
       </c>
       <c r="O100" t="n">
-        <v>150.873</v>
+        <v>146.935</v>
       </c>
       <c r="P100" t="s">
         <v>594</v>
@@ -8248,7 +8256,7 @@
         <v>604</v>
       </c>
       <c r="C102" s="1" t="n">
-        <v>44059</v>
+        <v>44061</v>
       </c>
       <c r="D102" t="s">
         <v>605</v>
@@ -8258,31 +8266,31 @@
       </c>
       <c r="F102"/>
       <c r="G102" t="n">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="H102" t="n">
-        <v>66969790</v>
+        <v>68263933</v>
       </c>
       <c r="I102" t="n">
-        <v>202.324</v>
+        <v>206.234</v>
       </c>
       <c r="J102" t="n">
-        <v>777569</v>
+        <v>642814</v>
       </c>
       <c r="K102" t="n">
-        <v>2.349</v>
+        <v>1.942</v>
       </c>
       <c r="L102" t="n">
-        <v>738978</v>
+        <v>715954</v>
       </c>
       <c r="M102" t="n">
-        <v>2.233</v>
+        <v>2.163</v>
       </c>
       <c r="N102" t="n">
-        <v>0.07</v>
+        <v>0.069</v>
       </c>
       <c r="O102" t="n">
-        <v>14.244</v>
+        <v>14.572</v>
       </c>
       <c r="P102" t="s">
         <v>606</v>
@@ -8415,7 +8423,7 @@
         <v>622</v>
       </c>
       <c r="C105" s="1" t="n">
-        <v>44056</v>
+        <v>44059</v>
       </c>
       <c r="D105" t="s">
         <v>623</v>
@@ -8425,31 +8433,31 @@
       </c>
       <c r="F105"/>
       <c r="G105" t="n">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="H105" t="n">
-        <v>78738</v>
+        <v>82884</v>
       </c>
       <c r="I105" t="n">
-        <v>5.298</v>
+        <v>5.577</v>
       </c>
       <c r="J105" t="n">
-        <v>1108</v>
+        <v>1546</v>
       </c>
       <c r="K105" t="n">
-        <v>0.075</v>
+        <v>0.104</v>
       </c>
       <c r="L105" t="n">
-        <v>1514</v>
+        <v>1611</v>
       </c>
       <c r="M105" t="n">
-        <v>0.102</v>
+        <v>0.108</v>
       </c>
       <c r="N105" t="n">
-        <v>0.052</v>
+        <v>0.053</v>
       </c>
       <c r="O105" t="n">
-        <v>19.13</v>
+        <v>18.764</v>
       </c>
       <c r="P105" t="s">
         <v>624</v>

</xml_diff>

<commit_message>
Updated testing data for 2020-08-21
</commit_message>
<xml_diff>
--- a/public/data/testing/covid-testing-latest-data-source-details.xlsx
+++ b/public/data/testing/covid-testing-latest-data-source-details.xlsx
@@ -110,7 +110,7 @@
     <t xml:space="preserve">Australia - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.health.gov.au/sites/default/files/documents/2020/08/coronavirus-covid-19-at-a-glance-19-august-2020.pdf</t>
+    <t xml:space="preserve">https://www.health.gov.au/sites/default/files/documents/2020/08/coronavirus-covid-19-at-a-glance-20-august-2020.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">Australian Government Department of Health</t>
@@ -397,7 +397,7 @@
     <t xml:space="preserve">Cote d'Ivoire - samples tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.facebook.com/Mshpci/posts/1672992029533151</t>
+    <t xml:space="preserve">https://www.facebook.com/Mshpci/posts/1673896616109359</t>
   </si>
   <si>
     <t xml:space="preserve">Ministry of Health and Public Hygiene</t>
@@ -494,7 +494,7 @@
     <t xml:space="preserve">Denmark - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://files.ssi.dk/Data-Epidemiologiske-Rapport-19082020-aa6p</t>
+    <t xml:space="preserve">https://files.ssi.dk/Data-Epidemiologiske-Rapport-20082020-jh34</t>
   </si>
   <si>
     <t xml:space="preserve">Statens Serum Institut</t>
@@ -538,7 +538,7 @@
     <t xml:space="preserve">El Salvador - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.facebook.com/nayibbukele/posts/3155527237866779</t>
+    <t xml:space="preserve">https://www.facebook.com/nayibbukele/posts/3164190897000413</t>
   </si>
   <si>
     <t xml:space="preserve">Government of El Salvador</t>
@@ -582,13 +582,13 @@
     <t xml:space="preserve">Ethiopia - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.ephi.gov.et/images/novel_coronavirus/EPHI_%20PHEOC_COVID-19_Weekly%20%20bulletin_15_English_08102020.pdf</t>
+    <t xml:space="preserve">https://twitter.com/EPHIEthiopia/status/1296485928240918531</t>
   </si>
   <si>
     <t xml:space="preserve">Ethiopian Public Health Institute</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.ephi.gov.et</t>
+    <t xml:space="preserve">https://twitter.com/EPHIEthiopia</t>
   </si>
   <si>
     <t xml:space="preserve">The [Ethiopian Public Health Institute](https://www.ephi.gov.et) in collaboration with the [Ethiopian Ministry of Health](http://www.moh.gov.et) provides daily press releases of the number of tests performed to date. It is unclear whether the reported figures include tests for which the results are pending.
@@ -890,7 +890,7 @@
     <t xml:space="preserve">Iran - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">http://irangov.ir/detail/345469</t>
+    <t xml:space="preserve">http://irangov.ir/detail/345517</t>
   </si>
   <si>
     <t xml:space="preserve">Government of Iran</t>
@@ -948,7 +948,7 @@
     <t xml:space="preserve">Israel - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://govextra.gov.il/media/24691/covid-19-data-israel-12082020.xlsx</t>
+    <t xml:space="preserve">https://govextra.gov.il/media/24739/covid-19-data-israel-13082020.csv</t>
   </si>
   <si>
     <t xml:space="preserve">Israel Ministry of Health</t>
@@ -1007,7 +1007,7 @@
     <t xml:space="preserve">Japan - people tested (incl. non-PCR)</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.mhlw.go.jp/stf/newpage_13047.html</t>
+    <t xml:space="preserve">https://www.mhlw.go.jp/stf/newpage_13073.html</t>
   </si>
   <si>
     <t xml:space="preserve">Ministry of Health, Labor and Welfare Press Release</t>
@@ -1032,7 +1032,7 @@
     <t xml:space="preserve">Japan - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.mhlw.go.jp/content/10906000/000660649.pdf</t>
+    <t xml:space="preserve">https://www.mhlw.go.jp/content/10906000/000661150.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">The cumulative total reported in the press release matches the cumulative total calculated from the weekly and daily figures reported by the MOH.</t>
@@ -1066,7 +1066,7 @@
     <t xml:space="preserve">Kenya - samples tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/MOH_Kenya/status/1295334203220008960</t>
+    <t xml:space="preserve">https://twitter.com/MOH_Kenya/status/1295717267376943106</t>
   </si>
   <si>
     <t xml:space="preserve">Kenya Ministry of Health</t>
@@ -1154,7 +1154,7 @@
     <t xml:space="preserve">Malaysia - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">http://covid-19.moh.gov.my/terkini/082020/situasi-terkini-19-ogos-2020</t>
+    <t xml:space="preserve">http://covid-19.moh.gov.my/terkini/082020/situasi-terkini-20-ogos-2020</t>
   </si>
   <si>
     <t xml:space="preserve">Ministry of Health Malaysia</t>
@@ -1469,7 +1469,7 @@
     <t xml:space="preserve">Peru - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.dge.gob.pe/portal/docs/tools/coronavirus/coronavirus140820.pdf</t>
+    <t xml:space="preserve">https://www.dge.gob.pe/portal/docs/tools/coronavirus/coronavirus180820.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">Peru Ministry of Health</t>
@@ -1510,7 +1510,7 @@
     <t xml:space="preserve">Poland - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/MZ_GOV_PL/status/1296009007744901120</t>
+    <t xml:space="preserve">https://twitter.com/MZ_GOV_PL/status/1296371398386913281</t>
   </si>
   <si>
     <t xml:space="preserve">Poland Ministry of Health</t>
@@ -1601,7 +1601,7 @@
     <t xml:space="preserve">Russia - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://rospotrebnadzor.ru/about/info/news/news_details.php?ELEMENT_ID=15203</t>
+    <t xml:space="preserve">https://rospotrebnadzor.ru/about/info/news/news_details.php?ELEMENT_ID=15210</t>
   </si>
   <si>
     <t xml:space="preserve">Government of the Russian Federation</t>
@@ -1621,7 +1621,7 @@
     <t xml:space="preserve">Rwanda - samples tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/RwandaHealth/status/1295093748729352192</t>
+    <t xml:space="preserve">https://twitter.com/RwandaHealth/status/1296181973946425350</t>
   </si>
   <si>
     <t xml:space="preserve">Rwanda Ministry of Health</t>
@@ -1917,7 +1917,7 @@
     <t xml:space="preserve">Thailand - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://ddc.moph.go.th/viralpneumonia/file/situation/situation-no229-190863.pdf</t>
+    <t xml:space="preserve">https://ddc.moph.go.th/viralpneumonia/file/situation/situation-no230-200863.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">Department of Disease Control</t>
@@ -2005,7 +2005,7 @@
     <t xml:space="preserve">Uganda - samples tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/MinofHealthUG/status/1296074539823177728/photo/2</t>
+    <t xml:space="preserve">https://twitter.com/MinofHealthUG/status/1296425945960767489/photo/2</t>
   </si>
   <si>
     <t xml:space="preserve">Uganda Ministry of Health</t>
@@ -2065,7 +2065,7 @@
     <t xml:space="preserve">United Kingdom - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://assets.publishing.service.gov.uk/government/uploads/system/uploads/attachment_data/file/910491/2020-08-19_COVID-19_UK_testing_time_series.csv</t>
+    <t xml:space="preserve">https://assets.publishing.service.gov.uk/government/uploads/system/uploads/attachment_data/file/910857/2020-08-20_COVID-19_UK_testing_time_series.csv</t>
   </si>
   <si>
     <t xml:space="preserve">Public Health England/Department of Health and Social Care</t>
@@ -2145,7 +2145,7 @@
     <t xml:space="preserve">Uruguay - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.gub.uy/ministerio-salud-publica/comunicacion/noticias/informe-situacion-sobre-coronavirus-covid-19-uruguay-19-agosto</t>
+    <t xml:space="preserve">https://www.gub.uy/ministerio-salud-publica/comunicacion/noticias/informe-situacion-sobre-coronavirus-covid-19-uruguay-20-agosto</t>
   </si>
   <si>
     <t xml:space="preserve">https://www.gub.uy/ministerio-salud-publica/comunicacion/noticias</t>
@@ -2183,7 +2183,7 @@
     <t xml:space="preserve">Zimbabwe - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/MoHCCZim/status/1295057062544781315</t>
+    <t xml:space="preserve">https://twitter.com/MoHCCZim/status/1296519577103466508</t>
   </si>
   <si>
     <t xml:space="preserve">Zimbabwe Ministry of Health and Child Care</t>
@@ -2600,7 +2600,7 @@
         <v>20</v>
       </c>
       <c r="C2" s="1" t="n">
-        <v>44062</v>
+        <v>44063</v>
       </c>
       <c r="D2" t="s">
         <v>21</v>
@@ -2610,31 +2610,31 @@
       </c>
       <c r="F2"/>
       <c r="G2" t="n">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="H2" t="n">
-        <v>882176</v>
+        <v>901255</v>
       </c>
       <c r="I2" t="n">
-        <v>19.519</v>
+        <v>19.941</v>
       </c>
       <c r="J2" t="n">
-        <v>4027</v>
+        <v>4391</v>
       </c>
       <c r="K2" t="n">
-        <v>0.089</v>
+        <v>0.097</v>
       </c>
       <c r="L2" t="n">
-        <v>10986</v>
+        <v>11114</v>
       </c>
       <c r="M2" t="n">
-        <v>0.243</v>
+        <v>0.246</v>
       </c>
       <c r="N2" t="n">
-        <v>0.589</v>
+        <v>0.579</v>
       </c>
       <c r="O2" t="n">
-        <v>1.699</v>
+        <v>1.727</v>
       </c>
       <c r="P2" t="s">
         <v>22</v>
@@ -2657,7 +2657,7 @@
         <v>25</v>
       </c>
       <c r="C3" s="1" t="n">
-        <v>44062</v>
+        <v>44063</v>
       </c>
       <c r="D3" t="s">
         <v>26</v>
@@ -2667,31 +2667,31 @@
       </c>
       <c r="F3"/>
       <c r="G3" t="n">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="H3" t="n">
-        <v>1072406</v>
+        <v>1095233</v>
       </c>
       <c r="I3" t="n">
-        <v>23.728</v>
+        <v>24.233</v>
       </c>
       <c r="J3" t="n">
-        <v>5483</v>
+        <v>5714</v>
       </c>
       <c r="K3" t="n">
-        <v>0.121</v>
+        <v>0.126</v>
       </c>
       <c r="L3" t="n">
-        <v>13017</v>
+        <v>13231</v>
       </c>
       <c r="M3" t="n">
-        <v>0.288</v>
+        <v>0.293</v>
       </c>
       <c r="N3" t="n">
-        <v>0.497</v>
+        <v>0.486</v>
       </c>
       <c r="O3" t="n">
-        <v>2.013</v>
+        <v>2.056</v>
       </c>
       <c r="P3" t="s">
         <v>22</v>
@@ -2714,7 +2714,7 @@
         <v>30</v>
       </c>
       <c r="C4" s="1" t="n">
-        <v>44062</v>
+        <v>44063</v>
       </c>
       <c r="D4" t="s">
         <v>31</v>
@@ -2724,22 +2724,22 @@
       </c>
       <c r="F4"/>
       <c r="G4" t="n">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="H4" t="n">
-        <v>5440495</v>
+        <v>5508831</v>
       </c>
       <c r="I4" t="n">
-        <v>213.354</v>
+        <v>216.034</v>
       </c>
       <c r="J4" t="n">
-        <v>59882</v>
+        <v>68336</v>
       </c>
       <c r="K4" t="n">
-        <v>2.348</v>
+        <v>2.68</v>
       </c>
       <c r="L4" t="n">
-        <v>57022</v>
+        <v>57007</v>
       </c>
       <c r="M4" t="n">
         <v>2.236</v>
@@ -2748,7 +2748,7 @@
         <v>0.005</v>
       </c>
       <c r="O4" t="n">
-        <v>193.764</v>
+        <v>213.853</v>
       </c>
       <c r="P4" t="s">
         <v>32</v>
@@ -2828,7 +2828,7 @@
         <v>43</v>
       </c>
       <c r="C6" s="1" t="n">
-        <v>44062</v>
+        <v>44064</v>
       </c>
       <c r="D6" t="s">
         <v>44</v>
@@ -2838,32 +2838,24 @@
       </c>
       <c r="F6"/>
       <c r="G6" t="n">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="H6" t="n">
-        <v>1000787</v>
+        <v>1011805</v>
       </c>
       <c r="I6" t="n">
-        <v>588.151</v>
-      </c>
-      <c r="J6" t="n">
-        <v>19579</v>
-      </c>
-      <c r="K6" t="n">
-        <v>11.506</v>
-      </c>
+        <v>594.626</v>
+      </c>
+      <c r="J6"/>
+      <c r="K6"/>
       <c r="L6" t="n">
-        <v>9575</v>
+        <v>9572</v>
       </c>
       <c r="M6" t="n">
-        <v>5.627</v>
-      </c>
-      <c r="N6" t="n">
-        <v>0.036</v>
-      </c>
-      <c r="O6" t="n">
-        <v>28.15</v>
-      </c>
+        <v>5.625</v>
+      </c>
+      <c r="N6"/>
+      <c r="O6"/>
       <c r="P6" t="s">
         <v>46</v>
       </c>
@@ -2885,7 +2877,7 @@
         <v>50</v>
       </c>
       <c r="C7" s="1" t="n">
-        <v>44058</v>
+        <v>44061</v>
       </c>
       <c r="D7" t="s">
         <v>51</v>
@@ -2895,31 +2887,31 @@
       </c>
       <c r="F7"/>
       <c r="G7" t="n">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="H7" t="n">
-        <v>1341648</v>
+        <v>1378819</v>
       </c>
       <c r="I7" t="n">
-        <v>8.147</v>
+        <v>8.372</v>
       </c>
       <c r="J7" t="n">
-        <v>12891</v>
+        <v>14630</v>
       </c>
       <c r="K7" t="n">
-        <v>0.078</v>
+        <v>0.089</v>
       </c>
       <c r="L7" t="n">
-        <v>13155</v>
+        <v>12976</v>
       </c>
       <c r="M7" t="n">
-        <v>0.08</v>
+        <v>0.079</v>
       </c>
       <c r="N7" t="n">
-        <v>0.21</v>
+        <v>0.205</v>
       </c>
       <c r="O7" t="n">
-        <v>4.752</v>
+        <v>4.874</v>
       </c>
       <c r="P7" t="s">
         <v>52</v>
@@ -2999,7 +2991,7 @@
         <v>63</v>
       </c>
       <c r="C9" s="1" t="n">
-        <v>44061</v>
+        <v>44062</v>
       </c>
       <c r="D9" t="s">
         <v>64</v>
@@ -3009,31 +3001,31 @@
       </c>
       <c r="F9"/>
       <c r="G9" t="n">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="H9" t="n">
-        <v>2049288</v>
+        <v>2072738</v>
       </c>
       <c r="I9" t="n">
-        <v>176.821</v>
+        <v>178.844</v>
       </c>
       <c r="J9" t="n">
-        <v>22858</v>
+        <v>18492</v>
       </c>
       <c r="K9" t="n">
-        <v>1.972</v>
+        <v>1.596</v>
       </c>
       <c r="L9" t="n">
-        <v>17725</v>
+        <v>17796</v>
       </c>
       <c r="M9" t="n">
-        <v>1.529</v>
+        <v>1.536</v>
       </c>
       <c r="N9" t="n">
-        <v>0.027</v>
+        <v>0.023</v>
       </c>
       <c r="O9" t="n">
-        <v>36.418</v>
+        <v>44.363</v>
       </c>
       <c r="P9" t="s">
         <v>65</v>
@@ -3164,7 +3156,7 @@
         <v>81</v>
       </c>
       <c r="C12" s="1" t="n">
-        <v>44063</v>
+        <v>44064</v>
       </c>
       <c r="D12" t="s">
         <v>82</v>
@@ -3174,32 +3166,28 @@
       </c>
       <c r="F12"/>
       <c r="G12" t="n">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="H12" t="n">
-        <v>351879</v>
+        <v>358723</v>
       </c>
       <c r="I12" t="n">
-        <v>50.641</v>
+        <v>51.626</v>
       </c>
       <c r="J12" t="n">
-        <v>8649</v>
+        <v>6844</v>
       </c>
       <c r="K12" t="n">
-        <v>1.245</v>
+        <v>0.985</v>
       </c>
       <c r="L12" t="n">
-        <v>4701</v>
+        <v>4839</v>
       </c>
       <c r="M12" t="n">
-        <v>0.677</v>
-      </c>
-      <c r="N12" t="n">
-        <v>0.024</v>
-      </c>
-      <c r="O12" t="n">
-        <v>42.406</v>
-      </c>
+        <v>0.696</v>
+      </c>
+      <c r="N12"/>
+      <c r="O12"/>
       <c r="P12" t="s">
         <v>84</v>
       </c>
@@ -3221,7 +3209,7 @@
         <v>87</v>
       </c>
       <c r="C13" s="1" t="n">
-        <v>44063</v>
+        <v>44064</v>
       </c>
       <c r="D13" t="s">
         <v>88</v>
@@ -3231,32 +3219,28 @@
       </c>
       <c r="F13"/>
       <c r="G13" t="n">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="H13" t="n">
-        <v>4925446</v>
+        <v>4974215</v>
       </c>
       <c r="I13" t="n">
-        <v>130.503</v>
+        <v>131.795</v>
       </c>
       <c r="J13" t="n">
-        <v>45274</v>
+        <v>48769</v>
       </c>
       <c r="K13" t="n">
-        <v>1.2</v>
+        <v>1.292</v>
       </c>
       <c r="L13" t="n">
-        <v>49195</v>
+        <v>48444</v>
       </c>
       <c r="M13" t="n">
-        <v>1.303</v>
-      </c>
-      <c r="N13" t="n">
-        <v>0.008</v>
-      </c>
-      <c r="O13" t="n">
-        <v>129.412</v>
-      </c>
+        <v>1.284</v>
+      </c>
+      <c r="N13"/>
+      <c r="O13"/>
       <c r="P13" t="s">
         <v>89</v>
       </c>
@@ -3278,7 +3262,7 @@
         <v>92</v>
       </c>
       <c r="C14" s="1" t="n">
-        <v>44062</v>
+        <v>44063</v>
       </c>
       <c r="D14" t="s">
         <v>93</v>
@@ -3290,31 +3274,31 @@
         <v>94</v>
       </c>
       <c r="G14" t="n">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="H14" t="n">
-        <v>2087354</v>
+        <v>2113632</v>
       </c>
       <c r="I14" t="n">
-        <v>109.193</v>
+        <v>110.568</v>
       </c>
       <c r="J14" t="n">
-        <v>19275</v>
+        <v>26278</v>
       </c>
       <c r="K14" t="n">
-        <v>1.008</v>
+        <v>1.375</v>
       </c>
       <c r="L14" t="n">
-        <v>25484</v>
+        <v>25863</v>
       </c>
       <c r="M14" t="n">
-        <v>1.333</v>
+        <v>1.353</v>
       </c>
       <c r="N14" t="n">
-        <v>0.069</v>
+        <v>0.066</v>
       </c>
       <c r="O14" t="n">
-        <v>14.575</v>
+        <v>15.253</v>
       </c>
       <c r="P14" t="s">
         <v>95</v>
@@ -3337,7 +3321,7 @@
         <v>99</v>
       </c>
       <c r="C15" s="1" t="n">
-        <v>44061</v>
+        <v>44063</v>
       </c>
       <c r="D15" t="s">
         <v>100</v>
@@ -3347,31 +3331,31 @@
       </c>
       <c r="F15"/>
       <c r="G15" t="n">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="H15" t="n">
-        <v>2246595</v>
+        <v>2309447</v>
       </c>
       <c r="I15" t="n">
-        <v>44.152</v>
+        <v>45.388</v>
       </c>
       <c r="J15" t="n">
-        <v>35883</v>
+        <v>31932</v>
       </c>
       <c r="K15" t="n">
-        <v>0.705</v>
+        <v>0.628</v>
       </c>
       <c r="L15" t="n">
-        <v>37681</v>
+        <v>35159</v>
       </c>
       <c r="M15" t="n">
-        <v>0.741</v>
+        <v>0.691</v>
       </c>
       <c r="N15" t="n">
-        <v>0.3</v>
+        <v>0.324</v>
       </c>
       <c r="O15" t="n">
-        <v>3.337</v>
+        <v>3.09</v>
       </c>
       <c r="P15" t="s">
         <v>101</v>
@@ -3394,7 +3378,7 @@
         <v>105</v>
       </c>
       <c r="C16" s="1" t="n">
-        <v>44061</v>
+        <v>44062</v>
       </c>
       <c r="D16" t="s">
         <v>106</v>
@@ -3404,25 +3388,25 @@
       </c>
       <c r="F16"/>
       <c r="G16" t="n">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="H16" t="n">
-        <v>107672</v>
+        <v>109207</v>
       </c>
       <c r="I16" t="n">
-        <v>21.137</v>
+        <v>21.438</v>
       </c>
       <c r="J16" t="n">
-        <v>1059</v>
+        <v>1535</v>
       </c>
       <c r="K16" t="n">
-        <v>0.208</v>
+        <v>0.301</v>
       </c>
       <c r="L16" t="n">
-        <v>1838</v>
+        <v>1820</v>
       </c>
       <c r="M16" t="n">
-        <v>0.361</v>
+        <v>0.357</v>
       </c>
       <c r="N16"/>
       <c r="O16"/>
@@ -3447,7 +3431,7 @@
         <v>111</v>
       </c>
       <c r="C17" s="1" t="n">
-        <v>44061</v>
+        <v>44062</v>
       </c>
       <c r="D17" t="s">
         <v>112</v>
@@ -3457,31 +3441,31 @@
       </c>
       <c r="F17"/>
       <c r="G17" t="n">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="H17" t="n">
-        <v>115338</v>
+        <v>116785</v>
       </c>
       <c r="I17" t="n">
-        <v>4.372</v>
+        <v>4.427</v>
       </c>
       <c r="J17" t="n">
-        <v>918</v>
+        <v>1447</v>
       </c>
       <c r="K17" t="n">
-        <v>0.035</v>
+        <v>0.055</v>
       </c>
       <c r="L17" t="n">
-        <v>711</v>
+        <v>882</v>
       </c>
       <c r="M17" t="n">
-        <v>0.027</v>
+        <v>0.033</v>
       </c>
       <c r="N17" t="n">
-        <v>0.046</v>
+        <v>0.049</v>
       </c>
       <c r="O17" t="n">
-        <v>21.829</v>
+        <v>20.376</v>
       </c>
       <c r="P17" t="s">
         <v>113</v>
@@ -3504,7 +3488,7 @@
         <v>117</v>
       </c>
       <c r="C18" s="1" t="n">
-        <v>44062</v>
+        <v>44063</v>
       </c>
       <c r="D18" t="s">
         <v>118</v>
@@ -3514,31 +3498,31 @@
       </c>
       <c r="F18"/>
       <c r="G18" t="n">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="H18" t="n">
-        <v>142124</v>
+        <v>144521</v>
       </c>
       <c r="I18" t="n">
-        <v>34.62</v>
+        <v>35.204</v>
       </c>
       <c r="J18" t="n">
-        <v>1653</v>
+        <v>2397</v>
       </c>
       <c r="K18" t="n">
-        <v>0.403</v>
+        <v>0.584</v>
       </c>
       <c r="L18" t="n">
-        <v>1405</v>
+        <v>1575</v>
       </c>
       <c r="M18" t="n">
-        <v>0.342</v>
+        <v>0.384</v>
       </c>
       <c r="N18" t="n">
-        <v>0.113</v>
+        <v>0.109</v>
       </c>
       <c r="O18" t="n">
-        <v>8.821</v>
+        <v>9.157</v>
       </c>
       <c r="P18" t="s">
         <v>119</v>
@@ -3561,7 +3545,7 @@
         <v>123</v>
       </c>
       <c r="C19" s="1" t="n">
-        <v>44061</v>
+        <v>44062</v>
       </c>
       <c r="D19" t="s">
         <v>124</v>
@@ -3573,31 +3557,31 @@
         <v>126</v>
       </c>
       <c r="G19" t="n">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="H19" t="n">
-        <v>341323</v>
+        <v>346439</v>
       </c>
       <c r="I19" t="n">
-        <v>30.135</v>
+        <v>30.586</v>
       </c>
       <c r="J19" t="n">
-        <v>4990</v>
+        <v>5116</v>
       </c>
       <c r="K19" t="n">
-        <v>0.441</v>
+        <v>0.452</v>
       </c>
       <c r="L19" t="n">
-        <v>4488</v>
+        <v>4563</v>
       </c>
       <c r="M19" t="n">
-        <v>0.396</v>
+        <v>0.403</v>
       </c>
       <c r="N19" t="n">
         <v>0.01</v>
       </c>
       <c r="O19" t="n">
-        <v>98.792</v>
+        <v>101.4</v>
       </c>
       <c r="P19" t="s">
         <v>125</v>
@@ -3620,7 +3604,7 @@
         <v>130</v>
       </c>
       <c r="C20" s="1" t="n">
-        <v>44061</v>
+        <v>44062</v>
       </c>
       <c r="D20" t="s">
         <v>131</v>
@@ -3630,31 +3614,31 @@
       </c>
       <c r="F20"/>
       <c r="G20" t="n">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="H20" t="n">
-        <v>812835</v>
+        <v>820151</v>
       </c>
       <c r="I20" t="n">
-        <v>75.902</v>
+        <v>76.585</v>
       </c>
       <c r="J20" t="n">
-        <v>7206</v>
+        <v>7185</v>
       </c>
       <c r="K20" t="n">
-        <v>0.673</v>
+        <v>0.671</v>
       </c>
       <c r="L20" t="n">
-        <v>6276</v>
+        <v>6237</v>
       </c>
       <c r="M20" t="n">
-        <v>0.586</v>
+        <v>0.582</v>
       </c>
       <c r="N20" t="n">
         <v>0.039</v>
       </c>
       <c r="O20" t="n">
-        <v>25.721</v>
+        <v>25.682</v>
       </c>
       <c r="P20" t="s">
         <v>45</v>
@@ -3730,7 +3714,7 @@
         <v>141</v>
       </c>
       <c r="C22" s="1" t="n">
-        <v>44061</v>
+        <v>44062</v>
       </c>
       <c r="D22" t="s">
         <v>142</v>
@@ -3740,31 +3724,31 @@
       </c>
       <c r="F22"/>
       <c r="G22" t="n">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="H22" t="n">
-        <v>1990371</v>
+        <v>2035007</v>
       </c>
       <c r="I22" t="n">
-        <v>343.629</v>
+        <v>351.336</v>
       </c>
       <c r="J22" t="n">
-        <v>7198</v>
+        <v>7704</v>
       </c>
       <c r="K22" t="n">
-        <v>1.243</v>
+        <v>1.33</v>
       </c>
       <c r="L22" t="n">
-        <v>26574</v>
+        <v>27990</v>
       </c>
       <c r="M22" t="n">
-        <v>4.588</v>
+        <v>4.832</v>
       </c>
       <c r="N22" t="n">
         <v>0.005</v>
       </c>
       <c r="O22" t="n">
-        <v>201.101</v>
+        <v>218.672</v>
       </c>
       <c r="P22" t="s">
         <v>143</v>
@@ -3842,7 +3826,7 @@
         <v>154</v>
       </c>
       <c r="C24" s="1" t="n">
-        <v>44059</v>
+        <v>44062</v>
       </c>
       <c r="D24" t="s">
         <v>155</v>
@@ -3852,31 +3836,31 @@
       </c>
       <c r="F24"/>
       <c r="G24" t="n">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="H24" t="n">
-        <v>280943</v>
+        <v>288307</v>
       </c>
       <c r="I24" t="n">
-        <v>43.314</v>
+        <v>44.449</v>
       </c>
       <c r="J24" t="n">
-        <v>2498</v>
+        <v>2414</v>
       </c>
       <c r="K24" t="n">
-        <v>0.385</v>
+        <v>0.372</v>
       </c>
       <c r="L24" t="n">
-        <v>2479</v>
+        <v>2464</v>
       </c>
       <c r="M24" t="n">
-        <v>0.382</v>
+        <v>0.38</v>
       </c>
       <c r="N24" t="n">
-        <v>0.152</v>
+        <v>0.127</v>
       </c>
       <c r="O24" t="n">
-        <v>6.571</v>
+        <v>7.865</v>
       </c>
       <c r="P24" t="s">
         <v>156</v>
@@ -3956,7 +3940,7 @@
         <v>168</v>
       </c>
       <c r="C26" s="1" t="n">
-        <v>44052</v>
+        <v>44063</v>
       </c>
       <c r="D26" t="s">
         <v>169</v>
@@ -3966,27 +3950,31 @@
       </c>
       <c r="F26"/>
       <c r="G26" t="n">
-        <v>74</v>
+        <v>85</v>
       </c>
       <c r="H26" t="n">
-        <v>497971</v>
+        <v>694093</v>
       </c>
       <c r="I26" t="n">
-        <v>4.332</v>
-      </c>
-      <c r="J26"/>
-      <c r="K26"/>
+        <v>6.038</v>
+      </c>
+      <c r="J26" t="n">
+        <v>21456</v>
+      </c>
+      <c r="K26" t="n">
+        <v>0.187</v>
+      </c>
       <c r="L26" t="n">
-        <v>8665</v>
+        <v>20568</v>
       </c>
       <c r="M26" t="n">
-        <v>0.075</v>
+        <v>0.179</v>
       </c>
       <c r="N26" t="n">
-        <v>0.07</v>
+        <v>0.062</v>
       </c>
       <c r="O26" t="n">
-        <v>14.258</v>
+        <v>16.105</v>
       </c>
       <c r="P26" t="s">
         <v>170</v>
@@ -4121,7 +4109,7 @@
         <v>185</v>
       </c>
       <c r="C29" s="1" t="n">
-        <v>44059</v>
+        <v>44060</v>
       </c>
       <c r="D29" t="s">
         <v>186</v>
@@ -4131,27 +4119,27 @@
       </c>
       <c r="F29"/>
       <c r="G29" t="n">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="H29"/>
       <c r="I29"/>
       <c r="J29" t="n">
-        <v>18138</v>
+        <v>127008</v>
       </c>
       <c r="K29" t="n">
-        <v>0.278</v>
+        <v>1.946</v>
       </c>
       <c r="L29" t="n">
-        <v>78267</v>
+        <v>82448</v>
       </c>
       <c r="M29" t="n">
-        <v>1.199</v>
+        <v>1.263</v>
       </c>
       <c r="N29" t="n">
-        <v>0.032</v>
+        <v>0.036</v>
       </c>
       <c r="O29" t="n">
-        <v>31.129</v>
+        <v>27.996</v>
       </c>
       <c r="P29" t="s">
         <v>187</v>
@@ -4284,7 +4272,7 @@
         <v>203</v>
       </c>
       <c r="C32" s="1" t="n">
-        <v>44060</v>
+        <v>44061</v>
       </c>
       <c r="D32" t="s">
         <v>204</v>
@@ -4294,31 +4282,31 @@
       </c>
       <c r="F32"/>
       <c r="G32" t="n">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="H32" t="n">
-        <v>429773</v>
+        <v>431272</v>
       </c>
       <c r="I32" t="n">
-        <v>13.831</v>
+        <v>13.879</v>
       </c>
       <c r="J32" t="n">
-        <v>1078</v>
+        <v>1499</v>
       </c>
       <c r="K32" t="n">
-        <v>0.035</v>
+        <v>0.048</v>
       </c>
       <c r="L32" t="n">
-        <v>1455</v>
+        <v>1383</v>
       </c>
       <c r="M32" t="n">
-        <v>0.047</v>
+        <v>0.045</v>
       </c>
       <c r="N32" t="n">
-        <v>0.15</v>
+        <v>0.149</v>
       </c>
       <c r="O32" t="n">
-        <v>6.661</v>
+        <v>6.718</v>
       </c>
       <c r="P32" t="s">
         <v>206</v>
@@ -4738,7 +4726,7 @@
         <v>250</v>
       </c>
       <c r="C40" s="1" t="n">
-        <v>44062</v>
+        <v>44063</v>
       </c>
       <c r="D40" t="s">
         <v>251</v>
@@ -4748,31 +4736,31 @@
       </c>
       <c r="F40"/>
       <c r="G40" t="n">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="H40" t="n">
-        <v>2939840</v>
+        <v>2963741</v>
       </c>
       <c r="I40" t="n">
-        <v>35.001</v>
+        <v>35.286</v>
       </c>
       <c r="J40" t="n">
-        <v>25791</v>
+        <v>23901</v>
       </c>
       <c r="K40" t="n">
-        <v>0.307</v>
+        <v>0.285</v>
       </c>
       <c r="L40" t="n">
-        <v>25231</v>
+        <v>25126</v>
       </c>
       <c r="M40" t="n">
-        <v>0.3</v>
+        <v>0.299</v>
       </c>
       <c r="N40" t="n">
-        <v>0.094</v>
+        <v>0.08</v>
       </c>
       <c r="O40" t="n">
-        <v>10.61</v>
+        <v>12.442</v>
       </c>
       <c r="P40" t="s">
         <v>252</v>
@@ -4852,7 +4840,7 @@
         <v>263</v>
       </c>
       <c r="C42" s="1" t="n">
-        <v>44062</v>
+        <v>44063</v>
       </c>
       <c r="D42" t="s">
         <v>264</v>
@@ -4862,31 +4850,31 @@
       </c>
       <c r="F42"/>
       <c r="G42" t="n">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="H42" t="n">
-        <v>735598</v>
+        <v>747521</v>
       </c>
       <c r="I42" t="n">
-        <v>148.973</v>
+        <v>151.388</v>
       </c>
       <c r="J42" t="n">
-        <v>5685</v>
+        <v>12416</v>
       </c>
       <c r="K42" t="n">
-        <v>1.151</v>
+        <v>2.514</v>
       </c>
       <c r="L42" t="n">
-        <v>7853</v>
+        <v>8546</v>
       </c>
       <c r="M42" t="n">
-        <v>1.59</v>
+        <v>1.731</v>
       </c>
       <c r="N42" t="n">
-        <v>0.013</v>
+        <v>0.012</v>
       </c>
       <c r="O42" t="n">
-        <v>78.755</v>
+        <v>84.375</v>
       </c>
       <c r="P42" t="s">
         <v>265</v>
@@ -4909,7 +4897,7 @@
         <v>268</v>
       </c>
       <c r="C43" s="1" t="n">
-        <v>44055</v>
+        <v>44056</v>
       </c>
       <c r="D43" t="s">
         <v>269</v>
@@ -4919,31 +4907,31 @@
       </c>
       <c r="F43"/>
       <c r="G43" t="n">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="H43" t="n">
-        <v>2021151</v>
+        <v>2050053</v>
       </c>
       <c r="I43" t="n">
-        <v>233.509</v>
+        <v>236.849</v>
       </c>
       <c r="J43" t="n">
-        <v>26229</v>
+        <v>28904</v>
       </c>
       <c r="K43" t="n">
-        <v>3.03</v>
+        <v>3.339</v>
       </c>
       <c r="L43" t="n">
-        <v>21872</v>
+        <v>21889</v>
       </c>
       <c r="M43" t="n">
-        <v>2.527</v>
+        <v>2.529</v>
       </c>
       <c r="N43" t="n">
         <v>0.067</v>
       </c>
       <c r="O43" t="n">
-        <v>14.84</v>
+        <v>14.978</v>
       </c>
       <c r="P43" t="s">
         <v>45</v>
@@ -4966,7 +4954,7 @@
         <v>274</v>
       </c>
       <c r="C44" s="1" t="n">
-        <v>44062</v>
+        <v>44063</v>
       </c>
       <c r="D44" t="s">
         <v>275</v>
@@ -4978,31 +4966,31 @@
         <v>277</v>
       </c>
       <c r="G44" t="n">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="H44" t="n">
-        <v>4551287</v>
+        <v>4600949</v>
       </c>
       <c r="I44" t="n">
-        <v>75.275</v>
+        <v>76.097</v>
       </c>
       <c r="J44" t="n">
-        <v>41290</v>
+        <v>49662</v>
       </c>
       <c r="K44" t="n">
-        <v>0.683</v>
+        <v>0.821</v>
       </c>
       <c r="L44" t="n">
-        <v>27751</v>
+        <v>31185</v>
       </c>
       <c r="M44" t="n">
-        <v>0.459</v>
+        <v>0.516</v>
       </c>
       <c r="N44" t="n">
-        <v>0.017</v>
+        <v>0.016</v>
       </c>
       <c r="O44" t="n">
-        <v>57.151</v>
+        <v>61.233</v>
       </c>
       <c r="P44" t="s">
         <v>278</v>
@@ -5025,7 +5013,7 @@
         <v>281</v>
       </c>
       <c r="C45" s="1" t="n">
-        <v>44062</v>
+        <v>44063</v>
       </c>
       <c r="D45" t="s">
         <v>275</v>
@@ -5037,31 +5025,31 @@
         <v>277</v>
       </c>
       <c r="G45" t="n">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="H45" t="n">
-        <v>7713154</v>
+        <v>7790596</v>
       </c>
       <c r="I45" t="n">
-        <v>127.571</v>
+        <v>128.851</v>
       </c>
       <c r="J45" t="n">
-        <v>71095</v>
+        <v>77442</v>
       </c>
       <c r="K45" t="n">
-        <v>1.176</v>
+        <v>1.281</v>
       </c>
       <c r="L45" t="n">
-        <v>49083</v>
+        <v>52833</v>
       </c>
       <c r="M45" t="n">
-        <v>0.812</v>
+        <v>0.874</v>
       </c>
       <c r="N45" t="n">
         <v>0.01</v>
       </c>
       <c r="O45" t="n">
-        <v>101.083</v>
+        <v>103.739</v>
       </c>
       <c r="P45" t="s">
         <v>278</v>
@@ -5084,7 +5072,7 @@
         <v>284</v>
       </c>
       <c r="C46" s="1" t="n">
-        <v>44062</v>
+        <v>44063</v>
       </c>
       <c r="D46" t="s">
         <v>285</v>
@@ -5096,31 +5084,31 @@
         <v>287</v>
       </c>
       <c r="G46" t="n">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="H46" t="n">
-        <v>1236180</v>
+        <v>1259422</v>
       </c>
       <c r="I46" t="n">
-        <v>9.774</v>
+        <v>9.958</v>
       </c>
       <c r="J46" t="n">
-        <v>22035</v>
+        <v>23242</v>
       </c>
       <c r="K46" t="n">
-        <v>0.174</v>
+        <v>0.184</v>
       </c>
       <c r="L46" t="n">
-        <v>25431</v>
+        <v>24871</v>
       </c>
       <c r="M46" t="n">
-        <v>0.201</v>
+        <v>0.197</v>
       </c>
       <c r="N46" t="n">
-        <v>0.045</v>
+        <v>0.046</v>
       </c>
       <c r="O46" t="n">
-        <v>22.147</v>
+        <v>21.608</v>
       </c>
       <c r="P46" t="s">
         <v>288</v>
@@ -5143,7 +5131,7 @@
         <v>291</v>
       </c>
       <c r="C47" s="1" t="n">
-        <v>44060</v>
+        <v>44061</v>
       </c>
       <c r="D47" t="s">
         <v>292</v>
@@ -5155,31 +5143,31 @@
         <v>293</v>
       </c>
       <c r="G47" t="n">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H47" t="n">
-        <v>1526180</v>
+        <v>1547172</v>
       </c>
       <c r="I47" t="n">
-        <v>12.067</v>
+        <v>12.233</v>
       </c>
       <c r="J47" t="n">
-        <v>21230</v>
+        <v>18957</v>
       </c>
       <c r="K47" t="n">
-        <v>0.168</v>
+        <v>0.15</v>
       </c>
       <c r="L47" t="n">
-        <v>21918</v>
+        <v>20690</v>
       </c>
       <c r="M47" t="n">
-        <v>0.173</v>
+        <v>0.164</v>
       </c>
       <c r="N47" t="n">
-        <v>0.045</v>
+        <v>0.053</v>
       </c>
       <c r="O47" t="n">
-        <v>22.038</v>
+        <v>18.76</v>
       </c>
       <c r="P47" t="s">
         <v>288</v>
@@ -5259,7 +5247,7 @@
         <v>301</v>
       </c>
       <c r="C49" s="1" t="n">
-        <v>44060</v>
+        <v>44061</v>
       </c>
       <c r="D49" t="s">
         <v>302</v>
@@ -5269,31 +5257,31 @@
       </c>
       <c r="F49"/>
       <c r="G49" t="n">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="H49" t="n">
-        <v>394566</v>
+        <v>398585</v>
       </c>
       <c r="I49" t="n">
-        <v>7.338</v>
+        <v>7.413</v>
       </c>
       <c r="J49" t="n">
-        <v>3150</v>
+        <v>4019</v>
       </c>
       <c r="K49" t="n">
-        <v>0.059</v>
+        <v>0.075</v>
       </c>
       <c r="L49" t="n">
-        <v>5177</v>
+        <v>5155</v>
       </c>
       <c r="M49" t="n">
         <v>0.096</v>
       </c>
       <c r="N49" t="n">
-        <v>0.102</v>
+        <v>0.095</v>
       </c>
       <c r="O49" t="n">
-        <v>9.837</v>
+        <v>10.499</v>
       </c>
       <c r="P49" t="s">
         <v>45</v>
@@ -5373,7 +5361,7 @@
         <v>313</v>
       </c>
       <c r="C51" s="1" t="n">
-        <v>44063</v>
+        <v>44064</v>
       </c>
       <c r="D51" t="s">
         <v>314</v>
@@ -5385,32 +5373,28 @@
         <v>316</v>
       </c>
       <c r="G51" t="n">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="H51" t="n">
-        <v>232918</v>
+        <v>234520</v>
       </c>
       <c r="I51" t="n">
-        <v>123.485</v>
+        <v>124.335</v>
       </c>
       <c r="J51" t="n">
-        <v>1997</v>
+        <v>1602</v>
       </c>
       <c r="K51" t="n">
-        <v>1.059</v>
+        <v>0.849</v>
       </c>
       <c r="L51" t="n">
-        <v>1727</v>
+        <v>1713</v>
       </c>
       <c r="M51" t="n">
-        <v>0.916</v>
-      </c>
-      <c r="N51" t="n">
-        <v>0.002</v>
-      </c>
-      <c r="O51" t="n">
-        <v>525.609</v>
-      </c>
+        <v>0.908</v>
+      </c>
+      <c r="N51"/>
+      <c r="O51"/>
       <c r="P51" t="s">
         <v>315</v>
       </c>
@@ -5489,7 +5473,7 @@
         <v>323</v>
       </c>
       <c r="C53" s="1" t="n">
-        <v>44061</v>
+        <v>44062</v>
       </c>
       <c r="D53" t="s">
         <v>324</v>
@@ -5499,31 +5483,31 @@
       </c>
       <c r="F53"/>
       <c r="G53" t="n">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="H53" t="n">
-        <v>464183</v>
+        <v>466964</v>
       </c>
       <c r="I53" t="n">
-        <v>741.535</v>
+        <v>745.977</v>
       </c>
       <c r="J53" t="n">
-        <v>1977</v>
+        <v>2781</v>
       </c>
       <c r="K53" t="n">
-        <v>3.158</v>
+        <v>4.443</v>
       </c>
       <c r="L53" t="n">
-        <v>1498</v>
+        <v>1660</v>
       </c>
       <c r="M53" t="n">
-        <v>2.393</v>
+        <v>2.652</v>
       </c>
       <c r="N53" t="n">
-        <v>0.024</v>
+        <v>0.022</v>
       </c>
       <c r="O53" t="n">
-        <v>41.447</v>
+        <v>45.214</v>
       </c>
       <c r="P53" t="s">
         <v>325</v>
@@ -5546,7 +5530,7 @@
         <v>328</v>
       </c>
       <c r="C54" s="1" t="n">
-        <v>44062</v>
+        <v>44063</v>
       </c>
       <c r="D54" t="s">
         <v>329</v>
@@ -5558,31 +5542,31 @@
         <v>331</v>
       </c>
       <c r="G54" t="n">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="H54" t="n">
-        <v>1141679</v>
+        <v>1152140</v>
       </c>
       <c r="I54" t="n">
-        <v>35.274</v>
+        <v>35.597</v>
       </c>
       <c r="J54" t="n">
-        <v>12588</v>
+        <v>10461</v>
       </c>
       <c r="K54" t="n">
-        <v>0.389</v>
+        <v>0.323</v>
       </c>
       <c r="L54" t="n">
-        <v>9666</v>
+        <v>9586</v>
       </c>
       <c r="M54" t="n">
-        <v>0.299</v>
+        <v>0.296</v>
       </c>
       <c r="N54" t="n">
         <v>0.002</v>
       </c>
       <c r="O54" t="n">
-        <v>583.293</v>
+        <v>554.562</v>
       </c>
       <c r="P54" t="s">
         <v>45</v>
@@ -5719,7 +5703,7 @@
         <v>348</v>
       </c>
       <c r="C57" s="1" t="n">
-        <v>44059</v>
+        <v>44060</v>
       </c>
       <c r="D57" t="s">
         <v>349</v>
@@ -5729,31 +5713,31 @@
       </c>
       <c r="F57"/>
       <c r="G57" t="n">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="H57" t="n">
-        <v>1124122</v>
+        <v>1138828</v>
       </c>
       <c r="I57" t="n">
-        <v>8.719</v>
+        <v>8.833</v>
       </c>
       <c r="J57" t="n">
-        <v>1965</v>
+        <v>7608</v>
       </c>
       <c r="K57" t="n">
-        <v>0.015</v>
+        <v>0.059</v>
       </c>
       <c r="L57" t="n">
-        <v>9496</v>
+        <v>9386</v>
       </c>
       <c r="M57" t="n">
-        <v>0.074</v>
+        <v>0.073</v>
       </c>
       <c r="N57" t="n">
-        <v>0.629</v>
+        <v>0.637</v>
       </c>
       <c r="O57" t="n">
-        <v>1.59</v>
+        <v>1.569</v>
       </c>
       <c r="P57" t="s">
         <v>351</v>
@@ -5833,7 +5817,7 @@
         <v>361</v>
       </c>
       <c r="C59" s="1" t="n">
-        <v>44057</v>
+        <v>44061</v>
       </c>
       <c r="D59" t="s">
         <v>362</v>
@@ -5843,31 +5827,31 @@
       </c>
       <c r="F59"/>
       <c r="G59" t="n">
-        <v>129</v>
+        <v>133</v>
       </c>
       <c r="H59" t="n">
-        <v>134035</v>
+        <v>139514</v>
       </c>
       <c r="I59" t="n">
-        <v>2.463</v>
+        <v>2.564</v>
       </c>
       <c r="J59" t="n">
-        <v>1736</v>
+        <v>1765</v>
       </c>
       <c r="K59" t="n">
         <v>0.032</v>
       </c>
       <c r="L59" t="n">
-        <v>1324</v>
+        <v>1530</v>
       </c>
       <c r="M59" t="n">
-        <v>0.024</v>
+        <v>0.028</v>
       </c>
       <c r="N59" t="n">
         <v>0.001</v>
       </c>
       <c r="O59" t="n">
-        <v>926.8</v>
+        <v>669.375</v>
       </c>
       <c r="P59" t="s">
         <v>363</v>
@@ -6000,7 +5984,7 @@
         <v>380</v>
       </c>
       <c r="C62" s="1" t="n">
-        <v>44062</v>
+        <v>44063</v>
       </c>
       <c r="D62" t="s">
         <v>381</v>
@@ -6010,31 +5994,31 @@
       </c>
       <c r="F62"/>
       <c r="G62" t="n">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="H62" t="n">
-        <v>657506</v>
+        <v>673220</v>
       </c>
       <c r="I62" t="n">
-        <v>136.349</v>
+        <v>139.608</v>
       </c>
       <c r="J62" t="n">
-        <v>18091</v>
+        <v>15714</v>
       </c>
       <c r="K62" t="n">
-        <v>3.752</v>
+        <v>3.259</v>
       </c>
       <c r="L62" t="n">
-        <v>21256</v>
+        <v>21258</v>
       </c>
       <c r="M62" t="n">
         <v>4.408</v>
       </c>
       <c r="N62" t="n">
-        <v>0.001</v>
+        <v>0</v>
       </c>
       <c r="O62" t="n">
-        <v>1883.443</v>
+        <v>2254.636</v>
       </c>
       <c r="P62" t="s">
         <v>382</v>
@@ -6216,7 +6200,7 @@
         <v>405</v>
       </c>
       <c r="C66" s="1" t="n">
-        <v>44063</v>
+        <v>44064</v>
       </c>
       <c r="D66" t="s">
         <v>406</v>
@@ -6226,32 +6210,28 @@
       </c>
       <c r="F66"/>
       <c r="G66" t="n">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="H66" t="n">
-        <v>2363752</v>
+        <v>2389365</v>
       </c>
       <c r="I66" t="n">
-        <v>10.701</v>
+        <v>10.817</v>
       </c>
       <c r="J66" t="n">
-        <v>23680</v>
+        <v>25613</v>
       </c>
       <c r="K66" t="n">
-        <v>0.107</v>
+        <v>0.116</v>
       </c>
       <c r="L66" t="n">
-        <v>22584</v>
+        <v>22851</v>
       </c>
       <c r="M66" t="n">
-        <v>0.102</v>
-      </c>
-      <c r="N66" t="n">
-        <v>0.027</v>
-      </c>
-      <c r="O66" t="n">
-        <v>36.902</v>
-      </c>
+        <v>0.103</v>
+      </c>
+      <c r="N66"/>
+      <c r="O66"/>
       <c r="P66" t="s">
         <v>407</v>
       </c>
@@ -6330,7 +6310,7 @@
         <v>415</v>
       </c>
       <c r="C68" s="1" t="n">
-        <v>44058</v>
+        <v>44062</v>
       </c>
       <c r="D68" t="s">
         <v>416</v>
@@ -6340,31 +6320,31 @@
       </c>
       <c r="F68"/>
       <c r="G68" t="n">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="H68" t="n">
-        <v>151427</v>
+        <v>162323</v>
       </c>
       <c r="I68" t="n">
-        <v>21.23</v>
+        <v>22.758</v>
       </c>
       <c r="J68" t="n">
-        <v>2078</v>
+        <v>2657</v>
       </c>
       <c r="K68" t="n">
-        <v>0.291</v>
+        <v>0.373</v>
       </c>
       <c r="L68" t="n">
-        <v>2018</v>
+        <v>2544</v>
       </c>
       <c r="M68" t="n">
-        <v>0.283</v>
+        <v>0.357</v>
       </c>
       <c r="N68" t="n">
-        <v>0.182</v>
+        <v>0.173</v>
       </c>
       <c r="O68" t="n">
-        <v>5.499</v>
+        <v>5.769</v>
       </c>
       <c r="P68" t="s">
         <v>417</v>
@@ -6387,7 +6367,7 @@
         <v>421</v>
       </c>
       <c r="C69" s="1" t="n">
-        <v>44057</v>
+        <v>44061</v>
       </c>
       <c r="D69" t="s">
         <v>422</v>
@@ -6397,25 +6377,25 @@
       </c>
       <c r="F69"/>
       <c r="G69" t="n">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="H69" t="n">
-        <v>472683</v>
+        <v>506901</v>
       </c>
       <c r="I69" t="n">
-        <v>14.336</v>
+        <v>15.374</v>
       </c>
       <c r="J69" t="n">
-        <v>8488</v>
+        <v>9044</v>
       </c>
       <c r="K69" t="n">
-        <v>0.257</v>
+        <v>0.274</v>
       </c>
       <c r="L69" t="n">
-        <v>6919</v>
+        <v>8538</v>
       </c>
       <c r="M69" t="n">
-        <v>0.21</v>
+        <v>0.259</v>
       </c>
       <c r="N69"/>
       <c r="O69"/>
@@ -6497,7 +6477,7 @@
         <v>433</v>
       </c>
       <c r="C71" s="1" t="n">
-        <v>44062</v>
+        <v>44063</v>
       </c>
       <c r="D71" t="s">
         <v>434</v>
@@ -6507,31 +6487,31 @@
       </c>
       <c r="F71"/>
       <c r="G71" t="n">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="H71" t="n">
-        <v>2333126</v>
+        <v>2357772</v>
       </c>
       <c r="I71" t="n">
-        <v>61.647</v>
+        <v>62.298</v>
       </c>
       <c r="J71" t="n">
-        <v>27734</v>
+        <v>24646</v>
       </c>
       <c r="K71" t="n">
-        <v>0.733</v>
+        <v>0.651</v>
       </c>
       <c r="L71" t="n">
-        <v>21586</v>
+        <v>21510</v>
       </c>
       <c r="M71" t="n">
-        <v>0.57</v>
+        <v>0.568</v>
       </c>
       <c r="N71" t="n">
         <v>0.033</v>
       </c>
       <c r="O71" t="n">
-        <v>30.743</v>
+        <v>30.511</v>
       </c>
       <c r="P71" t="s">
         <v>435</v>
@@ -6554,7 +6534,7 @@
         <v>438</v>
       </c>
       <c r="C72" s="1" t="n">
-        <v>44062</v>
+        <v>44063</v>
       </c>
       <c r="D72" t="s">
         <v>434</v>
@@ -6564,31 +6544,31 @@
       </c>
       <c r="F72"/>
       <c r="G72" t="n">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="H72" t="n">
-        <v>2438135</v>
+        <v>2463734</v>
       </c>
       <c r="I72" t="n">
-        <v>64.421</v>
+        <v>65.098</v>
       </c>
       <c r="J72" t="n">
-        <v>28741</v>
+        <v>25599</v>
       </c>
       <c r="K72" t="n">
-        <v>0.759</v>
+        <v>0.676</v>
       </c>
       <c r="L72" t="n">
-        <v>22362</v>
+        <v>22286</v>
       </c>
       <c r="M72" t="n">
-        <v>0.591</v>
+        <v>0.589</v>
       </c>
       <c r="N72" t="n">
-        <v>0.031</v>
+        <v>0.032</v>
       </c>
       <c r="O72" t="n">
-        <v>31.848</v>
+        <v>31.611</v>
       </c>
       <c r="P72" t="s">
         <v>435</v>
@@ -6668,7 +6648,7 @@
         <v>447</v>
       </c>
       <c r="C74" s="1" t="n">
-        <v>44062</v>
+        <v>44063</v>
       </c>
       <c r="D74" t="s">
         <v>448</v>
@@ -6678,31 +6658,31 @@
       </c>
       <c r="F74"/>
       <c r="G74" t="n">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="H74" t="n">
-        <v>566013</v>
+        <v>572273</v>
       </c>
       <c r="I74" t="n">
-        <v>196.46</v>
+        <v>198.633</v>
       </c>
       <c r="J74" t="n">
-        <v>5023</v>
+        <v>6260</v>
       </c>
       <c r="K74" t="n">
-        <v>1.743</v>
+        <v>2.173</v>
       </c>
       <c r="L74" t="n">
-        <v>4574</v>
+        <v>4810</v>
       </c>
       <c r="M74" t="n">
-        <v>1.588</v>
+        <v>1.67</v>
       </c>
       <c r="N74" t="n">
-        <v>0.063</v>
+        <v>0.06</v>
       </c>
       <c r="O74" t="n">
-        <v>15.89</v>
+        <v>16.685</v>
       </c>
       <c r="P74" t="s">
         <v>449</v>
@@ -6782,7 +6762,7 @@
         <v>460</v>
       </c>
       <c r="C76" s="1" t="n">
-        <v>44062</v>
+        <v>44063</v>
       </c>
       <c r="D76" t="s">
         <v>461</v>
@@ -6792,22 +6772,22 @@
       </c>
       <c r="F76"/>
       <c r="G76" t="n">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="H76" t="n">
-        <v>33509273</v>
+        <v>33814105</v>
       </c>
       <c r="I76" t="n">
-        <v>229.619</v>
+        <v>231.707</v>
       </c>
       <c r="J76" t="n">
-        <v>291805</v>
+        <v>304832</v>
       </c>
       <c r="K76" t="n">
-        <v>2</v>
+        <v>2.089</v>
       </c>
       <c r="L76" t="n">
-        <v>272996</v>
+        <v>273007</v>
       </c>
       <c r="M76" t="n">
         <v>1.871</v>
@@ -6816,7 +6796,7 @@
         <v>0.018</v>
       </c>
       <c r="O76" t="n">
-        <v>54.765</v>
+        <v>55.201</v>
       </c>
       <c r="P76" t="s">
         <v>462</v>
@@ -6839,7 +6819,7 @@
         <v>466</v>
       </c>
       <c r="C77" s="1" t="n">
-        <v>44059</v>
+        <v>44062</v>
       </c>
       <c r="D77" t="s">
         <v>467</v>
@@ -6849,31 +6829,31 @@
       </c>
       <c r="F77"/>
       <c r="G77" t="n">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="H77" t="n">
-        <v>334270</v>
+        <v>345920</v>
       </c>
       <c r="I77" t="n">
-        <v>25.808</v>
+        <v>26.707</v>
       </c>
       <c r="J77" t="n">
-        <v>4796</v>
+        <v>3306</v>
       </c>
       <c r="K77" t="n">
-        <v>0.37</v>
+        <v>0.255</v>
       </c>
       <c r="L77" t="n">
-        <v>5070</v>
+        <v>4483</v>
       </c>
       <c r="M77" t="n">
-        <v>0.391</v>
+        <v>0.346</v>
       </c>
       <c r="N77" t="n">
-        <v>0.006</v>
+        <v>0.013</v>
       </c>
       <c r="O77" t="n">
-        <v>162.798</v>
+        <v>77.293</v>
       </c>
       <c r="P77" t="s">
         <v>468</v>
@@ -6896,7 +6876,7 @@
         <v>472</v>
       </c>
       <c r="C78" s="1" t="n">
-        <v>44062</v>
+        <v>44063</v>
       </c>
       <c r="D78" t="s">
         <v>473</v>
@@ -6906,31 +6886,31 @@
       </c>
       <c r="F78"/>
       <c r="G78" t="n">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="H78" t="n">
-        <v>4439484</v>
+        <v>4501104</v>
       </c>
       <c r="I78" t="n">
-        <v>127.521</v>
+        <v>129.291</v>
       </c>
       <c r="J78" t="n">
-        <v>61067</v>
+        <v>61620</v>
       </c>
       <c r="K78" t="n">
-        <v>1.754</v>
+        <v>1.77</v>
       </c>
       <c r="L78" t="n">
-        <v>62626</v>
+        <v>61321</v>
       </c>
       <c r="M78" t="n">
-        <v>1.799</v>
+        <v>1.761</v>
       </c>
       <c r="N78" t="n">
-        <v>0.023</v>
+        <v>0.022</v>
       </c>
       <c r="O78" t="n">
-        <v>44.438</v>
+        <v>44.486</v>
       </c>
       <c r="P78" t="s">
         <v>45</v>
@@ -6953,7 +6933,7 @@
         <v>476</v>
       </c>
       <c r="C79" s="1" t="n">
-        <v>44062</v>
+        <v>44063</v>
       </c>
       <c r="D79" t="s">
         <v>477</v>
@@ -6965,31 +6945,31 @@
         <v>479</v>
       </c>
       <c r="G79" t="n">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="H79" t="n">
-        <v>137194</v>
+        <v>138713</v>
       </c>
       <c r="I79" t="n">
-        <v>8.194</v>
+        <v>8.284</v>
       </c>
       <c r="J79" t="n">
-        <v>1463</v>
+        <v>1519</v>
       </c>
       <c r="K79" t="n">
-        <v>0.087</v>
+        <v>0.091</v>
       </c>
       <c r="L79" t="n">
-        <v>1475</v>
+        <v>1445</v>
       </c>
       <c r="M79" t="n">
-        <v>0.088</v>
+        <v>0.086</v>
       </c>
       <c r="N79" t="n">
-        <v>0.09</v>
+        <v>0.085</v>
       </c>
       <c r="O79" t="n">
-        <v>11.162</v>
+        <v>11.775</v>
       </c>
       <c r="P79" t="s">
         <v>480</v>
@@ -7291,7 +7271,7 @@
         <v>509</v>
       </c>
       <c r="C85" s="1" t="n">
-        <v>44062</v>
+        <v>44063</v>
       </c>
       <c r="D85" t="s">
         <v>510</v>
@@ -7303,31 +7283,31 @@
         <v>512</v>
       </c>
       <c r="G85" t="n">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="H85" t="n">
-        <v>3455671</v>
+        <v>3480283</v>
       </c>
       <c r="I85" t="n">
-        <v>58.266</v>
+        <v>58.681</v>
       </c>
       <c r="J85" t="n">
-        <v>25324</v>
+        <v>24612</v>
       </c>
       <c r="K85" t="n">
-        <v>0.427</v>
+        <v>0.415</v>
       </c>
       <c r="L85" t="n">
-        <v>22891</v>
+        <v>23541</v>
       </c>
       <c r="M85" t="n">
-        <v>0.386</v>
+        <v>0.397</v>
       </c>
       <c r="N85" t="n">
-        <v>0.162</v>
+        <v>0.165</v>
       </c>
       <c r="O85" t="n">
-        <v>6.155</v>
+        <v>6.072</v>
       </c>
       <c r="P85" t="s">
         <v>511</v>
@@ -7623,7 +7603,7 @@
         <v>545</v>
       </c>
       <c r="C91" s="1" t="n">
-        <v>44062</v>
+        <v>44063</v>
       </c>
       <c r="D91" t="s">
         <v>546</v>
@@ -7633,22 +7613,22 @@
       </c>
       <c r="F91"/>
       <c r="G91" t="n">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="H91" t="n">
-        <v>85349</v>
+        <v>85563</v>
       </c>
       <c r="I91" t="n">
-        <v>3.584</v>
+        <v>3.593</v>
       </c>
       <c r="J91" t="n">
-        <v>222</v>
+        <v>214</v>
       </c>
       <c r="K91" t="n">
         <v>0.009</v>
       </c>
       <c r="L91" t="n">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="M91" t="n">
         <v>0.008</v>
@@ -7657,7 +7637,7 @@
         <v>0.004</v>
       </c>
       <c r="O91" t="n">
-        <v>266</v>
+        <v>263.2</v>
       </c>
       <c r="P91" t="s">
         <v>547</v>
@@ -7680,7 +7660,7 @@
         <v>550</v>
       </c>
       <c r="C92" s="1" t="n">
-        <v>44062</v>
+        <v>44063</v>
       </c>
       <c r="D92" t="s">
         <v>551</v>
@@ -7690,31 +7670,31 @@
       </c>
       <c r="F92"/>
       <c r="G92" t="n">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="H92" t="n">
-        <v>399394</v>
+        <v>401680</v>
       </c>
       <c r="I92" t="n">
-        <v>5.722</v>
+        <v>5.755</v>
       </c>
       <c r="J92" t="n">
-        <v>2118</v>
+        <v>2286</v>
       </c>
       <c r="K92" t="n">
-        <v>0.03</v>
+        <v>0.033</v>
       </c>
       <c r="L92" t="n">
-        <v>1377</v>
+        <v>1506</v>
       </c>
       <c r="M92" t="n">
-        <v>0.02</v>
+        <v>0.022</v>
       </c>
       <c r="N92" t="n">
         <v>0.003</v>
       </c>
       <c r="O92" t="n">
-        <v>370.731</v>
+        <v>319.455</v>
       </c>
       <c r="P92" t="s">
         <v>552</v>
@@ -7737,7 +7717,7 @@
         <v>555</v>
       </c>
       <c r="C93" s="1" t="n">
-        <v>44062</v>
+        <v>44063</v>
       </c>
       <c r="D93" t="s">
         <v>551</v>
@@ -7747,31 +7727,31 @@
       </c>
       <c r="F93"/>
       <c r="G93" t="n">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H93" t="n">
-        <v>787665</v>
+        <v>789951</v>
       </c>
       <c r="I93" t="n">
-        <v>11.285</v>
+        <v>11.317</v>
       </c>
       <c r="J93" t="n">
-        <v>2118</v>
+        <v>2286</v>
       </c>
       <c r="K93" t="n">
-        <v>0.03</v>
+        <v>0.033</v>
       </c>
       <c r="L93" t="n">
-        <v>1377</v>
+        <v>1506</v>
       </c>
       <c r="M93" t="n">
-        <v>0.02</v>
+        <v>0.022</v>
       </c>
       <c r="N93" t="n">
         <v>0.003</v>
       </c>
       <c r="O93" t="n">
-        <v>370.731</v>
+        <v>319.455</v>
       </c>
       <c r="P93" t="s">
         <v>552</v>
@@ -7794,7 +7774,7 @@
         <v>558</v>
       </c>
       <c r="C94" s="1" t="n">
-        <v>44058</v>
+        <v>44062</v>
       </c>
       <c r="D94"/>
       <c r="E94" t="s">
@@ -7804,31 +7784,31 @@
         <v>560</v>
       </c>
       <c r="G94" t="n">
-        <v>159</v>
+        <v>163</v>
       </c>
       <c r="H94" t="n">
-        <v>51889</v>
+        <v>54709</v>
       </c>
       <c r="I94" t="n">
-        <v>6.268</v>
+        <v>6.608</v>
       </c>
       <c r="J94" t="n">
-        <v>763</v>
+        <v>862</v>
       </c>
       <c r="K94" t="n">
-        <v>0.092</v>
+        <v>0.104</v>
       </c>
       <c r="L94" t="n">
-        <v>687</v>
+        <v>698</v>
       </c>
       <c r="M94" t="n">
-        <v>0.083</v>
+        <v>0.084</v>
       </c>
       <c r="N94" t="n">
-        <v>0.02</v>
+        <v>0.021</v>
       </c>
       <c r="O94" t="n">
-        <v>50.094</v>
+        <v>47.437</v>
       </c>
       <c r="P94" t="s">
         <v>559</v>
@@ -7851,7 +7831,7 @@
         <v>564</v>
       </c>
       <c r="C95" s="1" t="n">
-        <v>44059</v>
+        <v>44060</v>
       </c>
       <c r="D95" t="s">
         <v>565</v>
@@ -7861,31 +7841,31 @@
       </c>
       <c r="F95"/>
       <c r="G95" t="n">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="H95" t="n">
-        <v>112048</v>
+        <v>113758</v>
       </c>
       <c r="I95" t="n">
-        <v>9.481</v>
+        <v>9.625</v>
       </c>
       <c r="J95" t="n">
-        <v>1404</v>
+        <v>1710</v>
       </c>
       <c r="K95" t="n">
-        <v>0.119</v>
+        <v>0.145</v>
       </c>
       <c r="L95" t="n">
-        <v>1292</v>
+        <v>1365</v>
       </c>
       <c r="M95" t="n">
-        <v>0.109</v>
+        <v>0.115</v>
       </c>
       <c r="N95" t="n">
-        <v>0.038</v>
+        <v>0.043</v>
       </c>
       <c r="O95" t="n">
-        <v>26.214</v>
+        <v>23.305</v>
       </c>
       <c r="P95" t="s">
         <v>566</v>
@@ -7921,24 +7901,24 @@
         <v>142</v>
       </c>
       <c r="H96" t="n">
-        <v>5969629</v>
+        <v>6061930</v>
       </c>
       <c r="I96" t="n">
-        <v>70.781</v>
+        <v>71.876</v>
       </c>
       <c r="J96"/>
       <c r="K96"/>
       <c r="L96" t="n">
-        <v>63964</v>
+        <v>77150</v>
       </c>
       <c r="M96" t="n">
-        <v>0.758</v>
+        <v>0.915</v>
       </c>
       <c r="N96" t="n">
-        <v>0.019</v>
+        <v>0.016</v>
       </c>
       <c r="O96" t="n">
-        <v>51.371</v>
+        <v>61.961</v>
       </c>
       <c r="P96" t="s">
         <v>571</v>
@@ -7961,7 +7941,7 @@
         <v>574</v>
       </c>
       <c r="C97" s="1" t="n">
-        <v>44061</v>
+        <v>44062</v>
       </c>
       <c r="D97" t="s">
         <v>575</v>
@@ -7971,31 +7951,31 @@
       </c>
       <c r="F97"/>
       <c r="G97" t="n">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H97" t="n">
-        <v>333667</v>
+        <v>336713</v>
       </c>
       <c r="I97" t="n">
-        <v>7.295</v>
+        <v>7.361</v>
       </c>
       <c r="J97" t="n">
-        <v>4125</v>
+        <v>3046</v>
       </c>
       <c r="K97" t="n">
-        <v>0.09</v>
+        <v>0.067</v>
       </c>
       <c r="L97" t="n">
-        <v>4169</v>
+        <v>4030</v>
       </c>
       <c r="M97" t="n">
-        <v>0.091</v>
+        <v>0.088</v>
       </c>
       <c r="N97" t="n">
-        <v>0.009</v>
+        <v>0.01</v>
       </c>
       <c r="O97" t="n">
-        <v>110.962</v>
+        <v>97.276</v>
       </c>
       <c r="P97" t="s">
         <v>576</v>
@@ -8018,7 +7998,7 @@
         <v>580</v>
       </c>
       <c r="C98" s="1" t="n">
-        <v>44063</v>
+        <v>44064</v>
       </c>
       <c r="D98" t="s">
         <v>581</v>
@@ -8028,32 +8008,28 @@
       </c>
       <c r="F98"/>
       <c r="G98" t="n">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="H98" t="n">
-        <v>1356698</v>
+        <v>1378519</v>
       </c>
       <c r="I98" t="n">
-        <v>31.022</v>
+        <v>31.521</v>
       </c>
       <c r="J98" t="n">
-        <v>21698</v>
+        <v>21821</v>
       </c>
       <c r="K98" t="n">
-        <v>0.496</v>
+        <v>0.499</v>
       </c>
       <c r="L98" t="n">
-        <v>17539</v>
+        <v>17954</v>
       </c>
       <c r="M98" t="n">
-        <v>0.401</v>
-      </c>
-      <c r="N98" t="n">
-        <v>0.084</v>
-      </c>
-      <c r="O98" t="n">
-        <v>11.963</v>
-      </c>
+        <v>0.411</v>
+      </c>
+      <c r="N98"/>
+      <c r="O98"/>
       <c r="P98" t="s">
         <v>582</v>
       </c>
@@ -8075,7 +8051,7 @@
         <v>586</v>
       </c>
       <c r="C99" s="1" t="n">
-        <v>44062</v>
+        <v>44063</v>
       </c>
       <c r="D99" t="s">
         <v>587</v>
@@ -8085,31 +8061,31 @@
       </c>
       <c r="F99"/>
       <c r="G99" t="n">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="H99" t="n">
-        <v>6193635</v>
+        <v>6265918</v>
       </c>
       <c r="I99" t="n">
-        <v>626.227</v>
+        <v>633.535</v>
       </c>
       <c r="J99" t="n">
-        <v>72026</v>
+        <v>72283</v>
       </c>
       <c r="K99" t="n">
-        <v>7.282</v>
+        <v>7.308</v>
       </c>
       <c r="L99" t="n">
-        <v>71034</v>
+        <v>71509</v>
       </c>
       <c r="M99" t="n">
-        <v>7.182</v>
+        <v>7.23</v>
       </c>
       <c r="N99" t="n">
         <v>0.004</v>
       </c>
       <c r="O99" t="n">
-        <v>256.308</v>
+        <v>235.116</v>
       </c>
       <c r="P99" t="s">
         <v>588</v>
@@ -8132,7 +8108,7 @@
         <v>591</v>
       </c>
       <c r="C100" s="1" t="n">
-        <v>44061</v>
+        <v>44062</v>
       </c>
       <c r="D100" t="s">
         <v>592</v>
@@ -8144,31 +8120,31 @@
         <v>594</v>
       </c>
       <c r="G100" t="n">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="H100" t="n">
-        <v>12272157</v>
+        <v>12446595</v>
       </c>
       <c r="I100" t="n">
-        <v>180.776</v>
+        <v>183.346</v>
       </c>
       <c r="J100" t="n">
-        <v>153225</v>
+        <v>175916</v>
       </c>
       <c r="K100" t="n">
-        <v>2.257</v>
+        <v>2.591</v>
       </c>
       <c r="L100" t="n">
-        <v>161563</v>
+        <v>162256</v>
       </c>
       <c r="M100" t="n">
-        <v>2.38</v>
+        <v>2.39</v>
       </c>
       <c r="N100" t="n">
         <v>0.007</v>
       </c>
       <c r="O100" t="n">
-        <v>149.675</v>
+        <v>151.5</v>
       </c>
       <c r="P100" t="s">
         <v>593</v>
@@ -8244,7 +8220,7 @@
         <v>603</v>
       </c>
       <c r="C102" s="1" t="n">
-        <v>44062</v>
+        <v>44063</v>
       </c>
       <c r="D102" t="s">
         <v>604</v>
@@ -8254,31 +8230,31 @@
       </c>
       <c r="F102"/>
       <c r="G102" t="n">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="H102" t="n">
-        <v>68944867</v>
+        <v>69580676</v>
       </c>
       <c r="I102" t="n">
-        <v>208.291</v>
+        <v>210.212</v>
       </c>
       <c r="J102" t="n">
-        <v>680934</v>
+        <v>635809</v>
       </c>
       <c r="K102" t="n">
-        <v>2.057</v>
+        <v>1.921</v>
       </c>
       <c r="L102" t="n">
-        <v>744795</v>
+        <v>709806</v>
       </c>
       <c r="M102" t="n">
-        <v>2.25</v>
+        <v>2.144</v>
       </c>
       <c r="N102" t="n">
-        <v>0.065</v>
+        <v>0.067</v>
       </c>
       <c r="O102" t="n">
-        <v>15.28</v>
+        <v>14.935</v>
       </c>
       <c r="P102" t="s">
         <v>605</v>
@@ -8301,7 +8277,7 @@
         <v>610</v>
       </c>
       <c r="C103" s="1" t="n">
-        <v>44062</v>
+        <v>44063</v>
       </c>
       <c r="D103" t="s">
         <v>611</v>
@@ -8311,31 +8287,31 @@
       </c>
       <c r="F103"/>
       <c r="G103" t="n">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="H103" t="n">
-        <v>152121</v>
+        <v>154431</v>
       </c>
       <c r="I103" t="n">
-        <v>43.792</v>
+        <v>44.457</v>
       </c>
       <c r="J103" t="n">
-        <v>4527</v>
+        <v>2310</v>
       </c>
       <c r="K103" t="n">
-        <v>1.303</v>
+        <v>0.665</v>
       </c>
       <c r="L103" t="n">
-        <v>2134</v>
+        <v>2247</v>
       </c>
       <c r="M103" t="n">
-        <v>0.614</v>
+        <v>0.647</v>
       </c>
       <c r="N103" t="n">
-        <v>0.007</v>
+        <v>0.006</v>
       </c>
       <c r="O103" t="n">
-        <v>149.38</v>
+        <v>157.29</v>
       </c>
       <c r="P103" t="s">
         <v>125</v>
@@ -8411,7 +8387,7 @@
         <v>621</v>
       </c>
       <c r="C105" s="1" t="n">
-        <v>44059</v>
+        <v>44063</v>
       </c>
       <c r="D105" t="s">
         <v>622</v>
@@ -8421,31 +8397,31 @@
       </c>
       <c r="F105"/>
       <c r="G105" t="n">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="H105" t="n">
-        <v>82884</v>
+        <v>87885</v>
       </c>
       <c r="I105" t="n">
-        <v>5.577</v>
+        <v>5.913</v>
       </c>
       <c r="J105" t="n">
-        <v>1546</v>
+        <v>1256</v>
       </c>
       <c r="K105" t="n">
-        <v>0.104</v>
+        <v>0.085</v>
       </c>
       <c r="L105" t="n">
-        <v>1611</v>
+        <v>1307</v>
       </c>
       <c r="M105" t="n">
-        <v>0.108</v>
+        <v>0.088</v>
       </c>
       <c r="N105" t="n">
-        <v>0.053</v>
+        <v>0.082</v>
       </c>
       <c r="O105" t="n">
-        <v>18.764</v>
+        <v>12.199</v>
       </c>
       <c r="P105" t="s">
         <v>623</v>

</xml_diff>

<commit_message>
Updated testing data for 2020-08-24
</commit_message>
<xml_diff>
--- a/public/data/testing/covid-testing-latest-data-source-details.xlsx
+++ b/public/data/testing/covid-testing-latest-data-source-details.xlsx
@@ -110,7 +110,7 @@
     <t xml:space="preserve">Australia - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.health.gov.au/sites/default/files/documents/2020/08/coronavirus-covid-19-at-a-glance-20-august-2020.pdf</t>
+    <t xml:space="preserve">https://www.health.gov.au/sites/default/files/documents/2020/08/coronavirus-covid-19-at-a-glance-23-august-2020.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">Australian Government Department of Health</t>
@@ -202,7 +202,7 @@
     <t xml:space="preserve">Belarus - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">http://minzdrav.gov.by/ru/sobytiya/u-belarusi-na-12-zhni-nya-vypisanyya-65-tys-893-patsyenta/</t>
+    <t xml:space="preserve">http://minzdrav.gov.by/ru/sobytiya/u-belarusi-na-23-zhni-nya-vypisanyya-68-tys-839-patsyenta/</t>
   </si>
   <si>
     <t xml:space="preserve">Belarus Ministry of Health</t>
@@ -245,7 +245,7 @@
     <t xml:space="preserve">Bolivia - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://minsalud.gob.bo/4519-laboratorios-reportaron-mas-de-100-000-pruebas-negativas-desde-el-brote-del-covid-19-en-bolivia</t>
+    <t xml:space="preserve">https://minsalud.gob.bo/4531-bolivia-acumula-41-111-pacientes-recuperados-de-covid-19-y-los-casos-positivos-llegan-a-106-065</t>
   </si>
   <si>
     <t xml:space="preserve">https://www.minsalud.gob.bo/</t>
@@ -253,6 +253,7 @@
   <si>
     <t xml:space="preserve">Official testing data from the Bolivian Ministry of Health is reported in daily briefs [on their website](https://www.minsalud.gob.bo/). The briefs often (but do not always) provide a breakdown of the cumulative number of confirmed, suspected, and negative (also called discarded) tests to date. We measure the total number of tests performed to date as the sum of the number of confirmed and negative tests.
 Because of the way the daily briefs report the number of negative tests ("pruebas negativas") alongside the number of positive cases ("casos positivos"), it may be the case that the number of tests performed is equivalent to the number of people tested.
+The reported number of tests performed may include non-PCR tests. [Official protocol for COVID-19 laboratory diagnosis](https://www.minsalud.gob.bo/component/jdownloads/download/30-guias-manejo-covid/445-protocolo-para-el-diagnostico-de-laboratorio-en-el-marco-de-la-emergencia-sanitaria-por-covid-actualizado?Itemid=646) (updated in May 2020) indicate that antibody (non-PCR) tests are an important aspect of the country's screening and diagnostic process (e.g. see pages 24-27 and annex 2). But the source does not explicitly state whether these non-PCR tests are used to confirm or discard suspected cases without a corresponding PCR test result.
 As of 5 August 2020, the most recent daily briefs consistently report testing figures in terms of the cumulative number of tests ("pruebas") performed. However, in the initial months of the COVID-19 outbreak, the daily briefs previously reported testing figures using inconsistent terminology such as samples (“muestras”) tested, people who have undergone tests (”personas, que fueron sometidas a pruebas”), and tests ("pruebas") performed. It does not appear that this inconsistent use of terminology reflects a substantive change in the reported figures, since there are no corresponding large breaks in the time series.
 In 10 briefs the number of negative tests was not reported, preventing us from calculating a total for that date. For these dates with missing official data, we use data provided in this [unofficial GitHub repository](https://github.com/mauforonda/covid19-bolivia), which we have cross-referenced against the official data for all dates.
 Our data for this series is sourced from a non-official repository of official data. As explained in our [FAQ here](https://ourworldindata.org/coronavirus-testing#do-you-rely-on-any-non-official-sources) we regularly audit the accuracy of this repository against direct official channels. Note that, due to the way the data is presented by the official source, the time series may be impacted by retrospective revisions made by the source – see our [FAQ here](https://ourworldindata.org/coronavirus-testing#does-your-data-reflect-retrospective-updates-made-by-the-source).</t>
@@ -397,7 +398,7 @@
     <t xml:space="preserve">Cote d'Ivoire - samples tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.facebook.com/Mshpci/posts/1673896616109359</t>
+    <t xml:space="preserve">https://www.facebook.com/Mshpci/posts/1676619775837043</t>
   </si>
   <si>
     <t xml:space="preserve">Ministry of Health and Public Hygiene</t>
@@ -476,7 +477,7 @@
     <t xml:space="preserve">Democratic Republic of Congo - samples tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/CMR_Covid19_RDC/status/1295660670885732352/photo/1</t>
+    <t xml:space="preserve">https://twitter.com/CMR_Covid19_RDC/status/1296733289567399936/photo/1</t>
   </si>
   <si>
     <t xml:space="preserve">DRC COVID-19 Pandemic Response Multisectoral Committee</t>
@@ -494,7 +495,7 @@
     <t xml:space="preserve">Denmark - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://files.ssi.dk/Data-Epidemiologiske-Rapport-20082020-jh34</t>
+    <t xml:space="preserve">https://files.ssi.dk/Data-Epidemiologiske-Rapport-21082020-pp98</t>
   </si>
   <si>
     <t xml:space="preserve">Statens Serum Institut</t>
@@ -512,7 +513,7 @@
     <t xml:space="preserve">Ecuador - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.gestionderiesgos.gob.ec/wp-content/uploads/2020/08/INFOGRAFIA-NACIONALCOVI-19-COE-NACIONAL-08h00-19082020.pdf</t>
+    <t xml:space="preserve">https://www.gestionderiesgos.gob.ec/wp-content/uploads/2020/08/INFOGRAFIA-NACIONALCOVI-19-COE-NACIONAL-08h00-22082020.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">Government of Ecuador</t>
@@ -538,7 +539,7 @@
     <t xml:space="preserve">El Salvador - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.facebook.com/nayibbukele/posts/3164190897000413</t>
+    <t xml:space="preserve">https://www.facebook.com/nayibbukele/posts/3173404349412401</t>
   </si>
   <si>
     <t xml:space="preserve">Government of El Salvador</t>
@@ -582,7 +583,7 @@
     <t xml:space="preserve">Ethiopia - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/EPHIEthiopia/status/1296485928240918531</t>
+    <t xml:space="preserve">https://twitter.com/EPHIEthiopia/status/1297581159547834370</t>
   </si>
   <si>
     <t xml:space="preserve">Ethiopian Public Health Institute</t>
@@ -751,7 +752,7 @@
     <t xml:space="preserve">Greece - samples tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://eody.gov.gr/covid-gr-daily-report-19-08-2020/</t>
+    <t xml:space="preserve">https://eody.gov.gr/covid-gr-daily-report-23-08-2020/</t>
   </si>
   <si>
     <t xml:space="preserve">National Organization of Public Health</t>
@@ -890,7 +891,7 @@
     <t xml:space="preserve">Iran - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">http://irangov.ir/detail/345517</t>
+    <t xml:space="preserve">http://irangov.ir/detail/345697</t>
   </si>
   <si>
     <t xml:space="preserve">Government of Iran</t>
@@ -948,7 +949,7 @@
     <t xml:space="preserve">Israel - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://govextra.gov.il/media/24739/covid-19-data-israel-13082020.csv</t>
+    <t xml:space="preserve">https://govextra.gov.il/media/25358/covid19-data-israel-17082020.csv</t>
   </si>
   <si>
     <t xml:space="preserve">Israel Ministry of Health</t>
@@ -1007,7 +1008,7 @@
     <t xml:space="preserve">Japan - people tested (incl. non-PCR)</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.mhlw.go.jp/stf/newpage_13073.html</t>
+    <t xml:space="preserve">https://www.mhlw.go.jp/stf/newpage_13127.html</t>
   </si>
   <si>
     <t xml:space="preserve">Ministry of Health, Labor and Welfare Press Release</t>
@@ -1032,10 +1033,10 @@
     <t xml:space="preserve">Japan - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.mhlw.go.jp/content/10906000/000661150.pdf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The cumulative total reported in the press release matches the cumulative total calculated from the weekly and daily figures reported by the MOH.</t>
+    <t xml:space="preserve">https://www.mhlw.go.jp/content/10906000/000661890.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The cumulative total reported in the press release (1,609,485) does not sum to the cumulative total calculated from the weekly and daily figures reported by the MOH. See: https://www.mhlw.go.jp/content/10906000/000661890.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">On 11 April 2020, the MOH started providing a daily time series on the "Implementation status of PCR tests for new coronavirus in Japan (based on the date on which results were determined" (via Google translate). 
@@ -1066,7 +1067,7 @@
     <t xml:space="preserve">Kenya - samples tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/MOH_Kenya/status/1295717267376943106</t>
+    <t xml:space="preserve">https://twitter.com/MOH_Kenya/status/1297506691454574593</t>
   </si>
   <si>
     <t xml:space="preserve">Kenya Ministry of Health</t>
@@ -1088,7 +1089,7 @@
     <t xml:space="preserve">Kuwait - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/KUWAIT_MOH/status/1296054390097350662/photo/1</t>
+    <t xml:space="preserve">https://twitter.com/KUWAIT_MOH/status/1296748941434851328/photo/1</t>
   </si>
   <si>
     <t xml:space="preserve">Kuwait Ministry of Health</t>
@@ -1154,7 +1155,7 @@
     <t xml:space="preserve">Malaysia - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">http://covid-19.moh.gov.my/terkini/082020/situasi-terkini-20-ogos-2020</t>
+    <t xml:space="preserve">http://covid-19.moh.gov.my/terkini/082020/situasi-terkini-23-ogos-2020</t>
   </si>
   <si>
     <t xml:space="preserve">Ministry of Health Malaysia</t>
@@ -1180,7 +1181,7 @@
     <t xml:space="preserve">Maldives - samples tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/HPA_MV/status/1296133369865134081/photo/1</t>
+    <t xml:space="preserve">https://twitter.com/HPA_MV/status/1296854798076174336/photo/1</t>
   </si>
   <si>
     <t xml:space="preserve">Maldives Health Protection Agency</t>
@@ -1247,7 +1248,7 @@
     <t xml:space="preserve">Morocco - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/Ministere_Sante/status/1296132593813946368/photo/1</t>
+    <t xml:space="preserve">https://twitter.com/Ministere_Sante/status/1296857850669670401</t>
   </si>
   <si>
     <t xml:space="preserve">Morocco Ministry of Health</t>
@@ -1490,7 +1491,7 @@
     <t xml:space="preserve">Philippines - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://drive.google.com/drive/folders/1pP9BFBJuu4UF5KpPMvnXeWJjq5bHJk8f</t>
+    <t xml:space="preserve">https://drive.google.com/drive/folders/1QUIqtJtcgNfZRKIt0BpECegkx-z7IDhi?usp=sharing</t>
   </si>
   <si>
     <t xml:space="preserve">Philippines Department of Health</t>
@@ -1510,7 +1511,7 @@
     <t xml:space="preserve">Poland - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/MZ_GOV_PL/status/1296371398386913281</t>
+    <t xml:space="preserve">https://twitter.com/MZ_GOV_PL/status/1297458560926801922</t>
   </si>
   <si>
     <t xml:space="preserve">Poland Ministry of Health</t>
@@ -1578,7 +1579,7 @@
     <t xml:space="preserve">Romania - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://gov.ro/ro/media/comunicate/buletin-de-presa-20-august-2020-ora-13-00&amp;page=1</t>
+    <t xml:space="preserve">https://gov.ro/ro/media/comunicate/buletin-de-presa-23-august-2020-ora-13-00&amp;page=1</t>
   </si>
   <si>
     <t xml:space="preserve">Ministry of Internal Affairs</t>
@@ -1601,7 +1602,7 @@
     <t xml:space="preserve">Russia - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://rospotrebnadzor.ru/about/info/news/news_details.php?ELEMENT_ID=15210</t>
+    <t xml:space="preserve">https://rospotrebnadzor.ru/about/info/news/news_details.php?ELEMENT_ID=15223</t>
   </si>
   <si>
     <t xml:space="preserve">Government of the Russian Federation</t>
@@ -1621,7 +1622,7 @@
     <t xml:space="preserve">Rwanda - samples tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/RwandaHealth/status/1296181973946425350</t>
+    <t xml:space="preserve">https://twitter.com/RwandaHealth/status/1297637879523561475</t>
   </si>
   <si>
     <t xml:space="preserve">Rwanda Ministry of Health</t>
@@ -1795,7 +1796,7 @@
     <t xml:space="preserve">South Korea - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.cdc.go.kr/board/board.es?mid=&amp;bid=0030&amp;act=view&amp;list_no=368171&amp;tag=&amp;nPage=1</t>
+    <t xml:space="preserve">https://www.cdc.go.kr/board/board.es?mid=&amp;bid=0030&amp;act=view&amp;list_no=368204&amp;tag=&amp;nPage=1</t>
   </si>
   <si>
     <t xml:space="preserve">South Korea CDC</t>
@@ -1917,7 +1918,7 @@
     <t xml:space="preserve">Thailand - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://ddc.moph.go.th/viralpneumonia/file/situation/situation-no230-200863.pdf</t>
+    <t xml:space="preserve">https://ddc.moph.go.th/viralpneumonia/file/situation/situation-no233-230863.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">Department of Disease Control</t>
@@ -2005,7 +2006,7 @@
     <t xml:space="preserve">Uganda - samples tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/MinofHealthUG/status/1296425945960767489/photo/2</t>
+    <t xml:space="preserve">https://twitter.com/MinofHealthUG/status/1296774060966379523/photo/1</t>
   </si>
   <si>
     <t xml:space="preserve">Uganda Ministry of Health</t>
@@ -2145,7 +2146,7 @@
     <t xml:space="preserve">Uruguay - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.gub.uy/ministerio-salud-publica/comunicacion/noticias/informe-situacion-sobre-coronavirus-covid-19-uruguay-20-agosto</t>
+    <t xml:space="preserve">https://www.gub.uy/ministerio-salud-publica/comunicacion/noticias/informe-situacion-sobre-coronavirus-covid-19-uruguay-22-agosto</t>
   </si>
   <si>
     <t xml:space="preserve">https://www.gub.uy/ministerio-salud-publica/comunicacion/noticias</t>
@@ -2183,7 +2184,7 @@
     <t xml:space="preserve">Zimbabwe - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/MoHCCZim/status/1296519577103466508</t>
+    <t xml:space="preserve">https://twitter.com/MoHCCZim/status/1297591437534666756</t>
   </si>
   <si>
     <t xml:space="preserve">Zimbabwe Ministry of Health and Child Care</t>
@@ -2657,7 +2658,7 @@
         <v>25</v>
       </c>
       <c r="C3" s="1" t="n">
-        <v>44063</v>
+        <v>44066</v>
       </c>
       <c r="D3" t="s">
         <v>26</v>
@@ -2667,31 +2668,31 @@
       </c>
       <c r="F3"/>
       <c r="G3" t="n">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="H3" t="n">
-        <v>1095233</v>
+        <v>1150552</v>
       </c>
       <c r="I3" t="n">
-        <v>24.233</v>
+        <v>25.457</v>
       </c>
       <c r="J3" t="n">
-        <v>5714</v>
+        <v>2589</v>
       </c>
       <c r="K3" t="n">
-        <v>0.126</v>
+        <v>0.057</v>
       </c>
       <c r="L3" t="n">
-        <v>13231</v>
+        <v>13752</v>
       </c>
       <c r="M3" t="n">
-        <v>0.293</v>
+        <v>0.304</v>
       </c>
       <c r="N3" t="n">
-        <v>0.486</v>
+        <v>0.484</v>
       </c>
       <c r="O3" t="n">
-        <v>2.056</v>
+        <v>2.065</v>
       </c>
       <c r="P3" t="s">
         <v>22</v>
@@ -2714,7 +2715,7 @@
         <v>30</v>
       </c>
       <c r="C4" s="1" t="n">
-        <v>44063</v>
+        <v>44066</v>
       </c>
       <c r="D4" t="s">
         <v>31</v>
@@ -2724,31 +2725,27 @@
       </c>
       <c r="F4"/>
       <c r="G4" t="n">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="H4" t="n">
-        <v>5508831</v>
+        <v>5706587</v>
       </c>
       <c r="I4" t="n">
-        <v>216.034</v>
-      </c>
-      <c r="J4" t="n">
-        <v>68336</v>
-      </c>
-      <c r="K4" t="n">
-        <v>2.68</v>
-      </c>
+        <v>223.789</v>
+      </c>
+      <c r="J4"/>
+      <c r="K4"/>
       <c r="L4" t="n">
-        <v>57007</v>
+        <v>58433</v>
       </c>
       <c r="M4" t="n">
-        <v>2.236</v>
+        <v>2.292</v>
       </c>
       <c r="N4" t="n">
-        <v>0.005</v>
+        <v>0.004</v>
       </c>
       <c r="O4" t="n">
-        <v>213.853</v>
+        <v>261.028</v>
       </c>
       <c r="P4" t="s">
         <v>32</v>
@@ -2771,7 +2768,7 @@
         <v>36</v>
       </c>
       <c r="C5" s="1" t="n">
-        <v>44063</v>
+        <v>44067</v>
       </c>
       <c r="D5" t="s">
         <v>37</v>
@@ -2781,31 +2778,31 @@
       </c>
       <c r="F5"/>
       <c r="G5" t="n">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="H5" t="n">
-        <v>1061437</v>
+        <v>1101206</v>
       </c>
       <c r="I5" t="n">
-        <v>117.854</v>
+        <v>122.269</v>
       </c>
       <c r="J5" t="n">
-        <v>13221</v>
+        <v>6219</v>
       </c>
       <c r="K5" t="n">
-        <v>1.468</v>
+        <v>0.691</v>
       </c>
       <c r="L5" t="n">
-        <v>9990</v>
+        <v>11020</v>
       </c>
       <c r="M5" t="n">
-        <v>1.109</v>
+        <v>1.224</v>
       </c>
       <c r="N5" t="n">
-        <v>0.026</v>
+        <v>0.024</v>
       </c>
       <c r="O5" t="n">
-        <v>38.872</v>
+        <v>41.34</v>
       </c>
       <c r="P5" t="s">
         <v>39</v>
@@ -2828,7 +2825,7 @@
         <v>43</v>
       </c>
       <c r="C6" s="1" t="n">
-        <v>44064</v>
+        <v>44067</v>
       </c>
       <c r="D6" t="s">
         <v>44</v>
@@ -2838,24 +2835,32 @@
       </c>
       <c r="F6"/>
       <c r="G6" t="n">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="H6" t="n">
-        <v>1011805</v>
+        <v>1039571</v>
       </c>
       <c r="I6" t="n">
-        <v>594.626</v>
-      </c>
-      <c r="J6"/>
-      <c r="K6"/>
+        <v>610.943</v>
+      </c>
+      <c r="J6" t="n">
+        <v>9602</v>
+      </c>
+      <c r="K6" t="n">
+        <v>5.643</v>
+      </c>
       <c r="L6" t="n">
-        <v>9572</v>
+        <v>9653</v>
       </c>
       <c r="M6" t="n">
-        <v>5.625</v>
-      </c>
-      <c r="N6"/>
-      <c r="O6"/>
+        <v>5.673</v>
+      </c>
+      <c r="N6" t="n">
+        <v>0.039</v>
+      </c>
+      <c r="O6" t="n">
+        <v>25.909</v>
+      </c>
       <c r="P6" t="s">
         <v>46</v>
       </c>
@@ -2877,7 +2882,7 @@
         <v>50</v>
       </c>
       <c r="C7" s="1" t="n">
-        <v>44061</v>
+        <v>44066</v>
       </c>
       <c r="D7" t="s">
         <v>51</v>
@@ -2887,31 +2892,31 @@
       </c>
       <c r="F7"/>
       <c r="G7" t="n">
-        <v>167</v>
+        <v>172</v>
       </c>
       <c r="H7" t="n">
-        <v>1378819</v>
+        <v>1442656</v>
       </c>
       <c r="I7" t="n">
-        <v>8.372</v>
+        <v>8.76</v>
       </c>
       <c r="J7" t="n">
-        <v>14630</v>
+        <v>10801</v>
       </c>
       <c r="K7" t="n">
-        <v>0.089</v>
+        <v>0.066</v>
       </c>
       <c r="L7" t="n">
-        <v>12976</v>
+        <v>12999</v>
       </c>
       <c r="M7" t="n">
         <v>0.079</v>
       </c>
       <c r="N7" t="n">
-        <v>0.205</v>
+        <v>0.199</v>
       </c>
       <c r="O7" t="n">
-        <v>4.874</v>
+        <v>5.027</v>
       </c>
       <c r="P7" t="s">
         <v>52</v>
@@ -2934,7 +2939,7 @@
         <v>57</v>
       </c>
       <c r="C8" s="1" t="n">
-        <v>44055</v>
+        <v>44066</v>
       </c>
       <c r="D8" t="s">
         <v>58</v>
@@ -2944,31 +2949,31 @@
       </c>
       <c r="F8"/>
       <c r="G8" t="n">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="H8" t="n">
-        <v>1384026</v>
+        <v>1474075</v>
       </c>
       <c r="I8" t="n">
-        <v>146.468</v>
+        <v>155.998</v>
       </c>
       <c r="J8" t="n">
-        <v>6486</v>
+        <v>8520</v>
       </c>
       <c r="K8" t="n">
-        <v>0.686</v>
+        <v>0.902</v>
       </c>
       <c r="L8" t="n">
-        <v>6998</v>
+        <v>8205</v>
       </c>
       <c r="M8" t="n">
-        <v>0.741</v>
+        <v>0.868</v>
       </c>
       <c r="N8" t="n">
         <v>0.015</v>
       </c>
       <c r="O8" t="n">
-        <v>64.882</v>
+        <v>66.707</v>
       </c>
       <c r="P8" t="s">
         <v>59</v>
@@ -2991,7 +2996,7 @@
         <v>63</v>
       </c>
       <c r="C9" s="1" t="n">
-        <v>44062</v>
+        <v>44065</v>
       </c>
       <c r="D9" t="s">
         <v>64</v>
@@ -3001,31 +3006,31 @@
       </c>
       <c r="F9"/>
       <c r="G9" t="n">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="H9" t="n">
-        <v>2072738</v>
+        <v>2135342</v>
       </c>
       <c r="I9" t="n">
-        <v>178.844</v>
+        <v>184.246</v>
       </c>
       <c r="J9" t="n">
-        <v>18492</v>
+        <v>12962</v>
       </c>
       <c r="K9" t="n">
-        <v>1.596</v>
+        <v>1.118</v>
       </c>
       <c r="L9" t="n">
-        <v>17796</v>
+        <v>19059</v>
       </c>
       <c r="M9" t="n">
-        <v>1.536</v>
+        <v>1.644</v>
       </c>
       <c r="N9" t="n">
-        <v>0.023</v>
+        <v>0.025</v>
       </c>
       <c r="O9" t="n">
-        <v>44.363</v>
+        <v>40.749</v>
       </c>
       <c r="P9" t="s">
         <v>65</v>
@@ -3048,7 +3053,7 @@
         <v>69</v>
       </c>
       <c r="C10" s="1" t="n">
-        <v>44061</v>
+        <v>44063</v>
       </c>
       <c r="D10" t="s">
         <v>70</v>
@@ -3058,31 +3063,31 @@
       </c>
       <c r="F10"/>
       <c r="G10" t="n">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="H10" t="n">
-        <v>204818</v>
+        <v>211318</v>
       </c>
       <c r="I10" t="n">
-        <v>17.546</v>
+        <v>18.103</v>
       </c>
       <c r="J10" t="n">
-        <v>4607</v>
+        <v>2680</v>
       </c>
       <c r="K10" t="n">
-        <v>0.395</v>
+        <v>0.23</v>
       </c>
       <c r="L10" t="n">
-        <v>3072</v>
+        <v>3126</v>
       </c>
       <c r="M10" t="n">
-        <v>0.263</v>
+        <v>0.268</v>
       </c>
       <c r="N10" t="n">
-        <v>0.446</v>
+        <v>0.456</v>
       </c>
       <c r="O10" t="n">
-        <v>2.243</v>
+        <v>2.193</v>
       </c>
       <c r="P10" t="s">
         <v>45</v>
@@ -3156,7 +3161,7 @@
         <v>81</v>
       </c>
       <c r="C12" s="1" t="n">
-        <v>44064</v>
+        <v>44067</v>
       </c>
       <c r="D12" t="s">
         <v>82</v>
@@ -3166,28 +3171,32 @@
       </c>
       <c r="F12"/>
       <c r="G12" t="n">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="H12" t="n">
-        <v>358723</v>
+        <v>370786</v>
       </c>
       <c r="I12" t="n">
-        <v>51.626</v>
+        <v>53.362</v>
       </c>
       <c r="J12" t="n">
-        <v>6844</v>
+        <v>2288</v>
       </c>
       <c r="K12" t="n">
-        <v>0.985</v>
+        <v>0.329</v>
       </c>
       <c r="L12" t="n">
-        <v>4839</v>
+        <v>5211</v>
       </c>
       <c r="M12" t="n">
-        <v>0.696</v>
-      </c>
-      <c r="N12"/>
-      <c r="O12"/>
+        <v>0.75</v>
+      </c>
+      <c r="N12" t="n">
+        <v>0.024</v>
+      </c>
+      <c r="O12" t="n">
+        <v>42.317</v>
+      </c>
       <c r="P12" t="s">
         <v>84</v>
       </c>
@@ -3209,7 +3218,7 @@
         <v>87</v>
       </c>
       <c r="C13" s="1" t="n">
-        <v>44064</v>
+        <v>44067</v>
       </c>
       <c r="D13" t="s">
         <v>88</v>
@@ -3219,28 +3228,32 @@
       </c>
       <c r="F13"/>
       <c r="G13" t="n">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="H13" t="n">
-        <v>4974215</v>
+        <v>5115490</v>
       </c>
       <c r="I13" t="n">
-        <v>131.795</v>
+        <v>135.538</v>
       </c>
       <c r="J13" t="n">
-        <v>48769</v>
+        <v>38756</v>
       </c>
       <c r="K13" t="n">
-        <v>1.292</v>
+        <v>1.027</v>
       </c>
       <c r="L13" t="n">
-        <v>48444</v>
+        <v>48161</v>
       </c>
       <c r="M13" t="n">
-        <v>1.284</v>
-      </c>
-      <c r="N13"/>
-      <c r="O13"/>
+        <v>1.276</v>
+      </c>
+      <c r="N13" t="n">
+        <v>0.008</v>
+      </c>
+      <c r="O13" t="n">
+        <v>120.017</v>
+      </c>
       <c r="P13" t="s">
         <v>89</v>
       </c>
@@ -3262,7 +3275,7 @@
         <v>92</v>
       </c>
       <c r="C14" s="1" t="n">
-        <v>44063</v>
+        <v>44066</v>
       </c>
       <c r="D14" t="s">
         <v>93</v>
@@ -3274,31 +3287,31 @@
         <v>94</v>
       </c>
       <c r="G14" t="n">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="H14" t="n">
-        <v>2113632</v>
+        <v>2204009</v>
       </c>
       <c r="I14" t="n">
-        <v>110.568</v>
+        <v>115.295</v>
       </c>
       <c r="J14" t="n">
-        <v>26278</v>
+        <v>31981</v>
       </c>
       <c r="K14" t="n">
-        <v>1.375</v>
+        <v>1.673</v>
       </c>
       <c r="L14" t="n">
-        <v>25863</v>
+        <v>26345</v>
       </c>
       <c r="M14" t="n">
-        <v>1.353</v>
+        <v>1.378</v>
       </c>
       <c r="N14" t="n">
-        <v>0.066</v>
+        <v>0.064</v>
       </c>
       <c r="O14" t="n">
-        <v>15.253</v>
+        <v>15.62</v>
       </c>
       <c r="P14" t="s">
         <v>95</v>
@@ -3321,7 +3334,7 @@
         <v>99</v>
       </c>
       <c r="C15" s="1" t="n">
-        <v>44063</v>
+        <v>44066</v>
       </c>
       <c r="D15" t="s">
         <v>100</v>
@@ -3331,31 +3344,31 @@
       </c>
       <c r="F15"/>
       <c r="G15" t="n">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="H15" t="n">
-        <v>2309447</v>
+        <v>2396892</v>
       </c>
       <c r="I15" t="n">
-        <v>45.388</v>
+        <v>47.106</v>
       </c>
       <c r="J15" t="n">
-        <v>31932</v>
+        <v>22824</v>
       </c>
       <c r="K15" t="n">
-        <v>0.628</v>
+        <v>0.449</v>
       </c>
       <c r="L15" t="n">
-        <v>35159</v>
+        <v>31272</v>
       </c>
       <c r="M15" t="n">
-        <v>0.691</v>
+        <v>0.615</v>
       </c>
       <c r="N15" t="n">
-        <v>0.324</v>
+        <v>0.349</v>
       </c>
       <c r="O15" t="n">
-        <v>3.09</v>
+        <v>2.865</v>
       </c>
       <c r="P15" t="s">
         <v>101</v>
@@ -3378,7 +3391,7 @@
         <v>105</v>
       </c>
       <c r="C16" s="1" t="n">
-        <v>44062</v>
+        <v>44065</v>
       </c>
       <c r="D16" t="s">
         <v>106</v>
@@ -3388,25 +3401,25 @@
       </c>
       <c r="F16"/>
       <c r="G16" t="n">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="H16" t="n">
-        <v>109207</v>
+        <v>114371</v>
       </c>
       <c r="I16" t="n">
-        <v>21.438</v>
+        <v>22.452</v>
       </c>
       <c r="J16" t="n">
-        <v>1535</v>
+        <v>2131</v>
       </c>
       <c r="K16" t="n">
-        <v>0.301</v>
+        <v>0.418</v>
       </c>
       <c r="L16" t="n">
-        <v>1820</v>
+        <v>1648</v>
       </c>
       <c r="M16" t="n">
-        <v>0.357</v>
+        <v>0.324</v>
       </c>
       <c r="N16"/>
       <c r="O16"/>
@@ -3431,7 +3444,7 @@
         <v>111</v>
       </c>
       <c r="C17" s="1" t="n">
-        <v>44062</v>
+        <v>44065</v>
       </c>
       <c r="D17" t="s">
         <v>112</v>
@@ -3441,31 +3454,31 @@
       </c>
       <c r="F17"/>
       <c r="G17" t="n">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="H17" t="n">
-        <v>116785</v>
+        <v>119166</v>
       </c>
       <c r="I17" t="n">
-        <v>4.427</v>
+        <v>4.518</v>
       </c>
       <c r="J17" t="n">
-        <v>1447</v>
+        <v>1101</v>
       </c>
       <c r="K17" t="n">
-        <v>0.055</v>
+        <v>0.042</v>
       </c>
       <c r="L17" t="n">
-        <v>882</v>
+        <v>891</v>
       </c>
       <c r="M17" t="n">
-        <v>0.033</v>
+        <v>0.034</v>
       </c>
       <c r="N17" t="n">
-        <v>0.049</v>
+        <v>0.06</v>
       </c>
       <c r="O17" t="n">
-        <v>20.376</v>
+        <v>16.632</v>
       </c>
       <c r="P17" t="s">
         <v>113</v>
@@ -3488,7 +3501,7 @@
         <v>117</v>
       </c>
       <c r="C18" s="1" t="n">
-        <v>44063</v>
+        <v>44066</v>
       </c>
       <c r="D18" t="s">
         <v>118</v>
@@ -3498,31 +3511,31 @@
       </c>
       <c r="F18"/>
       <c r="G18" t="n">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="H18" t="n">
-        <v>144521</v>
+        <v>150460</v>
       </c>
       <c r="I18" t="n">
-        <v>35.204</v>
+        <v>36.65</v>
       </c>
       <c r="J18" t="n">
-        <v>2397</v>
+        <v>1718</v>
       </c>
       <c r="K18" t="n">
-        <v>0.584</v>
+        <v>0.418</v>
       </c>
       <c r="L18" t="n">
-        <v>1575</v>
+        <v>1829</v>
       </c>
       <c r="M18" t="n">
-        <v>0.384</v>
+        <v>0.446</v>
       </c>
       <c r="N18" t="n">
-        <v>0.109</v>
+        <v>0.116</v>
       </c>
       <c r="O18" t="n">
-        <v>9.157</v>
+        <v>8.651</v>
       </c>
       <c r="P18" t="s">
         <v>119</v>
@@ -3545,7 +3558,7 @@
         <v>123</v>
       </c>
       <c r="C19" s="1" t="n">
-        <v>44062</v>
+        <v>44065</v>
       </c>
       <c r="D19" t="s">
         <v>124</v>
@@ -3557,31 +3570,31 @@
         <v>126</v>
       </c>
       <c r="G19" t="n">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="H19" t="n">
-        <v>346439</v>
+        <v>361092</v>
       </c>
       <c r="I19" t="n">
-        <v>30.586</v>
+        <v>31.88</v>
       </c>
       <c r="J19" t="n">
-        <v>5116</v>
+        <v>4867</v>
       </c>
       <c r="K19" t="n">
-        <v>0.452</v>
+        <v>0.43</v>
       </c>
       <c r="L19" t="n">
-        <v>4563</v>
+        <v>4772</v>
       </c>
       <c r="M19" t="n">
-        <v>0.403</v>
+        <v>0.421</v>
       </c>
       <c r="N19" t="n">
-        <v>0.01</v>
+        <v>0.011</v>
       </c>
       <c r="O19" t="n">
-        <v>101.4</v>
+        <v>94.629</v>
       </c>
       <c r="P19" t="s">
         <v>125</v>
@@ -3604,7 +3617,7 @@
         <v>130</v>
       </c>
       <c r="C20" s="1" t="n">
-        <v>44062</v>
+        <v>44064</v>
       </c>
       <c r="D20" t="s">
         <v>131</v>
@@ -3614,31 +3627,31 @@
       </c>
       <c r="F20"/>
       <c r="G20" t="n">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="H20" t="n">
-        <v>820151</v>
+        <v>835603</v>
       </c>
       <c r="I20" t="n">
-        <v>76.585</v>
+        <v>78.028</v>
       </c>
       <c r="J20" t="n">
-        <v>7185</v>
+        <v>9363</v>
       </c>
       <c r="K20" t="n">
-        <v>0.671</v>
+        <v>0.874</v>
       </c>
       <c r="L20" t="n">
-        <v>6237</v>
+        <v>6303</v>
       </c>
       <c r="M20" t="n">
-        <v>0.582</v>
+        <v>0.589</v>
       </c>
       <c r="N20" t="n">
-        <v>0.039</v>
+        <v>0.037</v>
       </c>
       <c r="O20" t="n">
-        <v>25.682</v>
+        <v>26.838</v>
       </c>
       <c r="P20" t="s">
         <v>45</v>
@@ -3661,7 +3674,7 @@
         <v>135</v>
       </c>
       <c r="C21" s="1" t="n">
-        <v>44060</v>
+        <v>44063</v>
       </c>
       <c r="D21" t="s">
         <v>136</v>
@@ -3671,18 +3684,18 @@
       </c>
       <c r="F21"/>
       <c r="G21" t="n">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="H21"/>
       <c r="I21"/>
       <c r="J21" t="n">
-        <v>333</v>
+        <v>309</v>
       </c>
       <c r="K21" t="n">
-        <v>0.004</v>
+        <v>0.003</v>
       </c>
       <c r="L21" t="n">
-        <v>380</v>
+        <v>351</v>
       </c>
       <c r="M21" t="n">
         <v>0.004</v>
@@ -3691,7 +3704,7 @@
         <v>0.083</v>
       </c>
       <c r="O21" t="n">
-        <v>11.982</v>
+        <v>12.103</v>
       </c>
       <c r="P21" t="s">
         <v>137</v>
@@ -3714,7 +3727,7 @@
         <v>141</v>
       </c>
       <c r="C22" s="1" t="n">
-        <v>44062</v>
+        <v>44063</v>
       </c>
       <c r="D22" t="s">
         <v>142</v>
@@ -3724,31 +3737,31 @@
       </c>
       <c r="F22"/>
       <c r="G22" t="n">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="H22" t="n">
-        <v>2035007</v>
+        <v>2063958</v>
       </c>
       <c r="I22" t="n">
-        <v>351.336</v>
+        <v>356.334</v>
       </c>
       <c r="J22" t="n">
-        <v>7704</v>
+        <v>6044</v>
       </c>
       <c r="K22" t="n">
-        <v>1.33</v>
+        <v>1.043</v>
       </c>
       <c r="L22" t="n">
-        <v>27990</v>
+        <v>27314</v>
       </c>
       <c r="M22" t="n">
-        <v>4.832</v>
+        <v>4.716</v>
       </c>
       <c r="N22" t="n">
         <v>0.005</v>
       </c>
       <c r="O22" t="n">
-        <v>218.672</v>
+        <v>219.768</v>
       </c>
       <c r="P22" t="s">
         <v>143</v>
@@ -3771,7 +3784,7 @@
         <v>147</v>
       </c>
       <c r="C23" s="1" t="n">
-        <v>44062</v>
+        <v>44065</v>
       </c>
       <c r="D23" t="s">
         <v>148</v>
@@ -3783,25 +3796,25 @@
         <v>150</v>
       </c>
       <c r="G23" t="n">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="H23" t="n">
-        <v>231883</v>
+        <v>239766</v>
       </c>
       <c r="I23" t="n">
-        <v>13.143</v>
+        <v>13.59</v>
       </c>
       <c r="J23" t="n">
-        <v>3845</v>
+        <v>1608</v>
       </c>
       <c r="K23" t="n">
-        <v>0.218</v>
+        <v>0.091</v>
       </c>
       <c r="L23" t="n">
-        <v>2956</v>
+        <v>2658</v>
       </c>
       <c r="M23" t="n">
-        <v>0.168</v>
+        <v>0.151</v>
       </c>
       <c r="N23"/>
       <c r="O23"/>
@@ -3826,7 +3839,7 @@
         <v>154</v>
       </c>
       <c r="C24" s="1" t="n">
-        <v>44062</v>
+        <v>44065</v>
       </c>
       <c r="D24" t="s">
         <v>155</v>
@@ -3836,31 +3849,31 @@
       </c>
       <c r="F24"/>
       <c r="G24" t="n">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="H24" t="n">
-        <v>288307</v>
+        <v>295665</v>
       </c>
       <c r="I24" t="n">
-        <v>44.449</v>
+        <v>45.584</v>
       </c>
       <c r="J24" t="n">
-        <v>2414</v>
+        <v>2447</v>
       </c>
       <c r="K24" t="n">
-        <v>0.372</v>
+        <v>0.377</v>
       </c>
       <c r="L24" t="n">
-        <v>2464</v>
+        <v>2460</v>
       </c>
       <c r="M24" t="n">
-        <v>0.38</v>
+        <v>0.379</v>
       </c>
       <c r="N24" t="n">
-        <v>0.127</v>
+        <v>0.122</v>
       </c>
       <c r="O24" t="n">
-        <v>7.865</v>
+        <v>8.177</v>
       </c>
       <c r="P24" t="s">
         <v>156</v>
@@ -3883,7 +3896,7 @@
         <v>160</v>
       </c>
       <c r="C25" s="1" t="n">
-        <v>44062</v>
+        <v>44066</v>
       </c>
       <c r="D25" t="s">
         <v>161</v>
@@ -3893,31 +3906,31 @@
       </c>
       <c r="F25"/>
       <c r="G25" t="n">
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="H25" t="n">
-        <v>138166</v>
+        <v>140985</v>
       </c>
       <c r="I25" t="n">
-        <v>104.155</v>
+        <v>106.28</v>
       </c>
       <c r="J25" t="n">
-        <v>885</v>
+        <v>320</v>
       </c>
       <c r="K25" t="n">
-        <v>0.667</v>
+        <v>0.241</v>
       </c>
       <c r="L25" t="n">
-        <v>1050</v>
+        <v>876</v>
       </c>
       <c r="M25" t="n">
-        <v>0.792</v>
+        <v>0.66</v>
       </c>
       <c r="N25" t="n">
-        <v>0.004</v>
+        <v>0.013</v>
       </c>
       <c r="O25" t="n">
-        <v>222.727</v>
+        <v>75.704</v>
       </c>
       <c r="P25" t="s">
         <v>163</v>
@@ -3940,7 +3953,7 @@
         <v>168</v>
       </c>
       <c r="C26" s="1" t="n">
-        <v>44063</v>
+        <v>44066</v>
       </c>
       <c r="D26" t="s">
         <v>169</v>
@@ -3950,31 +3963,31 @@
       </c>
       <c r="F26"/>
       <c r="G26" t="n">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="H26" t="n">
-        <v>694093</v>
+        <v>757057</v>
       </c>
       <c r="I26" t="n">
-        <v>6.038</v>
+        <v>6.585</v>
       </c>
       <c r="J26" t="n">
-        <v>21456</v>
+        <v>20153</v>
       </c>
       <c r="K26" t="n">
-        <v>0.187</v>
+        <v>0.175</v>
       </c>
       <c r="L26" t="n">
-        <v>20568</v>
+        <v>21085</v>
       </c>
       <c r="M26" t="n">
-        <v>0.179</v>
+        <v>0.183</v>
       </c>
       <c r="N26" t="n">
-        <v>0.062</v>
+        <v>0.069</v>
       </c>
       <c r="O26" t="n">
-        <v>16.105</v>
+        <v>14.557</v>
       </c>
       <c r="P26" t="s">
         <v>170</v>
@@ -4052,7 +4065,7 @@
         <v>179</v>
       </c>
       <c r="C28" s="1" t="n">
-        <v>44061</v>
+        <v>44066</v>
       </c>
       <c r="D28" t="s">
         <v>180</v>
@@ -4062,31 +4075,31 @@
       </c>
       <c r="F28"/>
       <c r="G28" t="n">
-        <v>176</v>
+        <v>181</v>
       </c>
       <c r="H28" t="n">
-        <v>517645</v>
+        <v>551715</v>
       </c>
       <c r="I28" t="n">
-        <v>93.426</v>
+        <v>99.575</v>
       </c>
       <c r="J28" t="n">
-        <v>7891</v>
+        <v>822</v>
       </c>
       <c r="K28" t="n">
-        <v>1.424</v>
+        <v>0.148</v>
       </c>
       <c r="L28" t="n">
-        <v>10189</v>
+        <v>7487</v>
       </c>
       <c r="M28" t="n">
-        <v>1.839</v>
+        <v>1.351</v>
       </c>
       <c r="N28" t="n">
-        <v>0.002</v>
+        <v>0.003</v>
       </c>
       <c r="O28" t="n">
-        <v>472.338</v>
+        <v>347.079</v>
       </c>
       <c r="P28" t="s">
         <v>182</v>
@@ -4109,7 +4122,7 @@
         <v>185</v>
       </c>
       <c r="C29" s="1" t="n">
-        <v>44060</v>
+        <v>44063</v>
       </c>
       <c r="D29" t="s">
         <v>186</v>
@@ -4119,27 +4132,27 @@
       </c>
       <c r="F29"/>
       <c r="G29" t="n">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="H29"/>
       <c r="I29"/>
       <c r="J29" t="n">
-        <v>127008</v>
+        <v>115009</v>
       </c>
       <c r="K29" t="n">
-        <v>1.946</v>
+        <v>1.762</v>
       </c>
       <c r="L29" t="n">
-        <v>82448</v>
+        <v>92959</v>
       </c>
       <c r="M29" t="n">
-        <v>1.263</v>
+        <v>1.424</v>
       </c>
       <c r="N29" t="n">
-        <v>0.036</v>
+        <v>0.028</v>
       </c>
       <c r="O29" t="n">
-        <v>27.996</v>
+        <v>35.467</v>
       </c>
       <c r="P29" t="s">
         <v>187</v>
@@ -4272,7 +4285,7 @@
         <v>203</v>
       </c>
       <c r="C32" s="1" t="n">
-        <v>44061</v>
+        <v>44063</v>
       </c>
       <c r="D32" t="s">
         <v>204</v>
@@ -4282,31 +4295,31 @@
       </c>
       <c r="F32"/>
       <c r="G32" t="n">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="H32" t="n">
-        <v>431272</v>
+        <v>433503</v>
       </c>
       <c r="I32" t="n">
-        <v>13.879</v>
+        <v>13.951</v>
       </c>
       <c r="J32" t="n">
-        <v>1499</v>
+        <v>1131</v>
       </c>
       <c r="K32" t="n">
-        <v>0.048</v>
+        <v>0.036</v>
       </c>
       <c r="L32" t="n">
-        <v>1383</v>
+        <v>1313</v>
       </c>
       <c r="M32" t="n">
-        <v>0.045</v>
+        <v>0.042</v>
       </c>
       <c r="N32" t="n">
         <v>0.149</v>
       </c>
       <c r="O32" t="n">
-        <v>6.718</v>
+        <v>6.714</v>
       </c>
       <c r="P32" t="s">
         <v>206</v>
@@ -4329,7 +4342,7 @@
         <v>210</v>
       </c>
       <c r="C33" s="1" t="n">
-        <v>44062</v>
+        <v>44066</v>
       </c>
       <c r="D33" t="s">
         <v>211</v>
@@ -4339,31 +4352,27 @@
       </c>
       <c r="F33"/>
       <c r="G33" t="n">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="H33" t="n">
-        <v>804282</v>
+        <v>848380</v>
       </c>
       <c r="I33" t="n">
-        <v>77.164</v>
-      </c>
-      <c r="J33" t="n">
-        <v>63411</v>
-      </c>
-      <c r="K33" t="n">
-        <v>6.084</v>
-      </c>
+        <v>81.395</v>
+      </c>
+      <c r="J33"/>
+      <c r="K33"/>
       <c r="L33" t="n">
-        <v>17785</v>
+        <v>18438</v>
       </c>
       <c r="M33" t="n">
-        <v>1.706</v>
+        <v>1.769</v>
       </c>
       <c r="N33" t="n">
         <v>0.012</v>
       </c>
       <c r="O33" t="n">
-        <v>81.369</v>
+        <v>84.745</v>
       </c>
       <c r="P33" t="s">
         <v>213</v>
@@ -4435,7 +4444,7 @@
         <v>224</v>
       </c>
       <c r="C35" s="1" t="n">
-        <v>44060</v>
+        <v>44067</v>
       </c>
       <c r="D35" t="s">
         <v>225</v>
@@ -4447,31 +4456,31 @@
         <v>227</v>
       </c>
       <c r="G35" t="n">
-        <v>165</v>
+        <v>172</v>
       </c>
       <c r="H35" t="n">
-        <v>380932</v>
+        <v>398550</v>
       </c>
       <c r="I35" t="n">
-        <v>39.433</v>
+        <v>41.256</v>
       </c>
       <c r="J35" t="n">
-        <v>2324</v>
+        <v>1458</v>
       </c>
       <c r="K35" t="n">
-        <v>0.241</v>
+        <v>0.151</v>
       </c>
       <c r="L35" t="n">
-        <v>2610</v>
+        <v>2517</v>
       </c>
       <c r="M35" t="n">
-        <v>0.27</v>
+        <v>0.261</v>
       </c>
       <c r="N35" t="n">
-        <v>0.012</v>
+        <v>0.014</v>
       </c>
       <c r="O35" t="n">
-        <v>83.045</v>
+        <v>73.72</v>
       </c>
       <c r="P35" t="s">
         <v>226</v>
@@ -4494,7 +4503,7 @@
         <v>232</v>
       </c>
       <c r="C36" s="1" t="n">
-        <v>44062</v>
+        <v>44064</v>
       </c>
       <c r="D36" t="s">
         <v>233</v>
@@ -4504,31 +4513,31 @@
       </c>
       <c r="F36"/>
       <c r="G36" t="n">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="H36" t="n">
-        <v>83461</v>
+        <v>84640</v>
       </c>
       <c r="I36" t="n">
-        <v>244.574</v>
+        <v>248.029</v>
       </c>
       <c r="J36" t="n">
-        <v>455</v>
+        <v>588</v>
       </c>
       <c r="K36" t="n">
-        <v>1.333</v>
+        <v>1.723</v>
       </c>
       <c r="L36" t="n">
-        <v>391</v>
+        <v>436</v>
       </c>
       <c r="M36" t="n">
-        <v>1.146</v>
+        <v>1.278</v>
       </c>
       <c r="N36" t="n">
-        <v>0.022</v>
+        <v>0.021</v>
       </c>
       <c r="O36" t="n">
-        <v>46.39</v>
+        <v>47.688</v>
       </c>
       <c r="P36" t="s">
         <v>234</v>
@@ -4610,7 +4619,7 @@
         <v>242</v>
       </c>
       <c r="C38" s="1" t="n">
-        <v>44062</v>
+        <v>44065</v>
       </c>
       <c r="D38" t="s">
         <v>238</v>
@@ -4622,31 +4631,31 @@
         <v>240</v>
       </c>
       <c r="G38" t="n">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="H38" t="n">
-        <v>32661252</v>
+        <v>35292220</v>
       </c>
       <c r="I38" t="n">
-        <v>23.667</v>
+        <v>25.574</v>
       </c>
       <c r="J38" t="n">
-        <v>918470</v>
+        <v>801147</v>
       </c>
       <c r="K38" t="n">
-        <v>0.666</v>
+        <v>0.581</v>
       </c>
       <c r="L38" t="n">
-        <v>830795</v>
+        <v>854645</v>
       </c>
       <c r="M38" t="n">
-        <v>0.602</v>
+        <v>0.619</v>
       </c>
       <c r="N38" t="n">
         <v>0.075</v>
       </c>
       <c r="O38" t="n">
-        <v>13.289</v>
+        <v>13.309</v>
       </c>
       <c r="P38" t="s">
         <v>239</v>
@@ -4726,7 +4735,7 @@
         <v>250</v>
       </c>
       <c r="C40" s="1" t="n">
-        <v>44063</v>
+        <v>44066</v>
       </c>
       <c r="D40" t="s">
         <v>251</v>
@@ -4736,31 +4745,31 @@
       </c>
       <c r="F40"/>
       <c r="G40" t="n">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="H40" t="n">
-        <v>2963741</v>
+        <v>3036711</v>
       </c>
       <c r="I40" t="n">
-        <v>35.286</v>
+        <v>36.154</v>
       </c>
       <c r="J40" t="n">
-        <v>23901</v>
+        <v>25401</v>
       </c>
       <c r="K40" t="n">
-        <v>0.285</v>
+        <v>0.302</v>
       </c>
       <c r="L40" t="n">
-        <v>25126</v>
+        <v>24984</v>
       </c>
       <c r="M40" t="n">
-        <v>0.299</v>
+        <v>0.297</v>
       </c>
       <c r="N40" t="n">
-        <v>0.08</v>
+        <v>0.09</v>
       </c>
       <c r="O40" t="n">
-        <v>12.442</v>
+        <v>11.124</v>
       </c>
       <c r="P40" t="s">
         <v>252</v>
@@ -4840,7 +4849,7 @@
         <v>263</v>
       </c>
       <c r="C42" s="1" t="n">
-        <v>44063</v>
+        <v>44065</v>
       </c>
       <c r="D42" t="s">
         <v>264</v>
@@ -4850,31 +4859,31 @@
       </c>
       <c r="F42"/>
       <c r="G42" t="n">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="H42" t="n">
-        <v>747521</v>
+        <v>767359</v>
       </c>
       <c r="I42" t="n">
-        <v>151.388</v>
+        <v>155.405</v>
       </c>
       <c r="J42" t="n">
-        <v>12416</v>
+        <v>6758</v>
       </c>
       <c r="K42" t="n">
-        <v>2.514</v>
+        <v>1.369</v>
       </c>
       <c r="L42" t="n">
-        <v>8546</v>
+        <v>8239</v>
       </c>
       <c r="M42" t="n">
-        <v>1.731</v>
+        <v>1.669</v>
       </c>
       <c r="N42" t="n">
-        <v>0.012</v>
+        <v>0.013</v>
       </c>
       <c r="O42" t="n">
-        <v>84.375</v>
+        <v>75.886</v>
       </c>
       <c r="P42" t="s">
         <v>265</v>
@@ -4897,7 +4906,7 @@
         <v>268</v>
       </c>
       <c r="C43" s="1" t="n">
-        <v>44056</v>
+        <v>44060</v>
       </c>
       <c r="D43" t="s">
         <v>269</v>
@@ -4907,31 +4916,31 @@
       </c>
       <c r="F43"/>
       <c r="G43" t="n">
-        <v>194</v>
+        <v>198</v>
       </c>
       <c r="H43" t="n">
-        <v>2050053</v>
+        <v>2118768</v>
       </c>
       <c r="I43" t="n">
-        <v>236.849</v>
+        <v>244.787</v>
       </c>
       <c r="J43" t="n">
-        <v>28904</v>
+        <v>26043</v>
       </c>
       <c r="K43" t="n">
-        <v>3.339</v>
+        <v>3.009</v>
       </c>
       <c r="L43" t="n">
-        <v>21889</v>
+        <v>21649</v>
       </c>
       <c r="M43" t="n">
-        <v>2.529</v>
+        <v>2.501</v>
       </c>
       <c r="N43" t="n">
-        <v>0.067</v>
+        <v>0.064</v>
       </c>
       <c r="O43" t="n">
-        <v>14.978</v>
+        <v>15.659</v>
       </c>
       <c r="P43" t="s">
         <v>45</v>
@@ -4954,7 +4963,7 @@
         <v>274</v>
       </c>
       <c r="C44" s="1" t="n">
-        <v>44063</v>
+        <v>44066</v>
       </c>
       <c r="D44" t="s">
         <v>275</v>
@@ -4966,31 +4975,31 @@
         <v>277</v>
       </c>
       <c r="G44" t="n">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="H44" t="n">
-        <v>4600949</v>
+        <v>4739968</v>
       </c>
       <c r="I44" t="n">
-        <v>76.097</v>
+        <v>78.396</v>
       </c>
       <c r="J44" t="n">
-        <v>49662</v>
+        <v>47463</v>
       </c>
       <c r="K44" t="n">
-        <v>0.821</v>
+        <v>0.785</v>
       </c>
       <c r="L44" t="n">
-        <v>31185</v>
+        <v>40577</v>
       </c>
       <c r="M44" t="n">
-        <v>0.516</v>
+        <v>0.671</v>
       </c>
       <c r="N44" t="n">
-        <v>0.016</v>
+        <v>0.017</v>
       </c>
       <c r="O44" t="n">
-        <v>61.233</v>
+        <v>60.46</v>
       </c>
       <c r="P44" t="s">
         <v>278</v>
@@ -5013,7 +5022,7 @@
         <v>281</v>
       </c>
       <c r="C45" s="1" t="n">
-        <v>44063</v>
+        <v>44066</v>
       </c>
       <c r="D45" t="s">
         <v>275</v>
@@ -5025,31 +5034,31 @@
         <v>277</v>
       </c>
       <c r="G45" t="n">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="H45" t="n">
-        <v>7790596</v>
+        <v>8007637</v>
       </c>
       <c r="I45" t="n">
-        <v>128.851</v>
+        <v>132.441</v>
       </c>
       <c r="J45" t="n">
-        <v>77442</v>
+        <v>67371</v>
       </c>
       <c r="K45" t="n">
-        <v>1.281</v>
+        <v>1.114</v>
       </c>
       <c r="L45" t="n">
-        <v>52833</v>
+        <v>64317</v>
       </c>
       <c r="M45" t="n">
-        <v>0.874</v>
+        <v>1.064</v>
       </c>
       <c r="N45" t="n">
         <v>0.01</v>
       </c>
       <c r="O45" t="n">
-        <v>103.739</v>
+        <v>95.832</v>
       </c>
       <c r="P45" t="s">
         <v>278</v>
@@ -5072,7 +5081,7 @@
         <v>284</v>
       </c>
       <c r="C46" s="1" t="n">
-        <v>44063</v>
+        <v>44066</v>
       </c>
       <c r="D46" t="s">
         <v>285</v>
@@ -5084,31 +5093,31 @@
         <v>287</v>
       </c>
       <c r="G46" t="n">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="H46" t="n">
-        <v>1259422</v>
+        <v>1321079</v>
       </c>
       <c r="I46" t="n">
-        <v>9.958</v>
+        <v>10.445</v>
       </c>
       <c r="J46" t="n">
-        <v>23242</v>
+        <v>14951</v>
       </c>
       <c r="K46" t="n">
-        <v>0.184</v>
+        <v>0.118</v>
       </c>
       <c r="L46" t="n">
-        <v>24871</v>
+        <v>20538</v>
       </c>
       <c r="M46" t="n">
-        <v>0.197</v>
+        <v>0.162</v>
       </c>
       <c r="N46" t="n">
-        <v>0.046</v>
+        <v>0.049</v>
       </c>
       <c r="O46" t="n">
-        <v>21.608</v>
+        <v>20.442</v>
       </c>
       <c r="P46" t="s">
         <v>288</v>
@@ -5131,7 +5140,7 @@
         <v>291</v>
       </c>
       <c r="C47" s="1" t="n">
-        <v>44061</v>
+        <v>44063</v>
       </c>
       <c r="D47" t="s">
         <v>292</v>
@@ -5143,31 +5152,31 @@
         <v>293</v>
       </c>
       <c r="G47" t="n">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="H47" t="n">
-        <v>1547172</v>
+        <v>1609388</v>
       </c>
       <c r="I47" t="n">
-        <v>12.233</v>
+        <v>12.725</v>
       </c>
       <c r="J47" t="n">
-        <v>18957</v>
+        <v>21913</v>
       </c>
       <c r="K47" t="n">
-        <v>0.15</v>
+        <v>0.173</v>
       </c>
       <c r="L47" t="n">
-        <v>20690</v>
+        <v>21759</v>
       </c>
       <c r="M47" t="n">
-        <v>0.164</v>
+        <v>0.172</v>
       </c>
       <c r="N47" t="n">
         <v>0.053</v>
       </c>
       <c r="O47" t="n">
-        <v>18.76</v>
+        <v>18.904</v>
       </c>
       <c r="P47" t="s">
         <v>288</v>
@@ -5247,7 +5256,7 @@
         <v>301</v>
       </c>
       <c r="C49" s="1" t="n">
-        <v>44061</v>
+        <v>44066</v>
       </c>
       <c r="D49" t="s">
         <v>302</v>
@@ -5257,31 +5266,31 @@
       </c>
       <c r="F49"/>
       <c r="G49" t="n">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="H49" t="n">
-        <v>398585</v>
+        <v>421983</v>
       </c>
       <c r="I49" t="n">
-        <v>7.413</v>
+        <v>7.848</v>
       </c>
       <c r="J49" t="n">
-        <v>4019</v>
+        <v>4179</v>
       </c>
       <c r="K49" t="n">
-        <v>0.075</v>
+        <v>0.078</v>
       </c>
       <c r="L49" t="n">
-        <v>5155</v>
+        <v>4367</v>
       </c>
       <c r="M49" t="n">
-        <v>0.096</v>
+        <v>0.081</v>
       </c>
       <c r="N49" t="n">
-        <v>0.095</v>
+        <v>0.074</v>
       </c>
       <c r="O49" t="n">
-        <v>10.499</v>
+        <v>13.472</v>
       </c>
       <c r="P49" t="s">
         <v>45</v>
@@ -5304,7 +5313,7 @@
         <v>307</v>
       </c>
       <c r="C50" s="1" t="n">
-        <v>44062</v>
+        <v>44064</v>
       </c>
       <c r="D50" t="s">
         <v>308</v>
@@ -5314,31 +5323,31 @@
       </c>
       <c r="F50"/>
       <c r="G50" t="n">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="H50" t="n">
-        <v>573251</v>
+        <v>581118</v>
       </c>
       <c r="I50" t="n">
-        <v>134.233</v>
+        <v>136.075</v>
       </c>
       <c r="J50" t="n">
-        <v>4811</v>
+        <v>3530</v>
       </c>
       <c r="K50" t="n">
-        <v>1.127</v>
+        <v>0.827</v>
       </c>
       <c r="L50" t="n">
-        <v>4199</v>
+        <v>4077</v>
       </c>
       <c r="M50" t="n">
-        <v>0.983</v>
+        <v>0.955</v>
       </c>
       <c r="N50" t="n">
         <v>0.15</v>
       </c>
       <c r="O50" t="n">
-        <v>6.677</v>
+        <v>6.666</v>
       </c>
       <c r="P50" t="s">
         <v>309</v>
@@ -5361,7 +5370,7 @@
         <v>313</v>
       </c>
       <c r="C51" s="1" t="n">
-        <v>44064</v>
+        <v>44067</v>
       </c>
       <c r="D51" t="s">
         <v>314</v>
@@ -5373,28 +5382,32 @@
         <v>316</v>
       </c>
       <c r="G51" t="n">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="H51" t="n">
-        <v>234520</v>
+        <v>238403</v>
       </c>
       <c r="I51" t="n">
-        <v>124.335</v>
+        <v>126.393</v>
       </c>
       <c r="J51" t="n">
-        <v>1602</v>
+        <v>926</v>
       </c>
       <c r="K51" t="n">
-        <v>0.849</v>
+        <v>0.491</v>
       </c>
       <c r="L51" t="n">
-        <v>1713</v>
+        <v>1697</v>
       </c>
       <c r="M51" t="n">
-        <v>0.908</v>
-      </c>
-      <c r="N51"/>
-      <c r="O51"/>
+        <v>0.9</v>
+      </c>
+      <c r="N51" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="O51" t="n">
+        <v>791.933</v>
+      </c>
       <c r="P51" t="s">
         <v>315</v>
       </c>
@@ -5416,7 +5429,7 @@
         <v>319</v>
       </c>
       <c r="C52" s="1" t="n">
-        <v>44063</v>
+        <v>44064</v>
       </c>
       <c r="D52" t="s">
         <v>320</v>
@@ -5426,31 +5439,31 @@
       </c>
       <c r="F52"/>
       <c r="G52" t="n">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="H52" t="n">
-        <v>594478</v>
+        <v>599513</v>
       </c>
       <c r="I52" t="n">
-        <v>218.374</v>
+        <v>220.224</v>
       </c>
       <c r="J52" t="n">
-        <v>4973</v>
+        <v>5035</v>
       </c>
       <c r="K52" t="n">
-        <v>1.827</v>
+        <v>1.85</v>
       </c>
       <c r="L52" t="n">
-        <v>4099</v>
+        <v>4122</v>
       </c>
       <c r="M52" t="n">
-        <v>1.506</v>
+        <v>1.514</v>
       </c>
       <c r="N52" t="n">
         <v>0.007</v>
       </c>
       <c r="O52" t="n">
-        <v>153.439</v>
+        <v>145.727</v>
       </c>
       <c r="P52" t="s">
         <v>45</v>
@@ -5473,7 +5486,7 @@
         <v>323</v>
       </c>
       <c r="C53" s="1" t="n">
-        <v>44062</v>
+        <v>44063</v>
       </c>
       <c r="D53" t="s">
         <v>324</v>
@@ -5483,31 +5496,31 @@
       </c>
       <c r="F53"/>
       <c r="G53" t="n">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="H53" t="n">
-        <v>466964</v>
+        <v>468685</v>
       </c>
       <c r="I53" t="n">
-        <v>745.977</v>
+        <v>748.727</v>
       </c>
       <c r="J53" t="n">
-        <v>2781</v>
+        <v>1721</v>
       </c>
       <c r="K53" t="n">
-        <v>4.443</v>
+        <v>2.749</v>
       </c>
       <c r="L53" t="n">
-        <v>1660</v>
+        <v>1675</v>
       </c>
       <c r="M53" t="n">
-        <v>2.652</v>
+        <v>2.676</v>
       </c>
       <c r="N53" t="n">
-        <v>0.022</v>
+        <v>0.023</v>
       </c>
       <c r="O53" t="n">
-        <v>45.214</v>
+        <v>44.079</v>
       </c>
       <c r="P53" t="s">
         <v>325</v>
@@ -5530,7 +5543,7 @@
         <v>328</v>
       </c>
       <c r="C54" s="1" t="n">
-        <v>44063</v>
+        <v>44066</v>
       </c>
       <c r="D54" t="s">
         <v>329</v>
@@ -5542,31 +5555,31 @@
         <v>331</v>
       </c>
       <c r="G54" t="n">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="H54" t="n">
-        <v>1152140</v>
+        <v>1176416</v>
       </c>
       <c r="I54" t="n">
-        <v>35.597</v>
+        <v>36.347</v>
       </c>
       <c r="J54" t="n">
-        <v>10461</v>
+        <v>8467</v>
       </c>
       <c r="K54" t="n">
-        <v>0.323</v>
+        <v>0.262</v>
       </c>
       <c r="L54" t="n">
-        <v>9586</v>
+        <v>8881</v>
       </c>
       <c r="M54" t="n">
-        <v>0.296</v>
+        <v>0.274</v>
       </c>
       <c r="N54" t="n">
-        <v>0.002</v>
+        <v>0.001</v>
       </c>
       <c r="O54" t="n">
-        <v>554.562</v>
+        <v>758.134</v>
       </c>
       <c r="P54" t="s">
         <v>45</v>
@@ -5589,7 +5602,7 @@
         <v>335</v>
       </c>
       <c r="C55" s="1" t="n">
-        <v>44062</v>
+        <v>44064</v>
       </c>
       <c r="D55" t="s">
         <v>336</v>
@@ -5599,31 +5612,31 @@
       </c>
       <c r="F55"/>
       <c r="G55" t="n">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="H55" t="n">
-        <v>99300</v>
+        <v>101730</v>
       </c>
       <c r="I55" t="n">
-        <v>183.705</v>
+        <v>188.2</v>
       </c>
       <c r="J55" t="n">
-        <v>1125</v>
+        <v>1497</v>
       </c>
       <c r="K55" t="n">
-        <v>2.081</v>
+        <v>2.769</v>
       </c>
       <c r="L55" t="n">
-        <v>1057</v>
+        <v>1098</v>
       </c>
       <c r="M55" t="n">
-        <v>1.955</v>
+        <v>2.031</v>
       </c>
       <c r="N55" t="n">
-        <v>0.116</v>
+        <v>0.114</v>
       </c>
       <c r="O55" t="n">
-        <v>8.644</v>
+        <v>8.774</v>
       </c>
       <c r="P55" t="s">
         <v>338</v>
@@ -5646,7 +5659,7 @@
         <v>342</v>
       </c>
       <c r="C56" s="1" t="n">
-        <v>44061</v>
+        <v>44065</v>
       </c>
       <c r="D56" t="s">
         <v>343</v>
@@ -5656,31 +5669,31 @@
       </c>
       <c r="F56"/>
       <c r="G56" t="n">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="H56" t="n">
-        <v>163308</v>
+        <v>173263</v>
       </c>
       <c r="I56" t="n">
-        <v>369.861</v>
+        <v>392.407</v>
       </c>
       <c r="J56" t="n">
-        <v>2261</v>
+        <v>2173</v>
       </c>
       <c r="K56" t="n">
-        <v>5.121</v>
+        <v>4.921</v>
       </c>
       <c r="L56" t="n">
-        <v>2272</v>
+        <v>2373</v>
       </c>
       <c r="M56" t="n">
-        <v>5.146</v>
+        <v>5.374</v>
       </c>
       <c r="N56" t="n">
-        <v>0.017</v>
+        <v>0.016</v>
       </c>
       <c r="O56" t="n">
-        <v>60.471</v>
+        <v>61.981</v>
       </c>
       <c r="P56" t="s">
         <v>344</v>
@@ -5703,7 +5716,7 @@
         <v>348</v>
       </c>
       <c r="C57" s="1" t="n">
-        <v>44060</v>
+        <v>44062</v>
       </c>
       <c r="D57" t="s">
         <v>349</v>
@@ -5713,31 +5726,31 @@
       </c>
       <c r="F57"/>
       <c r="G57" t="n">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="H57" t="n">
-        <v>1138828</v>
+        <v>1170251</v>
       </c>
       <c r="I57" t="n">
-        <v>8.833</v>
+        <v>9.076</v>
       </c>
       <c r="J57" t="n">
-        <v>7608</v>
+        <v>8789</v>
       </c>
       <c r="K57" t="n">
-        <v>0.059</v>
+        <v>0.068</v>
       </c>
       <c r="L57" t="n">
-        <v>9386</v>
+        <v>9665</v>
       </c>
       <c r="M57" t="n">
-        <v>0.073</v>
+        <v>0.075</v>
       </c>
       <c r="N57" t="n">
-        <v>0.637</v>
+        <v>0.572</v>
       </c>
       <c r="O57" t="n">
-        <v>1.569</v>
+        <v>1.747</v>
       </c>
       <c r="P57" t="s">
         <v>351</v>
@@ -5760,7 +5773,7 @@
         <v>355</v>
       </c>
       <c r="C58" s="1" t="n">
-        <v>44062</v>
+        <v>44064</v>
       </c>
       <c r="D58" t="s">
         <v>356</v>
@@ -5770,31 +5783,31 @@
       </c>
       <c r="F58"/>
       <c r="G58" t="n">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="H58" t="n">
-        <v>1670569</v>
+        <v>1714583</v>
       </c>
       <c r="I58" t="n">
-        <v>45.26</v>
+        <v>46.452</v>
       </c>
       <c r="J58" t="n">
-        <v>21841</v>
+        <v>22178</v>
       </c>
       <c r="K58" t="n">
-        <v>0.592</v>
+        <v>0.601</v>
       </c>
       <c r="L58" t="n">
-        <v>22024</v>
+        <v>22008</v>
       </c>
       <c r="M58" t="n">
-        <v>0.597</v>
+        <v>0.596</v>
       </c>
       <c r="N58" t="n">
-        <v>0.054</v>
+        <v>0.063</v>
       </c>
       <c r="O58" t="n">
-        <v>18.435</v>
+        <v>15.877</v>
       </c>
       <c r="P58" t="s">
         <v>357</v>
@@ -5817,7 +5830,7 @@
         <v>361</v>
       </c>
       <c r="C59" s="1" t="n">
-        <v>44061</v>
+        <v>44065</v>
       </c>
       <c r="D59" t="s">
         <v>362</v>
@@ -5827,31 +5840,31 @@
       </c>
       <c r="F59"/>
       <c r="G59" t="n">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="H59" t="n">
-        <v>139514</v>
+        <v>145167</v>
       </c>
       <c r="I59" t="n">
-        <v>2.564</v>
+        <v>2.668</v>
       </c>
       <c r="J59" t="n">
-        <v>1765</v>
+        <v>1113</v>
       </c>
       <c r="K59" t="n">
-        <v>0.032</v>
+        <v>0.02</v>
       </c>
       <c r="L59" t="n">
-        <v>1530</v>
+        <v>1395</v>
       </c>
       <c r="M59" t="n">
-        <v>0.028</v>
+        <v>0.026</v>
       </c>
       <c r="N59" t="n">
-        <v>0.001</v>
+        <v>0.006</v>
       </c>
       <c r="O59" t="n">
-        <v>669.375</v>
+        <v>160.082</v>
       </c>
       <c r="P59" t="s">
         <v>363</v>
@@ -5984,7 +5997,7 @@
         <v>380</v>
       </c>
       <c r="C62" s="1" t="n">
-        <v>44063</v>
+        <v>44066</v>
       </c>
       <c r="D62" t="s">
         <v>381</v>
@@ -5994,31 +6007,31 @@
       </c>
       <c r="F62"/>
       <c r="G62" t="n">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="H62" t="n">
-        <v>673220</v>
+        <v>697070</v>
       </c>
       <c r="I62" t="n">
-        <v>139.608</v>
+        <v>144.553</v>
       </c>
       <c r="J62" t="n">
-        <v>15714</v>
+        <v>4589</v>
       </c>
       <c r="K62" t="n">
-        <v>3.259</v>
+        <v>0.952</v>
       </c>
       <c r="L62" t="n">
-        <v>21258</v>
+        <v>14159</v>
       </c>
       <c r="M62" t="n">
-        <v>4.408</v>
+        <v>2.936</v>
       </c>
       <c r="N62" t="n">
-        <v>0</v>
+        <v>0.001</v>
       </c>
       <c r="O62" t="n">
-        <v>2254.636</v>
+        <v>1870.057</v>
       </c>
       <c r="P62" t="s">
         <v>382</v>
@@ -6041,7 +6054,7 @@
         <v>385</v>
       </c>
       <c r="C63" s="1" t="n">
-        <v>44062</v>
+        <v>44066</v>
       </c>
       <c r="D63" t="s">
         <v>386</v>
@@ -6051,31 +6064,31 @@
       </c>
       <c r="F63"/>
       <c r="G63" t="n">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="H63" t="n">
-        <v>363331</v>
+        <v>378023</v>
       </c>
       <c r="I63" t="n">
-        <v>1.763</v>
+        <v>1.834</v>
       </c>
       <c r="J63" t="n">
-        <v>8135</v>
+        <v>3946</v>
       </c>
       <c r="K63" t="n">
-        <v>0.039</v>
+        <v>0.019</v>
       </c>
       <c r="L63" t="n">
-        <v>3607</v>
+        <v>3919</v>
       </c>
       <c r="M63" t="n">
-        <v>0.017</v>
+        <v>0.019</v>
       </c>
       <c r="N63" t="n">
-        <v>0.103</v>
+        <v>0.114</v>
       </c>
       <c r="O63" t="n">
-        <v>9.693</v>
+        <v>8.751</v>
       </c>
       <c r="P63" t="s">
         <v>387</v>
@@ -6098,7 +6111,7 @@
         <v>391</v>
       </c>
       <c r="C64" s="1" t="n">
-        <v>44061</v>
+        <v>44062</v>
       </c>
       <c r="D64" t="s">
         <v>392</v>
@@ -6108,31 +6121,31 @@
       </c>
       <c r="F64"/>
       <c r="G64" t="n">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="H64" t="n">
-        <v>567646</v>
+        <v>580724</v>
       </c>
       <c r="I64" t="n">
-        <v>104.708</v>
+        <v>107.12</v>
       </c>
       <c r="J64" t="n">
-        <v>9071</v>
+        <v>8712</v>
       </c>
       <c r="K64" t="n">
-        <v>1.673</v>
+        <v>1.607</v>
       </c>
       <c r="L64" t="n">
-        <v>9539</v>
+        <v>9801</v>
       </c>
       <c r="M64" t="n">
-        <v>1.76</v>
+        <v>1.808</v>
       </c>
       <c r="N64" t="n">
         <v>0.005</v>
       </c>
       <c r="O64" t="n">
-        <v>182.44</v>
+        <v>182.465</v>
       </c>
       <c r="P64" t="s">
         <v>393</v>
@@ -6200,7 +6213,7 @@
         <v>405</v>
       </c>
       <c r="C66" s="1" t="n">
-        <v>44064</v>
+        <v>44067</v>
       </c>
       <c r="D66" t="s">
         <v>406</v>
@@ -6210,28 +6223,32 @@
       </c>
       <c r="F66"/>
       <c r="G66" t="n">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="H66" t="n">
-        <v>2389365</v>
+        <v>2463513</v>
       </c>
       <c r="I66" t="n">
-        <v>10.817</v>
+        <v>11.153</v>
       </c>
       <c r="J66" t="n">
-        <v>25613</v>
+        <v>23655</v>
       </c>
       <c r="K66" t="n">
-        <v>0.116</v>
+        <v>0.107</v>
       </c>
       <c r="L66" t="n">
-        <v>22851</v>
+        <v>23416</v>
       </c>
       <c r="M66" t="n">
-        <v>0.103</v>
-      </c>
-      <c r="N66"/>
-      <c r="O66"/>
+        <v>0.106</v>
+      </c>
+      <c r="N66" t="n">
+        <v>0.022</v>
+      </c>
+      <c r="O66" t="n">
+        <v>46.172</v>
+      </c>
       <c r="P66" t="s">
         <v>407</v>
       </c>
@@ -6310,7 +6327,7 @@
         <v>415</v>
       </c>
       <c r="C68" s="1" t="n">
-        <v>44062</v>
+        <v>44065</v>
       </c>
       <c r="D68" t="s">
         <v>416</v>
@@ -6320,31 +6337,31 @@
       </c>
       <c r="F68"/>
       <c r="G68" t="n">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="H68" t="n">
-        <v>162323</v>
+        <v>171552</v>
       </c>
       <c r="I68" t="n">
-        <v>22.758</v>
+        <v>24.052</v>
       </c>
       <c r="J68" t="n">
-        <v>2657</v>
+        <v>2292</v>
       </c>
       <c r="K68" t="n">
-        <v>0.373</v>
+        <v>0.321</v>
       </c>
       <c r="L68" t="n">
-        <v>2544</v>
+        <v>2875</v>
       </c>
       <c r="M68" t="n">
-        <v>0.357</v>
+        <v>0.403</v>
       </c>
       <c r="N68" t="n">
-        <v>0.173</v>
+        <v>0.172</v>
       </c>
       <c r="O68" t="n">
-        <v>5.769</v>
+        <v>5.818</v>
       </c>
       <c r="P68" t="s">
         <v>417</v>
@@ -6420,7 +6437,7 @@
         <v>427</v>
       </c>
       <c r="C70" s="1" t="n">
-        <v>44059</v>
+        <v>44065</v>
       </c>
       <c r="D70" t="s">
         <v>428</v>
@@ -6430,31 +6447,31 @@
       </c>
       <c r="F70"/>
       <c r="G70" t="n">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="H70" t="n">
-        <v>1948932</v>
+        <v>2158493</v>
       </c>
       <c r="I70" t="n">
-        <v>17.785</v>
+        <v>19.698</v>
       </c>
       <c r="J70" t="n">
-        <v>25312</v>
+        <v>26333</v>
       </c>
       <c r="K70" t="n">
-        <v>0.231</v>
+        <v>0.24</v>
       </c>
       <c r="L70" t="n">
-        <v>30570</v>
+        <v>31469</v>
       </c>
       <c r="M70" t="n">
-        <v>0.279</v>
+        <v>0.287</v>
       </c>
       <c r="N70" t="n">
-        <v>0.145</v>
+        <v>0.13</v>
       </c>
       <c r="O70" t="n">
-        <v>6.896</v>
+        <v>7.674</v>
       </c>
       <c r="P70" t="s">
         <v>219</v>
@@ -6477,7 +6494,7 @@
         <v>433</v>
       </c>
       <c r="C71" s="1" t="n">
-        <v>44063</v>
+        <v>44066</v>
       </c>
       <c r="D71" t="s">
         <v>434</v>
@@ -6487,31 +6504,31 @@
       </c>
       <c r="F71"/>
       <c r="G71" t="n">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="H71" t="n">
-        <v>2357772</v>
+        <v>2430214</v>
       </c>
       <c r="I71" t="n">
-        <v>62.298</v>
+        <v>64.212</v>
       </c>
       <c r="J71" t="n">
-        <v>24646</v>
+        <v>18983</v>
       </c>
       <c r="K71" t="n">
-        <v>0.651</v>
+        <v>0.502</v>
       </c>
       <c r="L71" t="n">
-        <v>21510</v>
+        <v>22498</v>
       </c>
       <c r="M71" t="n">
-        <v>0.568</v>
+        <v>0.594</v>
       </c>
       <c r="N71" t="n">
-        <v>0.033</v>
+        <v>0.032</v>
       </c>
       <c r="O71" t="n">
-        <v>30.511</v>
+        <v>30.934</v>
       </c>
       <c r="P71" t="s">
         <v>435</v>
@@ -6534,7 +6551,7 @@
         <v>438</v>
       </c>
       <c r="C72" s="1" t="n">
-        <v>44063</v>
+        <v>44066</v>
       </c>
       <c r="D72" t="s">
         <v>434</v>
@@ -6544,31 +6561,31 @@
       </c>
       <c r="F72"/>
       <c r="G72" t="n">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="H72" t="n">
-        <v>2463734</v>
+        <v>2538761</v>
       </c>
       <c r="I72" t="n">
-        <v>65.098</v>
+        <v>67.08</v>
       </c>
       <c r="J72" t="n">
-        <v>25599</v>
+        <v>19634</v>
       </c>
       <c r="K72" t="n">
-        <v>0.676</v>
+        <v>0.519</v>
       </c>
       <c r="L72" t="n">
-        <v>22286</v>
+        <v>23294</v>
       </c>
       <c r="M72" t="n">
-        <v>0.589</v>
+        <v>0.615</v>
       </c>
       <c r="N72" t="n">
-        <v>0.032</v>
+        <v>0.031</v>
       </c>
       <c r="O72" t="n">
-        <v>31.611</v>
+        <v>32.029</v>
       </c>
       <c r="P72" t="s">
         <v>435</v>
@@ -6648,7 +6665,7 @@
         <v>447</v>
       </c>
       <c r="C74" s="1" t="n">
-        <v>44063</v>
+        <v>44066</v>
       </c>
       <c r="D74" t="s">
         <v>448</v>
@@ -6658,31 +6675,31 @@
       </c>
       <c r="F74"/>
       <c r="G74" t="n">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="H74" t="n">
-        <v>572273</v>
+        <v>589920</v>
       </c>
       <c r="I74" t="n">
-        <v>198.633</v>
+        <v>204.758</v>
       </c>
       <c r="J74" t="n">
-        <v>6260</v>
+        <v>5797</v>
       </c>
       <c r="K74" t="n">
-        <v>2.173</v>
+        <v>2.012</v>
       </c>
       <c r="L74" t="n">
-        <v>4810</v>
+        <v>5521</v>
       </c>
       <c r="M74" t="n">
-        <v>1.67</v>
+        <v>1.916</v>
       </c>
       <c r="N74" t="n">
-        <v>0.06</v>
+        <v>0.051</v>
       </c>
       <c r="O74" t="n">
-        <v>16.685</v>
+        <v>19.758</v>
       </c>
       <c r="P74" t="s">
         <v>449</v>
@@ -6705,7 +6722,7 @@
         <v>453</v>
       </c>
       <c r="C75" s="1" t="n">
-        <v>44063</v>
+        <v>44066</v>
       </c>
       <c r="D75" t="s">
         <v>454</v>
@@ -6715,31 +6732,31 @@
       </c>
       <c r="F75"/>
       <c r="G75" t="n">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="H75" t="n">
-        <v>1591015</v>
+        <v>1652644</v>
       </c>
       <c r="I75" t="n">
-        <v>82.703</v>
+        <v>85.907</v>
       </c>
       <c r="J75" t="n">
-        <v>24383</v>
+        <v>13274</v>
       </c>
       <c r="K75" t="n">
-        <v>1.267</v>
+        <v>0.69</v>
       </c>
       <c r="L75" t="n">
-        <v>20107</v>
+        <v>19822</v>
       </c>
       <c r="M75" t="n">
-        <v>1.045</v>
+        <v>1.03</v>
       </c>
       <c r="N75" t="n">
-        <v>0.06</v>
+        <v>0.059</v>
       </c>
       <c r="O75" t="n">
-        <v>16.676</v>
+        <v>16.983</v>
       </c>
       <c r="P75" t="s">
         <v>456</v>
@@ -6762,7 +6779,7 @@
         <v>460</v>
       </c>
       <c r="C76" s="1" t="n">
-        <v>44063</v>
+        <v>44066</v>
       </c>
       <c r="D76" t="s">
         <v>461</v>
@@ -6772,22 +6789,22 @@
       </c>
       <c r="F76"/>
       <c r="G76" t="n">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="H76" t="n">
-        <v>33814105</v>
+        <v>34695406</v>
       </c>
       <c r="I76" t="n">
-        <v>231.707</v>
+        <v>237.746</v>
       </c>
       <c r="J76" t="n">
-        <v>304832</v>
+        <v>247846</v>
       </c>
       <c r="K76" t="n">
-        <v>2.089</v>
+        <v>1.698</v>
       </c>
       <c r="L76" t="n">
-        <v>273007</v>
+        <v>272990</v>
       </c>
       <c r="M76" t="n">
         <v>1.871</v>
@@ -6796,7 +6813,7 @@
         <v>0.018</v>
       </c>
       <c r="O76" t="n">
-        <v>55.201</v>
+        <v>56.182</v>
       </c>
       <c r="P76" t="s">
         <v>462</v>
@@ -6819,7 +6836,7 @@
         <v>466</v>
       </c>
       <c r="C77" s="1" t="n">
-        <v>44062</v>
+        <v>44066</v>
       </c>
       <c r="D77" t="s">
         <v>467</v>
@@ -6829,31 +6846,31 @@
       </c>
       <c r="F77"/>
       <c r="G77" t="n">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="H77" t="n">
-        <v>345920</v>
+        <v>368244</v>
       </c>
       <c r="I77" t="n">
-        <v>26.707</v>
+        <v>28.431</v>
       </c>
       <c r="J77" t="n">
-        <v>3306</v>
+        <v>6402</v>
       </c>
       <c r="K77" t="n">
-        <v>0.255</v>
+        <v>0.494</v>
       </c>
       <c r="L77" t="n">
-        <v>4483</v>
+        <v>4853</v>
       </c>
       <c r="M77" t="n">
-        <v>0.346</v>
+        <v>0.375</v>
       </c>
       <c r="N77" t="n">
-        <v>0.013</v>
+        <v>0.016</v>
       </c>
       <c r="O77" t="n">
-        <v>77.293</v>
+        <v>63.261</v>
       </c>
       <c r="P77" t="s">
         <v>468</v>
@@ -6876,7 +6893,7 @@
         <v>472</v>
       </c>
       <c r="C78" s="1" t="n">
-        <v>44063</v>
+        <v>44065</v>
       </c>
       <c r="D78" t="s">
         <v>473</v>
@@ -6886,31 +6903,31 @@
       </c>
       <c r="F78"/>
       <c r="G78" t="n">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="H78" t="n">
-        <v>4501104</v>
+        <v>4622637</v>
       </c>
       <c r="I78" t="n">
-        <v>129.291</v>
+        <v>132.781</v>
       </c>
       <c r="J78" t="n">
-        <v>61620</v>
+        <v>59120</v>
       </c>
       <c r="K78" t="n">
-        <v>1.77</v>
+        <v>1.698</v>
       </c>
       <c r="L78" t="n">
-        <v>61321</v>
+        <v>60080</v>
       </c>
       <c r="M78" t="n">
-        <v>1.761</v>
+        <v>1.726</v>
       </c>
       <c r="N78" t="n">
         <v>0.022</v>
       </c>
       <c r="O78" t="n">
-        <v>44.486</v>
+        <v>45.299</v>
       </c>
       <c r="P78" t="s">
         <v>45</v>
@@ -6933,7 +6950,7 @@
         <v>476</v>
       </c>
       <c r="C79" s="1" t="n">
-        <v>44063</v>
+        <v>44066</v>
       </c>
       <c r="D79" t="s">
         <v>477</v>
@@ -6945,31 +6962,31 @@
         <v>479</v>
       </c>
       <c r="G79" t="n">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="H79" t="n">
-        <v>138713</v>
+        <v>142936</v>
       </c>
       <c r="I79" t="n">
-        <v>8.284</v>
+        <v>8.537</v>
       </c>
       <c r="J79" t="n">
-        <v>1519</v>
+        <v>1250</v>
       </c>
       <c r="K79" t="n">
-        <v>0.091</v>
+        <v>0.075</v>
       </c>
       <c r="L79" t="n">
-        <v>1445</v>
+        <v>1311</v>
       </c>
       <c r="M79" t="n">
-        <v>0.086</v>
+        <v>0.078</v>
       </c>
       <c r="N79" t="n">
-        <v>0.085</v>
+        <v>0.089</v>
       </c>
       <c r="O79" t="n">
-        <v>11.775</v>
+        <v>11.219</v>
       </c>
       <c r="P79" t="s">
         <v>480</v>
@@ -6992,7 +7009,7 @@
         <v>484</v>
       </c>
       <c r="C80" s="1" t="n">
-        <v>44062</v>
+        <v>44066</v>
       </c>
       <c r="D80" t="s">
         <v>485</v>
@@ -7004,31 +7021,31 @@
         <v>486</v>
       </c>
       <c r="G80" t="n">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="H80" t="n">
-        <v>831677</v>
+        <v>869668</v>
       </c>
       <c r="I80" t="n">
-        <v>122.223</v>
+        <v>127.806</v>
       </c>
       <c r="J80" t="n">
-        <v>10571</v>
+        <v>6939</v>
       </c>
       <c r="K80" t="n">
-        <v>1.554</v>
+        <v>1.02</v>
       </c>
       <c r="L80" t="n">
-        <v>8669</v>
+        <v>9300</v>
       </c>
       <c r="M80" t="n">
-        <v>1.274</v>
+        <v>1.367</v>
       </c>
       <c r="N80" t="n">
-        <v>0.023</v>
+        <v>0.017</v>
       </c>
       <c r="O80" t="n">
-        <v>43.563</v>
+        <v>60.446</v>
       </c>
       <c r="P80" t="s">
         <v>45</v>
@@ -7157,7 +7174,7 @@
         <v>496</v>
       </c>
       <c r="C83" s="1" t="n">
-        <v>44063</v>
+        <v>44065</v>
       </c>
       <c r="D83" t="s">
         <v>497</v>
@@ -7167,31 +7184,31 @@
       </c>
       <c r="F83"/>
       <c r="G83" t="n">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="H83" t="n">
-        <v>304021</v>
+        <v>311099</v>
       </c>
       <c r="I83" t="n">
-        <v>55.685</v>
+        <v>56.982</v>
       </c>
       <c r="J83" t="n">
-        <v>3435</v>
+        <v>7013</v>
       </c>
       <c r="K83" t="n">
-        <v>0.629</v>
+        <v>1.285</v>
       </c>
       <c r="L83" t="n">
-        <v>2453</v>
+        <v>2611</v>
       </c>
       <c r="M83" t="n">
-        <v>0.449</v>
+        <v>0.478</v>
       </c>
       <c r="N83" t="n">
-        <v>0.019</v>
+        <v>0.023</v>
       </c>
       <c r="O83" t="n">
-        <v>51.72</v>
+        <v>43.106</v>
       </c>
       <c r="P83" t="s">
         <v>499</v>
@@ -7214,7 +7231,7 @@
         <v>502</v>
       </c>
       <c r="C84" s="1" t="n">
-        <v>44062</v>
+        <v>44066</v>
       </c>
       <c r="D84" t="s">
         <v>503</v>
@@ -7224,31 +7241,31 @@
       </c>
       <c r="F84"/>
       <c r="G84" t="n">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="H84" t="n">
-        <v>145723</v>
+        <v>149235</v>
       </c>
       <c r="I84" t="n">
-        <v>70.095</v>
+        <v>71.784</v>
       </c>
       <c r="J84" t="n">
-        <v>1168</v>
+        <v>453</v>
       </c>
       <c r="K84" t="n">
-        <v>0.562</v>
+        <v>0.218</v>
       </c>
       <c r="L84" t="n">
-        <v>878</v>
+        <v>988</v>
       </c>
       <c r="M84" t="n">
-        <v>0.422</v>
+        <v>0.475</v>
       </c>
       <c r="N84" t="n">
-        <v>0.03</v>
+        <v>0.031</v>
       </c>
       <c r="O84" t="n">
-        <v>33.402</v>
+        <v>32.019</v>
       </c>
       <c r="P84" t="s">
         <v>505</v>
@@ -7271,7 +7288,7 @@
         <v>509</v>
       </c>
       <c r="C85" s="1" t="n">
-        <v>44063</v>
+        <v>44065</v>
       </c>
       <c r="D85" t="s">
         <v>510</v>
@@ -7283,31 +7300,31 @@
         <v>512</v>
       </c>
       <c r="G85" t="n">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="H85" t="n">
-        <v>3480283</v>
+        <v>3535067</v>
       </c>
       <c r="I85" t="n">
-        <v>58.681</v>
+        <v>59.605</v>
       </c>
       <c r="J85" t="n">
-        <v>24612</v>
+        <v>30560</v>
       </c>
       <c r="K85" t="n">
-        <v>0.415</v>
+        <v>0.515</v>
       </c>
       <c r="L85" t="n">
-        <v>23541</v>
+        <v>22434</v>
       </c>
       <c r="M85" t="n">
-        <v>0.397</v>
+        <v>0.378</v>
       </c>
       <c r="N85" t="n">
-        <v>0.165</v>
+        <v>0.154</v>
       </c>
       <c r="O85" t="n">
-        <v>6.072</v>
+        <v>6.49</v>
       </c>
       <c r="P85" t="s">
         <v>511</v>
@@ -7330,7 +7347,7 @@
         <v>516</v>
       </c>
       <c r="C86" s="1" t="n">
-        <v>44063</v>
+        <v>44066</v>
       </c>
       <c r="D86" t="s">
         <v>517</v>
@@ -7340,31 +7357,31 @@
       </c>
       <c r="F86"/>
       <c r="G86" t="n">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="H86" t="n">
-        <v>1699085</v>
+        <v>1743622</v>
       </c>
       <c r="I86" t="n">
-        <v>33.14</v>
+        <v>34.009</v>
       </c>
       <c r="J86" t="n">
-        <v>15043</v>
+        <v>10249</v>
       </c>
       <c r="K86" t="n">
-        <v>0.293</v>
+        <v>0.2</v>
       </c>
       <c r="L86" t="n">
-        <v>8855</v>
+        <v>11977</v>
       </c>
       <c r="M86" t="n">
-        <v>0.173</v>
+        <v>0.234</v>
       </c>
       <c r="N86" t="n">
         <v>0.025</v>
       </c>
       <c r="O86" t="n">
-        <v>39.331</v>
+        <v>40.288</v>
       </c>
       <c r="P86" t="s">
         <v>518</v>
@@ -7546,7 +7563,7 @@
         <v>539</v>
       </c>
       <c r="C90" s="1" t="n">
-        <v>44062</v>
+        <v>44064</v>
       </c>
       <c r="D90" t="s">
         <v>540</v>
@@ -7556,31 +7573,31 @@
       </c>
       <c r="F90"/>
       <c r="G90" t="n">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="H90" t="n">
-        <v>910283</v>
+        <v>932946</v>
       </c>
       <c r="I90" t="n">
-        <v>105.179</v>
+        <v>107.797</v>
       </c>
       <c r="J90" t="n">
-        <v>6189</v>
+        <v>9444</v>
       </c>
       <c r="K90" t="n">
-        <v>0.715</v>
+        <v>1.091</v>
       </c>
       <c r="L90" t="n">
-        <v>6651</v>
+        <v>7788</v>
       </c>
       <c r="M90" t="n">
-        <v>0.768</v>
+        <v>0.9</v>
       </c>
       <c r="N90" t="n">
-        <v>0.033</v>
+        <v>0.03</v>
       </c>
       <c r="O90" t="n">
-        <v>30.114</v>
+        <v>33.777</v>
       </c>
       <c r="P90" t="s">
         <v>541</v>
@@ -7603,7 +7620,7 @@
         <v>545</v>
       </c>
       <c r="C91" s="1" t="n">
-        <v>44063</v>
+        <v>44066</v>
       </c>
       <c r="D91" t="s">
         <v>546</v>
@@ -7613,31 +7630,31 @@
       </c>
       <c r="F91"/>
       <c r="G91" t="n">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="H91" t="n">
-        <v>85563</v>
+        <v>86023</v>
       </c>
       <c r="I91" t="n">
-        <v>3.593</v>
+        <v>3.612</v>
       </c>
       <c r="J91" t="n">
-        <v>214</v>
+        <v>116</v>
       </c>
       <c r="K91" t="n">
-        <v>0.009</v>
+        <v>0.005</v>
       </c>
       <c r="L91" t="n">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="M91" t="n">
         <v>0.008</v>
       </c>
       <c r="N91" t="n">
-        <v>0.004</v>
+        <v>0.002</v>
       </c>
       <c r="O91" t="n">
-        <v>263.2</v>
+        <v>441</v>
       </c>
       <c r="P91" t="s">
         <v>547</v>
@@ -7660,7 +7677,7 @@
         <v>550</v>
       </c>
       <c r="C92" s="1" t="n">
-        <v>44063</v>
+        <v>44066</v>
       </c>
       <c r="D92" t="s">
         <v>551</v>
@@ -7670,31 +7687,31 @@
       </c>
       <c r="F92"/>
       <c r="G92" t="n">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="H92" t="n">
-        <v>401680</v>
+        <v>406172</v>
       </c>
       <c r="I92" t="n">
-        <v>5.755</v>
+        <v>5.819</v>
       </c>
       <c r="J92" t="n">
-        <v>2286</v>
+        <v>1525</v>
       </c>
       <c r="K92" t="n">
-        <v>0.033</v>
+        <v>0.022</v>
       </c>
       <c r="L92" t="n">
-        <v>1506</v>
+        <v>1722</v>
       </c>
       <c r="M92" t="n">
-        <v>0.022</v>
+        <v>0.025</v>
       </c>
       <c r="N92" t="n">
-        <v>0.003</v>
+        <v>0.001</v>
       </c>
       <c r="O92" t="n">
-        <v>319.455</v>
+        <v>669.667</v>
       </c>
       <c r="P92" t="s">
         <v>552</v>
@@ -7717,7 +7734,7 @@
         <v>555</v>
       </c>
       <c r="C93" s="1" t="n">
-        <v>44063</v>
+        <v>44066</v>
       </c>
       <c r="D93" t="s">
         <v>551</v>
@@ -7727,31 +7744,31 @@
       </c>
       <c r="F93"/>
       <c r="G93" t="n">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="H93" t="n">
-        <v>789951</v>
+        <v>794443</v>
       </c>
       <c r="I93" t="n">
-        <v>11.317</v>
+        <v>11.382</v>
       </c>
       <c r="J93" t="n">
-        <v>2286</v>
+        <v>1525</v>
       </c>
       <c r="K93" t="n">
-        <v>0.033</v>
+        <v>0.022</v>
       </c>
       <c r="L93" t="n">
-        <v>1506</v>
+        <v>1722</v>
       </c>
       <c r="M93" t="n">
-        <v>0.022</v>
+        <v>0.025</v>
       </c>
       <c r="N93" t="n">
-        <v>0.003</v>
+        <v>0.001</v>
       </c>
       <c r="O93" t="n">
-        <v>319.455</v>
+        <v>669.667</v>
       </c>
       <c r="P93" t="s">
         <v>552</v>
@@ -7831,7 +7848,7 @@
         <v>564</v>
       </c>
       <c r="C95" s="1" t="n">
-        <v>44060</v>
+        <v>44063</v>
       </c>
       <c r="D95" t="s">
         <v>565</v>
@@ -7841,31 +7858,31 @@
       </c>
       <c r="F95"/>
       <c r="G95" t="n">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="H95" t="n">
-        <v>113758</v>
+        <v>119571</v>
       </c>
       <c r="I95" t="n">
-        <v>9.625</v>
+        <v>10.117</v>
       </c>
       <c r="J95" t="n">
-        <v>1710</v>
+        <v>2007</v>
       </c>
       <c r="K95" t="n">
-        <v>0.145</v>
+        <v>0.17</v>
       </c>
       <c r="L95" t="n">
-        <v>1365</v>
+        <v>1626</v>
       </c>
       <c r="M95" t="n">
-        <v>0.115</v>
+        <v>0.138</v>
       </c>
       <c r="N95" t="n">
-        <v>0.043</v>
+        <v>0.057</v>
       </c>
       <c r="O95" t="n">
-        <v>23.305</v>
+        <v>17.592</v>
       </c>
       <c r="P95" t="s">
         <v>566</v>
@@ -7888,7 +7905,7 @@
         <v>569</v>
       </c>
       <c r="C96" s="1" t="n">
-        <v>44063</v>
+        <v>44066</v>
       </c>
       <c r="D96" t="s">
         <v>570</v>
@@ -7898,27 +7915,31 @@
       </c>
       <c r="F96"/>
       <c r="G96" t="n">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="H96" t="n">
-        <v>6061930</v>
+        <v>6327466</v>
       </c>
       <c r="I96" t="n">
-        <v>71.876</v>
-      </c>
-      <c r="J96"/>
-      <c r="K96"/>
+        <v>75.024</v>
+      </c>
+      <c r="J96" t="n">
+        <v>80302</v>
+      </c>
+      <c r="K96" t="n">
+        <v>0.952</v>
+      </c>
       <c r="L96" t="n">
-        <v>77150</v>
+        <v>86032</v>
       </c>
       <c r="M96" t="n">
-        <v>0.915</v>
+        <v>1.02</v>
       </c>
       <c r="N96" t="n">
-        <v>0.016</v>
+        <v>0.015</v>
       </c>
       <c r="O96" t="n">
-        <v>61.961</v>
+        <v>67.552</v>
       </c>
       <c r="P96" t="s">
         <v>571</v>
@@ -7941,7 +7962,7 @@
         <v>574</v>
       </c>
       <c r="C97" s="1" t="n">
-        <v>44062</v>
+        <v>44063</v>
       </c>
       <c r="D97" t="s">
         <v>575</v>
@@ -7951,22 +7972,22 @@
       </c>
       <c r="F97"/>
       <c r="G97" t="n">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H97" t="n">
-        <v>336713</v>
+        <v>340844</v>
       </c>
       <c r="I97" t="n">
-        <v>7.361</v>
+        <v>7.452</v>
       </c>
       <c r="J97" t="n">
-        <v>3046</v>
+        <v>4131</v>
       </c>
       <c r="K97" t="n">
-        <v>0.067</v>
+        <v>0.09</v>
       </c>
       <c r="L97" t="n">
-        <v>4030</v>
+        <v>4007</v>
       </c>
       <c r="M97" t="n">
         <v>0.088</v>
@@ -7975,7 +7996,7 @@
         <v>0.01</v>
       </c>
       <c r="O97" t="n">
-        <v>97.276</v>
+        <v>103.502</v>
       </c>
       <c r="P97" t="s">
         <v>576</v>
@@ -7998,7 +8019,7 @@
         <v>580</v>
       </c>
       <c r="C98" s="1" t="n">
-        <v>44064</v>
+        <v>44067</v>
       </c>
       <c r="D98" t="s">
         <v>581</v>
@@ -8008,28 +8029,32 @@
       </c>
       <c r="F98"/>
       <c r="G98" t="n">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="H98" t="n">
-        <v>1378519</v>
+        <v>1425351</v>
       </c>
       <c r="I98" t="n">
-        <v>31.521</v>
+        <v>32.592</v>
       </c>
       <c r="J98" t="n">
-        <v>21821</v>
+        <v>9350</v>
       </c>
       <c r="K98" t="n">
-        <v>0.499</v>
+        <v>0.214</v>
       </c>
       <c r="L98" t="n">
-        <v>17954</v>
+        <v>17866</v>
       </c>
       <c r="M98" t="n">
-        <v>0.411</v>
-      </c>
-      <c r="N98"/>
-      <c r="O98"/>
+        <v>0.409</v>
+      </c>
+      <c r="N98" t="n">
+        <v>0.097</v>
+      </c>
+      <c r="O98" t="n">
+        <v>10.303</v>
+      </c>
       <c r="P98" t="s">
         <v>582</v>
       </c>
@@ -8051,7 +8076,7 @@
         <v>586</v>
       </c>
       <c r="C99" s="1" t="n">
-        <v>44063</v>
+        <v>44066</v>
       </c>
       <c r="D99" t="s">
         <v>587</v>
@@ -8061,31 +8086,31 @@
       </c>
       <c r="F99"/>
       <c r="G99" t="n">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="H99" t="n">
-        <v>6265918</v>
+        <v>6489404</v>
       </c>
       <c r="I99" t="n">
-        <v>633.535</v>
+        <v>656.132</v>
       </c>
       <c r="J99" t="n">
-        <v>72283</v>
+        <v>71216</v>
       </c>
       <c r="K99" t="n">
-        <v>7.308</v>
+        <v>7.201</v>
       </c>
       <c r="L99" t="n">
-        <v>71509</v>
+        <v>71268</v>
       </c>
       <c r="M99" t="n">
-        <v>7.23</v>
+        <v>7.206</v>
       </c>
       <c r="N99" t="n">
-        <v>0.004</v>
+        <v>0.005</v>
       </c>
       <c r="O99" t="n">
-        <v>235.116</v>
+        <v>198.36</v>
       </c>
       <c r="P99" t="s">
         <v>588</v>
@@ -8220,7 +8245,7 @@
         <v>603</v>
       </c>
       <c r="C102" s="1" t="n">
-        <v>44063</v>
+        <v>44066</v>
       </c>
       <c r="D102" t="s">
         <v>604</v>
@@ -8230,31 +8255,31 @@
       </c>
       <c r="F102"/>
       <c r="G102" t="n">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="H102" t="n">
-        <v>69580676</v>
+        <v>71693547</v>
       </c>
       <c r="I102" t="n">
-        <v>210.212</v>
+        <v>216.595</v>
       </c>
       <c r="J102" t="n">
-        <v>635809</v>
+        <v>611382</v>
       </c>
       <c r="K102" t="n">
-        <v>1.921</v>
+        <v>1.847</v>
       </c>
       <c r="L102" t="n">
-        <v>709806</v>
+        <v>674363</v>
       </c>
       <c r="M102" t="n">
-        <v>2.144</v>
+        <v>2.037</v>
       </c>
       <c r="N102" t="n">
-        <v>0.067</v>
+        <v>0.065</v>
       </c>
       <c r="O102" t="n">
-        <v>14.935</v>
+        <v>15.379</v>
       </c>
       <c r="P102" t="s">
         <v>605</v>
@@ -8277,7 +8302,7 @@
         <v>610</v>
       </c>
       <c r="C103" s="1" t="n">
-        <v>44063</v>
+        <v>44065</v>
       </c>
       <c r="D103" t="s">
         <v>611</v>
@@ -8287,31 +8312,27 @@
       </c>
       <c r="F103"/>
       <c r="G103" t="n">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="H103" t="n">
-        <v>154431</v>
+        <v>158702</v>
       </c>
       <c r="I103" t="n">
-        <v>44.457</v>
-      </c>
-      <c r="J103" t="n">
-        <v>2310</v>
-      </c>
-      <c r="K103" t="n">
-        <v>0.665</v>
-      </c>
+        <v>45.686</v>
+      </c>
+      <c r="J103"/>
+      <c r="K103"/>
       <c r="L103" t="n">
-        <v>2247</v>
+        <v>2068</v>
       </c>
       <c r="M103" t="n">
-        <v>0.647</v>
+        <v>0.595</v>
       </c>
       <c r="N103" t="n">
-        <v>0.006</v>
+        <v>0.007</v>
       </c>
       <c r="O103" t="n">
-        <v>157.29</v>
+        <v>152.379</v>
       </c>
       <c r="P103" t="s">
         <v>125</v>
@@ -8387,7 +8408,7 @@
         <v>621</v>
       </c>
       <c r="C105" s="1" t="n">
-        <v>44063</v>
+        <v>44066</v>
       </c>
       <c r="D105" t="s">
         <v>622</v>
@@ -8397,31 +8418,31 @@
       </c>
       <c r="F105"/>
       <c r="G105" t="n">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="H105" t="n">
-        <v>87885</v>
+        <v>91548</v>
       </c>
       <c r="I105" t="n">
-        <v>5.913</v>
+        <v>6.159</v>
       </c>
       <c r="J105" t="n">
-        <v>1256</v>
+        <v>852</v>
       </c>
       <c r="K105" t="n">
-        <v>0.085</v>
+        <v>0.057</v>
       </c>
       <c r="L105" t="n">
-        <v>1307</v>
+        <v>1238</v>
       </c>
       <c r="M105" t="n">
-        <v>0.088</v>
+        <v>0.083</v>
       </c>
       <c r="N105" t="n">
-        <v>0.082</v>
+        <v>0.083</v>
       </c>
       <c r="O105" t="n">
-        <v>12.199</v>
+        <v>12.086</v>
       </c>
       <c r="P105" t="s">
         <v>623</v>

</xml_diff>

<commit_message>
Updated testing data for 2020-08-25
</commit_message>
<xml_diff>
--- a/public/data/testing/covid-testing-latest-data-source-details.xlsx
+++ b/public/data/testing/covid-testing-latest-data-source-details.xlsx
@@ -110,7 +110,7 @@
     <t xml:space="preserve">Australia - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.health.gov.au/sites/default/files/documents/2020/08/coronavirus-covid-19-at-a-glance-23-august-2020.pdf</t>
+    <t xml:space="preserve">https://www.health.gov.au/sites/default/files/documents/2020/08/coronavirus-covid-19-at-a-glance-24-august-2020.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">Australian Government Department of Health</t>
@@ -245,7 +245,7 @@
     <t xml:space="preserve">Bolivia - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://minsalud.gob.bo/4531-bolivia-acumula-41-111-pacientes-recuperados-de-covid-19-y-los-casos-positivos-llegan-a-106-065</t>
+    <t xml:space="preserve">https://minsalud.gob.bo/4542-bolivia-suma-722-contagios-nuevos-de-coronavirus-y-el-total-sube-a-109-149</t>
   </si>
   <si>
     <t xml:space="preserve">https://www.minsalud.gob.bo/</t>
@@ -477,7 +477,7 @@
     <t xml:space="preserve">Democratic Republic of Congo - samples tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/CMR_Covid19_RDC/status/1296733289567399936/photo/1</t>
+    <t xml:space="preserve">https://twitter.com/CMR_Covid19_RDC/status/1297508985793327105/photo/1</t>
   </si>
   <si>
     <t xml:space="preserve">DRC COVID-19 Pandemic Response Multisectoral Committee</t>
@@ -911,7 +911,7 @@
     <t xml:space="preserve">Iraq - samples tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://moh.gov.iq/index.php?name=News&amp;file=article&amp;sid=16380</t>
+    <t xml:space="preserve">https://moh.gov.iq/index.php?name=News&amp;file=article&amp;sid=16402</t>
   </si>
   <si>
     <t xml:space="preserve">Ministry of Health and Environment</t>
@@ -949,7 +949,7 @@
     <t xml:space="preserve">Israel - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://govextra.gov.il/media/25358/covid19-data-israel-17082020.csv</t>
+    <t xml:space="preserve">https://govextra.gov.il/media/25413/covid19-data-israel-18082020.csv</t>
   </si>
   <si>
     <t xml:space="preserve">Israel Ministry of Health</t>
@@ -1089,7 +1089,7 @@
     <t xml:space="preserve">Kuwait - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/KUWAIT_MOH/status/1296748941434851328/photo/1</t>
+    <t xml:space="preserve">https://twitter.com/KUWAIT_MOH/status/1297858722606309378/photo/1</t>
   </si>
   <si>
     <t xml:space="preserve">Kuwait Ministry of Health</t>
@@ -1181,7 +1181,7 @@
     <t xml:space="preserve">Maldives - samples tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/HPA_MV/status/1296854798076174336/photo/1</t>
+    <t xml:space="preserve">https://twitter.com/HPA_MV/status/1297944752265007110/photo/1</t>
   </si>
   <si>
     <t xml:space="preserve">Maldives Health Protection Agency</t>
@@ -1247,7 +1247,7 @@
     <t xml:space="preserve">Morocco - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/Ministere_Sante/status/1296857850669670401</t>
+    <t xml:space="preserve">https://twitter.com/Ministere_Sante/status/1297944286143623168/photo/1</t>
   </si>
   <si>
     <t xml:space="preserve">Morocco Ministry of Health</t>
@@ -1578,7 +1578,7 @@
     <t xml:space="preserve">Romania - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://gov.ro/ro/media/comunicate/buletin-de-presa-23-august-2020-ora-13-00&amp;page=1</t>
+    <t xml:space="preserve">https://gov.ro/ro/media/comunicate/buletin-de-presa-25-august-2020-ora-13-00&amp;page=1</t>
   </si>
   <si>
     <t xml:space="preserve">Ministry of Internal Affairs</t>
@@ -1601,7 +1601,7 @@
     <t xml:space="preserve">Russia - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://rospotrebnadzor.ru/about/info/news/news_details.php?ELEMENT_ID=15223</t>
+    <t xml:space="preserve">https://rospotrebnadzor.ru/about/info/news/news_details.php?ELEMENT_ID=15234</t>
   </si>
   <si>
     <t xml:space="preserve">Government of the Russian Federation</t>
@@ -2657,7 +2657,7 @@
         <v>25</v>
       </c>
       <c r="C3" s="1" t="n">
-        <v>44066</v>
+        <v>44067</v>
       </c>
       <c r="D3" t="s">
         <v>26</v>
@@ -2667,31 +2667,31 @@
       </c>
       <c r="F3"/>
       <c r="G3" t="n">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="H3" t="n">
-        <v>1150552</v>
+        <v>1172592</v>
       </c>
       <c r="I3" t="n">
-        <v>25.457</v>
+        <v>25.945</v>
       </c>
       <c r="J3" t="n">
-        <v>2589</v>
+        <v>4977</v>
       </c>
       <c r="K3" t="n">
-        <v>0.057</v>
+        <v>0.11</v>
       </c>
       <c r="L3" t="n">
-        <v>13752</v>
+        <v>14451</v>
       </c>
       <c r="M3" t="n">
-        <v>0.304</v>
+        <v>0.32</v>
       </c>
       <c r="N3" t="n">
-        <v>0.484</v>
+        <v>0.472</v>
       </c>
       <c r="O3" t="n">
-        <v>2.065</v>
+        <v>2.121</v>
       </c>
       <c r="P3" t="s">
         <v>22</v>
@@ -2714,7 +2714,7 @@
         <v>30</v>
       </c>
       <c r="C4" s="1" t="n">
-        <v>44066</v>
+        <v>44067</v>
       </c>
       <c r="D4" t="s">
         <v>31</v>
@@ -2724,27 +2724,31 @@
       </c>
       <c r="F4"/>
       <c r="G4" t="n">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="H4" t="n">
-        <v>5706587</v>
+        <v>5758034</v>
       </c>
       <c r="I4" t="n">
-        <v>223.789</v>
-      </c>
-      <c r="J4"/>
-      <c r="K4"/>
+        <v>225.806</v>
+      </c>
+      <c r="J4" t="n">
+        <v>51447</v>
+      </c>
+      <c r="K4" t="n">
+        <v>2.018</v>
+      </c>
       <c r="L4" t="n">
-        <v>58433</v>
+        <v>60277</v>
       </c>
       <c r="M4" t="n">
-        <v>2.292</v>
+        <v>2.364</v>
       </c>
       <c r="N4" t="n">
         <v>0.004</v>
       </c>
       <c r="O4" t="n">
-        <v>261.028</v>
+        <v>276.863</v>
       </c>
       <c r="P4" t="s">
         <v>32</v>
@@ -2767,7 +2771,7 @@
         <v>36</v>
       </c>
       <c r="C5" s="1" t="n">
-        <v>44067</v>
+        <v>44068</v>
       </c>
       <c r="D5" t="s">
         <v>37</v>
@@ -2777,31 +2781,31 @@
       </c>
       <c r="F5"/>
       <c r="G5" t="n">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="H5" t="n">
-        <v>1101206</v>
+        <v>1110089</v>
       </c>
       <c r="I5" t="n">
-        <v>122.269</v>
+        <v>123.256</v>
       </c>
       <c r="J5" t="n">
-        <v>6219</v>
+        <v>8883</v>
       </c>
       <c r="K5" t="n">
-        <v>0.691</v>
+        <v>0.986</v>
       </c>
       <c r="L5" t="n">
-        <v>11020</v>
+        <v>10314</v>
       </c>
       <c r="M5" t="n">
-        <v>1.224</v>
+        <v>1.145</v>
       </c>
       <c r="N5" t="n">
-        <v>0.024</v>
+        <v>0.025</v>
       </c>
       <c r="O5" t="n">
-        <v>41.34</v>
+        <v>39.452</v>
       </c>
       <c r="P5" t="s">
         <v>39</v>
@@ -2824,7 +2828,7 @@
         <v>43</v>
       </c>
       <c r="C6" s="1" t="n">
-        <v>44067</v>
+        <v>44068</v>
       </c>
       <c r="D6" t="s">
         <v>44</v>
@@ -2834,31 +2838,31 @@
       </c>
       <c r="F6"/>
       <c r="G6" t="n">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="H6" t="n">
-        <v>1039571</v>
+        <v>1048935</v>
       </c>
       <c r="I6" t="n">
-        <v>610.943</v>
+        <v>616.447</v>
       </c>
       <c r="J6" t="n">
-        <v>9602</v>
+        <v>9364</v>
       </c>
       <c r="K6" t="n">
-        <v>5.643</v>
+        <v>5.503</v>
       </c>
       <c r="L6" t="n">
-        <v>9653</v>
+        <v>9675</v>
       </c>
       <c r="M6" t="n">
-        <v>5.673</v>
+        <v>5.686</v>
       </c>
       <c r="N6" t="n">
-        <v>0.039</v>
+        <v>0.032</v>
       </c>
       <c r="O6" t="n">
-        <v>25.909</v>
+        <v>31.573</v>
       </c>
       <c r="P6" t="s">
         <v>46</v>
@@ -2995,7 +2999,7 @@
         <v>63</v>
       </c>
       <c r="C9" s="1" t="n">
-        <v>44065</v>
+        <v>44066</v>
       </c>
       <c r="D9" t="s">
         <v>64</v>
@@ -3005,31 +3009,31 @@
       </c>
       <c r="F9"/>
       <c r="G9" t="n">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="H9" t="n">
-        <v>2135342</v>
+        <v>2144401</v>
       </c>
       <c r="I9" t="n">
-        <v>184.246</v>
+        <v>185.028</v>
       </c>
       <c r="J9" t="n">
-        <v>12962</v>
+        <v>7221</v>
       </c>
       <c r="K9" t="n">
-        <v>1.118</v>
+        <v>0.623</v>
       </c>
       <c r="L9" t="n">
-        <v>19059</v>
+        <v>19071</v>
       </c>
       <c r="M9" t="n">
-        <v>1.644</v>
+        <v>1.646</v>
       </c>
       <c r="N9" t="n">
         <v>0.025</v>
       </c>
       <c r="O9" t="n">
-        <v>40.749</v>
+        <v>40.688</v>
       </c>
       <c r="P9" t="s">
         <v>65</v>
@@ -3052,7 +3056,7 @@
         <v>69</v>
       </c>
       <c r="C10" s="1" t="n">
-        <v>44063</v>
+        <v>44066</v>
       </c>
       <c r="D10" t="s">
         <v>70</v>
@@ -3062,31 +3066,31 @@
       </c>
       <c r="F10"/>
       <c r="G10" t="n">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="H10" t="n">
-        <v>211318</v>
+        <v>218864</v>
       </c>
       <c r="I10" t="n">
-        <v>18.103</v>
+        <v>18.75</v>
       </c>
       <c r="J10" t="n">
-        <v>2680</v>
+        <v>2385</v>
       </c>
       <c r="K10" t="n">
-        <v>0.23</v>
+        <v>0.204</v>
       </c>
       <c r="L10" t="n">
-        <v>3126</v>
+        <v>2881</v>
       </c>
       <c r="M10" t="n">
-        <v>0.268</v>
+        <v>0.247</v>
       </c>
       <c r="N10" t="n">
-        <v>0.456</v>
+        <v>0.46</v>
       </c>
       <c r="O10" t="n">
-        <v>2.193</v>
+        <v>2.173</v>
       </c>
       <c r="P10" t="s">
         <v>45</v>
@@ -3160,7 +3164,7 @@
         <v>81</v>
       </c>
       <c r="C12" s="1" t="n">
-        <v>44067</v>
+        <v>44068</v>
       </c>
       <c r="D12" t="s">
         <v>82</v>
@@ -3170,31 +3174,31 @@
       </c>
       <c r="F12"/>
       <c r="G12" t="n">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="H12" t="n">
-        <v>370786</v>
+        <v>374374</v>
       </c>
       <c r="I12" t="n">
-        <v>53.362</v>
+        <v>53.879</v>
       </c>
       <c r="J12" t="n">
-        <v>2288</v>
+        <v>3588</v>
       </c>
       <c r="K12" t="n">
-        <v>0.329</v>
+        <v>0.516</v>
       </c>
       <c r="L12" t="n">
-        <v>5211</v>
+        <v>4973</v>
       </c>
       <c r="M12" t="n">
-        <v>0.75</v>
+        <v>0.716</v>
       </c>
       <c r="N12" t="n">
-        <v>0.024</v>
+        <v>0.023</v>
       </c>
       <c r="O12" t="n">
-        <v>42.317</v>
+        <v>44.233</v>
       </c>
       <c r="P12" t="s">
         <v>84</v>
@@ -3217,7 +3221,7 @@
         <v>87</v>
       </c>
       <c r="C13" s="1" t="n">
-        <v>44067</v>
+        <v>44068</v>
       </c>
       <c r="D13" t="s">
         <v>88</v>
@@ -3227,31 +3231,31 @@
       </c>
       <c r="F13"/>
       <c r="G13" t="n">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="H13" t="n">
-        <v>5115490</v>
+        <v>5169166</v>
       </c>
       <c r="I13" t="n">
-        <v>135.538</v>
+        <v>136.96</v>
       </c>
       <c r="J13" t="n">
-        <v>38756</v>
+        <v>53676</v>
       </c>
       <c r="K13" t="n">
-        <v>1.027</v>
+        <v>1.422</v>
       </c>
       <c r="L13" t="n">
-        <v>48161</v>
+        <v>47018</v>
       </c>
       <c r="M13" t="n">
-        <v>1.276</v>
+        <v>1.246</v>
       </c>
       <c r="N13" t="n">
         <v>0.008</v>
       </c>
       <c r="O13" t="n">
-        <v>120.017</v>
+        <v>118.604</v>
       </c>
       <c r="P13" t="s">
         <v>89</v>
@@ -3333,7 +3337,7 @@
         <v>99</v>
       </c>
       <c r="C15" s="1" t="n">
-        <v>44066</v>
+        <v>44067</v>
       </c>
       <c r="D15" t="s">
         <v>100</v>
@@ -3343,31 +3347,31 @@
       </c>
       <c r="F15"/>
       <c r="G15" t="n">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="H15" t="n">
-        <v>2396892</v>
+        <v>2427941</v>
       </c>
       <c r="I15" t="n">
-        <v>47.106</v>
+        <v>47.716</v>
       </c>
       <c r="J15" t="n">
-        <v>22824</v>
+        <v>31049</v>
       </c>
       <c r="K15" t="n">
-        <v>0.449</v>
+        <v>0.61</v>
       </c>
       <c r="L15" t="n">
-        <v>31272</v>
+        <v>31033</v>
       </c>
       <c r="M15" t="n">
-        <v>0.615</v>
+        <v>0.61</v>
       </c>
       <c r="N15" t="n">
-        <v>0.349</v>
+        <v>0.335</v>
       </c>
       <c r="O15" t="n">
-        <v>2.865</v>
+        <v>2.983</v>
       </c>
       <c r="P15" t="s">
         <v>101</v>
@@ -3673,7 +3677,7 @@
         <v>135</v>
       </c>
       <c r="C21" s="1" t="n">
-        <v>44063</v>
+        <v>44065</v>
       </c>
       <c r="D21" t="s">
         <v>136</v>
@@ -3683,27 +3687,27 @@
       </c>
       <c r="F21"/>
       <c r="G21" t="n">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="H21"/>
       <c r="I21"/>
       <c r="J21" t="n">
-        <v>309</v>
+        <v>422</v>
       </c>
       <c r="K21" t="n">
-        <v>0.003</v>
+        <v>0.005</v>
       </c>
       <c r="L21" t="n">
-        <v>351</v>
+        <v>317</v>
       </c>
       <c r="M21" t="n">
         <v>0.004</v>
       </c>
       <c r="N21" t="n">
-        <v>0.083</v>
+        <v>0.089</v>
       </c>
       <c r="O21" t="n">
-        <v>12.103</v>
+        <v>11.264</v>
       </c>
       <c r="P21" t="s">
         <v>137</v>
@@ -3895,7 +3899,7 @@
         <v>160</v>
       </c>
       <c r="C25" s="1" t="n">
-        <v>44066</v>
+        <v>44067</v>
       </c>
       <c r="D25" t="s">
         <v>161</v>
@@ -3905,31 +3909,31 @@
       </c>
       <c r="F25"/>
       <c r="G25" t="n">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="H25" t="n">
-        <v>140985</v>
+        <v>142160</v>
       </c>
       <c r="I25" t="n">
-        <v>106.28</v>
+        <v>107.166</v>
       </c>
       <c r="J25" t="n">
-        <v>320</v>
+        <v>1186</v>
       </c>
       <c r="K25" t="n">
-        <v>0.241</v>
+        <v>0.894</v>
       </c>
       <c r="L25" t="n">
-        <v>876</v>
+        <v>863</v>
       </c>
       <c r="M25" t="n">
-        <v>0.66</v>
+        <v>0.651</v>
       </c>
       <c r="N25" t="n">
-        <v>0.013</v>
+        <v>0.014</v>
       </c>
       <c r="O25" t="n">
-        <v>75.704</v>
+        <v>73.671</v>
       </c>
       <c r="P25" t="s">
         <v>163</v>
@@ -4077,28 +4081,28 @@
         <v>181</v>
       </c>
       <c r="H28" t="n">
-        <v>551715</v>
+        <v>571675</v>
       </c>
       <c r="I28" t="n">
-        <v>99.575</v>
+        <v>103.177</v>
       </c>
       <c r="J28" t="n">
-        <v>822</v>
+        <v>6146</v>
       </c>
       <c r="K28" t="n">
-        <v>0.148</v>
+        <v>1.109</v>
       </c>
       <c r="L28" t="n">
-        <v>7487</v>
+        <v>10338</v>
       </c>
       <c r="M28" t="n">
-        <v>1.351</v>
+        <v>1.866</v>
       </c>
       <c r="N28" t="n">
-        <v>0.003</v>
+        <v>0.002</v>
       </c>
       <c r="O28" t="n">
-        <v>347.079</v>
+        <v>479.245</v>
       </c>
       <c r="P28" t="s">
         <v>182</v>
@@ -4506,7 +4510,7 @@
         <v>232</v>
       </c>
       <c r="C36" s="1" t="n">
-        <v>44066</v>
+        <v>44067</v>
       </c>
       <c r="D36" t="s">
         <v>233</v>
@@ -4516,31 +4520,31 @@
       </c>
       <c r="F36"/>
       <c r="G36" t="n">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="H36" t="n">
-        <v>85203</v>
+        <v>85805</v>
       </c>
       <c r="I36" t="n">
-        <v>249.679</v>
+        <v>251.443</v>
       </c>
       <c r="J36" t="n">
-        <v>291</v>
+        <v>602</v>
       </c>
       <c r="K36" t="n">
-        <v>0.853</v>
+        <v>1.764</v>
       </c>
       <c r="L36" t="n">
-        <v>444</v>
+        <v>472</v>
       </c>
       <c r="M36" t="n">
-        <v>1.301</v>
+        <v>1.383</v>
       </c>
       <c r="N36" t="n">
-        <v>0.019</v>
+        <v>0.016</v>
       </c>
       <c r="O36" t="n">
-        <v>52.678</v>
+        <v>62.34</v>
       </c>
       <c r="P36" t="s">
         <v>234</v>
@@ -4622,7 +4626,7 @@
         <v>242</v>
       </c>
       <c r="C38" s="1" t="n">
-        <v>44065</v>
+        <v>44067</v>
       </c>
       <c r="D38" t="s">
         <v>238</v>
@@ -4634,31 +4638,27 @@
         <v>240</v>
       </c>
       <c r="G38" t="n">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="H38" t="n">
-        <v>35292220</v>
+        <v>36827520</v>
       </c>
       <c r="I38" t="n">
-        <v>25.574</v>
-      </c>
-      <c r="J38" t="n">
-        <v>801147</v>
-      </c>
-      <c r="K38" t="n">
-        <v>0.581</v>
-      </c>
+        <v>26.687</v>
+      </c>
+      <c r="J38"/>
+      <c r="K38"/>
       <c r="L38" t="n">
-        <v>854645</v>
+        <v>840894</v>
       </c>
       <c r="M38" t="n">
-        <v>0.619</v>
+        <v>0.609</v>
       </c>
       <c r="N38" t="n">
-        <v>0.075</v>
+        <v>0.078</v>
       </c>
       <c r="O38" t="n">
-        <v>13.309</v>
+        <v>12.833</v>
       </c>
       <c r="P38" t="s">
         <v>239</v>
@@ -4681,7 +4681,7 @@
         <v>244</v>
       </c>
       <c r="C39" s="1" t="n">
-        <v>44063</v>
+        <v>44068</v>
       </c>
       <c r="D39" t="s">
         <v>245</v>
@@ -4694,28 +4694,24 @@
         <v>144</v>
       </c>
       <c r="H39" t="n">
-        <v>1969941</v>
+        <v>1191948</v>
       </c>
       <c r="I39" t="n">
-        <v>7.202</v>
-      </c>
-      <c r="J39" t="n">
-        <v>873647</v>
-      </c>
-      <c r="K39" t="n">
-        <v>3.194</v>
-      </c>
+        <v>4.358</v>
+      </c>
+      <c r="J39"/>
+      <c r="K39"/>
       <c r="L39" t="n">
-        <v>134712</v>
+        <v>15799</v>
       </c>
       <c r="M39" t="n">
-        <v>0.493</v>
+        <v>0.058</v>
       </c>
       <c r="N39" t="n">
-        <v>0.015</v>
+        <v>0.127</v>
       </c>
       <c r="O39" t="n">
-        <v>66.281</v>
+        <v>7.876</v>
       </c>
       <c r="P39" t="s">
         <v>246</v>
@@ -4795,7 +4791,7 @@
         <v>256</v>
       </c>
       <c r="C41" s="1" t="n">
-        <v>44062</v>
+        <v>44066</v>
       </c>
       <c r="D41" t="s">
         <v>257</v>
@@ -4805,31 +4801,31 @@
       </c>
       <c r="F41"/>
       <c r="G41" t="n">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="H41" t="n">
-        <v>1345459</v>
+        <v>1433626</v>
       </c>
       <c r="I41" t="n">
-        <v>33.45</v>
+        <v>35.642</v>
       </c>
       <c r="J41" t="n">
-        <v>20356</v>
+        <v>19679</v>
       </c>
       <c r="K41" t="n">
-        <v>0.506</v>
+        <v>0.489</v>
       </c>
       <c r="L41" t="n">
-        <v>20225</v>
+        <v>21528</v>
       </c>
       <c r="M41" t="n">
-        <v>0.503</v>
+        <v>0.535</v>
       </c>
       <c r="N41" t="n">
-        <v>0.196</v>
+        <v>0.189</v>
       </c>
       <c r="O41" t="n">
-        <v>5.108</v>
+        <v>5.294</v>
       </c>
       <c r="P41" t="s">
         <v>259</v>
@@ -4909,7 +4905,7 @@
         <v>268</v>
       </c>
       <c r="C43" s="1" t="n">
-        <v>44060</v>
+        <v>44061</v>
       </c>
       <c r="D43" t="s">
         <v>269</v>
@@ -4919,31 +4915,31 @@
       </c>
       <c r="F43"/>
       <c r="G43" t="n">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="H43" t="n">
-        <v>2118768</v>
+        <v>2146693</v>
       </c>
       <c r="I43" t="n">
-        <v>244.787</v>
+        <v>248.014</v>
       </c>
       <c r="J43" t="n">
-        <v>26043</v>
+        <v>27920</v>
       </c>
       <c r="K43" t="n">
-        <v>3.009</v>
+        <v>3.226</v>
       </c>
       <c r="L43" t="n">
-        <v>21649</v>
+        <v>21688</v>
       </c>
       <c r="M43" t="n">
-        <v>2.501</v>
+        <v>2.506</v>
       </c>
       <c r="N43" t="n">
-        <v>0.064</v>
+        <v>0.065</v>
       </c>
       <c r="O43" t="n">
-        <v>15.659</v>
+        <v>15.324</v>
       </c>
       <c r="P43" t="s">
         <v>45</v>
@@ -5316,7 +5312,7 @@
         <v>307</v>
       </c>
       <c r="C50" s="1" t="n">
-        <v>44064</v>
+        <v>44067</v>
       </c>
       <c r="D50" t="s">
         <v>308</v>
@@ -5326,31 +5322,31 @@
       </c>
       <c r="F50"/>
       <c r="G50" t="n">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="H50" t="n">
-        <v>581118</v>
+        <v>590623</v>
       </c>
       <c r="I50" t="n">
-        <v>136.075</v>
+        <v>138.301</v>
       </c>
       <c r="J50" t="n">
-        <v>3530</v>
+        <v>3056</v>
       </c>
       <c r="K50" t="n">
-        <v>0.827</v>
+        <v>0.716</v>
       </c>
       <c r="L50" t="n">
-        <v>4077</v>
+        <v>3927</v>
       </c>
       <c r="M50" t="n">
-        <v>0.955</v>
+        <v>0.92</v>
       </c>
       <c r="N50" t="n">
-        <v>0.15</v>
+        <v>0.157</v>
       </c>
       <c r="O50" t="n">
-        <v>6.666</v>
+        <v>6.359</v>
       </c>
       <c r="P50" t="s">
         <v>309</v>
@@ -5373,7 +5369,7 @@
         <v>313</v>
       </c>
       <c r="C51" s="1" t="n">
-        <v>44067</v>
+        <v>44068</v>
       </c>
       <c r="D51" t="s">
         <v>314</v>
@@ -5385,31 +5381,31 @@
         <v>316</v>
       </c>
       <c r="G51" t="n">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="H51" t="n">
-        <v>238403</v>
+        <v>240533</v>
       </c>
       <c r="I51" t="n">
-        <v>126.393</v>
+        <v>127.522</v>
       </c>
       <c r="J51" t="n">
-        <v>926</v>
+        <v>2130</v>
       </c>
       <c r="K51" t="n">
-        <v>0.491</v>
+        <v>1.129</v>
       </c>
       <c r="L51" t="n">
-        <v>1697</v>
+        <v>1682</v>
       </c>
       <c r="M51" t="n">
-        <v>0.9</v>
+        <v>0.892</v>
       </c>
       <c r="N51" t="n">
         <v>0.001</v>
       </c>
       <c r="O51" t="n">
-        <v>791.933</v>
+        <v>841</v>
       </c>
       <c r="P51" t="s">
         <v>315</v>
@@ -5432,7 +5428,7 @@
         <v>319</v>
       </c>
       <c r="C52" s="1" t="n">
-        <v>44067</v>
+        <v>44068</v>
       </c>
       <c r="D52" t="s">
         <v>320</v>
@@ -5442,27 +5438,31 @@
       </c>
       <c r="F52"/>
       <c r="G52" t="n">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="H52" t="n">
-        <v>608767</v>
+        <v>613324</v>
       </c>
       <c r="I52" t="n">
-        <v>223.623</v>
-      </c>
-      <c r="J52"/>
-      <c r="K52"/>
+        <v>225.297</v>
+      </c>
+      <c r="J52" t="n">
+        <v>4557</v>
+      </c>
+      <c r="K52" t="n">
+        <v>1.674</v>
+      </c>
       <c r="L52" t="n">
-        <v>4045</v>
+        <v>4098</v>
       </c>
       <c r="M52" t="n">
-        <v>1.486</v>
+        <v>1.505</v>
       </c>
       <c r="N52" t="n">
         <v>0.008</v>
       </c>
       <c r="O52" t="n">
-        <v>129.292</v>
+        <v>121.038</v>
       </c>
       <c r="P52" t="s">
         <v>45</v>
@@ -5601,7 +5601,7 @@
         <v>335</v>
       </c>
       <c r="C55" s="1" t="n">
-        <v>44064</v>
+        <v>44067</v>
       </c>
       <c r="D55" t="s">
         <v>336</v>
@@ -5611,31 +5611,31 @@
       </c>
       <c r="F55"/>
       <c r="G55" t="n">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="H55" t="n">
-        <v>101730</v>
+        <v>104631</v>
       </c>
       <c r="I55" t="n">
-        <v>188.2</v>
+        <v>193.567</v>
       </c>
       <c r="J55" t="n">
-        <v>1497</v>
+        <v>977</v>
       </c>
       <c r="K55" t="n">
-        <v>2.769</v>
+        <v>1.807</v>
       </c>
       <c r="L55" t="n">
-        <v>1098</v>
+        <v>1060</v>
       </c>
       <c r="M55" t="n">
-        <v>2.031</v>
+        <v>1.961</v>
       </c>
       <c r="N55" t="n">
-        <v>0.114</v>
+        <v>0.134</v>
       </c>
       <c r="O55" t="n">
-        <v>8.774</v>
+        <v>7.465</v>
       </c>
       <c r="P55" t="s">
         <v>338</v>
@@ -5715,7 +5715,7 @@
         <v>348</v>
       </c>
       <c r="C57" s="1" t="n">
-        <v>44062</v>
+        <v>44064</v>
       </c>
       <c r="D57" t="s">
         <v>349</v>
@@ -5725,31 +5725,31 @@
       </c>
       <c r="F57"/>
       <c r="G57" t="n">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="H57" t="n">
-        <v>1170251</v>
+        <v>1185178</v>
       </c>
       <c r="I57" t="n">
-        <v>9.076</v>
+        <v>9.192</v>
       </c>
       <c r="J57" t="n">
-        <v>8789</v>
+        <v>5041</v>
       </c>
       <c r="K57" t="n">
-        <v>0.068</v>
+        <v>0.039</v>
       </c>
       <c r="L57" t="n">
-        <v>9665</v>
+        <v>8084</v>
       </c>
       <c r="M57" t="n">
-        <v>0.075</v>
+        <v>0.063</v>
       </c>
       <c r="N57" t="n">
-        <v>0.572</v>
+        <v>0.672</v>
       </c>
       <c r="O57" t="n">
-        <v>1.747</v>
+        <v>1.487</v>
       </c>
       <c r="P57" t="s">
         <v>351</v>
@@ -5772,7 +5772,7 @@
         <v>355</v>
       </c>
       <c r="C58" s="1" t="n">
-        <v>44064</v>
+        <v>44067</v>
       </c>
       <c r="D58" t="s">
         <v>356</v>
@@ -5782,31 +5782,31 @@
       </c>
       <c r="F58"/>
       <c r="G58" t="n">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="H58" t="n">
-        <v>1714583</v>
+        <v>1779980</v>
       </c>
       <c r="I58" t="n">
-        <v>46.452</v>
+        <v>48.224</v>
       </c>
       <c r="J58" t="n">
-        <v>22178</v>
+        <v>21110</v>
       </c>
       <c r="K58" t="n">
-        <v>0.601</v>
+        <v>0.572</v>
       </c>
       <c r="L58" t="n">
-        <v>22008</v>
+        <v>21881</v>
       </c>
       <c r="M58" t="n">
-        <v>0.596</v>
+        <v>0.593</v>
       </c>
       <c r="N58" t="n">
-        <v>0.063</v>
+        <v>0.054</v>
       </c>
       <c r="O58" t="n">
-        <v>15.877</v>
+        <v>18.403</v>
       </c>
       <c r="P58" t="s">
         <v>357</v>
@@ -5996,7 +5996,7 @@
         <v>380</v>
       </c>
       <c r="C62" s="1" t="n">
-        <v>44066</v>
+        <v>44067</v>
       </c>
       <c r="D62" t="s">
         <v>381</v>
@@ -6006,31 +6006,31 @@
       </c>
       <c r="F62"/>
       <c r="G62" t="n">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="H62" t="n">
-        <v>697070</v>
+        <v>701504</v>
       </c>
       <c r="I62" t="n">
-        <v>144.553</v>
+        <v>145.473</v>
       </c>
       <c r="J62" t="n">
-        <v>4589</v>
+        <v>4434</v>
       </c>
       <c r="K62" t="n">
-        <v>0.952</v>
+        <v>0.919</v>
       </c>
       <c r="L62" t="n">
-        <v>14159</v>
+        <v>12161</v>
       </c>
       <c r="M62" t="n">
-        <v>2.936</v>
+        <v>2.522</v>
       </c>
       <c r="N62" t="n">
         <v>0.001</v>
       </c>
       <c r="O62" t="n">
-        <v>1870.057</v>
+        <v>1637.058</v>
       </c>
       <c r="P62" t="s">
         <v>382</v>
@@ -6110,7 +6110,7 @@
         <v>391</v>
       </c>
       <c r="C64" s="1" t="n">
-        <v>44062</v>
+        <v>44066</v>
       </c>
       <c r="D64" t="s">
         <v>392</v>
@@ -6120,31 +6120,31 @@
       </c>
       <c r="F64"/>
       <c r="G64" t="n">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="H64" t="n">
-        <v>580724</v>
+        <v>619288</v>
       </c>
       <c r="I64" t="n">
-        <v>107.12</v>
+        <v>114.234</v>
       </c>
       <c r="J64" t="n">
-        <v>8712</v>
+        <v>3353</v>
       </c>
       <c r="K64" t="n">
-        <v>1.607</v>
+        <v>0.618</v>
       </c>
       <c r="L64" t="n">
-        <v>9801</v>
+        <v>10743</v>
       </c>
       <c r="M64" t="n">
-        <v>1.808</v>
+        <v>1.982</v>
       </c>
       <c r="N64" t="n">
         <v>0.005</v>
       </c>
       <c r="O64" t="n">
-        <v>182.465</v>
+        <v>216.718</v>
       </c>
       <c r="P64" t="s">
         <v>393</v>
@@ -6212,7 +6212,7 @@
         <v>405</v>
       </c>
       <c r="C66" s="1" t="n">
-        <v>44067</v>
+        <v>44068</v>
       </c>
       <c r="D66" t="s">
         <v>406</v>
@@ -6222,31 +6222,31 @@
       </c>
       <c r="F66"/>
       <c r="G66" t="n">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="H66" t="n">
-        <v>2463513</v>
+        <v>2487744</v>
       </c>
       <c r="I66" t="n">
-        <v>11.153</v>
+        <v>11.262</v>
       </c>
       <c r="J66" t="n">
-        <v>23655</v>
+        <v>24231</v>
       </c>
       <c r="K66" t="n">
-        <v>0.107</v>
+        <v>0.11</v>
       </c>
       <c r="L66" t="n">
-        <v>23416</v>
+        <v>24362</v>
       </c>
       <c r="M66" t="n">
-        <v>0.106</v>
+        <v>0.11</v>
       </c>
       <c r="N66" t="n">
-        <v>0.022</v>
+        <v>0.023</v>
       </c>
       <c r="O66" t="n">
-        <v>46.172</v>
+        <v>43.963</v>
       </c>
       <c r="P66" t="s">
         <v>407</v>
@@ -6721,7 +6721,7 @@
         <v>453</v>
       </c>
       <c r="C75" s="1" t="n">
-        <v>44066</v>
+        <v>44068</v>
       </c>
       <c r="D75" t="s">
         <v>454</v>
@@ -6731,31 +6731,31 @@
       </c>
       <c r="F75"/>
       <c r="G75" t="n">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="H75" t="n">
-        <v>1652644</v>
+        <v>1679614</v>
       </c>
       <c r="I75" t="n">
-        <v>85.907</v>
+        <v>87.309</v>
       </c>
       <c r="J75" t="n">
-        <v>13274</v>
+        <v>20479</v>
       </c>
       <c r="K75" t="n">
-        <v>0.69</v>
+        <v>1.065</v>
       </c>
       <c r="L75" t="n">
-        <v>19822</v>
+        <v>19646</v>
       </c>
       <c r="M75" t="n">
-        <v>1.03</v>
+        <v>1.021</v>
       </c>
       <c r="N75" t="n">
         <v>0.059</v>
       </c>
       <c r="O75" t="n">
-        <v>16.983</v>
+        <v>16.903</v>
       </c>
       <c r="P75" t="s">
         <v>456</v>
@@ -6778,7 +6778,7 @@
         <v>460</v>
       </c>
       <c r="C76" s="1" t="n">
-        <v>44066</v>
+        <v>44067</v>
       </c>
       <c r="D76" t="s">
         <v>461</v>
@@ -6788,31 +6788,31 @@
       </c>
       <c r="F76"/>
       <c r="G76" t="n">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="H76" t="n">
-        <v>34695406</v>
+        <v>34883220</v>
       </c>
       <c r="I76" t="n">
-        <v>237.746</v>
+        <v>239.033</v>
       </c>
       <c r="J76" t="n">
-        <v>247846</v>
+        <v>187814</v>
       </c>
       <c r="K76" t="n">
-        <v>1.698</v>
+        <v>1.287</v>
       </c>
       <c r="L76" t="n">
-        <v>272990</v>
+        <v>273494</v>
       </c>
       <c r="M76" t="n">
-        <v>1.871</v>
+        <v>1.874</v>
       </c>
       <c r="N76" t="n">
         <v>0.018</v>
       </c>
       <c r="O76" t="n">
-        <v>56.182</v>
+        <v>56.48</v>
       </c>
       <c r="P76" t="s">
         <v>462</v>
@@ -7169,7 +7169,7 @@
         <v>496</v>
       </c>
       <c r="C83" s="1" t="n">
-        <v>44065</v>
+        <v>44068</v>
       </c>
       <c r="D83" t="s">
         <v>497</v>
@@ -7179,31 +7179,27 @@
       </c>
       <c r="F83"/>
       <c r="G83" t="n">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="H83" t="n">
-        <v>311099</v>
+        <v>315854</v>
       </c>
       <c r="I83" t="n">
-        <v>56.982</v>
-      </c>
-      <c r="J83" t="n">
-        <v>7013</v>
-      </c>
-      <c r="K83" t="n">
-        <v>1.285</v>
-      </c>
+        <v>57.853</v>
+      </c>
+      <c r="J83"/>
+      <c r="K83"/>
       <c r="L83" t="n">
-        <v>2611</v>
+        <v>2707</v>
       </c>
       <c r="M83" t="n">
-        <v>0.478</v>
+        <v>0.496</v>
       </c>
       <c r="N83" t="n">
-        <v>0.023</v>
+        <v>0.027</v>
       </c>
       <c r="O83" t="n">
-        <v>43.106</v>
+        <v>36.652</v>
       </c>
       <c r="P83" t="s">
         <v>499</v>
@@ -7226,7 +7222,7 @@
         <v>502</v>
       </c>
       <c r="C84" s="1" t="n">
-        <v>44066</v>
+        <v>44067</v>
       </c>
       <c r="D84" t="s">
         <v>503</v>
@@ -7236,31 +7232,31 @@
       </c>
       <c r="F84"/>
       <c r="G84" t="n">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="H84" t="n">
-        <v>149235</v>
+        <v>150695</v>
       </c>
       <c r="I84" t="n">
-        <v>71.784</v>
+        <v>72.487</v>
       </c>
       <c r="J84" t="n">
-        <v>453</v>
+        <v>1460</v>
       </c>
       <c r="K84" t="n">
-        <v>0.218</v>
+        <v>0.702</v>
       </c>
       <c r="L84" t="n">
-        <v>988</v>
+        <v>1033</v>
       </c>
       <c r="M84" t="n">
-        <v>0.475</v>
+        <v>0.497</v>
       </c>
       <c r="N84" t="n">
-        <v>0.031</v>
+        <v>0.032</v>
       </c>
       <c r="O84" t="n">
-        <v>32.019</v>
+        <v>30.77</v>
       </c>
       <c r="P84" t="s">
         <v>505</v>
@@ -7283,7 +7279,7 @@
         <v>509</v>
       </c>
       <c r="C85" s="1" t="n">
-        <v>44065</v>
+        <v>44067</v>
       </c>
       <c r="D85" t="s">
         <v>510</v>
@@ -7295,31 +7291,31 @@
         <v>512</v>
       </c>
       <c r="G85" t="n">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="H85" t="n">
-        <v>3535067</v>
+        <v>3564065</v>
       </c>
       <c r="I85" t="n">
-        <v>59.605</v>
+        <v>60.093</v>
       </c>
       <c r="J85" t="n">
-        <v>30560</v>
+        <v>10640</v>
       </c>
       <c r="K85" t="n">
-        <v>0.515</v>
+        <v>0.179</v>
       </c>
       <c r="L85" t="n">
-        <v>22434</v>
+        <v>21199</v>
       </c>
       <c r="M85" t="n">
-        <v>0.378</v>
+        <v>0.357</v>
       </c>
       <c r="N85" t="n">
-        <v>0.154</v>
+        <v>0.151</v>
       </c>
       <c r="O85" t="n">
-        <v>6.49</v>
+        <v>6.616</v>
       </c>
       <c r="P85" t="s">
         <v>511</v>
@@ -7558,7 +7554,7 @@
         <v>539</v>
       </c>
       <c r="C90" s="1" t="n">
-        <v>44065</v>
+        <v>44067</v>
       </c>
       <c r="D90" t="s">
         <v>540</v>
@@ -7568,31 +7564,31 @@
       </c>
       <c r="F90"/>
       <c r="G90" t="n">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="H90" t="n">
-        <v>939231</v>
+        <v>948439</v>
       </c>
       <c r="I90" t="n">
-        <v>108.524</v>
+        <v>109.588</v>
       </c>
       <c r="J90" t="n">
-        <v>5923</v>
+        <v>5651</v>
       </c>
       <c r="K90" t="n">
-        <v>0.684</v>
+        <v>0.653</v>
       </c>
       <c r="L90" t="n">
-        <v>8000</v>
+        <v>7787</v>
       </c>
       <c r="M90" t="n">
-        <v>0.924</v>
+        <v>0.9</v>
       </c>
       <c r="N90" t="n">
-        <v>0.029</v>
+        <v>0.032</v>
       </c>
       <c r="O90" t="n">
-        <v>33.898</v>
+        <v>30.779</v>
       </c>
       <c r="P90" t="s">
         <v>541</v>
@@ -8014,7 +8010,7 @@
         <v>580</v>
       </c>
       <c r="C98" s="1" t="n">
-        <v>44067</v>
+        <v>44068</v>
       </c>
       <c r="D98" t="s">
         <v>581</v>
@@ -8024,31 +8020,31 @@
       </c>
       <c r="F98"/>
       <c r="G98" t="n">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="H98" t="n">
-        <v>1425351</v>
+        <v>1436206</v>
       </c>
       <c r="I98" t="n">
-        <v>32.592</v>
+        <v>32.84</v>
       </c>
       <c r="J98" t="n">
-        <v>9350</v>
+        <v>10855</v>
       </c>
       <c r="K98" t="n">
-        <v>0.214</v>
+        <v>0.248</v>
       </c>
       <c r="L98" t="n">
-        <v>17866</v>
+        <v>17257</v>
       </c>
       <c r="M98" t="n">
-        <v>0.409</v>
+        <v>0.395</v>
       </c>
       <c r="N98" t="n">
-        <v>0.097</v>
+        <v>0.102</v>
       </c>
       <c r="O98" t="n">
-        <v>10.303</v>
+        <v>9.807</v>
       </c>
       <c r="P98" t="s">
         <v>582</v>
@@ -8240,7 +8236,7 @@
         <v>603</v>
       </c>
       <c r="C102" s="1" t="n">
-        <v>44066</v>
+        <v>44067</v>
       </c>
       <c r="D102" t="s">
         <v>604</v>
@@ -8250,31 +8246,31 @@
       </c>
       <c r="F102"/>
       <c r="G102" t="n">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="H102" t="n">
-        <v>71700264</v>
+        <v>72382318</v>
       </c>
       <c r="I102" t="n">
-        <v>216.615</v>
+        <v>218.676</v>
       </c>
       <c r="J102" t="n">
-        <v>613827</v>
+        <v>682054</v>
       </c>
       <c r="K102" t="n">
-        <v>1.854</v>
+        <v>2.061</v>
       </c>
       <c r="L102" t="n">
-        <v>675323</v>
+        <v>680171</v>
       </c>
       <c r="M102" t="n">
-        <v>2.04</v>
+        <v>2.055</v>
       </c>
       <c r="N102" t="n">
-        <v>0.065</v>
+        <v>0.063</v>
       </c>
       <c r="O102" t="n">
-        <v>15.401</v>
+        <v>15.906</v>
       </c>
       <c r="P102" t="s">
         <v>605</v>

</xml_diff>

<commit_message>
Updated testing data for 2020-08-26
</commit_message>
<xml_diff>
--- a/public/data/testing/covid-testing-latest-data-source-details.xlsx
+++ b/public/data/testing/covid-testing-latest-data-source-details.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="626" uniqueCount="626">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="627" uniqueCount="627">
   <si>
     <t xml:space="preserve">ISO code</t>
   </si>
@@ -110,7 +110,7 @@
     <t xml:space="preserve">Australia - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.health.gov.au/sites/default/files/documents/2020/08/coronavirus-covid-19-at-a-glance-24-august-2020.pdf</t>
+    <t xml:space="preserve">https://www.health.gov.au/sites/default/files/documents/2020/08/coronavirus-covid-19-at-a-glance-25-august-2020.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">Australian Government Department of Health</t>
@@ -202,7 +202,7 @@
     <t xml:space="preserve">Belarus - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">http://minzdrav.gov.by/ru/sobytiya/u-belarusi-na-23-zhni-nya-vypisanyya-68-tys-839-patsyenta/</t>
+    <t xml:space="preserve">http://minzdrav.gov.by/ru/sobytiya/u-belarusi-na-25-zhni-nya-vypisanyya-69-tys-097-patsyenta/</t>
   </si>
   <si>
     <t xml:space="preserve">Belarus Ministry of Health</t>
@@ -398,7 +398,7 @@
     <t xml:space="preserve">Cote d'Ivoire - samples tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.facebook.com/Mshpci/posts/1677609049071449</t>
+    <t xml:space="preserve">https://www.facebook.com/Mshpci/posts/1678490098983344</t>
   </si>
   <si>
     <t xml:space="preserve">Ministry of Health and Public Hygiene</t>
@@ -495,7 +495,7 @@
     <t xml:space="preserve">Denmark - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://files.ssi.dk/Data-Epidemiologiske-Rapport-24082020-82ja</t>
+    <t xml:space="preserve">https://files.ssi.dk/Data-epidemiologisk-rapport-25082020-rg99</t>
   </si>
   <si>
     <t xml:space="preserve">Statens Serum Institut</t>
@@ -513,7 +513,7 @@
     <t xml:space="preserve">Ecuador - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.gestionderiesgos.gob.ec/wp-content/uploads/2020/08/INFOGRAFIA-NACIONALCOVID19-COE-NACIONAL-08h00-23082020.pdf</t>
+    <t xml:space="preserve">https://www.gestionderiesgos.gob.ec/wp-content/uploads/2020/08/INFOGRAFIA-NACIONALCOVID19-COE-NACIONAL-08h00-25082020.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">Government of Ecuador</t>
@@ -752,7 +752,7 @@
     <t xml:space="preserve">Greece - samples tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://eody.gov.gr/covid-gr-daily-report-24-08-2020/</t>
+    <t xml:space="preserve">https://eody.gov.gr/covid-gr-daily-report-25-08-2020/</t>
   </si>
   <si>
     <t xml:space="preserve">National Organization of Public Health</t>
@@ -891,7 +891,7 @@
     <t xml:space="preserve">Iran - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">http://irangov.ir/detail/345769</t>
+    <t xml:space="preserve">http://irangov.ir/detail/345900</t>
   </si>
   <si>
     <t xml:space="preserve">Government of Iran</t>
@@ -949,7 +949,7 @@
     <t xml:space="preserve">Israel - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://govextra.gov.il/media/25413/covid19-data-israel-18082020.csv</t>
+    <t xml:space="preserve">https://govextra.gov.il/media/25556/covid19-data-israel-19082020.csv</t>
   </si>
   <si>
     <t xml:space="preserve">Israel Ministry of Health</t>
@@ -1008,7 +1008,7 @@
     <t xml:space="preserve">Japan - people tested (incl. non-PCR)</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.mhlw.go.jp/stf/newpage_13139.html</t>
+    <t xml:space="preserve">https://www.mhlw.go.jp/stf/newpage_13172.html</t>
   </si>
   <si>
     <t xml:space="preserve">Ministry of Health, Labor and Welfare Press Release</t>
@@ -1155,7 +1155,7 @@
     <t xml:space="preserve">Malaysia - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">http://covid-19.moh.gov.my/terkini/082020/situasi-terkini-24-ogos-2020</t>
+    <t xml:space="preserve">http://covid-19.moh.gov.my/terkini/082020/situasi-terkini-25-ogos-2020</t>
   </si>
   <si>
     <t xml:space="preserve">Ministry of Health Malaysia</t>
@@ -1307,7 +1307,7 @@
     <t xml:space="preserve">Netherlands - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.rivm.nl/sites/default/files/2020-08/COVID-19_WebSite_rapport_wekelijks_20200818_1224_1.pdf</t>
+    <t xml:space="preserve">https://www.rivm.nl/sites/default/files/2020-08/COVID-19_WebSite_rapport_wekelijks_20200825_1217_0.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">National Institute for Public Health and the Environment</t>
@@ -1434,13 +1434,17 @@
     <t xml:space="preserve">Panama - tests performed</t>
   </si>
   <si>
+    <t xml:space="preserve">https://twitter.com/MINSAPma/status/1297671113905000448/photo/1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Panama Ministry of Health</t>
+  </si>
+  <si>
     <t xml:space="preserve">http://minsa.gob.pa/covid-19</t>
   </si>
   <si>
-    <t xml:space="preserve">Panama Ministry of Health</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The Panama Ministry of Health reports the cumulative number of tests performed ("pruebas realizadas") on [their official dashboard](http://minsa.gob.pa/covid-19) with a time series dating back to 9 March 2020. The page with testing numbers is not the first one shown but can be navigated to with the arrows at the bottom of the dashboard. The dashboard shows the cumulative number of total, positive, negative, and control tests ("prueba de control") performed. We report here the total of positive and negative numbers because: 1) the time series only includes positive and negative test numbers; and 2) the total they provide seems to include control tests, which we understand to be used for testing quality control.</t>
+    <t xml:space="preserve">The Panama Ministry of Health reports the cumulative number of tests performed ("pruebas realizadas") on [their official dashboard](http://minsa.gob.pa/covid-19) with a time series dating back to 9 March 2020. The page with testing numbers is not the first one shown but can be navigated to with the arrows at the bottom of the dashboard. The dashboard shows the cumulative number of total, positive ("positivas"), negative ("negativas"), and control tests ("prueba de control") performed. We report here the total of positive and negative numbers because: 1) the time series only includes positive and negative test numbers; and 2) the total they provide seems to include control tests, which we understand to be used for testing quality control.
+Starting 15 August 2020, the official dashboard is no longer being updated while it is being restructured. We now source the daily testing numbers from the [Ministry of Health's official Twitter page](https://twitter.com/MINSAPma). We continue to report the total of positive ("casos confirmados") and negative ("pruebas negativas") tests.</t>
   </si>
   <si>
     <t xml:space="preserve">PRY</t>
@@ -1510,7 +1514,7 @@
     <t xml:space="preserve">Poland - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/MZ_GOV_PL/status/1297820944896077824</t>
+    <t xml:space="preserve">https://twitter.com/MZ_GOV_PL/status/1298183333340483584</t>
   </si>
   <si>
     <t xml:space="preserve">Poland Ministry of Health</t>
@@ -1601,7 +1605,7 @@
     <t xml:space="preserve">Russia - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://rospotrebnadzor.ru/about/info/news/news_details.php?ELEMENT_ID=15234</t>
+    <t xml:space="preserve">https://rospotrebnadzor.ru/about/info/news/news_details.php?ELEMENT_ID=15238</t>
   </si>
   <si>
     <t xml:space="preserve">Government of the Russian Federation</t>
@@ -1795,7 +1799,7 @@
     <t xml:space="preserve">South Korea - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.cdc.go.kr/board/board.es?mid=&amp;bid=0030&amp;act=view&amp;list_no=368210&amp;tag=&amp;nPage=1</t>
+    <t xml:space="preserve">https://www.cdc.go.kr/board/board.es?mid=&amp;bid=0030&amp;act=view&amp;list_no=368215&amp;tag=&amp;nPage=1</t>
   </si>
   <si>
     <t xml:space="preserve">South Korea CDC</t>
@@ -1917,7 +1921,7 @@
     <t xml:space="preserve">Thailand - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://ddc.moph.go.th/viralpneumonia/file/situation/situation-no234-240863.pdf</t>
+    <t xml:space="preserve">https://ddc.moph.go.th/viralpneumonia/file/situation/situation-no235-250863.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">Department of Disease Control</t>
@@ -2005,7 +2009,7 @@
     <t xml:space="preserve">Uganda - samples tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/MinofHealthUG/status/1297887233287114753/photo/1</t>
+    <t xml:space="preserve">https://twitter.com/MinofHealthUG/status/1298238895956664320/photo/1</t>
   </si>
   <si>
     <t xml:space="preserve">Uganda Ministry of Health</t>
@@ -2145,7 +2149,7 @@
     <t xml:space="preserve">Uruguay - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.gub.uy/ministerio-salud-publica/comunicacion/noticias/informe-situacion-sobre-coronavirus-covid-19-uruguay-23-agosto</t>
+    <t xml:space="preserve">https://www.gub.uy/ministerio-salud-publica/comunicacion/noticias/informe-situacion-sobre-coronavirus-covid-19-uruguay-25-agosto</t>
   </si>
   <si>
     <t xml:space="preserve">https://www.gub.uy/ministerio-salud-publica/comunicacion/noticias</t>
@@ -2657,7 +2661,7 @@
         <v>25</v>
       </c>
       <c r="C3" s="1" t="n">
-        <v>44067</v>
+        <v>44068</v>
       </c>
       <c r="D3" t="s">
         <v>26</v>
@@ -2667,31 +2671,31 @@
       </c>
       <c r="F3"/>
       <c r="G3" t="n">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="H3" t="n">
-        <v>1172592</v>
+        <v>1195148</v>
       </c>
       <c r="I3" t="n">
-        <v>25.945</v>
+        <v>26.444</v>
       </c>
       <c r="J3" t="n">
-        <v>4977</v>
+        <v>6132</v>
       </c>
       <c r="K3" t="n">
-        <v>0.11</v>
+        <v>0.136</v>
       </c>
       <c r="L3" t="n">
-        <v>14451</v>
+        <v>14762</v>
       </c>
       <c r="M3" t="n">
-        <v>0.32</v>
+        <v>0.327</v>
       </c>
       <c r="N3" t="n">
-        <v>0.472</v>
+        <v>0.545</v>
       </c>
       <c r="O3" t="n">
-        <v>2.121</v>
+        <v>1.835</v>
       </c>
       <c r="P3" t="s">
         <v>22</v>
@@ -2714,7 +2718,7 @@
         <v>30</v>
       </c>
       <c r="C4" s="1" t="n">
-        <v>44067</v>
+        <v>44068</v>
       </c>
       <c r="D4" t="s">
         <v>31</v>
@@ -2724,31 +2728,31 @@
       </c>
       <c r="F4"/>
       <c r="G4" t="n">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="H4" t="n">
-        <v>5758034</v>
+        <v>5814709</v>
       </c>
       <c r="I4" t="n">
-        <v>225.806</v>
+        <v>228.029</v>
       </c>
       <c r="J4" t="n">
-        <v>51447</v>
+        <v>56675</v>
       </c>
       <c r="K4" t="n">
-        <v>2.018</v>
+        <v>2.223</v>
       </c>
       <c r="L4" t="n">
-        <v>60277</v>
+        <v>62014</v>
       </c>
       <c r="M4" t="n">
-        <v>2.364</v>
+        <v>2.432</v>
       </c>
       <c r="N4" t="n">
-        <v>0.004</v>
+        <v>0.003</v>
       </c>
       <c r="O4" t="n">
-        <v>276.863</v>
+        <v>329.611</v>
       </c>
       <c r="P4" t="s">
         <v>32</v>
@@ -2828,7 +2832,7 @@
         <v>43</v>
       </c>
       <c r="C6" s="1" t="n">
-        <v>44068</v>
+        <v>44069</v>
       </c>
       <c r="D6" t="s">
         <v>44</v>
@@ -2838,32 +2842,28 @@
       </c>
       <c r="F6"/>
       <c r="G6" t="n">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="H6" t="n">
-        <v>1048935</v>
+        <v>1058509</v>
       </c>
       <c r="I6" t="n">
-        <v>616.447</v>
+        <v>622.073</v>
       </c>
       <c r="J6" t="n">
-        <v>9364</v>
+        <v>9574</v>
       </c>
       <c r="K6" t="n">
-        <v>5.503</v>
+        <v>5.627</v>
       </c>
       <c r="L6" t="n">
-        <v>9675</v>
+        <v>8246</v>
       </c>
       <c r="M6" t="n">
-        <v>5.686</v>
-      </c>
-      <c r="N6" t="n">
-        <v>0.032</v>
-      </c>
-      <c r="O6" t="n">
-        <v>31.573</v>
-      </c>
+        <v>4.846</v>
+      </c>
+      <c r="N6"/>
+      <c r="O6"/>
       <c r="P6" t="s">
         <v>46</v>
       </c>
@@ -2942,7 +2942,7 @@
         <v>57</v>
       </c>
       <c r="C8" s="1" t="n">
-        <v>44066</v>
+        <v>44068</v>
       </c>
       <c r="D8" t="s">
         <v>58</v>
@@ -2952,31 +2952,27 @@
       </c>
       <c r="F8"/>
       <c r="G8" t="n">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="H8" t="n">
-        <v>1474075</v>
+        <v>1480047</v>
       </c>
       <c r="I8" t="n">
-        <v>155.998</v>
-      </c>
-      <c r="J8" t="n">
-        <v>8520</v>
-      </c>
-      <c r="K8" t="n">
-        <v>0.902</v>
-      </c>
+        <v>156.63</v>
+      </c>
+      <c r="J8"/>
+      <c r="K8"/>
       <c r="L8" t="n">
-        <v>8205</v>
+        <v>6729</v>
       </c>
       <c r="M8" t="n">
-        <v>0.868</v>
+        <v>0.712</v>
       </c>
       <c r="N8" t="n">
-        <v>0.015</v>
+        <v>0.022</v>
       </c>
       <c r="O8" t="n">
-        <v>66.707</v>
+        <v>44.605</v>
       </c>
       <c r="P8" t="s">
         <v>59</v>
@@ -2999,7 +2995,7 @@
         <v>63</v>
       </c>
       <c r="C9" s="1" t="n">
-        <v>44066</v>
+        <v>44067</v>
       </c>
       <c r="D9" t="s">
         <v>64</v>
@@ -3009,31 +3005,31 @@
       </c>
       <c r="F9"/>
       <c r="G9" t="n">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="H9" t="n">
-        <v>2144401</v>
+        <v>2162146</v>
       </c>
       <c r="I9" t="n">
-        <v>185.028</v>
+        <v>186.559</v>
       </c>
       <c r="J9" t="n">
-        <v>7221</v>
+        <v>14342</v>
       </c>
       <c r="K9" t="n">
-        <v>0.623</v>
+        <v>1.237</v>
       </c>
       <c r="L9" t="n">
-        <v>19071</v>
+        <v>19016</v>
       </c>
       <c r="M9" t="n">
-        <v>1.646</v>
+        <v>1.641</v>
       </c>
       <c r="N9" t="n">
-        <v>0.025</v>
+        <v>0.024</v>
       </c>
       <c r="O9" t="n">
-        <v>40.688</v>
+        <v>41.925</v>
       </c>
       <c r="P9" t="s">
         <v>65</v>
@@ -3164,7 +3160,7 @@
         <v>81</v>
       </c>
       <c r="C12" s="1" t="n">
-        <v>44068</v>
+        <v>44069</v>
       </c>
       <c r="D12" t="s">
         <v>82</v>
@@ -3174,32 +3170,28 @@
       </c>
       <c r="F12"/>
       <c r="G12" t="n">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="H12" t="n">
-        <v>374374</v>
+        <v>380606</v>
       </c>
       <c r="I12" t="n">
-        <v>53.879</v>
+        <v>54.776</v>
       </c>
       <c r="J12" t="n">
-        <v>3588</v>
+        <v>6232</v>
       </c>
       <c r="K12" t="n">
-        <v>0.516</v>
+        <v>0.897</v>
       </c>
       <c r="L12" t="n">
-        <v>4973</v>
+        <v>5339</v>
       </c>
       <c r="M12" t="n">
-        <v>0.716</v>
-      </c>
-      <c r="N12" t="n">
-        <v>0.023</v>
-      </c>
-      <c r="O12" t="n">
-        <v>44.233</v>
-      </c>
+        <v>0.768</v>
+      </c>
+      <c r="N12"/>
+      <c r="O12"/>
       <c r="P12" t="s">
         <v>84</v>
       </c>
@@ -3221,7 +3213,7 @@
         <v>87</v>
       </c>
       <c r="C13" s="1" t="n">
-        <v>44068</v>
+        <v>44069</v>
       </c>
       <c r="D13" t="s">
         <v>88</v>
@@ -3231,32 +3223,28 @@
       </c>
       <c r="F13"/>
       <c r="G13" t="n">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="H13" t="n">
-        <v>5169166</v>
+        <v>5205010</v>
       </c>
       <c r="I13" t="n">
-        <v>136.96</v>
+        <v>137.91</v>
       </c>
       <c r="J13" t="n">
-        <v>53676</v>
+        <v>35844</v>
       </c>
       <c r="K13" t="n">
-        <v>1.422</v>
+        <v>0.95</v>
       </c>
       <c r="L13" t="n">
-        <v>47018</v>
+        <v>46405</v>
       </c>
       <c r="M13" t="n">
-        <v>1.246</v>
-      </c>
-      <c r="N13" t="n">
-        <v>0.008</v>
-      </c>
-      <c r="O13" t="n">
-        <v>118.604</v>
-      </c>
+        <v>1.23</v>
+      </c>
+      <c r="N13"/>
+      <c r="O13"/>
       <c r="P13" t="s">
         <v>89</v>
       </c>
@@ -3278,7 +3266,7 @@
         <v>92</v>
       </c>
       <c r="C14" s="1" t="n">
-        <v>44067</v>
+        <v>44068</v>
       </c>
       <c r="D14" t="s">
         <v>93</v>
@@ -3290,31 +3278,31 @@
         <v>94</v>
       </c>
       <c r="G14" t="n">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="H14" t="n">
-        <v>2231463</v>
+        <v>2255966</v>
       </c>
       <c r="I14" t="n">
-        <v>116.731</v>
+        <v>118.013</v>
       </c>
       <c r="J14" t="n">
-        <v>27454</v>
+        <v>24503</v>
       </c>
       <c r="K14" t="n">
-        <v>1.436</v>
+        <v>1.282</v>
       </c>
       <c r="L14" t="n">
-        <v>26655</v>
+        <v>26841</v>
       </c>
       <c r="M14" t="n">
-        <v>1.394</v>
+        <v>1.404</v>
       </c>
       <c r="N14" t="n">
-        <v>0.063</v>
+        <v>0.064</v>
       </c>
       <c r="O14" t="n">
-        <v>15.922</v>
+        <v>15.572</v>
       </c>
       <c r="P14" t="s">
         <v>95</v>
@@ -3337,7 +3325,7 @@
         <v>99</v>
       </c>
       <c r="C15" s="1" t="n">
-        <v>44067</v>
+        <v>44068</v>
       </c>
       <c r="D15" t="s">
         <v>100</v>
@@ -3347,31 +3335,31 @@
       </c>
       <c r="F15"/>
       <c r="G15" t="n">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="H15" t="n">
-        <v>2427941</v>
+        <v>2458866</v>
       </c>
       <c r="I15" t="n">
-        <v>47.716</v>
+        <v>48.324</v>
       </c>
       <c r="J15" t="n">
-        <v>31049</v>
+        <v>30925</v>
       </c>
       <c r="K15" t="n">
-        <v>0.61</v>
+        <v>0.608</v>
       </c>
       <c r="L15" t="n">
-        <v>31033</v>
+        <v>30324</v>
       </c>
       <c r="M15" t="n">
-        <v>0.61</v>
+        <v>0.596</v>
       </c>
       <c r="N15" t="n">
-        <v>0.335</v>
+        <v>0.353</v>
       </c>
       <c r="O15" t="n">
-        <v>2.983</v>
+        <v>2.829</v>
       </c>
       <c r="P15" t="s">
         <v>101</v>
@@ -3394,7 +3382,7 @@
         <v>105</v>
       </c>
       <c r="C16" s="1" t="n">
-        <v>44065</v>
+        <v>44067</v>
       </c>
       <c r="D16" t="s">
         <v>106</v>
@@ -3404,25 +3392,25 @@
       </c>
       <c r="F16"/>
       <c r="G16" t="n">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="H16" t="n">
-        <v>114371</v>
+        <v>117997</v>
       </c>
       <c r="I16" t="n">
-        <v>22.452</v>
+        <v>23.163</v>
       </c>
       <c r="J16" t="n">
-        <v>2131</v>
+        <v>1533</v>
       </c>
       <c r="K16" t="n">
-        <v>0.418</v>
+        <v>0.301</v>
       </c>
       <c r="L16" t="n">
-        <v>1648</v>
+        <v>1626</v>
       </c>
       <c r="M16" t="n">
-        <v>0.324</v>
+        <v>0.319</v>
       </c>
       <c r="N16"/>
       <c r="O16"/>
@@ -3447,7 +3435,7 @@
         <v>111</v>
       </c>
       <c r="C17" s="1" t="n">
-        <v>44066</v>
+        <v>44067</v>
       </c>
       <c r="D17" t="s">
         <v>112</v>
@@ -3457,31 +3445,31 @@
       </c>
       <c r="F17"/>
       <c r="G17" t="n">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="H17" t="n">
-        <v>120299</v>
+        <v>121286</v>
       </c>
       <c r="I17" t="n">
-        <v>4.561</v>
+        <v>4.598</v>
       </c>
       <c r="J17" t="n">
-        <v>1133</v>
+        <v>987</v>
       </c>
       <c r="K17" t="n">
-        <v>0.043</v>
+        <v>0.037</v>
       </c>
       <c r="L17" t="n">
-        <v>987</v>
+        <v>981</v>
       </c>
       <c r="M17" t="n">
         <v>0.037</v>
       </c>
       <c r="N17" t="n">
-        <v>0.055</v>
+        <v>0.065</v>
       </c>
       <c r="O17" t="n">
-        <v>18.134</v>
+        <v>15.431</v>
       </c>
       <c r="P17" t="s">
         <v>113</v>
@@ -3504,7 +3492,7 @@
         <v>117</v>
       </c>
       <c r="C18" s="1" t="n">
-        <v>44067</v>
+        <v>44068</v>
       </c>
       <c r="D18" t="s">
         <v>118</v>
@@ -3514,31 +3502,31 @@
       </c>
       <c r="F18"/>
       <c r="G18" t="n">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="H18" t="n">
-        <v>152824</v>
+        <v>154159</v>
       </c>
       <c r="I18" t="n">
-        <v>37.226</v>
+        <v>37.552</v>
       </c>
       <c r="J18" t="n">
-        <v>2364</v>
+        <v>1335</v>
       </c>
       <c r="K18" t="n">
-        <v>0.576</v>
+        <v>0.325</v>
       </c>
       <c r="L18" t="n">
-        <v>2025</v>
+        <v>1955</v>
       </c>
       <c r="M18" t="n">
-        <v>0.493</v>
+        <v>0.476</v>
       </c>
       <c r="N18" t="n">
-        <v>0.113</v>
+        <v>0.121</v>
       </c>
       <c r="O18" t="n">
-        <v>8.837</v>
+        <v>8.269</v>
       </c>
       <c r="P18" t="s">
         <v>119</v>
@@ -3561,7 +3549,7 @@
         <v>123</v>
       </c>
       <c r="C19" s="1" t="n">
-        <v>44066</v>
+        <v>44067</v>
       </c>
       <c r="D19" t="s">
         <v>124</v>
@@ -3573,31 +3561,31 @@
         <v>126</v>
       </c>
       <c r="G19" t="n">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="H19" t="n">
-        <v>365353</v>
+        <v>369889</v>
       </c>
       <c r="I19" t="n">
-        <v>32.256</v>
+        <v>32.657</v>
       </c>
       <c r="J19" t="n">
-        <v>4261</v>
+        <v>4536</v>
       </c>
       <c r="K19" t="n">
-        <v>0.376</v>
+        <v>0.4</v>
       </c>
       <c r="L19" t="n">
-        <v>4759</v>
+        <v>4794</v>
       </c>
       <c r="M19" t="n">
-        <v>0.42</v>
+        <v>0.423</v>
       </c>
       <c r="N19" t="n">
-        <v>0.01</v>
+        <v>0.011</v>
       </c>
       <c r="O19" t="n">
-        <v>102.502</v>
+        <v>91.689</v>
       </c>
       <c r="P19" t="s">
         <v>125</v>
@@ -3620,7 +3608,7 @@
         <v>130</v>
       </c>
       <c r="C20" s="1" t="n">
-        <v>44065</v>
+        <v>44067</v>
       </c>
       <c r="D20" t="s">
         <v>131</v>
@@ -3630,31 +3618,31 @@
       </c>
       <c r="F20"/>
       <c r="G20" t="n">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="H20" t="n">
-        <v>843326</v>
+        <v>852414</v>
       </c>
       <c r="I20" t="n">
-        <v>78.749</v>
+        <v>79.598</v>
       </c>
       <c r="J20" t="n">
-        <v>4767</v>
+        <v>6835</v>
       </c>
       <c r="K20" t="n">
-        <v>0.445</v>
+        <v>0.638</v>
       </c>
       <c r="L20" t="n">
-        <v>6691</v>
+        <v>6600</v>
       </c>
       <c r="M20" t="n">
-        <v>0.625</v>
+        <v>0.616</v>
       </c>
       <c r="N20" t="n">
-        <v>0.04</v>
+        <v>0.041</v>
       </c>
       <c r="O20" t="n">
-        <v>25.208</v>
+        <v>24.176</v>
       </c>
       <c r="P20" t="s">
         <v>45</v>
@@ -3730,7 +3718,7 @@
         <v>141</v>
       </c>
       <c r="C22" s="1" t="n">
-        <v>44066</v>
+        <v>44067</v>
       </c>
       <c r="D22" t="s">
         <v>142</v>
@@ -3740,31 +3728,31 @@
       </c>
       <c r="F22"/>
       <c r="G22" t="n">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="H22" t="n">
-        <v>2169579</v>
+        <v>2201733</v>
       </c>
       <c r="I22" t="n">
-        <v>374.569</v>
+        <v>380.12</v>
       </c>
       <c r="J22" t="n">
-        <v>6037</v>
+        <v>7862</v>
       </c>
       <c r="K22" t="n">
-        <v>1.042</v>
+        <v>1.357</v>
       </c>
       <c r="L22" t="n">
-        <v>30410</v>
+        <v>29920</v>
       </c>
       <c r="M22" t="n">
-        <v>5.25</v>
+        <v>5.166</v>
       </c>
       <c r="N22" t="n">
-        <v>0.003</v>
+        <v>0.002</v>
       </c>
       <c r="O22" t="n">
-        <v>330.543</v>
+        <v>410.667</v>
       </c>
       <c r="P22" t="s">
         <v>143</v>
@@ -3787,7 +3775,7 @@
         <v>147</v>
       </c>
       <c r="C23" s="1" t="n">
-        <v>44066</v>
+        <v>44068</v>
       </c>
       <c r="D23" t="s">
         <v>148</v>
@@ -3799,25 +3787,25 @@
         <v>150</v>
       </c>
       <c r="G23" t="n">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="H23" t="n">
-        <v>242114</v>
+        <v>245983</v>
       </c>
       <c r="I23" t="n">
-        <v>13.723</v>
+        <v>13.942</v>
       </c>
       <c r="J23" t="n">
-        <v>2348</v>
+        <v>2546</v>
       </c>
       <c r="K23" t="n">
-        <v>0.133</v>
+        <v>0.144</v>
       </c>
       <c r="L23" t="n">
-        <v>2610</v>
+        <v>2564</v>
       </c>
       <c r="M23" t="n">
-        <v>0.148</v>
+        <v>0.145</v>
       </c>
       <c r="N23"/>
       <c r="O23"/>
@@ -4013,7 +4001,7 @@
         <v>174</v>
       </c>
       <c r="C27" s="1" t="n">
-        <v>44059</v>
+        <v>44066</v>
       </c>
       <c r="D27" t="s">
         <v>175</v>
@@ -4023,30 +4011,32 @@
       </c>
       <c r="F27"/>
       <c r="G27" t="n">
-        <v>150</v>
+        <v>157</v>
       </c>
       <c r="H27" t="n">
-        <v>7623</v>
+        <v>7979</v>
       </c>
       <c r="I27" t="n">
-        <v>8.504</v>
+        <v>8.901</v>
       </c>
       <c r="J27" t="n">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="K27" t="n">
-        <v>0.019</v>
+        <v>0.02</v>
       </c>
       <c r="L27" t="n">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="M27" t="n">
-        <v>0.045</v>
+        <v>0.057</v>
       </c>
       <c r="N27" t="n">
-        <v>0</v>
-      </c>
-      <c r="O27"/>
+        <v>0.003</v>
+      </c>
+      <c r="O27" t="n">
+        <v>357</v>
+      </c>
       <c r="P27" t="s">
         <v>176</v>
       </c>
@@ -4140,22 +4130,22 @@
       <c r="H29"/>
       <c r="I29"/>
       <c r="J29" t="n">
-        <v>112150</v>
+        <v>127561</v>
       </c>
       <c r="K29" t="n">
-        <v>1.718</v>
+        <v>1.954</v>
       </c>
       <c r="L29" t="n">
-        <v>93324</v>
+        <v>97097</v>
       </c>
       <c r="M29" t="n">
-        <v>1.43</v>
+        <v>1.488</v>
       </c>
       <c r="N29" t="n">
-        <v>0.031</v>
+        <v>0.03</v>
       </c>
       <c r="O29" t="n">
-        <v>31.946</v>
+        <v>33.238</v>
       </c>
       <c r="P29" t="s">
         <v>187</v>
@@ -4345,7 +4335,7 @@
         <v>210</v>
       </c>
       <c r="C33" s="1" t="n">
-        <v>44067</v>
+        <v>44068</v>
       </c>
       <c r="D33" t="s">
         <v>211</v>
@@ -4355,31 +4345,31 @@
       </c>
       <c r="F33"/>
       <c r="G33" t="n">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="H33" t="n">
-        <v>858138</v>
+        <v>872550</v>
       </c>
       <c r="I33" t="n">
-        <v>82.331</v>
+        <v>83.713</v>
       </c>
       <c r="J33" t="n">
-        <v>9758</v>
+        <v>14412</v>
       </c>
       <c r="K33" t="n">
-        <v>0.936</v>
+        <v>1.383</v>
       </c>
       <c r="L33" t="n">
-        <v>18740</v>
+        <v>18811</v>
       </c>
       <c r="M33" t="n">
-        <v>1.798</v>
+        <v>1.805</v>
       </c>
       <c r="N33" t="n">
         <v>0.012</v>
       </c>
       <c r="O33" t="n">
-        <v>82.555</v>
+        <v>82.453</v>
       </c>
       <c r="P33" t="s">
         <v>213</v>
@@ -4734,7 +4724,7 @@
         <v>250</v>
       </c>
       <c r="C40" s="1" t="n">
-        <v>44067</v>
+        <v>44068</v>
       </c>
       <c r="D40" t="s">
         <v>251</v>
@@ -4744,31 +4734,31 @@
       </c>
       <c r="F40"/>
       <c r="G40" t="n">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="H40" t="n">
-        <v>3062422</v>
+        <v>3088313</v>
       </c>
       <c r="I40" t="n">
-        <v>36.46</v>
+        <v>36.769</v>
       </c>
       <c r="J40" t="n">
-        <v>25711</v>
+        <v>25891</v>
       </c>
       <c r="K40" t="n">
-        <v>0.306</v>
+        <v>0.308</v>
       </c>
       <c r="L40" t="n">
-        <v>24926</v>
+        <v>24895</v>
       </c>
       <c r="M40" t="n">
-        <v>0.297</v>
+        <v>0.296</v>
       </c>
       <c r="N40" t="n">
-        <v>0.09</v>
+        <v>0.077</v>
       </c>
       <c r="O40" t="n">
-        <v>11.112</v>
+        <v>12.952</v>
       </c>
       <c r="P40" t="s">
         <v>252</v>
@@ -4848,7 +4838,7 @@
         <v>263</v>
       </c>
       <c r="C42" s="1" t="n">
-        <v>44067</v>
+        <v>44068</v>
       </c>
       <c r="D42" t="s">
         <v>264</v>
@@ -4858,31 +4848,31 @@
       </c>
       <c r="F42"/>
       <c r="G42" t="n">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="H42" t="n">
-        <v>777635</v>
+        <v>782633</v>
       </c>
       <c r="I42" t="n">
-        <v>157.486</v>
+        <v>158.498</v>
       </c>
       <c r="J42" t="n">
-        <v>4838</v>
+        <v>4998</v>
       </c>
       <c r="K42" t="n">
-        <v>0.98</v>
+        <v>1.012</v>
       </c>
       <c r="L42" t="n">
-        <v>7437</v>
+        <v>7531</v>
       </c>
       <c r="M42" t="n">
-        <v>1.506</v>
+        <v>1.525</v>
       </c>
       <c r="N42" t="n">
-        <v>0.014</v>
+        <v>0.015</v>
       </c>
       <c r="O42" t="n">
-        <v>73.117</v>
+        <v>65.65</v>
       </c>
       <c r="P42" t="s">
         <v>265</v>
@@ -4905,7 +4895,7 @@
         <v>268</v>
       </c>
       <c r="C43" s="1" t="n">
-        <v>44061</v>
+        <v>44062</v>
       </c>
       <c r="D43" t="s">
         <v>269</v>
@@ -4915,31 +4905,31 @@
       </c>
       <c r="F43"/>
       <c r="G43" t="n">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="H43" t="n">
-        <v>2146693</v>
+        <v>2175060</v>
       </c>
       <c r="I43" t="n">
-        <v>248.014</v>
+        <v>251.291</v>
       </c>
       <c r="J43" t="n">
-        <v>27920</v>
+        <v>28401</v>
       </c>
       <c r="K43" t="n">
-        <v>3.226</v>
+        <v>3.281</v>
       </c>
       <c r="L43" t="n">
-        <v>21688</v>
+        <v>21993</v>
       </c>
       <c r="M43" t="n">
-        <v>2.506</v>
+        <v>2.541</v>
       </c>
       <c r="N43" t="n">
-        <v>0.065</v>
+        <v>0.061</v>
       </c>
       <c r="O43" t="n">
-        <v>15.324</v>
+        <v>16.291</v>
       </c>
       <c r="P43" t="s">
         <v>45</v>
@@ -4962,7 +4952,7 @@
         <v>274</v>
       </c>
       <c r="C44" s="1" t="n">
-        <v>44067</v>
+        <v>44068</v>
       </c>
       <c r="D44" t="s">
         <v>275</v>
@@ -4974,31 +4964,31 @@
         <v>277</v>
       </c>
       <c r="G44" t="n">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="H44" t="n">
-        <v>4773326</v>
+        <v>4819124</v>
       </c>
       <c r="I44" t="n">
-        <v>78.948</v>
+        <v>79.705</v>
       </c>
       <c r="J44" t="n">
-        <v>33358</v>
+        <v>45798</v>
       </c>
       <c r="K44" t="n">
-        <v>0.552</v>
+        <v>0.757</v>
       </c>
       <c r="L44" t="n">
-        <v>42288</v>
+        <v>44161</v>
       </c>
       <c r="M44" t="n">
-        <v>0.699</v>
+        <v>0.73</v>
       </c>
       <c r="N44" t="n">
-        <v>0.018</v>
+        <v>0.02</v>
       </c>
       <c r="O44" t="n">
-        <v>54.515</v>
+        <v>50.986</v>
       </c>
       <c r="P44" t="s">
         <v>278</v>
@@ -5021,7 +5011,7 @@
         <v>281</v>
       </c>
       <c r="C45" s="1" t="n">
-        <v>44067</v>
+        <v>44068</v>
       </c>
       <c r="D45" t="s">
         <v>275</v>
@@ -5033,31 +5023,31 @@
         <v>277</v>
       </c>
       <c r="G45" t="n">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="H45" t="n">
-        <v>8053551</v>
+        <v>8125892</v>
       </c>
       <c r="I45" t="n">
-        <v>133.201</v>
+        <v>134.397</v>
       </c>
       <c r="J45" t="n">
-        <v>45914</v>
+        <v>72341</v>
       </c>
       <c r="K45" t="n">
-        <v>0.759</v>
+        <v>1.196</v>
       </c>
       <c r="L45" t="n">
-        <v>66495</v>
+        <v>69119</v>
       </c>
       <c r="M45" t="n">
-        <v>1.1</v>
+        <v>1.143</v>
       </c>
       <c r="N45" t="n">
-        <v>0.012</v>
+        <v>0.013</v>
       </c>
       <c r="O45" t="n">
-        <v>85.721</v>
+        <v>79.801</v>
       </c>
       <c r="P45" t="s">
         <v>278</v>
@@ -5080,7 +5070,7 @@
         <v>284</v>
       </c>
       <c r="C46" s="1" t="n">
-        <v>44067</v>
+        <v>44068</v>
       </c>
       <c r="D46" t="s">
         <v>285</v>
@@ -5092,31 +5082,31 @@
         <v>287</v>
       </c>
       <c r="G46" t="n">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="H46" t="n">
-        <v>1333884</v>
+        <v>1357628</v>
       </c>
       <c r="I46" t="n">
-        <v>10.547</v>
+        <v>10.734</v>
       </c>
       <c r="J46" t="n">
-        <v>12805</v>
+        <v>23744</v>
       </c>
       <c r="K46" t="n">
-        <v>0.101</v>
+        <v>0.188</v>
       </c>
       <c r="L46" t="n">
-        <v>21059</v>
+        <v>20498</v>
       </c>
       <c r="M46" t="n">
-        <v>0.167</v>
+        <v>0.162</v>
       </c>
       <c r="N46" t="n">
-        <v>0.046</v>
+        <v>0.05</v>
       </c>
       <c r="O46" t="n">
-        <v>21.672</v>
+        <v>20.032</v>
       </c>
       <c r="P46" t="s">
         <v>288</v>
@@ -5154,28 +5144,28 @@
         <v>45</v>
       </c>
       <c r="H47" t="n">
-        <v>1619407</v>
+        <v>1661966</v>
       </c>
       <c r="I47" t="n">
-        <v>12.804</v>
+        <v>13.141</v>
       </c>
       <c r="J47" t="n">
-        <v>4988</v>
+        <v>20461</v>
       </c>
       <c r="K47" t="n">
-        <v>0.039</v>
+        <v>0.162</v>
       </c>
       <c r="L47" t="n">
-        <v>16798</v>
+        <v>22585</v>
       </c>
       <c r="M47" t="n">
-        <v>0.133</v>
+        <v>0.179</v>
       </c>
       <c r="N47" t="n">
-        <v>0.061</v>
+        <v>0.045</v>
       </c>
       <c r="O47" t="n">
-        <v>16.432</v>
+        <v>22.093</v>
       </c>
       <c r="P47" t="s">
         <v>288</v>
@@ -5369,7 +5359,7 @@
         <v>313</v>
       </c>
       <c r="C51" s="1" t="n">
-        <v>44068</v>
+        <v>44069</v>
       </c>
       <c r="D51" t="s">
         <v>314</v>
@@ -5381,32 +5371,28 @@
         <v>316</v>
       </c>
       <c r="G51" t="n">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="H51" t="n">
-        <v>240533</v>
+        <v>242823</v>
       </c>
       <c r="I51" t="n">
-        <v>127.522</v>
+        <v>128.736</v>
       </c>
       <c r="J51" t="n">
-        <v>2130</v>
+        <v>2290</v>
       </c>
       <c r="K51" t="n">
-        <v>1.129</v>
+        <v>1.214</v>
       </c>
       <c r="L51" t="n">
-        <v>1682</v>
+        <v>1700</v>
       </c>
       <c r="M51" t="n">
-        <v>0.892</v>
-      </c>
-      <c r="N51" t="n">
-        <v>0.001</v>
-      </c>
-      <c r="O51" t="n">
-        <v>841</v>
-      </c>
+        <v>0.901</v>
+      </c>
+      <c r="N51"/>
+      <c r="O51"/>
       <c r="P51" t="s">
         <v>315</v>
       </c>
@@ -5485,7 +5471,7 @@
         <v>323</v>
       </c>
       <c r="C53" s="1" t="n">
-        <v>44065</v>
+        <v>44067</v>
       </c>
       <c r="D53" t="s">
         <v>324</v>
@@ -5495,31 +5481,31 @@
       </c>
       <c r="F53"/>
       <c r="G53" t="n">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="H53" t="n">
-        <v>472865</v>
+        <v>474282</v>
       </c>
       <c r="I53" t="n">
-        <v>755.404</v>
+        <v>757.668</v>
       </c>
       <c r="J53" t="n">
-        <v>1778</v>
+        <v>1025</v>
       </c>
       <c r="K53" t="n">
-        <v>2.84</v>
+        <v>1.637</v>
       </c>
       <c r="L53" t="n">
-        <v>1756</v>
+        <v>1725</v>
       </c>
       <c r="M53" t="n">
-        <v>2.805</v>
+        <v>2.756</v>
       </c>
       <c r="N53" t="n">
-        <v>0.024</v>
+        <v>0.022</v>
       </c>
       <c r="O53" t="n">
-        <v>41.11</v>
+        <v>45.566</v>
       </c>
       <c r="P53" t="s">
         <v>325</v>
@@ -5542,7 +5528,7 @@
         <v>328</v>
       </c>
       <c r="C54" s="1" t="n">
-        <v>44067</v>
+        <v>44068</v>
       </c>
       <c r="D54" t="s">
         <v>329</v>
@@ -5554,31 +5540,31 @@
         <v>331</v>
       </c>
       <c r="G54" t="n">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="H54" t="n">
-        <v>1182845</v>
+        <v>1191500</v>
       </c>
       <c r="I54" t="n">
-        <v>36.546</v>
+        <v>36.813</v>
       </c>
       <c r="J54" t="n">
-        <v>6429</v>
+        <v>8655</v>
       </c>
       <c r="K54" t="n">
-        <v>0.199</v>
+        <v>0.267</v>
       </c>
       <c r="L54" t="n">
-        <v>8883</v>
+        <v>8916</v>
       </c>
       <c r="M54" t="n">
-        <v>0.274</v>
+        <v>0.275</v>
       </c>
       <c r="N54" t="n">
         <v>0.001</v>
       </c>
       <c r="O54" t="n">
-        <v>928.075</v>
+        <v>1006.645</v>
       </c>
       <c r="P54" t="s">
         <v>45</v>
@@ -5728,28 +5714,28 @@
         <v>234</v>
       </c>
       <c r="H57" t="n">
-        <v>1185178</v>
+        <v>1193262</v>
       </c>
       <c r="I57" t="n">
-        <v>9.192</v>
+        <v>9.255</v>
       </c>
       <c r="J57" t="n">
-        <v>5041</v>
+        <v>6833</v>
       </c>
       <c r="K57" t="n">
-        <v>0.039</v>
+        <v>0.053</v>
       </c>
       <c r="L57" t="n">
-        <v>8084</v>
+        <v>9035</v>
       </c>
       <c r="M57" t="n">
-        <v>0.063</v>
+        <v>0.07</v>
       </c>
       <c r="N57" t="n">
-        <v>0.672</v>
+        <v>0.602</v>
       </c>
       <c r="O57" t="n">
-        <v>1.487</v>
+        <v>1.662</v>
       </c>
       <c r="P57" t="s">
         <v>351</v>
@@ -5943,7 +5929,7 @@
         <v>373</v>
       </c>
       <c r="C61" s="1" t="n">
-        <v>44059</v>
+        <v>44066</v>
       </c>
       <c r="D61" t="s">
         <v>374</v>
@@ -5953,27 +5939,27 @@
       </c>
       <c r="F61"/>
       <c r="G61" t="n">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H61" t="n">
-        <v>1312787</v>
+        <v>1464715</v>
       </c>
       <c r="I61" t="n">
-        <v>76.615</v>
+        <v>85.482</v>
       </c>
       <c r="J61"/>
       <c r="K61"/>
       <c r="L61" t="n">
-        <v>15892</v>
+        <v>20079</v>
       </c>
       <c r="M61" t="n">
-        <v>0.927</v>
+        <v>1.172</v>
       </c>
       <c r="N61" t="n">
-        <v>0.04</v>
+        <v>0.026</v>
       </c>
       <c r="O61" t="n">
-        <v>24.999</v>
+        <v>39.075</v>
       </c>
       <c r="P61" t="s">
         <v>376</v>
@@ -5996,7 +5982,7 @@
         <v>380</v>
       </c>
       <c r="C62" s="1" t="n">
-        <v>44067</v>
+        <v>44068</v>
       </c>
       <c r="D62" t="s">
         <v>381</v>
@@ -6006,31 +5992,31 @@
       </c>
       <c r="F62"/>
       <c r="G62" t="n">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="H62" t="n">
-        <v>701504</v>
+        <v>710063</v>
       </c>
       <c r="I62" t="n">
-        <v>145.473</v>
+        <v>147.248</v>
       </c>
       <c r="J62" t="n">
-        <v>4434</v>
+        <v>8559</v>
       </c>
       <c r="K62" t="n">
-        <v>0.919</v>
+        <v>1.775</v>
       </c>
       <c r="L62" t="n">
-        <v>12161</v>
+        <v>10093</v>
       </c>
       <c r="M62" t="n">
-        <v>2.522</v>
+        <v>2.093</v>
       </c>
       <c r="N62" t="n">
         <v>0.001</v>
       </c>
       <c r="O62" t="n">
-        <v>1637.058</v>
+        <v>1535.891</v>
       </c>
       <c r="P62" t="s">
         <v>382</v>
@@ -6053,7 +6039,7 @@
         <v>385</v>
       </c>
       <c r="C63" s="1" t="n">
-        <v>44066</v>
+        <v>44068</v>
       </c>
       <c r="D63" t="s">
         <v>386</v>
@@ -6063,31 +6049,31 @@
       </c>
       <c r="F63"/>
       <c r="G63" t="n">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="H63" t="n">
-        <v>378023</v>
+        <v>383130</v>
       </c>
       <c r="I63" t="n">
-        <v>1.834</v>
+        <v>1.859</v>
       </c>
       <c r="J63" t="n">
-        <v>3946</v>
+        <v>3588</v>
       </c>
       <c r="K63" t="n">
-        <v>0.019</v>
+        <v>0.017</v>
       </c>
       <c r="L63" t="n">
-        <v>3919</v>
+        <v>3991</v>
       </c>
       <c r="M63" t="n">
         <v>0.019</v>
       </c>
       <c r="N63" t="n">
-        <v>0.114</v>
+        <v>0.11</v>
       </c>
       <c r="O63" t="n">
-        <v>8.751</v>
+        <v>9.121</v>
       </c>
       <c r="P63" t="s">
         <v>387</v>
@@ -6212,7 +6198,7 @@
         <v>405</v>
       </c>
       <c r="C66" s="1" t="n">
-        <v>44068</v>
+        <v>44069</v>
       </c>
       <c r="D66" t="s">
         <v>406</v>
@@ -6222,32 +6208,28 @@
       </c>
       <c r="F66"/>
       <c r="G66" t="n">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="H66" t="n">
-        <v>2487744</v>
+        <v>2512337</v>
       </c>
       <c r="I66" t="n">
-        <v>11.262</v>
+        <v>11.374</v>
       </c>
       <c r="J66" t="n">
-        <v>24231</v>
+        <v>24593</v>
       </c>
       <c r="K66" t="n">
-        <v>0.11</v>
+        <v>0.111</v>
       </c>
       <c r="L66" t="n">
-        <v>24362</v>
+        <v>24609</v>
       </c>
       <c r="M66" t="n">
-        <v>0.11</v>
-      </c>
-      <c r="N66" t="n">
-        <v>0.023</v>
-      </c>
-      <c r="O66" t="n">
-        <v>43.963</v>
-      </c>
+        <v>0.111</v>
+      </c>
+      <c r="N66"/>
+      <c r="O66"/>
       <c r="P66" t="s">
         <v>407</v>
       </c>
@@ -6269,7 +6251,7 @@
         <v>410</v>
       </c>
       <c r="C67" s="1" t="n">
-        <v>44057</v>
+        <v>44066</v>
       </c>
       <c r="D67" t="s">
         <v>411</v>
@@ -6279,60 +6261,60 @@
       </c>
       <c r="F67"/>
       <c r="G67" t="n">
-        <v>158</v>
+        <v>167</v>
       </c>
       <c r="H67" t="n">
-        <v>262275</v>
+        <v>301561</v>
       </c>
       <c r="I67" t="n">
-        <v>60.785</v>
+        <v>69.89</v>
       </c>
       <c r="J67" t="n">
-        <v>2692</v>
+        <v>7584</v>
       </c>
       <c r="K67" t="n">
-        <v>0.624</v>
+        <v>1.758</v>
       </c>
       <c r="L67" t="n">
-        <v>2889</v>
+        <v>4552</v>
       </c>
       <c r="M67" t="n">
-        <v>0.67</v>
+        <v>1.055</v>
       </c>
       <c r="N67" t="n">
-        <v>0.348</v>
+        <v>0.151</v>
       </c>
       <c r="O67" t="n">
-        <v>2.877</v>
+        <v>6.618</v>
       </c>
       <c r="P67" t="s">
         <v>412</v>
       </c>
       <c r="Q67" t="s">
-        <v>411</v>
+        <v>413</v>
       </c>
       <c r="R67" t="s">
         <v>27</v>
       </c>
       <c r="S67" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="B68" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="C68" s="1" t="n">
         <v>44065</v>
       </c>
       <c r="D68" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="E68" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="F68"/>
       <c r="G68" t="n">
@@ -6363,33 +6345,33 @@
         <v>5.818</v>
       </c>
       <c r="P68" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="Q68" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="R68" t="s">
         <v>27</v>
       </c>
       <c r="S68" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="B69" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="C69" s="1" t="n">
         <v>44061</v>
       </c>
       <c r="D69" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="E69" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="F69"/>
       <c r="G69" t="n">
@@ -6416,33 +6398,33 @@
       <c r="N69"/>
       <c r="O69"/>
       <c r="P69" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="Q69" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="R69" t="s">
         <v>23</v>
       </c>
       <c r="S69" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="B70" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="C70" s="1" t="n">
         <v>44065</v>
       </c>
       <c r="D70" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="E70" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="F70"/>
       <c r="G70" t="n">
@@ -6476,141 +6458,141 @@
         <v>219</v>
       </c>
       <c r="Q70" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="R70" t="s">
         <v>23</v>
       </c>
       <c r="S70" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="B71" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="C71" s="1" t="n">
-        <v>44067</v>
+        <v>44068</v>
       </c>
       <c r="D71" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="E71" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="F71"/>
       <c r="G71" t="n">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="H71" t="n">
-        <v>2445546</v>
+        <v>2467528</v>
       </c>
       <c r="I71" t="n">
-        <v>64.617</v>
+        <v>65.198</v>
       </c>
       <c r="J71" t="n">
-        <v>15332</v>
+        <v>21982</v>
       </c>
       <c r="K71" t="n">
-        <v>0.405</v>
+        <v>0.581</v>
       </c>
       <c r="L71" t="n">
-        <v>22863</v>
+        <v>23162</v>
       </c>
       <c r="M71" t="n">
-        <v>0.604</v>
+        <v>0.612</v>
       </c>
       <c r="N71" t="n">
-        <v>0.032</v>
+        <v>0.031</v>
       </c>
       <c r="O71" t="n">
-        <v>31.517</v>
+        <v>32.227</v>
       </c>
       <c r="P71" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="Q71" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="R71" t="s">
         <v>23</v>
       </c>
       <c r="S71" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="B72" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="C72" s="1" t="n">
-        <v>44067</v>
+        <v>44068</v>
       </c>
       <c r="D72" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="E72" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="F72"/>
       <c r="G72" t="n">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="H72" t="n">
-        <v>2555515</v>
+        <v>2577726</v>
       </c>
       <c r="I72" t="n">
-        <v>67.523</v>
+        <v>68.11</v>
       </c>
       <c r="J72" t="n">
-        <v>16754</v>
+        <v>22211</v>
       </c>
       <c r="K72" t="n">
-        <v>0.443</v>
+        <v>0.587</v>
       </c>
       <c r="L72" t="n">
-        <v>23807</v>
+        <v>24047</v>
       </c>
       <c r="M72" t="n">
-        <v>0.629</v>
+        <v>0.635</v>
       </c>
       <c r="N72" t="n">
         <v>0.03</v>
       </c>
       <c r="O72" t="n">
-        <v>32.818</v>
+        <v>33.458</v>
       </c>
       <c r="P72" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="Q72" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="R72" t="s">
         <v>54</v>
       </c>
       <c r="S72" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="B73" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="C73" s="1" t="n">
         <v>44055</v>
       </c>
       <c r="D73" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="E73" t="s">
         <v>45</v>
@@ -6644,33 +6626,33 @@
         <v>74.098</v>
       </c>
       <c r="P73" t="s">
+        <v>444</v>
+      </c>
+      <c r="Q73" t="s">
         <v>443</v>
       </c>
-      <c r="Q73" t="s">
-        <v>442</v>
-      </c>
       <c r="R73" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="S73" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="B74" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="C74" s="1" t="n">
         <v>44067</v>
       </c>
       <c r="D74" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="E74" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="F74"/>
       <c r="G74" t="n">
@@ -6701,33 +6683,33 @@
         <v>19.838</v>
       </c>
       <c r="P74" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="Q74" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="R74" t="s">
         <v>23</v>
       </c>
       <c r="S74" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="B75" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="C75" s="1" t="n">
         <v>44068</v>
       </c>
       <c r="D75" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="E75" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="F75"/>
       <c r="G75" t="n">
@@ -6758,90 +6740,90 @@
         <v>16.903</v>
       </c>
       <c r="P75" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="Q75" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="R75" t="s">
         <v>27</v>
       </c>
       <c r="S75" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="B76" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="C76" s="1" t="n">
-        <v>44067</v>
+        <v>44068</v>
       </c>
       <c r="D76" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="E76" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="F76"/>
       <c r="G76" t="n">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="H76" t="n">
-        <v>34883220</v>
+        <v>35128661</v>
       </c>
       <c r="I76" t="n">
-        <v>239.033</v>
+        <v>240.715</v>
       </c>
       <c r="J76" t="n">
-        <v>187814</v>
+        <v>245441</v>
       </c>
       <c r="K76" t="n">
-        <v>1.287</v>
+        <v>1.682</v>
       </c>
       <c r="L76" t="n">
-        <v>273494</v>
+        <v>273028</v>
       </c>
       <c r="M76" t="n">
-        <v>1.874</v>
+        <v>1.871</v>
       </c>
       <c r="N76" t="n">
         <v>0.018</v>
       </c>
       <c r="O76" t="n">
-        <v>56.48</v>
+        <v>56.631</v>
       </c>
       <c r="P76" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="Q76" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="R76" t="s">
         <v>27</v>
       </c>
       <c r="S76" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="B77" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="C77" s="1" t="n">
         <v>44066</v>
       </c>
       <c r="D77" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="E77" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="F77"/>
       <c r="G77" t="n">
@@ -6872,201 +6854,205 @@
         <v>63.261</v>
       </c>
       <c r="P77" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="Q77" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="R77" t="s">
         <v>54</v>
       </c>
       <c r="S77" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="B78" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="C78" s="1" t="n">
-        <v>44067</v>
+        <v>44068</v>
       </c>
       <c r="D78" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="E78" t="s">
         <v>45</v>
       </c>
       <c r="F78"/>
       <c r="G78" t="n">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="H78" t="n">
-        <v>4733485</v>
+        <v>4792192</v>
       </c>
       <c r="I78" t="n">
-        <v>135.966</v>
-      </c>
-      <c r="J78"/>
-      <c r="K78"/>
+        <v>137.652</v>
+      </c>
+      <c r="J78" t="n">
+        <v>58707</v>
+      </c>
+      <c r="K78" t="n">
+        <v>1.686</v>
+      </c>
       <c r="L78" t="n">
-        <v>59397</v>
+        <v>59111</v>
       </c>
       <c r="M78" t="n">
-        <v>1.706</v>
+        <v>1.698</v>
       </c>
       <c r="N78" t="n">
         <v>0.021</v>
       </c>
       <c r="O78" t="n">
-        <v>46.523</v>
+        <v>47.343</v>
       </c>
       <c r="P78" t="s">
         <v>45</v>
       </c>
       <c r="Q78" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="R78" t="s">
         <v>27</v>
       </c>
       <c r="S78" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="B79" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="C79" s="1" t="n">
-        <v>44067</v>
+        <v>44068</v>
       </c>
       <c r="D79" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="E79" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="F79" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="G79" t="n">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="H79" t="n">
-        <v>143748</v>
+        <v>144564</v>
       </c>
       <c r="I79" t="n">
-        <v>8.585</v>
+        <v>8.634</v>
       </c>
       <c r="J79" t="n">
-        <v>812</v>
+        <v>816</v>
       </c>
       <c r="K79" t="n">
-        <v>0.048</v>
+        <v>0.049</v>
       </c>
       <c r="L79" t="n">
-        <v>1278</v>
+        <v>1262</v>
       </c>
       <c r="M79" t="n">
-        <v>0.076</v>
+        <v>0.075</v>
       </c>
       <c r="N79" t="n">
         <v>0.088</v>
       </c>
       <c r="O79" t="n">
-        <v>11.367</v>
+        <v>11.384</v>
       </c>
       <c r="P79" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="Q79" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="R79" t="s">
         <v>27</v>
       </c>
       <c r="S79" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="B80" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="C80" s="1" t="n">
-        <v>44066</v>
+        <v>44068</v>
       </c>
       <c r="D80" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
       <c r="E80" t="s">
         <v>45</v>
       </c>
       <c r="F80" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="G80" t="n">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="H80" t="n">
-        <v>869668</v>
+        <v>885575</v>
       </c>
       <c r="I80" t="n">
-        <v>127.806</v>
+        <v>130.144</v>
       </c>
       <c r="J80" t="n">
-        <v>6939</v>
+        <v>8646</v>
       </c>
       <c r="K80" t="n">
-        <v>1.02</v>
+        <v>1.271</v>
       </c>
       <c r="L80" t="n">
-        <v>9300</v>
+        <v>9210</v>
       </c>
       <c r="M80" t="n">
-        <v>1.367</v>
+        <v>1.353</v>
       </c>
       <c r="N80" t="n">
-        <v>0.017</v>
+        <v>0.014</v>
       </c>
       <c r="O80" t="n">
-        <v>60.446</v>
+        <v>69.174</v>
       </c>
       <c r="P80" t="s">
         <v>45</v>
       </c>
       <c r="Q80" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="R80" t="s">
         <v>23</v>
       </c>
       <c r="S80" t="s">
-        <v>488</v>
+        <v>489</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c r="B81" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="C81" s="1" t="n">
         <v>44061</v>
       </c>
       <c r="D81" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="E81" t="s">
         <v>45</v>
@@ -7099,27 +7085,27 @@
         <v>45</v>
       </c>
       <c r="Q81" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="R81" t="s">
         <v>23</v>
       </c>
       <c r="S81" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c r="B82" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
       <c r="C82" s="1" t="n">
         <v>44061</v>
       </c>
       <c r="D82" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="E82" t="s">
         <v>45</v>
@@ -7152,30 +7138,30 @@
         <v>45</v>
       </c>
       <c r="Q82" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="R82" t="s">
-        <v>494</v>
+        <v>495</v>
       </c>
       <c r="S82" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="B83" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="C83" s="1" t="n">
         <v>44068</v>
       </c>
       <c r="D83" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="E83" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="F83"/>
       <c r="G83" t="n">
@@ -7202,33 +7188,33 @@
         <v>36.652</v>
       </c>
       <c r="P83" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c r="Q83" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="R83" t="s">
         <v>27</v>
       </c>
       <c r="S83" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="B84" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="C84" s="1" t="n">
         <v>44067</v>
       </c>
       <c r="D84" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
       <c r="E84" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="F84"/>
       <c r="G84" t="n">
@@ -7259,36 +7245,36 @@
         <v>30.77</v>
       </c>
       <c r="P84" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="Q84" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="R84" t="s">
         <v>27</v>
       </c>
       <c r="S84" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
       <c r="B85" t="s">
-        <v>509</v>
+        <v>510</v>
       </c>
       <c r="C85" s="1" t="n">
         <v>44067</v>
       </c>
       <c r="D85" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
       <c r="E85" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
       <c r="F85" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="G85" t="n">
         <v>177</v>
@@ -7318,90 +7304,90 @@
         <v>6.616</v>
       </c>
       <c r="P85" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
       <c r="Q85" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
       <c r="R85" t="s">
         <v>23</v>
       </c>
       <c r="S85" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="B86" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="C86" s="1" t="n">
-        <v>44067</v>
+        <v>44068</v>
       </c>
       <c r="D86" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
       <c r="E86" t="s">
-        <v>518</v>
+        <v>519</v>
       </c>
       <c r="F86"/>
       <c r="G86" t="n">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="H86" t="n">
-        <v>1756427</v>
+        <v>1775475</v>
       </c>
       <c r="I86" t="n">
-        <v>34.259</v>
+        <v>34.63</v>
       </c>
       <c r="J86" t="n">
-        <v>12805</v>
+        <v>19048</v>
       </c>
       <c r="K86" t="n">
-        <v>0.25</v>
+        <v>0.372</v>
       </c>
       <c r="L86" t="n">
-        <v>12989</v>
+        <v>14807</v>
       </c>
       <c r="M86" t="n">
-        <v>0.253</v>
+        <v>0.289</v>
       </c>
       <c r="N86" t="n">
-        <v>0.024</v>
+        <v>0.021</v>
       </c>
       <c r="O86" t="n">
-        <v>42.29</v>
+        <v>47.458</v>
       </c>
       <c r="P86" t="s">
-        <v>518</v>
+        <v>519</v>
       </c>
       <c r="Q86" t="s">
-        <v>519</v>
+        <v>520</v>
       </c>
       <c r="R86" t="s">
         <v>23</v>
       </c>
       <c r="S86" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="s">
-        <v>521</v>
+        <v>522</v>
       </c>
       <c r="B87" t="s">
-        <v>522</v>
+        <v>523</v>
       </c>
       <c r="C87" s="1" t="n">
         <v>44063</v>
       </c>
       <c r="D87" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
       <c r="E87" t="s">
-        <v>524</v>
+        <v>525</v>
       </c>
       <c r="F87"/>
       <c r="G87" t="n">
@@ -7428,33 +7414,33 @@
         <v>11.896</v>
       </c>
       <c r="P87" t="s">
-        <v>525</v>
+        <v>526</v>
       </c>
       <c r="Q87" t="s">
-        <v>526</v>
+        <v>527</v>
       </c>
       <c r="R87" t="s">
         <v>27</v>
       </c>
       <c r="S87" t="s">
-        <v>527</v>
+        <v>528</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="s">
-        <v>528</v>
+        <v>529</v>
       </c>
       <c r="B88" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="C88" s="1" t="n">
         <v>44017</v>
       </c>
       <c r="D88" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c r="E88" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
       <c r="F88"/>
       <c r="G88" t="n">
@@ -7481,86 +7467,86 @@
         <v>12.36</v>
       </c>
       <c r="P88" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
       <c r="Q88" t="s">
-        <v>533</v>
+        <v>534</v>
       </c>
       <c r="R88" t="s">
         <v>23</v>
       </c>
       <c r="S88" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="s">
-        <v>528</v>
+        <v>529</v>
       </c>
       <c r="B89" t="s">
-        <v>535</v>
+        <v>536</v>
       </c>
       <c r="C89" s="1" t="n">
-        <v>44059</v>
+        <v>44066</v>
       </c>
       <c r="D89" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
       <c r="E89" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
       <c r="F89"/>
       <c r="G89" t="n">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="H89"/>
       <c r="I89"/>
       <c r="J89" t="n">
-        <v>8070</v>
+        <v>9264</v>
       </c>
       <c r="K89" t="n">
-        <v>0.799</v>
+        <v>0.917</v>
       </c>
       <c r="L89" t="n">
-        <v>8070</v>
+        <v>9264</v>
       </c>
       <c r="M89" t="n">
-        <v>0.799</v>
+        <v>0.917</v>
       </c>
       <c r="N89" t="n">
-        <v>0.035</v>
+        <v>0.027</v>
       </c>
       <c r="O89" t="n">
-        <v>28.661</v>
+        <v>36.555</v>
       </c>
       <c r="P89" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
       <c r="Q89" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
       <c r="R89" t="s">
         <v>54</v>
       </c>
       <c r="S89" t="s">
-        <v>537</v>
+        <v>538</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
       <c r="B90" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
       <c r="C90" s="1" t="n">
         <v>44067</v>
       </c>
       <c r="D90" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
       <c r="E90" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
       <c r="F90"/>
       <c r="G90" t="n">
@@ -7591,52 +7577,52 @@
         <v>30.779</v>
       </c>
       <c r="P90" t="s">
+        <v>542</v>
+      </c>
+      <c r="Q90" t="s">
         <v>541</v>
       </c>
-      <c r="Q90" t="s">
-        <v>540</v>
-      </c>
       <c r="R90" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
       <c r="S90" t="s">
-        <v>543</v>
+        <v>544</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="B91" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
       <c r="C91" s="1" t="n">
-        <v>44067</v>
+        <v>44068</v>
       </c>
       <c r="D91" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
       <c r="E91" t="s">
-        <v>547</v>
+        <v>548</v>
       </c>
       <c r="F91"/>
       <c r="G91" t="n">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="H91" t="n">
-        <v>86265</v>
+        <v>86419</v>
       </c>
       <c r="I91" t="n">
-        <v>3.622</v>
+        <v>3.628</v>
       </c>
       <c r="J91" t="n">
-        <v>241</v>
+        <v>155</v>
       </c>
       <c r="K91" t="n">
-        <v>0.01</v>
+        <v>0.007</v>
       </c>
       <c r="L91" t="n">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="M91" t="n">
         <v>0.008</v>
@@ -7645,55 +7631,55 @@
         <v>0.002</v>
       </c>
       <c r="O91" t="n">
-        <v>654.5</v>
+        <v>647.5</v>
       </c>
       <c r="P91" t="s">
+        <v>548</v>
+      </c>
+      <c r="Q91" t="s">
         <v>547</v>
-      </c>
-      <c r="Q91" t="s">
-        <v>546</v>
       </c>
       <c r="R91" t="s">
         <v>23</v>
       </c>
       <c r="S91" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="s">
-        <v>549</v>
+        <v>550</v>
       </c>
       <c r="B92" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="C92" s="1" t="n">
-        <v>44067</v>
+        <v>44068</v>
       </c>
       <c r="D92" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
       <c r="E92" t="s">
-        <v>552</v>
+        <v>553</v>
       </c>
       <c r="F92"/>
       <c r="G92" t="n">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="H92" t="n">
-        <v>407412</v>
+        <v>409632</v>
       </c>
       <c r="I92" t="n">
-        <v>5.837</v>
+        <v>5.869</v>
       </c>
       <c r="J92" t="n">
-        <v>1240</v>
+        <v>2220</v>
       </c>
       <c r="K92" t="n">
-        <v>0.018</v>
+        <v>0.032</v>
       </c>
       <c r="L92" t="n">
-        <v>1715</v>
+        <v>1765</v>
       </c>
       <c r="M92" t="n">
         <v>0.025</v>
@@ -7702,55 +7688,55 @@
         <v>0.002</v>
       </c>
       <c r="O92" t="n">
-        <v>631.842</v>
+        <v>514.792</v>
       </c>
       <c r="P92" t="s">
-        <v>552</v>
+        <v>553</v>
       </c>
       <c r="Q92" t="s">
-        <v>553</v>
+        <v>554</v>
       </c>
       <c r="R92" t="s">
         <v>23</v>
       </c>
       <c r="S92" t="s">
-        <v>554</v>
+        <v>555</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="s">
-        <v>549</v>
+        <v>550</v>
       </c>
       <c r="B93" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="C93" s="1" t="n">
-        <v>44067</v>
+        <v>44068</v>
       </c>
       <c r="D93" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
       <c r="E93" t="s">
-        <v>552</v>
+        <v>553</v>
       </c>
       <c r="F93"/>
       <c r="G93" t="n">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="H93" t="n">
-        <v>795683</v>
+        <v>797903</v>
       </c>
       <c r="I93" t="n">
-        <v>11.399</v>
+        <v>11.431</v>
       </c>
       <c r="J93" t="n">
-        <v>1240</v>
+        <v>2220</v>
       </c>
       <c r="K93" t="n">
-        <v>0.018</v>
+        <v>0.032</v>
       </c>
       <c r="L93" t="n">
-        <v>1715</v>
+        <v>1765</v>
       </c>
       <c r="M93" t="n">
         <v>0.025</v>
@@ -7759,37 +7745,37 @@
         <v>0.002</v>
       </c>
       <c r="O93" t="n">
-        <v>631.842</v>
+        <v>514.792</v>
       </c>
       <c r="P93" t="s">
-        <v>552</v>
+        <v>553</v>
       </c>
       <c r="Q93" t="s">
-        <v>553</v>
+        <v>554</v>
       </c>
       <c r="R93" t="s">
         <v>27</v>
       </c>
       <c r="S93" t="s">
-        <v>556</v>
+        <v>557</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="s">
-        <v>557</v>
+        <v>558</v>
       </c>
       <c r="B94" t="s">
-        <v>558</v>
+        <v>559</v>
       </c>
       <c r="C94" s="1" t="n">
         <v>44062</v>
       </c>
       <c r="D94"/>
       <c r="E94" t="s">
-        <v>559</v>
+        <v>560</v>
       </c>
       <c r="F94" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="G94" t="n">
         <v>163</v>
@@ -7819,261 +7805,257 @@
         <v>47.437</v>
       </c>
       <c r="P94" t="s">
-        <v>559</v>
+        <v>560</v>
       </c>
       <c r="Q94" t="s">
-        <v>561</v>
+        <v>562</v>
       </c>
       <c r="R94" t="s">
         <v>54</v>
       </c>
       <c r="S94" t="s">
-        <v>562</v>
+        <v>563</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
       <c r="B95" t="s">
-        <v>564</v>
+        <v>565</v>
       </c>
       <c r="C95" s="1" t="n">
-        <v>44064</v>
+        <v>44065</v>
       </c>
       <c r="D95" t="s">
-        <v>565</v>
+        <v>566</v>
       </c>
       <c r="E95" t="s">
-        <v>566</v>
+        <v>567</v>
       </c>
       <c r="F95"/>
       <c r="G95" t="n">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="H95" t="n">
-        <v>121807</v>
+        <v>123268</v>
       </c>
       <c r="I95" t="n">
-        <v>10.306</v>
+        <v>10.43</v>
       </c>
       <c r="J95" t="n">
-        <v>2236</v>
+        <v>1461</v>
       </c>
       <c r="K95" t="n">
-        <v>0.189</v>
+        <v>0.124</v>
       </c>
       <c r="L95" t="n">
-        <v>1730</v>
+        <v>1803</v>
       </c>
       <c r="M95" t="n">
-        <v>0.146</v>
+        <v>0.153</v>
       </c>
       <c r="N95" t="n">
-        <v>0.057</v>
+        <v>0.056</v>
       </c>
       <c r="O95" t="n">
-        <v>17.399</v>
+        <v>17.928</v>
       </c>
       <c r="P95" t="s">
+        <v>567</v>
+      </c>
+      <c r="Q95" t="s">
         <v>566</v>
-      </c>
-      <c r="Q95" t="s">
-        <v>565</v>
       </c>
       <c r="R95" t="s">
         <v>27</v>
       </c>
       <c r="S95" t="s">
-        <v>567</v>
+        <v>568</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="s">
-        <v>568</v>
+        <v>569</v>
       </c>
       <c r="B96" t="s">
-        <v>569</v>
+        <v>570</v>
       </c>
       <c r="C96" s="1" t="n">
-        <v>44067</v>
+        <v>44068</v>
       </c>
       <c r="D96" t="s">
-        <v>570</v>
+        <v>571</v>
       </c>
       <c r="E96" t="s">
-        <v>571</v>
+        <v>572</v>
       </c>
       <c r="F96"/>
       <c r="G96" t="n">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="H96" t="n">
-        <v>6423409</v>
+        <v>6521640</v>
       </c>
       <c r="I96" t="n">
-        <v>76.162</v>
+        <v>77.326</v>
       </c>
       <c r="J96" t="n">
-        <v>95943</v>
+        <v>98231</v>
       </c>
       <c r="K96" t="n">
-        <v>1.138</v>
+        <v>1.165</v>
       </c>
       <c r="L96" t="n">
-        <v>89046</v>
+        <v>91319</v>
       </c>
       <c r="M96" t="n">
-        <v>1.056</v>
+        <v>1.083</v>
       </c>
       <c r="N96" t="n">
         <v>0.014</v>
       </c>
       <c r="O96" t="n">
-        <v>69.723</v>
+        <v>69.862</v>
       </c>
       <c r="P96" t="s">
+        <v>572</v>
+      </c>
+      <c r="Q96" t="s">
         <v>571</v>
-      </c>
-      <c r="Q96" t="s">
-        <v>570</v>
       </c>
       <c r="R96" t="s">
         <v>27</v>
       </c>
       <c r="S96" t="s">
-        <v>572</v>
+        <v>573</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="s">
-        <v>573</v>
+        <v>574</v>
       </c>
       <c r="B97" t="s">
-        <v>574</v>
+        <v>575</v>
       </c>
       <c r="C97" s="1" t="n">
-        <v>44066</v>
+        <v>44067</v>
       </c>
       <c r="D97" t="s">
-        <v>575</v>
+        <v>576</v>
       </c>
       <c r="E97" t="s">
-        <v>576</v>
+        <v>577</v>
       </c>
       <c r="F97"/>
       <c r="G97" t="n">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H97" t="n">
-        <v>351845</v>
+        <v>355057</v>
       </c>
       <c r="I97" t="n">
-        <v>7.692</v>
+        <v>7.762</v>
       </c>
       <c r="J97" t="n">
-        <v>3457</v>
+        <v>3212</v>
       </c>
       <c r="K97" t="n">
-        <v>0.076</v>
+        <v>0.07</v>
       </c>
       <c r="L97" t="n">
-        <v>3744</v>
+        <v>3645</v>
       </c>
       <c r="M97" t="n">
-        <v>0.082</v>
+        <v>0.08</v>
       </c>
       <c r="N97" t="n">
-        <v>0.016</v>
+        <v>0.03</v>
       </c>
       <c r="O97" t="n">
-        <v>63.304</v>
+        <v>33.44</v>
       </c>
       <c r="P97" t="s">
-        <v>576</v>
+        <v>577</v>
       </c>
       <c r="Q97" t="s">
-        <v>577</v>
+        <v>578</v>
       </c>
       <c r="R97" t="s">
         <v>54</v>
       </c>
       <c r="S97" t="s">
-        <v>578</v>
+        <v>579</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="B98" t="s">
-        <v>580</v>
+        <v>581</v>
       </c>
       <c r="C98" s="1" t="n">
-        <v>44068</v>
+        <v>44069</v>
       </c>
       <c r="D98" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="E98" t="s">
-        <v>582</v>
+        <v>583</v>
       </c>
       <c r="F98"/>
       <c r="G98" t="n">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="H98" t="n">
-        <v>1436206</v>
+        <v>1452006</v>
       </c>
       <c r="I98" t="n">
-        <v>32.84</v>
+        <v>33.201</v>
       </c>
       <c r="J98" t="n">
-        <v>10855</v>
+        <v>15800</v>
       </c>
       <c r="K98" t="n">
-        <v>0.248</v>
+        <v>0.361</v>
       </c>
       <c r="L98" t="n">
-        <v>17257</v>
+        <v>16715</v>
       </c>
       <c r="M98" t="n">
-        <v>0.395</v>
-      </c>
-      <c r="N98" t="n">
-        <v>0.102</v>
-      </c>
-      <c r="O98" t="n">
-        <v>9.807</v>
-      </c>
+        <v>0.382</v>
+      </c>
+      <c r="N98"/>
+      <c r="O98"/>
       <c r="P98" t="s">
-        <v>582</v>
+        <v>583</v>
       </c>
       <c r="Q98" t="s">
-        <v>583</v>
+        <v>584</v>
       </c>
       <c r="R98" t="s">
         <v>40</v>
       </c>
       <c r="S98" t="s">
-        <v>584</v>
+        <v>585</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="s">
-        <v>585</v>
+        <v>586</v>
       </c>
       <c r="B99" t="s">
-        <v>586</v>
+        <v>587</v>
       </c>
       <c r="C99" s="1" t="n">
         <v>44067</v>
       </c>
       <c r="D99" t="s">
-        <v>587</v>
+        <v>588</v>
       </c>
       <c r="E99" t="s">
-        <v>588</v>
+        <v>589</v>
       </c>
       <c r="F99"/>
       <c r="G99" t="n">
@@ -8104,36 +8086,36 @@
         <v>185.096</v>
       </c>
       <c r="P99" t="s">
+        <v>589</v>
+      </c>
+      <c r="Q99" t="s">
         <v>588</v>
-      </c>
-      <c r="Q99" t="s">
-        <v>587</v>
       </c>
       <c r="R99" t="s">
         <v>27</v>
       </c>
       <c r="S99" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="s">
-        <v>590</v>
+        <v>591</v>
       </c>
       <c r="B100" t="s">
-        <v>591</v>
+        <v>592</v>
       </c>
       <c r="C100" s="1" t="n">
         <v>44062</v>
       </c>
       <c r="D100" t="s">
-        <v>592</v>
+        <v>593</v>
       </c>
       <c r="E100" t="s">
-        <v>593</v>
+        <v>594</v>
       </c>
       <c r="F100" t="s">
-        <v>594</v>
+        <v>595</v>
       </c>
       <c r="G100" t="n">
         <v>142</v>
@@ -8163,33 +8145,33 @@
         <v>151.5</v>
       </c>
       <c r="P100" t="s">
-        <v>593</v>
+        <v>594</v>
       </c>
       <c r="Q100" t="s">
-        <v>595</v>
+        <v>596</v>
       </c>
       <c r="R100" t="s">
         <v>27</v>
       </c>
       <c r="S100" t="s">
-        <v>596</v>
+        <v>597</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="s">
-        <v>597</v>
+        <v>598</v>
       </c>
       <c r="B101" t="s">
-        <v>598</v>
+        <v>599</v>
       </c>
       <c r="C101" s="1" t="n">
         <v>44062</v>
       </c>
       <c r="D101" t="s">
-        <v>599</v>
+        <v>600</v>
       </c>
       <c r="E101" t="s">
-        <v>600</v>
+        <v>601</v>
       </c>
       <c r="F101"/>
       <c r="G101" t="n">
@@ -8216,147 +8198,143 @@
         <v>18.291</v>
       </c>
       <c r="P101" t="s">
+        <v>601</v>
+      </c>
+      <c r="Q101" t="s">
         <v>600</v>
       </c>
-      <c r="Q101" t="s">
-        <v>599</v>
-      </c>
       <c r="R101" t="s">
-        <v>601</v>
+        <v>602</v>
       </c>
       <c r="S101" t="s">
-        <v>602</v>
+        <v>603</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="s">
-        <v>597</v>
+        <v>598</v>
       </c>
       <c r="B102" t="s">
-        <v>603</v>
+        <v>604</v>
       </c>
       <c r="C102" s="1" t="n">
-        <v>44067</v>
+        <v>44068</v>
       </c>
       <c r="D102" t="s">
-        <v>604</v>
+        <v>605</v>
       </c>
       <c r="E102" t="s">
-        <v>605</v>
+        <v>606</v>
       </c>
       <c r="F102"/>
       <c r="G102" t="n">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="H102" t="n">
-        <v>72382318</v>
+        <v>73016779</v>
       </c>
       <c r="I102" t="n">
-        <v>218.676</v>
+        <v>220.593</v>
       </c>
       <c r="J102" t="n">
-        <v>682054</v>
+        <v>634461</v>
       </c>
       <c r="K102" t="n">
-        <v>2.061</v>
+        <v>1.917</v>
       </c>
       <c r="L102" t="n">
-        <v>680171</v>
+        <v>678978</v>
       </c>
       <c r="M102" t="n">
-        <v>2.055</v>
+        <v>2.051</v>
       </c>
       <c r="N102" t="n">
-        <v>0.063</v>
+        <v>0.064</v>
       </c>
       <c r="O102" t="n">
-        <v>15.906</v>
+        <v>15.708</v>
       </c>
       <c r="P102" t="s">
-        <v>605</v>
+        <v>606</v>
       </c>
       <c r="Q102" t="s">
-        <v>606</v>
+        <v>607</v>
       </c>
       <c r="R102" t="s">
-        <v>607</v>
+        <v>608</v>
       </c>
       <c r="S102" t="s">
-        <v>608</v>
+        <v>609</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="s">
-        <v>609</v>
+        <v>610</v>
       </c>
       <c r="B103" t="s">
-        <v>610</v>
+        <v>611</v>
       </c>
       <c r="C103" s="1" t="n">
-        <v>44066</v>
+        <v>44068</v>
       </c>
       <c r="D103" t="s">
-        <v>611</v>
+        <v>612</v>
       </c>
       <c r="E103" t="s">
         <v>125</v>
       </c>
       <c r="F103"/>
       <c r="G103" t="n">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="H103" t="n">
-        <v>160216</v>
+        <v>163129</v>
       </c>
       <c r="I103" t="n">
-        <v>46.122</v>
-      </c>
-      <c r="J103" t="n">
-        <v>1514</v>
-      </c>
-      <c r="K103" t="n">
-        <v>0.436</v>
-      </c>
+        <v>46.961</v>
+      </c>
+      <c r="J103"/>
+      <c r="K103"/>
       <c r="L103" t="n">
-        <v>1993</v>
+        <v>2219</v>
       </c>
       <c r="M103" t="n">
-        <v>0.574</v>
+        <v>0.639</v>
       </c>
       <c r="N103" t="n">
-        <v>0.006</v>
+        <v>0.005</v>
       </c>
       <c r="O103" t="n">
-        <v>160.356</v>
+        <v>204.382</v>
       </c>
       <c r="P103" t="s">
         <v>125</v>
       </c>
       <c r="Q103" t="s">
-        <v>612</v>
+        <v>613</v>
       </c>
       <c r="R103" t="s">
         <v>27</v>
       </c>
       <c r="S103" t="s">
-        <v>613</v>
+        <v>614</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="s">
-        <v>614</v>
+        <v>615</v>
       </c>
       <c r="B104" t="s">
-        <v>615</v>
+        <v>616</v>
       </c>
       <c r="C104" s="1" t="n">
         <v>43950</v>
       </c>
       <c r="D104" t="s">
-        <v>616</v>
+        <v>617</v>
       </c>
       <c r="E104" t="s">
-        <v>617</v>
+        <v>618</v>
       </c>
       <c r="F104"/>
       <c r="G104" t="n">
@@ -8383,33 +8361,33 @@
         <v>38171</v>
       </c>
       <c r="P104" t="s">
-        <v>617</v>
+        <v>618</v>
       </c>
       <c r="Q104" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
       <c r="R104" t="s">
         <v>54</v>
       </c>
       <c r="S104" t="s">
-        <v>619</v>
+        <v>620</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="s">
-        <v>620</v>
+        <v>621</v>
       </c>
       <c r="B105" t="s">
-        <v>621</v>
+        <v>622</v>
       </c>
       <c r="C105" s="1" t="n">
         <v>44066</v>
       </c>
       <c r="D105" t="s">
-        <v>622</v>
+        <v>623</v>
       </c>
       <c r="E105" t="s">
-        <v>623</v>
+        <v>624</v>
       </c>
       <c r="F105"/>
       <c r="G105" t="n">
@@ -8440,16 +8418,16 @@
         <v>12.086</v>
       </c>
       <c r="P105" t="s">
-        <v>623</v>
+        <v>624</v>
       </c>
       <c r="Q105" t="s">
-        <v>624</v>
+        <v>625</v>
       </c>
       <c r="R105" t="s">
         <v>27</v>
       </c>
       <c r="S105" t="s">
-        <v>625</v>
+        <v>626</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated testing data for 2020-08-28
</commit_message>
<xml_diff>
--- a/public/data/testing/covid-testing-latest-data-source-details.xlsx
+++ b/public/data/testing/covid-testing-latest-data-source-details.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="627" uniqueCount="627">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="629" uniqueCount="629">
   <si>
     <t xml:space="preserve">ISO code</t>
   </si>
@@ -110,7 +110,7 @@
     <t xml:space="preserve">Australia - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.health.gov.au/sites/default/files/documents/2020/08/coronavirus-covid-19-at-a-glance-25-august-2020.pdf</t>
+    <t xml:space="preserve">https://www.health.gov.au/sites/default/files/documents/2020/08/coronavirus-covid-19-at-a-glance-27-august-2020.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">Australian Government Department of Health</t>
@@ -202,7 +202,7 @@
     <t xml:space="preserve">Belarus - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">http://minzdrav.gov.by/ru/sobytiya/u-belarusi-na-25-zhni-nya-vypisanyya-69-tys-097-patsyenta/</t>
+    <t xml:space="preserve">http://minzdrav.gov.by/ru/sobytiya/u-belarusi-na-27-zhni-nya-vypisanyya-69-tys-650-patsyenta/</t>
   </si>
   <si>
     <t xml:space="preserve">Belarus Ministry of Health</t>
@@ -245,7 +245,7 @@
     <t xml:space="preserve">Bolivia - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://minsalud.gob.bo/4542-bolivia-suma-722-contagios-nuevos-de-coronavirus-y-el-total-sube-a-109-149</t>
+    <t xml:space="preserve">https://minsalud.gob.bo/4550-bolivia-acumula-50-397-pacientes-recuperados-de-covid-19-y-los-casos-positivos-llegan-a-112-094</t>
   </si>
   <si>
     <t xml:space="preserve">https://www.minsalud.gob.bo/</t>
@@ -265,10 +265,10 @@
     <t xml:space="preserve">Brazil - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://static.poder360.com.br/2020/08/entrevista-coletiva-ms-19ago2020.pdf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The number of PCR tests in private labs has not been updated</t>
+    <t xml:space="preserve">https://www.saude.gov.br/noticias/agencia-saude/47401-brasil-nao-possui-casos-confirmados-de-reinfeccao-por-covid-19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Up to August 22, 4,797,948 million RT-PCR exams were performed for Covid-19, of which 2,652,551 in the national network of public health laboratories and 2,145,397 in the main private laboratories in the country</t>
   </si>
   <si>
     <t xml:space="preserve">Brazil Ministry of Health</t>
@@ -398,7 +398,7 @@
     <t xml:space="preserve">Cote d'Ivoire - samples tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.facebook.com/Mshpci/posts/1678490098983344</t>
+    <t xml:space="preserve">https://www.facebook.com/Mshpci/posts/1680281235470897</t>
   </si>
   <si>
     <t xml:space="preserve">Ministry of Health and Public Hygiene</t>
@@ -477,7 +477,7 @@
     <t xml:space="preserve">Democratic Republic of Congo - samples tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/CMR_Covid19_RDC/status/1297508985793327105/photo/1</t>
+    <t xml:space="preserve">https://twitter.com/CMR_Covid19_RDC/status/1298904810050260992/photo/1</t>
   </si>
   <si>
     <t xml:space="preserve">DRC COVID-19 Pandemic Response Multisectoral Committee</t>
@@ -495,7 +495,7 @@
     <t xml:space="preserve">Denmark - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://files.ssi.dk/Data-epidemiologisk-rapport-25082020-rg99</t>
+    <t xml:space="preserve">https://files.ssi.dk/Data-epidemiologisk-rapport-28082020-mm29</t>
   </si>
   <si>
     <t xml:space="preserve">Statens Serum Institut</t>
@@ -513,7 +513,7 @@
     <t xml:space="preserve">Ecuador - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.gestionderiesgos.gob.ec/wp-content/uploads/2020/08/INFOGRAFIA-NACIONALCOVID19-COE-NACIONAL-08h00-25082020.pdf</t>
+    <t xml:space="preserve">https://www.gestionderiesgos.gob.ec/wp-content/uploads/2020/08/INFOGRAFIA-NACIONALCOVID19-COE-NACIONAL-08h00-27082020.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">Government of Ecuador</t>
@@ -539,7 +539,7 @@
     <t xml:space="preserve">El Salvador - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.facebook.com/nayibbukele/posts/3173404349412401</t>
+    <t xml:space="preserve">https://www.facebook.com/nayibbukele/posts/3182381598514676</t>
   </si>
   <si>
     <t xml:space="preserve">Government of El Salvador</t>
@@ -583,7 +583,7 @@
     <t xml:space="preserve">Ethiopia - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/EPHIEthiopia/status/1297581159547834370</t>
+    <t xml:space="preserve">https://twitter.com/EPHIEthiopia/status/1298669531615961090</t>
   </si>
   <si>
     <t xml:space="preserve">Ethiopian Public Health Institute</t>
@@ -676,7 +676,7 @@
     <t xml:space="preserve">Germany - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.rki.de/DE/Content/InfAZ/N/Neuartiges_Coronavirus/Situationsberichte/2020-08-19-de.pdf?__blob=publicationFile</t>
+    <t xml:space="preserve">https://www.rki.de/DE/Content/InfAZ/N/Neuartiges_Coronavirus/Situationsberichte/2020-08-26-de.pdf?__blob=publicationFile</t>
   </si>
   <si>
     <t xml:space="preserve">Robert Koch Institut</t>
@@ -692,12 +692,13 @@
   </si>
   <si>
     <t xml:space="preserve">To determine how many laboratory tests regarding SARS-CoV-2 are carried out per calendar week in Germany and how many tests are positive or negative, the RKI has started a Germany-wide laboratory query. However, the number of laboratories reporting data seems to vary from week to week.
-The report published on 19 August 2020 states that “from the beginning of the collection up to and including calendar week 33/2020”:
-– The cumulative total of samples tested was 10,197,366;
-- For calendar week 33 (which ends 16 August), 181 labs reported 875,524 samples tested;
-- For calendar week 32 (which ends 9 August), 165 labs reported 730,300 samples tested;
-- For calendar week 31 (which ends 2 August), 165 labs reported 578,099 samples tested;
-- For calendar week 30 (which ends 26 July), 180 labs reported 570,746 samples tested;
+The report published on 26 August 2020 states that “from the beginning of the collection up to and including calendar week 34/2020”:
+– The cumulative total of samples tested was 11,208,091;
+- For calendar week 34 (which ends 23 August), 182 labs reported 987,423 samples tested;
+- For calendar week 33 (which ends 16 August), 188 labs reported 891,988 samples tested;
+- For calendar week 32 (which ends 9 August), 167 labs reported 733,608 samples tested;
+- For calendar week 31 (which ends 2 August), 167 labs reported 580,064 samples tested;
+- For calendar week 30 (which ends 26 July), 181 labs reported 572,311 samples tested;
 - For calendar week 29 (which ends 19 July), 176 labs reported 538,229 samples tested;
 - For calendar week 28 (which ends 12 July), 178 labs reported 510,103 samples tested;
 - For calendar week 27 (which ends 5 July), 149 labs reported 504,082 samples tested;
@@ -752,7 +753,7 @@
     <t xml:space="preserve">Greece - samples tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://eody.gov.gr/covid-gr-daily-report-25-08-2020/</t>
+    <t xml:space="preserve">https://eody.gov.gr/covid-gr-daily-report-27-08-2020/</t>
   </si>
   <si>
     <t xml:space="preserve">National Organization of Public Health</t>
@@ -891,7 +892,7 @@
     <t xml:space="preserve">Iran - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">http://irangov.ir/detail/345900</t>
+    <t xml:space="preserve">http://irangov.ir/detail/346050</t>
   </si>
   <si>
     <t xml:space="preserve">Government of Iran</t>
@@ -911,7 +912,7 @@
     <t xml:space="preserve">Iraq - samples tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://moh.gov.iq/index.php?name=News&amp;file=article&amp;sid=16402</t>
+    <t xml:space="preserve">https://moh.gov.iq/index.php?name=News&amp;file=article&amp;sid=16464</t>
   </si>
   <si>
     <t xml:space="preserve">Ministry of Health and Environment</t>
@@ -949,7 +950,7 @@
     <t xml:space="preserve">Israel - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://govextra.gov.il/media/25556/covid19-data-israel-19082020.csv</t>
+    <t xml:space="preserve">https://govextra.gov.il/media/25774/covid19-data-israel-20082021.csv</t>
   </si>
   <si>
     <t xml:space="preserve">Israel Ministry of Health</t>
@@ -1008,7 +1009,7 @@
     <t xml:space="preserve">Japan - people tested (incl. non-PCR)</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.mhlw.go.jp/stf/newpage_13172.html</t>
+    <t xml:space="preserve">https://www.mhlw.go.jp/stf/newpage_13239.html</t>
   </si>
   <si>
     <t xml:space="preserve">Ministry of Health, Labor and Welfare Press Release</t>
@@ -1033,10 +1034,10 @@
     <t xml:space="preserve">Japan - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.mhlw.go.jp/content/10906000/000662290.pdf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The cumulative total reported in the press release (1,619,514) does not sum to the cumulative total calculated from the weekly and daily figures reported by the MOH. See: https://www.mhlw.go.jp/content/10906000/000662290.pdf</t>
+    <t xml:space="preserve">https://www.mhlw.go.jp/content/10906000/000663894.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The cumulative total reported in the press release (1,707,901) does not sum to the cumulative total calculated from the weekly and daily figures reported by the MOH. See: https://www.mhlw.go.jp/content/10906000/000663894.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">On 11 April 2020, the MOH started providing a daily time series on the "Implementation status of PCR tests for new coronavirus in Japan (based on the date on which results were determined" (via Google translate). 
@@ -1067,7 +1068,7 @@
     <t xml:space="preserve">Kenya - samples tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/MOH_Kenya/status/1297506691454574593</t>
+    <t xml:space="preserve">https://twitter.com/MOH_Kenya/status/1298263711564488707</t>
   </si>
   <si>
     <t xml:space="preserve">Kenya Ministry of Health</t>
@@ -1089,7 +1090,7 @@
     <t xml:space="preserve">Kuwait - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/KUWAIT_MOH/status/1297858722606309378/photo/1</t>
+    <t xml:space="preserve">https://twitter.com/KUWAIT_MOH/status/1298953484306350081/photo/1</t>
   </si>
   <si>
     <t xml:space="preserve">Kuwait Ministry of Health</t>
@@ -1155,7 +1156,7 @@
     <t xml:space="preserve">Malaysia - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">http://covid-19.moh.gov.my/terkini/082020/situasi-terkini-25-ogos-2020</t>
+    <t xml:space="preserve">http://covid-19.moh.gov.my/terkini/082020/situasi-terkini-27-ogos-2020</t>
   </si>
   <si>
     <t xml:space="preserve">Ministry of Health Malaysia</t>
@@ -1181,7 +1182,7 @@
     <t xml:space="preserve">Maldives - samples tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/HPA_MV/status/1297944752265007110/photo/1</t>
+    <t xml:space="preserve">https://twitter.com/HPA_MV/status/1299028491674025989/photo/1</t>
   </si>
   <si>
     <t xml:space="preserve">Maldives Health Protection Agency</t>
@@ -1247,7 +1248,7 @@
     <t xml:space="preserve">Morocco - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/Ministere_Sante/status/1297944286143623168/photo/1</t>
+    <t xml:space="preserve">https://twitter.com/Ministere_Sante/status/1299034987212177408/photo/1</t>
   </si>
   <si>
     <t xml:space="preserve">Morocco Ministry of Health</t>
@@ -1434,7 +1435,7 @@
     <t xml:space="preserve">Panama - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/MINSAPma/status/1297671113905000448/photo/1</t>
+    <t xml:space="preserve">https://twitter.com/MINSAPma/status/1298761952492224512/photo/1</t>
   </si>
   <si>
     <t xml:space="preserve">Panama Ministry of Health</t>
@@ -1514,7 +1515,7 @@
     <t xml:space="preserve">Poland - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/MZ_GOV_PL/status/1298183333340483584</t>
+    <t xml:space="preserve">https://twitter.com/MZ_GOV_PL/status/1298908108161511426</t>
   </si>
   <si>
     <t xml:space="preserve">Poland Ministry of Health</t>
@@ -1582,7 +1583,7 @@
     <t xml:space="preserve">Romania - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://gov.ro/ro/media/comunicate/buletin-de-presa-25-august-2020-ora-13-00&amp;page=1</t>
+    <t xml:space="preserve">https://gov.ro/ro/media/comunicate/buletin-de-presa-28-august-2020-ora-13-00&amp;page=1</t>
   </si>
   <si>
     <t xml:space="preserve">Ministry of Internal Affairs</t>
@@ -1605,7 +1606,7 @@
     <t xml:space="preserve">Russia - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://rospotrebnadzor.ru/about/info/news/news_details.php?ELEMENT_ID=15238</t>
+    <t xml:space="preserve">https://rospotrebnadzor.ru/about/info/news/news_details.php?ELEMENT_ID=15255</t>
   </si>
   <si>
     <t xml:space="preserve">Government of the Russian Federation</t>
@@ -1625,7 +1626,7 @@
     <t xml:space="preserve">Rwanda - samples tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/RwandaHealth/status/1297637879523561475</t>
+    <t xml:space="preserve">https://twitter.com/RwandaHealth/status/1298361056834785284</t>
   </si>
   <si>
     <t xml:space="preserve">Rwanda Ministry of Health</t>
@@ -1799,7 +1800,7 @@
     <t xml:space="preserve">South Korea - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.cdc.go.kr/board/board.es?mid=&amp;bid=0030&amp;act=view&amp;list_no=368215&amp;tag=&amp;nPage=1</t>
+    <t xml:space="preserve">https://www.cdc.go.kr/board/board.es?mid=&amp;bid=0030&amp;act=view&amp;list_no=368248&amp;tag=&amp;nPage=1</t>
   </si>
   <si>
     <t xml:space="preserve">South Korea CDC</t>
@@ -1921,7 +1922,7 @@
     <t xml:space="preserve">Thailand - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://ddc.moph.go.th/viralpneumonia/file/situation/situation-no235-250863.pdf</t>
+    <t xml:space="preserve">https://ddc.moph.go.th/viralpneumonia/file/situation/situation-no237-270863.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">Department of Disease Control</t>
@@ -2009,7 +2010,7 @@
     <t xml:space="preserve">Uganda - samples tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/MinofHealthUG/status/1298238895956664320/photo/1</t>
+    <t xml:space="preserve">https://twitter.com/MinofHealthUG/status/1298965036740812802/photo/1</t>
   </si>
   <si>
     <t xml:space="preserve">Uganda Ministry of Health</t>
@@ -2094,28 +2095,28 @@
     <t xml:space="preserve">USA</t>
   </si>
   <si>
-    <t xml:space="preserve">United States - tests performed (CDC) (incl. non-PCR)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.cdc.gov/coronavirus/2019-ncov/cases-updates/testing-in-us.html</t>
-  </si>
-  <si>
-    <t xml:space="preserve">United States CDC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The number of tests performed. The figures are the sum across states, some of which appear to include antibody tests in addition to PCR tests.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">On 13 May 2020, the United States CDC's testing data was modified to include tests performed by commercial, hospital, public health, and CDC laboratories. This new data is available on the [Testing Data in the US](https://www.cdc.gov/coronavirus/2019-ncov/cases-updates/testing-in-us.html) page and [CDC COVID Data Tracker](https://www.cdc.gov/covid-data-tracker/index.html).
-Initially, this data was explicitly described by the CDC as only including viral tests and excluding antibody tests. As recently as [18 May](https://web.archive.org/web/20200518050707/https://www.cdc.gov/coronavirus/2019-ncov/cases-updates/testing-in-us.html) the site stated that 'These data only represent viral tests. Antibody tests are not currently captured in these data.'
-However, as of 26 May 2020, there have been a number of media reports noting that the testing figures released by some states – which are aggregated by the CDC – include antibody tests in addition to PCR tests, as discussed in [this article](https://www.theatlantic.com/health/archive/2020/05/cdc-and-states-are-misreporting-covid-19-test-data-pennsylvania-georgia-texas/611935/) in The Atlantic. 
-Within this time, the CDC have also changed the way it described the data to be ambiguous as to whether anitbody tests may be included in their figures (see [26 May 2020 update](http://web.archive.org/web/20200526082029/https://www.cdc.gov/coronavirus/2019-ncov/cases-updates/testing-in-us.html)). Our dataset aims to report only PCR tests. But because any antibody tests in the CDC data are not disaggregated, we are unable to exclude them.
-No time series is published for this new version of the data. We therefore started collecting on 13 May 2020 the cumulative total of viral tests reported, which is updated daily.
-As of [26 May 2020](http://web.archive.org/web/20200526082029/https://www.cdc.gov/coronavirus/2019-ncov/cases-updates/testing-in-us.html), the notes to the data provided by the CDC are limited. They state:
-- These data are compiled from a number of sources. Not all tests are reported to CDC.
-- The number of positive tests in a state is not equal to the number of cases, as one person may be tested more than once.
-The CDC previously published a time series that only covered public health labs and did not include private lab tests, which were occurring in significant numbers. Daily figures were provided since 18 January. This data is still visible on [this page of the CDC website](https://www.cdc.gov/coronavirus/2019-ncov/cases-updates/previous-testing-in-us.html).
-Note that, due to the way the data is presented by the official source, the time series may be impacted by retrospective revisions made by the source – see our [FAQ here](https://ourworldindata.org/coronavirus-testing#does-your-data-reflect-retrospective-updates-made-by-the-source).</t>
+    <t xml:space="preserve">United States - tests performed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://healthdata.gov/sites/default/files/covid-19_diagnostic_lab_testing_20200828_1201.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Department of Health &amp; Human Services</t>
+  </si>
+  <si>
+    <t xml:space="preserve">United States Department of Health &amp; Human Services</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://healthdata.gov/dataset/covid-19-diagnostic-laboratory-testing-pcr-testing-time-series</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The number of tests performed. The figures are the sum across states, some of which may include serology tests in addition to PCR tests.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Since August 2020, our principal time series for the United States is based on the CSV file made available by the Department of Health &amp; Human Services on HealthData.gov.
+It "includes viral COVID-19 laboratory test (PCR) results from over 1,000 U.S. laboratories and testing locations including commercial and reference laboratories, public health laboratories, hospital laboratories, and other testing locations."
+The source notes that "data presented here is representative of diagnostic specimens being tested - not individual people (...). Data presented might not represent the most current counts for the most recent 3 days due to the time it takes to report testing information. The data may also not include results from all potential testing sites within the jurisdiction (e.g., non-laboratory or point of care test sites) and therefore reflect the majority, but not all, of COVID-19 testing being conducted in the United States."
+It is also explained in the description that the data "excludes serology tests where possible", which may indicate that not 100% of the tests included in the time series are PCR tests.</t>
   </si>
   <si>
     <t xml:space="preserve">United States - units unclear (incl. non-PCR)</t>
@@ -2149,7 +2150,7 @@
     <t xml:space="preserve">Uruguay - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.gub.uy/ministerio-salud-publica/comunicacion/noticias/informe-situacion-sobre-coronavirus-covid-19-uruguay-25-agosto</t>
+    <t xml:space="preserve">https://www.gub.uy/ministerio-salud-publica/comunicacion/noticias/informe-situacion-sobre-coronavirus-covid-19-uruguay-27-agosto</t>
   </si>
   <si>
     <t xml:space="preserve">https://www.gub.uy/ministerio-salud-publica/comunicacion/noticias</t>
@@ -2187,7 +2188,7 @@
     <t xml:space="preserve">Zimbabwe - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/MoHCCZim/status/1297591437534666756</t>
+    <t xml:space="preserve">https://twitter.com/MoHCCZim/status/1298314387917340672</t>
   </si>
   <si>
     <t xml:space="preserve">Zimbabwe Ministry of Health and Child Care</t>
@@ -2661,7 +2662,7 @@
         <v>25</v>
       </c>
       <c r="C3" s="1" t="n">
-        <v>44068</v>
+        <v>44070</v>
       </c>
       <c r="D3" t="s">
         <v>26</v>
@@ -2671,31 +2672,31 @@
       </c>
       <c r="F3"/>
       <c r="G3" t="n">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="H3" t="n">
-        <v>1195148</v>
+        <v>1246917</v>
       </c>
       <c r="I3" t="n">
-        <v>26.444</v>
+        <v>27.589</v>
       </c>
       <c r="J3" t="n">
-        <v>6132</v>
+        <v>7766</v>
       </c>
       <c r="K3" t="n">
-        <v>0.136</v>
+        <v>0.172</v>
       </c>
       <c r="L3" t="n">
-        <v>14762</v>
+        <v>15536</v>
       </c>
       <c r="M3" t="n">
-        <v>0.327</v>
+        <v>0.344</v>
       </c>
       <c r="N3" t="n">
-        <v>0.545</v>
+        <v>0.591</v>
       </c>
       <c r="O3" t="n">
-        <v>1.835</v>
+        <v>1.693</v>
       </c>
       <c r="P3" t="s">
         <v>22</v>
@@ -2718,7 +2719,7 @@
         <v>30</v>
       </c>
       <c r="C4" s="1" t="n">
-        <v>44068</v>
+        <v>44070</v>
       </c>
       <c r="D4" t="s">
         <v>31</v>
@@ -2728,31 +2729,31 @@
       </c>
       <c r="F4"/>
       <c r="G4" t="n">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="H4" t="n">
-        <v>5814709</v>
+        <v>5972680</v>
       </c>
       <c r="I4" t="n">
-        <v>228.029</v>
+        <v>234.224</v>
       </c>
       <c r="J4" t="n">
-        <v>56675</v>
+        <v>86268</v>
       </c>
       <c r="K4" t="n">
-        <v>2.223</v>
+        <v>3.383</v>
       </c>
       <c r="L4" t="n">
-        <v>62014</v>
+        <v>66264</v>
       </c>
       <c r="M4" t="n">
-        <v>2.432</v>
+        <v>2.599</v>
       </c>
       <c r="N4" t="n">
         <v>0.003</v>
       </c>
       <c r="O4" t="n">
-        <v>329.611</v>
+        <v>382.713</v>
       </c>
       <c r="P4" t="s">
         <v>32</v>
@@ -2775,7 +2776,7 @@
         <v>36</v>
       </c>
       <c r="C5" s="1" t="n">
-        <v>44068</v>
+        <v>44071</v>
       </c>
       <c r="D5" t="s">
         <v>37</v>
@@ -2785,31 +2786,31 @@
       </c>
       <c r="F5"/>
       <c r="G5" t="n">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="H5" t="n">
-        <v>1110089</v>
+        <v>1147944</v>
       </c>
       <c r="I5" t="n">
-        <v>123.256</v>
+        <v>127.459</v>
       </c>
       <c r="J5" t="n">
-        <v>8883</v>
+        <v>14701</v>
       </c>
       <c r="K5" t="n">
-        <v>0.986</v>
+        <v>1.632</v>
       </c>
       <c r="L5" t="n">
-        <v>10314</v>
+        <v>10362</v>
       </c>
       <c r="M5" t="n">
-        <v>1.145</v>
+        <v>1.151</v>
       </c>
       <c r="N5" t="n">
-        <v>0.025</v>
+        <v>0.024</v>
       </c>
       <c r="O5" t="n">
-        <v>39.452</v>
+        <v>40.91</v>
       </c>
       <c r="P5" t="s">
         <v>39</v>
@@ -2832,7 +2833,7 @@
         <v>43</v>
       </c>
       <c r="C6" s="1" t="n">
-        <v>44069</v>
+        <v>44071</v>
       </c>
       <c r="D6" t="s">
         <v>44</v>
@@ -2842,28 +2843,28 @@
       </c>
       <c r="F6"/>
       <c r="G6" t="n">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="H6" t="n">
-        <v>1058509</v>
+        <v>1078767</v>
       </c>
       <c r="I6" t="n">
-        <v>622.073</v>
-      </c>
-      <c r="J6" t="n">
-        <v>9574</v>
-      </c>
-      <c r="K6" t="n">
-        <v>5.627</v>
-      </c>
+        <v>633.978</v>
+      </c>
+      <c r="J6"/>
+      <c r="K6"/>
       <c r="L6" t="n">
-        <v>8246</v>
+        <v>9566</v>
       </c>
       <c r="M6" t="n">
-        <v>4.846</v>
-      </c>
-      <c r="N6"/>
-      <c r="O6"/>
+        <v>5.622</v>
+      </c>
+      <c r="N6" t="n">
+        <v>0.042</v>
+      </c>
+      <c r="O6" t="n">
+        <v>23.864</v>
+      </c>
       <c r="P6" t="s">
         <v>46</v>
       </c>
@@ -2885,7 +2886,7 @@
         <v>50</v>
       </c>
       <c r="C7" s="1" t="n">
-        <v>44066</v>
+        <v>44069</v>
       </c>
       <c r="D7" t="s">
         <v>51</v>
@@ -2895,31 +2896,31 @@
       </c>
       <c r="F7"/>
       <c r="G7" t="n">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="H7" t="n">
-        <v>1442656</v>
+        <v>1485261</v>
       </c>
       <c r="I7" t="n">
-        <v>8.76</v>
+        <v>9.019</v>
       </c>
       <c r="J7" t="n">
-        <v>10801</v>
+        <v>15070</v>
       </c>
       <c r="K7" t="n">
-        <v>0.066</v>
+        <v>0.092</v>
       </c>
       <c r="L7" t="n">
-        <v>12999</v>
+        <v>13109</v>
       </c>
       <c r="M7" t="n">
-        <v>0.079</v>
+        <v>0.08</v>
       </c>
       <c r="N7" t="n">
-        <v>0.199</v>
+        <v>0.188</v>
       </c>
       <c r="O7" t="n">
-        <v>5.027</v>
+        <v>5.309</v>
       </c>
       <c r="P7" t="s">
         <v>52</v>
@@ -2942,7 +2943,7 @@
         <v>57</v>
       </c>
       <c r="C8" s="1" t="n">
-        <v>44068</v>
+        <v>44070</v>
       </c>
       <c r="D8" t="s">
         <v>58</v>
@@ -2952,27 +2953,27 @@
       </c>
       <c r="F8"/>
       <c r="G8" t="n">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="H8" t="n">
-        <v>1480047</v>
+        <v>1497421</v>
       </c>
       <c r="I8" t="n">
-        <v>156.63</v>
+        <v>158.469</v>
       </c>
       <c r="J8"/>
       <c r="K8"/>
       <c r="L8" t="n">
-        <v>6729</v>
+        <v>6882</v>
       </c>
       <c r="M8" t="n">
-        <v>0.712</v>
+        <v>0.728</v>
       </c>
       <c r="N8" t="n">
-        <v>0.022</v>
+        <v>0.024</v>
       </c>
       <c r="O8" t="n">
-        <v>44.605</v>
+        <v>41.069</v>
       </c>
       <c r="P8" t="s">
         <v>59</v>
@@ -2995,7 +2996,7 @@
         <v>63</v>
       </c>
       <c r="C9" s="1" t="n">
-        <v>44067</v>
+        <v>44069</v>
       </c>
       <c r="D9" t="s">
         <v>64</v>
@@ -3005,31 +3006,31 @@
       </c>
       <c r="F9"/>
       <c r="G9" t="n">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="H9" t="n">
-        <v>2162146</v>
+        <v>2211141</v>
       </c>
       <c r="I9" t="n">
-        <v>186.559</v>
+        <v>190.786</v>
       </c>
       <c r="J9" t="n">
-        <v>14342</v>
+        <v>20336</v>
       </c>
       <c r="K9" t="n">
-        <v>1.237</v>
+        <v>1.755</v>
       </c>
       <c r="L9" t="n">
-        <v>19016</v>
+        <v>18908</v>
       </c>
       <c r="M9" t="n">
-        <v>1.641</v>
+        <v>1.631</v>
       </c>
       <c r="N9" t="n">
-        <v>0.024</v>
+        <v>0.023</v>
       </c>
       <c r="O9" t="n">
-        <v>41.925</v>
+        <v>43.899</v>
       </c>
       <c r="P9" t="s">
         <v>65</v>
@@ -3052,7 +3053,7 @@
         <v>69</v>
       </c>
       <c r="C10" s="1" t="n">
-        <v>44066</v>
+        <v>44069</v>
       </c>
       <c r="D10" t="s">
         <v>70</v>
@@ -3062,31 +3063,31 @@
       </c>
       <c r="F10"/>
       <c r="G10" t="n">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="H10" t="n">
-        <v>218864</v>
+        <v>225474</v>
       </c>
       <c r="I10" t="n">
-        <v>18.75</v>
+        <v>19.316</v>
       </c>
       <c r="J10" t="n">
-        <v>2385</v>
+        <v>2274</v>
       </c>
       <c r="K10" t="n">
-        <v>0.204</v>
+        <v>0.195</v>
       </c>
       <c r="L10" t="n">
-        <v>2881</v>
+        <v>2405</v>
       </c>
       <c r="M10" t="n">
-        <v>0.247</v>
+        <v>0.206</v>
       </c>
       <c r="N10" t="n">
-        <v>0.46</v>
+        <v>0.474</v>
       </c>
       <c r="O10" t="n">
-        <v>2.173</v>
+        <v>2.11</v>
       </c>
       <c r="P10" t="s">
         <v>45</v>
@@ -3109,7 +3110,7 @@
         <v>74</v>
       </c>
       <c r="C11" s="1" t="n">
-        <v>44058</v>
+        <v>44065</v>
       </c>
       <c r="D11" t="s">
         <v>75</v>
@@ -3121,21 +3122,21 @@
         <v>76</v>
       </c>
       <c r="G11" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H11" t="n">
-        <v>4152652</v>
+        <v>4797948</v>
       </c>
       <c r="I11" t="n">
-        <v>19.536</v>
+        <v>22.572</v>
       </c>
       <c r="J11"/>
       <c r="K11"/>
       <c r="L11" t="n">
-        <v>48904</v>
+        <v>92185</v>
       </c>
       <c r="M11" t="n">
-        <v>0.23</v>
+        <v>0.434</v>
       </c>
       <c r="N11"/>
       <c r="O11"/>
@@ -3160,7 +3161,7 @@
         <v>81</v>
       </c>
       <c r="C12" s="1" t="n">
-        <v>44069</v>
+        <v>44071</v>
       </c>
       <c r="D12" t="s">
         <v>82</v>
@@ -3170,28 +3171,28 @@
       </c>
       <c r="F12"/>
       <c r="G12" t="n">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="H12" t="n">
-        <v>380606</v>
+        <v>392089</v>
       </c>
       <c r="I12" t="n">
-        <v>54.776</v>
-      </c>
-      <c r="J12" t="n">
-        <v>6232</v>
-      </c>
-      <c r="K12" t="n">
-        <v>0.897</v>
-      </c>
+        <v>56.428</v>
+      </c>
+      <c r="J12"/>
+      <c r="K12"/>
       <c r="L12" t="n">
-        <v>5339</v>
+        <v>4767</v>
       </c>
       <c r="M12" t="n">
-        <v>0.768</v>
-      </c>
-      <c r="N12"/>
-      <c r="O12"/>
+        <v>0.686</v>
+      </c>
+      <c r="N12" t="n">
+        <v>0.033</v>
+      </c>
+      <c r="O12" t="n">
+        <v>30.67</v>
+      </c>
       <c r="P12" t="s">
         <v>84</v>
       </c>
@@ -3213,7 +3214,7 @@
         <v>87</v>
       </c>
       <c r="C13" s="1" t="n">
-        <v>44069</v>
+        <v>44071</v>
       </c>
       <c r="D13" t="s">
         <v>88</v>
@@ -3223,28 +3224,32 @@
       </c>
       <c r="F13"/>
       <c r="G13" t="n">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="H13" t="n">
-        <v>5205010</v>
+        <v>5293936</v>
       </c>
       <c r="I13" t="n">
-        <v>137.91</v>
+        <v>140.266</v>
       </c>
       <c r="J13" t="n">
-        <v>35844</v>
+        <v>47671</v>
       </c>
       <c r="K13" t="n">
-        <v>0.95</v>
+        <v>1.263</v>
       </c>
       <c r="L13" t="n">
-        <v>46405</v>
+        <v>45674</v>
       </c>
       <c r="M13" t="n">
-        <v>1.23</v>
-      </c>
-      <c r="N13"/>
-      <c r="O13"/>
+        <v>1.21</v>
+      </c>
+      <c r="N13" t="n">
+        <v>0.009</v>
+      </c>
+      <c r="O13" t="n">
+        <v>107.468</v>
+      </c>
       <c r="P13" t="s">
         <v>89</v>
       </c>
@@ -3266,7 +3271,7 @@
         <v>92</v>
       </c>
       <c r="C14" s="1" t="n">
-        <v>44068</v>
+        <v>44070</v>
       </c>
       <c r="D14" t="s">
         <v>93</v>
@@ -3278,31 +3283,31 @@
         <v>94</v>
       </c>
       <c r="G14" t="n">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="H14" t="n">
-        <v>2255966</v>
+        <v>2303242</v>
       </c>
       <c r="I14" t="n">
-        <v>118.013</v>
+        <v>120.486</v>
       </c>
       <c r="J14" t="n">
-        <v>24503</v>
+        <v>27019</v>
       </c>
       <c r="K14" t="n">
-        <v>1.282</v>
+        <v>1.413</v>
       </c>
       <c r="L14" t="n">
-        <v>26841</v>
+        <v>27087</v>
       </c>
       <c r="M14" t="n">
-        <v>1.404</v>
+        <v>1.417</v>
       </c>
       <c r="N14" t="n">
-        <v>0.064</v>
+        <v>0.065</v>
       </c>
       <c r="O14" t="n">
-        <v>15.572</v>
+        <v>15.38</v>
       </c>
       <c r="P14" t="s">
         <v>95</v>
@@ -3325,7 +3330,7 @@
         <v>99</v>
       </c>
       <c r="C15" s="1" t="n">
-        <v>44068</v>
+        <v>44070</v>
       </c>
       <c r="D15" t="s">
         <v>100</v>
@@ -3335,31 +3340,31 @@
       </c>
       <c r="F15"/>
       <c r="G15" t="n">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="H15" t="n">
-        <v>2458866</v>
+        <v>2519489</v>
       </c>
       <c r="I15" t="n">
-        <v>48.324</v>
+        <v>49.515</v>
       </c>
       <c r="J15" t="n">
-        <v>30925</v>
+        <v>30059</v>
       </c>
       <c r="K15" t="n">
-        <v>0.608</v>
+        <v>0.591</v>
       </c>
       <c r="L15" t="n">
-        <v>30324</v>
+        <v>30006</v>
       </c>
       <c r="M15" t="n">
-        <v>0.596</v>
+        <v>0.59</v>
       </c>
       <c r="N15" t="n">
-        <v>0.353</v>
+        <v>0.334</v>
       </c>
       <c r="O15" t="n">
-        <v>2.829</v>
+        <v>2.997</v>
       </c>
       <c r="P15" t="s">
         <v>101</v>
@@ -3382,7 +3387,7 @@
         <v>105</v>
       </c>
       <c r="C16" s="1" t="n">
-        <v>44067</v>
+        <v>44068</v>
       </c>
       <c r="D16" t="s">
         <v>106</v>
@@ -3392,25 +3397,25 @@
       </c>
       <c r="F16"/>
       <c r="G16" t="n">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="H16" t="n">
-        <v>117997</v>
+        <v>119301</v>
       </c>
       <c r="I16" t="n">
-        <v>23.163</v>
+        <v>23.419</v>
       </c>
       <c r="J16" t="n">
-        <v>1533</v>
+        <v>1304</v>
       </c>
       <c r="K16" t="n">
-        <v>0.301</v>
+        <v>0.256</v>
       </c>
       <c r="L16" t="n">
-        <v>1626</v>
+        <v>1661</v>
       </c>
       <c r="M16" t="n">
-        <v>0.319</v>
+        <v>0.326</v>
       </c>
       <c r="N16"/>
       <c r="O16"/>
@@ -3435,7 +3440,7 @@
         <v>111</v>
       </c>
       <c r="C17" s="1" t="n">
-        <v>44067</v>
+        <v>44069</v>
       </c>
       <c r="D17" t="s">
         <v>112</v>
@@ -3445,31 +3450,31 @@
       </c>
       <c r="F17"/>
       <c r="G17" t="n">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="H17" t="n">
-        <v>121286</v>
+        <v>122975</v>
       </c>
       <c r="I17" t="n">
-        <v>4.598</v>
+        <v>4.662</v>
       </c>
       <c r="J17" t="n">
-        <v>987</v>
+        <v>896</v>
       </c>
       <c r="K17" t="n">
-        <v>0.037</v>
+        <v>0.034</v>
       </c>
       <c r="L17" t="n">
-        <v>981</v>
+        <v>884</v>
       </c>
       <c r="M17" t="n">
-        <v>0.037</v>
+        <v>0.034</v>
       </c>
       <c r="N17" t="n">
-        <v>0.065</v>
+        <v>0.067</v>
       </c>
       <c r="O17" t="n">
-        <v>15.431</v>
+        <v>15.019</v>
       </c>
       <c r="P17" t="s">
         <v>113</v>
@@ -3492,7 +3497,7 @@
         <v>117</v>
       </c>
       <c r="C18" s="1" t="n">
-        <v>44068</v>
+        <v>44071</v>
       </c>
       <c r="D18" t="s">
         <v>118</v>
@@ -3502,31 +3507,31 @@
       </c>
       <c r="F18"/>
       <c r="G18" t="n">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="H18" t="n">
-        <v>154159</v>
+        <v>162301</v>
       </c>
       <c r="I18" t="n">
-        <v>37.552</v>
+        <v>39.535</v>
       </c>
       <c r="J18" t="n">
-        <v>1335</v>
+        <v>2065</v>
       </c>
       <c r="K18" t="n">
-        <v>0.325</v>
+        <v>0.503</v>
       </c>
       <c r="L18" t="n">
-        <v>1955</v>
+        <v>2305</v>
       </c>
       <c r="M18" t="n">
-        <v>0.476</v>
+        <v>0.561</v>
       </c>
       <c r="N18" t="n">
-        <v>0.121</v>
+        <v>0.115</v>
       </c>
       <c r="O18" t="n">
-        <v>8.269</v>
+        <v>8.661</v>
       </c>
       <c r="P18" t="s">
         <v>119</v>
@@ -3549,7 +3554,7 @@
         <v>123</v>
       </c>
       <c r="C19" s="1" t="n">
-        <v>44067</v>
+        <v>44069</v>
       </c>
       <c r="D19" t="s">
         <v>124</v>
@@ -3561,31 +3566,31 @@
         <v>126</v>
       </c>
       <c r="G19" t="n">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="H19" t="n">
-        <v>369889</v>
+        <v>377494</v>
       </c>
       <c r="I19" t="n">
-        <v>32.657</v>
+        <v>33.328</v>
       </c>
       <c r="J19" t="n">
-        <v>4536</v>
+        <v>4549</v>
       </c>
       <c r="K19" t="n">
-        <v>0.4</v>
+        <v>0.402</v>
       </c>
       <c r="L19" t="n">
-        <v>4794</v>
+        <v>4436</v>
       </c>
       <c r="M19" t="n">
-        <v>0.423</v>
+        <v>0.392</v>
       </c>
       <c r="N19" t="n">
         <v>0.011</v>
       </c>
       <c r="O19" t="n">
-        <v>91.689</v>
+        <v>92.417</v>
       </c>
       <c r="P19" t="s">
         <v>125</v>
@@ -3608,7 +3613,7 @@
         <v>130</v>
       </c>
       <c r="C20" s="1" t="n">
-        <v>44067</v>
+        <v>44069</v>
       </c>
       <c r="D20" t="s">
         <v>131</v>
@@ -3618,31 +3623,31 @@
       </c>
       <c r="F20"/>
       <c r="G20" t="n">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="H20" t="n">
-        <v>852414</v>
+        <v>871133</v>
       </c>
       <c r="I20" t="n">
-        <v>79.598</v>
+        <v>81.346</v>
       </c>
       <c r="J20" t="n">
-        <v>6835</v>
+        <v>8615</v>
       </c>
       <c r="K20" t="n">
-        <v>0.638</v>
+        <v>0.804</v>
       </c>
       <c r="L20" t="n">
-        <v>6600</v>
+        <v>7069</v>
       </c>
       <c r="M20" t="n">
-        <v>0.616</v>
+        <v>0.66</v>
       </c>
       <c r="N20" t="n">
-        <v>0.041</v>
+        <v>0.042</v>
       </c>
       <c r="O20" t="n">
-        <v>24.176</v>
+        <v>23.963</v>
       </c>
       <c r="P20" t="s">
         <v>45</v>
@@ -3665,7 +3670,7 @@
         <v>135</v>
       </c>
       <c r="C21" s="1" t="n">
-        <v>44065</v>
+        <v>44069</v>
       </c>
       <c r="D21" t="s">
         <v>136</v>
@@ -3675,27 +3680,27 @@
       </c>
       <c r="F21"/>
       <c r="G21" t="n">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="H21"/>
       <c r="I21"/>
       <c r="J21" t="n">
-        <v>422</v>
+        <v>148</v>
       </c>
       <c r="K21" t="n">
-        <v>0.005</v>
+        <v>0.002</v>
       </c>
       <c r="L21" t="n">
-        <v>317</v>
+        <v>241</v>
       </c>
       <c r="M21" t="n">
-        <v>0.004</v>
+        <v>0.003</v>
       </c>
       <c r="N21" t="n">
-        <v>0.089</v>
+        <v>0.101</v>
       </c>
       <c r="O21" t="n">
-        <v>11.264</v>
+        <v>9.924</v>
       </c>
       <c r="P21" t="s">
         <v>137</v>
@@ -3718,7 +3723,7 @@
         <v>141</v>
       </c>
       <c r="C22" s="1" t="n">
-        <v>44067</v>
+        <v>44070</v>
       </c>
       <c r="D22" t="s">
         <v>142</v>
@@ -3728,31 +3733,31 @@
       </c>
       <c r="F22"/>
       <c r="G22" t="n">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="H22" t="n">
-        <v>2201733</v>
+        <v>2315324</v>
       </c>
       <c r="I22" t="n">
-        <v>380.12</v>
+        <v>399.731</v>
       </c>
       <c r="J22" t="n">
-        <v>7862</v>
+        <v>6042</v>
       </c>
       <c r="K22" t="n">
-        <v>1.357</v>
+        <v>1.043</v>
       </c>
       <c r="L22" t="n">
-        <v>29920</v>
+        <v>29715</v>
       </c>
       <c r="M22" t="n">
-        <v>5.166</v>
+        <v>5.13</v>
       </c>
       <c r="N22" t="n">
-        <v>0.002</v>
+        <v>0.003</v>
       </c>
       <c r="O22" t="n">
-        <v>410.667</v>
+        <v>348.417</v>
       </c>
       <c r="P22" t="s">
         <v>143</v>
@@ -3775,7 +3780,7 @@
         <v>147</v>
       </c>
       <c r="C23" s="1" t="n">
-        <v>44068</v>
+        <v>44070</v>
       </c>
       <c r="D23" t="s">
         <v>148</v>
@@ -3787,25 +3792,25 @@
         <v>150</v>
       </c>
       <c r="G23" t="n">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="H23" t="n">
-        <v>245983</v>
+        <v>251532</v>
       </c>
       <c r="I23" t="n">
-        <v>13.942</v>
+        <v>14.257</v>
       </c>
       <c r="J23" t="n">
-        <v>2546</v>
+        <v>2080</v>
       </c>
       <c r="K23" t="n">
-        <v>0.144</v>
+        <v>0.118</v>
       </c>
       <c r="L23" t="n">
-        <v>2564</v>
+        <v>2304</v>
       </c>
       <c r="M23" t="n">
-        <v>0.145</v>
+        <v>0.131</v>
       </c>
       <c r="N23"/>
       <c r="O23"/>
@@ -3830,7 +3835,7 @@
         <v>154</v>
       </c>
       <c r="C24" s="1" t="n">
-        <v>44065</v>
+        <v>44068</v>
       </c>
       <c r="D24" t="s">
         <v>155</v>
@@ -3840,31 +3845,31 @@
       </c>
       <c r="F24"/>
       <c r="G24" t="n">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="H24" t="n">
-        <v>295665</v>
+        <v>303031</v>
       </c>
       <c r="I24" t="n">
-        <v>45.584</v>
+        <v>46.719</v>
       </c>
       <c r="J24" t="n">
-        <v>2447</v>
+        <v>2497</v>
       </c>
       <c r="K24" t="n">
+        <v>0.385</v>
+      </c>
+      <c r="L24" t="n">
+        <v>2448</v>
+      </c>
+      <c r="M24" t="n">
         <v>0.377</v>
       </c>
-      <c r="L24" t="n">
-        <v>2460</v>
-      </c>
-      <c r="M24" t="n">
-        <v>0.379</v>
-      </c>
       <c r="N24" t="n">
-        <v>0.122</v>
+        <v>0.094</v>
       </c>
       <c r="O24" t="n">
-        <v>8.177</v>
+        <v>10.591</v>
       </c>
       <c r="P24" t="s">
         <v>156</v>
@@ -3887,7 +3892,7 @@
         <v>160</v>
       </c>
       <c r="C25" s="1" t="n">
-        <v>44067</v>
+        <v>44070</v>
       </c>
       <c r="D25" t="s">
         <v>161</v>
@@ -3897,31 +3902,31 @@
       </c>
       <c r="F25"/>
       <c r="G25" t="n">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="H25" t="n">
-        <v>142160</v>
+        <v>146128</v>
       </c>
       <c r="I25" t="n">
-        <v>107.166</v>
+        <v>110.157</v>
       </c>
       <c r="J25" t="n">
-        <v>1186</v>
+        <v>1271</v>
       </c>
       <c r="K25" t="n">
-        <v>0.894</v>
+        <v>0.958</v>
       </c>
       <c r="L25" t="n">
-        <v>863</v>
+        <v>1011</v>
       </c>
       <c r="M25" t="n">
-        <v>0.651</v>
+        <v>0.762</v>
       </c>
       <c r="N25" t="n">
-        <v>0.014</v>
+        <v>0.015</v>
       </c>
       <c r="O25" t="n">
-        <v>73.671</v>
+        <v>68.048</v>
       </c>
       <c r="P25" t="s">
         <v>163</v>
@@ -3944,7 +3949,7 @@
         <v>168</v>
       </c>
       <c r="C26" s="1" t="n">
-        <v>44066</v>
+        <v>44069</v>
       </c>
       <c r="D26" t="s">
         <v>169</v>
@@ -3954,31 +3959,31 @@
       </c>
       <c r="F26"/>
       <c r="G26" t="n">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="H26" t="n">
-        <v>757057</v>
+        <v>813410</v>
       </c>
       <c r="I26" t="n">
-        <v>6.585</v>
+        <v>7.075</v>
       </c>
       <c r="J26" t="n">
-        <v>20153</v>
+        <v>18724</v>
       </c>
       <c r="K26" t="n">
+        <v>0.163</v>
+      </c>
+      <c r="L26" t="n">
+        <v>20110</v>
+      </c>
+      <c r="M26" t="n">
         <v>0.175</v>
       </c>
-      <c r="L26" t="n">
-        <v>21085</v>
-      </c>
-      <c r="M26" t="n">
-        <v>0.183</v>
-      </c>
       <c r="N26" t="n">
-        <v>0.069</v>
+        <v>0.078</v>
       </c>
       <c r="O26" t="n">
-        <v>14.557</v>
+        <v>12.837</v>
       </c>
       <c r="P26" t="s">
         <v>170</v>
@@ -4058,7 +4063,7 @@
         <v>179</v>
       </c>
       <c r="C28" s="1" t="n">
-        <v>44066</v>
+        <v>44069</v>
       </c>
       <c r="D28" t="s">
         <v>180</v>
@@ -4068,31 +4073,31 @@
       </c>
       <c r="F28"/>
       <c r="G28" t="n">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="H28" t="n">
-        <v>571675</v>
+        <v>615008</v>
       </c>
       <c r="I28" t="n">
-        <v>103.177</v>
+        <v>110.998</v>
       </c>
       <c r="J28" t="n">
-        <v>6146</v>
+        <v>9513</v>
       </c>
       <c r="K28" t="n">
-        <v>1.109</v>
+        <v>1.717</v>
       </c>
       <c r="L28" t="n">
-        <v>10338</v>
+        <v>11373</v>
       </c>
       <c r="M28" t="n">
-        <v>1.866</v>
+        <v>2.053</v>
       </c>
       <c r="N28" t="n">
-        <v>0.002</v>
+        <v>0.003</v>
       </c>
       <c r="O28" t="n">
-        <v>479.245</v>
+        <v>388.346</v>
       </c>
       <c r="P28" t="s">
         <v>182</v>
@@ -4115,7 +4120,7 @@
         <v>185</v>
       </c>
       <c r="C29" s="1" t="n">
-        <v>44064</v>
+        <v>44067</v>
       </c>
       <c r="D29" t="s">
         <v>186</v>
@@ -4125,27 +4130,27 @@
       </c>
       <c r="F29"/>
       <c r="G29" t="n">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="H29"/>
       <c r="I29"/>
       <c r="J29" t="n">
-        <v>127561</v>
+        <v>143755</v>
       </c>
       <c r="K29" t="n">
-        <v>1.954</v>
+        <v>2.202</v>
       </c>
       <c r="L29" t="n">
-        <v>97097</v>
+        <v>106496</v>
       </c>
       <c r="M29" t="n">
-        <v>1.488</v>
+        <v>1.632</v>
       </c>
       <c r="N29" t="n">
-        <v>0.03</v>
+        <v>0.033</v>
       </c>
       <c r="O29" t="n">
-        <v>33.238</v>
+        <v>30.599</v>
       </c>
       <c r="P29" t="s">
         <v>187</v>
@@ -4223,7 +4228,7 @@
         <v>195</v>
       </c>
       <c r="C31" s="1" t="n">
-        <v>44059</v>
+        <v>44066</v>
       </c>
       <c r="D31" t="s">
         <v>196</v>
@@ -4235,27 +4240,27 @@
         <v>198</v>
       </c>
       <c r="G31" t="n">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H31" t="n">
-        <v>10197366</v>
+        <v>11208091</v>
       </c>
       <c r="I31" t="n">
-        <v>121.71</v>
+        <v>133.774</v>
       </c>
       <c r="J31"/>
       <c r="K31"/>
       <c r="L31" t="n">
-        <v>125075</v>
+        <v>141060</v>
       </c>
       <c r="M31" t="n">
-        <v>1.493</v>
+        <v>1.684</v>
       </c>
       <c r="N31" t="n">
         <v>0.009</v>
       </c>
       <c r="O31" t="n">
-        <v>115.08</v>
+        <v>114.404</v>
       </c>
       <c r="P31" t="s">
         <v>197</v>
@@ -4278,7 +4283,7 @@
         <v>203</v>
       </c>
       <c r="C32" s="1" t="n">
-        <v>44064</v>
+        <v>44067</v>
       </c>
       <c r="D32" t="s">
         <v>204</v>
@@ -4288,31 +4293,31 @@
       </c>
       <c r="F32"/>
       <c r="G32" t="n">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="H32" t="n">
-        <v>435109</v>
+        <v>437750</v>
       </c>
       <c r="I32" t="n">
-        <v>14.003</v>
+        <v>14.088</v>
       </c>
       <c r="J32" t="n">
-        <v>1606</v>
+        <v>749</v>
       </c>
       <c r="K32" t="n">
-        <v>0.052</v>
+        <v>0.024</v>
       </c>
       <c r="L32" t="n">
-        <v>1306</v>
+        <v>1140</v>
       </c>
       <c r="M32" t="n">
-        <v>0.042</v>
+        <v>0.037</v>
       </c>
       <c r="N32" t="n">
-        <v>0.155</v>
+        <v>0.122</v>
       </c>
       <c r="O32" t="n">
-        <v>6.47</v>
+        <v>8.201</v>
       </c>
       <c r="P32" t="s">
         <v>206</v>
@@ -4335,7 +4340,7 @@
         <v>210</v>
       </c>
       <c r="C33" s="1" t="n">
-        <v>44068</v>
+        <v>44070</v>
       </c>
       <c r="D33" t="s">
         <v>211</v>
@@ -4345,31 +4350,27 @@
       </c>
       <c r="F33"/>
       <c r="G33" t="n">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="H33" t="n">
-        <v>872550</v>
+        <v>903432</v>
       </c>
       <c r="I33" t="n">
-        <v>83.713</v>
-      </c>
-      <c r="J33" t="n">
-        <v>14412</v>
-      </c>
-      <c r="K33" t="n">
-        <v>1.383</v>
-      </c>
+        <v>86.676</v>
+      </c>
+      <c r="J33"/>
+      <c r="K33"/>
       <c r="L33" t="n">
-        <v>18811</v>
+        <v>12426</v>
       </c>
       <c r="M33" t="n">
-        <v>1.805</v>
+        <v>1.192</v>
       </c>
       <c r="N33" t="n">
-        <v>0.012</v>
+        <v>0.018</v>
       </c>
       <c r="O33" t="n">
-        <v>82.453</v>
+        <v>54.5</v>
       </c>
       <c r="P33" t="s">
         <v>213</v>
@@ -4441,7 +4442,7 @@
         <v>224</v>
       </c>
       <c r="C35" s="1" t="n">
-        <v>44067</v>
+        <v>44071</v>
       </c>
       <c r="D35" t="s">
         <v>225</v>
@@ -4453,31 +4454,31 @@
         <v>227</v>
       </c>
       <c r="G35" t="n">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="H35" t="n">
-        <v>398550</v>
+        <v>414645</v>
       </c>
       <c r="I35" t="n">
-        <v>41.256</v>
+        <v>42.922</v>
       </c>
       <c r="J35" t="n">
-        <v>1458</v>
+        <v>5846</v>
       </c>
       <c r="K35" t="n">
-        <v>0.151</v>
+        <v>0.605</v>
       </c>
       <c r="L35" t="n">
-        <v>2517</v>
+        <v>3031</v>
       </c>
       <c r="M35" t="n">
-        <v>0.261</v>
+        <v>0.314</v>
       </c>
       <c r="N35" t="n">
-        <v>0.014</v>
+        <v>0.016</v>
       </c>
       <c r="O35" t="n">
-        <v>73.72</v>
+        <v>63.715</v>
       </c>
       <c r="P35" t="s">
         <v>226</v>
@@ -4500,7 +4501,7 @@
         <v>232</v>
       </c>
       <c r="C36" s="1" t="n">
-        <v>44067</v>
+        <v>44070</v>
       </c>
       <c r="D36" t="s">
         <v>233</v>
@@ -4510,31 +4511,31 @@
       </c>
       <c r="F36"/>
       <c r="G36" t="n">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="H36" t="n">
-        <v>85805</v>
+        <v>88166</v>
       </c>
       <c r="I36" t="n">
-        <v>251.443</v>
+        <v>258.362</v>
       </c>
       <c r="J36" t="n">
-        <v>602</v>
+        <v>723</v>
       </c>
       <c r="K36" t="n">
-        <v>1.764</v>
+        <v>2.119</v>
       </c>
       <c r="L36" t="n">
-        <v>472</v>
+        <v>588</v>
       </c>
       <c r="M36" t="n">
-        <v>1.383</v>
+        <v>1.723</v>
       </c>
       <c r="N36" t="n">
-        <v>0.016</v>
+        <v>0.011</v>
       </c>
       <c r="O36" t="n">
-        <v>62.34</v>
+        <v>87.574</v>
       </c>
       <c r="P36" t="s">
         <v>234</v>
@@ -4616,7 +4617,7 @@
         <v>242</v>
       </c>
       <c r="C38" s="1" t="n">
-        <v>44067</v>
+        <v>44070</v>
       </c>
       <c r="D38" t="s">
         <v>238</v>
@@ -4628,27 +4629,31 @@
         <v>240</v>
       </c>
       <c r="G38" t="n">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="H38" t="n">
-        <v>36827520</v>
+        <v>39477848</v>
       </c>
       <c r="I38" t="n">
-        <v>26.687</v>
-      </c>
-      <c r="J38"/>
-      <c r="K38"/>
+        <v>28.607</v>
+      </c>
+      <c r="J38" t="n">
+        <v>901338</v>
+      </c>
+      <c r="K38" t="n">
+        <v>0.653</v>
+      </c>
       <c r="L38" t="n">
-        <v>840894</v>
+        <v>858659</v>
       </c>
       <c r="M38" t="n">
-        <v>0.609</v>
+        <v>0.622</v>
       </c>
       <c r="N38" t="n">
-        <v>0.078</v>
+        <v>0.079</v>
       </c>
       <c r="O38" t="n">
-        <v>12.833</v>
+        <v>12.699</v>
       </c>
       <c r="P38" t="s">
         <v>239</v>
@@ -4671,7 +4676,7 @@
         <v>244</v>
       </c>
       <c r="C39" s="1" t="n">
-        <v>44068</v>
+        <v>44071</v>
       </c>
       <c r="D39" t="s">
         <v>245</v>
@@ -4681,27 +4686,31 @@
       </c>
       <c r="F39"/>
       <c r="G39" t="n">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="H39" t="n">
-        <v>1191948</v>
+        <v>1233486</v>
       </c>
       <c r="I39" t="n">
-        <v>4.358</v>
-      </c>
-      <c r="J39"/>
-      <c r="K39"/>
+        <v>4.51</v>
+      </c>
+      <c r="J39" t="n">
+        <v>21018</v>
+      </c>
+      <c r="K39" t="n">
+        <v>0.077</v>
+      </c>
       <c r="L39" t="n">
-        <v>15799</v>
+        <v>15044</v>
       </c>
       <c r="M39" t="n">
-        <v>0.058</v>
+        <v>0.055</v>
       </c>
       <c r="N39" t="n">
-        <v>0.127</v>
+        <v>0.149</v>
       </c>
       <c r="O39" t="n">
-        <v>7.876</v>
+        <v>6.719</v>
       </c>
       <c r="P39" t="s">
         <v>246</v>
@@ -4724,7 +4733,7 @@
         <v>250</v>
       </c>
       <c r="C40" s="1" t="n">
-        <v>44068</v>
+        <v>44070</v>
       </c>
       <c r="D40" t="s">
         <v>251</v>
@@ -4734,31 +4743,31 @@
       </c>
       <c r="F40"/>
       <c r="G40" t="n">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="H40" t="n">
-        <v>3088313</v>
+        <v>3138782</v>
       </c>
       <c r="I40" t="n">
-        <v>36.769</v>
+        <v>37.37</v>
       </c>
       <c r="J40" t="n">
-        <v>25891</v>
+        <v>24976</v>
       </c>
       <c r="K40" t="n">
-        <v>0.308</v>
+        <v>0.297</v>
       </c>
       <c r="L40" t="n">
-        <v>24895</v>
+        <v>25006</v>
       </c>
       <c r="M40" t="n">
-        <v>0.296</v>
+        <v>0.298</v>
       </c>
       <c r="N40" t="n">
-        <v>0.077</v>
+        <v>0.089</v>
       </c>
       <c r="O40" t="n">
-        <v>12.952</v>
+        <v>11.273</v>
       </c>
       <c r="P40" t="s">
         <v>252</v>
@@ -4781,7 +4790,7 @@
         <v>256</v>
       </c>
       <c r="C41" s="1" t="n">
-        <v>44066</v>
+        <v>44069</v>
       </c>
       <c r="D41" t="s">
         <v>257</v>
@@ -4791,31 +4800,31 @@
       </c>
       <c r="F41"/>
       <c r="G41" t="n">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="H41" t="n">
-        <v>1433626</v>
+        <v>1502546</v>
       </c>
       <c r="I41" t="n">
-        <v>35.642</v>
+        <v>37.356</v>
       </c>
       <c r="J41" t="n">
-        <v>19679</v>
+        <v>20359</v>
       </c>
       <c r="K41" t="n">
-        <v>0.489</v>
+        <v>0.506</v>
       </c>
       <c r="L41" t="n">
-        <v>21528</v>
+        <v>22441</v>
       </c>
       <c r="M41" t="n">
-        <v>0.535</v>
+        <v>0.558</v>
       </c>
       <c r="N41" t="n">
-        <v>0.189</v>
+        <v>0.173</v>
       </c>
       <c r="O41" t="n">
-        <v>5.294</v>
+        <v>5.767</v>
       </c>
       <c r="P41" t="s">
         <v>259</v>
@@ -4838,7 +4847,7 @@
         <v>263</v>
       </c>
       <c r="C42" s="1" t="n">
-        <v>44068</v>
+        <v>44070</v>
       </c>
       <c r="D42" t="s">
         <v>264</v>
@@ -4848,31 +4857,31 @@
       </c>
       <c r="F42"/>
       <c r="G42" t="n">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="H42" t="n">
-        <v>782633</v>
+        <v>802572</v>
       </c>
       <c r="I42" t="n">
-        <v>158.498</v>
+        <v>162.536</v>
       </c>
       <c r="J42" t="n">
-        <v>4998</v>
+        <v>12274</v>
       </c>
       <c r="K42" t="n">
-        <v>1.012</v>
+        <v>2.486</v>
       </c>
       <c r="L42" t="n">
-        <v>7531</v>
+        <v>7864</v>
       </c>
       <c r="M42" t="n">
-        <v>1.525</v>
+        <v>1.593</v>
       </c>
       <c r="N42" t="n">
         <v>0.015</v>
       </c>
       <c r="O42" t="n">
-        <v>65.65</v>
+        <v>67.461</v>
       </c>
       <c r="P42" t="s">
         <v>265</v>
@@ -4895,7 +4904,7 @@
         <v>268</v>
       </c>
       <c r="C43" s="1" t="n">
-        <v>44062</v>
+        <v>44064</v>
       </c>
       <c r="D43" t="s">
         <v>269</v>
@@ -4905,31 +4914,31 @@
       </c>
       <c r="F43"/>
       <c r="G43" t="n">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="H43" t="n">
-        <v>2175060</v>
+        <v>2231154</v>
       </c>
       <c r="I43" t="n">
-        <v>251.291</v>
+        <v>257.772</v>
       </c>
       <c r="J43" t="n">
-        <v>28401</v>
+        <v>27211</v>
       </c>
       <c r="K43" t="n">
-        <v>3.281</v>
+        <v>3.144</v>
       </c>
       <c r="L43" t="n">
-        <v>21993</v>
+        <v>22890</v>
       </c>
       <c r="M43" t="n">
-        <v>2.541</v>
+        <v>2.645</v>
       </c>
       <c r="N43" t="n">
         <v>0.061</v>
       </c>
       <c r="O43" t="n">
-        <v>16.291</v>
+        <v>16.388</v>
       </c>
       <c r="P43" t="s">
         <v>45</v>
@@ -4952,7 +4961,7 @@
         <v>274</v>
       </c>
       <c r="C44" s="1" t="n">
-        <v>44068</v>
+        <v>44070</v>
       </c>
       <c r="D44" t="s">
         <v>275</v>
@@ -4964,31 +4973,31 @@
         <v>277</v>
       </c>
       <c r="G44" t="n">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="H44" t="n">
-        <v>4819124</v>
+        <v>4934818</v>
       </c>
       <c r="I44" t="n">
-        <v>79.705</v>
+        <v>81.619</v>
       </c>
       <c r="J44" t="n">
-        <v>45798</v>
+        <v>57640</v>
       </c>
       <c r="K44" t="n">
-        <v>0.757</v>
+        <v>0.953</v>
       </c>
       <c r="L44" t="n">
-        <v>44161</v>
+        <v>47696</v>
       </c>
       <c r="M44" t="n">
-        <v>0.73</v>
+        <v>0.789</v>
       </c>
       <c r="N44" t="n">
-        <v>0.02</v>
+        <v>0.022</v>
       </c>
       <c r="O44" t="n">
-        <v>50.986</v>
+        <v>45.975</v>
       </c>
       <c r="P44" t="s">
         <v>278</v>
@@ -5011,7 +5020,7 @@
         <v>281</v>
       </c>
       <c r="C45" s="1" t="n">
-        <v>44068</v>
+        <v>44070</v>
       </c>
       <c r="D45" t="s">
         <v>275</v>
@@ -5023,31 +5032,31 @@
         <v>277</v>
       </c>
       <c r="G45" t="n">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="H45" t="n">
-        <v>8125892</v>
+        <v>8313445</v>
       </c>
       <c r="I45" t="n">
-        <v>134.397</v>
+        <v>137.499</v>
       </c>
       <c r="J45" t="n">
-        <v>72341</v>
+        <v>94024</v>
       </c>
       <c r="K45" t="n">
-        <v>1.196</v>
+        <v>1.555</v>
       </c>
       <c r="L45" t="n">
-        <v>69119</v>
+        <v>74693</v>
       </c>
       <c r="M45" t="n">
-        <v>1.143</v>
+        <v>1.235</v>
       </c>
       <c r="N45" t="n">
-        <v>0.013</v>
+        <v>0.014</v>
       </c>
       <c r="O45" t="n">
-        <v>79.801</v>
+        <v>71.998</v>
       </c>
       <c r="P45" t="s">
         <v>278</v>
@@ -5070,7 +5079,7 @@
         <v>284</v>
       </c>
       <c r="C46" s="1" t="n">
-        <v>44068</v>
+        <v>44070</v>
       </c>
       <c r="D46" t="s">
         <v>285</v>
@@ -5082,31 +5091,31 @@
         <v>287</v>
       </c>
       <c r="G46" t="n">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="H46" t="n">
-        <v>1357628</v>
+        <v>1397400</v>
       </c>
       <c r="I46" t="n">
-        <v>10.734</v>
+        <v>11.049</v>
       </c>
       <c r="J46" t="n">
-        <v>23744</v>
+        <v>20617</v>
       </c>
       <c r="K46" t="n">
-        <v>0.188</v>
+        <v>0.163</v>
       </c>
       <c r="L46" t="n">
-        <v>20498</v>
+        <v>19711</v>
       </c>
       <c r="M46" t="n">
-        <v>0.162</v>
+        <v>0.156</v>
       </c>
       <c r="N46" t="n">
-        <v>0.05</v>
+        <v>0.045</v>
       </c>
       <c r="O46" t="n">
-        <v>20.032</v>
+        <v>22.373</v>
       </c>
       <c r="P46" t="s">
         <v>288</v>
@@ -5129,7 +5138,7 @@
         <v>291</v>
       </c>
       <c r="C47" s="1" t="n">
-        <v>44065</v>
+        <v>44068</v>
       </c>
       <c r="D47" t="s">
         <v>292</v>
@@ -5141,31 +5150,31 @@
         <v>293</v>
       </c>
       <c r="G47" t="n">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="H47" t="n">
-        <v>1661966</v>
+        <v>1708010</v>
       </c>
       <c r="I47" t="n">
-        <v>13.141</v>
+        <v>13.505</v>
       </c>
       <c r="J47" t="n">
-        <v>20461</v>
+        <v>15191</v>
       </c>
       <c r="K47" t="n">
-        <v>0.162</v>
+        <v>0.12</v>
       </c>
       <c r="L47" t="n">
-        <v>22585</v>
+        <v>20753</v>
       </c>
       <c r="M47" t="n">
-        <v>0.179</v>
+        <v>0.164</v>
       </c>
       <c r="N47" t="n">
-        <v>0.045</v>
+        <v>0.049</v>
       </c>
       <c r="O47" t="n">
-        <v>22.093</v>
+        <v>20.281</v>
       </c>
       <c r="P47" t="s">
         <v>288</v>
@@ -5188,7 +5197,7 @@
         <v>296</v>
       </c>
       <c r="C48" s="1" t="n">
-        <v>44057</v>
+        <v>44068</v>
       </c>
       <c r="D48" t="s">
         <v>297</v>
@@ -5198,31 +5207,31 @@
       </c>
       <c r="F48"/>
       <c r="G48" t="n">
-        <v>152</v>
+        <v>163</v>
       </c>
       <c r="H48" t="n">
-        <v>2291327</v>
+        <v>2434444</v>
       </c>
       <c r="I48" t="n">
-        <v>122.03</v>
+        <v>129.652</v>
       </c>
       <c r="J48" t="n">
-        <v>19573</v>
+        <v>7257</v>
       </c>
       <c r="K48" t="n">
-        <v>1.042</v>
+        <v>0.386</v>
       </c>
       <c r="L48" t="n">
-        <v>15431</v>
+        <v>13199</v>
       </c>
       <c r="M48" t="n">
-        <v>0.822</v>
+        <v>0.703</v>
       </c>
       <c r="N48" t="n">
-        <v>0.098</v>
+        <v>0.059</v>
       </c>
       <c r="O48" t="n">
-        <v>10.206</v>
+        <v>16.832</v>
       </c>
       <c r="P48" t="s">
         <v>298</v>
@@ -5245,7 +5254,7 @@
         <v>301</v>
       </c>
       <c r="C49" s="1" t="n">
-        <v>44066</v>
+        <v>44068</v>
       </c>
       <c r="D49" t="s">
         <v>302</v>
@@ -5255,31 +5264,31 @@
       </c>
       <c r="F49"/>
       <c r="G49" t="n">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="H49" t="n">
-        <v>421983</v>
+        <v>429513</v>
       </c>
       <c r="I49" t="n">
-        <v>7.848</v>
+        <v>7.988</v>
       </c>
       <c r="J49" t="n">
-        <v>4179</v>
+        <v>4149</v>
       </c>
       <c r="K49" t="n">
-        <v>0.078</v>
+        <v>0.077</v>
       </c>
       <c r="L49" t="n">
-        <v>4367</v>
+        <v>4418</v>
       </c>
       <c r="M49" t="n">
-        <v>0.081</v>
+        <v>0.082</v>
       </c>
       <c r="N49" t="n">
-        <v>0.074</v>
+        <v>0.071</v>
       </c>
       <c r="O49" t="n">
-        <v>13.472</v>
+        <v>14.109</v>
       </c>
       <c r="P49" t="s">
         <v>45</v>
@@ -5302,7 +5311,7 @@
         <v>307</v>
       </c>
       <c r="C50" s="1" t="n">
-        <v>44067</v>
+        <v>44070</v>
       </c>
       <c r="D50" t="s">
         <v>308</v>
@@ -5312,31 +5321,31 @@
       </c>
       <c r="F50"/>
       <c r="G50" t="n">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="H50" t="n">
-        <v>590623</v>
+        <v>603604</v>
       </c>
       <c r="I50" t="n">
-        <v>138.301</v>
+        <v>141.341</v>
       </c>
       <c r="J50" t="n">
-        <v>3056</v>
+        <v>4191</v>
       </c>
       <c r="K50" t="n">
-        <v>0.716</v>
+        <v>0.981</v>
       </c>
       <c r="L50" t="n">
-        <v>3927</v>
+        <v>3717</v>
       </c>
       <c r="M50" t="n">
-        <v>0.92</v>
+        <v>0.87</v>
       </c>
       <c r="N50" t="n">
-        <v>0.157</v>
+        <v>0.159</v>
       </c>
       <c r="O50" t="n">
-        <v>6.359</v>
+        <v>6.306</v>
       </c>
       <c r="P50" t="s">
         <v>309</v>
@@ -5359,7 +5368,7 @@
         <v>313</v>
       </c>
       <c r="C51" s="1" t="n">
-        <v>44069</v>
+        <v>44071</v>
       </c>
       <c r="D51" t="s">
         <v>314</v>
@@ -5371,28 +5380,32 @@
         <v>316</v>
       </c>
       <c r="G51" t="n">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="H51" t="n">
-        <v>242823</v>
+        <v>246867</v>
       </c>
       <c r="I51" t="n">
-        <v>128.736</v>
+        <v>130.88</v>
       </c>
       <c r="J51" t="n">
-        <v>2290</v>
+        <v>2040</v>
       </c>
       <c r="K51" t="n">
-        <v>1.214</v>
+        <v>1.082</v>
       </c>
       <c r="L51" t="n">
-        <v>1700</v>
+        <v>1764</v>
       </c>
       <c r="M51" t="n">
-        <v>0.901</v>
-      </c>
-      <c r="N51"/>
-      <c r="O51"/>
+        <v>0.935</v>
+      </c>
+      <c r="N51" t="n">
+        <v>0.003</v>
+      </c>
+      <c r="O51" t="n">
+        <v>316.615</v>
+      </c>
       <c r="P51" t="s">
         <v>315</v>
       </c>
@@ -5414,7 +5427,7 @@
         <v>319</v>
       </c>
       <c r="C52" s="1" t="n">
-        <v>44068</v>
+        <v>44071</v>
       </c>
       <c r="D52" t="s">
         <v>320</v>
@@ -5424,31 +5437,31 @@
       </c>
       <c r="F52"/>
       <c r="G52" t="n">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="H52" t="n">
-        <v>613324</v>
+        <v>629443</v>
       </c>
       <c r="I52" t="n">
-        <v>225.297</v>
+        <v>231.218</v>
       </c>
       <c r="J52" t="n">
-        <v>4557</v>
+        <v>5602</v>
       </c>
       <c r="K52" t="n">
-        <v>1.674</v>
+        <v>2.058</v>
       </c>
       <c r="L52" t="n">
-        <v>4098</v>
+        <v>4276</v>
       </c>
       <c r="M52" t="n">
-        <v>1.505</v>
+        <v>1.571</v>
       </c>
       <c r="N52" t="n">
         <v>0.008</v>
       </c>
       <c r="O52" t="n">
-        <v>121.038</v>
+        <v>127.915</v>
       </c>
       <c r="P52" t="s">
         <v>45</v>
@@ -5471,7 +5484,7 @@
         <v>323</v>
       </c>
       <c r="C53" s="1" t="n">
-        <v>44067</v>
+        <v>44069</v>
       </c>
       <c r="D53" t="s">
         <v>324</v>
@@ -5481,31 +5494,31 @@
       </c>
       <c r="F53"/>
       <c r="G53" t="n">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="H53" t="n">
-        <v>474282</v>
+        <v>379508</v>
       </c>
       <c r="I53" t="n">
-        <v>757.668</v>
+        <v>606.266</v>
       </c>
       <c r="J53" t="n">
-        <v>1025</v>
+        <v>1365</v>
       </c>
       <c r="K53" t="n">
-        <v>1.637</v>
+        <v>2.181</v>
       </c>
       <c r="L53" t="n">
-        <v>1725</v>
+        <v>1113</v>
       </c>
       <c r="M53" t="n">
-        <v>2.756</v>
+        <v>1.778</v>
       </c>
       <c r="N53" t="n">
-        <v>0.022</v>
+        <v>0.044</v>
       </c>
       <c r="O53" t="n">
-        <v>45.566</v>
+        <v>22.982</v>
       </c>
       <c r="P53" t="s">
         <v>325</v>
@@ -5528,7 +5541,7 @@
         <v>328</v>
       </c>
       <c r="C54" s="1" t="n">
-        <v>44068</v>
+        <v>44070</v>
       </c>
       <c r="D54" t="s">
         <v>329</v>
@@ -5540,31 +5553,31 @@
         <v>331</v>
       </c>
       <c r="G54" t="n">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="H54" t="n">
-        <v>1191500</v>
+        <v>1212790</v>
       </c>
       <c r="I54" t="n">
-        <v>36.813</v>
+        <v>37.471</v>
       </c>
       <c r="J54" t="n">
-        <v>8655</v>
+        <v>10026</v>
       </c>
       <c r="K54" t="n">
-        <v>0.267</v>
+        <v>0.31</v>
       </c>
       <c r="L54" t="n">
-        <v>8916</v>
+        <v>8664</v>
       </c>
       <c r="M54" t="n">
-        <v>0.275</v>
+        <v>0.268</v>
       </c>
       <c r="N54" t="n">
         <v>0.001</v>
       </c>
       <c r="O54" t="n">
-        <v>1006.645</v>
+        <v>1083</v>
       </c>
       <c r="P54" t="s">
         <v>45</v>
@@ -5587,7 +5600,7 @@
         <v>335</v>
       </c>
       <c r="C55" s="1" t="n">
-        <v>44067</v>
+        <v>44070</v>
       </c>
       <c r="D55" t="s">
         <v>336</v>
@@ -5597,31 +5610,31 @@
       </c>
       <c r="F55"/>
       <c r="G55" t="n">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="H55" t="n">
-        <v>104631</v>
+        <v>108099</v>
       </c>
       <c r="I55" t="n">
-        <v>193.567</v>
+        <v>199.983</v>
       </c>
       <c r="J55" t="n">
-        <v>977</v>
+        <v>1190</v>
       </c>
       <c r="K55" t="n">
-        <v>1.807</v>
+        <v>2.201</v>
       </c>
       <c r="L55" t="n">
-        <v>1060</v>
+        <v>1124</v>
       </c>
       <c r="M55" t="n">
-        <v>1.961</v>
+        <v>2.079</v>
       </c>
       <c r="N55" t="n">
-        <v>0.134</v>
+        <v>0.127</v>
       </c>
       <c r="O55" t="n">
-        <v>7.465</v>
+        <v>7.868</v>
       </c>
       <c r="P55" t="s">
         <v>338</v>
@@ -5714,28 +5727,28 @@
         <v>234</v>
       </c>
       <c r="H57" t="n">
-        <v>1193262</v>
+        <v>1204031</v>
       </c>
       <c r="I57" t="n">
-        <v>9.255</v>
+        <v>9.338</v>
       </c>
       <c r="J57" t="n">
-        <v>6833</v>
+        <v>11477</v>
       </c>
       <c r="K57" t="n">
-        <v>0.053</v>
+        <v>0.089</v>
       </c>
       <c r="L57" t="n">
-        <v>9035</v>
+        <v>10380</v>
       </c>
       <c r="M57" t="n">
-        <v>0.07</v>
+        <v>0.081</v>
       </c>
       <c r="N57" t="n">
-        <v>0.602</v>
+        <v>0.524</v>
       </c>
       <c r="O57" t="n">
-        <v>1.662</v>
+        <v>1.909</v>
       </c>
       <c r="P57" t="s">
         <v>351</v>
@@ -5758,7 +5771,7 @@
         <v>355</v>
       </c>
       <c r="C58" s="1" t="n">
-        <v>44067</v>
+        <v>44070</v>
       </c>
       <c r="D58" t="s">
         <v>356</v>
@@ -5768,31 +5781,31 @@
       </c>
       <c r="F58"/>
       <c r="G58" t="n">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="H58" t="n">
-        <v>1779980</v>
+        <v>1846260</v>
       </c>
       <c r="I58" t="n">
-        <v>48.224</v>
+        <v>50.02</v>
       </c>
       <c r="J58" t="n">
-        <v>21110</v>
+        <v>22009</v>
       </c>
       <c r="K58" t="n">
-        <v>0.572</v>
+        <v>0.596</v>
       </c>
       <c r="L58" t="n">
-        <v>21881</v>
+        <v>21979</v>
       </c>
       <c r="M58" t="n">
-        <v>0.593</v>
+        <v>0.595</v>
       </c>
       <c r="N58" t="n">
-        <v>0.054</v>
+        <v>0.062</v>
       </c>
       <c r="O58" t="n">
-        <v>18.403</v>
+        <v>16.109</v>
       </c>
       <c r="P58" t="s">
         <v>357</v>
@@ -5815,7 +5828,7 @@
         <v>361</v>
       </c>
       <c r="C59" s="1" t="n">
-        <v>44065</v>
+        <v>44067</v>
       </c>
       <c r="D59" t="s">
         <v>362</v>
@@ -5825,31 +5838,31 @@
       </c>
       <c r="F59"/>
       <c r="G59" t="n">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="H59" t="n">
-        <v>145167</v>
+        <v>147820</v>
       </c>
       <c r="I59" t="n">
-        <v>2.668</v>
+        <v>2.717</v>
       </c>
       <c r="J59" t="n">
-        <v>1113</v>
+        <v>1783</v>
       </c>
       <c r="K59" t="n">
-        <v>0.02</v>
+        <v>0.033</v>
       </c>
       <c r="L59" t="n">
-        <v>1395</v>
+        <v>1439</v>
       </c>
       <c r="M59" t="n">
         <v>0.026</v>
       </c>
       <c r="N59" t="n">
-        <v>0.006</v>
+        <v>0.009</v>
       </c>
       <c r="O59" t="n">
-        <v>160.082</v>
+        <v>114.466</v>
       </c>
       <c r="P59" t="s">
         <v>363</v>
@@ -5982,7 +5995,7 @@
         <v>380</v>
       </c>
       <c r="C62" s="1" t="n">
-        <v>44068</v>
+        <v>44070</v>
       </c>
       <c r="D62" t="s">
         <v>381</v>
@@ -5992,31 +6005,31 @@
       </c>
       <c r="F62"/>
       <c r="G62" t="n">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="H62" t="n">
-        <v>710063</v>
+        <v>730330</v>
       </c>
       <c r="I62" t="n">
-        <v>147.248</v>
+        <v>151.451</v>
       </c>
       <c r="J62" t="n">
-        <v>8559</v>
+        <v>11010</v>
       </c>
       <c r="K62" t="n">
-        <v>1.775</v>
+        <v>2.283</v>
       </c>
       <c r="L62" t="n">
-        <v>10093</v>
+        <v>8159</v>
       </c>
       <c r="M62" t="n">
-        <v>2.093</v>
+        <v>1.692</v>
       </c>
       <c r="N62" t="n">
         <v>0.001</v>
       </c>
       <c r="O62" t="n">
-        <v>1535.891</v>
+        <v>1215.17</v>
       </c>
       <c r="P62" t="s">
         <v>382</v>
@@ -6039,7 +6052,7 @@
         <v>385</v>
       </c>
       <c r="C63" s="1" t="n">
-        <v>44068</v>
+        <v>44070</v>
       </c>
       <c r="D63" t="s">
         <v>386</v>
@@ -6049,31 +6062,31 @@
       </c>
       <c r="F63"/>
       <c r="G63" t="n">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="H63" t="n">
-        <v>383130</v>
+        <v>391502</v>
       </c>
       <c r="I63" t="n">
-        <v>1.859</v>
+        <v>1.899</v>
       </c>
       <c r="J63" t="n">
-        <v>3588</v>
+        <v>3156</v>
       </c>
       <c r="K63" t="n">
-        <v>0.017</v>
+        <v>0.015</v>
       </c>
       <c r="L63" t="n">
-        <v>3991</v>
+        <v>3608</v>
       </c>
       <c r="M63" t="n">
-        <v>0.019</v>
+        <v>0.018</v>
       </c>
       <c r="N63" t="n">
-        <v>0.11</v>
+        <v>0.1</v>
       </c>
       <c r="O63" t="n">
-        <v>9.121</v>
+        <v>9.971</v>
       </c>
       <c r="P63" t="s">
         <v>387</v>
@@ -6198,7 +6211,7 @@
         <v>405</v>
       </c>
       <c r="C66" s="1" t="n">
-        <v>44069</v>
+        <v>44071</v>
       </c>
       <c r="D66" t="s">
         <v>406</v>
@@ -6208,28 +6221,32 @@
       </c>
       <c r="F66"/>
       <c r="G66" t="n">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="H66" t="n">
-        <v>2512337</v>
+        <v>2559261</v>
       </c>
       <c r="I66" t="n">
-        <v>11.374</v>
+        <v>11.586</v>
       </c>
       <c r="J66" t="n">
-        <v>24593</v>
+        <v>23483</v>
       </c>
       <c r="K66" t="n">
-        <v>0.111</v>
+        <v>0.106</v>
       </c>
       <c r="L66" t="n">
-        <v>24609</v>
+        <v>24271</v>
       </c>
       <c r="M66" t="n">
-        <v>0.111</v>
-      </c>
-      <c r="N66"/>
-      <c r="O66"/>
+        <v>0.11</v>
+      </c>
+      <c r="N66" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="O66" t="n">
+        <v>49.032</v>
+      </c>
       <c r="P66" t="s">
         <v>407</v>
       </c>
@@ -6251,7 +6268,7 @@
         <v>410</v>
       </c>
       <c r="C67" s="1" t="n">
-        <v>44066</v>
+        <v>44069</v>
       </c>
       <c r="D67" t="s">
         <v>411</v>
@@ -6261,31 +6278,31 @@
       </c>
       <c r="F67"/>
       <c r="G67" t="n">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="H67" t="n">
-        <v>301561</v>
+        <v>313229</v>
       </c>
       <c r="I67" t="n">
-        <v>69.89</v>
+        <v>72.595</v>
       </c>
       <c r="J67" t="n">
-        <v>7584</v>
+        <v>3612</v>
       </c>
       <c r="K67" t="n">
-        <v>1.758</v>
+        <v>0.837</v>
       </c>
       <c r="L67" t="n">
-        <v>4552</v>
+        <v>4744</v>
       </c>
       <c r="M67" t="n">
-        <v>1.055</v>
+        <v>1.099</v>
       </c>
       <c r="N67" t="n">
-        <v>0.151</v>
+        <v>0.168</v>
       </c>
       <c r="O67" t="n">
-        <v>6.618</v>
+        <v>5.94</v>
       </c>
       <c r="P67" t="s">
         <v>412</v>
@@ -6308,7 +6325,7 @@
         <v>416</v>
       </c>
       <c r="C68" s="1" t="n">
-        <v>44065</v>
+        <v>44068</v>
       </c>
       <c r="D68" t="s">
         <v>417</v>
@@ -6318,31 +6335,31 @@
       </c>
       <c r="F68"/>
       <c r="G68" t="n">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="H68" t="n">
-        <v>171552</v>
+        <v>177771</v>
       </c>
       <c r="I68" t="n">
-        <v>24.052</v>
+        <v>24.924</v>
       </c>
       <c r="J68" t="n">
-        <v>2292</v>
+        <v>2119</v>
       </c>
       <c r="K68" t="n">
-        <v>0.321</v>
+        <v>0.297</v>
       </c>
       <c r="L68" t="n">
-        <v>2875</v>
+        <v>2586</v>
       </c>
       <c r="M68" t="n">
-        <v>0.403</v>
+        <v>0.363</v>
       </c>
       <c r="N68" t="n">
-        <v>0.172</v>
+        <v>0.192</v>
       </c>
       <c r="O68" t="n">
-        <v>5.818</v>
+        <v>5.221</v>
       </c>
       <c r="P68" t="s">
         <v>418</v>
@@ -6475,7 +6492,7 @@
         <v>434</v>
       </c>
       <c r="C71" s="1" t="n">
-        <v>44068</v>
+        <v>44070</v>
       </c>
       <c r="D71" t="s">
         <v>435</v>
@@ -6485,31 +6502,31 @@
       </c>
       <c r="F71"/>
       <c r="G71" t="n">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="H71" t="n">
-        <v>2467528</v>
+        <v>2522949</v>
       </c>
       <c r="I71" t="n">
-        <v>65.198</v>
+        <v>66.662</v>
       </c>
       <c r="J71" t="n">
-        <v>21982</v>
+        <v>27110</v>
       </c>
       <c r="K71" t="n">
-        <v>0.581</v>
+        <v>0.716</v>
       </c>
       <c r="L71" t="n">
-        <v>23162</v>
+        <v>23597</v>
       </c>
       <c r="M71" t="n">
-        <v>0.612</v>
+        <v>0.623</v>
       </c>
       <c r="N71" t="n">
         <v>0.031</v>
       </c>
       <c r="O71" t="n">
-        <v>32.227</v>
+        <v>31.82</v>
       </c>
       <c r="P71" t="s">
         <v>436</v>
@@ -6532,7 +6549,7 @@
         <v>439</v>
       </c>
       <c r="C72" s="1" t="n">
-        <v>44068</v>
+        <v>44070</v>
       </c>
       <c r="D72" t="s">
         <v>435</v>
@@ -6542,31 +6559,31 @@
       </c>
       <c r="F72"/>
       <c r="G72" t="n">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="H72" t="n">
-        <v>2577726</v>
+        <v>2634903</v>
       </c>
       <c r="I72" t="n">
-        <v>68.11</v>
+        <v>69.621</v>
       </c>
       <c r="J72" t="n">
-        <v>22211</v>
+        <v>28283</v>
       </c>
       <c r="K72" t="n">
-        <v>0.587</v>
+        <v>0.747</v>
       </c>
       <c r="L72" t="n">
-        <v>24047</v>
+        <v>24453</v>
       </c>
       <c r="M72" t="n">
-        <v>0.635</v>
+        <v>0.646</v>
       </c>
       <c r="N72" t="n">
         <v>0.03</v>
       </c>
       <c r="O72" t="n">
-        <v>33.458</v>
+        <v>32.975</v>
       </c>
       <c r="P72" t="s">
         <v>436</v>
@@ -6646,7 +6663,7 @@
         <v>448</v>
       </c>
       <c r="C74" s="1" t="n">
-        <v>44067</v>
+        <v>44070</v>
       </c>
       <c r="D74" t="s">
         <v>449</v>
@@ -6656,31 +6673,31 @@
       </c>
       <c r="F74"/>
       <c r="G74" t="n">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="H74" t="n">
-        <v>594215</v>
+        <v>609258</v>
       </c>
       <c r="I74" t="n">
-        <v>206.249</v>
+        <v>211.47</v>
       </c>
       <c r="J74" t="n">
-        <v>4295</v>
+        <v>5146</v>
       </c>
       <c r="K74" t="n">
-        <v>1.491</v>
+        <v>1.786</v>
       </c>
       <c r="L74" t="n">
-        <v>5464</v>
+        <v>5284</v>
       </c>
       <c r="M74" t="n">
-        <v>1.897</v>
+        <v>1.834</v>
       </c>
       <c r="N74" t="n">
-        <v>0.05</v>
+        <v>0.048</v>
       </c>
       <c r="O74" t="n">
-        <v>19.838</v>
+        <v>20.71</v>
       </c>
       <c r="P74" t="s">
         <v>450</v>
@@ -6703,7 +6720,7 @@
         <v>454</v>
       </c>
       <c r="C75" s="1" t="n">
-        <v>44068</v>
+        <v>44071</v>
       </c>
       <c r="D75" t="s">
         <v>455</v>
@@ -6713,31 +6730,31 @@
       </c>
       <c r="F75"/>
       <c r="G75" t="n">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="H75" t="n">
-        <v>1679614</v>
+        <v>1756920</v>
       </c>
       <c r="I75" t="n">
-        <v>87.309</v>
+        <v>91.327</v>
       </c>
       <c r="J75" t="n">
-        <v>20479</v>
+        <v>26500</v>
       </c>
       <c r="K75" t="n">
-        <v>1.065</v>
+        <v>1.378</v>
       </c>
       <c r="L75" t="n">
-        <v>19646</v>
+        <v>20077</v>
       </c>
       <c r="M75" t="n">
-        <v>1.021</v>
+        <v>1.044</v>
       </c>
       <c r="N75" t="n">
-        <v>0.059</v>
+        <v>0.058</v>
       </c>
       <c r="O75" t="n">
-        <v>16.903</v>
+        <v>17.166</v>
       </c>
       <c r="P75" t="s">
         <v>457</v>
@@ -6760,7 +6777,7 @@
         <v>461</v>
       </c>
       <c r="C76" s="1" t="n">
-        <v>44068</v>
+        <v>44070</v>
       </c>
       <c r="D76" t="s">
         <v>462</v>
@@ -6770,31 +6787,31 @@
       </c>
       <c r="F76"/>
       <c r="G76" t="n">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="H76" t="n">
-        <v>35128661</v>
+        <v>35751747</v>
       </c>
       <c r="I76" t="n">
-        <v>240.715</v>
+        <v>244.985</v>
       </c>
       <c r="J76" t="n">
-        <v>245441</v>
+        <v>327964</v>
       </c>
       <c r="K76" t="n">
-        <v>1.682</v>
+        <v>2.247</v>
       </c>
       <c r="L76" t="n">
-        <v>273028</v>
+        <v>276806</v>
       </c>
       <c r="M76" t="n">
-        <v>1.871</v>
+        <v>1.897</v>
       </c>
       <c r="N76" t="n">
-        <v>0.018</v>
+        <v>0.017</v>
       </c>
       <c r="O76" t="n">
-        <v>56.631</v>
+        <v>57.764</v>
       </c>
       <c r="P76" t="s">
         <v>463</v>
@@ -6817,7 +6834,7 @@
         <v>467</v>
       </c>
       <c r="C77" s="1" t="n">
-        <v>44066</v>
+        <v>44068</v>
       </c>
       <c r="D77" t="s">
         <v>468</v>
@@ -6827,31 +6844,31 @@
       </c>
       <c r="F77"/>
       <c r="G77" t="n">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="H77" t="n">
-        <v>368244</v>
+        <v>378014</v>
       </c>
       <c r="I77" t="n">
-        <v>28.431</v>
+        <v>29.185</v>
       </c>
       <c r="J77" t="n">
-        <v>6402</v>
+        <v>6128</v>
       </c>
       <c r="K77" t="n">
-        <v>0.494</v>
+        <v>0.473</v>
       </c>
       <c r="L77" t="n">
-        <v>4853</v>
+        <v>5057</v>
       </c>
       <c r="M77" t="n">
-        <v>0.375</v>
+        <v>0.39</v>
       </c>
       <c r="N77" t="n">
-        <v>0.016</v>
+        <v>0.022</v>
       </c>
       <c r="O77" t="n">
-        <v>63.261</v>
+        <v>46.213</v>
       </c>
       <c r="P77" t="s">
         <v>469</v>
@@ -6874,7 +6891,7 @@
         <v>473</v>
       </c>
       <c r="C78" s="1" t="n">
-        <v>44068</v>
+        <v>44070</v>
       </c>
       <c r="D78" t="s">
         <v>474</v>
@@ -6884,31 +6901,31 @@
       </c>
       <c r="F78"/>
       <c r="G78" t="n">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="H78" t="n">
-        <v>4792192</v>
+        <v>4913924</v>
       </c>
       <c r="I78" t="n">
-        <v>137.652</v>
+        <v>141.148</v>
       </c>
       <c r="J78" t="n">
-        <v>58707</v>
+        <v>63265</v>
       </c>
       <c r="K78" t="n">
-        <v>1.686</v>
+        <v>1.817</v>
       </c>
       <c r="L78" t="n">
-        <v>59111</v>
+        <v>58974</v>
       </c>
       <c r="M78" t="n">
-        <v>1.698</v>
+        <v>1.694</v>
       </c>
       <c r="N78" t="n">
-        <v>0.021</v>
+        <v>0.02</v>
       </c>
       <c r="O78" t="n">
-        <v>47.343</v>
+        <v>50.653</v>
       </c>
       <c r="P78" t="s">
         <v>45</v>
@@ -6931,7 +6948,7 @@
         <v>477</v>
       </c>
       <c r="C79" s="1" t="n">
-        <v>44068</v>
+        <v>44069</v>
       </c>
       <c r="D79" t="s">
         <v>478</v>
@@ -6943,31 +6960,31 @@
         <v>480</v>
       </c>
       <c r="G79" t="n">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="H79" t="n">
-        <v>144564</v>
+        <v>145948</v>
       </c>
       <c r="I79" t="n">
-        <v>8.634</v>
+        <v>8.716</v>
       </c>
       <c r="J79" t="n">
-        <v>816</v>
+        <v>1384</v>
       </c>
       <c r="K79" t="n">
-        <v>0.049</v>
+        <v>0.083</v>
       </c>
       <c r="L79" t="n">
-        <v>1262</v>
+        <v>1251</v>
       </c>
       <c r="M79" t="n">
         <v>0.075</v>
       </c>
       <c r="N79" t="n">
-        <v>0.088</v>
+        <v>0.086</v>
       </c>
       <c r="O79" t="n">
-        <v>11.384</v>
+        <v>11.66</v>
       </c>
       <c r="P79" t="s">
         <v>481</v>
@@ -6990,7 +7007,7 @@
         <v>485</v>
       </c>
       <c r="C80" s="1" t="n">
-        <v>44068</v>
+        <v>44070</v>
       </c>
       <c r="D80" t="s">
         <v>486</v>
@@ -7002,31 +7019,31 @@
         <v>487</v>
       </c>
       <c r="G80" t="n">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="H80" t="n">
-        <v>885575</v>
+        <v>904343</v>
       </c>
       <c r="I80" t="n">
-        <v>130.144</v>
+        <v>132.902</v>
       </c>
       <c r="J80" t="n">
-        <v>8646</v>
+        <v>8836</v>
       </c>
       <c r="K80" t="n">
-        <v>1.271</v>
+        <v>1.299</v>
       </c>
       <c r="L80" t="n">
-        <v>9210</v>
+        <v>8843</v>
       </c>
       <c r="M80" t="n">
-        <v>1.353</v>
+        <v>1.3</v>
       </c>
       <c r="N80" t="n">
-        <v>0.014</v>
+        <v>0.015</v>
       </c>
       <c r="O80" t="n">
-        <v>69.174</v>
+        <v>66.848</v>
       </c>
       <c r="P80" t="s">
         <v>45</v>
@@ -7049,7 +7066,7 @@
         <v>491</v>
       </c>
       <c r="C81" s="1" t="n">
-        <v>44061</v>
+        <v>44067</v>
       </c>
       <c r="D81" t="s">
         <v>492</v>
@@ -7059,27 +7076,27 @@
       </c>
       <c r="F81"/>
       <c r="G81" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H81" t="n">
-        <v>731313</v>
+        <v>758569</v>
       </c>
       <c r="I81" t="n">
-        <v>125.003</v>
+        <v>129.662</v>
       </c>
       <c r="J81"/>
       <c r="K81"/>
       <c r="L81" t="n">
-        <v>6368</v>
+        <v>4803</v>
       </c>
       <c r="M81" t="n">
-        <v>1.088</v>
+        <v>0.821</v>
       </c>
       <c r="N81" t="n">
-        <v>0.012</v>
+        <v>0.018</v>
       </c>
       <c r="O81" t="n">
-        <v>81.641</v>
+        <v>55.48</v>
       </c>
       <c r="P81" t="s">
         <v>45</v>
@@ -7102,7 +7119,7 @@
         <v>494</v>
       </c>
       <c r="C82" s="1" t="n">
-        <v>44061</v>
+        <v>44067</v>
       </c>
       <c r="D82" t="s">
         <v>492</v>
@@ -7112,27 +7129,27 @@
       </c>
       <c r="F82"/>
       <c r="G82" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H82" t="n">
-        <v>1745928</v>
+        <v>1832813</v>
       </c>
       <c r="I82" t="n">
-        <v>298.432</v>
+        <v>313.283</v>
       </c>
       <c r="J82"/>
       <c r="K82"/>
       <c r="L82" t="n">
-        <v>19289</v>
+        <v>15168</v>
       </c>
       <c r="M82" t="n">
-        <v>3.297</v>
+        <v>2.593</v>
       </c>
       <c r="N82" t="n">
-        <v>0.004</v>
+        <v>0.006</v>
       </c>
       <c r="O82" t="n">
-        <v>247.295</v>
+        <v>175.208</v>
       </c>
       <c r="P82" t="s">
         <v>45</v>
@@ -7155,7 +7172,7 @@
         <v>497</v>
       </c>
       <c r="C83" s="1" t="n">
-        <v>44068</v>
+        <v>44070</v>
       </c>
       <c r="D83" t="s">
         <v>498</v>
@@ -7165,27 +7182,31 @@
       </c>
       <c r="F83"/>
       <c r="G83" t="n">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="H83" t="n">
-        <v>315854</v>
+        <v>327940</v>
       </c>
       <c r="I83" t="n">
-        <v>57.853</v>
-      </c>
-      <c r="J83"/>
-      <c r="K83"/>
+        <v>60.066</v>
+      </c>
+      <c r="J83" t="n">
+        <v>7996</v>
+      </c>
+      <c r="K83" t="n">
+        <v>1.465</v>
+      </c>
       <c r="L83" t="n">
-        <v>2707</v>
+        <v>3417</v>
       </c>
       <c r="M83" t="n">
-        <v>0.496</v>
+        <v>0.626</v>
       </c>
       <c r="N83" t="n">
-        <v>0.027</v>
+        <v>0.021</v>
       </c>
       <c r="O83" t="n">
-        <v>36.652</v>
+        <v>46.535</v>
       </c>
       <c r="P83" t="s">
         <v>500</v>
@@ -7208,7 +7229,7 @@
         <v>503</v>
       </c>
       <c r="C84" s="1" t="n">
-        <v>44067</v>
+        <v>44070</v>
       </c>
       <c r="D84" t="s">
         <v>504</v>
@@ -7218,31 +7239,31 @@
       </c>
       <c r="F84"/>
       <c r="G84" t="n">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="H84" t="n">
-        <v>150695</v>
+        <v>154771</v>
       </c>
       <c r="I84" t="n">
-        <v>72.487</v>
+        <v>74.447</v>
       </c>
       <c r="J84" t="n">
-        <v>1460</v>
+        <v>1338</v>
       </c>
       <c r="K84" t="n">
-        <v>0.702</v>
+        <v>0.644</v>
       </c>
       <c r="L84" t="n">
-        <v>1033</v>
+        <v>1136</v>
       </c>
       <c r="M84" t="n">
-        <v>0.497</v>
+        <v>0.546</v>
       </c>
       <c r="N84" t="n">
-        <v>0.032</v>
+        <v>0.029</v>
       </c>
       <c r="O84" t="n">
-        <v>30.77</v>
+        <v>34.725</v>
       </c>
       <c r="P84" t="s">
         <v>506</v>
@@ -7265,7 +7286,7 @@
         <v>510</v>
       </c>
       <c r="C85" s="1" t="n">
-        <v>44067</v>
+        <v>44070</v>
       </c>
       <c r="D85" t="s">
         <v>511</v>
@@ -7277,31 +7298,31 @@
         <v>513</v>
       </c>
       <c r="G85" t="n">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="H85" t="n">
-        <v>3564065</v>
+        <v>3617982</v>
       </c>
       <c r="I85" t="n">
-        <v>60.093</v>
+        <v>61.003</v>
       </c>
       <c r="J85" t="n">
-        <v>10640</v>
+        <v>19009</v>
       </c>
       <c r="K85" t="n">
-        <v>0.179</v>
+        <v>0.321</v>
       </c>
       <c r="L85" t="n">
-        <v>21199</v>
+        <v>19671</v>
       </c>
       <c r="M85" t="n">
-        <v>0.357</v>
+        <v>0.332</v>
       </c>
       <c r="N85" t="n">
-        <v>0.151</v>
+        <v>0.143</v>
       </c>
       <c r="O85" t="n">
-        <v>6.616</v>
+        <v>7.011</v>
       </c>
       <c r="P85" t="s">
         <v>512</v>
@@ -7324,7 +7345,7 @@
         <v>517</v>
       </c>
       <c r="C86" s="1" t="n">
-        <v>44068</v>
+        <v>44071</v>
       </c>
       <c r="D86" t="s">
         <v>518</v>
@@ -7334,31 +7355,31 @@
       </c>
       <c r="F86"/>
       <c r="G86" t="n">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="H86" t="n">
-        <v>1775475</v>
+        <v>1837006</v>
       </c>
       <c r="I86" t="n">
-        <v>34.63</v>
+        <v>35.831</v>
       </c>
       <c r="J86" t="n">
-        <v>19048</v>
+        <v>19468</v>
       </c>
       <c r="K86" t="n">
-        <v>0.372</v>
+        <v>0.38</v>
       </c>
       <c r="L86" t="n">
-        <v>14807</v>
+        <v>17275</v>
       </c>
       <c r="M86" t="n">
-        <v>0.289</v>
+        <v>0.337</v>
       </c>
       <c r="N86" t="n">
-        <v>0.021</v>
+        <v>0.02</v>
       </c>
       <c r="O86" t="n">
-        <v>47.458</v>
+        <v>50.239</v>
       </c>
       <c r="P86" t="s">
         <v>519</v>
@@ -7461,10 +7482,10 @@
         <v>1.098</v>
       </c>
       <c r="N88" t="n">
-        <v>0.081</v>
+        <v>0.062</v>
       </c>
       <c r="O88" t="n">
-        <v>12.36</v>
+        <v>16.162</v>
       </c>
       <c r="P88" t="s">
         <v>533</v>
@@ -7502,22 +7523,22 @@
       <c r="H89"/>
       <c r="I89"/>
       <c r="J89" t="n">
-        <v>9264</v>
+        <v>9364</v>
       </c>
       <c r="K89" t="n">
-        <v>0.917</v>
+        <v>0.927</v>
       </c>
       <c r="L89" t="n">
-        <v>9264</v>
+        <v>9364</v>
       </c>
       <c r="M89" t="n">
-        <v>0.917</v>
+        <v>0.927</v>
       </c>
       <c r="N89" t="n">
         <v>0.027</v>
       </c>
       <c r="O89" t="n">
-        <v>36.555</v>
+        <v>37.264</v>
       </c>
       <c r="P89" t="s">
         <v>533</v>
@@ -7540,7 +7561,7 @@
         <v>540</v>
       </c>
       <c r="C90" s="1" t="n">
-        <v>44067</v>
+        <v>44070</v>
       </c>
       <c r="D90" t="s">
         <v>541</v>
@@ -7550,31 +7571,31 @@
       </c>
       <c r="F90"/>
       <c r="G90" t="n">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="H90" t="n">
-        <v>948439</v>
+        <v>988383</v>
       </c>
       <c r="I90" t="n">
-        <v>109.588</v>
+        <v>114.203</v>
       </c>
       <c r="J90" t="n">
-        <v>5651</v>
+        <v>9437</v>
       </c>
       <c r="K90" t="n">
-        <v>0.653</v>
+        <v>1.09</v>
       </c>
       <c r="L90" t="n">
-        <v>7787</v>
+        <v>9172</v>
       </c>
       <c r="M90" t="n">
-        <v>0.9</v>
+        <v>1.06</v>
       </c>
       <c r="N90" t="n">
-        <v>0.032</v>
+        <v>0.029</v>
       </c>
       <c r="O90" t="n">
-        <v>30.779</v>
+        <v>34.187</v>
       </c>
       <c r="P90" t="s">
         <v>542</v>
@@ -7597,7 +7618,7 @@
         <v>546</v>
       </c>
       <c r="C91" s="1" t="n">
-        <v>44068</v>
+        <v>44070</v>
       </c>
       <c r="D91" t="s">
         <v>547</v>
@@ -7607,31 +7628,31 @@
       </c>
       <c r="F91"/>
       <c r="G91" t="n">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="H91" t="n">
-        <v>86419</v>
+        <v>86806</v>
       </c>
       <c r="I91" t="n">
-        <v>3.628</v>
+        <v>3.645</v>
       </c>
       <c r="J91" t="n">
-        <v>155</v>
+        <v>204</v>
       </c>
       <c r="K91" t="n">
+        <v>0.009</v>
+      </c>
+      <c r="L91" t="n">
+        <v>178</v>
+      </c>
+      <c r="M91" t="n">
         <v>0.007</v>
       </c>
-      <c r="L91" t="n">
-        <v>185</v>
-      </c>
-      <c r="M91" t="n">
-        <v>0.008</v>
-      </c>
       <c r="N91" t="n">
-        <v>0.002</v>
+        <v>0.001</v>
       </c>
       <c r="O91" t="n">
-        <v>647.5</v>
+        <v>1246</v>
       </c>
       <c r="P91" t="s">
         <v>548</v>
@@ -7654,7 +7675,7 @@
         <v>551</v>
       </c>
       <c r="C92" s="1" t="n">
-        <v>44068</v>
+        <v>44070</v>
       </c>
       <c r="D92" t="s">
         <v>552</v>
@@ -7664,31 +7685,31 @@
       </c>
       <c r="F92"/>
       <c r="G92" t="n">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="H92" t="n">
-        <v>409632</v>
+        <v>413006</v>
       </c>
       <c r="I92" t="n">
-        <v>5.869</v>
+        <v>5.917</v>
       </c>
       <c r="J92" t="n">
-        <v>2220</v>
+        <v>1806</v>
       </c>
       <c r="K92" t="n">
-        <v>0.032</v>
+        <v>0.026</v>
       </c>
       <c r="L92" t="n">
-        <v>1765</v>
+        <v>1618</v>
       </c>
       <c r="M92" t="n">
-        <v>0.025</v>
+        <v>0.023</v>
       </c>
       <c r="N92" t="n">
-        <v>0.002</v>
+        <v>0.001</v>
       </c>
       <c r="O92" t="n">
-        <v>514.792</v>
+        <v>755.067</v>
       </c>
       <c r="P92" t="s">
         <v>553</v>
@@ -7711,7 +7732,7 @@
         <v>556</v>
       </c>
       <c r="C93" s="1" t="n">
-        <v>44068</v>
+        <v>44070</v>
       </c>
       <c r="D93" t="s">
         <v>552</v>
@@ -7721,31 +7742,31 @@
       </c>
       <c r="F93"/>
       <c r="G93" t="n">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="H93" t="n">
-        <v>797903</v>
+        <v>840416</v>
       </c>
       <c r="I93" t="n">
-        <v>11.431</v>
+        <v>12.04</v>
       </c>
       <c r="J93" t="n">
-        <v>2220</v>
+        <v>40945</v>
       </c>
       <c r="K93" t="n">
-        <v>0.032</v>
+        <v>0.587</v>
       </c>
       <c r="L93" t="n">
-        <v>1765</v>
+        <v>7209</v>
       </c>
       <c r="M93" t="n">
-        <v>0.025</v>
+        <v>0.103</v>
       </c>
       <c r="N93" t="n">
-        <v>0.002</v>
+        <v>0</v>
       </c>
       <c r="O93" t="n">
-        <v>514.792</v>
+        <v>3364.2</v>
       </c>
       <c r="P93" t="s">
         <v>553</v>
@@ -7825,7 +7846,7 @@
         <v>565</v>
       </c>
       <c r="C95" s="1" t="n">
-        <v>44065</v>
+        <v>44067</v>
       </c>
       <c r="D95" t="s">
         <v>566</v>
@@ -7835,31 +7856,31 @@
       </c>
       <c r="F95"/>
       <c r="G95" t="n">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="H95" t="n">
-        <v>123268</v>
+        <v>128027</v>
       </c>
       <c r="I95" t="n">
-        <v>10.43</v>
+        <v>10.833</v>
       </c>
       <c r="J95" t="n">
-        <v>1461</v>
+        <v>2251</v>
       </c>
       <c r="K95" t="n">
-        <v>0.124</v>
+        <v>0.19</v>
       </c>
       <c r="L95" t="n">
-        <v>1803</v>
+        <v>2038</v>
       </c>
       <c r="M95" t="n">
-        <v>0.153</v>
+        <v>0.172</v>
       </c>
       <c r="N95" t="n">
-        <v>0.056</v>
+        <v>0.044</v>
       </c>
       <c r="O95" t="n">
-        <v>17.928</v>
+        <v>22.609</v>
       </c>
       <c r="P95" t="s">
         <v>567</v>
@@ -7882,7 +7903,7 @@
         <v>570</v>
       </c>
       <c r="C96" s="1" t="n">
-        <v>44068</v>
+        <v>44070</v>
       </c>
       <c r="D96" t="s">
         <v>571</v>
@@ -7892,31 +7913,31 @@
       </c>
       <c r="F96"/>
       <c r="G96" t="n">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="H96" t="n">
-        <v>6521640</v>
+        <v>6727860</v>
       </c>
       <c r="I96" t="n">
-        <v>77.326</v>
+        <v>79.772</v>
       </c>
       <c r="J96" t="n">
-        <v>98231</v>
+        <v>106111</v>
       </c>
       <c r="K96" t="n">
-        <v>1.165</v>
+        <v>1.258</v>
       </c>
       <c r="L96" t="n">
-        <v>91319</v>
+        <v>95133</v>
       </c>
       <c r="M96" t="n">
-        <v>1.083</v>
+        <v>1.128</v>
       </c>
       <c r="N96" t="n">
         <v>0.014</v>
       </c>
       <c r="O96" t="n">
-        <v>69.862</v>
+        <v>70.851</v>
       </c>
       <c r="P96" t="s">
         <v>572</v>
@@ -7939,7 +7960,7 @@
         <v>575</v>
       </c>
       <c r="C97" s="1" t="n">
-        <v>44067</v>
+        <v>44069</v>
       </c>
       <c r="D97" t="s">
         <v>576</v>
@@ -7949,31 +7970,31 @@
       </c>
       <c r="F97"/>
       <c r="G97" t="n">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="H97" t="n">
-        <v>355057</v>
+        <v>363802</v>
       </c>
       <c r="I97" t="n">
-        <v>7.762</v>
+        <v>7.954</v>
       </c>
       <c r="J97" t="n">
-        <v>3212</v>
+        <v>4513</v>
       </c>
       <c r="K97" t="n">
-        <v>0.07</v>
+        <v>0.099</v>
       </c>
       <c r="L97" t="n">
-        <v>3645</v>
+        <v>3870</v>
       </c>
       <c r="M97" t="n">
-        <v>0.08</v>
+        <v>0.085</v>
       </c>
       <c r="N97" t="n">
         <v>0.03</v>
       </c>
       <c r="O97" t="n">
-        <v>33.44</v>
+        <v>32.916</v>
       </c>
       <c r="P97" t="s">
         <v>577</v>
@@ -7996,7 +8017,7 @@
         <v>581</v>
       </c>
       <c r="C98" s="1" t="n">
-        <v>44069</v>
+        <v>44071</v>
       </c>
       <c r="D98" t="s">
         <v>582</v>
@@ -8006,28 +8027,32 @@
       </c>
       <c r="F98"/>
       <c r="G98" t="n">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="H98" t="n">
-        <v>1452006</v>
+        <v>1494243</v>
       </c>
       <c r="I98" t="n">
-        <v>33.201</v>
+        <v>34.167</v>
       </c>
       <c r="J98" t="n">
-        <v>15800</v>
+        <v>21507</v>
       </c>
       <c r="K98" t="n">
-        <v>0.361</v>
+        <v>0.492</v>
       </c>
       <c r="L98" t="n">
-        <v>16715</v>
+        <v>16532</v>
       </c>
       <c r="M98" t="n">
-        <v>0.382</v>
-      </c>
-      <c r="N98"/>
-      <c r="O98"/>
+        <v>0.378</v>
+      </c>
+      <c r="N98" t="n">
+        <v>0.117</v>
+      </c>
+      <c r="O98" t="n">
+        <v>8.558</v>
+      </c>
       <c r="P98" t="s">
         <v>583</v>
       </c>
@@ -8049,7 +8074,7 @@
         <v>587</v>
       </c>
       <c r="C99" s="1" t="n">
-        <v>44067</v>
+        <v>44070</v>
       </c>
       <c r="D99" t="s">
         <v>588</v>
@@ -8059,31 +8084,31 @@
       </c>
       <c r="F99"/>
       <c r="G99" t="n">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="H99" t="n">
-        <v>6560686</v>
+        <v>6755457</v>
       </c>
       <c r="I99" t="n">
-        <v>663.339</v>
+        <v>683.032</v>
       </c>
       <c r="J99" t="n">
-        <v>71282</v>
+        <v>68043</v>
       </c>
       <c r="K99" t="n">
-        <v>7.207</v>
+        <v>6.88</v>
       </c>
       <c r="L99" t="n">
-        <v>71262</v>
+        <v>69934</v>
       </c>
       <c r="M99" t="n">
-        <v>7.205</v>
+        <v>7.071</v>
       </c>
       <c r="N99" t="n">
         <v>0.005</v>
       </c>
       <c r="O99" t="n">
-        <v>185.096</v>
+        <v>182.732</v>
       </c>
       <c r="P99" t="s">
         <v>589</v>
@@ -8165,7 +8190,7 @@
         <v>599</v>
       </c>
       <c r="C101" s="1" t="n">
-        <v>44062</v>
+        <v>44068</v>
       </c>
       <c r="D101" t="s">
         <v>600</v>
@@ -8175,39 +8200,43 @@
       </c>
       <c r="F101"/>
       <c r="G101" t="n">
-        <v>54</v>
+        <v>178</v>
       </c>
       <c r="H101" t="n">
-        <v>74830464</v>
+        <v>81462633</v>
       </c>
       <c r="I101" t="n">
-        <v>226.072</v>
-      </c>
-      <c r="J101"/>
-      <c r="K101"/>
+        <v>246.109</v>
+      </c>
+      <c r="J101" t="n">
+        <v>636249</v>
+      </c>
+      <c r="K101" t="n">
+        <v>1.922</v>
+      </c>
       <c r="L101" t="n">
-        <v>891584</v>
+        <v>740927</v>
       </c>
       <c r="M101" t="n">
-        <v>2.694</v>
+        <v>2.238</v>
       </c>
       <c r="N101" t="n">
-        <v>0.055</v>
+        <v>0.058</v>
       </c>
       <c r="O101" t="n">
-        <v>18.291</v>
+        <v>17.141</v>
       </c>
       <c r="P101" t="s">
-        <v>601</v>
+        <v>602</v>
       </c>
       <c r="Q101" t="s">
-        <v>600</v>
+        <v>603</v>
       </c>
       <c r="R101" t="s">
-        <v>602</v>
+        <v>604</v>
       </c>
       <c r="S101" t="s">
-        <v>603</v>
+        <v>605</v>
       </c>
     </row>
     <row r="102">
@@ -8215,126 +8244,130 @@
         <v>598</v>
       </c>
       <c r="B102" t="s">
-        <v>604</v>
+        <v>606</v>
       </c>
       <c r="C102" s="1" t="n">
-        <v>44068</v>
+        <v>44070</v>
       </c>
       <c r="D102" t="s">
-        <v>605</v>
+        <v>607</v>
       </c>
       <c r="E102" t="s">
-        <v>606</v>
+        <v>608</v>
       </c>
       <c r="F102"/>
       <c r="G102" t="n">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="H102" t="n">
-        <v>73016779</v>
+        <v>74792493</v>
       </c>
       <c r="I102" t="n">
-        <v>220.593</v>
+        <v>225.957</v>
       </c>
       <c r="J102" t="n">
-        <v>634461</v>
+        <v>742340</v>
       </c>
       <c r="K102" t="n">
-        <v>1.917</v>
+        <v>2.243</v>
       </c>
       <c r="L102" t="n">
-        <v>678978</v>
+        <v>692794</v>
       </c>
       <c r="M102" t="n">
-        <v>2.051</v>
+        <v>2.093</v>
       </c>
       <c r="N102" t="n">
-        <v>0.064</v>
+        <v>0.06</v>
       </c>
       <c r="O102" t="n">
-        <v>15.708</v>
+        <v>16.606</v>
       </c>
       <c r="P102" t="s">
-        <v>606</v>
+        <v>608</v>
       </c>
       <c r="Q102" t="s">
-        <v>607</v>
+        <v>609</v>
       </c>
       <c r="R102" t="s">
-        <v>608</v>
+        <v>610</v>
       </c>
       <c r="S102" t="s">
-        <v>609</v>
+        <v>611</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="s">
-        <v>610</v>
+        <v>612</v>
       </c>
       <c r="B103" t="s">
-        <v>611</v>
+        <v>613</v>
       </c>
       <c r="C103" s="1" t="n">
-        <v>44068</v>
+        <v>44070</v>
       </c>
       <c r="D103" t="s">
-        <v>612</v>
+        <v>614</v>
       </c>
       <c r="E103" t="s">
         <v>125</v>
       </c>
       <c r="F103"/>
       <c r="G103" t="n">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="H103" t="n">
-        <v>163129</v>
+        <v>166117</v>
       </c>
       <c r="I103" t="n">
-        <v>46.961</v>
-      </c>
-      <c r="J103"/>
-      <c r="K103"/>
+        <v>47.821</v>
+      </c>
+      <c r="J103" t="n">
+        <v>1379</v>
+      </c>
+      <c r="K103" t="n">
+        <v>0.397</v>
+      </c>
       <c r="L103" t="n">
-        <v>2219</v>
+        <v>1669</v>
       </c>
       <c r="M103" t="n">
-        <v>0.639</v>
+        <v>0.48</v>
       </c>
       <c r="N103" t="n">
-        <v>0.005</v>
+        <v>0.004</v>
       </c>
       <c r="O103" t="n">
-        <v>204.382</v>
+        <v>233.66</v>
       </c>
       <c r="P103" t="s">
         <v>125</v>
       </c>
       <c r="Q103" t="s">
-        <v>613</v>
+        <v>615</v>
       </c>
       <c r="R103" t="s">
         <v>27</v>
       </c>
       <c r="S103" t="s">
-        <v>614</v>
+        <v>616</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="s">
-        <v>615</v>
+        <v>617</v>
       </c>
       <c r="B104" t="s">
-        <v>616</v>
+        <v>618</v>
       </c>
       <c r="C104" s="1" t="n">
         <v>43950</v>
       </c>
       <c r="D104" t="s">
-        <v>617</v>
+        <v>619</v>
       </c>
       <c r="E104" t="s">
-        <v>618</v>
+        <v>620</v>
       </c>
       <c r="F104"/>
       <c r="G104" t="n">
@@ -8361,73 +8394,73 @@
         <v>38171</v>
       </c>
       <c r="P104" t="s">
-        <v>618</v>
+        <v>620</v>
       </c>
       <c r="Q104" t="s">
-        <v>619</v>
+        <v>621</v>
       </c>
       <c r="R104" t="s">
         <v>54</v>
       </c>
       <c r="S104" t="s">
-        <v>620</v>
+        <v>622</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="s">
-        <v>621</v>
+        <v>623</v>
       </c>
       <c r="B105" t="s">
-        <v>622</v>
+        <v>624</v>
       </c>
       <c r="C105" s="1" t="n">
-        <v>44066</v>
+        <v>44068</v>
       </c>
       <c r="D105" t="s">
-        <v>623</v>
+        <v>625</v>
       </c>
       <c r="E105" t="s">
-        <v>624</v>
+        <v>626</v>
       </c>
       <c r="F105"/>
       <c r="G105" t="n">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="H105" t="n">
-        <v>91548</v>
+        <v>93892</v>
       </c>
       <c r="I105" t="n">
-        <v>6.159</v>
+        <v>6.317</v>
       </c>
       <c r="J105" t="n">
-        <v>852</v>
+        <v>1574</v>
       </c>
       <c r="K105" t="n">
-        <v>0.057</v>
+        <v>0.106</v>
       </c>
       <c r="L105" t="n">
-        <v>1238</v>
+        <v>1269</v>
       </c>
       <c r="M105" t="n">
-        <v>0.083</v>
+        <v>0.085</v>
       </c>
       <c r="N105" t="n">
-        <v>0.083</v>
+        <v>0.086</v>
       </c>
       <c r="O105" t="n">
-        <v>12.086</v>
+        <v>11.657</v>
       </c>
       <c r="P105" t="s">
-        <v>624</v>
+        <v>626</v>
       </c>
       <c r="Q105" t="s">
-        <v>625</v>
+        <v>627</v>
       </c>
       <c r="R105" t="s">
         <v>27</v>
       </c>
       <c r="S105" t="s">
-        <v>626</v>
+        <v>628</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated testing data for 2020-08-31
</commit_message>
<xml_diff>
--- a/public/data/testing/covid-testing-latest-data-source-details.xlsx
+++ b/public/data/testing/covid-testing-latest-data-source-details.xlsx
@@ -110,7 +110,7 @@
     <t xml:space="preserve">Australia - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.health.gov.au/sites/default/files/documents/2020/08/coronavirus-covid-19-at-a-glance-27-august-2020.pdf</t>
+    <t xml:space="preserve">https://www.health.gov.au/sites/default/files/documents/2020/08/coronavirus-covid-19-at-a-glance-30-august-2020.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">Australian Government Department of Health</t>
@@ -245,7 +245,7 @@
     <t xml:space="preserve">Bolivia - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://minsalud.gob.bo/4550-bolivia-acumula-50-397-pacientes-recuperados-de-covid-19-y-los-casos-positivos-llegan-a-112-094</t>
+    <t xml:space="preserve">https://minsalud.gob.bo/4558-covid-19-ministerio-de-salud-reporta-1-035-contagios-nuevos-y-65-fallecidos</t>
   </si>
   <si>
     <t xml:space="preserve">https://www.minsalud.gob.bo/</t>
@@ -398,7 +398,7 @@
     <t xml:space="preserve">Cote d'Ivoire - samples tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.facebook.com/Mshpci/posts/1680281235470897</t>
+    <t xml:space="preserve">https://www.facebook.com/Mshpci/posts/1683118181853869</t>
   </si>
   <si>
     <t xml:space="preserve">Ministry of Health and Public Hygiene</t>
@@ -477,7 +477,7 @@
     <t xml:space="preserve">Democratic Republic of Congo - samples tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/CMR_Covid19_RDC/status/1298904810050260992/photo/1</t>
+    <t xml:space="preserve">https://twitter.com/CMR_Covid19_RDC/status/1299647693489418241/photo/1</t>
   </si>
   <si>
     <t xml:space="preserve">DRC COVID-19 Pandemic Response Multisectoral Committee</t>
@@ -495,7 +495,7 @@
     <t xml:space="preserve">Denmark - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://files.ssi.dk/Data-epidemiologisk-rapport-28082020-mm29</t>
+    <t xml:space="preserve">https://files.ssi.dk/Data-epidemiologiske-rapport-31082020-lo27</t>
   </si>
   <si>
     <t xml:space="preserve">Statens Serum Institut</t>
@@ -513,7 +513,7 @@
     <t xml:space="preserve">Ecuador - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.gestionderiesgos.gob.ec/wp-content/uploads/2020/08/INFOGRAFIA-NACIONALCOVID19-COE-NACIONAL-08h00-27082020.pdf</t>
+    <t xml:space="preserve">https://www.gestionderiesgos.gob.ec/wp-content/uploads/2020/08/INFOGRAFIA-NACIONALCOVID19-COE-NACIONAL-08h00-29082020.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">Government of Ecuador</t>
@@ -539,7 +539,7 @@
     <t xml:space="preserve">El Salvador - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.facebook.com/nayibbukele/posts/3182381598514676</t>
+    <t xml:space="preserve">https://www.facebook.com/nayibbukele/posts/3191496677603168</t>
   </si>
   <si>
     <t xml:space="preserve">Government of El Salvador</t>
@@ -583,7 +583,7 @@
     <t xml:space="preserve">Ethiopia - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/EPHIEthiopia/status/1298669531615961090</t>
+    <t xml:space="preserve">https://twitter.com/EPHIEthiopia/status/1299752756551520263</t>
   </si>
   <si>
     <t xml:space="preserve">Ethiopian Public Health Institute</t>
@@ -753,7 +753,7 @@
     <t xml:space="preserve">Greece - samples tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://eody.gov.gr/covid-gr-daily-report-27-08-2020/</t>
+    <t xml:space="preserve">https://eody.gov.gr/covid-gr-daily-report-20200830</t>
   </si>
   <si>
     <t xml:space="preserve">National Organization of Public Health</t>
@@ -892,7 +892,7 @@
     <t xml:space="preserve">Iran - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">http://irangov.ir/detail/346050</t>
+    <t xml:space="preserve">http://irangov.ir/detail/346157</t>
   </si>
   <si>
     <t xml:space="preserve">Government of Iran</t>
@@ -950,7 +950,7 @@
     <t xml:space="preserve">Israel - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://govextra.gov.il/media/25774/covid19-data-israel-20082021.csv</t>
+    <t xml:space="preserve">https://govextra.gov.il/media/25848/covid19-data-israel-24082021.csv</t>
   </si>
   <si>
     <t xml:space="preserve">Israel Ministry of Health</t>
@@ -1009,7 +1009,7 @@
     <t xml:space="preserve">Japan - people tested (incl. non-PCR)</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.mhlw.go.jp/stf/newpage_13239.html</t>
+    <t xml:space="preserve">https://www.mhlw.go.jp/stf/newpage_13273.html</t>
   </si>
   <si>
     <t xml:space="preserve">Ministry of Health, Labor and Welfare Press Release</t>
@@ -1034,10 +1034,10 @@
     <t xml:space="preserve">Japan - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.mhlw.go.jp/content/10906000/000663894.pdf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The cumulative total reported in the press release (1,707,901) does not sum to the cumulative total calculated from the weekly and daily figures reported by the MOH. See: https://www.mhlw.go.jp/content/10906000/000663894.pdf</t>
+    <t xml:space="preserve">https://www.mhlw.go.jp/content/10906000/000664890.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The cumulative total reported in the press release (1,768,968) does not sum to the cumulative total calculated from the weekly and daily figures reported by the MOH. See: https://www.mhlw.go.jp/content/10906000/000664890.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">On 11 April 2020, the MOH started providing a daily time series on the "Implementation status of PCR tests for new coronavirus in Japan (based on the date on which results were determined" (via Google translate). 
@@ -1068,7 +1068,7 @@
     <t xml:space="preserve">Kenya - samples tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/MOH_Kenya/status/1298263711564488707</t>
+    <t xml:space="preserve">https://twitter.com/MOH_Kenya/status/1299691592748597248</t>
   </si>
   <si>
     <t xml:space="preserve">Kenya Ministry of Health</t>
@@ -1090,7 +1090,7 @@
     <t xml:space="preserve">Kuwait - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/KUWAIT_MOH/status/1298953484306350081/photo/1</t>
+    <t xml:space="preserve">https://twitter.com/KUWAIT_MOH/status/1299663124493197313/photo/1</t>
   </si>
   <si>
     <t xml:space="preserve">Kuwait Ministry of Health</t>
@@ -1156,7 +1156,7 @@
     <t xml:space="preserve">Malaysia - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">http://covid-19.moh.gov.my/terkini/082020/situasi-terkini-27-ogos-2020</t>
+    <t xml:space="preserve">http://covid-19.moh.gov.my/terkini/082020/situasi-terkini-30-ogos-2020</t>
   </si>
   <si>
     <t xml:space="preserve">Ministry of Health Malaysia</t>
@@ -1182,7 +1182,7 @@
     <t xml:space="preserve">Maldives - samples tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/HPA_MV/status/1299028491674025989/photo/1</t>
+    <t xml:space="preserve">https://twitter.com/HPA_MV/status/1299757834071023617/photo/1</t>
   </si>
   <si>
     <t xml:space="preserve">Maldives Health Protection Agency</t>
@@ -1248,7 +1248,7 @@
     <t xml:space="preserve">Morocco - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/Ministere_Sante/status/1299034987212177408/photo/1</t>
+    <t xml:space="preserve">https://twitter.com/Ministere_Sante/status/1299760106150731777/photo/1</t>
   </si>
   <si>
     <t xml:space="preserve">Morocco Ministry of Health</t>
@@ -1435,7 +1435,7 @@
     <t xml:space="preserve">Panama - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/MINSAPma/status/1298761952492224512/photo/1</t>
+    <t xml:space="preserve">https://twitter.com/MINSAPma/status/1299488397359280128/photo/1</t>
   </si>
   <si>
     <t xml:space="preserve">Panama Ministry of Health</t>
@@ -1445,7 +1445,8 @@
   </si>
   <si>
     <t xml:space="preserve">The Panama Ministry of Health reports the cumulative number of tests performed ("pruebas realizadas") on [their official dashboard](http://minsa.gob.pa/covid-19) with a time series dating back to 9 March 2020. The page with testing numbers is not the first one shown but can be navigated to with the arrows at the bottom of the dashboard. The dashboard shows the cumulative number of total, positive ("positivas"), negative ("negativas"), and control tests ("prueba de control") performed. We report here the total of positive and negative numbers because: 1) the time series only includes positive and negative test numbers; and 2) the total they provide seems to include control tests, which we understand to be used for testing quality control.
-Starting 15 August 2020, the official dashboard is no longer being updated while it is being restructured. We now source the daily testing numbers from the [Ministry of Health's official Twitter page](https://twitter.com/MINSAPma). We continue to report the total of positive ("casos confirmados") and negative ("pruebas negativas") tests.</t>
+Starting 15 August 2020, the official dashboard is no longer being updated while it is being restructured. We now source the daily testing numbers from the [Ministry of Health's official Twitter page](https://twitter.com/MINSAPma). We continue to report the total of positive ("casos confirmados") and negative ("pruebas negativas") tests.
+The reported number of tests performed may include non-PCR tests. The [official weekly COVID-19 bulletin on 22 May 2020](http://minsa.b-cdn.net/sites/default/files/publicacion-general/boletin_14_covid-19.pdf) lists a set of actions taken at the national level, including: "Algorithm request to the head of the ICGES virology laboratory for the confirmation or ruling out of COVID-19 cases, using serological tests" (translated). This implies that serological (non-PCR) tests are planning to be used, or are already being used, in case confirmation. On the other hand, an [official epidemiological report published on 12 May 2020](http://minsa.b-cdn.net/sites/default/files/publicacion-general/informe_especial_1_covid-19_panama_.pdf) states that "The diagnostic method used for the detection of SARS-CoV-2 in the laboratory was the Molecular Real-Time Polymerase Chain Reaction Test (RT-PCR)" (translated). We have been unable to find any official information that clarifies whether non-PCR tests are being used for case confirmation.</t>
   </si>
   <si>
     <t xml:space="preserve">PRY</t>
@@ -1474,7 +1475,7 @@
     <t xml:space="preserve">Peru - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.dge.gob.pe/portal/docs/tools/coronavirus/coronavirus180820.pdf</t>
+    <t xml:space="preserve">https://www.dge.gob.pe/portal/docs/tools/coronavirus/coronavirus250820.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">Peru Ministry of Health</t>
@@ -1495,7 +1496,7 @@
     <t xml:space="preserve">Philippines - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://drive.google.com/drive/folders/1QUIqtJtcgNfZRKIt0BpECegkx-z7IDhi?usp=sharing</t>
+    <t xml:space="preserve">https://drive.google.com/drive/folders/1VCjxPkiFPyceTiyJzRvn7eO616twBOpy</t>
   </si>
   <si>
     <t xml:space="preserve">Philippines Department of Health</t>
@@ -1515,7 +1516,7 @@
     <t xml:space="preserve">Poland - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/MZ_GOV_PL/status/1298908108161511426</t>
+    <t xml:space="preserve">https://twitter.com/MZ_GOV_PL/status/1299995274182623232</t>
   </si>
   <si>
     <t xml:space="preserve">Poland Ministry of Health</t>
@@ -1583,7 +1584,7 @@
     <t xml:space="preserve">Romania - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://gov.ro/ro/media/comunicate/buletin-de-presa-28-august-2020-ora-13-00&amp;page=1</t>
+    <t xml:space="preserve">https://gov.ro/ro/media/comunicate/buletin-de-presa-30-august-2020-ora-13-00&amp;page=1</t>
   </si>
   <si>
     <t xml:space="preserve">Ministry of Internal Affairs</t>
@@ -1606,7 +1607,7 @@
     <t xml:space="preserve">Russia - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://rospotrebnadzor.ru/about/info/news/news_details.php?ELEMENT_ID=15255</t>
+    <t xml:space="preserve">https://rospotrebnadzor.ru/about/info/news/news_details.php?ELEMENT_ID=15269</t>
   </si>
   <si>
     <t xml:space="preserve">Government of the Russian Federation</t>
@@ -1626,7 +1627,7 @@
     <t xml:space="preserve">Rwanda - samples tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/RwandaHealth/status/1298361056834785284</t>
+    <t xml:space="preserve">https://twitter.com/RwandaHealth/status/1299458252950982656</t>
   </si>
   <si>
     <t xml:space="preserve">Rwanda Ministry of Health</t>
@@ -1800,7 +1801,7 @@
     <t xml:space="preserve">South Korea - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.cdc.go.kr/board/board.es?mid=&amp;bid=0030&amp;act=view&amp;list_no=368248&amp;tag=&amp;nPage=1</t>
+    <t xml:space="preserve">https://www.cdc.go.kr/board/board.es?mid=&amp;bid=0030&amp;act=view&amp;list_no=368269&amp;tag=&amp;nPage=1</t>
   </si>
   <si>
     <t xml:space="preserve">South Korea CDC</t>
@@ -1922,7 +1923,7 @@
     <t xml:space="preserve">Thailand - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://ddc.moph.go.th/viralpneumonia/file/situation/situation-no237-270863.pdf</t>
+    <t xml:space="preserve">https://ddc.moph.go.th/viralpneumonia/file/situation/situation-no240-300863.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">Department of Disease Control</t>
@@ -2010,7 +2011,7 @@
     <t xml:space="preserve">Uganda - samples tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/MinofHealthUG/status/1298965036740812802/photo/1</t>
+    <t xml:space="preserve">https://twitter.com/MinofHealthUG/status/1299295338730336256/photo/1</t>
   </si>
   <si>
     <t xml:space="preserve">Uganda Ministry of Health</t>
@@ -2070,26 +2071,25 @@
     <t xml:space="preserve">United Kingdom - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://assets.publishing.service.gov.uk/government/uploads/system/uploads/attachment_data/file/910857/2020-08-20_COVID-19_UK_testing_time_series.csv</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Public Health England/Department of Health and Social Care</t>
+    <t xml:space="preserve">https://coronavirus.data.gov.uk/developers-guide</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Department of Health and Social Care and Public Health England</t>
   </si>
   <si>
     <t xml:space="preserve">Sum of tests processed for pillars 1 and 2</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.gov.uk/guidance/coronavirus-covid-19-information-for-the-public#number-of-cases</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Since early June 2020, the United Kingdom has been publishing a full retrospective time series in CSV format, with testing data going back to March 2020. We aggregate the data for the United Kingdom based only on two 'pillars':
-- Pillar 1: swab (antigen) testing in Public Health England (PHE) labs and NHS hospitals for those with a clinical need and health and care workers;
-- Pillar 2: swab (antigen) testing for the wider population.
-For both pillars, we use the 'Daily number of tests processed' and 'Cumulative number of tests processed' columns to create of time series of PCR tests performed in the United Kingdom. We do not include tests delivered or sent out that have not been recorded as having been processed.
+    <t xml:space="preserve">https://coronavirus.data.gov.uk/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Since late August 2020, the United Kingdom has been publishing a full retrospective time series of its testing data going back to April 2020 via [its coronavirus API](https://coronavirus.data.gov.uk/developers-guide). We aggregate the data for the United Kingdom based only on two 'pillars':
+- Pillar 1: number of lab-confirmed positive or negative COVID-19 pillar 1 test results by date reported. Pillar 1 testing includes swab testing for COVID-19 processed by NHS and (in England) PHE labs. This is a count of test results and may include multiple tests for an individual person. 
+- Pillar 2: number of lab-confirmed positive or negative COVID-19 pillar 2 test results, by date reported. Pillar 2 testing includes swab testing for COVID-19 processed by commercial partners. Commercial partner testing was introduced in all parts of the UK in April but data are not available for all nations on a consistent basis. Step changes in the series occur when new data sources became available. 
+For both pillars, we use the 'PillarOneTestsByPublishDate' and 'PillarTwoTestsByPublishDate' metrics to create of time series of PCR tests performed in the United Kingdom. These do not include tests delivered or sent out that have not been recorded as having been processed.
 We do not include other pillars, i.e.:
 - Pillar 3: this pillar consists (fully) of serology tests, which we aim not to include;
-- Pillar 4: this pillar consists (partly) of serology tests, which we aim not to include, and positive tests results from this pillar seem not to be included in the government's total for positive cases.
-The source notes that 'data on UK tests is updated daily. The figures for test results are compiled from different sources. Daily totals reflect actual counts reported for the previous day. Each day there may be corrections to previous reported figures. This means that previously published daily counts will not necessarily sum to the latest cumulative figure. It also means that today’s cumulative count may not match the previous day’s cumulative count plus today’s daily count.'</t>
+- Pillar 4: this pillar consists (partly) of serology tests, which we aim not to include, and positive tests results from this pillar seem not to be included in the government's total for positive cases.</t>
   </si>
   <si>
     <t xml:space="preserve">USA</t>
@@ -2098,7 +2098,7 @@
     <t xml:space="preserve">United States - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://healthdata.gov/sites/default/files/covid-19_diagnostic_lab_testing_20200828_1201.csv</t>
+    <t xml:space="preserve">https://healthdata.gov/sites/default/files/covid-19_diagnostic_lab_testing_20200830_2342.csv</t>
   </si>
   <si>
     <t xml:space="preserve">Department of Health &amp; Human Services</t>
@@ -2150,7 +2150,7 @@
     <t xml:space="preserve">Uruguay - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.gub.uy/ministerio-salud-publica/comunicacion/noticias/informe-situacion-sobre-coronavirus-covid-19-uruguay-27-agosto</t>
+    <t xml:space="preserve">https://www.gub.uy/ministerio-salud-publica/comunicacion/noticias/informe-situacion-sobre-coronavirus-covid-19-uruguay-29-agosto</t>
   </si>
   <si>
     <t xml:space="preserve">https://www.gub.uy/ministerio-salud-publica/comunicacion/noticias</t>
@@ -2188,7 +2188,7 @@
     <t xml:space="preserve">Zimbabwe - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/MoHCCZim/status/1298314387917340672</t>
+    <t xml:space="preserve">https://twitter.com/MoHCCZim/status/1299423733120217089</t>
   </si>
   <si>
     <t xml:space="preserve">Zimbabwe Ministry of Health and Child Care</t>
@@ -2605,7 +2605,7 @@
         <v>20</v>
       </c>
       <c r="C2" s="1" t="n">
-        <v>44063</v>
+        <v>44072</v>
       </c>
       <c r="D2" t="s">
         <v>21</v>
@@ -2615,31 +2615,31 @@
       </c>
       <c r="F2"/>
       <c r="G2" t="n">
-        <v>177</v>
+        <v>186</v>
       </c>
       <c r="H2" t="n">
-        <v>901255</v>
+        <v>1082679</v>
       </c>
       <c r="I2" t="n">
-        <v>19.941</v>
+        <v>23.955</v>
       </c>
       <c r="J2" t="n">
-        <v>4391</v>
+        <v>11097</v>
       </c>
       <c r="K2" t="n">
-        <v>0.097</v>
+        <v>0.246</v>
       </c>
       <c r="L2" t="n">
-        <v>11114</v>
+        <v>15679</v>
       </c>
       <c r="M2" t="n">
-        <v>0.246</v>
+        <v>0.347</v>
       </c>
       <c r="N2" t="n">
-        <v>0.579</v>
+        <v>0.541</v>
       </c>
       <c r="O2" t="n">
-        <v>1.727</v>
+        <v>1.847</v>
       </c>
       <c r="P2" t="s">
         <v>22</v>
@@ -2662,7 +2662,7 @@
         <v>25</v>
       </c>
       <c r="C3" s="1" t="n">
-        <v>44070</v>
+        <v>44072</v>
       </c>
       <c r="D3" t="s">
         <v>26</v>
@@ -2672,31 +2672,31 @@
       </c>
       <c r="F3"/>
       <c r="G3" t="n">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="H3" t="n">
-        <v>1246917</v>
+        <v>1305736</v>
       </c>
       <c r="I3" t="n">
-        <v>27.589</v>
+        <v>28.891</v>
       </c>
       <c r="J3" t="n">
-        <v>7766</v>
+        <v>12667</v>
       </c>
       <c r="K3" t="n">
-        <v>0.172</v>
+        <v>0.28</v>
       </c>
       <c r="L3" t="n">
-        <v>15536</v>
+        <v>18028</v>
       </c>
       <c r="M3" t="n">
-        <v>0.344</v>
+        <v>0.399</v>
       </c>
       <c r="N3" t="n">
-        <v>0.591</v>
+        <v>0.471</v>
       </c>
       <c r="O3" t="n">
-        <v>1.693</v>
+        <v>2.124</v>
       </c>
       <c r="P3" t="s">
         <v>22</v>
@@ -2719,7 +2719,7 @@
         <v>30</v>
       </c>
       <c r="C4" s="1" t="n">
-        <v>44070</v>
+        <v>44073</v>
       </c>
       <c r="D4" t="s">
         <v>31</v>
@@ -2729,31 +2729,27 @@
       </c>
       <c r="F4"/>
       <c r="G4" t="n">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="H4" t="n">
-        <v>5972680</v>
+        <v>6168229</v>
       </c>
       <c r="I4" t="n">
-        <v>234.224</v>
-      </c>
-      <c r="J4" t="n">
-        <v>86268</v>
-      </c>
-      <c r="K4" t="n">
-        <v>3.383</v>
-      </c>
+        <v>241.892</v>
+      </c>
+      <c r="J4"/>
+      <c r="K4"/>
       <c r="L4" t="n">
-        <v>66264</v>
+        <v>65949</v>
       </c>
       <c r="M4" t="n">
-        <v>2.599</v>
+        <v>2.586</v>
       </c>
       <c r="N4" t="n">
-        <v>0.003</v>
+        <v>0.002</v>
       </c>
       <c r="O4" t="n">
-        <v>382.713</v>
+        <v>488.511</v>
       </c>
       <c r="P4" t="s">
         <v>32</v>
@@ -2776,7 +2772,7 @@
         <v>36</v>
       </c>
       <c r="C5" s="1" t="n">
-        <v>44071</v>
+        <v>44074</v>
       </c>
       <c r="D5" t="s">
         <v>37</v>
@@ -2786,31 +2782,31 @@
       </c>
       <c r="F5"/>
       <c r="G5" t="n">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="H5" t="n">
-        <v>1147944</v>
+        <v>1180711</v>
       </c>
       <c r="I5" t="n">
-        <v>127.459</v>
+        <v>131.097</v>
       </c>
       <c r="J5" t="n">
-        <v>14701</v>
+        <v>8619</v>
       </c>
       <c r="K5" t="n">
-        <v>1.632</v>
+        <v>0.957</v>
       </c>
       <c r="L5" t="n">
-        <v>10362</v>
+        <v>11358</v>
       </c>
       <c r="M5" t="n">
-        <v>1.151</v>
+        <v>1.261</v>
       </c>
       <c r="N5" t="n">
-        <v>0.024</v>
+        <v>0.025</v>
       </c>
       <c r="O5" t="n">
-        <v>40.91</v>
+        <v>40.175</v>
       </c>
       <c r="P5" t="s">
         <v>39</v>
@@ -2833,7 +2829,7 @@
         <v>43</v>
       </c>
       <c r="C6" s="1" t="n">
-        <v>44071</v>
+        <v>44073</v>
       </c>
       <c r="D6" t="s">
         <v>44</v>
@@ -2843,27 +2839,31 @@
       </c>
       <c r="F6"/>
       <c r="G6" t="n">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="H6" t="n">
-        <v>1078767</v>
+        <v>1100729</v>
       </c>
       <c r="I6" t="n">
-        <v>633.978</v>
-      </c>
-      <c r="J6"/>
-      <c r="K6"/>
+        <v>646.885</v>
+      </c>
+      <c r="J6" t="n">
+        <v>12311</v>
+      </c>
+      <c r="K6" t="n">
+        <v>7.235</v>
+      </c>
       <c r="L6" t="n">
-        <v>9566</v>
+        <v>10109</v>
       </c>
       <c r="M6" t="n">
-        <v>5.622</v>
+        <v>5.941</v>
       </c>
       <c r="N6" t="n">
-        <v>0.042</v>
+        <v>0.033</v>
       </c>
       <c r="O6" t="n">
-        <v>23.864</v>
+        <v>30.074</v>
       </c>
       <c r="P6" t="s">
         <v>46</v>
@@ -2886,7 +2886,7 @@
         <v>50</v>
       </c>
       <c r="C7" s="1" t="n">
-        <v>44069</v>
+        <v>44071</v>
       </c>
       <c r="D7" t="s">
         <v>51</v>
@@ -2896,31 +2896,31 @@
       </c>
       <c r="F7"/>
       <c r="G7" t="n">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="H7" t="n">
-        <v>1485261</v>
+        <v>1514126</v>
       </c>
       <c r="I7" t="n">
-        <v>9.019</v>
+        <v>9.194</v>
       </c>
       <c r="J7" t="n">
-        <v>15070</v>
+        <v>13741</v>
       </c>
       <c r="K7" t="n">
-        <v>0.092</v>
+        <v>0.083</v>
       </c>
       <c r="L7" t="n">
-        <v>13109</v>
+        <v>13375</v>
       </c>
       <c r="M7" t="n">
-        <v>0.08</v>
+        <v>0.081</v>
       </c>
       <c r="N7" t="n">
-        <v>0.188</v>
+        <v>0.178</v>
       </c>
       <c r="O7" t="n">
-        <v>5.309</v>
+        <v>5.632</v>
       </c>
       <c r="P7" t="s">
         <v>52</v>
@@ -2996,7 +2996,7 @@
         <v>63</v>
       </c>
       <c r="C9" s="1" t="n">
-        <v>44069</v>
+        <v>44072</v>
       </c>
       <c r="D9" t="s">
         <v>64</v>
@@ -3006,31 +3006,31 @@
       </c>
       <c r="F9"/>
       <c r="G9" t="n">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="H9" t="n">
-        <v>2211141</v>
+        <v>2278391</v>
       </c>
       <c r="I9" t="n">
-        <v>190.786</v>
+        <v>196.589</v>
       </c>
       <c r="J9" t="n">
-        <v>20336</v>
+        <v>16482</v>
       </c>
       <c r="K9" t="n">
-        <v>1.755</v>
+        <v>1.422</v>
       </c>
       <c r="L9" t="n">
-        <v>18908</v>
+        <v>19858</v>
       </c>
       <c r="M9" t="n">
-        <v>1.631</v>
+        <v>1.713</v>
       </c>
       <c r="N9" t="n">
-        <v>0.023</v>
+        <v>0.021</v>
       </c>
       <c r="O9" t="n">
-        <v>43.899</v>
+        <v>47.233</v>
       </c>
       <c r="P9" t="s">
         <v>65</v>
@@ -3053,7 +3053,7 @@
         <v>69</v>
       </c>
       <c r="C10" s="1" t="n">
-        <v>44069</v>
+        <v>44071</v>
       </c>
       <c r="D10" t="s">
         <v>70</v>
@@ -3063,31 +3063,31 @@
       </c>
       <c r="F10"/>
       <c r="G10" t="n">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="H10" t="n">
-        <v>225474</v>
+        <v>232975</v>
       </c>
       <c r="I10" t="n">
-        <v>19.316</v>
+        <v>19.958</v>
       </c>
       <c r="J10" t="n">
-        <v>2274</v>
+        <v>3632</v>
       </c>
       <c r="K10" t="n">
-        <v>0.195</v>
+        <v>0.311</v>
       </c>
       <c r="L10" t="n">
-        <v>2405</v>
+        <v>2723</v>
       </c>
       <c r="M10" t="n">
-        <v>0.206</v>
+        <v>0.233</v>
       </c>
       <c r="N10" t="n">
-        <v>0.474</v>
+        <v>0.371</v>
       </c>
       <c r="O10" t="n">
-        <v>2.11</v>
+        <v>2.698</v>
       </c>
       <c r="P10" t="s">
         <v>45</v>
@@ -3161,7 +3161,7 @@
         <v>81</v>
       </c>
       <c r="C12" s="1" t="n">
-        <v>44071</v>
+        <v>44073</v>
       </c>
       <c r="D12" t="s">
         <v>82</v>
@@ -3171,27 +3171,31 @@
       </c>
       <c r="F12"/>
       <c r="G12" t="n">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="H12" t="n">
-        <v>392089</v>
+        <v>404683</v>
       </c>
       <c r="I12" t="n">
-        <v>56.428</v>
-      </c>
-      <c r="J12"/>
-      <c r="K12"/>
+        <v>58.241</v>
+      </c>
+      <c r="J12" t="n">
+        <v>6257</v>
+      </c>
+      <c r="K12" t="n">
+        <v>0.9</v>
+      </c>
       <c r="L12" t="n">
-        <v>4767</v>
+        <v>5169</v>
       </c>
       <c r="M12" t="n">
-        <v>0.686</v>
+        <v>0.744</v>
       </c>
       <c r="N12" t="n">
-        <v>0.033</v>
+        <v>0.029</v>
       </c>
       <c r="O12" t="n">
-        <v>30.67</v>
+        <v>35.027</v>
       </c>
       <c r="P12" t="s">
         <v>84</v>
@@ -3214,7 +3218,7 @@
         <v>87</v>
       </c>
       <c r="C13" s="1" t="n">
-        <v>44071</v>
+        <v>44073</v>
       </c>
       <c r="D13" t="s">
         <v>88</v>
@@ -3224,31 +3228,31 @@
       </c>
       <c r="F13"/>
       <c r="G13" t="n">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="H13" t="n">
-        <v>5293936</v>
+        <v>5440371</v>
       </c>
       <c r="I13" t="n">
-        <v>140.266</v>
+        <v>144.146</v>
       </c>
       <c r="J13" t="n">
-        <v>47671</v>
+        <v>85107</v>
       </c>
       <c r="K13" t="n">
-        <v>1.263</v>
+        <v>2.255</v>
       </c>
       <c r="L13" t="n">
-        <v>45674</v>
+        <v>51948</v>
       </c>
       <c r="M13" t="n">
-        <v>1.21</v>
+        <v>1.376</v>
       </c>
       <c r="N13" t="n">
-        <v>0.009</v>
+        <v>0.008</v>
       </c>
       <c r="O13" t="n">
-        <v>107.468</v>
+        <v>119.46</v>
       </c>
       <c r="P13" t="s">
         <v>89</v>
@@ -3271,7 +3275,7 @@
         <v>92</v>
       </c>
       <c r="C14" s="1" t="n">
-        <v>44070</v>
+        <v>44073</v>
       </c>
       <c r="D14" t="s">
         <v>93</v>
@@ -3283,31 +3287,31 @@
         <v>94</v>
       </c>
       <c r="G14" t="n">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="H14" t="n">
-        <v>2303242</v>
+        <v>2400522</v>
       </c>
       <c r="I14" t="n">
-        <v>120.486</v>
+        <v>125.575</v>
       </c>
       <c r="J14" t="n">
-        <v>27019</v>
+        <v>34769</v>
       </c>
       <c r="K14" t="n">
-        <v>1.413</v>
+        <v>1.819</v>
       </c>
       <c r="L14" t="n">
-        <v>27087</v>
+        <v>28073</v>
       </c>
       <c r="M14" t="n">
-        <v>1.417</v>
+        <v>1.469</v>
       </c>
       <c r="N14" t="n">
-        <v>0.065</v>
+        <v>0.063</v>
       </c>
       <c r="O14" t="n">
-        <v>15.38</v>
+        <v>15.975</v>
       </c>
       <c r="P14" t="s">
         <v>95</v>
@@ -3330,7 +3334,7 @@
         <v>99</v>
       </c>
       <c r="C15" s="1" t="n">
-        <v>44070</v>
+        <v>44073</v>
       </c>
       <c r="D15" t="s">
         <v>100</v>
@@ -3340,31 +3344,31 @@
       </c>
       <c r="F15"/>
       <c r="G15" t="n">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="H15" t="n">
-        <v>2519489</v>
+        <v>2599703</v>
       </c>
       <c r="I15" t="n">
-        <v>49.515</v>
+        <v>51.092</v>
       </c>
       <c r="J15" t="n">
-        <v>30059</v>
+        <v>26879</v>
       </c>
       <c r="K15" t="n">
-        <v>0.591</v>
+        <v>0.528</v>
       </c>
       <c r="L15" t="n">
-        <v>30006</v>
+        <v>28973</v>
       </c>
       <c r="M15" t="n">
-        <v>0.59</v>
+        <v>0.569</v>
       </c>
       <c r="N15" t="n">
-        <v>0.334</v>
+        <v>0.329</v>
       </c>
       <c r="O15" t="n">
-        <v>2.997</v>
+        <v>3.036</v>
       </c>
       <c r="P15" t="s">
         <v>101</v>
@@ -3387,7 +3391,7 @@
         <v>105</v>
       </c>
       <c r="C16" s="1" t="n">
-        <v>44068</v>
+        <v>44071</v>
       </c>
       <c r="D16" t="s">
         <v>106</v>
@@ -3397,25 +3401,25 @@
       </c>
       <c r="F16"/>
       <c r="G16" t="n">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="H16" t="n">
-        <v>119301</v>
+        <v>125419</v>
       </c>
       <c r="I16" t="n">
-        <v>23.419</v>
+        <v>24.62</v>
       </c>
       <c r="J16" t="n">
-        <v>1304</v>
+        <v>2211</v>
       </c>
       <c r="K16" t="n">
-        <v>0.256</v>
+        <v>0.434</v>
       </c>
       <c r="L16" t="n">
-        <v>1661</v>
+        <v>1883</v>
       </c>
       <c r="M16" t="n">
-        <v>0.326</v>
+        <v>0.37</v>
       </c>
       <c r="N16"/>
       <c r="O16"/>
@@ -3440,7 +3444,7 @@
         <v>111</v>
       </c>
       <c r="C17" s="1" t="n">
-        <v>44069</v>
+        <v>44072</v>
       </c>
       <c r="D17" t="s">
         <v>112</v>
@@ -3450,31 +3454,31 @@
       </c>
       <c r="F17"/>
       <c r="G17" t="n">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="H17" t="n">
-        <v>122975</v>
+        <v>125972</v>
       </c>
       <c r="I17" t="n">
-        <v>4.662</v>
+        <v>4.776</v>
       </c>
       <c r="J17" t="n">
-        <v>896</v>
+        <v>887</v>
       </c>
       <c r="K17" t="n">
         <v>0.034</v>
       </c>
       <c r="L17" t="n">
-        <v>884</v>
+        <v>972</v>
       </c>
       <c r="M17" t="n">
-        <v>0.034</v>
+        <v>0.037</v>
       </c>
       <c r="N17" t="n">
-        <v>0.067</v>
+        <v>0.072</v>
       </c>
       <c r="O17" t="n">
-        <v>15.019</v>
+        <v>13.971</v>
       </c>
       <c r="P17" t="s">
         <v>113</v>
@@ -3497,7 +3501,7 @@
         <v>117</v>
       </c>
       <c r="C18" s="1" t="n">
-        <v>44071</v>
+        <v>44074</v>
       </c>
       <c r="D18" t="s">
         <v>118</v>
@@ -3507,31 +3511,31 @@
       </c>
       <c r="F18"/>
       <c r="G18" t="n">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="H18" t="n">
-        <v>162301</v>
+        <v>168229</v>
       </c>
       <c r="I18" t="n">
-        <v>39.535</v>
+        <v>40.979</v>
       </c>
       <c r="J18" t="n">
-        <v>2065</v>
+        <v>1591</v>
       </c>
       <c r="K18" t="n">
-        <v>0.503</v>
+        <v>0.388</v>
       </c>
       <c r="L18" t="n">
-        <v>2305</v>
+        <v>2201</v>
       </c>
       <c r="M18" t="n">
-        <v>0.561</v>
+        <v>0.536</v>
       </c>
       <c r="N18" t="n">
-        <v>0.115</v>
+        <v>0.126</v>
       </c>
       <c r="O18" t="n">
-        <v>8.661</v>
+        <v>7.909</v>
       </c>
       <c r="P18" t="s">
         <v>119</v>
@@ -3554,7 +3558,7 @@
         <v>123</v>
       </c>
       <c r="C19" s="1" t="n">
-        <v>44069</v>
+        <v>44072</v>
       </c>
       <c r="D19" t="s">
         <v>124</v>
@@ -3566,31 +3570,31 @@
         <v>126</v>
       </c>
       <c r="G19" t="n">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="H19" t="n">
-        <v>377494</v>
+        <v>392785</v>
       </c>
       <c r="I19" t="n">
-        <v>33.328</v>
+        <v>34.678</v>
       </c>
       <c r="J19" t="n">
-        <v>4549</v>
+        <v>4591</v>
       </c>
       <c r="K19" t="n">
-        <v>0.402</v>
+        <v>0.405</v>
       </c>
       <c r="L19" t="n">
-        <v>4436</v>
+        <v>4528</v>
       </c>
       <c r="M19" t="n">
-        <v>0.392</v>
+        <v>0.4</v>
       </c>
       <c r="N19" t="n">
-        <v>0.011</v>
+        <v>0.009</v>
       </c>
       <c r="O19" t="n">
-        <v>92.417</v>
+        <v>111.606</v>
       </c>
       <c r="P19" t="s">
         <v>125</v>
@@ -3613,7 +3617,7 @@
         <v>130</v>
       </c>
       <c r="C20" s="1" t="n">
-        <v>44069</v>
+        <v>44072</v>
       </c>
       <c r="D20" t="s">
         <v>131</v>
@@ -3623,31 +3627,31 @@
       </c>
       <c r="F20"/>
       <c r="G20" t="n">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="H20" t="n">
-        <v>871133</v>
+        <v>896813</v>
       </c>
       <c r="I20" t="n">
-        <v>81.346</v>
+        <v>83.744</v>
       </c>
       <c r="J20" t="n">
-        <v>8615</v>
+        <v>5491</v>
       </c>
       <c r="K20" t="n">
-        <v>0.804</v>
+        <v>0.513</v>
       </c>
       <c r="L20" t="n">
-        <v>7069</v>
+        <v>7459</v>
       </c>
       <c r="M20" t="n">
-        <v>0.66</v>
+        <v>0.697</v>
       </c>
       <c r="N20" t="n">
-        <v>0.042</v>
+        <v>0.043</v>
       </c>
       <c r="O20" t="n">
-        <v>23.963</v>
+        <v>23.456</v>
       </c>
       <c r="P20" t="s">
         <v>45</v>
@@ -3670,7 +3674,7 @@
         <v>135</v>
       </c>
       <c r="C21" s="1" t="n">
-        <v>44069</v>
+        <v>44071</v>
       </c>
       <c r="D21" t="s">
         <v>136</v>
@@ -3680,27 +3684,27 @@
       </c>
       <c r="F21"/>
       <c r="G21" t="n">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="H21"/>
       <c r="I21"/>
       <c r="J21" t="n">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="K21" t="n">
         <v>0.002</v>
       </c>
       <c r="L21" t="n">
-        <v>241</v>
+        <v>225</v>
       </c>
       <c r="M21" t="n">
         <v>0.003</v>
       </c>
       <c r="N21" t="n">
-        <v>0.101</v>
+        <v>0.1</v>
       </c>
       <c r="O21" t="n">
-        <v>9.924</v>
+        <v>9.968</v>
       </c>
       <c r="P21" t="s">
         <v>137</v>
@@ -3723,7 +3727,7 @@
         <v>141</v>
       </c>
       <c r="C22" s="1" t="n">
-        <v>44070</v>
+        <v>44073</v>
       </c>
       <c r="D22" t="s">
         <v>142</v>
@@ -3733,31 +3737,31 @@
       </c>
       <c r="F22"/>
       <c r="G22" t="n">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="H22" t="n">
-        <v>2315324</v>
+        <v>2417508</v>
       </c>
       <c r="I22" t="n">
-        <v>399.731</v>
+        <v>417.373</v>
       </c>
       <c r="J22" t="n">
-        <v>6042</v>
+        <v>4918</v>
       </c>
       <c r="K22" t="n">
-        <v>1.043</v>
+        <v>0.849</v>
       </c>
       <c r="L22" t="n">
-        <v>29715</v>
+        <v>31184</v>
       </c>
       <c r="M22" t="n">
-        <v>5.13</v>
+        <v>5.384</v>
       </c>
       <c r="N22" t="n">
         <v>0.003</v>
       </c>
       <c r="O22" t="n">
-        <v>348.417</v>
+        <v>380.956</v>
       </c>
       <c r="P22" t="s">
         <v>143</v>
@@ -3780,7 +3784,7 @@
         <v>147</v>
       </c>
       <c r="C23" s="1" t="n">
-        <v>44070</v>
+        <v>44072</v>
       </c>
       <c r="D23" t="s">
         <v>148</v>
@@ -3792,25 +3796,25 @@
         <v>150</v>
       </c>
       <c r="G23" t="n">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="H23" t="n">
-        <v>251532</v>
+        <v>256212</v>
       </c>
       <c r="I23" t="n">
-        <v>14.257</v>
+        <v>14.522</v>
       </c>
       <c r="J23" t="n">
-        <v>2080</v>
+        <v>2236</v>
       </c>
       <c r="K23" t="n">
-        <v>0.118</v>
+        <v>0.127</v>
       </c>
       <c r="L23" t="n">
-        <v>2304</v>
+        <v>2349</v>
       </c>
       <c r="M23" t="n">
-        <v>0.131</v>
+        <v>0.133</v>
       </c>
       <c r="N23"/>
       <c r="O23"/>
@@ -3835,7 +3839,7 @@
         <v>154</v>
       </c>
       <c r="C24" s="1" t="n">
-        <v>44068</v>
+        <v>44071</v>
       </c>
       <c r="D24" t="s">
         <v>155</v>
@@ -3845,31 +3849,31 @@
       </c>
       <c r="F24"/>
       <c r="G24" t="n">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="H24" t="n">
-        <v>303031</v>
+        <v>310444</v>
       </c>
       <c r="I24" t="n">
-        <v>46.719</v>
+        <v>47.862</v>
       </c>
       <c r="J24" t="n">
-        <v>2497</v>
+        <v>2467</v>
       </c>
       <c r="K24" t="n">
-        <v>0.385</v>
+        <v>0.38</v>
       </c>
       <c r="L24" t="n">
-        <v>2448</v>
+        <v>2461</v>
       </c>
       <c r="M24" t="n">
-        <v>0.377</v>
+        <v>0.379</v>
       </c>
       <c r="N24" t="n">
-        <v>0.094</v>
+        <v>0.077</v>
       </c>
       <c r="O24" t="n">
-        <v>10.591</v>
+        <v>13.051</v>
       </c>
       <c r="P24" t="s">
         <v>156</v>
@@ -3892,7 +3896,7 @@
         <v>160</v>
       </c>
       <c r="C25" s="1" t="n">
-        <v>44070</v>
+        <v>44072</v>
       </c>
       <c r="D25" t="s">
         <v>161</v>
@@ -3902,31 +3906,31 @@
       </c>
       <c r="F25"/>
       <c r="G25" t="n">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="H25" t="n">
-        <v>146128</v>
+        <v>147901</v>
       </c>
       <c r="I25" t="n">
-        <v>110.157</v>
+        <v>111.494</v>
       </c>
       <c r="J25" t="n">
-        <v>1271</v>
+        <v>666</v>
       </c>
       <c r="K25" t="n">
-        <v>0.958</v>
+        <v>0.502</v>
       </c>
       <c r="L25" t="n">
-        <v>1011</v>
+        <v>1035</v>
       </c>
       <c r="M25" t="n">
-        <v>0.762</v>
+        <v>0.78</v>
       </c>
       <c r="N25" t="n">
-        <v>0.015</v>
+        <v>0.014</v>
       </c>
       <c r="O25" t="n">
-        <v>68.048</v>
+        <v>73.182</v>
       </c>
       <c r="P25" t="s">
         <v>163</v>
@@ -3949,7 +3953,7 @@
         <v>168</v>
       </c>
       <c r="C26" s="1" t="n">
-        <v>44069</v>
+        <v>44072</v>
       </c>
       <c r="D26" t="s">
         <v>169</v>
@@ -3959,31 +3963,31 @@
       </c>
       <c r="F26"/>
       <c r="G26" t="n">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="H26" t="n">
-        <v>813410</v>
+        <v>869430</v>
       </c>
       <c r="I26" t="n">
-        <v>7.075</v>
+        <v>7.563</v>
       </c>
       <c r="J26" t="n">
-        <v>18724</v>
+        <v>19194</v>
       </c>
       <c r="K26" t="n">
-        <v>0.163</v>
+        <v>0.167</v>
       </c>
       <c r="L26" t="n">
-        <v>20110</v>
+        <v>18932</v>
       </c>
       <c r="M26" t="n">
-        <v>0.175</v>
+        <v>0.165</v>
       </c>
       <c r="N26" t="n">
-        <v>0.078</v>
+        <v>0.079</v>
       </c>
       <c r="O26" t="n">
-        <v>12.837</v>
+        <v>12.651</v>
       </c>
       <c r="P26" t="s">
         <v>170</v>
@@ -4063,7 +4067,7 @@
         <v>179</v>
       </c>
       <c r="C28" s="1" t="n">
-        <v>44069</v>
+        <v>44072</v>
       </c>
       <c r="D28" t="s">
         <v>180</v>
@@ -4073,31 +4077,31 @@
       </c>
       <c r="F28"/>
       <c r="G28" t="n">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="H28" t="n">
-        <v>615008</v>
+        <v>639098</v>
       </c>
       <c r="I28" t="n">
-        <v>110.998</v>
+        <v>115.346</v>
       </c>
       <c r="J28" t="n">
-        <v>9513</v>
+        <v>1280</v>
       </c>
       <c r="K28" t="n">
-        <v>1.717</v>
+        <v>0.231</v>
       </c>
       <c r="L28" t="n">
-        <v>11373</v>
+        <v>9362</v>
       </c>
       <c r="M28" t="n">
-        <v>2.053</v>
+        <v>1.69</v>
       </c>
       <c r="N28" t="n">
         <v>0.003</v>
       </c>
       <c r="O28" t="n">
-        <v>388.346</v>
+        <v>383.24</v>
       </c>
       <c r="P28" t="s">
         <v>182</v>
@@ -4120,7 +4124,7 @@
         <v>185</v>
       </c>
       <c r="C29" s="1" t="n">
-        <v>44067</v>
+        <v>44070</v>
       </c>
       <c r="D29" t="s">
         <v>186</v>
@@ -4130,27 +4134,27 @@
       </c>
       <c r="F29"/>
       <c r="G29" t="n">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="H29"/>
       <c r="I29"/>
       <c r="J29" t="n">
-        <v>143755</v>
+        <v>135212</v>
       </c>
       <c r="K29" t="n">
-        <v>2.202</v>
+        <v>2.071</v>
       </c>
       <c r="L29" t="n">
-        <v>106496</v>
+        <v>114778</v>
       </c>
       <c r="M29" t="n">
-        <v>1.632</v>
+        <v>1.758</v>
       </c>
       <c r="N29" t="n">
-        <v>0.033</v>
+        <v>0.036</v>
       </c>
       <c r="O29" t="n">
-        <v>30.599</v>
+        <v>28.148</v>
       </c>
       <c r="P29" t="s">
         <v>187</v>
@@ -4283,7 +4287,7 @@
         <v>203</v>
       </c>
       <c r="C32" s="1" t="n">
-        <v>44067</v>
+        <v>44070</v>
       </c>
       <c r="D32" t="s">
         <v>204</v>
@@ -4293,31 +4297,31 @@
       </c>
       <c r="F32"/>
       <c r="G32" t="n">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="H32" t="n">
-        <v>437750</v>
+        <v>442185</v>
       </c>
       <c r="I32" t="n">
-        <v>14.088</v>
+        <v>14.231</v>
       </c>
       <c r="J32" t="n">
-        <v>749</v>
+        <v>1201</v>
       </c>
       <c r="K32" t="n">
-        <v>0.024</v>
+        <v>0.039</v>
       </c>
       <c r="L32" t="n">
-        <v>1140</v>
+        <v>1240</v>
       </c>
       <c r="M32" t="n">
-        <v>0.037</v>
+        <v>0.04</v>
       </c>
       <c r="N32" t="n">
-        <v>0.122</v>
+        <v>0.086</v>
       </c>
       <c r="O32" t="n">
-        <v>8.201</v>
+        <v>11.62</v>
       </c>
       <c r="P32" t="s">
         <v>206</v>
@@ -4340,7 +4344,7 @@
         <v>210</v>
       </c>
       <c r="C33" s="1" t="n">
-        <v>44070</v>
+        <v>44073</v>
       </c>
       <c r="D33" t="s">
         <v>211</v>
@@ -4350,27 +4354,31 @@
       </c>
       <c r="F33"/>
       <c r="G33" t="n">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="H33" t="n">
-        <v>903432</v>
+        <v>940882</v>
       </c>
       <c r="I33" t="n">
-        <v>86.676</v>
-      </c>
-      <c r="J33"/>
-      <c r="K33"/>
+        <v>90.269</v>
+      </c>
+      <c r="J33" t="n">
+        <v>9880</v>
+      </c>
+      <c r="K33" t="n">
+        <v>0.948</v>
+      </c>
       <c r="L33" t="n">
-        <v>12426</v>
+        <v>13215</v>
       </c>
       <c r="M33" t="n">
-        <v>1.192</v>
+        <v>1.268</v>
       </c>
       <c r="N33" t="n">
-        <v>0.018</v>
+        <v>0.017</v>
       </c>
       <c r="O33" t="n">
-        <v>54.5</v>
+        <v>57.961</v>
       </c>
       <c r="P33" t="s">
         <v>213</v>
@@ -4442,7 +4450,7 @@
         <v>224</v>
       </c>
       <c r="C35" s="1" t="n">
-        <v>44071</v>
+        <v>44074</v>
       </c>
       <c r="D35" t="s">
         <v>225</v>
@@ -4454,31 +4462,31 @@
         <v>227</v>
       </c>
       <c r="G35" t="n">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="H35" t="n">
-        <v>414645</v>
+        <v>428150</v>
       </c>
       <c r="I35" t="n">
-        <v>42.922</v>
+        <v>44.32</v>
       </c>
       <c r="J35" t="n">
-        <v>5846</v>
+        <v>3880</v>
       </c>
       <c r="K35" t="n">
-        <v>0.605</v>
+        <v>0.402</v>
       </c>
       <c r="L35" t="n">
-        <v>3031</v>
+        <v>4229</v>
       </c>
       <c r="M35" t="n">
-        <v>0.314</v>
+        <v>0.438</v>
       </c>
       <c r="N35" t="n">
-        <v>0.016</v>
+        <v>0.027</v>
       </c>
       <c r="O35" t="n">
-        <v>63.715</v>
+        <v>36.728</v>
       </c>
       <c r="P35" t="s">
         <v>226</v>
@@ -4501,7 +4509,7 @@
         <v>232</v>
       </c>
       <c r="C36" s="1" t="n">
-        <v>44070</v>
+        <v>44071</v>
       </c>
       <c r="D36" t="s">
         <v>233</v>
@@ -4511,31 +4519,31 @@
       </c>
       <c r="F36"/>
       <c r="G36" t="n">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="H36" t="n">
-        <v>88166</v>
+        <v>88829</v>
       </c>
       <c r="I36" t="n">
-        <v>258.362</v>
+        <v>260.305</v>
       </c>
       <c r="J36" t="n">
-        <v>723</v>
+        <v>663</v>
       </c>
       <c r="K36" t="n">
-        <v>2.119</v>
+        <v>1.943</v>
       </c>
       <c r="L36" t="n">
-        <v>588</v>
+        <v>598</v>
       </c>
       <c r="M36" t="n">
-        <v>1.723</v>
+        <v>1.752</v>
       </c>
       <c r="N36" t="n">
         <v>0.011</v>
       </c>
       <c r="O36" t="n">
-        <v>87.574</v>
+        <v>89.064</v>
       </c>
       <c r="P36" t="s">
         <v>234</v>
@@ -4617,7 +4625,7 @@
         <v>242</v>
       </c>
       <c r="C38" s="1" t="n">
-        <v>44070</v>
+        <v>44073</v>
       </c>
       <c r="D38" t="s">
         <v>238</v>
@@ -4629,31 +4637,31 @@
         <v>240</v>
       </c>
       <c r="G38" t="n">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="H38" t="n">
-        <v>39477848</v>
+        <v>42307914</v>
       </c>
       <c r="I38" t="n">
-        <v>28.607</v>
+        <v>30.658</v>
       </c>
       <c r="J38" t="n">
-        <v>901338</v>
+        <v>846278</v>
       </c>
       <c r="K38" t="n">
-        <v>0.653</v>
+        <v>0.613</v>
       </c>
       <c r="L38" t="n">
-        <v>858659</v>
+        <v>892578</v>
       </c>
       <c r="M38" t="n">
-        <v>0.622</v>
+        <v>0.647</v>
       </c>
       <c r="N38" t="n">
-        <v>0.079</v>
+        <v>0.08</v>
       </c>
       <c r="O38" t="n">
-        <v>12.699</v>
+        <v>12.551</v>
       </c>
       <c r="P38" t="s">
         <v>239</v>
@@ -4676,7 +4684,7 @@
         <v>244</v>
       </c>
       <c r="C39" s="1" t="n">
-        <v>44071</v>
+        <v>44074</v>
       </c>
       <c r="D39" t="s">
         <v>245</v>
@@ -4686,31 +4694,31 @@
       </c>
       <c r="F39"/>
       <c r="G39" t="n">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="H39" t="n">
-        <v>1233486</v>
+        <v>1282618</v>
       </c>
       <c r="I39" t="n">
-        <v>4.51</v>
+        <v>4.689</v>
       </c>
       <c r="J39" t="n">
-        <v>21018</v>
+        <v>11317</v>
       </c>
       <c r="K39" t="n">
-        <v>0.077</v>
+        <v>0.041</v>
       </c>
       <c r="L39" t="n">
-        <v>15044</v>
+        <v>15230</v>
       </c>
       <c r="M39" t="n">
-        <v>0.055</v>
+        <v>0.056</v>
       </c>
       <c r="N39" t="n">
-        <v>0.149</v>
+        <v>0.174</v>
       </c>
       <c r="O39" t="n">
-        <v>6.719</v>
+        <v>5.757</v>
       </c>
       <c r="P39" t="s">
         <v>246</v>
@@ -4733,7 +4741,7 @@
         <v>250</v>
       </c>
       <c r="C40" s="1" t="n">
-        <v>44070</v>
+        <v>44074</v>
       </c>
       <c r="D40" t="s">
         <v>251</v>
@@ -4743,31 +4751,31 @@
       </c>
       <c r="F40"/>
       <c r="G40" t="n">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="H40" t="n">
-        <v>3138782</v>
+        <v>3231110</v>
       </c>
       <c r="I40" t="n">
-        <v>37.37</v>
+        <v>38.469</v>
       </c>
       <c r="J40" t="n">
-        <v>24976</v>
+        <v>23841</v>
       </c>
       <c r="K40" t="n">
-        <v>0.297</v>
+        <v>0.284</v>
       </c>
       <c r="L40" t="n">
-        <v>25006</v>
+        <v>24098</v>
       </c>
       <c r="M40" t="n">
-        <v>0.298</v>
+        <v>0.287</v>
       </c>
       <c r="N40" t="n">
-        <v>0.089</v>
+        <v>0.087</v>
       </c>
       <c r="O40" t="n">
-        <v>11.273</v>
+        <v>11.503</v>
       </c>
       <c r="P40" t="s">
         <v>252</v>
@@ -4847,7 +4855,7 @@
         <v>263</v>
       </c>
       <c r="C42" s="1" t="n">
-        <v>44070</v>
+        <v>44072</v>
       </c>
       <c r="D42" t="s">
         <v>264</v>
@@ -4857,31 +4865,31 @@
       </c>
       <c r="F42"/>
       <c r="G42" t="n">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="H42" t="n">
-        <v>802572</v>
+        <v>824712</v>
       </c>
       <c r="I42" t="n">
-        <v>162.536</v>
+        <v>167.02</v>
       </c>
       <c r="J42" t="n">
-        <v>12274</v>
+        <v>9837</v>
       </c>
       <c r="K42" t="n">
-        <v>2.486</v>
+        <v>1.992</v>
       </c>
       <c r="L42" t="n">
-        <v>7864</v>
+        <v>8193</v>
       </c>
       <c r="M42" t="n">
-        <v>1.593</v>
+        <v>1.659</v>
       </c>
       <c r="N42" t="n">
-        <v>0.015</v>
+        <v>0.014</v>
       </c>
       <c r="O42" t="n">
-        <v>67.461</v>
+        <v>69.601</v>
       </c>
       <c r="P42" t="s">
         <v>265</v>
@@ -4904,7 +4912,7 @@
         <v>268</v>
       </c>
       <c r="C43" s="1" t="n">
-        <v>44064</v>
+        <v>44067</v>
       </c>
       <c r="D43" t="s">
         <v>269</v>
@@ -4914,31 +4922,31 @@
       </c>
       <c r="F43"/>
       <c r="G43" t="n">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="H43" t="n">
-        <v>2231154</v>
+        <v>2285649</v>
       </c>
       <c r="I43" t="n">
-        <v>257.772</v>
+        <v>264.068</v>
       </c>
       <c r="J43" t="n">
-        <v>27211</v>
+        <v>30119</v>
       </c>
       <c r="K43" t="n">
-        <v>3.144</v>
+        <v>3.48</v>
       </c>
       <c r="L43" t="n">
-        <v>22890</v>
+        <v>23844</v>
       </c>
       <c r="M43" t="n">
-        <v>2.645</v>
+        <v>2.755</v>
       </c>
       <c r="N43" t="n">
-        <v>0.061</v>
+        <v>0.063</v>
       </c>
       <c r="O43" t="n">
-        <v>16.388</v>
+        <v>15.94</v>
       </c>
       <c r="P43" t="s">
         <v>45</v>
@@ -4961,7 +4969,7 @@
         <v>274</v>
       </c>
       <c r="C44" s="1" t="n">
-        <v>44070</v>
+        <v>44073</v>
       </c>
       <c r="D44" t="s">
         <v>275</v>
@@ -4973,31 +4981,31 @@
         <v>277</v>
       </c>
       <c r="G44" t="n">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="H44" t="n">
-        <v>4934818</v>
+        <v>5117788</v>
       </c>
       <c r="I44" t="n">
-        <v>81.619</v>
+        <v>84.645</v>
       </c>
       <c r="J44" t="n">
-        <v>57640</v>
+        <v>53541</v>
       </c>
       <c r="K44" t="n">
-        <v>0.953</v>
+        <v>0.886</v>
       </c>
       <c r="L44" t="n">
-        <v>47696</v>
+        <v>53974</v>
       </c>
       <c r="M44" t="n">
-        <v>0.789</v>
+        <v>0.893</v>
       </c>
       <c r="N44" t="n">
-        <v>0.022</v>
+        <v>0.023</v>
       </c>
       <c r="O44" t="n">
-        <v>45.975</v>
+        <v>43.343</v>
       </c>
       <c r="P44" t="s">
         <v>278</v>
@@ -5020,7 +5028,7 @@
         <v>281</v>
       </c>
       <c r="C45" s="1" t="n">
-        <v>44070</v>
+        <v>44073</v>
       </c>
       <c r="D45" t="s">
         <v>275</v>
@@ -5032,31 +5040,31 @@
         <v>277</v>
       </c>
       <c r="G45" t="n">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="H45" t="n">
-        <v>8313445</v>
+        <v>8591341</v>
       </c>
       <c r="I45" t="n">
-        <v>137.499</v>
+        <v>142.095</v>
       </c>
       <c r="J45" t="n">
-        <v>94024</v>
+        <v>81723</v>
       </c>
       <c r="K45" t="n">
-        <v>1.555</v>
+        <v>1.352</v>
       </c>
       <c r="L45" t="n">
-        <v>74693</v>
+        <v>83386</v>
       </c>
       <c r="M45" t="n">
-        <v>1.235</v>
+        <v>1.379</v>
       </c>
       <c r="N45" t="n">
-        <v>0.014</v>
+        <v>0.015</v>
       </c>
       <c r="O45" t="n">
-        <v>71.998</v>
+        <v>66.961</v>
       </c>
       <c r="P45" t="s">
         <v>278</v>
@@ -5079,7 +5087,7 @@
         <v>284</v>
       </c>
       <c r="C46" s="1" t="n">
-        <v>44070</v>
+        <v>44073</v>
       </c>
       <c r="D46" t="s">
         <v>285</v>
@@ -5091,31 +5099,31 @@
         <v>287</v>
       </c>
       <c r="G46" t="n">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="H46" t="n">
-        <v>1397400</v>
+        <v>1455610</v>
       </c>
       <c r="I46" t="n">
-        <v>11.049</v>
+        <v>11.509</v>
       </c>
       <c r="J46" t="n">
-        <v>20617</v>
+        <v>14784</v>
       </c>
       <c r="K46" t="n">
-        <v>0.163</v>
+        <v>0.117</v>
       </c>
       <c r="L46" t="n">
-        <v>19711</v>
+        <v>19219</v>
       </c>
       <c r="M46" t="n">
-        <v>0.156</v>
+        <v>0.152</v>
       </c>
       <c r="N46" t="n">
-        <v>0.045</v>
+        <v>0.041</v>
       </c>
       <c r="O46" t="n">
-        <v>22.373</v>
+        <v>24.385</v>
       </c>
       <c r="P46" t="s">
         <v>288</v>
@@ -5138,7 +5146,7 @@
         <v>291</v>
       </c>
       <c r="C47" s="1" t="n">
-        <v>44068</v>
+        <v>44070</v>
       </c>
       <c r="D47" t="s">
         <v>292</v>
@@ -5150,31 +5158,31 @@
         <v>293</v>
       </c>
       <c r="G47" t="n">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="H47" t="n">
-        <v>1708010</v>
+        <v>1770064</v>
       </c>
       <c r="I47" t="n">
-        <v>13.505</v>
+        <v>13.995</v>
       </c>
       <c r="J47" t="n">
-        <v>15191</v>
+        <v>26201</v>
       </c>
       <c r="K47" t="n">
-        <v>0.12</v>
+        <v>0.207</v>
       </c>
       <c r="L47" t="n">
-        <v>20753</v>
+        <v>21805</v>
       </c>
       <c r="M47" t="n">
-        <v>0.164</v>
+        <v>0.172</v>
       </c>
       <c r="N47" t="n">
-        <v>0.049</v>
+        <v>0.04</v>
       </c>
       <c r="O47" t="n">
-        <v>20.281</v>
+        <v>24.75</v>
       </c>
       <c r="P47" t="s">
         <v>288</v>
@@ -5254,7 +5262,7 @@
         <v>301</v>
       </c>
       <c r="C49" s="1" t="n">
-        <v>44068</v>
+        <v>44072</v>
       </c>
       <c r="D49" t="s">
         <v>302</v>
@@ -5264,31 +5272,31 @@
       </c>
       <c r="F49"/>
       <c r="G49" t="n">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="H49" t="n">
-        <v>429513</v>
+        <v>445722</v>
       </c>
       <c r="I49" t="n">
-        <v>7.988</v>
+        <v>8.289</v>
       </c>
       <c r="J49" t="n">
-        <v>4149</v>
+        <v>3009</v>
       </c>
       <c r="K49" t="n">
-        <v>0.077</v>
+        <v>0.056</v>
       </c>
       <c r="L49" t="n">
-        <v>4418</v>
+        <v>3988</v>
       </c>
       <c r="M49" t="n">
-        <v>0.082</v>
+        <v>0.074</v>
       </c>
       <c r="N49" t="n">
-        <v>0.071</v>
+        <v>0.067</v>
       </c>
       <c r="O49" t="n">
-        <v>14.109</v>
+        <v>14.952</v>
       </c>
       <c r="P49" t="s">
         <v>45</v>
@@ -5311,7 +5319,7 @@
         <v>307</v>
       </c>
       <c r="C50" s="1" t="n">
-        <v>44070</v>
+        <v>44072</v>
       </c>
       <c r="D50" t="s">
         <v>308</v>
@@ -5321,31 +5329,31 @@
       </c>
       <c r="F50"/>
       <c r="G50" t="n">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="H50" t="n">
-        <v>603604</v>
+        <v>611639</v>
       </c>
       <c r="I50" t="n">
-        <v>141.341</v>
+        <v>143.222</v>
       </c>
       <c r="J50" t="n">
-        <v>4191</v>
+        <v>3718</v>
       </c>
       <c r="K50" t="n">
-        <v>0.981</v>
+        <v>0.871</v>
       </c>
       <c r="L50" t="n">
-        <v>3717</v>
+        <v>3788</v>
       </c>
       <c r="M50" t="n">
-        <v>0.87</v>
+        <v>0.887</v>
       </c>
       <c r="N50" t="n">
-        <v>0.159</v>
+        <v>0.163</v>
       </c>
       <c r="O50" t="n">
-        <v>6.306</v>
+        <v>6.154</v>
       </c>
       <c r="P50" t="s">
         <v>309</v>
@@ -5368,7 +5376,7 @@
         <v>313</v>
       </c>
       <c r="C51" s="1" t="n">
-        <v>44071</v>
+        <v>44074</v>
       </c>
       <c r="D51" t="s">
         <v>314</v>
@@ -5380,31 +5388,31 @@
         <v>316</v>
       </c>
       <c r="G51" t="n">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="H51" t="n">
-        <v>246867</v>
+        <v>251717</v>
       </c>
       <c r="I51" t="n">
-        <v>130.88</v>
+        <v>133.452</v>
       </c>
       <c r="J51" t="n">
-        <v>2040</v>
+        <v>1008</v>
       </c>
       <c r="K51" t="n">
-        <v>1.082</v>
+        <v>0.534</v>
       </c>
       <c r="L51" t="n">
-        <v>1764</v>
+        <v>1902</v>
       </c>
       <c r="M51" t="n">
-        <v>0.935</v>
+        <v>1.008</v>
       </c>
       <c r="N51" t="n">
-        <v>0.003</v>
+        <v>0.004</v>
       </c>
       <c r="O51" t="n">
-        <v>316.615</v>
+        <v>237.75</v>
       </c>
       <c r="P51" t="s">
         <v>315</v>
@@ -5427,7 +5435,7 @@
         <v>319</v>
       </c>
       <c r="C52" s="1" t="n">
-        <v>44071</v>
+        <v>44074</v>
       </c>
       <c r="D52" t="s">
         <v>320</v>
@@ -5437,31 +5445,27 @@
       </c>
       <c r="F52"/>
       <c r="G52" t="n">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="H52" t="n">
-        <v>629443</v>
+        <v>639044</v>
       </c>
       <c r="I52" t="n">
-        <v>231.218</v>
-      </c>
-      <c r="J52" t="n">
-        <v>5602</v>
-      </c>
-      <c r="K52" t="n">
-        <v>2.058</v>
-      </c>
+        <v>234.745</v>
+      </c>
+      <c r="J52"/>
+      <c r="K52"/>
       <c r="L52" t="n">
-        <v>4276</v>
+        <v>4325</v>
       </c>
       <c r="M52" t="n">
-        <v>1.571</v>
+        <v>1.589</v>
       </c>
       <c r="N52" t="n">
         <v>0.008</v>
       </c>
       <c r="O52" t="n">
-        <v>127.915</v>
+        <v>126.674</v>
       </c>
       <c r="P52" t="s">
         <v>45</v>
@@ -5484,7 +5488,7 @@
         <v>323</v>
       </c>
       <c r="C53" s="1" t="n">
-        <v>44069</v>
+        <v>44070</v>
       </c>
       <c r="D53" t="s">
         <v>324</v>
@@ -5497,28 +5501,28 @@
         <v>183</v>
       </c>
       <c r="H53" t="n">
-        <v>379508</v>
+        <v>381256</v>
       </c>
       <c r="I53" t="n">
-        <v>606.266</v>
+        <v>609.058</v>
       </c>
       <c r="J53" t="n">
-        <v>1365</v>
+        <v>1748</v>
       </c>
       <c r="K53" t="n">
-        <v>2.181</v>
+        <v>2.792</v>
       </c>
       <c r="L53" t="n">
-        <v>1113</v>
+        <v>1194</v>
       </c>
       <c r="M53" t="n">
-        <v>1.778</v>
+        <v>1.907</v>
       </c>
       <c r="N53" t="n">
-        <v>0.044</v>
+        <v>0.043</v>
       </c>
       <c r="O53" t="n">
-        <v>22.982</v>
+        <v>23.088</v>
       </c>
       <c r="P53" t="s">
         <v>325</v>
@@ -5541,7 +5545,7 @@
         <v>328</v>
       </c>
       <c r="C54" s="1" t="n">
-        <v>44070</v>
+        <v>44073</v>
       </c>
       <c r="D54" t="s">
         <v>329</v>
@@ -5553,31 +5557,31 @@
         <v>331</v>
       </c>
       <c r="G54" t="n">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="H54" t="n">
-        <v>1212790</v>
+        <v>1243540</v>
       </c>
       <c r="I54" t="n">
-        <v>37.471</v>
+        <v>38.421</v>
       </c>
       <c r="J54" t="n">
-        <v>10026</v>
+        <v>10613</v>
       </c>
       <c r="K54" t="n">
-        <v>0.31</v>
+        <v>0.328</v>
       </c>
       <c r="L54" t="n">
-        <v>8664</v>
+        <v>9589</v>
       </c>
       <c r="M54" t="n">
-        <v>0.268</v>
+        <v>0.296</v>
       </c>
       <c r="N54" t="n">
         <v>0.001</v>
       </c>
       <c r="O54" t="n">
-        <v>1083</v>
+        <v>1118.717</v>
       </c>
       <c r="P54" t="s">
         <v>45</v>
@@ -5600,7 +5604,7 @@
         <v>335</v>
       </c>
       <c r="C55" s="1" t="n">
-        <v>44070</v>
+        <v>44072</v>
       </c>
       <c r="D55" t="s">
         <v>336</v>
@@ -5610,31 +5614,31 @@
       </c>
       <c r="F55"/>
       <c r="G55" t="n">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="H55" t="n">
-        <v>108099</v>
+        <v>110249</v>
       </c>
       <c r="I55" t="n">
-        <v>199.983</v>
+        <v>203.96</v>
       </c>
       <c r="J55" t="n">
-        <v>1190</v>
+        <v>1129</v>
       </c>
       <c r="K55" t="n">
-        <v>2.201</v>
+        <v>2.089</v>
       </c>
       <c r="L55" t="n">
-        <v>1124</v>
+        <v>1081</v>
       </c>
       <c r="M55" t="n">
-        <v>2.079</v>
+        <v>2</v>
       </c>
       <c r="N55" t="n">
-        <v>0.127</v>
+        <v>0.12</v>
       </c>
       <c r="O55" t="n">
-        <v>7.868</v>
+        <v>8.361</v>
       </c>
       <c r="P55" t="s">
         <v>338</v>
@@ -5657,7 +5661,7 @@
         <v>342</v>
       </c>
       <c r="C56" s="1" t="n">
-        <v>44065</v>
+        <v>44072</v>
       </c>
       <c r="D56" t="s">
         <v>343</v>
@@ -5667,31 +5671,31 @@
       </c>
       <c r="F56"/>
       <c r="G56" t="n">
-        <v>183</v>
+        <v>190</v>
       </c>
       <c r="H56" t="n">
-        <v>173263</v>
+        <v>188539</v>
       </c>
       <c r="I56" t="n">
-        <v>392.407</v>
+        <v>427.004</v>
       </c>
       <c r="J56" t="n">
-        <v>2173</v>
+        <v>1909</v>
       </c>
       <c r="K56" t="n">
-        <v>4.921</v>
+        <v>4.324</v>
       </c>
       <c r="L56" t="n">
-        <v>2373</v>
+        <v>2182</v>
       </c>
       <c r="M56" t="n">
-        <v>5.374</v>
+        <v>4.942</v>
       </c>
       <c r="N56" t="n">
-        <v>0.016</v>
+        <v>0.018</v>
       </c>
       <c r="O56" t="n">
-        <v>61.981</v>
+        <v>55.745</v>
       </c>
       <c r="P56" t="s">
         <v>344</v>
@@ -5714,7 +5718,7 @@
         <v>348</v>
       </c>
       <c r="C57" s="1" t="n">
-        <v>44064</v>
+        <v>44068</v>
       </c>
       <c r="D57" t="s">
         <v>349</v>
@@ -5724,31 +5728,31 @@
       </c>
       <c r="F57"/>
       <c r="G57" t="n">
-        <v>234</v>
+        <v>238</v>
       </c>
       <c r="H57" t="n">
-        <v>1204031</v>
+        <v>1241422</v>
       </c>
       <c r="I57" t="n">
-        <v>9.338</v>
+        <v>9.628</v>
       </c>
       <c r="J57" t="n">
-        <v>11477</v>
+        <v>10931</v>
       </c>
       <c r="K57" t="n">
-        <v>0.089</v>
+        <v>0.085</v>
       </c>
       <c r="L57" t="n">
-        <v>10380</v>
+        <v>10105</v>
       </c>
       <c r="M57" t="n">
-        <v>0.081</v>
+        <v>0.078</v>
       </c>
       <c r="N57" t="n">
-        <v>0.524</v>
+        <v>0.537</v>
       </c>
       <c r="O57" t="n">
-        <v>1.909</v>
+        <v>1.863</v>
       </c>
       <c r="P57" t="s">
         <v>351</v>
@@ -5771,7 +5775,7 @@
         <v>355</v>
       </c>
       <c r="C58" s="1" t="n">
-        <v>44070</v>
+        <v>44072</v>
       </c>
       <c r="D58" t="s">
         <v>356</v>
@@ -5781,31 +5785,31 @@
       </c>
       <c r="F58"/>
       <c r="G58" t="n">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="H58" t="n">
-        <v>1846260</v>
+        <v>1890964</v>
       </c>
       <c r="I58" t="n">
-        <v>50.02</v>
+        <v>51.231</v>
       </c>
       <c r="J58" t="n">
-        <v>22009</v>
+        <v>22419</v>
       </c>
       <c r="K58" t="n">
+        <v>0.607</v>
+      </c>
+      <c r="L58" t="n">
+        <v>21998</v>
+      </c>
+      <c r="M58" t="n">
         <v>0.596</v>
       </c>
-      <c r="L58" t="n">
-        <v>21979</v>
-      </c>
-      <c r="M58" t="n">
-        <v>0.595</v>
-      </c>
       <c r="N58" t="n">
-        <v>0.062</v>
+        <v>0.06</v>
       </c>
       <c r="O58" t="n">
-        <v>16.109</v>
+        <v>16.662</v>
       </c>
       <c r="P58" t="s">
         <v>357</v>
@@ -5828,7 +5832,7 @@
         <v>361</v>
       </c>
       <c r="C59" s="1" t="n">
-        <v>44067</v>
+        <v>44071</v>
       </c>
       <c r="D59" t="s">
         <v>362</v>
@@ -5838,31 +5842,31 @@
       </c>
       <c r="F59"/>
       <c r="G59" t="n">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="H59" t="n">
-        <v>147820</v>
+        <v>156042</v>
       </c>
       <c r="I59" t="n">
-        <v>2.717</v>
+        <v>2.868</v>
       </c>
       <c r="J59" t="n">
-        <v>1783</v>
+        <v>2221</v>
       </c>
       <c r="K59" t="n">
-        <v>0.033</v>
+        <v>0.041</v>
       </c>
       <c r="L59" t="n">
-        <v>1439</v>
+        <v>1713</v>
       </c>
       <c r="M59" t="n">
-        <v>0.026</v>
+        <v>0.031</v>
       </c>
       <c r="N59" t="n">
-        <v>0.009</v>
+        <v>0.018</v>
       </c>
       <c r="O59" t="n">
-        <v>114.466</v>
+        <v>54.753</v>
       </c>
       <c r="P59" t="s">
         <v>363</v>
@@ -5995,7 +5999,7 @@
         <v>380</v>
       </c>
       <c r="C62" s="1" t="n">
-        <v>44070</v>
+        <v>44073</v>
       </c>
       <c r="D62" t="s">
         <v>381</v>
@@ -6005,31 +6009,31 @@
       </c>
       <c r="F62"/>
       <c r="G62" t="n">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="H62" t="n">
-        <v>730330</v>
+        <v>758027</v>
       </c>
       <c r="I62" t="n">
-        <v>151.451</v>
+        <v>157.194</v>
       </c>
       <c r="J62" t="n">
-        <v>11010</v>
+        <v>7219</v>
       </c>
       <c r="K62" t="n">
-        <v>2.283</v>
+        <v>1.497</v>
       </c>
       <c r="L62" t="n">
-        <v>8159</v>
+        <v>8708</v>
       </c>
       <c r="M62" t="n">
-        <v>1.692</v>
+        <v>1.806</v>
       </c>
       <c r="N62" t="n">
         <v>0.001</v>
       </c>
       <c r="O62" t="n">
-        <v>1215.17</v>
+        <v>1128.815</v>
       </c>
       <c r="P62" t="s">
         <v>382</v>
@@ -6052,7 +6056,7 @@
         <v>385</v>
       </c>
       <c r="C63" s="1" t="n">
-        <v>44070</v>
+        <v>44073</v>
       </c>
       <c r="D63" t="s">
         <v>386</v>
@@ -6062,31 +6066,31 @@
       </c>
       <c r="F63"/>
       <c r="G63" t="n">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="H63" t="n">
-        <v>391502</v>
+        <v>402070</v>
       </c>
       <c r="I63" t="n">
-        <v>1.899</v>
+        <v>1.95</v>
       </c>
       <c r="J63" t="n">
-        <v>3156</v>
+        <v>3766</v>
       </c>
       <c r="K63" t="n">
-        <v>0.015</v>
+        <v>0.018</v>
       </c>
       <c r="L63" t="n">
-        <v>3608</v>
+        <v>3435</v>
       </c>
       <c r="M63" t="n">
-        <v>0.018</v>
+        <v>0.017</v>
       </c>
       <c r="N63" t="n">
-        <v>0.1</v>
+        <v>0.076</v>
       </c>
       <c r="O63" t="n">
-        <v>9.971</v>
+        <v>13.197</v>
       </c>
       <c r="P63" t="s">
         <v>387</v>
@@ -6109,7 +6113,7 @@
         <v>391</v>
       </c>
       <c r="C64" s="1" t="n">
-        <v>44066</v>
+        <v>44069</v>
       </c>
       <c r="D64" t="s">
         <v>392</v>
@@ -6119,31 +6123,31 @@
       </c>
       <c r="F64"/>
       <c r="G64" t="n">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="H64" t="n">
-        <v>619288</v>
+        <v>664770</v>
       </c>
       <c r="I64" t="n">
-        <v>114.234</v>
+        <v>122.623</v>
       </c>
       <c r="J64" t="n">
-        <v>3353</v>
+        <v>10445</v>
       </c>
       <c r="K64" t="n">
-        <v>0.618</v>
+        <v>1.927</v>
       </c>
       <c r="L64" t="n">
-        <v>10743</v>
+        <v>11119</v>
       </c>
       <c r="M64" t="n">
-        <v>1.982</v>
+        <v>2.051</v>
       </c>
       <c r="N64" t="n">
-        <v>0.005</v>
+        <v>0.004</v>
       </c>
       <c r="O64" t="n">
-        <v>216.718</v>
+        <v>232.337</v>
       </c>
       <c r="P64" t="s">
         <v>393</v>
@@ -6211,7 +6215,7 @@
         <v>405</v>
       </c>
       <c r="C66" s="1" t="n">
-        <v>44071</v>
+        <v>44074</v>
       </c>
       <c r="D66" t="s">
         <v>406</v>
@@ -6221,31 +6225,31 @@
       </c>
       <c r="F66"/>
       <c r="G66" t="n">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="H66" t="n">
-        <v>2559261</v>
+        <v>2621146</v>
       </c>
       <c r="I66" t="n">
-        <v>11.586</v>
+        <v>11.866</v>
       </c>
       <c r="J66" t="n">
-        <v>23483</v>
+        <v>18017</v>
       </c>
       <c r="K66" t="n">
-        <v>0.106</v>
+        <v>0.082</v>
       </c>
       <c r="L66" t="n">
-        <v>24271</v>
+        <v>22519</v>
       </c>
       <c r="M66" t="n">
-        <v>0.11</v>
+        <v>0.102</v>
       </c>
       <c r="N66" t="n">
         <v>0.02</v>
       </c>
       <c r="O66" t="n">
-        <v>49.032</v>
+        <v>51.113</v>
       </c>
       <c r="P66" t="s">
         <v>407</v>
@@ -6268,7 +6272,7 @@
         <v>410</v>
       </c>
       <c r="C67" s="1" t="n">
-        <v>44069</v>
+        <v>44071</v>
       </c>
       <c r="D67" t="s">
         <v>411</v>
@@ -6278,31 +6282,31 @@
       </c>
       <c r="F67"/>
       <c r="G67" t="n">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="H67" t="n">
-        <v>313229</v>
+        <v>323049</v>
       </c>
       <c r="I67" t="n">
-        <v>72.595</v>
+        <v>74.871</v>
       </c>
       <c r="J67" t="n">
-        <v>3612</v>
+        <v>5115</v>
       </c>
       <c r="K67" t="n">
-        <v>0.837</v>
+        <v>1.185</v>
       </c>
       <c r="L67" t="n">
-        <v>4744</v>
+        <v>4912</v>
       </c>
       <c r="M67" t="n">
-        <v>1.099</v>
+        <v>1.138</v>
       </c>
       <c r="N67" t="n">
-        <v>0.168</v>
+        <v>0.178</v>
       </c>
       <c r="O67" t="n">
-        <v>5.94</v>
+        <v>5.612</v>
       </c>
       <c r="P67" t="s">
         <v>412</v>
@@ -6325,7 +6329,7 @@
         <v>416</v>
       </c>
       <c r="C68" s="1" t="n">
-        <v>44068</v>
+        <v>44071</v>
       </c>
       <c r="D68" t="s">
         <v>417</v>
@@ -6335,31 +6339,31 @@
       </c>
       <c r="F68"/>
       <c r="G68" t="n">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="H68" t="n">
-        <v>177771</v>
+        <v>185921</v>
       </c>
       <c r="I68" t="n">
-        <v>24.924</v>
+        <v>26.067</v>
       </c>
       <c r="J68" t="n">
-        <v>2119</v>
+        <v>3130</v>
       </c>
       <c r="K68" t="n">
-        <v>0.297</v>
+        <v>0.439</v>
       </c>
       <c r="L68" t="n">
-        <v>2586</v>
+        <v>2380</v>
       </c>
       <c r="M68" t="n">
-        <v>0.363</v>
+        <v>0.334</v>
       </c>
       <c r="N68" t="n">
-        <v>0.192</v>
+        <v>0.208</v>
       </c>
       <c r="O68" t="n">
-        <v>5.221</v>
+        <v>4.797</v>
       </c>
       <c r="P68" t="s">
         <v>418</v>
@@ -6382,7 +6386,7 @@
         <v>422</v>
       </c>
       <c r="C69" s="1" t="n">
-        <v>44061</v>
+        <v>44068</v>
       </c>
       <c r="D69" t="s">
         <v>423</v>
@@ -6392,25 +6396,25 @@
       </c>
       <c r="F69"/>
       <c r="G69" t="n">
-        <v>167</v>
+        <v>174</v>
       </c>
       <c r="H69" t="n">
-        <v>506901</v>
+        <v>552929</v>
       </c>
       <c r="I69" t="n">
-        <v>15.374</v>
+        <v>16.77</v>
       </c>
       <c r="J69" t="n">
-        <v>9044</v>
+        <v>3570</v>
       </c>
       <c r="K69" t="n">
-        <v>0.274</v>
+        <v>0.108</v>
       </c>
       <c r="L69" t="n">
-        <v>8538</v>
+        <v>6575</v>
       </c>
       <c r="M69" t="n">
-        <v>0.259</v>
+        <v>0.199</v>
       </c>
       <c r="N69"/>
       <c r="O69"/>
@@ -6435,7 +6439,7 @@
         <v>428</v>
       </c>
       <c r="C70" s="1" t="n">
-        <v>44065</v>
+        <v>44072</v>
       </c>
       <c r="D70" t="s">
         <v>429</v>
@@ -6445,31 +6449,31 @@
       </c>
       <c r="F70"/>
       <c r="G70" t="n">
-        <v>142</v>
+        <v>149</v>
       </c>
       <c r="H70" t="n">
-        <v>2158493</v>
+        <v>2403510</v>
       </c>
       <c r="I70" t="n">
-        <v>19.698</v>
+        <v>21.934</v>
       </c>
       <c r="J70" t="n">
-        <v>26333</v>
+        <v>33979</v>
       </c>
       <c r="K70" t="n">
-        <v>0.24</v>
+        <v>0.31</v>
       </c>
       <c r="L70" t="n">
-        <v>31469</v>
+        <v>32662</v>
       </c>
       <c r="M70" t="n">
-        <v>0.287</v>
+        <v>0.298</v>
       </c>
       <c r="N70" t="n">
-        <v>0.13</v>
+        <v>0.119</v>
       </c>
       <c r="O70" t="n">
-        <v>7.674</v>
+        <v>8.412</v>
       </c>
       <c r="P70" t="s">
         <v>219</v>
@@ -6492,7 +6496,7 @@
         <v>434</v>
       </c>
       <c r="C71" s="1" t="n">
-        <v>44070</v>
+        <v>44073</v>
       </c>
       <c r="D71" t="s">
         <v>435</v>
@@ -6502,31 +6506,31 @@
       </c>
       <c r="F71"/>
       <c r="G71" t="n">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="H71" t="n">
-        <v>2522949</v>
+        <v>2587559</v>
       </c>
       <c r="I71" t="n">
-        <v>66.662</v>
+        <v>68.37</v>
       </c>
       <c r="J71" t="n">
-        <v>27110</v>
+        <v>18753</v>
       </c>
       <c r="K71" t="n">
-        <v>0.716</v>
+        <v>0.496</v>
       </c>
       <c r="L71" t="n">
-        <v>23597</v>
+        <v>22478</v>
       </c>
       <c r="M71" t="n">
-        <v>0.623</v>
+        <v>0.594</v>
       </c>
       <c r="N71" t="n">
-        <v>0.031</v>
+        <v>0.032</v>
       </c>
       <c r="O71" t="n">
-        <v>31.82</v>
+        <v>31.108</v>
       </c>
       <c r="P71" t="s">
         <v>436</v>
@@ -6549,7 +6553,7 @@
         <v>439</v>
       </c>
       <c r="C72" s="1" t="n">
-        <v>44070</v>
+        <v>44073</v>
       </c>
       <c r="D72" t="s">
         <v>435</v>
@@ -6559,31 +6563,31 @@
       </c>
       <c r="F72"/>
       <c r="G72" t="n">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="H72" t="n">
-        <v>2634903</v>
+        <v>2701553</v>
       </c>
       <c r="I72" t="n">
-        <v>69.621</v>
+        <v>71.382</v>
       </c>
       <c r="J72" t="n">
-        <v>28283</v>
+        <v>19017</v>
       </c>
       <c r="K72" t="n">
-        <v>0.747</v>
+        <v>0.502</v>
       </c>
       <c r="L72" t="n">
-        <v>24453</v>
+        <v>23256</v>
       </c>
       <c r="M72" t="n">
-        <v>0.646</v>
+        <v>0.614</v>
       </c>
       <c r="N72" t="n">
-        <v>0.03</v>
+        <v>0.031</v>
       </c>
       <c r="O72" t="n">
-        <v>32.975</v>
+        <v>32.185</v>
       </c>
       <c r="P72" t="s">
         <v>436</v>
@@ -6606,7 +6610,7 @@
         <v>442</v>
       </c>
       <c r="C73" s="1" t="n">
-        <v>44055</v>
+        <v>44068</v>
       </c>
       <c r="D73" t="s">
         <v>443</v>
@@ -6616,31 +6620,31 @@
       </c>
       <c r="F73"/>
       <c r="G73" t="n">
-        <v>165</v>
+        <v>178</v>
       </c>
       <c r="H73" t="n">
-        <v>1799226</v>
+        <v>1976482</v>
       </c>
       <c r="I73" t="n">
-        <v>176.452</v>
+        <v>193.835</v>
       </c>
       <c r="J73" t="n">
-        <v>15899</v>
+        <v>17757</v>
       </c>
       <c r="K73" t="n">
-        <v>1.559</v>
+        <v>1.741</v>
       </c>
       <c r="L73" t="n">
-        <v>13380</v>
+        <v>13708</v>
       </c>
       <c r="M73" t="n">
-        <v>1.312</v>
+        <v>1.344</v>
       </c>
       <c r="N73" t="n">
-        <v>0.013</v>
+        <v>0.015</v>
       </c>
       <c r="O73" t="n">
-        <v>74.098</v>
+        <v>64.573</v>
       </c>
       <c r="P73" t="s">
         <v>444</v>
@@ -6663,7 +6667,7 @@
         <v>448</v>
       </c>
       <c r="C74" s="1" t="n">
-        <v>44070</v>
+        <v>44073</v>
       </c>
       <c r="D74" t="s">
         <v>449</v>
@@ -6673,31 +6677,31 @@
       </c>
       <c r="F74"/>
       <c r="G74" t="n">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="H74" t="n">
-        <v>609258</v>
+        <v>624609</v>
       </c>
       <c r="I74" t="n">
-        <v>211.47</v>
+        <v>216.798</v>
       </c>
       <c r="J74" t="n">
-        <v>5146</v>
+        <v>4481</v>
       </c>
       <c r="K74" t="n">
-        <v>1.786</v>
+        <v>1.555</v>
       </c>
       <c r="L74" t="n">
-        <v>5284</v>
+        <v>4956</v>
       </c>
       <c r="M74" t="n">
-        <v>1.834</v>
+        <v>1.72</v>
       </c>
       <c r="N74" t="n">
-        <v>0.048</v>
+        <v>0.047</v>
       </c>
       <c r="O74" t="n">
-        <v>20.71</v>
+        <v>21.128</v>
       </c>
       <c r="P74" t="s">
         <v>450</v>
@@ -6720,7 +6724,7 @@
         <v>454</v>
       </c>
       <c r="C75" s="1" t="n">
-        <v>44071</v>
+        <v>44073</v>
       </c>
       <c r="D75" t="s">
         <v>455</v>
@@ -6730,31 +6734,31 @@
       </c>
       <c r="F75"/>
       <c r="G75" t="n">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="H75" t="n">
-        <v>1756920</v>
+        <v>1795633</v>
       </c>
       <c r="I75" t="n">
-        <v>91.327</v>
+        <v>93.339</v>
       </c>
       <c r="J75" t="n">
-        <v>26500</v>
+        <v>14670</v>
       </c>
       <c r="K75" t="n">
-        <v>1.378</v>
+        <v>0.763</v>
       </c>
       <c r="L75" t="n">
-        <v>20077</v>
+        <v>20427</v>
       </c>
       <c r="M75" t="n">
-        <v>1.044</v>
+        <v>1.062</v>
       </c>
       <c r="N75" t="n">
         <v>0.058</v>
       </c>
       <c r="O75" t="n">
-        <v>17.166</v>
+        <v>17.25</v>
       </c>
       <c r="P75" t="s">
         <v>457</v>
@@ -6777,7 +6781,7 @@
         <v>461</v>
       </c>
       <c r="C76" s="1" t="n">
-        <v>44070</v>
+        <v>44073</v>
       </c>
       <c r="D76" t="s">
         <v>462</v>
@@ -6787,31 +6791,31 @@
       </c>
       <c r="F76"/>
       <c r="G76" t="n">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="H76" t="n">
-        <v>35751747</v>
+        <v>36696382</v>
       </c>
       <c r="I76" t="n">
-        <v>244.985</v>
+        <v>251.458</v>
       </c>
       <c r="J76" t="n">
-        <v>327964</v>
+        <v>269532</v>
       </c>
       <c r="K76" t="n">
-        <v>2.247</v>
+        <v>1.847</v>
       </c>
       <c r="L76" t="n">
-        <v>276806</v>
+        <v>285854</v>
       </c>
       <c r="M76" t="n">
-        <v>1.897</v>
+        <v>1.959</v>
       </c>
       <c r="N76" t="n">
         <v>0.017</v>
       </c>
       <c r="O76" t="n">
-        <v>57.764</v>
+        <v>59.822</v>
       </c>
       <c r="P76" t="s">
         <v>463</v>
@@ -6834,7 +6838,7 @@
         <v>467</v>
       </c>
       <c r="C77" s="1" t="n">
-        <v>44068</v>
+        <v>44071</v>
       </c>
       <c r="D77" t="s">
         <v>468</v>
@@ -6844,31 +6848,31 @@
       </c>
       <c r="F77"/>
       <c r="G77" t="n">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="H77" t="n">
-        <v>378014</v>
+        <v>393237</v>
       </c>
       <c r="I77" t="n">
-        <v>29.185</v>
+        <v>30.361</v>
       </c>
       <c r="J77" t="n">
-        <v>6128</v>
+        <v>5159</v>
       </c>
       <c r="K77" t="n">
-        <v>0.473</v>
+        <v>0.398</v>
       </c>
       <c r="L77" t="n">
-        <v>5057</v>
+        <v>5165</v>
       </c>
       <c r="M77" t="n">
-        <v>0.39</v>
+        <v>0.399</v>
       </c>
       <c r="N77" t="n">
-        <v>0.022</v>
+        <v>0.026</v>
       </c>
       <c r="O77" t="n">
-        <v>46.213</v>
+        <v>37.859</v>
       </c>
       <c r="P77" t="s">
         <v>469</v>
@@ -6891,7 +6895,7 @@
         <v>473</v>
       </c>
       <c r="C78" s="1" t="n">
-        <v>44070</v>
+        <v>44073</v>
       </c>
       <c r="D78" t="s">
         <v>474</v>
@@ -6901,31 +6905,31 @@
       </c>
       <c r="F78"/>
       <c r="G78" t="n">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="H78" t="n">
-        <v>4913924</v>
+        <v>5063593</v>
       </c>
       <c r="I78" t="n">
-        <v>141.148</v>
+        <v>145.448</v>
       </c>
       <c r="J78" t="n">
-        <v>63265</v>
+        <v>37466</v>
       </c>
       <c r="K78" t="n">
-        <v>1.817</v>
+        <v>1.076</v>
       </c>
       <c r="L78" t="n">
-        <v>58974</v>
+        <v>55076</v>
       </c>
       <c r="M78" t="n">
-        <v>1.694</v>
+        <v>1.582</v>
       </c>
       <c r="N78" t="n">
         <v>0.02</v>
       </c>
       <c r="O78" t="n">
-        <v>50.653</v>
+        <v>51.125</v>
       </c>
       <c r="P78" t="s">
         <v>45</v>
@@ -6948,7 +6952,7 @@
         <v>477</v>
       </c>
       <c r="C79" s="1" t="n">
-        <v>44069</v>
+        <v>44073</v>
       </c>
       <c r="D79" t="s">
         <v>478</v>
@@ -6960,31 +6964,31 @@
         <v>480</v>
       </c>
       <c r="G79" t="n">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="H79" t="n">
-        <v>145948</v>
+        <v>151044</v>
       </c>
       <c r="I79" t="n">
-        <v>8.716</v>
+        <v>9.021</v>
       </c>
       <c r="J79" t="n">
-        <v>1384</v>
+        <v>1276</v>
       </c>
       <c r="K79" t="n">
-        <v>0.083</v>
+        <v>0.076</v>
       </c>
       <c r="L79" t="n">
-        <v>1251</v>
+        <v>1158</v>
       </c>
       <c r="M79" t="n">
+        <v>0.069</v>
+      </c>
+      <c r="N79" t="n">
         <v>0.075</v>
       </c>
-      <c r="N79" t="n">
-        <v>0.086</v>
-      </c>
       <c r="O79" t="n">
-        <v>11.66</v>
+        <v>13.376</v>
       </c>
       <c r="P79" t="s">
         <v>481</v>
@@ -7007,7 +7011,7 @@
         <v>485</v>
       </c>
       <c r="C80" s="1" t="n">
-        <v>44070</v>
+        <v>44073</v>
       </c>
       <c r="D80" t="s">
         <v>486</v>
@@ -7019,31 +7023,31 @@
         <v>487</v>
       </c>
       <c r="G80" t="n">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="H80" t="n">
-        <v>904343</v>
+        <v>925208</v>
       </c>
       <c r="I80" t="n">
-        <v>132.902</v>
+        <v>135.968</v>
       </c>
       <c r="J80" t="n">
-        <v>8836</v>
+        <v>4356</v>
       </c>
       <c r="K80" t="n">
-        <v>1.299</v>
+        <v>0.64</v>
       </c>
       <c r="L80" t="n">
-        <v>8843</v>
+        <v>7934</v>
       </c>
       <c r="M80" t="n">
-        <v>1.3</v>
+        <v>1.166</v>
       </c>
       <c r="N80" t="n">
-        <v>0.015</v>
+        <v>0.013</v>
       </c>
       <c r="O80" t="n">
-        <v>66.848</v>
+        <v>75.665</v>
       </c>
       <c r="P80" t="s">
         <v>45</v>
@@ -7172,7 +7176,7 @@
         <v>497</v>
       </c>
       <c r="C83" s="1" t="n">
-        <v>44070</v>
+        <v>44073</v>
       </c>
       <c r="D83" t="s">
         <v>498</v>
@@ -7182,31 +7186,31 @@
       </c>
       <c r="F83"/>
       <c r="G83" t="n">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="H83" t="n">
-        <v>327940</v>
+        <v>334344</v>
       </c>
       <c r="I83" t="n">
-        <v>60.066</v>
+        <v>61.239</v>
       </c>
       <c r="J83" t="n">
-        <v>7996</v>
+        <v>1951</v>
       </c>
       <c r="K83" t="n">
-        <v>1.465</v>
+        <v>0.357</v>
       </c>
       <c r="L83" t="n">
-        <v>3417</v>
+        <v>3075</v>
       </c>
       <c r="M83" t="n">
-        <v>0.626</v>
+        <v>0.563</v>
       </c>
       <c r="N83" t="n">
-        <v>0.021</v>
+        <v>0.024</v>
       </c>
       <c r="O83" t="n">
-        <v>46.535</v>
+        <v>40.922</v>
       </c>
       <c r="P83" t="s">
         <v>500</v>
@@ -7229,7 +7233,7 @@
         <v>503</v>
       </c>
       <c r="C84" s="1" t="n">
-        <v>44070</v>
+        <v>44073</v>
       </c>
       <c r="D84" t="s">
         <v>504</v>
@@ -7239,31 +7243,31 @@
       </c>
       <c r="F84"/>
       <c r="G84" t="n">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="H84" t="n">
-        <v>154771</v>
+        <v>157456</v>
       </c>
       <c r="I84" t="n">
-        <v>74.447</v>
+        <v>75.739</v>
       </c>
       <c r="J84" t="n">
-        <v>1338</v>
+        <v>588</v>
       </c>
       <c r="K84" t="n">
-        <v>0.644</v>
+        <v>0.283</v>
       </c>
       <c r="L84" t="n">
-        <v>1136</v>
+        <v>1174</v>
       </c>
       <c r="M84" t="n">
-        <v>0.546</v>
+        <v>0.565</v>
       </c>
       <c r="N84" t="n">
-        <v>0.029</v>
+        <v>0.026</v>
       </c>
       <c r="O84" t="n">
-        <v>34.725</v>
+        <v>37.871</v>
       </c>
       <c r="P84" t="s">
         <v>506</v>
@@ -7286,7 +7290,7 @@
         <v>510</v>
       </c>
       <c r="C85" s="1" t="n">
-        <v>44070</v>
+        <v>44073</v>
       </c>
       <c r="D85" t="s">
         <v>511</v>
@@ -7298,31 +7302,31 @@
         <v>513</v>
       </c>
       <c r="G85" t="n">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="H85" t="n">
-        <v>3617982</v>
+        <v>3674872</v>
       </c>
       <c r="I85" t="n">
-        <v>61.003</v>
+        <v>61.962</v>
       </c>
       <c r="J85" t="n">
-        <v>19009</v>
+        <v>21902</v>
       </c>
       <c r="K85" t="n">
-        <v>0.321</v>
+        <v>0.369</v>
       </c>
       <c r="L85" t="n">
-        <v>19671</v>
+        <v>17350</v>
       </c>
       <c r="M85" t="n">
-        <v>0.332</v>
+        <v>0.293</v>
       </c>
       <c r="N85" t="n">
-        <v>0.143</v>
+        <v>0.128</v>
       </c>
       <c r="O85" t="n">
-        <v>7.011</v>
+        <v>7.832</v>
       </c>
       <c r="P85" t="s">
         <v>512</v>
@@ -7345,7 +7349,7 @@
         <v>517</v>
       </c>
       <c r="C86" s="1" t="n">
-        <v>44071</v>
+        <v>44074</v>
       </c>
       <c r="D86" t="s">
         <v>518</v>
@@ -7355,31 +7359,31 @@
       </c>
       <c r="F86"/>
       <c r="G86" t="n">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="H86" t="n">
-        <v>1837006</v>
+        <v>1879813</v>
       </c>
       <c r="I86" t="n">
-        <v>35.831</v>
+        <v>36.666</v>
       </c>
       <c r="J86" t="n">
-        <v>19468</v>
+        <v>13664</v>
       </c>
       <c r="K86" t="n">
-        <v>0.38</v>
+        <v>0.267</v>
       </c>
       <c r="L86" t="n">
-        <v>17275</v>
+        <v>17627</v>
       </c>
       <c r="M86" t="n">
-        <v>0.337</v>
+        <v>0.344</v>
       </c>
       <c r="N86" t="n">
-        <v>0.02</v>
+        <v>0.018</v>
       </c>
       <c r="O86" t="n">
-        <v>50.239</v>
+        <v>54.071</v>
       </c>
       <c r="P86" t="s">
         <v>519</v>
@@ -7561,7 +7565,7 @@
         <v>540</v>
       </c>
       <c r="C90" s="1" t="n">
-        <v>44070</v>
+        <v>44072</v>
       </c>
       <c r="D90" t="s">
         <v>541</v>
@@ -7571,31 +7575,31 @@
       </c>
       <c r="F90"/>
       <c r="G90" t="n">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="H90" t="n">
-        <v>988383</v>
+        <v>1012884</v>
       </c>
       <c r="I90" t="n">
-        <v>114.203</v>
+        <v>117.034</v>
       </c>
       <c r="J90" t="n">
-        <v>9437</v>
+        <v>8180</v>
       </c>
       <c r="K90" t="n">
-        <v>1.09</v>
+        <v>0.945</v>
       </c>
       <c r="L90" t="n">
-        <v>9172</v>
+        <v>10382</v>
       </c>
       <c r="M90" t="n">
-        <v>1.06</v>
+        <v>1.2</v>
       </c>
       <c r="N90" t="n">
-        <v>0.029</v>
+        <v>0.028</v>
       </c>
       <c r="O90" t="n">
-        <v>34.187</v>
+        <v>36.192</v>
       </c>
       <c r="P90" t="s">
         <v>542</v>
@@ -7618,7 +7622,7 @@
         <v>546</v>
       </c>
       <c r="C91" s="1" t="n">
-        <v>44070</v>
+        <v>44073</v>
       </c>
       <c r="D91" t="s">
         <v>547</v>
@@ -7628,31 +7632,31 @@
       </c>
       <c r="F91"/>
       <c r="G91" t="n">
-        <v>224</v>
+        <v>227</v>
       </c>
       <c r="H91" t="n">
-        <v>86806</v>
+        <v>87291</v>
       </c>
       <c r="I91" t="n">
-        <v>3.645</v>
+        <v>3.665</v>
       </c>
       <c r="J91" t="n">
-        <v>204</v>
+        <v>157</v>
       </c>
       <c r="K91" t="n">
-        <v>0.009</v>
+        <v>0.007</v>
       </c>
       <c r="L91" t="n">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="M91" t="n">
-        <v>0.007</v>
+        <v>0.008</v>
       </c>
       <c r="N91" t="n">
         <v>0.001</v>
       </c>
       <c r="O91" t="n">
-        <v>1246</v>
+        <v>1267</v>
       </c>
       <c r="P91" t="s">
         <v>548</v>
@@ -7675,7 +7679,7 @@
         <v>551</v>
       </c>
       <c r="C92" s="1" t="n">
-        <v>44070</v>
+        <v>44073</v>
       </c>
       <c r="D92" t="s">
         <v>552</v>
@@ -7685,31 +7689,31 @@
       </c>
       <c r="F92"/>
       <c r="G92" t="n">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="H92" t="n">
-        <v>413006</v>
+        <v>417044</v>
       </c>
       <c r="I92" t="n">
-        <v>5.917</v>
+        <v>5.975</v>
       </c>
       <c r="J92" t="n">
-        <v>1806</v>
+        <v>1111</v>
       </c>
       <c r="K92" t="n">
-        <v>0.026</v>
+        <v>0.016</v>
       </c>
       <c r="L92" t="n">
-        <v>1618</v>
+        <v>1553</v>
       </c>
       <c r="M92" t="n">
-        <v>0.023</v>
+        <v>0.022</v>
       </c>
       <c r="N92" t="n">
         <v>0.001</v>
       </c>
       <c r="O92" t="n">
-        <v>755.067</v>
+        <v>679.438</v>
       </c>
       <c r="P92" t="s">
         <v>553</v>
@@ -7732,7 +7736,7 @@
         <v>556</v>
       </c>
       <c r="C93" s="1" t="n">
-        <v>44070</v>
+        <v>44073</v>
       </c>
       <c r="D93" t="s">
         <v>552</v>
@@ -7742,31 +7746,31 @@
       </c>
       <c r="F93"/>
       <c r="G93" t="n">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="H93" t="n">
-        <v>840416</v>
+        <v>844454</v>
       </c>
       <c r="I93" t="n">
-        <v>12.04</v>
+        <v>12.098</v>
       </c>
       <c r="J93" t="n">
-        <v>40945</v>
+        <v>1111</v>
       </c>
       <c r="K93" t="n">
-        <v>0.587</v>
+        <v>0.016</v>
       </c>
       <c r="L93" t="n">
-        <v>7209</v>
+        <v>7144</v>
       </c>
       <c r="M93" t="n">
-        <v>0.103</v>
+        <v>0.102</v>
       </c>
       <c r="N93" t="n">
         <v>0</v>
       </c>
       <c r="O93" t="n">
-        <v>3364.2</v>
+        <v>3125.5</v>
       </c>
       <c r="P93" t="s">
         <v>553</v>
@@ -7846,7 +7850,7 @@
         <v>565</v>
       </c>
       <c r="C95" s="1" t="n">
-        <v>44067</v>
+        <v>44070</v>
       </c>
       <c r="D95" t="s">
         <v>566</v>
@@ -7856,31 +7860,31 @@
       </c>
       <c r="F95"/>
       <c r="G95" t="n">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="H95" t="n">
-        <v>128027</v>
+        <v>136199</v>
       </c>
       <c r="I95" t="n">
-        <v>10.833</v>
+        <v>11.524</v>
       </c>
       <c r="J95" t="n">
-        <v>2251</v>
+        <v>2586</v>
       </c>
       <c r="K95" t="n">
-        <v>0.19</v>
+        <v>0.219</v>
       </c>
       <c r="L95" t="n">
-        <v>2038</v>
+        <v>2375</v>
       </c>
       <c r="M95" t="n">
-        <v>0.172</v>
+        <v>0.201</v>
       </c>
       <c r="N95" t="n">
-        <v>0.044</v>
+        <v>0.047</v>
       </c>
       <c r="O95" t="n">
-        <v>22.609</v>
+        <v>21.341</v>
       </c>
       <c r="P95" t="s">
         <v>567</v>
@@ -7903,7 +7907,7 @@
         <v>570</v>
       </c>
       <c r="C96" s="1" t="n">
-        <v>44070</v>
+        <v>44073</v>
       </c>
       <c r="D96" t="s">
         <v>571</v>
@@ -7913,31 +7917,31 @@
       </c>
       <c r="F96"/>
       <c r="G96" t="n">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="H96" t="n">
-        <v>6727860</v>
+        <v>7028390</v>
       </c>
       <c r="I96" t="n">
-        <v>79.772</v>
+        <v>83.335</v>
       </c>
       <c r="J96" t="n">
-        <v>106111</v>
+        <v>91302</v>
       </c>
       <c r="K96" t="n">
-        <v>1.258</v>
+        <v>1.083</v>
       </c>
       <c r="L96" t="n">
-        <v>95133</v>
+        <v>100132</v>
       </c>
       <c r="M96" t="n">
-        <v>1.128</v>
+        <v>1.187</v>
       </c>
       <c r="N96" t="n">
         <v>0.014</v>
       </c>
       <c r="O96" t="n">
-        <v>70.851</v>
+        <v>69.869</v>
       </c>
       <c r="P96" t="s">
         <v>572</v>
@@ -7960,7 +7964,7 @@
         <v>575</v>
       </c>
       <c r="C97" s="1" t="n">
-        <v>44069</v>
+        <v>44070</v>
       </c>
       <c r="D97" t="s">
         <v>576</v>
@@ -7970,31 +7974,31 @@
       </c>
       <c r="F97"/>
       <c r="G97" t="n">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="H97" t="n">
-        <v>363802</v>
+        <v>367423</v>
       </c>
       <c r="I97" t="n">
-        <v>7.954</v>
+        <v>8.033</v>
       </c>
       <c r="J97" t="n">
-        <v>4513</v>
+        <v>3621</v>
       </c>
       <c r="K97" t="n">
-        <v>0.099</v>
+        <v>0.079</v>
       </c>
       <c r="L97" t="n">
-        <v>3870</v>
+        <v>3797</v>
       </c>
       <c r="M97" t="n">
-        <v>0.085</v>
+        <v>0.083</v>
       </c>
       <c r="N97" t="n">
-        <v>0.03</v>
+        <v>0.035</v>
       </c>
       <c r="O97" t="n">
-        <v>32.916</v>
+        <v>28.859</v>
       </c>
       <c r="P97" t="s">
         <v>577</v>
@@ -8017,7 +8021,7 @@
         <v>581</v>
       </c>
       <c r="C98" s="1" t="n">
-        <v>44071</v>
+        <v>44074</v>
       </c>
       <c r="D98" t="s">
         <v>582</v>
@@ -8027,31 +8031,31 @@
       </c>
       <c r="F98"/>
       <c r="G98" t="n">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="H98" t="n">
-        <v>1494243</v>
+        <v>1550280</v>
       </c>
       <c r="I98" t="n">
-        <v>34.167</v>
+        <v>35.448</v>
       </c>
       <c r="J98" t="n">
-        <v>21507</v>
+        <v>14109</v>
       </c>
       <c r="K98" t="n">
-        <v>0.492</v>
+        <v>0.323</v>
       </c>
       <c r="L98" t="n">
-        <v>16532</v>
+        <v>17847</v>
       </c>
       <c r="M98" t="n">
-        <v>0.378</v>
+        <v>0.408</v>
       </c>
       <c r="N98" t="n">
-        <v>0.117</v>
+        <v>0.113</v>
       </c>
       <c r="O98" t="n">
-        <v>8.558</v>
+        <v>8.85</v>
       </c>
       <c r="P98" t="s">
         <v>583</v>
@@ -8074,7 +8078,7 @@
         <v>587</v>
       </c>
       <c r="C99" s="1" t="n">
-        <v>44070</v>
+        <v>44073</v>
       </c>
       <c r="D99" t="s">
         <v>588</v>
@@ -8084,31 +8088,31 @@
       </c>
       <c r="F99"/>
       <c r="G99" t="n">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="H99" t="n">
-        <v>6755457</v>
+        <v>7011895</v>
       </c>
       <c r="I99" t="n">
-        <v>683.032</v>
+        <v>708.96</v>
       </c>
       <c r="J99" t="n">
-        <v>68043</v>
+        <v>87955</v>
       </c>
       <c r="K99" t="n">
-        <v>6.88</v>
+        <v>8.893</v>
       </c>
       <c r="L99" t="n">
-        <v>69934</v>
+        <v>74642</v>
       </c>
       <c r="M99" t="n">
-        <v>7.071</v>
+        <v>7.547</v>
       </c>
       <c r="N99" t="n">
         <v>0.005</v>
       </c>
       <c r="O99" t="n">
-        <v>182.732</v>
+        <v>192.731</v>
       </c>
       <c r="P99" t="s">
         <v>589</v>
@@ -8131,7 +8135,7 @@
         <v>592</v>
       </c>
       <c r="C100" s="1" t="n">
-        <v>44062</v>
+        <v>44069</v>
       </c>
       <c r="D100" t="s">
         <v>593</v>
@@ -8143,31 +8147,31 @@
         <v>595</v>
       </c>
       <c r="G100" t="n">
-        <v>142</v>
+        <v>148</v>
       </c>
       <c r="H100" t="n">
-        <v>12446595</v>
+        <v>13447568</v>
       </c>
       <c r="I100" t="n">
-        <v>183.346</v>
+        <v>198.09</v>
       </c>
       <c r="J100" t="n">
-        <v>175916</v>
+        <v>163158</v>
       </c>
       <c r="K100" t="n">
-        <v>2.591</v>
+        <v>2.403</v>
       </c>
       <c r="L100" t="n">
-        <v>162256</v>
+        <v>167916</v>
       </c>
       <c r="M100" t="n">
-        <v>2.39</v>
+        <v>2.473</v>
       </c>
       <c r="N100" t="n">
-        <v>0.007</v>
+        <v>0.006</v>
       </c>
       <c r="O100" t="n">
-        <v>151.5</v>
+        <v>156.471</v>
       </c>
       <c r="P100" t="s">
         <v>594</v>
@@ -8190,7 +8194,7 @@
         <v>599</v>
       </c>
       <c r="C101" s="1" t="n">
-        <v>44068</v>
+        <v>44071</v>
       </c>
       <c r="D101" t="s">
         <v>600</v>
@@ -8200,31 +8204,31 @@
       </c>
       <c r="F101"/>
       <c r="G101" t="n">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="H101" t="n">
-        <v>81462633</v>
+        <v>83898416</v>
       </c>
       <c r="I101" t="n">
-        <v>246.109</v>
+        <v>253.468</v>
       </c>
       <c r="J101" t="n">
-        <v>636249</v>
+        <v>523870</v>
       </c>
       <c r="K101" t="n">
-        <v>1.922</v>
+        <v>1.583</v>
       </c>
       <c r="L101" t="n">
-        <v>740927</v>
+        <v>672164</v>
       </c>
       <c r="M101" t="n">
-        <v>2.238</v>
+        <v>2.031</v>
       </c>
       <c r="N101" t="n">
-        <v>0.058</v>
+        <v>0.062</v>
       </c>
       <c r="O101" t="n">
-        <v>17.141</v>
+        <v>16.007</v>
       </c>
       <c r="P101" t="s">
         <v>602</v>
@@ -8247,7 +8251,7 @@
         <v>606</v>
       </c>
       <c r="C102" s="1" t="n">
-        <v>44070</v>
+        <v>44073</v>
       </c>
       <c r="D102" t="s">
         <v>607</v>
@@ -8257,31 +8261,31 @@
       </c>
       <c r="F102"/>
       <c r="G102" t="n">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="H102" t="n">
-        <v>74792493</v>
+        <v>77063268</v>
       </c>
       <c r="I102" t="n">
-        <v>225.957</v>
+        <v>232.818</v>
       </c>
       <c r="J102" t="n">
-        <v>742340</v>
+        <v>737701</v>
       </c>
       <c r="K102" t="n">
-        <v>2.243</v>
+        <v>2.229</v>
       </c>
       <c r="L102" t="n">
-        <v>692794</v>
+        <v>714953</v>
       </c>
       <c r="M102" t="n">
-        <v>2.093</v>
+        <v>2.16</v>
       </c>
       <c r="N102" t="n">
-        <v>0.06</v>
+        <v>0.059</v>
       </c>
       <c r="O102" t="n">
-        <v>16.606</v>
+        <v>17.053</v>
       </c>
       <c r="P102" t="s">
         <v>608</v>
@@ -8304,7 +8308,7 @@
         <v>613</v>
       </c>
       <c r="C103" s="1" t="n">
-        <v>44070</v>
+        <v>44072</v>
       </c>
       <c r="D103" t="s">
         <v>614</v>
@@ -8314,31 +8318,31 @@
       </c>
       <c r="F103"/>
       <c r="G103" t="n">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="H103" t="n">
-        <v>166117</v>
+        <v>171237</v>
       </c>
       <c r="I103" t="n">
-        <v>47.821</v>
+        <v>49.295</v>
       </c>
       <c r="J103" t="n">
-        <v>1379</v>
+        <v>3521</v>
       </c>
       <c r="K103" t="n">
-        <v>0.397</v>
+        <v>1.014</v>
       </c>
       <c r="L103" t="n">
-        <v>1669</v>
+        <v>1791</v>
       </c>
       <c r="M103" t="n">
-        <v>0.48</v>
+        <v>0.516</v>
       </c>
       <c r="N103" t="n">
-        <v>0.004</v>
+        <v>0.003</v>
       </c>
       <c r="O103" t="n">
-        <v>233.66</v>
+        <v>313.425</v>
       </c>
       <c r="P103" t="s">
         <v>125</v>
@@ -8414,7 +8418,7 @@
         <v>624</v>
       </c>
       <c r="C105" s="1" t="n">
-        <v>44068</v>
+        <v>44071</v>
       </c>
       <c r="D105" t="s">
         <v>625</v>
@@ -8424,31 +8428,31 @@
       </c>
       <c r="F105"/>
       <c r="G105" t="n">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="H105" t="n">
-        <v>93892</v>
+        <v>97272</v>
       </c>
       <c r="I105" t="n">
-        <v>6.317</v>
+        <v>6.545</v>
       </c>
       <c r="J105" t="n">
-        <v>1574</v>
+        <v>1551</v>
       </c>
       <c r="K105" t="n">
-        <v>0.106</v>
+        <v>0.104</v>
       </c>
       <c r="L105" t="n">
-        <v>1269</v>
+        <v>1082</v>
       </c>
       <c r="M105" t="n">
-        <v>0.085</v>
+        <v>0.073</v>
       </c>
       <c r="N105" t="n">
-        <v>0.086</v>
+        <v>0.072</v>
       </c>
       <c r="O105" t="n">
-        <v>11.657</v>
+        <v>13.846</v>
       </c>
       <c r="P105" t="s">
         <v>626</v>

</xml_diff>

<commit_message>
Updated testing data for 2020-09-02
</commit_message>
<xml_diff>
--- a/public/data/testing/covid-testing-latest-data-source-details.xlsx
+++ b/public/data/testing/covid-testing-latest-data-source-details.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="629" uniqueCount="629">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="630" uniqueCount="630">
   <si>
     <t xml:space="preserve">ISO code</t>
   </si>
@@ -110,7 +110,7 @@
     <t xml:space="preserve">Australia - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.health.gov.au/sites/default/files/documents/2020/08/coronavirus-covid-19-at-a-glance-30-august-2020.pdf</t>
+    <t xml:space="preserve">https://www.health.gov.au/sites/default/files/documents/2020/09/coronavirus-covid-19-at-a-glance-1-september-2020.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">Australian Government Department of Health</t>
@@ -202,7 +202,7 @@
     <t xml:space="preserve">Belarus - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">http://minzdrav.gov.by/ru/sobytiya/u-belarusi-na-27-zhni-nya-vypisanyya-69-tys-650-patsyenta/</t>
+    <t xml:space="preserve">http://minzdrav.gov.by/ru/sobytiya/u-belarusi-na-1-verasnya-vypisanyya-70-tys-606-patsyenta/</t>
   </si>
   <si>
     <t xml:space="preserve">Belarus Ministry of Health</t>
@@ -245,7 +245,7 @@
     <t xml:space="preserve">Bolivia - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://minsalud.gob.bo/4558-covid-19-ministerio-de-salud-reporta-1-035-contagios-nuevos-y-65-fallecidos</t>
+    <t xml:space="preserve">https://minsalud.gob.bo/4568-bolivia-acumula-60-408-pacientes-recuperados-de-covid-19-y-los-casos-positivos-llegan-a-116-598</t>
   </si>
   <si>
     <t xml:space="preserve">https://www.minsalud.gob.bo/</t>
@@ -398,7 +398,7 @@
     <t xml:space="preserve">Cote d'Ivoire - samples tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.facebook.com/Mshpci/posts/1683118181853869</t>
+    <t xml:space="preserve">https://www.facebook.com/Mshpci/posts/1684886605010360</t>
   </si>
   <si>
     <t xml:space="preserve">Ministry of Health and Public Hygiene</t>
@@ -477,7 +477,7 @@
     <t xml:space="preserve">Democratic Republic of Congo - samples tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/CMR_Covid19_RDC/status/1299647693489418241/photo/1</t>
+    <t xml:space="preserve">https://twitter.com/CMR_Covid19_RDC/status/1300552942563610625/photo/1</t>
   </si>
   <si>
     <t xml:space="preserve">DRC COVID-19 Pandemic Response Multisectoral Committee</t>
@@ -495,7 +495,7 @@
     <t xml:space="preserve">Denmark - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://files.ssi.dk/Data-epidemiologiske-rapport-31082020-lo27</t>
+    <t xml:space="preserve">https://files.ssi.dk/Data-epidemiologisk-rapport-01092020-ffe6</t>
   </si>
   <si>
     <t xml:space="preserve">Statens Serum Institut</t>
@@ -513,7 +513,7 @@
     <t xml:space="preserve">Ecuador - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.gestionderiesgos.gob.ec/wp-content/uploads/2020/08/INFOGRAFIA-NACIONALCOVID19-COE-NACIONAL-08h00-29082020.pdf</t>
+    <t xml:space="preserve">https://www.gestionderiesgos.gob.ec/wp-content/uploads/2020/08/INFOGRAFIA-NACIONALCOVID19-COE-NACIONAL-08h00-30082020.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">Government of Ecuador</t>
@@ -753,7 +753,7 @@
     <t xml:space="preserve">Greece - samples tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://eody.gov.gr/covid-gr-daily-report-20200830</t>
+    <t xml:space="preserve">https://eody.gov.gr/covid-gr-daily-report-20200901</t>
   </si>
   <si>
     <t xml:space="preserve">National Organization of Public Health</t>
@@ -892,7 +892,7 @@
     <t xml:space="preserve">Iran - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">http://irangov.ir/detail/346157</t>
+    <t xml:space="preserve">http://irangov.ir/detail/346224</t>
   </si>
   <si>
     <t xml:space="preserve">Government of Iran</t>
@@ -912,7 +912,7 @@
     <t xml:space="preserve">Iraq - samples tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://moh.gov.iq/index.php?name=News&amp;file=article&amp;sid=16464</t>
+    <t xml:space="preserve">https://moh.gov.iq/index.php?name=News&amp;file=article&amp;sid=16522</t>
   </si>
   <si>
     <t xml:space="preserve">Ministry of Health and Environment</t>
@@ -950,7 +950,7 @@
     <t xml:space="preserve">Israel - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://govextra.gov.il/media/25848/covid19-data-israel-24082021.csv</t>
+    <t xml:space="preserve">https://govextra.gov.il/media/26180/covid19-data-israel-26082021.csv</t>
   </si>
   <si>
     <t xml:space="preserve">Israel Ministry of Health</t>
@@ -1009,7 +1009,7 @@
     <t xml:space="preserve">Japan - people tested (incl. non-PCR)</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.mhlw.go.jp/stf/newpage_13273.html</t>
+    <t xml:space="preserve">https://www.mhlw.go.jp/stf/newpage_13311.html</t>
   </si>
   <si>
     <t xml:space="preserve">Ministry of Health, Labor and Welfare Press Release</t>
@@ -1034,10 +1034,10 @@
     <t xml:space="preserve">Japan - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.mhlw.go.jp/content/10906000/000664890.pdf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The cumulative total reported in the press release (1,768,968) does not sum to the cumulative total calculated from the weekly and daily figures reported by the MOH. See: https://www.mhlw.go.jp/content/10906000/000664890.pdf</t>
+    <t xml:space="preserve">https://www.mhlw.go.jp/content/10906000/000666239.pdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The cumulative total reported in the press release (1,815,298) does not sum to the cumulative total calculated from the weekly and daily figures reported by the MOH. See: https://www.mhlw.go.jp/content/10906000/000666239.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">On 11 April 2020, the MOH started providing a daily time series on the "Implementation status of PCR tests for new coronavirus in Japan (based on the date on which results were determined" (via Google translate). 
@@ -1090,7 +1090,7 @@
     <t xml:space="preserve">Kuwait - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/KUWAIT_MOH/status/1299663124493197313/photo/1</t>
+    <t xml:space="preserve">https://twitter.com/KUWAIT_MOH/status/1300765420702633984/photo/1</t>
   </si>
   <si>
     <t xml:space="preserve">Kuwait Ministry of Health</t>
@@ -1156,7 +1156,7 @@
     <t xml:space="preserve">Malaysia - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">http://covid-19.moh.gov.my/terkini/082020/situasi-terkini-30-ogos-2020</t>
+    <t xml:space="preserve">http://covid-19.moh.gov.my/terkini/092020/situasi-terkini-01-september-2020</t>
   </si>
   <si>
     <t xml:space="preserve">Ministry of Health Malaysia</t>
@@ -1182,7 +1182,7 @@
     <t xml:space="preserve">Maldives - samples tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/HPA_MV/status/1299757834071023617/photo/1</t>
+    <t xml:space="preserve">https://twitter.com/HPA_MV/status/1300845834117017602/photo/1</t>
   </si>
   <si>
     <t xml:space="preserve">Maldives Health Protection Agency</t>
@@ -1248,7 +1248,7 @@
     <t xml:space="preserve">Morocco - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/Ministere_Sante/status/1299760106150731777/photo/1</t>
+    <t xml:space="preserve">https://twitter.com/Ministere_Sante/status/1300845577253650433/photo/1</t>
   </si>
   <si>
     <t xml:space="preserve">Morocco Ministry of Health</t>
@@ -1288,7 +1288,7 @@
     <t xml:space="preserve">Nepal - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://drive.google.com/drive/folders/1wbintzK9V_XDb6I2qqn5l1Blo2sVRMQ6</t>
+    <t xml:space="preserve">https://drive.google.com/drive/folders/1CUjrDYrYfsNGPyk_TWvvw3gTgXeAbF0U</t>
   </si>
   <si>
     <t xml:space="preserve">Ministry of Health and Population</t>
@@ -1435,7 +1435,7 @@
     <t xml:space="preserve">Panama - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/MINSAPma/status/1299488397359280128/photo/1</t>
+    <t xml:space="preserve">https://twitter.com/MINSAPma/status/1300589990620139523/photo/1</t>
   </si>
   <si>
     <t xml:space="preserve">Panama Ministry of Health</t>
@@ -1475,7 +1475,7 @@
     <t xml:space="preserve">Peru - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.dge.gob.pe/portal/docs/tools/coronavirus/coronavirus250820.pdf</t>
+    <t xml:space="preserve">https://www.dge.gob.pe/portal/docs/tools/coronavirus/coronavirus290820.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">Peru Ministry of Health</t>
@@ -1516,7 +1516,7 @@
     <t xml:space="preserve">Poland - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/MZ_GOV_PL/status/1299995274182623232</t>
+    <t xml:space="preserve">https://twitter.com/MZ_GOV_PL/status/1300720054711889920</t>
   </si>
   <si>
     <t xml:space="preserve">Poland Ministry of Health</t>
@@ -1584,7 +1584,7 @@
     <t xml:space="preserve">Romania - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://gov.ro/ro/media/comunicate/buletin-de-presa-30-august-2020-ora-13-00&amp;page=1</t>
+    <t xml:space="preserve">https://gov.ro/ro/media/comunicate/buletin-de-presa-1-septembrie-2020-ora-13-00&amp;page=1</t>
   </si>
   <si>
     <t xml:space="preserve">Ministry of Internal Affairs</t>
@@ -1607,7 +1607,7 @@
     <t xml:space="preserve">Russia - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://rospotrebnadzor.ru/about/info/news/news_details.php?ELEMENT_ID=15269</t>
+    <t xml:space="preserve">https://rospotrebnadzor.ru/about/info/news/news_details.php?ELEMENT_ID=15284</t>
   </si>
   <si>
     <t xml:space="preserve">Government of the Russian Federation</t>
@@ -1801,7 +1801,7 @@
     <t xml:space="preserve">South Korea - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.cdc.go.kr/board/board.es?mid=&amp;bid=0030&amp;act=view&amp;list_no=368269&amp;tag=&amp;nPage=1</t>
+    <t xml:space="preserve">https://www.cdc.go.kr/board/board.es?mid=&amp;bid=0030&amp;act=view&amp;list_no=368282&amp;tag=&amp;nPage=1</t>
   </si>
   <si>
     <t xml:space="preserve">South Korea CDC</t>
@@ -1821,7 +1821,7 @@
     <t xml:space="preserve">Spain - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.mscbs.gob.es/profesionales/saludPublica/ccayes/alertasActual/nCov-China/documentos/COVID-19_pruebas_diagnosticas_20_08_2020.pdf</t>
+    <t xml:space="preserve">https://www.mscbs.gob.es/profesionales/saludPublica/ccayes/alertasActual/nCov/documentos/COVID-19_pruebas_diagnosticas_27_08_2020.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">Ministry of Health, Consumption and Social Welfare</t>
@@ -1886,18 +1886,21 @@
     <t xml:space="preserve">Switzerland - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://covid-19-schweiz.bagapps.ch/de-3.html</t>
+    <t xml:space="preserve">https://www.bag.admin.ch/dam/bag/en/dokumente/mt/k-und-i/aktuelle-ausbrueche-pandemien/2019-nCoV/covid-19-basisdaten-labortests.xlsx.download.xlsx/Dashboard_3_COVID19_labtests_positivity.xlsx</t>
   </si>
   <si>
     <t xml:space="preserve">Federal Office of Public Health</t>
   </si>
   <si>
+    <t xml:space="preserve">https://www.bag.admin.ch/bag/en/home/krankheiten/ausbrueche-epidemien-pandemien/aktuelle-ausbrueche-epidemien/novel-cov/situation-schweiz-und-international.html</t>
+  </si>
+  <si>
     <t xml:space="preserve">The number of tests perfomed.</t>
   </si>
   <si>
-    <t xml:space="preserve">The Federal Office of Public Health presents a time series of daily positive and negative tests, downloadable as a csv file on [their website](https://www.bag.admin.ch/bag/de/home/krankheiten/ausbrueche-epidemien-pandemien/aktuelle-ausbrueche-epidemien/novel-cov/situation-schweiz-und-international.html). A note states that: "The data published here is based on information that laboratories, doctors and hospitals have given us. They refer to reports that we received this morning and can therefore deviate from the figures that the cantons communicate." (via Google translate).
+    <t xml:space="preserve">The Federal Office of Public Health presents a time series of daily positive and negative tests, downloadable as a Excel spreadsheet on [their website](https://www.bag.admin.ch/bag/en/home/krankheiten/ausbrueche-epidemien-pandemien/aktuelle-ausbrueche-epidemien/novel-cov/situation-schweiz-und-international.html). A note states that: "The data published here is based on information that laboratories, doctors and hospitals have given us. They refer to reports that we received this morning and can therefore deviate from the figures that the cantons communicate."
 At this page they also make available daily situation reports, which present the same figures, making it explicit that the numbers refer to PCR tests. 
-The data can also be accessed by downloading the graphic software file in their [visualization here](https://covid-19-schweiz.bagapps.ch/de-3.html). This graphic notes that "Since several tests can be taken and reported per person, the number of positive tests is higher than the number of positively tested people". (via Google translate).</t>
+The data can also be accessed by downloading the graphic software file in their [visualization here](https://covid-19-schweiz.bagapps.ch/de-3.html). This graphic notes that "Since several tests can be taken and reported per person, the number of positive tests is higher than the number of positively tested people".</t>
   </si>
   <si>
     <t xml:space="preserve">TWN</t>
@@ -1923,7 +1926,7 @@
     <t xml:space="preserve">Thailand - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://ddc.moph.go.th/viralpneumonia/file/situation/situation-no240-300863.pdf</t>
+    <t xml:space="preserve">https://ddc.moph.go.th/viralpneumonia/file/situation/situation-no242-010963.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">Department of Disease Control</t>
@@ -2011,7 +2014,7 @@
     <t xml:space="preserve">Uganda - samples tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/MinofHealthUG/status/1299295338730336256/photo/1</t>
+    <t xml:space="preserve">https://twitter.com/MinofHealthUG/status/1300727966385790976/photo/1</t>
   </si>
   <si>
     <t xml:space="preserve">Uganda Ministry of Health</t>
@@ -2150,7 +2153,7 @@
     <t xml:space="preserve">Uruguay - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.gub.uy/ministerio-salud-publica/comunicacion/noticias/informe-situacion-sobre-coronavirus-covid-19-uruguay-29-agosto</t>
+    <t xml:space="preserve">https://www.gub.uy/ministerio-salud-publica/comunicacion/noticias/informe-situacion-sobre-coronavirus-covid-19-uruguay-1-setiembre</t>
   </si>
   <si>
     <t xml:space="preserve">https://www.gub.uy/ministerio-salud-publica/comunicacion/noticias</t>
@@ -2605,7 +2608,7 @@
         <v>20</v>
       </c>
       <c r="C2" s="1" t="n">
-        <v>44072</v>
+        <v>44074</v>
       </c>
       <c r="D2" t="s">
         <v>21</v>
@@ -2615,31 +2618,31 @@
       </c>
       <c r="F2"/>
       <c r="G2" t="n">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="H2" t="n">
-        <v>1082679</v>
+        <v>1118923</v>
       </c>
       <c r="I2" t="n">
-        <v>23.955</v>
+        <v>24.757</v>
       </c>
       <c r="J2" t="n">
-        <v>11097</v>
+        <v>12883</v>
       </c>
       <c r="K2" t="n">
-        <v>0.246</v>
+        <v>0.285</v>
       </c>
       <c r="L2" t="n">
-        <v>15679</v>
+        <v>16731</v>
       </c>
       <c r="M2" t="n">
-        <v>0.347</v>
+        <v>0.37</v>
       </c>
       <c r="N2" t="n">
-        <v>0.541</v>
+        <v>0.55</v>
       </c>
       <c r="O2" t="n">
-        <v>1.847</v>
+        <v>1.818</v>
       </c>
       <c r="P2" t="s">
         <v>22</v>
@@ -2662,7 +2665,7 @@
         <v>25</v>
       </c>
       <c r="C3" s="1" t="n">
-        <v>44072</v>
+        <v>44074</v>
       </c>
       <c r="D3" t="s">
         <v>26</v>
@@ -2672,31 +2675,31 @@
       </c>
       <c r="F3"/>
       <c r="G3" t="n">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="H3" t="n">
-        <v>1305736</v>
+        <v>1348014</v>
       </c>
       <c r="I3" t="n">
-        <v>28.891</v>
+        <v>29.826</v>
       </c>
       <c r="J3" t="n">
-        <v>12667</v>
+        <v>15147</v>
       </c>
       <c r="K3" t="n">
-        <v>0.28</v>
+        <v>0.335</v>
       </c>
       <c r="L3" t="n">
-        <v>18028</v>
+        <v>19164</v>
       </c>
       <c r="M3" t="n">
-        <v>0.399</v>
+        <v>0.424</v>
       </c>
       <c r="N3" t="n">
-        <v>0.471</v>
+        <v>0.48</v>
       </c>
       <c r="O3" t="n">
-        <v>2.124</v>
+        <v>2.082</v>
       </c>
       <c r="P3" t="s">
         <v>22</v>
@@ -2719,7 +2722,7 @@
         <v>30</v>
       </c>
       <c r="C4" s="1" t="n">
-        <v>44073</v>
+        <v>44075</v>
       </c>
       <c r="D4" t="s">
         <v>31</v>
@@ -2729,27 +2732,31 @@
       </c>
       <c r="F4"/>
       <c r="G4" t="n">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="H4" t="n">
-        <v>6168229</v>
+        <v>6255797</v>
       </c>
       <c r="I4" t="n">
-        <v>241.892</v>
-      </c>
-      <c r="J4"/>
-      <c r="K4"/>
+        <v>245.327</v>
+      </c>
+      <c r="J4" t="n">
+        <v>41344</v>
+      </c>
+      <c r="K4" t="n">
+        <v>1.621</v>
+      </c>
       <c r="L4" t="n">
-        <v>65949</v>
+        <v>63013</v>
       </c>
       <c r="M4" t="n">
-        <v>2.586</v>
+        <v>2.471</v>
       </c>
       <c r="N4" t="n">
         <v>0.002</v>
       </c>
       <c r="O4" t="n">
-        <v>488.511</v>
+        <v>531.435</v>
       </c>
       <c r="P4" t="s">
         <v>32</v>
@@ -2772,7 +2779,7 @@
         <v>36</v>
       </c>
       <c r="C5" s="1" t="n">
-        <v>44074</v>
+        <v>44076</v>
       </c>
       <c r="D5" t="s">
         <v>37</v>
@@ -2782,31 +2789,31 @@
       </c>
       <c r="F5"/>
       <c r="G5" t="n">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="H5" t="n">
-        <v>1180711</v>
+        <v>1210568</v>
       </c>
       <c r="I5" t="n">
-        <v>131.097</v>
+        <v>134.412</v>
       </c>
       <c r="J5" t="n">
-        <v>8619</v>
+        <v>17441</v>
       </c>
       <c r="K5" t="n">
-        <v>0.957</v>
+        <v>1.937</v>
       </c>
       <c r="L5" t="n">
-        <v>11358</v>
+        <v>13053</v>
       </c>
       <c r="M5" t="n">
-        <v>1.261</v>
+        <v>1.449</v>
       </c>
       <c r="N5" t="n">
-        <v>0.025</v>
+        <v>0.021</v>
       </c>
       <c r="O5" t="n">
-        <v>40.175</v>
+        <v>48.014</v>
       </c>
       <c r="P5" t="s">
         <v>39</v>
@@ -2829,7 +2836,7 @@
         <v>43</v>
       </c>
       <c r="C6" s="1" t="n">
-        <v>44073</v>
+        <v>44076</v>
       </c>
       <c r="D6" t="s">
         <v>44</v>
@@ -2839,31 +2846,31 @@
       </c>
       <c r="F6"/>
       <c r="G6" t="n">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="H6" t="n">
-        <v>1100729</v>
+        <v>1118837</v>
       </c>
       <c r="I6" t="n">
-        <v>646.885</v>
+        <v>657.527</v>
       </c>
       <c r="J6" t="n">
-        <v>12311</v>
+        <v>10749</v>
       </c>
       <c r="K6" t="n">
-        <v>7.235</v>
+        <v>6.317</v>
       </c>
       <c r="L6" t="n">
-        <v>10109</v>
+        <v>7276</v>
       </c>
       <c r="M6" t="n">
-        <v>5.941</v>
+        <v>4.276</v>
       </c>
       <c r="N6" t="n">
-        <v>0.033</v>
+        <v>0.037</v>
       </c>
       <c r="O6" t="n">
-        <v>30.074</v>
+        <v>26.863</v>
       </c>
       <c r="P6" t="s">
         <v>46</v>
@@ -2943,7 +2950,7 @@
         <v>57</v>
       </c>
       <c r="C8" s="1" t="n">
-        <v>44070</v>
+        <v>44075</v>
       </c>
       <c r="D8" t="s">
         <v>58</v>
@@ -2953,27 +2960,27 @@
       </c>
       <c r="F8"/>
       <c r="G8" t="n">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="H8" t="n">
-        <v>1497421</v>
+        <v>1534792</v>
       </c>
       <c r="I8" t="n">
-        <v>158.469</v>
+        <v>162.424</v>
       </c>
       <c r="J8"/>
       <c r="K8"/>
       <c r="L8" t="n">
-        <v>6882</v>
+        <v>7821</v>
       </c>
       <c r="M8" t="n">
-        <v>0.728</v>
+        <v>0.828</v>
       </c>
       <c r="N8" t="n">
-        <v>0.024</v>
+        <v>0.022</v>
       </c>
       <c r="O8" t="n">
-        <v>41.069</v>
+        <v>45.699</v>
       </c>
       <c r="P8" t="s">
         <v>59</v>
@@ -2996,7 +3003,7 @@
         <v>63</v>
       </c>
       <c r="C9" s="1" t="n">
-        <v>44072</v>
+        <v>44074</v>
       </c>
       <c r="D9" t="s">
         <v>64</v>
@@ -3006,31 +3013,31 @@
       </c>
       <c r="F9"/>
       <c r="G9" t="n">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="H9" t="n">
-        <v>2278391</v>
+        <v>2281853</v>
       </c>
       <c r="I9" t="n">
-        <v>196.589</v>
+        <v>196.888</v>
       </c>
       <c r="J9" t="n">
-        <v>16482</v>
+        <v>13021</v>
       </c>
       <c r="K9" t="n">
-        <v>1.422</v>
+        <v>1.124</v>
       </c>
       <c r="L9" t="n">
-        <v>19858</v>
+        <v>17337</v>
       </c>
       <c r="M9" t="n">
-        <v>1.713</v>
+        <v>1.496</v>
       </c>
       <c r="N9" t="n">
-        <v>0.021</v>
+        <v>0.025</v>
       </c>
       <c r="O9" t="n">
-        <v>47.233</v>
+        <v>39.855</v>
       </c>
       <c r="P9" t="s">
         <v>65</v>
@@ -3053,7 +3060,7 @@
         <v>69</v>
       </c>
       <c r="C10" s="1" t="n">
-        <v>44071</v>
+        <v>44074</v>
       </c>
       <c r="D10" t="s">
         <v>70</v>
@@ -3063,31 +3070,27 @@
       </c>
       <c r="F10"/>
       <c r="G10" t="n">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="H10" t="n">
-        <v>232975</v>
+        <v>238965</v>
       </c>
       <c r="I10" t="n">
-        <v>19.958</v>
-      </c>
-      <c r="J10" t="n">
-        <v>3632</v>
-      </c>
-      <c r="K10" t="n">
-        <v>0.311</v>
-      </c>
+        <v>20.472</v>
+      </c>
+      <c r="J10"/>
+      <c r="K10"/>
       <c r="L10" t="n">
-        <v>2723</v>
+        <v>2554</v>
       </c>
       <c r="M10" t="n">
-        <v>0.233</v>
+        <v>0.219</v>
       </c>
       <c r="N10" t="n">
-        <v>0.371</v>
+        <v>0.381</v>
       </c>
       <c r="O10" t="n">
-        <v>2.698</v>
+        <v>2.622</v>
       </c>
       <c r="P10" t="s">
         <v>45</v>
@@ -3161,7 +3164,7 @@
         <v>81</v>
       </c>
       <c r="C12" s="1" t="n">
-        <v>44073</v>
+        <v>44076</v>
       </c>
       <c r="D12" t="s">
         <v>82</v>
@@ -3171,31 +3174,31 @@
       </c>
       <c r="F12"/>
       <c r="G12" t="n">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="H12" t="n">
-        <v>404683</v>
+        <v>415797</v>
       </c>
       <c r="I12" t="n">
-        <v>58.241</v>
+        <v>59.84</v>
       </c>
       <c r="J12" t="n">
-        <v>6257</v>
+        <v>6784</v>
       </c>
       <c r="K12" t="n">
-        <v>0.9</v>
+        <v>0.976</v>
       </c>
       <c r="L12" t="n">
-        <v>5169</v>
+        <v>4478</v>
       </c>
       <c r="M12" t="n">
-        <v>0.744</v>
+        <v>0.644</v>
       </c>
       <c r="N12" t="n">
-        <v>0.029</v>
+        <v>0.022</v>
       </c>
       <c r="O12" t="n">
-        <v>35.027</v>
+        <v>46.301</v>
       </c>
       <c r="P12" t="s">
         <v>84</v>
@@ -3218,7 +3221,7 @@
         <v>87</v>
       </c>
       <c r="C13" s="1" t="n">
-        <v>44073</v>
+        <v>44076</v>
       </c>
       <c r="D13" t="s">
         <v>88</v>
@@ -3228,31 +3231,31 @@
       </c>
       <c r="F13"/>
       <c r="G13" t="n">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="H13" t="n">
-        <v>5440371</v>
+        <v>5545473</v>
       </c>
       <c r="I13" t="n">
-        <v>144.146</v>
+        <v>146.93</v>
       </c>
       <c r="J13" t="n">
-        <v>85107</v>
+        <v>41157</v>
       </c>
       <c r="K13" t="n">
-        <v>2.255</v>
+        <v>1.09</v>
       </c>
       <c r="L13" t="n">
-        <v>51948</v>
+        <v>48638</v>
       </c>
       <c r="M13" t="n">
-        <v>1.376</v>
+        <v>1.289</v>
       </c>
       <c r="N13" t="n">
-        <v>0.008</v>
+        <v>0.01</v>
       </c>
       <c r="O13" t="n">
-        <v>119.46</v>
+        <v>98.514</v>
       </c>
       <c r="P13" t="s">
         <v>89</v>
@@ -3275,7 +3278,7 @@
         <v>92</v>
       </c>
       <c r="C14" s="1" t="n">
-        <v>44073</v>
+        <v>44075</v>
       </c>
       <c r="D14" t="s">
         <v>93</v>
@@ -3287,31 +3290,31 @@
         <v>94</v>
       </c>
       <c r="G14" t="n">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="H14" t="n">
-        <v>2400522</v>
+        <v>2458762</v>
       </c>
       <c r="I14" t="n">
-        <v>125.575</v>
+        <v>128.622</v>
       </c>
       <c r="J14" t="n">
-        <v>34769</v>
+        <v>26326</v>
       </c>
       <c r="K14" t="n">
-        <v>1.819</v>
+        <v>1.377</v>
       </c>
       <c r="L14" t="n">
-        <v>28073</v>
+        <v>28971</v>
       </c>
       <c r="M14" t="n">
-        <v>1.469</v>
+        <v>1.516</v>
       </c>
       <c r="N14" t="n">
-        <v>0.063</v>
+        <v>0.06</v>
       </c>
       <c r="O14" t="n">
-        <v>15.975</v>
+        <v>16.68</v>
       </c>
       <c r="P14" t="s">
         <v>95</v>
@@ -3334,7 +3337,7 @@
         <v>99</v>
       </c>
       <c r="C15" s="1" t="n">
-        <v>44073</v>
+        <v>44075</v>
       </c>
       <c r="D15" t="s">
         <v>100</v>
@@ -3344,31 +3347,31 @@
       </c>
       <c r="F15"/>
       <c r="G15" t="n">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="H15" t="n">
-        <v>2599703</v>
+        <v>2647702</v>
       </c>
       <c r="I15" t="n">
-        <v>51.092</v>
+        <v>52.035</v>
       </c>
       <c r="J15" t="n">
-        <v>26879</v>
+        <v>22650</v>
       </c>
       <c r="K15" t="n">
-        <v>0.528</v>
+        <v>0.445</v>
       </c>
       <c r="L15" t="n">
-        <v>28973</v>
+        <v>26977</v>
       </c>
       <c r="M15" t="n">
-        <v>0.569</v>
+        <v>0.53</v>
       </c>
       <c r="N15" t="n">
-        <v>0.329</v>
+        <v>0.336</v>
       </c>
       <c r="O15" t="n">
-        <v>3.036</v>
+        <v>2.975</v>
       </c>
       <c r="P15" t="s">
         <v>101</v>
@@ -3391,7 +3394,7 @@
         <v>105</v>
       </c>
       <c r="C16" s="1" t="n">
-        <v>44071</v>
+        <v>44074</v>
       </c>
       <c r="D16" t="s">
         <v>106</v>
@@ -3401,25 +3404,25 @@
       </c>
       <c r="F16"/>
       <c r="G16" t="n">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="H16" t="n">
-        <v>125419</v>
+        <v>131623</v>
       </c>
       <c r="I16" t="n">
-        <v>24.62</v>
+        <v>25.838</v>
       </c>
       <c r="J16" t="n">
-        <v>2211</v>
+        <v>2767</v>
       </c>
       <c r="K16" t="n">
-        <v>0.434</v>
+        <v>0.543</v>
       </c>
       <c r="L16" t="n">
-        <v>1883</v>
+        <v>1947</v>
       </c>
       <c r="M16" t="n">
-        <v>0.37</v>
+        <v>0.382</v>
       </c>
       <c r="N16"/>
       <c r="O16"/>
@@ -3444,7 +3447,7 @@
         <v>111</v>
       </c>
       <c r="C17" s="1" t="n">
-        <v>44072</v>
+        <v>44074</v>
       </c>
       <c r="D17" t="s">
         <v>112</v>
@@ -3454,31 +3457,31 @@
       </c>
       <c r="F17"/>
       <c r="G17" t="n">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="H17" t="n">
-        <v>125972</v>
+        <v>127804</v>
       </c>
       <c r="I17" t="n">
-        <v>4.776</v>
+        <v>4.845</v>
       </c>
       <c r="J17" t="n">
-        <v>887</v>
+        <v>1252</v>
       </c>
       <c r="K17" t="n">
-        <v>0.034</v>
+        <v>0.047</v>
       </c>
       <c r="L17" t="n">
-        <v>972</v>
+        <v>931</v>
       </c>
       <c r="M17" t="n">
-        <v>0.037</v>
+        <v>0.035</v>
       </c>
       <c r="N17" t="n">
-        <v>0.072</v>
+        <v>0.073</v>
       </c>
       <c r="O17" t="n">
-        <v>13.971</v>
+        <v>13.662</v>
       </c>
       <c r="P17" t="s">
         <v>113</v>
@@ -3501,7 +3504,7 @@
         <v>117</v>
       </c>
       <c r="C18" s="1" t="n">
-        <v>44074</v>
+        <v>44076</v>
       </c>
       <c r="D18" t="s">
         <v>118</v>
@@ -3511,31 +3514,31 @@
       </c>
       <c r="F18"/>
       <c r="G18" t="n">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="H18" t="n">
-        <v>168229</v>
+        <v>175346</v>
       </c>
       <c r="I18" t="n">
-        <v>40.979</v>
+        <v>42.712</v>
       </c>
       <c r="J18" t="n">
-        <v>1591</v>
+        <v>4122</v>
       </c>
       <c r="K18" t="n">
-        <v>0.388</v>
+        <v>1.004</v>
       </c>
       <c r="L18" t="n">
-        <v>2201</v>
+        <v>2566</v>
       </c>
       <c r="M18" t="n">
-        <v>0.536</v>
+        <v>0.625</v>
       </c>
       <c r="N18" t="n">
-        <v>0.126</v>
+        <v>0.105</v>
       </c>
       <c r="O18" t="n">
-        <v>7.909</v>
+        <v>9.534</v>
       </c>
       <c r="P18" t="s">
         <v>119</v>
@@ -3558,7 +3561,7 @@
         <v>123</v>
       </c>
       <c r="C19" s="1" t="n">
-        <v>44072</v>
+        <v>44074</v>
       </c>
       <c r="D19" t="s">
         <v>124</v>
@@ -3570,31 +3573,31 @@
         <v>126</v>
       </c>
       <c r="G19" t="n">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="H19" t="n">
-        <v>392785</v>
+        <v>403181</v>
       </c>
       <c r="I19" t="n">
-        <v>34.678</v>
+        <v>35.596</v>
       </c>
       <c r="J19" t="n">
-        <v>4591</v>
+        <v>4958</v>
       </c>
       <c r="K19" t="n">
-        <v>0.405</v>
+        <v>0.438</v>
       </c>
       <c r="L19" t="n">
-        <v>4528</v>
+        <v>4756</v>
       </c>
       <c r="M19" t="n">
-        <v>0.4</v>
+        <v>0.42</v>
       </c>
       <c r="N19" t="n">
         <v>0.009</v>
       </c>
       <c r="O19" t="n">
-        <v>111.606</v>
+        <v>114.405</v>
       </c>
       <c r="P19" t="s">
         <v>125</v>
@@ -3617,7 +3620,7 @@
         <v>130</v>
       </c>
       <c r="C20" s="1" t="n">
-        <v>44072</v>
+        <v>44074</v>
       </c>
       <c r="D20" t="s">
         <v>131</v>
@@ -3627,31 +3630,31 @@
       </c>
       <c r="F20"/>
       <c r="G20" t="n">
-        <v>210</v>
+        <v>212</v>
       </c>
       <c r="H20" t="n">
-        <v>896813</v>
+        <v>910872</v>
       </c>
       <c r="I20" t="n">
-        <v>83.744</v>
+        <v>85.057</v>
       </c>
       <c r="J20" t="n">
-        <v>5491</v>
+        <v>7876</v>
       </c>
       <c r="K20" t="n">
-        <v>0.513</v>
+        <v>0.735</v>
       </c>
       <c r="L20" t="n">
-        <v>7459</v>
+        <v>7984</v>
       </c>
       <c r="M20" t="n">
-        <v>0.697</v>
+        <v>0.746</v>
       </c>
       <c r="N20" t="n">
-        <v>0.043</v>
+        <v>0.044</v>
       </c>
       <c r="O20" t="n">
-        <v>23.456</v>
+        <v>22.867</v>
       </c>
       <c r="P20" t="s">
         <v>45</v>
@@ -3674,7 +3677,7 @@
         <v>135</v>
       </c>
       <c r="C21" s="1" t="n">
-        <v>44071</v>
+        <v>44073</v>
       </c>
       <c r="D21" t="s">
         <v>136</v>
@@ -3684,27 +3687,27 @@
       </c>
       <c r="F21"/>
       <c r="G21" t="n">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="H21"/>
       <c r="I21"/>
       <c r="J21" t="n">
-        <v>151</v>
+        <v>327</v>
       </c>
       <c r="K21" t="n">
-        <v>0.002</v>
+        <v>0.004</v>
       </c>
       <c r="L21" t="n">
-        <v>225</v>
+        <v>237</v>
       </c>
       <c r="M21" t="n">
         <v>0.003</v>
       </c>
       <c r="N21" t="n">
-        <v>0.1</v>
+        <v>0.119</v>
       </c>
       <c r="O21" t="n">
-        <v>9.968</v>
+        <v>8.421</v>
       </c>
       <c r="P21" t="s">
         <v>137</v>
@@ -3727,7 +3730,7 @@
         <v>141</v>
       </c>
       <c r="C22" s="1" t="n">
-        <v>44073</v>
+        <v>44074</v>
       </c>
       <c r="D22" t="s">
         <v>142</v>
@@ -3737,31 +3740,31 @@
       </c>
       <c r="F22"/>
       <c r="G22" t="n">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="H22" t="n">
-        <v>2417508</v>
+        <v>2447911</v>
       </c>
       <c r="I22" t="n">
-        <v>417.373</v>
+        <v>422.622</v>
       </c>
       <c r="J22" t="n">
-        <v>4918</v>
+        <v>8562</v>
       </c>
       <c r="K22" t="n">
-        <v>0.849</v>
+        <v>1.478</v>
       </c>
       <c r="L22" t="n">
-        <v>31184</v>
+        <v>29908</v>
       </c>
       <c r="M22" t="n">
-        <v>5.384</v>
+        <v>5.163</v>
       </c>
       <c r="N22" t="n">
         <v>0.003</v>
       </c>
       <c r="O22" t="n">
-        <v>380.956</v>
+        <v>365.368</v>
       </c>
       <c r="P22" t="s">
         <v>143</v>
@@ -3784,7 +3787,7 @@
         <v>147</v>
       </c>
       <c r="C23" s="1" t="n">
-        <v>44072</v>
+        <v>44073</v>
       </c>
       <c r="D23" t="s">
         <v>148</v>
@@ -3796,25 +3799,25 @@
         <v>150</v>
       </c>
       <c r="G23" t="n">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="H23" t="n">
-        <v>256212</v>
+        <v>258266</v>
       </c>
       <c r="I23" t="n">
-        <v>14.522</v>
+        <v>14.638</v>
       </c>
       <c r="J23" t="n">
-        <v>2236</v>
+        <v>2054</v>
       </c>
       <c r="K23" t="n">
-        <v>0.127</v>
+        <v>0.116</v>
       </c>
       <c r="L23" t="n">
-        <v>2349</v>
+        <v>2307</v>
       </c>
       <c r="M23" t="n">
-        <v>0.133</v>
+        <v>0.131</v>
       </c>
       <c r="N23"/>
       <c r="O23"/>
@@ -3896,7 +3899,7 @@
         <v>160</v>
       </c>
       <c r="C25" s="1" t="n">
-        <v>44072</v>
+        <v>44075</v>
       </c>
       <c r="D25" t="s">
         <v>161</v>
@@ -3906,31 +3909,31 @@
       </c>
       <c r="F25"/>
       <c r="G25" t="n">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="H25" t="n">
-        <v>147901</v>
+        <v>151940</v>
       </c>
       <c r="I25" t="n">
-        <v>111.494</v>
+        <v>114.539</v>
       </c>
       <c r="J25" t="n">
-        <v>666</v>
+        <v>1595</v>
       </c>
       <c r="K25" t="n">
-        <v>0.502</v>
+        <v>1.202</v>
       </c>
       <c r="L25" t="n">
-        <v>1035</v>
+        <v>1208</v>
       </c>
       <c r="M25" t="n">
-        <v>0.78</v>
+        <v>0.911</v>
       </c>
       <c r="N25" t="n">
-        <v>0.014</v>
+        <v>0.012</v>
       </c>
       <c r="O25" t="n">
-        <v>73.182</v>
+        <v>84.56</v>
       </c>
       <c r="P25" t="s">
         <v>163</v>
@@ -4010,7 +4013,7 @@
         <v>174</v>
       </c>
       <c r="C27" s="1" t="n">
-        <v>44066</v>
+        <v>44074</v>
       </c>
       <c r="D27" t="s">
         <v>175</v>
@@ -4020,32 +4023,30 @@
       </c>
       <c r="F27"/>
       <c r="G27" t="n">
-        <v>157</v>
+        <v>165</v>
       </c>
       <c r="H27" t="n">
-        <v>7979</v>
+        <v>8408</v>
       </c>
       <c r="I27" t="n">
-        <v>8.901</v>
+        <v>9.379</v>
       </c>
       <c r="J27" t="n">
-        <v>18</v>
+        <v>43</v>
       </c>
       <c r="K27" t="n">
-        <v>0.02</v>
+        <v>0.048</v>
       </c>
       <c r="L27" t="n">
-        <v>51</v>
+        <v>60</v>
       </c>
       <c r="M27" t="n">
-        <v>0.057</v>
+        <v>0.067</v>
       </c>
       <c r="N27" t="n">
-        <v>0.003</v>
-      </c>
-      <c r="O27" t="n">
-        <v>357</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="O27"/>
       <c r="P27" t="s">
         <v>176</v>
       </c>
@@ -4067,7 +4068,7 @@
         <v>179</v>
       </c>
       <c r="C28" s="1" t="n">
-        <v>44072</v>
+        <v>44075</v>
       </c>
       <c r="D28" t="s">
         <v>180</v>
@@ -4077,31 +4078,31 @@
       </c>
       <c r="F28"/>
       <c r="G28" t="n">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="H28" t="n">
-        <v>639098</v>
+        <v>688714</v>
       </c>
       <c r="I28" t="n">
-        <v>115.346</v>
+        <v>124.3</v>
       </c>
       <c r="J28" t="n">
-        <v>1280</v>
+        <v>885</v>
       </c>
       <c r="K28" t="n">
-        <v>0.231</v>
+        <v>0.16</v>
       </c>
       <c r="L28" t="n">
-        <v>9362</v>
+        <v>11035</v>
       </c>
       <c r="M28" t="n">
-        <v>1.69</v>
+        <v>1.992</v>
       </c>
       <c r="N28" t="n">
-        <v>0.003</v>
+        <v>0.002</v>
       </c>
       <c r="O28" t="n">
-        <v>383.24</v>
+        <v>521.926</v>
       </c>
       <c r="P28" t="s">
         <v>182</v>
@@ -4124,7 +4125,7 @@
         <v>185</v>
       </c>
       <c r="C29" s="1" t="n">
-        <v>44070</v>
+        <v>44071</v>
       </c>
       <c r="D29" t="s">
         <v>186</v>
@@ -4134,27 +4135,27 @@
       </c>
       <c r="F29"/>
       <c r="G29" t="n">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="H29"/>
       <c r="I29"/>
       <c r="J29" t="n">
-        <v>135212</v>
+        <v>145507</v>
       </c>
       <c r="K29" t="n">
-        <v>2.071</v>
+        <v>2.229</v>
       </c>
       <c r="L29" t="n">
-        <v>114778</v>
+        <v>119064</v>
       </c>
       <c r="M29" t="n">
-        <v>1.758</v>
+        <v>1.824</v>
       </c>
       <c r="N29" t="n">
         <v>0.036</v>
       </c>
       <c r="O29" t="n">
-        <v>28.148</v>
+        <v>27.889</v>
       </c>
       <c r="P29" t="s">
         <v>187</v>
@@ -4344,7 +4345,7 @@
         <v>210</v>
       </c>
       <c r="C33" s="1" t="n">
-        <v>44073</v>
+        <v>44075</v>
       </c>
       <c r="D33" t="s">
         <v>211</v>
@@ -4354,31 +4355,31 @@
       </c>
       <c r="F33"/>
       <c r="G33" t="n">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="H33" t="n">
-        <v>940882</v>
+        <v>966346</v>
       </c>
       <c r="I33" t="n">
-        <v>90.269</v>
+        <v>92.712</v>
       </c>
       <c r="J33" t="n">
-        <v>9880</v>
+        <v>16979</v>
       </c>
       <c r="K33" t="n">
-        <v>0.948</v>
+        <v>1.629</v>
       </c>
       <c r="L33" t="n">
-        <v>13215</v>
+        <v>13399</v>
       </c>
       <c r="M33" t="n">
-        <v>1.268</v>
+        <v>1.286</v>
       </c>
       <c r="N33" t="n">
-        <v>0.017</v>
+        <v>0.016</v>
       </c>
       <c r="O33" t="n">
-        <v>57.961</v>
+        <v>62.612</v>
       </c>
       <c r="P33" t="s">
         <v>213</v>
@@ -4450,7 +4451,7 @@
         <v>224</v>
       </c>
       <c r="C35" s="1" t="n">
-        <v>44074</v>
+        <v>44076</v>
       </c>
       <c r="D35" t="s">
         <v>225</v>
@@ -4462,31 +4463,31 @@
         <v>227</v>
       </c>
       <c r="G35" t="n">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="H35" t="n">
-        <v>428150</v>
+        <v>437531</v>
       </c>
       <c r="I35" t="n">
-        <v>44.32</v>
+        <v>45.291</v>
       </c>
       <c r="J35" t="n">
-        <v>3880</v>
+        <v>7589</v>
       </c>
       <c r="K35" t="n">
-        <v>0.402</v>
+        <v>0.786</v>
       </c>
       <c r="L35" t="n">
-        <v>4229</v>
+        <v>4638</v>
       </c>
       <c r="M35" t="n">
-        <v>0.438</v>
+        <v>0.48</v>
       </c>
       <c r="N35" t="n">
-        <v>0.027</v>
+        <v>0.032</v>
       </c>
       <c r="O35" t="n">
-        <v>36.728</v>
+        <v>31.157</v>
       </c>
       <c r="P35" t="s">
         <v>226</v>
@@ -4625,7 +4626,7 @@
         <v>242</v>
       </c>
       <c r="C38" s="1" t="n">
-        <v>44073</v>
+        <v>44075</v>
       </c>
       <c r="D38" t="s">
         <v>238</v>
@@ -4637,31 +4638,31 @@
         <v>240</v>
       </c>
       <c r="G38" t="n">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="H38" t="n">
-        <v>42307914</v>
+        <v>44337201</v>
       </c>
       <c r="I38" t="n">
-        <v>30.658</v>
+        <v>32.128</v>
       </c>
       <c r="J38" t="n">
-        <v>846278</v>
+        <v>1012367</v>
       </c>
       <c r="K38" t="n">
-        <v>0.613</v>
+        <v>0.734</v>
       </c>
       <c r="L38" t="n">
-        <v>892578</v>
+        <v>955098</v>
       </c>
       <c r="M38" t="n">
-        <v>0.647</v>
+        <v>0.692</v>
       </c>
       <c r="N38" t="n">
-        <v>0.08</v>
+        <v>0.078</v>
       </c>
       <c r="O38" t="n">
-        <v>12.551</v>
+        <v>12.763</v>
       </c>
       <c r="P38" t="s">
         <v>239</v>
@@ -4684,7 +4685,7 @@
         <v>244</v>
       </c>
       <c r="C39" s="1" t="n">
-        <v>44074</v>
+        <v>44076</v>
       </c>
       <c r="D39" t="s">
         <v>245</v>
@@ -4694,31 +4695,31 @@
       </c>
       <c r="F39"/>
       <c r="G39" t="n">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="H39" t="n">
-        <v>1282618</v>
+        <v>1312477</v>
       </c>
       <c r="I39" t="n">
-        <v>4.689</v>
+        <v>4.798</v>
       </c>
       <c r="J39" t="n">
-        <v>11317</v>
+        <v>15293</v>
       </c>
       <c r="K39" t="n">
-        <v>0.041</v>
+        <v>0.056</v>
       </c>
       <c r="L39" t="n">
-        <v>15230</v>
+        <v>15753</v>
       </c>
       <c r="M39" t="n">
-        <v>0.056</v>
+        <v>0.058</v>
       </c>
       <c r="N39" t="n">
-        <v>0.174</v>
+        <v>0.179</v>
       </c>
       <c r="O39" t="n">
-        <v>5.757</v>
+        <v>5.594</v>
       </c>
       <c r="P39" t="s">
         <v>246</v>
@@ -4741,7 +4742,7 @@
         <v>250</v>
       </c>
       <c r="C40" s="1" t="n">
-        <v>44074</v>
+        <v>44075</v>
       </c>
       <c r="D40" t="s">
         <v>251</v>
@@ -4751,31 +4752,31 @@
       </c>
       <c r="F40"/>
       <c r="G40" t="n">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="H40" t="n">
-        <v>3231110</v>
+        <v>3256122</v>
       </c>
       <c r="I40" t="n">
-        <v>38.469</v>
+        <v>38.767</v>
       </c>
       <c r="J40" t="n">
-        <v>23841</v>
+        <v>25012</v>
       </c>
       <c r="K40" t="n">
-        <v>0.284</v>
+        <v>0.298</v>
       </c>
       <c r="L40" t="n">
-        <v>24098</v>
+        <v>23973</v>
       </c>
       <c r="M40" t="n">
-        <v>0.287</v>
+        <v>0.285</v>
       </c>
       <c r="N40" t="n">
-        <v>0.087</v>
+        <v>0.097</v>
       </c>
       <c r="O40" t="n">
-        <v>11.503</v>
+        <v>10.291</v>
       </c>
       <c r="P40" t="s">
         <v>252</v>
@@ -4798,7 +4799,7 @@
         <v>256</v>
       </c>
       <c r="C41" s="1" t="n">
-        <v>44069</v>
+        <v>44075</v>
       </c>
       <c r="D41" t="s">
         <v>257</v>
@@ -4808,31 +4809,31 @@
       </c>
       <c r="F41"/>
       <c r="G41" t="n">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="H41" t="n">
-        <v>1502546</v>
+        <v>1624331</v>
       </c>
       <c r="I41" t="n">
-        <v>37.356</v>
+        <v>40.384</v>
       </c>
       <c r="J41" t="n">
-        <v>20359</v>
+        <v>18427</v>
       </c>
       <c r="K41" t="n">
-        <v>0.506</v>
+        <v>0.458</v>
       </c>
       <c r="L41" t="n">
-        <v>22441</v>
+        <v>20306</v>
       </c>
       <c r="M41" t="n">
-        <v>0.558</v>
+        <v>0.505</v>
       </c>
       <c r="N41" t="n">
-        <v>0.173</v>
+        <v>0.19</v>
       </c>
       <c r="O41" t="n">
-        <v>5.767</v>
+        <v>5.274</v>
       </c>
       <c r="P41" t="s">
         <v>259</v>
@@ -4855,7 +4856,7 @@
         <v>263</v>
       </c>
       <c r="C42" s="1" t="n">
-        <v>44072</v>
+        <v>44075</v>
       </c>
       <c r="D42" t="s">
         <v>264</v>
@@ -4865,31 +4866,31 @@
       </c>
       <c r="F42"/>
       <c r="G42" t="n">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="H42" t="n">
-        <v>824712</v>
+        <v>844706</v>
       </c>
       <c r="I42" t="n">
-        <v>167.02</v>
+        <v>171.069</v>
       </c>
       <c r="J42" t="n">
-        <v>9837</v>
+        <v>4892</v>
       </c>
       <c r="K42" t="n">
-        <v>1.992</v>
+        <v>0.991</v>
       </c>
       <c r="L42" t="n">
-        <v>8193</v>
+        <v>8865</v>
       </c>
       <c r="M42" t="n">
-        <v>1.659</v>
+        <v>1.795</v>
       </c>
       <c r="N42" t="n">
-        <v>0.014</v>
+        <v>0.011</v>
       </c>
       <c r="O42" t="n">
-        <v>69.601</v>
+        <v>89.288</v>
       </c>
       <c r="P42" t="s">
         <v>265</v>
@@ -4912,7 +4913,7 @@
         <v>268</v>
       </c>
       <c r="C43" s="1" t="n">
-        <v>44067</v>
+        <v>44069</v>
       </c>
       <c r="D43" t="s">
         <v>269</v>
@@ -4922,31 +4923,31 @@
       </c>
       <c r="F43"/>
       <c r="G43" t="n">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="H43" t="n">
-        <v>2285649</v>
+        <v>2353984</v>
       </c>
       <c r="I43" t="n">
-        <v>264.068</v>
+        <v>271.963</v>
       </c>
       <c r="J43" t="n">
-        <v>30119</v>
+        <v>34286</v>
       </c>
       <c r="K43" t="n">
-        <v>3.48</v>
+        <v>3.961</v>
       </c>
       <c r="L43" t="n">
-        <v>23844</v>
+        <v>25560</v>
       </c>
       <c r="M43" t="n">
-        <v>2.755</v>
+        <v>2.953</v>
       </c>
       <c r="N43" t="n">
-        <v>0.063</v>
+        <v>0.06</v>
       </c>
       <c r="O43" t="n">
-        <v>15.94</v>
+        <v>16.77</v>
       </c>
       <c r="P43" t="s">
         <v>45</v>
@@ -4969,7 +4970,7 @@
         <v>274</v>
       </c>
       <c r="C44" s="1" t="n">
-        <v>44073</v>
+        <v>44075</v>
       </c>
       <c r="D44" t="s">
         <v>275</v>
@@ -4981,31 +4982,31 @@
         <v>277</v>
       </c>
       <c r="G44" t="n">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="H44" t="n">
-        <v>5117788</v>
+        <v>5214766</v>
       </c>
       <c r="I44" t="n">
-        <v>84.645</v>
+        <v>86.249</v>
       </c>
       <c r="J44" t="n">
-        <v>53541</v>
+        <v>54395</v>
       </c>
       <c r="K44" t="n">
-        <v>0.886</v>
+        <v>0.9</v>
       </c>
       <c r="L44" t="n">
-        <v>53974</v>
+        <v>56520</v>
       </c>
       <c r="M44" t="n">
-        <v>0.893</v>
+        <v>0.935</v>
       </c>
       <c r="N44" t="n">
         <v>0.023</v>
       </c>
       <c r="O44" t="n">
-        <v>43.343</v>
+        <v>44.374</v>
       </c>
       <c r="P44" t="s">
         <v>278</v>
@@ -5028,7 +5029,7 @@
         <v>281</v>
       </c>
       <c r="C45" s="1" t="n">
-        <v>44073</v>
+        <v>44075</v>
       </c>
       <c r="D45" t="s">
         <v>275</v>
@@ -5040,31 +5041,31 @@
         <v>277</v>
       </c>
       <c r="G45" t="n">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="H45" t="n">
-        <v>8591341</v>
+        <v>8725909</v>
       </c>
       <c r="I45" t="n">
-        <v>142.095</v>
+        <v>144.321</v>
       </c>
       <c r="J45" t="n">
-        <v>81723</v>
+        <v>81050</v>
       </c>
       <c r="K45" t="n">
-        <v>1.352</v>
+        <v>1.341</v>
       </c>
       <c r="L45" t="n">
-        <v>83386</v>
+        <v>85717</v>
       </c>
       <c r="M45" t="n">
-        <v>1.379</v>
+        <v>1.418</v>
       </c>
       <c r="N45" t="n">
         <v>0.015</v>
       </c>
       <c r="O45" t="n">
-        <v>66.961</v>
+        <v>67.297</v>
       </c>
       <c r="P45" t="s">
         <v>278</v>
@@ -5087,7 +5088,7 @@
         <v>284</v>
       </c>
       <c r="C46" s="1" t="n">
-        <v>44073</v>
+        <v>44075</v>
       </c>
       <c r="D46" t="s">
         <v>285</v>
@@ -5099,31 +5100,31 @@
         <v>287</v>
       </c>
       <c r="G46" t="n">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="H46" t="n">
-        <v>1455610</v>
+        <v>1490975</v>
       </c>
       <c r="I46" t="n">
-        <v>11.509</v>
+        <v>11.789</v>
       </c>
       <c r="J46" t="n">
-        <v>14784</v>
+        <v>23843</v>
       </c>
       <c r="K46" t="n">
-        <v>0.117</v>
+        <v>0.189</v>
       </c>
       <c r="L46" t="n">
-        <v>19219</v>
+        <v>19050</v>
       </c>
       <c r="M46" t="n">
-        <v>0.152</v>
+        <v>0.151</v>
       </c>
       <c r="N46" t="n">
-        <v>0.041</v>
+        <v>0.04</v>
       </c>
       <c r="O46" t="n">
-        <v>24.385</v>
+        <v>25.299</v>
       </c>
       <c r="P46" t="s">
         <v>288</v>
@@ -5146,7 +5147,7 @@
         <v>291</v>
       </c>
       <c r="C47" s="1" t="n">
-        <v>44070</v>
+        <v>44073</v>
       </c>
       <c r="D47" t="s">
         <v>292</v>
@@ -5158,31 +5159,31 @@
         <v>293</v>
       </c>
       <c r="G47" t="n">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="H47" t="n">
-        <v>1770064</v>
+        <v>1816394</v>
       </c>
       <c r="I47" t="n">
-        <v>13.995</v>
+        <v>14.362</v>
       </c>
       <c r="J47" t="n">
-        <v>26201</v>
+        <v>8005</v>
       </c>
       <c r="K47" t="n">
-        <v>0.207</v>
+        <v>0.063</v>
       </c>
       <c r="L47" t="n">
-        <v>21805</v>
+        <v>19871</v>
       </c>
       <c r="M47" t="n">
-        <v>0.172</v>
+        <v>0.157</v>
       </c>
       <c r="N47" t="n">
         <v>0.04</v>
       </c>
       <c r="O47" t="n">
-        <v>24.75</v>
+        <v>25.212</v>
       </c>
       <c r="P47" t="s">
         <v>288</v>
@@ -5319,7 +5320,7 @@
         <v>307</v>
       </c>
       <c r="C50" s="1" t="n">
-        <v>44072</v>
+        <v>44075</v>
       </c>
       <c r="D50" t="s">
         <v>308</v>
@@ -5329,31 +5330,31 @@
       </c>
       <c r="F50"/>
       <c r="G50" t="n">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="H50" t="n">
-        <v>611639</v>
+        <v>621616</v>
       </c>
       <c r="I50" t="n">
-        <v>143.222</v>
+        <v>145.558</v>
       </c>
       <c r="J50" t="n">
-        <v>3718</v>
+        <v>3997</v>
       </c>
       <c r="K50" t="n">
-        <v>0.871</v>
+        <v>0.936</v>
       </c>
       <c r="L50" t="n">
-        <v>3788</v>
+        <v>3795</v>
       </c>
       <c r="M50" t="n">
-        <v>0.887</v>
+        <v>0.889</v>
       </c>
       <c r="N50" t="n">
-        <v>0.163</v>
+        <v>0.156</v>
       </c>
       <c r="O50" t="n">
-        <v>6.154</v>
+        <v>6.403</v>
       </c>
       <c r="P50" t="s">
         <v>309</v>
@@ -5376,7 +5377,7 @@
         <v>313</v>
       </c>
       <c r="C51" s="1" t="n">
-        <v>44074</v>
+        <v>44076</v>
       </c>
       <c r="D51" t="s">
         <v>314</v>
@@ -5388,31 +5389,31 @@
         <v>316</v>
       </c>
       <c r="G51" t="n">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="H51" t="n">
-        <v>251717</v>
+        <v>256350</v>
       </c>
       <c r="I51" t="n">
-        <v>133.452</v>
+        <v>135.908</v>
       </c>
       <c r="J51" t="n">
-        <v>1008</v>
+        <v>2532</v>
       </c>
       <c r="K51" t="n">
-        <v>0.534</v>
+        <v>1.342</v>
       </c>
       <c r="L51" t="n">
-        <v>1902</v>
+        <v>1932</v>
       </c>
       <c r="M51" t="n">
-        <v>1.008</v>
+        <v>1.024</v>
       </c>
       <c r="N51" t="n">
-        <v>0.004</v>
+        <v>0.005</v>
       </c>
       <c r="O51" t="n">
-        <v>237.75</v>
+        <v>218.129</v>
       </c>
       <c r="P51" t="s">
         <v>315</v>
@@ -5435,7 +5436,7 @@
         <v>319</v>
       </c>
       <c r="C52" s="1" t="n">
-        <v>44074</v>
+        <v>44076</v>
       </c>
       <c r="D52" t="s">
         <v>320</v>
@@ -5445,27 +5446,31 @@
       </c>
       <c r="F52"/>
       <c r="G52" t="n">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="H52" t="n">
-        <v>639044</v>
+        <v>648863</v>
       </c>
       <c r="I52" t="n">
-        <v>234.745</v>
-      </c>
-      <c r="J52"/>
-      <c r="K52"/>
+        <v>238.352</v>
+      </c>
+      <c r="J52" t="n">
+        <v>5159</v>
+      </c>
+      <c r="K52" t="n">
+        <v>1.895</v>
+      </c>
       <c r="L52" t="n">
-        <v>4325</v>
+        <v>4351</v>
       </c>
       <c r="M52" t="n">
-        <v>1.589</v>
+        <v>1.598</v>
       </c>
       <c r="N52" t="n">
         <v>0.008</v>
       </c>
       <c r="O52" t="n">
-        <v>126.674</v>
+        <v>129.604</v>
       </c>
       <c r="P52" t="s">
         <v>45</v>
@@ -5488,7 +5493,7 @@
         <v>323</v>
       </c>
       <c r="C53" s="1" t="n">
-        <v>44070</v>
+        <v>44074</v>
       </c>
       <c r="D53" t="s">
         <v>324</v>
@@ -5498,32 +5503,28 @@
       </c>
       <c r="F53"/>
       <c r="G53" t="n">
-        <v>183</v>
+        <v>187</v>
       </c>
       <c r="H53" t="n">
-        <v>381256</v>
+        <v>385820</v>
       </c>
       <c r="I53" t="n">
-        <v>609.058</v>
+        <v>616.35</v>
       </c>
       <c r="J53" t="n">
-        <v>1748</v>
+        <v>1271</v>
       </c>
       <c r="K53" t="n">
-        <v>2.792</v>
+        <v>2.03</v>
       </c>
       <c r="L53" t="n">
-        <v>1194</v>
+        <v>1298</v>
       </c>
       <c r="M53" t="n">
-        <v>1.907</v>
-      </c>
-      <c r="N53" t="n">
-        <v>0.043</v>
-      </c>
-      <c r="O53" t="n">
-        <v>23.088</v>
-      </c>
+        <v>2.074</v>
+      </c>
+      <c r="N53"/>
+      <c r="O53"/>
       <c r="P53" t="s">
         <v>325</v>
       </c>
@@ -5545,7 +5546,7 @@
         <v>328</v>
       </c>
       <c r="C54" s="1" t="n">
-        <v>44073</v>
+        <v>44075</v>
       </c>
       <c r="D54" t="s">
         <v>329</v>
@@ -5557,31 +5558,31 @@
         <v>331</v>
       </c>
       <c r="G54" t="n">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="H54" t="n">
-        <v>1243540</v>
+        <v>1262848</v>
       </c>
       <c r="I54" t="n">
-        <v>38.421</v>
+        <v>39.018</v>
       </c>
       <c r="J54" t="n">
-        <v>10613</v>
+        <v>8993</v>
       </c>
       <c r="K54" t="n">
-        <v>0.328</v>
+        <v>0.278</v>
       </c>
       <c r="L54" t="n">
-        <v>9589</v>
+        <v>10193</v>
       </c>
       <c r="M54" t="n">
-        <v>0.296</v>
+        <v>0.315</v>
       </c>
       <c r="N54" t="n">
         <v>0.001</v>
       </c>
       <c r="O54" t="n">
-        <v>1118.717</v>
+        <v>1081.076</v>
       </c>
       <c r="P54" t="s">
         <v>45</v>
@@ -5604,7 +5605,7 @@
         <v>335</v>
       </c>
       <c r="C55" s="1" t="n">
-        <v>44072</v>
+        <v>44075</v>
       </c>
       <c r="D55" t="s">
         <v>336</v>
@@ -5614,31 +5615,31 @@
       </c>
       <c r="F55"/>
       <c r="G55" t="n">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="H55" t="n">
-        <v>110249</v>
+        <v>113885</v>
       </c>
       <c r="I55" t="n">
-        <v>203.96</v>
+        <v>210.687</v>
       </c>
       <c r="J55" t="n">
-        <v>1129</v>
+        <v>958</v>
       </c>
       <c r="K55" t="n">
-        <v>2.089</v>
+        <v>1.772</v>
       </c>
       <c r="L55" t="n">
-        <v>1081</v>
+        <v>1147</v>
       </c>
       <c r="M55" t="n">
-        <v>2</v>
+        <v>2.122</v>
       </c>
       <c r="N55" t="n">
-        <v>0.12</v>
+        <v>0.112</v>
       </c>
       <c r="O55" t="n">
-        <v>8.361</v>
+        <v>8.961</v>
       </c>
       <c r="P55" t="s">
         <v>338</v>
@@ -5718,7 +5719,7 @@
         <v>348</v>
       </c>
       <c r="C57" s="1" t="n">
-        <v>44068</v>
+        <v>44070</v>
       </c>
       <c r="D57" t="s">
         <v>349</v>
@@ -5728,31 +5729,31 @@
       </c>
       <c r="F57"/>
       <c r="G57" t="n">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="H57" t="n">
-        <v>1241422</v>
+        <v>1271295</v>
       </c>
       <c r="I57" t="n">
-        <v>9.628</v>
+        <v>9.86</v>
       </c>
       <c r="J57" t="n">
-        <v>10931</v>
+        <v>11758</v>
       </c>
       <c r="K57" t="n">
-        <v>0.085</v>
+        <v>0.091</v>
       </c>
       <c r="L57" t="n">
-        <v>10105</v>
+        <v>10626</v>
       </c>
       <c r="M57" t="n">
-        <v>0.078</v>
+        <v>0.082</v>
       </c>
       <c r="N57" t="n">
-        <v>0.537</v>
+        <v>0.496</v>
       </c>
       <c r="O57" t="n">
-        <v>1.863</v>
+        <v>2.018</v>
       </c>
       <c r="P57" t="s">
         <v>351</v>
@@ -5775,7 +5776,7 @@
         <v>355</v>
       </c>
       <c r="C58" s="1" t="n">
-        <v>44072</v>
+        <v>44075</v>
       </c>
       <c r="D58" t="s">
         <v>356</v>
@@ -5785,31 +5786,31 @@
       </c>
       <c r="F58"/>
       <c r="G58" t="n">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="H58" t="n">
-        <v>1890964</v>
+        <v>1956416</v>
       </c>
       <c r="I58" t="n">
-        <v>51.231</v>
+        <v>53.004</v>
       </c>
       <c r="J58" t="n">
-        <v>22419</v>
+        <v>22082</v>
       </c>
       <c r="K58" t="n">
-        <v>0.607</v>
+        <v>0.598</v>
       </c>
       <c r="L58" t="n">
-        <v>21998</v>
+        <v>22035</v>
       </c>
       <c r="M58" t="n">
-        <v>0.596</v>
+        <v>0.597</v>
       </c>
       <c r="N58" t="n">
-        <v>0.06</v>
+        <v>0.061</v>
       </c>
       <c r="O58" t="n">
-        <v>16.662</v>
+        <v>16.518</v>
       </c>
       <c r="P58" t="s">
         <v>357</v>
@@ -5889,7 +5890,7 @@
         <v>367</v>
       </c>
       <c r="C60" s="1" t="n">
-        <v>44062</v>
+        <v>44075</v>
       </c>
       <c r="D60" t="s">
         <v>368</v>
@@ -5899,31 +5900,31 @@
       </c>
       <c r="F60"/>
       <c r="G60" t="n">
-        <v>181</v>
+        <v>194</v>
       </c>
       <c r="H60" t="n">
-        <v>554388</v>
+        <v>705560</v>
       </c>
       <c r="I60" t="n">
-        <v>19.027</v>
+        <v>24.215</v>
       </c>
       <c r="J60" t="n">
-        <v>11522</v>
+        <v>12088</v>
       </c>
       <c r="K60" t="n">
-        <v>0.395</v>
+        <v>0.415</v>
       </c>
       <c r="L60" t="n">
-        <v>11601</v>
+        <v>11937</v>
       </c>
       <c r="M60" t="n">
-        <v>0.398</v>
+        <v>0.41</v>
       </c>
       <c r="N60" t="n">
-        <v>0.053</v>
+        <v>0.081</v>
       </c>
       <c r="O60" t="n">
-        <v>18.846</v>
+        <v>12.321</v>
       </c>
       <c r="P60" t="s">
         <v>369</v>
@@ -5999,7 +6000,7 @@
         <v>380</v>
       </c>
       <c r="C62" s="1" t="n">
-        <v>44073</v>
+        <v>44075</v>
       </c>
       <c r="D62" t="s">
         <v>381</v>
@@ -6009,31 +6010,31 @@
       </c>
       <c r="F62"/>
       <c r="G62" t="n">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="H62" t="n">
-        <v>758027</v>
+        <v>777560</v>
       </c>
       <c r="I62" t="n">
-        <v>157.194</v>
+        <v>161.245</v>
       </c>
       <c r="J62" t="n">
-        <v>7219</v>
+        <v>10934</v>
       </c>
       <c r="K62" t="n">
-        <v>1.497</v>
+        <v>2.267</v>
       </c>
       <c r="L62" t="n">
-        <v>8708</v>
+        <v>9642</v>
       </c>
       <c r="M62" t="n">
-        <v>1.806</v>
+        <v>1.999</v>
       </c>
       <c r="N62" t="n">
         <v>0.001</v>
       </c>
       <c r="O62" t="n">
-        <v>1128.815</v>
+        <v>1088.613</v>
       </c>
       <c r="P62" t="s">
         <v>382</v>
@@ -6056,7 +6057,7 @@
         <v>385</v>
       </c>
       <c r="C63" s="1" t="n">
-        <v>44073</v>
+        <v>44076</v>
       </c>
       <c r="D63" t="s">
         <v>386</v>
@@ -6066,31 +6067,27 @@
       </c>
       <c r="F63"/>
       <c r="G63" t="n">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="H63" t="n">
-        <v>402070</v>
+        <v>405916</v>
       </c>
       <c r="I63" t="n">
-        <v>1.95</v>
-      </c>
-      <c r="J63" t="n">
-        <v>3766</v>
-      </c>
-      <c r="K63" t="n">
-        <v>0.018</v>
-      </c>
+        <v>1.969</v>
+      </c>
+      <c r="J63"/>
+      <c r="K63"/>
       <c r="L63" t="n">
-        <v>3435</v>
+        <v>2510</v>
       </c>
       <c r="M63" t="n">
-        <v>0.017</v>
+        <v>0.012</v>
       </c>
       <c r="N63" t="n">
-        <v>0.076</v>
+        <v>0.082</v>
       </c>
       <c r="O63" t="n">
-        <v>13.197</v>
+        <v>12.142</v>
       </c>
       <c r="P63" t="s">
         <v>387</v>
@@ -6113,7 +6110,7 @@
         <v>391</v>
       </c>
       <c r="C64" s="1" t="n">
-        <v>44069</v>
+        <v>44074</v>
       </c>
       <c r="D64" t="s">
         <v>392</v>
@@ -6123,31 +6120,31 @@
       </c>
       <c r="F64"/>
       <c r="G64" t="n">
-        <v>185</v>
+        <v>190</v>
       </c>
       <c r="H64" t="n">
-        <v>664770</v>
+        <v>711225</v>
       </c>
       <c r="I64" t="n">
-        <v>122.623</v>
+        <v>131.192</v>
       </c>
       <c r="J64" t="n">
-        <v>10445</v>
+        <v>2778</v>
       </c>
       <c r="K64" t="n">
-        <v>1.927</v>
+        <v>0.512</v>
       </c>
       <c r="L64" t="n">
-        <v>11119</v>
+        <v>10016</v>
       </c>
       <c r="M64" t="n">
-        <v>2.051</v>
+        <v>1.848</v>
       </c>
       <c r="N64" t="n">
-        <v>0.004</v>
+        <v>0.005</v>
       </c>
       <c r="O64" t="n">
-        <v>232.337</v>
+        <v>202.636</v>
       </c>
       <c r="P64" t="s">
         <v>393</v>
@@ -6215,7 +6212,7 @@
         <v>405</v>
       </c>
       <c r="C66" s="1" t="n">
-        <v>44074</v>
+        <v>44076</v>
       </c>
       <c r="D66" t="s">
         <v>406</v>
@@ -6225,31 +6222,31 @@
       </c>
       <c r="F66"/>
       <c r="G66" t="n">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="H66" t="n">
-        <v>2621146</v>
+        <v>2662508</v>
       </c>
       <c r="I66" t="n">
-        <v>11.866</v>
+        <v>12.053</v>
       </c>
       <c r="J66" t="n">
-        <v>18017</v>
+        <v>20440</v>
       </c>
       <c r="K66" t="n">
-        <v>0.082</v>
+        <v>0.093</v>
       </c>
       <c r="L66" t="n">
-        <v>22519</v>
+        <v>21453</v>
       </c>
       <c r="M66" t="n">
-        <v>0.102</v>
+        <v>0.097</v>
       </c>
       <c r="N66" t="n">
-        <v>0.02</v>
+        <v>0.016</v>
       </c>
       <c r="O66" t="n">
-        <v>51.113</v>
+        <v>62.65</v>
       </c>
       <c r="P66" t="s">
         <v>407</v>
@@ -6272,7 +6269,7 @@
         <v>410</v>
       </c>
       <c r="C67" s="1" t="n">
-        <v>44071</v>
+        <v>44074</v>
       </c>
       <c r="D67" t="s">
         <v>411</v>
@@ -6282,31 +6279,31 @@
       </c>
       <c r="F67"/>
       <c r="G67" t="n">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="H67" t="n">
-        <v>323049</v>
+        <v>336345</v>
       </c>
       <c r="I67" t="n">
-        <v>74.871</v>
+        <v>77.952</v>
       </c>
       <c r="J67" t="n">
-        <v>5115</v>
+        <v>5596</v>
       </c>
       <c r="K67" t="n">
-        <v>1.185</v>
+        <v>1.297</v>
       </c>
       <c r="L67" t="n">
-        <v>4912</v>
+        <v>4519</v>
       </c>
       <c r="M67" t="n">
-        <v>1.138</v>
+        <v>1.047</v>
       </c>
       <c r="N67" t="n">
-        <v>0.178</v>
+        <v>0.163</v>
       </c>
       <c r="O67" t="n">
-        <v>5.612</v>
+        <v>6.124</v>
       </c>
       <c r="P67" t="s">
         <v>412</v>
@@ -6386,7 +6383,7 @@
         <v>422</v>
       </c>
       <c r="C69" s="1" t="n">
-        <v>44068</v>
+        <v>44072</v>
       </c>
       <c r="D69" t="s">
         <v>423</v>
@@ -6396,25 +6393,25 @@
       </c>
       <c r="F69"/>
       <c r="G69" t="n">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="H69" t="n">
-        <v>552929</v>
+        <v>584232</v>
       </c>
       <c r="I69" t="n">
-        <v>16.77</v>
+        <v>17.719</v>
       </c>
       <c r="J69" t="n">
-        <v>3570</v>
+        <v>7671</v>
       </c>
       <c r="K69" t="n">
-        <v>0.108</v>
+        <v>0.233</v>
       </c>
       <c r="L69" t="n">
-        <v>6575</v>
+        <v>6464</v>
       </c>
       <c r="M69" t="n">
-        <v>0.199</v>
+        <v>0.196</v>
       </c>
       <c r="N69"/>
       <c r="O69"/>
@@ -6496,7 +6493,7 @@
         <v>434</v>
       </c>
       <c r="C71" s="1" t="n">
-        <v>44073</v>
+        <v>44075</v>
       </c>
       <c r="D71" t="s">
         <v>435</v>
@@ -6506,31 +6503,31 @@
       </c>
       <c r="F71"/>
       <c r="G71" t="n">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="H71" t="n">
-        <v>2587559</v>
+        <v>2628272</v>
       </c>
       <c r="I71" t="n">
-        <v>68.37</v>
+        <v>69.445</v>
       </c>
       <c r="J71" t="n">
-        <v>18753</v>
+        <v>28703</v>
       </c>
       <c r="K71" t="n">
-        <v>0.496</v>
+        <v>0.758</v>
       </c>
       <c r="L71" t="n">
-        <v>22478</v>
+        <v>22963</v>
       </c>
       <c r="M71" t="n">
-        <v>0.594</v>
+        <v>0.607</v>
       </c>
       <c r="N71" t="n">
-        <v>0.032</v>
+        <v>0.031</v>
       </c>
       <c r="O71" t="n">
-        <v>31.108</v>
+        <v>31.754</v>
       </c>
       <c r="P71" t="s">
         <v>436</v>
@@ -6553,7 +6550,7 @@
         <v>439</v>
       </c>
       <c r="C72" s="1" t="n">
-        <v>44073</v>
+        <v>44075</v>
       </c>
       <c r="D72" t="s">
         <v>435</v>
@@ -6563,31 +6560,31 @@
       </c>
       <c r="F72"/>
       <c r="G72" t="n">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="H72" t="n">
-        <v>2701553</v>
+        <v>2743434</v>
       </c>
       <c r="I72" t="n">
-        <v>71.382</v>
+        <v>72.488</v>
       </c>
       <c r="J72" t="n">
-        <v>19017</v>
+        <v>29407</v>
       </c>
       <c r="K72" t="n">
-        <v>0.502</v>
+        <v>0.777</v>
       </c>
       <c r="L72" t="n">
-        <v>23256</v>
+        <v>23673</v>
       </c>
       <c r="M72" t="n">
-        <v>0.614</v>
+        <v>0.625</v>
       </c>
       <c r="N72" t="n">
         <v>0.031</v>
       </c>
       <c r="O72" t="n">
-        <v>32.185</v>
+        <v>32.736</v>
       </c>
       <c r="P72" t="s">
         <v>436</v>
@@ -6610,7 +6607,7 @@
         <v>442</v>
       </c>
       <c r="C73" s="1" t="n">
-        <v>44068</v>
+        <v>44074</v>
       </c>
       <c r="D73" t="s">
         <v>443</v>
@@ -6620,31 +6617,31 @@
       </c>
       <c r="F73"/>
       <c r="G73" t="n">
-        <v>178</v>
+        <v>184</v>
       </c>
       <c r="H73" t="n">
-        <v>1976482</v>
+        <v>2058544</v>
       </c>
       <c r="I73" t="n">
-        <v>193.835</v>
+        <v>201.883</v>
       </c>
       <c r="J73" t="n">
-        <v>17757</v>
+        <v>15127</v>
       </c>
       <c r="K73" t="n">
-        <v>1.741</v>
+        <v>1.484</v>
       </c>
       <c r="L73" t="n">
-        <v>13708</v>
+        <v>14260</v>
       </c>
       <c r="M73" t="n">
-        <v>1.344</v>
+        <v>1.398</v>
       </c>
       <c r="N73" t="n">
-        <v>0.015</v>
+        <v>0.022</v>
       </c>
       <c r="O73" t="n">
-        <v>64.573</v>
+        <v>45.979</v>
       </c>
       <c r="P73" t="s">
         <v>444</v>
@@ -6667,7 +6664,7 @@
         <v>448</v>
       </c>
       <c r="C74" s="1" t="n">
-        <v>44073</v>
+        <v>44075</v>
       </c>
       <c r="D74" t="s">
         <v>449</v>
@@ -6677,31 +6674,31 @@
       </c>
       <c r="F74"/>
       <c r="G74" t="n">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="H74" t="n">
-        <v>624609</v>
+        <v>634745</v>
       </c>
       <c r="I74" t="n">
-        <v>216.798</v>
+        <v>220.316</v>
       </c>
       <c r="J74" t="n">
-        <v>4481</v>
+        <v>4914</v>
       </c>
       <c r="K74" t="n">
-        <v>1.555</v>
+        <v>1.706</v>
       </c>
       <c r="L74" t="n">
-        <v>4956</v>
+        <v>5083</v>
       </c>
       <c r="M74" t="n">
-        <v>1.72</v>
+        <v>1.764</v>
       </c>
       <c r="N74" t="n">
-        <v>0.047</v>
+        <v>0.042</v>
       </c>
       <c r="O74" t="n">
-        <v>21.128</v>
+        <v>23.532</v>
       </c>
       <c r="P74" t="s">
         <v>450</v>
@@ -6724,7 +6721,7 @@
         <v>454</v>
       </c>
       <c r="C75" s="1" t="n">
-        <v>44073</v>
+        <v>44075</v>
       </c>
       <c r="D75" t="s">
         <v>455</v>
@@ -6734,31 +6731,31 @@
       </c>
       <c r="F75"/>
       <c r="G75" t="n">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="H75" t="n">
-        <v>1795633</v>
+        <v>1825272</v>
       </c>
       <c r="I75" t="n">
-        <v>93.339</v>
+        <v>94.88</v>
       </c>
       <c r="J75" t="n">
-        <v>14670</v>
+        <v>22326</v>
       </c>
       <c r="K75" t="n">
-        <v>0.763</v>
+        <v>1.161</v>
       </c>
       <c r="L75" t="n">
-        <v>20427</v>
+        <v>20808</v>
       </c>
       <c r="M75" t="n">
-        <v>1.062</v>
+        <v>1.082</v>
       </c>
       <c r="N75" t="n">
-        <v>0.058</v>
+        <v>0.056</v>
       </c>
       <c r="O75" t="n">
-        <v>17.25</v>
+        <v>17.741</v>
       </c>
       <c r="P75" t="s">
         <v>457</v>
@@ -6781,7 +6778,7 @@
         <v>461</v>
       </c>
       <c r="C76" s="1" t="n">
-        <v>44073</v>
+        <v>44075</v>
       </c>
       <c r="D76" t="s">
         <v>462</v>
@@ -6791,31 +6788,31 @@
       </c>
       <c r="F76"/>
       <c r="G76" t="n">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="H76" t="n">
-        <v>36696382</v>
+        <v>37176827</v>
       </c>
       <c r="I76" t="n">
-        <v>251.458</v>
+        <v>254.75</v>
       </c>
       <c r="J76" t="n">
-        <v>269532</v>
+        <v>275612</v>
       </c>
       <c r="K76" t="n">
-        <v>1.847</v>
+        <v>1.889</v>
       </c>
       <c r="L76" t="n">
-        <v>285854</v>
+        <v>292595</v>
       </c>
       <c r="M76" t="n">
-        <v>1.959</v>
+        <v>2.005</v>
       </c>
       <c r="N76" t="n">
         <v>0.017</v>
       </c>
       <c r="O76" t="n">
-        <v>59.822</v>
+        <v>60.55</v>
       </c>
       <c r="P76" t="s">
         <v>463</v>
@@ -6895,7 +6892,7 @@
         <v>473</v>
       </c>
       <c r="C78" s="1" t="n">
-        <v>44073</v>
+        <v>44075</v>
       </c>
       <c r="D78" t="s">
         <v>474</v>
@@ -6905,31 +6902,31 @@
       </c>
       <c r="F78"/>
       <c r="G78" t="n">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="H78" t="n">
-        <v>5063593</v>
+        <v>5160518</v>
       </c>
       <c r="I78" t="n">
-        <v>145.448</v>
+        <v>148.232</v>
       </c>
       <c r="J78" t="n">
-        <v>37466</v>
+        <v>49989</v>
       </c>
       <c r="K78" t="n">
-        <v>1.076</v>
+        <v>1.436</v>
       </c>
       <c r="L78" t="n">
-        <v>55076</v>
+        <v>52618</v>
       </c>
       <c r="M78" t="n">
-        <v>1.582</v>
+        <v>1.511</v>
       </c>
       <c r="N78" t="n">
-        <v>0.02</v>
+        <v>0.019</v>
       </c>
       <c r="O78" t="n">
-        <v>51.125</v>
+        <v>51.746</v>
       </c>
       <c r="P78" t="s">
         <v>45</v>
@@ -6952,7 +6949,7 @@
         <v>477</v>
       </c>
       <c r="C79" s="1" t="n">
-        <v>44073</v>
+        <v>44075</v>
       </c>
       <c r="D79" t="s">
         <v>478</v>
@@ -6964,31 +6961,31 @@
         <v>480</v>
       </c>
       <c r="G79" t="n">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="H79" t="n">
-        <v>151044</v>
+        <v>153078</v>
       </c>
       <c r="I79" t="n">
-        <v>9.021</v>
+        <v>9.142</v>
       </c>
       <c r="J79" t="n">
-        <v>1276</v>
+        <v>944</v>
       </c>
       <c r="K79" t="n">
-        <v>0.076</v>
+        <v>0.056</v>
       </c>
       <c r="L79" t="n">
-        <v>1158</v>
+        <v>1216</v>
       </c>
       <c r="M79" t="n">
-        <v>0.069</v>
+        <v>0.073</v>
       </c>
       <c r="N79" t="n">
-        <v>0.075</v>
+        <v>0.07</v>
       </c>
       <c r="O79" t="n">
-        <v>13.376</v>
+        <v>14.234</v>
       </c>
       <c r="P79" t="s">
         <v>481</v>
@@ -7011,7 +7008,7 @@
         <v>485</v>
       </c>
       <c r="C80" s="1" t="n">
-        <v>44073</v>
+        <v>44074</v>
       </c>
       <c r="D80" t="s">
         <v>486</v>
@@ -7023,31 +7020,31 @@
         <v>487</v>
       </c>
       <c r="G80" t="n">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="H80" t="n">
-        <v>925208</v>
+        <v>931037</v>
       </c>
       <c r="I80" t="n">
-        <v>135.968</v>
+        <v>136.825</v>
       </c>
       <c r="J80" t="n">
-        <v>4356</v>
+        <v>5829</v>
       </c>
       <c r="K80" t="n">
-        <v>0.64</v>
+        <v>0.857</v>
       </c>
       <c r="L80" t="n">
-        <v>7934</v>
+        <v>7730</v>
       </c>
       <c r="M80" t="n">
-        <v>1.166</v>
+        <v>1.136</v>
       </c>
       <c r="N80" t="n">
         <v>0.013</v>
       </c>
       <c r="O80" t="n">
-        <v>75.665</v>
+        <v>76.427</v>
       </c>
       <c r="P80" t="s">
         <v>45</v>
@@ -7070,7 +7067,7 @@
         <v>491</v>
       </c>
       <c r="C81" s="1" t="n">
-        <v>44067</v>
+        <v>44074</v>
       </c>
       <c r="D81" t="s">
         <v>492</v>
@@ -7080,27 +7077,27 @@
       </c>
       <c r="F81"/>
       <c r="G81" t="n">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H81" t="n">
-        <v>758569</v>
+        <v>805214</v>
       </c>
       <c r="I81" t="n">
-        <v>129.662</v>
+        <v>137.635</v>
       </c>
       <c r="J81"/>
       <c r="K81"/>
       <c r="L81" t="n">
-        <v>4803</v>
+        <v>6664</v>
       </c>
       <c r="M81" t="n">
-        <v>0.821</v>
+        <v>1.139</v>
       </c>
       <c r="N81" t="n">
-        <v>0.018</v>
+        <v>0.009</v>
       </c>
       <c r="O81" t="n">
-        <v>55.48</v>
+        <v>111.598</v>
       </c>
       <c r="P81" t="s">
         <v>45</v>
@@ -7123,7 +7120,7 @@
         <v>494</v>
       </c>
       <c r="C82" s="1" t="n">
-        <v>44067</v>
+        <v>44074</v>
       </c>
       <c r="D82" t="s">
         <v>492</v>
@@ -7133,27 +7130,27 @@
       </c>
       <c r="F82"/>
       <c r="G82" t="n">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H82" t="n">
-        <v>1832813</v>
+        <v>2068284</v>
       </c>
       <c r="I82" t="n">
-        <v>313.283</v>
+        <v>353.532</v>
       </c>
       <c r="J82"/>
       <c r="K82"/>
       <c r="L82" t="n">
-        <v>15168</v>
+        <v>33639</v>
       </c>
       <c r="M82" t="n">
-        <v>2.593</v>
+        <v>5.75</v>
       </c>
       <c r="N82" t="n">
-        <v>0.006</v>
+        <v>0.002</v>
       </c>
       <c r="O82" t="n">
-        <v>175.208</v>
+        <v>563.333</v>
       </c>
       <c r="P82" t="s">
         <v>45</v>
@@ -7176,7 +7173,7 @@
         <v>497</v>
       </c>
       <c r="C83" s="1" t="n">
-        <v>44073</v>
+        <v>44076</v>
       </c>
       <c r="D83" t="s">
         <v>498</v>
@@ -7186,31 +7183,31 @@
       </c>
       <c r="F83"/>
       <c r="G83" t="n">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="H83" t="n">
-        <v>334344</v>
+        <v>340123</v>
       </c>
       <c r="I83" t="n">
-        <v>61.239</v>
+        <v>62.298</v>
       </c>
       <c r="J83" t="n">
-        <v>1951</v>
+        <v>2428</v>
       </c>
       <c r="K83" t="n">
-        <v>0.357</v>
+        <v>0.445</v>
       </c>
       <c r="L83" t="n">
-        <v>3075</v>
+        <v>2883</v>
       </c>
       <c r="M83" t="n">
-        <v>0.563</v>
+        <v>0.528</v>
       </c>
       <c r="N83" t="n">
-        <v>0.024</v>
+        <v>0.027</v>
       </c>
       <c r="O83" t="n">
-        <v>40.922</v>
+        <v>37.581</v>
       </c>
       <c r="P83" t="s">
         <v>500</v>
@@ -7233,7 +7230,7 @@
         <v>503</v>
       </c>
       <c r="C84" s="1" t="n">
-        <v>44073</v>
+        <v>44075</v>
       </c>
       <c r="D84" t="s">
         <v>504</v>
@@ -7243,31 +7240,31 @@
       </c>
       <c r="F84"/>
       <c r="G84" t="n">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="H84" t="n">
-        <v>157456</v>
+        <v>160479</v>
       </c>
       <c r="I84" t="n">
-        <v>75.739</v>
+        <v>77.193</v>
       </c>
       <c r="J84" t="n">
-        <v>588</v>
+        <v>1608</v>
       </c>
       <c r="K84" t="n">
-        <v>0.283</v>
+        <v>0.773</v>
       </c>
       <c r="L84" t="n">
-        <v>1174</v>
+        <v>1192</v>
       </c>
       <c r="M84" t="n">
-        <v>0.565</v>
+        <v>0.573</v>
       </c>
       <c r="N84" t="n">
-        <v>0.026</v>
+        <v>0.027</v>
       </c>
       <c r="O84" t="n">
-        <v>37.871</v>
+        <v>36.758</v>
       </c>
       <c r="P84" t="s">
         <v>506</v>
@@ -7290,7 +7287,7 @@
         <v>510</v>
       </c>
       <c r="C85" s="1" t="n">
-        <v>44073</v>
+        <v>44075</v>
       </c>
       <c r="D85" t="s">
         <v>511</v>
@@ -7302,31 +7299,31 @@
         <v>513</v>
       </c>
       <c r="G85" t="n">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="H85" t="n">
-        <v>3674872</v>
+        <v>3705408</v>
       </c>
       <c r="I85" t="n">
-        <v>61.962</v>
+        <v>62.477</v>
       </c>
       <c r="J85" t="n">
-        <v>21902</v>
+        <v>11687</v>
       </c>
       <c r="K85" t="n">
-        <v>0.369</v>
+        <v>0.197</v>
       </c>
       <c r="L85" t="n">
-        <v>17350</v>
+        <v>18082</v>
       </c>
       <c r="M85" t="n">
-        <v>0.293</v>
+        <v>0.305</v>
       </c>
       <c r="N85" t="n">
-        <v>0.128</v>
+        <v>0.123</v>
       </c>
       <c r="O85" t="n">
-        <v>7.832</v>
+        <v>8.118</v>
       </c>
       <c r="P85" t="s">
         <v>512</v>
@@ -7349,7 +7346,7 @@
         <v>517</v>
       </c>
       <c r="C86" s="1" t="n">
-        <v>44074</v>
+        <v>44076</v>
       </c>
       <c r="D86" t="s">
         <v>518</v>
@@ -7359,31 +7356,31 @@
       </c>
       <c r="F86"/>
       <c r="G86" t="n">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="H86" t="n">
-        <v>1879813</v>
+        <v>1923547</v>
       </c>
       <c r="I86" t="n">
-        <v>36.666</v>
+        <v>37.519</v>
       </c>
       <c r="J86" t="n">
-        <v>13664</v>
+        <v>21210</v>
       </c>
       <c r="K86" t="n">
-        <v>0.267</v>
+        <v>0.414</v>
       </c>
       <c r="L86" t="n">
-        <v>17627</v>
+        <v>18119</v>
       </c>
       <c r="M86" t="n">
-        <v>0.344</v>
+        <v>0.353</v>
       </c>
       <c r="N86" t="n">
-        <v>0.018</v>
+        <v>0.017</v>
       </c>
       <c r="O86" t="n">
-        <v>54.071</v>
+        <v>58.074</v>
       </c>
       <c r="P86" t="s">
         <v>519</v>
@@ -7406,7 +7403,7 @@
         <v>523</v>
       </c>
       <c r="C87" s="1" t="n">
-        <v>44063</v>
+        <v>44070</v>
       </c>
       <c r="D87" t="s">
         <v>524</v>
@@ -7416,27 +7413,27 @@
       </c>
       <c r="F87"/>
       <c r="G87" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H87" t="n">
-        <v>5849939</v>
+        <v>6416533</v>
       </c>
       <c r="I87" t="n">
-        <v>125.12</v>
+        <v>137.238</v>
       </c>
       <c r="J87"/>
       <c r="K87"/>
       <c r="L87" t="n">
-        <v>68947</v>
+        <v>80942</v>
       </c>
       <c r="M87" t="n">
-        <v>1.475</v>
+        <v>1.731</v>
       </c>
       <c r="N87" t="n">
-        <v>0.084</v>
+        <v>0.091</v>
       </c>
       <c r="O87" t="n">
-        <v>11.896</v>
+        <v>10.98</v>
       </c>
       <c r="P87" t="s">
         <v>526</v>
@@ -7486,10 +7483,10 @@
         <v>1.098</v>
       </c>
       <c r="N88" t="n">
-        <v>0.062</v>
+        <v>0.057</v>
       </c>
       <c r="O88" t="n">
-        <v>16.162</v>
+        <v>17.67</v>
       </c>
       <c r="P88" t="s">
         <v>533</v>
@@ -7512,7 +7509,7 @@
         <v>536</v>
       </c>
       <c r="C89" s="1" t="n">
-        <v>44066</v>
+        <v>44073</v>
       </c>
       <c r="D89" t="s">
         <v>537</v>
@@ -7522,27 +7519,27 @@
       </c>
       <c r="F89"/>
       <c r="G89" t="n">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="H89"/>
       <c r="I89"/>
       <c r="J89" t="n">
-        <v>9364</v>
+        <v>12151</v>
       </c>
       <c r="K89" t="n">
-        <v>0.927</v>
+        <v>1.203</v>
       </c>
       <c r="L89" t="n">
-        <v>9364</v>
+        <v>12151</v>
       </c>
       <c r="M89" t="n">
-        <v>0.927</v>
+        <v>1.203</v>
       </c>
       <c r="N89" t="n">
-        <v>0.027</v>
+        <v>0.014</v>
       </c>
       <c r="O89" t="n">
-        <v>37.264</v>
+        <v>69.662</v>
       </c>
       <c r="P89" t="s">
         <v>533</v>
@@ -7565,7 +7562,7 @@
         <v>540</v>
       </c>
       <c r="C90" s="1" t="n">
-        <v>44072</v>
+        <v>44074</v>
       </c>
       <c r="D90" t="s">
         <v>541</v>
@@ -7575,232 +7572,232 @@
       </c>
       <c r="F90"/>
       <c r="G90" t="n">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="H90" t="n">
-        <v>1012884</v>
+        <v>1023203</v>
       </c>
       <c r="I90" t="n">
-        <v>117.034</v>
+        <v>118.226</v>
       </c>
       <c r="J90" t="n">
-        <v>8180</v>
+        <v>6365</v>
       </c>
       <c r="K90" t="n">
-        <v>0.945</v>
+        <v>0.735</v>
       </c>
       <c r="L90" t="n">
-        <v>10382</v>
+        <v>9965</v>
       </c>
       <c r="M90" t="n">
-        <v>1.2</v>
+        <v>1.151</v>
       </c>
       <c r="N90" t="n">
-        <v>0.028</v>
+        <v>0.03</v>
       </c>
       <c r="O90" t="n">
-        <v>36.192</v>
+        <v>33.154</v>
       </c>
       <c r="P90" t="s">
         <v>542</v>
       </c>
       <c r="Q90" t="s">
-        <v>541</v>
+        <v>543</v>
       </c>
       <c r="R90" t="s">
-        <v>543</v>
+        <v>544</v>
       </c>
       <c r="S90" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
       <c r="B91" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
       <c r="C91" s="1" t="n">
-        <v>44073</v>
+        <v>44075</v>
       </c>
       <c r="D91" t="s">
-        <v>547</v>
+        <v>548</v>
       </c>
       <c r="E91" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
       <c r="F91"/>
       <c r="G91" t="n">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="H91" t="n">
-        <v>87291</v>
+        <v>87646</v>
       </c>
       <c r="I91" t="n">
-        <v>3.665</v>
+        <v>3.68</v>
       </c>
       <c r="J91" t="n">
-        <v>157</v>
+        <v>144</v>
       </c>
       <c r="K91" t="n">
+        <v>0.006</v>
+      </c>
+      <c r="L91" t="n">
+        <v>176</v>
+      </c>
+      <c r="M91" t="n">
         <v>0.007</v>
-      </c>
-      <c r="L91" t="n">
-        <v>181</v>
-      </c>
-      <c r="M91" t="n">
-        <v>0.008</v>
       </c>
       <c r="N91" t="n">
         <v>0.001</v>
       </c>
       <c r="O91" t="n">
-        <v>1267</v>
+        <v>1232</v>
       </c>
       <c r="P91" t="s">
+        <v>549</v>
+      </c>
+      <c r="Q91" t="s">
         <v>548</v>
-      </c>
-      <c r="Q91" t="s">
-        <v>547</v>
       </c>
       <c r="R91" t="s">
         <v>23</v>
       </c>
       <c r="S91" t="s">
-        <v>549</v>
+        <v>550</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="B92" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
       <c r="C92" s="1" t="n">
-        <v>44073</v>
+        <v>44075</v>
       </c>
       <c r="D92" t="s">
-        <v>552</v>
+        <v>553</v>
       </c>
       <c r="E92" t="s">
-        <v>553</v>
+        <v>554</v>
       </c>
       <c r="F92"/>
       <c r="G92" t="n">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="H92" t="n">
-        <v>417044</v>
+        <v>419970</v>
       </c>
       <c r="I92" t="n">
-        <v>5.975</v>
+        <v>6.017</v>
       </c>
       <c r="J92" t="n">
-        <v>1111</v>
+        <v>1599</v>
       </c>
       <c r="K92" t="n">
-        <v>0.016</v>
+        <v>0.023</v>
       </c>
       <c r="L92" t="n">
-        <v>1553</v>
+        <v>1477</v>
       </c>
       <c r="M92" t="n">
-        <v>0.022</v>
+        <v>0.021</v>
       </c>
       <c r="N92" t="n">
         <v>0.001</v>
       </c>
       <c r="O92" t="n">
-        <v>679.438</v>
+        <v>689.267</v>
       </c>
       <c r="P92" t="s">
-        <v>553</v>
+        <v>554</v>
       </c>
       <c r="Q92" t="s">
-        <v>554</v>
+        <v>555</v>
       </c>
       <c r="R92" t="s">
         <v>23</v>
       </c>
       <c r="S92" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="B93" t="s">
-        <v>556</v>
+        <v>557</v>
       </c>
       <c r="C93" s="1" t="n">
-        <v>44073</v>
+        <v>44075</v>
       </c>
       <c r="D93" t="s">
-        <v>552</v>
+        <v>553</v>
       </c>
       <c r="E93" t="s">
-        <v>553</v>
+        <v>554</v>
       </c>
       <c r="F93"/>
       <c r="G93" t="n">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="H93" t="n">
-        <v>844454</v>
+        <v>847380</v>
       </c>
       <c r="I93" t="n">
-        <v>12.098</v>
+        <v>12.14</v>
       </c>
       <c r="J93" t="n">
-        <v>1111</v>
+        <v>1599</v>
       </c>
       <c r="K93" t="n">
-        <v>0.016</v>
+        <v>0.023</v>
       </c>
       <c r="L93" t="n">
-        <v>7144</v>
+        <v>7068</v>
       </c>
       <c r="M93" t="n">
-        <v>0.102</v>
+        <v>0.101</v>
       </c>
       <c r="N93" t="n">
         <v>0</v>
       </c>
       <c r="O93" t="n">
-        <v>3125.5</v>
+        <v>3298.4</v>
       </c>
       <c r="P93" t="s">
-        <v>553</v>
+        <v>554</v>
       </c>
       <c r="Q93" t="s">
-        <v>554</v>
+        <v>555</v>
       </c>
       <c r="R93" t="s">
         <v>27</v>
       </c>
       <c r="S93" t="s">
-        <v>557</v>
+        <v>558</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="s">
-        <v>558</v>
+        <v>559</v>
       </c>
       <c r="B94" t="s">
-        <v>559</v>
+        <v>560</v>
       </c>
       <c r="C94" s="1" t="n">
         <v>44062</v>
       </c>
       <c r="D94"/>
       <c r="E94" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="F94" t="s">
-        <v>561</v>
+        <v>562</v>
       </c>
       <c r="G94" t="n">
         <v>163</v>
@@ -7830,321 +7827,321 @@
         <v>47.437</v>
       </c>
       <c r="P94" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="Q94" t="s">
-        <v>562</v>
+        <v>563</v>
       </c>
       <c r="R94" t="s">
         <v>54</v>
       </c>
       <c r="S94" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="s">
-        <v>564</v>
+        <v>565</v>
       </c>
       <c r="B95" t="s">
-        <v>565</v>
+        <v>566</v>
       </c>
       <c r="C95" s="1" t="n">
-        <v>44070</v>
+        <v>44072</v>
       </c>
       <c r="D95" t="s">
-        <v>566</v>
+        <v>567</v>
       </c>
       <c r="E95" t="s">
-        <v>567</v>
+        <v>568</v>
       </c>
       <c r="F95"/>
       <c r="G95" t="n">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="H95" t="n">
-        <v>136199</v>
+        <v>140714</v>
       </c>
       <c r="I95" t="n">
-        <v>11.524</v>
+        <v>11.906</v>
       </c>
       <c r="J95" t="n">
-        <v>2586</v>
+        <v>1848</v>
       </c>
       <c r="K95" t="n">
-        <v>0.219</v>
+        <v>0.156</v>
       </c>
       <c r="L95" t="n">
-        <v>2375</v>
+        <v>2492</v>
       </c>
       <c r="M95" t="n">
-        <v>0.201</v>
+        <v>0.211</v>
       </c>
       <c r="N95" t="n">
-        <v>0.047</v>
+        <v>0.049</v>
       </c>
       <c r="O95" t="n">
-        <v>21.341</v>
+        <v>20.426</v>
       </c>
       <c r="P95" t="s">
+        <v>568</v>
+      </c>
+      <c r="Q95" t="s">
         <v>567</v>
-      </c>
-      <c r="Q95" t="s">
-        <v>566</v>
       </c>
       <c r="R95" t="s">
         <v>27</v>
       </c>
       <c r="S95" t="s">
-        <v>568</v>
+        <v>569</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="s">
-        <v>569</v>
+        <v>570</v>
       </c>
       <c r="B96" t="s">
-        <v>570</v>
+        <v>571</v>
       </c>
       <c r="C96" s="1" t="n">
-        <v>44073</v>
+        <v>44075</v>
       </c>
       <c r="D96" t="s">
-        <v>571</v>
+        <v>572</v>
       </c>
       <c r="E96" t="s">
-        <v>572</v>
+        <v>573</v>
       </c>
       <c r="F96"/>
       <c r="G96" t="n">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="H96" t="n">
-        <v>7028390</v>
+        <v>7247935</v>
       </c>
       <c r="I96" t="n">
-        <v>83.335</v>
+        <v>85.938</v>
       </c>
       <c r="J96" t="n">
-        <v>91302</v>
+        <v>109443</v>
       </c>
       <c r="K96" t="n">
-        <v>1.083</v>
+        <v>1.298</v>
       </c>
       <c r="L96" t="n">
-        <v>100132</v>
+        <v>103756</v>
       </c>
       <c r="M96" t="n">
-        <v>1.187</v>
+        <v>1.23</v>
       </c>
       <c r="N96" t="n">
         <v>0.014</v>
       </c>
       <c r="O96" t="n">
-        <v>69.869</v>
+        <v>69.562</v>
       </c>
       <c r="P96" t="s">
+        <v>573</v>
+      </c>
+      <c r="Q96" t="s">
         <v>572</v>
-      </c>
-      <c r="Q96" t="s">
-        <v>571</v>
       </c>
       <c r="R96" t="s">
         <v>27</v>
       </c>
       <c r="S96" t="s">
-        <v>573</v>
+        <v>574</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="s">
-        <v>574</v>
+        <v>575</v>
       </c>
       <c r="B97" t="s">
-        <v>575</v>
+        <v>576</v>
       </c>
       <c r="C97" s="1" t="n">
-        <v>44070</v>
+        <v>44074</v>
       </c>
       <c r="D97" t="s">
-        <v>576</v>
+        <v>577</v>
       </c>
       <c r="E97" t="s">
-        <v>577</v>
+        <v>578</v>
       </c>
       <c r="F97"/>
       <c r="G97" t="n">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="H97" t="n">
-        <v>367423</v>
+        <v>381749</v>
       </c>
       <c r="I97" t="n">
-        <v>8.033</v>
+        <v>8.346</v>
       </c>
       <c r="J97" t="n">
-        <v>3621</v>
+        <v>3564</v>
       </c>
       <c r="K97" t="n">
-        <v>0.079</v>
+        <v>0.078</v>
       </c>
       <c r="L97" t="n">
-        <v>3797</v>
+        <v>3813</v>
       </c>
       <c r="M97" t="n">
         <v>0.083</v>
       </c>
       <c r="N97" t="n">
-        <v>0.035</v>
+        <v>0.025</v>
       </c>
       <c r="O97" t="n">
-        <v>28.859</v>
+        <v>40.137</v>
       </c>
       <c r="P97" t="s">
-        <v>577</v>
+        <v>578</v>
       </c>
       <c r="Q97" t="s">
-        <v>578</v>
+        <v>579</v>
       </c>
       <c r="R97" t="s">
         <v>54</v>
       </c>
       <c r="S97" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="s">
-        <v>580</v>
+        <v>581</v>
       </c>
       <c r="B98" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="C98" s="1" t="n">
-        <v>44074</v>
+        <v>44076</v>
       </c>
       <c r="D98" t="s">
-        <v>582</v>
+        <v>583</v>
       </c>
       <c r="E98" t="s">
-        <v>583</v>
+        <v>584</v>
       </c>
       <c r="F98"/>
       <c r="G98" t="n">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="H98" t="n">
-        <v>1550280</v>
+        <v>1597707</v>
       </c>
       <c r="I98" t="n">
-        <v>35.448</v>
+        <v>36.533</v>
       </c>
       <c r="J98" t="n">
-        <v>14109</v>
+        <v>41052</v>
       </c>
       <c r="K98" t="n">
-        <v>0.323</v>
+        <v>0.939</v>
       </c>
       <c r="L98" t="n">
-        <v>17847</v>
+        <v>20814</v>
       </c>
       <c r="M98" t="n">
-        <v>0.408</v>
+        <v>0.476</v>
       </c>
       <c r="N98" t="n">
-        <v>0.113</v>
+        <v>0.091</v>
       </c>
       <c r="O98" t="n">
-        <v>8.85</v>
+        <v>11.023</v>
       </c>
       <c r="P98" t="s">
-        <v>583</v>
+        <v>584</v>
       </c>
       <c r="Q98" t="s">
-        <v>584</v>
+        <v>585</v>
       </c>
       <c r="R98" t="s">
         <v>40</v>
       </c>
       <c r="S98" t="s">
-        <v>585</v>
+        <v>586</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="s">
-        <v>586</v>
+        <v>587</v>
       </c>
       <c r="B99" t="s">
-        <v>587</v>
+        <v>588</v>
       </c>
       <c r="C99" s="1" t="n">
-        <v>44073</v>
+        <v>44075</v>
       </c>
       <c r="D99" t="s">
-        <v>588</v>
+        <v>589</v>
       </c>
       <c r="E99" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="F99"/>
       <c r="G99" t="n">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="H99" t="n">
-        <v>7011895</v>
+        <v>7177430</v>
       </c>
       <c r="I99" t="n">
-        <v>708.96</v>
+        <v>725.697</v>
       </c>
       <c r="J99" t="n">
-        <v>87955</v>
+        <v>82772</v>
       </c>
       <c r="K99" t="n">
-        <v>8.893</v>
+        <v>8.369</v>
       </c>
       <c r="L99" t="n">
-        <v>74642</v>
+        <v>78205</v>
       </c>
       <c r="M99" t="n">
-        <v>7.547</v>
+        <v>7.907</v>
       </c>
       <c r="N99" t="n">
         <v>0.005</v>
       </c>
       <c r="O99" t="n">
-        <v>192.731</v>
+        <v>185.634</v>
       </c>
       <c r="P99" t="s">
+        <v>590</v>
+      </c>
+      <c r="Q99" t="s">
         <v>589</v>
-      </c>
-      <c r="Q99" t="s">
-        <v>588</v>
       </c>
       <c r="R99" t="s">
         <v>27</v>
       </c>
       <c r="S99" t="s">
-        <v>590</v>
+        <v>591</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="s">
-        <v>591</v>
+        <v>592</v>
       </c>
       <c r="B100" t="s">
-        <v>592</v>
+        <v>593</v>
       </c>
       <c r="C100" s="1" t="n">
         <v>44069</v>
       </c>
       <c r="D100" t="s">
-        <v>593</v>
+        <v>594</v>
       </c>
       <c r="E100" t="s">
-        <v>594</v>
+        <v>595</v>
       </c>
       <c r="F100" t="s">
-        <v>595</v>
+        <v>596</v>
       </c>
       <c r="G100" t="n">
         <v>148</v>
@@ -8174,33 +8171,33 @@
         <v>156.471</v>
       </c>
       <c r="P100" t="s">
-        <v>594</v>
+        <v>595</v>
       </c>
       <c r="Q100" t="s">
-        <v>596</v>
+        <v>597</v>
       </c>
       <c r="R100" t="s">
         <v>27</v>
       </c>
       <c r="S100" t="s">
-        <v>597</v>
+        <v>598</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="s">
-        <v>598</v>
+        <v>599</v>
       </c>
       <c r="B101" t="s">
-        <v>599</v>
+        <v>600</v>
       </c>
       <c r="C101" s="1" t="n">
         <v>44071</v>
       </c>
       <c r="D101" t="s">
-        <v>600</v>
+        <v>601</v>
       </c>
       <c r="E101" t="s">
-        <v>601</v>
+        <v>602</v>
       </c>
       <c r="F101"/>
       <c r="G101" t="n">
@@ -8231,147 +8228,147 @@
         <v>16.007</v>
       </c>
       <c r="P101" t="s">
-        <v>602</v>
+        <v>603</v>
       </c>
       <c r="Q101" t="s">
-        <v>603</v>
+        <v>604</v>
       </c>
       <c r="R101" t="s">
-        <v>604</v>
+        <v>605</v>
       </c>
       <c r="S101" t="s">
-        <v>605</v>
+        <v>606</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="s">
-        <v>598</v>
+        <v>599</v>
       </c>
       <c r="B102" t="s">
-        <v>606</v>
+        <v>607</v>
       </c>
       <c r="C102" s="1" t="n">
-        <v>44073</v>
+        <v>44075</v>
       </c>
       <c r="D102" t="s">
-        <v>607</v>
+        <v>608</v>
       </c>
       <c r="E102" t="s">
-        <v>608</v>
+        <v>609</v>
       </c>
       <c r="F102"/>
       <c r="G102" t="n">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="H102" t="n">
-        <v>77063268</v>
+        <v>78447059</v>
       </c>
       <c r="I102" t="n">
-        <v>232.818</v>
+        <v>236.998</v>
       </c>
       <c r="J102" t="n">
-        <v>737701</v>
+        <v>698161</v>
       </c>
       <c r="K102" t="n">
-        <v>2.229</v>
+        <v>2.109</v>
       </c>
       <c r="L102" t="n">
-        <v>714953</v>
+        <v>724522</v>
       </c>
       <c r="M102" t="n">
-        <v>2.16</v>
+        <v>2.189</v>
       </c>
       <c r="N102" t="n">
-        <v>0.059</v>
+        <v>0.057</v>
       </c>
       <c r="O102" t="n">
-        <v>17.053</v>
+        <v>17.482</v>
       </c>
       <c r="P102" t="s">
-        <v>608</v>
+        <v>609</v>
       </c>
       <c r="Q102" t="s">
-        <v>609</v>
+        <v>610</v>
       </c>
       <c r="R102" t="s">
-        <v>610</v>
+        <v>611</v>
       </c>
       <c r="S102" t="s">
-        <v>611</v>
+        <v>612</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="s">
-        <v>612</v>
+        <v>613</v>
       </c>
       <c r="B103" t="s">
-        <v>613</v>
+        <v>614</v>
       </c>
       <c r="C103" s="1" t="n">
-        <v>44072</v>
+        <v>44075</v>
       </c>
       <c r="D103" t="s">
-        <v>614</v>
+        <v>615</v>
       </c>
       <c r="E103" t="s">
         <v>125</v>
       </c>
       <c r="F103"/>
       <c r="G103" t="n">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="H103" t="n">
-        <v>171237</v>
+        <v>175080</v>
       </c>
       <c r="I103" t="n">
-        <v>49.295</v>
+        <v>50.401</v>
       </c>
       <c r="J103" t="n">
-        <v>3521</v>
+        <v>1893</v>
       </c>
       <c r="K103" t="n">
-        <v>1.014</v>
+        <v>0.545</v>
       </c>
       <c r="L103" t="n">
-        <v>1791</v>
+        <v>1707</v>
       </c>
       <c r="M103" t="n">
-        <v>0.516</v>
+        <v>0.491</v>
       </c>
       <c r="N103" t="n">
-        <v>0.003</v>
+        <v>0.005</v>
       </c>
       <c r="O103" t="n">
-        <v>313.425</v>
+        <v>192.726</v>
       </c>
       <c r="P103" t="s">
         <v>125</v>
       </c>
       <c r="Q103" t="s">
-        <v>615</v>
+        <v>616</v>
       </c>
       <c r="R103" t="s">
         <v>27</v>
       </c>
       <c r="S103" t="s">
-        <v>616</v>
+        <v>617</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="s">
-        <v>617</v>
+        <v>618</v>
       </c>
       <c r="B104" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
       <c r="C104" s="1" t="n">
         <v>43950</v>
       </c>
       <c r="D104" t="s">
-        <v>619</v>
+        <v>620</v>
       </c>
       <c r="E104" t="s">
-        <v>620</v>
+        <v>621</v>
       </c>
       <c r="F104"/>
       <c r="G104" t="n">
@@ -8398,33 +8395,33 @@
         <v>38171</v>
       </c>
       <c r="P104" t="s">
-        <v>620</v>
+        <v>621</v>
       </c>
       <c r="Q104" t="s">
-        <v>621</v>
+        <v>622</v>
       </c>
       <c r="R104" t="s">
         <v>54</v>
       </c>
       <c r="S104" t="s">
-        <v>622</v>
+        <v>623</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="s">
-        <v>623</v>
+        <v>624</v>
       </c>
       <c r="B105" t="s">
-        <v>624</v>
+        <v>625</v>
       </c>
       <c r="C105" s="1" t="n">
         <v>44071</v>
       </c>
       <c r="D105" t="s">
-        <v>625</v>
+        <v>626</v>
       </c>
       <c r="E105" t="s">
-        <v>626</v>
+        <v>627</v>
       </c>
       <c r="F105"/>
       <c r="G105" t="n">
@@ -8455,16 +8452,16 @@
         <v>13.846</v>
       </c>
       <c r="P105" t="s">
-        <v>626</v>
+        <v>627</v>
       </c>
       <c r="Q105" t="s">
-        <v>627</v>
+        <v>628</v>
       </c>
       <c r="R105" t="s">
         <v>27</v>
       </c>
       <c r="S105" t="s">
-        <v>628</v>
+        <v>629</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated testing data for 2020-09-07
</commit_message>
<xml_diff>
--- a/public/data/testing/covid-testing-latest-data-source-details.xlsx
+++ b/public/data/testing/covid-testing-latest-data-source-details.xlsx
@@ -1839,7 +1839,7 @@
     <t xml:space="preserve">Spain - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.mscbs.gob.es/profesionales/saludPublica/ccayes/alertasActual/nCov/documentos/COVID-19_pruebas_diagnosticas_27_08_2020.pdf</t>
+    <t xml:space="preserve">https://www.mscbs.gob.es/profesionales/saludPublica/ccayes/alertasActual/nCov/documentos/COVID-19_pruebas_diagnosticas_03_09_2020.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">Ministry of Health, Consumption and Social Welfare</t>
@@ -7499,7 +7499,7 @@
         <v>528</v>
       </c>
       <c r="C88" s="1" t="n">
-        <v>44070</v>
+        <v>44077</v>
       </c>
       <c r="D88" t="s">
         <v>529</v>
@@ -7509,27 +7509,27 @@
       </c>
       <c r="F88"/>
       <c r="G88" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H88" t="n">
-        <v>6416533</v>
+        <v>7042795</v>
       </c>
       <c r="I88" t="n">
-        <v>137.238</v>
+        <v>150.633</v>
       </c>
       <c r="J88"/>
       <c r="K88"/>
       <c r="L88" t="n">
-        <v>80942</v>
+        <v>89466</v>
       </c>
       <c r="M88" t="n">
-        <v>1.731</v>
+        <v>1.914</v>
       </c>
       <c r="N88" t="n">
-        <v>0.091</v>
+        <v>0.094</v>
       </c>
       <c r="O88" t="n">
-        <v>10.98</v>
+        <v>10.614</v>
       </c>
       <c r="P88" t="s">
         <v>531</v>

</xml_diff>

<commit_message>
Updated testing data for 2020-09-11
</commit_message>
<xml_diff>
--- a/public/data/testing/covid-testing-latest-data-source-details.xlsx
+++ b/public/data/testing/covid-testing-latest-data-source-details.xlsx
@@ -495,7 +495,7 @@
     <t xml:space="preserve">Denmark - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://files.ssi.dk/Data-Epidemiologiske-Rapport-10092020-77gf</t>
+    <t xml:space="preserve">https://files.ssi.dk/Data-epidemiologisk-rapport-11092020-1lyn</t>
   </si>
   <si>
     <t xml:space="preserve">Statens Serum Institut</t>
@@ -513,7 +513,7 @@
     <t xml:space="preserve">Dominican Republic - samples tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.msp.gob.do/web/wp-content/uploads/2020/09/Boletín-Especial-173.pdf</t>
+    <t xml:space="preserve">https://www.msp.gob.do/web/wp-content/uploads/2020/09/Boletín-Especial-174.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">Ministry of Public Health and Social Assistance</t>
@@ -558,7 +558,7 @@
     <t xml:space="preserve">El Salvador - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.facebook.com/nayibbukele/posts/3228038390615663</t>
+    <t xml:space="preserve">https://covid-19-gis-hub-el-salvador-esri-sv.hub.arcgis.com/</t>
   </si>
   <si>
     <t xml:space="preserve">Government of El Salvador</t>
@@ -567,8 +567,8 @@
     <t xml:space="preserve">https://covid19.gob.sv/</t>
   </si>
   <si>
-    <t xml:space="preserve">The government of El Salvador publishes an online dashboard that reports the number of tests performed ("pruebas COVID19 realizadas hasta hoy"). No information is given on the geographical scope and number of labs included.
-The official dashboard only provides a daily snapshot of the number of tests performed today, making it difficult to construct a historical time series. We construct a daily time series dating back to 10 April 2020 of the cumulative number of tests performed using data posted on President Nayib Bukele's [official Facebook page](https://www.facebook.com/nayibbukele), which match the daily snapshot figures reported in the official dashboard.
+    <t xml:space="preserve">The Government of El Salvador publishes an online dashboard that reports the cumulative number of tests performed to date ("pruebas COVID19 realizadas hasta hoy").
+The official dashboard only provides a snapshot of the cumulative number of tests performed as of today, making it difficult to construct a historical time series. We construct a daily time series dating back to 10 April 2020 using the figures reported in [this unofficial dashboard](https://covid-19-gis-hub-el-salvador-esri-sv.hub.arcgis.com/), supplemented by figures reported on President Nayib Bukele's [official Facebook page](https://www.facebook.com/nayibbukele). We have cross-checked a sample of unofficial figures against figures reported on the President's Facebook page.
 Note that, due to the way the data is presented by the official source, the time series may be impacted by retrospective revisions made by the source – see our [FAQ here](https://ourworldindata.org/coronavirus-testing#does-your-data-reflect-retrospective-updates-made-by-the-source).</t>
   </si>
   <si>
@@ -774,7 +774,7 @@
     <t xml:space="preserve">Greece - samples tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://eody.gov.gr/covid-gr-daily-report-10-09-20/</t>
+    <t xml:space="preserve">https://eody.gov.gr/covid-gr-daily-report-11-09-2020/</t>
   </si>
   <si>
     <t xml:space="preserve">National Organization of Public Health</t>
@@ -1556,7 +1556,7 @@
     <t xml:space="preserve">Philippines - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://drive.google.com/drive/folders/1OodGYxPVA7GNASFrFWV2JCbntw4Ftorw?usp=sharing</t>
+    <t xml:space="preserve">https://drive.google.com/drive/folders/1skFOAw2L0sTwfnCPtIrGBdewza7mZ6-7?usp=sharing</t>
   </si>
   <si>
     <t xml:space="preserve">Philippines Department of Health</t>
@@ -2002,7 +2002,7 @@
     <t xml:space="preserve">Thailand - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://ddc.moph.go.th/viralpneumonia/file/situation/situation-no251-100963n.pdf</t>
+    <t xml:space="preserve">https://ddc.moph.go.th/viralpneumonia/file/situation/situation-no252-110963.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">Department of Disease Control</t>
@@ -3816,7 +3816,7 @@
         <v>141</v>
       </c>
       <c r="C22" s="1" t="n">
-        <v>44083</v>
+        <v>44084</v>
       </c>
       <c r="D22" t="s">
         <v>142</v>
@@ -3826,31 +3826,31 @@
       </c>
       <c r="F22"/>
       <c r="G22" t="n">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="H22" t="n">
-        <v>2784148</v>
+        <v>2830499</v>
       </c>
       <c r="I22" t="n">
-        <v>480.672</v>
+        <v>488.674</v>
       </c>
       <c r="J22" t="n">
-        <v>6609</v>
+        <v>6925</v>
       </c>
       <c r="K22" t="n">
-        <v>1.141</v>
+        <v>1.196</v>
       </c>
       <c r="L22" t="n">
-        <v>31770</v>
+        <v>32848</v>
       </c>
       <c r="M22" t="n">
-        <v>5.485</v>
+        <v>5.671</v>
       </c>
       <c r="N22" t="n">
         <v>0.006</v>
       </c>
       <c r="O22" t="n">
-        <v>174.835</v>
+        <v>162.844</v>
       </c>
       <c r="P22" t="s">
         <v>143</v>
@@ -3873,7 +3873,7 @@
         <v>147</v>
       </c>
       <c r="C23" s="1" t="n">
-        <v>44081</v>
+        <v>44082</v>
       </c>
       <c r="D23" t="s">
         <v>148</v>
@@ -3883,31 +3883,31 @@
       </c>
       <c r="F23"/>
       <c r="G23" t="n">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="H23" t="n">
-        <v>400138</v>
+        <v>403755</v>
       </c>
       <c r="I23" t="n">
-        <v>36.886</v>
+        <v>37.22</v>
       </c>
       <c r="J23" t="n">
-        <v>2493</v>
+        <v>3617</v>
       </c>
       <c r="K23" t="n">
-        <v>0.23</v>
+        <v>0.333</v>
       </c>
       <c r="L23" t="n">
-        <v>3877</v>
+        <v>3948</v>
       </c>
       <c r="M23" t="n">
-        <v>0.357</v>
+        <v>0.364</v>
       </c>
       <c r="N23" t="n">
         <v>0.188</v>
       </c>
       <c r="O23" t="n">
-        <v>5.33</v>
+        <v>5.332</v>
       </c>
       <c r="P23" t="s">
         <v>149</v>
@@ -4073,10 +4073,10 @@
         <v>1.233</v>
       </c>
       <c r="N26" t="n">
-        <v>0.016</v>
+        <v>0.015</v>
       </c>
       <c r="O26" t="n">
-        <v>61.865</v>
+        <v>67.324</v>
       </c>
       <c r="P26" t="s">
         <v>169</v>
@@ -4503,24 +4503,24 @@
         <v>165</v>
       </c>
       <c r="H34" t="n">
-        <v>1082401</v>
+        <v>1094354</v>
       </c>
       <c r="I34" t="n">
-        <v>103.847</v>
+        <v>104.994</v>
       </c>
       <c r="J34"/>
       <c r="K34"/>
       <c r="L34" t="n">
-        <v>12078</v>
+        <v>13786</v>
       </c>
       <c r="M34" t="n">
-        <v>1.159</v>
+        <v>1.323</v>
       </c>
       <c r="N34" t="n">
-        <v>0.017</v>
+        <v>0.015</v>
       </c>
       <c r="O34" t="n">
-        <v>58.147</v>
+        <v>66.37</v>
       </c>
       <c r="P34" t="s">
         <v>219</v>
@@ -4651,7 +4651,7 @@
         <v>238</v>
       </c>
       <c r="C37" s="1" t="n">
-        <v>44083</v>
+        <v>44084</v>
       </c>
       <c r="D37" t="s">
         <v>239</v>
@@ -4661,31 +4661,31 @@
       </c>
       <c r="F37"/>
       <c r="G37" t="n">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="H37" t="n">
-        <v>94923</v>
+        <v>95485</v>
       </c>
       <c r="I37" t="n">
-        <v>278.163</v>
+        <v>279.81</v>
       </c>
       <c r="J37" t="n">
-        <v>524</v>
+        <v>562</v>
       </c>
       <c r="K37" t="n">
-        <v>1.536</v>
+        <v>1.647</v>
       </c>
       <c r="L37" t="n">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="M37" t="n">
-        <v>1.524</v>
+        <v>1.527</v>
       </c>
       <c r="N37" t="n">
         <v>0.009</v>
       </c>
       <c r="O37" t="n">
-        <v>107.059</v>
+        <v>113.969</v>
       </c>
       <c r="P37" t="s">
         <v>240</v>
@@ -5111,7 +5111,7 @@
         <v>280</v>
       </c>
       <c r="C45" s="1" t="n">
-        <v>44084</v>
+        <v>44085</v>
       </c>
       <c r="D45" t="s">
         <v>281</v>
@@ -5123,31 +5123,31 @@
         <v>283</v>
       </c>
       <c r="G45" t="n">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="H45" t="n">
-        <v>5757488</v>
+        <v>5818910</v>
       </c>
       <c r="I45" t="n">
-        <v>95.225</v>
+        <v>96.241</v>
       </c>
       <c r="J45" t="n">
-        <v>57779</v>
+        <v>61422</v>
       </c>
       <c r="K45" t="n">
-        <v>0.956</v>
+        <v>1.016</v>
       </c>
       <c r="L45" t="n">
-        <v>59334</v>
+        <v>57743</v>
       </c>
       <c r="M45" t="n">
-        <v>0.981</v>
+        <v>0.955</v>
       </c>
       <c r="N45" t="n">
         <v>0.025</v>
       </c>
       <c r="O45" t="n">
-        <v>40.176</v>
+        <v>39.365</v>
       </c>
       <c r="P45" t="s">
         <v>284</v>
@@ -5170,7 +5170,7 @@
         <v>287</v>
       </c>
       <c r="C46" s="1" t="n">
-        <v>44084</v>
+        <v>44085</v>
       </c>
       <c r="D46" t="s">
         <v>281</v>
@@ -5182,31 +5182,31 @@
         <v>283</v>
       </c>
       <c r="G46" t="n">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="H46" t="n">
-        <v>9554389</v>
+        <v>9653269</v>
       </c>
       <c r="I46" t="n">
-        <v>158.023</v>
+        <v>159.659</v>
       </c>
       <c r="J46" t="n">
-        <v>94186</v>
+        <v>98880</v>
       </c>
       <c r="K46" t="n">
-        <v>1.558</v>
+        <v>1.635</v>
       </c>
       <c r="L46" t="n">
-        <v>90390</v>
+        <v>88361</v>
       </c>
       <c r="M46" t="n">
-        <v>1.495</v>
+        <v>1.461</v>
       </c>
       <c r="N46" t="n">
-        <v>0.016</v>
+        <v>0.017</v>
       </c>
       <c r="O46" t="n">
-        <v>61.204</v>
+        <v>60.238</v>
       </c>
       <c r="P46" t="s">
         <v>284</v>
@@ -5634,7 +5634,7 @@
         <v>329</v>
       </c>
       <c r="C54" s="1" t="n">
-        <v>44083</v>
+        <v>44084</v>
       </c>
       <c r="D54" t="s">
         <v>330</v>
@@ -5644,31 +5644,31 @@
       </c>
       <c r="F54"/>
       <c r="G54" t="n">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="H54" t="n">
-        <v>402681</v>
+        <v>404766</v>
       </c>
       <c r="I54" t="n">
-        <v>643.285</v>
+        <v>646.616</v>
       </c>
       <c r="J54" t="n">
-        <v>1865</v>
+        <v>2085</v>
       </c>
       <c r="K54" t="n">
-        <v>2.979</v>
+        <v>3.331</v>
       </c>
       <c r="L54" t="n">
-        <v>1747</v>
+        <v>1755</v>
       </c>
       <c r="M54" t="n">
-        <v>2.791</v>
+        <v>2.804</v>
       </c>
       <c r="N54" t="n">
-        <v>0.024</v>
+        <v>0.023</v>
       </c>
       <c r="O54" t="n">
-        <v>41.175</v>
+        <v>44.191</v>
       </c>
       <c r="P54" t="s">
         <v>331</v>
@@ -6373,7 +6373,7 @@
         <v>410</v>
       </c>
       <c r="C67" s="1" t="n">
-        <v>44082</v>
+        <v>44083</v>
       </c>
       <c r="D67" t="s">
         <v>411</v>
@@ -6383,31 +6383,31 @@
       </c>
       <c r="F67"/>
       <c r="G67" t="n">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="H67" t="n">
-        <v>823471</v>
+        <v>838251</v>
       </c>
       <c r="I67" t="n">
-        <v>151.897</v>
+        <v>154.623</v>
       </c>
       <c r="J67" t="n">
-        <v>10828</v>
+        <v>10823</v>
       </c>
       <c r="K67" t="n">
-        <v>1.997</v>
+        <v>1.996</v>
       </c>
       <c r="L67" t="n">
-        <v>11109</v>
+        <v>11019</v>
       </c>
       <c r="M67" t="n">
-        <v>2.049</v>
+        <v>2.033</v>
       </c>
       <c r="N67" t="n">
         <v>0.01</v>
       </c>
       <c r="O67" t="n">
-        <v>104.661</v>
+        <v>104.8</v>
       </c>
       <c r="P67" t="s">
         <v>412</v>
@@ -6699,7 +6699,7 @@
         <v>446</v>
       </c>
       <c r="C73" s="1" t="n">
-        <v>44083</v>
+        <v>44084</v>
       </c>
       <c r="D73" t="s">
         <v>447</v>
@@ -6709,31 +6709,31 @@
       </c>
       <c r="F73"/>
       <c r="G73" t="n">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="H73" t="n">
-        <v>2776698</v>
+        <v>2823879</v>
       </c>
       <c r="I73" t="n">
-        <v>25.339</v>
+        <v>25.77</v>
       </c>
       <c r="J73" t="n">
-        <v>28421</v>
+        <v>38573</v>
       </c>
       <c r="K73" t="n">
-        <v>0.259</v>
+        <v>0.352</v>
       </c>
       <c r="L73" t="n">
-        <v>33518</v>
+        <v>34986</v>
       </c>
       <c r="M73" t="n">
-        <v>0.306</v>
+        <v>0.319</v>
       </c>
       <c r="N73" t="n">
         <v>0.076</v>
       </c>
       <c r="O73" t="n">
-        <v>13.239</v>
+        <v>13.094</v>
       </c>
       <c r="P73" t="s">
         <v>225</v>
@@ -6870,7 +6870,7 @@
         <v>460</v>
       </c>
       <c r="C76" s="1" t="n">
-        <v>44080</v>
+        <v>44083</v>
       </c>
       <c r="D76" t="s">
         <v>461</v>
@@ -6880,31 +6880,31 @@
       </c>
       <c r="F76"/>
       <c r="G76" t="n">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="H76" t="n">
-        <v>2153615</v>
+        <v>2210452</v>
       </c>
       <c r="I76" t="n">
-        <v>211.207</v>
+        <v>216.781</v>
       </c>
       <c r="J76" t="n">
-        <v>9634</v>
+        <v>21332</v>
       </c>
       <c r="K76" t="n">
-        <v>0.945</v>
+        <v>2.092</v>
       </c>
       <c r="L76" t="n">
-        <v>15654</v>
+        <v>16342</v>
       </c>
       <c r="M76" t="n">
-        <v>1.535</v>
+        <v>1.603</v>
       </c>
       <c r="N76" t="n">
         <v>0.023</v>
       </c>
       <c r="O76" t="n">
-        <v>43.919</v>
+        <v>43.135</v>
       </c>
       <c r="P76" t="s">
         <v>462</v>
@@ -7886,7 +7886,7 @@
         <v>564</v>
       </c>
       <c r="C94" s="1" t="n">
-        <v>44083</v>
+        <v>44084</v>
       </c>
       <c r="D94" t="s">
         <v>565</v>
@@ -7896,31 +7896,31 @@
       </c>
       <c r="F94"/>
       <c r="G94" t="n">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="H94" t="n">
-        <v>1145949</v>
+        <v>1162236</v>
       </c>
       <c r="I94" t="n">
-        <v>132.409</v>
+        <v>134.291</v>
       </c>
       <c r="J94" t="n">
-        <v>10490</v>
+        <v>11139</v>
       </c>
       <c r="K94" t="n">
-        <v>1.212</v>
+        <v>1.287</v>
       </c>
       <c r="L94" t="n">
-        <v>12097</v>
+        <v>12203</v>
       </c>
       <c r="M94" t="n">
-        <v>1.398</v>
+        <v>1.41</v>
       </c>
       <c r="N94" t="n">
-        <v>0.029</v>
+        <v>0.03</v>
       </c>
       <c r="O94" t="n">
-        <v>34.648</v>
+        <v>33.604</v>
       </c>
       <c r="P94" t="s">
         <v>566</v>
@@ -8000,7 +8000,7 @@
         <v>576</v>
       </c>
       <c r="C96" s="1" t="n">
-        <v>44084</v>
+        <v>44085</v>
       </c>
       <c r="D96" t="s">
         <v>577</v>
@@ -8010,22 +8010,22 @@
       </c>
       <c r="F96"/>
       <c r="G96" t="n">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="H96" t="n">
-        <v>429062</v>
+        <v>430235</v>
       </c>
       <c r="I96" t="n">
-        <v>6.147</v>
+        <v>6.164</v>
       </c>
       <c r="J96" t="n">
-        <v>1072</v>
+        <v>1173</v>
       </c>
       <c r="K96" t="n">
-        <v>0.015</v>
+        <v>0.017</v>
       </c>
       <c r="L96" t="n">
-        <v>959</v>
+        <v>983</v>
       </c>
       <c r="M96" t="n">
         <v>0.014</v>
@@ -8034,7 +8034,7 @@
         <v>0.004</v>
       </c>
       <c r="O96" t="n">
-        <v>248.63</v>
+        <v>229.367</v>
       </c>
       <c r="P96" t="s">
         <v>578</v>
@@ -8057,7 +8057,7 @@
         <v>581</v>
       </c>
       <c r="C97" s="1" t="n">
-        <v>44084</v>
+        <v>44085</v>
       </c>
       <c r="D97" t="s">
         <v>577</v>
@@ -8067,22 +8067,22 @@
       </c>
       <c r="F97"/>
       <c r="G97" t="n">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="H97" t="n">
-        <v>856472</v>
+        <v>857645</v>
       </c>
       <c r="I97" t="n">
-        <v>12.27</v>
+        <v>12.287</v>
       </c>
       <c r="J97" t="n">
-        <v>1072</v>
+        <v>1173</v>
       </c>
       <c r="K97" t="n">
-        <v>0.015</v>
+        <v>0.017</v>
       </c>
       <c r="L97" t="n">
-        <v>959</v>
+        <v>983</v>
       </c>
       <c r="M97" t="n">
         <v>0.014</v>
@@ -8091,7 +8091,7 @@
         <v>0.004</v>
       </c>
       <c r="O97" t="n">
-        <v>248.63</v>
+        <v>229.367</v>
       </c>
       <c r="P97" t="s">
         <v>578</v>
@@ -8338,7 +8338,7 @@
         <v>606</v>
       </c>
       <c r="C102" s="1" t="n">
-        <v>44084</v>
+        <v>44085</v>
       </c>
       <c r="D102" t="s">
         <v>607</v>
@@ -8348,31 +8348,31 @@
       </c>
       <c r="F102"/>
       <c r="G102" t="n">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="H102" t="n">
-        <v>1778483</v>
+        <v>1806428</v>
       </c>
       <c r="I102" t="n">
-        <v>40.666</v>
+        <v>41.305</v>
       </c>
       <c r="J102" t="n">
-        <v>26552</v>
+        <v>27945</v>
       </c>
       <c r="K102" t="n">
-        <v>0.607</v>
+        <v>0.639</v>
       </c>
       <c r="L102" t="n">
-        <v>22398</v>
+        <v>22703</v>
       </c>
       <c r="M102" t="n">
-        <v>0.512</v>
+        <v>0.519</v>
       </c>
       <c r="N102" t="n">
-        <v>0.126</v>
+        <v>0.129</v>
       </c>
       <c r="O102" t="n">
-        <v>7.909</v>
+        <v>7.742</v>
       </c>
       <c r="P102" t="s">
         <v>608</v>
@@ -8452,7 +8452,7 @@
         <v>617</v>
       </c>
       <c r="C104" s="1" t="n">
-        <v>44076</v>
+        <v>44084</v>
       </c>
       <c r="D104" t="s">
         <v>618</v>
@@ -8464,31 +8464,31 @@
         <v>620</v>
       </c>
       <c r="G104" t="n">
-        <v>155</v>
+        <v>163</v>
       </c>
       <c r="H104" t="n">
-        <v>14653196</v>
+        <v>16145887</v>
       </c>
       <c r="I104" t="n">
-        <v>215.85</v>
+        <v>237.838</v>
       </c>
       <c r="J104" t="n">
-        <v>164358</v>
+        <v>205659</v>
       </c>
       <c r="K104" t="n">
-        <v>2.421</v>
+        <v>3.029</v>
       </c>
       <c r="L104" t="n">
-        <v>172233</v>
+        <v>187241</v>
       </c>
       <c r="M104" t="n">
-        <v>2.537</v>
+        <v>2.758</v>
       </c>
       <c r="N104" t="n">
-        <v>0.008</v>
+        <v>0.013</v>
       </c>
       <c r="O104" t="n">
-        <v>128.669</v>
+        <v>79.229</v>
       </c>
       <c r="P104" t="s">
         <v>619</v>
@@ -8731,7 +8731,7 @@
         <v>649</v>
       </c>
       <c r="C109" s="1" t="n">
-        <v>44084</v>
+        <v>44085</v>
       </c>
       <c r="D109" t="s">
         <v>650</v>
@@ -8741,31 +8741,31 @@
       </c>
       <c r="F109"/>
       <c r="G109" t="n">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="H109" t="n">
-        <v>127529</v>
+        <v>128662</v>
       </c>
       <c r="I109" t="n">
-        <v>6.937</v>
+        <v>6.999</v>
       </c>
       <c r="J109" t="n">
-        <v>1391</v>
+        <v>1133</v>
       </c>
       <c r="K109" t="n">
-        <v>0.076</v>
+        <v>0.062</v>
       </c>
       <c r="L109" t="n">
-        <v>1137</v>
+        <v>1099</v>
       </c>
       <c r="M109" t="n">
-        <v>0.062</v>
+        <v>0.06</v>
       </c>
       <c r="N109" t="n">
-        <v>0.088</v>
+        <v>0.09</v>
       </c>
       <c r="O109" t="n">
-        <v>11.419</v>
+        <v>11.133</v>
       </c>
       <c r="P109" t="s">
         <v>652</v>

</xml_diff>

<commit_message>
Updated testing data for 2020-09-18
</commit_message>
<xml_diff>
--- a/public/data/testing/covid-testing-latest-data-source-details.xlsx
+++ b/public/data/testing/covid-testing-latest-data-source-details.xlsx
@@ -110,7 +110,7 @@
     <t xml:space="preserve">Australia - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.health.gov.au/sites/default/files/documents/2020/09/coronavirus-covid-19-at-a-glance-15-september-2020.pdf</t>
+    <t xml:space="preserve">https://www.health.gov.au/sites/default/files/documents/2020/09/coronavirus-covid-19-at-a-glance-17-september-2020.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">Australian Government Department of Health</t>
@@ -202,7 +202,7 @@
     <t xml:space="preserve">Belarus - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">http://minzdrav.gov.by/ru/sobytiya/u-belarusi-na-14-verasnya-vypisanyya-72-tys-609-patsyenta/</t>
+    <t xml:space="preserve">http://minzdrav.gov.by/ru/sobytiya/u-belarusi-na-16-verasnya-vypisanyya-72-tys-810-patsyenta/</t>
   </si>
   <si>
     <t xml:space="preserve">Belarus Ministry of Health</t>
@@ -245,7 +245,7 @@
     <t xml:space="preserve">Bolivia - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://minsalud.gob.bo/4614-covid-19-se-reportan-828-contagios-nuevos-y-50-decesos</t>
+    <t xml:space="preserve">https://minsalud.gob.bo/4618-bolivia-acumula-87-031-pacientes-recuperados-de-coronavirus-en-una-jornada-con-586-nuevos-contagios</t>
   </si>
   <si>
     <t xml:space="preserve">https://www.minsalud.gob.bo/</t>
@@ -399,7 +399,7 @@
     <t xml:space="preserve">Cote d'Ivoire - samples tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.facebook.com/Mshpci/posts/1698559853643035</t>
+    <t xml:space="preserve">https://www.facebook.com/Mshpci/posts/1700436123455408</t>
   </si>
   <si>
     <t xml:space="preserve">Ministry of Health and Public Hygiene</t>
@@ -478,7 +478,7 @@
     <t xml:space="preserve">Democratic Republic of Congo - samples tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/CMR_Covid19_RDC/status/1305842562977103876/photo/1</t>
+    <t xml:space="preserve">https://twitter.com/CMR_Covid19_RDC/status/1306605705252700166/photo/1</t>
   </si>
   <si>
     <t xml:space="preserve">DRC COVID-19 Pandemic Response Multisectoral Committee</t>
@@ -496,7 +496,7 @@
     <t xml:space="preserve">Denmark - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://files.ssi.dk/Data-Epidemiologiske-Rapport-15092020-f22p</t>
+    <t xml:space="preserve">https://files.ssi.dk/Data-epidemiologisk-rapport-17092020-fil1</t>
   </si>
   <si>
     <t xml:space="preserve">Statens Serum Institut</t>
@@ -533,7 +533,7 @@
     <t xml:space="preserve">Ecuador - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.gestionderiesgos.gob.ec/wp-content/uploads/2020/09/INFOGRAFIA-NACIONALCOVID19-COE-NACIONAL-08h00-15092020-ALM.pdf</t>
+    <t xml:space="preserve">https://www.gestionderiesgos.gob.ec/wp-content/uploads/2020/09/INFOGRAFIA-NACIONALCOVID19-COE-NACIONAL-08h00-17092020-5.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">Government of Ecuador</t>
@@ -603,7 +603,7 @@
     <t xml:space="preserve">Ethiopia - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/EPHIEthiopia/status/1305181115477643266</t>
+    <t xml:space="preserve">https://twitter.com/EPHIEthiopia/status/1306640280741974017</t>
   </si>
   <si>
     <t xml:space="preserve">Ethiopian Public Health Institute</t>
@@ -696,7 +696,7 @@
     <t xml:space="preserve">Germany - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.rki.de/DE/Content/InfAZ/N/Neuartiges_Coronavirus/Situationsberichte/Sept_2020/2020-09-09-de.pdf?__blob=publicationFile</t>
+    <t xml:space="preserve">https://www.rki.de/DE/Content/InfAZ/N/Neuartiges_Coronavirus/Situationsberichte/Sept_2020/2020-09-16-de.pdf?__blob=publicationFile</t>
   </si>
   <si>
     <t xml:space="preserve">Robert Koch Institut</t>
@@ -712,8 +712,9 @@
   </si>
   <si>
     <t xml:space="preserve">To determine how many laboratory tests regarding SARS-CoV-2 are carried out per calendar week in Germany and how many tests are positive or negative, the RKI has started a Germany-wide laboratory query. However, the number of laboratories reporting data seems to vary from week to week.
-The report published on 9 September 2020 states that “from the beginning of the collection up to and including calendar week 36/2020”:
-– The cumulative total of samples tested was 13,436,301;
+The report published on 16 September 2020 states that “from the beginning of the collection up to and including calendar week 37/2020”:
+– The cumulative total of samples tested was 14,557,136;
+- For calendar week 37 (which ends 13 September), 185 labs reported 1,120,835 samples tested;
 - For calendar week 36 (which ends 6 September), 180 labs reported 1,051,125 samples tested;
 - For calendar week 35 (which ends 30 August), 181 labs reported 1,101,299 samples tested;
 - For calendar week 34 (which ends 23 August), 196 labs reported 1,055,662 samples tested;
@@ -775,7 +776,7 @@
     <t xml:space="preserve">Greece - samples tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://eody.gov.gr/covid-daily-report-14-09-2020-1/</t>
+    <t xml:space="preserve">https://eody.gov.gr/covid-gr-daily-report-17-09-2020/</t>
   </si>
   <si>
     <t xml:space="preserve">National Organization of Public Health</t>
@@ -914,7 +915,7 @@
     <t xml:space="preserve">Iran - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">http://irangov.ir/detail/347120</t>
+    <t xml:space="preserve">http://irangov.ir/detail/347255</t>
   </si>
   <si>
     <t xml:space="preserve">Government of Iran</t>
@@ -934,7 +935,7 @@
     <t xml:space="preserve">Iraq - samples tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/MOHealth_Iraq/status/1305863011551375361/photo/1</t>
+    <t xml:space="preserve">https://twitter.com/MOHealth_Iraq/status/1306621144095752197/photo/1</t>
   </si>
   <si>
     <t xml:space="preserve">Ministry of Health and Environment</t>
@@ -976,7 +977,7 @@
     <t xml:space="preserve">Israel - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://govextra.gov.il/media/26905/covid19-data-israel-08092020.csv</t>
+    <t xml:space="preserve">https://govextra.gov.il/media/27002/covid19-data-israel-11092020.csv</t>
   </si>
   <si>
     <t xml:space="preserve">Israel Ministry of Health</t>
@@ -1035,7 +1036,7 @@
     <t xml:space="preserve">Japan - people tested (incl. non-PCR)</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.mhlw.go.jp/stf/newpage_13592.html</t>
+    <t xml:space="preserve">https://www.mhlw.go.jp/stf/newpage_13640.html</t>
   </si>
   <si>
     <t xml:space="preserve">Ministry of Health, Labor and Welfare Press Release</t>
@@ -1060,7 +1061,7 @@
     <t xml:space="preserve">Japan - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.mhlw.go.jp/content/10906000/000672488.pdf</t>
+    <t xml:space="preserve">https://www.mhlw.go.jp/content/10906000/000673391.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">The cumulative total reported in the press release matches the cumulative total calculated from the weekly and daily figures reported by the MOH.</t>
@@ -1139,7 +1140,7 @@
     <t xml:space="preserve">Kuwait - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/KUWAIT_MOH/status/1305846355638857728/photo/1</t>
+    <t xml:space="preserve">https://twitter.com/KUWAIT_MOH/status/1306556031540105216/photo/1</t>
   </si>
   <si>
     <t xml:space="preserve">Kuwait Ministry of Health</t>
@@ -1225,7 +1226,7 @@
     <t xml:space="preserve">Malawi - samples tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://malawipublichealth.org/index.php/resources/COVID-19%20SitRep%20Updates/September%202020/20200913_Malawi%20COVID-19%20situation%20report.pdf/download</t>
+    <t xml:space="preserve">https://malawipublichealth.org/index.php/resources/COVID-19%20SitRep%20Updates/September%202020/20200916_Malawi%20COVID-19%20situation%20report.pdf/download</t>
   </si>
   <si>
     <t xml:space="preserve">Public Health Institute of Malawi</t>
@@ -1244,7 +1245,7 @@
     <t xml:space="preserve">Malaysia - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">http://covid-19.moh.gov.my/terkini/092020/situasi-terkini-15-september-2020</t>
+    <t xml:space="preserve">http://covid-19.moh.gov.my/terkini/092020/situasi-terkini-17-september-2020</t>
   </si>
   <si>
     <t xml:space="preserve">Ministry of Health Malaysia</t>
@@ -1270,7 +1271,7 @@
     <t xml:space="preserve">Maldives - samples tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/HPA_MV/status/1305553559556165633</t>
+    <t xml:space="preserve">https://twitter.com/HPA_MV/status/1306278303028916226/photo/1</t>
   </si>
   <si>
     <t xml:space="preserve">Maldives Health Protection Agency</t>
@@ -1336,7 +1337,7 @@
     <t xml:space="preserve">Morocco - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/Ministere_Sante/status/1305553857481781250/photo/1</t>
+    <t xml:space="preserve">https://twitter.com/Ministere_Sante/status/1306278175211745280/photo/1</t>
   </si>
   <si>
     <t xml:space="preserve">Morocco Ministry of Health</t>
@@ -1356,7 +1357,7 @@
     <t xml:space="preserve">Mozambique - units unclear</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.misau.gov.mz/index.php/covid-19-boletins-diarios?download=609:boletim-diario-covid-n-182</t>
+    <t xml:space="preserve">https://www.misau.gov.mz/index.php/covid-19-boletins-diarios?download=614:boletim-diario-covid-n-184</t>
   </si>
   <si>
     <t xml:space="preserve">Mozambique Ministry of Health</t>
@@ -1399,7 +1400,7 @@
     <t xml:space="preserve">Nepal - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://drive.google.com/drive/folders/1S7mzBdZrxwfOtkfRZxPF5RzLCau2MfoO</t>
+    <t xml:space="preserve">https://drive.google.com/drive/folders/1DyALDeJ6etkj4yQGxQz3dQA2-WyK1kwM</t>
   </si>
   <si>
     <t xml:space="preserve">Ministry of Health and Population</t>
@@ -1419,7 +1420,7 @@
     <t xml:space="preserve">Netherlands - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.rivm.nl/sites/default/files/2020-09/COVID-19_WebSite_rapport_wekelijks_20200908_1159_0.pdf</t>
+    <t xml:space="preserve">https://www.rivm.nl/sites/default/files/2020-09/COVID-19_WebSite_rapport_wekelijks_20200915_1433_NICEedit.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">National Institute for Public Health and the Environment</t>
@@ -1543,7 +1544,7 @@
     <t xml:space="preserve">Panama - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/MINSAPma/status/1305637768949837828/photo/1</t>
+    <t xml:space="preserve">https://twitter.com/MINSAPma/status/1306364241025421316/photo/1</t>
   </si>
   <si>
     <t xml:space="preserve">Panama Ministry of Health</t>
@@ -1604,7 +1605,7 @@
     <t xml:space="preserve">Philippines - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://drive.google.com/drive/folders/1BVd5-X8E3759_0xihIXQF_swZ0YOiyi6?usp=sharing</t>
+    <t xml:space="preserve">https://drive.google.com/drive/folders/1MFv63kETEmXr86KqycuW6k11gwJ-wxt0?usp=sharing</t>
   </si>
   <si>
     <t xml:space="preserve">Philippines Department of Health</t>
@@ -1624,7 +1625,7 @@
     <t xml:space="preserve">Poland - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/MZ_GOV_PL/status/1305789702788661250</t>
+    <t xml:space="preserve">https://twitter.com/MZ_GOV_PL/status/1306514478528331781</t>
   </si>
   <si>
     <t xml:space="preserve">Poland Ministry of Health</t>
@@ -1693,7 +1694,7 @@
     <t xml:space="preserve">Romania - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://gov.ro/ro/media/comunicate/buletin-de-presa-15-septembrie-2020-ora-13-00&amp;page=1</t>
+    <t xml:space="preserve">https://gov.ro/ro/media/comunicate/buletin-de-presa-18-septembrie-2020-ora-13-00&amp;page=1</t>
   </si>
   <si>
     <t xml:space="preserve">Ministry of Internal Affairs</t>
@@ -1716,7 +1717,7 @@
     <t xml:space="preserve">Russia - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://rospotrebnadzor.ru/about/info/news/news_details.php?ELEMENT_ID=15410</t>
+    <t xml:space="preserve">https://rospotrebnadzor.ru/about/info/news/news_details.php?ELEMENT_ID=15429</t>
   </si>
   <si>
     <t xml:space="preserve">Government of the Russian Federation</t>
@@ -1736,7 +1737,7 @@
     <t xml:space="preserve">Rwanda - samples tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/RwandaHealth/status/1305218895217856512</t>
+    <t xml:space="preserve">https://twitter.com/RwandaHealth/status/1306676604601499655</t>
   </si>
   <si>
     <t xml:space="preserve">Rwanda Ministry of Health</t>
@@ -1910,7 +1911,7 @@
     <t xml:space="preserve">South Korea - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.cdc.go.kr/board/board.es?mid=&amp;bid=0030&amp;act=view&amp;list_no=368402&amp;tag=&amp;nPage=1</t>
+    <t xml:space="preserve">https://www.cdc.go.kr/board/board.es?mid=&amp;bid=0030&amp;act=view&amp;list_no=368427&amp;tag=&amp;nPage=1</t>
   </si>
   <si>
     <t xml:space="preserve">South Korea CDC</t>
@@ -1930,7 +1931,7 @@
     <t xml:space="preserve">Spain - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.mscbs.gob.es/profesionales/saludPublica/ccayes/alertasActual/nCov/documentos/Actualizacion_207_COVID-19.pdf</t>
+    <t xml:space="preserve">https://www.mscbs.gob.es/profesionales/saludPublica/ccayes/alertasActual/nCov/documentos/Actualizacion_209_COVID-19.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">Ministry of Health, Consumption and Social Welfare</t>
@@ -2048,7 +2049,7 @@
     <t xml:space="preserve">Thailand - people tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://ddc.moph.go.th/viralpneumonia/file/situation/situation-no256-150963.pdf</t>
+    <t xml:space="preserve">https://ddc.moph.go.th/viralpneumonia/file/situation/situation-no258-170963.pdf</t>
   </si>
   <si>
     <t xml:space="preserve">Department of Disease Control</t>
@@ -2136,7 +2137,7 @@
     <t xml:space="preserve">Uganda - samples tested</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/MinofHealthUG/status/1305858800059142144/photo/1</t>
+    <t xml:space="preserve">https://twitter.com/MinofHealthUG/status/1306550790316851200/photo/1</t>
   </si>
   <si>
     <t xml:space="preserve">Uganda Ministry of Health</t>
@@ -2223,7 +2224,7 @@
     <t xml:space="preserve">United States - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://healthdata.gov/sites/default/files/covid-19_diagnostic_lab_testing_20200914_2229.csv</t>
+    <t xml:space="preserve">https://healthdata.gov/sites/default/files/covid-19_diagnostic_lab_testing_20200918_0000.csv</t>
   </si>
   <si>
     <t xml:space="preserve">Department of Health &amp; Human Services</t>
@@ -2275,7 +2276,7 @@
     <t xml:space="preserve">Uruguay - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://www.gub.uy/ministerio-salud-publica/comunicacion/noticias/informacion-situacion-sobre-coronavirus-covid-19-uruguay-0</t>
+    <t xml:space="preserve">https://www.gub.uy/ministerio-salud-publica/comunicacion/noticias/informacion-situacion-sobre-coronavirus-covid-19-uruguay-11</t>
   </si>
   <si>
     <t xml:space="preserve">https://www.gub.uy/ministerio-salud-publica/comunicacion/noticias</t>
@@ -2335,7 +2336,7 @@
     <t xml:space="preserve">Zimbabwe - tests performed</t>
   </si>
   <si>
-    <t xml:space="preserve">https://twitter.com/MoHCCZim/status/1305564644992573447</t>
+    <t xml:space="preserve">https://twitter.com/MoHCCZim/status/1306645585802518529</t>
   </si>
   <si>
     <t xml:space="preserve">Zimbabwe Ministry of Health and Child Care</t>
@@ -2752,7 +2753,7 @@
         <v>20</v>
       </c>
       <c r="C2" s="1" t="n">
-        <v>44085</v>
+        <v>44087</v>
       </c>
       <c r="D2" t="s">
         <v>21</v>
@@ -2762,31 +2763,31 @@
       </c>
       <c r="F2"/>
       <c r="G2" t="n">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="H2" t="n">
-        <v>1369139</v>
+        <v>1403090</v>
       </c>
       <c r="I2" t="n">
-        <v>30.294</v>
+        <v>31.045</v>
       </c>
       <c r="J2" t="n">
-        <v>23199</v>
+        <v>12031</v>
       </c>
       <c r="K2" t="n">
-        <v>0.513</v>
+        <v>0.266</v>
       </c>
       <c r="L2" t="n">
-        <v>20226</v>
+        <v>20489</v>
       </c>
       <c r="M2" t="n">
-        <v>0.448</v>
+        <v>0.453</v>
       </c>
       <c r="N2" t="n">
-        <v>0.516</v>
+        <v>0.515</v>
       </c>
       <c r="O2" t="n">
-        <v>1.936</v>
+        <v>1.943</v>
       </c>
       <c r="P2" t="s">
         <v>22</v>
@@ -2809,7 +2810,7 @@
         <v>25</v>
       </c>
       <c r="C3" s="1" t="n">
-        <v>44085</v>
+        <v>44087</v>
       </c>
       <c r="D3" t="s">
         <v>26</v>
@@ -2819,25 +2820,25 @@
       </c>
       <c r="F3"/>
       <c r="G3" t="n">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="H3" t="n">
-        <v>1639697</v>
+        <v>1677881</v>
       </c>
       <c r="I3" t="n">
-        <v>36.28</v>
+        <v>37.125</v>
       </c>
       <c r="J3" t="n">
-        <v>26583</v>
+        <v>13183</v>
       </c>
       <c r="K3" t="n">
-        <v>0.588</v>
+        <v>0.292</v>
       </c>
       <c r="L3" t="n">
-        <v>23143</v>
+        <v>23369</v>
       </c>
       <c r="M3" t="n">
-        <v>0.512</v>
+        <v>0.517</v>
       </c>
       <c r="N3" t="n">
         <v>0.451</v>
@@ -2866,7 +2867,7 @@
         <v>30</v>
       </c>
       <c r="C4" s="1" t="n">
-        <v>44090</v>
+        <v>44092</v>
       </c>
       <c r="D4" t="s">
         <v>31</v>
@@ -2876,31 +2877,31 @@
       </c>
       <c r="F4"/>
       <c r="G4" t="n">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="H4" t="n">
-        <v>7076539</v>
+        <v>7178741</v>
       </c>
       <c r="I4" t="n">
-        <v>277.513</v>
+        <v>281.521</v>
       </c>
       <c r="J4" t="n">
-        <v>29503</v>
+        <v>54357</v>
       </c>
       <c r="K4" t="n">
-        <v>1.157</v>
+        <v>2.132</v>
       </c>
       <c r="L4" t="n">
-        <v>41029</v>
+        <v>39108</v>
       </c>
       <c r="M4" t="n">
-        <v>1.609</v>
+        <v>1.534</v>
       </c>
       <c r="N4" t="n">
         <v>0.001</v>
       </c>
       <c r="O4" t="n">
-        <v>789.019</v>
+        <v>912.52</v>
       </c>
       <c r="P4" t="s">
         <v>32</v>
@@ -2923,7 +2924,7 @@
         <v>36</v>
       </c>
       <c r="C5" s="1" t="n">
-        <v>44090</v>
+        <v>44092</v>
       </c>
       <c r="D5" t="s">
         <v>37</v>
@@ -2933,31 +2934,27 @@
       </c>
       <c r="F5"/>
       <c r="G5" t="n">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="H5" t="n">
-        <v>1379839</v>
+        <v>1413965</v>
       </c>
       <c r="I5" t="n">
-        <v>153.206</v>
-      </c>
-      <c r="J5" t="n">
-        <v>15331</v>
-      </c>
-      <c r="K5" t="n">
-        <v>1.702</v>
-      </c>
+        <v>156.996</v>
+      </c>
+      <c r="J5"/>
+      <c r="K5"/>
       <c r="L5" t="n">
-        <v>13111</v>
+        <v>13878</v>
       </c>
       <c r="M5" t="n">
-        <v>1.456</v>
+        <v>1.541</v>
       </c>
       <c r="N5" t="n">
-        <v>0.05</v>
+        <v>0.051</v>
       </c>
       <c r="O5" t="n">
-        <v>20.197</v>
+        <v>19.749</v>
       </c>
       <c r="P5" t="s">
         <v>39</v>
@@ -2980,7 +2977,7 @@
         <v>43</v>
       </c>
       <c r="C6" s="1" t="n">
-        <v>44089</v>
+        <v>44092</v>
       </c>
       <c r="D6" t="s">
         <v>44</v>
@@ -2990,31 +2987,27 @@
       </c>
       <c r="F6"/>
       <c r="G6" t="n">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="H6" t="n">
-        <v>1276075</v>
+        <v>1301170</v>
       </c>
       <c r="I6" t="n">
-        <v>749.934</v>
-      </c>
-      <c r="J6" t="n">
-        <v>23177</v>
-      </c>
-      <c r="K6" t="n">
-        <v>13.621</v>
-      </c>
+        <v>764.682</v>
+      </c>
+      <c r="J6"/>
+      <c r="K6"/>
       <c r="L6" t="n">
-        <v>11593</v>
+        <v>10135</v>
       </c>
       <c r="M6" t="n">
-        <v>6.813</v>
+        <v>5.956</v>
       </c>
       <c r="N6" t="n">
-        <v>0.052</v>
+        <v>0.071</v>
       </c>
       <c r="O6" t="n">
-        <v>19.18</v>
+        <v>14.093</v>
       </c>
       <c r="P6" t="s">
         <v>46</v>
@@ -3037,7 +3030,7 @@
         <v>50</v>
       </c>
       <c r="C7" s="1" t="n">
-        <v>44089</v>
+        <v>44091</v>
       </c>
       <c r="D7" t="s">
         <v>51</v>
@@ -3047,31 +3040,31 @@
       </c>
       <c r="F7"/>
       <c r="G7" t="n">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="H7" t="n">
-        <v>1756746</v>
+        <v>1783779</v>
       </c>
       <c r="I7" t="n">
-        <v>10.667</v>
+        <v>10.831</v>
       </c>
       <c r="J7" t="n">
-        <v>14050</v>
+        <v>13673</v>
       </c>
       <c r="K7" t="n">
-        <v>0.085</v>
+        <v>0.083</v>
       </c>
       <c r="L7" t="n">
-        <v>13864</v>
+        <v>13395</v>
       </c>
       <c r="M7" t="n">
-        <v>0.084</v>
+        <v>0.081</v>
       </c>
       <c r="N7" t="n">
-        <v>0.123</v>
+        <v>0.124</v>
       </c>
       <c r="O7" t="n">
-        <v>8.106</v>
+        <v>8.088</v>
       </c>
       <c r="P7" t="s">
         <v>52</v>
@@ -3094,7 +3087,7 @@
         <v>57</v>
       </c>
       <c r="C8" s="1" t="n">
-        <v>44088</v>
+        <v>44090</v>
       </c>
       <c r="D8" t="s">
         <v>58</v>
@@ -3104,31 +3097,27 @@
       </c>
       <c r="F8"/>
       <c r="G8" t="n">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="H8" t="n">
-        <v>1661933</v>
+        <v>1672256</v>
       </c>
       <c r="I8" t="n">
-        <v>175.879</v>
-      </c>
-      <c r="J8" t="n">
-        <v>7315</v>
-      </c>
-      <c r="K8" t="n">
-        <v>0.774</v>
-      </c>
+        <v>176.971</v>
+      </c>
+      <c r="J8"/>
+      <c r="K8"/>
       <c r="L8" t="n">
-        <v>10098</v>
+        <v>9530</v>
       </c>
       <c r="M8" t="n">
-        <v>1.069</v>
+        <v>1.009</v>
       </c>
       <c r="N8" t="n">
-        <v>0.019</v>
+        <v>0.02</v>
       </c>
       <c r="O8" t="n">
-        <v>53.795</v>
+        <v>49.635</v>
       </c>
       <c r="P8" t="s">
         <v>59</v>
@@ -3151,7 +3140,7 @@
         <v>63</v>
       </c>
       <c r="C9" s="1" t="n">
-        <v>44088</v>
+        <v>44090</v>
       </c>
       <c r="D9" t="s">
         <v>64</v>
@@ -3161,31 +3150,31 @@
       </c>
       <c r="F9"/>
       <c r="G9" t="n">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="H9" t="n">
-        <v>2674780</v>
+        <v>2767873</v>
       </c>
       <c r="I9" t="n">
-        <v>230.791</v>
+        <v>238.824</v>
       </c>
       <c r="J9" t="n">
-        <v>16259</v>
+        <v>36381</v>
       </c>
       <c r="K9" t="n">
-        <v>1.403</v>
+        <v>3.139</v>
       </c>
       <c r="L9" t="n">
-        <v>28528</v>
+        <v>31864</v>
       </c>
       <c r="M9" t="n">
-        <v>2.462</v>
+        <v>2.749</v>
       </c>
       <c r="N9" t="n">
-        <v>0.028</v>
+        <v>0.031</v>
       </c>
       <c r="O9" t="n">
-        <v>36.151</v>
+        <v>32.448</v>
       </c>
       <c r="P9" t="s">
         <v>65</v>
@@ -3208,7 +3197,7 @@
         <v>69</v>
       </c>
       <c r="C10" s="1" t="n">
-        <v>44088</v>
+        <v>44090</v>
       </c>
       <c r="D10" t="s">
         <v>70</v>
@@ -3218,31 +3207,31 @@
       </c>
       <c r="F10"/>
       <c r="G10" t="n">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="H10" t="n">
-        <v>273036</v>
+        <v>277645</v>
       </c>
       <c r="I10" t="n">
-        <v>23.39</v>
+        <v>23.785</v>
       </c>
       <c r="J10" t="n">
-        <v>1513</v>
+        <v>1684</v>
       </c>
       <c r="K10" t="n">
-        <v>0.13</v>
+        <v>0.144</v>
       </c>
       <c r="L10" t="n">
-        <v>2650</v>
+        <v>2533</v>
       </c>
       <c r="M10" t="n">
-        <v>0.227</v>
+        <v>0.217</v>
       </c>
       <c r="N10" t="n">
-        <v>0.325</v>
+        <v>0.337</v>
       </c>
       <c r="O10" t="n">
-        <v>3.08</v>
+        <v>2.966</v>
       </c>
       <c r="P10" t="s">
         <v>45</v>
@@ -3316,7 +3305,7 @@
         <v>81</v>
       </c>
       <c r="C12" s="1" t="n">
-        <v>44089</v>
+        <v>44092</v>
       </c>
       <c r="D12" t="s">
         <v>82</v>
@@ -3326,31 +3315,27 @@
       </c>
       <c r="F12"/>
       <c r="G12" t="n">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="H12" t="n">
-        <v>472132</v>
+        <v>482823</v>
       </c>
       <c r="I12" t="n">
-        <v>67.948</v>
-      </c>
-      <c r="J12" t="n">
-        <v>7475</v>
-      </c>
-      <c r="K12" t="n">
-        <v>1.076</v>
-      </c>
+        <v>69.486</v>
+      </c>
+      <c r="J12"/>
+      <c r="K12"/>
       <c r="L12" t="n">
-        <v>3690</v>
+        <v>3060</v>
       </c>
       <c r="M12" t="n">
-        <v>0.531</v>
+        <v>0.44</v>
       </c>
       <c r="N12" t="n">
-        <v>0.035</v>
+        <v>0.044</v>
       </c>
       <c r="O12" t="n">
-        <v>28.23</v>
+        <v>22.643</v>
       </c>
       <c r="P12" t="s">
         <v>84</v>
@@ -3373,7 +3358,7 @@
         <v>87</v>
       </c>
       <c r="C13" s="1" t="n">
-        <v>44090</v>
+        <v>44092</v>
       </c>
       <c r="D13" t="s">
         <v>88</v>
@@ -3383,31 +3368,31 @@
       </c>
       <c r="F13"/>
       <c r="G13" t="n">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="H13" t="n">
-        <v>6292160</v>
+        <v>6422063</v>
       </c>
       <c r="I13" t="n">
-        <v>166.714</v>
+        <v>170.156</v>
       </c>
       <c r="J13" t="n">
-        <v>56695</v>
+        <v>67482</v>
       </c>
       <c r="K13" t="n">
-        <v>1.502</v>
+        <v>1.788</v>
       </c>
       <c r="L13" t="n">
-        <v>57291</v>
+        <v>63214</v>
       </c>
       <c r="M13" t="n">
-        <v>1.518</v>
+        <v>1.675</v>
       </c>
       <c r="N13" t="n">
         <v>0.013</v>
       </c>
       <c r="O13" t="n">
-        <v>79.335</v>
+        <v>74.457</v>
       </c>
       <c r="P13" t="s">
         <v>89</v>
@@ -3430,7 +3415,7 @@
         <v>92</v>
       </c>
       <c r="C14" s="1" t="n">
-        <v>44089</v>
+        <v>44091</v>
       </c>
       <c r="D14" t="s">
         <v>93</v>
@@ -3442,31 +3427,31 @@
         <v>94</v>
       </c>
       <c r="G14" t="n">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="H14" t="n">
-        <v>2887903</v>
+        <v>2942651</v>
       </c>
       <c r="I14" t="n">
-        <v>151.071</v>
+        <v>153.935</v>
       </c>
       <c r="J14" t="n">
-        <v>27197</v>
+        <v>31646</v>
       </c>
       <c r="K14" t="n">
-        <v>1.423</v>
+        <v>1.655</v>
       </c>
       <c r="L14" t="n">
-        <v>31191</v>
+        <v>31852</v>
       </c>
       <c r="M14" t="n">
-        <v>1.632</v>
+        <v>1.666</v>
       </c>
       <c r="N14" t="n">
-        <v>0.056</v>
+        <v>0.055</v>
       </c>
       <c r="O14" t="n">
-        <v>17.957</v>
+        <v>18.186</v>
       </c>
       <c r="P14" t="s">
         <v>95</v>
@@ -3595,7 +3580,7 @@
         <v>111</v>
       </c>
       <c r="C17" s="1" t="n">
-        <v>44089</v>
+        <v>44091</v>
       </c>
       <c r="D17" t="s">
         <v>112</v>
@@ -3605,31 +3590,31 @@
       </c>
       <c r="F17"/>
       <c r="G17" t="n">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="H17" t="n">
-        <v>144759</v>
+        <v>147565</v>
       </c>
       <c r="I17" t="n">
-        <v>5.488</v>
+        <v>5.594</v>
       </c>
       <c r="J17" t="n">
-        <v>1098</v>
+        <v>1253</v>
       </c>
       <c r="K17" t="n">
-        <v>0.042</v>
+        <v>0.048</v>
       </c>
       <c r="L17" t="n">
-        <v>1355</v>
+        <v>1378</v>
       </c>
       <c r="M17" t="n">
-        <v>0.051</v>
+        <v>0.052</v>
       </c>
       <c r="N17" t="n">
-        <v>0.038</v>
+        <v>0.033</v>
       </c>
       <c r="O17" t="n">
-        <v>25.986</v>
+        <v>30.429</v>
       </c>
       <c r="P17" t="s">
         <v>113</v>
@@ -3652,7 +3637,7 @@
         <v>117</v>
       </c>
       <c r="C18" s="1" t="n">
-        <v>44090</v>
+        <v>44092</v>
       </c>
       <c r="D18" t="s">
         <v>118</v>
@@ -3662,31 +3647,31 @@
       </c>
       <c r="F18"/>
       <c r="G18" t="n">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="H18" t="n">
-        <v>236938</v>
+        <v>249023</v>
       </c>
       <c r="I18" t="n">
-        <v>57.716</v>
+        <v>60.659</v>
       </c>
       <c r="J18" t="n">
-        <v>6353</v>
+        <v>6137</v>
       </c>
       <c r="K18" t="n">
-        <v>1.548</v>
+        <v>1.495</v>
       </c>
       <c r="L18" t="n">
-        <v>5114</v>
+        <v>5460</v>
       </c>
       <c r="M18" t="n">
-        <v>1.246</v>
+        <v>1.33</v>
       </c>
       <c r="N18" t="n">
-        <v>0.041</v>
+        <v>0.036</v>
       </c>
       <c r="O18" t="n">
-        <v>24.452</v>
+        <v>28.062</v>
       </c>
       <c r="P18" t="s">
         <v>119</v>
@@ -3709,7 +3694,7 @@
         <v>123</v>
       </c>
       <c r="C19" s="1" t="n">
-        <v>44088</v>
+        <v>44090</v>
       </c>
       <c r="D19" t="s">
         <v>124</v>
@@ -3721,31 +3706,31 @@
         <v>126</v>
       </c>
       <c r="G19" t="n">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="H19" t="n">
-        <v>500285</v>
+        <v>515969</v>
       </c>
       <c r="I19" t="n">
-        <v>44.169</v>
+        <v>45.554</v>
       </c>
       <c r="J19" t="n">
-        <v>7758</v>
+        <v>7745</v>
       </c>
       <c r="K19" t="n">
-        <v>0.685</v>
+        <v>0.684</v>
       </c>
       <c r="L19" t="n">
-        <v>7644</v>
+        <v>7668</v>
       </c>
       <c r="M19" t="n">
-        <v>0.675</v>
+        <v>0.677</v>
       </c>
       <c r="N19" t="n">
-        <v>0.007</v>
+        <v>0.008</v>
       </c>
       <c r="O19" t="n">
-        <v>142.688</v>
+        <v>126</v>
       </c>
       <c r="P19" t="s">
         <v>125</v>
@@ -3768,7 +3753,7 @@
         <v>130</v>
       </c>
       <c r="C20" s="1" t="n">
-        <v>44088</v>
+        <v>44090</v>
       </c>
       <c r="D20" t="s">
         <v>131</v>
@@ -3778,31 +3763,31 @@
       </c>
       <c r="F20"/>
       <c r="G20" t="n">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="H20" t="n">
-        <v>1086466</v>
+        <v>1123221</v>
       </c>
       <c r="I20" t="n">
-        <v>101.454</v>
+        <v>104.886</v>
       </c>
       <c r="J20" t="n">
-        <v>15678</v>
+        <v>17890</v>
       </c>
       <c r="K20" t="n">
-        <v>1.464</v>
+        <v>1.671</v>
       </c>
       <c r="L20" t="n">
-        <v>14592</v>
+        <v>15333</v>
       </c>
       <c r="M20" t="n">
-        <v>1.363</v>
+        <v>1.432</v>
       </c>
       <c r="N20" t="n">
-        <v>0.079</v>
+        <v>0.084</v>
       </c>
       <c r="O20" t="n">
-        <v>12.717</v>
+        <v>11.901</v>
       </c>
       <c r="P20" t="s">
         <v>45</v>
@@ -3825,7 +3810,7 @@
         <v>135</v>
       </c>
       <c r="C21" s="1" t="n">
-        <v>44088</v>
+        <v>44090</v>
       </c>
       <c r="D21" t="s">
         <v>136</v>
@@ -3835,27 +3820,27 @@
       </c>
       <c r="F21"/>
       <c r="G21" t="n">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="H21"/>
       <c r="I21"/>
       <c r="J21" t="n">
-        <v>189</v>
+        <v>313</v>
       </c>
       <c r="K21" t="n">
-        <v>0.002</v>
+        <v>0.003</v>
       </c>
       <c r="L21" t="n">
-        <v>224</v>
+        <v>244</v>
       </c>
       <c r="M21" t="n">
         <v>0.003</v>
       </c>
       <c r="N21" t="n">
-        <v>0.115</v>
+        <v>0.064</v>
       </c>
       <c r="O21" t="n">
-        <v>8.711</v>
+        <v>15.527</v>
       </c>
       <c r="P21" t="s">
         <v>137</v>
@@ -3878,7 +3863,7 @@
         <v>141</v>
       </c>
       <c r="C22" s="1" t="n">
-        <v>44088</v>
+        <v>44090</v>
       </c>
       <c r="D22" t="s">
         <v>142</v>
@@ -3888,31 +3873,31 @@
       </c>
       <c r="F22"/>
       <c r="G22" t="n">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="H22" t="n">
-        <v>3026103</v>
+        <v>3134355</v>
       </c>
       <c r="I22" t="n">
-        <v>522.444</v>
+        <v>541.133</v>
       </c>
       <c r="J22" t="n">
-        <v>7674</v>
+        <v>7630</v>
       </c>
       <c r="K22" t="n">
-        <v>1.325</v>
+        <v>1.317</v>
       </c>
       <c r="L22" t="n">
-        <v>39892</v>
+        <v>41478</v>
       </c>
       <c r="M22" t="n">
-        <v>6.887</v>
+        <v>7.161</v>
       </c>
       <c r="N22" t="n">
         <v>0.006</v>
       </c>
       <c r="O22" t="n">
-        <v>167.312</v>
+        <v>163.76</v>
       </c>
       <c r="P22" t="s">
         <v>143</v>
@@ -3992,7 +3977,7 @@
         <v>153</v>
       </c>
       <c r="C24" s="1" t="n">
-        <v>44089</v>
+        <v>44091</v>
       </c>
       <c r="D24" t="s">
         <v>154</v>
@@ -4004,25 +3989,25 @@
         <v>156</v>
       </c>
       <c r="G24" t="n">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="H24" t="n">
-        <v>297387</v>
+        <v>308927</v>
       </c>
       <c r="I24" t="n">
-        <v>16.856</v>
+        <v>17.51</v>
       </c>
       <c r="J24" t="n">
-        <v>2013</v>
+        <v>6330</v>
       </c>
       <c r="K24" t="n">
-        <v>0.114</v>
+        <v>0.359</v>
       </c>
       <c r="L24" t="n">
-        <v>3164</v>
+        <v>3858</v>
       </c>
       <c r="M24" t="n">
-        <v>0.179</v>
+        <v>0.219</v>
       </c>
       <c r="N24"/>
       <c r="O24"/>
@@ -4047,7 +4032,7 @@
         <v>160</v>
       </c>
       <c r="C25" s="1" t="n">
-        <v>44088</v>
+        <v>44090</v>
       </c>
       <c r="D25" t="s">
         <v>161</v>
@@ -4057,31 +4042,31 @@
       </c>
       <c r="F25"/>
       <c r="G25" t="n">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="H25" t="n">
-        <v>352379</v>
+        <v>357309</v>
       </c>
       <c r="I25" t="n">
-        <v>54.327</v>
+        <v>55.088</v>
       </c>
       <c r="J25" t="n">
-        <v>2481</v>
+        <v>2430</v>
       </c>
       <c r="K25" t="n">
-        <v>0.383</v>
+        <v>0.375</v>
       </c>
       <c r="L25" t="n">
-        <v>2469</v>
+        <v>2473</v>
       </c>
       <c r="M25" t="n">
         <v>0.381</v>
       </c>
       <c r="N25" t="n">
-        <v>0.041</v>
+        <v>0.038</v>
       </c>
       <c r="O25" t="n">
-        <v>24.655</v>
+        <v>26.551</v>
       </c>
       <c r="P25" t="s">
         <v>162</v>
@@ -4104,7 +4089,7 @@
         <v>166</v>
       </c>
       <c r="C26" s="1" t="n">
-        <v>44089</v>
+        <v>44091</v>
       </c>
       <c r="D26" t="s">
         <v>167</v>
@@ -4114,31 +4099,31 @@
       </c>
       <c r="F26"/>
       <c r="G26" t="n">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="H26" t="n">
-        <v>177504</v>
+        <v>182635</v>
       </c>
       <c r="I26" t="n">
-        <v>133.81</v>
+        <v>137.678</v>
       </c>
       <c r="J26" t="n">
-        <v>2432</v>
+        <v>2178</v>
       </c>
       <c r="K26" t="n">
-        <v>1.833</v>
+        <v>1.642</v>
       </c>
       <c r="L26" t="n">
-        <v>1934</v>
+        <v>2134</v>
       </c>
       <c r="M26" t="n">
-        <v>1.458</v>
+        <v>1.609</v>
       </c>
       <c r="N26" t="n">
-        <v>0.012</v>
+        <v>0.011</v>
       </c>
       <c r="O26" t="n">
-        <v>81.066</v>
+        <v>87.357</v>
       </c>
       <c r="P26" t="s">
         <v>169</v>
@@ -4161,7 +4146,7 @@
         <v>174</v>
       </c>
       <c r="C27" s="1" t="n">
-        <v>44087</v>
+        <v>44091</v>
       </c>
       <c r="D27" t="s">
         <v>175</v>
@@ -4171,31 +4156,31 @@
       </c>
       <c r="F27"/>
       <c r="G27" t="n">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="H27" t="n">
-        <v>1138012</v>
+        <v>1176252</v>
       </c>
       <c r="I27" t="n">
-        <v>9.899</v>
+        <v>10.232</v>
       </c>
       <c r="J27" t="n">
-        <v>7162</v>
+        <v>10605</v>
       </c>
       <c r="K27" t="n">
-        <v>0.062</v>
+        <v>0.092</v>
       </c>
       <c r="L27" t="n">
-        <v>13430</v>
+        <v>9394</v>
       </c>
       <c r="M27" t="n">
-        <v>0.117</v>
+        <v>0.082</v>
       </c>
       <c r="N27" t="n">
-        <v>0.068</v>
+        <v>0.069</v>
       </c>
       <c r="O27" t="n">
-        <v>14.639</v>
+        <v>14.535</v>
       </c>
       <c r="P27" t="s">
         <v>176</v>
@@ -4218,7 +4203,7 @@
         <v>180</v>
       </c>
       <c r="C28" s="1" t="n">
-        <v>44082</v>
+        <v>44091</v>
       </c>
       <c r="D28" t="s">
         <v>181</v>
@@ -4228,32 +4213,30 @@
       </c>
       <c r="F28"/>
       <c r="G28" t="n">
-        <v>172</v>
+        <v>181</v>
       </c>
       <c r="H28" t="n">
-        <v>9076</v>
+        <v>9806</v>
       </c>
       <c r="I28" t="n">
-        <v>10.124</v>
+        <v>10.939</v>
       </c>
       <c r="J28" t="n">
-        <v>171</v>
+        <v>53</v>
       </c>
       <c r="K28" t="n">
-        <v>0.191</v>
+        <v>0.059</v>
       </c>
       <c r="L28" t="n">
-        <v>93</v>
+        <v>77</v>
       </c>
       <c r="M28" t="n">
-        <v>0.104</v>
+        <v>0.086</v>
       </c>
       <c r="N28" t="n">
-        <v>0.005</v>
-      </c>
-      <c r="O28" t="n">
-        <v>217</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="O28"/>
       <c r="P28" t="s">
         <v>182</v>
       </c>
@@ -4275,7 +4258,7 @@
         <v>185</v>
       </c>
       <c r="C29" s="1" t="n">
-        <v>44089</v>
+        <v>44090</v>
       </c>
       <c r="D29" t="s">
         <v>186</v>
@@ -4285,31 +4268,31 @@
       </c>
       <c r="F29"/>
       <c r="G29" t="n">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="H29" t="n">
-        <v>837074</v>
+        <v>865336</v>
       </c>
       <c r="I29" t="n">
-        <v>151.077</v>
+        <v>156.178</v>
       </c>
       <c r="J29" t="n">
-        <v>593</v>
+        <v>11531</v>
       </c>
       <c r="K29" t="n">
-        <v>0.107</v>
+        <v>2.081</v>
       </c>
       <c r="L29" t="n">
-        <v>8152</v>
+        <v>10095</v>
       </c>
       <c r="M29" t="n">
-        <v>1.471</v>
+        <v>1.822</v>
       </c>
       <c r="N29" t="n">
         <v>0.005</v>
       </c>
       <c r="O29" t="n">
-        <v>190.213</v>
+        <v>182.126</v>
       </c>
       <c r="P29" t="s">
         <v>188</v>
@@ -4332,7 +4315,7 @@
         <v>191</v>
       </c>
       <c r="C30" s="1" t="n">
-        <v>44085</v>
+        <v>44088</v>
       </c>
       <c r="D30" t="s">
         <v>192</v>
@@ -4342,27 +4325,27 @@
       </c>
       <c r="F30"/>
       <c r="G30" t="n">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="H30"/>
       <c r="I30"/>
       <c r="J30" t="n">
-        <v>167377</v>
+        <v>168483</v>
       </c>
       <c r="K30" t="n">
-        <v>2.564</v>
+        <v>2.581</v>
       </c>
       <c r="L30" t="n">
-        <v>144610</v>
+        <v>148347</v>
       </c>
       <c r="M30" t="n">
-        <v>2.215</v>
+        <v>2.273</v>
       </c>
       <c r="N30" t="n">
-        <v>0.053</v>
+        <v>0.054</v>
       </c>
       <c r="O30" t="n">
-        <v>18.828</v>
+        <v>18.439</v>
       </c>
       <c r="P30" t="s">
         <v>193</v>
@@ -4440,7 +4423,7 @@
         <v>201</v>
       </c>
       <c r="C32" s="1" t="n">
-        <v>44080</v>
+        <v>44087</v>
       </c>
       <c r="D32" t="s">
         <v>202</v>
@@ -4452,27 +4435,27 @@
         <v>204</v>
       </c>
       <c r="G32" t="n">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H32" t="n">
-        <v>13436301</v>
+        <v>14557136</v>
       </c>
       <c r="I32" t="n">
-        <v>160.368</v>
+        <v>173.746</v>
       </c>
       <c r="J32"/>
       <c r="K32"/>
       <c r="L32" t="n">
-        <v>150161</v>
+        <v>160119</v>
       </c>
       <c r="M32" t="n">
-        <v>1.792</v>
+        <v>1.911</v>
       </c>
       <c r="N32" t="n">
         <v>0.008</v>
       </c>
       <c r="O32" t="n">
-        <v>127.968</v>
+        <v>118.695</v>
       </c>
       <c r="P32" t="s">
         <v>203</v>
@@ -4495,7 +4478,7 @@
         <v>209</v>
       </c>
       <c r="C33" s="1" t="n">
-        <v>44085</v>
+        <v>44087</v>
       </c>
       <c r="D33" t="s">
         <v>210</v>
@@ -4505,31 +4488,31 @@
       </c>
       <c r="F33"/>
       <c r="G33" t="n">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="H33" t="n">
-        <v>454912</v>
+        <v>457092</v>
       </c>
       <c r="I33" t="n">
-        <v>14.64</v>
+        <v>14.71</v>
       </c>
       <c r="J33" t="n">
-        <v>810</v>
+        <v>1043</v>
       </c>
       <c r="K33" t="n">
-        <v>0.026</v>
+        <v>0.034</v>
       </c>
       <c r="L33" t="n">
-        <v>870</v>
+        <v>889</v>
       </c>
       <c r="M33" t="n">
-        <v>0.028</v>
+        <v>0.029</v>
       </c>
       <c r="N33" t="n">
-        <v>0.099</v>
+        <v>0.106</v>
       </c>
       <c r="O33" t="n">
-        <v>10.15</v>
+        <v>9.472</v>
       </c>
       <c r="P33" t="s">
         <v>212</v>
@@ -4552,7 +4535,7 @@
         <v>216</v>
       </c>
       <c r="C34" s="1" t="n">
-        <v>44088</v>
+        <v>44092</v>
       </c>
       <c r="D34" t="s">
         <v>217</v>
@@ -4562,31 +4545,31 @@
       </c>
       <c r="F34"/>
       <c r="G34" t="n">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="H34" t="n">
-        <v>1133027</v>
+        <v>1170292</v>
       </c>
       <c r="I34" t="n">
-        <v>108.704</v>
+        <v>112.279</v>
       </c>
       <c r="J34" t="n">
-        <v>7145</v>
+        <v>12395</v>
       </c>
       <c r="K34" t="n">
-        <v>0.685</v>
+        <v>1.189</v>
       </c>
       <c r="L34" t="n">
-        <v>14412</v>
+        <v>10848</v>
       </c>
       <c r="M34" t="n">
-        <v>1.383</v>
+        <v>1.041</v>
       </c>
       <c r="N34" t="n">
-        <v>0.017</v>
+        <v>0.026</v>
       </c>
       <c r="O34" t="n">
-        <v>58.79</v>
+        <v>38.982</v>
       </c>
       <c r="P34" t="s">
         <v>219</v>
@@ -4658,7 +4641,7 @@
         <v>230</v>
       </c>
       <c r="C36" s="1" t="n">
-        <v>44090</v>
+        <v>44092</v>
       </c>
       <c r="D36" t="s">
         <v>231</v>
@@ -4670,31 +4653,31 @@
         <v>233</v>
       </c>
       <c r="G36" t="n">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="H36" t="n">
-        <v>567691</v>
+        <v>591618</v>
       </c>
       <c r="I36" t="n">
-        <v>58.765</v>
+        <v>61.242</v>
       </c>
       <c r="J36" t="n">
-        <v>9827</v>
+        <v>11546</v>
       </c>
       <c r="K36" t="n">
-        <v>1.017</v>
+        <v>1.195</v>
       </c>
       <c r="L36" t="n">
-        <v>10316</v>
+        <v>10628</v>
       </c>
       <c r="M36" t="n">
-        <v>1.068</v>
+        <v>1.1</v>
       </c>
       <c r="N36" t="n">
-        <v>0.071</v>
+        <v>0.08</v>
       </c>
       <c r="O36" t="n">
-        <v>14.005</v>
+        <v>12.567</v>
       </c>
       <c r="P36" t="s">
         <v>232</v>
@@ -4717,7 +4700,7 @@
         <v>238</v>
       </c>
       <c r="C37" s="1" t="n">
-        <v>44088</v>
+        <v>44091</v>
       </c>
       <c r="D37" t="s">
         <v>239</v>
@@ -4727,31 +4710,31 @@
       </c>
       <c r="F37"/>
       <c r="G37" t="n">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="H37" t="n">
-        <v>97035</v>
+        <v>102080</v>
       </c>
       <c r="I37" t="n">
-        <v>284.352</v>
+        <v>299.136</v>
       </c>
       <c r="J37" t="n">
-        <v>479</v>
+        <v>3104</v>
       </c>
       <c r="K37" t="n">
-        <v>1.404</v>
+        <v>9.096</v>
       </c>
       <c r="L37" t="n">
-        <v>477</v>
+        <v>942</v>
       </c>
       <c r="M37" t="n">
-        <v>1.398</v>
+        <v>2.76</v>
       </c>
       <c r="N37" t="n">
-        <v>0.007</v>
+        <v>0.005</v>
       </c>
       <c r="O37" t="n">
-        <v>139.125</v>
+        <v>183.167</v>
       </c>
       <c r="P37" t="s">
         <v>240</v>
@@ -4833,7 +4816,7 @@
         <v>248</v>
       </c>
       <c r="C39" s="1" t="n">
-        <v>44089</v>
+        <v>44091</v>
       </c>
       <c r="D39" t="s">
         <v>244</v>
@@ -4845,31 +4828,31 @@
         <v>246</v>
       </c>
       <c r="G39" t="n">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="H39" t="n">
-        <v>59429115</v>
+        <v>61572343</v>
       </c>
       <c r="I39" t="n">
-        <v>43.064</v>
+        <v>44.617</v>
       </c>
       <c r="J39" t="n">
-        <v>1116842</v>
+        <v>1006615</v>
       </c>
       <c r="K39" t="n">
-        <v>0.809</v>
+        <v>0.729</v>
       </c>
       <c r="L39" t="n">
-        <v>1089205</v>
+        <v>1067767</v>
       </c>
       <c r="M39" t="n">
-        <v>0.789</v>
+        <v>0.774</v>
       </c>
       <c r="N39" t="n">
-        <v>0.085</v>
+        <v>0.087</v>
       </c>
       <c r="O39" t="n">
-        <v>11.733</v>
+        <v>11.457</v>
       </c>
       <c r="P39" t="s">
         <v>245</v>
@@ -4892,7 +4875,7 @@
         <v>250</v>
       </c>
       <c r="C40" s="1" t="n">
-        <v>44089</v>
+        <v>44092</v>
       </c>
       <c r="D40" t="s">
         <v>251</v>
@@ -4902,31 +4885,31 @@
       </c>
       <c r="F40"/>
       <c r="G40" t="n">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="H40" t="n">
-        <v>1592056</v>
+        <v>1652324</v>
       </c>
       <c r="I40" t="n">
-        <v>5.821</v>
+        <v>6.041</v>
       </c>
       <c r="J40" t="n">
-        <v>42704</v>
+        <v>29555</v>
       </c>
       <c r="K40" t="n">
-        <v>0.156</v>
+        <v>0.108</v>
       </c>
       <c r="L40" t="n">
-        <v>23723</v>
+        <v>26054</v>
       </c>
       <c r="M40" t="n">
-        <v>0.087</v>
+        <v>0.095</v>
       </c>
       <c r="N40" t="n">
-        <v>0.148</v>
+        <v>0.139</v>
       </c>
       <c r="O40" t="n">
-        <v>6.769</v>
+        <v>7.173</v>
       </c>
       <c r="P40" t="s">
         <v>252</v>
@@ -4949,7 +4932,7 @@
         <v>256</v>
       </c>
       <c r="C41" s="1" t="n">
-        <v>44088</v>
+        <v>44090</v>
       </c>
       <c r="D41" t="s">
         <v>257</v>
@@ -4959,31 +4942,27 @@
       </c>
       <c r="F41"/>
       <c r="G41" t="n">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="H41" t="n">
-        <v>3586848</v>
+        <v>3641581</v>
       </c>
       <c r="I41" t="n">
-        <v>42.704</v>
-      </c>
-      <c r="J41" t="n">
-        <v>27283</v>
-      </c>
-      <c r="K41" t="n">
-        <v>0.325</v>
-      </c>
+        <v>43.356</v>
+      </c>
+      <c r="J41"/>
+      <c r="K41"/>
       <c r="L41" t="n">
-        <v>25828</v>
+        <v>26263</v>
       </c>
       <c r="M41" t="n">
-        <v>0.308</v>
+        <v>0.313</v>
       </c>
       <c r="N41" t="n">
-        <v>0.085</v>
+        <v>0.088</v>
       </c>
       <c r="O41" t="n">
-        <v>11.762</v>
+        <v>11.32</v>
       </c>
       <c r="P41" t="s">
         <v>258</v>
@@ -5006,7 +4985,7 @@
         <v>262</v>
       </c>
       <c r="C42" s="1" t="n">
-        <v>44089</v>
+        <v>44091</v>
       </c>
       <c r="D42" t="s">
         <v>263</v>
@@ -5016,31 +4995,31 @@
       </c>
       <c r="F42"/>
       <c r="G42" t="n">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="H42" t="n">
-        <v>1948531</v>
+        <v>1998295</v>
       </c>
       <c r="I42" t="n">
-        <v>48.444</v>
+        <v>49.681</v>
       </c>
       <c r="J42" t="n">
-        <v>22141</v>
+        <v>25206</v>
       </c>
       <c r="K42" t="n">
-        <v>0.55</v>
+        <v>0.627</v>
       </c>
       <c r="L42" t="n">
-        <v>22580</v>
+        <v>22483</v>
       </c>
       <c r="M42" t="n">
-        <v>0.561</v>
+        <v>0.559</v>
       </c>
       <c r="N42" t="n">
-        <v>0.188</v>
+        <v>0.186</v>
       </c>
       <c r="O42" t="n">
-        <v>5.305</v>
+        <v>5.383</v>
       </c>
       <c r="P42" t="s">
         <v>265</v>
@@ -5063,7 +5042,7 @@
         <v>269</v>
       </c>
       <c r="C43" s="1" t="n">
-        <v>44089</v>
+        <v>44091</v>
       </c>
       <c r="D43" t="s">
         <v>270</v>
@@ -5073,31 +5052,31 @@
       </c>
       <c r="F43"/>
       <c r="G43" t="n">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="H43" t="n">
-        <v>989406</v>
+        <v>1016310</v>
       </c>
       <c r="I43" t="n">
-        <v>200.374</v>
+        <v>205.823</v>
       </c>
       <c r="J43" t="n">
-        <v>8120</v>
+        <v>14663</v>
       </c>
       <c r="K43" t="n">
-        <v>1.644</v>
+        <v>2.97</v>
       </c>
       <c r="L43" t="n">
-        <v>10891</v>
+        <v>11433</v>
       </c>
       <c r="M43" t="n">
-        <v>2.206</v>
+        <v>2.315</v>
       </c>
       <c r="N43" t="n">
-        <v>0.019</v>
+        <v>0.02</v>
       </c>
       <c r="O43" t="n">
-        <v>53.764</v>
+        <v>48.949</v>
       </c>
       <c r="P43" t="s">
         <v>271</v>
@@ -5120,7 +5099,7 @@
         <v>275</v>
       </c>
       <c r="C44" s="1" t="n">
-        <v>44082</v>
+        <v>44085</v>
       </c>
       <c r="D44" t="s">
         <v>276</v>
@@ -5130,31 +5109,31 @@
       </c>
       <c r="F44"/>
       <c r="G44" t="n">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="H44" t="n">
-        <v>2724185</v>
+        <v>2862734</v>
       </c>
       <c r="I44" t="n">
-        <v>314.733</v>
+        <v>330.74</v>
       </c>
       <c r="J44" t="n">
-        <v>45675</v>
+        <v>43704</v>
       </c>
       <c r="K44" t="n">
-        <v>5.277</v>
+        <v>5.049</v>
       </c>
       <c r="L44" t="n">
-        <v>32214</v>
+        <v>37372</v>
       </c>
       <c r="M44" t="n">
-        <v>3.722</v>
+        <v>4.318</v>
       </c>
       <c r="N44" t="n">
-        <v>0.08</v>
+        <v>0.081</v>
       </c>
       <c r="O44" t="n">
-        <v>12.519</v>
+        <v>12.292</v>
       </c>
       <c r="P44" t="s">
         <v>45</v>
@@ -5177,7 +5156,7 @@
         <v>281</v>
       </c>
       <c r="C45" s="1" t="n">
-        <v>44089</v>
+        <v>44091</v>
       </c>
       <c r="D45" t="s">
         <v>282</v>
@@ -5189,22 +5168,22 @@
         <v>284</v>
       </c>
       <c r="G45" t="n">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="H45" t="n">
-        <v>6006675</v>
+        <v>6127243</v>
       </c>
       <c r="I45" t="n">
-        <v>99.347</v>
+        <v>101.341</v>
       </c>
       <c r="J45" t="n">
-        <v>50504</v>
+        <v>62451</v>
       </c>
       <c r="K45" t="n">
-        <v>0.835</v>
+        <v>1.033</v>
       </c>
       <c r="L45" t="n">
-        <v>52859</v>
+        <v>52822</v>
       </c>
       <c r="M45" t="n">
         <v>0.874</v>
@@ -5213,7 +5192,7 @@
         <v>0.027</v>
       </c>
       <c r="O45" t="n">
-        <v>37.087</v>
+        <v>37.504</v>
       </c>
       <c r="P45" t="s">
         <v>285</v>
@@ -5236,7 +5215,7 @@
         <v>288</v>
       </c>
       <c r="C46" s="1" t="n">
-        <v>44089</v>
+        <v>44091</v>
       </c>
       <c r="D46" t="s">
         <v>282</v>
@@ -5248,31 +5227,31 @@
         <v>284</v>
       </c>
       <c r="G46" t="n">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="H46" t="n">
-        <v>9943944</v>
+        <v>10146324</v>
       </c>
       <c r="I46" t="n">
-        <v>164.466</v>
+        <v>167.814</v>
       </c>
       <c r="J46" t="n">
-        <v>80517</v>
+        <v>101773</v>
       </c>
       <c r="K46" t="n">
-        <v>1.332</v>
+        <v>1.683</v>
       </c>
       <c r="L46" t="n">
-        <v>82819</v>
+        <v>84562</v>
       </c>
       <c r="M46" t="n">
-        <v>1.37</v>
+        <v>1.399</v>
       </c>
       <c r="N46" t="n">
         <v>0.017</v>
       </c>
       <c r="O46" t="n">
-        <v>58.107</v>
+        <v>60.04</v>
       </c>
       <c r="P46" t="s">
         <v>285</v>
@@ -5295,7 +5274,7 @@
         <v>291</v>
       </c>
       <c r="C47" s="1" t="n">
-        <v>44089</v>
+        <v>44091</v>
       </c>
       <c r="D47" t="s">
         <v>292</v>
@@ -5307,31 +5286,31 @@
         <v>294</v>
       </c>
       <c r="G47" t="n">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="H47" t="n">
-        <v>1745311</v>
+        <v>1786342</v>
       </c>
       <c r="I47" t="n">
-        <v>13.799</v>
+        <v>14.124</v>
       </c>
       <c r="J47" t="n">
-        <v>27256</v>
+        <v>19864</v>
       </c>
       <c r="K47" t="n">
-        <v>0.216</v>
+        <v>0.157</v>
       </c>
       <c r="L47" t="n">
-        <v>17595</v>
+        <v>17750</v>
       </c>
       <c r="M47" t="n">
-        <v>0.139</v>
+        <v>0.14</v>
       </c>
       <c r="N47" t="n">
         <v>0.03</v>
       </c>
       <c r="O47" t="n">
-        <v>33.073</v>
+        <v>32.801</v>
       </c>
       <c r="P47" t="s">
         <v>295</v>
@@ -5354,7 +5333,7 @@
         <v>298</v>
       </c>
       <c r="C48" s="1" t="n">
-        <v>44086</v>
+        <v>44089</v>
       </c>
       <c r="D48" t="s">
         <v>299</v>
@@ -5366,31 +5345,31 @@
         <v>300</v>
       </c>
       <c r="G48" t="n">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="H48" t="n">
-        <v>2125808</v>
+        <v>2193319</v>
       </c>
       <c r="I48" t="n">
-        <v>16.808</v>
+        <v>17.342</v>
       </c>
       <c r="J48" t="n">
-        <v>17435</v>
+        <v>17949</v>
       </c>
       <c r="K48" t="n">
-        <v>0.138</v>
+        <v>0.142</v>
       </c>
       <c r="L48" t="n">
-        <v>19110</v>
+        <v>20145</v>
       </c>
       <c r="M48" t="n">
-        <v>0.151</v>
+        <v>0.159</v>
       </c>
       <c r="N48" t="n">
-        <v>0.027</v>
+        <v>0.026</v>
       </c>
       <c r="O48" t="n">
-        <v>36.469</v>
+        <v>37.867</v>
       </c>
       <c r="P48" t="s">
         <v>295</v>
@@ -5574,7 +5553,7 @@
         <v>321</v>
       </c>
       <c r="C52" s="1" t="n">
-        <v>44089</v>
+        <v>44091</v>
       </c>
       <c r="D52" t="s">
         <v>322</v>
@@ -5584,31 +5563,31 @@
       </c>
       <c r="F52"/>
       <c r="G52" t="n">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="H52" t="n">
-        <v>684204</v>
+        <v>695556</v>
       </c>
       <c r="I52" t="n">
-        <v>160.214</v>
+        <v>162.872</v>
       </c>
       <c r="J52" t="n">
-        <v>4534</v>
+        <v>5968</v>
       </c>
       <c r="K52" t="n">
-        <v>1.062</v>
+        <v>1.397</v>
       </c>
       <c r="L52" t="n">
-        <v>4444</v>
+        <v>4632</v>
       </c>
       <c r="M52" t="n">
-        <v>1.041</v>
+        <v>1.085</v>
       </c>
       <c r="N52" t="n">
-        <v>0.163</v>
+        <v>0.152</v>
       </c>
       <c r="O52" t="n">
-        <v>6.118</v>
+        <v>6.594</v>
       </c>
       <c r="P52" t="s">
         <v>323</v>
@@ -5631,7 +5610,7 @@
         <v>327</v>
       </c>
       <c r="C53" s="1" t="n">
-        <v>44090</v>
+        <v>44092</v>
       </c>
       <c r="D53" t="s">
         <v>328</v>
@@ -5643,31 +5622,31 @@
         <v>330</v>
       </c>
       <c r="G53" t="n">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="H53" t="n">
-        <v>285876</v>
+        <v>290907</v>
       </c>
       <c r="I53" t="n">
-        <v>151.562</v>
+        <v>154.229</v>
       </c>
       <c r="J53" t="n">
-        <v>3041</v>
+        <v>2264</v>
       </c>
       <c r="K53" t="n">
-        <v>1.612</v>
+        <v>1.2</v>
       </c>
       <c r="L53" t="n">
-        <v>2254</v>
+        <v>2297</v>
       </c>
       <c r="M53" t="n">
-        <v>1.195</v>
+        <v>1.218</v>
       </c>
       <c r="N53" t="n">
         <v>0.003</v>
       </c>
       <c r="O53" t="n">
-        <v>315.56</v>
+        <v>349.543</v>
       </c>
       <c r="P53" t="s">
         <v>329</v>
@@ -5690,7 +5669,7 @@
         <v>333</v>
       </c>
       <c r="C54" s="1" t="n">
-        <v>44087</v>
+        <v>44090</v>
       </c>
       <c r="D54" t="s">
         <v>334</v>
@@ -5700,31 +5679,31 @@
       </c>
       <c r="F54"/>
       <c r="G54" t="n">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="H54" t="n">
-        <v>175384</v>
+        <v>187579</v>
       </c>
       <c r="I54" t="n">
-        <v>25.524</v>
+        <v>27.299</v>
       </c>
       <c r="J54" t="n">
-        <v>3494</v>
+        <v>3971</v>
       </c>
       <c r="K54" t="n">
+        <v>0.578</v>
+      </c>
+      <c r="L54" t="n">
+        <v>3489</v>
+      </c>
+      <c r="M54" t="n">
         <v>0.508</v>
       </c>
-      <c r="L54" t="n">
-        <v>3237</v>
-      </c>
-      <c r="M54" t="n">
-        <v>0.471</v>
-      </c>
       <c r="N54" t="n">
-        <v>0.232</v>
+        <v>0.187</v>
       </c>
       <c r="O54" t="n">
-        <v>4.313</v>
+        <v>5.355</v>
       </c>
       <c r="P54" t="s">
         <v>335</v>
@@ -5747,7 +5726,7 @@
         <v>338</v>
       </c>
       <c r="C55" s="1" t="n">
-        <v>44090</v>
+        <v>44092</v>
       </c>
       <c r="D55" t="s">
         <v>339</v>
@@ -5757,31 +5736,31 @@
       </c>
       <c r="F55"/>
       <c r="G55" t="n">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="H55" t="n">
-        <v>706219</v>
+        <v>716972</v>
       </c>
       <c r="I55" t="n">
-        <v>259.421</v>
+        <v>263.371</v>
       </c>
       <c r="J55" t="n">
-        <v>6079</v>
+        <v>5864</v>
       </c>
       <c r="K55" t="n">
-        <v>2.233</v>
+        <v>2.154</v>
       </c>
       <c r="L55" t="n">
-        <v>4231</v>
+        <v>4265</v>
       </c>
       <c r="M55" t="n">
-        <v>1.554</v>
+        <v>1.567</v>
       </c>
       <c r="N55" t="n">
-        <v>0.011</v>
+        <v>0.01</v>
       </c>
       <c r="O55" t="n">
-        <v>95.232</v>
+        <v>97.885</v>
       </c>
       <c r="P55" t="s">
         <v>45</v>
@@ -5804,7 +5783,7 @@
         <v>342</v>
       </c>
       <c r="C56" s="1" t="n">
-        <v>44088</v>
+        <v>44090</v>
       </c>
       <c r="D56" t="s">
         <v>343</v>
@@ -5814,31 +5793,31 @@
       </c>
       <c r="F56"/>
       <c r="G56" t="n">
-        <v>201</v>
+        <v>203</v>
       </c>
       <c r="H56" t="n">
-        <v>410867</v>
+        <v>415425</v>
       </c>
       <c r="I56" t="n">
-        <v>656.362</v>
+        <v>663.644</v>
       </c>
       <c r="J56" t="n">
-        <v>1771</v>
+        <v>2046</v>
       </c>
       <c r="K56" t="n">
-        <v>2.829</v>
+        <v>3.268</v>
       </c>
       <c r="L56" t="n">
-        <v>1783</v>
+        <v>1821</v>
       </c>
       <c r="M56" t="n">
-        <v>2.848</v>
+        <v>2.909</v>
       </c>
       <c r="N56" t="n">
         <v>0.024</v>
       </c>
       <c r="O56" t="n">
-        <v>41.883</v>
+        <v>41.119</v>
       </c>
       <c r="P56" t="s">
         <v>344</v>
@@ -5861,7 +5840,7 @@
         <v>347</v>
       </c>
       <c r="C57" s="1" t="n">
-        <v>44087</v>
+        <v>44090</v>
       </c>
       <c r="D57" t="s">
         <v>348</v>
@@ -5871,31 +5850,31 @@
       </c>
       <c r="F57"/>
       <c r="G57" t="n">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="H57" t="n">
-        <v>48556</v>
+        <v>48963</v>
       </c>
       <c r="I57" t="n">
-        <v>2.538</v>
+        <v>2.559</v>
       </c>
       <c r="J57" t="n">
-        <v>443</v>
+        <v>147</v>
       </c>
       <c r="K57" t="n">
-        <v>0.023</v>
+        <v>0.008</v>
       </c>
       <c r="L57" t="n">
-        <v>274</v>
+        <v>230</v>
       </c>
       <c r="M57" t="n">
-        <v>0.014</v>
+        <v>0.012</v>
       </c>
       <c r="N57" t="n">
-        <v>0.035</v>
+        <v>0.044</v>
       </c>
       <c r="O57" t="n">
-        <v>28.627</v>
+        <v>22.676</v>
       </c>
       <c r="P57" t="s">
         <v>349</v>
@@ -5918,7 +5897,7 @@
         <v>353</v>
       </c>
       <c r="C58" s="1" t="n">
-        <v>44089</v>
+        <v>44091</v>
       </c>
       <c r="D58" t="s">
         <v>354</v>
@@ -5930,31 +5909,31 @@
         <v>356</v>
       </c>
       <c r="G58" t="n">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="H58" t="n">
-        <v>1395578</v>
+        <v>1417154</v>
       </c>
       <c r="I58" t="n">
-        <v>43.119</v>
+        <v>43.785</v>
       </c>
       <c r="J58" t="n">
-        <v>11809</v>
+        <v>9895</v>
       </c>
       <c r="K58" t="n">
-        <v>0.365</v>
+        <v>0.306</v>
       </c>
       <c r="L58" t="n">
-        <v>10448</v>
+        <v>10669</v>
       </c>
       <c r="M58" t="n">
-        <v>0.323</v>
+        <v>0.33</v>
       </c>
       <c r="N58" t="n">
-        <v>0.007</v>
+        <v>0.006</v>
       </c>
       <c r="O58" t="n">
-        <v>150.177</v>
+        <v>166.703</v>
       </c>
       <c r="P58" t="s">
         <v>45</v>
@@ -5977,7 +5956,7 @@
         <v>360</v>
       </c>
       <c r="C59" s="1" t="n">
-        <v>44088</v>
+        <v>44090</v>
       </c>
       <c r="D59" t="s">
         <v>361</v>
@@ -5987,31 +5966,31 @@
       </c>
       <c r="F59"/>
       <c r="G59" t="n">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="H59" t="n">
-        <v>131623</v>
+        <v>134520</v>
       </c>
       <c r="I59" t="n">
-        <v>243.502</v>
+        <v>248.861</v>
       </c>
       <c r="J59" t="n">
-        <v>1267</v>
+        <v>1640</v>
       </c>
       <c r="K59" t="n">
-        <v>2.344</v>
+        <v>3.034</v>
       </c>
       <c r="L59" t="n">
-        <v>1354</v>
+        <v>1365</v>
       </c>
       <c r="M59" t="n">
-        <v>2.505</v>
+        <v>2.525</v>
       </c>
       <c r="N59" t="n">
-        <v>0.062</v>
+        <v>0.061</v>
       </c>
       <c r="O59" t="n">
-        <v>16.092</v>
+        <v>16.278</v>
       </c>
       <c r="P59" t="s">
         <v>363</v>
@@ -6068,7 +6047,7 @@
         <v>0.015</v>
       </c>
       <c r="O60" t="n">
-        <v>66.704</v>
+        <v>65.661</v>
       </c>
       <c r="P60" t="s">
         <v>369</v>
@@ -6091,7 +6070,7 @@
         <v>373</v>
       </c>
       <c r="C61" s="1" t="n">
-        <v>44083</v>
+        <v>44085</v>
       </c>
       <c r="D61" t="s">
         <v>374</v>
@@ -6101,31 +6080,31 @@
       </c>
       <c r="F61"/>
       <c r="G61" t="n">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="H61" t="n">
-        <v>1433043</v>
+        <v>1459919</v>
       </c>
       <c r="I61" t="n">
-        <v>11.115</v>
+        <v>11.323</v>
       </c>
       <c r="J61" t="n">
-        <v>12232</v>
+        <v>10485</v>
       </c>
       <c r="K61" t="n">
-        <v>0.095</v>
+        <v>0.081</v>
       </c>
       <c r="L61" t="n">
-        <v>11098</v>
+        <v>10643</v>
       </c>
       <c r="M61" t="n">
-        <v>0.086</v>
+        <v>0.083</v>
       </c>
       <c r="N61" t="n">
-        <v>0.474</v>
+        <v>0.476</v>
       </c>
       <c r="O61" t="n">
-        <v>2.11</v>
+        <v>2.1</v>
       </c>
       <c r="P61" t="s">
         <v>376</v>
@@ -6148,7 +6127,7 @@
         <v>380</v>
       </c>
       <c r="C62" s="1" t="n">
-        <v>44088</v>
+        <v>44090</v>
       </c>
       <c r="D62" t="s">
         <v>381</v>
@@ -6158,31 +6137,31 @@
       </c>
       <c r="F62"/>
       <c r="G62" t="n">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="H62" t="n">
-        <v>2251763</v>
+        <v>2295811</v>
       </c>
       <c r="I62" t="n">
-        <v>61.006</v>
+        <v>62.199</v>
       </c>
       <c r="J62" t="n">
-        <v>21694</v>
+        <v>21769</v>
       </c>
       <c r="K62" t="n">
-        <v>0.588</v>
+        <v>0.59</v>
       </c>
       <c r="L62" t="n">
-        <v>22782</v>
+        <v>22521</v>
       </c>
       <c r="M62" t="n">
-        <v>0.617</v>
+        <v>0.61</v>
       </c>
       <c r="N62" t="n">
-        <v>0.09</v>
+        <v>0.093</v>
       </c>
       <c r="O62" t="n">
-        <v>11.158</v>
+        <v>10.796</v>
       </c>
       <c r="P62" t="s">
         <v>382</v>
@@ -6205,7 +6184,7 @@
         <v>386</v>
       </c>
       <c r="C63" s="1" t="n">
-        <v>44089</v>
+        <v>44091</v>
       </c>
       <c r="D63" t="s">
         <v>387</v>
@@ -6215,31 +6194,31 @@
       </c>
       <c r="F63"/>
       <c r="G63" t="n">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="H63" t="n">
-        <v>117029</v>
+        <v>119689</v>
       </c>
       <c r="I63" t="n">
-        <v>3.744</v>
+        <v>3.829</v>
       </c>
       <c r="J63" t="n">
-        <v>1441</v>
+        <v>1032</v>
       </c>
       <c r="K63" t="n">
-        <v>0.046</v>
+        <v>0.033</v>
       </c>
       <c r="L63" t="n">
-        <v>1421</v>
+        <v>1563</v>
       </c>
       <c r="M63" t="n">
-        <v>0.045</v>
+        <v>0.05</v>
       </c>
       <c r="N63" t="n">
-        <v>0.093</v>
+        <v>0.112</v>
       </c>
       <c r="O63" t="n">
-        <v>10.754</v>
+        <v>8.895</v>
       </c>
       <c r="P63" t="s">
         <v>388</v>
@@ -6319,7 +6298,7 @@
         <v>399</v>
       </c>
       <c r="C65" s="1" t="n">
-        <v>44089</v>
+        <v>44091</v>
       </c>
       <c r="D65" t="s">
         <v>400</v>
@@ -6329,31 +6308,31 @@
       </c>
       <c r="F65"/>
       <c r="G65" t="n">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="H65" t="n">
-        <v>861780</v>
+        <v>882915</v>
       </c>
       <c r="I65" t="n">
-        <v>29.577</v>
+        <v>30.302</v>
       </c>
       <c r="J65" t="n">
-        <v>10375</v>
+        <v>10641</v>
       </c>
       <c r="K65" t="n">
-        <v>0.356</v>
+        <v>0.365</v>
       </c>
       <c r="L65" t="n">
-        <v>10515</v>
+        <v>10347</v>
       </c>
       <c r="M65" t="n">
-        <v>0.361</v>
+        <v>0.355</v>
       </c>
       <c r="N65" t="n">
-        <v>0.11</v>
+        <v>0.126</v>
       </c>
       <c r="O65" t="n">
-        <v>9.095</v>
+        <v>7.952</v>
       </c>
       <c r="P65" t="s">
         <v>401</v>
@@ -6376,7 +6355,7 @@
         <v>405</v>
       </c>
       <c r="C66" s="1" t="n">
-        <v>44080</v>
+        <v>44087</v>
       </c>
       <c r="D66" t="s">
         <v>406</v>
@@ -6386,27 +6365,27 @@
       </c>
       <c r="F66"/>
       <c r="G66" t="n">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="H66" t="n">
-        <v>1832451</v>
+        <v>2042887</v>
       </c>
       <c r="I66" t="n">
-        <v>106.943</v>
+        <v>119.224</v>
       </c>
       <c r="J66"/>
       <c r="K66"/>
       <c r="L66" t="n">
-        <v>23292</v>
+        <v>26138</v>
       </c>
       <c r="M66" t="n">
-        <v>1.359</v>
+        <v>1.525</v>
       </c>
       <c r="N66" t="n">
-        <v>0.026</v>
+        <v>0.039</v>
       </c>
       <c r="O66" t="n">
-        <v>38.572</v>
+        <v>25.6</v>
       </c>
       <c r="P66" t="s">
         <v>408</v>
@@ -6429,7 +6408,7 @@
         <v>412</v>
       </c>
       <c r="C67" s="1" t="n">
-        <v>44089</v>
+        <v>44091</v>
       </c>
       <c r="D67" t="s">
         <v>413</v>
@@ -6439,31 +6418,31 @@
       </c>
       <c r="F67"/>
       <c r="G67" t="n">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="H67" t="n">
-        <v>881532</v>
+        <v>897077</v>
       </c>
       <c r="I67" t="n">
-        <v>182.806</v>
+        <v>186.029</v>
       </c>
       <c r="J67" t="n">
-        <v>9088</v>
+        <v>7360</v>
       </c>
       <c r="K67" t="n">
-        <v>1.885</v>
+        <v>1.526</v>
       </c>
       <c r="L67" t="n">
-        <v>7145</v>
+        <v>6951</v>
       </c>
       <c r="M67" t="n">
-        <v>1.482</v>
+        <v>1.441</v>
       </c>
       <c r="N67" t="n">
         <v>0</v>
       </c>
       <c r="O67" t="n">
-        <v>2632.368</v>
+        <v>2862.176</v>
       </c>
       <c r="P67" t="s">
         <v>414</v>
@@ -6486,7 +6465,7 @@
         <v>417</v>
       </c>
       <c r="C68" s="1" t="n">
-        <v>44089</v>
+        <v>44092</v>
       </c>
       <c r="D68" t="s">
         <v>418</v>
@@ -6496,31 +6475,27 @@
       </c>
       <c r="F68"/>
       <c r="G68" t="n">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="H68" t="n">
-        <v>443987</v>
+        <v>482321</v>
       </c>
       <c r="I68" t="n">
-        <v>2.154</v>
-      </c>
-      <c r="J68" t="n">
-        <v>1912</v>
-      </c>
-      <c r="K68" t="n">
-        <v>0.009</v>
-      </c>
+        <v>2.34</v>
+      </c>
+      <c r="J68"/>
+      <c r="K68"/>
       <c r="L68" t="n">
-        <v>2455</v>
+        <v>6584</v>
       </c>
       <c r="M68" t="n">
-        <v>0.012</v>
+        <v>0.032</v>
       </c>
       <c r="N68" t="n">
-        <v>0.071</v>
+        <v>0.02</v>
       </c>
       <c r="O68" t="n">
-        <v>13.994</v>
+        <v>50.87</v>
       </c>
       <c r="P68" t="s">
         <v>419</v>
@@ -6543,7 +6518,7 @@
         <v>423</v>
       </c>
       <c r="C69" s="1" t="n">
-        <v>44088</v>
+        <v>44090</v>
       </c>
       <c r="D69" t="s">
         <v>424</v>
@@ -6553,31 +6528,31 @@
       </c>
       <c r="F69"/>
       <c r="G69" t="n">
-        <v>204</v>
+        <v>206</v>
       </c>
       <c r="H69" t="n">
-        <v>878415</v>
+        <v>919134</v>
       </c>
       <c r="I69" t="n">
-        <v>162.032</v>
+        <v>169.543</v>
       </c>
       <c r="J69" t="n">
-        <v>2575</v>
+        <v>11297</v>
       </c>
       <c r="K69" t="n">
-        <v>0.475</v>
+        <v>2.084</v>
       </c>
       <c r="L69" t="n">
-        <v>9179</v>
+        <v>10867</v>
       </c>
       <c r="M69" t="n">
-        <v>1.693</v>
+        <v>2.005</v>
       </c>
       <c r="N69" t="n">
-        <v>0.012</v>
+        <v>0.01</v>
       </c>
       <c r="O69" t="n">
-        <v>86.13</v>
+        <v>100.355</v>
       </c>
       <c r="P69" t="s">
         <v>425</v>
@@ -6645,7 +6620,7 @@
         <v>436</v>
       </c>
       <c r="C71" s="1" t="n">
-        <v>44090</v>
+        <v>44092</v>
       </c>
       <c r="D71" t="s">
         <v>437</v>
@@ -6655,31 +6630,31 @@
       </c>
       <c r="F71"/>
       <c r="G71" t="n">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="H71" t="n">
-        <v>3024987</v>
+        <v>3090660</v>
       </c>
       <c r="I71" t="n">
-        <v>13.694</v>
+        <v>13.992</v>
       </c>
       <c r="J71" t="n">
-        <v>29097</v>
+        <v>33865</v>
       </c>
       <c r="K71" t="n">
-        <v>0.132</v>
+        <v>0.153</v>
       </c>
       <c r="L71" t="n">
-        <v>28564</v>
+        <v>30144</v>
       </c>
       <c r="M71" t="n">
-        <v>0.129</v>
+        <v>0.136</v>
       </c>
       <c r="N71" t="n">
-        <v>0.017</v>
+        <v>0.019</v>
       </c>
       <c r="O71" t="n">
-        <v>58.294</v>
+        <v>52.555</v>
       </c>
       <c r="P71" t="s">
         <v>438</v>
@@ -6702,7 +6677,7 @@
         <v>441</v>
       </c>
       <c r="C72" s="1" t="n">
-        <v>44088</v>
+        <v>44090</v>
       </c>
       <c r="D72" t="s">
         <v>442</v>
@@ -6712,31 +6687,31 @@
       </c>
       <c r="F72"/>
       <c r="G72" t="n">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="H72" t="n">
-        <v>398522</v>
+        <v>408715</v>
       </c>
       <c r="I72" t="n">
-        <v>92.362</v>
+        <v>94.725</v>
       </c>
       <c r="J72" t="n">
-        <v>2875</v>
+        <v>5453</v>
       </c>
       <c r="K72" t="n">
-        <v>0.666</v>
+        <v>1.264</v>
       </c>
       <c r="L72" t="n">
-        <v>4664</v>
+        <v>4688</v>
       </c>
       <c r="M72" t="n">
-        <v>1.081</v>
+        <v>1.087</v>
       </c>
       <c r="N72" t="n">
-        <v>0.144</v>
+        <v>0.135</v>
       </c>
       <c r="O72" t="n">
-        <v>6.943</v>
+        <v>7.416</v>
       </c>
       <c r="P72" t="s">
         <v>443</v>
@@ -6759,7 +6734,7 @@
         <v>447</v>
       </c>
       <c r="C73" s="1" t="n">
-        <v>44086</v>
+        <v>44090</v>
       </c>
       <c r="D73" t="s">
         <v>448</v>
@@ -6769,31 +6744,31 @@
       </c>
       <c r="F73"/>
       <c r="G73" t="n">
-        <v>188</v>
+        <v>192</v>
       </c>
       <c r="H73" t="n">
-        <v>227011</v>
+        <v>239172</v>
       </c>
       <c r="I73" t="n">
-        <v>31.828</v>
+        <v>33.533</v>
       </c>
       <c r="J73" t="n">
-        <v>3708</v>
+        <v>3552</v>
       </c>
       <c r="K73" t="n">
-        <v>0.52</v>
+        <v>0.498</v>
       </c>
       <c r="L73" t="n">
-        <v>2933</v>
+        <v>3076</v>
       </c>
       <c r="M73" t="n">
-        <v>0.411</v>
+        <v>0.431</v>
       </c>
       <c r="N73" t="n">
-        <v>0.285</v>
+        <v>0.236</v>
       </c>
       <c r="O73" t="n">
-        <v>3.505</v>
+        <v>4.235</v>
       </c>
       <c r="P73" t="s">
         <v>449</v>
@@ -6869,7 +6844,7 @@
         <v>459</v>
       </c>
       <c r="C75" s="1" t="n">
-        <v>44088</v>
+        <v>44091</v>
       </c>
       <c r="D75" t="s">
         <v>460</v>
@@ -6879,31 +6854,31 @@
       </c>
       <c r="F75"/>
       <c r="G75" t="n">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="H75" t="n">
-        <v>2978859</v>
+        <v>3099796</v>
       </c>
       <c r="I75" t="n">
-        <v>27.184</v>
+        <v>28.288</v>
       </c>
       <c r="J75" t="n">
-        <v>25731</v>
+        <v>36962</v>
       </c>
       <c r="K75" t="n">
-        <v>0.235</v>
+        <v>0.337</v>
       </c>
       <c r="L75" t="n">
-        <v>35544</v>
+        <v>36100</v>
       </c>
       <c r="M75" t="n">
-        <v>0.324</v>
+        <v>0.329</v>
       </c>
       <c r="N75" t="n">
-        <v>0.096</v>
+        <v>0.11</v>
       </c>
       <c r="O75" t="n">
-        <v>10.432</v>
+        <v>9.093</v>
       </c>
       <c r="P75" t="s">
         <v>225</v>
@@ -6926,7 +6901,7 @@
         <v>465</v>
       </c>
       <c r="C76" s="1" t="n">
-        <v>44089</v>
+        <v>44091</v>
       </c>
       <c r="D76" t="s">
         <v>466</v>
@@ -6936,31 +6911,31 @@
       </c>
       <c r="F76"/>
       <c r="G76" t="n">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="H76" t="n">
-        <v>2893600</v>
+        <v>2936840</v>
       </c>
       <c r="I76" t="n">
-        <v>76.456</v>
+        <v>77.599</v>
       </c>
       <c r="J76" t="n">
-        <v>17925</v>
+        <v>21873</v>
       </c>
       <c r="K76" t="n">
-        <v>0.474</v>
+        <v>0.578</v>
       </c>
       <c r="L76" t="n">
-        <v>17713</v>
+        <v>18063</v>
       </c>
       <c r="M76" t="n">
-        <v>0.468</v>
+        <v>0.477</v>
       </c>
       <c r="N76" t="n">
-        <v>0.027</v>
+        <v>0.03</v>
       </c>
       <c r="O76" t="n">
-        <v>36.436</v>
+        <v>33.388</v>
       </c>
       <c r="P76" t="s">
         <v>467</v>
@@ -6983,7 +6958,7 @@
         <v>470</v>
       </c>
       <c r="C77" s="1" t="n">
-        <v>44089</v>
+        <v>44091</v>
       </c>
       <c r="D77" t="s">
         <v>466</v>
@@ -6993,31 +6968,31 @@
       </c>
       <c r="F77"/>
       <c r="G77" t="n">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="H77" t="n">
-        <v>3016740</v>
+        <v>3060844</v>
       </c>
       <c r="I77" t="n">
-        <v>79.71</v>
+        <v>80.875</v>
       </c>
       <c r="J77" t="n">
-        <v>18719</v>
+        <v>22192</v>
       </c>
       <c r="K77" t="n">
-        <v>0.495</v>
+        <v>0.586</v>
       </c>
       <c r="L77" t="n">
-        <v>18237</v>
+        <v>18536</v>
       </c>
       <c r="M77" t="n">
-        <v>0.482</v>
+        <v>0.49</v>
       </c>
       <c r="N77" t="n">
-        <v>0.027</v>
+        <v>0.029</v>
       </c>
       <c r="O77" t="n">
-        <v>37.514</v>
+        <v>34.262</v>
       </c>
       <c r="P77" t="s">
         <v>467</v>
@@ -7040,7 +7015,7 @@
         <v>473</v>
       </c>
       <c r="C78" s="1" t="n">
-        <v>44087</v>
+        <v>44090</v>
       </c>
       <c r="D78" t="s">
         <v>474</v>
@@ -7050,31 +7025,31 @@
       </c>
       <c r="F78"/>
       <c r="G78" t="n">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="H78" t="n">
-        <v>2280220</v>
+        <v>2345680</v>
       </c>
       <c r="I78" t="n">
-        <v>223.623</v>
+        <v>230.043</v>
       </c>
       <c r="J78" t="n">
-        <v>12092</v>
+        <v>23289</v>
       </c>
       <c r="K78" t="n">
-        <v>1.186</v>
+        <v>2.284</v>
       </c>
       <c r="L78" t="n">
-        <v>18149</v>
+        <v>19318</v>
       </c>
       <c r="M78" t="n">
-        <v>1.78</v>
+        <v>1.895</v>
       </c>
       <c r="N78" t="n">
-        <v>0.027</v>
+        <v>0.031</v>
       </c>
       <c r="O78" t="n">
-        <v>37.732</v>
+        <v>32.774</v>
       </c>
       <c r="P78" t="s">
         <v>475</v>
@@ -7097,7 +7072,7 @@
         <v>479</v>
       </c>
       <c r="C79" s="1" t="n">
-        <v>44089</v>
+        <v>44091</v>
       </c>
       <c r="D79" t="s">
         <v>480</v>
@@ -7107,31 +7082,31 @@
       </c>
       <c r="F79"/>
       <c r="G79" t="n">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="H79" t="n">
-        <v>700414</v>
+        <v>709132</v>
       </c>
       <c r="I79" t="n">
-        <v>243.11</v>
+        <v>246.136</v>
       </c>
       <c r="J79" t="n">
-        <v>4987</v>
+        <v>4150</v>
       </c>
       <c r="K79" t="n">
-        <v>1.731</v>
+        <v>1.44</v>
       </c>
       <c r="L79" t="n">
-        <v>4640</v>
+        <v>4709</v>
       </c>
       <c r="M79" t="n">
-        <v>1.611</v>
+        <v>1.634</v>
       </c>
       <c r="N79" t="n">
-        <v>0.05</v>
+        <v>0.049</v>
       </c>
       <c r="O79" t="n">
-        <v>19.963</v>
+        <v>20.563</v>
       </c>
       <c r="P79" t="s">
         <v>482</v>
@@ -7154,7 +7129,7 @@
         <v>485</v>
       </c>
       <c r="C80" s="1" t="n">
-        <v>44089</v>
+        <v>44092</v>
       </c>
       <c r="D80" t="s">
         <v>486</v>
@@ -7164,31 +7139,27 @@
       </c>
       <c r="F80"/>
       <c r="G80" t="n">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="H80" t="n">
-        <v>2110024</v>
+        <v>2185923</v>
       </c>
       <c r="I80" t="n">
-        <v>109.682</v>
-      </c>
-      <c r="J80" t="n">
-        <v>21049</v>
-      </c>
-      <c r="K80" t="n">
-        <v>1.094</v>
-      </c>
+        <v>113.627</v>
+      </c>
+      <c r="J80"/>
+      <c r="K80"/>
       <c r="L80" t="n">
-        <v>20533</v>
+        <v>20572</v>
       </c>
       <c r="M80" t="n">
-        <v>1.067</v>
+        <v>1.069</v>
       </c>
       <c r="N80" t="n">
-        <v>0.058</v>
+        <v>0.063</v>
       </c>
       <c r="O80" t="n">
-        <v>17.338</v>
+        <v>15.99</v>
       </c>
       <c r="P80" t="s">
         <v>488</v>
@@ -7211,7 +7182,7 @@
         <v>492</v>
       </c>
       <c r="C81" s="1" t="n">
-        <v>44089</v>
+        <v>44091</v>
       </c>
       <c r="D81" t="s">
         <v>493</v>
@@ -7221,31 +7192,31 @@
       </c>
       <c r="F81"/>
       <c r="G81" t="n">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="H81" t="n">
-        <v>41424006</v>
+        <v>42095246</v>
       </c>
       <c r="I81" t="n">
-        <v>283.853</v>
+        <v>288.453</v>
       </c>
       <c r="J81" t="n">
-        <v>301699</v>
+        <v>346318</v>
       </c>
       <c r="K81" t="n">
-        <v>2.067</v>
+        <v>2.373</v>
       </c>
       <c r="L81" t="n">
-        <v>304976</v>
+        <v>311817</v>
       </c>
       <c r="M81" t="n">
-        <v>2.09</v>
+        <v>2.137</v>
       </c>
       <c r="N81" t="n">
-        <v>0.018</v>
+        <v>0.02</v>
       </c>
       <c r="O81" t="n">
-        <v>56.732</v>
+        <v>49.914</v>
       </c>
       <c r="P81" t="s">
         <v>494</v>
@@ -7268,7 +7239,7 @@
         <v>498</v>
       </c>
       <c r="C82" s="1" t="n">
-        <v>44087</v>
+        <v>44091</v>
       </c>
       <c r="D82" t="s">
         <v>499</v>
@@ -7278,31 +7249,31 @@
       </c>
       <c r="F82"/>
       <c r="G82" t="n">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="H82" t="n">
-        <v>462896</v>
+        <v>470218</v>
       </c>
       <c r="I82" t="n">
-    